<commit_message>
Added thumbnails and show filter
</commit_message>
<xml_diff>
--- a/Excels/maha.xlsx
+++ b/Excels/maha.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="286">
   <si>
     <t>SHOT NAME</t>
   </si>
@@ -680,6 +680,126 @@
   </si>
   <si>
     <t>Kickback</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8abMlyXEldo57RGTe5S219o5uNLqxENuAgEQah1rGNN/0W/VFkplkM5KNGSGTNBwaZzjkcAHRaHY30NW1vf3em5kR7q4PcR9mfoOswuyVlVW9lzdfpof78XOOB/BmvVlv1pv1Zr1Zb9ab9Wa9WW/Wm/VmvVlv1pv1Zr1Zb9ab9Wa9WW/W/98XH5yfgRTAAsIgZBiyR7g7wPAIggCA418ZBCMgQhUB6e4ASCZVVYJ0D/dwN3MI4RHhgf7D4eYAHBFERNhhmt2j5PzowVkz2+12DiiFQjMzczMTldUwmBkQ7h7AvLQkCoRFJJHz81Nv7fp2F4BqalYJEaGItNZElRFzraQkZTiqexbVLKusqqlFuAOkWSOQc4JHKala7Hb7lDVpSimZRYQDiAiPiIAQAANBEIGgI0ihgIEAhQigfx2fXgRFSFAU63HYHyZzjwBJEuYhoLn1RwrAPURIhAUIijCiXy9IRJAMsyADoIoEAw4/fg9ImlvUqkkfnq6HkkkgUJu1ZhYYc0oJ7oiARyDg4f2j+60HYqrh4NJaKfmwnxAegHsAQQgVbiE8RlQPFwadIaBHmLX0i5//TFUQpIgqk6ac1S08IhARIOABId3dA6JQqChTSjkJwFprsxBlTqqaANTWmnn4MUoDYe7ov7PV1sLd3F0Y8Pnly5fjsPrWB+/98HufJIlvXr7+8ndfHw6TEEtrdanTPEfg9GTDiGbVA24xzRMDc2vzvGzWq5/++A8S4jdf/nZezCKWWpNqKcNSFzNbDYO5X19fj6tVSWle6n6aTjeb9Xq1WZe3zk9q8OLuoEyAVzMVnIzDdrt+eXn3/OWr1TiWYRiHMRwiDHirbuHmnlVBuvWoO0aSiggZwQBIgPBmHqGqPTxyUhA5yel2dXN3Zx4IiAiJWtvSGjyomlMiUGsVVcICKkI3Z9+jfox10mv1iFChqCrh7s2j3xhF6rK0wz4JvvXuo4/eeTwOOavU2mqzpTrJzSpL/6kWzQ2BHmAWCItAvLient8ulze3w1hsMZEgxcyaOSmCcDcKCZBCiocDXBZLCebRrKaT7SYlBaR/C0mzVsack7hHa9bzh1DGIZFSsopQVBFxu5tAFoq4K6kqFDG3COlbSUgPTyI5FzDcXETIZibT4WACRtmePIDPh2l+eXl1vl2/89bT65tra2bekmpepZzEmi/zMpZ0mBZrzcybO8LdkETc2n4/vfv04bfeffrrL595jdPtRihLayWXYVvcmi91WI1jGVIiSDdLOaWcLTgt7dHDU1XZTbZalVbb7jBvt2NKeVnqalyVomMZkqbQntw1JbiHuQsZgIsDICIAChkIgMAx4wUkCwIkRCSAQCgJ8m4/kZKLKCUJwoEId3eGiKhQVJKKhQtTTqm2FmTP0wG02gBQWNQgwnBNqdYG2rokIMzDLCK5lozw569vc8rfevtRyTqOukJEMBBmnpN6+FCYlO7eAogQTevNWTk5Pb/cv/qLv6L7vJ9y1qEUTbk1W+YKBOAqiQKCFBHSQ9xRWQFZrwZg1B//8AdUVVUVmoVZM0dt1QzNqpkHgqSQKQsAd68W87xMS3MPd4+g8FguazMzB0UEbhGMJKRqhFs1j/BwVenbxZuBsIAty+7u+vnLV89evNodJglfalNhfyXubmal5KePH758feXehBSRJJnKpCmJHOblwfmDzXqIZh5B0SBySsMwpKQEzH1IOciccrgDQSFFFJzMzGMsueQ0TQsYp+uyGjeXt7vLyytVEdFhKKICkAL2wtjLGkNACIFwgAABEWGAQgpFBD2rgSDB4497OEHAhVBNgjAPd4sISUmoZLh3vBHwQGCuc2u1v6pwRLgIw+HhItisBqEEkFVEJCLce0aFW4s2M0SEu8Nc3XfTcnmzu7zZ3+7n3X65Pcyvr3eHqTaz2/18fTtd7Q67KuPZ0/H8oUtJJe+ndnV705aKiJyyB8zM3RgURqD/OhQChJBLrSTee+ftIZdWWzrMNReIBI61mYEgpTVTZSn5PpbQmpt7BFXYH3Kv33aEJR4WFAEY8CQqRcy8WpNAhDerHS40gIicc4Rf39wgIudSD4tNu2mabm5uH5yepISUy1DyNC8imhRnpycWzghhEmWWBEGzhIiUxOr8zcuLb7335N13ngAvX91NKkKylOTuaRhIEZXpMJchuxs4hruA0zJrk+vAtCxnm/XpZlzaMg7jblpeX1w2D0XwiDwgpCbtAJMSdCAIEnCAwgDZAayokhASRIQf4QoFcAAeICXiuIFxH2S1WkqyKtk9wAHw8HC3VNTck4t5ABGAmQWRhCmzNTpif1hyViWaA4GkykSztrQgkFNOqs0NwOvL3fX1ncBb85ySmVVrBh00FLBws2BZaxm+enVXyrCbDlfXN8s89c0jIpLEGlrPGwiVTI/+fILseb21Ns3Ts+cvTjabkjW1ZqLiZiRVVEhRxXFfdjgZSYVHQMsOAAPuHiARLiKgqCgl/Ih9SYaIgITQzRDIOS9LrbWmpAFYa/v93W+/+uLk9Pxks+2AWgMRnnN+6/HZ7X5nFjklgA9O128/eVTG7ZA3X3z1JQBRzUkVWLwhaBEXV5fb7eqDtx+9/y7im0uqLrWCSJp7FqFAVeChmkvBstRhTLu7auG3tzfLVOZ5eXx2crZdU/Xq9fX+MB03aEfdAUh04O1uiACPmJtBagj1fhOio3iS7q5K8xASx9THkCCo1JQC4T0QLbyXhQ77IqIXjFbb0owAiVJyq16rIUJEevVM2pG7uPnUGgAVIcI9EAGEua2HAW5Fc23mZhEWhArNDeERdG9zc3hQEICCS7WG5eXFZWvVrBIaR2AAAWs4IiJcQNApRAgFFJhZgO5G8rDfHQ47a6bf+96nSRUkAhRJSftdDsJT5YPE84hNOKxjNZOAkAASmYkHq2Ednj1aWPMA0TvQCHqEm7k7SVD662qtRbib11pbq27mzrPT01yKED39Pn704OmTR9N8MA8lRdnMdnc7i9gddq22Mg7jUHJJZSg5J9WkquGY66KaN5vVdsxzrULW5imre2zWo8OFKsqsOqwGJXNOWRkUa62ZJcBaW2x5cLLJSfaH2dxzSppkyIMmFQokGAyEEITEsRKSgqQqShUBICpyBMVAhAg19QAMTZK0QywCTkTSFBEq2ouy9XrpXpvVZiIsSVNKKtJaMzOhrMaswtqMgJCi0j9JVdZDyTkNRZXSmnmEtdqWVkperVe1LilpbVabh3cWgBQkQoUidICiTgjERfe7Ow8Ljx4gjEhJU8rmHghrrTc6RKhqr9fhTtFlngNOEoHmnt7fiDkdogVnY9oOTCbjOj0+keLp5NylRIKj+W2FC2qDSFRnMrhLGdKwFveaBn99ya++tt+8iOtmEV6roX88hSTgESgl393dXV9f397ePnr48PGjJ69evxZKyqnZAiwI7qb5629elqIn61JbNYu6zLd3u+fP/wnR1tuT1TgmZe+HRUTE1Y+Z5vL6Otwfnp+880gvb3YAg4zOvITkQZVsrQHU9YiIISfs5+1YxjGvhuFmNz178bo2fPTBex+9ry8vr1uziNCsOWezJpqgoZG8kxGBXjR5TOmwCAmKCqJ3hKIi6CBD4UHp6C4Ihjfv9ISKUAAXEkszdyM4lrzUqqpHYgkhZIiqwMwBVxF28iLQu8+UU2ttcVeiNheGMEpKwnY47KdlSQx3J1wlIlhbYwAiRKiC0JRFNeXNyW6/HHb7QBybhQjySJeYmVmNQJIAhO5MqVMh6IjSzNwA6a0xAumHb23yIAVMg6+2sR2DpVmiCJN4yUKyzak51iZ1oorf7R057lAb/GRqKy2ronbIJxk/+aT94KPDX/3H9tcXzay12iDMmnJOAFqrpLbWxjL4uoXHYq21ut8fzs/PNKXsQ2vt5upqNW6//+1Ps+g0T30zqWRHhJkgLNwjNKy/JlECIW5OCQeSllxK1g+/tbWIOs+7/TzX3hkdSRYFF4valo5EET4UdbPVuJxvzhowz75ebT4YN95aRDi1p62cc07JrUag1dqCqlJyLiWJZIvWWojQrJFws+bemiECgCCWdkzwRAQiVASpBVLWQG8zYr2iN29uEZFVSVarAQypqHAsqfNnQri5RYRHKSklInor1kiJcCFK1ub+4uXtPO3CoCoOt2arIYV788iSokeECCKCSCkbcH23H1JRFWnwYyACHtqftXsAm/XGWq7LQjrv+bxerN0jnKpk77mB9Bdf7KQkiWgeCp4JV+GjypCVhVVbDVSLO4spAmDzOLTeykQ4t4JR5wc5np7Jt95FeZD236x/8kOp/7H99QWFrGZuNk0TEYd5Xq9W+90uwkFt5vN82Ky3gNfWRLImICyIBw8fP3zrvVLGCAQipVRyAaVDmaRiDrMFkJJTpxJA5lxUhZICIWAqGhbH5k867hZVmQ77YRgg6q3O8+LuERFuHgF4TlmoAUuaVquNKBFRW02aRUSTTIdDa63jWhIqiYSZUTAOq81mS2J/mK6vr6bDpCm5ORglFwDm3nsoIVurZrYs87K0ed6Hd0K7WbMgSXaA0ZpN89Ra7QkwAiDCXdFZFc+aem1srTara6Fbm+ZZyPBG43ZVVkl9Y0qNMI9OJQsiDLDaHOwh4oichrJep2H49WefL3V2j/su6PjJIuoREiEq1uhRJRiUxI7Z3T06ox6wCEaEuaWrCKlOAOS8zP9wdXl9fdtaWw3Dw0ePtpv1uFor4UBvmxEAExAb4mfRHiMOwL++s7+7w6Nv5GfvLd//+fT6xcmnH40Xh7tfX5l5q4shQlWs2dXV5W6/H4bVfncnKY1loEizenNzs13nNu9JpiQe/s2L50lUcvJm7p5y7jfQ8a/KPW0g7Ll6vVp3fiUAcxOqKkk2M7hTFIyS8tLqMk1aijcHscyz9IJ37KUwjuukApHNap3GOkgex2HwrCkd6ZtogxQExnHIORO4vb0JZPc4OzuTpOFYq+QhL8sSQNZEoarW2nJKDmQVag5vbmbu0zQt8yKqtdZlnnPOFFmvVmY+L9N0mOc6wxmIVhcLWK1LXQDkXODhMKEikHLKpSzzfNhP0zJn1VorGYfdniLuvRzD3cOj821uUduCnndINwM4jGW7HV++vHj56nXAwuPIjSHgXQsB4Hc3VyUPpazD++boQQYEzNCZh073gJpqq6tRa6t1sa+/+op1eVKKbtfrItt5P/iSvTGXKcJTNmIT/ohMYWMp767zl8Pqu1dXnwz5b+f2srZ/9et2+4188rPr8Xzz6bf01xdm1XLWeZ4vXl08eviAdJU0z8t6s9rvlvF0uNvtWp3DvMg6Kftu/dU//O1vPvsHqibVlHLPaghQKSEeXkoBQlNOyt9T8SBTShEhoB9bZjVr5hbu2816NeYXr67MWofwZubmQP//riIxaZKUEG4WolTRlFNJGQKAbr1Ty6QnTQGKQqCdgQeYU+p8BkX7PWsSQiJCyeCx7IQbRJTSJaaIsGbmnpLKkR6IeTostXaUl1IWYa3WO4iUEkVyzsdEROSUV6sVhW2ptVbI71UKWq3jamxmvd/t7GOXwEAwOgtDKkHNWTXp7d1eNYMkNHjsdo5NAulweMB7MEWQhAAeXboiI7zTyU4Xc5AJwbo01bQ+3Y6fDEk4qrooEUKECJOaB90AerN9ShU8Vzzd3Qxz++756s7rzlWUoMwV/+ZiWv7f9OEPWcbV6bB/sSy+tOvrq1cvnyeV1bgqQ94fpmVeSLOwcSizN0ld7gyBuJNi82S5pLZU8uDWkZV3dgoIlSSko8usNEe43Ut6nTFUkErpyRyIy9fSmYgAjk8I4YB0FgLhff/1yx6f7lFLpGj0CiKMiAhHiEiQ2oU5Q/CoAoVHvza65imULofySNd20a9Xxq5byvG+gWNGjhA4CPLIMQVA8MjuCntrJSQl3EFAlOEMuIgKaRYQuHmACNecEWHNgqGU/o/9T0SIaudhUpbtenuYdrvDVOcGBvrV0YlpINyiZzWodkIx7e5uowudIBD9nggA3rVYJdN6vSo593o4jiMQ3m8fEYgGmiMizNC8hkcuqTq+uN3dDOOzzcW//BN59HT4T//XgZ8VIYexLHX+5fXU/rZ9/EfnH7+7+e1fvXLnKDMo87KUYRDIUMpQBvN2e3WThyJELgXH1+eAqkhr1QwpZXd4GBH3Lx0idDejCMKCYeE924HeKT5RmINee8sDIEC2LgehX0CAoHREfVRiDcGuTvuRfEYEKELQ0QBFJ7470PGgUEWDUErSnEoRkbYsyzJ12MdOMQJUjYiIELoFcC9OIgiYx7FXc4muUAVABuiI/vbAYDAiIE4/Sug9oOP3WoMjhEr0u5cueCPC2vJ7J0T11mP5qI4h3HueJYCbq8uIMIeIoHPUfaeRDIjmHkwBB6S2OUKBrme2YFc70XVgHjeOaVL96Y//YCw5JXU3JYexZJUIC/el1m4W6GVrqZXAxdX1PM2rVb68m7g+udzVTz6tkPGDd+O3z2DOzgZdTfHUFzmVz343v/10fbq9fva8jqtVkjKMpbYGi+3JZjockhDwnPTe+hAUNff+wr2r97x/fO4ipCjJRAfZfwwIEQhFBSqiSmGQkgRCqkApwO89BTjaKe4ND92dIGCQXZq978eP+acz+wQYuJeSukruEY7oxbdam+s8tbaEe8+8JDqP0REl2anrLkMFQYfxuIM60EanuXnMD9I/+BhmXc68107v4XnPo7BOQnSGwxFHlr3zHnHvpvgvAuyINfoDpB/jHn7Powg7vOqAggREuwYe7q5HwuZ48/d5gO6obVZR6bYNCMn0wePtarUZx9yZw5ITwGpuZn3zTHX6+89+ZxEl6+5uty75wbq4llXmN68OL15NF6+HfInHP613t3fQE5WUh3yznz7/an73x1XY2iHvXiNpUk2ByCmH3x2mm/B5ux4QvlQLdw8DqCQUBIXt02+9V3IKIIlQ9dXF5WdfPjs/3X743lspSQ+daVn+7rOvzOz9d56+++SBiLq7uX/25Vc3u/nDd54+Oj/pj7U2e/H68vnF9fnJ9t2nj/srj8C01C++fg7gg7eeDEOOiH6FF6+vl7ps1+vzkw0ocHf4NM3Xd1NSOd1ueuIzpzW7O+wADkMuWYkISCCmqTYzInIZBBYUUXGPeVn6u1ZVOEU15VyX2sxAEKK/p3HRJU6Ge6fd7qWrHh8R4WAARzbx2KceNxLvE+ExKI90Sr/ufUbrSVuEEEbvjT2Arn4c62CPZo9IR0qGIhzGNQNmVUSOdinv9g4ngggIo1mIhnl67523y1AAiOg4ZCGXparQ3M2hylbH3c0tI/JquL3dfvL+k+2m/Lu/+c3VPmo1lfKX/3h3Wmz+s8NXv3324Ycf5pzHcUw57eb68s93rfodd+OC7I4I92ZWrc6tLXVBUtGkbtYiyBAGRCK8pHKyXv2zH356thm7jQTg189f/Oar508fP/qTP/yBCN0DwN1+//lvny0LPv3ovZ9+/9tCODjPy9XN9eXNs+9/58PvfvyekgHUVv/uV58/e3X18Qfv/vd//BP3o4vs6ub2q2cvAPzpL/7g0YPTvtmX2v71L//dZ189/9EnH/74+9/uEgjJL373zf/6b/787OHJ//gv/quxlObuFq+vrv6X//P/qWZ/+vMfffv9t1ThTnf/y7/51b//u9+MQ/4Xf/ST7WbsZOx+N/9vf/Zvb+72P/rud37yg496xfOI//Srz//93322Xq/+hz/6yTgOney7uTn82V/8h3lpn3z0/kfvPJWcJMI8Pvvq6998+fX56faHn36kouFmHodp/pt//GJp9tajs7cfPSTZvVmvrm9fvL5crca3HzzowRRAne2bi9cesR7Gk+2qJ6S5Wa317rBEREol4PfY9T7/Hb1lpqLzfDh6Dzt2hDugjOpGSKeWQEkiSSWVcRiH4WhhUY0IixCwtmbNIyuBH33/41JSrSbe5mn39fNXd3c313sxt5vr22Wu8/6wO9xcX158M4yPHj3c7fYi+lmd/9jzutWLea5IJ0RIqnXe3aG1JZzmHt4dhn23AKqArNdrBKhCgKpEJ/253WxONuMRR3SgD65Xw4PT7fXdPmv3fUGBpPLowfmz1zc5JZKak4qkpGenm3EoqrrZrFqt1Rwe41i2q9ECKaWUVFQTmXI6PdmebK43m9V6VYTSs8d2PWxW5WS7PT1ZZ01d2G5tWa/G2vzRg5Pzs60KPQIRZ6fb1apsVqu3njzYrkt3pI3DvF2vzOzpkwdvP3nUtSkVPn95sRrHB6cnH77/dLNed4fk1fXdf/j77bzYh+89/dF3v91/QXffHw7PXlw8ffzgpz/4dtKEAOg3t4fPf/cidocffOf9H3znw6SJjIj463/4p9cX1++/9ei//cWPqN0nyavru//5//i/l9Y++fY7P/vedyI8As3s9m73r375Fy6DJF2WpStnPWMdyTNvgBzLtTBJastivb4CROfLBQEEGL5Zr3/+/e8kMwegOdNNieouwFSrN1NGEcnD0JZ6dXHH8P3+5qtnry6u7273h4vXk5YhpfTsqy9qa96c4PXr10nzdrtJwe95e/c7m59g+Le/vgFXd7vDyqu3enO4TVp6P9eBbcrZaqNqx+gRJCwc82L8LzrxUvIwZHPXlErWYCi0lLTdjLe7vQNJE+gEZcXteuwIfSh5tRrmuaYjrSq7w3R9fZNy2qw2pSiV41gO01JKSZrQ+01KLlqyAuj6LwPBKDmnJDmlLh8pGOAw5KTSPErOHZ4L6V27BTV1Jk8DLkfJEyWn3K1wPAI+R4CSUnfW9C6UIlAR0rabtSq9U8k4Eiin201O+diOQrsnNyd9eLYlnArpZAxlGIbHD8/GcbgHdcg5j+OQS3770YNxLB0tDJGmadaURUutM7stUXtdFESPL4EEgmaWFYLew4AQhDGJmUW4kA4BdTWU9XqVdrfXgyIhm5nbkXSh2XqUcSg5l4vLi/mwWMT19fXXz1+8vLi+ur59/epqqnb+5J0IowoXUPHx++8/fnTy959/JaqPH5//dCxfjRd/+kdPPn+df/fsaj3oPE3m1ZsTJhqd9AxB0mytdeE53A+HnaquhgFwFSWjb6rVWM7PTgnten8nERC63aykE9xwQEAodbNZ9ZeR89FvbeabzabktF6Nm/UmDzmJLs2aISedVESz5tJRsYWXVFQVoOYsgDtEkLN2e7qIJFVjhIeIpCRqUUpOJfE/dxgQ0ZRUNamIUCPCPMw9J3V3B7JIElr4bj9LTwOAeWgSFa3VPCJnVdGcEykINGvNGhHDUMZxII4tabu4qWYgh3G1Wo3eTMsRbibl+ekmpRwMmDswzRUiSTiOo4i4h0iEy7w0SUlSXpaF7ILT0RRMYXRB15tQcxnCJuvdJsO9ezyltQZEHP3lsV6vStZ0ero5OVkDSCHWLGkac4F7yTofdr/98jmIeZ6ePX95dXN7ebN/8fri8uIm3IO6v75o0RAxjPkPf/S9f/6LH1/eXX/21bO6LG+JEvLnfymXfvPkMT//p0PJIozrfVXKPVL1IJRsreJoEw/p/GEAEc1d07FuAgzkp0+f3O2tV00VIEIDTx8/aXIyDiPlXrUPnp2evP/BR7kUdwe8tQby7PTs0+9978F2FWRrvsTRsPTW07eG26n7gY9klcejhw/Sl988OD8lhHRRABjLcHJ6enZylnOiUBDOUE3n5w9XLUrOIsI4GkvPT7cpl6cPH6zHQZN2y+04ls1qNR0OD862R7c+kChjSQh/9PA0AofpcHpyklS7wg33nCVpwlFApLmTPN+uVeQI+UWOXzkNpYimiGhtUc3WTBNPNhth92KQzsM0A+aOnLQLq4gE+FxNJR0d592MeO/r6G0uSTi7897DOvvY+xLvJp3oNEcIxSPOt+uskobVibFrO1wWEzLmA8llxpPz093Vxe+ev7q4vntxcX23O7x49Xp3NwWcQjDm+Y6i29X4z3/x05//5JP1qlgsPfBnipKfDO98+fnFB5+0krtvvnVHDOk8mjgsIplbBLuj4dhxExFRm3f87QERqGqmXbx+2fw75n5PXcZ6Va6uvvnwrZNOckTAw5LqNB2ataTSvfk5JVXb312fFOm5obkjIMB2u5lMOjw7kr3Qk+366dtvr8ZBlYAIKQhROX/weFyNtS1DLsIja1CGdRo6+wGR7qDhyXbz3vvfevutk5y6tY8iouRb77w7Gx6dnxEeHlSJwNn5+Ycfffzh+0+22zUROSlFTrbrzWpdwx+enVC7RdfB/OD8wYNH9e23HmkSd4gee8r3P/iYsNOTbUpJRKZ5bq055fGjpyebkSLsBmDFUFI4t+vxZLvu9pLmLkfTHs1q18Xv+ZDopjQ7zhQ5yE4ydtrcAYQhpLbaDR5k6t7Es5N1Vkl//6tfjVkDNLO51qypmbkFyA8/eO/xyfb2N1988+ry9eXNze3tPBtVEnOnp+gB8r/74z/8r3/23ZKSR6zGYRyHNI7X3r6ZGx+nc+L2pqlwWRpAigIQCAUizJpEpZmat+N8T3ciBDxiXiqPVmkR0BlDTos1uA8lA9F3+2Y13N28Xto7KupuvS1fj+Xu9qLVt6d56bIUkyYK3KZluXfKEWDOmjVevfxG5IdHRywRgZz15Yvn9TvvmXlK7GSCCK9ePz9fvQ0P64RnQMi7m5dTherHrTVSRLzbF37328/ff/T9eVl6qVXVZnbY3+4OtZQPQbh5syYiCb7b77bjOymlgHRJUUQePHpUStmebIQacFAJW9qiSUtKQap2Xh0ivLm+evRg3YNMREdgt9/P8yx0VW1WPUg4ghD58Nufnq5lKAMQzb3X9P20dCPnvTe2k4fwCFEV3ue3ODIjIBEUMOig+FIBJNFe4kk52a4l5fT5P30xlN5xCxnjal1bPRwWEldXL56cbS9u9i9eXt7tDwBzUkMSWGdAhyFd3t2qak7a476Ucl3tXwwAACAASURBVLrd7Cta0v1Sv6g7g/vroZlQHM5EtACFSgo1pwKV7MnNRYgg9Dh+1jyauR6nqoTCcB9XgzsskFOK8D77oUlVOE1LTglUERFKba4i1XwoZalVRJLm6kuE7w8z2AfUjgbrCDdrFq6qEUZoSuGOlPt0Rj7S6wh3F5XeFJNo7goUM1LIGEverIbO8nqguxc1yXpVPNhJpi7eW6vDUNbjqnfajAhi3t8Nw9C9qR4hMJLz4W6zfrAaBhFGqBNwq/PibTo73ZSUOhQMj2q+312++9bJepUF6ozElFKZ5jllXQ2lO5kR2gdhvv76q/d/8skwZLiLiHm4L9Nc+Xudq8P73gZ4T+kMs76fCREVp9N7AyoqMocfNTEgEOuxnGzWqin97utnJWei0xkCiZyKtxaIlOSbr2U3HeapqQioSJE8Uiqa0vc//vDho5P/6X//5cvLK3NkhZNDzg/Pt3cv9naYY9DbG95e355zLcweDhKq7LYXCAWLLaOuyI6LOnksBAMMj2lZIgL3nEIAOaVwP0wL4b0FVOVxdmg3dZ2EQXb/qnC3n6mSQ3MuqliWADAtS3hoUd6PXZqHO6yZKhCpD8mZGcDaTJII1ftQa1itZhEpp2EYprkGXKt1TYKaNaWI8KCELw2iihBJRSkId8RSfalNKKR2XrXr7Xf7qY9LlZz7KIakFB6LeVdCvRt04e7YT0tOKqoUiQghTeJutwP6QJr29AtIAPPSztajJkm5SLcbBffTHK2uV2POCffDnohoZt3KwGOLfV8VeaTPeo9MUVgT1fCgKkC4q0g3YILafU2np5shJ3dP+7v9klNXltw9iYK7XpU1aRIlo0+xiGjOKdzGcfxnP/z0h9/96GZ3N47D85eX89LSZpSAZp6fnnz5Yn8zL7+crFrMdXpW73KWcRy8mQrdDb/XT+7F5eiOny4tSuqJutZ2r/wgABFdjUNE7A5Tn3jRTuwqhTrXpTZbDTmOg20QcneYENCkonrvc8Q0Lc19RRFBN4mK0PpkNPokRAiks5TTtJACQoUhKGUQwjzMfF4WESFVU6YIYRAGNOgEPXCYl+7A65ftlJ9jac1T6libEei+srv91GFDH/Oc9zWpzrWZ95rVOVq6wwP7w0FT6vPYIj1EcHt3IJBy7j2iAO4xTUu1mpP2R02hIMH98uaOlJxz96d4XSLC4bW2e0nuqEt15GJwst9wNLf+iDUlW8zDpXNsfXOym4MB8sHptuQ0L00AiY6GA6BEb0k7YKSqiopoSjnllESE41j+5Bc/+dH3Px6GknIeS351eXNzu+/5huT56UmfGU+pEDGutt47b1I0paNAJqr93UQAmo6lX/q/kxR6xFzNrbMDIqIBpJSFcbubAGhKlN5MiKjMS12qUXgPuAURd/vDYZqPEmOnsihLra1ZH45mBLu5PlDNVFRUc0opHWXveemjbCklSZq6rcrd0WdyBUkTeTRg3BvuRVVzznNtStZmPIJBUlj70CJw/yBEKOZxOBz6d4lqzoOmZN4Ohym8K09HiiQlba3NtZJUFVGNoAVq85u7AxhC2n3fk3M6zDMg4zBoEmuV4ZRw99vdQVXGcUg5r9cnkpSk1da8z9j23X1UdvsXEQhnp/RElOrHIZqjMuvuDutgsYsE52dbFaUwgUd/SJDdoXAUsNhFRQWiz4ACcI/b3bxaDUnp4UqOY7m8unlxcfXk8Wnvq09O1tP+dr/f5ZSHobg1Fe0jVxCklJOj5LEzAPeS8lHQ6PWRxySKeanmfSRCu9Uk56Sq+2nuCY8k+rkKgWmu0zwrN320qO+QeZ7nZTnZrjuh1ZvdZm2aJvNNV2Y6L0zINB/Cq6OfPOC1NkQs89K9qd2evyyzmTdr905lSSUDPLa/gGjqVH5b6jQt0oed+owJCGJeqpv31l9V+nzYNNVqfq9e0xlDKfv94er61qPnGHbRPiD7aa6LyYki0Mz6aQXTvOynidRxKKnrOhaAXd/uOsWdU2qtegQD89wO05KLqohbvbm+UCGJaake3oX0Yw0TRhCgSj8IA93jbR6ENzMhDVRRktYag6LoI28icrLZWIgHkooGJASpi58MpQidTDlrVgn2ssmT7cnff/7baVour3Yff/QOwXX4Zhwc8frytpTS1aFH5yfCaMthbrO3nEsmQjVpErMoObWucwaSjpuxHN3umrq9utP/3S671NY8UkoUJlUyxrGo6m4/eVCF0U9kYLco1/1cJaWOJlQkZ10akqZSSt+SwaqqRNTaNImAPZeICBjLXKML1UcTWwBYWnNzEBYuiHmaAZh30w6EtNamZe6cUWtWknbWybQtSyWlWSWRlORRRAf7MRu9cgdFzJtDiDD3Zkay5LykdnFzh/BlWXa7nVtJmiG4ud17eFJ1dLskvflumpelqWrS1GUDcwuPi6vbCLjHXKsAZpZE7w6HCPYkLWTScHdEzHP1AAWB4PHNH5OAdtMbwmHdk6Y5a6BGJEI1kfdHNFA7lFOVzXokwpyp5A5okES63H5/RVkPWSjteO5Bev+9t3/1xVfV7PmrC3iIIqmuVyXCnj1/3aoNozBivRpOt6vrm/6ybJ6M91PKouGAmYnQnWZG4Wpc7Q+TmiHQKYyjziTSmu8OU7WtHPVcEqByrnVaqiRBgA6SvaoepsUjAJpbhJecZwtJWVRFEJCMWK8G1awplZTBkAAlVFWT1NZKLt0Y5O6aMykAcklJJODeXI7TR33SF06Hw6yJiJjX1u4t0ABiqTXc3EKVqoIABPM8837YXATuJGKaa6sV6OpC923psBpbbaC05qoyDEOfk5qmKdw363E1Dt2c41lx2Ql5GYZcSiGjNV2Webc/eHBclXEYVdisudvt7d7cPBq7CHWkeDDNrTOAmhQux/yF8EBWTUpz+727VkUcSKHgfaFo1hHdUexaDasyGIJEEpWk9CDgSbI7Sk4q7n6PGzvdTLjZOOSXF7vnLy5qaymPqr7dbqz581dXu8M0DNnCc8rbzermdtdJfBEDhCKB6JhEJUnS/ibMvDVLKafWItBH6KXrHaSH397u6uNT6ZNAHojIKc/TMs3zatA+yqx6bOv2h2mZZ0nSlrYscylFl9kDJHvtNiCV7K0tffzJGYxACJk1Wc8xgGR1R+rzxGSfDAin00mWYSR4mBeU7AER2R8makoSd3f7u92ul/7DvJhZKgMimrUI9XB33x+mnAolpnmZ56Wjvd1+J5JUk7nV1ggibFqWudpqtc4ll5JLTkJxRLOQlMdxFM0dNpB6mKu7B2MoQwe+KWO398NUAxjKmIcCjwQsvry+vG5tUU0pJceRggFkN80BmBl7LwMoxcxAalKE/R5lqmozTyrxnxlOCWIoYz/rwSJON9thLEIFWtpsVv3QBEI1abh3Tpy0pKmUtD+EIYCY5mW7Wrm/fvH6crefxyEDWI/Z3C5vbl5dXD882wBISbfbNUKglKAHAx4hAUdQGF0qhnRXsLubaOoMmUj3dvK+YQoPrseBR18y3C0n3e+nCKzHkYpwrMcBgHk7HOYyDCox5iQSXUM095SP3HQIlUKRwzTj2OZS2M+B8lq9p0YSoiRZW23NSOk+UMDNWmvNI1SOUYiganJr7lBlLkUACltPqq05IqechA7tMqsohViPZSjZw8PZzCKCIuMwlJybRUc41bwfECGiokJQAneHwziuy1D6zQrggaU21UTKOJZjLASauYM555PtuqRs4SCSx35eRNJQkjWbl5pTrs2WVm93++gTKhHSPY/uqmoR2otmeJ/9ISUnkuxeAZE+eZ+GMbu7NSsi56cbFQ0EEfIv/5ufn51vlUxJSsk5p3tvtDg4rlddRxTh4TCN4wDi6vb26vquW19W48DAVNuLV1fm3ufxf/jpR7kkdHav+6u8uVu3mKoSAuExeyGg2scsQBxbld6+ALq0KkBKIkA/72NIaoFpmgBXUJWqqSO+m92+tmat1dbMAYaZ76e5kzK9Re9j0/Pc3L3b/NwhFCWnaW7u7HNUpIM5paX1Q7YQQTNfqnU+WVRURQQl8f7sggA4ljyOZSgZ4daBnXmEa0opqYpOtcGPHplShnEYV6vVUt3MImIYy2q1Xq2GMhQQ/dyN3u2RSk0U3d1NzepYSsqaVCVlIXfT4tbc2zjk3io64u7u0EfcctbolUSSgdNsIrJar1brVU652dHR2E9i8zgeIoYOaoEkKSfpAw8qoiknldU4dhFCVErKImytLsvS6uJhJafzs20n8AORzs5OHpxt727vhOJuXbo/8ieI3Ml+DwRrbQ9Ot+GYl3q727daAa7H0eCw9vzV1TxXVQT49NGD9Xq4ubFu9XSGQEQ0pQSQXru5hB1LM4aSyKEu5hFt7uUrADH3eV5EpROADAiZiwjlbj+1Zp2qwJHm7SjHQtEcIkk1R/huP9fWlCIq0XVDTX0jBn9PAEMo+2kKDzOz6HxohKPVNtdWUop+sBw0AtXseLyIB1Ssv5/AUltSpcINOH6bWeuNWnRnwDQtAUfI0WYZAcRuP5m16ACenZqOZWnRz3KT7O7NTMF5abe7PcJTUiL64Rhmbb+bjnaiHjJCGu+miaBISLfCUwPYT8vN3S7Ck0pSEZUMN6cLh5x7fgrRzm32bj+V1AkO1UQRc4eqeaiqgEw6DFmadNMtRZWg8Gy77gfBIZg8eLLdkOIAzI98SXegBlqrOSWvZhGt2ne+/f6TB/94OFSS89xInp1un5yvv35xqcS81KR0YFmWiAg4o5vi+6itlUz8f0y9yY8lSZLmJ5uq2vIW3yIyorIray9WddVweCRA8D/mjXeeSYDAAAQHIAfdnEbXkpUZER6+vMVMVUWEBzFPMk4OhCPiLWamsnzf7yMuxP16hZBioQNiSWm/y73Dy+nSe/NtPUuIcL6utfVtOUtU15ZTQvRl7aqGqOqOiKXktZqqtt4cRJ3U+jQODlBrrbUhETcgkWkcVLu71qaMPU5nJHBCU1uW6uX/xyYgcvB1WYUQ3LQrMjuAqtXW16bkDhuMy6Psa72jgjmsrYEFaRHMVJUBQPt2KQGBqrXWELCbLWvdLhDw3izIAfEo0t7cua5rTqJi1/Oy1tUdhKm3HnZvbf1aKwKJOAJcltCFw/PziZgMNvcokrvb+bL01twV3JZlSakgIZibae09ZloBdHN0diLmkhOYIW8LLkAQETfNKVVomVlE1qqA0URvh8Y0pIAPObj85W8/LGsN+wq+KSMQSBIIs4gkg87kZqr9dLoOQyEefvz89biforf4xT99+Pz4+nw6ffryNJRk7o/PL+fLGoIt8A4gQO7uIgSciQUQRZiFE0sucn93/N1v/unr8/O//Nfvr8sSplQkQKLadVmWklNI8c30/e3x759fi/DaWlNFYiJ6f3/zcvrxuN8ty4qssW3Y76ZhmEpOa2uMpERW22E//9PPfzGOY11XihUxwv1x33s/7Mbe20+iqySspjkPvbVlQdj+f0WCUnJXa2tFBFWchoSAXW0ah+vaCNwRCCBneT7Z7c3O3VttDt7VE5O6z7mA2bLWOLmZqLWWUkpMy3J1JDfV3rcdF8tamywLp3K+XmNF32q7LhVDEKYbYnUsCRCXZTVAVztfVwMIDd+6NseGQNfr0nrX1nNJ1+t1XStLBrDzeb2ubesW6c1oQMBM41jauva2nd9EwEwo1LsJEzGzkGpH5A20R8iESbjVZgi1Nvmf/uf/5bCf7g9TGFPMQ6hiQe8asjBSb2q1mut//i//ulxWVf9f/9P/8Z/+8//NhOZwulwOh92//eX7Hx+fhNncWm/XpSZmD5seAwOLYEoZSHIp79/d5iI5lSFzKWW3m9U853x/t39+ea1VN8kGQFe/XFaCNwsq4DyPx8NtMws4KAm5+mG///CzlIto15CxidBumj98/NYAWm3O4qAcExOWZa1dLfTVAECcfv2b30+7EhiE+KzGMrx7981uEAevrYO5ec8pffPNh8NuIvDWO4J3Bwf68PFbQEop1XWNzp6ZHu7vjPI3D/e1VoBYw8PxuJ+m+WcfH4iwtxaPt/08HXfD8XiTRM6XNTYrzJISvZzqzz++d/fTZRE28zgENWU5nc6+mbhwGAoSf/zwLj72WFkOJdWmH97tCGipqzkyUYgt1PTh9oZYrtcLszryp68vtSsSx+SeAGwDzPA4jLLN/Igw3HVOwjvJG18QvfbOREwbGLjkBA5rbQ6urUnTul4T3lASJuINARfaNdXrWoehiFDrm+egturmzy+L++sbqpCI0VzXupq7GoF1SQnAyQTDdsgYLkaiKC03Fh0QA+JaWyn55rCrtR0Oux9/fApsSjiBL8uahGirhYiZieBaOzMhUm9NzUuW6/W0L4dmJhgfESHa4+OPH2+zmoErEppZb/355el2IjMFpIAoAvjj4+MgN1EGkXl3i79QU42ewgzdDIyIg8q2STMREHG5vJ6WBvbhJ4KGmiERS3HwWhWgmaObm/nd/buhZFUDoCi8Ffz+/mEaS2BLCDEsnQ93D+N8czjs3UF76wba9d37j+Z+3O8lpbou1R3MkeTn3/1ynjjkHyEJZpF3794/3E2IoE0dAJhLybe39wj6/t29mddm9fyacjlfl03GABgGT2YqOX94fyeSaDfe4x2GTx/wy9evQy5JOPQEL8/PvauDO4QeFKYhm2pVM7C1NgGDro0oERESo5kk0R4zZDhdKlLaCjZkkewOQWR2JKDwZ6F2D3M1mCNsTn5CMXdCmHbzz3/2XoS1tcvSEKCrd7WmJoIO2M2uS0PwWpswIjpzcnRhdoDz0sayyaUNiFMWoW62LA1ZGckckKiUDMRhu0RCM01MOSd1c7XqGogwEg6hUYx90YAZmbmUpFtDsDmLDUCE1IPrg9WcAHtXEeEkqp1JIPDQ5pILtx67Iwc3g9pUHRF9qW1zyyF20Nqta2uNNvMaoBLUZpeGwOrg23rRrAd5gTTQvm6WxC9rC7QbM7krIgu5oq1r/8enLze/+ijCRNDV3VSBp6nknDmWnoRmVlu/ubtDrcIC1kWkret6PffegZARjTdrXinDb3/58Vfffatmnz9/bb211pwZCL795h0idesIOAzJ+rifh3WtFH0B4TgkbU0RHLC3KoDcDUpJCNDdEbB3AyDtRmhr7TtzZiIRapqERaR2F4nRbiAFzZQAAV0N0cziZlJTRBrH6Z9//+v37+6017/+7XtVRZanpydiyimLSEg5kqTb447RxyHnkmKwwkxJpHZdumdCdWu91rWVIRvQ0lUcDDeC7jxNTti65pzcVc2A8O724EBNVQjc4/mLD/f3XGRb+wsSkAgfDntJ/99GfDM4IaQgUQmbW12WWquIAMBaq7kxMYA3tXEYkRmIzMARTK2pmcewkAKbAgDu2M0D2hTjOwPovdduQKCq+vaMdPW1NQdARlUj5q5tXdfLdVnW6zyNpr23bfZt6uaG6NNYzA2cET38S+Y9J0Fmwc1Qeb6upr23FVyZMSfRJM+nS/SPyMTGBo6I45g/fvOw243n6/rw7pYAWu+1djWNwVhAGYUI3t3N8/S//e//ZzPLiRFxLjna7FA+i2lv7s+v1/u7HSkYORCphhU0QG1AwrV2TiLupeTeNCYCECplBGRC9G6MZnGOQ8wgEv83v/vN/d1xuV4fv35d10CUAyK6uak2VzNBRFdb1ryfirDsxnJeGhPlnMep3L/7IAlNw/gHw4zp64mIp/3dPBUCrG2V55X5KkTT4eb2ZgeAtdVz/eyAajBMh5wYCK0bXNpQEhGhlDzkWA7Wlyugq6liKqEoNFXDklNgI8dxGN3rOF2b8/UVAFjKMGZCUtVmyziPWcuqrpuMjpvafr8fJ6Mkqo5I5n5du+R0e3tMidfaQhVSW+OUbm9uCHqtPciX5tab5rFQxVCzEFGttXUdh7GU3HoXZkLo6kvt4248tIOI1NYRuqpe1oaMSRKAL+tKAF3NzK5ra62ZWu/dCWOryETmGLeUqjNAjJO+vrwSiwExAgmpIRDt550DLNerIxCLumvTeZ6//dk3f/n+R2JmAhGOy8TMa1MBRwA7na/ffnxw02XtSKS9Y7jy1T3uWjd3ZpF5yC+vF9Q3LImbbzxr37irjqHsYObf//Y3P/twT+BfHx9P52VtyiyqnYBIIJTHyMhEwlxrw6kcdpOq+dPJHIjxuN8/vl6ulxMAqPZ5vnl4d/+H391Qko75XNmgu6Z3H35+fPiQJJehrE6IhGX+5ufH4/tfJOGUGGKiC/BxON48rCXnUmJzj1LgQznMN++J+O64k5RCN/Ih7fPubiz5eHdIwog4qub9w3z3QojvHo6DiKO3plT2157WVn/28cPN7T6qVi7z7rku63p7e3f3/r0wN1V4PiX5CqrzPB9u71ISRHw9XfTvX92VmHeH424eEVBNO7zQ41lEhnE83N4Teav9df1+nMcx8eGwH8exNVXVa/X94UCUHNCRGMmQ6mllZvMQ9RARJYZlXSWl3X5uC6mDYLzdSZ2nhrZ0Ol+ZDRFEZCjpclnMntdW69paqw44DOXurpecP315IvCUc9fu6mY2jmUchthcELPGagfRHMQQyeF0WZ9fL0MmcE8iqgRApk6ITb1kDN9u75BLCgcoAQKQkxGwIUI4yYHBQUEJ+He//tV3P/9AiF+/fj1fLoiJ2RDUzRDIY0ZPmIgR3+iehEVkvxuJ6Pm0EOD5ciWScRqHxN38x0+fP399JAqZsg65SAojBjFy4IMo1B68ieTf0NfhhttkVSJs7mYKtvXwZgboX54vueRwnQC6A68m/3hamISYhJilHG7fO3insiCbeweVefjVb25qWxHw80lTyuBO5fCHP/5JtSHCa3Nb1MEgz7/9/e+0mwhX5K7EjGk6/vnPf2pdmTCVtG5q9Hy4H/95Omj3MuRGhIQ44He/mW/enXaD/OkP/+RO5+v6/HwtuzU9n1+m091xf9xNLIQAw7z4j1+W6/LhZ+9288jEgKBdV/vR/Omwm8f5OE4DODDjx5Tlr9//67//nZlSygCWk4xDAfd/fPqyrish5izXtV4uS8xhvz6+IBkBdfPgaLuZJEbk3ZRu7+920y4JEfH5epUkzAKhHXU1AOhvdN0IRHAz86CzgIOVlCVRUHlCAd9d4U0gG1oyAv/tr37x82+/ySKPXx9fX06tKQkJk7uhu2TilCSHNmcLYUkiSdIwhOAdulpXO59OXXWqQx3HsZR5nj4/PvNWulHvTW3brIXqKxqlyKFx9w3a5Kiu0bbIBijeDPC08Vhwg1MEcsfdQswIQSUNTgq8efnR3AhFJD6f6CxdLUTgYOAplMiEjKweaKI33SCEoIiIMUkuOdvGrvJYTqjGfmGbTsQ8Kjx/TAJAIvTr726TUFeXxDJIu6wdiNP4fNbTeqaQMDAdbu5vbrAhPp4VXCNyYD7c5XFnql9fnr48vTKjSB53+zTshjJKOiMaMw1DSkm0q6tFoYxEQx7MlYhaUzUToqDtxGsNbHQu5f7uUIapA9amCL50l1DfdVWtay8JHM1bzOiISJhq71IrMZla8FFzkt7BXMEAQDflNXoIegDxw8O7P/7uV4f9uC7Xl+fn4M/IVtR3ZCPinJIkTsxRsfE2GPShlHka99Oo2n74/DINBcCu1+uyrK+JEVCYAEGSIKCzl5xd1QCRUH9K+zEDgvCjO4AbJE7gxj9ZDRw26g+GDj6IfBq/Q0xk/bKsLJtC0R3cFQCJ0VS1N8OqncEd0IlYg9mz5TqBEVgH31Ry2/WPmwKHtqQBROW6rtzVrLcQ4eAGgwrx6RZbZAAcqVkA4P6HX3+43adWL1UdzA4j4JHadXn89Hg6L92st46IpQw5yWW5argNCJOEbbi7Uyly3M0kaOaPT09P//43c1/XNbGkBDlJSTSUdFHnRHMuxGxm59PCwvM0PD2dzQ2RIwqDEFJKvWNtDcG72t9/+Fw3XqWt6yrHw46ZAwc8Dqm79WZIhEAezaNjyglCA0iYUjrud62qI7jFb3pXY2YmMvf9vPuPf/ztNKanx8fX89UctHckkiRurm/TvDKUkqXkBAiMyCkJMRFJSlNJOI3Xuh7nce1+XWtXQwDrHApBQOzuJWcH01bjsSTISNaDrc+ICMRhIg+jOpoq4Eb73ZQhvpGqwjUXVzASugGlst9N2tra9E1TShbiCrS5FCAPyR9LoohdwhCrgrkTIrh1MLRwNsStiKoKYIbIhA7YAKD1IKy5GXMKmZqjaY8VdnSPm9YYAQ+74Rff3jOzuTNjyTkxjyXNU769PXz58vLl6fT0fFpqM+2XXjXw+qpjmaZp/Pr01Lshgllf1uqqrfe4OQHcTcuQUkqJcDcXQly47+YpQCiu0E1HFgTMKTFREmbmbBbOx1ap9x6mhErYzRDA3FRN9kNh2fAt69Ki9++tbZoFwrFkbT0uMgZ2giEXpsabYxndrIP3box0mMc//fPvH24P1+vl9XxSxZRy6xciKik9vzzX2sdxSkkO8ziMQ5IQ5BMaRqiROTDz6XL57uP7YRzCIRjDcQePkCtzd3AGACYGiFoxMYYSNA7KkEuqa1ilQ+4C8ZDfTGObqJUDKhj0J3XYSgXbWIngMeB0M+0KBG6O7n17nAe2CXrvBht+LCL0ANG2k9B77+ohkLIIhlLty9LGaUhCARKM79rNkRBQXLZAm3BZuXsnMHNG/+v3n5fabm930zhm4fBDiIzzNN7d7u6/nv72989/+8fn1i1wKyg0TwMRWl+zELpCAH7ciEAybU4dxK66m8dxSKoxQcTSDBAD7L16G0q5vz0SYkqYRESkJCEmd1BVBEo8ZYHarJuhW1cL3Kq083Mn7g7IqdzuwQBJgukW09jW2/mKY87IGGhv0FrP50TECA5QrS8Nkfi4m//bP//x/nZvpo9PLyIFBc2cFhKR0/n8/T8+3d/eJMGg95Qsw5AJycyaNmEW4fPlaqpTSfM8RlUSBb27x0g2Shxi8LdBQgAAIABJREFUNleH0AiH7YfAYVvh0nZSm6pv0YJERBzrCfAwWiQRZmqt19a3EzDEsghmTgiI9KbGo6hBVLWrMmLYijZYg3tUh9tjZ5uAuYUpMKhR/nbdmGrXeJwI8zCOITRS19hMbPk1sN1i5vEkBjPX3omZwAixrv1mx/M4EG0aHge4uZnf3x+//XD35cuHp6fXy6USQTfbIH/45mpAcHMiiDqQokkN45n11vrX51NV09okYDMp+DMY60ERwdolyTQMpQjEuFIoiSCkD/e7sZTWW8iiCOF6WeWy1kC7iKj5zMREKJJy5uW60iYwNkcXJCcSxHEsy+UKDGEPdOckMA7jn//0x3d3h97rpy9fkRMBIdDlciolg/u//Ntf0YAJbvbTtYFqf3l9PZ0IwHa73X43lZSIidDBYRxySiIiiJKKcHgcDYiQmdScEBwTIXY1UwUOFTiJkBt2U1BTpcQozJJRksSh2ZpuZXLoRRBFiCi9FVfm5mpq6MQsjPzmwXHzpg7MzMKMTGQbFm/jW2wAR8A43B18rd3dEN/+AsER1IAI1LbbYF2u+93sjkJJSZHCBIi1KvibL52zRWwTDAFKbl2tt69Pp971eJjneQBENWXGoQz73fD+4fj6enn+erouLeR8seHZ4iMQwshZ11brikS5ZFNrXZfFiPDbj3d/+f7RJBtYLlk4NI9wvixPT685J9W3KKAkLGzdllqdHICeXpfjfro5TFEJudt1rYLEhMDBp3QPQlprHTZeUjRthrgRrIEop4zMgBgrZEQqhf/8pz/87ONdb+uPnx8vVYV5WVvXxkjd7a9//0etbR4mdRxLMfaHm+N+P4R5JphjhCTMKckbk0eIKCdJWbQpIVbtrbsI58StdgdPKZUkkJhJzA3AEbGpiaFxvGxSN1dy0C1/1ry3UGhm0F6bR4nJLE4Rcdg33SWAI6paZP6hQGIBAwtgtgOGjPZtf+Rqb0xX3A47ACLsTZfa3X3IvLUehABkapISM0WMDaEnTlXtulR3ZyJidPXukCnlnAF9KhmZeq3CvAJo1+fnU62t9XkYizAFNI4Yh1LmMd/upqfn8/PrNZSMGgMIB3NLQrV6ztJa7b0Pw5DHMriPQzmdTp8fnxEc0NT0el1SYgQEU0ZvrXa1EMBlIXe9XLpqYyI3q7UvbufLMg05p6DUcGtN3AA4ahXVrmHOQFTtnUlwy2RzJlRzZALDcRymYYx1ryMB4K9/86tf/ern5P7p5fVS1dVXrdp7Eja173/88no6lzzgFi2IDzf7Dx/uS05h7iPQJKkMkSsiTojuxALgzCySsiR3zyk5IAu6elfoTVEDVOkpKTggeuutqwszE9rbBDwqrhSGFASiSL8iABdBVe3dNvavI6ArqNW6MV8dYIWUU6uVObFwVLfNtx7ZzIjA3HpvYK4edCNQd418TLfeFBFrQ/QebtMkjJ4lcZa01Goanam6WV2rCAORKqh2VdPILQWsVfEt81mEVcEMXl+v5/NapnRznOexSBZhRu9Dkul+P085JXp+Pl/XVZsDuAMOOSFhTlSbmubnl9fL9bKXfaxwxqHc3x7G6/J6vrb15Gb9qinLcS63u3cv58u6tGHM8zQk5i1VlzICEJO/qayJaRjnWhdTc2RZzBGdCd0wXWseRkksQAaYiIkpMOUYWcwxbGbmYehNDUGYfvXdd3/842+F8Ycffvz89SVmC1EDEeGPn77+4/u/Sx444TiM01TGafruu4/zNEWLCgSJhYVzEnNvDlqViREMHJbWJsChpG5uBokBgCxGBUTmIFEYbTpjQOSckYmFUSzZmyoVELsZIwnRVIr5G0obUZg9BasDkNm6ra2pYcmSOTNjVyVOTMncUkqmrq68YSWdEpqhEGWmnBmQVA3Buzp4BAnrDtmRTBXcwmPLIta7QVzxAIDqLsTEuC71bYZC4Ol0XWMrY27Q1MG023WhJJRTpCpx69Zf1uu1Hnb54eFm2E0MhASQKMv0YJaTfH58XpbzWuswZDVCR3VU82EciFm7Amh4hEspKcvhsP/GrdXWWkQjGAur+vW6iEjJKYmoh7fGIZibCCysrYsQE7rXnMTFzESQYtIMyLg0tQDsOkXUgLnH4VnXzokBvHdn5jIU8wZEP/vw/g9/+O08Dd///fvvPz1qVyRBMnNLwufL5fPT8/tvPh4O+3cPt/d3x908vX+4LaUgkmyS+ajZeZv0ukvgDwlVnRBNdV2C++DOjNjnqaR5uK61VkNESbmtK5OrY8kppYRujiCJzDzcdzlxSlyS5JQAXXswYNzUuqGZRjaPqnqSnNkd7E2pLZIAgYlqt9YtGOTE5Gq1e2u1Nh9K3u9K2LeZEQFZAJBEDb0DMAlYj3hhN1cmNsKuiujC6bAfr2u7LC2UZL4p511EcsnRPUSOCeJmT2diDwFKV7e+rOu66ON6UgU0vDnMCQnWBm7DNA7DsNtNN4fz4+tlvTZgEmQgF3NiGsfNt/iGmwXYcpVMI3w2wlTUHPyw3zsAIpgBq6o5oDOSCMW+DiSFRJKDk6BdhGK9KEzuIWBl3JDg5uqKbpxSRHUkJ3UARGbJSWr3u8Pxv/sPf5jHfD2//vDpixBRKV1DHket6T8+f52n+ebm+HB/++3H93c3x7KplmJexsGOI8QI+NgUauiAxIg5EjmChyBs5qrty+PpPRyGUnhLY0dhaISSZRRRi3AAByB3FCEUbF1T4v08TtPAhNfrGu2nua9rI3BCNoBY/kOIihkTRKwK408zDSZ0ULDIRuxuy7Kq6VI7C/WeOXvvxswOTsi9d3OLlAtC6VYRSQi19tp7TNhNbbX6eg5VrZuhmbdWibkkjnFj7z1WC5RCZkhIrK0reG9mAEMWBOvetdmXLydtVmu7v9mPQ6LNDwfTlEuSlPDltHaF1mO6DYSAEpox9I1piEQYxRybdTAlJJdU3mQs7r2HEMJImzqgG5IgxFPJoodt3YSwde3q/P5uH0VSUCzmaRDaGNhBborareQ0TkNXR9wa4P28+49//t3tYQbT/+tf/uvluoaaPqeURJDp3//6fTc/7Pd3N4f3797d3x/HoeSSJGgdibfJO711AT85tmKxEJ50ItrcwwDoKaWb466kBEitKxFnYUK/LBUAmSj09xsVHdwBVD1aeWbsfcvZJknM1M1DBeSbjY8CwLr9QUCi3jX6s3DAOmDIcVs3N2/mhEiSHOByXfe7eZsdgAtTeK84SZhvw3WrZjmFcRKE2fGnpKX+0+6JhEJ4AxujEZh/MsJA+C6RyM3N0YmCEGTaWrfevSnUptdldYckLIHBAehtJbC7m13JuTW71qrm2j0EioAYeRWhJ40Lm5AcwQ2ISCTkFG+jka3jAWaBcGo4OGwKTQfqqk29Nbusnd/f74lIJC5jH1LOOTFxWBTD/k9IhFSGIWgwSDzP8+9//cv7mx2C/pf/59+eXi5IHBs+Jgb0Hz49Pr8u8zTdHA/v3z+8f7ibp6GkLBIDLpSUs1AM0mgrUXwbIrhRJIUFQQggJgMsMI/DPA65SE6ScxKmnFDNkHhInAW7QWwAY/YGYGoKgUdwr127qjtoNyBKzLvduN2j4JE8F8fFJngEJySJGtAh7goAv15WiywPdWIcxiGLjGPpaoweQkuN/LttUbYl7SFBmHKbxolPTGFVdzdvWq+XxQFyknkaCEFSCm4KCyNCYg6ZQDcD30IvA+u5tB6yGUC8v51F0vlSz5eltgbuKUlv6+vp5ea447u7YRz3QyGk2nUbMEdAwnYFoZoCYU7ETMyiambObEEr2qAFxBEGkhIS8ea9AiDC1q2pAWIc9utaZZ85sZCEqxfZTcKIQqRuDKgQzhTrvTGRAbLINI53N7OZ/v3HHz59eXZg0I4AmVgIP399+vL4Mo7lsN/d3d68u7ud5iGLpEzCsV5CCbKEEEGsGoMv5UHZcDMFz0niKhSh+GkzyWOcZ+ZbSjGMJRMTAhzLJh/wN9ucMHGmknN4dMOCFw8MRNeup/OldVVVZmJO7hCO3M2pTAHNi9UKq5oZcJJam5maqqScc3K13VTW2nIW1V7KEH7M2DSYmZkFTDlobWCrGfSqoWIPXWemYRxlXRuzdANJCVHANSWO5VAQFTafrIBwyglyYnMX4da6AVHrTc2dSVLt7cvX83Vpp8tKUA+7AYYRSoZR0jz/bBp2U/709fTyutg2qwFG7GYApmqmxMwQw6cwVSMgKDH9FEwjGDNwEGGEiJJWYamtdbWUhAlXYcnEOTGiRxRJzLjDsWJgxGzb58UEYIzeY5lrgPz9D//4979+MoOcqaubGiKfL+enx+d5yLvd7v728HB33O/HQSSlzRqTEydhEQ7+Soz73mIMY9Eccw2cxpKTqGmoG8ABwJASuCFATuLWTpcFkIfMTKzuRCiuxrGLdGaKDXYoVaONbd0SeDUlxLW2dWnx7GrdCBTRmTbfTmRZICLn0rW7WViCp2AjmtVat64CvKvtd4MQrxWIsHeL/OFpHFtra13BnMCRKYsIQ23NwRlJUoo5fRnGaRgen14AIRadhK5OgW0Q4dBxCHPIyt29dyUScB+KABIRnU+X1mwcpalJAuu9dXh6WYhsnhNQ2ooyErjdH4a8200/fnp+fD7VpuEdB/BglHY1dEglI2Bwa2Nb4ujMFGBeJo7FB7PwlthEZpoTr93AQa1LU/7lx5vEskWgMTKQlIyh9wjFdozNiQAwThAHZBbt6w+fvvaukkRIaqsxtfry+Yubz/N8c3N4//7u4e44lixJElNKqZTMAe4K8xpt1FZh/sn4J5HSR9S7rrXV1nvrUUMyCwKob683Ma1Nx5JLEkDoreN2z/3ETyAHcDVEitxU7R4OYDevdbVugelBhJJEmJKEP4YQXDiueUc3dEcCAr+cVwDIWda18mbC85xkSCzkvTXagK3BLjA3s96IiRCY0AwIYZ7GOAFjjxytLyHV2gL5hoDxIhFAvYMpMQ1ZVHutVSNaXntwTMmBBd19WZuHHc+MEN23Eri2rt05iThmJCgCiIAEKeGYd0PKSF11E0YgiGAS3vxzGAInAoigSOLN9Rg6UUQAtXgxykQxs0w5TUNGThsU55cf75gZCIlZYuWUEqeQpHnOOYokZiTGN/UOOMBSm2pPORHgUmtcGa/n17bWcRxvbg7vv7n/+P5hngZmGcaSUso5dG8kHNa1tzp3g4N5Es6Jcdu7bYKat6QvRKYsqQWFAHxZu6mawTTmnCVKdSHo0R5v6wFmfiPvx8eFBEhmZo6w1b8uzDnJmKSwRJ5qKDnNwdXe1EObqfxyXQGg1vry/JqEWcQRc0rjNCYmBOtq2+ITIC5UIslJwN3ctjdnhojCMSrqbkAhITInwszM5IxI5AjGRLEvN4usbkNAN43AsHgbZgZqASXqrQn7cR5209ACxORorsuyrmuz1md3EIJoM0lgkGHKtyU7gLbeVbNQSswUIzoPdByAEWApOSVBACG0ONsc1BTdVZupElEIc2rXUHa0rvy77z7mlHNKzELCwsLETgQOLDmnFO8egYRxmsfeFYklZUJARGGpvROSCK/X83q5Ssr74/7d/f03Hx4ebg/TNCShnCUJIQCBsxASx5qBEAiRGYckuUiKqBiIzgpZmJAkUXo7dmFjhaI7tK69axYcioTZkQA5URZBcjUgFmaOBVD8gyHiiCKva7ROmDKPQ06JJaUylbu73TCOvm1ODTciGxDz2zqcTG2aBiYqQ2YiB1xbk5TPp6u5CREJqyptrllHwkQ0jonI3T0xs1ASZqLae2vWdHtThOhmLIjoYD4MKUkOm10EAYIbkYM7M0RWH73R8MJDEI5LBMzC827MubSmOUlOQsSqvta6LFW6ZgJIBASADEkw8W4qcy6IsK6RgLbVqD0cy2q+yQ7DgUIiRBtzwMEiA8V70wj3iflfStJal//hf/zvEwszIKC6rWt7OZ1++MePwKhqYb1HYrAtbZKF6qrILYE4oHZlEe9a1+V6PgPQOE7H4+Hu7njczylJThJfbxBDGTFuxkjZ3QBb4L13M1I2dHAwRIgabttLE8UCgIgMYG1Nu4EbEAIlVUdGRuho0SvV2sMNH+Ma355tYmbmzpLQMSWK3EgzV/OckoE74Np0rb23WIFDkuSb9AKSiLkPQ7muTXJOKbe6dvMhS2uaBebDpNqESd0QUR2YIhQZTc3UTRUgTnJvvZpC7abGKSUkDlIkgKnWacoOUHtPjGXMdlow0kbR3ByJgkqA1lUrQDJHYgFA3YIR4by05pehpJQkixCDq7VWu+rTy3mt7WapN8dJjjuYRkCAIcOQh9307WHYfX758vUlRBxu2NHVarjgDBt0kGmEoOamgghupfemXa9r6727afTIrs2MmEkYoRQGR2IWcCQ2gE/8NeZnuEkVEBDMbK0tQFempmQxVSWHZvr0/NqbjeMwztP+sN/tZhYxoKZIm2QZhVnhLU7X47GNjJiF+S3MBhHQEZmY2f2tUgEnEhIBwN60tY4AwiEH0NadJXU0d1+udVkbADoiGBqFKTNAcBDhgmoqxEFVQQB1vy7NzEsRNztf2rI0QhAWI33T30bMB9XeoSES16ZmGvRAABhKIqSUGEEjVnMYi6mGoNENVHVde2QQ1Katr62DiCAQCxELoKMTU0Yzg27OucT5bsvlioS1reGhtW3rRuC+Ia5DvAmGJDmxKZ0vHR3bUnvXYSzIDOCtV0QairTer0tb168vp/Pd6XpzmOEwwTgCFUgZ7vg45uPtfDktL6el1poSmwsCeRiwCZiwKYAqORkCE07zSA55rZfLRVXBQTITiLplJvmXf/1Lykk19hqQhOztdAi9lzA206A0MLEI9m4OoF1TYnPQro/Pz9eq0zhOh8Ph5nhzcxznSSTGEuEEwUiCczB3D+K/O4hQyZJTilaFOW0kTSbe6nkNqIrk4k5NTa2bA2N03j6m0PwAgvfWa9OAiiOgubce3Rm6GyClFFauzRUohGruQA5wXVYHC0GfqW5XPgs6uYGBunq3/uXrSynD7c3uWhsYqHpEXO/meTdnbS0MGUSSs7RO6K5gUTGaaVdVAw/0EW1IrriUhXGTQToQYus6DImYXbujEQIoqTWKsZU7eGeWnEczVdVaG5FIks5O4OB2rRprtN5UuDNTytm0E2FOkhL33lvVL4+v12U9XNb5rsNBgTMAwjjDOEy7dXg+fX06XS7rVvKHxh3RHVBbV9tq/2bLUhGdmMdhtNh7AkBktLvyf/jjr6PSimpFIy8CkRCSSG/N3cNWnoRYuBRuPRTokHIx09fT6XKpqeTjYX93c/P+/f3tcV9Kii6SmYLaDQ4OzohvW4DwHhEz5izRS8Z3S4QR8RFzemGSlIRFoyZTNTMhjBTpUrKUAZGE+XpZNgF+0LXcAZmYtxk/gjuESTzMOT3wURB5v5iTbNME2qJ7f3qgwlazY1c/HKacxB1VW8RrlFL28+imiL4s1d0ivKz1Hi5ZN79e67oGeptC6s1cEMnd3TSmw9EnIzsjlpxIQrq5qWpjR6HqiOyuFLUEIiJHjJcju6MjgbkkGXPqtnF9zb3kFEQLQmDBJCIsYUq4Lv18XXRZS+uECpkABYAhCe6GqeQBycx7t7XV1rpqf0M4bii4JELoSALuxJxzLNqTO6jZcl34j7/7RRimTc0BRMQ2j5Bv/RGRGxBFPCAUEaBIRGZmOF+X19MViY77/ft39x++ub2/Pc7TkJOUt+MwJYkdRZbEhMTbjDRQGSlRoN48iBXhPgIIvxcTswggEiUiNoBWq6omQVOYBk55GMcppWSmEXMd0z1OAo7CG1tPRAjZEUSiSIhYRiOGIaeUZchZgv/o5o4shPjTTC9qcybm2n2eigiHVru3RsTDOMxjUbXeWlclpEiZCPdX79q6uft1qb33oLM7sFkw65AIGV0SZSERmOch51jEhdGJEN9UtoDaDQKVGc00kjqqhlwCgah3V/drVXUSdHOYh8wsQMxEOae4OADf5lUshLiubbm267r62kZVEAdBgAyQoGSZ0y4LgbdmYTyOdQkzh473J/w+Imq3GqQu3NI+W28CAOaGKHHf9K7M7KDuuKGm44kZ0XlqRA4dAMhMr4u+vJ4dfJrm43F3f3f88P5+CMlIcNUROaJTWQBMiDCUrMGdciWCkjMg5hRSkm1eH0uNmHhISjHfAqTW1tZqSUl7S4I5iYO37oz+5evLmJiZC1NtHRCcQgpGDoogtmU4RwacE4ICpJzHYYy1QVdD9BikqDoTqiq8xTf27sg4FBmLpDLa+RK+qVxSEgZQt25v+DsII7ZbbX1de0pp3g0BkByHoubk5uTCIEzI7kbbJ0CRO2RmzsgGFq4ZMlMkBGPZqA4i4g4KZBbGF0dmAYRkrbsZkAAgkzcRlJTXpmGECUI+vNV04C6SxgFa1+uiaz2dzsvx5XJ4d4TbA8AAwJAK3KfjPB52r58eX19eNUbQEThJyMhuZqqWU1Jr5EAsdW0sLDnv5lkQQYgdrbuZYyJAdDOMuUbK1Ou6IbCZmSmOHWa0gAoBDMN4c5jvbo8Pd8f9fhaKlbhs96G7gwoKbJPZ2CXE0JXKUGIaviVRIQltAC0CNLAgPlKZAPF6XepS3YEQFDAJA3FKJWc+n156a5glGIVJ2JB+ShhQ9bV1DHKLmyPGfDWNZRhyysIoRICtx8LZzA6HeTfPp9Plcl0s5lWgDLifSpiFzBTcmanWPs/g5ikLONRW1RUdOuj5dCYmN74uS2utlHS7L4f9/PdPzzklAFJTYnLVWKA5AJiHvw4BgEBQVDsAADEYLHUFpMgzC9BV1H1CRFvgK7qaGcSiuVpDh7o2IonRmgiHzgeJI05EVbsrE+aU1KW39nJpa3u9ru329ZpvZ9jNgBkgw5DxY36/G3efn758Pa+tISCxmLm6O0BKEmUGCZWckZCAcuh8//y7X5bEsfINXS3EDANidW/h4kSizaGIIb1SMyBmd5+n6f7+9uOHh/u7m3kccskRI58kbWUYvWkQMTSowMQp8TSNkpiY45pDIiFmjryfLXWLkFCSpKy9L9dFtTNRbx1Ap6EghXvAEKDkPAxDyQkASZiBc94souY+DuM8TeZtKHkoKWUpOaTtDB4pDO6m8agVksNhrk0B0SwGrsFNY36Ddi3L2nsnBCLOeVvaN23n80qIdQ0IJZp631LGcDelaShxbiBhEt4ougDxml3NwZDITF2d3j5zMzfta13BzUzD4anm220bwvG32FLtZtZj9EjEvSmglyQAeK2NSCI5TSMTkjZljEOghDHiOJva9VpPp2u9XEutLAA5ARSADGVMt+NxyOTQ+7Z5d3dEV92sJO7QW41NACIuaxUA75twJrLITdXjwANV17ChcCmEoQpUz4VVIKGFcOOwn9893NzfHMb4/koiADUnDPVNmJIhpv/CKCJMCQgAwLqb9ZQEgMANefMkRHJMhB5ILq+XKyN2NQAwbWo+DxJrMgz/FwLLFoMaFDglg7jlEYacHQBAhzIQGBFX7WbGErHUxESX5YIBtSZU8y+PL45AyK2uERUfhhAgGHIutD321UwEmZCJVJWAcsIWYkiPvCEggnGQlAWJX5cG1+qAYF1JYTP8bbNQ62auIiYiwBzDS/DgCMU4gYmMMCz4vP1AUZWyEHCixGjGjvxyWpc1MvzA3YdRWjdzRWBHJgDHDYcboqWti0WIGWzXvtS+PJ5P5/X+st6+q3B/A7ADEIAZbvPNfr55fP3y5fl8XQAJnJxAzUEVESB0TYbXaz2dL3K8PaSUtNumUDMDRFVQ98ulvzlYTTuE1iYaOiFnZkAZBn54uP3w7vZwmJOQEDFRvDcCYGFESsnixMItkIuQGc26OmyBaA5oKYkQGbi7oaNHmA3Rcr7Gr5i7q7XWEUy4oDBSQoBr5OJs9G4HUN+QhS7CTGRmibHVzgRmEIb9qAN6by3inlIGMAbQTZkAhNx6q7W2poAUSlBQ6L2xspsLkzmI8BY5h5QEexJh6a2Zm6nJkEJU/rZ0p6gr1NxBo7kO5ULASjA8l+iEEL56eCszEBlswxRvQR5IROTeVBHMnEmIU2HtXtWS4GvvHUyQr+wl55QIEIEYzcIqa2oO3jYvDYSM2QmzMGK5Lsu61vO5rfX5dFnvn8/T/QGONwATQAYp8L7cj3l+fHl8Pq/LGn5VYgSnYER4rBsA5N39TS65dQWzN4U4OOK6rHVtCKYGoUTcFG2hWwdExKaw388fHu4Ox91QJL8ZlUITFwvm6MeFCRDdjYmCuk0iGQnQhYUJmyptXTemnMGhm7aqzasQQuzu/9/2ziQ3lmRLz6c1cw+2t8ubL59GEkqoQqEgATWQBtqe1qEVaFcCnl5l3oZkMMLd7DQaHGcK2oJAm5MRZHi4n+b/vx8RBHnG3e26LG0mdabLNoSVGNIdmdLrqgWCw94W4QgwZ7U/5crJsrZCpqjmW6UZicDgwysmLMHSLSrvt+KbMpBYRD1BVNwk5p6R+7QIWrts+wQg1WqxwT1Exd1tDI8yxkWQViwvAjLJ7d3t6dRffr5sc4dkSwOEdD+SOymJJDM9MNNI2hwGGHismEqwJxXD4AEWmTNqFbt0vV11BHD69Wo3qyOS17Os/i1UmzzItASECAD0SAKMSERHot67quz7+PHj8nK+3v98+eXTuX39CMsjwAqwwB0vt+tvP88//v796eUyomy2h2MgD/oI8H/653/YtjHnTI9hYWaXfe7DzH2OWRjJCK9RarlN17VhPTgSlnV9+HCPSNMhEq7b3IbtY+7TAHB4zBlIeB0OiSRi5q1pQdGJiJE+PN713sccRRmpZpuFCfl1DyICTGXZx7Tpc4ybRU+nG2mNmJUZI</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8abMsR3Ildo67R2ZW1d3eAjxsjQa60Ru7m+Swh+JQs5hG0hf9WH0YfdIyMslEzYwkajQiOeLWRC9AY3n73aoqMyPcXR+iHky/QYYwe2b3bfdmRXq4Hz/neADfrm/Xt+vb9e36dn27vl3frm/Xt+vb9e36dn27vl3frm/Xt+vb9e36dn27/v+++ODqkiTBQCApwnEYIj0CSCQSIJBIBoIAQDIjqUIVAZGZGaDQTFUISKZ7wMMzQCIyM4HM/o8RCEQmFBHw42FJZNHy6NFla77fHxIgISLu7uHRksrNOHo4MjwSKWtd+093T1V5cHWR3q5v7xNUVXcHRARCqdGMkkRdGwlRQaBGmEgpOppasRZwDxE2d5JFNTOn0daa++PB1MzU1CIjIgFkZmQiAAEpyEiQmUkgSYGAiQRBCJGRCYIpYGRShP0DbsdymBePzEwRZiIzAIlooAgQQEYICUqmkwKCyUR/DpBISHpLkoCqIPuGR39xCUl392bKhxe7cSgkkKjNW4vIHIoWk4jTh8p8886BzFOUHGsEsa4+jOV4mDMDycwIQEiSiEiCAEhkggSIBAQZ7pH2x7/4IxHt+yGqplqKuWemI9l/UAJMBDIiVShCigzFTISCZfX+koqpmiGzeri7R2YkhMgMz2QikeFrc2S2FkXDvb588fU0bD/8zvs/+dH3isizFy9/87svDsdFyerLusS8LMg4P98R2WoLZAaPxyMll6Uta9tuNn/48x8X5q8+/3JZa/NozUWtDMVrre6baQiP1zd3u81kJktth8N8frbbbcftZnrnwUVNvL4/imhmujdSLzbl7Gz38vr+y2fPd9NmGMZxGjOTJBLNmwfSQ4sC6LGPRH+1qqKkB8CkkIkWkZEqCiYyrRgAU708H2/vDx6JTFFhYm21NY8MoQ6lAFmbiwgQhLCf6h7pQET0UGjeEEmhqioZHi0DYGaCrGv1ea/M77z7+OP33tqMxRSt5VrbWp2C3VSU0sK9ZQ1nAmAio7848Pnt4evb5fp2P4yDtyogRdxbixQIEZlBAEKAIpIeoMytFpEWHh52drY1M4AkhUwiPKdJTDWBWltEABDKMJoIByuiVEoy7+9nEMOgEUnCVEhGZrpnCpk0pKea0khJd7g72Ny91lobkrY7fwhf9/Pxxavby7PNO0/een1z481buoXZlqNJda/LMgzDPC/NPcKbe2ampynD6/5wfP+dxx+++9ann30ZyPPdlqprdSvD2bmG5xzLbtoM41CUpLh7KVbKGMm5todX56a2X+o0Da35/nA4323UhmVdt9M4jGUqg6r2CkCBRYmMjEyCma6JTPZsD0kkkKZEJkSQWUQAkiCJjNNXgv1hJTkMJkLrJQWZniJCQgQqRU0ioFS14q1FNFETEkBtLTNFxF2EmplDsXWtjdxqAeA9A0dYMSCfvrwfyvCddx6WUsYR01gCiUBkmIqGcUxTCQ9PIINaNmdX49n5g+vDyz//q0xfj0crNo1F1FqUdanIYCIhFCEoQohA0gFZF4jsNhNAU1UR7VHWaj94qK2ZWWZEJEkV6VuYiaVWVnpEJCK8lwlSKVnde/olRRXVGwNiQpGMaNUzMzJMLYFSSq1rJElbfX729OmrV6+mcfPk7beMSWGBtgQiGzMiyjC89fjB9c1deJBSlEm6QuAq8sVXTx9cnZ9fnL398Or1/R6QAMaxqIioOJqJ6a5EpKiI51BKZq61DSyv744Onm2G882wnxdSHl1sx2l6eb2/P8ymRLqYiCAhPW2JsCf7SICpIu59r5CECjMJgCoEIk8RRBIdmgARGcxTGSEFbO6ZAWIcB8/IiOYRUYUA0hP1UD2zlCIEMj3CRKp7eAjZc3ZkToPVCPeIiB7YiqyRQiLx1YvrGnG+HZHJTFNRoSda5FR0MxT3qF6bp5TNW+++tT17uIruLso7771zu98f50OrqxdLePMGBBCnitezbIKZILw2Nb737tvZ/Ha/t3lpwwCyw4hekhNka02E0zB4ZkYk0Wp0/CACSN9LCWQ6wIZghJNKIjJMTKQ0D/cWmfBs3jJBsqEJYMUi/f7mlkizsdZlmQ/rst7f3VxeXKqxFJuGYV4WilgpV+e7zEgAFFWYDSDdM7OZarT16fNXH7z35L13HuOpvLy9FxURDsOQ6TaNpIjqcT6OwxAR4BTRhFiWpYmC98d5eHCxvdhOa23TNN0d68vXr91dxUB5s5XUIv0wsX/6kBPmAqgEID3l8bTAhEcQHYKw47YUyuk7imQPmohc11YKh3HISIr0jIlwVXogLCIik0hUb0yGsph5a5E8LmtRI9k8CJgZkeGxeAJZihWVFpGBV9f7u9t7RZ6yifvq6cRAqCA8PVPKlsPhd68OVsrhuNzc3izLzFMGEVX1iJ4pEzGoZiSzgzV0mFpbnef5q6+fnp/tBlNr3lghekp6FJpox5cUdkSpqpREIgJAehDR4g3QJEUgaiLCzCS1g1XtoJUWkcksPaXXVc0y4d6Oh/vPv/js4uzy/PxcKEQAEcli9uTtB/f7e4800ySuzod33340TmfjuP3Nb39HOM2KqpK1tQAz4uXrm+129+G7jz54V1NItXWtANRKBjBCRVR2iTCzUlirjGPZ74+OvLk9jsNQ1+Xh1fnV2Y6it7ev9ocZTBFBZvbdYwAUoGWSiUjyhJBU+xZTlMgOQZLCnuRE2AE+CYFAMiFGqEEyAwlkhIsSkIww1chs4RlevaEKCCHHoi1yrTUTqqJCglAyCdLDW6uRLCZMb70/y/TAZhwYMajU5uneIbwKIzwTSPfAGpEZAiZDbfLqzvX+5avWamtNhQlPQCikdGgYEZQAjQwQBCkI90hGNNLn43E+HtxTf/SDH1pRJBJUFRMREQEHwaXKA+UV8iwDPY17SN8twsCBvJrGM2SBu2eN3vQw8tTxRLTwpPRWBEDW1jKR6etaW20R4YGry4tSBrKnU7718OHbbz+a58XTRagircV+f18jDvNhrW2cpmGchqLDOBQrpZioRmJdq1rZbcfdZliXKsLmoaqRudtuMkOUImJmm2mkspgVE4LurdUwydZaa/Xq/Gw02R8XDy9maixlKGrUE8RCz0i9KXiDbVVNRVUIQkVBUijJZIqI9m0F1ahqyhRVZgI9qlD0hD9aOBKZ2VpbWxORYqWoqrI2b62pyGYcej8OpIiI9H4Dqrodh2I6DGb9EAa8tVbXUsp2s62tFrPVvTbvGJ8kBYZUERFJEFSSSQno4XDv7ugNECQji6mWEgEAta0ikplKiqoKI4AMEVmWGkghgWwe9sEZI9ggpeBiq+eDqmOz1UfnWlIuLiElCj0dd2uESq2hkjWowQiOpQw7yVy14NVNfv5FfPrc76q3gLeWCNMCSTmVbwxD2d8fbm5f397eP3z48K1HD5+/eA1StWRo1JrAYZ6//PpZsXK+3a6re0Zdlvu7/dNnr5G+3Z1P46hmREQkRTRC5NRTv76+jvDHV+fvPNbXtwdwAZBxCohhKEIJr5ncyZSIcbD9cd5OV9Nom810c3/88vnrxfHRd977+IMnz17ftNYSKFqGUVtLEVBoIZ4pkQlm5CnSlEJGpuSJX2gZNA6ppGQHL53VAAEDM1pGojBNRQgJAYGWEUHmOBRUqOqpf8iOlSkino7MHl4ernqq5mbm4Wt1FfQCqpKDCkXn+biu1QjPJtkomhmttQ4JVNgrmipVbdhe3R+Ph+MBkUAC+Q3JkZnhzZuDaWKCRCZVhJIgUT0DDo9KoFNgibCfvrOzQUZAB2zP42wKDnANsWYsQwEhbR1axNZ1ncXYbg+g+SG9ZZ4vbbIyFvWlnCl+9kn78UfHv/yP8ZcvamuttipSzayYEllrE9HmdRym3SYyYlnCWzvcHx48vBQdrIR7u7m+GTdnP/nBJ2Z6nBdGgqlSAoA3sPfbYYjW+xSSCcKjY1DRMo6jyne/e+aedV3387Iua2SK0BMZKZK1xbo2Klt1ZIyDROQ0LA/PL2tgWTBtdh+Ou4gayQABFaVpsaLpDYh1dU+oSinDVIxmzT2yAwwns4NT98joYYG1emYQnV7yMEV6JkeVHq2JPJtGj3RvGTATAas3JMowFOVgBiYiRRiREeGZo+lgEmBk1tYEEhkiGE2r5/OX1/Mh0lmUQXjNzTB4RoT0pBgIUjpuNBs8cX1/Pw6DijZCkilkIJgqwn60GJvNLlqtdWHyDfnl3jmR8MwOQoGEQOzPf7O3oifCM3lh3GYM5GYoHFoV1Mw18uBxTCboEccWkQwAmTvKJPPDgW9fyHfej+lBuX62/dlPpP1l/YtXEGG4L96WQ0DkeDyebTaHw104IQyP4zJvN1tKtrVRTK1kOMirh4+vnnwwTUMEgVTTYRiRDICEUgPh1cksQ+GJrZRig6iKSEfcNhg8IAS+wY5iJofDYRoninhry7JEBBAegYhMDMUokglT2ex2SsmM1qpqERVVnY8Hd6+tKo2SVBPA3UU4jtPZ7gzEcV6ur6/neTY1DwcwlKHvf+eZhGx1jYh1WZa1LssRGdHhSWsQzQSBFi2az/N8SjzRejsS0bTTVQhTzUxva63uXrcbhLd5XRUId0bspmkyi95yIsJTtBO/TKDVmmCSiPBMK2XcnZVh+vTT38zr3Ml1Jjv9SaaI9BxnIisR3igq2WFsZgQiW3MghYwIgB5pNwlpvQvnWte/ffb69va6rr6ZpocPH5yfnW82E0UyKHLqlUAB4oz8w/C3sh2p/3rf/uYOj57KH7xXf/qL+cWL8+9/PL067n957S2irWvHrR7x8ub1/nCcxs3hsBfRzbQBUVu9vb3bboeoe0KoRPjTZ1+bqap5NPcoVoSaRG95OighVYgkGDltd716IunpQlERCMP9lPWEg8lafVnmUobmTsq6HElRM2ZSBcBusxFVUrfbjbUi4zCO45hFVIVCQWShDIjNOI3jUBJ5d3eHLJF5cXGhZpm5Udrw1rLMIE2tM9vemllJpKmJaIZntBY4Ho+1riqyrm2ti1kRcrvduse8zstxWdals0prrZnRalvXlaRZSURGigiQxQYbSl3Ww/E4L4upeq3JmPczBREZ6QxEeufPmcjwpTYhOhPoHgCGabg4m168uD6+eIYeKaQkuwiSmRGOxN3ddRmmYdxkoHnFN0JEZgYpBQCpGU7SWluncaream1fff451vWtsdj5bjPobj1Odz7EDqXMiTRtkB3ikdDcp3F4f6ufDec/uL3+wWB/ufjz6v/60/X+qfzgH8V0ufvkw+MvX3mrrVhZ1uPzF7cPH1yxFKUt67rdbI/HZRiHw/6wrnNGmO5MBCQy/v7v/+bTT3+pqmpqVk5ySIaqgZnBoRgINVPVN6IHAVgp2duRnr5OcRbuebbbbDf27Pm1v5GMwsO9dVoBJ3KCqoOoEu4eoibCUqyUobOwkZ4JVSNgpgn0iPfmiSSoZp1RFJHszAVFRDKC0jksZERGkCJC7z18ZCefVU2l8+U5z0td10SGh5VBhLW5EKSUUkTErIggojMXw2azAem1rXUhxT2ITKC2tpmm1lyEBCkUCokuliGpqqCoMClWxExv7w/UE7ecKQAhkKSw72kkMhPS2z5E74giM7pu1uWB/ktECMtgbU0pu4vLzfcHVZnEgifKOoUw9Uy2CEa0OOr4NfOyDI+Pd+O8/OjBfOfrfW5MGMTa8D+/mpd/1z7+GctmupgO87oudbm+uX3+/JmJTNtpGst+npd1BhAR01QyGuHKAMDMCFHJdZnLMLRaFxwjMhl8w9FkpqqiPyQo2iFbRNdTE5S+MaJk5Il0un4lXT6D9B5ckJGZEOmIg0BmuixdzyWzxwSFhPSC1V8P+vNARKVHST/nJy0Y6CobAXSpsxNoXTMgQSBAYa8z/X0kgkn2hiaTBJmnn0sgCSLDQemsO0lVRWbkSQAFMiNFhSLhAaA/VyTLYOkZ0SL7ez/JmP34mkqSBLWUs+12ng+Hw3GtjYg4qbTR9WJkegYzI0MJipjqutwhIwUUY3Myu4YEABlAgmHb3VTKIEREDtMEIkhh76WipkSkZ0amN/fIMnDN/Gx/uBvGr7eH//JP54+ejH/9bxf+clDKOA7zuvybm8X/un3vP3nw/fd2nz9/EY5BZyKXdR2mUYVDKdM4ebT7m9dlGomYRsvIlFMFpzBbeGtWSiYzKwCPEJ5OkYf3VwayixC9Hevqn0AzEtkCb3JbIuhMSSadFEEGEUm80ToAvJHDEQAjIV0TToiyNhdBdl69WwvgGSlvIl51U4ZBRFqtyzwDHnFquJRBYeINDR5IRHqHPdJJyUwEyIge+UQSKezxncnMFGYkBWAwCbbacXZ0GYpEBkR739cj6SS5d1zXN2eN6Gf1mxZy7Y4JgpC71y8ckuH9DCXZiXgwmaSp4ATNqdLWJVWJ8EwEiUaRBALeaT2Q4qlW9Pd/9tPNVEQ0M4yymQZVIiPCa/P0oLKL82utAK6vb5bjshnH14eZ2/PX9/WTH7bk9OEH/vmXjIBpcebNHG/5yiv+6ov1yVvbq/Pbr5+2adqK2jSN3lqEn52fzcdDUU3EoJbMnudV9KRoMSMy3aPrDD3Ueu4WdsWG6G+wOyBoIiowESG1/wnY+385ZfJvTAUgusoPdlWJnRs7WRUIOUWynP6GAE/JEgCUb3JMTxteva5rPXpdezx982AUCJUU7QmuJ2IAp7SXnUM/URc9V/EN79lZE/QDdmqtT0aajquA6FwvED1BfuMr6d3viVPp/4+MnlfzG80i0Q07/TmkR3U/7RF5ooxIMk8SJRERylMa7dmLCUcSiGSrqwrxZjcpYh++fbbZ7DZjAcWUxQxka97cJSWY87r+3adfeMZgst8fNkN5sCvBshn59Pnx+bPl5ethfI3Hv+/7+5vEhRYdy3Dnh1//bnn/QSNbnfX4EqqiRiIHs2O0eTmgrbvtyGSt8HDA2ZVD7YR6++GH7w+DIVJNRfTF69e//O2Xu/Pzjz941+wkNyzL+jef/qY6vvPu4/feeqxKD2+ev/7si9v7+Tvvvf346rxXwVrrs1fXz17dXO7O333yUEX6O1jX+usvv2bKB+8+GsvQK2Br+fz6+ji3i914eX4OnorQ8bhe7/cm+uBi1+uOZ7Qa++Mhwc1QihnBJJBynOcWVYBxGISZTKH2BjwzpCMlgCKlDGutLRoDIp3GArrm4AQjU3sSItl7v5PLKhMMJMFegoUInII2gDe5F6cyTkTKqYYnenVLQlIoXcaPDHjP7pJy+nuyo8piSQKRKpg2GwCtNaEkHALxjERkvqk00putCLf33n13HAoBik2DUrUuqwmrRwBKtrYc7u4yctyWu7v5++89Pjsf//w//vr6Hq1VkeEvfnl3PvjyZ8fPP//yux99VEoZx42Vsp/jxZ/f1TUO2E9rlHBkRkTzVtdjq63msZQtxCI8M0gqI8nMNLOz3eYf/fT757ttz0YBfP3sxae/+/rJo4f/5I9+okKPIHm/P/7my684+yff/eAf/d7H3dCyLOvt3d3Lm7sff/87P/reB13AaGv9609/+9W/+6uPvvPkP//TP4yu2yKvb+4/+/ppRv6zX/z00dVFr5zN27/+X//PX/7my5988sM//PH3+qEk8fnvnv6r/+nfXT64+q/+sz+exqG1iIxXr2//m//x31b3f/6Ln338wdsimsiI+A9/9Xf/19/+aizDv/yTn5/vdiIkeTjO/+3/8r/f3B5++qPv/cFPvsdkbwb/+pe/+fd//auzzfAv//gPttPUcd7N/eHP/o+/OC7+w4/f++57b6tq93r96rOv/uG3X15d7n72g497K5ARh2X9f/7+N3Nr7zx88M7bD3jq//Ll9e3TlzebaXjy6KEIkIjItdWvn7/M5LQZLrZTL85z81b9/lgjvLAEvWfAk5uMvSA7ABGZlwPilC1JeESe8lnijVERoKiMJjaO42Yq4QkRsXIykog0b829S7O/96OPx6HU2iTqshy/+vrF/d3t7RHNY39zsyzrfFzuDzc3r19+PY4PH799vz+KyD/U5U99OG/t+eI7ljMhRL0u+/tYa4tIR/S0fELNmSpC0c12y4QqE6KqiaRIETnbbc+3U7L3heg+x+12vDrf3eBQTEkRIkAzfXR1cXZ2XcwAWikiLKoXZ7vNVFR1t5tq7axqTFM5226b+6m9VRVlrXZxtjs7355vp8009twJ5G47nG3Gs7Pt5dlWi6ZnAN7adjvWGg+vzq4uz0WIjEheXZ5tpmk7je+89XC7HXtqmaZytt21lm8/vnry1kOlQFIhz16+2kzj5cXZdz94cr6ZOjl2c7v/v//602FYvvPe2z/78UdCgQCOw3H+8vnLxw+vfv8nHxXRQJK4uz/89ndPfX/48fff/8kn3y2qXYX5j3/72+evbt5/8uhf/PHvq7JrjDe39//qf/g3a22ffPe9P/rJ93uldfe7+8N//2f/3suoostapUttgEC7JOpOsquiJMWUdandj4IMqmatTEkhIojcbcZf/ORjC/fMwQZjuPZOQbCurTU3xmhhZWyt3rw6IOthf//5189f3+3v9oeXLw9aNmb6u999HbWFN5I3r16ale35WYH+KNb3P9nNGP+3T++I6X5/3IZHq3fHg2jP4dbhhZm6uwrzhBeYGQkuSwWh3ZdEDkPZjIN7WtFiRiRFIuJ8N93eL5HZxSgBTeVsN6lYAOMw7LbDsrTQVAUph+N8c3NXStlsN2MZRGQa7TBnKUMppTMiIlqKjUUTNJNuO0NkGUoxHcwgImTvCoahmKo7hqF0YwEpEXBPipid4GIiBNJNi2MxM5XO2YIQRkKEZh0OdSMjKOxc4dlu25VEhGQGgGJ6eX7yDkq3oSYgKFYeXJ4Jg1JO5CJlGsfHjy6ncegGQSLLUDab0Up55/GDaRyy9+tZlmUVU7FhXVcyBSIqb7pTASiSSBFhba0UCE4W3wATVIp7JDyi0yKyGct2u7X7u5tB0zB6tGhrhmcA6btRpmkqw/D65at5XiPx+ubm66dPn726vbm9ef7i5bzm5eP3hGHEmiHCjz54/63Hl3/z6eci+tZbj//gavxsfPlP/8nbv35ln39xvR1tmQ8RHl4NReQNbkAUM3dPQigZcTzs1XQ7lZP1rdNawmkYLy/PM42UYtZLrZBnu63wpgfCm/fG3W6DzGI2DNo8PD3cz7bbcbDtZtrudmMporq21iLNCqWpFbXS0bJklFJUBKRa6f24FJTSMx5NqKq9xRelqawS41Cs2Il0kuj8kpmoqaoA0mu1R5gxAwEUUoWZuT/Mb1B/uIcWU8paWyLUVEWGoXRzUYtwb5mYpmHzpsICeHl9V2uAOW02m3HyCDNL0DNM5er8vAzWTTcJn5cV1FJkGkeKIFIU4bGszcxQrC5Lb7lOTciJCANAzxBgGIb02tiltjeUDdg8MkOl5xDZbTdDMbu8ODs/35HwkPDKLGMZgBxMluP+i98+C2Zdjl8+ffH69u76dv/85e2r19fpAeB4e+1ZmdyM0x/+9Af/7I9/drO//fSzr9a6viMk9c//g77K27cfya9+dRxNlHGzj76bvSHvDFP1hgykJj0heVqs4aonDyZBK3j7rSd3xxrZG87u2OFbjx+tPJumSURFqKJAXF5cfPDh98owZIQD4S3B8/OLH/7wJ5dnA8HVI5sDMBveffL2cDObKr9xdHo+fvjgHz57+uDyomOaTt6Ow3hxdnl5eanFRBTdKiP28MGjTY0yFKGIMhIF+uDibCjj44cPttMkpr3yTuO4nTbzfHxweTYOQ8c+mhyHgoxHDy4jeJyPF8OFFlEKMhFpg5oqAI9kZIsQwcVZx3y9kT6xaoPZOAxi1s0naubuqjw/m05HUJDJ43FJeHpYsTf0nIpwaY2i3dqP6MMeJ/c+RfqYCDIjPLow+v/p4bsJzb0FwUyjeOTl2XYwsTKduQxRawTWNUnHehRyIZ48uNjfvPri6xevbvfPXt7c7w/PXr7c36+IpIJgXe5J2W2nf/qP/+AXP//edjd5NhEkdRYa9JPxyWe/fv3hJz4OAERSVPLEUQiEcpLEWuSJTFCm9lycGWv1XjF7U66qRePl8xcR3/eME60bsdlM19dPP3xy/obmjsww1eN8CHdRkUSImBWzPNxfb4dLKyZkDTBTBLvdbl/Fiql2cQ1InJ/vnrz9ZDONbzxlFJgqrx4+mjZTq1UHCBkCEjZudj1mJInOBeHsbPfeB9999+2dFdOuEVD0TN559/2l5aMHF2RmRNe7ri4vv/vx9z/64NH52ZbIYgrq+fl2t91Vj0eXF52KF0kSDy4fPnjY3n3nsan0gpuZnvzww+9ltl5PRXRZ5tZago8ePznbbqVb4zKTnIaSid1uc7HbUEwZ4UnRulYRWd15aldPDDaz/yZ69jrNuERCBZHdiQewtoo8UTcJiuTl+dZU7W///u83gybYvNXVzdS99ZmiD7/z3lvn53eH3z59/url9d3N7WFdXIRp5ZQVAyT++Z/84Z/80Y+LKRLbzTBNg9j2LuKrec/H+pByd7uqcp4bKUINnjKUipipqoZEuLAPCgm7sT4y1rW96Vm6gy6GorU1ZAyl4xICebYd729ftfouVbKbt4DNVA7317U+Wda1exRFlcyEL0uNQHZGTjiYmsTL50+Fv4eTWw+SNJUXL57W778XEX2QqzdL16+eXk7vAOnuJPuozf721XGppp+05mR0oyMyvvzdr99/9MN1WdRESYo29+Ph/v44D+UjJjwjFlelSh7297vNE1Vll6oIUh8+fKhDOT/fiWhXM4RRW1OVQbUjim6+VeH1zauHV2fFCkVNAI6H/WFeVoGbSnXPEzebQX700Q93G07jlOgGi8zI/bye8nkfYQCEiZRkmqgIke7djZYIilBA/4aPi9Z649DNTxQ93+1U1X7z219PZaAkRQScNlPzOByOAt5cP3t0df7qZhoyOdEAACAASURBVP/sxfXdfkZSB5WQ0mVAwTCU1/d7VS2mvQ4Ow3ix294tUVUPdf1sf6hMvCq1dbrqpBH1gBPKYEXUPCJOpHN/fibTPZs30dNYVaeANuMYGZ4sVjKTRGSaqgkP81zMhNbPffNQsnqOw1DXFaLFylpXRBzm+WTv60w+QcJbaxmm2qlgIT1hZhE5jtb1OsXJTJOU7WZD0iMUJ6cXRcai283YFatOjYqKim43YxeYOz+7rnOr6zQO03Zidl0sAcyHu3EcVcQpHUCQWJb91eZyO5bOrERmhqzrHO1wdXlWTCnsHFpzP97fjm9dbDYjKUAaitqwLIsZNuMwFOsPkREm+OLLz/7xzz+ZxoKM5hKZLeq8tlNpSXQxQkX7EKEIKAJPVWRmCuw0RKdIB0WU8wIwRVXAyNhMw/nZxtTsiy+fDmpUhkdXf001vCVQTL786uvjvM7HVQSkGCUzRW0w/eH3vvv40cV//d/92fNXNx5ZVAIyFHtweX779K4e5xz1bs+725sH2ApLwCFUkUhHB/iCtbXJ9IQbYB2sdBtWZs5rO3F+nb/PLKVk5uG4dLadwOmMUfaH5WT7JEmqCQWHQx8vsGLDCcUC81Iz00w7OszMFumRpwhT6ex6p7mru4pCu6sSEd5a8wgrZRjGtdaI1HbSVcWsTxZ250xrIaJJUSun6p+5trlWJwUi6JEoQOTdYU5QKGUo9HAPMY3MtQaFnuxdL5KZ7TAvZiZiEM2uajDv9keS02B9P+PNHOVS6/m0NTMtJr0XAfbHGl7PNpMVY8JKZuKIbM2F3b4mQJ70km4/ezNSehqYiEYt8GD/pqBQI9rJr4QAcH6+m4Yhw+14f6ilxEkyThUDkgxkipmJ9p6jN+RDsYiYps0f/N4Pfv6jj28Od+M4Pn3+ellb2U2SaRyurs5/+3R/vyx/dvQWuSzr73w/mozjEJFq0txPwklvSMBkZpDDSahIQiCRWWvLzB6DClJ0mgYk9se5z3qcfARUCpe1Nnez4aRVJim8P87doCgqp1EQ8Div1X1Diki3YHSnVPiJk+zGvswAcp4XUsCkqmQMw0QyItxjXVeKWBGr9iYxSkL7GEGmH5baJxhOwj57WKO2PgpAUk6CZ8Z+PxOZyD7A10vturaWGUFTVRMCDRGB43GmaPfQ4o2Idn9/6B4WCrqBKQTzsq61mVofL6ZSIIi8vtsLaaWompm1unYZvrbam/Y86bHs5EiXGro0FeEAI7OYNV+6Dai7lt2jq20Q0vPBxflQbFlT8jQCnHkSlKNPjnWIoCoiNLOipwm8aRr/01/8/Oc/+biMpZhtxvL8+vr67tgdISQuL84yPAJlGDMxbDfM7O5KEVEqhEJRZWfRAqlUNUGim8zR+afEsjaPhECpFAmwWCFxt58BiBq7G19oqvOyrtUpfSdFhALc7/fH49wt9MjTO2htrS1U2J0VItrHUVvz/pmHUsy0j3kt6yqdwFVRMxEA4gGQakrSVPmmU4lIEKSqylDKWispJ7TbEzVR3WvzN7pnd6bRI47LfAo9kTIMauatHecl/DTObqqqVkxra8e1djG3q+aRaC1u9kcCQunjg6WUonpcFoDTNJpKuCMdZGbc3e9VbRpLKWXanmmflWrevAdNkhDkyRlyIvfRp+m7909F+zxW1+T7VGz2rqTLtiJXl2fdJ2hdUEAvTWSfvwcBiPI0VmGd4QYy4na/TpvRVDNdRaZpePX6+PzFq3cen4NKycuz3Xw4HI+HwUzHAe5UpZyC18xKxFDGUlT6bCm6zNxTWTdASP9gS60eQWifeQZYTEX1OK/dm9OPWmRG5rLWeVkfcgcRBVVFRdZaj8u6O9v188iAUtzbPB8jzzrh2a8jEOpxOSLdPYLMjLpWIJdlnZdFKMgQ5bquzaO11sfphGKlJPokGIE+jUEAa63HeRFlRIqoULqwuCz1NJRGqJ5k8nmpnfoCSCUCwzgcD/vrm9tubHyjlycoh3lttYkwgdr6a8l5WQ/HmdRpGsw0upKecX27F+E4FLPSWouEIudlPS5rvz8gvN3dvO4jukutEUlET35QFUhXh0XYJ7aQqaJ9VtDdCUlJFaVIq+0NbDnxLOe7XSQCMBMm+vekRHfwsmezYlpMO2ggcHax+7tffXE4rq+v99//6P3+6rebKfH65fWdlaH37g8fXIh6XepcYa0MwySEqlqhtyyqLUtkhGspZTsNfa5RVZDdh9FHZ4WU2lrzNFMRhTlSpmk0k/vDsZ+rOA2rCQGPdjguWk6myH6Hw9LSbBiHIiKZEljNNJO1NZXuisiIPg2HZa19WDzfKMEAavNvjN3qOS/LyadIGEGht7asNdORWb2VUvpFG9pirU36JCypBlAROa+11x9hn9HtTn8PgKB7/xKlWNXy+vaeyHld9vt9xKiqIry7P4S7mZ0mawVIHI7LslYxKaoeCTI83P365q7zD8taReDuKro/LpFQs6IUgSaRnpnLsp4mfnHyllAE0edZSD1d7eGZANUMRKsuNDMBWddObJKiBFV5vh0BRsCsGKhAz3bpCdOezLjZDEK0liAo8p333vn733zp7k9fvMp0ihbV3WbIxJdfv2ytmQ7C3I7l8nx73Q5kJHM9zt0K041yQfHmFE24u0O4m8bDcWmumXkydVIpFKF77I/H2nYiAYIZ3Zqy1javtZfaTkP0xHiYa7xx3mbEMAyzu2gRtT5NPtCmzVTUzKwUe4PFmqmaSa1RSqEwkxFuQ+lWomJFjYxs4W9uP8gTO5oRgdaaiCJaq06cqmQy1rVmRrirUrt6I7ksCymZ3UEJCRI5L0urDR0+n+qUjptprQ7APdRkGksvX/M8R3K3nTbTqNYHlSO6p4ccp2EcTrMIy4L7/SGAaRw2m4lkePPwu7uDu0f4SfxgN4hyXmsftzeV6JaEPisWVFMTnC4oAISqJplv+BMhKR5xMhkhABmnaRrH3jeYmZlISwpcxCRiKCYnVNddXeiV1T02U3n5sn717GWrUYqpycVuU2t79vJ6f1inqbhnMTs/m65v9kJNZEpXxXjydzGpZsZuMHWP1tzMtHn2k43TVQAkI+P2bt8eX1HemNEih6Lzsi7LvB2VIumpKmaWgcN8WJbFhNXbuqzDYLZ4ZFBOQMiJYuZR17UB33hr+t1HGtl5r05niKnpMACqpqpMJMMBjtMEcp5XjAkkqMd5oWgpcre/v9+fIUGVea7No5QSma15t19nxuE4WzEyl2WZl5FgROz3RzEV0ebuzYHMbMtal1o3m90wWCmllNIFouYhZtM4iRX0jkp0Xqq7Z2IopVtfadkOy2GumRinsZShM0G+1levb2ptZlKs9AmlbizeH5cAwv2U1QihugeJotKNmNKd38LWvJgIu8AjKpKJYdr0ipmRZ7vdOI7SxbfdZrP6as6EmBnDTxYJhqqNo8VhcQSB47zutpNHvHj5+v4wT1NB5jQNkXFze/vi1c3Dq20iu/cXeNWBj5/MUIKTrVneOMdIoDv3u/tZRNDNmr3ICyOJ5LQpClJON9iYyf39EsHtZurK22Ye+0s8HtdhKCYcaQKYiUe4RzHLPrOa0i0hh+N86nkpoHgEELU6hKZyQiaU1ry1CoqZBgMwd2+1eqaoDEPvkKmq/XYMpQzD0N2X7umZ3hqQnVJI1YjwiI79p2mYhpKZEfQ+LCPYjJOZne6HontLHUpGnDoySkrcH47TZjMMA4XK0x1ES21qBaKbaZDe+yareyatlPPdtpQSEc1phv1xFdOhqHtbazUttXmt6+3+2F3gPMFlZIRonyYjIR6td1mkmuabJkFO+q9yKFtv7llNyoPLnaqeLJ//xb/4xYPLM6EU06HoUArRnRAAOG02okaQIvNx3kwDINf3h+ubuwiPzO1mQsba6rMXrzwCSSF/7wcfT4Nlv74LTCC89akjIU0UzG7M7LSYWilmPM2tEz1jAwSXVhVUo5BKGYcyFI3EPB/7oGyfoU8gI2/2R2/eWmu1eWT32R075qD2790F07W2PtuTb0qDCo/z4h6nJpDabXC1tXa6nwbNvZ7kP6qqqihR9NQjdVi2GYZxHMaxINObg3RPMFWtj2/1VAqklWEYhnEcp81mbeHemDmMw3a3maZxHMfOA2c4ebLviyrF9ofFW52moaiJqZmBcpyXiBbRxnHkG8Pt/f2hRWOilJJkf2gPzq0pdbOdNtPWrPgbx5iHdzc6+kUhkp3QFOlVMvvX/Tq47WaT6A23lGIiUmtdl8WjZsMw6NXFWTHtQwjy4Ori6vJCJVUkwrs/ogdvJDqOUQqQa1sfnJ9nRq3r/f5Ya/PwzThmotZ4+uL1utS1rnWtbz+62m4nvCFI+tU6VC2m3XCdCWa3UhPANNpmOw6llGJvLMkg4JHzUkW7NH4yT/eLse4PS2stPJBAV2mQy7Ku1ZvHYUmKmUn3QdTqrbfcgJn2kxOZzTO8RfS8JvNxjszOw/rpbqZcW1v7UHy/XA4CoEceuglQ6C2+uWepUyAUycwO6k8X2CAzs0Uc56VfFtjp3H4Zyv1hPql9PcnydCmYZ9ZljUB0PBUxr+1uf8iMYpoATjcDtf1+Zp8AyNOWkNwf5k7Td+okEv3Gl5u7PRAmYqamUhRKinKysd+1JZQkBdqntYahqCjATrZFJAEPVzE1NbNxHMZxQJ5mH9QEkIvznZKqBGEePD/b8TTliYTzxNIRGd5qMW0qAXj1Tz56/63Hu8O+kVhrQ+LyfPf44e6rr18LsKzVlAEsS438psb3wU+05mMppoWKNnft4cTel8HOd1Ntfns/1/+XqTfplSTJsvTuJCJqasMbfYjIjKzMrBwr2E1yS5D/mEsuuScIcNEg0ASa1c0qZldmTB7+3N9gpipyBy6uPk8ufBEODzx3M1WRO5zznaH4uv8HxPNl6d2UNCyIae0jN5t9HeaO6um2n2pb80zQDlA8SIfN0wQAax99KBkMIBY6zM3UPLyPkUCLvBQA0NzWZcXWABNtF2lJWtYhvKD7cCdif23f+kgRUai7u+rw3nXYQCUDH304uHk6cGOob4wT9/x55q5jAKC5L2vPTysChhlCev4sIFQ1nHrvva8s5XI+r0vPVjDJEgBoqsvaAVEIifByGQjugJ+fXhLsJCJjKBK7+8tl0THcDDCWy9natI2UzLv1rc7PUVei+0hqLejBnA5hB8TC7OBSBUbKAUsfS36dOXVl4bkJRLr7QP7y1++XZU1UkkekFgO201AKsUmwMKip2fPLpdUJEX748HB12gEQBP76m7cff/70+Pzy04eHNtUIf/j8/HJePB2L6eQKinARQZbCDBTCUoRYpEq9u77+wz/+8tPnz//8L9+t65Ij8jRhDLXLsk6NEXCM4eZvb09/+/Akhdd1DFFEYcK391ePz8vVcX9ZOksOneN4mKdpbq323nOvAT0Oh/03v/r1PE/r0okJBwDCzdXRTE+H/RgDMff2UJnMfD9PNvSyLAShulVXrYqZ99EJ0AjmVhDJXOfdtCwDcNtGtCKP9nJzOgH4GJoWXRFxt3mewn1ZRzaGRNi7liq10HJZEMjDRmqa3YWl974sUgReLkveazrsvCxZaugGPLNWCgBe1hUcLOLlcgkgYoCAtfcIRKTL+TJUTUer5bws3AdxIYzn83JZNFWBm8MTMAKIcbebdF10bLacgkhCjKzqzMTELKSa68RUCyBRVJE+hgOufcj//L/8r6f9fHs6BkJaWyMcN5EktFaIScdYPAL8P/6nf72cL+bxv/+H//gf/q//OxVgzy/n09XpX//644+fHsrG7dHzokIMgRZOEcTAzEUKsNTW3r65q600kdrq1OphP1tEqfX+5vT56amvipQ6J1CP83lhrBHp5I39fj6drs1j1VGcubB5nI7Hd19JbZy8UgASof1+/+6rryOgj8EumDJQJGRelqHuHODhAEFUfvO7P+7nsvbhAUwKiFOb3rx9u68lwHWoB4BbEXn3/t1xPxHFGJZGywB4//4XgVhKWfvIjSAh3d3dGrR3b2/XZSAqILj59em0mw+/+PqeCfroqSo47ufrYz1eXReWy2WxdKMwN+HHx/7LX7wNx/P5wqzuwMxL11Ll5fklXsuJaWpA/P79fQpnUgc/1dbHeHd/RYTLMtLV7LAZIO5ubon5cl64WAB/eHhaVXPcj9uFAsRMiLtd64A5eAIILgUjiPl4qLm1izSkpHSEkJBbKQiwrj0CVbuMMZZl0A0xE5PENgBJtZFflj7tWs4dcqnVxxKBnx7XrLkAHICZA3AdD2yedUyQCHD68QkQYzuhNgbwRk8QRiJAXIe24dfHQx/j6uHw/eVBGHKG5o7nda0FESnCmViYkPGyDiEGRB1DA2rl5fIypoNaMAOhAzBFPHz86XLT3BxAEcldddjj48PzzG4GlD7wQPCPH3+e6Mo9TA2YzCy5oOZq7hho4OT5UJJIzVXf1rMiXi4vL+cL/OErM0tjUlIHudQIGGPAq+nNw2/v3rRWVL0IeoS7hsft/f1uagjhEYxoHghxe3vX9ldXx2NA6DAzHG73b97fBlwd96XWZVnSbIzE33zz68OMERBuSOjhIuXN27dvrveEYKoOIMyt1pubOwB79+bWHYfZ0/nS6vT8ssKm89kqF2JuRd6/u2ORq/0+8BbBs7b8+PCpJgCrTG2qnz49qRoAAQQCB8A8VTcb5g7R10UAcLhjArqEzVxE3BwgLOzlsgDlN04RXqQA5LoSAIggkMgcVIOZLKeFEOZew5BKABDgPO+/+cW7Ulh7v6wdAYeFmJG6FAhAMzsv40uFxxSbE58pEM9L37UigkzsgFSqMA6PpY9tkQCBxLUVInaPNLaBKzO1Vsw9kQKJ32YhEc7pZDb/TEDMreUkKYg2D7p7cKHX1wZUcz2gLMyFTZ0o9/1uHqUWWrtq2n0DAtZhSeVbegdA3MbuvqqbjzHodf9NCL6onwcGGXwRnnuoOjATGSRn1E2E+7mvvSNTmioSWgMQlzF++OHj1a/fCRMSurm5GeK829VaiNAtBDHcV9Xrmzv0VYTDnZkpYlnOZpq1Cr1SUadWf/vrr3/7q6/N48OHh6E6dAQzEnz97h6J1BQB51ZsvzsepmXtuVdmonkqNoYRgocOlQAytWlq8Oq8cwsATPDE2m03BxMxsweIcOG6uBbGCAhwRCF0wNTSoMVmrvXNVE/TPP3597979/7GRv/rX78bI4Di/PnzE2JrRZillKnVWuv1cU8cu6nWWt2DCFm4FFqHrxpAYOFDdV17m6oDLt2qsIchOAHsD7MjqXlDiAB1R8KbmxMiDTMmCicjR6T7+7tSi0cw5ofCInw8HkthBMpBMb7C2aXVIiIiEWNdxuiDRRBh6Wt4SWmwmU+7CZADKQA8wDe6bDAjIDkABSGGAahHsjYgIYgRqtYtcu5v7gKAAe42xnAAZFR3IlKNZV3Py3pZlv1hMlNVTIWsheY6c553Hp4ctQjoZhFa6oGICQIIXe3lvLir9jXchLmVokWW57N6sAgx53qcgKZde//u/rifn5Zx/+YGEXRo75ZCcABkYUJg4rf3cDjM/9v/8X+qehJ091NLyHKeSuLm6vH58Xx3c8rxIAIPN3RCUERgBBSmPnKhVpv04a8sCUJw5hzDovqg7eTEyItR+I9/+Mf7+9Nyvnx8+LT2sfEOAQBCNRfK2bT5UstxX0Vkv5vOy4rMTcq8292/eyss6s6ELDApVXlhLvPpej9PBNCHytMqdGGi3fHq5uaIgH2Ml/EhAi1gmq9KZQR0j08vo9WCTCStThMRuerwM2KouRNPbSLCMLfAUqXVKmWa5raDGPN8USjnzwEh0qa5pWmk+zLP+9JsWFh2MMjd43g8tDmkFPUoHOa4duXCNzfXpVBflcQhsHflIrc3VwC+DiMcWZt21To1IhTmPCSW3vsYu/1uqmWoFSZECre1627eXV1fifDoAwh12NoVCaUIhPd1DYDsFS59qA4zS1CjRaTZwiNqle02Q0gC5efPjyLszsRQiMwRCQ/7EyKcz5cIoFLcTM3nef7m6/f/9bsfmJkQWFgVgMINupoAKIA8Py+/+Oo+wpdFkQhdMQCIwiyyX4yIQGHZ76ZPn8+pqAAMC5BAQ4eIV8xJhGOAMu7++Lt//MX7OwD49PDx6XkZQ5OIm1vWIlJKEieJifvoCO14mE09PqFBENHxdPj582VZzuCuHof98f7N/R//cCVcBsrLYHcL5/t331zdfsVSpqmtwYiIbX73y6urN78qmwWJGIkxvppO1/drq7U1gfyIG75rp/nqLRHfXh9FOEcM78qhzHe7qVzdnIowIppZOdzvbx+J8O3NVa2CEH0YTaezlbWPr75+d317gnBE4un80+f1svSbm+u7N2+FeZjh43Mtn/rw42E+3Ny0UgHj6fkS3z9YeGU+nE6H/T6nHgM+08eXItx289X1LROuXZ/73/bzWgvVWqVOudi9DDieTsQlgJxIiFloPXciSh9PIDERMa7rylIOh3ld0AOZqBAj4uw0K8VlEJ8TVsyFdlM5n1eHx7X3vvbEyE/TdHMzpjb99PMDAtZa1NTNw303TdM0EQlTEJJBgBOgu4PkAvXpfHl8WlpFiBAubqhCbg5Eqt6qBAAjaVht9RXQsSlhEj0dGATiaBwcOBjpd7/79T/88itEfHh4eH45ExUmC4CwkSca0XbmZaGUUK5W5LDfIdHnlwUpzi8XJt7tdlNhdfvxp48fHj4Skbm7ep1aYY5wZCHEAEwVBhAKyQYs44zWIGJixMwdYRHwsNDw/GtgmAPGh88vrTbAlMYHAK3G3326CAkRM5PIdLqeAkK5eghgDFCep9/+9qqPHuEfnr2IQATX4x//9K2aEsZjj3ADjCj73/3+96YmIh3ZjJhJ9uXbb7/tqswkRdYsOwhP97t/mk+qsWu1MxMA7vAffjtf3z8jxOm4B4BWi3vU/VWZXx6fn++ujsfjXJgAqB3OwR8u6/r+qzfH/S6RuWa6+k8/xcPxsJ/2p2k3EQIRvi+1/NsP//kv/8YsUgIAW6VdawHxww8fLmMwQCt86XY+L8T0iOeHj58RgYjUzHM66FBEgHg/1dv7u8NhLyxMeL6sUkpllrSBmgUBmI5cc+QuMOlqwuKBYd6kUC0ellIHQNAI2PQ5vvEijP/xN7/+1S/e1cIfHz4+Pj7pMGBmkXBTiFoqlSIJ9wUsRYpIKVKkpCoBIMy9a7w8P6vbvE593k1T3e/nDx8fmIQYS2HT7ppuJk1oWM7Ec/W7NX2E4OjbRe+IXyBrEbCl3eCm/EJMGW1AYDpagBIS9ErOzufPHYhJmLOHTb1BvpaJI0vHJSISZzhIKvw2tSBiIDITllpbKQbIm3wXPdzNzCxebZlpd+Pt3JdXzop9Pvdk1cKrQ59l93C2p+UlQdyEdLq5PyEq4scXg0iuPsynm693s3s8PD74pydhZKm7w0mm/W7aibzkV79rUgqrhkcIYRFBwqmlo5vGUPMohdJBDNun7SJSa7u7PbZ5Hk7dDQC7mhAiQZjb6Cu1YgHsKdENRmbGMWztmvxBJpxqrVV0gIdvagcEQoagIGAkQPr67Zt/+sNvjse5L5fHx8dsT4W5FRpK3YKJ0thdRHhznKUuKaap7XfteJjsbz8+f3iapxN4XNbLsq65lRJmwChSkIg9afu5zETbtGLh7kyQWuBXx4SkUzz7k2Q/AdL/H8njvpFa02V2HhdmRqq06Y8y/yrcTYeyoRFF8ouA4ZXCs3ESCdUsIAg5wHKvnT85KRuEYIhmvS8yzExftyDJN/3CTNvWSICEYdnLAyIwpbwKACjg74pzYfLAMQYRtqkVqcvlnGs0ZmJh2F5CLFWuD3sSNPPPnz99+stf3WPtaxGpFYVpKjy1evbBTPt5Sn3v83kh5v08ff70nPrFV0YWllJMdR0DEMz9r9//rEOHW3isa5fr0xGJEMnNGItGrGMwp7sBw90Ja+E1PMOdpPD1Yd8TaroZeMjM8/qPiMP++O///Nv9Tj5//Ph0PpuDqSNRLQQQw4YQEtNU6zTVjDDKj0BYiKiITK0cEZdlvTrsV7XzpZs6ILrmQRQAMCJ2TQzQR3cIoly1u4GZR02qOm3y4ZwHqXuqQyMwRZqRTn5EggAMkZQ9U0SUUk/7WXXt+krcQ053LEHsd/VV15QDPfKkz+UCO4KS2P6Km0PcJGvhbgYJTCAgDwXIChjcQ1hSugIBaoaAiO4bqi91D0AYmEhUAebUsaGGEhECHubGLJflsnQ1NR3PltlrbtM07+f506dPYxhQmOmPazc37RqZFBUB4bVKa4URjvNERMuqh8M+ct8Q4Ga1CgbUJgiZ6FVCPV9YoyTJ27IO7CMXxx5uZnJohYQDUD3WZU0H8BgrIAchEzQCNYX0OxIz+1QLEREGQ35bYAbDjZAOh+nbP/3h/va0Xl6eXl7MoRTRoUTUqnx+fBzddvNURE6Hedq1PM+Y6TVchDKb4vn58quv3+6mFttzQiwITvp3nhcgOCXznBAAC+M2YEaIba26YT7zmcizK4er+fon2XXjVkAkyQkAMoiEMG/bSASxubs5Irg7Blho/k85PB/DImltDg7JBiNLk2u4juEBEOhg4aHmbnZZ191uqiLmnq67DceZNJp4NX7Bho0dQx3SBu3ukUB18KDUjCBMVYhpakU4zM9beAoZIO33jZBN18JfTgeP8EIgjRB4CygyPczT1Gqk09xjaYaImeizLL1N7e7migmFuZRShEsRnjBStop4JdQY+lCzGPgl+8dkvDwD4QggKuX2QNsJn9owJMBh/nJepyYiFBYCHD7Wl0uhHP/G6rgMA6Kr/f6//fafbm5O4frz5yfmioIUviy9CL28nL/7/se761thZkIRbrVmBJOH9a5VmITOl9XcD03meRYmQM6eNAertoklQUg0AUmI2ZwLsUMmQuRcDERIX+Xz+bu0RbUEbH9AkGi6cQAAIABJREFUmHmM0YfiBvvYxEr5nCGRJF0m0BEgwszUnBBqkVxRJNc2r96ssWJrajItECHA3NydiCEiB6hutvaViXe7CZkhwNwjt+6RmVmem4YItDCITaOWc6EMa0Mis/AwAvLXvzxsj6yr5oQtDQq4GcQ2eeeGzAgHAN/2mYkSch1qD5+f+vDulpcMllepQUCtVYpgt1rKbppaEwhXj8JsJSDq+7vD3GRoPngEEMuyyGXtgOiIhR3iQABIIFJqLeuyAgB4xiZQMr0RcZ6my8uFMnwTATyK8G7affvtn+/vTtr7Tw+fkAoXRKB+fplqBfT/8i//FSKQ4Oa4uyiq2tPT4/MLh9vxeDge5lYKbQ4UmKZahKVUJpSSiEnM44cZLT9uSAOIq3kBUDcGEpbAcDPzUMMiyMRSqRTJcMyuuoEIcUP+iHD+W7bryS1j3ohZNklSpOp1GAAzswgjUXrf6UuRikg5JwHYHrilj9jMMjmj8nAMhEACUCY203VZ94cZEIXEyImQRRix6wjfbn/Eam4RFQFEmJnMQs2y0iQCYerDN8JtPi7bKDQlVhsnNBEyueNP0+i6rn0MRKhtcrOu1ldXs1++v/3Ldx8dxCPaVDmzQT1ezsunz8+t8DDPeqAUEWE3X9ZOHoDw+flydbi9Ph2KEDOF+2XtAgjMyEmvdAdmCOwjeyAOsIAIM8hWGxEAa21MEogG4BBAUIX+m2//9Muv7rWvP374eOnGIsvaVY0JFeLf/vrD0sdhN0XENBXv9ObmeDzuADkPHmJkZBYsaeplkiKCWIqUyqaOFH3oGFEKlyJj9AioRZIIxCgennau4Z7K1Vz7uUcHD1QE9DB3HOYesJsK6BjbFYrMnGePAzCLlJSak7nRdrJhZQp3B3S3gEASM8tVPAYGGCG7OnLuTT2fXTNbVgWAWgTDMa2NgO4mUlm4SDE3QiiFu8LlskYEE3KuzQ1qlVpbYiUIYQx1BlzDwCkQKQqjGQBszg4d2Z2kan9z6wGCO1iKLtxYWLvWWjPxc5qg7XYtwqb28vzy08MnDEcAdYvzyoJI6O5MMdauygEuTFUYws/nYWrMEIF97UvYy+Wyn1otWTPTUJUIS4AwhJlpqRUACTyjowgZXBGRiTcLAsY0tWlXXwWGGI6/+d1vfvubbyDiw89P525hbr6oWmH28O9++PD0fJ7ahCzpOLi/OXz1/r6WwpIuNGultpYyeMEU2OcnxVhKrQXCvZVigYXRA9TC1IYBJgyMLS/EYWq2HUVqkJFZiBgWUhKQEF8y09LlZebDNNwgpWjgBuCblS2jtUiqjHVIYaKS1eGwYMoN29Ze2NDhqwMgMJK7gZomQMDGAKSBgG45LxJhjMpFisiyZbVQuMPmEBYhVndTV03CvEJA75r7zKnVjUcQruaXZcthMRsRHh6lUKtSpgab0wlTLpv08NoKA9Y9j6Hh7dPnp/PlcmQmYio8TfX+5uq5lvNlXdcFPHT1Inx1mG4Pbz6/XJal73ZlP+8yIqMPTbcsM2c/NE2NGKfdYfRF0QNQLk6C5BBEwJfeprkUyWI7D/AA2hp/zkE3MpHs5vTnEPNvfvXNn//8e2H68ccfkoEA4VnfMNOPP3742/c/1NpEYDdN87zb7ff/8M0v9vuJaBtqFGYRliIRoA5uQRzkGOA+IoBbFQc09VrIUycHCEgGUVIeCJGKKXKiKlmoikQ4rKrhDoTuDkjC1Ap/cXETURF3Lw4Qgcyk6mMMN6qVqxATmSlyIRIIlMJpviSIRCczkgcF4Y65VgIgdwcM00gRrvsgmh3YzTAcOe9GUjNwfz1vQA1EmBDXdU0rPLMEwPN5dYsErag6gKvGZVlKoSoSgO7ABIS8Lt107KZqgRFuhqVOpfD5w8PaA9DCQj12rbhRIIajeUxTu6GEBESEI0SdWinleDqAxzdf9wwjA3Bmcfe7yypFauEikl1qTlhzXlOYho7CzEzhWqoUd7ciSAJIjA6Efaj5pt8xcAHcuHUAvQ8RAXDXIOGptZdAQvrq/bs//+n3+3n67m8//O3Hn80UqQAggbHIy/nl54fHr96/Px4Pb+5v7m6vj/vd/f1Nm1ogp081wcy86S4QIziH+ozuude3vvowS3w9AuznqRza5dK7OhKyyFhXZnfDMpUmHBAYICxhxiyB0ISklFq4lQK4WXogQs0t0u+KSGTmVLBViQgPDHcL4NLSOq7qma9MBELkEV1t9NGHt1aPh4Yb3wARUCbKkihA0hGsHhtFKBmlROqGEVzK1WFaur6cBxJO0y5FXQBQipRaIRtS9838HTm95UAEIDEP095XZmaqgdJaSyve00uHiFLnUlOZhRBACESUy6UAR6RpdogtemdTzb+29WZmEW4e5iMcHQ6nYw7E3dxi6104eQsQEF6KbO6UnDeiFiEhZmIkECBMwkC4B1BYODsGcEHVCHMsSdejNPWvw2+urv77f/en/VSX8/MPP/0kxNR2w5SQCGiYfv/hYT8fr66O93c3v/z63c31sU211cIsVYREOJVxiEVkMwcj5XSCOZXbKf1GEXYHtf7x4TkAdlNlEQoFxMIwiES4zFXNkAjcHJEhuIhADDUufNxPu3kSwuWyGmFW0zE01DAtXq/uC4dgJALyVNdHqJsbZJIhYn4r4KrLsrr50gcxudWgMA1mAnBAzgxlCGAGJHFdEYkYzW2YiggSuYb3/nwGcxcKC0zIBROVwqoqhAl/ECQgEcroEsxcQx3mEFMVRBturjh0IMnUJK00Ac6YiR2bLhwpc44zRwfzLEy3tlMkyYRzs2fKTH0YAoIUwfyTDoEpgWAzJcsNCmWhA5xOCEJQVUYYw8yC390dhZKEAoi030/Zyqa/KtmcEF5b2+2mxCUjYgAeD4f/7ts/3F4dIvQ//ed/OV/WBHS1UkQKE/7lr98Pi9PxeHtz9fbN7d3tddtNU6lSioiUwgm2YNlmDpRfAmJioYiJMPctX6b2UERubw6ZOtPViKgWRozzMvIgUY/40k9FVp0RWyIOWbqcKD3OrBmIu7kUMGkr8brxCQQiVtXs+uDVn0XCy9JT9jMMEIFEEPH5spwOc66/IpyFVVUtGSoIaUIiCI9ahIt4nrgQiJvaETNkEYJyIZf+CkZEyN1gnjbCzCK5mvC0IxERRrhulxyyFLFXt/4XHE8uvxLy5e7dLBzMwwI8nU15qmViUU7eX4kYxJS23s3yh6+JIQkbQ0pnICBY/hsA1EIt+rDzapLdKW2MRRzDa9vYu9lxmQEzuTkSA2qWalen069/9fXt6QDR//n/+den5wWZ1QYBBwOC//Dh42XV/TwfT4fbu6u725tpai2fQEJEIOLC2wPG2zwy14zpUZCcPeQ8KL/iIjhNtZWCiB4wTXUMJcR16NxKKSSM3iNg43YjhJlFWEQYQu9jjSGSB4nWUkX4uN8ta1+Xbtusi9SHhgegAIabcOa7B25fKFhEWkUAItyQcT/tIryIXFYtspmcdYyAdANCfq/5nTnE2FyryARUJCDM1A1672tX5rLbtf1uGmY5okMioI3F4REp+wGCUgTR+lAP7BpAwmKhcHtVWcp50a3jDmeQ2BQ1ZG5mX1yy6OGUF1jiDCAIyFVZpBYCZnKBWIa6FDfHVBYiURWyiIyLDIPhqEOTtrflQwKamwOYuxwLlVryaAUkQS/53BO5pY0zciCrY2QTSFTm3XRzdfTQv/3tx59+/gxIbooOVEGIPjz8/OHhcZqm43F/e3N6c3sz76daRF7H/7l8dIiyueaBAIlTtQeAFGFuUYrIluSVWCZ8vUeBIRyAGTNroU2NGQHo6kSbh8490GlzPXKrJcLVAze7cF7ZMNSen8/JyWFGluIATBzwulff9gTZXbObu5uIjLSAupVSSy1udpjr2nVqrGpTa2rBxTFKQJimzi5F3kDIBksYDNiivsIBUFrj3Y7XocxlRKQRPptHNe++ndXuDhGMLMK1SC2pIqahDoCdVNW6ZSwVAmbedoQHEibKHgGQcAxL2o3ncCwScCjDjDDMuykmzxuJhCHLS0TDLfqZiAIFiSg42AWnGhYZwtx1qHotogTSWapI44Rz569tb4uIQcBMYVmOAwIAY6gjeWINv/vub//6bz+5Q62s7jmYfjk/f3p43Nd6OO7vrq/e3FydjvtWpBbJNUCRbOe3rOWcJ9Fr0ZDHBoYz47xrpXD+rBwVurtIAXAHrAJ9+PNyAZTdxMRsHoy5l2UH90BmQOCc2QSAIGL4MCsAqxsi976uS0ciAFS1LzOnLd8XLBwBsZJYujTBw2OeWmcGsL6OQFA1whgWx30rwilfDus2TIR3027o6OvqDhQATK0IE3TtEIEMhWvuyqa2203146enDS6QJzzmF80inlkQjIUIzMFja8sQo7HkE+DP566x2/EwJwIPr5VKaWbuZt2GBzAiBCQrJAtTBCBOd2rkBiS9pWbaSgNhhVdb7ZbmRl/cUB4RDsQsQkHOQeBWi6yqEMhuy3D+zVc3LF8IPcyI0trmFvFNVJkWKwJk4RxHSZHR+w8/fUxwDTOP3omFGT5++NkCDvv5+vr09s3t3e3V1GoVYeFaSmuFkCTTwgHoNSh5WxaRCOOrXgxVrXftYwy1rNiEOUcAWZMUxlVt10otghhjWGZovQoA6HULlNEx6BZmBp5LwtC+mhoihjthtCKVuXAmvgFC8CsXOTspBGCA5/MCgbVyX3qKtwCiirTKhUCHpkAJwREDM45SByIJAeUWCHB/2GESX7P4Cwg3Ruxd3R0CGXGzOWKERbgS41SLm/XexxjulkbkrL+FGMLXPszMRt+GnVteJEFYKUWE7IuzminhP4lycY8AZ8pPOESoChEC/R2BiwiQNRttUCCKV4ituYepuzGhmptbq2U3NeJiAW4mgRCRIVfEKXoAZyoWkQsoiADP6UBARMbar0v/4J/do9YGEMva8+N6/vykEYd5Pl0f3r65ff/2ZrfbMVObmjCVlKUyEW3yGQwDFNiAhFA4Qy1Dh/kXQhJu+gViLsJ9DA8Ii2V0ISegVqVVVoNakdF7H+6ZHA2UyVC0waqQA4ARwNSCc+AKEJChAFVEkNx9jJ6ZAG7Z6uV8DgPAIUwdwcZL//z5cb/flVYhkJhraSyB0LvaFvy7bdlDRJhIzUyV0dXHcgliREEzGDryTDdTRBIELoQB/BrNhEjCkqOEcGBEh4Dw1IPYAEJyNHCbCoeLj06hV/MkpT0+r+7WDWyog9dShGVb3OfA0SzXZ4hotgEimagKOVDCytxdCDUQIFppEDBUIaIDmsfmBQm37q6DpSDgsiyIjFJ2U+1rFamtbvMFzF4vN4kBIKVmr2RjjTCM0lpZuhISCyMAE3PhZRlMTITr+WVdlqm002l/f3v77s3tzfWx1hIRRVJBDBHGyFl+ZrmF4IxcKhehjM1L+h0gJDGfiJgpt+lmluweUzcHHd4EhTFpJYCDCUqR3seyALIQUXhoWL7E2/IhAImHar7srfDUSioWWq3HQ+tDX87L+bxGJDd6c6V09XDfz60P388TYpTCAKzuL+dLLeXpuVcBYSRhGwoIGzQMkRiPra6KfenEKV1MX+CiChbBCBIgEuDOG9gq2lQQyQzUrIgEmkhK5RAjfBNpbh0rIRZBhIqAbhruu6mIlM9PZyYkfE1EJwrKmjvrXdduq6pb5EvOiKOrOxIRMgG6mamGhxGS++BUJiIye/LhBqINIEZz771L0uddhYowibD8j//T/1AlxUsY7mvXx6fn77//kQM135gIpE2YQFyEfB2GqqUIAmQskgNov1xeXgJgnnfH4+n+7vp0mkuRWkqWXHnlpTwVIIQ4gacYERimGp6mKgB3QpCyQffzTveAwkSMFrguXd0hp/xUzQKZeNNooZn3PhyAAxgxOAWMyBjmAREsBSEqlZxkm4d7PjHgGL3bMrQPTb6lSMI4HIJEEJimiS7rkFJKq7quw2OqbagXxvm0cx0kGBa28UowVcNqbp5M9IAAd+9DI2IMMKdS09EeY1WCUOvzXAOgj1FKa7viL4aEroHwxXuHDD7UXQdIajsEmKxvQ/rzogrnVkpWLcLopkM13LLXEWHzcHUWmrjk6DqlMY7uHrtWkREcFcO8A9JQQwrT2M1TRCDzrjACRjS1ocPWdXRVcGciJgkbTsRMwrhlQBNKYCCJRbCwaXA+71twA5rHuq5ZkbxSgzMrB3Xop09PQ22e5zbvTleneT9zEQDqGry15JBuddoihkBgm0xVSfRJQjchXsnFEZ7DFQckEhIGQDPrqoiZfCMROhS4FHX0iLGsy5LB8gTgHlu4KW+2REBgN2Ph1IEhgCGc12EerUoJeblcLktHJC6C7okgCE/lDvREyzL3bfgGxASBrUoO8wbkeCCmVjw4vRTuqVjuHo5Aw7QP6yNqEUBmIUrEfETiID0sgmoTd3O35WKIMMYCSMwlYgQkltmJw1Qh8JWACrWyO70MoIhx7lqtTVOyxoYaAnFBU4twHREI9Fp8uW+aKze3IESQQghoCLWQhwAQFE4MFRMlBQeDAZ0J591MMyzL8nJeTDUAapXMsC7M8s//5f+ttahaRFhA4VyMACAVQfMozH0MBEx+ZxFUGwahZqUwOKj1h8fH87B5t98dDlfX19e31/N+Fi4shQnygsinyAEinF8RtExcG9cqTBzhzLKx0bLSRAY3JBZEKVMADstlBzB6OHSPXU2lLiKE2ejdAhN5laWD5eWbE4HCpGZImJVZzgVTkn1ZB4BbRJiZh3CwSI6Jw8LBk7H94eF5au3m+pCan019JnHcH477ajnQCyCSWspQTT6K5o7GfQzzTbZIxBEglAg/AEEEisxGJsSh3iaiLXnDsqg3VdzI8xYRzFy4RNFwX1YlZhFRDoJAiPMy3A2CTVWZCnOpNUwJEYRT+ZvDV0jqnLl7ELNHkAMz96G04Yak1m2CntLziID007kzooYva4cIEd7tpoS3bIxc9wjLIaERoapjRB8ossH5WHhc1gEer5qg8BARxOFDgYFRRvjzy3lZx9Smw3G+uT7d3V0f97sEYmW9j8wMEBDpwSRiJGSC+LICp1zUieTs8nUwC1uMyYYaUwPz0FShYarog1motjzeVDewBSKqveoE04iTPz3C3DAoODfNlgqtoAwfJkKITC6DsMxNJU8+EzMj2rxrx/0sItVj7T3CiaSITFMx1UDQYYAxSRtDh2p6wjxgXcfaFQGQSKTkiPKLBhcB1bPHt0xEKCIBsJl7bUuMIyI1R6III0KPwHAkAVBiikD1ACAgmSZsrT2dO7GEu+ooRTjYIgCjCm1mHwOADGXKdFi3TIVifvXhgqqnCQYM1tHdjAillNwWJgSzipgqAiU9c5pqOpjW3sNj9EV0ZCI8aAQ4lEJZxASAqm+rilctppmHQ63FAyLAws/n8/myMPHhOL+5u3339ubu+nCYmxQuXOhVOutu6WvaBiRIiMFAxJBjBLUgiHDjV0gDYuRQhbesZOLCJbCvK4QxyzCbK5dWp2lHCGP0Vsvau7sHUBFx97wrWSQ5U+5QhdSdKd9LZwTJaTAjE5m5WwSGsHxh5qT8pGRMXq2tVikMEGOswx0ZqhRmdI3RE2hNfaiUQiwRPoaaGiCPsbjH1Gp2ombBm46SEF0YkCBZz5uEPADypUQzVUIxtxSGs0hivAHJHdSISBDJgcZwd1iGU2zPwX6uAewOItwKh3mAbmsg2hI2wCEwJLPVCWNLakNTDUCLEEquNtbaTHOoi5Kicw9Vo+T1B9mwMYwTJyDiBswokUnxhAgUaKqeAase4ab5nzm7jABzY/QOAADuflnWp+eXCJh3++ur493t6d3b28x3IaH0ryV5vzBnQA4gEBBQvivGSLUWRK4liBkimDAQGPODCyJK4GUuScZYx+itiKpXjozWG+YM8fHj49SYhSuS5g4lbWeZJJ+R94ibv+ZV5lpKmXYTIgqihbsHUgpmnIFsG7igB3RzJppq2U1Spvb8fInASA93YQRPHW4RCXTKCNHw3rX3wVwP+2rmiDS16h4WThTCyJKB9VxEkPmL78tpexliU1WTQQAKc8qFQ0oJj1xQ5nIcs8orOBR8RWIERwoTQqllHZ6TEXdLwNmrpSqI6JWuDRAZ5g4AyIRUUsq7bYFFJDcK7sEsBp45aBScuvNai1kQBDH3rsm1OBz3gslihcAkwHEQsiatiWVX6uh9u5kJmdmACFWILJwCAnCa6tXV4e7m6v7u+nTYixC+crAAYSv6iWUzfCBsVvMg4V1rmcj+dzYtkWTxRrDlZyBxnQCgL+uyruFIiIhRRYBQSq2Fzy/PY/Rd2xVhJq5VclvpgYhorr0n2SsNKUkr4Vpam2opNaH/Q0d4roDh6jTv94fnl/P5vHgOEByQ4zQ3xEgMakqyeh/7PYRHBgn00V01kGLR5/MLIQXw0MVsTK1eH6ar0+67D0/CBYncDJk2/E0uTDOzZ7OiEhOaWa700eGyLoTgDkScM1i1yJizHLBFoG5kriBitYDAdQzKNJUAloIaubwPzwyMMNVt65dDW8xxiaulzRUBwTKDLHdkhOSYt45UccsoUchseCAUpNIqIQMm2gwFwoU2ePvWBLiGBRByhJqlEwaRNJws1q4ihORsiILTNM276eb69Ob+9vrq1KZWJUN+WEQgPzSMdFinCiX9EqXQbmqbKACDkAGjIGGabxDcLNesEcjMNkYfgwJr4d4HhEmpmObZsFr49ubUSgUCN0PAJMzkPqB3aMdJuJ4vT4WZmfMlBgBiCncg0jDwICFwEYDdbuq9E7MIq7oTE0TKWjzjck0RQpiAONzMiRHM7Xxea+F1rO6BkCDmIGJ3n1orVdSiNcFAElrNwyGvk9zWBygzm0ZAFABDBACPMLPRO6ZVFQCC+gh+1RqEuaEhYCBFGIRl/0tIy8WG+uQBBJel71pl5qRFAm4MvsixZUREMFLOF7KIN9VXExoxy8aJigBGN0vVRs4kCEHN0A3CHfByvuQdSITLqhIAfxeQMHvYdo1yAbdwM3cNnCowkIWp8tTEHTMV77Cn43H/5v769vo470otMtUCWN2DEEtpSKjDAiIXlCIkQswlF+KmEaRcZLPEEXByoQKYeTsEpb1cLgQ41AAhVNXsuJP81glyzf3qNHEgKoCB5ulLA4xWJZAidNcaIAhiN/e07AIKEzP1yxpI+eWEx88fHwOREEZPEK8BQK5Bp1baRIAYWzLwFsxuaoRYC48xPN9+BHBgijZJrUzMT5eOlxG5xbKtE2LKktzMzM2lSmEJFHNLl1+iZbfthgcRehgTp/OPLBwjdxKloHDd1eKITy/rZR1FJNuaqdWh3cIZOMVB4bmTixTfp41qC12BzXhMxLF1u5A5kK/7TZAEzXmKFTggOCBzUlJ3n0Fml8v6/HKWq+tDa3VzLoSlcVHVI+DlPLKacndzygHYqwiRiAhYph29ubt59/b2+uqQ4gpiKpkPAEDChFRLGgZjo/PmKDxCczIIBB6AkW4Bj4AsbwDd3UH0cvEACAuAcO2jI4BwA2bkghCXJW923ryZqS2CAPNUwoU7MeXMwcM1toK3iAwdXZXUSQqAUz49kNUwqurah6piensBAnDoEJMwFyEfIMJInAJCkZwFsmqHfApbAXBMO0xfY9sYQ6YDFtm0T69LQkQi8AhBwsh+zDcnJ3LlcHc0gM16xiQUHpQ6HwcgZpkqmUdXL0yqQwEK4ZmgtVIk84QZIMjJyd3MAW1YrpuQkBEjadHEvY/ARFZCBCTnMPtnNwdm9MhBKm3nbhpaKYuAhEVk+y5v3ty0WocauEO4b8Z9XPuy9o4OBoAIwhzhxAyALMyODmgeh8Ph7Zu769Ncm7RSOfEpr21meiIgr0JAh+DcmSIgUq0NEISJiYZZoi4YSXYM5hoxuo7owpnXkSgxdvL9vG9TG4CF6bKMFH+7OTO5p+gqMWw5xAGE0OEAQEIU7Ns1CB4hpeRbDAgZwqye6wOE8DCNCELyrckPJChSdauIi/dLRKxD3XC3K8vqDlBrqUWSV1Kq6LChPSwMHNEDxQwAghCYZX84znN7+vy49BUCFZQwwiyEtuECCgRYQEa0jBXgVcGxPbPBuc/N0ZxvOPaYWtnPVRUJdFl0zIbIFuDuFOFhiRohBN32vB5BudcOB0uLNYIw+6ZsRHMrWx+dlAeIILXNXJAWZGFyj4BgJEBXcyCQx+cLxoUZhSjhJcMy48jzDgGnEZZy1yy1GDFYYDskGZhfLroO+P/aO7scS5LkOtsxM/eIuLcqs7p7epockS/Sw5CABAjgiwCtT+vQDrQukjPTXVWZeSPC3X70YJFsrUFIfywUsurmjR93O+d857ZlXeW1E1+XXjqwihxjatNF25izNVikIkmTWb48fSamb99fayQLZEZKaz3zbfdiKYjIeU7zsDlu223b1tY6qAQNJqo6CMxhQB3Lk0DkbnWurLuLmcEeXo1VngGACZbOYPcoh4jNq5mhbCkL2P3y7VVmuJyYxLBwirQ5b0vb1kVVcj8zaZpVm4yHjTG1tybNyac5yh2bWQWJnphzvr2xRc3Gr2ixNFBmZKiwT9elhZXeXa5rTpAWWyEBQJSFOmpbVzoN0Hv7+YfPv30/mvZxzpe38/N9Fa6y4tqCeTVMS1WCgBliNpEoTEnR3YmS4/J1qCgRSm2ndC7Xbeere7zCjFFOIc+rbwBEpH/5y6+LSmtS9uasZlPwRRIhaBMiTgDAuvZ9P/f96MsyPSJ5W/sPz0+3+60JRCU8Wm9Lax5OQO89M6bn4ziXgEoPwtsxkWHMLZjI/mLOAjNnEDgFpJHLsjz24W4EFpVMmh4+Z1deem99uUxUEdqEMjzDP</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8Wa8uWZIltMxsb3f/pjPce+PeyJgyMzKrssiiWqIHoPuh4alBakBC4hXBb+KJB954ZRJIvEBD02oxSKhaVVlZWZVZlVNERtzpTN/5Bnff22zxsP1E1W9AsaW459w4536ff9ttm621bJkD365v17fr2/Xt+nZ9u75d365v17fr2/Xt+nZ9u75d365v17fr2/Xt+nZ9u/7/vuSHn70QUQFUhcHifnt/nGsIkLrOVAOhVIIQgGh/iggEgCCcIAgRdEnH2cMpSrL9GCIY+nx5sbb2FwLCiOXtCYxTmUs1IUS8xuzVS6ikPKyneZynKWV5drFdrXoIpF0ABPxb1/PN6woVAhEBIaogARLJBKLncXx/e67hAlkN+eXzawfubm8+ePmhaDCoZqomCoGo6rDqzVK/MhnKj//BJ//oH//983zzv/5P/9e/+t9uFJJSPhwe9je3v/+j35/n+md/+WsgQNltu+vdWlSA5e35N7tNQoSEyNOnf/qGoLT/yyDC425/PBwnERFR0ld99+xqbSIBIUlSVUjpcgJAgQIASq3uIUIGIEKGBwCKiIBBAdo+tT3ieK6P57FdoloWgVcHICoCuDsAMdOn99htcme2XDUAiBCiCFIAgu64fzxNYwkgK64uV5fbVa2e/uN/8g/7LhNMpgKeztOvvnh/83AOdx22ucsRFGF4tOAKUFVNTE0AeCkCeq2gbwdzseOx7Ib8ycsX7+/39PmzjeruYv3sMpmYCEUiWN0BEgrit29u93dHelEv57k8jIXSb7cv+83F4XBze/umS/y7f/j5px+9EFVAwBBB2xoRMCAiqlBVEqIQgYo+/Rkkui4J5O3N/f/9J1+cpqKiL6/Wf/jDTwrw8z//2avvftckQKaus9SZ0URy110/u9pu17vLQbbz3/8PPv8Y/wnw5e/9YPgf7bdJrcvdw82b91+9+c/+8/90f5r+i//qv42gCj7/5PqPfv9DSwnUoHu0qFhuTY128WxXCAqEy6ehQiGER53n8pO/+Oqvf/vGUpdNS60ffbD7u3/4qaoFJSIIZLVV3282g4qepykYluRwHI/nSRhBEUSpUd1FRFSEy5EUFRUIQfJ3r+//+qsbUIPRrbYCjudZDclSBEuZzEwsmYiIQPjDT692qw6yvKQIhBAVkh4E43iefvqL17cPjwyuOv3xD1/9wfdeEZr6lNZDEihUwMimv/fZyx9GWLYv3p/uTkGPAGiOdjhFVExVNFm2VBQ553maV4kvr/u5xLTj1fbqH/2b//Bf/exP3719ve5qh9MXr+eXz68vLlYpJRIRDAYgJMtcHo+l63Idp/NYYevV5urhdDq8e20a2ZL7nFPargeotRTRroSEigRhIposqRAUAEtOE4GoUkVSMojsxrHLqbiI0kN+8Wd/Ag+cz+9+eqOipqYG1UwGgdzl18k0J0spwH/+X0uV/1LEp8PocwjazWY4//d//i9n6ZIlGk10teq2m5WZiVpEeI1gtFRGMkgPitDEWj5WfdrWp2jwKHOyYehT0pw0WRZgu+k364HQICMIIuf88nrX5SQQER7OY9/l8CChAvcIRpcCImaqkLbhqmghR0ZEdF3qcwJ0rjWpUdB1IaKWDGAyVTNRqCiJZLjcrLbrLpzQlrIVCBFdLirqPLuZpWQMiqkQQ9fNlelcq1YjqYJg1Bqh0vVD16Wun/RMmgk9RBls6RMIUrwQRK2ecko5Db28fHbxsH8sdw/zmP74z//fvkuffe/V8Xj+y9989ZsvvujzV59/7zt/8MOPu5xEJYmRJOWTD5+9v69d7kEdhuyUr99+fdjfdt3wuH+4vLzcrrsaDMKWQ8hwBEJE2/kkJMiAtDKkgEir7hCRIKuHqEgr3AKElFr48Fjn0SAQCKBQireUIiJnKOCgiCIAAtpqNhF0UkmCQdE//hf/h19+KnkghWC7JIFEK5Lt1Ski0f6eTKTFQhDCoOhTHWIsrxFoRc5ERVUtqZmScESEkGRAvO5P5912FR6HcZpLLfsqQErKQFIGEzTItkOi1Hb4AHEPD5BwR5CgA/SoAvWIpBLhJgKF6rIhKpSlSoiacAEtRLtiWaBLrbXUAlIUIM5zFY+klqbqK6ophBRISilgQXiESRIL1KBItFINbWgigjmZNrxEhfI8ju9v7sl49ux6tbtKw2bgWCHXVxdD319crN99/fawf5zmYsnYkg4UEteX2+9+7L/+3cP+MD2eb44PN5su/Uf/3j85TIe/+ItffP3m/YtnVwBqdZBQZfAJ1wSp3yDFcKoJSVBFlwMhoioegJIETBvGC3qDAwhAJYD2rTScIWAgQAaIEIZAQYISQg2qCBjuFDBCtcU0gg03EhFQhRIUAbm8bAtCsOEyiiAoEAZUQIAmStJBUNVEWuRZmJqZNqwp7dMLPHA8T9WdkFJqK70E2CChKBGgQqiqAALts1PYEio82m80dCWMCIAMwhQUUVmOzBKeqlRRLO//BJaXrQ6BOFgjGNqiOci5eI1YDSl1KdHdKSoEkZJiyVo0gwIl3NsBEglE21IQKeeoDnIuxes0ZLOuWw1d3/fWJef0cJ4e9ocXu831bpU++fD68qKME4AFO1CIYFAFn73aDLn82c9vXr++ybn/5KNXn3z68Z//7E/6LBebju61OugejWAIECJCsm2OqGpECOCiqli2BW1/RUxIijyVUzbUHR4ATbjE6RIMdEpQniJGVUAJcYSCriIEgkRQwBbzqREe1XbAIVARLGRE4LEwFgBELBg3wHY3lrsPEtQG0xERJMyUEe6RTUi4e045ZDkTDZ1Ok7fXNhOGEA0PLtlGIKKAKJeb30ImTIxLSmpgD423hEdLv6BAQiEtM/EJM6mKqJCQJYcBohBEIBAM1lJJfzrXWt0rQyWSCbEcYhGDkNIOKGAiQXqER5BUSjBEhVQIaqkqIGOezqrqwdOpJEnCWkY/jzOj1nH68uE4bvMZqRAenOa7dhMYLLEkpRpxnn1Y7z76JOeUX7x8OQybr7/6ci5uimk+HY/n8zinxBoRLcmg7Ru8RnUvzlocoCo+evV8t+4gIghQg5VQgQQRZEs+AZqQT2xwgcUQQEknEsIhgLBUCkIESiGdjXswQGHjbggsQQ+haINZC4dsYS41SMDDSUhLnBC1p7gkg1DV6g6yehxPZ68xDD2DFHTJQAl3SV0yAdkOEwFGBLWFeIAMaahXZDlVqsqIp6P3RBLb3yn0hnQpKst3JCMkJUDBgFBEwZZixExUZKGtC7Vf6L5Xd68KmJmpAguumWuF9OkPhny66BSYRMbCMslTyVEVUdUntOEBBWT5GhjH0cxask4pVa83j8dz8ZQTRCJCIcmyrvNNdQGRVFMWg6qqCkhxp3upLlEHZeqjgx1K+ur1l//sX5xubu4M2HVJNc2zf/XmLqU8laKi01xFhBHjXIZhrZi3m/X+cPrBd78D8nA8bVYZAAIKJ8PMIhYdxOObXNDyGvANrloyNYHavpEIiCDYQjMgxlgKqmApqCKq0k44JASiYgBFlKQC3iqxtyBYUoFiiesGG1XQwpeB4/F8OIzXm2E3pFa5Ta3r0v5xMktD30OlZYbGv4MgFAhVARQhUErL07IQTFBUEUGC7aaCdAQbeX9KTwSBKDU0maqQCISEmiGqtFKBBeXaApgU4KLJlLmo2ofPdu5rkh6REkphEOnZTR3HNPXp6ipfvEz3p/jd7fR275VSfNX3neYNI8AotUYtXucgRVC8KhWQfugvLq9W2V7sZOhULFHFpF2qPOlG8JaeBYLIpu7hpcylHo+n48FLKV5LuM5ltv3bL968cdHt1eXFKoWqEG/e3W836+dXm7v96TSVz77zopTy/ouH3e4yq0xlmsv8eDhBYarLGYXUBkcMwieNAUIGotF89zBRF+oigYgAxnjSIQAwGrWIlrAaEBMBl9wu1HZyW+xGq2lYWIcvd0UCT6iZVF1CrSWWhWCQQim13NydSoFmy5aiMRGyQh5OQT1//LJDe7v2LmbGACWoBEVFQDNKq9DEQuxVBFAFoxV9NHRvKX/w8kP3+vBwT4gqa4Wo5NyB0bC8qjDaPiRRsSf9TCCiEgEu9D/Ok08l+iEjEgUIljo7pXqkix/4X/ym/vFNWb8d/85H9gc/6q761W/K6Y/fTHPQLHXZ2q53ixJEkKXWOhf3Ustolo6nY7643l49QzkszARiIqoiAqeYiJElGsdCCIUk4F5rqWWe53GaxulxXj3u74e5pmTr3bV1aVYLCItP03ScavV6Oo2PxzPrPE/z+VQeDseHm3fufnV1eThNV5fb51frBXS0EqJmQUqr/iKgR4QKg0IKommaHgoJoaIBOFBaZaRB2l1rJFDQUHNTXIF2cCUhGCISHtVrzplARMPFUYMNcgGwhfYt/zXqiaZqMWr1/WkO5G9ya2OLLT7uj+WD6kNnznhKoqEiMJOIiECEJm1kQAlHiFIpIk3tgUOeIIKIpR//63+02V389svXf/KnPyE0pkJDSpZznsdxEfcaoBZRgalClgQmqgBU6E3kp+xP0/7kATRIT0ZWzrUikKYfn16/Ez2lc+Bf/mq8vR3/nX97+u4nu8fj9Cc38+F4yl1aD6tWv4tHuKuZiMKSikQJl0Qvv3v9ehwfn+1WV7vVep1UIaqLJN/Ue9UEBhmxkCBVUdGUU0rmKYX6cZpRzjMgQK1j8bxGVtFSikDmcXx3Pk91niqOY1WFpX48zydHsmGscjiXYe1zYc7osy1wihFgWiCANn4gIBEMhTRaSJUAtAEtPAm834j0KtqqbIPgZDSdWcBg0+K5gAHRpld5C3QgIAr6E0Jagkyb2tGCbCHKIuLhpQRSMP4GkHNREFDOfp7mVd9BwCXUIKYChMJEoLb0S0AGJBgULLSgoQNQQFC7rdnqzf3j+/vHP//LX5ZScr9OmWIKssxjhItKE95EjPRS+eWb/YfPN9t110AonxhnBQhOpURICffqLSVJwjiWoKd/9n/65RY14t2tqcqfvB3L/1L+4d+Lz3+wui/1FzdlmmZ373LXdV02G72WabZsndkEFi/lWAn4XH/1m9/9MvzZ9fbv//j7292KYKNagDhDfKE1qtEwUuMvqmY5yewz+ih3nUmpCC9xOHRXL1JeD0Mn9Pv9MTTbevPhbj0Mw9IlK3Wcpg8//LDvunme3z4cv37/eLEdPnxx8cnLy8vdoKb6VAHbbdMmhiqckEWDT23HFGALRICirXkD4RP3b1x9yTKACDTYpBUhlvSUkiW1piALoCKiWgnDU7VZqlsrraoqANW05YAy1wasGmpqpJCtGwVExOk0Xl9sWjoOd2lHQ2BCbwrFk8LRdBA2/WaRalrRjAj88ldfvH8YX7+9q15zsmSaTSE55jnIWmehMsiWtIJBnqfyV795u918tNsMohTqohlEU6AXeUgWpLToyVOpEWGCly+vhx/9nr6/8aDNtfxmf1rf+uUHOWf+1ZsziOoxl1lawYbO80RSVIXMuQtGLQUiXbJnV9c/+sH3nl9vw2u4RwTD3aO408MjvFZ3r9VrmWsp01ynaSpz9egKduV806dsZmaWcj/0nUvu+z4YH7588dkn33lxfbFdr1Z9TqYqMY+ncZqGrNshr7f91W63Xa/HUl+/e3h7cwSw2wxdzq27d5qmL77eV/dkrcX2IOEqgNiSarSdeDYg5WzaXEPHEgQRDMHCJg1o58Vsey1mLXSuLleffHjdEEODXlhaNGrLqVIVbWmoIfKGY8OjlPn24VSq5JyTSTJNKjlZMuuy9in1yXLCZt2ZiprJ0gNcVGkB+I3+F0t1JMOejlr7KgIVG4bVu9vj6TyWMtfqppJyX71E9aYCNMV6IUcgQC/1kw8vvvud52a6iLSBpc0R4aU8HmdyUUGaAJcUqz5fb7v0+Pjwk7/oX7+P97dl2D5fDasI/j/7qfvl/vr3dp34w9mJcPd5nLqcKLLdbEuZz7U0bnx79/7dm3ebzW677lLWc8XM1e7i8vh4dz48CKJddqsb5ELG2yFwZ7Dphpfn+e75dt2omIe79uh3cy3B2KzXVxer8XyYppHBVZdUaIJ1rw93p6o8+igtNlfrl892283q5vbhT3/+1e3D49/50acXuxUWrEhVU9UkknfPWKamRZgJw5NpE4nMOrKGV32Sgxt5bMItscD9aH4A0dZ1aJkJpHtks0YUVNu9J/QbqZZL3781yUTUmoIQx/M0T77qciu3DfVw6XEJSCTMM+73p2dXWwXVtL0/yAbg2oERilrLxliUvNYWIERT7jdj0WFI293x6/fvlw/RJP9Cj1BABCYW8EaoI2pEuPvPf/2Vkx8+v3i2W3VdXlgtWL3OJTb9YObVHcx8YlFOTlNJ5/Ppd2+++u1XUxnl8x+tFcg5T+G/fDP/g4/Pr54PD8dHAF1O0zRH1KkUUy2lnM/n/eN+s97QOU3j5cVV6obT8fCnP/nJn2l6/uL5J68+sDqtB1kqxFMTXQXhi2iTjGSyJhXX07AaFCIqc/BxNrBe7Fb7/fGx1vPxoday7vrtkJJqzonhLA7IkGU1dKvVkLscsMfTsbf02Ucv94+nX/3uzVzKP/g7n19shuqUVkVFNOf87BUjKEAg5WStzxhBsZQSEOH1G1HSTIkmcFDVGB5Bj3CPICoZ7i2U94/T+/vDy+eXDSM12kRBEiUQHk/IXrgIT0JG03fe3RzujjM0Rzi5QEiBkC5Qf9L7jtN4sR066wCo2qLAkEJAFIwAFOagRyHh0c6F394f396Xivvb+8eb25vpfGqytqk2VtsEZ4+aUmpnQrXJsGwN0/Fc/uKvvvyrX+mL691nHz37+OWzLpnXmMayPxQng3CnkwKqtLoAqhmjnvaH/eE4zeehX2lKfZdTTrfn6WKqF9/pf/XVaZrnCL5//26cyno1HI+H/X6fcgIRwe12RzCnYbPZmOp4PsylHB73+8dTMlzshtTqRWrJ3rou59x1Q5eTWc5dSqvN9dv9qY7jRMzUQjmM7uB3P/1os8qHw8NcME3z4+Px/vGQUrrY5u16parnyUV1N/TDeuhyXq2H7aq/3K2TwmxYrfthWH359Q3I73zw7Pb+8fXNGQpron4woCDEtOs6qB7PZQpG0BnF/Tx7AHNgrjHXmD3G6jWCksYaTlYiBEEU91qj0edS66rTF8+2LZJU0IJb9W8k9KVnIWKqRNTqtdZpKl++ub9/HKcaUynjXKa5TnOZSplKlFKn6nOtXoOM64u+y3lBeU1EDQSBlnHZ2GcwSEYESi2l1F99+fD17ePpNL97/9arO12X8EKXO8udiDJinuecLKKmlFUVYC2l1aK5FKEE/PFx/OrdfrNKu3Xv7ofj/NW7h3PlcaoPj8fDOB7O03Gc51qGbBfrPhUPETckD//666+7ri+lbLfrMMP9fK8Px8f9NFVN6e37t6ths14NqlKqh9Mj2u/vNtvbu/vdbtv3g46ppZl5HsnVuu+12SFEPdw05S7F0ktrXF92z34Q3bu/PN2PhQ4eTzNFfviDTxX++s2br1/fUNKrD16dz6eHh8N26B9WIgQDx9NUXKZpMpMohaR3ebMenl3uprm+28/bVf7+Z5840gcffPrbr96JIKkm1W+aJ5aSQlLSeXYIJWhJW4tShdV9s+qP5zncQQThwlrrNM+WkomczufwUmt4uFoasgnz7F49Mpb2b8Pk7gTpEYuFT6SVulK91nk8l+M4ZbNV37kIXZA1WzKTFkIq4tGSJsXrw/1hnrzrrDoZAUgybYRFRKIJhYAJRDXcp+pR4/7ufqy2XnVeg3BEcyCICIIepRYSwiT828yY7o2511rJgKpAQ4jw43F+2J9IuvNiPTxOdRrH6k5G64+GIyKO5ykpgmRhEXKaHm9vby6vLmstfdf/4nS4POagXF5f1fHeyxTdpkzzarNarYbj6ahqpZRpGpMagLlMq9Uu5xV4juDQ98+vr8/nokJLpmIiUqVMxXVRDxDO3O/SsN6/+52pmMpUylzr59//LAnfvXt/f39y51hOx9Ph+YtX4zQx4v7uOB5OOef9JJJynseYJzOppZ5Vp3G96nM3rK4Guz2Wi916KtGtrj75+Hv7/eQeopqTmhqIQLgHiJJlO2zmUpeumyKrJEuqcrVO56mcprk1SCC43g1Nl6l1GMd5vVl3ZgBS1qHLnaWvvr5rTDI1j6U0D4A84dIntTiilhoRNVA9tquh73oRuCNAEkmVWPrSvjRKKchCOR6Lzy4CdxJsYpCqFHdb9CS0ri+A4lGd1xeb26/v9nNt3KaJMmCT4YOgMDbb3WTJfX7qRPmTOsCF14IN8q2GYSz88u0jiS5bMsvGzdB1KUHCJKkJw0W1eOtvttpv4ZX7/d0wrJ5dXe3fvX2W7Bo7w6jwz78Xf/3rnC2fx2m1XqsKIzTlu9ubq8vrAK4ur0qZp7mkbqWm0/m4Wm02u0ufx8P5qEK1aD6KRvUbB6zVP7i4ePv+5u7ufuh7it89Hl+9fLFb5fv7+y++fuclrq8vFqOByu/94PMIz6a1FDUzToT0uxeN9s0KgU5n34/hN8daptklr86q+pOf/9Xf/fHv//q3v73bH9HYPmNRAVRUdei6EGybD1cQAcJVJKlBkOa6A0wRIWqgs7iXUnJK/TA4QVURCbVCK3P97Zv7Et6n3GezpH1OWQ1Crz5VH+eqKipWw909J2NwLMUrm652nmaBiGoybYDJvWmliKAQZgrVTmFmzS1ZvaqYJSu1CKS4A/Tli6saFOth++z6+n5/aIIeRYRBaDKDKoGIKiJmNk3V1ILEE2Xz1m77RoUTcY+7x3MzCzBEDbXU4lVFRbTLbIbKdW/jXFM7II3EhnCcztM8C/lPX149W/PxM3nxr/D13cNfnx5K5S6rmATp1XPuUkqb7Sb3GYjT6TjNY53H9dA18Htz+/4nPysfvLgus4uUYAhFVM2QLF/vttN8Oo/8eNj+8hd/fhxLzijOi/Xqow+u6dPh8Xi52Th0GPq+77brzVzKbrubyxRgKp6SIeVSPFLvESG5eu1SiqC7AwmCcxmner683Lx9997x+9atqp9EwqmMCoiZhgOIIgEVgeXeckoiYgZEuIpQ+i5Xrx4O+lzFayVENZtirl4DxQMCmR1SBLDUSYQHjlNgCjMXhgfnutiIghDMpmYmPlUPqBqUplCxbp27LhFyOo/hVcCcVSFOh4ipjfOMKrNKzmCweg2votYoanM/NMsugx4IuhfM5fHwePTwiJCFpDRQVxnWJLqHu3c5913Xmdo0T4xKIMJJYXDxUJEgp3nq+6yWo7a0KFMpfUpDnyFGxlSLiaj2XbIkIoQ3F4NGkJLUXiT5wXb733/xq3/8b63//Veb/+Z/YDp0pqIqZioiw9Afj0fVbr1ez3PZbYd5KrVMc0pdVkWoKUFq98mnP7jYrkup4WGmEAOkhisY4QqdS/nep9///mc/zDmradMQVOT7PzI1g5oIVO3yYttsUq2Zo2ZNzgz3plSWUooXBk0VQCk1ZU2Whr7vuz4Qj7X/R//uf5hzspS81Ool515NESxlquEIqKmqygIlRVTXw9pybgT9dD7O89xIqgdz8+ZHqGVVqKiouBevXquP41R9VmjxGrWk1FHQ5exBX8RFluoRtZZaagkPj5rU5KmjriJNcGwi3jSPZSqqCkTzynutTbuKhYoG2XoS9Dp7CFTxpHhoP3z48vlPf/azX//6N2CznDBAFZfmtaIjSrgjJ5UcjIiKiADcW8MtAiFcuvAi8uknH/fWlYjTeYxoAVxBBHi17j579WLo0nrQWmtSVQkj6YiUFNDcdTNlqvDj8N/9z/x7fwSY9uvrbToAhpBwpmRBnE7nF8+vH+6/UonqUSvCI5yB6EShfPny1fUHr9arFSwJgKBlM02tS0g0wtUa7GpmooIIS7nrehGqpTa6YaqWkqmJgsGUcvU6l9lEx/E0rFZmJpBglHmeS21C+WoYui43hluL57673G1Tyn3f5dzVOjffzjSPCjHTUisjRHScxv1+r2rVfdgMZqndsNVuU+f5PI7D0JsmZ52mOVsmUGqhRwkHLfUJ5hnkDFHFRBFDUkZQbZ6Oh9N5niYuThC4V/cAKapBJE1IrNUZFLFuvbKcvLpr0p5BhtcIzJysV4NU92zGiKapluoCGiQYqqpqTWPLppPX1WoTokAiKiSAprhqNJkuRMRAtdyfDwevDoFJ82koRflkmiPFLJ0Lj6ejMxaHmgihpVZIiOr5fDwefa88jnPa7i5y7gQIRp0nMl0/u5xVvzyM311/Qhx//dV49Wx7fnf6sEt3ydTsNB5FV9M0Rq2n9SqCAiPn9brfDEm1Gf1URB4e93/205+qqYjmlJpTXtWaWzTCVS2ZiVlnBtV2JlJKZgnSwAe8FtFkpmoWtXp4kD6XPuPu4fE8uy6sKkjWWqZpqqV4hFpSQcpd7joEg55SSim1qFWFe7TGpYjklGr16iU8SqkA3Rl0NPjSZrSa84KRLYuJu4NUtWDrI0pEVUvhUWoptbTOmJp2liiM6qTXUuRv5mhE1OZpJCNZtpzUzCDRNGGEionC3RGhlgi2aw7Co/bdICK1lmZxbSFANqtjCKCmDElJu5yJuL9/9Fpatyu8GWFFrZkZF0+KgRG1zpOoNy8alCoqaigVsG+G2QLy9s2bMo9cJgGeTPXhoJ4e9XUiGElRPdJ2e9l1SUSJODw8FPdaZumydXi9efjs+fDFfLi67P/y57fHaV4NpUocDvuol17OKaW7m9d0juPRVNfrQSQYhHgDAF/++pdfmvW5I9j1fZv0mcvUtGJTA2ApNTEpmTbputZKIprjiSJCkQRTE3gt1SmgiJhJKU6GWmpuLC8lln4Dn2YEFod7OFUF0QT/Bl6bJCymVurs4SBSSmZGCMNrdS6W2W8EXQJELMeEixDLJ09WM/oquJir+fTzxcImi9QuQlkcp839DACqyaK32cQAACAASURBVMzCHdKcwALQpLkXCaFZYlBNQQk6KAeBiDbnJwRNWH5y+S6u4WbSVTUC1Wu2JKZKE6/RrhFUy6khr+XD0H1eTB1LnxKCTFCFZgpodZrKeD43CjwXJ13FyFBVRn08xZ5w0qIiPB1Pj+OoAW0Ch6Wh1Op1/s1Ufxd+nkcv3fxwKqXKahjHKamY2nk8Ckh4l3O/XUd4m99qrN20+dgl9/08zyJmScO9lNLuGMMBqU+9dFWDoM0rUQRRA0AEpLWIIFLa6TdN4cW9ku3gQkRUXU0FS+O74T8RFUJU3aP1mj34ZPqXnHKjY6FEyq1JF86G6kRTazb1/bDbXeacx/PpeNg7GzZsxnPJJqrm7h6uao2UhUc7tCQU4tHMY8KgKskQNSFCSut9mupSixgR4lzmTJpjd/KQp750zgiGlMV5KWJtPGrxTUZUryrq0TxX/s2cTnPtNoNjAFm0Sm0ZlctPm+AWIiSj6zZeC8zUKyAkPIJRQTE1FQ221kZ1d2mW+AUe1iA9Kp9mDdphU5XUmCpZKpFE+76LiLtxfuehql/+6nS9Wr8vIuIJpCL3qc6FUZeRqiSroSN5PJ3IAGPpsAWlFRR6qWNnPdjkDCVYasGSUUCw1mKKuhghJJpDiiISomFqEbWpRBWzQNma861YwABvyKJ11MwsqS5eRT5Vu8Vc2mAMPSqjSVhEKTlnuouygfBllis4neYyHgmgSedizacpFEiY5tz1XucI9TYvLQglIyDtd2BKYYISBhWoNCeuLEqNKBp6FwGkeJVmzZDF+tp8Is204F5AaTMr3zTzl55Dm6cTNglNIija8pGaItC898EwtSrLfKcsEhtEEgChk2Gqtc6lFLR4hhIubO4iujCpiAMwYTCa4+bJPwm2aeRFJ6Z4VDM11bT0aCECcQYjQFHLytndx1JKrV22bAaJ4lFKaTRKIZZTqyS6eK6edrB5dg21FDNl+DyeAgqy63oQyVKtBSKgqMTiwVu8hXxy2UObMy9CQU2CaFW5JlDbXAMh4hBbXIQCkDXq3yplLeyTLuNIEAkT67rspUZ4hARLFJhK0/yF7V24GLE9mgOC2oxbbO1oIcPneQoT7VKeipfaxgCEcATM0mq1nedz9WY6IgDTJGqk0/Ekui74gSKZRgZNSJeIth0LmGOEy/IvWhteFvzdhqWWhCIBLrEjYMq9NYNwWcr/7DWR2k5yM9Xq38z+tZNf5hkgYSTINp7+zbjm8unFxdvgPKWpwQwPNteb9X3PWgnALZmoaWK05COMULUyz/uH2/O4UnK922m216cbKQZnn7NwfByLiUqCooU4I5gMKsb2Pm1IaBks83kcTcXMVHQuc2LkvjuOJw8XTSqyubzqkjI8It7fPZCxHjavPnz1uH8sHozwqIfDMZld7HbrPiUNVQP0PJ7f3uy7lC4v+hqwnFQ0IsbxfDie+5xWm60q5rmUOmVNm1W+u9+babfd9iaSO49OwcPx8Xh6XA3D5cWueVSTpbnUt+9uBRiGflgPbbrfxE7n0/F4hmjXpfVqHbV61PNprOHzXCCSLPd9l1REtc6nMk+1uCpS17UGfClzw9cMimpO1jzhDQWEF3dfrdaWbZ6rqmXTuZY61b8FMRBUFdQ6m2hprRVgve4J9XkudVaoqIIllCJS3KPSo252l2q5TGOr1SpPXjgVo9EoosXnbGopT1MJiEAoNEnALCKgC1QBSz0zI6hQCsP9fDqp6Xc+/Gg9DDEdjTWKV/p+HNOLZxd9l3LuTqfT4/FcSgmHIJIlocMrhOQsCEiIqMosuowgeFTVFFEZUmsBqNbcCapKKDrr6OdpjiGlly+fH4+P57FcbFf7xyMhF9vderXuVqvO1JTFy+3DQ8p96uzZ1c40aokSdTxP+8eAdCnZXCs0LnZ9zn3OuLk7iNlgQLaJ2tzwpdSUs6gFPcJErevTduhVapdzMA6Hc77Qq922DQuM46nvczLZDL1qNPE2Kbo+mejQp+e7taqJ0MzKpv/NXNRsu15//OqZqaacEbzdP/72d28aw7CcWwZLndWgGSNczKAKIqesgnkaN8PqPI0QsZQtJYGM4yQS69VQA9blXb+2rCB4OoFEIK+GJAbTCK+lBr3L/ew1d4NCuiGTCDMIu5yp1vd9g4ZkzFM5Hx66flXmEVjQqyxDhYufTED3aqqEe52xYI6nRmezuUPIUFNLKfddI80RNZwenpKZCqeDRmEgJVXIwC49f/G8z0lE1pthru8YZ4RELaVyPB0tJUwNHxBQiALWtFYu5joNooYDpDBCBRFETmnoB3e31F9vBqjW4DCsauW7m1tBdF0/l7lGLfc37nx2udmu8tCnLmUxe/P2TYTvD6fTeRJys9klw/3+4XA6S8RqeFyth/Wq63LSlCaPQezF5TqCs1NEz+cpmQzDWlTdPchhGEzi3I0OefXBi3/t808ud2sEofpnf/nXv/zi9cevPvg3fvx7UJgoBcfD8eZ+X53f//TjH33/EygElrv8sD98/f5urvHqg+d/+Pvfb7KMiry/e3h3cwuyX29Xm42qVGdEVdXzaRLl1dWVpdTuq1fuI1Q152613XGZbJa+78fjnpTVehhWaxFpfDMiopZg9H2vmkygSgaPJzWFugxDbg+hIaMw2OWcOrE09F1rXCbrTsB47lJKdRa1ZtSCigIONLMvw8lwteQRTxCGimVqNhgMFzEVBxVM65zdF6gsKsmSAInj9XY4Hmr1UBFRG7oupWStsQCImoHURpfg5+NBRNzDTFRSzomEYGrhLG1iS0VAgamlWmpzLKtol4dhtTqfjiIqakE87I+rIY9zEVI15T5ntcvrK4Tf3u/7rptKaZTEa308hIiuV5v1asPl4SJS67Hv+pRMVW/uH6ZplXJnaqvVoILTOA5dyim1T2Gah6HPOXfZprnshjROU+6Shlzsdv1qNVYcx+iHzrUTSKEcI09zadOOp9MiWzyM8dX93BpFueuOj2eIqfD28fzLt49tFjWp3T3sRTQldH2XzKKNCyDlnGr2Urk4DaN5JCIny7nLfZ+WJ+Vos2pF7sZxbkSKujwHKJlY6lTdLBGy7fR737m8XPc/+9Xrdw/HH33v1YfPLotHG567fTj+4uvbvlt9+mJztemaSAbB25uHnx6OXcqzaKWrQMQEBHSxpC8ObHh4+DIQJdF8F/DmmAokbVwDlowEnRCYGijJlJQ+aSlPDVlVMwt6mqbSD5nNm7ZYdBcEykCgOKWTDF1G/MXayL5Z445ozIxdTu5VhKIGwTieSpmb30FN4DG7C7qLy93peBYNgUDx8LCfy/zweHh/e59MV0PqVE3UUjqP4zTPOamzGelTP6wtmYDTXOapnCC71BF88/5hu1ntNuk8eupzsgQJSGuZyFQ9ma1Xw3mem+r2/v5wnL4CxMNV9f7uxgzvbx7++Kc/T2a1OoGoXj0guLvbz9WfhkFQS6GHqB6Ppy++etsAuYlO80mAbPoUUIvxp5QSEY3nm6pYMpVpnmcgfPYqw3olS69EnOFeVSWn1HdZTUjMcwGpKh5Mmir9/d1+Gg+Xu+1hnJPp1W59tV05ow3OjdPktVaZNqvLD67W0SzA5PF0VrUIj2V2i4iKplCCT5JQ4w/L/FWQbONhpFFaCx9NyRA1ERG058wExIu3GVEQ81zBEJWUNal6qUlEGBJALQVtLHZhyCoIwIDaHoJSalVFU/ubTQRMy6O1mnsYJGy5JWAEHW5pGTEC8Hgcn13vLrYyV65WmzKfHg/naR77lJnYeHjOqe+6cZ7nueauH+fZ3Vf90KXsuURQVGsNs3SxvXh2fZ26/P79+9mDki92ebNejVM3T6dslnOmMIl0WVLKKhZEUhXBXKoInDRGl7LJKmACWZgamTv96NUrWGLIFCHLLB3UdLPdiNkyHCxCcDEMqjglWwPW2h7mtBr6WnzI/dB3ADxqhKSUzLQJ9w3+RJNETFPOog6V6rXTBDIZ0nq9212VeQ5lPRdBnE5+PN9tNpvd5eWvX99/ffMQ1U1gpofTHPR5Pn/1+ub+/qGUKOGW0t3jWURKrQxfZiCWeZfFCdIiYZlmbwL3N88yifbbbVStPUhLRKUzm1mgmqGS46Pnn9JD5wf3qkmypWwGofqcyjy3cfOUs1mSpdtVTdpDLMQksdnYVYUqVhv5UknQb3ScmOY5PFTViWRCNtcoAFVRCk1tKtPt/X63GoZ+6PrBYxaBwgJ1LhWUzz/7/ouXHyJGn8+1fH2aqlnarNevXn707PnVl7/99eF0ao/UWa9Xue+unj3LOd0/3AM6O+4OhXG6uNj94PM/8Cjn834qUaJebTYecOLTjz9znx9Ps9nyQCsR2Ww311efPezvx9IeIrCIB1TrumEczwaFAgITEWrebrtuNc/nujwDigRSyt/55Hu79fp+f+sBTWoCAa8udq9efex1Ok8TsAyzi2K3vUg5e3h7Co8KiiOZffjyw6n6aTyTDGewVmc25JRaiLTuAUEVE0uAPj4eqy19C6j0w+aTTz4TyPjw/ndf3ZhicjD38zypdabiQUYl2XW9ilIBUMXayEzOXS3uClNzX55joqptUEBILg9p8ybDdimJKBSH/Ty9fQvUD9Z9ayzmLnfZ5nmkiH3+3Y9IJtFmXZznaRnSaUW4jSEbml8MqqU4jCqmClPNXe677KRXD1LFdJnsERFJKYHou2xmKjDRiFBTRj0cTofjaf/wOJdSq4fXiBjPp9N4SpKeP7/wGtM89332iIf9w+P+ULw2H3Kpc9d10zzP0/j4+Hi/f+z6TjWp6lS8en39+uvj4bzdrE2x7my9Wt8fz2/evp/n8/E0akpiCWTrco7n8fXrL6sj5dSqBkFG3N++v729tdTlLploG9ET4ePj/uHuRlNvpo2QqUiAtzdvH/YPZq2DCgTD43A+vXvz5vF4UpUGtqv7Ytio7hFmTdaHgrX6/d3N8fC42+26nPTJXlbm+eH+7ng+dH1PZ9S5TwmIGj6PZ1Zvoz2EkKweD8fz+Xis0znC3RFqOafWUIVqLXNEqIiayYK+JP1/RL3JriRZkqYn4zmqamZ39iE8MobKqGp2FYEGGuCKCwIEuOKOb8BX4Avw+QguCBBEFzqrurMqs2L08Q52zVT1HBHhQvRGRwCxyIxwv26meo4M///9QgzgKXx0T/UR5IqNmBEA4XRecq2e9vpSh6LarJt592jrYmbh/XY/iJAIs5AqtfO5u4tHILiWYr0TbW5YhCzyw4AwIgKFeXMwIoUBCiYHaxAupUDzTiul03YD0+Sazwm5mw/MKZVSLq/vbp5OJ3tea9FTLmA5wAmBWESQWoQFf/Xmrlv79HDKVsPcREgQ536upaqqcBRVYC16XNY1ABGKMC8tugGRDYKApSg/r/3z54cAUOHW3SNkuxwcgYiwiG4sgQgg4AAQYhYyl9SIvWCucliaCgZCjkQ1AYCF9QZuiHtEtO5m5m7CLFqmaSCWtLuNwk7cZhdhFu7pSTPfsG0RFr6sbRgkTcnCDCILI4MgAFEIcx1HIVg92tocYXWgCAQjQgjLQZsyEikE93BCA4h8kQjJMWGgnqsvDE9RBwCYWf4YLOLN3IMIAwjjvxGnUoSLiObeuweEWdjGRgASEkRCIEEINzMEEAgoRQHweD538wikVFtCloNZfyG8cECIsr3cRLEWEB4sJCLeN89salHgRaxcVQPRwj1iqHWaxo+fvyAhQ2ri0ANzB6yiSHB6fv7yMLx7ffnN1181//k4r+jpmcKhVoDIebJW6t4ZmFnNOkOczudpGNP5Zu5tXYZSVMrH+8dlnQlBRNx7BKTsDLeiFzycIojSjoWI5OBEmzhhAznkcUQozMY55gYIJBZEdwQmJtyWQO7een9ZwRkRHcYhGQhr64RkEBzuztsJ54GqgsGM7AgQazMI6L3lni3Lp2zUusfz6TxNk7sjMdsiRAjQLXr3IABGAOxBEaAqbW0kFduMeS1RrlSR8oBO6x84BhARBgYEBUd+PsQ5VOitp9wBABGDUHJ9wIg9ACkosUoWAcjC2VqsvSOSg0kpKsKIUEsx6w8P+Xzx5mhPYtH26zPnQss8srdFAQTzzlwQCfllz7PV/dsrQoRAJBw8lG/fvpoOh7//h//+H//xT4jBoipKFO7FzEW2z/3X9++HqtcX4w/fvvvl4/3nT/eBNNRKQsVqqZI6AeuNEOtQ2wIifHqaiShOTgyI9OnzQ+/2/bfv3txe9LZ+eTxm6S3ML93xC4YuHCJBRpu9Mg8sYmCilNdGREQQsahYFyZU4YCXfUwEESNYDjMBIA/B3hui93U9MZl574YE5BQOUpSFn5cVAYciZrF6S5YFCxXWtbdSShU+z/M53fOEEMCEBPH0+DAd9kzgzEXZzPOwWvomDCICRtaiq8X5vHTzKvmgBSNt5CoA3PCrgRuxMdwdmcydiCKQmRHJN1di2h6QAESYkTphFbXWnS0isqnulkdeRO8BaOlcDAAhAsHL/e79+w+4CcgCQhDNAZlIRK0bEAuZO2/SqQ14tGm5PECJEMnDGBle6B+Ya34Ad/j142d9eJr2ewCoWnAfEFiKEGC33t0RUESWdf35tw9ru7q7Pnzz5qYt83F2BHC3aTcAxDBUN1usO9hYCiOUUg77WJe1lOIBTBSsrc1/+eXDt+/eHvbj6TwDEmHPRy1N1QHRCZFYhWvhdKYhAgALi3lnQpWkc0Dq505Pka9ZDhTzNXRJmggW4UBERGZxjzBkJPdI1QETllKYaA5HxNRZqBYW9OgKdN6wLbCsKxAU1qW33p3yyQhHxCJs61KrDrV491NvT6cG219BWhiRmfoSEQ0RBMMQUof+cirnBovy9gInwtTYxYvslIHBzdJWjcBI9vselgID3c14rJNgOAaxu6+B7sBavDWLDm4YAQRuLmY+DXW13pqpUrqScn2CaB5BEQBMCE4YEcwI5kwqwsTERB7OISJi1mCDcnFOcYEglXoi+XPT6XT6+Zf3gXx1sQ/QYRiSqsLEZMK9EYlqCYxw/3x/7xE3F3sRjVjcukpRoXlZRdgRVsLwqKMyIzHvx8JIdai/fvhsBs/Pp+N8Hlr9p3/5a1G5OOzdm7srZVUf3ZwiB3lATLVoQruT/vLAyI2JgIWzsUknMcLGIqhFwp1ZPHxZLRkJqXBOtbkwWuuJZSTCSmAsAdbNLWczKlf7MU8OJW1rQwhGuhillMpMbr40OLr31pHgzdWumT0++OwmtRIiCgmwYXtxrDiJEvMmI3Dvvbsjhuc3i7jtASBx5BGE4ugsGIaBljcWKyFQB6AkkhDgus17U7UHgFcXu6uLyc3T0akYX57Oz8vy8eHp1eWFzd3D0Q1TVHE5Va1qz04FPex38MwGSIitYOnWs/JFcpFSSsm3PPdPOVND4ohtoAH0spyFQMSiEk4tWu72VQiJEGGolZnS1JrS+FygVdV8PZ+Oz9b783mJsGmcXt9e9N6fEYIwQtoyr25F9fZqz4DDWHvg6bwiIjH0c59Pz+u8lFIuL/a999TJ5G9OhAIUWYlGRBgRb8Nr5O7bVgZx45NRVnQvSi4IL6pmXYQBeF1bAp8KwTRVFWZhQvzo5j5Ya+9uD8qUyDt3+5cfZw8niD9+dTNVzWf408Pxy/1DKfL3394NQ8lSKTz+vz//epqXovru1aUIf5jKX3/6QCQB0B1JGJxFCADRSGolwt46IWLKF3qDcCqCSEzIqmH2Mj8Dz4sY2amjIVOQsHdH8lSZOoRuX3AQkiMIArF+8/ry5rDDFzj1T3h/f5yJ4Ol4srbeXB6w9cQ1mIeo6OV+3NUCAOd1+bcivRm/sJsI6YXSRkQUwKWgWfMIsyiKU63ePUdASfb6fSGVLTERHKbxzd0lAqxruxz07mK3WJzXplK+ffuqFE75Qu/tw+f7Lw8n0boftSgjkTCryjqfe7e1x+o41HEYR0QkxNPzyQyK6s311bz007J0s7DOzNH97uZwua8ZQHFx2NVheHo6BtKmiBJCxNY3biWjbPejIzORIwtzpxzTCLMwL8vaWvdUrnkIE6EwCxIUFSKGgMNuen13IVKKkhAuy3o6r4709vbyYj+mO7219sv7L89rN7OL/bQfCmBExGleI4KYRatIZQLC6BZIrCxIeNjthqqH3XR3c/1vv3z6/PBMhMEcomnzFCUMaGuzvm4VQHjiHxGBicwcYIuCQGI3Q9qqaQLyZEYDOaQ63JPLaQhuNo4TIiHlBNCGWsai2Zu4O2IE+DgM/8N/972FPR+fn9YjozeP7iHvPz840VAUMZhVRfrabIM1OAMCiLu5AyE4hht4OEeacQyALi5252UhIiFNyx4kryGLRsTdWN/cXhFRN6e3d0j4eDz9P//pvzr49dXF4TABBgZ2s6W3x6ez9eX2zVfX1zvv3np3MxUCxN77fHyaEYmFVTIKpNYKYVVIkS+nXVFtZud5fTrNf/z23d3NRVJ+mPXpdHp+Ppn7fqr7seRIybqsp/KEwAz7sTAn8IPXda0q1oQQrnaFWSJilGFd6TMhATDB1W4iDM/klbYSIQQNtdxeXyUCKHk+vXcA0FpqqbDpFAmZVAsR11LKUDeVXDkRMTHWOoyjxiYM75vHJEBVikoRGYZq5l+eTuH49u5iGpSRmAkRfvrw+OVxZZYfvvtqN2hsTVz89bcvnx9ngCBgp/TVWZ4HxEEQjgFZwNBLPR2OkM0QIgYLY6BZC4A6lF2VWiTzACCQCLVUhn57vRtqeXoc/vnpY5j3bu4m+8p/uN0BkVm4234an44nCkDqG9k+YW1IaWLekmmQHIiB3G1tJqq0NJLIPjnTSXC7nogAxyKMpDtiQGQSDBZW1UowSqoGIISrsKgi0X7Qt1cXROAWgNHWee5ye6j/4d99g5vuH1W4zecPX55vLnZ/fHeHtPGX5mX9688fAvmwG9/dXad8OMIZbRin4vY37169urlKGHdvDft5Wa8OU/27r29LYUKGiHlZf33/gaVMhf/9t6+LcH7pH++ffvrlfQjsavmbd1ey1W3wI8Wv73cIMAzlYjfmlmBpTUR3+0Nb16qlDiUFsOZL0TJdHtbzGVkk+1lAQt4fLkqRUqSUChBmbh5IPO0O4U1FVTUf30FVStWg7795+9XtZUAQkEU8zX9eDMPa99+8PUw1tsvXvxyX++fVmjvYpunFlBuHsiACWIjoRhhnxvRZIjDJMNTe+/P9I7JEhDAWVRYlJg8gJnfyxBEDIAsiz20Nd3NvYRYhRcq7N7eMDARh/q8//vzTrx8w+bK5+8IUYRORQkC2nySCGwyYu3mhzaiTtVpOpbYGjBDCi7CqJNkg2dLCbBbdUqS9uU9THpPnYVFGRFJAgGkcwp9Y+GI/8QtIwiNKUesdAEupIpiabHdvbV1XJ8ShyLYbxjgedZ5n915L2U9DQp28y8VU/vl82g061FKE033Reg/ry2KFi6oWlXQSiXCEr63HVJllrJr6ekBs65Ju+7GWnEzJTK33dV3CQYSrakLS3W3tfT0+r+tMhGXre8LMz+dnwgmJRFIBscGlTseHOlQtZRxKmjUd0HsHZBGVMmzIq2aAYmaCQCzEGuER6BC5zthq6Q2eZ5SNJyuCkQcQeEAPG1gMXFXdg0VSDeEeTP5ydBAzEzNZsvh8aTbP57GSsGiRZW7m0Xu4g3nI43mOwJexP7HwJjsPJ5Ycgwdi611YkRiS1oTbGsPNUNjxBYGZE56A3CYHkSAFIW9xUGiBCAmn9NbXboYJAU+oG6Jbd+vNYxpqjtlfSkM3C1XRImFu4bauAEAEDliUiTlfz7V3iGDCANCiTAiBFk5MItyaE2ItsumhibOEBqKiWpTzf7dqANDaDFBrkVpKHotM2aFGd5cX2J2HRAQR9t4AiTeiI0ENt3CzVD1sH0HeVMxB2VcRK4eHQZogAgBUVVVzg20OqSsx6wieU6T4HSmHgMSqAsmxcpiXBcLzP2HmCIZww7jYT4j38d/k7CHEaS0RZWv+O8GSiQGDMZ12nVIUABsbGgmZmAlKkSIakmuStGikGRTdcV4Xc+/u3Tqjy/H4HIEsnLMTFXEABhThZJUhMUSa6HO5LNg9fUqb8QNcSJhbLhDSDIPIAAAOoIhIzCL6+xIBhpbmAAPAsRba5mygQu7uAL11zjLbOccq7tbdhjqIonu49RwWEHN4MPM0jS/UkVCRta2tu2rdNlvuLJLwlQCoRdMEYsbCKCIewUSqkjURIXngy8gRVTnBEgnOQ8BuJqpFS2xzQoyX0BMWysWhO/e0niMuy8rMTAIEtDABnJe5W1eRUiQ53BkSgQiiWmulLb8BXoLRQEvdkBhEnnNUyD1ybvmiWy7UPbcmxBIBEc7kQx3yO6SXxI5U+jNTLdoglrnle0skKuKY50Vh4bTlpbB2o8kTVVVVASJwX9NYSiwEtRbwWJY1K/Jm5qRyPC+9t826jPT3P3z7pz//NM8NEDHMgdPXJswi7MFadGkdIt/FbVGgSoDD8fnMzLG9k4QYG/4JiVlUXv59BOG0/QIQjrXGCxaQmfOc7O7MwpJ7L5Ci4W4WzTqzuFsppdZhHAoij9PIWrt7eO6GGZkB0CxEJSfOYcEiEUGIEZARbGn1AqSAsO4Bkf74FFglv2RZ5m6WfVZKPDbFhAcRimCOcIiZmMPNwyLCIgjQvLsHEIHbMAyJE0s6JDLBCqkqECnh4WERuThHYipa0vPBrSMlYxRqHcaptG69tWYGG71sk7MmmMbD0hRNwvn+hJODExOTIHagvDhzQyjMUseqnLcRAaGIhDsyjcOYg4YtdWnbVW0uKlVllby12MMdPIy5VKX53NZlTmlFODUa5TSfl7VdXR7yo7++vLy8mNblKb2R24gWRZiJGYOJhQjypWHSQCAkFWGR9FSdZ19779YVJQ29PZtnpvQwZWQGMWHzbg5MySFGwlJKbhK3PStigpQzAq333rtF4VJKrRXCp3FMqCLnWgD96AAAIABJREFUxcyoQpYPEyIg5AgDAJxCRHJ+QUzCgoTu0aL97jTP3iUVWKosQmZu7KWIKmOgQ9SqCNg9WBL3stk4irJHBECtZTeNeTMRS1HuvQvTMA4B4B4iPAwFcNtYp/ne0RAoH7IN+C+UKq+iRZXW1m8ud8OQ1bfUWg67Xeu/IsLlYT+NY0DaMmYRdbdS9fb2dhB02/4+LU02GtfvNyAJU7dWRYfD/iaCiVrvTPTw9OgOIqTMdRiW+fz78jGfbBXesOsQiCQKr64PP3388u7N26Ll4f5o1tOHGkDnpQuE/1//7z8d9pVIzGxt7f5hZuF03yCgBTCCA6lQM0AAZkYhIZKiSiyqh8P+8mIw859/+2Ju1k2YNmc/YQQwS631929xHGtVnecmIkORXHMF4OVh9LBw3O+GoZbU3gPg7dVFt1Z0rIWZeRgqAAXAm7urUvTN3U0tirRty4rq9eXut4/3N5d7VcVtne/7sQS4ddvvRi2JYInGuJuGCB9qmaaxDJq+ShF9fXt1f1zubq53u52oJhrv+uricj/8+Nvpu6/fjuMowgGBgK9vbxDMw796fUciWcwMA/3w3dc///bhu2++enN3zQTn81yK7Kbx7c3lz799+PbdVzdXB1VxJ0B4fXu9tOX6+jCNQ0QKP6FU/erV7fMC3319NQyV0/If9Oruaj9NWmg/VY/OJEQ4jvXd65sff3n/7374Nu+SHHasHsvakLeVQJZ2TFxq/dvv310e9s/nuffWexdhQry6OIhwWoCHKlWmN69unp6eWoQgAaKwAJABZhJEIA3T9Pr166uLSyA5nc/bQxY+7K+vnMSt/Zd//auHIYA7hfswjqUoRtQ6XV9ffvX2dS2yzPP9/QMunVUu3r2tRUopKqwqQx2uLi9uby4fH+9792Vt5/MiIu62lV3b0ZJrBiSIcRi+en01r3F7dRCmFxAdvr67vr25Meev37zKPzAyIeDN1eW333x7udvVWsexMlM4BOs07b///odhrLmFy9OXSL/75g+rl7u7W6bMlgV3vLzYv3t99/S83l5f5qtJErXUu9vrd+/evbq9LEUIWZSJcEG6vb7+xqddBWbd+hmDYZzevH1Nw+Xt7Y2ocBrxIMZx+P6771v3i8u9MGfdYG616t9+83Z/uRMmUUGkbo2I7+5uv3r9/M3Xb4i4uydVdhjqH77+7uZ6T5jZIO4RvVsz3+/3HhlZl9wyQKLpcBgUSlEISBICEt5cX3//xx++efd6KJycGGIi50BgZGKyIA4IwFKHv/vju3/4u79xoPN5JoRu1lpvrW+UU0ZOGgrzm9d3w1D/03/+MxKpiGpBJniZdYXF2k1FM5zn9Pzs1i0CUUFLzE3MHMMAwDf4OyLGNAyvXt/+4d1Xh/1ubcvTw9O8LPlyEDELi4iqZKJAqaV5P53Xi8N+be3Lw/Pz80mElzXZ4rCNbplgM2cRIx52u2nfiAiJYXvFQqTUUpoTEud0Pn2wtapZb20V1VIKAABvmPLj8fn5oIi57UIAYALGOC89vCNmphIEOCKWUmUFS9SnB2Ks65JOQGUmTsYeeIQwqdKHD7+V11eliAoFIlLOcihb2py85OBAGJ9Pp7X573GzidZYu9t41zzMTZxVmZjcotSidRDmqsJC2yeQYleIcSyqmt4LogbEx+OXq91lTXTX5nimy8uL8DaMu1olEjhrboiH/aG5p6NoXVO6BUnwEGYPAwckUuVxGFeztGZn0G3rXqdpP01tXZ/nc16urXsPePvm1YeP95+fjoiJyAGAyBKsd3s8Pp3O83k5zPPy+PjUW3OPMu26Fm4ugZx9cgJmLi52f/vDd998/W6a6ul0+vjhw8PDQ3MnTCUcIZGKljKoSi21DoWJENgCEKXWejhMn788WHd8oaRAEhly18GJm2ESLqpLN48ccAEGqWop4kZMlMGqZmbha1t77z1CVVUlnYcBgQSPTw+ny8pCyhlLAoiAwoDQLGqRLco6AoC0Fl4MgIZxCHfvZr0vvQ91BJHeHRjNgyjLmtDC56U9n8/gCsRM2Lot5kJ4/3x+gS0EAMxr01qD7HReX93kw+oeMTd7fLyfCRyIhAGAIRDtPK+X11dPc0NiUSEkc386zVvUNTFL3vjeMyw0TIRzR7YxfSxaWwgBmUXUkIlstfXheH56ui84xff5mMJG/SAqRZZV2XrINun8+PkLMwHp8+k8n89Jlzjsp6vrS3f/9PFL1rLLMqcA8Or64jgvhFREcDPCp3HAI7DWihDH4/P5fAoAh3jz5u2HxxkJs6PjCLq9Pvzw/Xd/+OqVFvFuH9//+uHTPbO21h3ZwcycRAPgy/3jIx+LqigLcyllGArfP15dTG4t3JgweYJbvY/YzdJISIm4yNo8rLXOtMXOEAI3QCZyWK1DALNjwLJ261aKIDMzpzA1Wy0RnnYji75A0mObDhGLUEruMkUeEEVsbc2sJ1Vyc6GGW/fA8HBiVpWc5BiRiIzTVKsORXe7KV8HMweIXPGknQTy6ELyCAIgoRzlA0DvhsTTOBCGipZS3N0t6VuxrjMprX1lZue01hExIUaW7slNBIhxKIeLwzDUtRnlOwvQ3VSFEFq3Ze2AEDn3RhQtHnY+z8yUs8N1be5WatGl997SMVqLIODHz1/Oi6/ryhRMMq9tXlYkWJb+8HjMnOtNOYfg7kOtiWZZzjMhWTgAzPNKWi4H7R739/etrQA4jPtaK6sJsxDLH959/cfvv/767etS5OH+/ueffmzN069H6Mu6sI4ibOZh7u7ruhKhWadGTFyWZV6klqqChWmoUgqfF8gcsexxmKiWzIFDZA6AWnUcByTCTAZBckAgGoYByZce5u5mQCqi4zRdXV0B0tq9uFOyJ90B8NXtjVRdW3p4CKBDIABeXh7MofXE+CIydQ8VHsehdV/XDojeG1Jl1XEchKV1Fw4EdyA3C+Kb6ysinNe+y5R5j3nt+8OhDF6GsqxNVfJSas0uLw8A2Fuc5zkl12trgHS42Hvvx+dTDpIjfFlWR9rvdwz+8Hjso6OwIJrH9fXVOJbj8bm3lpKK3rxO01dvR0I/nmYCDHAPmJdeilq3p+OpV8k4stN5ZtXDYQ99OZ1P7oHEhLK0Rctg2JhJVNxDiERkKLr07uZIoFKQeGIBDGHptA3hXoY/CRdmVekeRPl5IotAUKl0eZhOSyfG8zybGYtc3d1eHqbjar01+V/+p//x669eQcTxePzlt6fz6YyBRNjczcNsdSDB6L0zQXe31ohyWpQVzSZnQKS2tnE/AMBQa+tnQGGmqpWVzdzMzYIIzKO3vq7NvT+flnldB5Agdofn0+xugHQ6nc5zY0n9ZD+d19Zb7/B4PLEwImBA9358nkm4N3s6zfvdQBgI0K2fzufW+tPpdJqXqgUIoPvxdPYAJl5bW5oJkwMBhSNDxNra3HqtNWeta/NUiQXRYjD3vCJpabauvZktCzYHDgKk1u04L601BFrMemz3fl+sJTkWcXVwEBJCBKFy2O3m9qhSuO64jkQYEMMwTuNZGINLcEmLimE7TPtmR0SSMgxFkNnMxofzl9Oy5RNNE6firY6Hp9XtqFMF3SXnIwJe3dxRPfyXf/23o87d1c1EpAinuZOZxjLVUrr7cl5YUqt3TP4cZOqVoagIRG9SSKbdFGVcAd0iAIL07ZvXS2vg8etf/qu7s4rL+GxU6zjtAf/P/+N/Px6fvzwc53kZp0FYWlvPy8rEx+PzdgAOIzMGxPNxTlMKMolIUWUmJCwqIqLCN5eH3tdPX54+fXlCFka6vDq8e333x2/fEYX1jeY1jtOn+8f74/lqv//u69eqjAS92fE0//rxSwTtduO71zeaHGj387K8//yESG9ur8ZBcxcRAKfT8nSeVfSwG4pwNpFu/nw+n+ZWi15d7EU1i7Z5XZ+OJ0Q67KdaNNddAWARy9rBfZwGFU3c69rW3ux4nsF9mmpuMiAiPJbe29qIYKi6EaEilrUtywoBpRbV/NIJIHr35LHLViq4WQCidVt7BwBmgQBiIBTbMO9NtQBAxlB1B/dorYc7C+evExtfK4tgygRwM0eCsFjaEg5Pj1/auhBzYeZhco/j09Nff/y5dUOEqnLY110tpzVV5mIRYP74fKyl/PG7P6yt/eXHX4SZCc0NAkXQLE6n89L9+mInRdvamyWWNnPEwM3WL7+2+YhSFjk4sJnN8yr/+Kc/p34VAzzgPC9INI57ALeHJw8QJlUx64BIhLY5R7fBzO9EqrQhMpPKeHmB5rA0c4ciZX84fHg4nk8ngrDw1uD27o5Jpmm/WPzpr+9VhRG6GREhF3c4ntd//utviftKIRsiAsVPH+5hG0qnuhPdHWD9eH8M727pvsZwM8/1FxFLijbTJUiAGUObz01K6xAhIliYSSBTQXtLSVzvLQLyn8QoRB7bGjbAIzxyIbW58QKJEF1Ya1UzCMgCMDIPKn/ZDU2ckgNMdCfESyxZ9hAQniu1jT6VY/MAQjBzYhpqVeHn87ln3k2EiOTP4G6quhvHJGXcn58ffn3flmYRAVFUVIUxhqKlagcnIvfsSllE97sdMxbg3TAtbS1VhQZE6LaZl/z5dJrXzToG2wO2NcHhYZ1FXCqShEWuRKW1/rLcxfNpNrNUMrs7INRSmGkYdF3i/umZCMFpqIppU2QECGRUFhEeh6FoEY7W+fri8OXxqTtYb18eHva7aRyHQTUQPnz8+Kd/+qdxGhDQzNraai1SilsnkhSkwIb1wkR/IWLyoVM8YrlJBEeSFAPFpraG/GOB+8bCQczwr1yieWTj/LvZFjabOUbvHlvGIZobBuBmW8wQTgdAKSXMIMkU6KkjRHyZB9HmXkEMk9a7dAvvLX8zenEK5ZMkKZ7IhzReeNYWDlgYkdAtAIJxM5MiEREdptK6PT+fI6C1pTWwbhHee6/DcHW4eDo+ndcFMFqzpziH9e7e2+Kem1kPh2ksLHwY9WK/A8DATiTpmWutr913u3Ech3letQhQ7KYxk2O5e4DWoqXI0/Ho1jPgJyXU4GAR1BYiMCfkwiTIEQ2MTWpRFnFAa2teAZmSp0VVeDcO5v7p8+dPn75M427aTUiRqhVVZmKWLEWIicyNGKdxAADrz/vdcDwtgP54/7CubRqGdRqmYbi+up6XbuHKPNTKB0rmaDARpeFgy4dLtjQRu/VEmmRRn88WkiAkt3vTu6dwPQCQlQhbW8Eh50J9XebzDEjDOGxyt0wwDWAmd8CwLDfDoygzCVICTN0jkDhH/KLarW8TGs60WsofLxVk9DJxb71n/HAqo4Uljy/LDitFqOG5uoGwbtvz7MTWOhfOyIFw9+jsJdB6s2kalOnhdIYXdC5ADEMRpnWdCSNdIghmreX6pQhB2vYgkOD6Yr8bh/OyMlM3c4damKUQkZkvqz09n4dSmjVCjAhGGoaCiBlCBUJFeSh0GIu7d/dNcAPuFh/f//bxKbTIq3e3qoWRInxeVilFgdCWrsq+pheIxqF281L0+XT65f3H4/E41Kp7TAC2Mg3jkKwRj0iMXimScJhhqNNQhqofPt0/PB65ai5nTvP5PJ+eRAC36NQcgJkbEY6lAHrrISrebekNAhIQGNG1CEKYpy1iG8FD1ikACfNM/VXOGMKaQeabEoR54DhN0zSFrfPSRHjjCopEhHkQxFQ1F+qRa518bgQJBLes+yACgsANUA3gbuZJmcxlths4gpuJSka+IVJgclMaBCGCcuLIkySQlFDoPYkC4BAIoWkyQoAgJg4ozHldCBN1RRXqOfsAyJasFGZiiCk2QGvQphfavqBaNMtaj/De6lj++uNHYgEKZkl1YO9WlJ6eT+8/fCylLK0RIkL03lp36z0ni+vaAeLu9upqPw1VmJO+C/Pc/u/HLx/AX9+9/o//8Dd5H3n449NZAKGvfTcNrTWVCAdEEqbz+fz+0+dPnz9HGLMSAoBXlWY2juNuHPLAE2FiViZP5DcAEU+DTNOwLGub/60Xad1gPrsDEySwPUfmiHSYBosQ5rN1j0iGh1uTcLNQTKYFMhoAFkEWISQPc09HdV5UkGnxzDxUZZaqEgDCiMiiYma996HWVOucl54UgxyeEWH6nQjRwpWIiETYI3p3VY7I6RzIds5RgBOQR+89HSAIFOBo4dHX4/N5GIf9NLFQ6lbMk0qR6Z8QHsiU2lJwcIgwtwgmFGKkDTODm0sZhSnTj39X8ySIJQy2SvVFAuCb2gQRgAjMrK19XlfwGKYBidyjrevz8fR8OgmDubd1fTg/mnvaVITgcqfL4q0tg9A0jbtRI4DBuRYiKFICAiFFWbjfH9yauUc4YQ/voqx1eHg8KSFAmNs8N3HzoqKiTDgUNbMA+MtPP/38069L63kvyKYZoeuL4Xg2Vdnvp2GsRUSYA2KeV/AeBGb26ctjXO/XZb67vvzf/tf/eW1t7RnTBnnLxlYNAiCpUD4jxCSihGnowJdMyIyHRKGMagl6+Ujzjku+K6ZljBOiC93MzHlb0W3Vm5vjNoRBxDRTojv6ZsoMRFLOei6LvUjVXQAiOgJtHNiIHv6CU/HWPMXtefpmZPJht6TCdj9NWoqHEWz9k1nk75DXpQcII1JK6GgcSmy9DPRuFr6ly7o7gHsKGsI9wEN104ZFgEfSCSDF9+5eVJgxhIswgD+f59Pz8+FwKFWVqaiMc7mYdmu303leV0N0DJCih/2EgOd5YaJhrCkTtywfIOTF+BoQQhsNI9nZEC6Ef//vf7i4vGjmn7/cj7UwYfKXBSG/WhAuAP7jz5/+5S8/HU+nbXFCxKyqKsIeWFVWQyJ+Oj6fzzMQ9nWttVxdHg77XQp8ze14PF0fptubS1VFJFFhFsq0KQLc+sdsUsWjY+KxU66CEZl/w+wOGxsaIhVYnJUgbxapjewOLsyZlYAMDKIcmOEplhcjikS65LI1U5JARwQK9nTmumcmlCOCey4QLcCtQ4RBz6mJR5j1jZ0eMa8dM+YpPOGHiKhFPXwoNSDWtrp5nsMAvq4rAnCGioG35q3F1iQArGsLNwcU/t2miB6QaHEzX3oLs1K19wBC4Rin8fn4FMAY8dIRIRESC+U7zHyh5fLq8iX3KNPp4/LyAMgQFgEb7iUs/EXMmJ7zl8yLzBrYgtWE81vK6J2N5shurbPot999+9XX77ytz6fzsqzr2tfej8ezpLnSwz5/+fz+tw/vP3x6eO4oLsREVErZ7yYEAiTMU0NYmXZTKaUEhFzshlpEWIWZkRn3OohKVRnqoEUJsVZ1wDBHhrX1MAsiLWLW1vNJVJlIVQNIhV76et+ag4Bwa2bKCmiIQIREnZCI0ANiU4V4olYSGOjWi5aUGIajg1l3xJDkbYKvHuMwrGtHxiIlxWpJq2aEYHJrgTm5cSEipu1sBHCXAOxmFL7bT0SUA6RUIKtyqm1Tq4XMY9XWrFkEwG63c7dsTpkokHqyHiHAjYg8nDYgwBbCYB4RJuDH00wbbkfHnbKQIC+rkQ6SCyamfFdjC6ShCOtODEAEoNtKzr1n7DCzAEg2JO7Rzc0dPJjBHYMIPGjb5bu7E7E7dDMPyElDQERQys29Q+8OiKJVhnJRp956b2vrXfRJai3Pp9OH9+/v7x9ba8hQCxpkUcJusSy91lJKmaaRWCaCr9+9vr7e5xaPkBBNRMehqqjkcR2bBPfFoyFFKCQiQrUgARMHYl+7QyMkIPLY8pEDgiC6pWiCmYmL5mXjDu7OBOn7EhFhZOKMn0jlXt56nhkXSAFg7hjg4knGI84SBxCQpZi7x7baFwYksG7z2q3b3Nah1rFqrfqip4AkSHQzMUcMQhalvjG50K1DODIpKUR0Dwg/L6ubk6B3CEQP37LwAhCjFDEzYjIjiFSzSqr33Lxtuz4A0mHwdW0tfG3LyKgy9EwN2DgZnEKFHLJERPMOifJG9IRiQiCaZ/gisptjRBKNOZDF1tUcLSU2saH2IjCEBCLzNyBCXpxSEG6IsLbuEaDRu3X3jOGqSm01Llq6r4by6fOX4/HZrEutINxRKizNMMKrlnEah7Hup+nyYrefhuubm7tXtxf7HSsrMzOnsCxV3ds3DRGw1fuZlLb0jijmkDnfgH6ez1cX0ziqKK0pYWFWwXntDM6lBMWoQsn+JGLcrO/djRDGoRaloVYkXNeek9bVDBx7IlY9ACkQwD0tmRE5wHpJcSXMx5GJItA9AGJpHdHdY+2OiFrEA57OSyodskvIBtHczV2VArB7EIm7ed5SpN0MALQImQOKWQc3N19aBwcSGQcmQiZiFe9WiuSGwMzS99rMMIBFJhV3M/MAZJ6kBJeldYOwF55PRICbkRIShiMCmuf/m3ahcE9R9NbNpss8q0PCxNJ2JmahoVKEZhtrOUqOQKSE0CNAeIYzBGAwsgNE2FSLIwJQM/NuGdK4zqtFIDIwioicV+NawNhXgyAdWEplojIMF/v99dXFq1c3t9eX+904VK3DoCIqLInX2MoIknTdE22zyq2STwRlQt5BKTwEApB4HFMvhCJi4UpQGC3CzUiYGAiwdWchJk6hpFtm02NgtN4ieGleJK0AlK5wZqnha+u9d/NNt9Gs53QEtm4tkhGRKlt+aeDWdV1aws0iArSoaonwIvmnBBE2AxHu5iwgklI8WZfVwQjCU49OSGFh1rozElJUUlcGwOvLCoTPpzOxCGH+HCRCnIQxEOFcVeVHF2HWIZKxT4AquVmiua2rnU+nUksOEz2CwDELO+LWXoIqgATDIraQJodIwh5klRzMJEKpdiFChwgEMvbwlOo7bJm43SHCzR27uTUzd+gp+OvR03g5qIZq6917c7cMDzJzyU0FAiYFl5iUiJinYby4PNxdX796dX1zfTGNo6gUYWIW4SKSlh5ikqTObCsFTEMAYmwTIkjjGXAq0QgIKXuW9IaGea1gbQWkdW373ajK5j4qB2Rw1xbZlMy4gBBWZvIIhLAI7B2ZI9Jr5udlWZYGGzQ/JHU+qW7J/hUylgtYtHsHhxy5Q8A01RSmCjYk8ghBNOuHaQdpagoSonCDsLSSCKILEpC5c4S7I9JhGte+cbvdnTbPILh1cFDmBBq8gPERrCNTyUWIQ/ji3fI/TH6PkQuTB/a+FiQZedDdeZnJbRx5GsfmsKzm5kgOBoShKpEZekH64rjpbtZxO6fckCjj/4iglIoIRNG6t9aByMw6GFKoVkQuAenEDocAg4huvq6ttw4AQpQKSiLWWhZCt56dMnOIVnF3JiQKYiICEj1M+8vri9c313evri/2u1JERNOorSrCKCxAUEQAIkfzhLGhDranDQFcE6OgEu4QkPmZ+cmmKDQARFgDTh2X1gfVsRZkas2yc044TN6E+dRuM3DzAAT0tgYiUO/WOiOezdL0BuGEmLPHtE54RBJjAdAgIIKwK4QnwdJtntdxLBBxnlchGAp2QLeOzEjsvWUnGuG0WSQgItybMAoJoltva3eEaC2UEVkDYp5ttk7AyBsuL/dIpAIQ83IepzF9bPO8qHCPLkwGQYHgwegR0Frr8eLwJ2bCDlGitNbPS+++5OpetYgwZkdsllIu5EDACHRwFS6aFHdHYCDwbtk0MCMiBHKhPAeZtkyeYCLP06k7ZZuRniekYShQaw6O0haVUYNC4MjuAGjowMwyMCCFB4pgLeP+4nB9eXl3d311edjvJyIuhYWlFM16kRl/vy5pc41uNiHmHD0k25sAoTdr3bbdsLtWFWIRWdsKQMS8NsvTugqPY1FhADIPxfAIcw/z3E8C0CZeI8q6IcH4EWAB0d04l81UlFW2i5tYdoN6xNraunrrLYsVErbeWZgDmpkIX+wHj6i1SlFwj5xxxBZzAcgAIZKXLGVSUXYkCODeCWErEgA8/Dy7QyfEvKYSGpP2UoJYwx2iFhqnHYTHS5KaeYvIVxfdApVzTp00DQhovSGRCotQUZwXSrrv2qJWZs4nhjjZxBiF+GUzh0SMgCkEMqMAR6TmHuGoat22PQ1SKpbj95xib2m6ROCUr6ZWYbscAHK+TkyIjOy9GQlDeA9gJ3MrQhuzF2sZhuHi6nB3e/3q7na/nzjnZqrMad4UREgO2GYlS1kpEafdfGN/5Hdvmy+OCcAZGQmFmUkQwdyZuBn0tSeEohQF9yQoI1FxJwIBaN2WFyZvHpPubm454fEN/ImIuQjexrLJ/S8iyR5fzXsi/MJTxbShh903Rx1g91DVjckEHcK8W178u2mowsSYaaoRfag5TU2jsVu4dVsyExjCnVIzAoAhQgzo2XoEQTigA+Rg1gNqKZCSBnckBI8tfTafCc/DRpGxsOZ4F4ICCImRihQiVoBo3TFVHwlUASQO8CCGyJCv35H1gJkSLCQRUauaByOx8MaZhfAAVXRnAENkM+9mTDnb2pTLAJvAnYjWtmZ+VwtDkmEqhcnC57n13mzpyCThMUzj/rC/urraSv7DWEoNiIRMp08px+hZ4rwU+4D4cmPi9nunpEWEkFgZN6rm5s7nFHJ3i+79eJ6ZqDJKkhbArBuygLm7ZZUQ6f0I8ExIwqTkbjEZRBuCf6NGoEOAOUSEmS9LHwpb+BrYveOGBc1SDTLRL2Xtva1fjsvVYb+rZe6WzOVuxkil6sVhzxQIsS4R4MIcAR5obphsL4d5tXVtvXdCkqJCAozuaeJNyVTK0DdBk6gmYC7VPnkfunuAE4AHuVsgpY/3/2/vbJIcSZbkrPbjHgFkVnVV16v3RmYzwiNwzxXvf4rZUCgzb7q7KhNAhLuZcmGOIs9ASV+mpGQCAYSHuZnqp1ABNSEzodpEap6BcEvwcc46j0WGNd22Vul96o0RYEAE0F+USpD6nMEkxUWNq3qT8iULIBwjVSGwZ</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8S68mSZIddszMPSK+131kZmVm13O6q9k9bA1FiRRFioBAaCEQhAgIWmg7v0lLQVst9QIEAVpIoggShEAImHdPd89Md013V1U+7/t7RIS72dHC4+bwNwjlubmJzPt9EeHmZsfOORbAd+u79d36bn23vlvfre/Wd+u79d36bn23vlvfre/Wd+u79d36bn23vlvfrf+/L/nys2emChEBBZiLX90dqgcDXd+paQRFAEIACkBAlj+gEC4BIkSkSzrOHsHlX0JEAWDd591unUyEpAgJgCQICuQ0lXmualCihs/Fa42kKfXraRqnMnUmlxe7oc+qArQLEIJCESEJCIB2B4SISrs2iCw3qaoiGE/zu9tDqaEiqyG/ePakMm6ubp69fG5CDyY1mJkCEDUd+t5S6tcmXfnJP/z0H/+n/+A0v/s//9d/+4f/9zsVS2b7h/v7m+sf/a0fTbX+9Od/DRLC3bp/cr6GCAi2+xQIQaDdtsjjQ8TjpT/+LygYAMKDN3eH/X4SFVGl+2ronlysVQSQABlUEUK6nPD4XEWklBoeBNpeOcGIDzvWvh9o1wAhTtP8cJjatWnKQrg7BCIiQHUXQNVEQIgIztY5Z1seKwXCx0gAEUKpjNu70zgXBCzhyW51tltV9/Rf/dN/NHQdADMR8HiafvXb99d3p3C3YZP6PqqLSrg/7puIQiUlU4JeCsCoRRjrlZFpf5y3Q/78+bO3d/dS5s+2qrvd6slFZypCUfXKGr48acpv3lzf3xzDZ/MyzuV2nCnDdvui32wf9je3169Swn/07335ycdPTbWFqIgEQ0VBkhRRVREVIaliIiIQURWIgh5d30Hw/t3N//On3xxPs6p+dLn+vR98WgW/+POfvfjicxMS6FLWrjOhmnQ5P3lyudlsthedbcvf/+c/+AT/NfDbH/5w9b+l35hY1+W7q3fvX736/d///f04/zf/3f8Ihoh+/7Pzv/u3PlYzQkDWCJIkREAyYjkX0nZyOTYUSBCqSgbDp7n+6c+/+eVv3ljKOaV5nj99cfYf/u3P1TSIIBiRLG/6br0ZVOQ0FUdNavvj6Xga20lGsHgUdxVV/ZsEoSKiEIKMr1/fffXtNYkAun4tIuM4imhOxoi5FDU1MxWFiAq+/Ox8u+q0Pd/2nAkxodMZJI+n+ad/+erm7iGCq05+8sOXv/s7LwmkPqfNkNupB5lNfvT584jI2X7z/nRzqJESGGFGhggIVRFRTcmSpaKSU5rLtDJ8dNmXEvPZcL69/E/+43/0xz/7k7dvX6+70uH029f1o6fn57tN7iwCHtHOMIkyzw+HknOKaT6eCmyzWl/cnQ77d69MI1sOny3Z2XrFJVERQJBCYDlompKYassaLe0JIKoqVJGUEoTjdtWlVDJF4S5/9Wd/HKQcD+9+eq0C0yQmSZPTAem6/DqZ5mQpBfgv/nsN+W8hddpPPlPQIobh+Jf/8l/P1ueUiTDR9dBvNr1ZErFAeGmhRZJBgKxBEWjba4EuyYDLxgncS5fKMPQpaU4pmUnOm1W/3gwi8JCIAJFz+ujyrMsJEJXjw8n7Pnn0LXDbxmePFmSiighCVKGibNcT0XfHnFWRpjonSxTk1JmJqkKhZskM2uJJ1HCxWW1WXRAQKhS61A0SwWBEmauZmZkaxADKKqfJJY2lWsoQAM5AdQ/Vru+63rr7WU8uUEYASoBOaMvKXisZUr2mZCmlodcXT8/v7+7eXz/MU/rDn/6//ZA//+LF4Xj6xa+//fVvv+67/IMvPv7dH37aZW2FjAEKP3355P3Nu77rZ0lDd+nQ129f3d/f9F33cH9/fn6+3XQeDC6VkURERFBUDaCoCD1UlICKBAhpuweKaNBreDt70CXh11IODw8+jm1rFQAUEtoKsOAEAaL9JRCEaKs0lKCTyiV68Af/+l/5xWdiAx/Lo4iKaCy4ACRUWhYmIUmXTNaOTKB9uwAgyAhQAiBDYCKipka1pCArJCLYkmL1+9O4kz6CD+M0l1rvnRJmCiI0BAK1v6nUqksgg+4SEU54kAGXCsC9ilqEq2qEmEAEYrL8akAVEFGFUolYSr+QkKXMidfqpZQFz9CmuTAiaUpTjRXEFkDDlLKDQbjTVNXMKyFCBlvqgBCIiJyswSRAVXEa5/fvb4Lx7Ol5v7vshm3PUxG5vDhb9d3Z2ebdqzf7+/tpLpZ6ggqBgMCT87MvPvW//ubh/mF8OD3s7252nf2X//Q/30/7n/38L9+8eT88uSBQazFLUGEESREAjOUhqgjCoUYGoI9YrVWnx58hNMFjAWNEAywQCUIEDkrIgh9bymxFOkJUEWQDgIACjAgSQUAJEgp4QLT9VkSoGRuWFHq0KBIh2DK5tq1YLgEQkKoKisOFoqLLsSLNzEwCgqAQFBEiiMNxLLUKpJRK0ttBaFVzwciAQFW45P4FGqsAIq2kq8CDCgkGHESQasJWDgS6gDujClSEFJUPyFIoohRKgCTFo1UaUQEZU3EPDgNSnyw8BEtcJhUTFVIgZiJARG3Aoj2a5cgSKVtUkl5K8ToPnVjutquuHwZL5hzvTtPd/eHZbn2xW6VPX1yeb8s4LyUPiABFGFTB5y82ffY//4t3r19fd3n45OPnn372yZ//7I/6rGebjlG9RDAkQqhsh+exA4gIUUSICOCt+LREryoKQs3CCaVAKaLSdpp0p9BaAlr2rt0nQIPww/OCtBSiQqFQwaXuUIAgDe2LtGXLhqLbRqtIIBbMDzAAAQPQeGxfWvVcHuyCqT0CEFNluLsmE1LoNaUcQqPi8ejMkxNUQE2F9BAiEB8CQVQhokTIAo2gIhS0Ho2Ixz6PANxj6ReEyoAIEBAFyIaIVXRJzmh1gw0DQxgREbWWCCoQFApqjcowYVJAEAgRa6UB1uoLYQKS7hEMkAxh209REKW4CQjO00lF3eV4KkmTshxQT9Mctfo0fn2/P63zqKk4gpzm65ZjGCyx9Fol4jh7vz775NPOUvfs+bNh2Lz69ptSXA3TeDocj+M4p8xaIwBGyNJ8wiNq8Rqciwtoiu+9eLpdd6IiCIiGV0IV5gy0dgsCYQBCtr41IIogFKLBANgaP0CrkwwTafkKISERXKoGSWnNyWO+0KXhXTJXi/pKMuAtWsHAYw1vFTToIgqpXgHWGofjWKuvht6DIsjJBFKr59wlUbR+R2SJ9xZP7cgJSQks4NVUINoCES28uFS4AE01nATpbFsSj0hSkCCKCBBqEIhHZCxxxmj0BEVEAVENr6BHrYAk06Kmj43OXKton353nY/bTgWTyFhYJqG0CinWujgVCbg3FC4RoYogxnHMZq22pC7XKFf3h1PxlI1iDDeIWrJVd+0VTklqkmCaVFpqFHe6l+oSdaXs+uhgD0W/ff3tv/hX//Lq6kaBsy5BU5n9mzc3OeW5FIiWuVJEGMexrFdrYD7brO8Oxx989j0BD4fjepVlOYcuDDGLaFlFIlrb/6EXh1Ig9ICKhIAILHtHIkABGY9hJIgglzBbwFWLeWF7/CIi9gGVySO/Ei2kuZTzBbw1SCmiH8BZcH8c9/vxyWbYDSlaaJv1Ke33U0pp6HuIBEVEDGjAFQQJUbV2SxLSmiH5kPmtxWc8NhxGlqgtIikfmKEIsNRqamoSAOgaCpPWI6s2RqRh0FYeGiAQEKUWg718unVfk6j0TjEXBpGevK/jKU19urzIu+fp5hjfXo/v7lBFSln1q866TUSQ4bV6LbVO7QnRa1AB6Ybh/Pyiz/bRToZOxRJUVDSZqrQETgJBEAqhAWZCj1JKLeVhP56Oh2kuUYu7lrnYw5vfvnldRJ9enO9WKUQJvH13u9usn1xsru+P4zR/9r3npcxvr+/Ozs6zylimMk8Ph6OopAZ9SF+wGLMhSHfGksWCIYAAzjCoI1RUfOEc7JHOatVuCSYueKGVEpDCVoShItqajlZ6F6z7CJCxcFXLx/079CNkYWMgghaDc42rm0Mt1JyypVi2UApwewzq6ePn3VKupJVFbUHWyjwbqDPB8tyJ1hc9hh0b29lwrUi2/NGLF+5xe3sjKkWFlSqSug6MlllEhcF29lRF1fBYNCGynEoyGMfR5xr90DEoggh6nZ1Sa6SzL+vPf+1/cDWv39q//7H+7o+7y27963r8g9fTHDRLOdvyvBooBUGWWutc3EudR0u2Px7T2fn24hnKw/IQFCZqSoh6u3GihATpDYeSBNzDa5mnaR7LNI4P83p/f9fNJaU0bJ9ob7Mo1TjXaZoOU529jsfx/nDyWuo4j2O92x/urt65+8XF+eE4XZxvnl5sIiigPNK2DDb8sFx9MJQSIWTLTwJhCIXaOJOFPyGolMZStl0LXcC0on0+QNKDSK1UMZzFa865dUs16BER3kA3gHYIZdl9xlJqG85hrdPDcXYkXSpviycSjAAP5VmNoVN+yCWEisCEwdaKSmroGoxwAAptjUYD9Hgk3oFk6W//3t/Z7M5/8/WrP/qTPxVq4izMlrSRdvL4Oa2WqTSOBAxaa0cb9ccQUxD3x2l/DEd4jVaGs8ZcKwNp+sn4+p3oMR+D/+ar8fr69E/+0fT5J7uH/fTHV+VwOKTcrde9iJJwr+5UE4iKJRX14oEcXr55/WYcD5e74XI3rNedCVUBsUcSkqqawAilBASiSw3POaWUawrXfJomlmNpDV0dH062HXqIz4RAyji9Ox1LrafKw1hUJHX96VSOjmz9qcr+VFfrmOboOuSkjeFqTZgKFjL3kWBrqUdEwFAhHjsrLD8GqQAFSlBFW+kLtNjyhRIHSbGGynUpIKamj63hIwTDvyMDqAoooiBbs7UwtA5BMObiklKEL7wI8KHaHk/1NI1DvxMhuBTHpSQqRRQaH2QQBhAkGwCFolEGgJJU7TZqw7vbw7vbh5//4pel1L4fErNpkJzLHF5Ule1BtAur9es3dy+fbrfrvsF0NqjZ2HCwlFoDHl4bqgU1cRwL6en/+jf1bCfV490tVOWP3s71/yj/8O/zyy9Xt6X8xZVM8xjhOeeu68yS+zRPnlNOSUtldb87OMCY/Ve//hpRn17s/t7v/WC37YNQaRWKEQyEPmpBrasDIaaqajnJXAs6L3fZ4BXhtRzuu/OPtFut+w6Mm/sHal6vzy5321XfWTL3qKWM0/y9l9/rujTN9d3d/tX7+7Pt8PLp7pOXlxfb3syW/qmxVIQsqgQKAUoSiiQKP0AlIgkYrWkkiIWtaJTwktAhfxMB+qGEiIikZO1LhRCICaHaqGXQKGiymLChuNbPNhpVyJjnugClpZg2BqPVkoiIw3F+ctawJsNDVJWNkFn66HYQgmwtb8NvEIkA0Vo6eNS//urrq7vT6zfXTjezztQsQWSeK1m9zC2TQVuzCZLjVP7y1293m263GahQsp3hWLSARYWQdgWtbhBzqRFhgucvLocf/1jfv/eIXHz+9d1pfVXOP+pSjl+9GQlUr/M8y2PbUua55ScBc+4iotZKokvpycXFj3/4/acXm4gSNTwCDK9eqjOiuru7l1q91lJLLfM8T9Nc5hLeFd3Vw1XX5UYnp64b+t41d7kPxMvnzz7/9ONnl7vtZrXqupTEEPN4GKd5yLJdddt1f36222zW41xev394e/UAwXY99F1uxfN0mn77+sHdU1Kh8HSrUQUK1UZ6YOnuWz8qsSh4C+P9yGIAjfdrTSsBMduci1rLLhfnw6cvnyx0goDSgkkgZqoN3zTupbEEojCFiETUMtfr20OpknLKZskkqeZkyazL2qfUZ+1MNuts1rgbMV1ivF0WQ0RiubKl5Q3TDzkVj3Dehm719mZ/muZ5mmp1M0mpK7WEOxrt1AiadrcUgl7qpy93n3/8zFqiF2n5nQx6da/3DxNhLc4bg5ZNV71dbPt0/3D3pz/rX1/x6mrqN89Wwyqc//Zh6n55f/mjTZZ6d3JGePg8TblLQl1v17XUsc6NJL++ef/u7dvN5myz7nKWU8XE4Xx3sX+4Ou7vDRGNkFmqPQl6BALOyoBHI4jPT/uby91aBCIo1WkD++1UC+Gb9fr8bD2fHh6mkcGhS0lognVvdze3VeMQI8RS7vrV8Pzp2W67fnd996e/+Pb6dv93fvzp+W619EpCFVOVpMibJ6yTiJCqSYTeYBPFLCW6R1RpmYVg6wgbr9W6PC7aU6ipqCOkFWSiuveWnYSYSKgxgsnQEhNESBgkSAhUlzIuwOF0muZY9elReW+f13iUhjh1Kry9Pz252FiyRcVW+SBrqS78v+rjWRAsQn5jbSV3q82p6NDn7e7w5v17Ih6rn4L08KaBJtPqoaIiElGCUd3/8qtXTrx8ena5W/V9FlJVI1i9znNsVoNZ1FAOXcvIRERgmksaT8ev337z21fzNMoPf7QRlS7n0f1X78Z/8Gl68aS/+3rffAHzODlrmauqlDqfxun+7naz3TFimqbzs5S7/nA4/PGf/MlPU3ry5OmnLz8yn1a9KARNbcVSkFibPKmqkhM9WL2inlZDryJiMlc+VEX4+W51f394cD8d7mqZ1/2wWeVOI+VEdxYHMGRZDd1qWOWcQu3hcOg0ffHxR/f701ffvJ3n+R/83R+cbYba8H2T11PKT583FR5gSmaLAhiEWsoKupeFckUkTVC0+pBMgwyPGhEeJAsXhlNU7vfj+5vDy4927Q6b/gKBidAkPNpRJ6BLEwqC4bWU+u76cLsv0BThi9jAwPIhwsc+7DCNZ9uVWcPlzWfDWIQ5BSICogaPSifh3rwbfn1zens/V95e39xf3dxMp4OaAkgpNdUkCBENd00WpC5mhCaTkxGnaf75X33zV199++xy+/nHzz756DJnC/dprPf72SlB1GjiEdXAYBVQ1BD18HB42B/G6TQM65Q05y53+eY4nk119/Hw1bfHeS7BeP/+ahyn1Wp1PDzc3T+klNuR3m53IFLXb9YbM5tO9/Nc9w/39/tjUjnf9qqqyZKqmiW1nHPuU9d3OeWULOW82l6+ux/LeJwpM3QO2U/uwO989nK9yof93TzLNM0PD/vbh0M23W277XqlaqepqqTNOq+Goeu79apfr4fL7WAqlvvVajUM/devroV4+fzy+mb/+vokgJq0XQws0lQ39IAepml21mAwZo/TVEKkBKYac/hUYypeSIpNNWrQiQBCUIrXIBENFKw6fXp5tiRHoFGQixVHl/zS6qqpMLy6e/VpLl+/urndj5PHNJVxLlOp01ymUufic6lT9bnU1rhe7rq+S4/CyN8Aokc8Jo1cd3cA9Khe58m/+vb29fv9YZzev3/vtXiEqbYU3aVsqRNTeszTnDuju1nSZELMdWppfC61Yb6Hw/jq7e1q3Z2t+1p8f5xevb8/zjjM5X6/35+m/TgfTmOJOiTbrfs0O0WKSY7wV69fdV03z2W72bol3M53dne4v5/mojm/ffd2tV6tV2tVKaVGRAS6LpUyb3eb6+u7s+2m7we1zOoQmaeRXK1WgzYxWMSdatb35o5o3E6QlN2zLyO/+8XxepwlEONxpsoPv/hE4K9fv3v15opML54/P52Od/d32yHfDSoUMg6HUgLzOCfTqIURfambzerpxXYq/u523K667//OJ5X5+Udf/Oab9wqKWbKG8RdtTVWT2hwFENCTpYZrVFCjbobhcJrL7Fg6L3qdp1JMsxmOx2NUr1HdqapDl4R5dq8euTFWjdwCGAGI0xkwRbgwSghLqbXUcZoOxzmnvOrDxZoAmVM20yalqqlX92hS1nx3e5iLd0lrCOkgktkijYkEFzm6NSRBznOtHrc3t6dZ1+ute12wvbfixgCjlkIBIhmWI2giQI2meEv1GqxJTKABj+DxON7dHQm4Y7ceHk5lmqbWbEKUQndE+PE0JYUHUb1QOJ3urm+uz8/PvNRu6P9iv7885oCcX1yW+dbrSF/P07Rer9ab4XA8imipZZ5GVRNwLvMw9LlfAaeIGPrh6eXl6TiriJmaGSmqUYo3Ll4V1aPvz1O3vnv/TVI141Q41frD73+eEG+vrm5vj+6cpuP+eHj20YtxmiJ4d7sfD6eU0r4INOcy+jwllVrqyXSe5qHvu6G/WKXr/Xy23UwlutX5Z5988XA3VdJEzDSZtYpU3UlUx663sdQkCIECySSlpCLn6zRO5TTNEDFVAE/OVg3v1bPhdJq363XOSkrONuTUWfr29bVCVFUb7CdbM4BolTNaM+g1Sq1kuKN4bFb90HUQPJ5DmDWVB6BUJm1kAZJAjofiSbFwF5xRBDCVubqZAkQgECAUmGo4ebnd3Ly+uavexA7KkgRDgh7MkPDN7mwej7UWhDael+GNMyMpsNYdCGU19NPEr9/tA+zNklnO3ET0pu3KVSxQVbXUSCZhUBdC6Y77u6uhXz15eXH/7u3TpJd8ahhV/Msv4ldf5WRpHKf1ei2ijEid3VxdX5yfE3J+flHKPJeS8qCq0+m4Wq03u3OfT/vTSUXUQkUB6lJIIECtPpydvb16f3t91/d9iN88HF5+9Gy77m5vrr/+9p2XuLw4/yBu/PDLHzBqNqulmoliJqTffSQIWppVhJhO1HH0q4dayuzMq5Oq/ekv/urv/eRv/fo3v726PzqYCPeoDKVARVWHLofohhTVRV1CKDQlATTPZdcEwYAa6CzupZQMG/qhEFQV0VAt0DL7b97cFve+y30yS9pny5og9OpT9XGuzRpVg+41J2VgnKuHNwnqNM0CFUWyBNAj3KN1SOEUgalCpVNNpgEqpNaqZmZWyixqpRYAXsIRdDZQul6vLy8vb+4PqnAubhBAFiMMGPTWjdY6mkqEQhjtTzAWdTgAg4g7r/cjeBI1BtW0lrm4q5gIutyJVhXZdDYWT0sLuLBLGKdxmkch/4vnF0/WfPgcz/5IXl3d/vL4UGrsOhOVIL167rpkttmuc98BcTgdyjjWeVyvOgaBeH/1/s9+Xp89uSi1LsoaKWYmSClf7rbTfDpN/km/+dVf/fl+nPuci/Nsvf74+SV92u+PZ5sNqf2673O/3aym4mfbTSmzg6l4SoY0l1IjZQ+o2lQ95xSB6lWQRPRUjlM9nZ9v37575/iRdiv3owidJJ2BlCxcBD5LqApgubecMoTJRIKuADF0qXj1cCDmQncnRDWroiGI0QmhzBVCASx1oqwe7sEpzFw41kCp1VSCAhZATMVMfQpvzoCFp5Buk7uUKTyepvAKRJdVRNwdWRUyl8rKSRU5tXYvvIoZYIADpTpFoFAQzogqzpjrYf/wUIMR0fQMto0JYWgEBLy9edflvu87gcxlRpMzwklleNMRm/VpmsehT2I5ahAR5Fxql1OfOzUJx1RnFTXtu2RJAMBVEC7NuJE0PTX54dn2f/rNV//kH67/2Yv1//C/hB1HEzWVxv4Mq/6wP2iX1+t1mctmO5SpHuqUinVJVUNVIQzkT7/48nyznucai1ihFPNaVMBwiJZavvj0Bz/4/IeWkyVjiCoB+f6PTZOJWCPNL87PqruJOb1UpmSAQhBeRUDKXIuXGnRVE0ipczazlIa+7/qejIcy/OP/7J93qVPT6u6l5K430yDrPHl4BJJpUyrCXUTMdFitU8oggzweDnOZIyiQCLcua8BJM1Ntdi3xWtyj1jJOcy2zihavrFVzEkjKmcFaWyKDR6nuUepcq9dKuMJUF7crROju0VBZzOM8z5OYCUMI9+K1tP/ZGjJhPFqQGLVEkGIAPBxQG4bnHz392Z//7Kvf/LrpcoGQWIg3af1CVHqRlCCZJL3yMdCiacZsQx/BCDH59JNPutxVj+NpDPdgRK1Nzz7fyecvng2drgcrxZNqYjACKtF4xNx3hToWxmH1P//v/Pu/RyTth8td3pMm0PBIKUXgeDw9e/rk27tvgMbBIhweQad2BPj8xcvLpy9Wm9VOUqOELJlqElE2k0wyaeYahVlqkm1Olvth8U82PNocxKqiwoBl8+plntV0PJ2GobeUm69rHsda3cMB2axXOScz7XJXqvd9d7bbpZS6vutzLrU2YXuaJhWxZGWemwPxdBofHu7NrNS6Wq/UTEVCZL1Zl1pOp3EYBlVl+DiXbIlAqYURxZ2hOWUkywuXqZwpqqIWDKiN8/G4P0xlZttchtdo9nqVRveqiLTGV8S69cosuxfXqR/WwfAaQc7zmLqtKKL64lknIOK1AGJCBlXNFrlZsulca7/ZkiKaml1qsRkTQfFosW2E5dSdDofqDkDN2owIoOTiDiBENY2Fh9PR2QC3NG9BqYWEqp1Oh8Oh3ilP45R2u11KWUSDtcxFYJeX57PK1/vxi/WnwYdfv5ovnmxPb4/P+3RnpqbH01F0NZUxSjmu11GpasFpPfSbIZlKE4sBuXu4/7Of/VRFxFI2a/RmMhM1EQRdpZnJNaWsKh4eEaYp50TAzEBUL6amKaloeKnB1hv1Cdd3D9NUG6++UFm1lGmaSyGbpU67nFPXIcLJLpmlpKo5m0A9XB+ZzZxSrbW6R/XilcEgw11UTRWQeNxIMFLKonAPBDRp+2oRCa+qKRillFIKybnUZJpTIunuoNdaHs0bFDWBzPNE0pIly5ZMRBEebBSUiGjzyKeUImLxL4Feo+87Ua2lfmgzFk1PGE4RqilDUtLcZUTc3T+UMn+w9DRtS1U+MP9Bmoh7qbOoBNE8AlRVqgLN9rfYdEl58/Z1mWYKTZqVuan5Dsi4T69SgGGCYKTN9jx3WUWI2N/dFg+fZ/TZOnm9ufviaffb+friPP/FX9w8jNO6r1J8/7CP2Pk85qQ3V68jYjzuLdl6sxJxtAzuCPjXv/7VN7+VnHsAfd+RAbEyT4++LRMgpUyhiiYzEUbAwxFRw1WtWQVFWrpDqTXcG8OdzEopJMyUUFOUUj+QSCKPnlJd+PLWu6AZIwCTFEITM5VSi4cLRZMmS4B4eFSPxn8uJaN5xtDKK0GgeWygiDZGRETjo0mI0LHMGJAUBkLOlUcAACAASURBVIUGiEAfJcCFqgeae1Ys0QMSqql5wZtswCYGaBJQVEkBPSh7abRq802i1mpmjeNtHT3bFamKSEDCq1kStWQ6eVNoIICKmekiiDabs5fFpy6PvC8WU64lAdSdqjKeRgokZPaJ9GZgFkVE3JdTsxxLFPGaDscHHT9M5MHSULxGmf/a67dRj9MpPJe7cSqzrdbj6ZSSqcnpdBI4IV22frMLRK1VBB4UUhUBilpKeZ6riKUkXr14DR8hoHsoSCFFdVI1kWbZWqzYy82JmKamgYuiQFTN3cOLs+GQJt2YmnnTewFCPLzZbFSTNE8q6eIaCAYCuevY3DriSAkgGbUGKkqqptqMw10/7HbnOafxdNrvH0iPGq7RHIGNe3avHkuOqOHhYYIAGj/X2jQKJaS19RBxUaCSVKoka9khSI1wurBZjAGJR9quKfQIRjM7kdAlsmszs5GMqM3FyfAmZIkqoRqEtQgwACZSyXYCIBKALZ7PaB/T9Zta5mTmrk12q+EIA5v1NTV3BqLUGo2Ibgp+0J1c6Ltlog0GimpaxkpaRRMb+lw9bqbyrlZV++arh8vN+v0sKg4ITbrO5jkQtZ00EVmtOhKHw54IYchiCSSoQZK11pPq0Jh3s0Sw1CJVYctEhddoNHnLXtFs01SIQCOpRXgtTi5jjxER3nTRNjwUEQvJBIVp49mb/F3ZEtrjwFKDF+4fLAasYE453MUUDEQALgQdk09lOpIhQVgbhxNdWFyqout6rxJBj0q4iYrEosULhWoKbYNpFipZEQv9hPTBDrkMN0Cq1yaEAXw0ADfcE6rqtTSLsGBx1n+YBgGXIShTNL2IWMp8Mo1AREPztJQg9XGoqMkHCCoCkADCVGoppZTmOGwjSLqMtjCk+VZM4M2sotoGaSOEYJsMaJ5jAeAeZmKmKTyoAFRAZ5smF9WkGu4+eil3tessm0FQ3OdSqhcFVNXEmjO5SUp4dIkCdGfKrLWYKiPm6RhQkF3Xg0iWai1Kg1DJ5vxi86i2iSJp08gQOBgKqMmj04RJ2kROq4ZcTC9tbsJZfblJWWCHQ5Iu5xeCaFO+Xub26JurxEScsVRGb6UKIKOW5Z4c0MAySKZC0muZDiKpSzaVWqovU8AMUExtWG/KPFbn4tAHzbK04ffAMn7ChfuFiNCaL5ZeW+9P4aJcsKXl4GLuD7RtR7SoeuRUBXysBUDKpgI1ltK4spinKeW0zFa0cwtQ2AZmVBWQMo/A8sWP0wfaxlY+TDUI1KMiPCgRtSmsLXdDre96eiUARzJRs0RvSbcSUNEyTfe8OZ1OKlxvt5bSq+OVVoVLn1TgD8fJTJs81xi7iEhq2nRothmJ1isq6fM8mSKpqck01QTvcv8wHcNDRNVsszvrOoNHDb+6vgUwrNYvnr982D/UGhFRvR72+2R2ttuu+5w0VBMgp9Pp3c19snS562ci5WQiNTCNx/3x1JutdztAap3meU7JNn2+ub03026z7Q2Sew+qYP+wPxxOq9Vwvts2e3NKNpf69v21kMOwWq16CgwQ09NxPByOEOm6bj0M4dWjnE6nWn2uBZSUU5f7lFRE6nyq8zgXmjJ1narSa2k1351BUc1Jm5PCnVCJMju5GgazPM+zSs4Z8+y1zKSpQi0E0qbPaqmmKNB2ttfrFSilzrXMjeUFStQiIsUXV9bm/MIkTeWkIg1ULo5ugUkmaxt4SUnM8uhtDkMAqlgbdpFlmkYsd8wSHqpKRNQ4jSdV+d6Lj9fDENPRooR7Db8/jenZ0/M+59yl4+n0sB9LKTFWoSdNwmBUkWC4SEBFXFSbkS0J3CEabaDKay3g8pUi1oS2rstRx7m6Dul7z54djg+nsex267vDnpTzs7Nhver7dZfUjKWUm/v7lFJO9uRyZxa1eqkxTaf7BybRlNJcKizOdkPOOXdydbtXs97YW54h7XUSpdZkWZK6B1ShqevTbr0CS9elcOyPx7zbXmy3re6Mp0Pf56S6GfrWvJtYMumymaWhsydnaxUVExMpm9Wv50ktb9fDJ8+fWtLGYFzfPfzmmzcNB1uXSYEydVY9hiRRi6QEAEmyZIXM82mzGk7jBIh12TSJyDhNgrROuQKW8m5YmSlEiD1ABPPQJ0tQDY/qcwS7Ps/Fc79SYdd3pFhVAbucKdavhsX7yJjncnq467qhTJMsgSULr/FYfQXhQTVjVF8K9GNdUGs8bTS2xsRSzn3XnAgRHu5OzymZIOa9RmVEMlWVYejT06dPui6rynqzLuVNeG1jxUCMx6OZtlm9ZeBCDRBoXsp7AI/2aD4OqjWAbil1fR/0nLv1diUKJ/ph8Mp3769a+zmVqe7r1c01HZdnq82mW3UppWymr9++YcTD/nA4jSB2m60abu/v9oeTgKv+fr1erVZdzslSmoKD8tn5tgaKu6iMp0lNh9UgauHhjL7vTPLpNDLLRx89+8kPPj3frRGE6k9/8ctf/vb1Jy+e/wc/+VIfxz/3+/37m7vw+P5nn/zo+5+qArDcdbf396/fXY+VLz96+pMff5lM1VRF3t/cvbu6Jjmst6vNRlXd3SNEZTrOYXZxfmFp4au8+sOdi1jO3Wq7a0VTgb7vT4d7UFbDalgNKtpI0ViU+toPK1tkAzK6g56SQlX7ITVzaDAKLbqcU6eW+y41SlatU2C0LqdU5slUG1QQUcKbybeRvRGeLAUDVWMRiZb35zT5ScRUAoAwpZybGQRow20JQMJ8uelP+1IcIjCzQZBSTgDdA5D2ZhhQBE7gdLhvYwumSJpSMgICJauZCQWmjzPpklI3z8VsOSBdGtab1WF/gJiaRuD2/mHV96dSBEyiqeu6pBcX5xG8vb3r+q7M3rqlUr3ujyJpNaxX6w0D4zhpQj1433fJkiZ9f3u/nfqcetW0WvcKHMZxaHZyM4JJdRhWOacu2zTNu1Ue57nLySHnu22/Wo1VjmPNQ1+1E6BQjpGn2RkhguMxAAni7hSv7mbSCe2y7w8jxVTq1cP41dv7ZvNJyW5u70Q0J+n6Lpm1dluBLmfPZA2SKuoeomxsWZe7rh9SlyPatECo6pC74zgBYEhIqIFksoX2M0sEzjr9/suzs+3qz3/16v3d4Ue/8/zlk4tSCaGKXN8d//Lbq2FYffJ0fbnpG1WhIm+u7v/s4ZBzNpGyIDOBQMMWYzAaWYZ2QKAhj69kiACD7ghKsjZxTTUDEeFoIlEDmoI+aS21sU+mCrNMT9NUhiEvM2fLNE+AEkINIUoEs/XQANjewANYIxO0McCUIHOyWguUCoPIOB3L9ZxSUl2Y5HkKWeF8t9sfT6KhAghu7x/mab7b799d36akqy6JqlEsd6fxNBeYLpMVJrkbVimZgNNc5mk+Artdr4g37+6229XZOh1Hz0NOKTU7ZYRD8lzcUlqvhtM8i4mFvL89HKZvIeLV1fT25ioleff+9g9/+pdq5u4MhHt1F8X1zX1xf5z4Qq2FEaa63x+//vYtW1esOo9HEeQ2si8iXGB0mUtE8wiyBYqZTJwVCJ/dZVgNkgUBwkqZq1dTzSn1fRt5wjwvgMTDk1l1v7q5H8f95W57GGdLerHdXOxW7gFRE47j5F7nedquzj+6WLN5NsD94dTYNV8mBNs7GxQfhtkeq+SjC1w/DBy0aYNHh8cy89JeV2CWkoAQL67WGErOsxOhKpY0mUapSUUihEAtBYspkwCVKm2KRKhKgZVatTn1WhPS5Hcu56I1LqQtkjxBslZPCwoQET7sxyeXZ2dbqZXDaj1P4+F4HMexz5mJj7g49V13muYyl9QPUyle62oYUkp9TjXCTGsJs7Tb7p4+eZKzvX13VZwh+fwsb1arU8llPJlZlxPJZNoZUkqqFi4pqQBzLQJ1hiFyyklWidZYLEBEImf73ssXKskhpcbSmwFqutlsYGYLJykgI7wR5RWySo1G0Xbjq1Vfqw+pH4ZMCKNGiGVLZmSNWKbXCUDCTFNOooRIrTXnJGAypPV6t70odQ6wegHidKzH0+16sz4/O//rN7evrm4jaKQl3Z/mCC/z6ds3V7c3d7N7s/3d7E8iUhalhCQfPZdtMBPB9hoRAdg8LO09WioCbxOt0caRwYCKQrpscynNsKnQJ08+I0OmO3pVlZxSzgZSY05zKc1enFIySyoANcTtse1t7ZCoGJVQk4rlHRepCd4QBL3ONSJUlG3gueHKlp3VNEIszdN0c3u3WQ19P3TDEF6bdzs8mij2/S++eP78BWP0+fTL37w6nqpl26xWL15+7/Ly8tuv//p+fwIA4WozdH1/cfEkd3Zzdycis+P6oTCO52dn3//yR3Q/HO+Keyl+sV5Xijs//+yzUub9qZhqkCamws12++Tiyd397VhadRNGm3ZM1g8+ntpIkbZHC02b7TAM4zS6L68RQDCl9OSz7282q/vb6wIkXSzV52e7Fy8+cZ/G0xgipDFCBZvdLqfs4QvuTVJrJLUXL743Fz+OJwTDgwivnlRSzsUrF64faNPJlgJ6ejhUa3ybAOhX608/+1xFjzfvbq+vBChEWDeXopZVlREeVUDVzpq3GgIxFXpo7pKX0tQaRhgkCNFl5vuDzOLuTdDIZmoGyP3xfpzeMcqLba+iapK73GUr00iIff+L7wmpIuthOByP8zzqI8veOl6Cas1ZCVWZ3CEwk+aS7bvUdZmE19qSoZo2fl/FLBkofWdm+XGqh2bmUQ8Ph8PpdHd7V4o3W0s4x/F4PB6T2dPLC3ef5rnvOo+4v7u/3+9Lrc03MJe574a5zPN0ur/f3z08dF2namY2lzrX+c3rN4fDYbvZqMi6S+v16u7h9Ob9+3maTqejpKxqhCQzFRmn4+tX3zhhlhcCFIzg7c37m+srSX3X5fbgGim8f7i7vb1Ry5oMjxNEBK+v3j7c30hKOZmJtgHh4/H05s3r/f7QuHhBm4FtM2LuEU1uazPdNeLu+uph/3C22+VszSMJoMzl7vbqcDp2XQ/Sy9R3GaS7z/PJq7dh3haC1ePucDwcDj6N4bUSAc191wqjqJZ5bgnJmn9GtUFAVYlm2mEQkpORNDVpuJ08TKNAbOG70fWrrkvN++TuUylRC1if7oac1JJls5x1Go/hkf4/pt5jV7ZkSdMz6b5WiC2PSi3uZfEWOSEBjjghCHDEGd+Ar8AH4AMSBEgQTaD7Fruq64pUR28RYrm7mXFgK7IaOTlIZO4TOyKWu4n//35wd4SpFLNBRB7rNIZ+vwqB0FEK5x6NgNwdiImACapoLdp6dOoUjiSIiBCIK3oDkYZ5LVhEw70wvXpx93Q8HKxVFRHK4U0EIqxb7u5hwF+8etlH//RwQiLA4eaiJCDn5VxrVVUbqlqRuQgvreeyUBjbgGGB5LNgYCnKh2V8/PQQgSrck6mSw3BI5B2ryr+Zq8EZEQRZeAxTZmJcrWsI6x47Vf+UNvIAQLew0cGRKBAwHYTuzkyqOm9mYQnwcJ9UHKAvLopMOsLMY7WxrL5zX1qfJklTr3CA8kLMkFLHUJVaZ2FYPEbrQNAcyAMxLggqEkIRMCwCNMIRO0Kk34SIPJCJLywgyIo7rVHDLF8JsaCbeRDRakFwB6IARvAARwSzGGbhYb5+0RmCmASREEgIwt0MACQAqwoAPp9OwwwCASlXwPmU5XIfAYnQI5CAEBkjL+X0HbOQCNtYq/6L6wLyGiqlIkaP8Iip1s1mev/xIxIR8FQLADqg+WAgFUWC4+H08eHp61c33371Zfefj+fuTrnvmKYZAFi4LU0quQ1CZFazQaDH02meVqChu7e2TKWolPefH5d2JgQRtnw7GOM/c25DgIcnhgCJc3VKAMwcYbTuFdatvBCbkDClOppYEcMxmIjSye5u7mOMXJBn37Cd6/rv+0AmA2en5EflR6WqhMiETAgQrRsEjN6BCH3tJdPTPjwOp9Nmswl3JEZbhAkI3GIk84TzLSUHEBVog1kBlxUZSUSBBJDCV0x9MDg65DrZISjYE4F7ESqNPmA90AERCQWRkIAAHQEpaN3qQgCyMESEQxuGwA4uRVWEkbAWNasPn/MmSDjWBWe0lvrM2fjYSEUVIgOC2WAtK3sh1U6XF5RSRCbIv5pr/ebLl7vd7k//+F//h//wZwBgEZVCBG5mEZwAJuu/vX0313K7n//47Ze/vP/84eNnRJzqRAyl1FIkzWTWByHVWloHET49HYjoPE7ISEAfPj6MYd9/++Xr+6vR2qfn53AHCGFWFbOBWXBRWjmQiYIuS0dwJCIaTKwsmACLCCUWERvCjCq8AtIAIRK26eGBlEcLAcboAzF6W85Mw3wMQwR0ggARJeHT0jCwFjGPNnqyLJipqLbWy1Qqy+l8TOEErZor5Iinx4fNfkcM4FyUzRwRBXHJ7U8EECiyqnaL46m5OWuuWiP3S+nuXAUMEZEoUA4wJ17BjhCpvkO3QKJLOYUEIMKMNAgLq9lws4iAIAIeKXLxiDEC0BxEC4eDIILqNeFbzoJjfT0ppSEiFR3DgFjIzFczQvIH84WYuwcIXurFtQfNo41JCAEc4de3H+vD07TZAUBVxe0WEIvIKoA2AwRhWdr4+dd3bdy8uN5//fpuLOfHsxO6OW63NRynCcwHmLnbXCszFi27rbc+SlF3QCJg7f38l1/effvVm/1uPp7PQIQwAFxYOJ2JHoMYiVW5FE6dDxKAswibMROqchbC5kYBz3mfIYpKqicYyWTV8RZNdQCxkofHMM7GAiB1/aUoM52PDhfGTCma+28lOuGKAlqWBgSFdBl9jPXyAg9ErMLWl1pkqtXMzq0/nTokSAQQVYWRmcYS3RsQCoYBuHC4I+f+mi4OZQQEAk7vfBpS8kNjYo+RfwBEJGdkQIy1hAUfxpuy4RoBIWTDMdAcuRTv3WJAWKoi3Vx8+DSVbt7bUCUKIslRLSKHu9G6ogAkijBmRIt0ZDITMXoABwiL0UCA32GTtL5eRgIhgoJueDqefv71HSJeXV8BRJ0nRsoPgMV770ysWgHPHvbx04Ob393sWQrGaQwvVZT5OLoKo8VACIhSCgsS0W6+ZoRpmn9++96Dng+Hw+lcp/rnf/lbVb7ab90t3BEo9zmpIUhHjBDWonjxcUc4ITMhJcOdGBGFKRVZIqJMUxH3tA2DLwMRMGiYM+dTj4xkvTNzuBFhJTZ2AO/dzC1soMrNbjJzFlKiNpKxglez1lKI0AJ6g0ezMZiQX91uxrDHpzj70DoRrnNMMBABJO4WLMIsKXolhNF6AOYEbnX9UvbOCXpEJHKPlPqFJR6NWBgJrV8gyCvCAfEyX0OAm+vNzX6XUCKIEIDPT8fzeXn/+PTy6trOw8PRLVVgcrUpWuvT8UxFPAagY/AqcIpA5ABAgjEGEhExGohEKZMKp1ceAVbtS2LAApDzuFtFNEhYVAKie5h71kl5+s61MqFHeAQjAGja5YtKFjdPh6PZOJwXd9vO21f3V2MMIQjAAB3LuY2ohfebHVNM0zwcjuclqWDD7HQ8LMtSSuGrXd5ZROtkKx1H5skUCncnEmb0CCEcts5kkNZOPs/pFa+CEAFFxcxEBABbb0lrqYybTVHJExPfXyjUX97vlROZCW7+n/72WwKJfvziblNXO/iHh+f/+/PnieUfv30xVw1MJWX8u3/+9XTupfBXL69F+N3H8tefkn8L5kgiYEMkZ+ghdSLC0QcTYxgxnU4D0LJhJiIRjRTFrcI1IEJm8mGIwIAk7O7ogJRMEVjRZLi6D3LW8M3Lm7urLV6YuD8hPhzORPj0fLDW7q72OCyHMOYhKuV6N22rAsC5LX8t4t1WaX78XuWtx2wAl8KW4lynUngzVbeRkyXOzw+RUtIPjMxEsJ/nNy+uA6C3fj3ri6ttszi0rqLfvnlZCkPE8LDR3338/OnhJIq7zVSEEUmEVaWdz6OPNqI5TnWe5jn/otPhMKwXLXd31+dlHJdlmIUNZgbzFzf76211B2a82u/rVJ6eDqmZZyIRQpQ+BjGnkVmFiSg5rAWdhXkQARBzTona0kbv7p6SN2GmrBoIqwiyINh+s3n18kq1KBMzLks/Hs9M9ObF9X4zEyEB9tF/efvp0IbZuNptdnNJOdDx1MKBC7EWLpUBiGJY4OW17bbbuep+u3lxd/v3Xz68fzwQYRCHaKAToihjRG/DRoMEDbqvzgRCQhqrBDJ5GuzmRFn/ACE6YZb/bk5CKZsiQnNw83meEQkpwpHApqnMRVMpmcu6CJ/n+t/96XszOxwOTw/PjNGHW4S8/fgQRKUoQZBoETm1VayEaAgMwG7mCOTgGD5yThOYSnDEq93VqS9MFKyISHTRK+GKlNvO9dX9DSENd3rzAgkfD8f/6//9Zwe/vbna7zc50R3DltEfn07W2/2b+9vrrZv3MdxNhVIGuDw/nRCZhVWKSABMUwW3qqRI15tdUenDTkt7fj7/8N2XL++vwMDRmfTpeDwcTua+29TdXFQkEMykHY9PCMy4mwsTAwYh995qEetCCDebwiIRsdGpLfQRkRgY4Wa3SdgsEURvjAhA01Tu726yGEAIQhxmAaBapqlCEvqIkEhLIaJaaqklNz1SjsSERNM0zZOubA0cYZ41UREpKkVlmqqZf3w8DsQ3L642kzIRIyLTT789fHo+MMsfvvtiO+nvGrO//vbp4+MJAwnZ0SgwwpDT/xCEidtJ7xZToXyWkIgoT5BgZlx9LlCmsi1S63pBp3NAtTKN+5vtVMrT8/T/Pb6H8G7D3GVX+av7LRCZhbttN/Pz8xEDkEZg8r0jPJFuiWNhHINIHJCB3GwZLiJMw9lX0y2tBQoyEhEDzkUIqRbKo04wWFhVK8EssIromKuwqCLRruqb2ytac1igL+fzkLt9/W/+4dtVZwjBImM5vf10uLve/vDFixxzAcB5aX/55R0AX23nL+9vV000BKPXeS7uP3758sXdDREA4Ogd+2lpN/tt/S++vC+VCRkiTkv77e074rKr/KdvXxXlAIyw95+f//7LW0TYzOXHNzdZ5xHA3yh+fbfFgKmWq82cDoBl6ay63e57a7WUqZaEu1gsWst22i/nEzKLCKyTI97urqYiqlJLDYiR7RXzdrv30bWoimYzW1W1Vgn64Zs3b+6v46KbfDr1xTGsf//Nm/2mBmD2n5+ez58Pzbo72AXgl6rtnKsBoIlquhcwR7juAUAsc62jj+fPj8QCEcxYVVk1B66IFEABKKIEACxIvLQW4eY+3C1cipavXt0TMwC4+19++vmnX98JMtEqLKYkDAGzaKwkRmLixDojsJkRCzEx6GXKBADwexyJgxdhFRHOIRwQExO7xVjlvqumKF1SKactuUFQRoTNPIU/CfN+PzP+m2NCVd1GBE615loRMMx9tNaaE+JUBFaBVTwVaefzMC+l7LdTDjV8yH5bTn89bqtOUynKabru1s2sL6Nz0aKqQhAGrMwB3pcR28os06R4UV73toQHEc5TyeqZicYYbVkAQJi1aH4VzLz3MfywnM9EWEqJiIgw9/PxwLQhSkccMntKJg7PD7XUUnSep3Q0RXrQkUlUdUqxZO8GKO5GmD5FyU/EPCf7ySkioOSHWLYRIopuSEEAAwHMiki4a1GzUBZKiEEE5xKaCJGYmZjRAok6+NLsfD5NlYqIqpzP3SLGSMRGyNPhnOxCSJMV82rtAWfOMRU6+BgmqoRkK4M8cvpi7pyKeEw1B+XUc83ewNU9y5zD85WmSUiA0fvSh1EynDH132g2wszMN3OFgOFOmI4mNw8RrUoWEebLaGvngyjMIpzCAmHLUVMAaFEmylGOEJEIR0fEqrLO/lF0FR5QUS2aKEZM63nvZ4Bai1QtgBEQxMmUCjMnzrUfBq1eEY+OQMySsTUVwxMeB4nfz3eORZCYAZGZkYiZI1kbtpJHRLUUzRLbPCIME1CfmRWyiv8p9zPEovo7LOa8LOBuYUTEIklpQYyr3RZ+/ZSfWq5ggAQhCFkkqWXo4eQAzAiAgsmyQQJh/r0JIFp73KqiqigQiGS2UtQCAMkBzksz9+E2fBC6PB2OAMjEARHuKpLjMyIJd0AmBvLfwUrAKBn6wcSwykRCkjoZllYxWJe9q2oGMCEfkl+4CKi15xoRAaep4CVSTpnSj9TMhBgZ5RKG527mPtciyhf1phMRM7u7KM/TnBjiiFDRpbcxXLVQzqYiWISYYmBAlFpW6V6GjTCHBzOpClwWgRAEKOl3KUWSLkGEDoGAZiaipZR8+3PUmS6EhKkhoAePpCUEnJfGsioBqQkjnNp59K4qWhQhQtdtMiIU1VqnXPsNvzjjCIsWQAh3YjZzEk4HoWgyVyC9nB6W0DFihXAGcotpKkSEYAnphkjuI4lQqcXCT2OsqHYWEU4HCnNVJszpHSJQbhEIEEvRogoXi/BYA3Qw+XtLWxDIPMZwJ5Hn06m1XjVbXv7TH777p3/5+2kZ64w4HEAJPd8jD+ZSzr3DheqVWykVjqkeDycWGb0BwMo0ygsU85GTrNjSh4KEQgyEU60Xq2WQcDgihpmTCtM6WVCVcB/m3Y0MA7yUWmudakGkebNlKbbaBQmZkZgAh4eIEq8FCrHACsjFlbsZNMbI2dAwiwhmCo8AJEILB/fzspg5EHBQOjXSnukRQiCX8KHc4ltYuHl4GBDjsOEeeQnUaSpSVk43AhFH9IggYlVJeJoDMAkAEHMpAoAeod0uQxio0zzN1UZvfaxKQoTckiFRek1t9eQYM6uwRypTHIlFBPtABEjvS4SwIPNcy8jDloGAWMU9mKFOG0ZMRzTiuguGRPMxqUp2BhHuAm5uESpchNq5t3Y2M7MAwI4bOZ3PS++3us+dz93N/upqt7x7WAEP+Ymh5CWNIcSc0TUOUdbgTtRcXgFExMm9LcvArqp5CGaMF3HmAyFQ5Ih3oA/zvKvBIQiLltxN+yVJJBA9gllFeFgf3aqySqllArTNZjIPSyIcIwCqrNRrRwQAgZXPGQAAIABJREFUFmKm5DOJMiKxKBGKaL7a1luuxmHFSGEmV+T8y8Izuq+IZEM0FQVE8xAWznoTAhCLciYc1aluNzOs+xIphXsfojRPk0NgoDDNU4l0qAKIClPmBFw2PLk0YgYIAlJVFW593N1sp0mTs1wK7HbbPn4lhKv9djNv8nIgEhVxt1LL3f3dpOw+3GKYnZeWD0N6pQAgUQBmo6he7XeIwUhjdCR5fHxwAGVS5Vrrclouk0REd2AQYWJGWiN0ROnl3dVPHz5/8epVLfXx4dnGgMjLiU5LFw//P/6fP+93MyF72Ln1zw8nFskeM5/d7EtUpFtGCQkzEkpRYaFS6m63vbmazPyX3z6Z+bAhxHkvUiq9RKZSYZ0qxxhWqp6Xs4pMRZBWsO71fnY3B9hv5qkWFs7pyIvbfbd+LXMtzMxTrUjoTq9f3JSir+5vay3plgiEInp7u3334fPt9a6o5pwZwXdzBbBhttvOokyACTTcbqbwMc913sylair6SOXV/c3np+XF/e1ut2XRBNLd3lxf76a//3r89qvXm+1GmFPR8vLFHcZwhy9e3xNLVirTRH/49quff3n3/ddfvH51SwDn87kU2W3m1/fXP//29ruvv7i73knRcAeAV/c3rbfb2/08T3ERuNaqb17dH1t8+9XdPFXEFAHhy/ub7WZTlPbbGjGIBInmuXz16u5vv7z9hz+8SVpu6jLI/dRGlpMGiMnIZaq1/vj9Fzf7q8PplGhqEUHC6+udikYAIdRJi9KbF3ePj08WK1ycmQHFL1DvAJw3m1cvX11f3yDx4XhK17aHzbtbn0ncxn/817+mXxScPLzWudYSCPM0393cvHn9olTty/njxwfqA0W+/vJNrVJKUeGiWmu9ud7f3908Pn3u3c+tn86Lqowk6q4yAyQhWLHmsZmnL1/enduH+5s9CycVDQJfv7i9v7uz4C/evFDh3DYw0s3N9XfffHuz25ZaN/NEhA5ALJvN7vsf/jDPE/Eaw4CIXMsP33zVRn314o54jQZhgOv97s2rF8+Hdn97k42IINepvry/+eLLr17fXZciaW1nJOx0d3v7jc+7isTKkpBHmub59etXPF/f392JyFrpAGzm6bvvfhjm1/udCAMgUSIw9A/fvbm62jFhUSWm3jszv3px9+bNl19/8YqI8mCDiFrr119/d3u9SeVgTu3NrZtvt1erOOcymCei7W4/FchnydwEEQlv7m5//OEPX3/5ai4UEe7ATO4MCMSMyMQGEUhUy/THH778x3/4EQAOp4URhlnvo/fx+8I+ex1mfv3yxTTVf/fnf2FiESmqSGkaDiAKj6WbqOaG/nQ6Wu8WgazAFcYiuWbPFDNfDa6wmeuLF/fffPXFfr9pS3t6fDqfF0BEIiFhJRFRlVKKMpdauvvxtOx3u1cvx8PT8/PzkYVH8xU0kctXEoTIO5GFdtt5t90jE1HaWwIIRbTW2hyZSEQy8ZEwpipuY2lNVUtRB+CL8ujp+XDcFoBgXgOzgoIAT62520WHHBGBhKVUaeCeXsuIiNFacq9FVp5o2nyZsSi9f/9WX95MRZgYKSKgBgBS6yPAiwpe0g2Z6Hg8tmGp6gFYyRzNIup9S3J/uDITkXuUUkqpIlyKChMmvYJomAPCPFVVSQv40gyJnw8fb3c3qoUZkrLugNc3V+CjbjazakKPzd2DtvvdWGkLNKw7oq+iWGahSOwPgKhsNlMfI0AAGRkZqXefNvN2s229HY9nSGBmH+bw+vXLt+8/f3o6IGFWWWld8TAzf3p+Pp1Op/PutCwPD482zN3rZtdFeZgkMwHA3RkAr6+3f/zx+2++erPZzMfD4f27dw+fH7unljzNv6RSSqmqWkuttea6yYIIuday2+3Kh0ezPMwo1UIXkwMhoYQDIIuolqUPj5yRM0aIllLYjYk4oea5cG6999EtJtXCl5Y4lfxPT5+fr6oKS0aseyAyCiFCtyhF1z15YACWWvk8Ammep7Bw726jDZ/qDCJ9uLC5AxCHmXmI8nlpz6fTthYgZOI2ejNnwofD2d1WRRjg0hetE9A4nJdXiJE0+PBzGw+PDydBB2AWCGAIRDsu/fr25uncCWkdGLk/HxYHywaTVTHXAdbMPcI4zZCY2RVoHr0txEAkrArGQL6cl4fD4fnp8QM2//7LVfuxjjaoFF36f5a0gvHuwwMRA+nhcDwvS+ZA7Hfzze1wsw8fPxGRMC9LS3LEze3V82khppKj3Swygty6I9Q6IcDz8+F8OniEI75++ebd8xkXlJSEYujd7f6P33/79Zevi/Bwe//2l3fvP7No78MzgtmcRAHi0+fHB6aqKsrCXEqZpsLydLPbuPfwwYzmkUducvmGWbitHgZfRVseo3djSqYBACJ3QCbyaDYgDYbkSzMbVooiJxlTVlxGuKhsNsnBg1WtgrSeuyJZTHAKjRFZpPVmbgGwgkUMIo42LDAiHNO6AsgMRigim81cap2Kbrdzfq1TF599lojkD0/tQA6QmFlLySNtDEPizWYiDJVSSrlEPbm5t3YmpTY6szjHRTxBiODuZrbGNkLMU9lfXU1TbX2kYhYBhrsWIYQ+bOkDAxIvCkii4hGn0ym/2RbWl27uZVJtZYyRI8xaBCHef/x8Wqy1xhRMcm59aQsgtdYfHp+JgBDtopxz92mqiUldzucMTgCH89JIynXV4fH58+feOxBOsq1T5bMJsyDpN19+8eMP33z1+mUp8vD5808//ZK7T/egsGVpXCYRdnN3C4s2FhrsNqgRM5XWzgtXrYVRBaeqWtjOkbNZWeOysapm2DEyBEQtutnMCTpnZGIIxECapwnI28iTLEMjdN5sbq6vgaUNK2aEhJhfGHj54k5LWcaAVYudRydd3ezMoA9LIAoSu4ewzPM0Riy9J0AGqXAp8zQxyzAbzKu1cEQw397eMuK5jY0bODr4ufXd/qpMVmtZeleXZFO3Ma6vrvIQPZ3OiJCUa0DaX+3d+vPhwDkSMV96c6D9fovuD4/PY2NEQkxmcXt3M1d9PhxH77n2bcPrvPnizUzkh+MZIC8fOC+9FLVhz4djb5q16fF4Fin7/Q6tHU7nMENRAlpaL6U4mgixCGTclvBUy9IsD2ZVRaQNCwCoko21CU/NCGZJS6AiA4KJu0cRZBIQKoDX+81xMWI4nZq5MfPN/f311fa52ehN/qf/4b//6osXEP58OP7y6+PpdMRAZIo2LGIsPRAQE6yaT0wnWPnZnItMQmVBwtbHpAUg5qmOHkDEzKVUFnaPYfb7fql3a72b9ePpfF56LYCEFng8nnMB8Hw8nZdOJGEOPo6npdsYy3h8PrFwqkCHj+fDmZj6GM/HBjNm9eo+Dsfz6P3peDqel1IUgQD68/EcEMx8br03yzkIkDgQoLc2zs2ybYWAZXQbbmME4WKw9ABEAjoP7631EUvHNoCFEKiNcTj2PhoCtuEDiJGAcTTrYyTZtBk65pOHwrrbbc+fH0utXLdcJiIKgGmeNlMVxqASrCuOFPp+t2sPz0TEpdZSmHFYTI9HOHYWFJ2m3ZxWIS7z1VP3CJWKutGJkSACX95tadr9x7/8/elwLKrmLsJFZD2DieZpqkWGxbIszLzf7cOf897JdA8EExWB6N0r0bTdYJkasGdVT+XNq1fL6OH+9i//yd2INXQ+DCrTvB2A//v/9r8eDofPn55PbZmmSVV6a+dzI+bnw6EvLRDnaWahcDselkyYJaHMmcslZCmSTvAXN/s22qfPT+8/Pufs8vpq/8XrF3/87ktc7c6OiJvN5v2nx89Pp+v97vuvXpXCANhHP56Wn99+AqTdPH/x+k6ECcndj+fl/acnQHp9fzNNmtnhDnA6Lc+HM6tebycVTpy3hZ8O5+dlmUq5ud4pa24pWmuPz0ck2m02c9XshCPAItoyHHw7TaLq4WHRR2vDjoezg2+nSoSY+u6I1kYfnRDmmkkdFg5L721pDlBLucwvKSKG+XCnABaKwHAzd0Ays9YH5GAW187OLEYf7l21pFcUEjVm0Wy4uXB25xCwIsYo5f7uuTlAAI9oSwPwx8+f+2iUiYB1ExaPz09/+/vPybGfqlxt61zLubkDCEt2Kk9Pz7WWH7//urf+r3/7hYWF0C6jA/c4nk6t+/XVtqguY1g3S5BciuLN+qdfl/MzaVlo78hmdl6a/Ps//4tqDcx9NpxOCxLNm61D2MOTAwqRKidLF4kgLEfqq+yXmJkA1j8S0WaabQ/meFpGBBTV/dX+7afD6fRMiGbWR9y/eMUkm922DfjzX39LM/6wTiQkxRyezu35r79lD09MQhhByPDTu8/pBVm5fIDuDqf+4fNTXBBfaf2wMIjAvxGpZiQ7ATp4Ev2Y1pTuvBrSas0kGTVnvQ8zz2TbsUSgjeHghMSX1AH3EQERY4Wdw6oKySmOKqvWhMP7JfjbLYYNjwyryD1OLjAQI5ewkHelu0MEM5nn0CPW7Q4kPGEQ81QnVTocThnOBqvcFy0cwph1t50JyQKOT4eHX9721s08AFS5SEHwWqROxWIQi4ejOTiplu12w4Sgsp03y1hqKekpHOZmhgj+dDwtrTXzsFS2goet0WIeZiwSXJBk3UQiSu8ZxIdEeDqdzSzPSXcDhFqUmOepnFt7fDgAIzpNtSBzGvTy5lZlYZlqrUWJcYzu+y3AoY8Y1j9/etjutvM8V1XAePf+wz/90z9Nm5pbwt56mUoRNXdkEmSkXPMRwiXjCNegBET8PTc6L0FcFSU5QsmsG4IcMgMCoa/oSMyc14vqeP0Jv+MRzUYEpr0sN5LMq+MyyXeIoKJp8eA17tQveuYIiMSY5SbYjEfvSYOKi58gh1/5j6zsUAxwcDQ3RAgLB1BhQRiJQkBE8sTkktB+0m7xfOgY1sfSWp6PbjbqNN3sr54OT+3YgdBjPB9OZuZuvS+ebkCmAJunqszbjV7vtogYwITi4ITY+hjDd9vNPM/n81mLAMVmO+Vb1oYhiBUtRZ8en8wHrDnggZCHvVNfkACdgquwILkPcHapVZnEEa1380wGccZQLSqynYt5vP/46cOHD5t5t9ltc8wjwirCQsySVwozuRsybeeKEcN8u6mHQwPwh4fHpffNPE1T3czz7c3tuQ0zV+FpqrynkRD1iJSn+sVbn3HZROQ+IoII3T1XqznvzbFCRvJC3iApZSIipt4bGDAxE7TezscjICcqGxD/DWxJlLjDHNBGRBEWkVX/kPHDyI4AgCqcDQgnv4qJgDxszYxdnWsAAS3xxBk8hyAiSTL1MBgpQf39/Mtcsku4tcFwF+FIaX2+NsQwH8M3m0kFH55PKw0wHCCmqYhQa2eCTKoLAh9jwQgIL8IAkKpxBLy93mzn+dw6EtqI8JCZhSsh1mqt+9PhNJWnPkYiLphoqgUBitnShoqr8KRwNdcRbiOYc5MdbvH+7W/vn1yLvPzyXrUwUXicl0VywmTLUCVvHu7CONdpmJcih+Ppl7fvn5+fp1p1h0wIpMo0TZMWqaoewYTMXBLBwjxNZTPVadJ3Hz4/PD5PtBGhgDidTsfT8enpKdtCTK0HgIUx4VRKoI8RouLDltEhwNKeFZ72AncgckLOjyMHCh7AdNGsQP73lnCbJMlBmAVu5nk7z2HtvHRhDsRAJ5IkrCDEZiqwSgfW4A/CS3YLsTtEBDEQrhGJhOHgPhwQPAAgSbLgEB4hKc3IKGw0RILoYURojAiKF/1VvmYw90v2bQSCAq2zHmHOBAXieZ6KCjONjso0zM2NABJmXjJfFiLiKmtJoiSMOBMT01Q0t7Ee4aNPU/nXn98zEYgm4JwJx6Ai+PS8vHv/QbS03nNpPUbvw20MQrTw1gcE3N/d3Fxt5iLICB5EcD73//Px01vwNy9e/bf/1Q+wamT98XCSCLA+dpupja4cTkBIInQ6nd59+Pju40dwE9G0XVXR7raZ53kzlaKqeaJliZbhy0AsmyKbTV2W1pa/DZVh5qdTzryEBS+0aSLabiaPEOaTDY9IaaRbl3D3yNBdRBS0ACRBEWWiYTnxWO+pXMMgBjHPVWXVhgAxpte8m9kYU62ISOinZVxoR25jjUHNOV+ECxMiKXOy01kZMkAdQXN6R5SRPBk4kWpYuuQs2eiHw3Ga626zZaF8ge52EWxnDEV6dCjtCOBg4W4pr0IAGqMBpmE7EJGF8/RbTTF0ecrcc3KbMmUgzOBmYgwHZnCzpVlrZw+YpwmZwmNp7Xg4Ho5HIXD3sbTPp8dwpzX2Cq63ujS3vlSh3XbeTCXCCVxKYQaRghABToxEuN3t3bp5RAzC4T5UWev0+Hhkyl2snU9d3K2oJL5/Uk0lx19/+unvP/3WeqcESzgFIiPfXk/PpyEi+/1mrlVVWBgczu3sZgFg5h8+PcDN/nw+v7y9/l/+5/+xt9FHN4cAUJaLfWCN2xXmQGBEZs5VRq1CgKtwB1czGGHmMARSlhmM9PtwN42vmUFMCDgsC5qc2GYOcNqZUtCyBo7Ayl2C7B04QUtZakWGBQSmGmMF/UOKCtzcPL1qMWwgICE6hJube5jtd5u03222c9Eabuvpt4YWJquH8u4UKWuRR7Cd6ho9ksk5YRCQhHB3cQjOJJIAAC+aAUaS/0NCwozAh+cNIEwhrGIHGMfjcjgdrnZ7KapCVWWayn67a70fz633nlJkVbnabgHxeF6EeZq0aAlYxUYQGVSamiLjbAHDSy3gEcFC9Kf/8serm+s+xsdPD1MVRnYwdxBCLCqIULQA+k8/ffjnv/x0PB4DfLWakUhVIYmAWmQxZOanx8NRzwTYR6ul3Fztd7utppDQ7PH5eLff3N9dF9UcTzMnd2PVPjFeDJ4saxxaroizbwPI2PS43PqIkZE/hChMyJxdvWfTAr4O83KPDiBCjAwr7dwgEDiIKSATwiJpF55+BsTUYqxX8AVFnRIYNwuI8IGMyQDrNjJO0D2WNghJlCKh6EiIWFUt5+YerXezwax5XLZzQwAWysCSMbz1seoOAfoyHAwcSSi/8/mWmANA2PDWu4epqnkAoAhvyvT0/ATImSqQ/SoAMgtLXi98peX6GjyciQDJ3ec5rq73BOQYuI42IY+Yi0ETsth1j/CwPE1Tp38RhqFbIOb5QuRmQaLffffdV19/NXo7HU/nzMTu4+l4EgJUlQj7+PHj29/evXv38eHQUIBTeV7KfrsFICBCZABSCWHabMtUqoEpb6eadkUSRmas0ySqk3KtUy2CSCleNXPCaN2gmxPVIsP6OJ3SsyZaECCVDgEO7sMsv5Yew0d4StEROiGTIQISR4T7uHgsDVfodJgN1ZLIp+xF+xi8mvbd3c8Rm2nqbRCjSEUMD4a0kdK6sANIqpcLIyHHurmH6hKAZgbh+90Gic1GeIiwe6hy9tGp8WTGqZbWPWWJm8021lkUIDEgjG6RxJu1e02feqpPyAHMItwY/XA8U60+OokULqLMSKc2WGdlhLz6s7nFZKCQhbkTAVzsMoHIOUmAiKRDInjxMIdMgQnPHGBMFQZRREA67IggPMZlCIqRzk0yM4uIAWM4IKpWnYrUzdSH9TbG4IcnKbWcjsff3r59/PzQ+gCGWtBWDjy6wXnptdSp1mkzCcuE/PXXL29vrmop2S4RhgpP0yzCKX3JBpAufQggFWGXiADRoCxSELAJwMhCBAA92eUQCJBvviZFt25SIWjrb4vMwMQiJMQsGZ9miTjK74p7AeS1G3WI8CwMItbQ+zxAZ6mWSWzhAMQcSDFGtGV0t9ZaKWU7ay3l4qddy8puFmZZPYrKGCPvZXcDNyQiFnd0dws/LS2ToG1tGtKbAxwBiKocEUiQuhlC4bWix2RKru4AhqlG6+0EZi14QhFJokWeYSs1C9NbjAHeMkw4ABC7BaEDrDLKND724YhAhMRcBNmpLcMxAB2JLYIIs3YgxOD89ZE9Vce2dmHgw9jMo4T0YZ6T1VAVbmOoqvtiIO8/fjo+P3czqVOwDeIa3CPCotYyzfNmnrab6Wq/v9rV67ubVy9f7nazrrpOzrlf5nzham9YpdpIlCNKHI6EGS4OAIh2Pvfrq81m0q7UhpsBMhWmZRlIXrUAkark4QNEus4Lopsz4mbS1HkSYh85/4MxLACH2e/43hx4CoOvY7J1eJWz2Qh3D0YNCA+CiHM3wgj3xQwRRdURng4LEBdhIrCcyUZmeYUIAtEwRxYAS1IOC48ICFdlDwqIdTZhY2mWM78yKRMisQqZe9pThtvolsSzMda0vFnF3dKjQMRsVVpr3dawg2ws3c0t50uRD2S4mzMirF41vxjJ1oCDLG3TvmE5VCFUYaoUsE6Rw8NhRVdl9AQm73PlowEjGQRGpMbYg6y4WTpu+3JeMmKLCEVVzs2oVHHvbQD0ApRBrdM07Xfb29ubl/e393fX2+001zpNVUREWDWfOr6QBFKykjOsdG4hEYAw/c6nF6D1ewbTlDZuYkABV4GiNCwsTGB1RjUzZbmwRnCNvAewiKWbQ7RmUnSt7lVZSZgDoi2jm0GqawRtWNqeAyI9C5HtISIiEJMHUvjSRusDEQHDAScRLgUiquSvhCI03JV5mHNOLYhEuLfull9QSDoM9eYQY/RUdGEREUakmxtFpOPxjEQsDOEptxemiCBP8F1kpCsAQvgwAwdJzoeymZ4JAXpvdjodapliZV9AggOUKYBwpMuCgAIRs8gCgOwgCMMZCYLzmBTJtEMi8oxrcQT3tfn0CyI5hWYRPmBYd8tcdQDEMSwgmKQWcech7oPCk3mM5qYiskqRIrL0QyVi3kzz1fX+/vb29cvbm5ur7XZWkZTMs4iKiiCvbjlGCgKM1B5mLU4B+U0GzLaQKJWZOTRhvshcE7/ce0PEPny3mUXZ3efCmX6GgL6qF4kjAENEcvoXWWq5E3MufdzjvCzL0mElzI/UquU9HXhxX3gAgrLaGFmg5DphO0+B4G6MnZggghG62e08Zb+LAELkPhwcEZhIEvzFFO6B7u5IuNtu+ujgyWJ2vLhFwizAdH0kHQkiXBDDBjMBQ0F2h+bLMMsszXyp5iRCATh6E6TdxKNsz6czxtjWMm3nMWDplo0FIhBEOndSZIog61zRzcalGoRAILc4W2eCUgQRmGAZPvpIZg8MIwrVmltUXs/EAmC5ul1a9z4cgoiFKcKIWUU7wbDBEe7OQSxFwm2VR3MGJetut7u+uXp5d/Pq5f1+t9EiJeWzTCIijNnbiQitcpGcqkMePemCgnBhLiqq4u4QwELCnLsj4rQ6gyIDgw88d6si81wQqZthRP7wwHCniGBCgHXatOKZwUcekGN4H4iJH0x9iQOiiCiloT4gl0qYAJiICPKRusggGMNO57adS3icz40JtOAINB9MjMTmncHz0uSct3DW7l0EmQTRx+ijGyCOHkLIRd3jNMxspDHfhxOsvUri9E/ttJ1nQClFltNCwhEj+zkPBA9gdwezPkau8mmdKFp4La2PUxs9lqJKjEKFhTHCbJgZC4c5YEZmIbgX4RBCBA8nYCQYw7JZSSB/IFda50SI6x6PKGONrI/VtJwdBRPNU4FaAwLDMSMTRgB4Eu/CAWGkoVUKAxMMAAAq07zb7W9vrl+8uL252W83GxFWYREpmQ7CzIyZt0o5BQNkkXS/8QqnhYgU/EMfNkbKDUGcsSAxi0jvLYCIpfVOGB5RlTe1iHIguYdweIR5EikBMBm6mHmdeXghUjhkCeLrXROAVJRVCDMoRmQ7q3u01ltfacuIKMzuJkjA2LuJ8PV+co+51IyqDAABdKPuFhGI7BGpVY4goJQEI6cREkYmbaWAxt37cPdBhO4USAnsjFVSEWbuEbXSZrN1d8YYvSODW88nCgHBApURsr6vuXgYrYOgkIaiCp4Xar2PYW1EVQZJOScxXKw9xATgEAxIypArLgBzCnfE30ktamY5jU6qPBKu4VcR7quBBYh/zzxLJx/6mqQFq1mLiXwMU2EFHwbOxdyKkhQmBJIi8zxfXe1fvLh7+eJuv9sgU9GqysykLCRESLJOT3O3CDnFzZBvXs3ZEBHDYv0lKe3ixATESkyE5G5IYuajjQhovUkpGCMjr5ioiCcdrndr5nnfXZzM4WZpZ7mMXpMCtl4xAWt3XRIGTthG2BhtpD2TMUJYADG6QyRbH81dRIk5iBgZY4xhTIQQ2zqVIozQRhCAhdeqsK6rVu/RGLbYMFtXT+GJhGAAQU5XdaQBbd2DIDiAOybOGMDT5hnhlE53kgALH4C06vqrQjgAOQAk9JNUCyFrPs85uIZVAAI5oANEjEFAuU5FwCD0boAowgBQikYErm8vZEg2QCgmn3+1mtuwNJisMz1AQDDzDDaxPogRiHw4Mk+lFGGzcV7GGMOWQSnWnzfTbr+9ubl5+fLu7u5qv93WWhw8HfHZ+KTYH9c+kgAhxQxEQBTJLQBIAU4oI7JmxB2sXRCuIBomd+/DDqdFiJRJkmUaMXyIi+W8vXsbI88wADSHiJH3Vdq+mYmYwcMiUnd2WW/6QLQlWmtFpQQs2Hx4QAgR0JrZERFEZG4Y0Ed/eD5d7fe7qSzdIAVGZkhYSrne75CCIKLHcBAhRDCH4UGYAXq+NOtttNGYWKXwamXN4JBAAoyElK/c1lJKHgkpr0diJTQfAVkjpUiaA4NYEMCBMNCckEgwMCtVlAA8LmdhYmY3I+W5aBBZ0gI8zShESGaWXxEASKxzhs0mxyouc3JYMzagj5FQPo8cm2FWH+uRFeb2+xBplTGPPgIBDLpnDbxS/YUIAGXa7G/ub16+uLm/v7262k9VWdSBiIUgh/frJ5qrxJwXMCESqkgpTMQYjszK7AgUgEwQwIR5XuQXVEuNo</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8Wa9mWZIltMxs7zN8w518jPAIj8qIqMzsLJKCaqqpAgHigUFIjYTEc/OXeEQ884gagRAvQNOFGjUtlaoqK4fKzKjKmH280zeec/beZsbDPp9X/wbk2yWX3yv/7j2DbbNlay3bwPv1fr1f79f79X69X+/X+/V+vV/v1/v1fr1f79f79X69X+/X+/V+vV//f1/02fOHQgwQsZMjZb3ZHEoxB5qmIWGYz/+V4A7Q/BUDTuSmBLgbETWBx6RmDoDgDiIAhEUX16tFYCJyB7kD7k71QximnHJhAhOKaspaigUOoVlMeZymqYl0ebbq+pYJmC+A3J0IBHL3ekn1K4CY3n0NAHBwYHKMU3p7e8hmDOq7+OThVTG7u7t7+OSxwNU9iIBFGAAxc9e3IqHthbr8k3/00b/3H/zxkN7+H//L//uX/9cNg0OU/Xa7vb394Y9+OKXyy998BTjg60V7db4AERz1RgHUCwfgcMLpNk5PCPW5OqF+yKFqd9vD/jARERG7a982VxcLJgLI3B3OIAc1Mbz7SQTkUszMHYCTwwA1A0D1F9Wn5k71aQHDkHbD5A4ALJEIWhQEIiJHMSUCkxChXuvZKsYg794C5tupt2YEKmr3u2EcMwBhXJ33Z6u+FA3/1X/6J13bwCFMRH4cpt99e327OZq5NIvQtaZKIDPF378/ZpYg7DAtClMzJdNFJ46wP6ZVF54/efTmbkdl+njNvFr3lxdNIGIikJoX1fpoHPTNy9vt/dE0ieVxyvdjcnSrsyftYrXb393fvgyCf+ennz17+kCEHaj3Zm4MBtzhBGYiEiJ3ZxIiIhAxM+oeaGIDxvX13b/82ffHMTHzo8vFTz/7KDl++ze/evLJ7wmbG5oYuWmETERCDA+uLpfL5eqykUX+h//402f4r4HvPv988b+Gr4WkaePm+u31i5f/5L/5J/tx+m//+38KV2L+wbPzP/zhByzBiWFW1Bw+36x7jQGqu+HvN62TkxEY7DA3nVL5+W++/7uvX4vEGENK6aMnZ//2T54zsRFM4W5B4rJrFouOiYYxK5XAvD9Ox2FwAOZwz2Y5KwvznBxAIK7RCrjbd683X35364DBm3ZFhHEciTgGcbeUMsv8ByCGf/b8ctVH5noHIDCRE5Gbq5u7H4f0yy9e3G0OZtY39JPPn/74B0/dEdoQl20AGEIwi8w//OSxFYuNfHN9vDuamcDcIG5GIK8BLhRYQgh5GmLs05T66I/O26ya1v35+vxP/9Gf/uxv/vrNm1eLpjQYvn2dHz24OD9bxiDmUHO4Ocjdc867Y4oh2jgdxwJZ9suLzeGwf/NS2GKIVpKInK06h9ScUXemO6iGKlNgEYGDQM51/xIRwExMCFHgNC7HppGskYhM6be/+Jmr0Ti8/cVfMLOwkCBwVDcQmhhfB+bQSBSD/7P/gYz/O7hOh1GTUX2PZmb+z//sXyRqYhAHC/Oia5fLXkSIxcy0mLnVlGXugBc1AjEzE9zBPKeZmkQIUMtNyF3bhsAxSJBA0ZaLbrFoiVjVzR2OGOOjy3UTA0DMx91R2yaqGWpONFO3aMYtcWACwdUhzM5MbuQwM2vjITbCxFMqIYg7YozCzMwgYpYQpKZ3crDgYtktF42ZA8QMgAEjZjczg3vJSUWCBGYjEgbQhziph7EUyeLkXGBupagRN4umaULTTnT0IGKkcDi4VgHA4FSKO1CKhhhCDF1LTx6cbbe762GTRvnLX/1528jz33t62B9/8+2Lr7/+tm3bTz/54MefP2tiYAaRuMPdP3p6eX2nbRsTpOtEnV++ebnf3DVds7vfnV+uV32n5moQgTu5mbmbgwARcmJyKJycwSAHmOYyARDBYKXQvIsx7+Rcsm/2JR0FAnJyMLNDudYMYGCCOaj+BDh8LscGg7rXR2EO+ov/+8/0/DnFtkKBU4iTnYphLZFzlTcEYTpVmxqvTIQ5UXt9wjUHEoSYmElERAhAMTd3NzicStkOw5p7U90NKeWSSyFAmN0dxGQMtnk3EuDMREQMh8JMXQ1q5GZKAJnOhcsYMCKBE4OIQc4EImICiJhq1NXn65ihC9X8XErOJaNuHMeYCswCc5iK9mAhkDuBYojF3QhqJiQc3IuCYOp0umQHXF1E5tzvDPZhHK9v7t3twdVFv7oKi0VnYwEuL8+6rjlfL1+/eH3Y7caUJYgDp0xOl+frTz6yr77fbPfjbtgfNjfLJvyX//l/sh/3v/7tFy9fXj+8ugSgpdSn5+7u9fWRmTNX5EBmzlTBHxHPEIiIGW4AuwFgrvWLXGtyIYeDjIjcbQ4LdxBcATIzgMiNiGn+ANjABLipGqGmBhhqZBHc3WHmzMwVjdW66RWbgSpwIuL6KwE3JwJRvW53dZ9fK8HNXVxERLji2hkoOZljf5xKUQflnCsmq4jQawiQVRRXM6exkNeq7QRnIoebGxOZGYHd1MDu5mB2pxqWRLU6AM5y2hIzupv/BSfAiEjNi1XYTQDMPSUtZn0noQliZuQgOAjCJPUtOYkQw5NpfbUA1VpX30VsgqnDLJWsKXUtSWz6vmm7TgKrT5th2mwOD88WF2d9fPbk4nyVx0REZk4Es9pGGBOeP1l0sfzit9evXt3E2H307PFHHz371a//qgl8vmpcSynmZkbG4Aqsa0TBXc2EGWZGgBIzgYlAYGdiOEhkzi1EBAaBYO5sqvVeyAnkFbib12ImcHenU8QazAF2vOtk3GrYmIEF9RfV6uR1z1fAzcSGcmoA5j7KDWDzGnWnzFYjisCAwtQACJO7a9EQBA41jRxNnJxtxgg0TYrTi/M5EVrtFeh0/URsMAbATO5EJMReYwdm5iAwHA5zqxkY5IAxagDx3NIYsdTE5fNfXO/BzagitFLyaVcRCKVYcWP2IPVhScXoFdqBnJwgBHNXMzc3VwabG4iYxOEll3qpaRyZoUWOQw4SyHOGDuPklsuYvtvtx7swcJPM3DC9vGWpe9qzksPgyGpDsbZfP/u4Cdw8fPSwXSxfff8i58yCaRwOx2EYU2i8qJrRnBmIAKh5LkWLp1KIIIQPnjxYLVomNyZhqCqBQWL+bvuiZm83dwa8ZikjkrlsmROsNrMFwLxDDXADz5WbHLUw0gzt3wF8poq5QGS1DLuRwb1uFia4K1hkjspaKYmpmMKtqO6Po6p1bWsAAU0I7rCs1DeBGI65vrtrzV1Ec5TAHWxuNViYTv3GqeGsYVHxuzujoj0DkRPMDU7uZhTi3Ag7RKh2MBASIhY6lROvdRSAm8FVtbCTsEhguBC7k+dcQF34cRePZw0DE9GYPU/1+dVdyczMRErmCiOv9dsYcIzjJCIA3C2Ermi+2R2GrCEGUC3zFELgEG5USQ2BOQgJM1PN5KTqilyUvHTkofOWZJ/5xasX/+zP/vn17a0A6yYwhzSVF2/uQohTzhW01ko3jrnvF0BaLxfb/fGzTz6A+/5wXPZRQewGhbuJyFyjQKaKUysx9xOoiAbkAMig9fkaGdUgdK/FwZwEZu+aEDcQAyRMOgM5YlDFNAQyB8OV2EmhbrXwek2YFYHNcHCORlc3Pxym/WG8XLTrjx64wWEi0oSw3U8SQte24EpNEM95kJwAAxPDHOxk5OQ1dYOI3ODMDKuQo2JVd0NRdybY3IsSYO6etXAQDsFNAXNjEoIRE4hnhoNQcRvX3WVMXpBzZpKnD1amvbqbWQhIxc08XN6UaQxDG64u4vpxuD/a97fT640aUSp90zUSl6bmZJqLllxKqk/ISjEwgbquW59f9FEerqltWCQYkxAHZhaqaAdAMYAZgMCCsBZTzSnlw348HA9pyqbZlKeUw/b1d29eZfCDi/N1H4yYgFdv78+Wi6uL5e32OI7542cPc8rXt5vV2XnDNKUpl7TdH4kQApt7RafFfe5A3VXdak0xg5OBKgoFqZ9qnhPBxWq+nHkHI7CBqFYqUN3+tYyQOQnXcgzMSWWGLLXqYGYR/R1PdnpZfGqLaa6mTqCcy/X9QRM4SpRg8w/y4rQ5mvPw7HFTy3TNKcyCufK5OoKQwiE+83WA1zrKRAATnMy8skEOUIjx0eOnqmVzf+9MxGTZRSjGBm50yoowuBshEJGc+LN67WaY+2m346ipWNtGIDjg5lpScVK1cP6Z/ubr8he3efFm/Dc/kB//uLlo+1U+/sXrKRlEOMbokQCgdbdaWDQXK2lSK2UaWcLheIhnl6uLByg7ApiF4FIJPqa6aZiRDeZQB1PFZjDVUnKeUhqncZh2qT9s75tUgki/vqQmJBYHHZJOaTqOJWkZj+P2OGhJJaVhyNvdYXP7VlUvLs4Px+nifPXgYmFmVLE8nFncHW5qVuu1u5kRmZM7wWr77M5OMycHdzDc6vuXutFxoqNP1DCTK05ZCKeqZGZFS5TogJkXczU1c53pU/rXWBcwyBxUIaUwqRXV3SEpIs+c7YyO3M0A3+dHV9o1omxcezy3Sm7N7Yd5DBVsuwOqRuQ8d5w1YAiOumcohJ/8wU+XZ2fffPPqr37+cwKrZUQIS4wxjeOcZt3c50uuLLbDBeRzA+qo6dtpe5z2g6mZmpG7uUX2VIo7wvQHw6u3xEc5mvw/X463d8N/9Cfp+Uer3WH62c10OOYQmkXfEktlZdWchUBEEplESY2jafn+5atx2l2u+st1v+zBQizvekoygAmBK1CdWxiRmaEJIZSoNupxmjwPuQKvPB40OiIRpZwJnMv49tUxlzKoH46ZhUJohykfC2Joh0L7sfS9TtmaSDHOHWKtchUAnEg1xvz4mBxgMBww5ndsCJ2Ae20BnUkAc6/iiM+R5vO/5B3RT05EwsJMZnNOeff9E4KbyyoDTqisMp+i18xSVgrB3N28wsKZ6QUdcxmm1LWRKuNfk/L8cdQ+BzMLa5XdqN3s/CRovm4n52bFoX97t3t7t/v1b/8ul9LGLjRBijhZmkbzUoG4mTPB3FLx715vnz5crLqOeI7y+WEBBsu5FIMWLarzByPGMbtp+D//RTlboZi/vXUK9LM3U/7fy5/+kX72eX+Xy9/e5ClNqqVtmxgbCUHTlCaNIYYguVhW3e7U2XXSL7/6/nemDy6Wf/RvfLZetbWvrE9Z9d2WMABWc7IDTCwhBKEsiRrLmyjQAtOcjvv27GFoFn3bwPVue3COi8XycrXo+06Y1L2kPI7pgw8/iCHkUt7c7V9eb8+W3QcPzj58en6x6kTkX2/AZ2zsREQFTgZhAAFzL8i1pjkAGDkbef2+z98km5G7k/MM5tzfcewED0GEpcJtJjgRMc99ZjjhpVODykTEqCwVDHBPuczXOjNxsLnyubmb2eE4Xp4tZnVBK8UVAKvBZOTs77rImRiZxQiCWaUsrZh/8+V31/fDq7e3aiosMUiI4oWKF1W4JiIyV555ZLjbOPkXX79ZLT9cL/oK52YKqO6JinfNQADVb7g7Ui5qFv7lvxr+5I8WP/n9+Oc/S8PUTIw/vz2s/rx88of88WP67RuFI5mmlBd9jrFhYtXJ3WOMDDpbrYZxnMYJzF23WC0WP/rsw7P1QsukrnwCHsWt6qGwU+sNNbWUSkpTUSPvmq7tw62EPmtRVZA0QkXdSczsk48/PFsvhWuLAlUrJe2GqZSpa7BoYlj2V+fLlPVue/ji27ffvd1+9tHlJ88eLtpY+dtTdoEEIbNT7QLAFWtVssJPBJX6O2jlM9nm6pV+qhC1MvynVdnY2hsQERuBCTA1DyClkzx7kmUr5U7kNTUU81LKcUhd01CMtd/AKQu6uxC5iylKLiEGInY3YWaeWWumGSrNzUsVpt2YuRZ+ITLAmSLLB48urzeTME/TpChMsRQrJasq1eSHWStzq3gUpuWjx2cPL1ZzI1VlAa/Aw8ktMLdRshY4qzuxE3tRK6WE3X7z879pX76129vcrh70XW/m/2o7NX+3vfzROqJspuIOLSVNITaBnJarVcpJS65g4/b2+u2bN8vl2XLRxsjHjMn78/Pz/fZuv9sI2UycE516PJiqwd1M1bRyoeF82N9drRbM7O5F1aX1dj2V7G7L5eL8rE/jfjeM7t41EoiEfdHw5u5Y2I82giQ2MbaLpw/Wh1V3c7v76y9e3t7vf/rjj8/XPRFVkpZZmDgEiqtLz3mujcwEFRY3A7OExrWYFa5BZX5SBtTmRsC8FgafaXaDcc2FjlKsbUVrH0jCbAYPFZubg0/sP4jgTExMBCX2wzBNk/ZtJMAZgBC5G1mlLMjhNCW/3w0PLlYUnH1OowIvVkNojuCqEaIGPQPm5HAmuLTNclDumrA+O7x6ew2YmTM1ROzuVRUQIhYxVdQYdTXTUsoXX79U96cPzy7XfdcGmrtUL1pStmXXSfCi7B5pburNzMeUwzAcv3/14tuX0zTg8x8uiCjGOKn+7u30xx/Fpw+6++92cDQxTGky12lKLJxzHsZhu9ksV2tXm9J0fhZi0x72+7/++c9/IeHh1YMPnz4KOi3aWjzATD7LGlxfEJxEggNqQYt6OfZ9xyASSsV3RWDlfN1vt4edluGwKTkv2mbVN5E5RnFVdwWoi+jbpu/72AQj2R0OLYfnHz7a7o9fvnidcv7jP/z0bNkVq00Sg4hDjFdPq4JjQAxSyV53c+IQI9xNc0U+AIQZRBWgsYi7mrqqqZsZipsVRyAm2u7Hm/v944fnM8Izn60lzLUbnRPe3IVXktjMNaXy9na/OWTj4KpVx630s5sT00mR9+M0nq36RqpmQLPkYF4rMt7JQG5q6oAVrz/qdnN4s8nF72/vdjd3N9NwZGYAIcSaHWs3bFo4hJoTpMZZKZVGHcf067/97ouv+dHF+vkHV8+eXDVBtNg0pt0+F5CZqbmq1zx96mtFXMtxv9/uDlMamrYPEtomhhhuj9PZlNcftl++OE4pmfn19dtxTItFdzjst9ttiAEgU1ut1w6PoV0ul8I8DPuS8m6/3e6OgXG27gIzVYMHsUho2hCbpmmaGIPE0ITQLy/f7I5lHCdHcs5G+0nV/ZPnHy77uN9vUqJpmnb7w/3mEAKfrZrVomfmYVJiXndtu+jaGPtFt+ra8/UiCIk0/aLruv67Vzdw/+DR1e397tXtAIIQOWAGA0Bg4qZtwXQY82Ree8OsOiRVoBimYkltUhuLFjOnMGZT9+IwwBxZtag5oFpyKV3Dj65WMzFCNUbBcxE+MeFEVC0lbqpaSpmm/N2r+/vdkIpNOY8pT6lMKU+5TEVzKVPSpEWLudvlWdvE+PeWD6tsvqNqn05mZuozpjPkknMuX36/eXm9Owzp5vpNKequVTIB0IQgsSFiN0spxSBmJcTIzE5ecq71OOVMIHfd7saXb7eLPqwXraruD/nF282Q/ZjKZnfYjeNxmPZjSiV3QdaLNmR3RmGIqr169app2pTTarnyIH6fNrw5brdDziLNm7dv+sVi0ffMyLmYuZo3TcwprVer29vNer3s2n4cdyUpg6Y8wvq+a4WIhYVI1SVIjGIGg8Os9murq8+8efvr492QSd0OY3LQ73/2MVBevXr76vWNenj6+MkwHjfb/bqP9z2Tk5sdjrkUjDKJ0JCzuWuMy2V7db5KWV/fj6tF/MHzZ4r46NHzb168JXhkYaFaXwgUhMAcRFLJIJCZhFDTBpOrlmXfHYeUVcnJzFW8lDylHEIkwjgci6qVks0Dc9NEQsiqJVuIte97p26aGRm05jMHuRu551JKKeOQDsMURfoumos6Va05CFfpnInVVBVETl429/s0aRNZnVSVgCBSGWcC1edaGxNmMvUKxu9u78fMi0VbVOHmM81YWV6znLMTwU4guOZKWDGHupOWYq7MQhBAze1wmDbboxvU/GzR7cY8TlPR4u5OTDA1MdPDMAV2dVhxuNs0bO7ubs7Pz0vRtol/ezycH4ICl+dXKd1pmVwXaZoWy75f9IfDkZlyLmkamQWwlHPftzF28NHM+6a7uroYj5kJIswiBJTiaSq1BySGqcd2Hdvl5vqvApMwpewpl09/8FzI3r69ud8cSsGYD4fj4cGDJ9OY1Wxzd5j2Q4xhNwGhkTz6NIlQSToEpGnZtk3btZe93O7L2dliSmj684+ffbLZTrVHiyEIUS2FqgpHVqxaSTkLs7kxkxDHKEKUF2Gc8jBNIBYWkF2tF2AKjFy6YcyrZRclOBCjdDE0Qb5/dV+zWAj1XcO92meq4WJ2PWqxXLI7VD2prvq+bRomzhUHmoUgPrMvpCqoGhYiGR2PuQRmgqo5kJCrDyqrydw0u5nXvnBSU7Wrs9Xdi9ttqYpIbWcMzgZ1dY8gL8vVeZgOVrI5Vd7OXVFZV3dCoJPo17ftlPHtmxlWBZEYfNlqIwK4zB2KESOrBSZjSIYzwQzb+9uu7a8uLrbXb6+YLpqr4CNx+ey5/e6rKByncVosF0xkrpHau9ubi4tzd5xfXJacxinFdsEs03jsF/1idWnluD8MJBTIiBkoxMQzleul6KP12eub6/u7Tdt0Rnq/2z95/HDVx83m/rsXb0uxy6uzCkCI+fPPf6ClNEFKycLCNhlRd/aQHM6ShMiRRqNhVN2VnJN67Bck8ovf/O2/9Qe//9W3395sjuRwNRbRUqqPiljatmkdSxALwSsBXrs56oiblNeoxgcmcjNTsynlJnjbdcXgwsTsxAmcJ/vm9ZtStImhaUIQ7kIIQeBeTFPWMRUhhpCpl1JiZHcMUzGrUqyPUwIREYsIw4uamp74dwM8sBBxEMQQKpVgamCOLEkTSErORMjVf+BOREzc94vLq8vN7jA7PqpbBSYhOnE11DGDWVIZmUndyHwmLczVnMn9pGoUtbvd6DBAABeiVIpqIRJixNAwFRHqmzglDUSzbEBEBh/TOKVEbv/Fo4sHC909p4d/iRd3m787bHK21UogbOpq2oQmxLBc9rFt3XQ4HqZpyGlcdLGqEDc3179UffDgQktxAKZOJETMHGK4WK3SdBySP+uXv/vi1/thirEtRc+Wyw8fXbpOu+3hbLVUcNe1XdssFsuc83q1Tnly96waRc5CnLK6tFmNJYyqjUQ3y0XJAzEfhyHocHa2fH19rfghh17tUC08lrMDQYIp4BqKV4o+tG0TIsElMKAOMqBpYynZrJiZw3MxAphDYErF1L1kIzJ3q7Iyc2yaWNTK6IRy4FJDIRXj6gAxMDsTi0iZ1A1gIgQWEqJm2TRR3GmYRi1ZyJvAYDYzEAmHMSU4XJmc1NRUiyozT1Wq9ZzNhIiI3VHUmDhZmfJ+fzioalXcyeFQgFwVQc2cgLu7t01smqYh5jSNgGnV/x1we9cqOzylsbRNLWXq7kAupRFu24aJzDHlrEYS2hgkENi9CMO1Eg8WRB4Kf37W/U/ffPkf/rvDf/Z4+T/+zx72TS19wkRMXWj3xwNzs1gsU0rrRZdzLimlEJtIBKsChXH8+PlnZ6tFzsXURBgkICpFmdxMmTjl8slHP/j0+acSGxGeOUymT38kFAQkBLDI+dnKfAYfxYxFalNtqhVr5ZyzZjcXZge0FBEOIXRt27Stm+1L++//x/84NEE4aClZcxtbEoZ7SpOpOsDMTEzMaipMxNz3ixiiu6v7cDjknNScADWPMQAwsyARjMDsILdciahxTEUTgYsWL1lC44QYo5sXLaZq5lnVSilacipqxU2FpXKzMCOiGkBVWJ3SmKdMzEzm5q6llDLjfJxyzqytuuakTmDGbBYn7rqnjx788ld/89XXX1fvCLy6TpzdCNV5lGEFMRCLu5lpVd9U1YkAs+rFc3NXYvr42YdNbEqxYRzVVM1QihPM8GBFzx8/7CIveimlBGIOJmrupEECgBjbDBoz9ND90//N/+FPHSLt4nIV9nCGs6mHIG44HoerB5ebFy8YpkWzUqem6gwTImN//Pjp1aMnXd+TBAbMLMZILDMDCBKugrUzMYsIk5mFENqmdzKRUBMtMccQqn3EzUIIRS3lKRAN09i2XQziILhNKeWcKwjru65pYggSQtRSmrY9W68lhK5tYoyllMpnpzQRWITqEIcQH6dxt90yi6r2i44lEDPcl6tFSmUch65rRYJqSSmJRAClZJ0Ti4Q2kEgBPIGYy+QgQeBqVhunw+F4TFOuFLYDRYupwb3q8sxC7MUV5s7ctguJokWVA7fu7kWLG6ZpkpYF5KZC/M69m4synEHBjZlZBAYWCsKj5n6xMmIgOApICQFwJzYHqZtXMo5DaI/7XVHj6mEjIrBXB57Nbm0iGQoOw0HdTgYYcuKcMwhMYRj2h4Nutn4cUzhbn4XQVL2vpOTgq6uzkfjFfny++Mhx+OrldHG1GN4MT9twJ1ECHYcDcT+lUXNZLHozJ4h6WvVN34fA1d8nBNrsNj//1S+ZmIVFQuWrKsMBJlNlrl5RCVEIbG5mGjhIFICCiAMlZw5BmIWlaDFTd885dwF3m/2YMkAiolrckUtO01RyVnchBlNs2hgCHAYNHGITCBybUHXxyqKDKISgRVVzKVa0wFzdTbVeu1e348yDuoQoTEUV7sSCOmNE5KrMbO4551KyqhdVIQpR4NUrrUVzNW9YTZ+gKU3mFkMUCRKEiLzOT7ixCBG0qLtLYDdYNRsZmWrsGgaXkqvTmEFW6Q1yVyOasSaztG3jpvfbreZSR1Fc2RxEHoTrPkc1MpGblpwm4krUgMWYmFiQC5FUW0udmnn9+lWZxrk1nf3kpqYADzt+EZzdmU3Vw2p1HprIRA7bb+6zWs6Jm8gNvV5unj/ovk3XF+fNb357dxinvs05l/1ub7bWNIbAdzevTW0c94FDu+yIzMyI3LSA6Luvfvf9txxjB1jTtnUaLqVUJY36GEJonJyJgwgRKsR2MzMlljmfEUMkEHIpplrVwyCSc5ntZWBhyjlV3tVNiepwVB2XgHmds3GcxEUhNoKQCFMuWU3hFAKLBIAq/119EnOzNcukZkb13cy608mKTMQOAwmdoPLJ3Ef9oMQAACAASURBVFp3ujlB8I7APOmo1VAEZw5SKXgCnwaUhNjc6sjau6iZPSfutCUiqY8agKm+81fMJpQZ6TMxG9xURSIxsYiqgQxghwUKImyEkxXNVTOqBEHqxg4jhHr7EgTg6qVKw2hkZFw0VzbOffadbLO5Q93FCqyE/XEnIxsqHU4htLkUzemrVF4UPabRS7PZDCln7vtxGGv5GsZj7R9ijKvl2qAlK3Gw4k4Q1Bug2DYpFyZiaUw151x7eldFdTURJCViqdbhOvZjVqpXmsDCAaheLWSQcFAtqurm4zs7FyszV8RX9Zw6tAiAmc2qnmiluhjMYRRjdLgVc1IEqfGk5qU4SxYJ1T3Y9N16dR5DHKfjYbdVNy+m7BUOBw7MVMtldR+Zwl2Jub5rApnBXGdsAAcZQZQcKNWbxsI0T2OaKSmMKrkKkPtUkZODCCHE6neqJYpBJOyu1czmbqalSv4V380OJBZ3ZwcRgx1wISleqgRW53bqoMAc725Nuyw5swirVqyo6k4Gd5HAxObuMLeSixK8ggp3Mi/qNCeKurmpmiUoVLe8I6tDSJq2UbP7lN/kIiLff3m87Bc3mZgUcBM0TcgpmxaqRTpQ1zdwP9gRZphdt27ulYgy1VLGKN1s5HQGPJUMPdn4YVqMGfOMD2btpMIVsImIWdHiDlfkWu+Kag2k2Ys4vwCqdL+ctGWCuRJkNi7bbNJ3VXU41I3ds7cxOinY2clhrrnix+kw5eFYxSMiEAVmmBrDHRBGbLpSUjC2irAY1epWQ5uIhevEIkAQAsiqW+Qk1hPVwQ9iEIpqdWES1YSFd5Ms7KyaT9NC9U+lmgHQ3PBRFfnrYEAtHizETtX9pu7uHEDFzSp9CbiaMgUAMAOZgErOOafZykmsZgTnal2r41lGVSut0ypcBVR3Ry27J0HWYWYiEAnBVImlupbUzczZCSxBvKgOOa1LE2JoRIysqOZMWROBGeAY3Z3qL6vovspt7mrGAsslBJjZNA6VPIlNJIdI1JKIKgHpwqi+GJBzlRgJwgRyhsFM4BzIrdYhJweH2XpChGp2mN36RhknYmg2r0NcHIwKKmBM0rbBci5112nWOmqsMBhV8hsn178mB3O1LaO4zXNf7DD1PB2YQgghZbWiJ3c4YC4S+n6Z0pS10gFVLgzCbLV9JSJ3Qs1o71KPuLi5wuw0IOMwclJXOLgSr+RU5fXKd1eX0DwZUltJAuAxSk2XlYs2M9UR3tAsA/icjMgZZOTsRMw5TQ6H82zzIYD5hGPpHZJRKzA1J7cqn9ZfDBC1beulADBFFBahYAZxA7maB5ac0mZz14wd3FbrM4nx5fGacnD1Nkb2aT+ORCzBgUDu5GymzLF2gtXfxEwMro6vNE6VEGGSlHPwJrbtMB7MjIlJZL0+axuBajG/ubuDo+8WT54+2W4PqsXMi5XD/hiFV+tV18bAJhwMNI7D25tNDM35us/gKEwipjaM4/FwjEFW6zURUsq55MjS9/H2fhMkLJfLGMChqx7rw353OOwXXXt2tqpeihhDmvTtzbU79V3bL/pq+WEJw3E4HI4gapq47BelJLMyHoeiJRUFECU0bRuYwShpLGnI2YSpbSIxu+mUkpPXPU1MIYSqN6tV8jO7Wtt3FCWlIiwiXEpOU6WUXaRaexkEK5kAqw5weLfoCJxTynkgZiIpnpWzEBVVLe5WFusLFknTJER1cpTrZiQIVX8ccrEYWSSOY6lAmsgYgSgBp9FFoA2txar0ExGKaj4eRfjJ02errtPpwF6QNbnthiE8ujxv29jEsD+O+8OxlJQmIrcY2N1gmQDzxFDUEwVImQFnYlUjYjZTc9acAWPhmq6JnBkcopYx58yhe/T4wfGwG8e8Wi02u72D1uuzrl+0fdeIiCDn6W6ziU0IQS4vzoS9ZC1mwzDsduY1bZQC9sW6bWLTRLq+23PgVqgTTs7mXns9iVGEixozg6VtZdn1RLmN0Ry7w/FSVuvzRXVop+ForbPQqmvBILiIRKb7GJm5a8PVuq92XBZOi/abNLHE9aL78MmVMIcY3fx+u/vqxWshqLPE6AAD0hCb9kLFMkIAQMSxC0ycp2HVLaZpMiIJMYTAoHGcInnsgxpCE5u2j1HMaTjuK6qIbSfCTFLcNKfs1jYxZw1tT4S2iQ6IMLE3El2k7bpq+e3c8zQdDru2bacpMVCnqhkMdjrNL5m7q3LVIMrsGSYihzCz14LCDLgwSwxd21ZFDa6lmJlGkcDQ6cCWyJwDN6De2/Dg4VXbRGLql4tcsquCyEpOxuF4EAnJ/15TJWYHAwF1jhHV8InavLiTWR1XQ4yhbTtVDbFZrnsAaui6rqhfX98Q0LTNlKds5fb+VtWuzharRdO3oXoE3rx+bW7bw+F4GAm0XK0CYbO73+9Hgvdt0y/6Rd+0MbCEZNaxPDhbGSwVI9AwTYG47ztiUTVz67pWKIztqE5PHj38B59+dL5aAADRL379t7/77vVHTx//4T/4fLbAO3aHw/Xdpqj94ONnP/r0IwBEEptms92+urlPWZ88evCTH34mwlWbur7bvLm5g2u7WPerJRMXVVPbMw1DYpeLiwthnk8YUd3eq7CE2PTLdR1zA9C27XjYObzvF92yJz/NnmrZF4WVtu04sIB6gvfNYX8UYWbq+sAUKrTIrh5ijA2F2DWhWp8CyxE+DEFiw2lyYXKneu6Ge53gd1RaySRKKUZEmKdZiZxOBwHMs4ggI4QQo5VirjAwc5AAQvR0uWqHfU5mTCCWtkEIMVTSo7JQM5YmhWM4bEFcDxwQkRDFvZ41UpikWuyqr5eIhJuUc5R55Kppur7vD8dDlZrMsdnu+q4dp0xwYQ5N0zBfXJ6b+f39pmmblLUavIrp7nAkCotuseiWDozDxIJytLZtQgjMfHO/naY2xpY59H3LhOM0dE2IIXAQDC4Nd10fY2iiTCmtuzhOKcbARmfrddt3o9JxzLFbqLQEJKOjxalkNyPC8ViP/8BmtBd3qU7PNI3udyPARHazG798s+XZ3iP3mw0RhRCbtgksBmeW2o+X7Bnm5hxmTO3mIYQYm9i2oY1mdZ7XXLmN8TgmkLsCbGbscAkSQnBjCcGBVcM/+ODsbNH/6suX15vDj37v6dOr86xWSY/bzfGLlzdd0z97uLhcttXoS0Svb7a/2B2aEBKx1jnceShGZkuJQs0BaCl1XpqI6iR1pfPUYIbAIGaHswhmty1LIHKqW7QJXHJRdarhIRJdwzTlro1qtQWhOgk7k5Igt2zukVqwwZwZJAQnAldyvrprzD3GUDSBwBxAPo1DylOUyJWyVUuqBJyfrw+HAVzHo3G/2aWcNrv929v7INx3kZlAHEIYxjElSJAqNwk3bdexBGafppymdAStQ8Ow19eb1bI/W8bjOMUmhBBABiIzBWIqKhIWfTdMqZ5FcL3ZH75wwNWMme9vb0Lgtzd3f/nL37KIFnN3s1JUiej2bpOLnehuKjm7mjDvD8fvXrxxdyYi5jQdCYhSAXblx6zyyWbFHWZ2IqV5SonhpkkLdYueQnXUc/ZStAgjhtg2oU4lppSr91rNAnMxu7nfjsP+8nx1GJOIXKz6i3Wv5nAIY5wmLZpoWvVnjy4WbvMgy/44VH5OZznb3cAsJ66vqu3Aye9LRCdDE8ydjKpMBYKTEUmdoJEQQsWX2ZjZ1QCklL16XiIHZqvOkjrQV3KGaTX5zm053J1ByuwEzloYmE2S1VZV5yrmbUGVu6pe+Tq6oGosRECdfdodxquLs/WaSrauX+XpuDsO0zi1MXqYHaEhhrbpxmlKKce2m1LWUvqui0FKrAQSl6wi8Wy1urp6EKK8fXuTzYzi+Tos+8WYSxqHINLE4PDA1AiHEFhE1UMQckolEUjdxS3GGBjBee7b4cSIHD548oQlmGMqPjOxBhZZrpfEUgehKmpxK0wM4uK0CPOBMSEGYurbtpTShbbrGsDV6vRsPS/D3h37UkcwRRBiJLbKcTQsgAdBWCzWq/NcsgFlGuA2DHoc75bL1dn5+Vev71/ebM1M3CXwfpjMSk764vXN/d0ua8nqInK3H4golwzX6sCt47TvDo1zpvnAj5nf5voOQVQ7cIIbGSG4O7EzoQkh5UREwszA1dXH7sbTvTpYKIYQg8CNLYc0JTipa4ghSKijsPBCJHOz7VJHc9iZnIlL1bqZZiKjUs9jTqZWUxyzVOqRqPYEFTmGKU+3m82q79q2a9rOLBHAxOol5+JOP/jk+ePHT91GTUP5+uVxKiKyXPRPHn949eDiu2++3B3HGuaLRRfb9uLyMsSw2WwcnNTv9tnseHG2/vTTH7nl47CdsuVSLhbLYqSK5x8/LyVtjykwF/MgAmC1XF5cPdht7odsZs7C7kYAsYSmG8dBiN+Nr5EjLldN06c0lDopAjhIQvzw409Wi8X99lYNHOajcS4u1k+ePtMyDdNUaQJzE8Z6dRZiVNMKfoNQUQ0Snjx+mooO42BupmxeinoUhBiLqplWIzTgTEIiAO92xyKzbEFMsVt+9PEjBg2b6+9vrpmRFRbblCaWhplNq9fWGwnMXI9+qFKzGoUmai6AEQdoBrG7s8hpDpAdLoCWeuKCNyGAiJnvj7txfAOUR4tWmJhCdUyXlB2QTz/50N0Dcd91h+Mx5aHyQ6A6zlidXVS7XxJKRTGTWxyEmxiapnH3UhSG01kJXPXXegBJ2wThyAypJ/yIuJX97nA4Dvf3m5xLUTUtpjaOx+PxGEQeXF5o0SmntmnUbLvZbHf7Mh9W6Dmnpm2mnPM0bLe7+92+aSKzMEvKJZX8+vXrw+GwWC4DY9GERd9vDsPrt2/TNB2PRwqRWZxIRJgwTsPrF9+rQyTWIfLq47+7vbm9vZHQxiZKVbeJiLDfbe7v7khiCAEnB7bDb2/ebrZ3IiEEYSK4mtnhOLx+/Wp3ODDLPEisRdXMSr1tkSCnAcuiurm92e336/WqicJM9TiqnPLm/uYwHNumNXfPU9vEemJRSkcrSjg5dxxF9f5wHA6HMo2upTgMHNs406gsOU3VyMnMBGYmdw8iVDlWgroBFIIYvB5TUVnR/4+pN1mS5FjS9XQ0c48pxxpQwAFwBml2X3JBoXDFBYULrrjjG/AV+AJ8P3JBEQopfbsvm91nAg5QqCErIyPC3c1UlQv1QF8BdkBlZmW4m+nw/99/niZA5NzZBJQ6liJX+YAtrbn18P6wH4RJhJm5Ks3T2cwlR4taillHonTtX/XsCBjpHhfmnMKt84xVQANVpWpZzFtrQY4kiOkF4xxXImH3qIpFFN2V6fXj/fH80q1X9XwQkSEMkYRZhKhZGPBXbx9b75+OZ0Jy7GamQqp6mS61VhUVD9GKxEVpXlquTYR57mAWSL4RdCxV+Tz3T5+/RKAqt7bqZ3J0nwMkVc1rP1U1BEiCzExmzCxZkuaeNO1ZBLTK+3O5ie5hvYED4J4QzczM3I2ZVMs4DtlFhfcqAgjz4oWQRLq7OSTj6mpbsXlpQ01XKQkHCM9MFDkuDRGpw8gEzaL1BgiLA0UgBK6rU2JBYTAsgtTdEDoCiKa6l1IVAmmHyr3KilLCbrZuIFjQzHNKFbnncEQC5AgPSGtkWDeHMAu3CACOICIhJFo3sd4NASgCi2oAni5TN4ukLGSRlWCTX9/Z691BDISQOwDz8AhhYmZEyTc+7a/rhQpUtQCAh/eIWutmO0zTQgTEMhQdx6pauKgIqygiXC6XT0/HYTN++81Xh90ITISUxLQ6DEMdDvs9MQ1Vc/gopOFGAOfz1K33pTtEhM/zotCF+eV8nueZMUFiEhFCaabLvU2uuZxoHd4wJc0JmPINgCx6CTF9zcyoQkzr2lGEhYmIGIkBzNzc++pNwXATpu0wbGqppZjnVt1tdUCCmbk7MakwU2qlYmneWj9P07w084BAXrlY0T3Ol0t3tAhEJrBKIQQIYWatp/cPu1MgkUgAsxREBFj/2tePKS1TBJTbLyckJiFCYo5kuCEjMYsEICIDZkmOiMJ8xYcmmIhzZweASMIIFIFt6YhsAVKKpKWiltKsP+NzBKWVPyUOSOvDRsgQgWRoKREnREYEcxNWIsJfPT3I135g9cECIQBvhvLN21fb/e4//If/6h//8T8iEquqCBN2dzcXIUBsvf38y4dx0LvD9vffvvvpw+cPH5+BcKiVhIqWWsvaG/eGQKUWbChC58uFGKMbMZnRp8+f33f//tuv394f2jJ/eT6l61W0liLNsnhHJrwKlijLYMRfbZ2diVSEchYQQcRF2JoSoQrD9XcDQUxp1A0GJwAkpIDejdCXZWHGZmHdkJAcPFCZWfQ8zwBYi7h58xX/J0LC0nqvBavoZbrE9dRByJFSHJ+ftvtDUASTqpgFEgji7CnP8bzoi5ZmfplaN69yJTMSreqEdUmMkSopIgJwDybubkwEAQlUJIv8r4iE+UQyMXFHq1WtNXdxahiMyJ6StBQmAHqAqEhAMLEq3tD2F/ola/PAoBX8hkQkotYNCIXInbO/TL08ExOBmVuAEiOih0suQ1ZGMTFTR4gOP3/4pF+Om90OAYsq7TYeWIsw4GLd1smezn354acPS++PN/tv3jws8/wyOSK42XY7BsQw1HCbewewoVYmrKXsdtHmXop6ABMB69KmP/3t/Xfv3h52m/NlXqEQESKcv2wDJ2ImEpWqHP8+2AEVceuUzxmhkoYZIpyOAQBEqCqwQg8gZNXtVGZfHwcF9zAjpPSDMEIQ1lKE6Xy+pPvS3YdScgqZJ0UAQcC8LEQgXOberDshrf0/YhHuy1xrqVXd/NLa8dxyAxEQqEUYiLnPC7hj+pMiSFa6W35mmFflyhRBQl4ntTkzQFYCC0MUJgIkROcsMREAGMPNXEYiKeAYTG4RgeGNtHhrFh0Tlotg5uLmw1Cb9dZMmWh1hgYhITqEY1AaaRwxIJgBLJhIRJgpgZocKCJmPaU4eapRHsrISCBCFBiEl/Plh7/9goiHwwEhyjDk92MicmlLE2YuFSaIsE+fv7j7/WEvUiAu1q1UUeHzPBfhbpBQpjoWYSTmx/HASMNQf/zlozu9vJxP82Vp9Z/+7c9V5XDY5qqbEIk44b0MfBX5YK0Fr593hK/3ICELc5YCnNolUBZlqkXcQ5g8UpSLCNHDObLAQ2DqrTNTuBEhEzIDgC89Rc5dQO92o7kxSbC1JRtJPIxaSyFGM2gdns1ba0T85nbTzZ6/xORdayUkYGAkQBAGBGoeLMIsAWgYCNBbC8eka2XlD4jrNJ2QApCZIndNgWABSICihEBgOUhLScavbMO1urg7bG4POzdLMe0TwNPxfJrt45fjq5sbm7qFo609ihw2VaseT06KHh3BAfi6m4+IdGJj721lcpKKQCmDyrULDVg7kpy4QFyXs9cVLaKKAMAS3s0JQSRLIBprZSZ398R/gqZ2pxTJI/3l5dx7P11mD9sN28fHg1kXjCCCkDZf3KOqHG63CDCOY3c4z3PWHGbtfD4t0yyl8GHXmyMEUUpWE4CAvmqR3FMELBQWxGhG67pj1X8xEUTAWvswREBRMTMRAcC2LIiBEYVwOxYtktfNB/dwa62/u9+rMmY36/5vf/05HAj9t1/db6sSgkd8+vLy9PS5FP37bx83g+bQxDz+n3/9aZoXUf761a0I/jKWP//NCTkAzJFEwLsIQhBQSBmIqfeFkZGNkC69QxiVfFlIVc36ihZGgAjCVMwHIjAAi1h3Isd1bR4raQZ//ZeI6Tevb+/326yPLEARv7xMRHh8OVtb7g97tJ6YC/MQFb3ZjttaAOEyz38p0pvBr+fpejQRADGRB5XC5ql6pSK8GYpbwkRXi8q6isFfjwPYb8c3DzcIsCztZiiXm+1scZmbqn779lUpqRCM7u2XD0+fj2cB3I2Dapo+WUXafOndZotmONRxGMacu5xOZ/dWVG9vb5fWz9Pcu4V1Fo5mD/c3h90QHsR82G/rMByPLwHIQkwsQojSemMiRGZiFUGmAGciJmcRbg0RmUmEBWluS28tcb4eLsRESCRMoCpMDAH77ebt44GlFEFhnpflfJkJ6e3jzWE3IiAhNms/vv98Wbp1u9ltdmPJVuQyLR5AxKqFtTASoXcLzCOVaL/dDIPut9vH+7u//Pzx09OJEIM5RAOcGAUIAdqyWF9g1Vc6oztEDpzcLFVlOSB0N8S8+JEQ07OFiARGKO79V9KquY/DiExXsEKMpYxVU8qYAKgAH4f63/7992Z2Op+OTy+M0cx7hLz//BTEJa9MVlXty2KRtVUgUiC7WxgEQURYQtUZ0sWISPvdZmoLEQvJysUHyoYzm4NtrW8e7ojQzODtKyJ4fjn/n//4LxFxe3s47MdV/eZ9Wvrzy9n68vDmzf3dvnfrvbmFMgFitz6fjpczMq/ABACopUD4ULAQH8ZdUendzvN8svm33757fX/j4RHAwsfT5XQ6u/tuGLabUpgBsXVZLpcjARPux4JC66PQei1iTQjjdjOIkAcOik3p00fMRul2P6Ykn5C8LSljGWt5uLsjBgAicAJMSaaWUmuBdCB1IkIthYhLraWUvI5UT0hCgrUOm1HdICAEu7sDAUaoaBEpIkOt7vbp+QyObx5vdoOsHSDhX35++vLSiPkP373bDtknIkD8+afPn14uYEjEHoaBEYYrKiCQPAwAnFmvpi9wX9s4FsQ5RDiFZhBRS9kMUkuKudHdiFC1MrWH291Q9OVl+Ocvv2B4c3Nz2RV997BBIjc3j+1YX44njAAyRKEVJhJUMIIAnEiQjJAckIHMfOkuIkzdJQF8mC3+FX9PjDAWIYIqhRCRWdCZVVQqwUbWQzNCBiXRioS7Qd/c7onQzQCxLZepv9zvx//6774BXHXOLNTny/vPp/vD9rdfveIcSwBM8/LHv30AkJvt+NXjDQAmx5HB6zgW9999/erx/pA9V2/tX/plnm/2m/EP39yXooQIgZd5+vn9e+KyK/z3370qwkkq+PB0/OuPPyPSZtTfvb1jXq+Uv3D89H6HEMNQ9tshO4l5bqxlu921ZamlDHXIusJi0Vq3w2GaTkwsquu8gGS33w9FtEjRGgrdevNA5u3m4L5oWUc/RFi0lFIj8He/efv2YZ+z9Qh/vvTZCW35/jdv9pshyRLu9vQyP52XbhYpg8wxqQdC5Nlu2EQKEgGkPQ2I8njlsZbe+svTkZggkBlqURYhYo9ABAIJQJFCAMCExNOyQET36G4WLlX169ePnJpi9z/98MOPP31gRCJNBXCyDwNYRcwxQUxX8xIikJlTXkUgq6kC1kaAMLKbKMIqlEMmDydmJnZLlmcaMjxSvrwOaKgqAyApI+JmHMKfhWm/3zBRntsBXjRHaDDUmjJxRDS33pY2d0Qciq4qZ4ChyDzNbr0U3W1HSoCPyX5bLn++bGsZak13LkA0Y7e+zNa4qGpRAQiHUOaAaPMc28rM41DgSqpvbU7T5WYoqYZgIuu2zFMACnMpGgAQaJbow5d5mpCwFI2IFCFPlxPjhoiYGRDTGQYAp9OXoVQt+aZAjsKtd0AmUS1DVkLNDIDDLV9nIglYBdXJnch9NP5KJaV1mIBuqYj2CHcTqeGupbiZsBAzIXs4JyueeP36TGQRRB1iXvo0nwelIqoq09zMoXczA/eQ5/MlS9u0dDBzRHrig4Sy2bRAsx6iSAiWZpF8lMLdk3AGicFJP2bEtbOhVX/BuHKpUvePhGjLYr1bTq3oqmp3b97RPIahIibhKAc3YQ6iUkTC3cLa4pHDOQQRYUYIBojGAuEk6IGlCBFHgIflgLWFE8KgsmrzmZUZAIGpqNSS+xkwN4DobQYopWjueVbPEQAimBmt0JAgRAsgxB6GmA8JAUKFYpa0Q7OwdZGXkyfmWHd0TMIp/Wo9fd2hWrQkWR3ME3lN5h3CiViEVi8FrtMlkQIY4eAB0zKHu4cloynfYe+x346IBGCIa7KApOmMWISsZVhHAAAzIwQypcos8Sj5iQdANs6UK0fRUIAA8asjbKWW4DTPa1PtndDl+HKOALkCUUXyxiUWilTkEFN2xfmJMi2d10YU0rkVQixCzbNH9YQH5jmYCzFiUWXCnIrCXJOsHIE4lpItNiKoYHrqWus5NnHOlxHNu7kNZVDFtHSn9RyZ3EOYN5shVg81FJG5Ld1MdEiBfDgLMzKRYwCWoomeNSPmRBitw5rryYoejEjdAAFUGYLzWMjjt5upatECqxVhddFAAAvnoD08kibkCPPcmDkVfpmiM89Tty7KVSVfzlin7aCqtdb84M1/7d+hlIoIHk5EuUJAR0xUcEBQdIvIDREEERNLBEQ4qW/qgP8OxIIEjCIhM9VaWsQ8d8AgQObUVoUHVCosnOcirIMqSgJyksXSt7b01s2ZeB0PeUzzQkTNvXcPUnm5TL21qERApPQPv/vun//tr9OlAxBAT3lVblVF2EJEZWrPCPnI5DIKVRmw9j4zU+++Dl0wJb+5sGYVWfcdAKlVZA4EHMYa13ohT1MA6O4swoSCiICqkhvibp1Zwq2WOtQ61ErE42bDqt0SJsVInLkdZiGqlLopMhKBpCkG8CqaWsf/EWDdYk0VobRmpahhnqduni20e/DKC4PwIELhNZSCmYk4wjwsXSYEaNYTOQDhwziIpAorhckM0FKUJqJrFRzAzHkNlKJZWcpiyElXgVqHYVOtt9b60g0zyzIlYUTJiDVzAA93EhIR9wggd0chJiHshkAouQQgEmIehqqYMgFaiyJwJBqHIZvR1XWXN27eUExFmUUQMdjZxT3cgwWr0nRpbZ56zx0KLriRyzRNrd3KPsdKd7eHm/12mY4ODjkqIgRMui9jEIlQAhbAmTU1ACrCkoBJvIQvi/XeVSRLrW4dCYkp98+UU1lmbNbdgVAwP9oopeJ68CZAGD0QAFID0bv1brWwllJrhfDNZjALM2MWYgRAFcptf7rMm+hq/AAAIABJREFUOCP9AN1JRJCQUYkp5Qnu0VpL1yckwJNWv5Yqi5CZG3sprCoY6By1FATsHiy/vjkASEXZISKg1rLdjDkQIpYi3K0L0zAMAeCOIjgMFSisOyKKMIu6W4IfYEUtQ6pVCUmLqvDS+/12OwyFhYW51Njvtq39RAiH/XYzbnJsScSqYualysPD4yDotv5znppkFR2rShCZhMmsF9Fhv7uPGyZqvTPRl+OzO4iwMtdhmKfLekkDQnj+nlccBASCiOKru8MPH57evX5TtHx5Opm1K9qDL8siHv6//1//ab8b8iie5vb0ZWIRD8uv7A7I6Igq3DqskzRhIdKSOzrd77Y3N6OZ/fjzp5S8SELtU7wRwKy1Vlp9dDCOQ1GZpq7CtZRMbAiMm90Y4Rax34xDLcnQAsCHu0O3VmSsVZh4GAoiucHrx9tSf3zzcF+r4jWFRFXvb3a/fPx8d7NTlWtV4buxAHgz22/HVC6ER2PabmqEj0NJx0HWniz6+vHm6Tg/PtztNlvWghEYcHd7c7Mb/vrz6buvfz+OowjnB/z64Q7BPPyr1495cCLCUPn337378edfvvvNuzePt0x4uUyljLvN+Ob+5sefP3z39Zu724MKezCgv364W9p8e7ffjENko4hQq7599Xie4ttv7sahIGGYA9Crx9vtdlOE9psa0ZGFEcehvnv98Ne//fx3v/+WMACRmZN+PS0NiYlw5cIgMEmt5Xfff3172J3OU2+tm4kQEd0e9iKSlqJhkCqbN6/uji8vPffkiMwCQJ5yWIgAGjeb16/f3BxukPh0OadbOTyG/c2tsbj1f/njn5Kz6w7hMYxjKQUjah3v7m+/ev1Yq87z9PTpCzZj4W+++qpWKaWosKoOtd7eHB7uD8/HL735vHS8kIp0T3gTAeWdmDJBRIhxGN69vpvbp4fbg6xrf4igN6/u7u7uPPjd20cRppX5D/c3N9/+5rub7VhrGYcsuYBEtpvd99//bhjHNcsnjWKk3/3m3eLl1eM9E69BpAGH/e6r14/H03J/d0O0xsbUWh4f7t599e7V400tedRJimMfbu9/8+1mW5FEszSmgGEc37x5TePNw/29qPA1lG4Yh++/+751P9zsUz5JBN691PKH37zd3WyFWZUBqVsj4lePD1+9OX/z1Wsm7DkxchiG+vU3393fbIk4R6xh0d16t+3+EIEOyFlVgSPSdrcfFErRdYnIgIz397e//e0fvnn3eiiZhhbMnGomJkJiYstaq9by+99+81/+3fcOeLnMlN64Zq0t66I959dEwvz69eM4DP/3P/0rCQtLUSWmtfFFAoy5WZZDgXQ5nc2aeyAL8BB9ETfLTT1cK1lE2Iz11ePDN19/td9vlrkdn79M05IaFMpAGBFVqaUwc6na3M7Tctjullf98/F0ejmzcF/sekBjdhZZSUSgCO2228224fXESi0oSxlqaU5I662UPIlaxa0vrYloyUYsxXEALy+n01YRMdOD8+sQwmVu4ZYXb3q7iUBLlQXcfektwjFwWea0xCpTsscAwMGFSZU+fPhZX93XIkKEBBFYIwCptR4QRfna94AQnc7npZvkagnAHQK8WfjwuLibuwQVEWNyj1qKlCrCtQjzumRDQrMAjGGoqpJfh5YGzC8vn++2N0WF+ZqCinRzcwhvw7gZqpqtF6QF7fb7nuEvSIs1QOwOiJj+BA+EoFSWbza1dTfgSF4NUms+bDabza63+XS+ABIpL83M8c2bV+8/fP50PCNRzmzxGh7QrR9fXs6XyzTvL9P8/PxsrZtH2Wy7CHcXR77GgxAgHfbbP/z++2++frvbjC/nl4/vP3z+8sV8tSgAcY5baqmqqqWOQ80JhjsB8VDLfrf99OlL74apoqfV77TOsYgwnABZWLXMrUfO6IIhQlVLkTD+9RQ0sx7WWmt9saiqRVTW6RwAUjw/fzkfKgtp5r9FABILB0a30KJ5Imadp7XK3B1wMw7u4b2Z8dytDiOytm7AgO5I7GbdQ1SmeT5dLmMtqbdbel/MifD5dHF3vA6Np7ZoHYD6eZoQD9m0RsC0tC/Hp3MewCwAQI6Edprb7d3ty9QAWVUAKdyP59nDmgck8xsgIrqFuXv0ZCbhOo6F7r4sMzMQC4smQL5N09PpfDx+qTj491+viRieKAZKEbKZrLZ2hA8fvxAxkp7O5+kymzULOuyGu7tubh8+fE5l4TwvqQe5u7t5mRZCStHwKgBBdHMHGOoAEKeX0+VycoAAePX67fvnCWkRwgBgRLy7u/n997/5+qvXtYh1e//+pw8fPoto6x2AHMDNWNTDn56ej8wlS1KVqjIMw9PT8+Gwjd7COzOapSISmQkAzRL+nACLSDZGQG+LEWdvEIDEPYgJLRazVC4I+dJ6765FiZKpw9meuIeybHebJPykESzPBSQWFXNHSuAfEmITactia+iyMAVCuIdZRwiLIOaMtUekYBDRzWastZRSdtsBAAHzLwIiDIginPTh1Palu51EqqojEGCzjsibzUARyRjPb2c9LGxZJhZqvXOqWXL3RAmYNzO7Dkp8GOrhcBjGurRO66eL5qFFGGFJSQiAm3cDRBBVi5guF2LJOm9ZmrnVUqbSemvZMqgKIXz4+DS3Ps+NCZjoMtuyTEC4zPb8fMxuzMz7VZcx1OKAjDhPEwBGgEPMl4VVD2M1989PX3prADiMm1KriomwEMtv3n39u++/fvf29VDk89OXH374S2/RHTzc3Jd5Fh1ZyM3MPDDaMjdKSTPTjIvIPE+lVBEuDEMVVXFvuSZj4Sznq3IkoSSn81VzLwsBIgiYmkGuQw2K1pPOH0TMouO4ub29IeTWc/4ABJ7sh4eHO62lLQ1VIOdX0QPw9rDrga315MUQk3mI8jjUbrEsDRCtG7Oy1GGsLGzdOwdAMEE3B+K7u1smmpdmVh08HOal7Q+7Mm7qUJalu0J6pJbmtzf7AOzNz/Ocw4+5tSA+7HfW+/HlLATuGNGnuQfQfrdF8Ofnl9Z6bn66x8P97TjK8eXSW8vzv7U+bMa3b0dEO52nVClDwGVupah3ezldMrEaAE+XSbTs94h9Pl0u5sEkgLS0Vkt1NCbkouBABEWlqC69ew8kFGEi2XIghrIYebrbIa7h2ggRKKpp8mjmIspCFOAjHXbbS+tINE2XbsYit4+PN/vtaemtV/kf//v/7uuvXkPYy8vpp5+Ol8sFgYAivJlDt5aPRe+NGNzcWkNaJ9pMDITMlFje1paxDBAwDqV3z+1CKUVFzL2bhwUSmEdvfV6aWz9dpnlpAIHE5nA6T+ZOSC+n0zR3Ygpz8H6e5t569/58vDDTCnTo/eU8MXHr/XiZdzlRDnfz8+XSWj+ez+fLXGpBROh2Ol8igIjnpS3dmMgDg9mRIKC1dmmWXNYeMDc3M+sWFLPB1D0lxZfmbendbJ5psSAlQGrdTtO8LA2JZrMelGqqvljv3bwjYnMwEBJCVCXfb3dTe1YpVLdSa/rEhnEcx4swAmtwSWVRx7bf7BZ7ISAuQ3bcvduwueB5YQapw7DZMCMCcRkPx8X9RTcVdFuFECkcbh62VHf/8se/HFWLu3UTFVVOgyYx7UqppXTzeZ5ZZL/fhb+kGCggiMANs2QsTYhk3I6gm0Y4WwRgIL59+3puLTze//H/83ASCRnPhqVutjvE/+1//V9eXk6fv7xM8zwOg4i0tlzmhYlfXk6tLQA4DCMLhsfpNOXPxUIsoml9BCxFREWJ72/3vS8fPx8/Ph1Tinlzu3/3+vF3370jCLNUj8B23Hx4en56udzudt99/VpLIt/t5TL99P6zA+2341ev75UZiCL8fJk/fD4C0puH22HQHHMFwOkyn06TqO63Q5EM3CYPP50u57mVoneHnarmgGBaluPLOQUmtWhuxALBLabWwX3cDCqa9v6lLb3Zy2UC982mYrKuIiJiXnprjQiGQeGKApiXlkVM1VIyqoQpPFLRCAhClE1hGnLNbGkdAkiEIqm9Ep5w26a1gAMLImLv4RGt9zBnZlmTCTMpxXNEnwYtu4anTG1Gh+fnT21paTvQsrGIl+Pxz3/9sZlhQKlys6mbsZwnBwQWMQtwfz69lFJ+//03bWl//MvfRJgIwy0nqeFxOl/m7nc3WxFtbcWluvsa2mXWP/+0TC+oZaa9I5vZNC/yj//0r1pLWo094DLPiLQZdx5ufnQHEVIV8w6AxGjXfBfODwo5KzAEQiZmUhlvDugOl8UCoEjZ7fe/PL1czmeCMPfW4eHxkUm2293U45///F5VmFJKTygFHI6X5eXPP+dO/dcpGmL88MsT/LvIDQIwzIGWD08vYf3KhcZIwBn4n5CIBVZiE7g7E6aGFNfYSMzNa2AwMYtAgPXerblH7633FgDWmgcQreUmhPccAl1z2mBlPubEEFRFi7olGKAnyszde2/5ZObqPVZV6xoxtuqcKbU3zsy2/s/wa4QNIeSRP4xVmU/nSzqrIEKEAbIkN+HUCrCFn4+nL8f3rTXziIiiUkQQo1YtRfu6xQoEN2RV3W23jAjK281mXpahKMlAAElqCQQ/ns/TwpT08ZVymjFd5B5uJBJUkSV83VdJ63318hJOl6mZIUIAhRsA1qrMMgy6zPF0PGWQ31AVmFVyWxdEqCIiPNShqApj6+32sIvnk3n0vnz+8mW33Y7jMKgGxi8fPv7zf/p/x01NoklbWq1FiqbNOHUKKRzPtdAqtUsbCKJ55LQPIFZTZZrjY81ERSR3p3XvhRae4fO2QmRTEpq8xLhKUrx3C0+wJLpbBGQLEbCKIxBAi16Ti665I4lGgsA1LHl9A8y4NTHz3m0VBibwDtdUZeIsdwAiOacRq+0KBJkJ3ALCmTILa/V9bDfae5xOZ4BYlqUlMNC99z4Ow2F/OL0cT0s6MfrL6ZLevqXNsGoAHBiGoYjwftDDYQuBgB1IIpwR59Z7t+123GzGy2XSIoGx3Y75IvFqXNKqenw5uvUM+Fmt7ck/6zMhOFJIYRIiN0R3kxQSBWBrLX+/ie7NO3E7Dub+8dPnjx8/bsbdZrdF8ByfqDDLqk6m3FC7EdFmrABh5vtNPV5mwHh+em7LMgybZVM2w3h3ezcvvZmr8DBU3tPqGeQgStXu2o27h7kRkXvLIBcLh8CUmgUEI2ZRvG6HCQPo1yOwt8UcmJgZlrZMpzMwD3XI8a/5VfAk6B0wnFevbKiycCYvZ16FE3OKUoqyuUUAIwWjpEjVU6S67nTzdGqtR0R2h0igLEgQoeGWNJc1HQcRPcUDaeGCILDuIgwA5j26BTgEurs1326qCB1fzhG2knMhxqEIU2sTIvCVZtzbjBgQXoUhIFXjBHhzs9mN47Q0JLQe7lErC1ViKBZL85fT+UlL80aQQFwaSkGC3m1eOoqr8FDgMNYebt3zuMm35eP7n98fXYu8evegWhKsOc2zlKoB2JeuSm1xCxeiYajuzqSn8/lvv3x4OZ6GorJHQQqhfD5UtRSFSDkaaxEmYuFhqJux1KIfPz09HV/GqqLsEZfpPE2nox4h0CMyzyFteUQ41gLhzUJUrFvr3VdmakSEqiCgmRMCCl0RwgARGECrlQSutBW3Fo6RE/9UPGzGcTuO4e0yLcqUxhqiVaVCCGNVRAYwd7SVBQBr8DayJ+CQMnEbAT2JsGHujr5KVLAHIEIzE1WRvOthjUz0FkFEhmlIIc5M0IgAhN49cisAgQB6LUogiCqnmWEcalFloqpLEezdzSzlDMQyFE5Ckfs+QwiISVMeQsjMuZpDyKFJH8fypx8+ULJWWFQlCeJF8PiyvP/wsRSZWydEBO+9NXPrnQjNY1kWQHi4v73db4ZB+BrGOM3t//jyGcAfX73+b/7htwGIYR7xfLxIBJj17WaYWwNxciREZTpeLu8/fvz46XOECRUiBPBSuJmPddhuN6qsIrJu2BNhnSJM2gxlMw7zMrfp0ov0br7OtUBYMC1FAIS03QweLqwX6x6RAW7hjcPB41emRbLONSUqSB7mvmZ157dMRa4wDrUKcyZICGFqXKxb9z5oTczkZW7ETIgZAMoEgMSUBRywICOJsHt0N2VN3HVgxicykkQYEbp778Ys1/oK3MKsnc7noQ673ZiD/ryyaW3cmChzDmnNOnZwyJzFYMTMnVpaXyX7EYCoTH5l1f57Rt1VM5IKeeZUmlzPSIgsNua5zfMCEMNYkcTNW1tOp/PL6SwMZn5elvPl2d0JgYlF8Garc7PW2iC43QybsUQANZeqjCRFMHYRlrKY3Xbv3sw83Al7RBOVosOXlxMjI5hZzPMs4VaSJ4gEVax7APz5rz/89W8/L0sjJMrkKERGvjuML5euKrvdONShKhMzQEzznGlsvdvHp+e4PSzT+dXd3f/8P/0PS29LswSqswrnKJqZApEwJXuMRMwiTJDKRFoNeYm/QszIy9yHM+LKVsRsuNKWh8iczW83dzMk/FWbFxBJiafUftFqQ8xUQ/DwCGbMZWjElYSfi8SUgKZqE8IB3KK75ZKhWU8/gSc43yOs73dj/qnNdiha3Z0oElJr/xk/OwXMUhmJUs83DgoeScHq3cydMCF2GUAGTHDFwIYKE6GIZJ9JmdLqnqiYIszMEaFEiH4+XU4nPxy2pWpRLspDLYfdblnaeVqW1iggILTIYbcNwGmamTlzPiLW4jgicg1AlBlnKMQeXrWERrgx4z/8F78/3N62Zp8+falDEcAA7waCgNmHl6KI8pf3P/7rX348n84Bnko6pqJVmCQCa+HZiImOx9P5MhNE670WvT3sdruNihBTmB2Pp/ubzcPtTSkFKEVFmr7vtUPN0TcSMmUM1q9izESvcdLVVi+NIQCTEiPliUhr6JVH4lIhn5IkNDCACDGuQst0GEAwMQVg5kELc5LjKRVJgJnSmLKZuArPPWNLIdnMlMvM1nusKlWf50bMIhQ5U0BAwFqKmQ+1RsTSmq0TbQKAZVkw0mJJ4dF6X7oR5rnsy9wcHDwo6VmYMcBgHgjYrS9T9zDVYp6oFdqU4fhyRGRDp3XLgphSWuHsZg6l3BxuPDx/Re4xjvVwuCFCh0DzHpFHe9KP1iYYIQDcIOOfIwAzBIWFMCIcE1CSFnoMN2fVb7/77t03X/e2XM6XaV7m1vvSj+dJCFFFIezjx0+/vH//y4fPX14W5FRukday346Akj88ACu7KG3GYRjUPFRoqFVFWDmDDes4CMtQZBgGLULEpQhk3gHgsnRwc6aqbL0vU8s/KazImME/iW+yfo3ldnczF0FDRGjk2Qdg/nU9GVICa6cc7m7dtSr4esOERbeOiMyAHh4+BWyG2tpCyFo00Y3Z2zIiIrs1BEbi8ChC2WASoANU18ikEIj9bnvtZF2IHVxZU9WdnzgjDYMsPVL+udluwi1lLGlx7b3nzOMq9kyTIl1FWZijDQaLU/Na3DqxlEFz83hZjHVQYqDg7NARICDfM8smBoKvmnFcO/dUqlM23SXcIlpbxzRMkMrOAFyTgDD7EwgAM2t5X0Oe/ZSDlXDsrQOSyqBDkboZerdl6a3z81FKLefL6Zef3z89PbfWgKIWtCxJgd1imqwOVIftOIzMPA789dev724OZSjg6aA3Za1jLarrehURAnMJGO5ILCwSHhGqBRFYOAI79aAEtFAghYOjBwBhWAePyJXVwJp5Vys8LOV8gkIigsy0TgcCYE1rg+5OSEAEAWaOGOLrQn1FsQIgIEsxcwcKzxEJMEFrNjczs2lZhlI2Q6mDrAkamPMtsm4WihCELEq9Wypj3Ru4IzGSAkS3cPDL3NycGLNKdY882vMiLkWS4G9uAICQqUMSER7emufoAFmGwZfWpu69zcIgdWPuuRGKxNGlSDOryYjFDQA9AJF6D1zH0msEAAIuPQhzliSEyGStmXkCP/OeQEqOgKwlSgCIpEHN87iL1bPjANFVu3nWoCLE3bpoMZ8D5cOnz+eXU7OmdQDmTlyhNYvwqLUM47gZh+1mPBy2h81we3/3+tWr3W5UTb4VB6RFFlkk10EBEIkqTaRbwNIdwGK1KgBhfHm53B4246BitHQ3g2wmlqUTOJUiGLnldfe1JkNEjJRQbwdV5VorIbbeYV1DWQB2s3BYUWOI4Z5lyjo5y50aBK1nYTByrgQAYmkNEMB96YaIqmoIx8sEtCmFEZJquMaZJxoSCLoFssDKCGAW6REQoSLEHsBh5m7uPs8WEMw8iiYTWYXNXVEJojv3ZsSEgK23VPFsRnZ3swgIpi2bybIszQFbRGYk5qbNWRBTnBZo4W7O60YyAOJK0PLEDBCusD4ENI9wyx+GiCIk02Su7T6k1tVj/TTWKCEEJjRgChuLAqIDWXfz3nt368u8RDgig6CwyLQYl+LOfTEALMCiAxENw7Df7e7ubl493D7c3+62Y62aiylRLry6rQBRiJgFr14SoqSFIxGiOGSDjgEJogQgxHHANVIARMBVoCh1C3NDZiFogIu5cro/Iccf69MSvrTuEPPiujbzqMqkpCwBvsy92TXVRsR6zy4s7XoBtq7tkpzDK1ZwWZa5OaZdC1BFpJQcPhGtlqrupszdnEWYg5hJpC+Lm+WcjJmJkFpzsG6OSEyAJdOL8fa2IuL5fEESltR8IjMJUwSQd2FOJjUiAwSEdQNwFxYiCCU3nwgBWlv65XKupQRkW+OAjGAZa0zdLUOsCBEpRfbgmYNjWcMSECMQ4yAU/3mSQGC20sRpxFpDrDw/APPuYK1F+AKJTIPee65YaikebCK9N3CziNyGacKCADHH40SMikSyGTeHm+3j3f2rV/f3d/vNOIpyUSVCYSk5KmMiyu1TMtrySoJVqJbMRxBmgEhobj5aIKLMq48uCZbWOhAszXbbUZgjYqx0HZ5Bgnop/RCAwsKCOdVMjhNieGRuj18u87w0WFn4ISop5c2HbKVlpMKdpfeWIzwIAMDNWADIowkaMkaAIHSz280mR30IJIRhYeCIwATpPFQm87UpxKD9dlxaiwhEyHlB5M7CLCJEiFfYcIq3ANxy1p2q4sncvZtnLJdBkIUhS4D1ZVFEHsV1c5kX9L4ZeTNumse0WIRbbwCBiJUpFwwIBAKAmE9Kd3R3cHJ0QrRusxkRlaoEFJR6WgdEg45mCKBVEZgJS06dIMIrIPTWl9Z77xD5RrODCVLRMs/o3hncOzA4S5FwTxQkEyGCSNlt9zc3h1ePd68f7vf7UUspwlJUkERZmFkygoLSi00AgJEJy1cmDQKEMBRVVcoc0tVtGmsN7OGAJIISMVmfZhtKGasgc2uGKQgMCEL3ld4DQNlge8dk8nZfVwHeOyJMtsZvpVVZlJXS6ggQgYI5g4r8ghFC1yvT7XKZtmP1sGlqTDEU7RBmwUxAHH253kJOK1mOANx708RsIPXee+8A3loIEyM7+GXy1joCI5P3bAkj0HPqcpmm7aYCaRGa58YJ1WZ0RAoBB8bwAGu9h1F+HxYGMrASsLRlmq37VIoygXBlQQS0tuQ0Lnw9c1JnqkqCgmscJCJgd4MApuuKJagUBDCi1Uucb6eni6v3dHvlf2LmgRhqyY1ypt03M3QXQTOOIBTHYCaWyoEETuhEtYy7w/bu5vbx8e725rDbDUSZ8M2l6JVFtc4lUpKPq+occd32wHUlFwjYe289VdagzlBViIRlaRmaiXMzQXD3qjKOqsIA5B6MEUHmDnZNEV27qGx7IVXXsXaYaGaUawKkWoSFKCHQTNuheERrfVp67xYWiZI0N2EComYmwre7sUdsq2rRLG8FyCO6ea4nA0yEMt87fwamHLxnMDJCOGAQsIe1yRyCgB0QUCnDdSK6OwH2MAeohbebjYcTWO9OCB493JkRkMEMBZEKAcBQ3QwCW+9rVaeq2qYZlma929Ki1jyzhZNllxmJnO5fYAiigrCu6bLgQ0RvFgFIYt1SXkaMRSmAryiVDE3PUwjcVysHoOeabd0s568CHVl6awqkhD3Cnd1NlUWJkQCqjMNwuN0/3t+/enW33+8QsdSiosyonBGAKMTAcF0ZrchjJswqfjXHAiQmJGFBiAlxS5O25GVHzL15NwuIy9xEC4ILZaYWlRSmAraeKdGYWNIIDI9wizQV+pqEEAiMHJ5hjNDMA7CU5JXTYm7dloxKJUIKYQHCWDy7DAA0d1ZV5kBiNHTqvTExQmw3pYowx7JAomhqyoESUhHhEb3bbGbWc/QaAL5CJ3hdMgQgBlCA5yJdcu6qqoxZOTlxmAERWreUr4U1iAhSYWQuyf9xpABCYiTQgsiOmdeOzLhexEhCuYzDNfcz16M52DAzwNzeQaklLJCJhcPBwN0dAlXBnVN3ZOZmjUjWPcM65yRzTx2DtZYgBItAomHUomzWp6X3pU3eORd827rZ7be3tzevXj083N1s95uhqAOsDwevlQ2vCKAc76Q2Jwgj+SmpOs74URVCImVePQEIOZ4lEmJ082Z2nmYiqoyc9M3w1nthsUjdrifpHZFyjB4dEYGRHIIw8vJO7RcTpbUdI3IOZRbz4rVIiVgiu9RY8XqIiGAeuf8G997b5+Pldr+vtSzdMKK7uTmhl1oO+12WOhBLNxdmCPBA846543SfF1uWpbeOTEVLnqPuFAG5/0HsACCUhlco62wvB8JEDATs3pECAZzJ3fJwWmFSTkhgTsgqiIgEACbsAG2eUnNqZqxcqwCSO5BymEdYrjIcVodH5KUQmBWiAKNkXbG6Sog4wNu1801kCa7Jh0npSD1L+qsTbY8RkYVadtbZruZjkcI7GTa7u4e7h4e7x8fbm5td1SoimdYDlFMlYqL1WqbIWKDUTJXCIiqMqXpYM1lXzUJgYrQBgJCJRAYHWLpbQ</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8abBm2VUduPY+59zhm9/8Xr6cqyprLpWkkpCEoASSAEWHLIwNNthM7Q7sIEw7bHfj6KajUYQDBwb3QDc4PLTdgLuDSQgEQiCZFhJISCWVhlKVKmvIzMrpzcM33+kMu3/c76WypqwU0b86ake8F+8b7nn33rPv3nutvc4BXrfX7XV73V631+11e91et9ftdXvdXrfX7XV73V631+11e91et9ftdfv/u9E7Hv02MclgYhONvPJ5Yb1zQQQQhCDEBAFIaU1EWmutqWFoXFjvPCMEa4uqcM5L8BICi0PweeXqd1gcPFqdDkWxDdIA0sKhl+wNp4vNNBnbaUQTo3oLS83uvA6+0e9PXZHMdbs62XAh1jTo9zmJq6JIG8m5c/cpWz535erxE8fLaTZ44XyVTTqtttFUObu81n30nQ9sHKZJow0mRUxEpa200lVVNRoNY0z/YK8qi7wos2nWv35tkmXLx08sLa30enOtVpfZmNgQq267y4qNiZlJMU+moxcunt/e3dFKLS0sjEYDVqqRNiprBdJImiBcunT1Y5/8c++CYmXihOFPrC0++OAb7jx7lln3B/04ivKisFUZxRHA3ntGZa0DQQKImUBVORVImjRNlLBSxmj4cH3jWn+4L85FcZymjdNn7+g05/YOdr2XIi+yfHpsLe11ExLs7o+efuri+unje3s7ZZkDJCLEpLUxWkVx3G4lWnNRTMuyJIiIQJwXL16mk1yCL63zXpjZGGWi+KE3PLJ6bJ1ZATBaBcF0mlWVLaoqODfN8jzPnPNV5VZXl5aXFtrtxtbmzp/+2WOf/+KTIQggAoIIBPrv//Q/T9ZODXNZbPHGYbl7OBofDmxVSlF0czsKfhzKuNU2SQSRVitebaGqis2DSZVlJ8Mk3+0/74phViRii7LI8iK4Inhb5IUtyjzPbJ4fW1yLV1Zyz0uJXswrWensHA5Wmo31qez1s+fn4u7Kypn73zzX7Z0dDoqvPJWd660urG8m6fFReXF6uI1gRbiaPPTwW7/v+J3nn7+e3dlbbJmP/8r/Mt67durY8UgjasvxE/Pf9ujbcfwDr/VoVXCH+1eunf/Up/b2d97w6LvveMMbka7exjM5BZqv9tnHf/+3L17dJY7StB3HjVZSfP8H/osf+LH/Eqxfa1gPVIAGCCggDtR7yTeKK0/t7lxB8K1Oc/6+NwCL3/hMclAM8NHrK0D6whf/eDwepM02BGWVBx9MpLq93rETy+g04UaYTKXKIB5See+IkutXNre3r44mFqDIqLSR3PfgI60zP3LLMz8E+kCQ0Yg69wMJAKBf/rOf3tzc9M56IRGCiA+im8srfcfKhL1xWYkjKSeHOya3dwc+Nq6uTicXUpoEl2VIk8iSLljpvDh32M93Ro3DcetYst9tnW6qdLM/CHyh1Rrl1FHRjiND7IlA6A8Ojs31hNOCuD/XyotwYmkOla9OtZZ1RJ348miwd+Gr7sS5RnvhzY313Wz6mYOnv/3hN7av7Nxx78n+6PDM2tLBwcHW9Uuf3Xjh5OJJ9O4wTdM5ccd4b8Pa6uBwKPtYaq1/9dNXH/47I6Bzy7sTQafkbCPWvVZLnLs9J6tu4WTTrUv/x6//nomSRrPXac+XZX5sdfXBB99wG04GQAHp0d8JqMJkA63ezf8uOfXAyVMPvPLRlL749SlAup12p9Po9uaEKJtMiChNE5PG1XQaxUB8D3oLhBLoA4WGAag7+OTGxrU0TY02Wsux48dfy8kAELACpNRRN956/FMf/cSf/jmRkFJaKAgBAi/6D//gI4G4yIvxaFIWhUyKeFokNiBJLiRqd1LspJo6zU6nGc+1ioKf2sKxplkm1+kqxEm+0jiJkOzb6W7e9G5xJa3iqCyLY3NxVWLHOa/NMCvt5mZzbmU6pXYrbcTGRqY7yrYq6yJFvuo1zMH+wcHB52X1uMn9PWfvO1UuZSTxA2c3TTKf9lohYGV+/fji8YVkOu5fff5r3D127lu/58qXPpOV5XA82T4cHFs8FpsY21tYvbWfAZBxvy9e4ihSxK/15drCTX+/NLB98Bd+dTTJ5udW02Y3MmY43Dt54p573/zm2xv5ZtOARqvxzRxSHAWSG0bzd9+HagJtMJ520wTtBWAR6B9c/8LgwvWVlcvzp48jagEKiIEWYJVRaXPe2SKIU0qvPfyDt/GvW4C5+fW18x/92X/xr/vDgQSQkBcAAmFA9PqpO+NGsj/IutOszLN8MrV57mx5aVqIZsx3mjpqtpNe0yBIFHBGHKZh0o58K77wwl72/P5yq6mgknuWbFmOS9diGtpqoan75XSRfRZJb6HpTUNFOo3icVkVzu5JnA2L8jAbd9se9m4VL6pkA3J9VPKZ9cW5RsP3yqTlF+bWo9Yol9HhJG01Vk6dvG/RRDjz8IP41BPPhI1rc8ur5XSQ5cUomwYIAdPBYfM1w1MohwcHzKSVykfD25vO8qbpvNnn8D/9wq987aknIGJ9mQY3GA4H/V0TqQtPPH7nww+BXtNpBPCAAgioAADR7ZyP7Fze3tlcO9lB7+UOvQjOwSm6DaAL9IBidPnZjWsXxE+z6cHW9QtxotM4Xlpej06cxmSv3VOnT61dvHhVfPHwt7wXOH4b5/AiJ8Pky//9B3/54sUXQghBmEAi9eWJiNcrJ04dW1nMKj8cTdmX3cg9tzGcZlmeF75y3lVxrM4uxNujYjGmY5OpfWIrOBdOti/40Gi1zyijCj+Ocd3KUPRcR/Unor0b7mediee9giOaNMCRWdBmPUmuwNhGnDSjZGleC+UT77OiKKQRaz3fXjxz5+l775w7e/Idp1aXm9E04PrBcGdclJVLWo1200QABCnhfW+4Z2N9ReNw5/r1uZ1tfP2Z0o0Ph+OLzz//0D1vf4374/xgf79NiCJT5pPbuKEAujf93b7x11NfOv/JP/vUcLhPQG9utSiLw/2tyXT0Ox/+0NbGpXd/29vf897vQXf9liMTcCO91h7mgBxQwC18tKJWt1da9E6+0qeLKC8j20NnDVgAFLC9u32VpAJzAAWJ47i7fu5utO8Gtkdb1wnV3PKxu/S50XCA+fe/1t2QFz94QHj6J//Rv3j8y1/zQSBEgAQBEQEiIgL90d/8tVZ38c677jh37q5obj6OzaqaZ58f7A8i9i1ttwaFbqrE6b5zp08204mfbo2ud9sj6+5rNf3nLvWzCrE055MyVoWVWFO3abAleuRbjYZPZKzksH+QLKkX9g+t6DRZmEtiR7plNCmZJvFB4XKtiMp859KG3Z1e/MIVRautNNaN/srxu86sDZoxtOgQroFP0OzS1hfn9pZXvfil1aXji60kbG9s9tWVqw/B3TRzr2ChLIvpdG6up5SalsVr3dNb2b/6pV8BaGXlTCNtC8n+7lXrKoDWV4+fPnGGVZSNp43urccoAA3wTbW8vtmVX2wW/ctoNWF6aM6ntwjdzROTS5+jYb/ZuoK5lWzjSjY90IaUanW68+vHj6vlc8AqsFlcfdqYOG2vYGG9u5h0ceY2rnsKVDf52bV/9k9+/tN//lkfHFDXZAggEgkEAETQjTiO7Pj6U4+Prz9rmk1v2mvHT508thQtdoYVhkV+crU5LfKFVtgduucHVeg0QiPaLisfMM5sudp9zjpHQSuvScZluGMhjky6uTMuFxKdclmV41FpjO4PDjlKMN7pRXlR7GpjxOgmqCGiCGShK4oL0n0UrDaAHeE0TaU7d/jlBqJmo9nevLYcNXpFJ5oLNmo1O0uLPSObVdVuN0/ce8LuD7OxP7m2fmsnA2ArK8HHJmbN/qXFzTdh//xnf2E4HKyvn00b7aost7cvee8J9ND99/ztv/6BNzxw77HVlXhl+bWGuf0TGGLY93mprEdXgQ1MBLRe5csrrbPvB7aABQCjwVfiJFpbu6Nz5izoODAHVMDFyeVnjEmSZges3c5eXkr75GtlAwDQN/3f/r/84L/86B9/0nkJNcCEiDCRiKCObSDSZ88cP7bcGY6LyzvTJZ2sd6ncf+YLzz6mTCtZXtdpb7XZHRbIcyYV9cvSaM3kFgxv7rsN8UXTRI6qvEoNO+8JsjWsYKlc6ZVZlhhKI9UNPMlJ+xJKjz2VlW1ESgsZsFHEIKWYIcwcKVbM2qhIaWM4MlEzdk1dNRPdTqg99W0MFqNup9fBnEJUnl5Kv/58NRhUawthcU4fLgw6q6+KCm8yEe/AMNqIUq/99VeyD//GH05yc/LE3UWZ5/kkz8beOWIm4D2Pfuuj3/atzUYzWlq57fEEoFt9Hg5QVogT1V26BfJ9samjMmtnaWlh9f57gSWgDUTAsNj80tee+MJ4tK+NAtg5mUzD1W39/vcnpx+4NTfkb342fu3f/K//92/9QVU5QCQQCAICBHJ0XczsWef9nUNyIW7dc2YlCtnzFzarQIBaWE2Lg82N3aevPJ0g6RLHxhjnKogEb8ts6p2dKijxxzvKVXKQ+V5MiebC+QgUSBUUlUVlnWitWkmc5eJtqUzcL20zMZrZO6ugSTEJiAGRIKIwo/eYFDMAYYDEi/fiXXBVkWea0RCPVgParLaSndyR8r3UPHBnJ+rJa95+73xlSxHR2jjxtzdnL7Uvfe0SgCAO4pk1swI8QK1m8u53PTp36iwATPtozt3eeC93MgcIUOFwC0yAIGkiMrftZDdsc/vpzwz6O7hwsSwrYup02krpw72rtpwQ6yKvS6p0c89tbPlf+bef+uvfO3jHu3/01Qf8xpP5l5/49//uP/5uWVY1siRAhEggIBAYELBmDoAe5SCnJ0V1No2vXt3bPCjmjh/vznXTbqvb4MLs7m1cH17/erAu4qSLODfGGqWSWJEwoaFkf5CzqxrWLVe+MuoFj4iko8CpmmQcQRHE2pDEprI+aqZxI50/c2e2/UJlKxIBNCRoUaAA8RAhUtWsWgkMMCEEL94jOG8rb31Rlq086+ZN1WqcmGuVMbW6hGKznVqdvtrd+YYNRyNrbQgSQrDefZPTBgAQeOetLaMoTpOm9W4w2HHWeu/uOLNy5oF7Z1+7XSerzQP+JrCpke/BlUiaaCzcHgh9Jcuv7G1f2d7eH0+mQYKzPiA00uTUqZW773+o3exYJ6Nx8eUnNjZ3tssqgOhDH/ryhYubP/IT/+iWQARXnvrIz/3if9g/2BcREYIQRISEwMQgKCJipYiYFav7Hv2urLRZ5UIQpc3i6pJKmzqKrBetuJmk62tLc3MdDrYY7NLhfhhMpvDCkqTRXNPE7Lt53t0ZtA5HkfiqG0Wa1iZFOphKyxzkjiEIstJWFHxMsjaXHj91x3e863uSdnvn6gWunwEhnrVB6qAmdWojIIhIjZJJQhAECRIkzCwmSuN4KFErloYMjXJoraD3ABBulYbK0dOPf25xrtdMG5V1S/e86Zudu6984fzm9ggARAKwv7c5Hu4H0HQy+J73PPqWd7zrFY5xh2BzU7H/cmP4EcoBjJ5RBqaJuANfgt3L+NjbNjOY7h2AuZE2oyROkkYUp3lht3cON67vHAwO86IYjNQXvrLTHxQ+iA++KMrzz17/9Cc/+t53znNy+pWHHT32j3/6f/7qU+fhxQMkPPMwECmlWCmllNZqFulF/cj/+K97ced4jsq6ykgV0I5prqkHmc3K0IiooRE1GsqkCy22XB36aVZMlOZWohKWUW4LiOloSTDQDoy2rZBVoXRjpYIi633EshBBHWRxkHRh/s573vD973rft73tbdvbuxsbLxCYmQDUpWOd26n2OgkQCcGj9rxw9JuEACbSrGKjRo40Vb1oDCOgDubvBeyRq73CvMYpfeE/f3yx1200mmVVLt/3yG1NWH4VZgYdP/bRTzoxQcLezsbe/mZRTCCoqnwyGf7Ej/3d9TN3vPTYySaSpZszzisbp4BFmcHob6AZ3firOxkARHM9To1JGikRR5FJ0jhNkzhOiXWe2Reujr/45Z3BwAmRCIo8H4yG48lkZ/vwNz/0Z+14454H7ntZYHvmZ/67X/rEJz/jvZeaxQAxM0OxUlppZsWsFTGIxAfvvfrl//TLevXsGxbue9/yqZHHYTmcFEUzIu+ds64aHdphf2lpbqkdXbu2M82q1lzHO7u/vUOjfttVC8EtJqw5XBtN3ahoEpfMO8z9xIihwnnyPqqK9CCPi+B7TT2/9KYHHjx5x9meju6668z5554b9g8IOKL0IAgkN4JbEKl7sUEg8AFEwMzJjGJmNpp1lJpGlEYDcBDfoKV6mhuvGjw4+dqn/3ih0zE6ysts7aGXIKzspQxkbcbceP83f+MjcdxsNtreW4CVUkHC4cF2EoWf+vv/IO68uEFp+0iXX6PMv2EqRTbwgz1OCfxNNQZezVJEjXR+rru6vHJsdW1hfm6+uzA/35vvLSzMZaU+/1zWH1rrQ1VVeZGPJpNsOnXeeu+Lovrzzzz1tS9/5p1vbMWdO48u4Yl/+bO//Nu/96dVVQqYiECKmZmVYsWsiBUTAeSDBO+8t8479Ysf/GC3hei4Gs23u35xvjV3YIvJeDDa257s7R3sHJw7tby82CaXGxO1uh1RiRMZjaZ6u19s7e+Nx44xDLyYqPbAVkOrGJnRjmRa+k7My4mYUYEy6OVm1W6fOXnyb77joWMrMdIq7UUP3nH2s499sSoLIBAR1zilxsQyo90FQUAIYQaVCYqZmbRmo7RSuhFpFWuT5giF+CZ1T8NZUA5uvMrs0pN/8fH5VkMrM5lOTr7521/86Ss52Yvf/8TH/miSlSaKtDZRHI/H/a3Ni6Pxwf3nznz/j/0Y6MVxS32T0SjpcKwwGIBKmFejLb4p05h+SUZ7FGlK46jbSBfWO8un53qdx75w7cKl/co6a31lqzzLszxzwXnvffDeBwnh8rXd3/id/2fzymMnFycN2fz1//P3fv03Pz6eTIhAxMxMxMTMxMQsgIj4EHxwwbsQnAshBKdHwAkAwO489Ld33Xb34Z07RqPt/Stf9wdXFOx+Zqcv7K4stEy7U3mDmJJmp9HsUtvt+spqZIODtCzQbLp2nCtuxIpJsqkQYBRlXlXdlmvLfDdtJe171lcjKXF4iHYDSbx4bPG97/6Oj/zBR5wXgp/pebxHjVoEIhLAJKDgQSAirVVelrFWReWisowi02p63UzhgCCsNZSGUvD+FiFkfmml3UgVJMsySAG6TRKrquvxf/wT3/+Lv/JrX/rSMwghyydFNi6LCZN/5OEHQK/mpt+MmTkszgEZYF/d72/fIjS/g5qbwCZ8DmoClO1c//Rnnn3iyevOB2atlC3KUFaV884757zz3tf1PQlNM/tbH/rsh//gMyeOLW7t9vuDCROBmIiIZgyziITggwgkBJnVPYIgAvGifuqDH+wCzwFXBrgnwZkWzq7q1qnemfvPnTz1UJ5l/YODUI5H/X4+HsdxpBT1J1VZFpVScSdd6rWiOCqyzHrXjkwMeBsaimMNG0BAFeBZR0kMlZxZWXrwWC81KlbKsIJWYNw533vy0rXDgwOeeYUIbupYiIhQCB51tcUEgmbFirVirXVkdKSN0Rymu8Ql0hWJ1ykEmOQmmse+pDZS/au9JNWKra3W3/ydtz1h9SDT9vLpR+4+/bFP/Mnh/lZZTq0tBL7bavzo3/mhtdN3/VW9oUS+C7bgG/HPAOEbBMerlJuvbjdzcrsAAwnYYTS9/MxzH/uTrzz2xWtFaSXABZdl+Xg8KsrMOe+8Dd6H4I9cJ4QQGOwDHfbzsnIKBCaCAlEN24KIeCcSQgg+eBERCYIw49FE1A9/8IMeaAF3JkgBBSTAGrDGaLX1uXvuWDz74PbG7oUr215pC5UVrqiqpqZ2U2tFzcTExgRS/XEWbNlmiooqNRwb3UNoj8uUlEvjdpLev758vKkTLZFSsdap0aQjKOZWOtdofeXJp71zECGiWbE2I8JCEKnfrxsZ9fXpuhgg0prjOIqgi3ISqRzNJVp4GLoRilE+3jNpCuijRvU3bN6PqHLe2dJVKw996zczeQGIATTmlx45d+KzX/ySrUoikMj66uLf/cG/lXQXX3OIVzEN04CdQnKoG5WZAjSggFtj1ZecYe1hN4dzi+LZ0eVnNi5eevb8xccev/L8pbyqQhCx3uZZNp6My6rwwXvna0eZHS4gYq21MoZZEdXQkkSoBv4QBJHgQ+1kdV8TMw+rT4AAUf/2gx/sAClweMQAOoCAz17cuTbwIU2Cic7edd8dp45554LNE+UVgmaQeJYgwi6Ewbj0VVCMlMUGJiIPmhJzGqtW0k2TY+tnFrptP9xlIs2sjTZKJVrBaDCtNJO98fT6xmYdbIkZ4gGqeY0abALEABEUK8WstGLFRivN2mhW2hAnVzaus2ohXTBpQrprUoNQgswrkE9NUod9xSjLfP6+b/lmvOEbkze3tnjXytxffO7xg8Gocu7ec3d84Af/NvivSnQBAEM3wQ7TfUTyzbSkXjbOSxsMfag8H4y3tg6fvXB48arLCl8URV7mZVFZV1W28s754IN4EVCto66LL1bELHXB5Zz31nvng5MgIj4IJATAiwiIAMiMUwoCMBOTBin96Se//tzV/d3rl184/3xEQbFMxtOyKFxVOScmicnEzXa71W2tLM13G+2tvSwhl4vo4AFntRllYbEMJZRqN53N2taW3YbXzFBIdCONolYvinB47dmUKTF6FMVpPIyVio1OlEIjQjP90b/xAUvRF/7iU0E8BxEQQwJIMUEkBHHOVQQCaWUjrUvrosoWlY/LcpJHWueNRvPZrfnLSN775mU7GZqWAbrgl0aymel4/3CQGBB5HDyPhdtPdjcGDAjjh99078/9zH/z87/0b5594fI73v7tUP9flO3UQauW0JV17Lw9KwELtI7c60ZUq8+2kIO+tb6wZnOPJpktS+u9h7BzRVHk1lnrrPM+hABICBK898GHIN476613zjnrvZMQgrg64M26mQDdCArERAIwsSICs2FmEdI//9/+DyaKAOK64TnLT/XCALFTB2R2cDi4TtcAHUetxYUoQqyx0x/khW3N9UxenY2jF9JorplGWZhScEQsNNeOI2+LwaAYHBZXq0ZsqNHItIqiPI1MrKMojhaUiriNNOKG+aHv/97tzevXLj4fgJpaDhAKNa8WEOB9cBwq5yvndFkZpY0uDJM2xigTmejt9539s+c3Ln3tcYCK6mnFappnSlE+nQ76u8NBPyumTkKz1VxuLdHm3pkTa4o1plMs3L4X3PBai9KC44feeP8//ckf/9/+/f81zbMwHLEu0Hx573yMMke88DKnr45ibXiltHgLJ3vJ81NLVOLZic00bSVAgAUIh1evX9u6cv3wyfP93f3MByilJEjlcuucdc65yjlnnRPxIQTrnLd2BjydC+KC9wG1K3kSEgghQBgMFgaJQBRIiKlGoaxIsWZNREGg7rjjbqUUcKMtWEe9+tC6WUUgMBMRgvPleOKKioMTkWanPS1cOsgVcTnXPN00kYp1pzXJi1N33aNMfHDhyWoyCGXBIgQc0SxKK6W0ZqWM4oZiABAX9Xpvffu3f/7zj+XTad0mwA3aFgCImBjEREqxImYiQJiImZXWWuu5drMb6WefOb+8uPTlz//Z01967PxXv5iN++PDnfGwX0zHZZVXZSEBm5e3Nq5em2u1CNRdW9MLJ17LvW72jS2oBoo95CXaC3bUZ6aHH3wgipvNRuv6tWuXnnli/ey5m4/YP/9so7WM0WTv6qVmbx58w6UUAOSjpz73icneVT/a03aoYr6pPrthguIg398zrZqce4lT1ljBAjkwAfrAASZ99HdxuItuD2nb+OILX7r27KWhtQGAd34ynYwmozzPyqp0VWmd885WVVWWRVWVtiqtrayrgncheJG6hKkFGEJgARMpnsUnJiJirdgYbXQUKRVprZk1M0kQHUIIIoQQArMiBIADAI/AdRUIIUIIqCcWoKqobGmhVcSBrJ9qztvJYqdhU60akpd2pwyLZSU7l4P3EoS9qyxrpkLrSJuyKLI4iibTOImacRQr1RKPSKPaSM++/bv/2l/70K//qq8qEAUvoMBAoHpChEFMvqqsZqW4IiKllDKF1iaKTGMan1xbbLfb7bX15aW1/e1tV9kkSuIkCsEXSnNV5ra4/76H21HvEx/68OXtnUip3l2Hx2dp89YkQh17higz8AGyAu0FEFmHqnL33nPuYBRY6bm5lTh5aV21uHoMrRZaraXFm1HCJrAAxEg7cwsnKmsX734IdP7px/9ycGAVayI0my1WJorileW11rGT6eorgowKuIwaxUmJfobxBMPxcDgcDvukceLkOjB48utbl65OQ2BidmU1moymk0lZFWVVOmtrYtY565y11oWaAgtBgg+CG9CMCDQLWgCIwUcxSDHXlZxSTFQziCQSxPsQgtcheOecYiISBALXq+lAAYFAADFTTTPUGIYAcC3/dqMyIpheqzvXSBIz8tQO9uDaRpzMm8lhOekbEzlnXRByriQwFUapyOjIGM1sIpNoEylmCY1GhDjg4l8ua3rkkbd98QufF1/JETImkkBEXhx7sqKYFFsmEJOplCrKxERlUWV5Ho1Hc/MLIDm2evzZ809SkDRtNpJIIGnSKMoCk+F999zbO37HaG9/6/xTk7JoL589mrBbAzoFAJOJG+cYFzptQSdwZaMzbw77Sptet5W0uhBfZqOXHpq8IlV7DABwHTi+fv+9YXIA4u3dS5NxeubMuWaaeme73XlutRC9OrZ48s/w7OPotvDgt6CyOOhv7GyPJ6OidBK8UmxMhP71/mH255+7uH84mWST6WSaF1Pn/Q3H8v6Il/XOOReCD+J9cBKCCIAwo9FYAUKkmGoqk+sEyaRqmraOapgxUkFCXeAF752WGjAIM4KAJNT4TtUOWzMoBAIxakAhQF3HQUCkRcgGN6nGZWi3k+FguLE7/pl/8F6XDx/L9uvz0awAACAASURBVCdZVuSor6SqWdacY22m2iitzDRrJnFilCJow5FiJMmD95978Nu+K4rTz376T0F1rK17AkIcgifPwTlfoFKKqCKllNGqtLYoq+FkYkMI3rV9yEcHoayiOJmfX00jCuLqToiJ4qtXLvdOvOXuM6cPLjyrg2+1moCDn0DVS49uyCTrmunGAioFAK013WiFvW20F0ExtAOHKI45aSa6iwiAis3LZBrxLZDjcWALaHGr9eRz/+4P/tPG8eUTC0l37e3fenQOU/gMqk6XdVnmgCEOdzHsD577+tbzz4+E+Nq+kKqqSiRoEwmIQN773A43fv+x53anG1vDqqoIbIxxPglSVJWtbGWryjrrfR3IqhDqSFavvhQc5URmAvSsuFeKiVkxgVkxg+QbhKevXSuEEIKvW9WAaJCgrsiAEDwIzFx7Y90bFYEgHOkjAQAkNUdHtV5SpJpU4MpW9sq1nR//3nd97w+9D2VeFOXTz1zoC/I8eIHzgcQWirOi0Foro40pJlkeR1prFRmllWYf0BAk/of/4X+9u7Pz3PmvOhs8AgVhBoIieAJb5wkoK2agVKowuqxcVuR5VfFoNBqPV8tyPtJzc4s06HfanTTWIg4QY6Kl5dXpNMP08mg6OhyN01ZTJQRYqCZggPLIzwZAAFoAA30gBRKgAiqM+yANrVHlyIbWBu/di8R/Lwe4tkJ8i+7TGnAZ+KP//ec/3YoW3v+me+5oCS4+Zoejg8Hhzs5OI02OH1tL4phAIJTTyWA4HE+z/cFwtLVVbe8NnNW57c0vJklqTFw5V3uQdX5U0t6W2+qXAiFiH5zz3tpymk+LLC+rzDnvXOWd96Gq49BsMRwRSZ0PFSvNNb2hVf0zazfVbiM1O+tCCN77mtpFCKAAUM2naSYFwIdAEljpWfkPBAlU51CiOrDVzW1SFLwAgaiGGkQidVE+zd3S0rGH7z0LrWCaZ06eKIvi0pWNgxAKFM4550NeOa1LVlpHphHHWZankWlEcZmG1IfIepQWgx30Vv7eD//Iz/3C9eHBrvdBABJ4CRAhISKvPFnrmVlZV1Z2mhf1BRdlmcaDyXS6urR0fG0tz/MkiZtpwgSwtJrtxupxtFbKaxeeePxLu/v7b7jzDFwOFEfsYQwI/A7KHI21I/F+heDBJmw/x1E0GUzYpA0JdavFRAkQYNJvQKmXm4RX/2z27P6Tf/qxwz2+825tyP/hH390NB0dDIej8URC6PV6a8vLjTTRSmdFlk2nEiRAyrJ0ZWWmZZ5NddxQcSPLS++DD857V5R26mi/iPenYZJnRZ5XtiqrqqqqsiqrsnDeurr96J1IIGIJIgCTCGkmYtZKK60irZVSRtUQDAwmEsyoj+C8rZvlXsSF+rYclXRHfG/QAYEDhZpcoxCIGCBmJvIhMOoeEInUIjAOPqBGDYTAII+gmCVAAGYR/OrvfWZ7f/Cedz4YiI4tL6VJfP65F/b3DzKQd9Y5V5SVVqosojKxRVVV1pXWiRArDSGUFTgH7fTWu9/znd/xO7/3u7PWhxAjBJATD0eKiCwRk9bKVHbKuRBCwGgyLWMdfPDB9xZWu525NG12Oi3FUFrrVhutBSCK0+b1K9fTTutb3vkOGAYMUCHfgY7gK5QFjAYmcAHVGFXlC2vdhiszmUiWu6XVORQVlCbFaHdazRaS+EWQ/SWV3suQwUvs4x//D08+frjUnf+B7/pOlxVXNraevnr9hZ3DrKgSw8cXujsHw2YjiRQTxNrKOlejbxEfB7iqwnBcCQjkgw/BV5V1HE/RGzsEIIlShnJh5Ny0KHJrS+ddLbgSCUIQIQkBALFSrDQrbYxSJooirU2tJwMgBAninXPBWmedtc5V3nsRLyHgKOfJUe4jMDMEWldF6bXS2milgghCALGq624RL8JMIszwnpg5QIgYdRSU+jH1CARihg9MGE7LD338S3/++HOn17qnV9uLC/P33c3ngd39g1y8OF9WldFcFmWWZ3FssqJqW1dUzgVoECoLYhiNMHn3o2+5dOHZL3z1q1SfmYAg5MUJAU4AVEJEDHYiAup0eseWG5FWElxZWnHF6tJip91pzM2BBBC0uzMpVactkfnAD/yN3unTiBpwY5QlKltM9iKt2BikMXwFW4AVXJhm+WQ8arfblWdSzK0uvIX3CAEs2sT1TZ3ZK6yDuZXybPjch144741OT650FtvpVy5e2tofnN84dKTi5lwgunRQXTu83o55sZt206SRJo0osr6a5hkrAnGs9KA/QJourczPzbWXVhZM3Hju8uTJi31xhXOusjbPsprC8M56CUQgoVrfJ+KDEBOxiSJlojgyURTpWGmtlWZmEIIPPjhX2cpVtiorWwbnnPcCJ0J0kzaQBGGm3VLMpLVyPqjj66dMjfmoTklH7esgQTzAMyh7JJ+ooYBAjjqQBJKbU0a978skq7YOxgf9PDbUSJNGpATI88I5CxEIkSJFSik2Nc1qojSO0jhBEoMYjSYaTczNvXFx4XNPfC3PC0jAUR+q/s8h1IqA+jWrKFpaWDyzvr4812s2UmJqxnGn1WgvHYsWFtBsodGASma8qEpPrfWOv/FhqAbA4CZcBmN0p0PtNpqLcCWMhomgdRiOijIfjSd56fqjaavVas4vwftqkjuf69aK1hrm1TlVX9x6A4Rk4b5H3vZuO86/+vWnnrv4/ONfP//Y81eqQFGctpvtbneu0+6mzU7h1W5/FCuab7caSSJMvaX1ux5667e+5wMnTqxJyH/8H/7YW7/vffe+7R0nH7hHufCpz1+8fG1rMB5OJuPxaDgtJmVeVrYMIdSCPh+8907qFUBxkjba7Uar3e40m51Ws53EqYkMsxIEW1VFmWf5NMvGRZ6V5dTaynkvwYkEkRAk1OKampUggIi00krr4ENRlFqbSGsVROBmhRsT13rWGeIMEHhihtRanaP2FUBCxAHgunarse4MAwPey85gevhEudwz59baSytrlfV7e/tFnlXOZnmpeWqMTqJps5HmRTHJylbDmjRFI4V1EAJFfO+5v/nd7/2Pv/27tgohhHCkggwIIbAEcQJRimOt4hZUMi6dc9Rrt5pJArhGrFSwMBFUctSQntnqg2884mpaANCo6zMPxADBGHiPILCW46YfZ1leGC3zcwuJ0WCGrYiJxAC4ZY0PDIeYf+1O5Zsevn+0c+WTn/3swWjqSSmlmKjWeSZpmqbRyvJyXhwrJ/2RDQ88+KZ3fPt3L9/7ILxAEfDmN7/vEfQ6QAtwG08892u/9ZmLV/diE5sospUb07iaWB88ABCFAGurIEFrbUyUJM00SaM4ibRmpQGG+MpZW1ZFkZdVUZVFaUvvK+8DgpcaikrdFwAJAhFJAFONDohZKc2Adc5WlQ1OnTh5uhauElGt/pqtIK6rNKYaXtaMbc2eBQkzBoVvFHsEoRlsnSle6zHE+TAu/M6gyMuw0Gsnkcry0tkqoK4JRbHSig1xHEdJEieNBpIYRoMYLND62OLCtReu7O7vH0lrQxAJIs6HyocgxCaJ0laSJKw0AM3USdN2u4Fadqt1NLeEqAkkL66bIiC+qcXeAFKgQpVBKRChqlCUQIKkRT446xYXl1vNlncuNlE+zUwU62YbJsUtN+koD3Z0Z/41/Wy4s9+l/L619QuXL5cuKK1wVO/UenutdZKk3bmFuZXl/+qnf6q5dBoAZmqqHKmAYqA8eObib/z+Fzd3siSJjYmstePJaDKdFEXhvQ0BIbgQgtZRq9ma6y3MzS32ur1ms53ECSkVvC/LYjKdDEf90XgwHg+yfFpVWd2FEvGzbFIr6cEkJLN+Jc9qO62NMiJSeecqD3gRUuvrp7VSUneqCBKCAEopZgaC90JMdfeTiGS2SO9oDVUIMzcLMuNHbshJBDzj2kAgF8I094VDp93WHIqisNZKCL4ewQdmTuI4TdNOEiOOoAwgcBYS0Gzd0259/mtPVVUpEoIXL/AhWB+cFy+wPpRlMZ1MSmsVITEmiXQ7bTbSJHjriiLiWC2sv6xIurESnYASyIApyhyVD6M+lQWCgpjtza18MpYQ4iSNjJ71f13I8kxrrYiQvEbvvDzci3qvLRY62N623jajSMS9+c4z03F2MBlDECQ4751zAknjOE7M+//W/Wtrj7y4DCyBEcB2c/v3/ujLz17cyfJ8NBqPxv3RaDzNp7YqQaSVjqOokTbnevOLC0vzc4vtdjeJEyJ23k2zyXA0HAwPBsOD4XB/Oh0VxdS6Kng7e7SBmrOtHaBWadftQGJiVlopYzQTuxCcrXzwdR4VCbqqSiLWWgWIOK+YtdEAnKsA0srUJVCdJUEgUIAQfJAafwbU6cczKxKCeDCDiAICSa0Ul+ABluGkmpa+HbXavTAZHVRlmRcFgxhI4qQzGnc64yiKlpjR8khiMOqWeuvcne979J0f/pNPFEUQCs674CUECQTvnc3DJJsaFTnrVfDknIaLomh5ruMDO5sNty8vnj6LaOlFE5v3hztbJooaSSqQMs+KqiSBUjzJCq10mjbTRnNpYW48GVVlzopJpYo5jaOiDCGEPM8E8pqCipoif01TrC2rEw8+/P4z92bXnhn3B8MyL0XlRV4WmUhg5gHT2947/8Y3nXlZi93Dl8jGn/rs+SfOb1jroyhiImQQUXEcKaW1NjVjz8QAXAi2qrJsmuVZVmR5Pi2LvKxK723wblabYDa3hFkH/KjjNBMM1Yo0CBGBiJSCCHkfrHMyo2UBgEDq+PpJJtR7ONY9bu+d945nawpQR++jgvuor153ucMRPAC4Ts5Es1UjhBkkqHv5xDV+CEEKRx5x2kgVvC1zHwKTMkYpxVoZFak4iuNI12o5iMB7aD6zsnzlyvXtvT1nvXMhiBCRD0E8fPDBg0QQPInEhpkYRJExDIACvG2woZc0y6l004mE4J0tyxJAUVTa6LqC0EqL+LIstAqJ0WmjkcYRE4o8rwVXpS21jpQ2ut26NZwMk8Ht5M3p4eHB4W4jbS6srs2vn+2tHHv00Xd9x3ved/mFywf9g+C9QO56sPn+71vTuorMS/YI2sfB9l9+9tlPfPqZ8bSsqtJaC+I4jhvNVhKnkYmY2QepbDWdjvvD4cHhzu7ezu7e1v7B7nB4MJkMiyKrbBlmyp/ZrgVHWrSjTjmYWbHSqhYAMhNRrW1m5lBraoKjWfkOAERBBGp15TgrYlJA8NZaW9WpFrO9LElCoHqFOGaJWIKfVWGzM5iRxzMvFNRLRenoaThqN8zeEBLvUYkxcUNxsFVRX1e9jC64UNnSFiVZG0uAtfABwSOJz3Y7X/z6M9MsQ70lB5EGmIipfhzAEGNUrBUz18RjZCIJjhCqomiuLUHftAiKSdmihrBxlDDrdrcdJ41YqzSJ016bXJVExjQaXAsRFOfTafCu0Wiw0j6I9957m86t3not023mzWIw3tq51mg0k6TRaLZP3HHX6p13rZ1af887HwX0xUsXGh35sb/3poXOsen4uW53CtzzjYOH1z72J5//1F9e7I+mEhAgZVGMJ5PhaDAYHB4eHu4e7O7sbu/sbm7tbO7sbe/ubfUP98aTYT7zLRs8hEKdsoBaVDqT1zDV4hqjtNYqOlo5Vy8OADGYiEi5mRLXHS3CDTcoCi9era/feMoJikjgg6uJWVfTxFK30rn2GvGzRMk3HIj4aD8FIXxD8DsTWM4C6KxZdqNk8yHYQIEbzPBVDoS6TevrjAjxzjsXJDhtLTkH4kavkxK+/vylIIGZNEFrFem62UZakWHWiuqXMwdnIggTQrDa+mj11M0CMs7HWmnTadfCXDRisBAzhQAJ2kScxNAK9W8gYk7iOPigjTHaTLOMmBvzi98YM3PwAv0iWFD196K5F6fsVzI/zTc3r8ZJkkSJiSIBtFLQSjeTN771zW956C1rJ+Q73/2Trfbbu933AheBx4C76ypt74Xzf/jxL27tjbzzzruqqoqqGE9Go9GgPzjsDw8H/f3haDCZDLN8WlWFdw71QhLMlBegWeOSiJm1VkZrrbWJTBzFSWRiE8eRjo0xWpsaHtYlu1YKpJxz3nsXwlHJXseV2epIBKjVlXWlapmvQEBKK+b6SQ3OM2tiqlck+OBJwKxupEIcVXk3SLUgN+pEQMAzJHJD0Ss3QOvs+2DhlNiILcS7I+kJKcUk5MV7EAAWUSEghPX53s5hf3t3v5Y+1asENJPSyiiOI0NHPk4Acb11BykixeKtbc/PIe0ehR+PKKC1BLMANYQWVPnmhYv7+33NBgIloPllmC50gnpikgaaTW610GhwM21GsS3KpNcBHYFWZkQvxp5F5rKJ6b22kNK4cO365ThJoihVihFAEG2iGlHOry7efe87buqhngNWgI8AClj56Ec+8cTTl/Iss95Xtprm0yzLyrIoq6qy1tkZo8GsldLaxHGUGJ0orRUzkVJaG22MiY1JoihO4jRK0jRO0rgRJ2kSp3GUGK2VUiAmBAmBCEopoyNi5V04WoTncDS9M7BMM/pBz3jV+kfgfRVQ9+EVAFdV1sEoQ8LMBOba2xSrWt1LECISLwJPMyViqBtQgAQBvDAzUyCeuaf4oBTXdZ4IAiC6DY6m9gCjMbPSzForIpLaKYMECYlzkWbN/L53vu3K9a39g4P6aglgTcx1Z0wJxDqX5UW9OEpRIBKWIBITT0aXn+/Mrc5aAgcb169emut1ijJ77sKlPC/LqhqOszhKdBwbZbwPb33kDfPdBZXEz3/9vLAqrC3LjKBMHCdRBIK1YfdwfNcjRytZXp4/82ma3tbOKypJmNn74L0LLnjtyjwnQtRu19H0ZbYK/Cjwm8ClK1svtBqNyMRFWQQJWuk0SUPoee+stbUL1CnHe1e3umtZmJdAR0uS6nRD9eNJs9Krft87531wzgXxkBBFkdKaSVXOBmslSL1PENd0tIR6TxQiEiGBsHgtdUeH6Ma3wXJEz6Le/tG6ikBKG++DUkSkRBxTvYZPzXYnkKCIoUCEuh0rJPCgOgtRHdtmexeFo30MauJJRCxFEq+Q7fNoqOhIUxmAetGweBdFhtFKk2ML8+99x1s+/J8/ZYsCJCTEDCYCM/5fyt7019bsOO+rqjW80x7PcMfue3ticxJFihQl2kkEOYYHIAH8JUAQJP9egjgfEiAJ4iAO5MCwZUcDLYk0xWbP3Xc689l7v+Naq6ryYb3ntkSbErM/XOA20Oece/ba76p66vc8BUizBULGELu+t8Y4awyhMWit2Z09W3VX0NQAwDFcXF0P43h2eT4OgbLHFeBwaGkY224khH/2f13nEfLLs7P1apXSZJCqurau7PrRe4+Ibz5562twN9MkAAbQrzSHNE128euZBpwrfCEsIYyRK8sOLQ3DoJyK7TGYX1UC/tfnL/7Z2cvr3X6KzG3bJmZjqPTlYtF4V5AhgyaXz8w8jlM/dMPQJ04ir6f78ynQuYlXFlBJzJI4pRQ5RVUmotJ7azwQcYp932elI1+QxlrQjPwYmAv614Iq2MyXZf4HERAVFVVZEUAx32L5/+AUAVHVUH5vjRIYuAtfyUBSfo9BUQGIiDUZsECid0JKLvVQ5nZZmTPSpgpCpG4L6UC7A9wluNzBeDEUReEdAnhrfvDNrz0/u/y3f/bnKaX8VM3DMREhIpo/nDqFOE5jP5ZlUXhrrDW2a8fPPiq/fR/A3+5u69L345hVZSKsynqz3sQkr16d7/e3y7pan56s1qsYUgqTqJRV2TSLk+PT85sdDoMhPLTt1dUNCECOt8qN1l9hcmMMtvj14gs8ee+yUJVSjDHUdTOMYT8NS8RysYTiP0o7InffCeF/V5UU0+Xl5c3uioUL7zer7Wq9WS7XVVF57xEwphRjGIf+dnfTdvsY46xJzODEXFDN5ksQEQYFIrDela4iY0R0zNdxGBHRF6UmDilkFFJZkGhWJxDhNZwBapkTkrubeREhCoqiUg7dUlBQc8f+gAJzYlEg8r5QFBAxhohshnQVFOdhO4owKCZgo5jzPIgQVY0BFiX8K6dPAQGSsqplWkjqYXdgEc02J44hLpqqrKqKU2rqsiT6ve//xtn11aefP2ONAJhl4Vyfsgqp0Rm6034cvXM2jx3InH352dNv/ybA8TgOMaXb25uyKKrNGgBENHLy1h0fbZ0xm82mahoi08PknUscHz16tFwsb3btfncLgPvD7sXLcyAHfQDv50b2r9NBMcXK/LqGckOGDBCZrADFFArvUsKry/P46tnR9mi13kDz1yNFFa6vLoahCyGsV5uiKD//wp5fng99D4BJeBxH7wpf+MKX1loWdt4tF0tCyOaAGCZRhtmEAbmcBSRjwJEz3lZlY4xnlr4fpjAwC4CSMc5aBJg4zUq9ABAocC6ZAOaJFKgAqM32znwf57peVFBRacaIQFEIAVAE5wIEEUGncSBjrPVElDghKpKxlC9OEM3SsSAjZN8BgqoBRGFGMgIRAFWynwnySVaJaqjDEiLI/qAKnMlMlhRTSMypYOHJUlUW//BHv/0/98PFxYWyKMJc8M1d7QyEJkkx8hjGYfLOBWvM7uYGPv0U3t4QofP29PgYCcIUjbPTOBkx6GzJJaxUEB4+uL/ftzfX1288frDdbOum+vCTZx9+8omqOufatifC/f623d0sHtwHyDsnIvjXB0uF+W409Le/rHWAZJ1LMXpnr6+uqqqs61pF6rJi5nHoyl86Z7ubsb/NEiCa/b3jB/n9ubq5mqZRVG5vb1iSs64oykWzVMCs1COoNaYoigwaCXAun4mAiLx3J6vFolnsBybrOGmIIyB6XwIAMxvrnLUxJmedc34OSVBOLIAiwLP2qfNs3bIKihCpSEZnBBEFkWajLqFyVvgz/5a7iWxLAdAYhpSQyFljCDCpolDuRGefQcaLAOd7LacezhWcIoEmIMS5KSBkYUN0IAepwLbN1ZaCgmhSQRDmNDlbendytP2Hf/eH/+sf/Ku2PShLlk/wNUmiAmgBQITHKVkzWEuGSJE++cXP33nzyThNAMY4E6bJGAOqzjmVsO96FEkp1WW53++7vvfOfvHsxdn1NSd8df6yLGtCM4XJeb+xtir9MLQLvQ8AICBhotcXZ5i+gpB/rXNmWcQgCWgI2RhiVWSz2pLF+uj4dS/31UuZ+ECEnNLV1SUhHR+dppiQzOXVxaE/aAqJY+KIQFVVOeu7oQsxEqI1zlq6S8/MvwzTNP6dtx69+fC0JH921fevbnIIgDHGgc9uEiJ01ubihIxlZsjM552DRBUFGFRAFVAMoDk+PjXGZKEUXl9jd/ANvq6/Xr/foHea62vhBYUlccjNCsxReYoEhizMlTxAHojmKdlMwonkYfp8Pu4YJlEAjGosMEiQOxgV80ESRSRVZeXteln44tnZeY7GzbWkQUMGrZnj3uZPRhYAiSwRgB4tNjftITHHkETFe5fnGL4ovS/GYdis1867m5t917YxxTBNt/v27NWrRVM3dX3v9Mg5bwwxp1VdPHr8dH10HxBhSimMpsnqg8AwDIdddfy3RiHPr/2rlwronCO0qpxlQFUuihJVSISYf9lqcPGl7M7+/IMvrvbtOI5te1CAzXbTVAtjKIbU9S0gIJokPExjStESGWPnAbVqyr4moMcPtu+9/egH3//Gf/qj77795KEBenXRXu1aEc4JGmGaxjDGMFnrmCVM0zB2fd+GqQ8xsERJzMrZHAAiMF8yhEjm+Oj0r5aACLOcC3PsC8NXaWQgyrnKR52FkNcTLFVlYeGESNmSDKo5diVLdyJ6h3/LHcwB2dA0T5hEmEVzakMGpNBbmCBFvTvQAJotNgC5h8CTzQoQz69uXgsuZNBZa8gYZ2zu0fEOLwFw1hBCH5gKzywKsmpqEb7d70Xx6Og4pTiFsNkcXV5d3t7cIqi1ZtHUVVE0TXP//v3VYjWFICpn5+dh6OumWq+P77/xNgBCYpBEdTn/UobusLtuTh9ClF/ZMGb1EQAArl48L5zLgxhVIMSUwjAMHCcFUE6FL8D52f7Zt/D5R1/+5b9rd7efvbp5eXmT34x+6Luuc96uV+vj7dFysQagxImIQDWJhDjGFHNfaYicsWVZNlX9G998+z/90Q+ePnm0WS26tieAs4vDy+u9SmLJxL+kxKoyjv0wDDEMiVPiOIUQ4sQpCyhJ5xyX+UJExCcPj6xKSoyGEDKsipIVf8qcD+H8OFEQ4PxmYcpqWlQgxbkdzSMoAAhhDArGWu+KxHw3xkAEkJwwCZiB/9yj6Lw4I4cCIYASkqoS0YjYYkV60LbHfFRFEckYo6riDCI5Z37wzffHKfzk5x9yjHdDAAIEuktOUkRmmWI0hvohODddvnrxaLNcLxtR3O9349hfXt2enJxcXl2FyH0/yiYUvjCI1pqUWAGstU4lJlHg5y9egsqiropVY4zt+hZiBO9B5atijBOklFIClr9pLsUMwGAdAAxDb5dLZ0zihIDW2hTjNA7OGhtjVRackokTYAmXr85++uPPP/5g6A9f//p7j0+3P/7IEJP1VkTarm27tq6a5XJ5/9790+PTtm/3h33bHvqhH8Z+ilMMQSTFlIJyTAFRvHerRQ0AV9eHvhtXVbGoPCiEyIYIEb0vkHAYgFmm0HNKiGKcJXRTGEU4ccIIZIDIGUQwCoD3T1Z//4ffzfUZJwEkAs2SleIstGYRK+ttZACVkEQUDYkyAua4lTtx1iDOtyJqihOn5Lw3xoBm7ZZytDaLGEIVEGEFMIh6l3aGoECoKpxvdoiDLSssMY5tOxcAMyKwaFSdJLbWVHXx29/+xhDiR598qsz5lneIuachIM43A6IxNE6jG41T8+LZy3rVLBarrh93+/2D+/cfPXwMBHEK0zRdXd9UdfUb3/nOze3ugw9/EWJkFhUVgJPjE+bgjbMEU4iN991hDykCmTSO1t2dqRg5RSKaR3S/6rW7gbrO52wa+8LbqlrEFBAMIimoH8QFvgAAIABJREFUNXYaRxV2znJKK0gwXT776Y+fffEZWfu973zLWosSnXOgwCoIWJYViIpy23YpRe/Kpq7rskpHxyGGME1TmKYwxRhCCClFkbRo/LKpjVFrTQxZGzXbZWkJe2ZO0TqPiM5aLSvrrHM+pDiNA6fJWmyqZoqBOaowi6Q4GEMWfFVWv/2t9x7eO7HZcTdbTTLdDUTAkmN7EigiKQBqAiRFJSQAptdPMVQmIAXO/1EBFdVkUiTGkCL6oshgiWbzO6gyKikIIAJnEJcgK6UgIrlpUGaAmNJgioLiFAP0s5dPWAAgFIUzaAiGENbL+ke/+e1xnJ6/fIlzRhKyCDAgSVZoFBUntMaY0TpBOLRUlKJtUfiqap69eBViIkJmeP7ipQg/fvTIusF6772bwoSIiRMiXlyeeVcQaEicK0KRkKbJZsna3BE7cYohlGX9N6fSHm4ul8ffvDuZ0ziOa1VnHZEJIaiwsdYQcpK+75w1VeFxiss33/nNt96rx5ux29/srkhFmPPYO0EqrSVjVEBBmDXoxGytJWudyRyONd55lsTMiPro/uob7z1989Hpatks6vq9772TRLqu266effDl7s9//mFIUVTGcRymnox11lvrSiqcs8INcwIQ62yIIcZglJltShNDvH/y4J03HoGoZRY0Ckq5NAPCXIYhIGcmRIXnFhQVKEfmk86nTIEQRRQRGIVmrBLznHKmOMahN8YZawGYAJEMkELGJbMrAQARRURUcBZwM1SizKYL5t7RUqY2cuy6DhSQ0BojIslZQziGyMyrRfODb389xnR5eQmaCW8CZjGEONsBE6UpRGejAPlpTCmlOJ0cvVl6n1m/l8/OvfcPHzxYLpbHp/cWTWWMG4f+Zrfb7/YHbcM0xRSHfmzqyll3tF0DYtv3MUWcphQnVxUAAIkhpSRMf9s+vJTi63GVsKQ4xRiccykJSwIFAAHN2Ck454GMfefdNYB+8ovP/v1HN/trns1KHCM77wAhpQQZB0UlYxHAWDXGElIfxrZtM6bBKSVhQ/DeWyf/5B/9vfffeTelaCyh9cAJAO6fPnx+Pv3isy9jl/phGMcupDiGgzA7b5tq4V2ZkQ5ODABudjOJpJScPVqvfu/7v1FX1ZTYrJdrQMqulzwimOF7gKzS3xny9G6OoHezyzsbSMbKMnT2etgA8xMyl0kxTCzJkMucCKEhNIpzTzC7keWuG9Wv+pE8cfvWN9579+2nt9dXU4wirMIKZCwhzCP6EJOC1kVx7/j44mY3hbz4LbfMaCwhmtdlZFIlJGusqxa+9G3bdf2wXC6y+Lff3T588OCNx4+Lqtquj8qqXC2Xxtr1elVYByAnR0ePH9w7PtouFw0RhphC4nfe+joRjeNYHh2BIUgCYei7FomK9THAr0SH7DiY1exf//KDvySDdVUXZZ1/0ZwSMxtjRNlZt1yunbVkCC7O/vj/+T/+zZ/8EZJuN5ur/fjBl+chRVGVxG3fdd1hCmPKsYwAuVDp+vbq6vLy+ny3v+36Q993w9iNw3h5c7s7HL79tafr42NEA8KAJMqEuFnVnz97+fLiOrGO4xjjZIisdRxlGKcpDCo8TdM4jTFOMaWYeJzGmMT74v133/vN997yrhpjtKwMMnNpgPN2EETMxGzmf3LoGqOgSI5UyJYlEUXMpRRZAmVGIMgBCgQkBlFZU87LBYVp6p0vnTFZqMsXKQCIpvxdDFESydP13CWIqjXm5hD+i3/w+9vN6sc//qPD7eHQ98Iqypvlqq5KQEuA/TghwKZpfvRb3/lXf/pn/aHNMFxi0RCtAWNQQSfUpEBo/Nib29tuKoZhSDEq4jQOy6Y5Oj65vtkJmKauVKFpmvVqfbO7vb2+RsLlogHAmJhjbLt+GEOMqevH3WFvjWNO88w7TsCSUkJNIH/TxinXfDX9zHF2UxhXtFVjnVNr7H5/G+NEZBQghNBUPl1d/Zt//r/9xZ//ya7df/29tzTpzc0NzAs9sr0yTOPIkgDBGee874eycIVwGseeJc1sDiGBJYRxSh98+MmHn3waorT9kIStsczRkBXVb73/9l988EkmEfcM3XCrKkSWELOZgMgYY+a8WjJlUZVlsd1uifx+EEeRRaywqKQ8txaUjCxmchKy74nuDk5+YmnGeQyKAM5Dg0xDkhEWIAVEJJCkkq1/mG9YJTImxYiAzpjXCnLm8ii7RvMXnIFOye4GFv302cvnz589eePRG4//yRfPz/7wX/5BPw1ym5UdZS2cMWhomKJ36cHJ8d/9re/+4Y//bOz6bMdRgSABmSyREUNGAZCMaRbDzTBYS2RMCGG5aNarzXa9cUVZVfVmvTZkRPGnP//Fxx/9/Pz8su0Ozrl5lYpqjCyqhDhM6fr6clHWMcZ5+jQOLJxiLIrib0mHKb+iOQpfhtilEMZp9L4gJAYmQ5acgnBKfd/WtR/a/qNPPr5p+6rwL84vfnr14dl+yAyqpoRIVdUYMuM4DFOfQuiG1qCxzi2a5dHR8VaPQ5imaQopCLOqWGvqqlSg69ubX3z0mZLWVX19u9sf2uWiOXQtSCqcceuNtdbsjSircmIGBYOIhiwRkREQQsgIauF9VTW3XVzUHszSLOpmBmxV50S+WVGfrXU6S2UzWkJ3gTBfKaqZnkWY5+dwJ41B1j7nu+8O8NGYgioQUkphJr7hzmOVg3SZVXgewiIRUUr89OHxg5P1b/3d3/vGf/KPj0r45NNPh6ELYW4D8yDfGMpKxP2j7aJpXl1dcUq5rcgDNAUQARYBVWdt4dx//ts//J1vfeODL76YQlguFkdHJ64s75/ed75Q0Zgis375xWdt1xZFsV6vFQgQfeGrokgp5UmgJH786M2j7fE09esHDwFAugOn1HVdVRTFcgMCv1I/c19NP88++ySF4Ly31hrrnXOZ5I0pckoKUFbVZrMtHzz67m/+4L1vfv/nP/vJsxfPd32bFK8HEdWYIqgWRVHXi6KosgKfUopxCmGaphEQ67JqFstFs2rqpioqay0CNE359I0HXd9PIXT9cHV7u9vdVlUpIjHxF8/P+q5ThMJ7RCzLMrN/3nkyFlRDjDHGmEKKKXKapnEY+iTcNM3JyZPbbjR1Vc+10F3h9XquCTAXSZL14Ly2B4FnWV/uQG6c5/uzAIsA83uveodSAOagwIzXcpZzTU6codlOM0c1Sy73Zr8DIhkS1gfHq3eePHjwne8D+Edf+87vfvudz7/48vr6apoCs+RisHCuKqvSWW+Ltx49Otoeff7iRV6I+dXUcxZF0VkipKcP3zz57g94t7s6HHaHw9n51c3tTeFcN3S3t7e3t7dn52evXr28PH/FKS6XK0DdrjeJ0zj0GSkIIQroZnV0/949SXHz6DFETt1BUur7vixLv1gDApi/PcX47NNPQhic89Z7SzYLMbMVCAFUU4xVWdrNFptm9eD+hz/56fX1q7Ksk+hVFxUgp0ApgPO+KauqapzzxjpEUpEQY98fhrGPMQKANdZai0S563z3ycNxHNu+M4hlWTR1PYVgjO2G4dXZbTf0MYQYAxJaMkQkrCGEkIIqE6G1zlnnvPfeFb601hPhern42ltf67u9qapKUUT+Kmmb2bNspBK9S6PKKL0Iw11qEWSV4e41zxXnDkGyQ3mexGtinlVZQrTG5qbaGsvCACKsc2Lz668NOfQ0zyF0syi+8e6Tx1//YY70cdtHP/yd78Su+/LZl/0wphAic4x3xK+Cd/7dN5/qJM+uLmLKSTizRpenHzMjifTuu9948PTpZx//4qPPvuj6ri6Li6vLTz/9/ND1IcXPP/t06LuyLIrCG7LWmtv9vt3tBJQQmAVUrbUK8OTR47pZLk7vQddzGFKM0zSWReWbBRj3qwGyr16vPv14HFsisrYoysIaryrMUZjnBwCos6bangAiJPi3f/gHaLT2fn843PaSWFUZkHJWEBA658qyqsqq8IV1HtGIyDRN/dCOQz/FgKrGGWc9GXPvdNUeDiGGpqmNMWRce2gVdbve3Ozas8ubvJ6GlVXVGPLOVVVVlVVVNmVRlkVZVnVTNU29qKqqKktDtiz86fHx8WZjqqoAAAR5Pc28cyzNzeWdM0Hnk6T5STbr85pHlKqv56Kvd+XgnGmBoAKis9Ev72fMvzORJJzdDnnklM2hMyV5933zV/XO/uA7X3/zG9+D4RzGSyi24Ndf+/53V5i+/PLLtmunMYzTOI3BGEuAaOyhn95/+k6zOvr02eeaDxaRihqTk0fRICrKPYQF96fL+mefPdscbU6Pjo21Nze3aAwI98MgzNujrbIcujbFFFNUFUMISCwsqszS992TN95cLVeL0/sw9Mo8jj0CbO7dh3oFiL9OKPuLj38xTeOcXYcGiVTEWg8IYRpjCs5aY02zOQJjoBv+9b/8PxXFehBMt62EGJkVEIRlDFOKgZmJyDrrfeGcL3xRFIV1nsgoQk46BoA8C3708Oj0aHt0tF0tllOIV1dXVV2tlysgc3Ozf/byAmC+wHIJHTkkThndMxmBVpmmMcQxhpBSNIQCUJVUObIsSpgvKcmWTMEEgKiklBtRAQHFObszg4+IObyFCUkh26UAVDjBV2SkNZitxqDGWppzARXye66KZBB0CsFZO0siiq+n5jPhg8jMgrpvu7JcAkwwDTANED6A40cAyx/+k//uaLv8n/7pP7283McUhYEFRCAaR9CumtWD43uP773x/OzLlKJKngvNY1lmnqbxrG/D8/DP/+iPGRTAkHWLwnvvCaHvhxQCGdrtD3VZhinOC2YQOGkSVlERZeaYxqurV0+evJPzZVgkxVgUHljBAKT/aMzxL7+IKDu1M2/tPaMxM7hFmAUgZgZmcC60h8JTEh/Cvqit86Tda2MQGTKcUi9t5FT6wjlvjGnquiyK1WqdbSOZt0opjdPITNM0NYvGWzvFQITLxbKoit3uYJy5d7o1RMyJkDLRkxPWmBMokCEkasq6rhvnC1UhNFVdbdab5WIJaM+vzy2oQB5TzsxElmwxx74IZMIWFFVgjqnKyiogkYLQTOULvy7XTF6Kl+krUbDGAcySXJ5p50vaEIEqMzvryFhlSRoSM2Hm/XmWIlQBNSXZbLcQdjD2kIKGEcePYL2FxVvv/p3/7NEf/C/TiG0LY5h4ryp43Y5P7z14dXl1eXVToPOuZGGaDzqKzqGDidPHz89+77e+/fDtd26/eH5xdSkizpACjEOvojlMtet6yrjOGNHQFBInBoTErMIhJDLQtlcpReAEmgebcbPZAhmAX6s4AwBCUlBhZuYQJxrIOy/KCFBWDSEWRVmUZS4x+77dblaROUza9sb7Se7KaiKyxjCCKsQwcYrOee8KY4w1ZNGVRamqMaVpHFWHbBeIMe0Ph1zdJ2Yiury8TEm4Y2NL79wwDoREZFKcYgogfNe2ARCBsLG2qRtjnTGmrqrCl8YYApnG0c4S2cw/ztGzgK/H53N+Qub4M6uBCJpTlMkSgoiwilEEAks+fxvmJJwAyRqjICkpzRpwTgc0xjlEjJxUZJomX7g4hcQhp16BGqXZEprLNO/98dEGbs4hZr8ncxDtD7447yP84S/ai1c3j+7fP6rLMExXZ5fbxda58tnZ+auXLy6vLjkmRIPEMFtgUQUS8jROHMZhGB7dOz3btZvVAsmVhXVFPD+/EGYkyEZV51zXD/3UIQIzIyInFlAiAtSqKMZp6LtbyFhEDCLSHvabZg3wK0XaX3qJCCjkZohjYOtd48qiHsYOQYuyquvaF0U+Z213qOpmYXCMujk6eXEuz1/evk52RTIGcG7HRGJKoGCsEzGEOcGOU+QxjJySseh9UVfFoq7bfjhMbd7QulgsY4x13Rzaoa6K3QFY2QApqDHOGIuJU4osSZlH5nB90XaHpmrqZmkNWet8spvl2tHCzga+LDDcLeTJigZ+ZZsjVVRIiCYfO9C7Nb8CgJzdos4VxjgEzeFYuZ1UVWYmUAZFNNYYZx1Zkw0XzFzVCwBtDwcAztJWNt1na2EOXACFR/fvr7YngB0PKYYJEQEkxtS1uw8/f/nssm17eLNe/zf/7X/1L/7vf/Hq02dHx0cIcHV9cbO77sZ+GgclUy8rhZC5t+xhCSl1bdft967wj++dvLq+IWM3q6ZpGk7p5vY2xsjIhAZBU8r7GWZIxTo7oxxEx9uVIXNzewEpJU7CjGSXzQL8/4+dJnkmoqC5H08xjOOUncMhjAhKxhbFHBz5yaefffb550fb5RD7qqgXtc/FtADMRQihRX9XL6uIACdhVlRJnFLMQe6AWpAnovOLawI52mxUoe06Y/Fos42RP/3sczDG2ZkeAwBvLRsLKsaKY8cpRUk56HiahjCNt/tb71xZNvdOTx6fNpvTtUXIGqwqyh01cUc8ZqOmZqB7Hhjk2MhZSs0UDqElsrYgsiwpTJOqGJPjbiTNC8uUCL133pcCEIZ+nEZCs94cWWu6ro0pemdVFVFAjfWekFiSCjhrAPHe6T1O0RwdGSK5PkspAQKzDMN4s9sNfT+MXeGLb/7u76ya1f/43/8Pl7dXu/31OAxxGuM0xDgheevXY39uiRBAEFKUfXt44+TBxaFd4/LRenl+eVU1piq8qL737jt91706PwtTDBxzKO6iLpFwGKcwxX6cAMEaW3j71pM3qsKVRQnM4zAkjsZYsz6Cws07JP7m1xSg8M5lp4kyi7OQUgxhDFMw1nhfZBABsjME4MWrsy+ePUc9Pdos+3YoCyWixJwV0Cxx5+olV2JZ7wQFZklpijFyijn6aUJ0NsQoonroOkTKyP0Xz58vFsvjo+P94WAMZCORoBIZkagKzjg1oN77vBQKeV4qrKCqKcXrm+vrw4O/9/t/J4ddZUUVFQXnmWUeImSpFmmeEhhQEVCcB1L5MkXrCmssIEzTEFMABWcdAKYU52qe0FlX+NIYO4Zp6NqYQtOstptjBb26vkgxGSJQQqPeF2VZAcA4DinGsqyscyJycrQ+7G82nuDokXOF211MfccpRY6SuGkaCZOk7sVP/91qffTGk/sff/jZ0PfeWmtMXVagGgJrxJfPWluLMbh0clKlJ9vaEieVtus3SH//e9/58OIKHHlfhsRVVT68/yCEsesHQEoxLJrSGguEcYpDCMLKnOqmTjHtQzg+UYhhmgZO7IoCbAEIIL9GE1B4ACjLah655HFzil3fNnVTYOW9Q6CirIAsGAMAu92Nd6asl5GtNWLJZRZhrgoQZifRXeemOs+k88VKROQKURFJwmkYhudnV1H7qR+rsloumuPjzeqRP5y1+1273x1Wy9og5aYQDFhyU5oAkKyxaNVYBFKVnPVpbA6oMqL68afP//jPfmpzOaYoAISzqkpgRBVVGDKUhggKrIyzZAaCSHmUbZ1BYo4xBhUBBEOWhYFjBnyMsYWprHOR06HdT9NYVfXx0T1jzG5/1fedITS2sM76sqjLynsXmbvDbpympm6Wq02YelDZLJu+21UWiqNjaJZAVOBViJE6u6zx97++5K594w3+yU/+2Bq3Wtnt8fKw3wHz0Wa7XG3b/WHXHkqfnr71hk235xcXZurUHt32JfSjXF4C0qefff69b37rydH2SmSz3fbjdHl5udvf9sNEROvVMoVm37beWUXiGG/2hxiCsz4y7/eHmLhcPHi3a1OKClqWDZQOIOOd/8E5SwoWfynJ1rkSVBSBmVUFwHCY+qGzzgEUzlkRkRTzCpLfeO/+2w+/b21eD0kvz/fOfjSMOWxLFWj25b5WmAizRImAzjrnHACkkEJeD5bCbt//43/wg3eevjl0YwwwDv0IY3OPHp/eL6rq9qb9+LNzHmat1BprjQkxGlC08/pABEdm3liR7SApBiqKP/rTn9mMsioAgBDSXXIogM6ZyJrTuAHvtJO8dEXRWEAjwjFNzFFVDVkETJxEEgACUuELa23i2O86USmLcrs9IdLd/nYMrQFjfZEzwwtfeV+W9WIa29vb22nq63p1fHyPOYVpLIpitSgkhn4ciu4ATQ0sUC+XCjFyVbht0wZJD05rsEYBvXNPnj4IIV2fXytg6bzfHhlfRInOcVR/fO9R1/WjL8umYTI3u701tuv6P/l3P37//a9Bs4iLxfF2XTobQrD2MIb0/MWZdRbRJNGz83NCqOoSFLJnr+uHEGIOzc8pdvNWlCFBDPOB+yuFGHAC66A9gCQoy7zIYhj63DGqMCgIiIjkxRExjMvlqd1s9XDIX6Oui7I4dY6cK5glqlvU5aHrXkP3PG+MIyJUtLOde+YGDaIKS5KkIkiASClx38a3Hj41RInVWlKFJDyFiYWHNv7Bv/qz7vkwE/zC1lBIGsLEwmycc46MaiSmvLsOLJmqqoqiUiArOrd0eUGcgoLg7AwBVNA8PwcC0HltLM0tIaQUkjBKyh8bEWZlYQWCTOjHGPuhE1HnC+9siumie8VxAjLeeXTWO1+VzWKx8EU59N319WXb3sYYV8vNyck9Ud3dXqnqvaPtdlUiwjD0276HZg0q0LVgi8XqqKoX1hqsS0VrjQNEEdMsyn/4j/7BH//Jn372wacE6IuyLspDnzS7AFUXy7LwThX2bWuNKax/eHpsjf1///TH3/ved5EfdO0uRF00lSVikWXT/OwXvwjjRMaoyhRT2/cnR1tC2h1aZ21VlSGEcRq8K5artS0a2B3A2L+yzenuhQB3NPx02Mvuqjq5B81qGPaU7yYAFiY0IhLjJCLMKYZgAXBzBAAQ+HrfJg4IILJv+2Ga8ruABEZUWDmGhCZaY511SAYBcXZyi2h2jUTVhESWbE5W/MlffrpYrt569HiYphxS0I8hhOC9n6ZQVUU2A+WRoiU0aJJySilPDXPECyQAVGu9MQbzIi5ASzlEKs964M64mz2HSgoxj87ndJZ5eKnEGpSRRVEgI4oi+SfztmwWy9VyU5ZlYmaOKSaRNIUwxVA4b6tFUXjvS+9KXzhDVoRvbq4O3Z5j8s7dO32wXh+lOF1dXXGciqJ8dP94s2oQYRrHdrdbnJzCcsW312PXkbGGLBCisaqmWSwzYlhVzaPHj3+oYbXe/OzPftKHCQENWjLGWZdSMGS9t4CYOMWQbscdgb75+I0g8sHPP8CqKo+PFs1i0SzHMcYUzi4u2kN7eXlVVWVRlMM4rJfLcZyqumqqcgwxe2P6vnPGI1lIAcpKuo4MwuKvB9gqQEoABaRARCnp/uWz612b86CnMAnzbBgzNt8+1thxmqoQwCMYO17d/OXHn8YY8i8fEWJkaylTNpAUBFgSR+HssnQWkbLKmh+6nBKgWuMICQgIiAinELtuPLu4ONpuGPS2bWOIiaXrBwFdLipC4HlaraJAxlAiUeU7B5G/O15m3taU+WiwMwqNpLPMyir5XgTIHgDC7KrL2IMiqHISEWUVVSAAsNYuFsuqbOqqdt4XzhnrzEwJm/xYhmyIEsU5ZkGYNceKAGhTN3W9aKqmKH1K6bC/2e+vRcQ5h4jvv/W4aRpRmKZpv98twgRFY9bbcPhiOhzGaUBA55ySr5s1s4zTeHr6MKXYNIvf/Ts/6qbw0b//Sw2xKhahn5y3AJKnGyxpGqeqKschfPHlMwV57+2nX375/HB9G9A8f/FqCrGpqimEuirffvqmte7s7Lwsiwf37qWUjo+2iXkYJxURxGEYYwhDbFnSol40i0WYQnN6/5efZ6yQItzuuv2NSCJjX52dX99ebLf3irJKKTGnLEYoc84MDGFcLFZQVVny7cfp0Havs5hMXuCVe8I7AoLICEviZEQyZEVkMpMnmhffGGsomxQz6kdo1quFqr54dTHFwCLOWlUEAyf3j94cw4//4oNMv+aOkgiJKMVJFVARxCQyzjrrnCGb9xISUUrJAgiikdm5JqrmK7/cXWweAADmBSqSUYyY1zUBOV94X5TeW18Q0jgNbXtg5ew3MuTyPHM2kCJkEYhmWCNvOMsTbRDVGGO87GOYYgqI5IxDxKoovv7eU2/tGMaU26kQoFjCalXXi7Y9dF0XkzSFpWxsNlRXzXq7vbl81ay3t7s2AbrNhsd+7Id+6FIH621DIClxTKnvh6aq7t0/uTg/f/Xq4t7x0de/9t5hGnjodvvD7tCeHB0jUVlUr84vDdFbTx7XVU2Gzi+vn7945bxDBEIzhZg/NtkaxCLt/raomv9ISrJF2GygG61zQz9NIbx89QJRELUs6xjDOKowMwKS4ZSEk68WMU7x8tKtVlCVXXsQBZCUEWFOoojeW7jjuHIzkIfEiCiqlKu+OSF7Rqdn9AqUFUCk64ez84uqKPaH1hceEae8jM7Cxctp2B+MIZrd/yiihsgYoxEyXwGkEBARKiLjZ4+IisYY7N06unk5HeTAqNeuYYC8kCW7eqMqSBQh5wpjbJ5OhWkM46C5Q9DZaIx3jAfOg9fsX8d5YAUZ+clUt858GoIhAkXKHRQiERCZJw/vvf3mY0AIIRVFvVofARgABqyKzaY6HKYQYkzsvLE2S0SL1ZqQhqElX93sbhXg5PRkGIbrqyuL6BNPQ6grL8yg6qzrum6zWb//3jsvXl3+7OcfPX3zjSfvvX8TR0Qa+uHnlx+XpbfWPX/xcr1abtYnbdv147io68369OL6NtstVTWmwCnVzYLICCdfVilFSPGXF2crwDhCfxBm62xMElMwhCmmoijGscipdUhkSBLHGKO1YQLtzG5TVVCV3dBnSs8X3pAREQDMnui7oLv5Lci5mvMuuezchYyHKigkQAuaLUBKOI4hxuCsy854Z0hVjh/dR6BPPviFcbYsXIjpLuJOFdSQISTOgKKoasz/wJkyA1QjoGoJ8sIxm1tOFJV80hXnBxqyCrLm3</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9W6+tW3Yd1Frv45tzrX0796pz6mLHTsUJxpGdiFyECGChSEQiEgh4jARPecozvAQhIR544CVCQgQBz5AgISElUsAoUq6CJCTYLsupctmusqvq1Lnuvdfaa605v9EbD62PuSsxvwCdWdbx3mvPNed3GaP31lpvvX/AF68vXl+8vnh98fri9cXri9cXry9eX7y+eH3x+uL1xeuL1xevL15fvL54ffH64vXF6//vL5IgKImEAIBYfyYo6Mf/df0EWP8ECK9/CICAhPVh/x9voyD6f+vn//y/AgCTuhq8n4S0Ba42vv04bx7mj270Y19BAOsr8M9+FwiQKClArUMjKAoiAfknJAS/gQIgkP0FAn1igiCQv/cc+hP6mCSxf/ty7dDfQB/I5UPXHwjo9Tf9sxflx8+lD8QHJuL19SPgL/MPAPTpUby8wb9Hxjoi33l/ToDsPytIAgwSIkmCZAAggvLfggJB/9ZaRBBBQiWwqkqEVNCcGI8PGQxhUhJCTEjJCnKqyBQQQKEIgcnqKyIfhKAgSj5iKgSBAOUP9FsAqS7XpQRS9GUIhO9+YYYoSEQQX3/r8I33r77zo4ebez27ji+/cfijP/3sWx/e/dIvfy6wSmRBLEZ4LcVOEQhiAilGqAApRAQgQQGKDEiKPom1GtcZAUqyjzeQyVkiiCmhyJBUYAQgXZZwEACmEOtGe9mipv/NGzUCAn1FAVR4afRKKAGBBEDKa9hHhBArGAVfT4EokAEiBDFIklQhessRgUD4ZAiACf92kZlEUAGGfzNiS2QwoMgMYIwIxkhEcMsxghlkKBmZMchMjkCQkczIJAMqMIiS9ll71T4xZ82qV+c5SJAVCERBIZWSIRbAiEDv0aQvjZgsRGBKwShUAGSIRIkMX+UIQbGuFCmAEeAUEAqHgiJSrLXnUukYVahgnOd8cV8CDyOOh3h0jDcebYdxH8yCMqUiMyCQQSjBimABzA49XlQkO9KEpGCBEQ5Ivf6QyoqCFIwVnxigJCEzRFQEEJDAGL0ZvKmcFXwO6njoBQ0pUwqwenkkIIRAhIgBRbJWFA0vEolBCPE6YGDvBcSgShFkOmiGAgl6UVKhZCBEBYNB7iCDDDEIBAPhhTW4ExnJZEQgI0aKjCRHMiMyGMktchvcIkZGJJKRgZHMyBEcGZncIjLAAAqgqnSeOM2579rn3IW430cQoSgACGcSFKdDqFAEL6FKCBaEQCFACetOEaQY3s0SA5DXZ2cu+G4jwCoAyk50AVaQeymDoAQqFCX96Iaf3j1cH/I4kMwtxxa5T4ETCoCKJCrJ6pSQgINQ9If7thYU1d/IS+xRgCQBVVExWQGm77gEwDcbAHYxmER59SHEGdKKf/Bahxh9ioIUBEhOznBSgoQSwmHdFzi4g4TP22G+V3+tMOSDHs6gAYiKjsv+oLqclDp9J0IOeJSXphgQlA6c9CVIhNNKkRksMBPMVDAiEMHB8JobyW0wI7ZkRkRgS2bklnHY/ENnagA4zxqzYs8zi2TUPA8MZ/FQlnYiEQXJsCBgtMFGEJ2VSiFVdngDAwQLEihnG5WIklcmigqwABDJQjEXHPLVK6dXYIpRvdQgYc4qjZIicEgw67wbhE0hh6pAsJKoBS0WYJEUVAkOUZ3l+mTKEePy1aKcrcqxbCU/khOKBEsFTCBQTIqhAqoMeKYc7CvEioWF6DwCQgFW47MoVnLhKaCkZAO5QRZFYF7wmI85xEaRDkmOAbjcG9AApGHXXEAToKK3jpF4dPKEwEiAXnUkiQQiSDCCwchgJjKQgcwcycOILXMkRiIZY+Qx87jhsGVGBERqFh/2Ou8VMZMA6jwz4zzKx9mppdC3i7OqAh3OwMAkUEBQ0CDLG4pCqdgfUVzAti7oE9EZSkRUQfDbvHlluEehLtdjxdbq1VAKahvMyPOcECSHgN7GkujQBQQLgBR0jgaI6ajg+yTMyLxg7MZc/d/eleXr35toSsa8WQhSEhBFRcYUSshAqcIA2ymBhBc6IbEKTBhUBDAvsLyxIAJQ+LRjouhgSjgzqCJigbqOjCyyiFxZOzrpcDGIEKEF332rot+LhfuIYAQZXnAEGREy8O/UGTGCW2Ibcdx4yDhsPIwYwcOWW8Zx5KNjbiMAUHjY63ie9/ueJy8F8ewkC3jjFzoHRgC18mRTIZ9fyZypBMN9X1WzLxQb3jrCh1hqmlYGa9SK+CVQhegc4t81R6JU6NDjYAYkuSUJnPaVHbwf5eh1uZrOIgJ3A6IVzQMrCDhWsrMiQajEEFTG9EIBA3K21SJRWPyHUmkCZCYDsQWgPF7xfq+9alaUBrn3XQcApI8YkgZCF7orBDVBNhggpWBzBbCaDgTAmAKCSQg0Ig5UMDqGQ4woY1NvhwhfFlyWtVO0I1o4jomIivW3CGNAmB9kcERmcmQcRhxGXG1xfRzXI66OMcZ2DF4d88lVXm1JRtW8e5i3pxoPDE7fTagOGcMwFcHhcKVS+VhyLp5ElBMdG+w5YHhpLhqpDSRVTrdFhC8mSENalnklIEWwEnFuLYAlRe8xhTo0FsxGGCM0kueq+/M0uiiCJn6+qCBK1RxcUlQFe2kl0B9log6ghMGQTIkTolMbfM19K1vgCXEGf0xYIAFswRGxhTKUOgN445jbyIcTn580S4b3SyWAFvwgIqHqDzL1ORNh+EuEmNTOMAvACu8MM/c+Q1DBENkKg1ep37aAnYIQIykiva+SJJQ0fPQy9af010VEhJLIRBCZ2pJj5JZx3PLqkE+O+fh6e3o1Hh3HYYzrLd98sj17lBE8neqz2/Pnt6cte/WLUuFwGINQwexYgUtQUpFRF32HQtEcWRRLDJp6KtSh3LzfyYgUhUHsK9aJUNMgRYlCpANclF7rLp2kTdzYWxcjc8uo0l5z8f9YElpIovUL1UXHgU+y4YtJN6AhFjtQXwSn4iW+rDvLmJ09WVQBG0FxeuluI95/HA9zfnZ7d3uPfYqBDL75iO8+Pbz15PD9F9vN/QRTLDYYlZSghBAKApnGF8QwyRTB6rvdP2nkTotL3ouWU/p/fdgIQZHRodQrJ9iKV4SZGhKYEUkqI4kK/jPRi0AEgpERAWbkYI6MQ8Zh5JZ5dcjrY75xvb337Oqtp4dnV1fX1wNvHPHWFUYcXrx68vGr4ydMonpPAMXjXoPUhRwabwJnwefZaU8UMYTZN5EMB4DmXL6HS4VqJbHIEqpVESxtoTNJORrKW5RWHCBFNeilfIyMCEbEcQtCNeVdqwa/cHZfOS2EvRgEwLn00ZZYGi6gwKSmmJIiKKuenXAnWObdAQCz5cDeQhPIkXzvMQ55+v7nDy8fSFQSBVThs5s67w+/8PtyZHz7I57mxAJrrwVUQw4DB1ZvFi7gFYpGyYZj0wQF5ZBKqkm+j6o3TDPsQuyUlxWycxDoYGpCFCArOJxwg2JEkjmYNANQBjOQyaDpJzOYEdvgccT1cTx7tL377PDu+0/wpWd49wl+8m3gPwTeBf4X/Mr/8aVgCbtQilk479qCQ1AYpGNWmKDkktXZEBIXITzIktCBj6JQYmCxCYWguKAZpReE92GAAssiFmKqRKAiHO0E736hLJGwr6e2mIctgJgCRMg5RACSLZzCUhw663UyR/qAu/7QgH9atGeoRCo6p5FUQAFdGKqz14qzNHLMLz0ZlO7OoGSyjbWN7k+6fTh/8Mb17f3+4j5uz9qnL43FNgdb66qrDsDE0snZ5D3YFDVFUWAauoRQcM6Rr7twWWrKABwtQMdGBSPQMqIJZkYGK2jlLCOUFmtJA/8MZHAEx0CSmczkSBxGHEY+Oo5n1+PdNw744Al+4X3gDwL/XkcP/Nv4ud/G7a+/c1f3Z92d5t1DZCzkZ/UZJDqYIGA6Qxm1LKUDRmdIdBREQdk5yu9woLIuKbIiLDFaGA2jaiEKgnz6Ta6loHnqIqxEkq1BHzceRq40XsVm6lYrjeyopIaZvzW2BtSdNawxREtoLWcEaP0VVHZYpIDS+jUCVEGCkoiRRdXTYw6HQt9/QEIgIvhw0vWGQ8apRMyIsuxBiiEQ6U9UicMFKTQN8ol7j8RK+WBXdyxw8rJOiQDTux9QK4lcnIgZMUjfaON8ZQRZQSQzAkGOyEgOMhPWybbMsTXwHyOPIw8jD1seRl4f8/FhPHu04Y1rfPUZ8PUfW2R+/Rm8+Wh7NA4jRoQAw6G1Iy7lD68JNpD04WVYrDVcCGknWiyLCHSeavAZSlMnkERGdQFFViJaB2pVOlYYsJRIpRAkSr6mBWKkRsTVYVwfIjMgs+GQ10yrT0GYbgosILlw4wqrbKWF00ci45rW4gtLcmoOAC7MT3HRXwpRKrzaxUwGjbQXCoS8zKm9cJrYZ1cRg8qIdGYo10wiwh9s+aPFDBoPEAku0b+Vir4nK0maK/ane/2tWxSXXEkGa/1BveCiw1hEjmQERnTQyogtcozYcmyZh21cHcZhy6tDXB/y+jCuj4fHV9uT6yOeXOG9J8DX8c+/fgZbr45ZJWGWVPOC9csyOahCCr5NE6yABX31EYMZGUhvy4CWbC42qyoSVAULqAoREf0t0xeUKwpWGMkRYoVZvIXrAKjWsiODST6/2x9ORbggW8HqWvBSjYITDez2ZvAhqLTK6B0PiPUVWAffuq2BY8NMVayYub6mK8tvPrLKoyiHwaX9QA9VDztmYWQ8GszcBrPkKFLJzHBJ2NHxsvop7MCE08WSNroYaI7N2W/ss2D/WcHwKk06l3b8itbIyOx6k4F/Y/8IRWgEI2MER6aLSyO5BcaILfO45dWBhzEOYzsetqttXB+243HD1QEYwJ/4Pevsu3h1wul8f5qnfT/P815zzgquIOO8Ze0lG3EllcJSYrxbAAd55YwV/VqDdjjAilfQkhIEhBeOKFmHA7oiZSbF4hJ7GHPFdiAsnsVh8Dzr/tzybriowDLmuRgtojF/dvYRxQjvea91JRVidcpVGvsv00XXKbEUZ8o33oA7Akzy81e6eZjDKEhxkUFKmHt89mo+Oca/+NXrn3hvm6jzLJCzYm/xCpnThZpWybAUDAY4SJFZvtKMoCVcsAb6Bl0kMWIt/zCFi5Xtw2HWKodlzy5uWp8imGFRhNG+DJLMTjR0fZRERmRkJjMQgQJUhYcH3N8Aj37POvtr+Oz2xavT3el0f56n85xz7t5nxIRSJpGOKFEOT10kLwFDBMOM2ngLMjVj5SpoNwy7iPKNi8qXjEsxMjn3amidxdQJ0evFSi5IYSQjOSJnaZ8idkU52UMAyzUiaCOiNWIWsYdEXm4o2yISaKgE76tqzLAEhIDVAN+xHR0cSsSgjiOeHnQcQYUQLQsDDvoEbBK5fdgHBex9aLDgkoImQDGBLTGGlmyhFdfK66JRVzuyBEBd0nJ0FV9XkyxGEc1RTdeJFiALyzJjDWip20C19LYCzdLsfB2ICAXDqtasOs95f9pv7k6f3rzCZ7e4efF7Fhnwq7+KT+6e355f3et0rvOc+6xZGjB69NZaZ62iXSbFGWIhgnuJUEXQ8qZ/aZmwaI6JtTiqF1CRFFyEbrGeCGGaHcZCh7Kfoj8NRMl5jdgCGYrQedZ0WdxWEIVjVVO52L1vW3jiRpZlsyX8OyDZlVQi2aTZy0zNEyyWYlrcEIJdnFWAxwGA1xtqzrtzaf0+V6AvxsO5Pr09X2/7w4PmtFRm84flVExhApvmCCQw4QJcgCHtIFGFAJQRSydaJ9A1mvUj9nWoMHRed6XrhSvQtgTexgf7UPyX7BjbUlJ/kaASZum0VwbAPShgGkpmzusDHr375J9fZHf/Mb796Yef3D+/Pd2cHh7OddrrPLFPDfZZuPI0fFBYrhdAUAYm5TsKYOFOsMKUrbgWq6BkWjYDEl24nF6dtse1bt9In2sNsEXT3vck92AElRkUTlP7rnrtyKnm/kFp4pIZ2x/nSBWX/UP6Wldnz+Cq5ZpX9nvQiu1EiBpUIfaLvjWhmxOuH+Ot6/zeZ/cUuMwpgNrvItRkJjLx6JBvXOn5vcizsLH5ekOKOTlldi+mojk47OIKQZxQLG1H1WHWpX9rL5IyAhZ6WoO0nmNEZ9QZaLtGtPcmFiwE7KWzOSurqgLnaWq+QwkI55xK1NxnqApQRD066BHeBO6Aa8cx/Npf+vwffPr81enzm9Pz29PN3X73sJ+m9qlZNQqRmuKIFtRBlXeJbyNIVfhUyZQQYYUUARbsS1k1O1LahYig6lJjuOipJS+MLgBPyZ7EFtjAQoU4hS61qa+VDoPnqhIiDKZksa+dr6Bcb3jNDMWGj9OYEy2FddL3+wpJUZjBS2y2ah29UHtzTfPPSUK6O9VHz/dimzkTlvDoJaLQls7OSc7wt7BQBRcoUaA/3dvPu3cOu46MYWGHg/WxCeusQFmTNJ7p6nvLe8mVpS10oDXBljVidmEg0BqJIU5x71rMBIKzZDbX9lRVYc6qijk7kRXqT/5rj4F/B9iBvwn8rbv/8Z9854cP96fzw1l3D+fbh/Pt3fnuPM/n2mvOwtCKM+pjd4gpiKjBkEqRKxhbKFoWLkAR4eLzwjhD2JfUap31op92QcrCYiCqvVpsf5sTtxNhG7AY0EiO5JOrbRaqyhcL6w5pCVKWjgkXuFBqg7KYVk+cboSkvPIcWwTOQAKisrdW1xhqwc1wjUjgMfPNa0G6OXXC7MyWtgVrIzT5698/3b07zopX51qmC6+EKaQ9YQISlZmAZnEvRiDAMZTgjpyz9QGibaadK5EuOzPmwvhgm2W4CKeStruuBMvoqKucKExm6rxjhHZ2DGzYHRQqCijWhhIPdhSMKoQKVcJnD8A9cAf8jX/6X/3jD5/vdw/ztM9913nfH87z7lyn83w467TXPq1qujqklTcRnYAYISD7YlPM4HRxTa6buBCavY8c9ZHBiShK5IBCMaNromEPpU8HAjmAIlxkRSLmkiKBkBqkPLnaRvD+NGVabB5gryWTmg2Cpd4iCvsW0F4ftR+AospxeAmEueyD6fpooAouRwVsK2fr10+v4g9/aXz9zfjOhzc3d/u2eJ/rvjBQIGepSnfn0zYOs5b03IbkbaFgBPagyZvDaJU9BBNIJcFBFItDIjQ7FiONQrFUFmiSy/YWJJQBtpe7ALsE1FWRojUsUVNIaAoo7GQ6aydKKx2nCzaQojSlPM+atZfqr/zS5//+z/wlfONr3/1vfu2ffv/Vw0kPe82qfdY+te/ztOs8y1608z4HNK1vujINSE15iFWGBtvYrk6YarnfkuEqMbYWABsTS9HRJmSDl88yACelsKlR9iKDCYpqmIsgi2Qmt+T1IbbBKpDKqGUIM8Mttc2+Liwfywhsrqbl3GKX6SmW8X7zkHJVAI0YDHJeG3OjSKAkvbifH97gtz+9z/SV0wQAlYKos1gkqYedDyc+e4Snx7jbqWKGZml32GjEF4wqcSoa65OAJJ4mwoyPGqDCluRoRTn0Grtb+nDECgbEGCvas/FxLdmEADsjTyRrGpir3LnglYZCKbEpJiZADmmfBdZEJEt1GOPTl/jL/+Vvb/HdDAo4nWuvmhPOOeeaNetc2nedZ52mBvte2Mxfr1lnG346R0HV8hKd9nfnOPVle13ulIQoKdg1+OoSkK8QFkjC6kexRyGqFGmmSa8NWgvegsdDjszTFMv8DMtvU0sH4ZLPfPQFceU8M84AdjM/1Iig+mBQKsbotN2E4FIOXVoVK8S98Lsv5ie38/k9Zr0m2WeQVcVVASc+e4XTPF1fxRvXOR7i1RkJPrvm/Vk3uy94MTAy9sKcbRpy4OsLCgFRynB1LMI7sAa8NVetKdgEKCAVFZpmwaFSC5YoicCuyIYqipjRR1sIy0raU+mEEmK5cD1PO0ayxMk9Kw+Dbz4an7zcHx6QqUAIdZ6oqr2o0pRKqlluFNgL56mBLj7N9i5gqcwNm2cHALhW7b8kYYdyI2Y2+fevhHrfWhBjxWJ1atOPHaH2EfnTllBEq+HR3BAEx4jjYIkPp33C+7qKy4EYugAX2TPYgghb0uzEVVr7H3bly0kT5HCVpvO3l2zj6VDNLVGKp1f19nVKDNR3zzpNK0JqC50oMTEtJ4R0e89f+537d5/yjcePhO3Ffd3dg9Ah+TABRLQxobuELoorLzYSKFAFsp1LZOQwb2BLAa0h2oMKEjWbjzpb2pTc1gcxQyoglxnLrUMsISZqiAW7FCaQZTuwBgvMqiAj9FbmT3/50d359rPb+ySDNVWzOFU1UZhVbPZQNaumeJ5zWH4Q5ea4WGu/+X8vJbLNgGBFu08JIWFdl1x1dJW3mhzl7I81M+tCJ3vJCkwJ5AzUcsdnS2ntCgdjHkJX2zZLp1kr+iYZXHWnEKRKRrHge6NlsrTCKfv4atXGWDBLsD0khULDAa4V5t+tEXx04D4xiPuzPniGm1cPRmNlkLfqom0ZX4gaxN1Zn97oD3zAN5/EL//uXiLJ60Psd/skIWRoTlLNX2ztpWN/FyTcP5NilcBZighUOhEGhSq7NQFgrjrGhFCKUKEsBBSLjJoiGQVFVXGL2FUOSYHY5Q8GJ8p4QknthYhBMWLUPIy8Po4M3J8qlmA3pVmSMFWqqKqCakKqKV30MwJpxcbopJzzYAd6dc9UK52T7S8QqjrGCfuiks0rgiFFS9bOE27VVMtkpGk0GatBJFr0NtcLSRrB4zEPI/ZZNZEx9wgsuG/7ODiDWZ10bO/KoJdBM+dODV1usgJI0lBRq8iEpcvLJMV77eY0n2y5BZ4d9fnt/bc/2s8T3R0CXeodJUW2ANd2UeLVGafz/Mrb+f3n46OXEurmwfuZCK9/MaZAIhSzL+1aZRf7U7NjEFXFKCgDAYyElIVSLS+bYGIRKiuIupi02i1QZbcqqpFZYV6M0oQkq20E7BUNSayUHl2Pn/360+sjTvt+f54RaNwqzNIUVJB2SVMFSaq9Yi8Otn3GUdTbHAm6422d6x4Gn23OVDsMMyBR2Wgo4A7QCKFYDKpP2YC9pXYxiKmImEueIKsbEbp8Y4UwOCIPyQzc3J/vz1PapFoaSOslDaVsaHR9yTtb6B5LEojlTk1pEvasFh1i6dp2+wAcnkAkkMRx4O3r+uDpePnq4Zs/2l+dqis/NorYQu5sXW2IZudEAfzw8/Mf+lp89Y3x8c1ZiFltafbb2uuyCCsbQ1jXXo3tsHJu7iWrdShNlojEJKJ1ddIOeDN4orhcnO4Ft0gbJd8d61bgsrCUSzeGGJqTAhRVUy19Ue+9ke883TJ53tUyPFEqIao4VSoXjPwf7pr7XiPcNhNO5VHde9UcZNo40SaoRYhsg1hbbqLQjWqSMJhT5hNWcoda0E6yCkoFOLl8YJ3b2hTh5u1aToQcgcPIID5/tb98qNJ00rNVp7q4YtVvWRusZEUxnA/StUCGbNoPJ7sqRQiz3TWtzQLrfgEq1RaxZRwzHk7nb318enXSBLIFpyq1bdUv0qfGMWIEGCOkT27x4s5+/x/TrVvsKPK1a8OiElmkStlCpdkVAUVwV3uep4WgmkKgVMm+QdH3iE1RBWGyNN11qG4SRNi7a3uRWL77DpqJ0rSLsjruTAjE3UN958Pb4zbO5zo7U7ZGD6oKqJpVJhiqkgCz7OEDW2S7bCdvDu1+SyNWi1Od1lqTpVCc2Z1zNTW8ktjevU4qdJu7SxukOAPMQGESIjcUyg5EL+WmjQAqc1xt3AZvH/abuzlrCulFYfLx401WLkQWLoAfnYR63cQyPAe6eb6WdA5UypHMEVI4DH7lzeOrB33pan/3Gv/wew+f3NrI6zkL/vT+GgpKUkXmceAwfMeVzJH49GY+vTq6dlemSqx2lJLtwAtfs0I7SdwBJVkVcgbUpb/O5W06E0rapYiMqQgEADcTo9TqdGfeoKqCNqpWFNGSqFisUCgwfduqEFCZ/PutOJ3nb3/08OLus9/59O60lzChYdLdpQJBtgr4/gsl7tOKXVfmyRWiACBbdep0s5xb3QrhIgDcg+5LFRfzqXvsO1uBYikqqDSfjXAnYyCJzWJctnBV7SJgiAnWNnDc8tHhEIHzRHUFrxoF0ZcSAa4SguOK2EUoSHDDjzfLcs6E7RugbIg2Zw64HQQRuNp4yDhGPb3Gr//o5kcvq1i+ot2s2MvZ0cj9n+6qBYkgk0jUCPzup3d/6CtP/8hPPrKOyLX42wre+MvkJ63UYHl4WvlTy5lNb9Dhz71i8C0Rpniu2suEvKyxEmI72zwNABBLKBn8uc+jqljOyNIUplDFKc7SLFY1AjuOuL3Dh5/u51lz4qx9r9qnXC+fpSpU2XuIUs2SVMP9CqZt7CalApLYW5jBLGRLSZI4qSAbjLfhRM61F12Mwk5RTcsNZRfCK6jRQgdCOPmwZtv0nFaKyI1x2EYOJbvq3CK+CzeWIM2w/C+LMifRmp9ZrWFU+8sM6+y9c7v8fJ36bBiJePmw75/e/6F3cPvq/P3PZ0lRKJq/GfZ0b+uqMC6gB1ctGGQEj9sg4s/94k/8ubj6V/+Tv2/s6BDad1wZhNDl7KX+eLtraazofgWqF2SVZ2ss6gNVMYCqinQl2VHLqCy8npfi6ZhZahfE2qFiwWW4KiEUPeyhOcYefHyMR8dUzHnR5RTAnLrkd4I7O5BK0pSCmBH2rYvwpCAEu/XeM2rSN9N3yHUzehVaOmevP6NjFDgdGKPn8tAtsG2i5jR7JSub9k3YKUm7hJy7IoRtxPUxrrcNYFm2R6DKHZB9UtjLzQeAV8wiT+EOcufBS0juoIsS5/o7LyNoGAhqI44x3rrC440fvjjfneG6krG/UG2HMhb0q9otIbAYaryKc/Es/ur3Xrzz9LANBw+Yc0MAE15ksIVaW3JL62rVQpnUQrlKSnMqn3wTMi29XN5XdOSqYilKqMK05AiAFSi0jVHqU5DUEUhV7vp3Aa2Akvaas7TX3KuO2wA599VCh4sAACAASURBVHmu2nftVXtxTuzSedd51r47vFV/QnFcGkvDxdoq85q0I1Ou9cNcfaERBbYCwV1uEHImJCd2qucI0GZQ9b0ugqwWFJHkbqzOXi9NvTsnmyBFbYnjyG1w1mwW4248MmqlzhawfLWSTWF72UgVQSzXjrmpb8iqljXZjJaSkYFnVzpGfOPdwTp/cjtdbjP2jNX0FUC5VmiiWzWhDQxUMiBOBKbOqdj5t7/5ybvPnrzzePvhi3OrxB5mwTIKy1T23BSoosip2tvEaRtVkeaaE9EzkahAA6oUZ4OaZrTTXWZ9eoDhlFyqc75nN+EbDTPC5UVUzTWYAFXlyVGqvXD3MPcqFc/T0560Lqg0y9kDqHW1a6+QZkR0VShdJYokRnQkZdrci0BEeo6RCyAhtzIbbSxYWtERg2kbS0eLQjAa3qf7u9w7FATdpElDPatg3XcUii3jODASp73K5mMP7ZLZqo3HSwtbccL9oMCINeBgJUUSIdiWvPAjI439vTeYQrx4QLDeuuYPn5/uJ+Ce/WW6d2zcmwtZT21pw1YmI5vznOea83ya+/0nLx9+6f/54Z/4xpuOnu3FzI73bunNsFsFjPJJJcJuAE908Hc1AgABTWe0NUms075KMmu1/t8sCRqAqCiEhF2YhVmqiqmubhv4YKEXh2csfgzh/jzn9Co+S2U7ZGFWAYwS1g9rL+6FqtrFAdjWCnhoRoDdzhQMEyjrlWFPdaG6U646aXOFdiGBtv6TCqg0MpYHnEWMKK8k9UCPiwRvPr30ioVOamRsmbZ8VRM09NQFVqKAlIYb/Nl1cKB7Hbr6Eu0ntyFwxcBWhrtT1Ol11XMDqCfHuN/nZ3dzn+q5AdFFLBkTqaslQaAHjrlO4Fsij4Y6zwLwj7/z6Wk/v/fmGy07qOWiJgG+r01n0S0B8kRELpOZ73oQW2ddMlDVqEi+sHAtf4FGT1Rwa1hPRnER0JUadp2kTZNChCKY6nWFleR96SXcneu0zz6W/g/kYSQFSLY59MwI9CSV4VafbhC+aHxeWYZZZmYEzHs5gGmJM1hyVCUQmDZsWa/iTm091AEJVGCI5XpRKcjNSgmECFtUFo9qEoyAghqJXbg/rWIieh2bFwquwWcAgKfvLWuTUSB6dB7pA11KsZGtTRzeC16OQUqe9XXzsH9+d7ncXjhLy+777vEe8o8WFxCzWDESyUHs+46bV/Wt77/89GU9OfDm1MW6RoyqpnujZkXSS8yGR38ubZzi5d63/3pZBYwCLDs7wtc6v1gHrybT03fAa1nWsSSVR8dV9UZHlWj0xIjipPuwHk51v5fr5bDmTPdqy52apijG49O7UhoG74ikvf+w4wqXLKDufmpWHU3iIkKuZGSnOF1YS0DC8C1hlZuNG/v0MvH4BdNYm3PskmewJAU3YWfwkNgGNbHX3lYMVVdAUUC0ozbKgyFXpfz1EuqIT6wC7HLcsjWDDicufBCQIuL9x/nOdX1ye759mBBb+fbGbkzhKnU7WIrKni9SGUHgLG3CLpUwgKeP4iffffzW48MPXpypennWqsm5rYIQ5qSiLONWzWru4hgWYKldwVqaHYgsVbArsl1JU1v8lj8GuByq+RTbpEX4AGLpnRVkaUYD96rKaHmvc/XDueZeCs2epNoxrUAL7CoKEwpbDFKzEAMqRAJmiC1tEUTU5eqzgZaoGrbYgQDmMl9QaJm9NYxadLPA8PgJ9P1vOtipoqEGXtfZfXkkd30dDnkcidBslbmW5Te4hsO2vOQNo1ZeL8NCiLZ3tx57gXaEEIFmpH1OFQy98zi/8e44xvm3Ppm7NOXGZU5HypquO03YTeVhCp3aJEwAhXTFI+t85gzc3NfVhvce89kBn93tpl8XQmGtQkuP12upjEuDAJZlycC7eTNgA0Sv1WqIuuSQbObdpRfPtbxc9Qi8LhP3rEITYLu5yPSUHDQsJHja62H3UurLr5WjgSihB32prQETqZoR62zIYFSgMoqc2bZBQ2anUbVjeo1ii6iEBV4FkSEX7IiBCCoC/uquGHZbOya4OocdbRBGJt1ezdXzz7ze4vq4ZcSsWepJWSSBnvvktAeXOzuNIVhB0f2zvIgv2Siw04yZDUj3UyEYY+Cn3zt+47185xHA+vhm2Yc9eNmUulEJG6RpSXgNtqJmQszEGDwGtmQQr071Gx/eHQ/bV97KQ0brGphkA9pO3D1poiXkXj5YO70rFr44sElNTNcJSiznQIYUwpT7RnqhcO3wnmUh1dS0KlWaar/J7NJkS/ECy4dkRmHlViCVsntP1v01L9hBUlV7YlFlIZ2kbXQ2kgX8s54fGaGMSio4DBIDkSEGBhhu548ki0QwSZEV8E/cas8l7Pp8B5QkCzOaVIvs4NKICiSwZV0f8rjxNOv2fnpJ+9ytZMa6s+zdZ25mP3kQZ6H8OxFij9YUqQxPqXOXIkhlYASvDqra377i739/Y8TNfeOaDnhqs1uyNZBe9JR62jYJRuowIgMA97YdR4nf+/h8+7D/3Feuv/xkJNsEHJFLgPOCSmPAcp+vCXLneG/51VDtGFuOp9UDjaTZHa0S0o0SwJIeNJcC0ZANyJLkiqDc52Ih2HnJLhhArFnl6kFpnzOstVnYa+OKIO2aKsG1Tvn/nCgXYexAgg4AQQaVsedactHLURlFIClEZSjJgEMCg57dnK1COvy1UiRPMQ3uESVEdmPB+k6fvv1IPFMaGU+vx3Hwxd3p5b1W8HORpan+hTkgZMuk23mi+0fMLydceLABpVO8mkiT6XF5oUdb/MJXDn/sJ6+2wA+ev3q1C8sh6RXsiUHVO97MuCTjhpTbG4Hg3ELdUiPMOkMl1P/1m8/ffHr1paebW+g8/6vTDkucoljNBtlaVJsp7KqwONYmKHX4o8hLl7+KmGpfoMOtGtoghebVWMbTqp6i6CIW2voSEh0PVVEsKyD71HnXvjugNQ+uHozRwbZ6pJRtRy69zhGXiTSYXCQvwz021V02FgToyJFof1aH1aIypIpCMExE2Omrcxbsq4WneJFy60RXmUpcvUW2uLVoPDP0+GqQ8YPP7l+dqq8WKQ/Td0XV294bivvSAbHgZgEIbmIpgj3DgRbEE3RXQuQIkKH3ruPdx/Hyfn50c/qnHz7U9L73OdhiZFdgIz0ZOkcTeuZalKEp2BiXARQ8O+fV3YNOL99/UoNVPVq1g9XSuAqRlkywYhFNF41wvMXQASOCnrfcRQG6st/H69zeJLAVivZTFR2cDcjRTUduPiBVVRF+0gTojoKaRQKnydPehElLHe8Curi4Vkpl8SsYqjlaPlM540W7HzKdydz7h0TsnWSzjQ61NhkUKoERnhJQkY6ii2BCcv9jQ3FTgCLCQklITrXrUtMmwthybGPcPNT3Prl7fruvdhc0UG6xradFEn17PPTayZG+jmt+0aIB3ldO84pgBt+4wtffOPxLP3X1+98/vnqY/+i7Lz554YVdJDUNS2uNYmTVJXNizVBnqYV7KKcmkWMgqnayFL/v/WNgZjw8u97KNosyichLP4LjENsOhku5z+0b7XOwtqFuJ/T/r5Yi1RlWzeQotNLr2gy8J/tfzJ0DlyaD9qiW0yE751Ei0wt/zjp3g6dmAazqXbdCc7UcgArh7Fg/LMMjLSo4Z9kfjvRtYD/4wPPSCAizbDRQ2u5QGSzPbEoyBXUwJh1IbSHqbdaCaXHV76LjUbtmbDHw7T8MPn913ndkBjHLg4LcV+d2utfPvfBHy0NXjDhXT2wsJ/QivqiIHh22hd5/Y/zsB8c/9lNXf/ZPvYeff+d3/trv/uX//Xtnt3U4IbAHeHGRSgsd4c0RZoSTQMSEci9AydB5xl5RQiYeXx1/+Ontdz7eT7uhmEZiyS228LdkQWa3Y3WKa5NmK4cC4K5rogccsdvZHbIaTYJLAmjjirTaVaIJeOttvYJLXN1gRv7MUOvjbKvMvnPfp1DTepl4AfvtrXIoMGZEls5SDU+8Lfd/w8lEYZdeeEQMk+qiCJVsxnGeMUqlNv0xWdoYUTWN9loeXH2Vakq+6FrLccXys3Oi3wP09ZUOA4fBveYHb109PrzEaz3ZBtx0aTKiFpkgu5TU7JiGirDDmAi7ReHdOZIktoyvvXX4d//4Wz//J9/FL/4U8GQcf/CD52esWpZ91qX2nvuL3LnPFmTSWcSZqmyhZkksTYgZDODVw2kvffjy/LU3r776TJ+8qmNqgkmdW1bpfC8welK94/ES49FZ0jYPLHWDvcjU+ay1Ih//am90+bJ/bksVchkK2QJjrXnkDn70o4RcDZO4CydpToFdmyerxWQnUa0utiYcAljuMDNO91wZkowMGBdHBrfhIfIlaiAYmFMn7QB3AJOTTOyFCFGcjC6bGJe1P7/vroWy0uvuQ5DlqRsZhHqmgbXnbXBLAnz36WGMbM+/sW638pJuYyWJhOUMZEYkK4zE3U0UTAQ4OboQyuAgI3AY/OM/df3zP3GNX/wK8KeB52++8Y8+uZmWQUMoRVnPbDEzzFWt216AqrlMKXZpyE9KmMBISpooffeH8+W5nh7nz33w5Btvj/PcM1RanpFW/LtOKlkJx8Lb4TJUy2pRLM+LsBrvI1laeQFR8EzAHos+1bit1Uy3lC6NulXLWM2TlylKLPfq5Q4//YH7xNmjyVu9sFznGlaVrcxdMPFxJapGhqENW5ZjRYBQBDLrOPIw4nCIYyaILUni7uGc53Rzr7+wXIIKefQS2l3gZhs/ycHuWcPVxRItoPrCJRuG9jNKQFZgnHYU96dXMUtt/eXesZALHHvhRIUiQoOOveGZqC3UGs96vmFrDoxAAl96zH/j557i7SPwdeBngJ9+cf9XrZxE9RCkJXc7YVV3ohqcotl6YXqStoCpateNqqirLd57dizw0+++/PD5HKx/+aeePuy3r/b64a0pdzv/XZnrk/OUETlwrsE3HpBpXtpkREtXq4DzDfrRMGvAQvXTjIortqmhnOsBLsQspFOcrhtRIEKc5bYgBjl3nPZZhSpVyyQWAFRWyjBfp7EAe9CBMsIFnJ0e19bCUoyMbYvHR77xKN58fLw6jscH3NzXRy/ys5sHO4Kh7g9o+71LqWs6OeybdaHDLKcfcnXBEr3SsmGC20gRFKXDCAhb8uq47apsGdLihq+NXIy2V8diYASCFd1ZC2hfg9Ycr5VApEiOQBJvPYqrQ6LtZ/fAD//bv/HdVjbbsOV+jBZTO8xFRdXUerxETfjoC5UV6hqtRBQfHvTlt7YP3nr2re/fXA19fHP6uT8Q7/8wvvnJnuFr4sXaG3Bp9GYCBOQ+2G7aXnJ+F0icFpxVY0eFd7mf8tTDUCpE9rMi2iFBYJcSl0fIWFjwQwB1qWJxogJ216FY59KcQTKy5u6rVot1rmUHwFlLE7CfNgAve6Q1gmBY6xrBQ/DJVf7Ee4//0//pPwD+IgB8+h/9xT//V/dZ5zn30vCCWSX0iQAmG75WV6iaUPsamQwyLhihWSvYxm6jQM1Zh4y783z/7evr6yEh3WdZoW6qazNDd7PAGl+5SayZmUAMdeF8Yd6AH9L25uN448ivvrO9fHV+48kT4HeAv4IPv/c//61v7wVZOCdYywLr9pzFJ3ZnO9lqbUjQe06uNCgzNFiHLb/53Zf/57eeb4G3HuXt3f7qdP7S0/zmR3bLq3m2LJGDLFuvGrU1ap1yBOh80P1805MQmcSOiiKjtNS19SZ1870taW7B88CiJcRhdsnTT1hYygimBQGolmTC015kDo5TT4kDMMvdpCgiZR2mnREmMqGRHh1vNJNEey0zsI18dMx//eff7kUG4O3/4o/+wWfXV35K2eyhnF0pcudRUKkevnpRa7sZDl3jaihOzIy5FKTyJJQIO/qxDX7+6vTO00PS7XqxJUeyH6hGZDARwfQ08kXiXaUlpAi5s9mVsdVzYgCZW+C9p+M68td/cI/fvcdf+61/8p//jX/zT/+vz2/nvruMA7gpgezpLwuRVTtKLBoA5Ma0KVfLGWr5Y1dsg2PD81c4HlHQRy/rdCqB7z9rC0YjMLYG3di+2XrLa5BH+uPHPADsrhwrHT2JyCIvSiEPcVn90FNdEtLloFtWy4tcdFGhBXgkuEoeb15+rmVhN7l0ZaJ5cLTEjiGhLLy2H2dOaDgILMjrKtp6JCjoObGHQ6tqfv2Rf+GNX/qHH0cw6LY8wDNZOKg5Ax6tYqB5KZMJS1YLt/CJ4nnfDyOW/60TRiAiZhB76YfPH772zvVvfnJfii3UwxG7H6RWw1FiGaS6+OmJwE1hhycMdMXDfjMpEvse33jr6g9/7dHz27tf+7XPfvOj2//ub//o+x+d704qUNUuNXT/D0BQjcxa2FqaqKX9yH44VYdYTmIEMEv3e5Tm7T0/3fBkO18f+fYjDfJ6JDmBlhJt01rMtb+HSCvbaqy27LErT0wQl9LTRewG2uwtuDcXXRIoSgpP00vYd4Juay1PpIElptnuT3NRAcSu2ufYUmirGRz/LPFqjW3raFoshGquh3OYknbnse0Mdqfwfsff+5XPge9e1tk//ubnD3v1RP1a7B8BTiwXLZqxmD45yKGTQ7H3vQqaXXMEk/G6IgRK8fnt6Tznl995tJdUPG756NBPghkRkWGzryUnXRJKW4DKzokeVdlKmEhFgIgPHvGPfLB97Ske9ocPno0Xt+f/7Vc+++YPHj6/q5qXTjH1yqJWBvJpNfqVBQYB4A7NiSBDZdX06TFG7MB89aBPX54Jnc51+6CPbufDXv/KN548OuDRZmjjrNlfwnAG8Jjq5fFqStsovk8bi8hXr/lVAqfLCdX5Ixxfegg1KQ/GbxnddXBOOQWqLfIeQCx4nVZVFXZxn3sVSpyTpSpp9gAr+1fdA8HuLmiLWw/t8p43bDQHnqU6Tby6r9/60cN//xf+LeDPA/8ZfvnP/t/fenF7jwePhHSlz4uGl7P3udWa7ErYS2g8td4mNIcmwKhyMKIfYhWAPr45f+WtKzzd7s/7LgRjdF0/R3KLHNlwv83ltPgaCxgPN5YZTEe3JpdQI7ANHgefPR6UvvOj+7/+y5/8ve+8urnX/dm2kH4KphpBIkD0NHuWUvox2Nn3yTs+iMjgPuvmNO923NzXZzf7/bmrIiHdnuK//ps/+LXvv/jZLw1qkWdoFfW7WoE2whT8hGi6RNj0xp55Uf5GRnhDs5+Nrd4T7GeWCSBSnbccR2J5XyEXOlyIx+WUCEPiUk3AUw0mZrFKpTY7TvnlacBVtQwg7duDKsZFgRaC3LEiQlVUYJ969TA/enn/d391/sM/89f/xO9/cn11fH477x72fd/3qipM95eBVsixbIBgoKYWQfKwOjvyoldfiDFnRK5+Mkwpzd/AqIqf+cpTPD087FLhoXb6WdquxwGg0mMdegfCg0PFCWQ4TThIWpRkEHyU/Im3D199wp/98tWz6/GbP7r/u99+/ve/8/KzVzVr8UobB9cig2jb6hpK7x4/b56Vr1sWnzvw9iEeznh10t1J5xnLgEvtnKzHR337Y/0Pf/ejv/CLX/9TP52/8dmrh/aAAd0zATd5VveTvvYIS9YQ7F0DV0MumuHKjz4iCD843pJrd5q5PTYbJ/sRSMSqFZ0vzxmSB7xyVgXZDyStIsgZ2suT62p2tIzVadStjO5Na28m2um5g5ttNBY/7CcpaE4Sukftpft75Jj/5Lf07hv7pzfz1Wnfd1XR0xQKXRewAA2BgdAs6uHuPAZzbAiWZs/g5KREitrBCBzWKKAAUNKsCmgb+NmvPsP14e40S2fL+RECxlgloKKomK3k9HMYyCHUeszFJeEHwQx86QmPqHcejbcf5+3N6bc/fvl3fuPFD1/MlycCWCXwRhrCpV1zWs3u9nuPJLaKJvpRhyBqYkscDvHlN/JbH556bfrCSqBe3eHhKKB+46Pzb3788hc+eOMPvvXwDz7c25WFnuPcCIxc9W50MXedSImeW0u0YOBiZFeb+rlGy/qoC+jvHge1TbQgFiamF6ydZs5p2VOPV3tnj56e2nfD46pZEQHupSajzUj6mS9z6Qk1up4YgdqryXXZ/0ThPKuK56mH2McZH744vTrVZzen8xnnQnnUJUqVl7o5MJPp6naQh8G70/mI3EbSxl2k96Z0agkOO5gejhwRUFVF1RnA1QgE786zagvusCmOXfyBg2UpGNOgKLgFi6pqp0gnFuc44jr1dMvHh3rneru7n9/+6O7vfOfu4zsqtqujT3bH1PTcY3boNyGoRrhdg5Y5LUVP9bQxmSjx9qz3nsQ7T7Je7Pd7j3UwOztPvryvfUcQn96cH96ef+C9w289r08eRHSUXhuDTthYT+Ow/q3GZW4X7tqO+YM8p+l13QAdljvjwF1EDoy1msF6PpTWPIdwd08n0ImiaoJV00auvXKftPetYDuEq6JGh5ekmJIQU/h/23uXHVuyJDtsLbPt50Tcd1ZVVqqZVf0gwIbA5qNJgAAHkgaaEhDnnOqT9AEaaqQpZwQ4aYAgQJAEKXY3G1J3VVeyklV58z7ixjnH3bfZ4sDMI/kNwnUgE5k3IyPiuPve22y9zEZTGyqlcd2xciC0IzmSLiA4iXU3Mm9b7lGxfYTyQP9K6NfHSCmlIZ1OnrEpbrbcwxwyPWmFZ1N1wmi4oE5zad/n3OfdPV6cDcOua/XXGAVdHgTxEVNgIUEDDBFRVWi9EH3W1E7AQf78zfL6nj956X/1Yfvnf/bu//n14+OmAOhYULk3bIt6KIq+ZJWr5cip5q3eiQq7hUrHh9YjBXXbdJ35T/72698+5j//Dx/f3aLL9fIjEuYAcJ1y4x7TrMroOgqSPchRbDFL57MdeUitNKr+G2Qyy5HVsyifBoDwaOisBPuBEhcoD/yx0n1+wAd722vXEpEi94Qpd8FKr71PRh4ZOsf2WPYiMHH4dYp+qFd4VOecR72r4hvtaLjEJ7SXhm2PkLYZWW2WUlkDvZ+AQR1JlkdooA1zR+zPRtyyaIMSYzHhxGzsNEdJ9pSZyDm3e8Pf/oMf//R//BLOda+obU5xSaQFaN4nBaupd5b5wYVoTvBY1WyPs97c8dUpE/avf/npz3993SIyRUTJTaqaWwaV2AvQC/Vy76iOp66g1Q/oMGhkGXoNUpO5n2a+vex//Luv/9+3l3/9VzmzvWQnw23iboDA95f9+dne3C+f9lk7FBCYKld9MZyolfO0QTVgwdq0VK/TgewItRQqRP+o3iBVAyTiuGd9ZuLoLCGzSnfXYfGpzWlKJkUKoCJT5DYVCSqERJ7rSUT7QRyK4l9xtL9ADAriRHrSTKlG86uRykhVEDMIprYpBma/ZFAH9DZVfxwwaMSVs/ppd79t+3kB5NeNhv3Ja8/OqBAZRe4BypiDHCP/8Os3eH2H1GWbJT3NSjnPDm9BCV6q8TCMtCyGG7X22xpTN+zF8N97ZdeIP/vVh+8v02hnF0xJy8QemFk7GZJmjHB6NuVYETh1H7onBwAVlV1VVSPuAKF92j7xJ7+4fPHyfHc6LbbORD39n73mrx/0uOH5WaeBVHz5jL//mn/63UQWBAOlw2RROstUTtDE4WPJKWAjDJpAG+n7rO3qrVowqhnj1oFWJ6DCYsqtiWYvakeJSTM/5MNFVecBDNTXZHHkIWSm0jLCLLLLNxwuOiTQMzaTMGX60HG7CkkzeMMOLbEpHq11VlXBKdEZIV2hGLrD8R7Gq8NcUQC9eYF154XXLQ99XhAJywL/o5XvhpwZQeh0Xr58eYYb1nhca6IFWEJSM0OFWha6VfxQVudziJoLlK/dXyfDF8+4LPw3f/XpcZ1OHDW1W815I7aJy651lyh3KnkrYDZL7VI7XLt72aYOPQk3VEG3dcxl3m5B8//73353GoOAw0KZwt3A67O/XdOEbz7Gf/lw+8nL+69f+J9/t+eBspKWtUdgQIokFGaonBaodv2iry2q4ysVBIxPeaoE5LUUyzFQoMuTiqf0mKSgoYoajeipsFCixgoc5n9ZHEhlGYLdohQbFQbKQ70EGpI1yKpwHEFPMSTdgpLWHTLiGAILeypDOzytT/3KgizPipOVxN4ETXXj7KYXxHkZr852wE3VBU4ceysRfQdhSpD57Gw/fX3GswFy3aLdNAkJkRGqeVMssV1JUluQ0hU/xaz2O4GTkW7/8dvL9RYU3DDIk49hiLBraE8tjjd3+eaZ3Q/zGvnTqHMQfCquG/xko+FqmSbAVqyDmKmEzR3vPun7j3t1a/W8f/WBZszgcPzq7fqv/vLjGPHzL+yLez+PE22ICE1ptoHTRhGYkRHzhgjAUhPaRWRKuSO2yMwooQQ6RggtaofUQCb73DmajIrZs4QJLjYK2Gddr6Zajp7H0yScPQKgeqNM7cqZOWvkZlQzWuhM7QDCABMa4HHDJJqr2NBubFq6A4ry2htLI1YOqd4rgXYGdYt7hOYJQSpxMixLYUOFG6MS5LoIbCt53YMk+Px8+vGrO7y+x+3xttcXiDU+owoUKFhoUN1EPvmR7ADru7OQnc/2cF3ffno0Y4JRYfOSGZaRyLHuce1qPk8LhmMzk7Rlbv05+37U3l37pJPKfBI6udW0Igk4Obd6wlIkfNCkSDxucg8zjeEv7pdfvd+/eXf7B7/34s/f4k//67qt7ZwrL29opwYJIRUTkxjGHDhIN7NRy8uQxKhFn8euWIX6f6ehqDrjaGer12y9kUBX5dOXrKWjBEsSMQvajB67rhrmgXovWXJaRk3BaFTP4qjPulsqEwhQpUgBup6V8d1GN9b01kRWoChLHXGobN3MzYaVLSobyK4PYsoMJ28z1q0Jqn5H+51Lt2O3hgwBIsTnd+Pu5Hh5hvs2Q10AdkBhihIjLdoFltlNUzvP9MM9glHrnO8eV4BGngfOTiSuE48rLpu2iJQycwtdQ+vkGgi1CQogOqWyPxK7sPAsqOFJ5AYFpwAAG9xJREFUviOTsLgNY0jLUmN7W9JaKvU19fZRCVx3vX/cPq357accxP/2R89OXve4eUwplQlFE0QFVMaMnADcFjOnk7YYCbq5V1xOYadd/lRtxV4aAg6vSo2ztSd6KquPqsjap+6AJWIsmlKs8SnJqJHN8IRnemVo1S9Y+Ej2b15bfhqaBC0foB9xV1Ff3D0JdUT0WsoP9KZ25nrJ0Lxkf86suXpCKjAjk7FNPm5ZZ0stLwmGYcAyfFmKQSr7lSl5f/Jnp4HzAnKdSVqSx8gLEU3CZccOQrJmvw8BfbE158V++tIzMiIIuJtEMIfn2XO4itF3G6eBFye+OY/nZz87h7kP0HwxwSp6zVWGwtova+mWt6PVZhldvfBxBZDnxbdgFyfVngiRuO14f8nLpsc1z6a/+M3689f+d7+qLSSqtVXOzFBCR067YIKTC7jQaDbIUbGuUubcY0ZBFqDenMfSfkMDDoVTnyFll2A3z909lPibKUbm4fWSlEFmdumCGuvYm1Z0Hyc9bY8iJAcqlahjlUciLEgrR2h2a6lix9sWaCDpkFfSZGU1AFMHe9S2o4LPSuCk6P5TmjMGzM32iMOOQlZwjRLwYYhU0IINJAAcjtfPB0B8ul1vIRWWK5RnpcQ/hybAVE1ivb3FnQDSixPunfcL3j7MVM1BCcIqoZmo52ZY5Ba1Bqv3TMmMQ3Y6ZUTZfVmurTzGDxqKMEdLGiERnpxME/ZpGTiftK8F03YmWNEULkTgsuKrF3nnWBzvP12XNmhtxMlQNptQyZIxDZEI8lQNTioRQebM1Nxplm7UjJm+yIWXd7xMg2blqhw76t6Mw5PKAUjUaU9pCtWuC9wYDvIHb5ukBEd534vWL7jDD9qs7AIFcdjTZqnkyER6Z26gsndLWqR2BpK4W/x0HnMKzESUErdaTSBq+FHdabfIRJZyF7USIzKGaXGsIWOmBlEZQW0emKE9UU5IMUsYnZGvX56AgVtc9x01KAO1fScRqaWl8WVMMpbAvlSDlb5853aNfHzYY5Z1IFIL7Mkaa8NyeFs6djKiXEwm2aygXJjbVIkDf6hsSJTGr8RcPXyBgphF3wYyMQgbp9zXKI6w271DDfu4Ydvxab19/cXdy9NYlm0MmzqDo+olxZYxRcBqFHBKNUIgCU1FqtKzNfxkNg5JQyT9m4/ZuIYSGYpExRQQZU7BodLLLFS1aKIQwgqFLa9gyy8AZCQwmd4Thhpbglqmy2gqrpOTatvMRI4QvAYA1PPpb1CJTgOKZfBHr+7uzsun67pu2CNqZBOhSr0iUxjFbC+OHcrqz2CooRgJOva0PQANY1NG2cBLJ+2yBntWRELg020e8w61h8gGqZob0eAhgSINqVSY9wepZIqUfVzjbtFl3aFocLuVBTbMhycQBpvSnrbtlohEqxqcmSOVpaasoS4q/KwiGDsU/oBuywqXUmWnSJihxe189rPlu4sykcdgIAlOfvGCD7vePs6Pl/mzl3eAu7vEFmlJmQMIZTbdxU5h6fo9izOFoKL+agfIjohgiW4yApoSpaivgBQsbw2gKXimC9OANsQZCGdaUughBF6yqpkR0kzPAHrtpUTrmUU8ksOjAk2UUMYo4qiOyUKKpVJAOxUyuS/DO/QAnKW6qYmcs/D3w4ZchK5RYLotykgoZ61+v87IFFBosAPHxEAwqsq3qjudNErffVwxBQDr3EOVgln0cP6Qi4tUWA1Sq1tI0JyKFBMzEreQQoUB1ROisAx4GzAQ4gyIMdxIT1gmoZDg4XItC32PyPY+qKmAFk/ySJYKkUoYZ8BoUkbiTAJ5o509MzGrGgEAuulk5s7vV7y73R6384nz3uPjPgp6zA4magyicTEUaWdCgmY9MFSpydlfHZqFtwHZ9F/PGahOTsaanzJNFRSaR1dadX8V3kUqqLHR6rBF0TIt8uhVamRv587V5l7faNQfK3coBpLp9QrTFdRSwLayZstgzvn+8WrOmEf7UZ0t3RiZNZOowSEFu2fMSCATMwLSyXOYtojeZpUZ0QMYNTM2wTuxrzJgkO8+hSKJgT33fSp3QKnBOrG5M4rWrL+MEBQyYCqLKkDaotiTTFPN7iw7Kp3htJCccqv/pFn4gErhDcqoGRlOa6FsNeX1NJt3woEQqeWe9dtREmYy0pQZOyJac1NKDMAy8/01v3iGdx/jw+t8+7Dt++ZzumxHIjNTyCkEikaGmRt9dLld/ppG8wFFnaYIKWeHmkHuMC4l60kcq0Q6xqgWCGPtm2jRHQ9cvzK1s99tmGEKhZmxUkKbCGpepw7EGtdU3XfHygwBFafes1iOuDrUrw6T8uFxBdwNo0LfKSSiZkahjI2dJThV1Yn1gJ/MnEEioX0WflrbdgLlMX4y4FbKhrfMz3RZ48PjfAN9+rjus7R0FHbAKJMhq5gqnCQZBJmIUCvPbIyaJ1578FJbyOJZlEHh3cNYIZipUTFxC0FmgLlBGDySDg6FW336So7VIW01do5qZaEJIEwRcV0VuxbX+Y6xwqCcEGiWkZYZkQDm45q/ebwx87Zvg7hGTYtIaFcicwqgDHZ6/Tu/u14uj2+/aQ7p8BFBMwtHUKBl7RV6zyPeDEfAirLzPLtQlEyVqNL9gVpgUsa5+tDl6zrk7H0UAcBUZ1GR8B5HYighXRpTDmJYxy2Y1Mg9u6eqP5TSZLACl+V4cv00RdD7Z4kLypIwLBu+UjeQ5CA5rKIagMSaWbLgYRy0I26kEmYMyhR/8dvLG/D9Zc+oSq5mkaEV6U9By4cUlKgaqon/0ZuY40jnO4+wjl1yiMMKTjRCblxIKVJjz3Zg9O7F6BJZLYoAhRq91X+S6qSaWnAEU6l9ckDnhS/vhyz3SGySoeWBiGVAwE/ux4/vx+PG53fjYV8rZye5WqIs7eqViRc/ev1P/9n//ov//Mt/86/+xbu//g80UqHarvx8fvFmWZbHj+/26yP6l1JWL15OJ1lZSRAQdgDZmywIvnn14o9+/2dvb/M//+Uvc10Llz+SP2sek6RBTqjtLU0uy0oiL2UiCOZMHwt4Ik/DTmk5nt25W6knRbpZGpAt4WcFMxvpxBgiI8N2GLL0SRUxVLLpdAvz1qsnOEgwqwE8LXF/Om09DEQyzCBFeoK2lGqkIApoTw63UP6nX7z/+1gf1z2lIrXAtm2xBVhoegJR22ALG4nBdEOEpTZavUmdHFY0jgQnUrGwDE3aE5FIcUBw7kjlEfl66LcOvgFPKCieVrapJBYEywPrjpcv7NnZ3UcIp2Xd93RD9B3WbeLlnV0zFudtyx/dj7PjcaZhmgLpxojiUZNJjdN49eLV//D1z++fP3srcAYMxA45fTk/e/7s/sV2ve7XBzbuwtRuWoQqxGcBFIVbmNnL5+f1dttn0O3rr3/+x//4f35347vbv/z2L/9TJ02y1cpWCk9MSMrI9MVBRmEZVe4jo85KlZ/Fw3xBLgDHy7sc7rUDDNdpWFf9PYGyxCxpZpASOQORiszIKXBGGTHTKIObl/fAMgPE3Mt0RKMti8UWx5CQudsPuOAYTXOlgYnFOUXs+I+/eIdfv/t03Q1xGhaHNjZVTWEQZi3rK+I+WlwvLotByNjQCTxZUbk8TosyJblhULMAP7kbh6abbckyGlZ4QhXTRkIKiEG5Ms1rLGaRA4SK6UZF6DCmtl33Z1a6x4s7v94Cuw6JNi5XvPjS7u7cnS/P+J1Xy/NFt31Wc1myGGKv76b0t3/9y//r//w/fHnxq7/49xmgTWSx9uEZ7379y8uzl+vjB0WgP2cdKbuhEgnwZNqCdP9y+epHrz58sO/ePyrs/br+8sOnT4/b5fIRQqaEqCKu8Bu6UtPKOVf+5OoxQMmLQuz3DWLOPXbnKreMGJdVbmFWNEIOH4SsogGMVI/3LbtStFcOAKDFaNH5C2U/bWIopZRLjIHvHHvq8RZvXsXzOzaMa2PfBZX4jOexGDmVkpUG5ho04zffXfFx3SOHj1Rp8SPLr0RJVsL/4hcOWX8lB8pdEbX7tHsERwpYVVqlnDFtAmos01K4V1ZSzxxugu2FctdrJJjBy+rQcsFihjuBsj7+0t4kZurTNe/v5hidiDOcM+lRikYT4v2DLm902eeb03jmuh8crOREC0o5pFAtXjInvvnTf4dyK1XH1aAKMpPr5bJeyepmEqyYcwrdETfUxlZvret+ue2XbUMiOX/1//3Fb779RrT908dSogItOjcUEFaJvDPkSqYM6aGo8Wyp6orrZ9WQExTyLeVY93S3xTI9c5pBM3OwgI9CHFntTkqRJqW7Dws3Lq6KEXBPcgBZ9x0Ts15r2HDb95jJk+vuPArLdPq27VXcDdMXL/w0WheyzuW24nJhJq7bVmaan7xcIqZIpWfWkLmuDwlOhdJnItKlTvWBoIwjhrTEV6WBCWBUMCww9wnzigsDqZlCxxUxkxGAuIdFZgDWFGcflFbJWA2VN0n8ZJA1phsA33fgDoSPEebUnhDLwE/HZctv39vffK2/8dI/7Xq2wA2n4bdtdgwBkpaWXXgmqwgPB2gOKdVHjfWJyObBUPl7gcolVlp3Mz0Xdb3im9vbuo8ENGN9eEB/iGygDTzqhYlS9aTDkSGMJGcPHGukvPVudbYIndMO2TgNDjcgjWbgjClW7IxKbknaDIUwI1JOyF3LgBObxbA8L6PsLlJmemRmYps1NQNmlplJPVzn87tTFWiDWW37MAB4duLLe3dDSo+r5ow9EtBMYNOM/OkrUwnFzIxJuhkq7Mk8gQVipoUCskB++07ffLcaHEwvVZxYeb7Otr+RuUcqYU5pTnWZRuQeVrLk6q4jpGPmJohq3JnKw5Va6AbyEOUVbQGclpwzLpu9CtiSd8DzO6y3pgYFLEQAD7f8cM2IfEj8/Mf3310fPtxm3WqzyALCjGTOMKWLGuQyahPHHhkpZAb90GtnJ0C1LOaY3tvbeEA4DCmF0GTCvbUbUL93VT4fY2kbYg3SEwKDrCOQWa1KtRo1sblKFeLw8nBEqrzWCBFp5IigyVE4XWXIAcCw+uRyl1tLb2ZQwD5BhtRwOxjD4DYycH/CJwCJ37yP5/f54myOmODDtSHXbeLPv/n0xfPT7//09Ow89pHrntseKQw3bPHpug1LgIvz2dm8cicHTsbFuYxhjoEShLmRW+Q3v701S1O1OUsyULW7jrFUyslllPgHma0vMjcvyWBqUobcQ1YT/I69jCpN5vEdm9tDtwtF+osnNwHrFqEkTrA4LRwOKbeACfvOi3A9BZC3SYKX21zcFp9AZJCgj9JJkeAysO6YE+4Yhho6lL2fWI317MCNgs2fiF4CmTUYsqVcAvlU27J4MCMbjW5YLiHIi8JVa70AysoXLFkqiCFFrcJMoAXYZRMoNzmHF0lOqyK83HqRNgXRDDG8dCkqQdOA3MyR5hQo2YxYg2CUQmWYAeYGt8Sw4cuHh7nutu757feXr97c3Z9wW+fbD7PGKkXg19/FX//mdrnl3/ubz7ct3l/mumNxvL4/IfPd4/7xksuQFlsckqXSk+ndOi2JtaoBKaWHG7972AwH+V+3iaZK+UYDsZHDfE1pDwos89jSjF9p00F45Nz3quA4Z4+Zzo5wRB7CWvFpYolKgleHx3ngGmBjLnbyE5idPUwCiIQ7np/17ra9Pp/uXQaRNsx2hYNmHIOpNIMV9tXgAAlGRqaxhyakisxpD2xJSDp3Jg8ysoAKGhXlFzn+EMAPCV6HAqNXD2mV3r2DI6VMSx05g8d7SXQcoAiqxjhPAoSN8xi0SNA6ZqenPNfPQ1q9k8eM05zJijdwwC3NxrCRI2rsHp7KYomgG5Y7//LN8uu3k8Jv3+VvP16eL1w3XCefSauEestNtzXff4r3j3G51tw1/OHXL/Hy/P4xvn/EsxNnIEPDg5ZuTsRjCYlIYu6JGRLs7YNFyEze88KaGCOroKobj1QAnkWT99ZdjkJMaCYiNCeuW80fxeLaAweO0k2rVTtxyPf0w3sHCOuey3hKcoCbzicsbjsLUhFdIM7DL+HPad9f1tfPY7znXTITy6CUbji5BNGoMDLPQyFzhym38MUls6iASRU4qjqkxGA6CY6SuYJP8wl0jKtHx3SLGemleSmeUtnZjjhIB2LUG5ldx6lok6oLRQKDNZYJIry3zNrPzDiz/lUFyY9RCXhFM6VAyaulKOe1W/ScR+yw4SDdIiphRuQkbWamuMC+eHn6dJ2PFxC4rrytCuHesE5EUtDdSc8Xe/bM/+uH7fuH9bZpGEn9r3/vd/DydFnnzLxtJnCPWFxOmgc0AUZWZidv+1x3zsTDZXXI0WMyKudUMsNk6VVqJrpqfH1GFusLF0kveWG9OCnc9loxqGFyZi14yg6J736n1A8JOqsVQZXTEVoWujvZgiswjhZGKZiTxsu+n5e7d+t085f3CWekoEoXRDfYYJqPwciiEwnxLKUse8qtlVu5sgpDjpIMiDRFIpLz4CX7zQDaqQoJFTZMIWo+YXbGduOUJSMAnupS1vlAdtN46L1rN4NQxLVEjsQscDyFGUmmnAJHmeJMNdaeyN4ZenwYKQWGYWqWy64G4SBVLqBI+Z6cKSO+eHmKuQq6TYVgifTCOzOEPSyl629XoyI5TMNxf+I//F9+F4utWzw/NwwfMkROVKgDKsXhtu23Xesc9oOAFi2sbQg1WoXJlMGlmTmnzif044eROVxg7lFNeQRsRm4TSvioASpHj1uwFTr5rB5FLUuC2SRiaTDx4szBApZzuA83WHpiZvPUEXr7KdcfcZg/rIkUklnYmbzcIUAXf0ct6PXMnWEGcwFLo2MYhecpKSyoDaSyaLpZVUeUYUKcWip7tWWjaXn0PFIdYlbK29IUAgBtuAicht2dVG8ZUgnrdB/rX5hl47Uc+/T0liEYWfIuBEIlxS9EhCSMu0Tzkg4ZQVp5Q6pTy2YioCiiVJEwJEJYhr16OW7v90w8P9tPXtr7x7juKWEQ51FKYaspN2cXoP/pj77E3/kKH7aU7heGUMApMARBkfAtcp1x3bAHHQlzzOkUGUaw5zTC5Ee+H8oPYpl3C8w0FVURl8JQKgVEOUAOhLZmRFoOp5G3rciVLklay2eHrkzoNithDtbwYxghM1fmadDKHlJfQip12WJd1+umy6ac+f2nEEjWo5WONpCc1SeaWWbbOo3pBLgfIKbRojsUKNNo9HIw0VCaDJsHO8mTtZHsKckNNCh0yFuA4+w8mMuqytzj+R3Pg6LXrNnjVWUKkZnJGX1kjXVqZC1KGukygFOiitxkMTzultWBlhqFXVgecpzDvBhyM5bqsHh0q3I8786nH72yD5f1J6/8Z1/evbrsf/XtbQOG4X6BydeZzxc6dQmA9k/+0c9wMry/Xm97BbhLilY4lZbTYOlm54HTYIq3dRpQ4pE6aHjE51SpDtANJ1ossQUjteeoE9IPmo8JM2zRSabHOLDK8tEY4g7rAsSekoj79aqds8LvyAQGfNu17nOMZfQ0GWTCDVMYjsVTMpGXbb595OKIiYdVi2HmjEDBKwEh3azjCp1Zlol6PMNANBVpPUgrm2WXSNU0JDOhpce94VcBf9ii+mXzUt9UQJYZEcdxySPnvFW3o5IqCFVAYg0dTIR4W21Devn7w8Y+M8yoTJCWC81HTRPIY+cs5DFr6QV6VCsEYB6+gTI1pEBnumsxL1TJE8PTnJKZmYSPjzG+stNid2feJq67Xjyzr788PV7nw6dQaCG/+vL8B189x/sVbx8frtu2/5BCWbPb1QZ+Pw04CfMPDzGaWRVhpkyqPCkdmqg0g5OXPV/f+V7g4HEI9pxkzVJS1AI1ykYqMKxSs3ReOHe/9hD6xpZKhRZ1qlQFIZHKhJ2w7fH9Rzw7K3LWrlmvpMMYxBCodQ7Cp2ZGOXI4wLVM+FbPogDA/s4iIxkdeyCZlVb4eL3LJqnuJlVT0pylCG2nc8kW0qxOMxTNbpbdoQOhlOTwZBpAJL18xRgDd+CuuO05Kvu6OepIMgNbaJ9WdWAqR/ULoipGbTfTzDSYielqiREkG0yyZpWF0aselGbIrVR5kBKb3Bx3Y5pJoOBCWoK0fZ97IiIva6xzRqqraeV5Mcnp9t27EOL3vnzx4m7gsuJhvaxz2/cur9J4kJzDzQ2EueO2KbUPCH1HrFW2pYTiNEAwZz5b/OM1zksm8WkdwVkpJou7IdOEYMswkU9L3SxnVD3u7h1Z2AYeoidUQoEOKam6cApkngcva368xJevT6nM1HnQoIc1BWyBTzedxiacnp/scZ2b6KabptFtNClZhj30wROS0cLBDEenaR57tkrFASWTNTwUpnqpC2UEJJoK8XQvE2hlvtK9YcfSwExROWlR+2FtnCncScvAnHlZ4Z39V3YpAsiSVargFAgYhZL1Q2g1doaosMwyi0vlLopWLgCQh7VbZRy+hQNEYRDco9dVoCKU2hU9iCnsMy433HYL5Y+f8YuXy2UNYaYMbie388lf3p3x4qzUZZ3bLM9O4YSBLsEz06tTudz20eQSSVVCNq3urDkrqCBf3fkwv21zOEZ6yf9FmXU3apU6qKgfFsIMG5YDWGcNoDE3mAVmK08LsC2+s8rsY05S8Tc8Lbw75WUtO7otDkFbmUyATGRS4sdtfn/BnNjT3LylDyUrKRwfkJw/pG3aceeRcPdKaqnkSgrKyE5rKOlXhTihl6kViE8rK4mxWhdLIfeal8bh/Usya7UmGpizvdFc32ObYccJk3VkESwgfwEiuQyMkFX6I5oWUDdgVSZmxYZngy9ISm5Wukt2zUMAGYgEzY1pR9a4NarS3e9t7yjAL5+fFetf3rZMjOF//Ac//otvP3665h6arVbETGHqtx+3j1etW2lXK3SggiMTm0gtw/ctlFMgNaWawkNK1CCycplIOPXTF+ctx8z9uvOyaY+MmQFbwC0wpJS2mTMQgT3ttqv4swAErruW0Zy0Dq8AE0lTtsm5TMMTWgAHQjGGzcnctc2UFEoTdwlATMJwm1h3/Zd3CCCnbnuue6cw5SGLV3NegYPuKRjCzaQQ5dXl1pHM+r+i4L0e7a5kD1Ux0BKjBkV0BZQ9Iq5o0OovGp2vTZ01lukYsBfcIzOR4VkTvtgiA3cZfZBTUtqo1Ng7R/mWDyCOTcKyYzLYypDu29FfzoP1/+Gf6xvYAbM4jv+hgWMEtU1AeHXiLXQLkBjk3/rp+M3DvG6QtIsGfPXK/sEfvP7Dr1/92TcPf/Kn38843ER4Cozscs0NmS3/LT6Fh3ajf1PrTHMjfnRvAn79kM8WRGI2KUJCzjaX1bDSgFLYhZkAWqyRlcZRvtYmAY8P/9/9vQAlHj90lLYbeLaUYhDbrgrOLEDSqUG8XGpKGbbQ1pH3/Tbz+IfjLpA996eehpp8PAh+VjT7cTf6F336zyW0PtR0x+NDi4br6/vnApWhX9+pm56jUXWluMXTD+/PS9U0rJYM9Wb0+fp8fb4+X5+vz9fn6/P1+fp8fb4+X5+vz9fn6/P1+fp8fb4+X5+vz9fn6//3138Dh2KPUWuMKLQAAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9S69sa5YdNMac34qIvfd53Hszb6ZLmWW7ysJVSNjIlkDCWKomLYMEtMw/oGeJDg0s0eEf0DINJNzBshCWMA0QlrA7UMJICBUl7EqpnFn5qFv3dV57R8Ra3xw05pwr9nX9A3QiM0+ex46Itb5vfmOOOeZjAR9fH18fXx9fH18fXx9fH18fXx9fH18fXx9fH18fXx9fH18fXx9fH18fXx9fH1//f3+RBACKoghKIimIIKEAKIAEBOy/In8kf6zfCkggCem7f13flP+cn1CfJCjfAO4/V9+wvwuqn64/UYBBAgUZIRESzPJq826g/T1AfkN/vPrPzFur30t1Y1B9zvN7xvP7V18EtP/52doAvYhAr+ZtxW5XQ0ri7TYJ5ML1t+V15Yf2d9wuZF+z/esFsv467yY/LRe5v7O/vC+et0WBCIZEPv+B+uh6a+4ARewfnzu9/0Ca0HfuRwTvFycCNMs9FAgyLYSiMEmDACNEQvWbMDC3xthrApFG1B0ZJZlZrQMB1oeG1Z7mO5V/hIEiGb1fA5h1/zK1AZsA5v+H8lJvRkQaFcrrUd0NKEkAp2S5d4HoBYYE0RC13hLBKcFI5YqkPUghq0Wl2nJzVW+7HgrCAoGyNRMABGRlE3k8ogwb0LMDmjYVUbdNSHh2mvMn6o4pySiFiRE0KkzffVP+zO0rUP8AUUgMoaHNklDsq6n9vFIiTUoLzaORvzO7HeYAvBa6LpXGuhAJvDuYAcZ6iyW4AblIFMUgrO0idkgyNHqUFYlMgwmSzIWnsW84f8oAMMjRRx1GEyYB0E2ARZ9CJ3vBATWIEQRMgiVilHnN/RtCsaOhAqKICJFgFFbkdkTAAEXsQCDt9lMmkb+jBCgEQ+FNoL7cxPw9dnCSBOb7c/eQe6OGxEa7UP5IbnPkHQi54kAUKO+2te9zHcUADYSmYGAIbNQLtp3kyRXzj0EhQFIKMd0UicgltsZq7R6AhUn5oWC0DTbcWX5ov1kyIY9/34gQFF8c7OY7ATZuEQjCgmEi2k4SC22HJ4kwCKSRIXr9aAIg024NAWO+u8EPhIlMs84bMlhvawFBnYr2Fe1za9+eQXkQpNVW5nmRpujlvBD59xHtqEW1weX/1X7LxJm7FRF5NbsLQORvCrKFXNL6tHyX0o8T6vOChrd9ZRKVCAQDopQovPtQRZ7hIBOdE+OVrgEBUQZOgArRGFEbCxJKoEtwitykdoGhyMMfunl5pKmVm6vjQ0XdHeqj025BWSRu0dKhGtRHVf2O3esaEFPyMdICCg0cZU9q98f6m8Q4SxRhgZU1npWlsTiOGQ2I/EGjSCNJgiTrjzCW+ZGwtsS0erP6YqOBtETUfBcsDZ0USTOQsLzQNMr6SIJKIxUMEOsFmAhL30diFEjRYGgIE62YaHo0UHntzJvSM9baSN3+22BR5IqglXk1ra2rzB2tCyYKEPKEJQ1KvKkfTTA2i2ZXzEPa/Jk74awtAcscUbhaNtyOiwTDiRCNAiwCdruHZm557+U+0cebReF4++E+PsUpAZhYnp6UH51mdePMJSjwsH0ZrMyqNnM3usS03HQrFLQ2lWBZC0gD5RANVmbMti4zgDSj5QLVn9smnbn/xvxLg9W/prOnkdYfJ9AokE7AZEn8ZAmVSuODWf9kmuNh8XRpBzdQIRQZLVrQJoq6bjPdDd8iKEfityw/XGkPBMVe1HJ6RgDWZpM+oPlGXmX5bqYnIFhUOL8//733oS4tbXPfrd0O0A6RAOlJ9fIgJqVGXUzys7q79ED9/t3nFPfu3U6qXgegv0OAi2jyRVIMykQ4JNEPw/tIyZk+svyj5aZRQO5+LQrRy4EiNkZPG7E6B8Y6b+HW12I3M0twMyq/0Or3ZcKJV5boyUJESzOjSE/gtNoSWRmZG6OR0kjbuZF1xIHe2v3Eng7+2YM5dTyaM0jOsGQ06R/7oBSdAXh/cKOtkZSXCUSGIjDqRapVKp+VUJEXGmXItZbWV2XcQ1BWBLP/GyDQTLfQC1DFGPWtjA7gkrJbgWsS/ty9dmnPD1BREYPKzVnjlPbAvPGtTaBojHVMYkU8WrXID+qggoQfh/VNqd2O9s/kDRnVVr9703IFVggelsQUz06Y1acW6pTrSfuJNCEz2H6E2/eZwUAzgfA20kQTcj+ciWTFKEkZCJODtQFJHJtXoMKZiu2Ogz+8x8ljXbd1237w8jAVM2TGCGutI9+UWwhCp+HLQIjXLRK1zYowJkN8Zgd7LKZGx6iwtGwvo9yb+9G+YahbunmwPL6w1m5UHKh+urSGQvVc/f5y5oeJQhRVwQ2kg7JILoGm81QenvKpeUg76oWsPLGVlaO9JtmHCZB1pEhCfhwkyvUkPCAxeAfnJlV5COvDCoJtd9SFyir3SqhtC9zhhdZYXnSqqFsCrZnBzMQd8LAbJQ0OyswAeX21WbOU5EEZWpTPU51hS1igUrFIFnB0+96dbDt/+6TzFo9XffVunTHNzWhmRXT77JPUIO8XHoZEW6e2uQclifkGBOruojnLvm4Z5fXJJVCBNtRrqHYORagaUxLcovhM8ZrENqm3JH1cE/mGXrtZa8cshYTfFWOCGXTtOiCT3TH1hV3bIpKdRgOQdmhU9E50bEZFkRNA8MXdLVltWnnZrz2DyCZe7VLTqFAEob108RMjwWDfkjVVd1ry0jagdK4wJp6ln4TBzZS2n/Q/rdzqvDY/K34nIyCa51db3WwSpgZ89rHIQHAYXi/rel3fXjChDyu24BS2KZo5aQY3GwWkcrPDwHFwOAQTcVljV4+JHf8Lj3ZnljoyiFYyd76cQKwGpQIRSITXZ+7eN3WiCjnUYkkBM3rnxMhrkErw1J8CyzKOioK4S95R2xflKXPn+idaH0BjVlPXJhK3GLo8ADJeVlF2CjY8mYeUMhRJRdKDvNoC1+aMO3nITS9pZ/dMTSTz8yOdGJnrLavjlb7PkJEBAJhZB0G2kSQ8vYgJyl9pxA1knp3HGJ44HySj1In0A0VnosR5kibgk5PO5/l4wVV2nYhIsQAhnC8bjzi4mwVBXxg7Ey7kinXjNtsBAqnsJFHjbTGTt0rBVhtqA+rsIAJkEDZV+1LeMc3USsIich8ApwWib9tKWkmfBlUgIaNFmRJuqQiBpdTl9eVH5JkwmDK89d2qVKKCnjl7M0SUUB8l5rCusoMO1HqnGg2glRU/uLvdOHVFZSQ4mx8kUSrV3lgGxRvdfQZ65fb3KBKkeccxOziBNJozfWZDl6UjdE8hw+TM2ELu5QKSt7GVDgNLAaE1g8vrbYLTFCfP54t7O5peHvXV++0cnLMD7yQyiAiGNIY3vdHumJKErRPnFR1dthPAvtxoc7Q6kLWqNxqC8jzRDqS4cRKOkjN2X/KMwYgp1Ox4iQoXVY5DCiselqaMQOsYclGs8GMHuWR7ke5FKtdcEQEVlRk0BsGUh2AlIda9lFrOZFwgY4+C8xAQIOWnUYuVXx25V3kBJGkyUSjaQ6tdLGDKD8zA1NrYdj6X2JV8qzwXITMv8cPYpgWHmSk5l6fpmDnppmRhTpL5TzTSU0cjPcOGImgklNKYpQFKoiVYC4jQD17Zts5vHmd0JFhSFZvICqFpZgYHm6oKEq8Tl9l+6Ja+3alEY1WD0r72jVUpfyiTUYTtUnvyLu55ZUT6kzap3fIySGUzmybTmamgqTd2dyxF3thnqfYdjQ2ZwYNgxsYDJOY5KSoFpzogaBO3He52Y6q/YDDJYiqHlSdIK1OwBEIzsV15etwCuzTZDFgKweo/CXYZpRbprm81Q5A7ISZohpmkJ5fJnrE0mu1sD4VF/btc0JQeeXOZdd+SaAzJEWGEwggpYCjhrN5P6rTY49MsUalpUDrb5EYS1i22uR6WOHguvgV42TBTCM9kXJFt3hLHefotkY0oc0GlZPegt2DSABoiCZ9JKtIkSaR3UrVwq1lfKQVqYMqkTgtX8UxoVvtvIhejkdIqqshjwYBMjCL1O9X0Ym8297CiULuXXxVn1kWXUaeibVLsrq7gXYJZJphblEAHUWQTkwpCe6mKG7JJWn1N/hzUDpE0utUpL37mFmZF4Y0wlwNm9JRIjG7mhBucGJ7vN3cMmhuHwZyDGMbF08PaQuTXWEW06QoiV4NoTiQOH7/166+OIxc01VPdss7JhIUInC9xvl4NenEySU6ZwSryYyd4MwxIDSnqq5S8s47eLShrhCrCjF6+9GGFN8WX0ppQjrjQ5Ha0EERhYRkYiirj5t6sf1w77FaiG4HMT6EjZtQnJdz04dxrFIxqAoHJgqAQ9pR5fjS7OITfiUoBvxvWTqMiSmOHw631N6zIKv0TBccliioF9xsEmTmMJnZmKePbGxuDG2VmbnRr0Z/mVpmBxJH0rZ7ki0rFIYmYGd3LotPCYNblFc2dbr+rmM7pNL2+X0h8+36rlW5aVwnwIr4MIALLwu+/sA9XO29g1TiYATIBJgWNt9CsvqvIOa2zR6gLqYwbhCL3N/a/O18Uk0q7L1tUiVWlG6FKlxxCJreTjRmhyrJbW/j+PQRold7vqFWlFLYZ1xWJYGQEQodmLZJulSAoSb5WOh0XdjtP9iml1ib4yZ3s1Ba7HmLHz473KrTsLAch0qmwphlJCaz5kzFAWCUDKuNUTogkMcxo9OJkMDPvUMBJM3OaWaIazeBen2A0N7hZ6oBGukHsGpRnzqnFysTvEoTWTcD80af29fv1ukVHTSxI6aigLBaYU4/XLSLvS7Er+fk/RuyCZNtMe5RcKbUfYG/2jcejjKqvEYK844pa6sakPg3l8kIlzYVa8ycoRdMPtQCgttfc1kyMdxhSpU97himdkpo1YdcygJZQioprR9nddEUHAEVRM5UFC/TTAjPLIgxaM9u8RJbvt+JdSVZRme2MDTLtU4J/Z3gajNxi/7lWyEgiYSxFWk8IY7pOyzjAymnaIM0TsehuRpopwSyB0i35R3uGCk9qjZrFaQdlQdcNf+a1B+LNh4g6VRVQsagy0XJX+tDPXo77xQg/DNRxtWjpN5l4lIa6Z0O4H310fVRfktq5VyKk3deODunEW1oqwswm8M3IyJk4R9vh1EqmqBUAMvVVmliFYlUpA0uFKFnMjmW7lFNqTK4aWrGpZEdFO2V5jYV7XY/KiEuL87vF+uzXT7G/0Zg3lCAebNeZASaLkTUhMqGUjDREVWxdAMadPzVitaMkuTtKhxsX43DzwWEcg8PgpuGehkhL0mYkvagnUCyUOxFpNGEfT4E8Dju43R0NxG98fjiv8e2H2djTuNJJukxBmDEEIYy8P1lMkhqOKS7JBpSmj8X2pFBpCY1SBCpaSA+ZrLhPAFrEbSPMdygXuXWS3lHsPrY22/pMoBX5stUd1eq9u1JbMWDbYdqIFSYFZPQbhqVwUtwe1lUbWeda4Y8pHQsFmWzPS2XKkBTlp6UDZD5ztHuc0AnYLrlh1ZXtdnZLOHYaPGtzGZ7HiGaAuSx3LpWztKp0ms5BmHEY3TicwzmMw+FOJ9zpZp6oZnSzxXvprLKa7PwP9wVsLbBPHgFsQgROCy+rjotPxTcf5oxKXksEPaWCYdgBRorr1HmVIV7dA7BlcAs+HM3JCKXMeXAdFqwrqgCxtzWBIc953P7KdfPojVvMEBxtemwLSikkD83ObMxu8FEBT5O6IklqxAAAVaahzPHmQnGTYcD+slYg6pw0kVWVglXCN/IiWRFz3uMeGqMUYQF+XCwdXuNxFVqbtSvOAoq0y3SMtbeeFtZZcLbsBUJ7+EiU9JX5cne7hZZOq8ofusHdFucwc+cwDDfP37svZm5mbm5cHG6WoWxZcp6Izr4iQ5pbzcxNJE1weFpjivdHfu+BP/9mblN92kFoGLVnLVN1g0JU4DLjugaA+6PdD//0hTPCjKSGMQCFBBue8cVesV7QI8B3j8ZoH439/5vu9NWCplCycbJSUqnIE0y+n3V+WfbM3e3a/gEUlK7Foq2LKu1YkDvzlHWNU8l+7b3LjqxLq/YKEj0XjNROk4VNzUnrluinJd1apkrTmFTA0Mpq+8Lc3Pqj7ahb4JcxQOSlONvyKSPcQDO3ZFTycqMltLpzmI2ENG9Icxtui5kPWxzDzB3mvri5qe/Hd2grKRmdeOwompWkwn7vSU+H49e/t8w5v3o30xiGZTgZaXMzMouVAGmyiLDrpqdVj+cNmgtFTAAvT7g7OMQttE4ugyFFpZaVWd88+zt2iEq3olJDtDfzGAVV9VpbS5Q3r0AzVGt70zpbTUj5LR2qVTSRVZsVhTZnTJNozaWk3q68bX5FdYRXakc5BjYl2DFbFWAjQ4TW6av/BX439hYU8BZm3mKqovetlhetBUR28S3RBYZoBcsTZaCUmUk6I4UMAu5wkrDh5QoPjjFsGN1tcSzDhtliNhZb3BY3X7iYDffDqBVy8yw+M5NuK2jahf09bJJUjKQYVUDb1P2BD0f7o6/POz3OGogpCIjMqbSglGmUACHNwBZ6/zjfX7ReY506Ln7dgqQbZ2CL5FbFfcGAnDeJIdKi0D6/SiDLsvagH/XzyeW4q7PFcdRpqgob6jAlG017iZSEnxebF3iX+obKCOw+Mr84GZZVZQfAlB6ii4EI5YJXm0f72NiV5epKqKjKT0t69fpP6hKVXi187ki+FIkbQuaulaCPfgtktNLYaGbpKGFuzhQpzDKKJM1scS7OxS095mFwcR/pLgcP7svCZfjBfTgPI+3M3JjZTzcQcFrTsxYd627RqWbeJBsAsC0wjD/+/uEXX1/WLaLamBApzRfNK0Efu/uDJEbKKLSYWkMzZNSrOwPs4Hxxxw8XPVO0i+RUXFAZTysZZae6KqvbXeieJUy/TthNjasP3wvdytoqBKlvq4JFNSciLCqItGavNx9dqa4ibqmtpNpn6A+t6sU61J31zhoGawutU8DyngQJPy1VFltQ2FhoFahlFUDxspbXmwlYHnnbK6dT17AOCaxy5SDpJqc75VYxgzvNuJiNYYMcw4dxGTaGHRZbnMfFD8s4Dj8c/Dj8sPhx8eGekgczhVnhS2V68l5UFrGLQOzfoGJghMiIiODlup3XyHoNlWrWAUUhuFiaTtY2kdAUIxAAgmtw3eL+xM9e+HnF5y/GeY3rrOjKRJUwlB+dinx6hcx0W+vqu2jaNpTgh/KihVcEditJT5JY0A2KBUDRu9aerBKJ/Vlp3R2XJOtA5YUIooppiBIoTAhYmhOrFL0OSFK7Isl76Fg/RIl+WtjONHWVxgNmdiIvIs9OCrnP6sMpoNkSnEy1bK/LAEknUgwzmpm8oo4SzYZzOIZxJKotXNwOww7DjodxXPy0+N1x3C9+OtjxMO4O3uEnvL6pdAiVrTXrT5cXvBEzRCVTACgrcmLO+O0fHc301dstxD1TiS7ASEva04aZ4otyyVB7qC10ucb90V4czR2AXWcM7oClpupStiaS7B6NKP+yu3hDCwhCeiqrr0qgamGjGmwSNerD0JJscp3mP5WlKCgqcavdbG10ejHuSZLOJEF5C7m6Qq2kENWB0R/NPa2Wa0Wri7bIOKA8s+0CDlFtm6VTpNwc7SFvMGKZNS8sq+CvazSUNpWlgmVbTIXWUsgYBjdfnMNtWbCYLctyXPy4jNPB7o/j/jRenPzhOO7vlofDOB3cnYuP4bSONFMcK8OQCQpVYcTOsZ+hmpqJ427w/mh/5Tdf//7P3r19UvVd1mq2zXafaTsTlB+p2DZybwxagx/OMRzLsIfjeLpuktw4y7XZzsCrBqaPddsMiGqu3cF392u9kfkPpu9u6V7QVVEyrB0/i47pO372Bu/VQGrd4cist2jVTSwgawvv8teQeQkfGSzo1tyq9t4lCzpAv1+8UaqsrTXgqvopcb0QOOWLmaa1/5NRLeAY2amP8pgwyml0eur+qcfCPFXZgeF0xzLGYfCw2HH43dEfDsvDnb88LS/uDq/uDy/vlhen5e44FvfT0hFF3peyaRKz/lQesyCn6S8qZFJtK/lwtFd3Yzh/+uX5sm5ZbhV16FGA1WwvmyJRmZoma4kH1WeLdcN10zARPA69OPnLk7lxC2x69rEVk1hn04OdLlSZww4pjUbF+/d4r717+zpRrXFYQSPYJZ5pJI3m9T0371vKRGo4iTgVcHbgCWa9TJ1EtiEREGZHjHlNxdNwY/2CBi368D4TAfbDKpOF4KboNEKmaSPFoPLe6VFLyrXqggdQopYVwyiCKIrmYuXbmflKNyw+DsNOi98f7P7kL05L/fd+3B3GMLtsuq7zss13T+ubD6U4zsCMNWRLRATNYGFZuWOEGVSlyaDq5M7KZ8fxsHzz9ny9riSNEQETJmQpN3ZInysbME2BgWAU65aqHCe3Hh+u+uXX648+46sHW0yfvDw8PMb7y9r4lJZFPK8RYa1gqCOHDge6AGLKXOFE9IUVFnQhZnq4jvYAJhiUrbLFW+7scKcTuFEP7Ox1FyWCVrX/lQhQpJYNRX9TtQ5IsjCYytlTDGbcEBoGwG1GEKYq5dh1tgEGblkKq1hB2qsud2wvQLQUn0yYxoHyDVnrWuH7s6ABuzPNZIA7D8NOi90d/eHor+8Pn748fO/l/eevTp++OPLgl6d52bZv353/5O3ZzUhEZLmYz9hWN58xqey8SwAwMu9egpnFRPLIkD5c47rG/Z1H8ZMuvA62CCUzgMMydABXSLPK0DNVnIxCfXwVOkNfvN3uDsvpTm8/rDP8brGDzW+eRNAsS7apvdA7vZXYq1+Vz83QIXmaQ/aT3Ypos5u94ocizpXGiAxXHIxnebVncV3anVXffIp8QjTPYKMusgUTAOXFVbUna7vgcb8NhMGF6ELygvsRIiU3g3LeRNm5xOwUYJkam5nWBqhUuXLztAoLOlNvu+wD7u1cdktYwYwwmJe7hRmGY7gdDzgu48Vpef1w/DOf3v/GD17w1z/Fv/pn8fI/PQJH/N1X/+P/tPzqbQjbjMuqy7Zd17haJqbCg9MiMyNkpYgjHXohcrJHAfbqbhk2D8M+XFfAgRyHQhkdbq6yr+Zqw4iIDbV9zFZPUgpxpNO2sPfn+MMvrp+99Jf3vD9R0N3B3pwhYTGc419yYnlAu/0zqswoF7uKNsvZWLvTLr3NjCLDcipCamVW4Qsz4ypD4e9M/0q1xFahRUV+kCGkGpFTgkp0CiPjgRypU04ZqNUlUaxuSmFWZKIne5gfl4TKrAZr1M5zZFlMW1+jKszpLhoqK8dg1anLjCUyJO4aoMo9kW6pbmQQmgVkthjcfRiWwWX4cdjDwe6Py/3deH2/fP7J3W/88GH81g/xV/9tHP/jNuq/jH/l/375L94+Xub5Ote5rZu2GRHaQiHNQGQ5X5JtAWBANWOjc7lm8cNX4zd/4MP1h188nrfCDtDcsXh69paPMiivQTCVwuscdbSEXmwjJbMNIu046E5Il4nrJtBmREuks6biNF1DOTF0/In2ng10RcLare7eunSYIl7dy1kF6agEdIYdVjmFLKCBMg1uO+hl+ckzp7pHH7j59MS53XunkbAaClPmupG7YpwW8FBp6otjcSBzUHABCkcXbVT8WiTTlYBX7l6popPYrxLqmK9CiQ6l8uaR0UMCT3nPxbkYF7fDYby6H4fvP+Av/xrwN/Gd17+DT06v7pf70zgt43Tw42Esiy9uRhsOo5kjHTY7XChfILjBDZI9nPDjz8bivE4szlf3djr66cDDwOLd50KaBdmNRnvxZUldLDG15KKcHWQCIuy6xtMa3767Lo5Bvr7zzx4IwukgBW/ymhaS51m3u2Tp9G1A0TgQeBbTFBu/QUS9RYVaIjiMpwOOQ6NgIoWgAiyzzIWgBGHKGCmfJMdKwEuz68gjHeK+rn3l2bPUcSdKpKHRqqRyCnOWkx8md6Eb+yoqQpf+V5iy35VVzNQByH7fbOnuuyuRZloF3qzeFwKq5iXjMB4G7w4Dr4/Av4Z/+fUKd+Pu4MfDOCzjMPywZP7AD8MyB2p0MzPrqiTuZzSlFxyc5ysi8POvztvU/dE+e+nLqMBPdeQxhoNZqWuEqCDhXjFaiUt7aL4rLISgy6p1kxlD8+A6jSw4Sw+YR92qta08844TvcuowKpSasBeoWs3+1PngvJlHb2yeHaVw/hwHJIg1ybsFfltckjAo+RkDrMo8QLM1sXcx3TxvEXQ0Yeta9bzOzol0aIOuxZ9BiNI2CCXqotIPFI1HHSEAe5R006CLdHudiQLN/caug5u0MibxeWdr412bPkes8w1/7t/ys6+TCt2cLi5m9kYlqZmxzF8WCayzOhON3fnPiNkCyqQoHU82GXTGjLy89eHh4OX1AcjfBwGzcglTS0zNunEjNGoUOahfRVbc92Ad4+xqaYwQdt1C0vX2emnWoqM8ttBZjUX9+ivirrKHm9haNqS9otINSluYkQ5S27CdRMCNjBShCKSqNYIx3LWMtsbNtWQ4kA2LrU1E6hSBhQPoyCrmVeVaXUSebydGKx8VgNhaGYdicMZ5g4iokrcVDcfALuQIX/duurZrFVBVhlWVCRcPS+zemnKaDNVK6XgKSS7itAMrVvguv0pIwPwu3ia61R0AG6Euy+OOXwqDuGKqpvhDBKYWmQREQwqQrYFhI3IGIiXbS5OZrkbxww/X64RGb5teSKiSUvNWRNbjqMQkjdnU5bgOOKy6emyHXwMh8zm7BC4pD/rBewWaACdIUIL/gSCUb1CzEllPfRgB0GWiLhLe8qdkomKyQnI7c5Cxi1ynmSNFawCRYSi8pRC9ccBgm6HwRjRPGn/brCH6aXNVYXxFHYQ0yijzD/pBuAzILNBLI5pts1iZskusyRNlFcIMrpJJ1TjV1JUTwGEqsk2tEqZVuQUCsBLShVmaAohbaF14nwJbPtwxmevf/YzfFjP19hCOTmO6RQWbIFF25w1SI4hN65TGXvHmNokcRgeTnYa9tGD8CEAACAASURBVPZp+5M3Z4GPF7192l6/WCbm0xWhGapiBJLSDGDL1hQYlKM8pFzb5CGZ8tYO1CA5hfdnffZCB6cwT4uFeA1zk4SZpsZ0PGlzVkHXnpYSEKkMtZwAJwNyYT7jL2qGl47BEnayV4WVPZU5BsipJoSRudf8sqpeImuYZEHnbCIhQQ6LRrqdClbwJ0/pkoyUTrJZJ2ZdTfn+rmErpxaBiZghUotjuKwnlCQK5tK2ytdxcFowi28qJek9aUNU1KZILAhBiWkRObVgitvkusX7y4Y/d/pTVvaf4Wfv3r27Pl3nddU6s1wiy279sNiwkcn4ZfHj8DH8MHw4x+DiPIzx4rQM59H5w0+WN4/x1fsV0gz9yTfbJw/2cKogyLgp1rmt2zZnxJwTMbP8U0XerFd411WtYZ5GBAyIy6bHc5jNo9vw7v8jjo4l44GmF8lWM7Doj8yUsYrdJ7NAiCK3vQQQqgYNNkkjAAZg1IYMu4ucmltNniq7Bjst0dFh+W+1iMVmQtr5XlIxw46pIhScrZrAMnNgpVMM1DBUtDxXkb+FiZLsOmMA1tU+sY8pri+s8FM5QausvgLwjoh3ivqdDGNWEQpUUIjQCHGm64w4r7rOwI8+B/4v4F8HAPxveP/38E++ev/2+vX76/vzvG6xZaZcdaCMNoZC9mxohkFy14gI+fBww9uph9O4O413T/N8FQgFv3p/ffmW66rDmOtZhOa6kdwCMwTAjaE6H3lTAXSavXyQZfaekCwUBDTxzWPcn3A6DEO8und9iHUym60OjvNWK7jrmllFxyrojVsAEz0nQAHu5zVVPKEYnuW42qRBQTPNgJsUjJzAAQtMZgdeqGaS5EBgKbXFWaiWk3oEMlDoh8BE6nUwsWtcWmYrTZdhbZWARrrn1B6kzC9kaUECukDOzmcQdKciET1HVlc4SZVwopqA0MQhCe7OxLKi2pQ1XgFERPhQFa8igmvgsuHpOh+fNiCAnwFfAP8L/uEfffvmer7E43W+O2/vL9tljaiZsUB1H8lg7lhCAcwIdNZhGMOxTVyn3LkMna/z6XJRKbFYp371zXVxX+fctqoPCnXeXZyZPWxRymWTkzkUWY0N5aE6T0MA+HCJbz7gYVtBLDSnroQTkg7DL3OXYdFzYVFzja2HsVpWiVjtZCZ7RJoi07tw5mRdCbSkQAQNUzAoMpUWQbdy1WCJDWBQHs0Uob2YL29EPUqHvvcntjMu8Mh8ZxGkPZNb/a0zMEqZyHkK6KYcymvjavpmCBtkoFeKMGGvMprF8AQYrJL8LHeiTodgtz6VHCBIDCGEEEMWwgxtE9ctLtt887jhf/3n+J0D8O2/+Ds/ebwocwDXbZ6vcV7nZYstZoilYasGBgNmnFkVb5zJCWl0IWSa4WbvzvrsHt++X2uBKMmerjwztokIJoAxE0XTYHDlSFJICGFaBVr1lZU82gMuFmsCFfxwsWERAg/x4s51npfVrSaGdNxaoXamtFxEzTkGpVlyi/ZthgBFllOAaE7G2HejuLSmzCAZfUoOZdVFdu0mlxLhqjYZQqU63gJgkZ4jH3gLXYoI0hrMih7WvxdKCQQHEicBZAFLHqoupcl7tj0hJsxgTUnoGRXNJ6AWR8xMVX+XudIALCRXXrKUU0vzhMkiNCVJIWyBLeZls7sADf/zP/rik9/9JoTzmqk5hjQjrpvWGeumdYt1QormeYigEEnIszy4BnLTzMKCmYO6bgpwnVCXLUOcoWzjiyBEd0qYkSVl5Q/QKUUrGL1J8chkdpPkKOLLKX24zIPztPjTdQLz/uAUVmDp070X+qgdFbGf0agYci9MQ6sZWUFfym2al+/xYUjIqYzMCLWU3RohoMJGCDUQGXvOuvxxaha3CqB0lsgajZxPoJuIUpyBJpWU3FVOQ2Y58SS9MStzUsEISiGpBnsQygSOceSvBChZetZdpt3DoACGlGGBRRU4UAF53rknNkRgStvUZrpuGhbufHnvlyt//tXZjaJlnIoyNc2JNWLbsEVsM30u0ulEaOYwgG4rKp0PMKOFgtwCj+f12w+X5NcKCtzSCVFGufPgdp17C7+MSSgIKWBCph4rEFJxzw7lsb+CQATfPQnSYYnhNmecBk4+3l1UwgI7mY4OM8t1796pK7LU/jj1CAbFCTgVTfNUipfYIkjaTw5g95pGgDbtvMeeY5+SVEprlWnNi9q5twzVWlMhZKHZZO1wZZHLYIFBRU2grhbDhFvm2DoA4nTYfr4yEglpA12RxWTVGkqBXgEJ90LQ5AdWQWVaeNWHthAFBDBDc2r18M22oYeTv7obX814vExmVUlyXLkUU0gUXKfm1OzkppTyGyRlFjKUMNebQxjrcL289/OmUGZ7UyyzTXFYuHRO0A0rkB82BWfajdVg7l7uLGm20MyNzSWOOm+Jf9fJt+d5WHF/xHAsCxYGxcVN0DqzMkZZTHPrKg8DZ7UyymaRHLF+Dey8KNmcIBkZwKwD31IYWqu0VDBaN0ld2VClvkoNmc/KyMVEwR5ALIlhYdkouCdm5c8CpD0EpIgBgphRE7UzZBRSrbu53JI8Wr+pdELiEKq7L0eR4SY3osWe9CBhckQEzUPYi/Gqiw0MYRZQhdm4Xq93pwe8n0/rzOuoXlBMATNCgQnNqS00pTmzEA0Ryqy5pJhS9zcmKGTty2KchALnq0pLApnjmdTFdbSICLVwAYUQCq9EDSQalaMdk3d37V5aVsaPoKxYo7AGDHq86jBAhHPeHxdc4ho08uA4z05o1f5HPR3FYF3ErWa6rLKe8ueC2O3ESnJcgOa9IdqUfc0wckpl2nnMKrWQu85yeSx33TAbKkEu4796mkKl7KvqaPaUEEEImhQjVbBKC1RNDwzZDYm9JqGC7Jvx3o4yMsPLUDW6V6FTbg66+E6AQuE0NGRn/qa4Z7oBhDCBOef/+ZM3n7xczJfrOgFznyRdRD7ZKV0tpIiIzFhgRhSMqaIwdSwaJfTlEtqMLYQ3T3NYYx0ozuSimzRUp9cZDkxoZjxGC6ViQKNmWDuT/PgogOghY2VflVcuxTEp2RbQJe7vQgdenuhEOu8yrNrUwZ7+VOc9azQVyV5QdWq2j79CZmJ0W1cWdpVrV83Uy2mlebIq9Zd7l+Jq67Cli1bUZqzStoxIS9US87E53dOY6aOcoUwyO5NU3UkprxI1tydtep/ZUsyDu0rStXaZvdAEItJV3cqEsKsp2KVCCyFyHdPKulkmdcE8yec13j5t//Sff/3V2/WaiBWagW1inXPddN1inbGu2xqYESFIE3vs0lw2L4OlrhQoZi2cGwx6OO44HYJJAWqdWGeGFFN9zLOwQsAEZliXTHSgWIJHRwOZ94bV844a4BSYMkmLy6jDonVbF4YhTgvcciZ9Oo8QaJglEaS1sOcv59aoZmS1MF9csJ1Xryf3MCJvBKNK7TM+zVJ7ONSF+IkB2XFQbKXqEYAkSik1k6mrydid5J13rXiYGSDDXxzda+mNXjI0KdIN0X1SVp4WpaskkOZEyULQjmnrn1hpx3yr52eiTHrUYCnW4KD+1ejZL2fE+8frN+8vx8NxC/SoboUwhRl6vGy/+vrN9TqXMRLPpoSs4wTzeUpJcFLc1J4/JM10cFscdwe8/fB03XhJzVRNvgMTyiEg83akJXipy7ml1fhUeiJKbS1+w5Yv2XJRv0k0LA4Bx2GngxbHdfLg3ALbntOpV8YxVvRFqdQUM2yXrh0r89BUZhM3J462VVB3A2Nonbb1tI9dzxK0X3OfILU/A9LoCkTKNZDR/UCq88g+gI30QIzyc3lnmUhIhTftLiE0krp4qswsgh+1HBW6VpiTsSVUFNGUMj1vNQh54Xt7DIiSCCpHNwMSh9tX767fvrve3x0g04gEvRAfL9c/+PmX18vlL/z6D9dNgLbQTZbO+tGSUyMzLWEclJQNRvlMO1vnZsTB63tLpcnYMXBZwQWZWvM6U3MTYmY7qzkjmCVnSZgNDEWOh6zybDCDucxHZU4U28b3kjsu67xb+PJ+3g8o+w7Jqd5FwDgmZNFFSFWYTSNjz37CWYmWHO2e6JYeo45Ark6NESCHxyhjZW9+trRiB77UBqqyQ02gKnbPs1e5tarASx5nnP0kvAxH8hAMFlKS+5GphHmE6Fk+mznv1GyLe0X5DCKj2CYjjVrB8Hz2VRmWG7Nf3Z+FCmoLB1OQUoqtAQ7Hum5vPlwOhwMQ2moy0Zzxsy/fvHs8f//Vi+FLOs2MFWtdFaneqc+BG2Q+FRICqe1YTgD9cNHb8+yj78JkxXKxTjltGRbSnDBTyOrpiOFJ5ihEPYq0kKzdTUTDScd0pUkK2BI1JkScidPKwxLXOe+Gu/H9WYCnRGWAUrlgVW8r5wNU1FnkRf3pmWxT2VqlSvKmG+MqFbOUkkViIr10mU8nuqCWqcpGqxWgnnSSagZHNeLdinJTvMj8GzKMFUaxLEIy2lalkmU3EmcWgKNbqWx/Bk1qzaX5aJ/LDCgzH2neyi91QYQrq8puD32qOEX7uJ+suN5mkDan3jxePn11D5gwnR7Qh/P65TdP2xYv7o8ppCXspwOLymOLAK2fehU0hyYmZKEsknfni5PNqfOW3mVCO67lQBesMUdjLYXBuCrn6G9ZyLALvFUylE/jFbIbOElh7552rMjnadT0Bovr1Gng5RI+dJ1jnVLouhNAlKKV2U6D5bNyBHSjWzasRjvufq6S0kNEZcFUuDQjSDObBE1b3i+L2eV8qIyh2ThSXbpIU0uUYftGxl5Ikc+STAoVnSoxRPb6oS1EgEl7nFjuNx/dlcJCk8fkjyy4ZDG/3g60EynkUisXqq/JPoPMPUeyuzwrCYpZkAPDDD6eL+ucU4ipTTFDT+f1fL2QtiyLGr5K02nIJyoOy7CteEahViKo7g52d2iKkx6itDYGuhMf/Pz1WBw1xJdF9s0S3pKSZK1Tka92RVQ1T+6uKA0GgSpVSQud4nnF2wuu20TEg8ePXuL1HQ8jSVkm0SrBZ3AKhFlXI7WmmensVArTi85nqmEGhzPDoLzHmqdZlan5P5bckP6J6EjPhHRTOSYxzOiGYXIL5lwB7kOc2IMRLAUvgYINIWs0vE5afYNZnY+kOEhBiR38dusFume9l7c0D5bCbUyxI+lBbotqs3XZ5uPT08Pd9umr+6wRDKsymSk5fUqXdT1fpvvoB1phi5hzDl8gBDr5i7SPlL53AqFQ6p5Sc+Y80yQWirGtU55aLoBbA1nFHCA/uXM3/PHXkXoEzbfJTYpgPZNhF95yTXYqJFAW2WSV5Z+saRoR2CYpTQKTcnvaArBLBDkn/MUpxrC3jzqvYB6a4sg5bjhdY1Ae2p+enG6lG8aTjwdoVaRas+C7Rz+ngF1mdnkk9kVRKFXYXNadHryDz5prYnLZ7BMkQbJQ+r6ocROpOtPMYuTid79bt9BVHL8HMkiJLE9KFxhlisWsU2OZyt05pVvU/IfqGZYUMicqpjguY5vLt+8+XLb40fde2jIssudWEt1M0Dbx4Xy9Ox1njk7MNtTgdduu20ZbyNLQ02mmfrCXlpZXgSw7MlGVBAa4RcQWoQx/NnVwpsBetBl68xQQsiUx65dyztMzVSO/qJooC0+SK3LaLt7mIac6Bo5NrA59SrJzKDZOhhHrU7w8ju+98j/6cktoMkTUhmaNcrH6vMxMt978bKsw7WG76ESANIPCHJ6j7Dohg6TI+2PvK2ltUfJWezQMw3DlPJQZjDAyZsQ2sUVMwNUzSJWic2By1ONVMz9W9lbkCQDhGSPs2Jp0pGu4s81870/1mrZpmTehMQTX/oimisnbjo2vH+7nnI9Pl6/fjR9++jKZhCy1RKNhTr0/Xz8LVOtuJRlxXefjeV2WkRPJoiwkEw9QP6Amte7i6cbMgkEK4Qev9LM/Pkfx4+rlbsOJ5kX29nGDtG1tV2JodhdIjVA0IrIILSoguKWcSmgoS0vkq+1naGYNCbPTsSueBeG8xTHp0ZwA582GNCvRlIJ+pURRM+e5Kx2sVOCOTkyqHVOhHKAJbLmfyShysnp2dlU6o4aaA+j51IvzuNjdkZ8+LMfFZ9i7p/Xt4/WySptBmAgzKrrvFEnsymWko8zwPbP5JC3RreZIMZ1iSrupeaZO0Q+sbVKPrrMDyPI/2ZvL3TjzH935+uGBxLfvn67bXh9ctu/moXh8uqwxQ1AoIsZwc9+mvn73tG0xS8KNOSNjpoAkRnT1e9t0iuBuHG4PR8xt+4NfnT9/dVyGQS15w7Iwrg+a1smnK7bQecXTGk+rzlum22Eyywm6rLHz2WaYt1A9nimYlYnuyn6JOCHMWdVMCmWxLiG3iJjXiBd3CVfIqRP5mxAgS8VCTaKk/Xtmc36wWjSzalrglneV8yBz1CEyWhRrerE64cN9I5TE0MjFcBh4ONmPPjv9w3/wt/673/3yH/wfX/z9//zfen0/jkuOelWPhyr1i3R0rW9nx1i4nJSwB4wxF3DnXuk/szwKnfWvfwH3AqX8256rVepGKsJodkzgdFyWZWzbfDyv+QYVWHIMi8D5Oq9r1g0hRBruD8sUvnz74fGyhjQ7zow9h1RErWCkHL3BzAiOQaN+/+ePgr+6g9fwicyICpVTvhUr724khC0UgSkGYo2g9OkLfPJKr+9FNlqxaKN6Co4QOT+pknplf0k5MzIWPYlHRSpBzhl3C45jlFuucowAIpIq1NCThJ8E4S0fsCFkzWp2OxZxJGgM45xzsgoTsnUyjALD9tpasG0VqMlPORjWhtv9wf/W3/xt/Nm/nQv02X/47798GDmXzspmhHwmuZGW+iFKTsD+IPiMkSx/OEMa9qFJwTAgjz2EFAHvEoVCsyqurSbYiiHYZWptkwDphtOyBPjhvFZhaoIgcXCbwnWbT5drKNKkILy4PxHzfF2/evOUqW6hetDzMFjr1/0l8DofKazJyHXi/ugzKqwpfE80rDOiCISCzJOKYUCWSAuSSXxxwnGJQZhljs9uYVCS73KkTRdzNAcQYEQNJ8q4ZOw6eiYnY2Y8fjpUJNkniLsnzOKXcpxp52DGv0RI0UXVFcxlrihgMwzksKjKhzr8pg6+sZO2AkIUB23Z7K/9R38Rt9fXNZ2sqvgN9N0pVdtOn/3KGrC6UTL0iDoMJRh8J4mxT+Er0aIFDVLsEVe3IqTcXDRq7hRQALgsQ4jr9RqTwdLXJRzHyGdJv3u6zsCcEREReLg7DB8S/vibt0/XVYE9BujoJ916XY9lQ3QT8eF8eWcPJ19nPttVVJpiPR4FlZCFgKcrzqsUIdFoRw8zZb6eBhrXcIEKLk5aJqL2kC2jc9spIEr+qSfLhbRluyxrJRtDa61rFngz2gTDavnP00+ktoIWmcCwuvZJtWpR1R4J15rPniqG3qHqzxS7c7h9Ul5dtotAIV22+ZO////sVvbP/qv/4cNlEwL1WPkC5lYggsSQQEw1e6xnDaO1gLzHGutB01Q1CavjrLTbnICTUXOmPtXvzSLbqtEtjawKkBBVbw7IrnPOmAOjXSQOR1doQ7x/um5TtIAsoMXt1cPp8Zvr+Xr94psPP/58lGqy46nQz4a9JWezGpCm44LHq+4O4/3lcjRO7YYdtZeKLiPCOiFhQ7hT0HAuA+uM65XuSGGP0Awa4N7CWHqerA0rJCgJv9PTJaDFxDYg0UOCLabAVPZtWBUUDcc2DVDU6JT0t1JUUrJ4mkimtiC1S4wqFcoxPgWJW8Q2n9GCypDusJWauYSc0p9laZaTUue0p6v+9t/9yX/5+nc++a0f/9f/ze/99//k5x/Ocd0int02ETULRpDCX9+PqoKX0WPveS7VtMwi2Xsmrurxxln9kdUgnV5NnRv9iB1Z/y33gUE0L/k3PT4MvGzbu8czoE9fPhyGJ3lzozR/9c2HBMFPXp7MmJ4gg6yv336YgXWdr17eHfKR6YZUnXcAZ6bFbvoDF8e66bTYf/DXvvfucf7eT9+fN1w3Bav3pm1knxha2Rkz1lO3yGVwcY4BdyAYighOCMouJrLquRpC68ilI8h/TsBgKJ8FYyCWkXWUpfVZzzAXGZPNmULd9ZGZ6spA1KighIbqXtXN+VQ5hVvlThYngPOWXiofxZzIps4Vkty3KrFTyYYALcO/d3/8g9//4u/941/86pun8xbrZIgRUHXF1fmKbEBIaduQZbGjIsKC7qbrgjClNLJZ9S/axwv1Cc5KDVSMmgereHDH9VClawNZ5xCCYiKgORUz0v+lQxluyXIv6/Z0nQrNmIoI6P603J+OAp+u27dvn9Km+uKzqCl1KUARVYshSeuGEP/qb97/m7/zw//iP/lLP/r+SV09kyqymqCxpa/sBIgShbMSU+5xWrLUQNmLtnh2H4HZe9jlCBnH1waCvZ69xqXOaxnlC3ETAVPfitOAuczyIGXSLmdBxv6E7hYjklpZFg3JOutdqlj5lLTk4Ty0ZKDyPbr5cBZnSoBKu1YoxOvk2w/Xp8tEYM54vOK6aoaywlSZAs5mDjKnm5XlVlUiy2wtAyOChCfFgSML8TKQyRxUIXbyAqvC9coCVGaeLXDk2SuWoFJWstNpKi8wq1+RD8LJ8mJjTkKYj0+XLSk1CGgYvv/6AZhCfPn2/TajGDKLQ3b0mHx4RlTv4+J4ceTDyfFrd/jrP/rrv/26AjVxqsy6LhCAYgrZ2rI3HwhZm2RbINtZE0VDnDPJAOozihoASolPpUsoUqxP+1+3GUJq6BGZh8nvry4Bt+oodoqWBXtR56qeZmbsLk+wSV5R7tbXIDAqiiCdHA4fHR+hCx1RtSAoYFU3yShkkuaMberd0/zlV09vHi/DsM5Yp1JXyqRWsromYiQ0CNCsnqNclqIeQpVMrZo6sUsalZAImrO412TNnycZ6fSyXQAdyefb+2xJ4gyZZZagygWyXsOAUMwwd5kxtrDQ0zV7Ndljv/nq4XBYlst1Pj5d358v33t5x24HKSDTbjOZuYETp6O9urOv3q345RMcv/ezd7Pwpt+310WgenFkYpXs5wAKy6TBtiEopwMzkTiUuQkq5waU8qsd+J/54ooJgsLktmJ41jxYl8IUOKVlD+c2c++mZJQiDDc5Tl2GyeLCWclQT01EMaCMCOoc0gyDNMRMco1C4T6sKdi1pxRliHBYYMYF/OmXj6fD/RisJiA5MNXOWiU1ZRycqSqyfV3qs2bIQJ3OvYDDkKWvaPnWPBmCpWpiNS4A++PS0xYzjGXTBLAqq7O7oJo3M4Gd2IPUyhRBw3HxGRR0vqxzonBQEHAYy+uHUyi20LsPFwlBRVBVyC8phSaFSiyYE2+e5mXV43l99wdv/tHf+f1/+pOnLSzz2kzAF/tyE9WVU9DySe01iD6zNlkQwGxR76iotc8ucMnIujLee9FEPuMhu4YkTM2F4ZwZuCgqLM/3RkzLh+amg8kxSG5eDRNmmUqtwivBwljzAKz6blAJnVarAjByGSr5HGakUwUWxSPNx4GwuEHaDBUN/cXX52/ebyQyGgdnUobcPCE7zavjpCR6LwSiOQbpTmM+ZKIoVvWQIQ+pVemkuRGW4+yaFtmuWVQokadz7xVGCQeRa1+VsIBCsc5o+NWUKN4dPBQhnNd1m1NV+K+MTV7dn7Lx4d3TdUZUB0pLYPtPlgBVf8sPlxnS//7/vvtv//EvzteYNbKEWaLYZPKWqUwBQSoJcLjllCsyhtcR8ZySVnBYDicNTOUWykH1r0mZMrLQutUzyxmRxfrscq3UhLz0lnxKqerRfU6jeT4DsOdAsZ6XGqzp5nXyiSiVLG8o5B7LkFlkz03p56xqYJIvvvdr3//xXzi+/BRZnR0QlFNXIvDl2/Xr99fkF1OZzsqTXUuY7IdAQAMEZTRVeRDbXxcAlqhRsVNPrmeV2aQSZ31qkceR5V/T4ljcrFK76ZACRokhOaionpvLdYu7jLHNTKE4HRdI28T1Oi/rXJbyWXkBp4MnGT5fruuMAz2l0WCwS/jb4xfk0BWhh8Pyk1+9+/LtU0YAqScBWbnBjmwqj4v2SLkOSV7V4ZkJk3m+IM2QIRRNl/ptqdDnR+6xZ6emQAnbpHuOIwrc5gf1hUPDMEsxr5K/Jr2I8Kn9we2VkcmIi+l4cwBlfxuV0fEwahjW3WVWTAvC6bx/+Xos7p4KARAl+1owiG8e12/erzMzzimtzYx5Q6pk0ayDm+3NlmLxLdZM87qNDSmG4Wzun7pFBT4FYH2cTF0z166yEY6l0rXOVVAsmgTOwNNlm5U8iuxqOS0DQNLPD5er9toDScAYNnxA87LOGWqOJwSjiskAUcrOKLrTOR8OePPh+idvtvN1RkKGlD/TXm03TbCkgzyaVbOSD91OEpLUJ7ISA6qCrtrT7NjXFNlJihQqVDX/jGaFMTGDmyLmLB+QZ6QeXaNhyMF1IMmaWOlmbvVMGTMO2x8d7nmN2e9IsB55apbPkZlhW0QOXvDDwd1zCklqKSlUrdd3f+7P/+g3f+svLsupGEIKwVBoPl3w5jEUWEYiBVnJO+TcpHz+S+7/uNHEfeJS3V+uSVWhITW/DE3r2cJllR1dWjPNQoA2KtUHe9c2sF1xPuU7ZFbS6Ien65xh7llzsQWWQXDMudLi7fun77+6N88ikGrSjFQSpAi0w9u99e4ts0QRB8cPX42n8/bFW3x4Wi8rc6aVVf1+mhpQ2f+bHqXMuFhn2zmpkMwsxHyWWUgw5zZrwGgqleUptX8WUTpmdSfvnG2dOg4ooUdlrNFRUxJyU84VY3YPB+WpuQisUvxk4VkCrVQsWYp+jdzfS0y3CDd8/ud/+/Wnn3/xi59+9auf5iTxCliJv/RX/o2/8e/9jT/+5S//6A//8Ns/+RWBrO/OxyesG95dtk/vxzGHEmSlevm/1EEyzWRA1W17nteqBSnIt26Eh9Xz9ZpkNFNEPZRqn0K6h9D55+AuleyJtOQ9R0nknQAAE/VJREFUrNDSwQkMMzPTjMu6Pl3/v/auZcey7KiuFXuf+8jMqq7ql7HdGIFAlph4hgQeWjJfwIQfQPwAU74AJCaM+AT4BySEkCxhWQI3suVuP3G7u7qrKrPyvs7ZOxaDiH2y/Qsoz6DVlcrHPefsHTvWihUrWi3WjQxVPuMdWnPdHS/nuV3tpvRkMrx8c5olQSW6zPwhA4zgtmq24N6NE+140dJ9U9AcxxkMM/uhsQmoOIQPia0j7hrNGHMxs40lNOhWkpRSJkCBsoLX8UHEwIFqpPsIVl/eDnBo6WqK/tffonKTMBaLLcWmDMCkBR4DnV5iqY2m0kBeRDHD5vrpbr8/Hg7L6U5BwFj13ii5uNlsv/L1r1uZdld7M9CKek/rQvrz5882m+l8vr+cj1ADzerkrUkNQHMdT+16i2IjignhdBFCx0BGwfLUHJS81kY0qk75rTbIkBH08l/jXvJnPZLUrFWZ0iFAwGhgHUdJcAwIKO1AIWopm6me+qV1vXh93G1qJXtnL+GqCEkdOp79ly9uf/f95/sNHLg9LJ8dL2bmWPabTSH6CAMa3IkgKV1FivywsAvn2fcTbw9tWRwFDL/pWPyMjletTyKclaJdNc+gsYiFMP2gK5ycVEqAzsjOYq1FizKRdchop880NZvCAYTyTF5LllZXToRAD57MUUtpoTcNjZcEodJc+UYN6OOF0lCLPXn+vJj11rTUwaC6sWfsa8vp/guru7u7V7urp1bLfDws8xmC5N//3r9fX+/+578/PN+9hmRTTX0iitABvTn1m6sqxD6KBCBGt0bHYQJ2hG9oCO0CBmgsljge4vkkm/FAAI5YP+AQ1mcfFQ8vYpgGamxZqrsZ4Z7y82HC5SqFeHK1PZzPEl/fnabJfuf5DSuWptvjfGnuDV0S8OsXx5d3ywfv7kn77DxbLeFAfnO9YR5F+UeT8kkfOULoTnfdn91lvS+3h/niGEObviSLzCdigSQZSW4G6uAOhQE+uwfwlLvFMbpuS+UZGyAvA63BHF/qhEJoddTj40lxxnVlekhC7mRxdaqWgpIJ8UQop8/ECdvBqlSW2UQz+aUY4Ytk6pc4edydiPoLJHnHpx99eOpTX+b9zZOEdhHNXJ989KN/+enH7i1pz949qUmQRfJL87lhf/V0Ny/n4wEA1H38kqwXu7ujIstxqflQPHQJcFgZpuupzn/oaMpcPrJYjhr2+jJ88IwMFyipkSb1JBEz9kXN00Ve7bZX0+YwN1f79OWby9zeudmczvPL+3mePSofTaC4HNuPfvma1bbbMpl5awX16fV2MFjJJyuBxiAzREmXBdUiRFlzX5q6sxZ4C6iflPTALpnlI7PVwGQQUIipcm4C3IUePZsKc93xnevTVmBtdYeZI/Ya1neaud/c/bKwmmpBdO1Xi/6hbOfp8klijZgZtisrBWNWQ1CKsr159v4HhF5++ktfDqfbV4D6cjEg/WzdDS6m1wnnU78cxLJcJsn7csJwwDERfQlEQpbee25GkGGg1ynb7K6udufj5WzuLbLubLnKdwAAdYC/bKBgKpKx9jgFBGDabQPw7F4EAUu3gGQtEguG4sPzFBOgoNS1MpX0EFzF4QRHsfLu86fL57ezXMLL+9MXr8/hfw6yGMI3yhgnLSH4RYstBr71bL+b6nDQCPQ2CIHMoTlIiuxlqOZv31QbVfOHAkAwefn+4sk4Vx03BaKAtYLUpgSutr6C545VgRPBT7kRFRDIRz1rlP8ylYC5xNOibQ1NrROQW8xJjB0qdve+3W5Yy7sffO18nF9/+uu6meT9vW/83lc++OAXH3384hc/29882e+vvJ23+93FL71fgjQO2osjeQFcgMGKuRHu83K6DekfVNI7GJnliGMOVHoQBYxHF8/zXDdtmS/efUSgTEtHtky4KjKwQOq0kusxTsr14AyAQ0TV39mDERLJIGLAjr42sa3JNxADpjxMjKhI4AvARAGU0p9Uu019/+2bz1/dLUtzmBeFEtsQZUcR2k327vP9zW4CbV7a+TKT9tV3biztWFbDI4yTYTC0zHFiG/M4+Ha7q/eeHn9+Gcr/Ly207CyPbUw5wO4oNNOmMqh5KXQTDM1a0EQ+7OUKHtBE1hcGIODYfpmmjfAHycjWvU4wUc4RBBgDzig273/4zd//q7/52+9++zufXZa//su/OLz632k7/dl3//ytJ/vr66vXv/l1mw/z+V7w3f5JZJakjnevfJnTaFrgQHWl9CoVi/4jODpAoYcnHtGjuybTJM9XGnrs4NJPp8X0eTu3URWJ9lI8EM0SgAp0oISKL1cwOcoPyhNuVJqz0yeXR7Ssm+QDmrqZBQ04QFUEQAKgO2i+2qGMNFcWmNhIXO+207vPXry6m+elS2dxU/HNbzy/vW+/evGG1DvPrv7gq2+lTHcESLOMqFSw96mbDtiZhe6g1aTmNpkv2Oym5XpXqnX3TOCQ525A84xI0ZoloTX06q4qASjoPdrYXdbVY7uuyzxWTi5eR7ARAQMUB96ImQR6NL8JcorRsQcRZRQzCtVhQnfnt/7kT7/77e8AeH87/dEff+v7//oTu5o2lZfz4f7uzntbjm++OB13T57XaWusZdq0dgbgvQfxgcwxEUaCUlAkEBQ5fKo0sqAfHK2vvLsygRcgd59b2/daStQDA0K6aMNVOZ9tjXDPodnONDCFWxiPTRnT/IEWixWJeCDRlUq6o5g5YYgxGSyIguMwcEqKndI4h7Na0yWAtpvq195/a740GD59eWq9Pd1Pd4clHRRGMpneSHm0pT8UcgY0xtmJkQVlDcGgMAKajIcLjNpNOF4sOlhWARa0WlmqICo56h2n2Qo1bXMlyrOZIUyBmoOkEX2Iajm2wpqrVUNMVR+gHsVMXaTRvMeoJYcKc0qSY+xwqROOj37847jrTw+Hn/zwB8e718e7V//5H98r1T7+4YftfIRa78vlnstm15e5bna9LcvlqAc3m/jdwbGnXQ0i0RmioFwLq6gopDdZOxRBMxZ6d0oO+mTBfYWNTgrPYh8Z1Yny9nUpBRjiXI5kn8O6Ie90nITB/WkVYawlzLWc+WW6NrsfEr9yrc8iVcPEGu9G8kxVs+2mTrW8vr+8ejPXYs397nghwOLvPrkqJWnVyCTXvzm+GEjDRmUm0k3Eq4/eiE0l1M/nw6uDz00tvQHijLCR9A99rXEqZgWtoaelIRXttdn5HO1VJLh0dSVNwgzaQWmT5FQUhcLB96QPmUZsq8Zpiu1BM8akzrBNi++4fXl7287/9aOf/dM//P3Pf/CvfT618+XFr37+2c8+no93yDPR+nJeLgdfzu18WOaTfFRoGE8j3oRtCgibu3pPHkD5nPKVBEols/2NYC3YVlxv+WTHJ3t7srf9NskYpSYmc1lmAkoJNbvUw+IKHSjjTFtTLTgyS4mvRMj3+DzxLvUQPNKEM6GUkG3UKQHigPxKC5F0/osP5y4zuDNmFUcAe/HqsHQ6DMKbY3/15v6950+UE1a0ZgFxXKW0CwQasyyW1SRmxYeiL93Ql6UBwGbipdOiOoQRYOMpIzkvUpuKyXBe8Oa+18mrMfzyYhRuPOXeQ2c28G6CoNgN0SrKYpCxebDzEe04Pj4uLQdP5d1BkMU5R6p7P919/s//+HdUYvD8rKHoHS0RAUDN3aNolr0A3XPfJR3l3lvHNOX0NkFguNKkMjfacgplZoWejYmFu6pttc2k7WT7CTTtp3Kz191RdyecZ7WecW+0ObG88ySKdSWT/qhUWjiBJgUFhfCWwvoWgcQTHAxawlRlrTexhI0ok/VT+1Lw44Ab6/mW8Q4BO6Zqr+7O7piXNDVUx3nx957tx8880CkBo4NQ8ZFmxN9I5k+pey+E92Vu80efHA8XeEOP+OSjasL1XCNFK6ospXIzqZpBWDqWhW32S/NlwTJjWbA0tjmRWJayEDcZYJOQ1RqjtYRAbkCBJWIYZ+tuUwg3EIa0XAFCvhBQp+SE8NwSkRll1M7yy8NRMx5pOg5llLWgAG2q3Fbr3udmq4htZCciOFVsJ+42tt9wv9XVxq63drPjfmO7CZuCaeKm2qZwt/H9xnaTb4pxmCdYjD8Qa5AXGKq6ceJQye33fKPJhQQzmFszb5NJ7kJMXzik6qcIWvsV2Rkm2zH9kpT3QgsWTQOahFbBGGUxkexdLm4mtk6r6O7e22nxWmy7mYqsFDTPnw6NAEmXMzqT7EFzGKSGu6v3u2NbXEYcGjrQGjROJ62pQjJmNobo2lS87HCl6F6Jxn8Hzd0BtIJ5DnAb8vR1AEgkRh7qUculRkkNEdezICONZI6DHZaP+rskqvfeWSzInfghgmMsBYDRQRDVTx8T4ALSYfAT+ftiHxpsZJsxB0WyiSob7So3EwivxaZiMZ61FkYzcBcus7xqU1FpU8Vu4vXW3prtcPE3Zw8Pw2VhHYXKiKTpuCU4g1JA5KXw5D4COgkJJMZrYc/ULy01gofLj54bKwaneTBC8DBmYDrUjEJ2PmIXlsvy5v5i0OK43nNT6+vD3DvfLPi3H35RiP3GvvnBkw/e2d9fWmuwWhNVECGCNe9RsckQHIe6QfCl99vD0ruWTofmHrg9+qXzlPWYcgALQ4L0jh0NbNWE3DFxaBoMXHReLHUucdPBHnJMcA7bBmYlWUy22taaCsdwG2B19I7sx51Sd8jdVhuUsbZCRxTKES80d4z5M91HcAsfjhLEXAAzF+DVOBV0RdVehMx8WzlN3IRli2FbtJlQyGIWQ5msAB1LHt9G40RDwc0OV1td7/n0Ui/dL0uZm6qi+kAbrkrRS+LJeyGkiFCwFwKkHpXAsOfM3u3I98YJlnZnWV5Z96gPYzhBRaPlK2NG1vCNvq/87G7+9PPj4dIlOPBsTw9ldJzLLhl6a994Z/vxJ68+/ry9dT194ytPplIC5YpOt5ilkC91xOowfSdsmqbFTy5spzDsBO0huwty0NNCiHBp1C6xHsQYKaone5YAAQBQEkKFBEwgDOyuUmFEoebBpvjK8gAONWCjB2gudw8bOaZ+I7sJEIJGhDQjh2wn6FCu0gJ4/DlHOOc7Gdmv9RQFGbdEuYk4ge6QoxZuK0oh4WbYTWU3sUTvS8TRGNNS7cos9GmlRG2pkqD6boPJsHXOC+amSik7HDOuOVg8Ig5y72b64xHGCGkUPVKuiZGFxOEPxDFWBnQJbjLklHAphucBCNlIVBMK/NIuP/nNabfBeeHx3CfmFrw96njJWASLSMu3d+XDn778zUEg7s/L8exv3Uzw7vHAwnfooRDlU2KdwN58fjPtt+V46bWgGHsfnGhm8JmBj5bfiEwh41R+cqS+iXBPpgAWxp+QGb1jzFbLbM8j4RKXCLO5A/OojaEEy4I6QVJJG4UAgdYTBtId3VVqR9acYydlc4Mp6QmzPIZIr8bCADqB8ayaiqEaNxOAnBhOYm7o8uhSCRWamW1CKx6rUOqwSEI0Jra6fG50pbV+DlHt3txa7+cFNR7CmtgTRWpD+ipnnoCJW3N1hEPrWm6K28zVqGhdNuTuyxbF5MwSZyT5PtBnqn8uL16ezrOOMxF1FkZLHG5PQKRWRFhVFONx0fmo5igFEO7O7dmzp+zN2yX0R2A204SuzBUKcTOwWC+lPLuZbu/70hnjxgZfmD1cWjG3zKVwt6IcVpiFhtxeirvNJe2jV5qRofponA3JWqRTHPyZAVbgbc3JMC+YCmo6OGYE6S5m6tndS8+UbaRnwVpx6OykHAxRQs5kU+lJTaTEPrxnaITLW2MtvqlmDM6bLg7bWXfpNAdutu6KPmaJQu9OubuiVxrZ7eHuMvfuoHsD0JpqehUBJpM8SnDwnhOYZRizXkbjVg5GiEpqcAVBWsUhi1XbFmvMQ7M1vB8yqTNPvW/8DND7J5+fX917DrZV5okxT8hCRRguhoTkrdsdtDErUKDDw/E8t1ZLBRapK52Lk/RzRLE8GFioYzLtJ9ZiocyxNRnHykgEZWvp3JEFm2AoQHi1ktSXKaeLrBlmoLY1xivJyBQcUJbOe3Kgkj4s1aIzamkx9CNp8cBYkcpL5pTci1UL4gcmFKOMoV5hineRPSZGGSeFXymzZ8ZGCFyaTjMuTZepWzbulCwdSKS6W4wPgeii3IeHPwaJiT6kw0xDEQ9NSOQc3a0290ghQ4vSveVnENLJAYgpXV/a74BCWwuLjNO7MWanRU4YrvuR7LgpG/eIhDPJ9HgvKV7mfJ4/v/e2yEzR4hjQvbvAIacISU1AUoFWPBNuNrjPOJwu+x2XuREie+CweJ9ZcRPBXg2U9xrrNSbFWpd7joXEaClP3sCATiwEm1Ti05iBkIf/lAKEj0cfB3PU1LPHRkEaonX1UWnu4y3FF3NZg/tCJ5YmH9YAyi7tQAAibF5k15xqpJ7qEmHVhq0TRyxAJmphSeDoYYKhVLG6uy7NT2ex2GSKggrVhvFKHOoemnYJHmevZ0fZQ9+va8m5PY4hIIgki7LuzslGsWWt9gZREZs5E9SH/82Ea00tkPVQDSo0HmuU8/IrHFRsJrx5dCpJQxJaHHNfQVd+JwfFkMA2SZ38Yjp3rV8jb3ZWUhCMQRQM3BeHi6LeQJeq4XzR7ZyJZtIyo8KWH+Uh9c/2Qnv4IHj4TwIkYCgykn1CVnD0cBsomTTQx5k4Ym7e9ShHpJds/FF/eIqK9HQ/oaShw8NTwkgUMtten4KA0Q8tjfcVrKHYXeKQi3O8SeW4p/V3eFSjhNGfk2nqqFaut/Nb6iwOgPl4PV6P1+P1eD1ej9fj9Xg9Xo/X4/V4PV6P1+P1eD1ej9fj9Xg9Xo/X//Pr/wA/a5bW+b2BaQAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8S48tW7odNMY354yI9cjMnft1nlXnlOveso11jW0QNmBMD2S5wy+gAy06/AYaSDRo0kWidTsIOkgWAgwNBEKAhI19ub6uW7du1ak6j/3KnblyrRURc37foBGx9imZf4DOVO7ckbki4/nN7zHG+Cbww/hh/DB+GD+MH8YP44fxw/hh/DB+GD+MH8YP44fxw/hh/DB+GD+MH8YP4//vg11PufpMCTmrBessEQkAl396sjPrCZJCIgh5MACTKOQCyxZUI9SgFgyCsIQEMNEEA2DwQK04nnxqaK7qoFASzOiuPjFnRRACExggBWNrmJpcCAGA1gsHBa3XSEjg5bNlY9nhsg2te/1/Pr0cCN//koCW/QFezrGeApc//+ee4/cHXq+Hl5MuPy+fGiHR1ktfTr/uAJCEJIKgiOUH2uVyue6rdfN3LnHZHcsf8PIMJBqXW+NlfwL4nXu8HFjrp/rd53G5xA/3DAhwKMSQmNjl5fFobqweIUiI5U+0PrNlM/+l3+vE+Gg/nA5tgos6PnhrSgZbzmvp93981e17loSILCSaqBroXLtd6rvEDc9jmwtOb0YQlBHqNhnnNjzp0ymoyFelHdph8jeH6btvz8fR7+7iquftbaZxevSbq7QdjAavIIVGK6DhNMbx5FON1uCBJsjhyxuRZEQg8P1LBbDaxPrgdHlry07f2xxF8YPBCB8M8oMtrpYQFyP8YKPr+yTX10gt2yREgjBAthwBMBohgiQI0kSBJAEzUQbKPtgoZCAIQlwshTSEgaIZRErL7xBY9qIEGe13jA+GxUyXY5EIrBdwMezlbhQwKtb7AEApLhN6eRSiSwYwqCq1wCz1Q7na9QI94vFUH0/jXNUcLRSOABTr9xrI/8Zfe/nV14dC1immxza77/dpnj2BTfKmlNGVVIohI9yyR9enkijqytLLTzaYNKd4NDuFXz3dzqbSpfNYFZDlufpmm0pKw6aUocRhfn0/aor5FH3G7VW62aVo2O3x9MWwKZaICKiGGQVVj2HQ1TZXj9a8OlzwgEeEIyfaJk3epiOah5cEDzX4BISWaSkBXNzE6rWWSU1imbnrHCcVWg0EJLW+rtWGL/4GF2tdTHg5gLRO9sVYKQgy2WqfMIRAowTYug+MAmAQGaCZRCMVy3mMAGgMUCbSQAmMtByE4DoxYrVyIChAizcywQmTRBgEGUgyuMwCXebXxYEBBvrFwX0fGWK1YsMynQUjkqmAuz5fbbsIjbOfrZJmCDASIMKEMFjADUnI+33/sx/bL3753kwtM4DNJllSmxHnSF0yI0mXGEaFGXxuZd8NZh1pc4yznyOiaQtunvSnu2m3H+5n2c5gfHg3bp/2fm7RYgRf/+bw+PbcpHB0BTmbjzLj5qrrO17vCibP170fmkkoqq7Jozmae7RcPQKoHh6JwmbTlSdpijgc5vM52pBhqR2b7udMVYd7tLDYEKE2RpxFqitszpDCqCY5SNPi+QBJiwsMkiHw+5AL6UOY0hLWxZCW6KRL9Izl1TnjEj1sDZCXcLm+ZpJLpNPFaARqcbW2BDfCQDBWswNAGQSawQGZcXn3S6g1XKYQVn9JyKiLv1zdoABbnf8aJ7nY6OrvL0H1+wi7TloYJYgkOXSp7xJCIUSohVpAQQdcioAuqU4A+TzX66v8xadX+dvHx7GdT3hoMzOmqru3yp3fPivCchEgARrJ5m4yDvnx1JTRauTBYtY8NhUe3o25szpG6dNmk09vp0g4PNTT+3l5dIZYfbkx9cmbWvXpUXbd2S6f76eByQxmJnrQLCs3i6xebFJ1hkcBd9elPO1m+nZXDu/OU4MndANaytURCkViZ9OuR2J99OntmF3PnnGsGJ3clnaa21nWISraCAARgcre0BxBShxrAEgUwAhpCVtCrMGYsXoRAkv8+ZA7SlrenoW0vmBJgAI0MT7kkN8b8+8kg997HVICSBkkwegiTARjeSem1eOSWHyfmS9h10DQSZoAE0VyNX0TaevJL3nhknyuVg4RDIkkpTCDGWVBs67kviQJk0tCbZgj3BFiOFoghNAy45Cn2qaWrp/306m9fzXdq54OgvE4aRbqhCeQCHK5VdIgowfm1kZgBJya5uaPYk7jYdq/HO6+Ot98vjkda/2mXn+yu/vu0YZyfdudX51PJ1diSCAybXudN0OeHnz/vAwFM9Aem59qt08h9CFimbgQQSOA1BSEAX1Ou5ysS7MHEnJJCQ1qkS2Z+kRg9QJ1YLse2l5jlzbn+vQlz2eNYeXZ7vTq0GxGtnxr87sKCUhPr0p2O80RjCa+uq+EffLESqa7TlWP7gEwMB0gh8nqOnPpUEgUCIUQQAJCsVQUAhyXN3kxz9XQJMOSkIOL7QLUurHssCZia8qFD3a55IKroxHIWJyrIWBmiiVY4uLhuIRPGeiJXNznckiCRheMlK3Z/4dcN7IxZRqYEs3Yd0XSVEVLLVid7ggIQhM81rIghBxAc285P/l4+/TNeO/tCLdkpSlc3jDsspJ9yBDnWbkDadYwo7kk4xwqZqWz/maTU7r+aGOzyiYBauead6Xvs2XDkNCaN7XlKSS1sVVn6ZKBbFKTJaZNHk9z3xlLTlCYEUHSHUudm+Qir/rupuvevpllkTtAiibYMkkBqqQk0BJsckRYZ8N13m/VZXoJ5rx5PmyvHZ7ufjsPzNvPg6Frdde3XUwx32Oiz4q7qj7xyx/tN4MRuDvPbzCnzBI6fAsf2SE91rmDQWqu5motFBgnd6DFYgGgWGONQGsirrVqiTVIrbnk6sl0qU0Ca2TVhwpOq8dbfiRCS7Klf67KXosYfnCTWOMSlnRtCbiwJXhSXIojBsC0uhjy4kpzRk8a1As5pb5kQs2Vcga4FptaK+tYzg0AyK1pbkoWJduLL/Z376fTydWp60gjA5ttYjLSQsqBnIwiIrqO1sDezqc6XHd5Ujfk6X318ES00btt0ckFbq47f1sjsd/YPEIBKxSVizGYE6PB39bd89Inu/vu2JdkgYDUqfQAGGE1QpKkxBBUkn10s//85VV7dTe+fZynlhLP57CkkLmizwlbQVBQ8Hx3YkodBXKaAgqWVHrbXBe2mO5bPGr7tNvepl0qV0y3Uz6wvvMW23QXp/Goj18MV/s8t5hPiMzNwF5436yeuaM9zN0mGQPuMTXV1qzi7nF0+bmCxjKkBD4c21gDpCloSDRQFEIk1ZoCGgpBTTOqX0q/BA+QCF2KYl7qY168HfHBNFcEJj7shrjAPh8c4IrorJmifrfiXi6J3+d5AGQAiSEkogCdkLN12XLi3JwK8ALlXCpZW5w3ICE392kGpMip3+Vnn23ufzEdIvyERPR96nOicSlkDDDKJTaUxBJoAQtwijp7fVBrTY8W1UPgoUZ1htgARhudtOngcoVHzthf582+mIPJh6ucDRRSx02X5mOr72cOxt4yrZkn0REUSCSgS/n59eaLF1ffvT++NfjcHs56P6rrALUa+PhZWj2HK8ESqHARIiS2JnaJJkI5Iw3p8VXdflJSRmzUh+3nhD4eR8+b9C//lSf10D57OVSP7x6m92nc7/J+l7dQ21mj3aSOte5SMiFcU/U5sp086jw7EmV92uxLJ5sjZomEwXJGV5i4wBU0s3FqoP7gpyoJv/gtXt1h6GAFFE8HBLiUGIkQojl8KTMFByIgIBz+wdoueIy+zxdXK8Tib6QlQvslOC72qsBS2XyI2VyBEoBgc9IADH3pMpOxJINk1FKKRlxOZ8iBJcbkn7786GE8neep0rd9+eyL6/vDXO/PDQEYCsE1Di3HWnCZvrOhy92Ok4cNPQPYpblF6stUw3KGBxDdVYkaEoaXm+lY26k5OJ5anZgTSp8MbM6yYdnmeYq8y1sO7eC2yxsRs2wgc4gMwEAhTBCtGJ/v+59+sv/F683//Uufb4ZzH/GuHcbWHPstzRhBSziPLYNMQCHNQNYWk2w7ZA9kgYmbXT5tIyUjMLhNo//R+9PHc5eM7cFD8fJ5/1jrb74e/+jV8fZzCkiU0bKZjMmQE0uyBMGMgClpir4kGIPKXdptuh7sjjOTwCDZ9Ug5DckJ9iUZDea3N/jrf1nhmA3vT7a70fWVkuG7r1NryszXG+0git+eYElbkKbZaIbjOWhMxqlqntf42JpckKMBcfnuAIQgQpAhrfYEX/Ox1f/57yDTy6RtAXd6hoFDsZKtS5yKJUNOQjYzj4YQkhCCG1KgBfK/9/f+5pv3x3/26zd//PWrw/kRwqc/vn79/5xbJUKpMJcVN0pApuVEr8oGCC60xU9SzeHhbRS2ab6by3UKZ32o5bbTqdX3k21zeLhCWTEq07y616ClxIxD7YeMU7NZjch9wqMzxIgFkCJggGiBoFAsXW/LJ7ebF9d9fdrzSbcP9Lf1fKjzm+lJp2jhUmRz4XzyROSOOSt3TNm6ZxvruNTepHKn4bbkTlCM9HEjf1Hru5xOdOk3f3Z8tRlvb7t/8uvzlOMWFlIVBq1oRsTyIgKrI4DQFBdwzlbQO5PJzBlLWSgTzJFp0jCkzaZMPn/80j//CMcz2p/hoy/jL3yKTYfTow4HjEd7+WR4sUvd6ZiSzgZIH2/BxLavfYfX71K/9d70+l06jbi5ij7j8ZBOJ0ZbrykcLkTogqNKARc9FIA7Qliol6UoXpyiFn9JQFgKblAKL4kpWZeYqGJAFp0OSXCHA8nhCUbkvttYpg2WKbZo9Xi7G37242d/9tX9eawpmdEW1iInFtGyWY2l4mkIUC1E4FRbADCN99OwSdMUBqRNmidPycx0HpuC4SibrEPFEvCTyZXmNuS0EXB0h3Kf2+Qk0EKeLECAC6mhBSVSTrkrXb/fbvpOQy6lUOielrytd4fqY1XKc/M0ieTs1qrSxJJ0tcP+Ns2d4UP2QbMiySWDhUxG0lLdKD0SxkjlboyfPe0/O/kv3p0BCqyOmVCsyMOSLruYJEEKa4oF14DWShmAGVaIIi3IHCJAksbzXOeIj59g1+M8oQaeP8GPX4CBbypIoqSnT4Zng+8ymqgDEvTJk6SMcQ8AjzW9fOqZOLi3lJ4/U58xVyLldqIUWUmSQqGQDOSCw0QwpNCKhAVCscxnCpAUAQfCGVBKSxkf7iEP2PoniSbzpWCJkBIYCFu9Y/7P/5s/eXP0u4fjXO8Zx5K1cT59uumHcjxMh8lzXosTCE6Nkwc1jW3b2eH9mIY0Ptbuqjs9zGmbW/U2eRnS6W4adlm9Hb853Xy6D/L9b46NiKzxEEs9UjorQ5qPrn2uYXPPkozHZpJ1KVKTQzWQUzI0gCFKBoRZTla6HrnbXPW2ySAy2BS52LDvelPpcwvz0Pks0mgiGeI4aR8hmokAzQCDJUC+oPpGJmOQMuzNzuE3m/Tbb+v//seH4+S4cAkhjYEIcZmHCw+GaIiFuWlL4RKxJMcL7pq4PkkuiTpWMley8zyGlDu0wFev8c1r/mQvAscT2ogQLOdhsFSI2aossj7aRlfiTF1fwQPl7JsBLXAWSu8vnoPCd3cCrZ78kuFDRsrsAreBQjC0uKrFXVkAhHGBkAlBfbHavAnewiNysi4byFr9cKre4kMGqA8Y71qogET+L//BP4I1sDJ5V/K2t21vfWegPX26uQaOc1QFAHd5okcokIzHY1VO49isT6djzbtSp8bM1Nn4OG+e9u3U4th2L/f1WKNp/3Tz3W8ex2PMp4CBhJ88cvKmNkW6Ldql0+y5MA/mRC2dP9bNLOtkYBJM5hGQDIqlss9p23XJ5RlG2Mq883RWtIpCGocnXZQ8v59jDDPjlZ23fSoJF6bPljzLFnIKpBLhpoPak5Q7cd/zarBXDw2C9dSKkS+ZQyTki0cDYoEZPaQacGmhERaQ1chiiYKDhQIRkqjEnDJiclAf3WJTYAOs8PZKux7VYRVN6LP1yWw8DubelSc735HJckjfvoqqlDsvCQ8nHGdcdeh6nI64Dxurji1MH2DYxY2vDIGttgDItJKqtJXaWuhRK4VXmzK3mcJ5apO3p/t+O5RkQHCcfazhERFogQgufAACsbCIQn64f5sWQUVmydOjpVI4DDkVm+a23RQuCLSQjfLF7gkiZ3j1vivnx6lc5cPr8+758PBmLBvLfTm+Gvcvhnpq48O0uS5em0MO+UwYECi9IWk8VkuM2WE8vBl59pt9Nz3OjjR8Opy2qTyqd7eAgUYahYCHaq3T7Cj5arNZCRkQUDIYOIc9e1qOEfdMw4stHd1NN70eNcXw8cZ2xcxWkQIA0BJC8kZAihXW3O/ST59e/5OfPwTxdGOPVS1cwfVjYAniLfx8gbS+r9oA9wWnXdnMheFJC6mJIBWQLaWfUYrmGDYw4jTjfERzqOF0wumAmEFi15slOPk4p3NK227aBRJwP+fvaomml88e+wIJhzs+/VRGSMiJ4+yuRXnwgUQiRVgsTANW9jeMNNJAMuwS5KkY+r7vk+WuY6Skm1Rv9/3NfkimFnJvtS3AIarTXR4IrdzIitOmDArhChcmgJoMdfbb6+797JNru8k50QB8iOqGmFrZbebJU2bOqeSc+5QtlSH1fWaXcmLfGzxP0zxsSx3j/jdH60yp+YwF9o0KbqzrM8NrddsV7tLhLE2RZq+/iTTkbtvr4QyTAQYYFs0RvMFd6LvttmO2ADMtKNGGfc+Htt2UsUbfFytGoFznss3jd7N1ZkYkckF4lqhH7Ip9NvQH1YhoUBH/7c8/HrfW/TKd3Z9s89ePLUQBEStmDa0EegsPskplSZFBKCLi8vmSni1U5YX/pqTF0GiGOrfm8WKLl9dICV2PJ/t4cYvdBvcT3r/FOKb+xth80DRc5ZrS41u86OEtxlO8O+Une9tsduOYHg7el3Z7NZWMw4ixMppIeqxVi4BYtUkC6EGsVBolJYOZA0zLAyKIuILCSMHMLKkUdl3abwqgc9SUk4dqxeRwV3Mo4BcAZUFus06RB+SOSKDgTp+jnr3mWbB+KGuIJhgKoSk6sO+zqqds4WJim1q/yTG1/W3fDt7tyGe9H2r/pM+ZcfT+pusep+lhtkKdYFlqSlumwnpsm5u0uSmndyPIclPiOvnsGRy67ELXF0yVtkpcGIGQgZaIktIquQEUBBKt7JLtc+ksg8NQghYMQGWX44lSXu/0wiRrdZWAv4t6rmnH66t0U/pNSr8+T6IQMWRuc6ruC1a8wEmCjGiQAso2h4eYl2QtpGgQg2JoPRdk5AcPd8H0ZUxzbRG62WHocK74019hblDF/TuMIzxSIMYaqSSv8Np++yYwa3+dy3Z/u9lvXZa0t+yVu8304xfTfJ5evT7evffDg7f5wgbEwvtfyIgFQoUuqo2F1uKSTgZgF99XMkNBqDlyaWBEIEJdSSm7rbYLu5TcYSuusfABLmQ1xUkQkNEPljriyhR4fPTN3pKBMBgsFiJBc1NnMGJ8rBVBN59c3SrEMgfmiDmsKmYlQZPCI2+tH/L9qyklkkiJ/Sb1+z5O1bLtng6WjCUNrkF8+93p6tMtadPrcbjazK4hYBAhhqhF/oUIIKXNkLeIBgaTL36+td58moINmhO6AkkBZOQNrTOmtD5oiQQNZpgQ3x2m+dXMxOuXFlv7b7/75vVhTpNtrnIufLax+6mlhfxfgGvDheVZjqUFMqDkDaElxi9uzBb1EFfZZCyBNyRaTrRZHsLtFrWiAW54/hH6K2THd1/ZL7/Ock3Vu02e85NvX59+/vr8k6fbz7/8Ynd7ozeHN3eHx1r//M3xNNXawl3nMY6nm7nO8PmS4C/GlmzZJNaCMiDDQmWKZlxm3aqzXGZETtbCi+Dhs1iIqfrdcdp2OSKm6gC6hEakgMdaR3usIi4uOaxIEhZqZ3Fqglmm9anflNyZUQYrUDajopCbnPpiw8ZaYkTErvgq4lMLbZ4P7k3Z8k2GB000alZ7aOHhs0D02fbb0tXmZH+dM4TRr5/18VAB7K+74SgMyEPugTYFCSlSIIGSQpCHR6BP+33ZD+k41lYbUoHDjnXXUWCoYW5kWUMFwGRW7KJ+wapKJJek97FzPoEd/NXdFC1ucroVTi1yRS28HfLLNP3oR9dXT/IdR5oUsSQzq85ngQhkzb26e8QqVFvMbGESCa1QblxENwDk4ST6AZsBd+/x5h4vn6IAxyO+fdeNE4xotVaPSfzTuxrJfvTpR88//+TnX999/frh7vF0f67nuU2TT82NbC1+dRg3QxmS1RUpA7ho4JYbjoXAEknEwgh/r8TkpbKRSmafOTVIaNLNzo9HnKb27v587ksoDueaoJyWxPPCbC4T2EGCgRyBRMEYy2QLYoUPQrXYouKRilkGGdYlbTdl1xk7TrW1lOdTsyHVsSkBgE/Vtjkmp4nZ8t4YMZHOCMM8B4lcaFloLNvcEemh2c5sm+eGlDV0iXetJzGqa77dd+08NykhEiKITCjcI2AoYM5MiXN1oGj26WFiuGWOguc5PelBqYXcLooZLKDvhYWREalLNN/+Xpkf9PafTj77e9iivei6lAd2hV1Of/LV4Ybl2RcJWhMuW6GKNRItQi5fVJaL7zDaqsBICYIFTYBCMCrTPFoEmfTlSxhwOmOsLJ0gvD3g4SSJ+03yqK/vx8l1OLaffLrfbewf/slvb2z8bBMbtzq2t4dxnH0KREQ4PeJ09pt9SgneVpRiFV6s4m9dqplF2LnQcgaKNC0CqEX+KynETDTMTS0wTuP7x83YWlQdxwkI44qlw6BAukjqFtljDqmFGEy25H0BWipislKSpUWrRBlri1NtbYyTUS3lYGuoJerUZMIc6mmZMYkmOJwqGfVVTVvTErqDlskmy8ZkMiIzZ+t3pad09mGT1cEpXbMB3GQfSgqVoY/z6FwVp4sWcJoqQHbFp1BEq3F8d6bzfNRmx6HP59PsZkuCiUtE02IYiwvSiqNaYulsNFmnq5fF38f1lK8NDwd/bP7Y4iWsUbtd+fp9HTxCaaHBVk+IVeJjIshEJlxy4AX7X+MQzAwXIf6Sk1uyCEi6vsbtNQ4TfvkdjmfuOrGizuiT2OFqk6fqcTh2ho+f9S9uek3zj/bz3/m9vSU7TO0X77f/6x+9/ZNvTl/dt6PYPNyZOkQu5i3ZonhbmO60AhxrVcCLIpIXfGYt35cqJpEEPEgxFzy5UptwrHE4Tc1z9TiObQFjF0HIkhn4RTOy0F+WCpnJjFhlnXRTbTCzlC0lS+Smz8MmobfRwxJd6jbZm2bE+3djy7z77tELDm/OdYoADq/GvM/jsR3f13JdxjkO7yZkY2cgLSFTXU4lmZq6PsXsMrNi2aM4Um/dx4M97/vbbjOkTZf2113JiTQaUzImE3UeHccZYP2uHt5O81lRI2ZXwN3G5s1SuRrWpwgyFFo11lzdmRQgkYjcLTi5WeHNT/pDanWKmZiL/dpRZxhwM+RdZixPapn9izJPApmMiZaJRZJ90dhzgTIur+CiA18Vq0tnigSYACFlbPfY7bTdQAlvH5LEZHhzOJvr89z+8pX//ov+Zms63/+Vl2Ww8Lky/An1+y/6v/qjzV/6qNsaF+7bguda16Jjxc1oDKOFFIoFcl7K4SVnXMAjUsbFAapLC93pvOjCp2oCWvPz1I7neZpbDXrwQ0LmgjsiVo5fQlYn40XvCyTSE+RCUipGY0fbdanrbG7RXB3Y5ZSAY4vHqYZiPNU0lPFU8zZP5yrCEs/HObzpbDXZeDeOpzaT89TqJOtIR8zNhq6dmkKlrEp6jZEKc4O/mYbbTZZyn7rwDqkbSjtLsTwNuvR4GnGese9Kl94+KokqmucqoXRps+XJihXKQy4zSaSEINLaF7SGulAQKbOQ4bCEfJWefbG9eY9ffTe+biVch+o3JUfyF9v83i/SVURKC2+EBXgjVMhYNKpazREUF70jARNN4AeBIhPpaKJePsftNcaKX32Nq4KBiIq+j9ZoCTlREU2swXeHo53j886/+Gh/u83fvT8a0n3lfmdXJ3t53X3zvj6Mi2JP80h2vgjcUkofP+mSwYNzteoRCinHop+KJXHkyj4FaDIhJ3qIgEKbofUFltSV3HXZA1NVDdWm2dXaipYtnUHSyoq6kBEGg5KWLAJkOLJQBsudUTCIgWiaJ2+zKoJXeDzVx7GdpyaEyZipRCmQMiUr9Kay69txno5187SfhPdvxnmUKNJSMW+YqyNxPjY87x/ejptd2uy742EcrobUpfn9VBqjJOwLPXW1TOOczWIpoFM8nkc8jvjkavN069NZ7qkky4kH7YZcBstua2wU5TJXBMMikUy2VvNhCMIEW2VTJI32Ypsfzj6mjEA4vjnX20IUezLks2qssBjMbOUrtRS1kpY+wu9b2BYp17qfGdOHvhEk4xI3TjMLNY6YgCd7MqvrMc9oU7rdKJUUzHufrjr1Ga3Vn39bH1/s//B/e/P7z9OzTXp9bg/u78Y4BzriprNMrkqhFkorrPLiqvvZx5skVoW7S2iuRfK/tEXkRAJzUxPCw0M0c9fUYsG1mnOqmCv6rpSS6Uo5heiyuUYNLSddNBa4sO8SsiGSqKpFsRmZWFoyl9YjxTTiHBXA4f38eJhR7JtvvR/K4/GsRLpKjzbF1bP+8dV0+0V3fD1urku3Le/+/P7m070lvPv6NE+ObEEKSoaUGaFa/fq6x+zHs+d9inPMdcKjK0d05rP6XT7+9oCbjQ1dKZZkVW1tLDXW2jA3dGXoSzjkDlmdWt8hFc5CKYkpVWhp21mhoarQWiaCASkZYOhygpqCZuiIz/f9//nVvTJTCyXehaZAF4rMWyRDLHK+i7h+QcMQUPMQkWlrBb6KzBfxIS0W1gkKgOiSGXU6OQ2fPsPVDu/f4v2DbfaeE/oB243qBrP09lA3nZojZs/dsN+2c/gU+GffzM+2+pNfnd65Nl1SuOg3fe6stoZsMmCbgyYDP7stxTBO83mOkukhD5mYk4E0MhMpccgWC/OCRLUAACAASURBVA5EZfB+jHONTI+w3aaSECwlAy3nKDkt7bchLYFyEa7g0sipQBCZfYLBQnKkwByeZBGWmAJqNcZzG4E2x91hHqOZpzlkpzrPzRITkTzM7HSonmy8n53yWTOa9SU5JLRzMC+NDFoihSbPV5a6PD/Mm03qujRNFYkM5H3x+5m07b73wv1Pr9MxIPTJSpfm0wLCi0ZFoAF96S2BlEekINOma7VO50rf2tB1rhYX3ekicqQWreYCuEQ7ttyTkhkJJthfS7sf32z+QbxXyINGNuHb0b/IpRI3ls5au9wW3SSWKEwAqKEExCoVWhJCULG2U0mWv1f1dzkZQDN5lITzDACPM88nfBF48x6/+pa1yiFAzze2SfGIsr/e/sUrvBzsb34y9Nt0msdf3k1/oe9ajVfvasrc9Ljp7bOt/WjfHdjOqQFWUrrZJEp35zrXyERfytQ8kWbRHMez7ze5L1aSneZKYFPSZDZWhcJogrtkgdoWOMgEJLOLaG0dHwSVH6h0CNldRlOGFVgmzmJVSlh0giEdx3YY23yKCqfx3DxaeJMLZjJDKZaTjdVTSu1utiHNp6nbZxYe3o55V9jbPPp8qgSKMSUzY8oFLhN22zIQp/t69XwTLY5359tPb9rdGPfzrklVxdJ+sAQOfTkfRwELwRiK5i1LTzOe9/n1aUaEZWunIHJ4RAu7yI4vlMbK712Qb6i2+bHGieFAk84t3lt0+vk8FkOPOGLRiODrOT5vUXJKYEzwjXOR91w6wRZhQkgVGsMlBBmxZPhr0RsLrb6gaECXKMkVfW8/+sSHAXe/xat7/Cs/xdUexyMeJraKnOKLj3a3m3p/nr6tQcAyDPbiyn786e7v/6OHHz0tBjuc4vyiO5znQelHV/mm5NttHgxvPBK53wwlYW6xLembu/k4+u9/bAB+826W4suX26f7Mlb/9Zv5xVXXdWgV357m602RbOk+j8C21/mMECLWGnupYM1iwXCWamLVRfJ7+W5GhSA0hEGuRDJBnaGQQHV5+OwKRbLk8HmOeYra5IG1WEuRyJyZkxlVOiLQP1opVqq62WvT+VCnKSyYMjKRu1xb5JR2+5KbCO6fDTkYyXZDv6s6I3WFcMTX4/VH+32Hlshtfnyndo5IiATleDjVp/env/3Z5uzX//XdZK3WmqcZk2Ny9H1ZbYuXBnIyYklI175tSgg5WGefxghwLPPb88Q3wt3ST2YRMtMsvBrjy6EcoHxQ7IG8LEtga3PbIsQkZuDk4RFGY4SUtMrtDd+LPZCMXU60iECfkAKHR0yOcEyPOBb84jesNXUZV5v02ZM+H6eh8HyWRu86zEMS+I//7PD+fc3ix8+S17Y9aZ4whV1ti4vnwj99Xd/PsR/ys10i8P5YQXt51Wmvvth5DhAf3fSnc2yHBLCFmmKf8td342nym10nX3oGKfHNfTo8+ti4D7TqZosyKjLpSQTC4IFlIxad41oHAAotXULQumQBHUaKiKZQAsOyBbAKlUQt1LuwNO4trVpmQcAMRqRH9gXbksrkDoxTMJCgDOshVgfQ97kYNIm9b4bsx5aedrlL7Rj9sz7NykO+ycN1Kfur7kjEGO26f/s4Dr13PQvt6d5wy69G//ndCSX53LbRSrLbp0ObQ8YWi3R06Zrkpc9b6wIWKxNOKVpDASmU4E8/3391P87fns6VpNZkTvzl2X9yhZKoSX6k3RpsDZgrTHupPNd63j8gwVpER0YwrcEkGwEb5wpy03sqqI5ffoPrm3ixR5ex3arLUXL64uVmOxgfYVShxojCFMVn4pt7//nr+vHTfH3y89go9ZYmRskpJfv2vn1zRAifXOch2VxjrKD5WPXu5J9ldil9etMFcDhFXzh09qPnvYGHc/vstnOHkc3jwtnycOzeHyvF1trcUqaaN0hmWNo7QgtSA1v4zQwLMGAkcqIlytANtt9aMuu6tZD2UIRjURZQAsKxajLxwX9esr9FEh6ojqmqzpiaTzWmyb2turEC9UQXTGBOTKH+aVmU58wmVwAtI4GcYgCf9Pl2293uum0yFt08Kc+f99f7ft8N/9pf+QP8O/8ufvx3/62/+fFpdkAt2bNn3ZOrFFSfGcsNrEaiD7TeCkdi0VfFAulQvN7n3VXPxrf34/1DnReEwmhmyxICp4hfn+YbpgSWB6IFFmJ6kdiaLWh4CNE8xHUmRvjaAiujpXXhA3TZTNFaeKjLOD7i3QPGal1SCN+9wm+/yYX6+En34iZHa1meLAiMU83G2tqfva8D024oD2P85jC/G+McCqSUcl+6X70ff/Ewgdj2+ZObzsipqct8d6h/+nbKCRS/uZuMjFDfWzYezt4le3uYfvWqTlUw3J2qh+yy+EOXU07gYhqtVfdWQ5cmFBrs4mjW74Qt8GQSh8TmisDtNnV9/masKSXLJrHVhvU9IIioi0R0zfWW/5boCSJ0aYkRUgITFhovXCEilBISmMmuYwMo5WIpZIJVcV+aAj3zplNFedpbn5/fbv/G7316dTX80Vev/+zr85OXQ79J5/ezHeK2D5z/Gd5+9Ztv3kXz3hrndn4XU+PubppD8zCUDVfuI3jpmcQ65RZ81ZbrJonHk2tSXOsXvz2dD+0RlswuSdWyQgV+fqyfbrvSUdXqo0mgi74oScBMtEUWTShEJCm4th9RRi7dqOICQxpDoumTF/r8U3z3Fq/e2stP2m6Lhc/OOd1scptV3AHNzvtZM6PVkE2jpEkbx7tTvOkiXAiSHDa7d8fTbx8XRpsf7cv1Jkvhgepxqvi9F8OTTXp/anf37elVd7PpsMGfvz6dx7jZ5ZzyTae7o3/xon84h0tpxbUFWJeT1waEK8zZfNENX6oAYsWE4yIYWFIKp6YqM5acihIn2+Wy6UvC6s8gMcnymt6tevYFYV9f3IfosKCeCMDs+4UCFhhw4QGNsGzcJCvW3NlxGt33OWbF27GMSsdmQv+063b5alt+8uLp7e99lP/FL//gL36eshlovXFj6O2jZxn37//xf/fL//R//PVXr+t8Fo5x+mamw8XDfXNduGMA5GWdgvWqF2LA5AubDgcEefz4avtv/u1Pxo+7qSPATCMXvQVJnMFfjXUAGLL7rIpoa0HP5lZhDrZFbb8c2NaNQIQMSCtTjU2Xuy4FANjtDn1C6TBsiEBz3L/H45kE5jm+u5se7s4Ia0hTpIcppikQ5epqe4jaEvoMVKhirnZuuD+Ov313rE3Zcpf42ZMuZ96P+upuLjl9ftsPyaam51fd73228RZvjlXQ033/k483Ap5fld3ObobUAk93RaAZCeSim6txhdvW5TPkIY9VF7QsELTSAL/TzBJATiWDahEla66QYhjSZpNpmOaFmllU9KBZRKx68oV45WUNHq1w3LKEROZCoxKEr1j04lTFBBBNUMY0elwr33aHx9r3NiDNx7l3Y1S45ZRevNj/pb/xJf7138dmY++O07ktfkOZHz3b/+QPPsfHtwj+9kHR5fFV9TMG8Mk+5116927MQhh4UUlwFWavtA9XFm4pZxLAkiwP9tP99kzJ4XVRy3NVyK/CM3wd7Sdd7hpjXhK8WFaRWJ6zV/fJ5aGFzjUt7ZCrY9SFbzYkcK4NxkQ9u0Xf4XHEYdRf+BK7HncdamMye3pdbnb7v/t3/qW//KNn/8Uf/vd/68vbv/YvfP5//F//9GefXo9N78cHCWY2je04x9yah861vj00Y7p9tivz+GxXJN2dmpE52Vd358dzlKwvnw/Hc3v9roI2fMqc7M1DlXSzT8+u893BD6e2HbJHFCMMn72cnmzj/sDTOQnmWnoKIiJaYPlSwC/6hPVrWcflP/j3/9Zf/9nLu7u5jvHzX9796a/uStL9+Hg/nbyFByBxFTg0hFa96FIvgOvKWVrkLpCAQCpYV7RxLU5E69oNZsmUObewPm+vSnWcplZH55V5x/Mhbp73mLzeTc8+vn6uHjljcw28xOZP69gMZKJVPL0esOuA65e3w1Ss7LNimF9PkzBsSuooyc8133SLYECSZLx4cq352bKyFEVZCAWp5//y87cf/TzNHiWpRlokP00OgMkAVvD1rn55Hua5sRmSUAGGaHB3aa6rHNK0LHNgCUyrQnpxi0w0UuPsAnLmLuN4xMMJrUGBWvF4RDgjmZXdf/SH/xnwB8Dn/+Hf+yXwP+GPf/2zp3h8nP7wf/jjP//zd3/14+35MRSkh4XXpuo6OzbP+6cv989bzkmnqm1vBDz00xcbD1Zv2Zh3ZZridl92vU2uYnCwyzZWfXd3/tnnV2eHr2uEQIrjCedxaWvAontqMheqoznqhdP8sADCGuKI/K/+jS8///Tp60P9q3/nD4AdkADi/Tf/yX/8X/39//kfuge19gvJl4Z6/9CluOgyPqB0CohIRFpFWWsTxpLfLFI/GmhmmyQPOCynefThad9m16zNs36qnoMq7K63P/mLL/HRFVCBCcfzfJo765Bkk+/7DolA+ehHtwmAWdklTUWH1nV0qnUsY8WH1RMr1pteoNrF6i9phQUUnq0rOX35cYfqm3R+8qDpqNOZp2qWltXJ/l+q3jTWsuw6D/vW2vsMd35zvZqremZzaHGmyJCUGJOiKUVDHCWRFDlwpCCIjAAGkgAWECMCAgSIfySAgsRGHMFCrMmSTUVzTIo0KY4i2d1s9sCeqqprevWme++705n23mvlxz63KDca6AYa/fr1vfvss9Y3tsD+mQmrYegckWftdq1b+RAoWoVExIWgKqJqOoY7FCYSQghsI57CUEATQ1D4EACkqQqh9jg8RZJjYwu9LgqxO8Ps0z/ygf/mH/88kAFLAMB14M07r329KN2Lt07mZWOtJCkTK0uwpMLcqC9F2dLGuW7eS7u9/nve9Y7r57pf+OJfH03nEvxebva2etd2tl4/nL95PNno2dNZfTJ153bSznamilXtepm9dK7T7fBi5lVBCkp02IOv4VWDtM65+I6I9hHV9QSF9RtTWxQtCOwf/Kvv7Z0b5N1ehk6S2ssXRklm62VRNS74tZIgStklni5DFFOl1rPewxmNQYAx7a7RumihQWEJUCJmImZLomhqAXM6SKYPisXCdUdpMau9V9dI8FSX4dk35l/45t1Pvvvmf/5rP47zGy+9eM8tQpKIphRU2TASAwh2BxmhIoihpGu0Ejaog6SGbONt5TVLCQwToqFM2pDD9g1KFACSEDVWgTnpJ8mZat6hkJq8F8KJ6hIuqGEEkOXWBHvad1f6WTkPJqH+Znd8WsThNSh8EFWGBqnieg4RUoi0HyADSC0jxjYxhl3Z6KD2YAPDggYNcG509Tf+0X9i3vdfAVeAN4BngVeBC3jzr7/23Ovfev7gxbuTizv5pXPDbmbKrj2eOOdReHfaiKQ0GOS9XkIJaptkg/67fu7vvuvn/iGwQv1Xy3/y//b7NR4/97H96xCHt6b/92ff/NrLYyhNl/XRqbOWHr9kd0eWSZ2XqEkBQi/F8aoFFoKS1dbYYomsaRVXgdZ6WrS3mghAsJv7W0fjs4t5/+L5jX6/88ILb03Plt954eazL98KAmutIYiIaHxE11tFCwODwvqaiPMZIbXg6NVSVcTvr13HDJNXXRS+KeEdVovm+KQolsE3yimXhcTQLGUY5iwJnGXfm4ZX/uClp39C/+r1O1RrKB1lKRueFzVmJeAwyPs2mbkquonIcpLSsgRbm6eS1r7QlA1ABm0SImGdGsFx/gIRK7MJQJepNzC3Hzg74ISIrclXEf5C44O1BjAqqtCGwnJUDVfZNMhwu5un2Z17Y1HVIF7aR5ysUd/CPpBIHkSUTVIyCmGGMnodsokuK9w7oU5XkxxBz/0v/+3P4ZlfBibAV/DK68995/vveGw/3d959bk3FqtiRe7xa8PNjn3+xvg2uMuhDtIARTflDbPVzaaT8sGrE/u4vbKz/+lPPwNcAC4CObIf6v+Dnwd+f/XPfrv3/AL9FFc2/u4jvWd6eP24+saxhKBbg7RyPk+ToPCqvGZyrYEqXIhsrqyjiYRILSOCHxTtbPQ3ckMBKOxP/dh7zu/3//q7d774xVc+8fGnn/n0J4C5TfjL33qFVJXZWCOuEa+iShJFemvVc/sttUeNAcswTKZVSYAprnNr1Iqh0CagYTiR4szXy4iWggrRKAszsBb9bvL41d2nH9t/4spu0es++8WXbkznOdQUYvpqHMYnK5wugAadpJdaLikS5UnCxnIQUJJkmeYulBJNPNLKqdrflQBi0Zg9R6xgVcLlfjbYyMIJDIhjxgI/vP8YgDVog8wU0yRcT1E1PJ0tr13ce3A4c3UTREObF0PSeEDiwhpTybhF0SgxrBIie72/EYyiCagdJcx9M/rZT3wGz/wwcAC89cV/+gcvvHl0YWjvPTjqd3NS2d/uvL3eaBrPxO97agdCt4+XTVkXS+dqtYrpolrOqsrTndfHT169jtoBrwEbQAB6wA7wK73/crf83f81uKq6fbroaGcnuw59bCs7rv0blXzv9jK1pqhF1xPQ5ihkSYSumFtGBaTyUElrCFjf1xQvNAMWiIEK7NMfewJny7c/fv7ytW0YeuGPPzer3XxRsNLFc+cevXru1v3Tew8ORRxCPEwa1j8wbgRMGmLKBsOamKm7jlBiSHgosAMILqBWrYOKFx/aLRUP8VMDNuh1ksev7z1+ZWdr1O/myaRsvvzdl+aFUwnskYtm1hq1944WlxZjLJuY3cREAkozYjbBKxN7IGc/XDWLjTxewMTU/vYKJgVHKL+NK0kMnR9lkkK8EMAIBNGYhgEhEnUsEJM5RgZoAE6d37PZgfeH47OL50dvvHXsYkZFFD0HCMisxXWRD7RETGxAzkuAJgltbsDmmBxjZ3jxw89c+ulPPLP5I58GVgj3yuduvXzz6P7R5PLm3qpyq1U97KcC7eeJptw49LL+smredmV0OK8OzorpvK4K74oglga7na2N/OxsOj482X7kPcCbgAUYy2+gvwk82nnvB/SFr2cZ8p7tb/itvayc++6k+eFuuvOTT/yzv7z97TfP4rglisSGyqNqYIhaVLYlQX4AFenDNUvbEV7XYm6L0wX29i8bO757ur0zeOYn33vjyy/9/h9943i2vHa+/8i13cceO//FL8trN++2P4miLJsjnb32cAMKQ+1Pj5SUiXjk+ltkhhA8pAniCBIgCtgW721/CECCbpYMetmg1x30sjy149PV8c0pCGw4BGlUn7ywtWm73/z2W38r4aaXzWMYhxATpQkbS3GrE+amcia4bscu2MawQ265zYg0h6gqYGUAG1liDN8bV66WRMgSOQGbaDbBoIfEaJKENNfECmCgOnXSr90oM2ercmPYT9MkLCoL9VAmCEEDINyuthHZASXcGgrYqDG0N+xujPbf+fjG3/7Q5Xe852m87SOAg5sgeaQzPHrh9QebvaysPbFUdWgaGQ7T0SCzAhGtnK+cV6N7o7zTNdNBNlvWPmA4ynY38ySlZx6/tv3hp1q4ALdf+Jd//sdfe+Mf/frfB67hiV8l/2t48dks4cQm6KjrJ+VWKnNBcD96Lp0WvcPZmYKI5OqeWgYIoX2TtjS6KKASdK1q1JYlimdO15uB/fxv/vknf/EZbAy2n+wj6aI6g/eXdofPviKzZfH8S7f7/W5V1QqSIG2iOFqlpcTwNwIUFBkuRjS/U8vAqAKW2hgLgQQiryRQiVdwPLrSnjYGoChLd+fOdGej//iV7UE/v3HrAQG5ZXhBQmpps5ud63Vfe/HOb/3RS7PdfOaaeFJFYFMiIrJWamfVlk7NALRsZGgsSKmNW28xVI0JDKQQCFLweFGdLirvNIhaw1BDhpNETSY7l23XeJNa1+ZkKAQi+mDlrlrDkOlsTpaCIL40GSpCSspsokdAQVA1TKlhNiZL2Hl5/9uf/Hu//JMYdL7zuW9MCodOB9gFnkBy887nflODMTbJEzOdVnmfU2uWi8aHsDXKialvrJOwPcwPl2XlayLaGWUXd7u9LAmsLohJ0g//0KPALpACb7z8h//2n/zrb3z0fU9icYbBd4EP4un/OTn8749vPrcxTNKErVEorYb+xtHirPYf2ks3e9uff37inUwWMMB4hsZpnIsEJKJBY1RUjKxqx7KgIGnNm6oICnt662Wc9tHdgekCGW4ff/Gz37h1c0KKDSsX0vq1W6fj6bTNpaT4lLZC8fXftVwTR7+TIgjizKgKYhijzCREUPaQmFQfL8L2nUlrOEvAQL1yB9VUxe8OuqNhfnQ6FUCcJIDtGFOFxbTuenP1+rnbR8X9eemUFCGCwpYNIMIkSs2qdoRtBFtI0k3UJNTqxai9O+Pxbh9QDbWvlt7NBS4QjELjQGdYd/d5uGe5Uk5ZhTQoNLqApA4YL93GwE5V0hQ2oRoY9s1H37//5ecPJ3NpETPS6EoxbPa2Nj7zsXf84k++P3n/U8C7gG/h5fun8yJQ+tk//saq+Prtu7P/9MfeV1TV//F7X5ouVz10uoaHw+5wkEHkdFw1Xs5td4TNxjCvmnB/VWxu5U2jnZyZaFH6qnZZZndGmxcf3QM8Jl/709/+yl98/eWjs0XdVAffet25V69++gz4DD7xs9//F9/s7a6uPd5Pulw58Yq0Z4aXetlh8X5F+vatz7122s8hAsuInop4kwVBEHIKF+A8wjr7OOq2H36/QWGN8UgZTcBoE6jqV49eu3s8WUhm+JnLPcuuKBbOwxAJa4yWUIIJsSCilXJBwdy+pSW0Rye+wA1FQw2EgJaDaeNW42TGoHao/AE/BhHxXiez4s698cKtss0kKUM/sGSWZu5gftJ94tzGxuDGYVH5GiYuJZEhg/cIoGHf7ufUlTRduoJcMm5Oz1nYSENGpDmel9YQq9AH8wallmXQkYCMKhF5a7Sbhf5GlmQc6jXM2j4qUU3A49pt5KaTsLDf3crdsvmVn3vq3U8Mv/vmZDKvGTGlmsiYvQujv/9Tn/7gf/HzwAeADtAFCPqtX/+dv9jd2Hjv0xf+7K9e/vb33lpN629+5ZUWfkyptEmT+5OTkhl51274bHpWOicXz/d3B3kRQpqY85tdAh2drY6mpRftdm0ntU8/chWDvPr2V//Pf/nlV24djM8qY/nwwfif/+FXz+aLp775/V/6tQp4z8f/wU9/7Vd/89lXV+nbOpev9vLMGKZ+jwbXBmcn1cWq/OS796b1W0enWJTwAcwalKEsJKLkBS60wcfxnKmsFY6CCObYbkroZnj5BD9yGavF73zptUZk6UJmeNizh5NV+07MwMZKUHWQACFlD0OtWY8VhluSwSssr5HbVikDMEXvGqlKYO/aA99SOvGEra9GANawNbS3OxwvV6eTuSWQYe0n6cqHpT9rFmeL7elscjZZ+J6nh90MIgxylTDrpV27N8rSxOhJVb400arkntG0g/U0Ga9Q0YdpGZSNrNXktHTZkGK+joLzVIcbYCMg+5BnMwxVofVVHEQPV835Ueogm7lef+/eh9+58ft/eefwsALIGmKmwSD7+EcufuajT+Z/++eAHwcA3ID7IpIUp8WVc+e++uxb9+4Vt+4cryaV+OAhzkkIATVoX9OELdOqcEHsxjADYzwub9+b1/thVjadzNZNmMyqu8fLPDeDftrvpqN+r66b3/2//uS579+ezIuzuQtB1Ovrrz3oDJPKhbIq73zuuSufUpwfJRc2N4vVKy/My9vl5fdsbO/mlpmYtva7RBgdVwe9nVV5miUEohgWywbaWkBjWAjaVUDb20LWO4ESbI+B4zlKj3v3jr90897JpG60CDrK+HBaH55VXsVYStgglxBYfQiVhKZFaVmU14JH4nV8fkxXkzW/TkqExHBmiZQCSdPAt+DAOvs0nhQGAZ0suXZl9+LeqGiqmc7T81lqkdbUb8CGy9xa7ydHs7psQrnSPIv+ZCg0KEHLKoA1KFaF0542HX4ALeGp8Lz1N45/a0SJv4Yw6On9jc3z+VvfKdSoiAgpANOhzNr4wUUfE6FVKicGfn3yZk0Ylj7NWMSbDn3+u8df/vZRo2qIeh1z7XzvJz5y4aMfuIJPfQZ4HFgAFiDcOfmH/9PvNaW+8+mL//EnP/hnX3jhrRsn0VapgqChdsEaeC8A+r3UaRCvAuQdMxpl01l16+7M9hLLenC8XFXN5kan0zH9PDWGmia8/MbtG7cPZ6tqWfiq9AqVIsxY6ka6mzYE/zt/+vVPnc3yBA92u+mizo9gTvzhV6fVu0dXrvWMBRm7sdcjY+7fDBo25sXCRxf+Q8Ah/tW06jsDhIcUONbEN2AzVswqXN6tvnrzs196yYTgVF2QWRnuTYqidk6USK1lMBmWQCaaCWyAWqKgzD94H3tGQlGsAVFQaBXTSmQM4qrFof12WxYBrUwwygDThC9f2n7nkxcevbp7//jk/v0TSqQzyHJDyKjx0l0oGVqdTrxCMqpbbyJBwUGZuPS+CRSIG+9pqZXTFaF7Pqu7maqg1S7F+IQWHxIxfc4GvfzB1Bk2qh7wDONV2FhOiOLmzMqR9FAhbh1Sa0Qa0yqcz9IVNwfL4vj58sm3X/ihjHlcPfXY6LHroyQx2N0GEmACPA+8HbiFJpycrZaH84M7x9P3lz/57z/z3Ru3F2clfOsg3OjxTl/rupnO6iwzo2GaJWZVNko6GCRJamaLerysOjkvCre33el1kiyzLshkWh+Ny4MHy6bwGpSJxAiE6sILBClvJ/n3Xz0Qxh/VZZaaqm6u9gbbA5esKhQ6+eaEPB55amgMTG43d7K9cbpfdje6zXxVRRQJREbBBolBMOA48gssITBUWvYpCv9sxgai4fsnf/aNt3q2OW2wqCQIgfx4vsos1gktgLZWrfVuF1OWCfEvD82uBpbAEc5iNQSwMpOCnGiUAWqE4dqnQVsGjZEkZmtzsLc92NnodnMzWc3rqrHeLELd72YhqJ00VCkYAQiMaT9ZjwLqyQAAIABJREFUGOI2fR8EsgwVdsswPqpoK2tCGE+D5mkw6CYo18CfKggS57LoGaiDPzkqZzNvFHE4i0FzEXWjoBEHYmot3Igm4zXuGjRGJHAAc62Xz/efeWJ0eFD0tjcy1ZfvzuuGrl4tgTHg8JWv4qO7OLv7G7/39WVRNV4ThK9/7eVnv/OGMegMbFP5VGiU22GXU20W1qSpISXXiKgHoduxqWUoNblFUXNirl4adDKTMJ8tmpNJOZ1Vs0UTVHzGofSmCglIWH0IkuL6Vm6UbMfmud0e9O+dTueV80LNIOutKlY1gtmzZ3cMX3tiQERseHO/u3lUnO/woSFRGCYDUYZlTROowDCCwAhU2pdVPC3tXjgYdLBsfu8vXl9pdb6LlxtZ1hBohiDRYAuwQViHYIpqADmKyX3tG9lLGyAQgxkiPrFWbamxxEyxCEeY2uhkPOS1Y5QYmKnf73SypNfJRsPOdFWcNbN8mCSGB6ALFdJ5WCx9bZgsuUDLrj3JTIxkg5IEtUzMLBKM8vxYzo6WpNx45NtZAXSdszYGN4pnRNgZ6weOWR670n3h5sw3kqCNKA8ebYpVLEkybONVGCublGN3V6Twru51nnlm+IUXisXKP3WpPxsXb313nA7SFdBN7cff/wh2evj+izhY/PPff+Hvfej9mJfPffdms3JB29ieJFmeGzb3TzTU2ullTqVxftQRl9osY4BckNIFaykE8SqiqJrQSa2N326j43lxNC4VcEG6vSQQQuGDkg+B1BhCB6b0cnZS7503lrGYNZN0CojU7ua0usM0GHTOFzV5oSDj70yznC9c7SpI2CTbeX5rmVtyAUzBMingmROisBajtwkuAhVom7oOYtjHr+yAdF4UOxtsVaalFD627DFi+DATmIVUFUFFwUE0GPYcNIDilhHgNf5ENdQKB+N/1ca8CUNq4AOauKatFZi0ll8SIUlMniVZYrp52gS5eXLcBJ+mxnspvK4qMUJhaGtDXUWVmaOOqdatlEwqSpaRZCwVwJSwKZeBjTFWyRollFUztHVi8kE/e8s1usZrlUSFrVgH0oHFVBmkGhO0gqiwsao+PlHRXRHpu0iYkkKA3NKH371xOC/pzJ+/NnznY9tf+c7RJOHtVVhWTbbTn50Vf/lbz752a/JgUh4Xbu9//zdksJgsRqlPR+HBqfqsunzFpQGr+9zPs/2NNCjSUCNollpm8iGoIw+pG00z082ToGIt9frZsnKuCYeT5WRad3sJoIk10Y0kXjgEhYqIMfR33r19e9k8f2NlWCk31y4Nq9LfvrewHdPp2b3dwWKjt3FSZHfGKkqVP3j2LO+ZrG+b4IWo308sCk+wbS6QGlK0YTbg9dgWS/liFlrUFFna7GNZJEb7OS+XsnTUBEXsYDPkleroGLUUvCBhqGqAJuCMhFVqiMILJMSbLUoLoW0SUxTmt65rGASvTllFVBDlEw+XuG6WdDvZ5kavk9vTWXEynYws7XRSWMyKZhbEJ3yggUBDkxwbXrYcK6KXEiLWkrGkCRnDiUqdsGX2BLCCqBS708iV3eRHP3jtt56/c3RWaZs/QKray8yiasqiIaHWWA60Fl8okawxXbRDR3z1t02ssreZjRf1cy+c7CPJTv2X/uitGy5sXOmX02p5CBqXn/vqW7MqNMxHq9Ik9nN/9b3VquxsTD/4jmre4ODbdvOc39yCFiAjligzIGbjyLnWVd+EII2alAhoamG4OkhVh7fuLYylsnTOydZmh5nK2jNjVYam9m4dGgfgHZfzjz7WezfnVxfhNYcx0+S0rER6w2RzlHHCo8wULrws/uluxovCGlrO61demD753q0oLOOEUkuNk/VMseae1rdZFAX9YEVYI6OMWX18b5EastBpFQqnMR4zscQWTuCANphCo2sSSkSGTM4cj86aZ6C1BF+1zRGJ11Zb4caUJmQtQSW+aPRhCyTBGt4Y9Tf6nUEvD+DpdPaubX17l2hRXdmwcOFA5LVQnzThOIS3SFcPkYlInGo01xOIAhN3Gbk1o9T0bHSHRIdhE7hchPf/wi9f2b4AbdWOUDDRM1dH/U1L1ogKWn1i23oZYdbo5I9JN/HVGZeP+AQfjuuv/PXpm4dNYbgRPT0uO5NKZnUNhJE5KsO0kNJrLSEdJHlCR8fHt8fHmztVr49GsKqCOkiJsoBvuA4hfpyNmqVQU/uqChH0Fq/WmjShVeFWhasKR6LLuXNe9na6UBSlWy6b2VlTlV7aigCAdHeT/4P3bPZzYxSPdfjHruQ7Oc9mVV2HXmImp+X8tDo5Xt48mEwtnzx2dff9by+H9u7KTV5bju8VEtSJepG4CIGgEqVNGkTXmG0LoUWG4CGWJgI+W8prd+dpCng5XEnpVFWJYS04iZJFiERlUKSuSFTZKFjVQIhCO1210EbbERnRSSIyHIi8CKAMGJZWZ9MGNAIGYPR76d52f3PUSZJssXT12TgZl5M7S5mWLz13elYjyZgTk1lKRKSsqKpIAlohSnQEIjEcIAFEKWk3sYPEbiZ2y1LKJmFOzO4w/1v/3juRbZ3WrFFlC4jKVpo8erFTQ1zjg2oABW1LGmK4P9pfOvIgiNEsGlcEkEIqF04LPS3CndPCF14IRiifNFw4WkgIUSZCatFIOK2Ke8tFQ35nCO+RWgwGOtpEpwMlaOCi0Spo1QQNLnCSpdZYCkGGg2xjlKXWAORVXR2YqdtJbEIbg2w8rk5Pi7Np1TQhSU2vm3Dc2BIiwvseHVzZzjoDo6r5KH3yvZs//vYBoGlqxpOykycbm1m3k5R1UA2LPPvAL366GZzbFGTA4Svz2cLVtfdCQUQRGUXxQnHMbzxcaFkBFxCRW7fmo1Rhn3+rPDha5gMqan9acRPiY0tgEpBAvaDNi2FVaZunWvmeqldtdSBY36RoL7b4kjGGYEhURSTGKZNAg8IjdkOCYFK+eG5zd3sIpaIOq1nRTKblALZrB5nxQj6oBZrSZZ1EDFzpg2usTcnEhHiKrqI4uQchStkwsSEV4owUZC1d6yYfvD74yK98EvOvD1a3tpicybw2CnN90O0NzPR24+qoFYUqSxt4HLlaorZrOgCG2mq32Cao2qoxRFVfn1RFE54YdXJDrm4WKykbG8uKFOpJnQ8CBWm/i60NJCkOTnF0Svv72pQoSjRegurJvOwkydWuUbF5xv1+mhhqap+k1odQNcFY4oTLpZutmibIcunSlLPMDjsmywwZOj5ZhSqowCgyax/dzxKlVeNVsfX2XtbnXW8/9LbeS7fdrAgbA3VOjcG5zU4Qunvv+N9+8/Wf+NmP1cfv/MZvfW4+cau7RZFo2XjnWVQFrKqi5IWaQI3Xh7yTPsRN/wZ4ZV+6cZY7l3Vw7DD36mXNSUEbJ1UD74U5CgHjYqUR1fBeg1MBUaKKVkAZ6XMiRI68jchm1XXbEpSgEnU8CiUPYlhCv5t7rz7Q0cmyXJz5WuaWeonODcgSA85rYk1d+UgxkGmvb6a2cJoUiaHglahN8SLDJsgu645xmSVfNy+/0ez9i29+8Gp+3iLNOpImr58ugvrulr03qRczb4QGaS+oqPj43BjE2AMgVrK1zxIxxdQMwz+AJWN0rt6eu3EVLvSNNTx2mlhr0PJzfj0sqSKxKg5LQd2gt6n9DUBhJN/foLuntQt6ZUiPd5NvnVFR+kFPnNPGiZaunRYs+v2027GdQZJktpNRklg2VBT10Wk1Pi7nyzowYJlXfm+UbPWSs8IvSZKeodwsFm5J+syVzoPXVw/K0DSBS1rMai+6qn1Zh3v35+NP/tB/9F//2CN3jr/7l9+eHVT1+WxVhiZIUA7KBkYA0RAEPsBrm0mra2cA1iOTAnY6O9tK3aKgCZsqiJMoMgshGFEqGwlKJDGInZU8KXwQ8eIb9QKKYKUFPGloZY9KiCHgrUaB28tPlKBoP+hYamoAhU0tsX1wNG88Fauiz4XpcnAqZxISFwBhSTtJE4QM2HKSGol6WMQ4TBIVKKzhoKpExiJT3TbhXMdvdSXPYA2dzOX7r81/9Wc+gMOTcTFtHIWGTe0yNquFO7pbNhN3ZYv29/LjaZjOQ00a8ui+5Eh1sBW0jt91lRMpUVv9putz71W6GW127VEhk1rPW6K2XrqdSuNNn/fACYoatw+QGSSKvINh38imPZk1j24mH9pMaZjMJ7Ubl71epkEWhWuaQECScJYYm/k0NVlmVMU5YpLjk/Lug0XZeGEKXSYvpvLW0/bQSghOeCGeG8qVZo1kXT4b1x+5lG3sp8/drKYpXbs66vdttFoui+ZPvvZtJX3HzoYnqmf1mPyiCo2PefhxoFCOXkmOJHNrk4a2tCatSUVb1nUBaRiz3LhAQQUKZvLrsxo/vvb4CIfggxPn1Ln1XsFghZp4iqm1rRvYqIHkNmCTIqAhogEIYFY1bT94f9BNs6QoZDqZWlvqgEk1B0HbwtREKW+QCLs6NCp+OzOZpbZRAUot/MxGG6DjZbCUHdW9URchOZsugcAWiwZb253/8Zf+t15aBAqVZoOsenpXJjN/cKThLDSnTd6RTGUz97mxNw6dX6jZpei+hQQmJvioFqC1y8LEtZeE1VArpqPC6b1ZmDohZsNE0I2t0dPvvDTa7k5n9fNv3P/+3YONXtlNYQw2Rpgrki6qCncOPWr80H72rn66cb5TZzbfMFq76ay8dGF4fr/LzFUV5otmWdbFyhelT1Mz6Cd5ah+crO4fLshSt5M2jfeFVwsj6r1s9y1EBzkfV8iJZgu3IkpFjeHO1e57oRuW75p8sJk3IV42EpMVv/HSrY13PKrGijTlmfchYodkmZgVAmvIGiSmpXPawX+t246Ni6KwzoUlYCyVtTZOQqxiaI1oUAGsxiJGgagP3sM1aOrog6XWjM6tr0yltUgSAIOYLsfMDI1Z6CIqIqpEUXxukaem3+/N5/X0bCVSJx01HSbVJogyDFmG1i4QhY613jFAyBIYjvt0C9mo9jrUHaUbrIOT5fZ2/siTu1fOjdiYo+P62efurKaLnYudX/gPP3zpA4//d7/0G5MyZJv1fVe99xq977q9eYyjY1dCbh3Utw7KENQxzxqtK90myS8mkRtTDWgBDiZAVUgkxgSD6Af5TEwh6EJFSQe9NEnMZz797p/5hQ/jiXPACOgBc7z6xp//6fMv3Xzt/viN2/d17wosgSz6Btf3squ5uXAxz/rGVRiM0qt5l4TPZrWrzePXNobnMy9SNb6qfeXCsnSLRf3a65PT00JEQAxqhDgdJXDBT8UrbfZAQvdXDVtVT2e1T1IOHpvDxDWhHvtunuwN80raxUgJho0gHBxN7vSH5JwopA7MYMRoYTVEYDGslpAaMCE2VAjFTCAEEzu7EQTmfecZCGKxNOZ0pkuHKPJhY7wn74UtTGaICUGdU9dIXWkQ5dgHqK3iOv4h6xPGhmK8LRGsYcPExExaey0b+KBi2rYcA3RMvlo2xeIs7+j2uXRzO08yTq1hsFcxKRnLnBlkxllFbsWYOKQJKbHRIJtNeORc1ttO3LgZ5HTu0dGlK6PHL4+yhN88PkUqTGZW18eTMimaW0e3V4WrbVKDt3JKmd72xJVyI2lWaji7OQnl0jlGlvJGZhdT5R7ZBFBlywm0FqK4CwR1E5t7Ln2Ip/2sdCzqFTkjsWbn0uCnf+RckpvdC+e2Mr777Td3VjNcZJDFzubj5/oXOpvzxejN+4vBTrHbxXBirqH/9E7n3OWO7ZioKnhrEvJuurfT3d3KE0vHp8XhaTFfNItlPZ5Wb948e+Pm2b2DxWLVBEOmb3pb2eZet7+RZaTFg7qsA1nzriv5XmphSYQmK9fJyTIpqFw2s2PncnP1ev/ckOCaxaJZFMF7ubh/HmJu3DzYmK02ja8Q5k7OJBSNGMOJtWwIqhLEudBKvFqF/r/zZ5SyWu+1IWKhysMHSETJmEQols2zgWEiUBNC8OIaDSFqdlsxOK3Fikq69pzQw2HcxJFcSUXFkABBRQ3Ff5GcitfFsmbxJH5rs5P0LeXE3mqq1odQQiXY1GYp571U5whsvSeRWFVBxkJUXQiUUVXJbO7tbqIcjk4WddmUK2dIhgO7vztarpY37o9f/ZP7XoUsxuMqsXx/lDHrYOln0xrjahmEM3NW8NWtxMmAi2Yrc/PDJpxLOrlGyzSBSSXCs2iTh+IQCoBjRJBhg8Re7BCW1dnK/z+ff/53v/xi49xer/OxZ65f2d/cGnYv7W68cuMYir/z8Wfe9bahn56dLG5099HrGWsJRIbozIdVIUxNP0+LlTs6KRTa6ySzWfXgZLVYNGqYU+Ju0uma8zv9zVFSF+HkeDk9qZazqnYwbDqGE7YPTqu8bxKYtlBV0MzdYuXNRrq7300TLJaNL5sBudXSn4zdC28uzjSMoNcugRo7P3Rj5xsR4hh+o60c8WHXh7TwVsy6DFFnIBADE2B9ULYghXNw0vqWIiqkKsRqrGU2IWhw8E68i1lYkIBW88HtdCtExBpl+CBmJjJgJuZYTateEBQSLVOeNKgCJjONNAnr5k5y/nJfVKYTF1QJMZJIbG4lMYsmiHeO1AUKLafZlg4pUR2w8H7l+L7q4UkzGNH13dEnPvzUZz//XNUUj+zvrVb+4x+4oP0nf/03v/v9+9ON3H/sqfTe/WZQB+5lr78xm53UapvjSUOU2IbMKvQGBQ/RJc81jg6a7JLVNP4/hwh0t8mz1HZAr0X/FFdTCuLm/rVXl2+WNF5VlQZDXC6Lz36xZMvj2eq9T1x779suvnbnuKzc09ff/eFPf+yLLn1w56W0Y9K4rBFeP9YqYMh8eLwqVr7fS3sdc3CyOjwt1PLoXC/LTK9j+52k3zNVKfduz0+PiqJqgrACqWUiJL2u5UFZTJRlRrLZSclRfdbMRXvn8p3dDojuj+uTWT2ZNZMzt1qGxCmXPtTh8nY2OVjN525RixXRsPa9xlwCkYfOuXjbRPh8rUBrsS5iWC9qACg1Ad639gxVkCoJsY1yNgkuOBdcA4m268h0xiR/aTW1cVUw8VZjKMRaywQmFhUNJIAEsGhQUhtTXFUJQZ0l0+1bzbWb5bMy1EXJhow1hogcGatsuKwDQGBPYoIaUnbeh8qrBqyqu0dSqIzHTSI036WDB/M//P9emM3nNslWZZMmyQs3ZqUsh317aXt456g6XtT75w2BLu/t7T/S/8I3HywnS5oiFyHw/QfywfM67KhvaBgwqjD2AiSqPp6iKGNZBxq2uQ7UhqERCAGh16fayXQRRJWVgobSaTaU0MhksfrCN18panfncHo0nn3nlTs/9a13stWvfHfx9n3zoceG28PkZEk3FrCGiiJ0c7O1kacp3T1aDfrZey4M0pQtkzEM1rLyD06KOw8Wy4UTCTFsl2omIQ/ko2zVSZtO7ko/HIoppIfkhKm/nY02UxfkZOYOxtXpuD6bu3qlDNka2M1RcnlpRk7SmQyJxWLpmOCjjy2CF/9OHplC1v6AtoI4/lOCKGwQEpAwnFMfDezC69wusoYASBDnpGngRVRIPCQAQkIRl6CH635s+2KOtihDhPgW1/hi8UCA1DCklHHW7YlICJVhpAmKiTuqZ7t7/Z08OShrFWgQWNPrmghv5rmNOEKxlJUzBK2WzcndBUEtCcaVUxVHmz3jG33X9cGNB0Vw4n1zKsvMprOT+tU3T+a1GJNcyNPTE3Gu65rqU+/tVT3bsL01SQg+CeQAV2tTSmdkHVA5bPXUqJ4FbSlRpWhlirl9LYkXJe1rtSaIN7vMieXTwoBBwQc0LvgyXL60NyurabX61vdupFm6KioFfv/fPNfrp5zqV96sXzkOb3t0Q4hOFy4hNKSdjkkSUzbu8oVBnpo4H8cb9HRS3Ttanc1rr8odDoE0CJVCgVVZczzzjmvntvgsNLSo3Ekxzf1skzb382E/WVVydFYdjpuTk2a5ClJLaml3Mx2ImnnIA2xCqnalmkLJUQhtJA4RS6x1JA6CJiBErklaWfVDtDYyJ1agQuTB3quXqE9RkIkvTTJGFd6JayRmpElQ8VAPhRqCGIrFqBQbtpiZ1TAiWxNNpUEkdpiABNAggAeH4EOhCRmCISQpVCh07aSsbdUQGw3BJjZq2VQCDNWN5F0bvJrUSCOkVNchVEIsw372xJWtF2+Ml957H4zq/fuz6VntQV5D7ZuE9eR0JU6tSEPhZL6sxL9+Wl7eSl4/XJ3cdrObxXQhXacmSC2UMD84Cue2uKj96VRXhYwbTvb0/IUo/o2hIdF6baM8uY1HjwklbNKeGabMg6j2VlIlDxUdT+Z12RhrhFB7AddsSJzA6HLRZLlSak6m1eqlk8ce3Ti/29kZ5cFT48LRrEisCXCNkyRhDWos1Y2/eX8xnVVM5EVc4xUgB3EkTGoJHd7b3nj3O869UE7PVhUJhpe7Ozu5AONZ/WDSHJ7U07GrK6WAxCGTIAeul9huyibliNiXPgRBUPWiXmFAYMOGlQgIXsmF1vUU5Y0tSKvtq1MAG5gDwSs5iQJTTqyCApgNAVAJ1Dh1DlCIp9Bo8K0xKQJGzATTei2YYRhoi6LRamkRO9GIjE1TmG5oAlSBEBIPBoWMgtPOMOl0bZobccEoiFM25CBN4zk1hkig1hIbCkHj1+obT0aJ6KPvPP+P//V/hnHx6//DF77z2oNOktw+Ko7mVW+QJKkJrqkcgvMuyLShB66qvAAg4gu73cv7+YO7zqn6MswrRaIrQkgsTtyztn5knyxJMGoz9FxQb2LNHChR8a1+owVzDBFBgzUM0a0OD3vmbimuERiQJ6iQ1wAsixKiiZKwSEPMGphUEEIIC8p7QRMqCr1xa5Y/lSWLxhj2laSpHU/K7VF+YatvM3r11nwyKbyG4UbW7dnxWVXOXIBSjMW2kREhAzpbVkens+W8zDJc/eBO3jOryt85Kg9O6vGpK5dBPQ26zBLkzGcNpYaVohsCQcQJvGhQDQKnGgIJGWvYGAMSEMX2k6hHDGsGQNqczFYgZCdJ3ukaZS6lFhUmISbieCMBSiGIbzQEBAfxKi6GlAPUft5K4LZNpx38aS0KaTkgFaU4/SsR5YbVCZTIx91BiUCi23sdTqBAaDuktd9LWCTrWrbGWMzOqiQzBJqdOVWoaFMFL2rBf/7Xt3d/8fd+5Wee/tS7trBaPXrRLGrt9TdNmuyMzK2jcnFWU8CJ0weNr4OIKql59FL3R9+x+5F3776gal5fxgySwwq1SFA3DsHn5onLdG4T+ZKroJbVlYI8ZkzpGswhgrZNcED87IzRCyNrElOvnKoiIIaMOrDRmKvEieqq1pg3HVcJYvJB6hWnPW5YZO5u3ZldutC/uN0LrJNxNeoneWoOjhdFE/r9dH9nu3bhwXh1dlZb5u2dXlH7xbwONioMiBPWBIf3D2+78blN3t0eOtHTRXP/qLpzt5xNvThkuRnt2bxHBMh+GlZB5r6spadIoQ4U0BYjB0VQeCUmstYaA3gTha36Nwayh3zTumAIINgzm5Y2YZJKfcRjWzvl+t9p/ftBfSOhbtti7drGGSdcIhhD1jCbKPWJJffr/xYDYBGoD6EWKTSUbXe4YXWEhHTTJATJjc0yS0AAXPAuaO011IFcMIlJu0nVhGLmi4pjPKKIxF4Tp/idb9x68ebB9VH2w7t594Ab1a2NjrF2t9/71A8/jo3Ov/qdl/7yL16sRYmZRUF6NCk//+yDu6fLg8LXJawx88ZVEvsqoYrJIkwX3NvhXiZNAQTNliIKzWPlM5MBOQIxSSRCtA3RSbSXkRrOUgtANQRVDlAj3mEt5tUESjGI0ESaHpySq4QLRUYVhePDpbFaLsJTV0dhK7t9d15Ws8aJIRZFlvHudnd3J9/ezuer5uBwVS6bLDO9YVKLelUFbSbJvj/Z6W48dW3jcFbeOSzuHtQPDqq6FAMddqk/oiSnCJqa3Ga5pa0MtUgTUARaRayLFCwURElJrYn3GQMhdq20XnFEvdC/w2zGbcmqaYViwQugUNHAwTFBgsBYVSXLcDFUx1JKui6WXOcgS0Td2FgYa9pG5shskVGAGEwURJogddBS1CWtu8kqpZZ6HbYsk6PSJtTtZlnOxhqbIku40zFkyauGRjwQRGzGWdByKaES3yi4ZbmLgOOV2+/YRaWpgVs1B+PS9CbfevHeb3/pzfOXs5dfmjqFSKSJwNCikbvjUpwbz/R0Gc7mPrQfVOv2Wyzp/hRpL+mSW6z8vAAsfECeMdYZQESAkpJoO6aqJVXHiVcxZC3Qph+ogNKAkqFeGVEfqokSEZOECOSz1TqBd2qhSLjScHpU0b594ZXx5b3utYuDzHKWJ8NuyszeSSPBNVJW0kuS69eGi2X+xu3Zyd3FaJBc3Os9stP56LXhXqJvHZU3D1Z3HxSvv1lWlR8O2feZjbKIcxqcZ4VhZWPUKBm2CUmemL2079XOm/LEwfmIyjMhsSZNIp/GzC0HFO+z+LXLQ6SDED3cVg0rMTRoiBsASVChSA4piNmQSSgDTJqorM09GkVppBBtG6WjAlXaAp9Ib4W4aMIwGSaG1eCFTSoiAXCUBHRzjPZs3rGudL6kpig7CbElm7JJDHJKMmMzYzOTGjLWMvOwE8qOPzmUmAPLTBAKTm6d6ny1Opw2jw1ykyiDai83Fu59T27aKlRerEUQxPDYAILoqJ9ub+Z3xotxLQIQqeH2EGhA7XDnTjhZUlHLcgLnsHcV169FCYpCA8hGyjiScMaQ8yg9uinylE0SUUyNTemkKqBUpUbsqqU0smaqbWKJCnkYRjBQBxvEJ7xa+XOqW9tpWYfFqrGG2dRHFkroZMmgl2wO8iev9NLEzIr67nhlje4/NtzP+bFzn</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8TY9lWZYltNY+59x734c9M3M3/4rIiMyMyMzKpCqToqtRNa2iuhsKIbXEjAEjJqglBvwHhkj8AIaMaMGEIVI11YC6BbT4aKqylF1ZVZGRGRkRHuEebu728b7uPefsvRmc+zyy+AkojhQe5ubPrt337j5r773W2gf4Zn2zvlnfrG/WN+ub9c36Zn2zvlnfrG/WN+ub9c36Zn2zvlnfrG/WN+ub9f/3xa6HK7pAwiWxVtTiDoiADhAO9IMMPWISqBeDq4uQQC42je5G0lc9nz5MIVKMCq/mxVzEnayjU5AIJ6fJtkc7jijuahAiBYB08xQQhU4AHpJYcQA0VzIXFHN3APD5xkGHAyRw+oIOJ+AAQcAdZHvV1/9Etu/D316LgJN099NlTz/e/orTj8zLAbbLgKdL8W/eEr++FKXdAOCAkO5Ogt7+gwNy+p2Ee7sZOE83erp8+wGnk4Cf7pKO9s32K93nO5nv8u0ndHrv+PqG3cHf/MS+/rxObwSnl7192wY3UA1OF5EU2l34VFDVFXCHYX4ifnrXAOL3P0xCPl6nw04nqDt2e9WMEIwEXDzgwdVwdbUa+mjq41hrsa6jO+9vp5vXeysWEz98d/M7P3wYqg8hZNWj+yGXtAyarVSHehg1SLgZ82df7l/dlt3etqNdnsnjp31RG7e+XjIB/SqouilgDiDQp+L7rU2TwqjVKkTh7iinSLFT6LVYId/GDuDuFMLd57fd3vn8MTrQHvxvRO7pkeI3v+LfDFr+xgsIh4AQurUQExCAsIUrhCCFDooTIIVwAdtlSBCQ0x2Q3iJPaEBoj10EhBPC+WUtmFqMYY5ZuABOOd2Yz1cHhC26SBgpAEiDt8uYz7uq/Wpy3hTm/hufhZtTADdndqvO4hgWabXsAajq3T7vDrkUK4aqUIUDZnDADQrEP/jJk+cvdx1RMqatFtP1UmoyQNxQFQhMKXYpxEAFRRjEQwhmEFoAIIAj9TyMuS/C6GOuk1DdbdIucHmZdFIzh3h9XVxNAhW27PhgEzebzpylr5dXwzJRquXs4yEvL4f93aRjHXquOxPpfK/M7gFKFrOxOJMUVVXSjVGMbuaToqqXShhJ7wOFkosd1OkwuLRN/PVni7e7GpyDiW3vi7tDZqjwr/e6+wwvcDposPZTPgMR38LKHJYOOHV+2mjXJMSdJATiACFwEA3M6KSYNPQxEhDq21ATGCTQW+DOAKsuQnOShhYgbLtJ5hslCHeZ48m/3k4nNGsgPr/DGf1Ah1Ewvz8EmXPBahHPFp27HUYLgiAspMzhDnOIwAwUuCNenKdV2nz8qzvSawpWdbmUnJlHy+ox0oRB4HB3aDWt6gaA7lbVEBicm0UU8919TouuVhT1w7Fker6ti030u3FztYgP0vG2VKGZaVatGHp0XYjgNOnZEB4/HZYi5T7zUay5JxHEaw6rhwu9yTRgWcOoAnpF7ThVi8BxrADZi5xFJjjlaLYdp+NoVvlkvf7hs4dPLhafvNz+0599vt3m6EidFDVzOOEKN4if0mhLzk6wfQECBoifArEFGdBCtv0rnfBTHvX23P2Ua6S9ZIaGtw+4XYptk4I45WV3ETpc3CEt8igwwkERKEGIixNUIQR0QmAASBUAM2g5AaFhTtxCOgmZ8zX5dYgZGOY30MqWGaYNLR4hcANg7hCSNLoIFikOnbhLruqGqlSDGc3dHGZznnHAHPFYdLPp3n9nHb/ab4/78WD3WiTymP322lOP88sgoW1NBz0ESgoxilatarnaZR++82i5ORumsVYaaLWYVhtrDYn72xwjj4eaD1Wrh1W0V0iRQhCg0B2ovtjERQhBTYaYzmK+h5lfXC3gHmPUQBSVVZCDpYPK0dAHXTCMqhJiDNMmho2wDx5xdLs5xv1RYw0/effpP/jxex8+Of9nP//yp7c3+iWS18vLOFafqvuq092kEyRBi9ejQZCc4qjGLsDdDxlTgROhPZNWebytP041iMNJmLeCZq5KCLhbKxZtjlp3b88YDU/sN4rEBl4NOAm4NsycC6QZFDEHscDR0itJtMRKNiSEARAaCQEACpVzHidbZueM60IClSfg5ddF4VzQtXqgba7g3j4IAbsu9l0w9S5FdRb1olB1c6jBDGpzfedAnLLm3i4eL6Z9ucVx63K4NUTfjyiOOmJDkpEkKUEsxhAiJbi5a7XNEL59tXj8YGHAZC6EG6DOrEE1jxb7YBnbr47DRVdy3d/XXFzNHeiT9JFJKF2k+fTqmM6ju+iu1m1hCl1Hvzdi4lmwDJ+cq8gofe+czCYnsB66GGS7EKxCGMQ7SabaeUy8TOsff/fRv/WT9/DO+bs398Oj4cx9mcuDKxyOPiKky8XxJcp2YhdDh/y6glgGWQ/dBBdoH3m7Ly/uTJzPLkMMrGpjwb2a01kx7ednVNVbN+Ogu7etbD6HzwyBJ4j7urT2U2/BU/yegnh+rc1VoxtAd1JO7dCMuQ7IDEKcf6Al+rcJuuEt2IDNHeJyaoSErYRzEjLDm2P+2loQzpkTTkqIHiEMLoghyJBSjZqKgaEassJ0BjB1qAM+78xo7kUtRl48Wz58Nd65HVZkYspQU1MuViklihBwc5hb9GCKUmwR5Nll//hi6Lvw6s2REoYUQiABVTUNbkhdHA85OY+3eXIbi6nZcTIAUdwmq1FDiCbMRXefTGmIIaLrgh4ydpDXReGFtuiTQAKIYg7EyB60AqqlyGhWXYiWGyiUKLxcDu8/2eBqhc0wVUXC5UVcV48JXa3sutXjxepM3eTmc12E6CtQ7cL7izTcuVpv7yzT52+m62lcdvzu++uhIxyvp+mN1dB5qrJ9Qc3oTPZaEoKbq3mtWtShfszmjmKtCgfaRm8p2PEWUdzmftZ8fvxvOz3MQOmnfs8dJ6hxt/ZKnbHubdjOyPq2QZ5x1982m8JWd0I453uhQ7xlewFBE8wFwRyL7iLaOWO0CAnRo7DvYkIoBSGcsmS7bZ8fRQsyA6Ka52KBTB2vvnP2+s+Ph+qk9wMhgcblKnSdkDCDqru5Kqorij5Z9U/Oh/UqpUV4//KiB6ebXKYKteiM7r3SDzosoxj9LqeL6NRcTAERuFOzVXFNSmF91PMsTa+n+EYTa+oDsk9Z92N1+BRNwG4rq0BfRjEmiMeQDZPZZBIAEZjD4OYuDGeL4XI1YEg45OfPb8PtYSBA5kkBhhRTH4Z1YsXxduTBFw/T6jycxfTovg8HXa/Cb39vgy+2X+69jvb0ql+tu5xrHh0xLHt27m9qsJErCXe5LCXCoaq5eFZj1rtdKbCpGASpDwF+u7dStQFNpLMBi83pt6rB0XdwImeW6s4ZFc1gJwKitSZf1+0nPsTmlgxv0XRun0/g6IA47DegdeY43gLsKcLbvmg/2roTIQToHQPotB4xxZAio8gYWw87dw5wUEh1ztUr6IilmuRKwAKHs+7hs/Xu0/s79XqwAA6D9IkxCE6FMQMhzoLLIVwNab1Oy0XsUtxc9KsUj8vu1auDS7EIi+5QPRakyCRpmfKu6qGgE6kWFYte+k7cjJP3YNoqH/bTWvIq6E1JxyrZ1XxP5lExuqmmKMsQul1ZBTnv49mQRKT2XQ0WQCEhcBVzdCE+uzx79nCNPuL14bNXd9HcBWoGeFWGXlqKkYTUy/3rvOo6SawLTyrLSXPF7a6cb+K/+ePzeu/vPh4m9S/v6l2s63U8W3BAqGtq4HmIyLKOSczVLBeb1HioXmrWEInYh37VdY7Jjnp0kgKkJDF4FMAhAjKUXED5nQ81CD5+7tdvpB8sRNC538FBNyc8EO4s5uagQ+FuMFDd3WZE8Zbq3rYyp55jRp23+fpvlpvic8/iBsHXPGJrk+mAuNBESGLoYhcZRFK7IXEhAxvKGomKmYMxR/z2w6vtdJxqpnO5CO99cH63y3k7VgIQJAFCqzTNzd0EFMHQhYtluBhijFx1Hcy9AAGLFJ68f/bVp1ubtJilMzoMe3VUnnfqKJO7ohZ0HYdFoNBUIyOLlc8P3W3dPOnqIo59ON4XPSgKDWAf/WhWgkfeZY2VN1Zuxro55lWfLgPYC+dyQ8yrA4uYnj5Yp8sVhg63119eb1U1AAbWgkwsh6iG4CIRixWPyyhBAB9qqKYRnMw//ui2VAsX8enj4T7rp8+PP7/eP3wvuJuEGAyRhDCIxMgUEAJdg5BUIlsfI4N6ZezjapE6SLfPmJwCEKljjN4HEuhjpHB7KI8e2L/xI5SKCbg7YH3BzcaD+4sXQQtCCBc9VzBzf3H0GLB0ICDTRXw/kkCMPmaWMgNSVZq12pxqro65Tn/Lqc6gM/PS7mg8YGtc7NTTwBGAalBzVRfhkCTFkAL7JJGehIxeCTO0cBeDRgSDCuJ/8g//zvX97qPPXn/05fX9YQvynW9vrn8+ssBdYx9jlJbj4PDKIAjOXjAkcfHAsF5EjZz2Rfuw3+dhkzbnw/HmwBJsmrgIapDs2BVXsyR2VDNAqAZLMAQCVg3ObvLxl3v2YX0eu2Usq6AGWYSadXqd+z4kuO2Vk+XbTJFsmA4lw7uh6xlaz++AuKcYVl1CCoC/vt5/+WqftUqQ1FGidFdLRlgjheBx4HARQwLhR5Y3K9/cCxFSFxPrz35+e305bDbdn382aucP4eqm5gaDCwE14wwTIicOWBvauFMa6cgIp0DnCokIcAEDBD4s0rCQqeanj/VbT7Ddozje+dC++wx9wH6P+y2nIx9fLh8N6MYDhHtaFD5dCMTrpgwBL2/DclGj4NWNj0fZbHyIuL/jOEarbu5mruZqNLgZ3WA0t1Y1Qg0tCs1gDQIdINS/bk3MZiyku8NSkBC8CxR6EiK6ABWAQA0iEIMJRBE3Z6tJ0+ZiGK7DzljL9uHZ8P1vPfjk89tj1iCQ1gJAYdYLYiQIAYpapFxtFnTUoiGF4z6zC8exFrN+kEOljjSBdnQy77OZsbr09D1oTtUYk3XCammIEdCsrojw+KaOL8blw05WnY3a9SG/syhJajEsLJrpOvnk2NUlJQahnJImXN1g7CVIg+xD+ctPb17clgqmYJtVWFwwdzKXHwIyMAFeGkuPEDLNIzm5dzKZvMiRk3941b1zqJ/eTnOfrp5ale7SGHcn3dEehLmrKlvfeSIySAaS0rjQVoHTfIa3Y8nZ7NkFlj32I4rh6hLvX8EMtcDFJcUHF91VqqsOR4PdSQp89iAoa97AKlbKJ1eAYlvpgVcPrQ/IRSSGcnQ3uLu6mzucM9Vs9Fb8GRymRnczpzlxamzNOfP77uqIhAjdtVaDKSSoOdxFPDqqUBoMCtQQA9SAgPiP/8kvrvf46s39ON6p7rpoffLHjxfDIu22eVdKDK2UI8AQKYHmULNa/dnD9cW6Y8fpbhqGkHclbnh3X/pF7CUOwMH1eF8cbq6aJI91Omou2rJGSiEYKD5cdovzFM3GlxOjGHE8aFikmOGsGpxdWEze3Uy87HUTrVq3RhThyFgch4KOIgKBuqu6GxapCyCy4c3hZ5+8qnBS1HCcbGUB82YBBSAlNEoCBEWcIJYIB58K9rX2yb64hf18tx21FREEzX00Nr67lcGth0fjet1r+595k4CaABZlFiJErAXZXDgRx2NxIPYoik9f4sVrXlw6iMMONcOdCLLogwR4ZZUovT5aax+wo5+fIVekbMseh4wRnhbaYu7FrQFSjzpvhpkKa9zvXLg3xtlNDK0yYrsv0uUkuaUoWc3Ui6oBKUgX6EDOujuWotZIEdIF0FPb6ydRNf43f/xTRwELRLsUlp0sFtJFUsKDq8W5D/tiOvOPLnRzUXVze3q+frRZQl0UmyHFJGmN4u6AZuu60BcsF7EGmcai98huR/XJvBQQRAyeZHJnNvHUL0O/HNLlQqdSj6pnFnop+0rzxVlnQbbHvBxCfD0tXNKjBQLDsa7W3XqV/KivD2OKBFkdqubGLnbOiEPdXk9/9eYurpIfq0ThWXdcdSEGnz9mMiBGzowxQCCQh76uJVWyY4oUEl/dmYNhEDdCDB68iSQnjZ5oqiEdbrCi7i7u2oodwgMkUEiehMOZuJAgQagGij+5wKIDB4TklxssE6YVQkExWXWxixL3+z567eR8aUtSgqjKly/rpCkuagzYH7HPuBjQ9djucK9hKrqvSm9aaguyxqhBWp/YpCQRABAn2RTYk/zqXQxnyziVKvD9yFzrg81i6GMgSTtMtVRTg6qrsbq7zcm3lYDuiDdvvhIBxELgmOI2MO2w6ENIoZZuOcSZmzGL4qZwNzd/MPQXQ7c/TH0KC42dCAyuXqj9EIPDwKD28GJ488m9drRVzCUXctbHBaxq7CwSTlezgxok9ewve1tZmVSD6ybBrFbU++LmhyXr0S+yylejXHSry6F+vueDRYxR3Bhjda9qpZpZOGT//KtjH7af3Nx+iWn9/mp6NSFb/3TgMlHmjdrSGQLcXSvc3cwt6Bj0ctHFCSlK38VDqUG8tuRhjRdtSinN9HgSrmaN1OnOalXd1A2gNKoeiBQA7kbOSpYTgcFgqrpcAMRhwvEAM6nFjgccdrAMoS/7KEQJ3JUwhrTq8hImHu5yvC5npvakL32CGba3fPTuTCvEyNvJqp9+bStIrYEPyMaZzU1qq5Jkpm2buu8Bshxi3wcJTHSKivDBptuseiFNXdWKWqleDM0DUR0w6KnVVSBKAN2sslTXUoRkRIA/XKTezFSN0hRjIaq7u68krIc4VUWMkW5qSKG62QAdCXctGs+6s1UazR9f9XfuX97vLME7qLUqGDGKF1XzbpHS475GwVT7ClnEkMSLdV1Adg8M5+nYs+5UxxrP0vEM070ubo7nqxjP+zza42fLHSsFxb1WU3M33u3rJ8/v77b5r3ev9+bDw9Qt4/HlFJJIaLwkQGeAw4VYxfCtYbhDNnOFR+eHT88++nSvtKuzeHdUkk0lspmXaGHigFQ1Dyym4a0mbXTzxnI2ZbIhmIi3wAtsNJYDFEHOpSoer/HoDDGg63C5sUcXWC5wm/HmK4yZQyK0Lpm7s5Al7F85F6zVjod6O8bLtSz785vt+GaLKPrgrKaIuxFTpStJM2uSViufZjW9MSBNsm0fiBiCNAELgAkI6rlEJSUgQCQiRe9TPFt06nYwa2BcqmeFKqrCAbW5M3JAgcijhd5jLyCFXIpsBrlYpfM+hshReADQvCXe3ARc9QnAYawSmM47M1jw/UFlLQbERWASAUzR9+HK+65aebZ89dVBC1zcwCgQ0oqJi1fTQ9XzGFZRhdvPtotV1y2DR4qLZA2Hmva2fzP2571PLo71w77elHxXfvD9J3fP9/f3k/RQolSrZm7I1fa7/U2u27H7RLdOI1Jco5uiRGFjuE+mLwooJKGvtRxK2oTlKl7G9OhR97w/3k96vohDLNkgoLu5zRVa4znVTUB3jG4RTA3W7O1z9Vm6/lpJn/lTn8slkCzFzHyzxNBjN+IXn6JWWMbtiOkI9eCOsWoMUQtKrp/c7KJi2aXh/PLd87OLqS4SFklux9zH6d0H2XJ5+XL7+gb3t1bKTL+at/q/mT6ah2P2Fs0VQ+vV57KNdDdCwBDEDEIW9S6Zm5u7O0JgDCKknXRXYWPgT1rwLP4iWlEvJDUNcnEuZ+u47GXRBbq7u7rMhgGHOIIwMPRJVkPoU7Si06QiLObHUnGUAHj1votQ78+TVqOmy2Aktj7JwLQUjCpCo0sfYJSs3BZZiNNyBFcpu0/bPD0vF48XFIwvp9Uqrc87KWZg18eH62GxWW88Pu2Xf/jvfft//+mvP9mNxVDVTOGgqVYbC/Tepm0sMJp7pIRFCEPbrTjZGUkhAybzF/d5epXDK55dLXTJ/+WrF/lAX8vQyZNVuN6VvXuQ2SpGBIihmXpcyeAONTd4MK9aW18Ha9LibNGBwGxuMFs/RzCITGbuuFwiZ1SHCq6eYNiABV/8mr/+IrjLVMqw2uzjxZvr/a/fTD9599H3fvRu2qzzp9dTmV6Pdbyth5xz8cOx5JKW3eWL650Wcxe4aVOf5GSiO3FmTfpyUtBa59bYuMxOKJBIQnUjTA1VncCY/c3uuOxjrpaLCj0JGGGGGGAKC1CFotk+EA0SxBc9H17Es0USYVDXbIdccxBbJEQQdNVaIGQXmBxDCsMQivhhlzmEcarWS7nPwyrawRhYjrq+6KX4YhNrtux2uehe+N6Kk0iJw2XX9eJ7xgF0HJ8fzq4G6QMC0ipV5XqdalY9aIgCQ98H3eXUS2ce9vaTHz36e7//A3znCtV+eL399Uevq86bjIQIEt1h21xqY9yreaJEkTg7CaWpi7PLwY2+653n0B2+up2gtgqhN+SJWPJ8GfbXx0UXvvve2fI83nKkAGqgzzbDk1nS3Y9aS51FS3gTl2bRO5Bt2+JUKFHgbi2J9gssery+wZtbvPMUyXGzxYs3acwSgpbCbH4w/vKNrtfrv/93f3uzSh999ubF7f5mN94dy25fc8kgzXC/3cfA5RCrFn17Jy3gpdmABV4hbM1m+56cfHMyd49Oogvskoy5AqJeNivbbrk95jf347GPtfpuzAKEMJtG1Oc/BRBAic4QzbDo5GITN+tu0ZEAzetxmirKKsWFR6GbWXXN1Rzd4CH2dbL9mFOHPHk91kPRsAylqAvdjCO1OI4lOiRXutSiEA9Kq04yJOk6ShTvGFcBiXHZY/J6PbEP681islqyxi5W4dnlUO4m2ytIji6w5borB80vt92/8yPIox9+/uZPPv4FzAmKIIh0nUWjOu52kw19o/+aTN0kwtlexVZJgYLUQzLX3xvGO73+q6yT93SCVxcr6X25TN0Qdpk//3R7yXjxfoS3xpSz33rWGRsDSzdv1pzGV1LYnF1hLgqJk9UtMJhB1ULCdx6BwP6AUdkld8ebLbbHQGDVd7XW69vpbir3h/q7P1i9fL39q19u7+622+3hbpdvjzpmrWa1uruX0pRodimRBpicvPjNagCHM8CtNZtCGCGYm01STn46gOLuDfHgyBXVuD2Mt7v+ONWqdhhrS5cwaLu2AQ6Ek9QARKEPPWNAFA9CcXhBVDIEptAcEkKGSDfJ2d7sSycHng8pW7cnI48H3R4L70z6btoewiIcdiUu4/GmLlfJD94vwm5fqwHudIgwdYwEStv/blG4DAUa2EXh9PneOy4f9KEPd9t8yMd+Ff1CfBk4eu9htUqP1qvtLj/8nz7Cjw7TdjQ0mQxBKER1IvnhWA8NZkTg7tY+AJ48987Zu4wQGDup9NDz7EmqN/W8hjV5vzOttoKo2PJyePmmVPOlvjVcQOB2MoedEmNDhVOFIiRAt5NLh7OJEDP0BhEzM/eLDS7PcD/ily8xTlh1QEbNGKIWcLNIU6l2v13A370arjb96+vrv/9ePP/g/Pa4er4b/+XHd//q0931pMU8q1txD1hIxyjMBs4yNwQzhyFebSb2ZpSdE2pjq5uYIe6WAuCuZgySEi7OfDz6Yazbw5RTzLUecmkpdg6quaUA7CTVE3G54tkqpgCttSBYbRa25PAYxYSBWAwxMm3HfKz5cKgf3d5//vn28So97PveXFIIBYddRTA18yj7Usde+siLB8PZkBYejlX3h1wBgBJsvUiLlNzgkavztHrQCcAgkRLpelsThQfVgy1WCeaIjIYV0pNvrb9/9eDbF6urzXrd9Tgo/uz5n//ylZ5ssFY4jWqkDjxM6stOSG2ZwRoNyFNTSMdMb4lTOnEUs9AtcfHBsP1o6krIsOtc+rHnIJer+MVd1QJrFi9+7Wtoj0XAIARcSDG6OWVmOptLcu5wlUj2Vskh6Vpmk5ejD1iusVr5YgEXXG+F5iJ8tR0fdf5+r8MQXsQhcXoS/OlylYKuzmQRU302LMQ+e5N/cZ1f71UBQKbJQqwzCYOmgjfizNVsbjJFmoEHhoZ0rVRzB2BCj4FmbUc2izpypbvkYmb1WGrOqu5FoX4SNwF1uJ00K0cchpgi+0SA97sSQ1is0+TU1mvQewmrPsbAyVTdp6I62lg8dPLBB+vx3qft5Dnn4q5qQB7rL14f7yYNAevV7uHDfrNOIYX7XZ6y5WKhkxiCJNbJgpPVIxCqkdItJBrCkwhzP5geqmSkVRx3ZUD8177/9MN3H3x4vlr98BnON+gXuDzDp9f4q1/aaQBFzSUypEgRj053r62PB73pc2wW9nlsxQmj0WJC52IOigwbPvp2WN/6r6/rm8yzUc87WAyP1/GTu2ytuG0pU76eDXI3Igbi1FOe/DcEaHSBCAQIPrO0hhAozc1PPrnyBxtsR/z6C2w69IBXDJ1nFZHmyjeFZ8P1zX57yH/vdx7/4N3zz17tq1kXuO55tQrV4qHom30Fxc1zVomnKSUiCd+57EmqaSnI5k1ibzbM1p+0LFkNLXkaWhOAVoMuFtonUNB3IXVRa83FinlRNFLDTqJIG0JpllpzxEin0gsrvTrGsSCGrmcWCdLoYgQDBJatTGYVsQtGO9+s1hebd7+1cdV//ic/9QoEGSetkTcHnQok+M22vnxVFwuslkLhcVR1RFKNWrxMJoPUotsvDqsYgiEHWPEuxbQMEkUS87EetlPJMOqv8Crs7Id/eIHs6Ab0ESHgg6cPLs+O+zqaV7gTQwygp6P2lZHMjcbRkxJUnHDIyTnocNPmEDI4jCRF8Gg9vDmUUdQEXx7rxRDY48E6frVXV5i1IIPMXhZ1FwDmGoOgkVQzk6HwNlnXqh8wnOxfgDSvxxAORSNxOKASlyv0A7oexxF1kgcLjykWx8OgZ50g2jjlX77Kf/10WnfbZbTquCvVIiygCzzv4yLkogbClF5N2Iyx/uS8/96ThbirWbVZWXc06hiARxHQa/HsdLNqHsisnIoJqlqoamOGmSz6mGIUMmQzoCimiqozejUZwE7UtQKxI8z0MJLqknBUHG+mi3XEMgqp6lO1EUUN29s8Hoq5l7F4wevX428QO98AACAASURBVOdf7vxJmIq91BIByTDj4WgU7zs6qOruMMOYDWSpdLrBtrts1WIModPMWAkfaPvKbOtNPx1r9zIPikRZdqxB7tyL25cv7o6vx+P99P33Hv2tPwq4WKM4Xt59/Pw1AiSwD9J3rcN2mUDhufrr6tbspY3Nr2bulJboAGMUQNAFHHx2XPSQd9fDp78eGYXZ35iN2WKUIYXHq3DnOk9DNQncW8HftrIVBcjYyiHSnU7hXJIBTpojztJBJ0Hoh2MB8e5DrNd4c437HVcbj4LYY7mkZY7m9zu9WvhUoBb7RVpM9c+/GL94XT7Y8DDqp7dlEiMNpgvhRS/7rHBGwUDvOm/Ww3cuUiKORY/Zuoiqrm6BHkNwIAgCEYUexcwdUQAS90c7FgQK3FZLo8GMIYhIc4tGQKwRcyeXdvNaNuXUCHXEEAXCsehUbGUSaHeTTFrO+xDcUXyaSt4z5/r6fsrVATf3av78q91X1/uzVZcSpqpCCUKn7yePYR7/ioIYPEaBeDW+tTON2ejadziMpb48ODx0IuZ9H9bVmXXTx4tlt8x2VpGOFva5fzCcP1z//g+//e1n5198fP3TP/7zf/1vf4D3fxu55HK8vOgVVkElVIAARE+dlImHXd2b8tRmNl+fK1qI+aT1YDG5wClCR4T8Xrd+Z9XvbPb7qMuLyT7oRQOuVuFY33r/MLs+3EGKw4VVLYJvZ2VP2GXw0MxVDC0FgUCXKDAyABqDHycAuJ+kHLU4rt/gs5esxQsU8MteOvG7EC7OVxcb+7tPV8e9f/tJ/NOPb4rbg9Xi9at9IFPgg2U4ZnywiZtleOUZwdwYUzgfAuA3+1LUAzEkTBWBKuJFsT/UzUr6GERkKtXBZSeAjAXmJqSCpjBHdfc2MuIew2lm+rRaI986+tYkCRDfHPRiCBN4SJIjusIAr6ACZq5qh0O9zzXvc3HxQFerFVpZzRy8Pxbba4iMdBGDsxhCMzAIu+Bdahm6MaUnJ1aghOCCacTdvRZ1iAoI1PhFDsL1SjbreEZ5Z9FtovRnsasmB/3RB4+f/cOffLheor/A8+dIxNU6RO+TVEp0LwJlG8ZwBpxFOTjHO7FGG5HeesD56btVLdtqAquGajaK3Vgd/OPjoQvSwQ6gO77M9s5ksQurIT6os4EVjagwNuNUaykdnoFJ1dC2JJrCxKbuqL81RAuRgrh5NV8s+d5TLBZ4/Tle7/B3fgtnK9zf4e4IcwuQ7z5brbvyespf7Sycaxdw0fP33l2W4MNzef9J1IOWC9k7ONnVqkuo31p1YcGxagFFeL5YROFUbdmnX7zcHSf9wdOluX3xJlPk21f94qzf5/LFzfjkvEtRtNqL27JZJJtZQHG3obf9ro0Bq3ki3V2aySUKYKhtOoEQh8q8B42IdwcvtTpZ4UUxOUnEPkikw61aNa/F1CkCc6vFrQ25V9Zq09RoPY9iEp0mNg8IWnCkGKI4yVyN5pGgIAWJUVIERNwVbw9Y8NlSou5323q/t0i/TvnpEJ/1adOLd8d/9i9/8R89u8Af/R7wLt69Akb84uf7PLZRMAYGhxFm1hBnsxST7jDathgIGg0uJ0KVgLi6qbrk7OXoCDoGvBonGw236g5CjKiwr8b64TLuIs5TOFoTok8Dj0RzOAtYyex+VGszXTQ3ccwDvbOTuqFqEA4xEGbuSVwM99s2MsS8w5b4xWeojl64WXXPNl06HENvu72mUTVRHQ/X/Z9+eZdErhZxXJjeBD3YqOwj1kM4Jhwn/evXCvfNKjxaRQA3+xIET84SN7GLoZiJ4Ml52h3qZiGguFMNqyhf3IxjwcW6Q2mzgHDzVzfhbmdZWYvVNI+Lwj2F2erdjI0N1QQIberJEM19VAa6zNOgMCPMKQFOtbn1l0gHXf2kvMLhqo0CgxCZLgVCaySNAIz04HQxN1OnIQoC0METPBBZzWF2Gh2brehzEBCOCr7OdjvmTz1fily8GbV0P3j6yd969xI/InAFHI4vrg/tRBA2X4pmspqnwJ6yjtItWC66L+/r3s1ORrpmPsSJiARMi0cRqHcWvvf+6lfX4/TVYaykAErSnhd7b7KhC87g2WxtIvx6qKj1FCK0hpLNUYhGpXkjOiEQhBMREkXgPJZKYhgYI4ril1/i8qI+XKFLWK7YCboUvvN4sRiEByRHoJta6uObSf/i+eH/+tl21LJ+N/YE1TqVCp+CDYtYTX55k4/FHfJe1/UBU7axeqCPqjc7f/eBdTE8u+jNeTzYotNlF9676gnsjvqty76xklVPlh337SHd7yvpVa2UEshaa3MLRKIKElFttj216bo2ah8x9+JuwmGQCOTRuiRR4M0z2EyhrapVtsM67G2h53CHniZttNUjBnd4cDOvqmquCjiCoyM7t2gCA9zmOgknVXsud+Z57TnLO7eGfbHno/365sXzl/f/4S+v/4P/DPjJGuXui7vDNKnCVXycdKxaSASmIbBCt7pYhHcuehH5bFcOk56ohnYmijeevjkRz89C7QOLXd+O99taKM0fEwC6ZLNPtvnHq2WJGI5xqgWJmK0PdDHhLH06ZgUMBlANYf4IgSiUAAWE6KLAXdXV0Afb7qGOsUiK5o4XL/Dli5CEzx70D8+i5xxdJbibT1kvV+nlvixD75FH8ot9TWr3k5tThD3DIftf3xzvqlHiMuHJeRJwUh2ifHEzfrXTJ+eRwJdvxsfnfS26XEQJvD+Uy3V6fjPd7ew7j/sY/c2+RJFAA8TBLkmK1Ipm5TGwVDvlTgRADVHmXEmbFYEASE8MgZEi6per9OAiOSkxSKCb1daq0iHSgMzM7e3ATGtiT2XgPKzn8wBPY4saGdOsvTCIeCQFNDNTrzofjDPnHXrTQJwApc1qeSMCBCR2Zj/7avfH//evvvgffwbcIz28GIYy2VT8MNr2UA5Hr9XcESl0n+4nn2yziFdn/VnibGY9IZCQhDX+VgTbvR7uyw7l488Or7887sDARr3SxSH4dKy3u9oZojHsQhObpBrNRSHesMqh8zkBmGuBebpCzHkyiwDoIykwMwqePfb33kGX8OqGlxssFlieAcIUZdOHkqvnSvBYuS1eqpeiO52ihHfPFr3Ky5v8aqdZvToY4jCs7qZ6O1U3J/3pWTobQjuOYFLLiu8/Sd+66PdTud26OS/W3eVZfH49fXVTQHQhbLpwc6hDFwKDGUWEbs2k3gWS7matd1c1c3tbnOLrAdRZKm2PVhTMlUL0MXQuyGEVu1UfBFSjWVPsAiNImU/WaFc7nXHjsz0Gra2d4yy0ox+8ns6TIkQEQnERFRRItpaXW6g1gWKep52rmVmzgQfxQA8IxOT+0xfb//p/+FP8k/8HOD5YrKZD3R/K/UGn7F1k34c+SB+Fwj1wl30aTbeljHoK6BYEmK/ejhBQQM0V37lY/8EfPBmfpNwRYCQpLcmyCP7qPscCGNJeMNHcTd3UoZBqUk1q48LdZ2fqfEwFjOYU8+ZaJWXRdX0SJem8XCMJug6Lge6oFW9ucTiSwJT91W0+3E9uUiAV4f5YclZIDL1sax2iDFFUAZViMlVuj/lmXwUiEjqRdy/6EORu1M/e5D6Fdy67JHEs9mjTf+/ZUKteb4sBj87Td54tzPxqE1fLeD4EM79YBac101gXbXNWKNW9OaRghmrms3oMwzxqoP+fYRYgWqBCXWXoJBczD8MiLRYRpGkxpzslGCBKw1xnkHTx5nKZiz6GGfiagBrmyoTzeSktU0Eo7iFoQHEvbuaG5jriWwqAbSRrPiYJdGukAxBhIBX3pf6vv7r+p3/yF3/0t7/LR2c90y4fQxQZwtk6SR+qep0UJFbxLuv9893toe7CPLU6z58AcBPxWRAyi13suvC9s/WRcIPmNnjL00E7BsOLqjf7ep5kNNH7qKYtQ86lrVOL6lQbAQoaRdwROLu/2ERRqBBC5GIgQvCH5xh6bEfsJ/7gEqsBMSFXxCQPz/te8P7lt7Dbvbi//vf//u92Kf7Zv/r4xx+8lw+jdESlH/w46ZRRPXfgVv1+X/uzvovcRL9YBne/OVQJIQo/vS/7UVPkd68Wu2O9vikQWaRIyvVtNvjlOj04i7e7uj3Uoe+qWRfE3b/1zrSKfnOPcRR3qe50N4M61VDNq8J81p3sRNg6oYb4j/7j3//dHzy6v8t1tI8+uf340zd9lPu83ZapTZ+7Q9oeRJvfmZ8T3x47418fFTcT37MAaGZ0NHkRnL8PpylDddg86epzcTdjoxP0+Yybk7fSWzcyn/ukjpdH/eOfPf93/7eP+GTz/tOH+xdfYh0RmJJocwEZVuvYB5nu7cW+vq7epk+aX6GNvBIGV8y+vxADZOA//8vrRz8PxXMMrI0aE1c1J5tt7pOafx+L6l6PsWabj75ovAXMzHMxcze34HQ3GkOz3Zu5M9BBRCEcY60gY8AqYbvF/QFV6YpcsN1H92CO3/rBb/2n/+U/Av4I6JD/W3Qb/PQv/uxfbN7c7v/xv/jVkPXhwOlgKEbTHu7gONV91UcPhsvl8MSnFLjLvhoiaGb48PHQrKAx8HzdlWIX67TqOVXvItUlJY7Vvnpz/MG3zw7ZVIEAh3vFrmCaYJir6+pUR1VUtVxPx7ecMMx/YzIv/uHvf+e9dx/eHvTH//aPwSUAIOKLT//z/+K//5//z7/U6iSbN89tPtGBb7MwwbdnwpxOxQlEkHnO1GZb+uyOB0EGQ8NVM8PsWPf5lMOWKIUz7AAuRpV5aNrsZCUAAP+zj178V//d//HbP3hwKLlPobirY5pUIkTcDCjs+7Ree5iqHsssawJwaUmdsNkar071EGKK8t1nnY666uzi1svBtsd4yGCwhuEBcmv4asgPx24CErsa/1+q3ivI1uw6D/vW2vsP5z+p8+2+eXICBphBIAHQIEiCYBRFSqQlkgqm6bJUfnBZpQf7yZbkF5WDqqgHW7YplwjJpmXKDCLBZAIEEUhwBoPBREy+sW/n0yf/Ye+9lh/2f+7AL1P3ZbpPn3//e631peWCV1YEAkSDqgtBFSpEBXMKP25Ja1FqWwJQwgA0eFFCkkGA2uPgFHkR1jZQZFgE2umnDz/0wM987lngB4ElcAHpfwb8wdHtkyLll46no0WzDk0H2XQqmYElZqajpStFuMO99Wy9390ebDz76KMJ3MsvvTqeV6JhJ6MLm8PrW+tvHI7fPTpf79mTUXV83uxtp3maq8iyDt0OX97NOxlPShc1TGzR72m5jB7PmFVDGvV3q4Zs9WTaAbHN2Yu807//969t7QyKbi83vTSzV3cH1EmXi8oFCT5KkETi4ZR4GFqlDYu0HvlV0Yv/sBxx2qjla6XC8dQwK0gDsYiKUtQIKBHJCtVgcEtvR1a8NUyoBcDwIk5IKXpIKKXbixkd+SyB1KFpBIXJc5sX1qtOzhuWMOwi9WKCrujueKAjjHK/K4wqGIUKM/VscpaGtGMGCTVLdSdhOuMQlA2pqjEQkZNEN4zNZ8zdbHvQv3vr3IdAQjHoz/loQIaUEjwj0tXS/qr4TaU2ba0ChGEhgxwugONX16D2SND9x//5T3/kb/8XwCXgPeBNYA5s4OaL33r19tdfvPXWvfNL270rWchAZwmNy5AwGi/HTXApb24VWW7U8kmghx69+tRP/uKPoQ8c4Y0vHPz6H+1dyfDo7vdduA5pcHv6L/+ft77+2kgFo2l9dNZ0MuoXxdYwI5ALIIr9ixQJJg6iJKJBySiIhKCG1DClRv37EUktrRn7XihsSLK3bpw89URve6NvE/7zb7w7W5TfeuXGt9+4I6rWWI78fVBpzcgxt0gC2nYD991kgCGkCYiUqQ3GWcEfSkzEEIa0GF4EUwXxB+lKnNXGt4LQctMcGKJkQClgjfqAQETI163pg1zjxo2vPa3ZLDFZYgzIC8BcOz87XJ43fhk0MLW1H6sfT0IitFLGEIsChaFu3753LyR9NERpX/I5gwiirgk2YUV0PuhZ3+01WVLkl3c3+nn26mv3REVURUIIqhBSUJK2iI6qQlj5fmZLYlQEccLodjRJMKlw5xSdTkgyLBbm1/7Hf4AnPgf0gLcweW78wptrz55gbfjS117/0ovvfefO+d5mMVk29w6ry4NkEbAIoqCZAW11eqkZnTWju/PuA/nWzsZTH74GbAKbwMN4/FN7//jv4r1/NfrCH24EQT/DteHffbD3dKFvHFfPMRSy1U/LJmQJiXLQQFACG+OMgQLOg0ghEsOGSMWwmFgqtM0pUlm17IBROIH9+b/2yUHPfuPFW3/0xy//1Z989lM/+2PAmf6afuX576gqsRrDzkNUJWDVRkWYtu1p9bvqpmXEXCoAKispQGznCCCjQAAF0tACJO3Z51WwF7ECRMzEwgBqkkZMvHwMjBWT2J2d4VqvY3uhrprxEhJkntpEyTRijaaW85ybQIvTxexkftjPpynjvlxnVTtXfkUAAgaxCuHaIC+GiR5r200SwaC9b0kJZFkid14arftuINrrZrtP9M/Hy9u3R6rqg2o0KQBSe4KwRYwki9wXEYwiNRxtscy6t66kaBxqx0UqSUh+8ad+AU98FFjDnf/7D3/7z597/c4z19e7r9/c21wfnZ0+88hmp8O5MQo9GJfz0h0vA2dJ44MaY9mW564Z1/OzyiL5wEOPwnngLeBDAIAu8Bge/G83/lZv8YXfVHH1jeNJLvlm9jD0sc3ssApvl/rK7UWe0LyM5i5S1Y2hT+1KHbyajyJIyNE+Fj2fbYpLy7rEgyEK++ynH5XD89rJw1c2TGj+7N/8jimypgkMunrhwsXdjRv7JyenpyEOEjH9VFvfDq0Y0xbKZ1gbn6CGsKIQpeX2mFhZg6CBOlIfolytbfi0lbBrm1wZq7pGKx98AEX9UqNkg8t9tpWagu9hecgQZkC3azHGdAtT5KkPQWd+MmnEhbBoJM3iJ24Tc7SF51qIJl70RNbQbj/zKQUvDJio/tOIqmoMGw8wCXumVCHnqWxNKnixfX7ysYsHB2NX+xBaIIcUGgJBYQy1DXGMb6Wodai9KCMxvDZEkuHsEGWdPfPExR/53mcvf+gRYIrzP7r72r3X3rtX1XXt/fhodD6aFblhwnY/g8IHvbZV+IC1fnowq5ejZbP0flRLI2opW8/EuP39o/Hp2doDCfAdYAAsMf02Btex/snuxefkdD9NOeuaci2TvXw+9sXIfbqXrf3s4//rH9x4/u3ziF2JirWoHRoPAxZSohDRv1Wvf783Q1RMIay4kigb/kf/4Ifp4oUNo3fvjTc3utc/cv3WG3c//+++tn862d1a/+iHr1+/unt6Mj2fLsUHlWjljMo4+u7ULFIYhrVgarNJYy5qVNgZpsQyGXIktahXlSDBvT9OgigmYHJQFiCohtZjSquXI55Ia6211oUGPTRW5wrHGkQNcWFN15KtwvnB4t5xNXIIValOOU8aJuaYpxTvYSUghWMOgIA4NNiw6ZWt3v6sPD0rbRdM5IWqiqbnEEi/j36h3a70e5oPKElYFfWJFh5r28NOYcsyHJ/MFo0LdUCM8WpjlE03synZaGCbBKfMPWt9ELAmGX380TDoI82uff8zT3/m2Uef+PiTuPIIYNHp/PHvfO2Vt/aL1G4O0ibIfN4QkFiTMOepscxZahsf+h1b5JYyZkuUmbyXXLjUv3K5d2G7+/GnHvj4z30SsIAAb/zm//Cr337h9gc/+b3AJ/DAB2j/OamW1lJqbbdjOl2bDyxUO71kuGgOvd49rVQ1sfTBBxvLODrHeBr7VGZmUfFeayfBrzJgvkt/pqvCoYD5oT1ce5Q5x/reENsdjBbnJ7P9g/Mbd09U+XxalWV9cno+nZfq7me08X3sV1fhlQRYAzYAyAe0F4aQKixzYogNqSVPWgOBCE7hiFrHUBS7xnwAiipCmBV0FUEnAoGyjC9d3tnd28kSotwHQwFtFjAEWAaUIajcPG/ulp7IuDogZ3hUeWKidF+VWj0JEjSGgjIxKNS6hjTJksPRcjZ3SZ+ZyQnqksqlsbnsXjZra9rfNLZr2ZKxINHqBGbmObNqeLKoj09m02UTIyiYICBVpInppDZjjhK4SXBsTCdN2CIA2xvDv/kTn91ef3K9e+HSheEjP/MZrP00sIEbfwFLJ+8ef/3Ft3cGBRECRAPmc5elnKe2kyTd3IqCmebOe5E84UEv3VsvHrky2NspurndGAx+9oc+2rv2QaCL5u0v/6sv/V9f/PbnPvHE5ScHYADP4qEP3fvK/+t9WXSMNWwNMcNbOjuvzsf1XmHXN7M7p7WE0O/5ZYlbR5gtmcFsmMiIqvNa1dIIwkq3LQJ/H7RvZXkwP/1o9djTXSQNyhGqUXj+9c//xp/funN8spS9rt3p2dv7p6fjqXMiXletf1tuRAkxyVLBBJuAI3saIh8AUZjW4QKypEyO4FRJBYHUKVq7AwhRzAMyBAOKqXncut7iI7KGh2v94drA1erNkrpGGH5FrarQYu4tg7p8t5ZJFbjylWo3hyl9kyewbKLPmoCYdKcVmZXYotG84Y7FZOIbF5IhEVMQVJVWM93a0+FulrC3mVXLAIxR8iQjLhc+82EmcjaZL6pmMi0RIIosYxcEhhNLRWIzw3HPwDT4LLO5tVsbmz/+6Y/913/vxy//6A90Z9ULb916Y/88HTc75g42Get7f/L533v1ncOD01EvsanlbpF0MrNYuNnCdfIkMZSnVqHEPG5qYzlJeGOQbQ6zQKicZpav7O598rPPoDfEyStf+PyXf/NL317U1QcfvuT3z4vpreTSGvD48Mr8a7/yp/PKJ4UhS6UTL0SW0q5NK79HGAyz2+fVpQuOCMfnWCy5zSom8oLGa+VC49AE+IAg8DHiSlbXW8zbtiYgMSDFxU3M5s+/eXB0MpqUWlh6bK/wfjmfzXyLyCtaKp4AlfD/07exabussLJSxQa/BcU4Xm0UYw9iSFKLubSxTjF1B23KyfsVvx07iDlJbZbn84VzTdW/vJpBENoYTaVGNEAbrw4Y9MzFPMkDkkVdwqWj6vRCodx+/FWeuq6kYRSAw0mJUpZLL+vCZBQKYsuhyH1vLbMpaU3E0KAmdgqqIlp5HJ7Nt0kq74seZ4Wty+bv/c3H1nr8z379zfkSMbQiSnAZfPnC9i/81Md+8hc/hZ1HgQ8A1eTPf/Wlt+545UFv8IWvvfrPPv+ls3vztaJvMz4+OU26ydzYjuWiY7qDbLiWnZ4u7xxOd3d6JjU7G8XBaNkpkp1Bp3Z+2bizSVUH7eS2k6Uffuw6dgZ49flf+fyfvPzu/tl51e3al16/8bXFcrao/vrn9j/xt38eu5/77M986y/+zZe+9eY8e7x7+WrRyS2IsjzJr/XHx+XVRj774a2xu30+waxECCKGWRGUFBTbbK9wAgkA3vee3D8bAtiOJWQWr57gM5t45/TLL98UxaLR3Jphl987dETCpDYzxiJ4hScJ2qocBab1LLYZz0FjJFbsAUlWIb7KxASTUFDjEXxo4yXbOBPElqllFGIifmxxqO3aYS1lnbx24pfLJKuN7bXHVGMtpJanV9S1GMKV3XR7mGaGw0lSvTaWsuJuohv56ugLrbQAq2xXytZT65OzqukM4CRAWdXnGcIaceTySaCG6T4xIXGCHZVubdZ0Okqsu9ud7mb+Vz6581tfve0bZbAxTESGeHO39z0fe+jn/pufA/0ssAXci3Pbsg5/+sJ3todbD17qvfbGq+PzRXBycHIqThDUO+H1PgPjSSUqScLbm53ReXXvaKGASWhS1/0ssUyTMtw8mrPhXmF7Hbu1tiZB//h/+b0vffONk9PZaFZDUM39K6/cyvuJiN68d/rBv/yz3vf8B+YHn0p//7mU3OsvTpa3yivPrm1u5cYQW7O+Wxjm3uFyv781nZ+maevmCQoGS6sXaN1RLfD9XW0Z7s+bKQvOljia4aXbf/RbLztfV05KH9Y6yb1ReTqviWAsrG1909KQNOIb0kYJ8IzotKCVVBetmzluboEAlkBQa9hagqjABB8kSvZlxRNE/VZL0WtbMFsngxCYrQXbqnTBL/N+ykmr7Lm/9kGV4QVqqtoRkRdZLBvtJGUHB+KX5Ll0LCkA5ii1CC0vGY2ykA9cXC+2slsvlmCNxqgYF5JZIrS4DNoLWoiQMHsogQNkf1rtJplDGKTy/R+5dPNk/qfPHTlRIsSswg8+tfnXfuDalb/z/aAfALYAADfOvvJbR2eLg9PxA3sXv/3K4Ze//GZdOwntXVAHCT6ktUIlTU2nsFXtEpv2uqkSTk/LO/em42UtDBNwcLo4n9WDflJ0sl43SROG0ouvv/Pq27fOptV8XteVJ0W1CNTJFpXf3eudjsb/8t999ZcRFvPFaK+rzaxzT82xu/e1Uf3M2pUHukSUJDzY6QjT/nuiYW22nPoW4sb7Gr5VAx1ltC163w6f8TaB7SQG5yUurX3x3774zsGBCdqINkFntTscc+2cV5Aha4jIiKiQeiUEDib6wVoWEisgzVowEVP7BAESgiGOsUOJQRNWBl1tCYbVzdSWsKgTitOqrmSJKrJc1gjeGrG5QbvyQ1sIjhgqJMSEpdM6iLKpGiFxy0bmTL29vOomEY6XmI4XZ3ISUkCpb/Nunh+OayYj6qjNJQAM2BqKkScUM5sIMBR1ZzFJINBcwnLus75pKDx38/QvXpOyMdsbeVnJY1f63/vU9vc/vb3740/D/CBAwClQA9losvyn/+J34fHww5f/47/+ya8+9+5v/f5fxmIuIoAypG95tmjG0yrLu50syRJTNt4Y2tosxrNqPmtqo6RyPqm3Nrq9rikyKypn5/XJyfnde/Nm3kA0GIrhCvVStKm7G5mKvvTqrSxL/vm//lKvoNnCXS36w6IyjcMinHxjRF6vPz4wzGx0fSvbOikvLov1olosXOxvCGBSQ0gYwSKgtZwYgkiLCsXLDwTbSSxK8W9GmwAAIABJREFU/+LzN96+e7xR4GTsZjUH1cqF8/kyTd7PCmhhNwARWCKKscqG6b4ojQxIYYy23lMCRecZqYKjxFRX0Eism1EUAb3vzrivrG3fFRIFkXcBWjMLpzbJVrmIq/8jXp4MtQYayM3l5LDe2khcFc7OHHWzYKhjUa+asuhYgEBX2GLlwslRORk38fOqgjn+WYaYyEd9NjPFJlW07TKJVJkQlOYNtoWaBDJ3673Of/SzV2bT2i7l+sWiGGaVMnb6wDkwAV4AHsTy2wdn89IFnftXX3zPleGRh3bshbReelSBA4YZb3TzrvUNwblQlX6QJSpwEoos6eamk5uzWX00W3a6Sa+b9btJYmi+aE7Oq5Oz8vy8bkTqRKUSu5CE2LPW3idFvrtZBBe63aRbZNtrvTduHwjIKy72sgdGjgDrdfTNcWL56iN9EJHhzd3O+nF1IbNH1hHUtJ2SJAaphSr8agTU1dKdduRksMJu9AscTb/6rRvbG9olmlRm0YiATJtiRKxKzAKFwIXIW5FvgVaNi/5CC5zcz+GJLRe1il4DMDkBvKolAaPNYFtdVnGSAMXg/1YQJBQPbxQYiYBYQLApJTGkuuVAW6hVRGx0REgwaiZHzfiogaLx3NnKlqobzvskZQJUAxMCVm8NxZSbB690pq7xLqQACBZt/9WmY2gUaQIxyUNb9aJGVgnU75rtS/n5yOnMffTJnWZe3XpltPHA+uKdc5elzzx0EbMSg1OgWf7JS8Vn95rX93/jD15onIeoEXntlfe+8+q7RabwIqyDjEQpt76XU10kRScxRHUdytLnuWlMKBtfVn62dNE1lOXMQuNZc3C6qGpfOcm7NpTOeIpm8fg+dAw1pZucVVu7hXpZzt2dgyNr9PhkMVK+zbq+1l2flCSBgh49f57mZu9KR0HBmHQj6ySUG/LaOvCCkmmNRQpApK2butIjBgErSGAvXN305zMmt9Ux02WYVH7pV0IwgijEEBlSggfUqgYKVrwhTwpqo8JDiLlqCsDEZVf8fkPIq+MaolhGBK1CA++vfUPbZ3FkFlZcNxRRihaTB4kozY1JKYZjtKMpgUAkmliyKYWlgilJbLlQZrZWKeFAqMumb+vEJP1e52bTYFVxVUmCJKAGhIHFCIRAymwUvu0NFIHUELVrB1cOlKBqAcRVfB9/asA9vHmrGW51P/Lk9p+9eHx2VrtmPPH+sYd3nn5yD5MKf/Z733hh/+vvLv7hhx556c17R3fPyMcpTajntnaWxuvr7/Fanu0MO0E0F0cBecbGkA8iDiJau7AofSe3yugUtp8ky8q7RkbT+eHpIklYBGliwFp6T0vloIogSrnhH3ly85XTxd3TpQRJe8nVi53lvLl5b1KsZUmHLu0MZ8NefnOUHY9VFFXYf36U9baTnBsvgdEtjCUVVUNCxDFfy/CKplsZnNp2TWBWGm6L3cHo1lmRm8Imd+pm6bkOogAbIkYQOAUYahkuEJMaFWUkoAxg8Q3EqxeENvu2HQVip71ib8gSqQWAELklifknLc30vpK6BU1YSAxTzLRj0lb3tnJvGzaxzALEcUwlhcZRw2jCxpBVaiwbY0MEf5mXwW424dpO92NPX/63r+yfLypgtSMVKFI7K5tq6VQDKbeKfqZVCxkxZLREaZyMabUVknB5M7uwm331haPtxm6ZdP/t8e2j2j66Vu6Xi6Wbn1e//buv3fqfp0eT6mRWnXna+JU/fOOdfQt/9WppMnn5Pd251Fy8gGYOuiWWOTNECdsGJkYgGfIa/FJNShAyDAiaEKpayroJQLVwk5nr91NrqHLeMi2Xvq6Dk0Ah2u/x4eudzz01+LDLv/XV8ZuCivjsZDlrms2tbrcwWZFsdJJx1YwSejzPsSitofNp/fq3zx99Zj3qY03C1sC3LN77ho77j17vT5otYARhUIDFrNw/nndT1hBOSyl9ECEQMgtiahx8xDZVA0BEEqAkZMlm5MEIITQty9SKYVaoCTRGHkIUQmqYyLAqqVeVNgyAcH9dzGonLgCKonqAWzcfTNQ9srWUJISYQUhMIgxuUTlBYiGkYtgUTJ5MChNMqOOdCbHWeVfP6TO/+Et/9k//p/FsIhxlTkTEH742LFOi0cpFAsTdAFhp51bfahyq7iN9UYwijfNfff7oxu3lQ8N8Pqq/eHO/LGy61yu3U2/DG3enr9+YzXxwVufO94v8uRfeOjg7efKDs6cf0JsnKN9m8fBLLOfwgRsv8ZJ2Yjwx1aE2QbwIkCrnHetcOKuc8zpbNvOlC0GDyoXtQonK0pVlqBvvRCQoRBWihIvr5kefXisyygN9oG+v9ZI/mvrJtEHKKWN0UmZZI5WfO90Ydk4ffeBxlrvvvrd/uNx8Y3q2k2NgnVOPlYVrhT6KyvvrB+T9zkxXhyFCpYwljk4XRapl40/mofEUop3bgE0073OIXg3cj/0AG4UBjAhR0PbwErexkRQXyTAMg0ybNwAiQ8Qx1zrqi4TiyEiCuDcGQnFXmSo0AC5egAQDSslYspYyAyqXqCoED45Ki7bHs0xtrENmtGttPzEbSbqeUsKcGmNpe1j80Pc9iWJj4jgmn8VvaivLH7hUVOJd44NC42dRD9IYYRx7CIWuMjGVoPGgEQDF0di9ebO+OW7mjdBSoDATp8cLdSHJzLyWJm78NAipjqvlzeN741BuDdQFpBaDga4NURQQAgIvmlAHWdaexIlJg2hTBWN5OEitZQKsNTEktciSzWGepLy12VnMm9OT5WRa17VXUJLYWOTFEhE+8fjw6maW9Y2IFmvJh75n7XOP9XyQNDWnJ+Wgn61vFoa58iEErYf9j//cD8+1WFdKlQ6/M5nMXOXF+3biUpAIx9UWIZALcB7OI+4TdqH9b2yogsK+d2M5XTbDBKNaZw1q33JKETAQcJCgYhCpmjZwDSLRXE1BQ+u7bW+g2J7H2EAwEzNg2ijUNnACLQ4CVlJq98/GKggBQ6OqQURBympilKUoQ03CeUHBq3hvbMKGlEFCqsQCk5D3Ioi0FZMhCDgjEJkED3az77ne/8Tf/xxOvrFW7i8NeZN69ap4cFAUPR6/F5rGt4LO1nAe81lXdnLSWCgJkatUtJviSVWdytLpW0eLx7Y6gzyxKn4eJkvfNOS9MBNAjrTx0jgnpMOhbg6Rprh3itMzurSndYnFAj6IC3oyqbOELxTplGynm/Y71nsNXtPMqKjzzqZcz5vGaVk55+XosBFRYylJbdYxRZGcnZdaiwYloJ+bB3cyIzRrhEjXn+p1evaBC+kzDxVv3WvqxkuAb0KSmt1hEYK+8+6dr7yy/Qt//68sD8++9mt/MDt1i/1labRsfDQBCBhKQYwX36xCXELci0itW+J+ARXAfv3l00TUeT2qUAZx0tauAK0dVUF8EGJibhViRKIKCeQDQmQFEoKP+0xB8TlE2JapzaY38ZJd0UnaGjNXhZPe56goxsgSGwQhEjUCFoEDiCVVm1AIShG44va3tfOKImGIB0BqiAA2ZIJssG7aJjfsy+a1d6rd/+MbH72UXLTUzbve2rdGUwmh2OY7o2YxCVa5l3QEPnIobTbj6pxx245JfIuozbjiFp4hVei9uRtV4Wo3GeRGIDO2lU8izqgk0QkVe78sUe8w86gbDLakO4AG5NzdW5PbZ7WTcL1jHyyS5ydKtet1rbHUeG2WLuqyOKHBWraY+0bC+jDrFjbPjLXsgkyn9clxOTophSGJSRfu4ka2VvBo4Rc2ZL2EchrPXGnkYw92jt5ZHtfS1F5FRk0lQOX8ogq374xHP/Gxn/nlH7z48ntvPf/69F7V7HYWlTRehcgIwbBABBxEfYAP8IIodcR9NX88SwR7eHJ6oavjWs8D156daBzgvbAX1I0GglVdLRJXABI0+OCdBq9kVu1R/Hm0Al5XyzCV2y3kooE0rgsglbCaJ7HSzbb6LGawIQ7CDupUA+L9pAkMkWWQaJoZQbRAgZkoROe3GmNCNCMY5Kp9o9sdt9mRPFdr9fBc3np78V/9jU9W37kxrqZNA1+zKeuOtbOpw+2yHjfXN3h7Kzs+b86nS2c4pF7iShCAVGDQdoQAUWi3QLOuKKw4/NLMye2lu5KQQEd16NqkTZHnFnokZqXQKcAW8xq37lHS0YyQdzDoGlm3J9Pm4fX042tZ6Cejo9Ke19aYxdJVTkgkSThNbZpQmpmilwwGaYBAYA1P583de7PxtAmEUECV7dIZr7vDpHHBq5nV3hiTKU2bJuva81H1Aw92Nkr/8u0lF/batWGeGyGtXFgu3e/82TdUw7WtDaeoJs2J+lnlmxAxUY5vOiPiaxqxWeVonW7h2fuXiV2W9YQVlheCJiAoYghY7CBDUBhdNemiiuDVu+AdXBPPibYaHnlfJaZQNa0hNsYnRjZJRVSjzCOKytoCakIstnHllhoIHJxTUcAC0THPYAMr5GdBko7NovaC2r3fShCw0VqRBxnMm02VnUE3BJ6cL8akZMKspvXN3j/6W/99kSwChaUkw7x+cjuMpu7eoW6Ncn/ms8Jl6jcKn5v03cM62GC3TYRlohWWiBTC96UEukpAUzWrP5cIqUVh+bD0cxf6CQi8vt577IOX1zZ657Py228fvnnn7lqv6qQgg+FQXQ6TYzHHzYOGg3l2L/tgNx1ezGfMde6rylUu7O0WCnJOZ/N6WfnZUuIkn6VcdOz6MJ9MqlsH06BadJOqcboISjBBncNGn+HRy/k4aIdwPnMlKBFvEltcpe/VbDPn47yX963z2jhPqknC7MI337gzfPhKAHyQchJ8EAUZgI0yVBmGybJaA1IERggtoalxcR2vfChV4ycWpstVHZogQQloTSciEBUGwEJqJMa6OHVOXa2IPZe0OouVIRKg1ebHNqo1rnUhZgASPLVFVFvfCq2CqWPHpgZEGhQwIAtEAp7iykNmC8oNZUZNGwlFaNfOdTvcHaYDwuC96eZm8eCjO9f21ojM0al74Zs3FqP51uXOL/3cp3eefeAf/tL/Nqpdui6HbvnsdfOxB+zbRzg58ks0N/abd/dLHyQQjx01FTYpdC4FarGVCKRFfQlRdMrCAEoQjrc1AELj9Oa4KVV6/U6S8A9/9kP/4d/5FB7bBdaAHjDBm2//4e99++X33rh78s6dA7n8ECxBGX1LD29m1zpm71Kedu1shit7vbXcTCfh1v5sa63zoce3s8RUzi9Lt6xD2bjGiwQ5HS3v3JnVdQCpRGNlYRJRmTbG8lpBCNhfNGxJHMaNTxMTPDYGtq5Dde57RSaDZOlj9h6UUXSKRbV47+7Jw20eLEIdMTMxHFXBqoK4QjQxYLS6ivfJAGr1Z6QwH9s1akQLO63odK4L1xoVDZsmaPAwCZnUMJME8U6bWppaRLgVTbaKRlppLaAxasGwScDMZMAEG2VkzM7DNxp8m7wJghgoQwhqoLY9skKQhJlggnINdYBQ3uHBprW9VK2lVhypREaCrjfugZ2su5n4s6qX2wuP9K5e3Xj0yjBL+O3jE01UofOmPh03WVm/c3h7WYbKpg14qwPL/NTjV+b9xJdgzt87C9XMN5Y6GQ8TMxurLZhSZhFjkJBW3hCpMUJO3Tnl3pY+xBFoXAYWDaCcmQzvXhv+1c/s2Mys7+xc6CaHL95cn41w2QIGW+sP7/Uv5euzxfC9e7PhznIjw/DMPMzdx3fynUu56RhDlBgczClJk8t73b3dXpbw0eny8HSxrEJd+/nC3TmY3bw1vXVnenSwWLoQrNpukvXTfJB0Eluf1GUtnQ59+GoxNIkaQHS0DJ2cLZMqypmfHDvtpQ8+UOx0SZtmPnezhXeOHrp6ua71nbfv7i6rnvEVMPMyFimdGMOpZWYGNITgvUTVNK36bW6J71ZdAYJtghqBCNVOfbjPiHMAiW+TNdqV5x7Bq2skhKjMYERm6r7iYnXYsDIqkEW8iRBURIkQRKP424hqzFFgiAUIEjEPRiS9bBBqGF6DQhNkGQ23bKefcmarAKiQsjAsQRQ+CGdUljqZOrvXAfTobFKXdV06Q6Hb5wvbF+fz6Tv7hy//zo3gCTaMTqs0pf0qE9K1eZhOapxVsyCc23GJa+upkx4v6o3UTQ99umdMGptbtEsO1SgE0ubRRg5YV65QMiDLFzPSWT1d+s9/8cXf+sZ3WN161vnk0w9c31vbGHYvbg1ff+e4rsOnn37oUx/9BE+no/JOfsl3uxzBCzJQx7NpYxJ0Urss3f7hnMn0CnM6Ko9OlmXp1RASSMZJ317c7G4P06oMZ8fz2WkzmzZVFdLE5DazbA6Pl/nQGiGbERGJVzcL0zKkG9nOhYyYJuOqLptCfDZvZmfu6++MR0Ev5ubqVVSLZHzoR03jFAQwBSBpaUMVigu4JTp3WnVDdMG1sIXCuiCJqgRtnDqBKjNHkD0Se2IsM1HwQYK6RoMHKG4Jlah14BWEGYtx7GJAQmwiXBYnsZhyFUQlBmwqyCPubBFBlA7CwAgbiDhoDR9DVi2sIbZkO0ZsC+Gs6FDEH14FnQWZNeEu6Pi4Ggz08cubn/r4w7/5x9+umuVDF7aWpfzgJy5y/6n/7leff/t4st7VTz9O9/Z9t3amk7/x1nR60qjxJ6OaYaxjs3RFb8FD6lKgSk/3Q3bZ2AygaNKKBGsbN9T+xRpJf2oZN1U3bt56S96c6fmiOhnPupbG6eLwS3Nj7em0fOahy089tPun33x7PC8/8ujlz/7YZ15fe/3Fb/3F5dwkNmLR/NaJW3jdLszBUVnWzfZ61xg6OF2cTWrKuNfvJIY6edLt2kGRVLW7t784O5qXdQgQES1SS6C8N4D0F9WxGHKW1joWTuqRn0H7u9nWVuEVd06WJ+P6bNKMJ2E5c9YDy4oFl7vZwe3lZOqWTTABcRUZwUYUO7TdxPu0gNKqEaLvSrNQ2KAQQhB4Dy+skFU1VIiwJWMptv9No02jAqiwBLlPSa7smwC0BZuimJ+ILTFBhURBokFJlTV4ioEf7UwA8QCBEk0MmNQqBdWQMDIhy9awJRDxfCJZ1zB7BBOUWeG8+KrSIDSvbx+FpYSzUz8HZjvm1t3x6ejlyWTCNq1dyBLz0ruzBvX6IL1Y9e+c1meDZmfPMPTa3oXta/0vfWN/duZpgjwoHO8fyPc8E/oF+YoHXRmWNA4Q4ZgJ3So62r5/JQOAMDS054+DandoaifjhUMAIzTC3DjTTbXxo+niS3/5xpu3jw9Px1UT/st//rs//NzbvX7+jZdnT+wm3/twd72XHM709ZESdFn7XifZXOup4nhSXbrYf/jBNWs4jucAl1VzcLK8fThfzJvAoMIYNYkR9sar5MPOtJMtO11f+eFATSXdkJxYDLY6w35aunB0Xh+cVifnzXTsm1q7hi5spuVGqgvXq0Ky1AGRGJ4po9FVIlRrRRXcdw4jSKvRaH0o30VDWVGIYWF2IXhdGZkClIKqWksABR+ck6Zpq54EldBiJIYgiAADAWBWZjAEZFp6wHAAECCtfVSdixjcaj8jAQYmIUMEUQrtZUeklsHRVackBnnCRWZNQouF1k6UaDlrTu5MSTU1KmfkVYPDVt8Gpx96sP/m3bl3Qb07O59bTibH1Rtvn02bkJj0cp4fn0g1TIKrfvTjvXmXG7Y3zsmKMQKr6mq4Cp0hnKJqeKsHqzKRuKxHYpCDtFFALWtG7Q6nCISQGtrICcPEnDgL9TAIqL2kLNevbE7LelQv7h2OKEaahfB7X3m1W5i0Y7/6TvWd4/qJhzeD4nwRSLUJLknYeg6iFy90E0NEZA0xkxc9PFscHi+mCyeA7dogAR68DOQMVKVrfuKzHzbjo1Fd0qx0J9WowHRddna6RWGnpTs6aw7O6pNTVy29OAwKvryRcBmKqe8EtcYEqyyyFKDVZDMI1IpZGGSCBCct9N/muHxXiEvkp6yQikl8UBciitjaNFoqyZBKcF6bRkOIuAZCgDgQwAZRv6wkRGDDTHHLTOu0JiYmlvdzDQQCUdWYIqsKhbFkDThAg3qvjbTxPGzBgK80BHCiF/aK/rBrMw1BbEKlA4LWlZc6ELQzyB7cW3v95vnC++DVqL99dzw+WwqjkeAWjaFwerJQHxLVWuqTcVOLe/N0eX0je/NwcfRuM75Rns+k75UDaoUFHR7L9jovKz09D8tKTyvK9iTfNavaYNpoLo3Ddvu5ATKkxMgL28uYB0mkS0xM0/B6Pp41lTOWhdQrcjZkHJwqMJu5QpQzOjkvZy8fPfzgxu5OZ7ufNV7LOhxPyoRNI9JJLAiN80VmyxD2jxfjSU1MzvumCWCgEWkAA02Zc/PQtZ1rT+185Yvn5/OKLG1e766vp03Qk/Pq4LQ5Om3Oz32olQJylaxUveP7ljNjOIGSukBLSIhLxARBxcLGwG0GEfkmaCSaZMVvIqpqV+dMAOvZBCYX4IRCCLHNi5MDJwRVL+QaabyoQLwEF39nC2eoAbPGJP32Mot2mKjZj55MtGQ1QtsjWkucaGCCUhKUnAaHAAQbV720WaQcL82CNtfzy9trD1xYTwZyODtzQSIvFJpAhkjph5+9/E9+/edxMPuVf/Llb711mIJvHSyOJlV/LbGZrZtGq9Q71wQd1XLofeXaJuvSdnHpQrZ/swmqvpRJDU10ThQS4MgHNtd21XLwREnORQMNAbDxndaVTCHKhKDMgKhaQ1DdKKhf2P0yVHVgRhCoCHkIYb4sSZAoxKg0wsbEPEMllPOQqYFVLd27N86z3DARibpGssSMp3WRFJcuFQp668743p1p1fjBWr7bteNJvTx3gYhUfBBkNu57ZKU7x+OiNrNZ2R/w5Sc208yM583to+rgpDw/lXIZrFJ/yFqrTF3mmBKTGU4YAvigAeoFXtSpeFGvnBNbY6NoRIEAeIEPqwy88F0TQJwMAHuWdXxmg6KUMi6MJyZijhQyFBrUO6iHeBEH8ZBwP7kYrc2biRnWKBEx37eUoGWYViSBgts19U6NJSMEUfYqArbgBDZhGAS0bQ5AiaVebq/vbj5+feeRqxu9teyFO/jO+EQADdLU4gIs9Le/dnP7l3/jP/2pJ37yI1u2Kq/t0qQJeTbMu+la39w4Xi4XtQY6dXLQSC0Iokz00KXeZ5/e+b4Pb7/oAr+98EQQOSjRqAbBSCCFPHolGa4hT0IVkHBwpUEqUUXbygdWYsmV3ZkNiAxdGiQm5boUKGlQ8gIiR2oCAoGhKTCvhFKC1/uDrFelpSQdagh+1ty4Pbt6UfY2e8G501HZ76Vs6O2b49myGQ7zRx9cV9DR+fLkdKmK9Y1O7cJ81oREQTDCZCkpkhdeeHNZuCvbZn2tUzk5OG/2j5Z3bpezqVBAr8/DNZtmTEjFZWEZZBqaoGk7QSPEgEql9lkJiBNjjSED40EMYbnftGnb/rfzga7U/BNrxaYUdCmNIiB28a2YFoS4SUTEq2/UOwQPuh+BGACrMVbMWrYGHDcc3X8AvMqUip9gFQXjA9I28RSSEDLV79q+ykRqEPeLmICkkUGRba0Xg37OSHroVdWJiohAghioKhrR//0r733zzbsPDNNPbHXye1RDN4ed1CS7w8GPfvJhrHX+z1976Yt//FpcpWQYgByNlr//zXvvHU0Plq4uJWM6baQRRHW5AOdTHS3k0jp6GZqFUpB0Di0gObcvGa/4DqK4Dk9UA5BaLVJSw2miIFXRoMoeynBBjcIDrEiIOAQJCkMRdySGq4VLQkqO9ORwZgzKmX/02roAN+/O3q0mGlhJ9O7cGt7YyHd2Oo88MJzW7uBwOZ/WJjHr/bwWCUCWdJ65sneVF5fW6Pre4O758tZBefvO8vjE+QYWMuhzp8/GtAosk9ssN7TOkSHXSUMLUtdqBOPgp6SWYQ0bJlEyMTlkNXRGkbO2+Pn91xCWLBGzlE5FoEwQCSLE8WQYC1Wyxjj2TGyMrpRoq72CAYE1Hi9jjbVRG4v7toJWHUsqqkFUWi4S5GEsyFJI2bVRCi1I0ap5BdQIHNWs775zZBWpTTY3BkmS5h0sZuIr9XH7CKuSVIGP536vsLNKEwO/bA5OK9Mdf+OV/X/9p9mFS+krr5x6kIZWXk6geR3unC5C7U7H4WQexvOgimjgit/ZbEH7I6TdPNd6vvSTJTihZl2KDKvAU1op72J+gxqCJYIn60UNGbvScAoAsZ6cQXARBVAfNFFAmaOkE2osOQsXYCtBwpXK6GSJbX7p9dMrO8WDl/p5avrdtJMlTHBevZfah6oOBdmrV/qbm9k7t8b37s7Xe8nDF7sfuLr2/Q93s8q/vb9cNnLvoHr3xhKqW2tcQS1bCDWNch0MBQaxhWGmRF1CupbkG0niAk/88riGi8ttlImThLPEUNTS0opAwkqmsUI6SN8/ahbWsKGmkZWxnDQgoM1qAYOZbMIZGWN1dS+1nHzMzIxG3/vy69j/qRAIIQQYjumZAKllsWpTFRcHYxgHlkAxDr59D4SU4jI1H2As9bv5cNi9uLe1ttYf9Dp9n+xtpLPMnxw1KhoIlqCBfSM3RjIrw+FZ/WA/takhaDXRG3P/scfWtXR1UGuoWeXlKjgEHfY6G2vJzdPZqGl3DsQvT0VFqar0zm05mvtyqdMxgsOFB+SBa7bdJxjjKKEEVlKIMlMTpArKJHlGxrYplyLaJr0RkkAVhBSslLJAmUgR4OON5mEZnoAAFgkJzWZuZxfDbrYsw2TWWEvHTEnCICo6ybCXbQzy3WvdJKHxvLk9muWs159c38742la+1U/Xiirp5oen1Re+fsBqdtZslpNAQ+A8IW7XtxNHBY3EPSQa6nAyDzudhBLi3HZ2KWVhF7QWJuSp7aTWMC9rGOb3n3pbudr+7H1kj</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8SZNl2XEm9rn7OffeN8UckVMNWRNqAGogAQIECYJjs0ljd4vsNtNk3Elm+gXa9w/QTitpJ5mpF7K2lrrNZM25xW42CRIogAAKqELNWTlnjG+8wznursV9LzKrtdFaVmeR+eLFy4g89/r5/PPPP7/AF+uL9cX6Yn2xvlhfrC/WF+uL9cX6Yn2xvlhfrC/WF+uL9cX6Yn2xvlhfrP+/L3phh5jIHGaWnFSRDe5Q884pkFeBhGCGZK5Am5Ec/v/xpwPmICLAAbgDhP4LwuMXvvkwgJIBRiioEkQmNTeFdnB4YGKACERE5ARyBwAidyciONyd3N0JzFQMYI5OYeymTh1BvRgQMyX25AS4EznAm59GgKkvFxCCMBEhq6tBmMzc4HAiQr8hg8PBoKe34sHWYLpqIkmzao0J5ubucMsgIgpuGcZEQBGoKOj64fhi1kjgNulqlQ20bDQwtdli4KxeFhQD65Dn7N0sW0IcSlZFCwtwQrtyNzDghAByuBPIAaL+ggBOTEROTuTOQlXkZWsOLwLvjuOwDOZ6ct5NG4ORkwOAwwlCROTqIAdAlze8v4OBUUVOaklRCNTI3W39r0GAgVicGeYgQzmk8Ps/v1OJd0pZc52oSdp0ls0WHY6XujeSa5MojC7TqmtndT5b4GRp2dY/tN8nbBMpDhAc/Yb74OpvPwCYgXgdT8zgyxADiAFDEXE4Yh1gaydcGZfDIE2rqdPmQi17FTiEKOSRiYJIv39zMBHIYQ53Q3K4e1HR9rWy6fIs5ZZybpzONAI710YScAGvyRNAzASASAB3BPe61jsfNVVRFBIMnDptmlYkOpDaloiIACIRcTPNyQyvXNn61a88Oz2ZVeTdqk0w7xo1U7Kc3OEEqAKVsPH1Z/bfeHb72nhwd1ovV81ZkxfnTQM9Pl81KS9XeTgMXbLd3eFoWNw/jKdDb+ZpdWsB4jAkbbumSRZ5tUrzk6w1GCgCF8HNiQTExMGRxd1Q8KCUqztlQfzgtLtxtHPr4amzP3/18OVnDooYUmp+9LP7P/14mt1dTd2zOjOPxzSqQpe8SabJzdzciODGDmem4ZCYBaBRJcs6t0vXbIkAgAkemIceC5CDjPeOQhABRx4G6nIsxMaR88AN9miRk/P+uDyauIPapMLcJgIZAUxr/GGHAy6Ag/or2iPWBrf6QHLAAOmDjCAEB5hA9BjSmFEKiXgsuIwYlmFUkLsKIW6LtsZgVhVmEYpgCgYjFxIwyJ3YzJ01ODt4MOZByWoU4EqgmhgYDHg0kAwIu7gZPDCImdwYBBApuSYBBWI1MzVTFybtWgeByNVZGHDPGYQQggPvH08//Q8/OojVKzcOimwh1wNxjlQqULCzqJupOXFZFi8ebn95b3zjYPTGzX3UqRuGz94/eSD+0/ce3TqdlWApaFKG7UGwbU5DH+zEcjdWk7D6ZElq1f5kwtac1lJYeYWX87w6104tBIql97sZjGPXuJmL8OFW+czR1t6kpDjfGRWn0+Jgd7Q1LMaj8mLetcmLIg4HyCo5I6mORqEquO1sOlcmLwuRwotIOfl0mSmQuzNzTiYCZurRjrODIExGzkJhizN5CCBQIBSKAADWJw0HIQoKpuxSVVR13d4Aw4K7jJah7uam+jmEdHoMZP3ry+/9v3OrA0QbIKQ1RNMTsRjIO8dQLEAAlyghiKoVFVNFQpxb0iarwikLgQByUTK6zNNODguFDHaCqWVTI3cDpUzwclC6oyPProZNeKqDyJ0IDtN6kd3MzLtkmsxMVUGu/W8wkGdjJiJxCCgTnJjqlD+tF5/OFgOmpyfF0Ugk56uTKqlWRKzggl2xvTu6ul089ZUbOBpjELHoirp90YBHs5Pt4dmyaevMREWQFPxevbKDCcGEpZpEPD/K54kccTQIg6pcNcvzJsZ2MLZ6pvVUDSSEID6JPM+elCbDWIR4NtP5qglBXn56d39S3Ho0390eMiirpWRVFcbjwelF7UJkLBKSqgQaRYa7O+rWWg25UzWQO/WJlOBGCtSdZqVxRVulCFMt4AENt4o66ao2YnfzQUIgNRA5vGRyJjgpjMAhxqrQYXRiUqBTz9mTcjJdR4yDCD2nuQy1PnSejCwnuD1+fUnN7IlQu/xwZgQCCYO5UQ9KsQrqQMoEhnusKBSirZG6GRMZ3GAQFneHuBuDXAqwUJctGZzIMlFm9hRKVveW0CnUlZgBNjg5gR3Onq1eqWVrkHMyNzVzApn7Gsnd3aG22RIRelR2hjugteODi/bDKcaBrre+U/DVEeVMwTEuimJUjoJgWmN/iAdz7FSoEw5HB9PVzZt7J7PVIiXLKEd8p2viCMOuO52LTwiwaqfIBUvg9kED83JQFONqq1HnUGTMj2fzi/rRSWvmqUNBoYwoihirQpNPF/XVg617Z6uqCK+9cBilRAxHB1twnc3o+Hx5Ngswg3jXajbA3Twx06BaZ0YzC0wgUjVVc9Bogpx8ujCCD0JYuWuyp69uHx7EquC29XmTk9p03g26FHqCYtafVRKGgMzFiIYxBIIlcnM37wxtRmePObuvMQHeE8U+afpj0PLNJw1wB2OTVR3cxx9tMi+BGOpwJvQEnGzRNgYIUVEKqZOuwzIOhIDUuiVoyoElqRI5ZaK+8DByc1VKbkrqyanxEAVCnSO5p+yWjAUk3p8XcQI0q6TG3UmTWTYH4D3UY82FDWvwI/PLg0UEZ3CGEcwdZI6Lzo/rNIx0dZGe2h5scXH1yt5Te6Otw8kHt6cvXdvBuAIT9oYw3Xl2b/D+o+3tys4XEGvEmpyeHrKfT2VQzOJkVQQo4oDJqTwoSCidd2wmkW++8tS3v3zzynh88vGts/sn//fbd7/37vGk8t1xKSTtqitiUQzC1rh6eLoIka4dbm2PaNlYEJSBtsaDrUkVTxaanJkEAs8KZyd3NDWSqDkJB7DC15cqRvrHv/3MaBju3lt8enf14GG9cmuBqXe+gq20Td60lk1zYxNF6OsUEGDcmgczYdLAMVBRScmW1XI2M2S1lF3zGszWOOQwX7MugIi8vxe8Oe1+mT7pcditaRk9jsT1+wIJiEGiQgwibMitecsUSGKkkoTMYYCZRDdxCEmAJkcH8DqCObKbJ1OFg1iywhwi5to512owN3MQhMjchchdiaTtNLWu6gSn9dGwfsN+SRHgAMyJYQaHs7t5/7vXRw/mUHMATaZbC71bL3aKGK/sfmkwuHnjED9/DbdOMWuxXeJwhDsXEFibM1M25QE96nJVUul2Me2i2OFxnhfD86qgnYJaZQDwwdFwUo0926Nbx+/zyF+f0LPPf+XNV976Lf2b73zwb//oh3dunx7s0KAM5rkKYX9czGZ8Oq+fv7rjQBU5a25aS9kOdkaDatalBCZV5eAEsuzm5K5JiaU/XSA4BwL5c8+Mrl8djId8/ah668tYNvnkvL17uurqzEaz2hap7VrrVjqpgqvLN58pIjG5EzwQMdgcFqvkNIoeTLP6srV5m+eNnS+tTvANYtElOaPPZU964s1NQQzQOlEKgwjc55xNsBIggqLAYMijSkYcms44e1AEgISye4bVpkqQKBKFmJmJmJwyCYXI5SSGgsoRV5Pg5HWyjt1BYWXeuAyDlLKEJ1MDHMy02YqBnYiwmOX5uZHDzPpN9KD7BIaTg5h7hCOA4TAi2hTgPe6p9VeJiLzfdaP+4b2z//j+w+9/cuKfXWx12WdNacAiYadE3R1W8e/efXCa06IwJdofg6ZdB4vjWMBpuqrqjhFaJxiVg+pga3cynhxcP+IY73x6fj5P7/3w1vHSmtHorV9+9Xd+743R7tYP331YL2phjMeFGZ0tu/Eg3DjcUqcYWbO3WU0hjEdni3mTvecFRAQ2okJEBAQWgZsTkRuIiRmvP7+7vxXgFAIXkSdDubI/uHlt/NTRaHsSKLJH5ABEDh0Nkwd2duuJsDkscnAJiHEgXponyy1ZC20UnSLpJj86iD9HzrDBJ/p8xuy/sE3wgdDLPOvQ3EhnRBBBEAqRIhOIW+9YaURhi8IoswmmrlPKHeksK5OUwoWIFI4O1nliA1I5CLEgZ2Sj7JoJpM6ZibQYhPWvduqFlP6AuqMn94GpXhlA5v2fjzcBAM7eE8s14yTA4GREZGRwwF3JyR1km6P1uFACO2xRd3/+w8/+3Y9vMyFGPtwajoR+4SvXtpKOjoZ/+fFDq0Attkc0MltcJLkSItyUcp3Lwq7U86UHnkxk77BVGY93m2V37eCIaj586uDmV57+6Me3Tr9zcfvjB698+drv/+G3fvs/+/k/+79+9K/+97+rjxdN60ZcFOGZ/erD41TEYOokQdVU0/ZkMF2mplMY1DRDCFAYzJnYYb1s6WLCNK7CNnh1nHzsvk2x8uEwFJFFvCp4dzteuzI6nncfHS9+dn9WioYmy7dfHBSRs8PcDAQhKWIcDpgptV1KXavemLXJFp3Na8+6znrreLtkYxtI88s3fSOtbUSQze0FMXCpsREYkIBYoCy4GvB2GXeE92I4DGFXZBu87bKLcOR8RGGX2AktcuuazDsiBJGCg5CqdsklEAt3pvOcjUwSsFBnG0zKXruo1Zl8IxpTXzqBkdXOj5MmXZ8f6qkjAeT0BOF8XL70gqivJTJzJ2SHar+ptZh8eXHcneBE7HAHZbV53Z6t2h9/evaDOxfvfXactF012jXp6T0qF9pli7scK9FpyplvHBX/8IVBqOtfuk7f3I5bg51TjVSEAtHUz88uBqPxUy/e+OzWg/F4cn66+OyTR+Od8a/9g9d+63d/bvvqwQcfHj+4expD+PaXj1aZDKRqarZqLWetm7ysU5fdHQ4n7zUzuJO5Wk+ZAWIiwtXt8nAUoQB53WrXZjMPgZmImAgUhMaVDAehYe86l5NGvv38UAIx9Vo7K3msBh6LyLRaLUxzNmqyNp0vu7xooOs6gC7/6i/ik1XmY4h7YvEGt9ahRo8/yAxmVAWioKzkoAw3nHdBY+LKqADDndwZ2GY5CnJgYUu5AmdGh9xqajUrk4uwkIhQoM50lTMI0nJapjjgYlzAoe6NGkBMbut4ABGcuG19dpKQ100CONzJqedqfSPgsVjj1EPhpQDI7q6AKri/Oj09uIRs3mA+rZPrhjOQMG0NaWcAZpD70S7dGEt3kTDEaKcMQer7bTXk/+ZX9l+YxEWXbu6XN54rDx49tItZbunmU0fT1kaj8t6dh/Dw/CvPvPeTj7s61Z3ev33+6cfHw2Hx5tdufuNbL199+vrBwd61g63tihZNDgXP65zVzZFVl23XNNm873tYH1V9y2RT18HgDAwjj6ooQ9ZAReAqhqqQInIQJhI1JSOQsKEzO7to7VEbei3EYGCou5q7hKw+rETcDayeTT2b5QzblFxMmxrsiepy0x/YQF2vejiMHgPB+vpeZti+VQIERik0jCgUQ6OKqQC7m4HMPZAbUIiUgUE+EBx52FV71rEge0h6jHaZkzsF4sQqbehyVjJytlqz6rAcEEPNxACFGVh6hLEemOCeu4Ts3m/O7fKo9Ap0n2DNQEzuvm5x9HWOEfHjILuMqssyfN0JostsCiLvw1bEb14bfPXF3Vv3z8/n3eho+OwuwrJJZONxfOmw3Db8tdmbz46vvHWof3N3ZxQP94a4un3nbx5uYfYLdvq6LoIfPCgng6cPb9++1yyWX/2l1z/78Pbs5KINxcnp/O3vfkQBN1++8sILz/zB73xjZzyc3bnzyr379+6f/eSDR/N5M1t1Tdttj6vZMpt5JofJZenjcCKTHt3dQeg0d4VrpMA0iDwspABr4+rGJZkhmwo73EP2lLI6BQyL1OXOegoIZh5UBUQ8p9yXU05mntVN13H2OVrMm67lhsz0Gmz/Jq91gMurC36iofkk8hGBmaqInQhxb8kDmTgFWmNhFagU7k+aE3FAZATFwPhqiA2XZ6z3tD1x1Ekpa04uBRGck3ngcsgwiIEcI8Y8WTInBhH608fEnt0J7raOjzX7pL6PuT5IQK9nPGZgIMD7vvDlXrBmBT0cPgayDTUF9x0R4UFBT+0XeyPZfnpbmergW90y11ZU8upTgz/41gFm+ukHF3/wm09jP0qhYynw8zcwNffMIq+/toPZxfjB7asp/srNpz64svturWef3js42CmKYjZdLM5mq27VTRfnf3Xng79/792//unVoyuvvPD0K196/pvf+rlvLlbHjy6aRf3ue7c/+uD2n/3Vz27f7dQom2tPON0FBrD1TECoZHDJLVvK5oWwCJiZiQ1draTu5OZkokQEpVhyLkz+ye8+EwtJTWdmas5STHa2QN62aTWfJ7WcrclWtzZrvG43GdA3LO0JYeLJ7rivWfIG6vpv9XlzUz0wb8Q2QhExqGhYUCgpMS3cs5u5CXMAyhAGEQSYQ4h6PaLPS0Yw9ZJoT8L1sni6LEZOyamFGXtIpCuzSFyFzMSB3I3UAogdtO6EWL+TZqGpttbocVQRzNdfXnZBLl+vwcrcAXWoYR1AT5wrwtpGwAQJXFZhazLY2xuWZVDNQphMOFE+nrfnrXYpXx1Zsey0seFO+Ke/uF/+w+fxwfn17cHkn76EOye4O9+6toMvX8GffLDUvL1dbd3cfvTeSUvYHtCXrvvi048PFo+eteWLlN5/0JxfzFf1LOWVQg3wZT67e/HR+5/96Cef/O3bdz74ZBGHgxdfur5986UX3nj9F379537vt19/+dXrRcl13VrOrknViYmJnBCEiECGYkgs3CUbVLEogppOl+l8mZqkOZsmM4epm2GxSp8+WvpM5Q//wTOHV8aT7VHbZmu0Gg25KIdlXC7r1CWAW7U2+bLzReOdXp7UJ8BoI70Sb9LEJrguT/b6NBN4c4Nog4o9PxuUNBpQNZCKKQqI0LjO1BemwjQpRYSEADAxaG0CISJyUKfWg6gI7UyG++5XKJylPCcta2pbhTuStU0yIS6ExFmtYqmIR0IlyB1ZdTZXXbowKZB9rfytRVpb0wC/zIa+gTRHdqivgwx4YuP97oSqivf2x1cOJru7Wwc7o61xtb1VFoWU0SZbIZnPs120ejTy33uxiJ3Olvm1l8avffs6ntvDDz6b/OZL2CZ8dIZZi199AQXje7fOFM/+2pcwXdQPZ0vQV968hkU6n66c2t2B18fnP3vnA9x/MElzaVIkE6YqhyCczLN617Ynx/NPbq9uP1xoswiSA9twb/v5V57+5W+89NWvPXdwZSyRq0qqkotIg0iV4Hyqal5EGkWuQihKGpQ8X6S60zKyOVadtp12nakidbmp9f6qja2G3aIcV8XRaHS4PXj7R/cGUpSDooqSu2Ru1lMJkLplW1/WDTF+DGZrscMex9/l8stUu5HT+EkgdIAQGLEXNZhCIGHpaxslXmV7pF3XYhx4S8KQrXIWIepvM5O4MyGbQxE7rc9rIRNHjUzm0iGbV0KDJjfJdJ6boWDEFCRAxZncKqLAUhGfs54rBE6OAGSGOik5XYYasOGlj70yWztY1miax0eINwxBAqoyjiflsIqDqoxBokiIZGpELmSxABO2RhUXXK/aP3yz+sXfPfrw39w5mcs3XhriSwf46SNwwLMTPDrHRY0rO3jlCu4eo9QXrl/Dmwf44wdlSROPeP3I/tVPFPRohVsrfnhrmloNAaZtzM14WGDuk2IYOT4iW6FojXI3P7l/78cpr1bd2bQ5PNoZDJiJHBju7n/9668y0zs//nixaHt7j2R9uk7HZ83x6cV8nkcSmqV2w9wqAuNi0VlfEMElcBkEhFWbU9IwoDCqylEZA9P2oEhfpjv3ViEIw8VyEUPynMw7dTW3/kLzht1jTb94w3b7GLJNj6bvAV3iXp8fewMZXxqaCE4QRhQumEtGQRwZTMTOACmhMz3NdmY6DLYLmQQZM1dCRGACCYmSmiez3lABoWnWqXvJBWnuzF8aDb40qI7r9v6ymS00z1VD1gHzSCRIJVwYbxXhykt7f754sFgk996BB+vJv6w3YZ9XxIiI4FvjsKwzAOdNocMoB3E0Gg1LLstQRZZAIiwglvXRSp0b6fWrw2vbYtkXys8ehl/85QPc3Nqt8OzVavtL+zia4F++j69cQVPDCF2Hrz4PbbFaoAj4padRGSqpM26+vI9le/tscZL49szq1Wp6vjRxHhTz0yZsBQExU4kcUtpRH+kiuXBZRW6XF7j1MZtTm/3KwRDEKaflsrk4Xyw7ajs+PV0RMTMRQcri6lODMIknx9PxsgvA3UZDKepGRLGIYDCZCK8oM/Mip9y6Bw6Ppjkr94X5OBSHu8RAu2wmRJUwEdU9nimZO23KQ+/DiyBPeM8u0atHu74UcFtHGG1u0uMXG7U2CkYRW5F3mAciQSDMjH5rqLMu1bOjVZszJ9V5toKxJRIZkRhMfY81G4SQFQ86zc7boFaVia4Oyu0qTMrw1KQ6r/OdRXdc1+3UfKW5lOUojMbltWv7Lz+1f++s/d47jxjIAAkFct80Z2E9UPV7gwEF+XjIubXUPsFZGRJijEXfgxLmEEWYhAGnrNqqM1lVOEWZbIfxThyI13eb37xZ4qtXcTw/Xtqbz4/x9adwe/nBg/ql//oI9QqPGowmeHYX0znmCbsT3BjCGjTNIuMojvFwNU3+YJ5OV9ScTpvO4kQMpo1XByyNi3kgWrWJmOAWzAe+nLTtdnexWJ2ezqars6MHN/bG28OqlFElO3vbpVizWDx6eLFa5d7WyZyalBerFooHq1wQ0aJ1dyqEBeREwlxwDOxOg4HUcOsUFYWLWTe/qM2UHVnt+tUtJiKzo2HMFgYhkHVt6+dE3hdaly3Lz+dB37CTx6bZTad8rWLwpobYxGUfZOv8Emhchp1BGAcOQQggQXAWQkZcdPki6TR1yWnoYUgg0NJg6jmnSE4Ocx+IwCDk97rWQ66ynKuNKqqAVVJ3GHxUyPPb5eFAzpp81qa6ztRo1eWDw3R1INujUhnkCAEOd0VmsMMIziCCmxNgGUyIBVh8Vm/qUlp3V808KUriIFFCIIIwMXOXkprtTgZVEdgXMVTe+vnUVgOSnL/22h52S/zHOyctXnltD3tj/Iu3X/radUTgQcZHx3jjBjSjdnwwwyvXMRZkx6q5W5dPHedi3E1bfdRY29BildlZJrx4lENFoRSufa1jZ5UQ+n5spLDqNHkd+e62Hu/h4IX47P742Tw+vHB+tPBVR4NBxRLcO4erITW5blt1V/WU/LNpPhhgIECnydG347DiTjgEFtNINGmNOgqzi9UwOLmX4hKLi4uurOTh2Sqt8nAQComj6CNJAyZswOwywnpkc1+7NmzDfH3DvXr888t7wJsi4FIQwPrNldt5zt55Cxk7BlFG4KqQgjgEPqiKWdIHq/BgWZ+nNIcMJOyVYbeITnrSdE3Kqwx4d1CGrcCndeJhlGyN+36I0V3NAgvDlRBAkzKWInuDYp7ynXnN6tO7D/7u5PTep81hJSlrMrQGE2bY2gPZdwUYri4RMLQJ2XztDOrVpt5G4LlrfJZT0666NNzdrspQFJG3RuPtSdl2dvfu8Wp61qmXlRRRJPB/9UbAzx1h2s5+Onvq6gg/fwO3z3/88fT1/+JVPDzD3z1Aynj5EA9P8eNzPFzhWwc4mSJnnNvPHjn5PKD5bEXnjbSrlBWDMXumtNRiN5CTu0dmS3257u4omIjQdLkxHhRaOVU+Xdx6Z9TeLz/hF/YOXts+aIejv96u/lY4JVV1AF1KUIMrlECo1W7PaSCYFKjYAzuRECxnWFZP2BmVVaLlogs/+/CT65OSmW5sDV558VodYqO0WLWzVZsXTTbvEmat1tl0Q7aIeg/RmrKseT3hcRA9bks9Lj+dnwjNTe3pgAhilN6H0bpPk14k5RqFeBApOVTMBdNuFZ/bGgj5rVlTQ7vsS9PTpHtlOR6Ws4UtUqfq01rHLEMOZfJlZyvFtSIOhDt1kDOTkGdnYlchNwdhlvn2ab41s5Kb3CJlZKPk7gIGGRMRsbmj76Gv06P27nd47+hwI+JLrZrBEspqa6va3652t8q9STkeRTecnC/nyxVZdiU3NLVVg6Iq/B+9NsFrR/june991v7Grx3g2gT/y7uv/+IN7Jf4/sX9T6bXfvkpjCI+OX/4vQe2vXftkxp0hjuz795J5+f2zuqi7ZbtwDUjN4mCFyNpZ8kFYcRSSkyILMsuObuD3CES4L7qSOFVwSy8qNuaqD5dTmfLrcHJiwfF3qjQW6vh+cW+USc8S2ZmTutGrzCZuzm1pqtVrwV4hA6EBgGDCFM8aGpTAxA6xWmThiGcJP/K83thEJlleuveJys5WaaLppnVdrrQ05VfVo7uIF5bHJlA9jhXriXZ9S14ImP6BsMuI2+jbkRBERCJAjujFyzY3OsMzwa0PZbcWjUDCY2ZMpGxwVvTrrXztmMHSJ3BxFV/s5XbrMvsR0XYjVGYK3FzWmXtVDvDKtky2SylZfaV2rT1i4YKQdkPcTCiUyBkd3bSdf2yUZ0DwTzAzcWzVSWlrKknpRuTGufcLOeP2ibnsQiXkduU25R3RtWNg9HD2/cWF2uTaFXJr762P/n6ASTghxejrYg3rmKVf/qT09f++6/jwQXemcog4vVrmK7ww+lHUz2f029878HAp7dPz79z17rOTtNCOVsW7VQzxQkzsSXECjKKkRErRudNslAGUwc5sSf1bBYLirHMGRcpi7Cu2ot5s2xQ19Jk3DpZUZP3CIH5RPPSQuvUwBvz5L29E04UmPqyqXN0yWbZY4NJgSqIsEhBITRubAvLV6pB7dgTlqyvbFVlyu/m1cUqLZtuVqPJjykI1iaHTbg8McK0ETM2uLXxAvXjJ76h0Y97AIQioBSvhAKziAAOz8RExr2i7k4Oyu6rnB3oba19z7MXV5yMXQJ5Jm9BZgYCm8SQI/CwbZNrJVIInzT5ZNU2ZgwSJiEZFxSYA+hspXTnb+0AACAASURBVI0iswvzAKpOSSHkeR1j5NBN7jQIwz0QOXObrbcA2oZ4msHY2ECuXZcvpsumqXfGg+1JOagKW9WVJQi5wwwnF7l48xv49reBT//6x3/zlecqvHaIv77/2sv7uDrGX9z57kezr71xhKMtfOfDP33n4ox5sZz+bcJytbwQnS48m2ZLMiY35Dab6HhU5VnnDCkgZJRNIG2jSrlk1qxEHhhNo0VBZclEaJJql8Kg8LpZdJ05wf18ledNCoGicNNp7ixaFxwTpg7cuTsjW1ZwZ6Rk2dhgTuRuHfy4YaZ0bbf89beeDv/ohauDQn42Wx7ulKOyuHfeyDLBeBDiflncp6ZufdGuhUp6rIN/rhmAJ79FsF5e6uX+PpFsPI++kWr7f1cIboyKyQgUJAhk7Rpid+sLWiY2IpD3Nh52KoiTmIPYCAQxVBILokVWdTMnJ2IYibF5yvho0X2KLgofVbGEB+GxUPY+E5KwDSM9M4n7lUwbm7aWAYIsE3j9v4f2pSNTb/LgvkFHcBgxBcBNQJo2F4AZLHCHZtXcbm/tv/zszu6kBGExX3Unx4MAKciVPNr2M1dvfOkZ4OfuvTv97rz4pde2UMZbf3H32f/2DeQO70xnxjQ5xMMO3z99sPILcp/P35mZFViWlDvKIDe4RGusaywOCzZp6w6RQlWQB3anxHXTUowM6szLGAikRkWkGIK7d53lDFVHk7uMwJSzrjozcAxMsGVramAwB0SBZo0MOBXM7JYJxpRNiQmwzknJFVZW4T//jZf/u3/2anjrxs7eKF6bDn9q9uNb0+miOei6Otlprfdm7Z1p82hBuadm9lg6eizo+xNMfwNmfPmtS7TbKGeXZUT/5zjyi3vDF44GHehBUy81JzWDgdjdmKkvHpx6IcWcic2jw+AsFIjJPTtmqkoGBFojLRuRwBFgakows3urVLK501B4JCiFuXciEgu5uacxdZ13qo3i/YtunonWeqwr+mHRXjJjoo0LnQBGUaDOoAQQWMAOEBeR4FrX7Ue3HgSh529sqer52cVeThEyHoZV9nKreO4rz37zrWeBs//5f/vLZ159Bb/zFn72bk2MZ4/wye2/eXd2juKT0+K5f//gX3/3fMncrjw3XZs9FJK6YGZZIQW7UlenrDoaFLZKRkQhSGDKEJC3uclalNyz4jIA5uYs4u5QRVJtOw+l56yqaDol4o1BCrNa29Rv3sqCe++KMNQQ+yHaHlOYAnl/twJwdHX7xvW9lB1XJ0GBMsqb17aeCzJ3PwaalT6Y1R+drN6+N/3oNDcZgicG5jZA9bgZsGkJ9NaMJ7tSn0uml8G3GfB0wt6Ar02KL+2Pr21Xp233g4ez26u6zZoNZv30Ry/lwtzInNgLChIBWFJ0rp0RHHZJ//pepEHEnUDkHKiX8pU8ExOwMF9qjoRxkEkhUYgIpUshPgxQo+w+G5b13VYNDgQQ3BTUmzvMNx4f7nUOZkIsJCXtr28IoH7WUZiZNKfb986v7lVVRXdPz4YjjkajIpoljsPnX3xq9/A5rO48ePjoS299A/Sr/+effvz7r1wDFO9ffHSRp5F/8JPzH6bph6cdhpJbrVvVCBOh1vsRXSmCJk2NhpILRtNkCAkZh8CtFhIWbQKTCJO7MAlz13kmBzxAc7bU2Spj7MjmWVWzsyhA5rRsc5fMHESQQCKUWhMhZGemIK4ZIlD1QBSYUvJQxa+/9ezRweDvf3b8znur/+l//Nvwl5+e/vrze8/vDMem7bILtR4vug9PVm/fOf/gNHdpU072lh9/jEa4nD35vJnsUrOwDfL1fZgnlbb+A4GwN4gHw/JwXN3cHrwx3n7r6tZffPzox8eLaaeZKcPd+4AzcYWE6AC8MwOQiRzM/aw5EzmIHDDLZORCTMLkMLJe0nf3DETqGxKU4OdZ59nGkYciUTxwn3G5iT6pZGemF7MMeDYw2DaNp8vpejj3+3SmGEmi5gRVABAx7lMpGYgO98fjUfno4iEmed4VwWypltRuPn/9jVefBnb+5C/+aPvKzqvPX2tPb/3Jj2791u++PD4L7QddzWim6f7s0cV0Ue6ENllOaAxSRYaAPJuxkLNok1LC1m7wTs3gpYg4uwuzqa8aDUNmYnYiIjdqshpbECGlrNp0mYvNiINTl7wAg7DsVNVViZmIvIjUD2T3sSBMcHdihntAVTKMjq7vf+trT+9tVR/fnxHL+dnqL7//MLxz/3TRtm9e33lhb9wkuzddfXQ8/8Hdi/eOU5s31SVt+NZGpPXP94wfBxzWH8NmbG496fSk3oF1AyoyDobF4SheKcPWMGJS7u4O/9lW9ead6X+4ffbZoqlV1eABDHEUKefOXB3SO3oYadNRNV1bDgkkguzEjiqwMK0yJdaNpkcKBCY3kBPIktl5soWiYB8ElEQSuI4chG7uFO8s1NVlPdJF61/i7GSgHtad+o4+a1myqfV1ABGJUO/flsAn56uL6XJxOrsxKQ7G0s11MixKpRvPXf3mW88C7V99572dw4OXnjr8/g8+aVj/1w93f3+89ac/+s6ygzc+s0VnmSlqg6bLyhxKhrKRqVoxCq7etcoFF6HI89YCw5wEZF6ypCYltVIiOamDQV22VZdkFMRJzVKnWb2ogrvD3cxTdgpInTm8itx1RoAECswpqxv1g2nCbsoOlRi290Y3n9p79fmjrUF592T1Z9+7fTytk3E2k7oNBLozXd1bNfujwdFwOK+7H9+f/uRR2+aNh3GTHOk/AbCeq9kmjW7aTWtPNm0GMeyJ0hSPsRCEQaSdQbFVFYNCEAXCCIKd4YvbwxevTb77yenbD6fndWplbbLOkSs1VcDRzxhl9s4ssyubK8zXIc1OBflAuGAMRE5rTUaAmgdiJDMCh/6/zASHwmr3uoMTnpFiOCqIqRpA98ufnDQOj76mDuZO7CDqDZi8ZgkG4hCsF8R7HkMkzAz0Tvs21cuYmuV9bO0PLtyLvfjc4faNG0fF5Drw6YPzixcOrleh+tu332fPH7z74f/wHrWz+jCFIdKy0TgUTVDVTl0GwiSklM0JxEK509TkwXYpSl0GhJCzFKWwBPNZY9TLwU5mKTC3SRVeMGDepdy2TjHEwOLM5illNVFDCDQMZdfojFzYAgciN10/3iQEgrsz8SAOi+qNV5954cb2Ytn+1Xu37zy4mC3rzh3EZZCjAw6/+PTBJxeL+7PmnenFsjtf5XT3Quct/PPmi8t42vD9DbJdfsbW79FmOGDDCD+3nviRMGDaZSfariKqAGa4IwpGBarwC5Pq9QeTf3/r5N3T1Tyl5AhCQZgCmburunPpVrFkNfR33HqPomciQNjVHZOAYlTUOWeV7NZXGdab9cFwX89HAwbOTrfr7jqXW0VM3D4zCfcWcrZShQUCESlc++zpIIKBuTckq4EoRkqJuBc/zEHEZG48KFmbOjVUG91ZdSsl+2h69bXD6wd7QPGv/8Vfqns383/zR+9+74P3q+TT2d12PgtXsVwNx2Sw+UF0ay0pm3s5cDJ39lx7KMgNms0dgxHQqDOcPAqDObpb1jYpD8XZI7xN3psLqZR+ti0l7zord5mIBVC1nI0EIUrJQu6zZA5n5iBuqqpCpMKI4m3nw2Foo9y4ee1s1d363q3cLLour+qW1KJBxXe3OQnCf/nLNx8cL//4Z4/+5s75g+Xy9oXOm02QbYLksnFEm2exYO2NXysal5NBfd/JNvMba+l/E52X7VHy9cM17i2X379/8dLh6KkwxiCAGOxIiigYV9ULxW9fnXzz0eI7H5/89HRx0Zq5IlBvvWMnhQQYs7gaM/XjEwY2W49TmFB2L4WrUNh6Ws5VmcjMYRC4uYPhRAxHdj/t7P5FG67Kgnno+fndctau3NbIRcRuru7eD7FzP/7U8wWPhav5Wmwm65U/Yo8xN65LUIq+dzQ6HEeHbF3dPdweY/npv/3zH2TY+e2zf/ne+zJJdoZuWWts2WJQOc9mg0ExwqhZtdp5wVEIBnX3nGUoqtSutBxxsKCqHMg7DyMBKDi3XVYDqYqL9R1h0iZ5MY4BpDk3bXYmigIYOZpW1SgOJIgIqEt51SkxhC2wZAWTgcBCMLihdhzs73Q5zafdxfGFBE2E1m0AKtmKUZxsD2on+ed/8OqYaVzFprMPjxd3Zmr6WI8g3tSPl4Pml6rsZeVIj9XXtYjWM7O1/LSZvXhixpMIJBgWNKrY2KdtfjrKeGeIcQGm3oyGIIiEqii3Bi8cbX11VC5TmrY5q/dPN2Dqy1AQY/0UonVmp+zo1JzYgfXzXQDrm+C9vwMEInEQszBYiEExSCFUCU9rtUq2tkoyj+ogv2j6uQwmYiYyJ9vMSa8pA/XzLAzAFNRLJiBmBMHBfkme60apjAdXq+2tohyG3atPP33l6r/747c//OwzaX01X83pdEjQuWvb2hbFjsmoaVvZLWrEi1SeJVQjHsKJ0LXGbKGIKdtqods7pYByhxzImxy3Y3CpnC/muUsaB1xK0GSq3rXamA9GRQla1d1q5VxSMYxCQhmLVVaiYiBFEDJf1LnOFAqqYhwE7hKyQwoKHCypiuwc7mdLs/PZ7GLBquZWQ+AQxX6Bsgh151k1IDCYF4bOve76Ce7Hjown+5W+cV375TtYo9eT9WZv3lqHna8pP9ZC1MbW7H0ngJypVftsUf8fHzz4dptfe/kqdsvHSMgBnhEF24M4iP/4yuSrn57++a3Tu8u27RNkP5quxsRwcu7nwJzYzNBlC4ECkwiB2VWzuxAZbK0bExGb9YKbUF5bX+RKpEf3lu1+dbBXxGG4XvFccTxN/X5CYDf3lK3fvQnY3U0AMEuAGYHAmwe0sUgRkVaW3Xa3Y2P22cN6VPL59O8/+ft7s4vT0ZXIK5y1Z8NrgebKCjWVoghTdGZEHobBL2yhviKu9rZ42VZtB2vKSsy5aTILQmTv4JGsNSmIEMSQktV1ppJDIeSeczbVugVXFEBdsqZVmEsV+h5uSp4VXACByC1rrjtjkWEVKvaUtFWEgoPAsyu43B4u0iota2udIwvDMpWeVZ0I5eEIo6I+71YXnfzzX3l2umo/Pl69fef87TvLy/4SNs+NWjP3/2Ra6bLMfIKA9THX02Lf8DcmrIdPNg9L64GwEIyHPB7IoIyFSHK9M23qi9VzZYFSensN4GBZp24mjMvJla0394dHRNOs806zoc2uTuogYu29YgQ1EHF2N4IHYXcC+gdYmTuDiIR6gxtAJMwAOxGDBcLCGBI183TvrE2Cvf3B1f3hZ49WORs7iJmjkPcNgUvx2QHynpAS97OwBDDR1kj2JmG5sqS+fzQooxREJ+fd9OHq5M5D3eJxWXqDBdrJKMQZedJcaSEiHeekNGRitobmXYqVFaNi0YUll00Zw//D1Zs0yZod2WHH/d77jTHm+OZXM2pCVxWABtAgxG6CbEkURCO5oZkWNBllJi5kNJN+gpZaaSWt9QNkJpoGE9kttlqkuhtUN6YuFFCouV69KefMmL7p3uuuxRcRmdW5eJYv8nvxIiL983v8+PHjWSoBs1mbD0yZOI0khrpFlxbEzqaK1aqrO7Elpc5RRPQxBKpbnw6S1Lq6abpGlTgtjbHGKq2q0AU1OVlHRqmtteo0SU2RMku8WkQhuNQA0CjRGc24WjTaCQtbljG0J8qNKiy7qMtF7KoQ22D+q/f2T6+a3xxd/fkX519chmvmgcD6NdMybLiMbc3I19OJXwf42/y3CdbtcbkN38zSuOBB6orEpAmTklc5rdvTi+p1YqQWKusn4k3mZIIxGGe7O+V7u+Wt1C3qWAVpo/SNT+Ketu9PLDAxO0MUe1U3bySWxARSQ2QMc+9jw0zMWCt8BIBNbUZIla6u/OnpSn30jay6GKXvR20Qa1SijaZOe5WUbhoFAMiQTobWGFouo0lod+AaL+pREIc2VF0YJORraTpxE1MIu5bbptGRSxsmNb5teOq4UR+16nw5dpYNggpiLNPKJWchOWtltDs2SkIauyidpCMmsIs8W0YxlJTWgWKnIto0EoiLoaWAug7Bg4y60jhD6uNyFYTgSuPYUoe6iYE4zckaaSqpWjUps2MIgodPuPWitRjR3JiJRWHZKEGEiT2DYu8TgJha++llVbXx0WXz5UWrW8SxofV5c3TSumV93UqnDcFxfc7ia99TXzHcCM3tIWwJr0yTb+wNkoyE18O2QbDy8YPL5cn74Qdnq7f3BihS5BYOSBjWwBhQhCHkKZz9xnTwjfvTs6PFv/r87P3LVRSIRF4L3MFqrFUBRMkYVtKocH38qUKJjTKUiaVneEmjkLKqMpEgKhMGmblfOoKcL70p7VUlrSHjDLEiQg1D1ffOE4AaGICYYmSGaoSCUoei4LbzXsNOliTWxJLKxNZLXx+3nNg0MW1Xr6rl7bv7dgmoRoKBUtCokQwREYK2EplhnZVaGIgJG4fY6rzyVOYLl80kSRLV1WowMJmVNHDjpRZKChhm9VAgRnQBtiRL3HS+x0jGqJKSUNOqD2pyNoasaoyhC8LOsIV0WrdKhpKMhVRiRGJM4TKWxkfb0dCgRy25oQC2oMjK0yIEsZ2gEfvxebNq/G9P5pfNJjdt4fqNMnMLx26SYduicvulG2RFvUZjG2Sbi/uAKyze3Bn+4cvTNw/LQWpO6u6D8+WnV/Ws0y7K42X1P39a/2+fm8wmZWpHafJgkLw6KQ6GCUqHzCB3sITE4WC0dzD4p7vD/+EvPvty0agyBGQMaNNWVfToCcwMIUXCzH1fHNwP9jFAa5daeO2pbupb5aXh/dxljIPMnazCVRcfzaNhsHXWSBAbbOQgbYj97JNS36PQXuOuIrd28zQzF1c+EF0uvEiVJrZJfCux6mi0Z4c76SgkeLqKlz4qhwCfUunBoOADBsZ4KHHruzQxDIJIILKJJYGItm04OMjFSydQw/PIq8Nxl7vpIs5WzTHLrUJzFiAQpPcWzlOnEV235qXIsDFEAU0bopC1TASOUrUalDIHEu7a6APZDDZBF9iH2Iik6sshIWMDTQgWFFSU0AIJgWFsG3wAL6PpxH5wsrhaNr85a8KmHb7W8+j6wKJNHqLtrPlGebGlPhibhpJey2O2wUXb8N1UDKOEDwbusEz2d0rslw8L97DtMGvPjmY/PV5+fFVftr4NfhW644ZF6edHmlgu2QwTd1hk39gp3rkzwl6BzIAMbg3/xbsP/vufPTqqGoC470NxTz0oYMAS121QiLJlIbOdc+idZgElS5AowhAiJTjm3dSmzhAkJXtvSLkp5/XiZNkpeSIIlNgYgu2xIBRABIihAiakCe7cLZ5eVG0kgc4rPZ23oNZApyMTPM5Ou/kiZMZkTTi/nJ1O7CTLkp3Etj0nLCa11CIAUEmzhAOCwhSwliVK1YixJklsaFWMhi5EBjvTdOZU7UkXukQviiTCphTQtmeh4gJjx13bdZFYASuUWAZ3bWg7KKtJYBTRow0AqTFGvdRdVLCxDDISWURYZOh1OAdHdI5UkBF1wkvRilF5BaScRe7UC1TVJOg+PavOao030hJtKgCir+WkNTAjgNatJL0RUv336x4Nr6EY36BCerEgEe6W7ju3R28elMOdHAOH3CFLMc6Kg/KVu5Pv7ZdvDdLcGB+ljar92Cli67Houud188H57C+ezo6er3bqMBTAEKb5Oy55/3TRaUxAhoiUjCEDGAaEzCYv+xgZMIYYPZTf0DVMTNTPa4lCGVNnppnpB5IBiK4Nv5+uogckSIyIUaBQEY1CuraBWN+eRA/vFtNd9+Sibr3cKrNBYk6ufCByVlPHCr29l04n+WLecocq+DbEJsTpNHMdqcZglFLjgqlihEpRWg0QVpsbANHzxawZj9LUchQGU6i8ZJznNg1UzburlXc555mxytHYo0qfV2r3c8oGFxUuJG/YmVSSlCigraXuos04KYwVtFWoGqHEJJbb2rdemTQpGWzmsxhUCqaR5QDpRFJQS8JsUqNaOpfbxsfaa6JqFF2MdSem83HVAb1J7Tr5/03kvjZt3Dy+1ZD1FxFuILYbMrU1Z7a1BuL1qWoIL0/S79+fvH1Ymp0cZQLHYIYhWIvUYZSV+4MX745+9+7oB9NymLD3aDuJvaNfFFW0IRzXzfun8/efzU+OVsnCO8uLVo9XjYItwRhIVGfYKpQZAPfkMDQokRpr+kRMZIg3rtv9YapAaczUcWK4jzAFRQFUhqld+rgii95lQ0BMIohKiBAhWbtTKxGaNl51oSOKQUepXTbhaiUpUVmQKPLSUYZlE3QZ4CUtzav3x7nj+XlVVzFI5KGxSoBtQ3CWXGkRhRKwM+TReF3V3c5ObsEhKqk0q5hNXULkorucdV1UV/A4cY6t78LZVRNIdqd51+jRUoh4SVqXuckSeF00plLOBpQao21YVugk5pnRSE0TFWQtmYwAoY4zpilzzhIUM0ZTOpTmUrVVXTizt1PcOSxdbkOrvo2XbexUbJS1jII2pix0A4ptKVnZyPm3FNr20NRNS2rjbLLheDeZrCfLsZFuM2M3d8PEuF6ynThYA8do+84lYAzYIDEYpMnh+Aev7vxg3snx4i+ezt4/Xx3XnY8kECg1EcdVfVLVPz25zKwDtIsaVSxpCmMNsxKILNQb7g1te1VHF4UICRNT76SnAmEyTABRzhg6m7u+p0QaSSQCKkSp0W9M05MQykHZBqnqrqujaJQoAggpMdgQkWrEstbuxN+65eJ+uoqRFAd3rEZFVN9CVAwlVdvZVltVK/TsZDkoXFd3TdtqQnu7Ozm4d061CRgUHHOiLFDlzoc0c5aJAphIgigjdcZE03XSdoGt5olhsKrOq9h6dQPHxPO6I6gSi2FmrmEuheYhRLYYZkYjVquFRueMCLo2VGpSUnZgw00dWi8ja9J+2IqhY1dOktBGLzKr1VXdF4uYjZJyYOqUrs6jMJGQ3cZKHxb96dIPAzNvjbvA24JA1/ijjy1ZJ4l1CK5nOTf5bDuivQ0ybGXQzL2zHvotGEHBG5sKBpgRARAsIy0xKPhg+MNX9n+4qLuj1Z8/nf312eKyDVFElHuNQSU+kESgkUAwbYyOkVhrCMZIAu4InSBENapM5KOyku0LOgExqxKxGuHUorRk1nY0zCxKrCqGoESjjNG2SOx4kI2Gaetj3YSq6VofQpA1NBOIAZFCuFzIQWq7SZEVpm1xedk8OqpiIN9J18SSTYfggWJgjTMk2o9RNZX6J1dtURRJAlKXOiY1GYHZNKqG2iYOh44iERvrpFqJKy0pLMyibUWQFjZxxES+i3XrvcioTDRI7aNjDqzkyFiNndZVaIO6EUeyF2KvAlaxm46SVmVe1w2Z1GBvQMZ4CboSLRUE6kiXiUmNDYu4bAIZZxybNthau66tLxAjjCGK5EFmYDZk0E3CojdZ2UCv7XgwbcSx6xNzW5luuY+bV27z2Yak7f9qGDBRiYeJuTVIsVOsGRTePi9ADMObrRYb8ZqzGOZmp3jx/uT7t0dv5K4JWgWJQTYuCHAEBvehHgVBYpR1z9H1CEzJC3pVj6wHlsiQAaSfqnGMUWILSwYAmX5Mi9etWYrQX582H591ofZN0wSvvdMLKSGKBkEEQaHcM7UqdLtIvjkd+apbqdSMTqUTSBcmiQtBUGv00jBqEiaJXppGo9XGYLWQ2bKeV6uTi3ZyWOSTVBxMIBb2QVdVHA2dY0OEGGNVdeU0s8TW02zeqWhWmiy3NtCi8rNVVIvdSdpVsW4lsdY7Nc7kKcVaV3WMROnYZs60826+8n0vbtbKyrMx1Bkjk7RCcrkSjmbHYWBoZXl8t9ybpvNGl6suLn3sEKAQTQ2TELwwMTGno9QUbrN0Ysu4bsZGcIPj6EPtmv7exNzaBmGjGuob8LSJKsObf7sJViJYizxhj/B81Z7Pm3uVT5VgNnG23l6hYLOBeJuOvW7Y4cRiWg5uj9+6PfrhOHXAstMuxr6FZAC7RpoqQlBEQSfCQR2BiQAEgYiIalQlsIEyGWYxSoXjjJkJhsmAZN2XUhVE6KrVP/1i3gZVcAja1p0SSUTwXeiiBO19crSXnlqbptyjP9IwaMUKPOHeuBwPU6voWkGrqpqNk87H1HFdB+8pEFlHNiPKmBJDkZrKK5G1nAiR8KrqmJHl1pCJIm3VCSEfOhPJ17padmw5LZAaK16vlm3VSDm2g4QXywBlm7KwJglS0GolXQBSGowdd7pYhBg0zTgq6kZMP3KbUp7bto6X85CI7hoERXl3eDDJ6sY/O6vbWoNXCaJETFpCFeaqEWt5MC2zSWoGax3Wpim5xVU3ok1xnZkUN77ZKDVoY6GzeY4b4XUj5fVfmcMk52HOqaUqhk8uqudH8/G8GSghMTAG3EcoQLoJ1Y2LVa9RMwxSJA5lir3ywd3x9yb5GLTysY2yNZ+xPWWrAEQEQYgAR3AMFYkgEVUYUVXV1FBuTGpNYTl1RCAouJ89WU9WCSk9XbS/PGpVEUQdI8lsMUhFEKPGgCgSFWIA07f2hQgdST50D+9MJqWbiAZKiiIZ5WmSMkJsl74mnd7ORplddbFZ9gauqlE09A0KMaC6CY8/W8xn9TA1PujVqi0z4xJLIO9DWHVuYCxzCrdc+tjGNKW0dFa5aeK88lFoZ5pw5HkdUsviSAl5aqiT5SpEqCvNIHdhpU3jDZN17L2EGB1zMEhLYxOqF229ktsOeyZOD0fjw0HVtV89W6wuQ9dGFagld+CIuAvqVUWJS5eOs8GoMIX5enW5YbmuRRbb6nLbt9lGHq3Ziv6nuqlJ+2vMRvB4XVMARMgTZJmxjpgZhC7qWd19cLb85GiG8/pWJ0gcErNuuTsD0c02KIbZ0HGG4CwMgRmpwyS/fWf47YPR/cStvFT99PTmjuhd0xQqSl6FCamxhtFPPYmu9yCUlkeJcb2BKrFQn/bJgAUQUFQcr8LnF632Va+qs5RmWQwxj3cz3QAAIABJREFUiK4JEcAlJjGsof+kZG9o37g72t/JhuP8aRcu6tgGYcJpW19edF0d84mjxCSZu5r50MZhYdkQEaXMHCg2Sr0HZSRf6V5CqJrLqvF1Z5ahuqq7y8YwZdOMiTma1bxNADcwSWI4YFb52GqW2fEwWa2CDyhyGwxZS4PU1MvYesCiHLsEVC+9eLFsAK07McyGSRPkpdMYl5chBn0pgc2S4b3x2ax69my5WvjQUoiSGCoyTpzxOWmDLHEuseVOsb8/3JnkpnTXWWfb5F530G/oeXpMxgrlTX3KWHenthdsclsv+6HNj7b0bB98ZUbDlDNnnDMg6oQa0SrGi1Y+uqz+8tnlxdHiYSU2YWQOhkCMfiCkz2p9SnMGImurhR79pSl2i+m9yTu3R98fZEHiVROiaK9kjEpM6MvNCKiqNcYRRe3zMkdVQ2yZEsME9EtmSNdNhT4tiurjq+7JPEA1KLyCiUejPMsdiKR3CspsmSeqEFEVHTvz2l5SJJYML71+eVUtVm2IsIpYd6dn3bLDuEgi47zu2kpIcHu/NIbyxL6wV+4N0lFhLGnrxTga5FxmHAS+keNFO6+b5qozdTdbNsGxs2lbh8+/OA8hZiOXOvYtVlVIhcqRJdCyjllCZWEidFzawtL5ZSAQpRiUTltdLjpH5Aw1PvioKasYNpnJc9dWYbXwTnA7Exlms1VTzevQha7VLoiCU+YkMegiZcZZUxhX7pS7e+XedLA7HpvC3iDDcA2Q6CaPvy02t3O/W5SGr3G4JOtHenJqW2NuQzk1mOQ8yu0ws2XKznI/MycEUQTVOsbnq+Y358tu3r1ADNdLuvu8yr2KCQZgg6jrBw2vi14mJA6jzByUrz7c+eF+uc/msglNjL26X/oUrITe+JrAQCRmaETP0KpltgaWSXX9P/Qz6kHQRf3gpLpsFKAgPWrTInf7e4MstSAURZo5AxUyLFEz0rcmyX5hmI0wFl04vah8C6hmSkndLr2Q5RcOB3Uny+ilUlHYnPLUOCbnVJmyxEwGiTU8q3wbpGrjrPKLWmLQaGhIMMrLTk6PqqPn82fHi8uL7vyyvbyqgtfGy2zedG032S1iIE90Zz+1CQO4e6sITTy/ag0jHdrUmmbuo5fEmBBjFdQSLJtokRcJSFeXPnQ6sTQpbaNR6o47bTppAgWFBy/UjfJ0P09HVO7sTg5u7d+/d3j7cHd3upfnI8ubzSa6TTw3z0fatKG2GsZrr+N1Ctz+pY9FxXoOb90w2KC3/gkTg9KZkeOxM7llwyxQib2eR6EkkCh8Ujd/9tXps1Xz46vd0av72MngbL/4cJ1bjGy6XRsnxa1aHARK4CzK7JsPd795WftHl3/86Oznp6urpgtKosLBMCRlcoaHhBApgtogtfdN1L3cDRNOmABE6UWzHMR/dtU8mncBtF6uqfBCx2erskhGk3yoSdeENsAaUqXc2ZdTc2eQpCAFQidRVFbRga0iaDCt7Od8zlRTYKvakaqazMxW3cWpArAGzlKRuqywQeNgJ0nZNKFrO+RRQyfiNTUIql4QotZNDILeY3d5FT6bXfXDQyCdt105zJo25mayczD45iu33n1173//N79OqDIJ8szAw3t1bEW1jiIiqWMyZJxJE6qrkLF9eGf48uFwMrSGKHZhMWueX8xLNTZP2xDS3Axyt1uUxWi0tzeejAdF5pwzzK71arcgvY+qPtq2tV1/JLFcrwe4pmc3+5r6r34GHTcFQptaATd+lDkqEh4kdpjw0Fk2FCHRUwRC1AjAGBGFUuXlw4v5Sdf9cNF8++V93B8jdxABAUGQWBQpuojGg/q2ooANYrxWWjKQWtwau4Phj988+PHp6sMvzv/vLy+/XLRtCEEkRrYUi4RHiSXSxpjLRo+qMO/ifmH3M1c4FoWPsYny759XH160nXDQEEGi6J2CG6/Pj2ei6r00TQsgSV1i5H6mDwdu7CixJjLVUaVqqRW2YGNC7WMrWUoT0pkPnjV2AuLBvjVE3UXnG6hKlposo9WqCx5BpKMgILKIBjanXIxttRENqqIURaOCN3d7z5sLVCNOn9cnzxuFHn81v/fq3o/+9rvffPvBn/7lV+PhWUeGCHUduTe970IjymDLhhyzo9TYO5Pi1dcnt3cHZWYMkyFihkQhNpPdSZLYk/PLz56cXqz87u7eiw9u3dkfjQeFZRbRKLqqOtpPbxSVG/bB8HV4ga7Da3sI4joI19asBPRvUrfwbgvdsNYp5hZvHbrDUVakZpCZ3LFZO/VLn816iiQKAVHXiIcLppdGxY9e3MvvTTBIkFlYA0twZt3b7w1t+38sCh8R17YJ6Gm0bfM1CGYNns9+8uXFnz2eHa3aTsQSFY5HjjNnYtSzNh6tPIP3cr4zcANnIPKLk+qvL/2ijqmhZeUVCF76lR0EsEFqyRGXo9RZq0Tctr+Tm72Bza0pEhOZ5yF+elGfrII1SPOkqhvUcZAaJLhiHJMuLmNu6LU3xtbx8qqtLryqjEeZyykAbSPsiUSOrpplp0qIittMOdOllysvXaC61S1pAIDWEq61j25v2WAIqcHDlybffPf+ajk7O71iy01nqyuPphWXeKh03ojko5zLZGeavzgdHw7yySgdZE4BJkqdGeZOVe/c2X3zzYcY5bicf/bVxaOjWVoU92/vHu6M0jKFMQgxNv5iVtFeupG5ypqpXPf98Ddx2/Y87c/E9eg597vu+tJqHWTXKym2xK+CCA8G/A/fOPjGftkiXtRdLbGNEtfT9Rp6o7F+w4jQegFHT8AyEuLC2YMs+ebB8OVXDnB/gtytX6IxYIUx685XF9crSfo/DUC99pKhCkNQReXxfP7hRyd//OjyqGr7nWLOmNJRyjRv8XjZtVF3UtwfJom171e2EdjUQPDbz467xkdRHyBKZCJgEtZ//q27v7xozyAXV9X5afWjO+WDsUutGWUuCJ23/v2T+SJwZhWZWdQtdSgURQJ15gJ66lQD3RnnxchQJ+iIBJYRSChh6zgGqmvfrPzJVVt1Shb3DHdRL4MsI8RS12hsoXHtcNjfWUYh65FSTHMMHHq7B07VGLOYxU7gCIYhgn6pFVGvgyE7yX7vW6+QjyqYjNLRIJ8tqyCaJ/bVO9PhKH/z9Yf3Xr+HMoEqfETTAYw0gUuQOVgLEVQtzpamtOsVhT2N0MuB6G9IZ7eM2gZvbUrNzXDd9UKGtUh7q9fApiI0hFem2R883PkPHk7euT95a6dM2VSd94KA9dI7XRv1s2o/NgLRfsGmhqC118vWP100aSeHWYJBin7ws0+w66v7HXO0ifo+yPrjv5/EIhDBGkzy/f3B9wfJ2Li7ZbKKMQgvfVwELaw5KCyTntW4akJtUi7K4/OZet3bLQU6XzTrhaeIzMyE/+LdW//1P3h97OO//vjo9Lz5nYPyvXvj4ENmTWpZCEer9ukqKMQatik3qkKIXjlSQZo7ww7mwGni6nlbL2MkbUOsqrBqw1njKxFYSjPOclMUaaMxDSiIGtGlIDK4YONgDBn5m6C5TxD7AxwOkRi2PWTz2jUaN+CnF8lHQBVR1gVfkaXTYfHk+dXp1XK+ai8W1adPL44vV8fncyY+PJw+fHBYTkooEBWJw2SA6QDjHMMMeYIkQeqQWEQ1hbnOUlv4v7WRArbY7Zqb2IK5a4+gzTXbs3XbZdrmRWfwzsHge/eGr9wa4GBg7oxv75evORuiND72p56qEBkFVFR7d3+s5yR7Jb+qRtVFG+6TyUuLzIEIlmF6QY+sA46wNvF2Bs4hNTAMA1gDVZzX+Phscdp89mT58Vl90oa//9re792fni1qJWSGg2grUiTmwWuTlsysszs7g0XVXV0u08Tu7QxPLlatj1GUmYnwYGj/x3/8Nu6PXhim95j/xffu/5c/emUxb45mVWI5qH45bz6fdVGUiNPEpI6J0CqCRPHC4IGhFBzaWJOEjGsTl21YtjF2GgK8aBSxSkElCDxFJeQCq1hFXbXaRRCpsQRad+wsb6glgIA8wcOpyRw7w4bJMfVbAwmItFbIE8P0HWZAFYYxGBdVF45PZleLSgnL2p/Oq9ZHIr21P3nx4eGDO7vZOEdiNzmT18MgPQ8QAqLCMaKa0l5XAGvqa9MGuEb5X0f3W9L1ZibbNgaYrtuStI1URmHwu/cG374z2tsvMc0xTjHK7U75wt7gnSIhRROiV42qUFJe6wiJoLRRihApQRRN8Gd1eJnI9cLu/ljUzcCCKAz3x8MGJxqQgg0MIXUgwrNFulPuf/eFB3lyIGS9mG/svpmaD5/NuxgtkzG8KpKliDHG2nwyHTy4My3LbLHynQ8+hLb1pGINGcL9cf7tw+EkMdjNX3p5d/rCFKP08vH8p08vvegXi/Zo5b303lac5i4aFRECxFKAxg5OaeRgwV0dV8sQoUgMpdQpWh+7Rn2QCtGTdoZbRIIOGvUCn7GZWmVhgUmQDp3LCFCKMLzO5sZgp8ROQc5aJjIMa2FYmdisyXaKCsvILIjQKVRhHcTh8qJqWi9RbWq6EGaVz1JzsFs+vHewOx3uTsrRpESRQwEBLAOMZYOqw7LFo7P6qzMnCogp7Ubws2VocR0rWziPzaim3khsG7x5HYK8ufhmPutjbjfj796ffOvueLA/wChD7pCmKDOMUt4p7u0N3xkVI8NBENdrB8kY6m3H+tVxov0WTm0jX/r22aK5G7RILDIDovVeT9zIw1ERBD7AB0DXDYqoSBmj/K/++JM7Z3O6NchvD41jHJbIHB0vf/psdV7HkygLEalld2AuLttVI8My25sODveHznFi+OxiSeu6A7lFFdqL8/a1YY5p3iOGO4w/+fj8tG6boIF6jRoSgzduD//+SzurRmYh9MShV/hOHWhimKyNqs1C23mMTVAlMCmRBoSZNDNp5l07D1xrqaYSkdQWw4RK2IGjKNIImK0hUUZUmDXfuTvkzHFqKU+NZTCzMZzY/hNWQ6QMUeSO+k8oKvYOSlXMl56UCGwSbX00hh/entw7mA4GZdeFMk/vHkxQZugnHBMHw6g92giii6cXf/LnHz17fM51ZwoL2vAOvI2bjcWB3KDKrqPqhph7e1xuxWq8iTO+0Qxl4O7I/fDhzlv3d5LDAUYp8hSFgzNr9rVw2Cn2dwdv7Q5ezF0Urb10UcJacwEvCCqxL5xIFWbp/adXtczae4ZRJLBmLRt3vL5R+s6B3Zh3YLP7mADC3XEez6snX1yMu4gHY4xSDLNbuX2xSIj1uApL0YHjkeVdYh84GLaWd0b5ZJhdzptnxzMi6gcCdjK6O0hOquZqFl4rU+QWqrDmq8ezZ/MOJANrGVpHWEf/0auHP/7OvR/dGd7O0uezqvIxMHURnZcU2HUmMQxDXZRQITaqtYrXtUoq9rgVE8sGXKsslqGadX4VQh20t86qRVaiASrXSDpPkCcmccyE3Fln4Rxnjq0lZ4yxiIoQ13khKAh44cE+E04vGwJgwI6I8OKd3Zfu7xzujWPks/PFZFy+eGfXlMn6rMgTpG4dMWWWp25xvvpX//Y3v/j1Y1NsRpK2+GxbAWxPSNmE11pYe+MMXVPs8fp4vU6BW2AHEOPFcfaDF6Zv3BlhnK3zmTHILZzZ0K2E3OHOpDgYvXJr/J1RatQ0wddegmjvWexATGSo1/dzK3g8q88uqteDokzgDGy/G0xAhNStly3SRo7dZzgFrEHp+NZw/OIOHozXml5rMMqnL+y8bem3T2fnVfDA0Np/9g++dZibSW5uHwyNMzujzCX8+GhWNw2BmOhbB4O93HSgs6Y6uvKvGcujFJmdNuFnT65EkVn4EFeieeb+yTdv7TzcwSB7sF/84W7RRjledR2hDeiCFKqHKSeW1HEn6vtXq9efrgIk2EkpstQBTacqoADpoA00qmUwUwzag1oSgGAYZUqpYyIuclNmiVn7HAGkISL2nJKuB8OgEJJF28wWkYmNBTvsT7PXX7z18oPDLM0uZ3XV+Lu3pncOxnmWgIAoiJs1DiEiTTAp7hZOvPzs1083fSdai7bYrL/XDXNBm37513iK/n1vSptr+L8tOTdxyptu+n7Brx4M37w1xijFILlus/dvy6y3jSNPQECZYHdw73DwrUlx19lNcde7+3DfYhCQBmkUp1X7yXl9u+6GziJzsIykV6H0S00UzEjNWoTZC+tEEQRnFS4bNAFdQBBEgWU4i3H6/TJ9fLr65HT19sPd3//Pv3f/D156/YcPXv1Pvvfm77/8GumT5/PLVXN8sjDMr03cewdZlhhFjIrTun7/eFVU8ZB54uxPHl3MG7/oZOEhhL1x/k/fu4+dAoaQON4p3r01/u7u8NYgV5Zni3be6QB6P7M7pcsTW4nUnUCh1K80gwKZRZEYAS+8eL++5S1jkKK0/PBg/MM3Dge5PbqoN6PaFIEyM3lmMmudZWsoKgUNMUgX0cXYBoJq4phIuwgoui541aZTS2QTmo7zO3uDl+4fvPjgtjP2ctmmqZ0Mi0GeWpXlyeL5lycnj85Wz2bV6ayb10WIyFPsDV6elpmzpjDXg7jrbETXGOtmG2BNamwrgGtP5OtHeiDONyZn+8izhJ2cQwy19y8QWWfXP+gnA/rICZu94n02Kh2IsDfYuT168/boe7fG7+2WwzJfVW0VVaAiIkSq8BoXPnwxa9Jld7t/zsSsESUDIaIHR2vh70afzkCMOF9+8vHpB789dqf1KE8wTtdKuHH23Z3BT7+8dNb93hv7KFKUGfI94G3cf/mNV7u//H8+ffT8apLgb98rJ5llQ47YMhRUh/jx2fwvvzr/+bNF00RDUgUNIkJ4+/boh9+5i9KBGZCe4R3tDd54OP17D6d3cv7F+epoEUrC65Psb90fvzxJaolXbb+nYE05OYvMmQ66Jv4IzDgYmf1BMshNnqTfffOF//aff/u1W8W/+9VzH7SnLUQld7BGAISoQYIGeBGv7IMsG2UmiFQeoee5mcigiziYFg/ujPZ3siKzo7K8f/fQGDo5XwYvTJQ4s1i1H/z22Z/+xSd/9f5XH3529OkXZ189n83n9SDGIk+wP3ppXJjC9mLRPvCv+5vbR24qMraPr2vMr0O3a8Usrc/irUJ2kuJHL+x+687UkH58tTw5nuN4NVnUiLruFHmsCVXuUaHgoonLjhkYJCgS7OTJwfDe7uA7g9RFnTWxiVEBpb7jRY3EL+b149PVvSrkziC3MJskvO2UYWueC6ggsdhJd3NXX1R/8vjczf1hYtej8EQYZ99W/V9/fXzH2lsmASxuDYA9QDH0Dx4//dc/ffTy2L0wTtX09IsySKBV0DrGLoR50ybE9zIrUc5qD0v/+PVbL/7OrbWcibEOtf51ZvbFw9G7hf358eKruVfv39wr/9NXd//W3eFO5ua+m/kIghISQp5wFaTptDemyR32yiRPKbNWgeOr8K2Xbr/7n731d/fK//NnXzWtAPABTeh9T+FjiBLbII2XysuqldrDMuoOqw4hIiiSBKx859bku+8+fPH+JHNoOl83ur83DSF+/ujs6GRWZulkUqyW7a8/ev7LDx8fn8xPLubPT+ZPji6fHM2OzheybPYM2zw1BV8jM9xIZnSjCN3mtC2ptqUtrpPZjXNzmxq3TfdBgtd28/duj75/f/rCqDhddT95fP6Lx+dnj6+msyavAyAwBonpZyzhpfr8/KjMJm23xvg9nM8tdor7++V7qVu0cdHFoFAlBYtSo3pSd7+9WJpZe09pfTpvp2v6WYaoa6aNCI6QJBi4fWfay+YnR1dPni8OF13RCRYebciL9JdfXRyfV6maW+yQOuwACMBienryL//dZ3WnI9fPFfc4StqobVQfJapGIUBH1jSdP2s0Se1/8/0HfH+MxK4dyNdik80naN3uXv7dcfbXx6snM38xb26Pyhde2Hnn4eTHd0Yvj7LP5s28iwnDWFSdbteA5ikssTVkDTHUUfv+51dvpeXDf/T639vJ/5d//2UIqkATsGy0C/Hdt2/fu7Xz7KKuhU2aNUGbVlYturA5hR3YIGV66cXDOwcDQ3JxVZ1fVfN5e7C/kybu8qq+mtf3b08P94YEtG0cDYvDg8nh3mhnUg4HuSqdnS8/fXT25OiyWnUmt9dvk83XvFsIa7XZzQKTN3kOG6kENr/BnnLHTUIEa67EMHwMs65b+RgUQfSqDid1+3xVf3A6/+TJRXW0PLhqbBvXiXHR/r+/ePrp8eytYYbDIZzZRLrCWowzs1e+Pi5ecqYO2gWN0KgaASjVEV8umour+s0AWIY1X6tctq9pe7ozIbX3LdfL7uNZ9cuT2W+ezr96Pv/k86vlZXNZh589ueqWLbO9o8CUMSRAcHnxP/3L35SJMYqqDU3QECREhYKhTMS92ZUhBF16ufDy0m75hz94iEGyPh3yFH/wOrqAxq+3dSQGRTLcL3/86v4Pb48Wwj/58uLVIhtOSrtXvvJg8rvj4f/15VUPUruIKOjXa6eMlMmwEqtlGqaGEH712eWbtrz3H7/yuqF/+8vHijWNvT/N/vD7t/7Zj1975xsHb7y0+0/+7r3/8L2Dlx4M0hyXq1a8WosiJy/IEzsaZqLx+PTq5GS1XHarqhsNB4f7kzThtgsv3t9/6d7u7cPxSw8P3nnjzrfffvDe2/ffe+veu2/ee+f1e9949WB/MriY1b/++Jkpzfo3e5Mq6wub6xbTJnqwuQy8aeFszlBs9f3b3mhvvUEgIHcoU4qIl233eLl6smgWvo2qEdKFuGjjZ1erXxxdfvz44urJLD6bP3l08VeLRtv43t4Ao2w9K9Cfxz23mFiM0uHh4O3p4FvDtLTOx9AGjSQKRI1Htf/4fDWp/K5hZPZ6Kks2+Ew22VgIhjFKXyiSoo3PV+153T1fdZ9cLX91sjyv/HkdPzlfPj1b1iG8rGpsi4uLn/zRRx98cZY5s1z6phWNIqJVG4+beFV1ISAFMsMGqFVnTVx08Tv3J9/+xgFSXt8wTcA7D3H3VczPsWrXdVNfoGRmuFu889Lk9x/ufPR8EeftuEhgzXSYtZX8+nzuBWzIGBOC9h6Ya8ZVNbfETASV0P71Z6d7rfvuH77ycm4+/PLUGqRWd3NqFtVHF4snF/NFVa/qJjFda7rKyuHt/OFhMhgadXQ5j4Vll7CPflHVdRW8jzFI18Y7t3cHRVJm6Yv3d1994eDuwXjvcLxzazI5nEwORpPD8c7+eO/25M6DvVde2n/9/l5ZpibnayMM3h58G2S2bVDqjTyn28jbIJ+t6QvdOIKxqSqYUCYY56bMTGbZEK+3bwOqrKLKDOIuxnkXnizqj64WHy07myUS/eKyerDsuGciLK+jrSeRE4M8xTix+8P7h8NvT4s9a+ZNWAZRQKDzED+5Wl1d1A/q6AAYA4sb487YrNIBQEgdptnhJHuLzFUdrtqw9AiqIuIM116fLrtHV80vHl1+8dHJ7Okyzd133rz7zVd2q7Nl58PzRXvRRFIUhg7yNIierPy89j6oSmwU8zYa5x6Q2c0cks0L+PwYzRyXSzQBUMS4Ptb7mHOMSXrn1vCPfv4szuvDxEHjDunPTpczL8zGGGaDEHvTUkA0MZxZMgxjyCSsiXz8/IyX/Hd++MLA8M8/Po4CMBLI/GR5UnfDETU+niy6yzrYQIVhHwIMXVbd2aWUDqkzQmijbzzUKxRV1eR5vr8/enhr+sK9vTsHYzPMkVokFolFniJzPV+HUYG9YXJ3en9vZAp7TZjx5k7DlobdOBjcBPXrnHez47ThO3gD5tZaZwIUlnvKjIaZyQw70wtbCQTblxmGVYU0gowaIstmUAxyJ757fLH66fOL2fHqYR0MgMSAaA1u4kZk5gwGCfYGBweD7wwyE3HVBS8aVTvVZ6v2g5NlfVm9VAc4g9TCAkTrhtX2nTNgLcrETYs3BtkEsmxjHfqpYxo5Zuc0z4xzuzvjF+5Od3dHrz+cig9f/PXjIePeKM0tXbXhbOWbEEYJ7+aWSa7aeFGHWRdVNTX68dVqedV9A4zcwhJEcbFA7dc35dZwdcsMGUaZvBr1v/uTT22IUyLD9AcvHby8U56u/FUXnSFrOaqsGihgWG3/FhPY1NiSA+TL4/OLi3h7mj+9vAwkLx+WUBmIciOPu+isKSwdDlNKRGr58KipglxehquF5IZyu2Y6fOxHdyhKnM+b3eng4b3dB3d2hqN8PRkEwBkkBolDkSBP4RKwBTsUzhS85lFpQ2Rs+dn1Mbr5XfTfy6antG4DbEae1sHKm5LuBj5zBpOMJjmPMpc4ToiUJYoaItHer6yXWhAxxtMin+STSTEdpCT1sgrLVfdk1f7qdL46X91fBRO+vjm2f/WGYA0Ki53yhWnxbpn5SPOu60IMqlWMjxbtb86r0bLbN4zUwvH1SGDfM1lXPQxnMc0OpsXvFsme48xwHcSrpgrfNDGgTO2Dw1Fh9WCvcMdXl4/OVyFCaJzw7TLdLWxUPq9C5eMo5Z3cAqg6UUXdxab1T2bLT87bu17GgxS7Bbpu/UpAsATTz4vy2liaAWKTu08fXf7mq9nFqjXODix/9zt3/+Er+68N88+vmkqiMYDqokHbwbA6y9YSGaioTZgsPzm7+PkXRx7RpeoVQ2vaVhhUt6E1vDNIJqWp0shCx7N2ddleXcqq1Zy1SJ1RCp2EqOghsKKu29miGw6K6bgcl4nrWSpRtAFtQNOh9YiKrsWqwmyJ40tT2g0s3habW/eDzQmom2MUuD5zbjTT16Q/byqArc62f57MYFqYSeIGmSmMAcFy7zigDChD11o2k2T21r3y/t3J3qQcF+xb39R+ufJCqAOeLptfnS4vz1ajWTOou/UijO3/t44Sg2Hmd</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9yZIlSZIkxixq9p67x5KRWXv1Oo3GLNQH9AGnIRAIFxA+AP8OIhxwGJrpbkxTVWVWxuL+nqkw4yCi5tG/AIqXVbG5+1vUREWYWVjUgG+Pb49vj2+Pb49vj2+Pb49vj2+Pb49vj2+Pb49vj2+Pb49vj2+Pb49vj2+Pb4//vz/427962N7ug0CQAEgCDBBEgCADNBgEECRJwggGQZD9KwMiARNABMgADAOAAdMwVX82bBsAIMP1d9A2CBsg6jVioN8NTODDm9gjQBu2ePF4yWMMwgBJ4WBasJ0GZNk5AViA7ppTMWIEUB/WAGEABknYIpwiAUDycVfelRZE0DABob8XBBjcr+PxzX69jqiV6DcOkhHsz0TKhiH588+350/3x3eXhzeXMQjCZi2UaQi9ArDr766/0pATt1veX6ZlyxLy0MunOS68PyuniVptx+DTu+3Nh+u+R2wR5NhoG6YlCf2KcL3F82LcPs9Pf7xFxNP7cX3aR4DgIAIcwB7cyYgIwbamcyqnZiplyTOtRAxeLtvz813g/hDP0rS3/+X/+PsPf/Vuuw4SMRhBBsdgjAiy/mUEg4gRIxiBERHDg2MERoyNiOAIB2MAUSHIAERTgGCTEpKUNG0JFVhTzpRhySYkmIggRnAwtoiBGMM00v/p99cf3gzTsjPxQz7806efn97tliJJxwvu05rpTChzTj3foQTkY+a8gXSQoCse3LGNDnDqfkspJR/P+vjz/fnjTakKBQugCQYAIoIPb/fvf/30q9++ff/hYds4EEF6JoPbPmKg9qIAyzJuX47/+v/8OO/54ddPH375OPbtdWvBKdFMw0obKVsybEFGHrrf8+cfX376423e0+mZ1l3zUAx8/un+8adnyF8+3vOY2759+N3Tr/7q/dv3l6c3+5v317dvLtzA6Zk47tNy2nWBkAYIQamXz8f/+3//+fkPX7777dMvf//m8e2+My7EhbySjzGeBi/cNsDpnDruut/my+243fT8opeX4/aSD2M3eA/d7VvoCzw3bJv58GbENiIYgxwcIzq2RkSsOAsOkhvHwOBgaI/B4CAHYwxEcIARlfMQYGczEnICYMhKQ4YgIWolU4AlQjZIBGMQI2KQMTgqddBTT++u33+/WZg0JEz/8Pbh+rDLqTTAPUcqPeF0BtJ5u1EJA06kDMmGpkBYTkM2JNkSMkXe7zfP+zEP0b5chkVUDq70TIyI/cqnt9cPv3j87leP3//w+Pi0j2BtSxoEIlhZzQCBhJ143uOXv3/z4ZePD28uEXGmdQuiUVc+Je1paUp2Ts103tOijRHx+Di8U4CnZQQipbcfrr/ON/XjEDgQxPXxsj+Mh6fx9G57ershoOkxtT/srgS7sixBpG08vdnev78eX+6QH677fuVG7sAeYyc20KCAQ/YGD2oQW4yHfbv7MhVz7NNJWLAEaWO837Yv92PztEHJjMrhgICAAMiseqeqoIiEERoewgQHhFovMWzTZIRdgVGlpgqShmFBkKyATNMgHKx0QnDQHhEkBjiCQGxdwg2buE8TGAmOcGBe/LjtMoiI4ZRJMAKbMRC2xbFF1PU2PCHIsraQbCGUEiYGZuaR97tevswvX47783HclZmmSdp1VQKhbcT1cXt6v7//8PD2w+PT20tchoCCHDBGEJXxCBM2BAIwdXmz/e5vP8QgAjZ4rvYQbZO2ZcqZ08d0HjkP3e553PK4+3g5jkPByDCECFoGMQIjtn3j/jAeHrfLdWx7jD32LcY2xoaxEWAekg2YBEahJBKd7x1A2sHYtutTQEZjDx6yNYU4jM0MI2wIOWV5ClM+rIQPYm7mNhRAgiLSaRnYQnAapA3ZQ9AAbYgetqCCWrYEBpWqTU0ZUctkyA4aZLquK9MkIWGEosIKphUwINalJ2EPEAMUQQ9GEEEzGJUOwaBlkrOvOy/ifXjYSfgsf2EAMaHGUm6cF6y0ynCtbD2tpQQznTPv9zzuOW85785DLrC6hdOiaQQYxNj3h8fx9O7y5t3l6f3j05ttf9hqpxioVRBcH5cIuOKIrr0UDrLWmoBpCySUkGBLEzlzpuah49Bxz+M2b3fNe8675hRsBOgBJMAqIzG27RIPD9v+sF0fxvVh26/cRrDALSruHTFiQAeF+muBUzkhA2mnJdNWkmnLEChAStFmWIcVSWVSyJTFTKWcdkJJ5EKY0z4sSdMx09tjhM0IZHoLwJQcEYCsEMFabVLhMFXQ1R60EhiglByN8AcL0gOoQGLaAZM0RABUVyEyqPoKQQOICJKBAKomoK6hCwjPBGAM6q4g3ZRFVmF0EnYAgkNI0AXZA3ZKti3YyglJmZpTeXhOzZmalozgGAFDlJKiB2QwgvvGy9P28LQ9vb0+Pm0PT9v+MBgGK0WcGa1Cny7UJ4Kqgtu8yGrSg4KulpzpnMr0nJpHVpDNqeMuTVXpZ5ARAyJBjRHgiH3j2GO/xH4dl+u4XMa4cERxkkZ+rF1DbNs2IdpgbAEJNBBGIukMZ04JhBmWhARkaFiSLBIJMwGmJVtZKc0pp2BZBWnMmU4hoTQEbx8/3neIM2Kj5SQ3w05gyCCtZIzalay9GYCLCQUoa5BWKuqvLq5qxMk4m3VWOLlKdBEdRMM4M8jmnQ3UDQHRQQYb0zYpZGyDd3FnhRJQML2qK4mwEzBsZ/FOVMnOtNcunIfWr1ZCBskRGIMkleGwNwQ3Dux7XB+27XE8Pm4Pj/vlYdsftm0ng4CBMFnRGaajoEfhbFtNIO1w4SCEZVkS+xJO5PTMOQ/MqePInMgJF34iGAiQG21soNJjcH+IbYvtMvad2z62C7dtMJZc0Atf/BqVYcklIRCmTKiwX8BOx4DFUcWe9eOmiKitKxiIKctQhpgmp21iwqZsgoCdtGBzQ8gbt+OWTqW9Xfc5tVMirRhRhRPuKxYE0h4MW8KwPcQkkGYgqgoMh4IsjFu4hKx1JggLIKXKRSttVRy6slf9EWGbhFYoknEcTngARzhg3MELwkwYqqpsyUjBSFlpCRCtnFn5305J1JRSmsqsNTNp00EyGC17IIixjW3jfo3Lw3658vKwX6/bdh37XhIJS1JhVM5yIVYA6ZYPlDZc1EOSixkVVFUls1Q6p/NAyppGwqqEiAgIGAhHr0xESN42Xq7b2LlvMfbY9oiBbQRIVD2Go9aTzS0NJGVXIDa4cAVEVSkmBpBQ9PVQyQbDSCJSpg2FZGRIgggNZMLDKdLEBiKYdgRqUeWNQt4Vl0GZqIBEJT8y7QpqSuboIpYCh2EoGHIOFkJjkILDYYSglpPs0tK+3mHRUUXUzmlJyuj8YJhVYAC7FDNMuSIKkDZiykaIJLKqYopHR6okJTQ9NSHTyGnJSmem5ZRtETTNQGQ4PDZyIiIAx+AI7pfY9u16jbGP63Vs13G5xLYNDjTsY+cOMoDR27mlMLoTLW27UqssslBRpi3l1BSckkRHOIYBahs0kBg50mYqGQFiEBwxBrc9IrjtESO2jRyVXs0IF0Zd1TrYyqhH1FsjljpXl62vC5EqFAnB0bXXClBCgM6AYsycCoh0WKZCXd0YERiDOrZhJQAhFBtlT/kax03bdZMLlnkUMwCCssLhwKCYoUEmPGrtSBhJhwtno9knDZkBNDBrhg/AwZJGRVD1UYsnRCe5lQib5tV6CIci0yNcCog3IOUjWFKt3ETFmJITc0qyjoKLgo2SVQy5kDtXeQgODEWC25YMkqiLt+1xucR2GfsW28PYK3MEwCAUpF04G+CKrSXrlgZqLdAmq/ZQymCmICmreillAbU7TCVsEyERUfsSYwyCDGJspWIyttahWvtEp7HXyBJFDDY+GWMTi9uorgVVyxAZsu0IyIAdUYXHpcKbdfVpIIQI2worIUpLvg+y9C0WhSzqFdogSthG3O9ze4hCpq2tmAQsJh2io6VK2ZF0QLKHwhymCdmL1dVmQiyZxFiYvkhfFAUDosXyJc5zQeTWqKNzIRCw7ES6itws0HFsCbc+bimFKWU6s2oTpJbWpVWLLKLxYZWPqDwAMiwHwDEiNmyDY48oVX2PCJgwS5EQgKw9z8pY9bvCJdi4cGG1LyyWfofSqFUaCw0VrojuroiBBMPMABQNKwgiGOzKHh5bDAY3jFGVvmK+SzaLfKDkJZTCxKDrNXt9q4PTy95QpnUYllIFIqKkBnRiJkE77JLWi06wsmSRFYKMYG8Vw44tgDDGFgVuIoLRjaTqntS2YPRb4aIyBRqQ1gAL2rvFVnfOKr0ZXtiMpX1U9WWxhaL5ZrHwKKW2W0FAvf6AHUQCR+ZOoNgJK4HokFONeAyokHWiKKYt9GLTTJvFrsN0NOA9NX6DG0QwthiDY3BsMTbGYIxARDDqA8LdVRDNyh6uT8tMvzKfTp5Ol0LNlKq4yXblVaguNYiIMM2SxqzaASoxjlHy7wgEB0d1aFz/GIDAqDTVxAl0AAD7Ta7dW4JBawBw0ZVSGogguoqSlPsyuCTRoDOMIIJgqAgbCwvQ9VYJRWVuRmlP8DY4nK6ISrmpCm0RG4oStjZVWx82A4NBIjocI8wYsDGwNKrq8Kx4rdxfSIYtSizZwSzJKYJBFwZv5WMlClBSwnd5NyxKNmcB7JM995VTg+iqWAXyAKBX0WnTbGjWEKvQIQJUfeANEdX1Wn0RtrYZaLEzorALmmPh7GJVGUHJ7rKs7lzJqgvcy8l6J4wgUOtvOAARpkhS8AACwdEbr6I9ghHgqP5LhznpQWRWuaodvfqeFNw7e/VMXYSNS2hu3NPJvXe7XruhVmkI0fwHK4nXQjYTiuoGwZAQsABvkiTYjkEJatR9alpVRsVC/o3YWgWo4jEQIqP2h6HwwGiyVILSYAXNapCjuwj1dQYXav0qDaBV3H7vsj1FHdYgwpktTFGdz+WsS63VhNbhCG6IPJ8newGrjFgAG/swaHsb42nsn+bLSv8Ncuq92a5NTwQ756AuXq14uNY1gGpXt4ALAGqGVx13IzvO6SiFjR4bqrwiImwMAwwXRTXHCKh+fsSIcAW++z3UmygYVsuK3gI0O9MteLAaacKCqg1XZQecQvd/e/sY1aF2CYKkiSQMJnpfl/Ae9UYC3dhd2GFTd7MV+9CRjZUEDBiyhqMJnCu5RsgY6NCwrOHROxmrP101PgiJMaqp8irHVneRjApaIwKp3inh5rzoVFR5IlM07sf2uDsqx8FdedSV2EuGQdXv0Yu/+uZfSyyyjGAR33ahBPYYb7fr53zp7V1AtfCRXQKwyIDkQDcYDHMwhnkgJ2goKm1guTEKhamgqAMeGA5JDR5GUz4zIhqgAoyuZAswEVHN+iCCozdtfzshvaawcD05WCCpMoNbX6kw0/poa/nUeeAVNJ9bf30jWjwtXFTxedoBonSoMuZ0HDkte6PhdKa269ayV1+ngMKlk7b+2I3CavMU7CEqBdbOdwge9Lq8cUpitZyxSH9//iqUYFVnnAIAsCw1ZcaRZFnmS+ZbUKJtSSW4FJsME3BWnJmEggN0Vu/2REtFT3LBwm7NNHyZzn99/lhvuPuPdqEbBUY1HmybHh7AqkQ4rLlSBVhgO+GoK1QIUavpVeVKHeKgaDjONlWg4LbtQQIUFBE0HR5cYkpFeTuLVp4qpLcUm0po6Lzm4gNoAavzba1CSFmacvlhbK3sAn21k4FatPpzSQKlGQigam+zQEptqvrqZkNZOiZ6nw5RXKogVfDSVDVQXeWCsuvbQhY5WHp3cbt2KlS1gkDapT7gtcF+XjLWMwmOgqw6OWfFac6uPTNlb1m9GiMCtfEKuVrrWasuFBEsoFEZvjfyQkfUa41eEK22eDEMKxiWqg+DgMzBXk68gqBFNKpkdSHvLeaVEH3C1o1jKjtCio53sFT0lOMPUaWkIbsYI1DZrSKW3TQhXVRfZzNexPAqOVVOGugCWL42m9UsqkdfjMJOWP+uEoIa71bBqAZH/7f8gLUA8rCXd646uADBSFe3vd5kBdJaHUOqt9WBX8GNpT+lO73apRR7VXH0NmCTvjQgIS3AyfU0VlEwG4kErEzl6vrJqke1/AlgJgtXGyU3VffGsqclO+uLpo30AuLN+VAfQGBFN8xl1oQKNnXc1A8B0LomVQkoWIpVPViuQU9JtbruH1yRXp0wdgibjr949+F/+7v/sI+tgF9ZRyPKQEj2/5ryV9u9hYJA8cqlCKCbqCXI6kSe4oLQzckqwmoFsktirURlAquvdS0V+wPTQrdgzWJUbuC2kE11q6vXWfHlvj4ysP4dqc1lCgvkXePCvNV383VtV2lo5NXZE44VmV6ORobkCFglbHjxLpN2GgFMeaAjlyAoCKIWua63DteTuPU8UqkxeD/UpdVUZmBzyU9ySS1dRi1U66oaeSqbg4FwVCvlTHYu2NMlDd0fBYIiR6X0cBQglTUQZcygOt3Iq38uKxbFXsCunUXVHhb18+35v/z443QWdW0ngbUoE1UouK50CXbdnsRyYDTKbBLYOsQJZQFUOwe9G9EWhhNxNnSqiqUub+sfq9KZK/fLgJRmUa4zmXUAl6ujfp6nuywKjbZxAd62QaeCnDO363Vdd4egANMKRCn6oqLE5DBNRckfCW9BG8yS72iCCUTBvLpmIhBamWyc4kUJa9W3gu1yAaHTEFl+JBYUw3FrkyRb79OC2qC5i4k4MBGMMg+Cg56tp5AsZtydlYI3dYXYpYoMVs9pUResNAcZFfmjUqFEFj0sH7vI6s64hHu5dcRyBtSu+ni//fzHfw6+vnZrBF4bDSWRtnFqYfEoTnkGIAmtdtFJCrtCnxWpvmh2AasXqOzVhahC0EibJcLjzOOstn9paHbW7lHvRgMsORpZu91sySlCUkPTUqe3v/2L7z9d8wjkYS6cXi/S0r8NRUuHveTmQKa3jZkag8oGH00ZCdFjwpsrugiHmVG6cSiTUYsZlfVkBBelBTIFVC/aRjgzxpaZ90nk1kVIdNhwuLxBEARgY6SgFvAKxhT/Z0Qvkk/Gw+4Yk2Uyo4FIbAFjDLrMDdmaDE4R+sJx90EEurlfXUPXExT9fm121CXsXlprVXzlbaWTlaxaRr7CjIXMLAcKC9dzYNHMUrtPVFA/seAiXxl7bWeecKggC0DlmZmqBAqwxaqfOCV/s95tZ7Ny4jcVQD+zanqi+oRcSKteMsYv3l9fLnr8zaOc+74LKhjfULQqykLurVp3cuitM0aoumE+FS+3ArdEUhML/nPhGKolQLZAtEreSQF6aqCoafC45eN1/Ort6J2SbnTrrsG1o21EXykwOKeBiFi1sS5hLNIWGBE72II/Q/CBTKB8xCYYLGy0MUBE8PdvvvvP/+5//Jeff0plPetgv4FRkisXq1yEZClUvUcC1MkXF+zpOluQwtWO4c7YUKL20rwbDbSGeVLaBlKoFmmn+QIhWfEqsBl6IdyWJarZp8W+2ncLpdlU31giMxcHZSqr3adcr0gAjIEg2+9n2p6Hxt/85u32YX/41QMHLGx75DRH86VeNMbCLi3GVj6XPZbIyq+EgtcSQCxVkA0etYhLR1J4EewCnecVKVhKIjMZAVjTD5f44V0XIan6rYW5XwFWmDtG7TbZSqugEFBcjp3owDXN0HbFoKu/IJXSWK1pDAOlvFcbEYf06eXlT8+fzTITrUJyeiFWVkHvzZXs0R+wTb52vUZ0Sv3qg7DXQ9axtpLbB3gqQOfzdrqKxlx0OqI+YkW5GmAvJXB1eOraILOW/VR6K5+5sC+W3l8ctpa84lGipJwuIMdwcJT0PtNNA6a3bRsU88jrZb/f5uXhaqgFPzKlcjuVzqWlfzvYUDuQM/fLNlNbWekHw5AxAlWkHd3cZCKxVolAsmkS22whaTTKrZ81CKViRB6OLe4znRvgrEs37Q2rlDQqieC9nMaFUcfgbB4Zp5LBpWQ0ZOfSHfi3Hz7cj/lffv6xiBWiWotcyi0M3/L4bz//CYHIqhNth1ihgkIEDbx9/qGTFbqUVozUO2KVojAKTCSirvPC642IWgYp9bELW5NfmKakpd4WNVnCS4dVXdtTx6h+gFv0qSEBwxSyhOYlT1i2Az250yu4BCUgyhUoaHgr5cMNmy0QG0lPKMFATkkrbxfcFZv2DYba60BaCYIxMDNB5jQp7cOpwCj3SOWEEaXmtMe/YJmBiNKFLHEM96cvL3jXEpOYd8VGpTKxD3z5NOexc6e7G+1hzvQYTQhNpXvnlmrWlZ4ghptodnZlW5G8pFHQ/qfPfz4Oje7dv7I8AhYx0KBv5adld+j+Uz1xfbhV17uBUCitk1A3aty0t3PIioAFwKr6qpvUscr++p6uCYW3uyiUfF2Zhg3Hoky9TJgBOe1wuAoCTsFMjv4JrRTYkGztkE7QhRmrKV5uWyRw8gx7I3rXZBuGSDilTCVjcN5m2/Ot6ga2BFJVPWEr3TVcsKdIzDkB6F5OKiEhMVNdtgxPt0E5bUjLZqhpw5mwnamqqFkvmQUkBTPTJHLqfp9pmDUzgTUagB51dOvLao5mqY3ShTKrSg66xKry0Vdt5OBg+RRtJsioOcHig9GctCOpPSBgrU2qOaC7gFbU1G8loxaF6KLm4AKi/dbQ+K4V41MzPkUwg2WQ6XUv9bL43CvkbuAgzCxqVK7d1EpcpRPFcn+xYrXjDa+TC3ZLcq3+v1IPVs7jEtBIRO+WUnbz3AirBBjY+rWFeeR+idtzPrwbkoNQmCpbQ3sSI5ziIJIMJBnB0DRKfVCJnVSl8DBTCloiEQlEeQMA2+meWddiQSUUQDYbck6PoFKmR2wzRXIeeb0OvgaYXsFwwYqVkUuw3Df44JImvJqZWKzA5ayxa0i9jDeDlqIAZ6xOejOgssKBOmsY3Kb1dgmxMVFXL8NdEDsrNviuxwJZ7R7BGcE8v176AlQS+LKy9/8L36+tVi8pa7pYONcz+oSIRhettfClqXp1FNHCV1XMRVFf5ZJXlFJLQzLIA4CRJfqgGn3d7wK4FW+PoNLXh+2mqVQ3twusLzrdfTtSVikEQ1CYU7HFnDkikA6K52VtECwFQ9TmdteWqyEEtoRomDFY1WZlo2i81SYqAHNKE1HNgyLj7jGCJRmwr21Vu2L77RXBKxY+7QgRaP9XJQ15JcnerSswyVMbqDqpgu9FX5tRdj3mUhda50K3h/A6koJxJrNz12sFWyzWtHAWGkuuF+vIRNuKmF3dCqoRJKP0rjazfEWWSlJtZHjuhH7/S14u45pXtVyq1ro0wVZ+DTgiItQijryMpfWWm4ZGdlcHykRwDGpq9ftqYave1/ZflMhg1JMZpFNNz+vzSNVSOPnMAjHtHaUXck6flzN6IakFTQCWXYfgnOnMmZjVzuqGGlPdIaih5qZPCLcaBCyDfq9LKQTwKzizvTo8aySo61bwTHt9kU90pWVURO2/9UAnLC0hx62IrS82rWuHXJc8vbZe3fJMTdacJbRfSgvAOzx66L+cs2AzJwDEiBVBtQ6dnEqkR/fFq2WuMz0196rnaA63lg2oXFt/UcOCLgxCcO0grh1zghcY3so9JDkUmuIW89DYKEfQGFXLQGqQNpXeLqPeq+vAEpcGGTKqfxRVJbJ89N2EOkoIraZ0FR8ojOp61SVpP4RWaqoVkDCGpqXyNLflRekGC6NC314EslwlBYgrDmM19VsErVZus8y2VVRf/esM07sc62KzQ9mLetbwhRSglm4mMNaMAJbvpL6i85qd3tbXx9Ip+kqfhKCRqNvg49IfS7l9pQwsbbK5WnWxBDV5q4x1xgJI6yQAWSHIbpDX3uw+nruRcHZ5W/6QyleKCGQy6AhmEjg5KKv0uTdy5ds06OOmbYRt5ar3BcalcytoNYWUSUByqs0Ndg+Xdu2RlTVnkd2PL04gSVlK9Ky/zjK+VtaFMtfmKfSIPNJeAopqXqmmH11PsAhLy5I12FcDecEFt9k9baBl0EKx5y/schmv3c4G8KiTZzqX9ItVNld5/Gv1V4pq66j6KkGCcv2k8P3l+vs333VIaWW1Tjytb9Y3W16fslOdBee5hm0hPjMrzDrSgSIc6BmZusr1nk1wOSMWsu8/oHC2v6INtQidWfVvrD6FqFc16sZm9Ti0aM/SdbxVA0DgBsz73C+XXt7EGChRY1XuoTTROX+mtz2q72QPIK0apheyxIIwQBWzVWOMms8gWFPWHtllv3sevWOk03MQwfvMIK3gxuNQimYzkqJ7EWE1b8pO6baCVkSMVjejE1UbwjvXLsy+SoAXPPCZCD1gAatF1WRDbdy3jaAU4aoCcoSqV9U4a4H9yo3vL09/8/0v/+XTz9MG1JP0WNLiyjltDfYJ47uKrQoMW8sRhWoydhJWbdiVVGtkoNHja74kOiFWQK9Utn4tj5FXfvMZM1idF5RXoY3HI3CsXOPe64utcPwPf/kdBvZf7eMSSmz7SJnLdndSLRtR9tjBnBjbUGaMUHp1XIDGnTRiweIGeH7FPNCiNaUvNdzrlIOcWQ5crKeQADlTsZGDj6kPb4YNKVG+sFVg4WqEd0Vrcuga8CsDzml+W6WRbTAjWRKXrUyUpb/7BoWosLi8O25qE6NgnLsx3r3/LlJYqL92f/0o/3z78l9/+rM8q8pjEZj69l6sBea6TtYLNvzjqtor2S5W6MJhy5HThGWBOJ3hCyzrznqawmTTYjU0KxX0hzGW62Gt85ncG18KKeeU4WD0mVyquVrOu7fiwH0+FKzM8rEojVDzsZ4wh+Xo+jVs5j2jzt4xYrAhJU2kkqMawFY1fSoc2MZSC4z2rNOLX7GQQKTN1o7tPETSmXG95Mv8+PHm3+yFGepZlR41TmjLGlxY/kwMsqLOZSCMGJA8ogTwCtT6rQA5lhmWUKeyMTqdnCCKJXXXZIsAqK0eteGyfFPVTMAJvuo9pZG61yFWp9tkGW7WLkRrq8s5JBpisN50b0GfxlguZV+ry53pEwUay0zczx4AACAASURBVJ1YUtnaUn6FXiWACQqxq79NlTKotWWwiELXDCxDCgYRZSpYiHrhSRje9kGQuM3cY3/a7jft11C3quyyi8gOKNv3AjinYuNxy8edR3qLKD6+TGTmiHJ9wW4jWI3wMwPIKN9ayKqBVq/UFcFM1xFBUQPx7ugn+eXPLw/DsO+3jK1SRtnOqhNNEql+ztq0YDm6y+Vjm6VdK2EkOQQU2Wl+6FcELxBTjNGl2VX8z9HMljFqp0tG1DwYDS8zZNnVyP5+VG6UXZHYebW6IFC5Ck5bTJE7JZvCKNtzUHSrVFxAZhaS7Z3KrBBSV5UzA1XQqe03UUp3u7Kqlnb61So//DeW5dfctn6pxSVY0+zlyJVRFwEEJuDx+7fk/fnhy317e9neP9xvc7uMyt9jCZXVVTu1TSybxjw09jhrcVWBlfhXfepcvaStE4CsdLBAWTQkblIUNb2YM6v7tD8MyX/6l4+//OH6m188oFoZbRTP17qD1cfpzA7AqSDq/NMeg11cL1ZJwiL/aACv5V6EwTKv1+UKor7Ux2W1y641ul6BzkxdCGN1oQuaNl5iOzo7NAoqtPnKZ1Xq69o+xM6IDUe8TBb+N5FUm6DjoPD46cFw933XS/q1FVn99Vcn0UpFq/hz0SDYbaUp+iK5njYTmS0AboMEZkryPLzdPn/+x99e/uffvP3ni/8vy3LOVjJyGduciNEZ1+kYoWnvIDEPj8E5NWLEEBKsyeWaU1GQa2/UFguijLg9E6Xe/pRTYwtlCSqV4JpmGgbGy5fnnBqP1zoMhT3UDTrS3lAmtgIAbKtWEQV1wQuEkGWgrQZ+9z9L8qqo1QpCqQfEikjJUfOdDe5LXFFxHhlD66w1n9JGdllY8dTRV8Cp2VUtbBdKt+64xHd136qOIgotvNDH38TaH2HnCr42VpQZYtXqs7CeFbDiqMte0RDCPbRyvnyTjzNFNMUHljMc9UKtDqN4TWXl1/Tp7bcP8aunfQtQ0HSModSIKDnMiLGiRMOhsMGQjTxy2+N+m+NpVyKYznV02XpJQO0ohZvtCaipE4J1dAdHT8/23CAKKUZwHhqDx937w5bOLz+9PL6/iphZwkTbiLL9UdHB1cmsbGtrieUAHdk6cI3jRFRHo9ozIYLtU2jVlA7aiRpubULb/KaDpggpZAy0+bwqWyevjqfCnyudFyHDUj4LhJXhvU3eq3HZ+RUw85zAQlnRy+5el3Ihc3TBVzmjvXhco3fCy3m/MjkKH1ivEmvt005qBNeA/StjwAm+SrZLRJ9/DdRcR0Yds1Dd2O1F+vGm59SPxu02L4/bcc+4rinKWLstxHYmQjMA5cQYm5Sag4Gcxo5RHYHRe5WinRFhcK0JWVcjukOSyCByYruwYFCBcskw55TtGLy/zNvz8cPvvpvTMzNqMqq8uMs/TaTagK2uPlkd8DKfnNMDLicdUkTNXQBs83A9cooj6hScVebhck8vP1kZ2hvZcMWgjbZrNL9EQ7J1oaqD24mc/UbRX+iQSC8DM5anAuqDnirIWCMZ5YrtcFL7LIqKLCbxmtN8TmC43hAXCUJjsrUHFlbT8gy6u64443m1qOQgxaxJniCKttXob+UUyuMf//rNT7fjj09PP/7y6fnw5XE/bhnbKM7CRqSd62Gc56pUcSKZU9s2JFXC6tEEEKcx5tSnbNTIMtowWZdd01HGoYja0C67LDGP3K8byS8/vYB8enfVbf7q3RjE6VfxqzOV61JSvarsqH0VTxbSr25YIxuczSsICd9vGQXI2syz8lObec6StHyfWnFVk2+9893Jr11kC696GXbOzLCEpspEK2mh1tKrqC4Srde46QPV4Oq119zmAsdOnZi6LZjqbYYVr4UMG//5jLVGdf0hF/xeYxzrHzvgqCzjvGd6TqNEnyjQ5uPw9he/fPtyO3jZtog8UuUjSlUWr76MqIg+L2bUvh+Ecdx1eYzb5/TFsHOaQ0nUeTfqQyzay2g4ENFzn1jHVppaZ2sSow4ZFSoRzcMBxhbHLV8+v7z94a3tz3++5X3btqjjwJBY9KqZ16uPxawU14MuNdFtVN8dryMsnWMCS/lKSlIOBpgovnEyx7pkQa8zjEA0rRUR6o5bS1AtnvZWPSOrgVKNuaJaRMULVCf9vCYzLAVbi8S2flbRGEuSQUeMl0PUqTo0tbFYLFFjyZarT1inG/V4RfVeQyuYyDqSu/fXOowjsfRPuo5TB4CI6Gbfek+odvQmBiJ+PeIF/Gnw/uXYrjEzN47GmUa46zZRB/yVxYWG8uDY4niZ49LyYHlFLDisRFTdXkdqyn25S7ut/sy2jZQiaAKzmx71dNvD7vTL5+eI2K/bvM8vH19mPl2qu9L+2AbvhQVXzW7OdXLejpVXqb8gnbrhVBefcBYIhfqY8V4q1okHfWqTamy452/bBWOwwfTso9FaEV1p/qRydRXZQbCcDd3w7yy96KZXxlU1SVa2OrsEOgWQ5gE27GoPKNtQ+/r5zqzfqt2CGK6nqs7dYqNrwKBsNUUya7UNrXE6G2VQhetAqjo3M7ex9CVvH97sTz88zoHPwNjG7ctxebjmlOpMsMFSLG2FyKjRH3ZzOpxHbpdxvGSMEbBIjPZPGWHUiJ4MVKQ3sHSfmGshNmbhLVNTDNSNS5QeWzB43I+XT8fT+2sAt9u0lWmL2V6PVumkNQPgXgV0lVs8hk3glkRRALe6Tqtt0emF1317uc8+S3u1qVabEAyGXFuONGo7uQWIGPSUx2ubq/EdgNJVz8TWyab5XOWUZrFdUIAzV1V4V7NATR+6nJUiWLiqflM7nHAixNLtGh7WzGxXzOYqcvrMtfR6f+6imTKZZzADKC8qCnzTnZE3sodcUi0+IMZ//P3j48Ou4MfHbcCPH1/epo89quy0NNCpv7kbACjLqFGrw0FP9amV9THLAvCVpgUuc5Gbq9uIWNKU+mNpnV1AcuyDwO3LkYfefPdA8sufnyH89hcPDw+RBT7oUb0p9+mKfV5F/xe1lKmC+CVidJanmhquHmRfdcMzjZSEEXAd19W4j90b4RrKaQTW9bdo2jlO8JXyuaSo89qfuu0qhG7ld8HtVyH+VNjcx7G+Er9GciS7cb9ekTqjpMMMJr4yWHMZKpdLYBm7+jkLZFf+qx12vuQru3XvXVfaL+VxzuqvOyIydb9r/Oa7IcB7OHD55z9f/vTl/rTfnnYQfXrgYgHnSVvRYHetp7XuNoHi8RWQPSq1pF2scD3drEtvXq9CAMHoznYwOCj584/PD28fLg/bPObzn+9jH7/6cLlewym5Z5bqSkSfDls94zqbvzlS5b5gn8LblxwtMFYJYW2FIktlzVRyfZD6MBVXtQJVoDsTrYvN6jS8ysbua4kGectGBqwJgtZvS+Z3k0vW9AdKwOxLijXE4M7UjZC6HBe0arzW66B2W7T50KoUUI2HDg+j+EQlCJ+ldy2Om9rVv+o0sbWe5NVVSCGnhWp0goya+r7ftL3f44fw9/P25b99/Ndb/vzLt/eHfavzM0fB414zid3CaXpdCarPY287RG36xYCWoX75MI1oY2Q3AioeewtrGTugOnMPwJefvjD48LjZePl0i5027reyEjFTdT5lxVlOnTNz9W7RjeAGT+riU+pd79oaL0qDg+GS1kBEKvd9HDfxEoH+MGdicnuL1f2t8p0FVUL1VB0hhf5MppDAym2wbakOoimpB64jnZp9CYme03epwlUeVpA1zE7XZiox2Gx/4sqwdVZqKQbNLKrmnI3HRmNlmMfJXV03kPACludb5tJlm/O+7lgb5tioo8u3CNUB1db2d2/56NtPz/Hjr9+//PJRMW4/vwwvIl+UprYVihuv0UOZQTONykG2gPCJT1nfUp3ymm2vOYN03UKlMCIsmZDHQMOPyh0Dx/P99vn+7hfvOGIeeft8vzxeNJVLY6gTtUnXMbY5MbZXMFOnx6D9UlwnOdmyAsMBJxDKPtsCafVEd1k2AGHs1DRGHyFXs/UFw/udNroDYSlGGK5503IClBlkpYNXvLQKdZkM0Top6XJVRbVNztLm1l8XzitoWHy2Rsqa9mApal64juvvXVjOZ2kuUJCwM0LRTnfqQF2aUmMrRy5kjYXuWDB4ZcMe689UUuds+vj9D/vL48Ofvn/z8Rdvx5sL6duXObZtRHkqKhTgPqmsLTjraOwujC1111th1HxAhxHcIKi/FbEq61lPq8KvVmfdG29Y+vkPXy6Pl6f3VxgvH180xRFjj++e9oeLB2Nmch2fYztnSR3EKg2FzAc5E15zaRLaI7QGztY2rnisA4trWEs1bQ/gzMDsbtFCKq1qYZC0GaxZc559VixM0c9Tib84DFeBpTuAl8npDIQT/2nR1PVUXT0WNliJtqKWja7UwdQyxZmFVhh21V6aSL2TZb9sJc9sSfqEg12Xz2euqtwZGxJymj0vhnnX+F//4fvffnjcL+MYHI9DHPM+Le/X4bYoLm2kjad1BvapVDr6VjcFVNCyLL/auGvWYIm0C/Wv62UpxihaYDlGMPjpxxdL775/4hi65+cfv2wPO+zLw/a4x/sHkqzDjiMW3bM10feaRPWMBbfvZNkATVaqQ1E6tjWiRvUL+EDLr0fECC74sGa0cK6L0YKxMjEGZ4rBqF1TGaJ96LCrFnX7cQVSdFY7U3sFsM6t2IxZZdZ6FYHPi31qH2wJfwnCPoOpRLITvjcqrBzH7vO4g6/QWNXP0/YNfFVA0eMWPnXehXi1EOFMw4otkL7fFT+8edgQ+x8+f/jT55hJYtu3eeQ8xBha6skSVPqec33cYEVxqyndf0XP2JzXCqifQpeSmr0sCCkrZ8YYNUat6UpOz59u9+f747uHSmzPH19KORr7NsZIUImWtNNliSZNRk5pVmhXk7Hn4oq2LMcxGsxOjUFNA20W17rPUuFhMo57Cmb5oVt//4r9GdWKphnkPLRtMe/SasIHMTCar3tFjNzMzk7NCqDsNq1zOnOZsdXBYp3QCkpKlCwxLWRlE5SDu7R7uST+poPS4qDdceoRoliS79Li0KNqHWmI6A5spcPqc71+86pIjb87gwD0V/owAhz/+DdvGHx+vk35/sOT94Hw8TzBumNrl15W27kKZ6X7Nk0UuWuLDfqADZz2UCK6l7Zkbp/vj7AxxmYpVoLYtnHc88uPzw9vL9c314CPe3756cv1Yc/M69PD2LjT7y/YgqbnVDBq7hfGCB73HGXxN9Y4slNijbIZsMdWgy0YEQWXC/jXB6yP3D42QFKsM4rqzZPtaFrNUQAovpTWdY95qM9K6L6Yz/5+Fz4YNb2DBrqZC1GXHiq12UuW645BDePOeu2CSw3RO4KBqAMHT3Ti9HrNblHHcl+tBLcqQGfnRuZ9HlNXLnbWXLmNHdyVi4vk1vlhndUyPYIEjsPx7nH/8Oby9Mt3aWxfDttjjHEZmqm5CKu7PpRMBUOWo9SRYiZ09ttVjZWfuNJ9mKyrtOg0nQA2GaksSARj28dx5Oc/frk+bdfHHXamvvz4Zdu3TG3bGINA3O+yPadHGW5ner52yCN43KemWywovd2RdZy4qSxmasD3+4xVT7Y6tkuOIOFR0/0RFnSA54URVidy1Sz0BA2DmLjfc79sdf+oFugbf3qArZ60nQsuG7uxbSsj1YVX5SQ1avLidHBU1HQB5lnSXIaoojzFHRb0pdGzcIX01EB/BVhliN4vHXqrDdagT18BM9W3C2s8Z2kriqZcGmz13HXcxTGViW0f84e3//qiTJG4PGwwpHRW0XOJDjjvrq2yS3hsNUEpyFZW0u0sXZVGcNYiZZ9gr6pnVc+z9CoS22UcL8enP3y+Pm6Xh0vEUOrl8y3vc2yRmZeHPQLOfH6emZhTBsaI466cVmqdToAqoHOqyqhk1U1SSsisq1nG4PT9Jbct6r43Y6PsvOey3AOpkmqVruETqO7GtjqCrQKUG05jY6bvL8c2gkTOqlekVXGONZ6kgjWGXPV6Ad4KzNWnXcAHWHhLcHVeuqnd3uomyA1yFtvga7OrAnv5HBfw4jkbXXMYq7nEVteFKqJcPU43pfPSNLhirTUMi2ZpEDNrXEPj3//uYR+8Pevnz7dnOZ7GdtmL8pSN4qxw0bcMsoWxVb5HgDGwiD3PvvKpU7IZwboBBoqQopSlvtHNhm0bL5+PL39+eXyzXx722IdSOfX5Ty8P7y/HLa+Pl+vjDkTej/vn26/e73AxBs+75swxIlpU/fr8klqKvvNh/Zm9ZdfblObMbRvlU6pbGkOY8tdslC3/Fnx5pYMrBLBk6tgGK5mRMYJ9OlOJtDVHr5bFCpChnSMdVx0W+upXryCp88+XI6P0klKMT7ljMctXHqo+hPykdOf9HxZv5VJ6+xLxVHFbp6/9W3eJaJq3TMEnzfCZdCvcC0HmNuK4a/z++/3HT7d//dOXeZv7Po4x4nGLdTMFL10ftqUa/K38PrZRLDjqiN7+BIzKT6gg6o8zSvOvueKCMiOKK+2XQcanH5/zeT68u1weL7FFHinj0x8+Pby9zGOOfTy+u5bV7OXj/f4yf/1uv1wA8XINpW4vJhBb6a/RB+G8QhaOgSNpY6w7CcF9CEPB2jJCsgzJtaVz1ffVqV6y+1fR0NQfhalGnX4pb3sA9DSEiJ7A6iNj/Hp9ynLY2ah82MCKhrrGdZxA47llSsIJNIsPdh9WJNWHh9WxBLUFqp52AGEByi6nSwwr7BxVq+16hvKDNuqxuLKqpMbfpZtUu9VaP7uym8wxMO8af//Xb//7y3F7PsJx3cFL3Gr5zq60ekpOghIjMDgMKxV1kxjXjXjGGIw1v8Y6s4iuewSPOisRrGN66nvGzhi8fzk+/fS8j3F9+3B52i3nXSl9+dPz9e01DwXx7sPT2IbSzx9v85hz+hfv9ndvxv2edVe549BxEyO2jV+L8CSi7tsqxNhYw+OE6/7ijW4Agy5JvY7K6JTnOqaw9vAyumD5xUoy/Jq+9QCTjTTAjQQ4EksXoNex5I1pqgaVtlm7tBWh6jKsKczmejbg7CjHYlpLLe7uMru75QItOqOqMyjXh1j3v1qynE77RmfFRlhejKc9Sh1ogNW3/+v0vMQF04mSFeU62dnj7/7qnb+/PH+64Z5h8nEfb6+uzubGbRvblft1uz5u16fr5ToYHCO2nds20Koj64oOFgrHNsYIRIwxOIJjBCM41h38NpZa8fLl/vzTC+zHdw/XN3uQ9y8H0vM275/v16c973l52N/98CYG510vH2+WyLg+Xt48bt+9GYCfP8/Hh8sI316O2xdFYN/Gvse+9TRNIw73EEMJMWeNJQihRtx6G9adX226jsAE6q5LOFu9nRTIU5BqItn3Yi1xru7w7YUYW2qqeFp6uiv6ogQjdDkSVCiMsf6x8ZCBdYh5FTius12bDzd0Kq9KnxzOJTSjGxMtgwKOPtUOp+ehxzXav7IoYOtaXyFIwCpUilbPivIWnFtL0lmZsR3Px8c/PueX+TwYt+P3+/7du8dxDQEp7cYT49NhRIwIjrrvCxhueFU3Qjotrej76XV7uUpR0R1hZs575jxyOoKXx+3Nd09BZObnHyctjnh5mSO47Rsn3rx/ZIznP99uX47nT3fdJoNjGwj+908vPzy+e3zc9u340x+/vH13fXpz/elPX/7wL/fPT/d3312vT2Pfx9i2mj2935WWpkqsyYltq3rvWUsKxcCo+/K13sT7POC67StHH97mpozRgwz1QWsAYEIRDg704QQlPGXlP5w47iyNLTFlNcfdpMEn0pJRdx6PjJq06nvsln5wqhXVNm7RoWyJKrsHlxJW9fCkBVxHA8RyHNDl/Op+VosXZN0+JtYWeNXSKksXKO1GeA04VKTb64aYgPgff7tdhh8v+1///rt/+Ptf//u/+/Xj014oioFtiz02mRzuE302RMSInjkeY5x3fUcRsL4bSu/xKR1HOj3rvKcAgh5QyglNRZRQF0i7dVoQ2LaR0/M+6RYHPn6+Pz1cAjxyJvXudw/bE//w8fnlmD9/uj08jriMzx+f73cdqQhsly222LYYW4CO6/XNwziyb0VdI5/cYgRK5U91J69QqARTZN30E7olt77dYgASwk6agREjulOyBsua8FVpjBadVhOcrT4sY1UdMaySrs4uSdV+LhUhvuJUXD7YLv2r3VJpBc3H2tdTELW+q+gXcaYbOSsyUY5a111Eql725E0f+tIKjR3VlLPcNx2rEimvNbTTMzEPzc/aHjbR23/+n/7qr3/73V/+7ru//M37x+tgjG0gYjA4IvaNJLdtRN22CgY5gjF6JnGMGKSJ9fuZ1oiaOAeDMUapuxF1qCLYfeAqtDDQ513jnOnuFhUwALLv6V0NaixcAGECFKYwXkXpOaeyF5wjSAu+300oEyTHZRQmnqnS4bFxifhBJ8hMl3BT6SAm4tp3LLnUYe/SLdN06cQC7nM6xLrHj6U2TOiYGhFZh1fDnr7NWUuUU7eZsmZaqQmQPmRDs+95U5u3bxRX9K+FUHUbpRC1O2dZWiPrCKAPDFYRwKyDeLQ+FboLvo7DaLxJDPXIxspdjhZM3Op8rDIGoO5DXHfqc4iCM5/z+Ce/excJbv/n//4P79/sdbVHxBjYxuj7MheXAZBZE/4MBCJsJvretDAK8htBj6h7a5ZBJq772AcMlEFU1kDdYdEdMeVyrHQ4ioh2VcfoGyh3fqseKbtmYBAOOHAxuOExXluO/19735IkSbLkBkDNI6t7HoXCj/AC3PD+x+KKnJnXleFmquBC1aN6rkApX5RUS0dGRXqY6weAQoHVL/7MXLBQePHJck0JdbyoX0lsamtpoH1pXvYUNzAQRgnNxpB/esiQEQEMd0606B0PSennHTpXZiFrXlBd23OQtHY2bwer/rM3+Q2tl/i0I1V32ul0QUigK/Ghr7IMZPmUM6uqTs2UYRUKedLbVemddTLv3Q0nCj5V2e6tnN1Fp3r6ttIri4U6VTnmrzzdgBaSVXyUOyGfrNs/FKewhPJJqCNTXlhqQgSbIyK0bYlZU38+jq6UYCcphYImKZeoALpeYGamylVpSjSOgI31UPI99c2vC2P9U5/pg2epuhC/9MlPwBqKBwRCCABGGnuDwhJINGKWhZf+Rts/75Cfo/a0+b8GuQoWsqACiaWJrK20jxhlrfpRedSUGtzjV8XOX0UMxlIHU7SigMLVq4sLpaGC5uMZiufU949gethHddy34tVP0a+NWjmeRq2bnj7o+bP+duiBtljpUdks+9G7pV1GZnU1l1VZyKqqgdtPulBZzDzpLnbKbRqSdbvyVNk76/1H/vs/boI/32fdP+//9MVopuz2ZkZwNfNrWu5qmbPuV5SVFUMEkoCWL1tUdMgrw6dD+b6b5fM+fl26rvAzcnrKS9AKgNgbBewnacpgTMAjcT/oz9NjgXhsDIQ8SPy6rRCm236+qb8Gnpqv5Nc5eA6WnzCGLlxjTk/3ZOSvkLaIdx/rWSn3HIanQm2UrRFSPoem3z/4NzjCAHH237rLAwPlOQ2fD+8Bif/Doenfrhmlk88TOMIyzLQTUA2vdBQvfCCSVtgOQdK0F/tsDXpT1GcBhLHaXb2B6tJhVSmN4hoseeoke9H2uRpts/+F/u+oyn/951k///nPnyuDokT6FTrkPeirNTC+23glgkuKwBURgWA0zbVBUbsl6FIM4J+wJK7gF4kbuVFNGtshYqklS3On1ihcEQRjsmSx5Q4fRGEix9/LuBl78NTA+lv8m9LiCV34/OVvTV8nrxkb+SjsfnVlEyr6XF7r16dtIkRGfGpH/Dp8NhRoO4KfB38EVsyH9AOzPQX6VD6NVJ2xGZwG8iOGqM8hm7z5xKr+T3e39/y9qcn6dSvq8xgM/cSCKtNw+rjaXDE7qbC7XT6t0cC7PZrdYGzfIpLRyQMY/qRvwOf5AuRaOu/7nxltBk8cYZGfyYAlArgiHAjCh4gocRNJLsmoIxG1FO2LIXD3Xudep6XYvcnSjEVCEQCquEwHNUKtz9czsQpIT53UcWUKqf74j50BPgmLmB0YbPFja8tH4jtiEWIYZz5r3Pzs8mZjgA/J0ndQA5tymkBU4RJe61fdBiCE1WEY0Oq2rgHKJwIVsnCEYBfeqMJtZOLiiOB6Be7nW+q5J3w6RkwNMKGrD6hxnofk0Tf8x+fqb6/Mv0XW+dN080hjTNp1IKft6KkoTqVnmGh58qOZ8kdj+EttPZXnrDvImhI+f+bCfjNydJwDS3cGoUg3spk0mS3/Da3FhEwfIGRSV7Akk1J/GpuY5rE9+sEN5HZTZCG7JWEkbE4RCMNrVv3ouESRpUYrqx2CWoL8VEJjVTxbhWlQrEJicCQQJzFrUEj2proHvOzJ+IaXexy0B0yk9ihsJLOhWufxWmKHsRUT/4QJZv3Pf1ItjAi4YzPQHd7+WytAYAUyp7r3Ry75iTp4cpzniLRLeT1l3OAWhZqFa3POWrqZmL982osuMf2rkZfHmrZ38MycRSss0BI2o6bhq95wUWzcsIaMJziiPgMkWV52MaocXd4ltHO5koUIRsNGZdEkwyYQKWlIthCXqCp0SRCUO1ikC0dqJ7UeVScQRUFLdCIxjzgloXrEs+HNfETwMC5xoYVhGlt8uKhp3IlxyTKF6RNK/jx/ncYgtOFGuTeY+rg+/JCFRbq73u45guyhheAS0EsTnixrtoGergUgcQgTuZuAwwpI+HGhDo5BYbXPWz4+gY9uv9mTeGoD9GumgwA9L/hsuu7YFcSpByEdhyXMFA8eVeEj3p3mnShgYfJmv0/6P5aMkxZiDjGbHAXbQ9hVOKhyl779HHQlMFM82TKKxvDoU+O+QzRv0IbrFPgK1ML63/96A+u//LG+FtdoFbw0MtQm7cRUKIgIiFgaHnMJemwUQrgiRmULcObwWuHgV8+ay1cMhi7+sk3veaBG38r1UVzSGQAAFSxJREFURefHFRRanLH7ruQxUZxTmZSCzi5WKCA5I9MdRFoJPRCTSECewTcHVCgmItgPFUxUrZhfvUXYH+qyP0WICECBJVyJJM6eqBYGAiysDoPCAl4Lp5eGAhJWzNe/s9lhhKZgH3lm/eqLC7iImVTtYpHIxHngnkZJ+hD05+en2SQOsPgRY80pzPrVOTE6iNLsV6rmQ7z8tya34CoC6drFOjO6Y+PYlXWil7hWmvtglhqks9eLO9f//K/Xf/5zLbGMS44+YKJgBmRHQIwQQgwxpAhfimgWigS1VFrx1MLGSRiZoJjZFVIbdkVVZ7D2VzGmkK1otVYV7KKEAhlds/R3RGfh0Y48LB1IuP2a2LxtolTtUIUel6HRPaTd0KlnqMYuX4E2anyBoK9ATwZ3snxdMegJOfGmgCBe8aTIT9X/0dZ54tyszCN2QfjVzRAI4RSuaCxrGpcunvv/prGNBQD4cU1JV4aIPRt0B94rD3CT/fpCGgeNZ86G3q8A4heIczyqskyIQECeXN91JAwGqnCMCCwj0Y4oYUbfAcLlnY50IpbKBqVT+BHIUoKJ6uLq++31tfS1eiytXeAl1AoDI3wIMoRWQjfxUECiqvDPrK+IKzKJOA4JdFXtllxBok8aQIiSyIQ9JMDjR9nn5ftOmGqrPKWAQhajBUdiw9/OomhIIl0pRchZ9HineUp7MJ39PMVjSZCwDbKEUAz8mUYdA2XFEs5xiIxHYniSQawFGk1XdNETAjgpsk9xNzSYDRGowh4PSLBAo59DErUBDi5zCnvMpfqx+NW3AjidN3Pwjs4EPfG3C05kPul1SgaQczqXEAsVOFO6TxvxaXL5IHYjjez2RejitsVbS/OCQMeOp6MHjtMIdsdVvVg30z3tEoRaA5uAcQkrNIepCQY1ETRIDTEkeK9FN4jTpW2C1JJel/54CWAPhGYPps7TVIB+rC6YquvmBLK8VFmPLMvPWeudunAmLRDKiT+d8kW2OJfhSmsEP+7f8AmU/ZgCbEeYXnMwO7Y9vtoNKrpkiLqC4uDMrW0JRhc9vPrhLoTAggIUduG0DoT4Q7hmPh8jr66nFSBYoCYi3oUw+Hj2duCZWdiHd95db+XTHD+ZcTTMQBZyMsWU/APe9hHnnDAbt7Duef99cIwC1pMOoKf5aIvBmJVzfcrryRcdaPvXeT11HhvlrmWgHK1LJEDv7TvrJCV1z3LE711/XFo78b5bqmBSpYwiaBHFElnbAqmq8goGKYbD73uzDU3qXCtgh3QFNHC8+7hPLfK6ujJY7kKUJ2ufpq3gAQWTkMIycog9dGC5TxEmca0IocDMVGkzT7rK5T6ZCIJUT/jsc8rd/bstptqKGzZKJJJNJLtQDrEqPlvDXPAa1ACPhqIOylCAhYMJJ28OtNGJrKvHXsF4aToDYmpbP7xCi2vzwVvwdKCVj4HfA0DU8+3aWIFlOObGZDNgD+bcTNoAPcApZCKm6ISNDSRwCvfBCvyIh2zIObX9sw1o9wxfPg1vP0udnf00zpdwUvZJh7gWQV7xQcRb/IKdXj/fp52+rsXXQrxksMU+sdRx6WvFWnjFrCcTS9Sfr2X4ku7KbJ9slw+/LsLYVft4jaLR39/7TpAOcgV3AXY3EGW460VjhZZJMmse5YFnwJNWAOn3MeE0iBN9E4ncfjuvFQc+mR+It/0KAkwUi6melnbazkkdd2WVxQxpCVF8LQCISizgEpageLisPpbEJcSasvokdE0f1yVULTCRhHLgWTXA9hwXCcHpHno7VmEC5/wnB7ydfG2YOAV1pC34sRp82sjBNfIBLSTs7JZw/t70cRB/XpMZ6wGuZ8hjik1k4QA7q3ynr3g2x4v+BlDZz4hLXbx7kD7UILcJ79MTMSSwJFzSWnyt61pDAMAoEokuVAo+qaossOaIlO0rIqJOYufJLBBfET9eIvm+cy2/1qoqUt/7ALyzEx5DU6JhFoGhhW33cT4rHkiUx0ulNyLWwbdPOVeDMPbOwc2uCJFVvk+188NOXyv8aWy7gywkamNw0RcfFNPOY6+ubUFEh/Orv7widCbvSAMLdzyUQeEiEmi3NwFNpuXgxjgFcUJXw2CddvuLX0IBxwCwc+jaT0sh4RTQfGtXA0ZtQJBxCXc9pw0QsQ13lm8MT0/iw9+6llb8Pogduv38WMN5mIZKLMn8cTUiyxFPluvw2K/Fckw5XrWTbdAuysQCEqzyFYwuGtel15qh6511ZxF8LS3hkADe+dkLAC1eYm5KTpPpBtmvJRu7Km8AuAI7uavVSWdnZeLVbaoqGB51hV9LXb25V674EZqYPSHE0cMYYHO0CvfBzqqgv15x92CVPws3mFU4BZYUtrPcBGNIDZMo6HEK5iVFYFyy1P8c7UoLu3xXqEcMujoxFrFimoPuv/qrPfd8wZ+qv0Hdjq7rgcRardo/+I2nv0uQ2Il8tGTkpOZ4st4oOAAcuM0muwvutO5pS08hA3xa4/3IQ/hAwSgkcQ7WI7XrHzcnTHa+HnDlEdd42Kc+rdtuXYxIP1a9J00eDbiEOviu+nmfRQhEFrcrM3cm7HVpn9KzgktPdSiCb+zc//ev+sfXFSG71opLVmvWVPfttfTnpRZ/Z43RCNqQC3WJR7PF4ApmGUCa5ySkIDNrtQ61rJAakujgQEeXM+7KTFx87zJn98cuOz8T2Nl57VpRVXe64K/Vt8aoeBsgl8qpJFmlRp2XV6ggFxlGYp9SGc37N7rxPgCwMBW0NJ3mPjiFP1/TrJE4ngqvnvYND0jREjMKygFgu/eMh1RoQumXRKqdGowmOshpcgmcp6j/FGSLSKKMv/aclfOw6R/S8zy98K456B0AFkYz0o1Yx/zWccDjM9oq9Ka/xZ3clZiyx4/4Fq/gH0vrTv98m9w1svhx5bsWY94SRWTpCoYAc5n/7T8heqktWwdY71N2ibD9ftfOIBjhFYMOEW5oYnNFdDNmGQW3aK2IryiQwZaasIyok73bWKJ9Ciedtdfiu/vJPbFuZ+1dJL66kAycbK/0YVJsF3gfLs0CqgO0ENKsTPeszGvxfYzRh9ZyLxbiIq6+8zZrYMtolBW9LhkwcAOXsA8QCGELPKMvOu2G+Byv68Pb5iBkXWCpWaPJVkiDj1/j0oMAf4h/43jACz0YRAfdu3D2E7GmJR2e8qO1BZymPJJdus7Jwkr19MTQ4+l71+mBKDtUJ21Y8hVNrFQBmUhnlO4sgJy9h/z377Pu9NpHLc8w7oN9DoWvFT8ufXXzgDqZbafXcP8regcTT1ZT1YrGjErUChg4ldWbLT3bAlpMc7L2GMswojkt9BbvHQ3XMeQ0K11EnbzLV+jHJRJ3+X1nZEszkeb3OfdOQO9zzsFr7T++LgUFXEskM2fRjFERBlVGJqryirhdEZ+nMMuMXffHWxVJ8mTpwRHV5RtwBfLYO68gUHwnQ88qKOBuhc+ZShzAS5MXOk2cj34TMBExRduaGREYaEvSDv721Hz5sJZlvJ6esQqn3xbYBzvxdQHGezCeT7k29ihKUNV75lGCjo+tUz5pnFpUdywkTrob0L/ufQWreOwAVvA+sKtlyWm6KuQ2OLWdQGX98671bz+3vZYAn2an1mJIktP43vkQYCCLxBUhYZdz13sX2RgsV7HsBt/KZBsBPx8RdJCMhiCbFKoCT6uoZ/wI0VY7xinu9PdtI2klKqu+t1oGvUIYYxIYed/51877HqxN1PskD0I6mYVfm4Gu0A1vFwwpBZ1xZBvXWLHXdUvnXAswKbqwFgidqnufbCNuqcpLFKyeFLT7+XxdqHZJ4aDHajHBO3A9qEG3CIHRSEZjIjkUeIexfUAATxsxStpupNk0OL4PSAQHWmsoVcC1cBoQy587naM+WIrRDJTbeKOqWEp1LmpdOwB3TPJTjWS6WZy7GXog4XOzkK2XlHgJKb53dlBumIVglteKoZgZzfPYcLraSHcISGFNe4gsf5/ax6GGyqMJtJ0jHyjifRrHmqNZjy/mOl4LWd7JKyD6CvYkGyRB93F7UJ9Tx3A5VrNbcU71WvkrBhZmzGDv6xXvPDt3mT+ukCLLVbhWlnXnVoO68LXilCuxZICmc1eEev42s8nQOoUfV5ykgTQCiM0VcCXFPO7Y10NPEaHMV/fs4jGwEYtS46layyNk6qesKe0E5OHIGxxBDnklTe7bRgPF+QxATIOYsBpgOyeHIC2vpSZQpsYSUXT5EhK0uWgFCKbA7oSg3iU+1T39CnYerqpj3BujhH4O+TM0PPqaerrdPLwBl0+5qhrpBBBUECvLmdbFysrxuKGrsgmt6i6VtQpo4CDL/urjWU7XpkGIsivTwIzWiZ1DxK7KAfuECDgLJ3RFjO+/bZaaw0gDrXVgl7ObqKq0L1FSlm20NGwSAuzSj9eS8ON1XUuZlYLpYwBxXCouoNpJhfNTEsr26Wp7/Gdea11CufYhBJkW7uMqMHyBf3w1Et42IQqiW9eddR+0q3mMhIlBvF50GpzNPbR7RkyDKhNolIaA9y6ofb4hkicjAsA+Wd+WtBbtkvS+q3cC2s7DdN3HEW0o1vYP6H0rgO/t75MuXGveOYIhZe4sR8QaGtbjppAu+969+P5UWQoIrRp6LRLYp0DMN06ezDQ6OWT6+2xCSwjVfbx+7vpaJHyGl2ky8NF+IHFw0niznTyC8XqpjO/79EdSgJCYALrKWeQg3sdwUozgLKquupauEIw7m/mhhDx1vaJ6rwZZMwDkiPHlUO/+tkXsqvv4MpfUaMjXK3Kb1n0qjZ3ZU3NmteZsn7PB+pnX6jPaLg52eSPZG8RsMsCPF2blRoiyltrFFrfrtIs7THKRoMoFWsA+p2fv0ds8SCPvmwbOqVC7MCP21tIrmA9c8HXJRBbrUR22vIAkcai2eQKYWXWfWu1LZl5LcL0TV4TLpcqDqlqhICFe7ODKEHbWv/9MUJmMqGstNS+s/HFFlU+aYhZsn6w2+yrD5vscDzbCLBh1krAlnZwu2p4s2KrCffLbReL79vq3v95f8ZWdhx/BIYFQr2DGTp9KmCv0dYXEbitOog3D/rEyrkipea4OkIVq341gtEgQ7lGXznrzaboaUBV6a+y4FuPjAHvaTa5Oz8KI3GVUrRWjcDlV8H1qp1dwLb3vrJztAYBfSybP8etioe5kr/T5Wu7JmiVmI09iGN/bVfW6tNoqpBBRCTn9bMZyHhsOCfbJHaHXUoh/6FXA4wjHHgmPcbkKwyp0R3Kyyly9wQPr5/aSy2r99J31Y2kflPP7PjsNYO8s4hXe6Z0WmEaWWyS/FD+u9ecPmSK5T5VwbuxF7hZo8X3qHGcbeWWRu2dyDa/ga4WIdGUpgHVpj91fF2xoTz+A33uO0injGQluCO9UCWHXGesanlN/vWv98bUM/nUfgRGOR+77c9e9UZUR+vGKFvW/TxI9WOuQVkg2yWNlkYWUV5dmHdBLh9lb1QEvo0QfG6xMamzuVtD22VWuRYHjI2zMfPaSNAYdRZvROvPhEj36flHe53zMDXvo5HvXFcqq9+5x+mZfnOYVLHNXZY/+nnwXups+Z2Q5QSaEtIdDk5GZzXX7ZFJcrp0wSua1uhfqIbGwQTZIMLqVALG0D3bWOcfkpY3CNu/M8ccu/J/79HKZMk+mjbss1Hea48ncXWYb5vIgf951Um1MgfIKmszjPFY0QF1XxH2fuxU1MFHXJcA/b777hyEpN7BgG3+986D+8bqMNuLMuFajIF3MZPbuWWSi3aLOuVubjynNsavWe1uPxQxybBsz65yS+OeP6xKBqoKiN4nXRUoBVJalOIyCZZ6eU5a6XgwqUUgXuGSFbLzvNNlqRDL6KfhO76wgI1odzJ46FItkaHXO3uV9Cva6AK6/3pV5qsausDLzzSYAQqgmreAwTL9WiyWqdUo2ft4Voa8VEXAvtGpdbuFGGTp1yvhalFqKgqb5Qv7n9z7pr2u9lihs6sGboY0Wy9gMJnq/sXoPAQkEraGD2OI3aRl1ymfSZRLcx3kyVi8GGrv3HqcQuSLukwD/+FqLvKsGhjGupbQtFIhiLHnNosAfr+sS/vzjx8n63s3a1T42EE+X03ZqBSGdM13un+8Todz7pF+gTZ9snVWmTWcyZm4bAN4nCUZMuhCxEv753t/Zs5QWJXqF/nzFn6+1FgVc1+UsRjfTGDcvO6QISmYCcCzhZLWiF25zf1GhD0w69KlCtIyxwnx4mgaxcKrynAJXUERW/nRV0YBo0efbdzjIU5C8QlVVs4CsEYxZQNBog4tFhlDQiCu7Y0n/VY6WSrME7ixSf756trs9KrtOsF2zuQwI6euKnVmAErezjSavwE5TVpmoba7oMoQ9CrQiTsJZS0DhEjPxzYSzF8KOKpcOgVeE5HDY0Y7xgIJBEvzzR9ynRB5bFEPXan8wXiOz8GNMhBYE3huc1WgeCb3U6tsQifj5fZrpj6WeuYugi5lQOF5XmOl6j8CQ09QW7HwXq33txTDLuE+VUVk7uX6+84p172OUC5J/XKvLoO9dTIp4FezCXRHRzAORJO0Ta1JcHif4/T5pX9FDepLYdpgAIMUYI3SV83iiokQt8c48x8/5cBUVhrlPZdVaEWSsEcA/E2SdPU7L73qsoMuyHytIZyKHIOY52TNZe5uk5IgW7lZIEpZ0Eq7z103nbiPCa619/OePHrhxd4hli2kjwnDex6JCaFAgnq3NWVhBGAo/OwDyvauy/uXP6yEw/T7nxxVgVGYjxgLbSmzFahueZx7ZuA0z7bYFOeVgr6lqV16iF8u3vMV4H1dmhK4rBLwbzyQE3Cdb79VbDu7Zl+M/XqGoGVEgy6ysOC5zd5B35bPylI/ZbSZ2ph7Fs637ZI+Iv8v8X/8jCLbvA832SI9ZpDPlbLR+sD36/SiQOThc809lnzaxBtaIuJ5VJ7+IcLRwqgPIg8kgguhnzphOHx0vezar5RsMGmKMaxjwTCLkQwA279fNztIMU42K1O0Y361+zRaIkVv1KWnFG/k3pc05NnBdbM39ksBuj9xfFRrs54whEI/WcnrkzxMzojZAVWlTT21q9KLwcZyOfmFr8rrf7KhcBtG7JoNjp61gG0iN64/GYwvGx4oqe1Ot5KpOFz08a+NU9dykm1tq79eCiO7X8OtWj+YyW+o3x4NucQzZt7g+3+uMvLTdW+WY8v2+fl+/r9/X7+v39fv6ff2+fl+/r9/X7+v39fv6ff2+fl+/r9/X7+v39fv6//r6fzj09AS1LFA1AAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9SdMlWXIddtxvxHvvGzK/HCtr6LF6EgASEyEKMIGUiUaYybjXRv9AK/0Umf6AJDOtJDNJKy2wkEhREACREECgG+hCdVV115hzftMbI+L60cLdb7ziT5DV67bMrDfEcK/78ePH/d4Avnl98/rm9c3rm9c3r29e37y+eX3z+ub1zeub1zevb17fvL55ffP65vXN65vXN69vXv9/f8njH606LRQCEAiFAhAQ+N/xr/YXIEB+R4Rk/IoCAQQkFGgHjN/EFwFQIP418XP4gfwc/idh7ZfxNol2PpG4MAFBgQKkiMJPkjcCGCF5F/l9P7nfnKjQAPUjACpCEAQ5HqwYi4oRNIoiPvZrVAhEFCoQVYKH0UQFEpcqx9cOxN0CyL8x3zpIEWH7kv8VB/HBiduHMH8DAzQmKuYAhEDoY0DM9835ZPkBAREaY2IYM0ogR8Cv1iBCAoRPMeOMAIwERYS0yiJaVCjkBCqEfngffbKy+73/7Pv9skBFSX9fZLYsCoufSUUQ9xz3SYX6qXxohGCYjoiCYQH+p38OiR/4IIZ5EZCiIvFtvx8cHVrdMsLMNM7kf1GgaTRupAIREYqYVaEiLt8PAYAqcer5LkUhFCoUNJrV3eVhOWGxUBs5TlW6UgQUKaoQioqKdJ2UTrtex4rrzUEWqhAIRMLDfCjgnoi4/7jOmHAfqWZfBBRAOpqIiQgRxwh7cTs0ioSnGQkyTkfSv4QwC4JA+qCZWz1IiMFEYARoVNBAkiAp5qYNxivMkH4wkjRSCZI2HXhWStcrIeNhEh8poVWBGIDxYF2/LIuVEtpMpE2qT4TPcg5f8y8RUbd7CeCKu1LRACyBumFpG+v0ZyEahLllKFU1/EYAaoyqmKDkJaXxhYWaX1Zcn8aVK8StkFUsLShOLHH5Io5HDqqO0IHIBFjLtJ0WHVaLUnvqqBBopwqIqgigoipdkW6hpahUK5N2i6IqEIGwAIQCRpNpsr4r0kmguTarC2hwjwnsc5sIdPKbFmsO7L8nikilmR+BRUhrWMT0XYYpwz8N7DOapP04HIGEUQRCA2CsIkA1CAjC/KsEIaQZRQiDufGZlSK107LoO4CqGTMENAJKgKwdBICqxO1JhJdjlHd3NwecjAbq+C05NoFCIuGUAkUil38eY+gmmAOsMXglZsHhz45C8Twlgado0KAiJmFqcOzA8SkhGgEbVCQfmOO0Y2HGwsDgmHM/i0gRMUU1C6wJfxMB4WalwikDnMTvJ8P2crdbD+O+1snefv9iedY3WBVxYxDARzWH0d2DMU/+nnnAjs9Jw/1F/w8ePPzV7c1n203MqN+XCKAQIyAGKGiiQlJVzJDsJyK5tAgFUpQwJxIKsfYpaTEHQlgGI58oIU082rl7UlBUxuo2G/fhU9G5PSCiiqp4oPIxY4MfmaGs0bKZ/eRfflbRxprQiJ5YjHLGFAHzkG5BSWucebitsmGeX4QKBGLpCx5LMTuACo2qEpYtBINVNSQNM/Soo3nSIzraXMcPJ9IVWPAdDdcSeOgU9RGDqqgEu7DK15/d/uJPn1/+6npxsXr4/XMpevfRycl5t1h22ocDitAS1I+I22ysgrh6ETpDFCgEA+3VsN3alLM087CM12IeFhSk0OlNi9TBZmERnwkVhTEAwBjObe4FtMbAqRAL0mbB5pzkNQAqimkU7YIy5FR1sz9I8EGP8HHlEvNAUTl2rUaRCLgjgEmTSRGIJRAF+dCMYEhKEqREJcxAE7Ua6nisdcsTtklR/7nDDzT/EcMoMagKNQ36JYGOcVT4XQRm5PQ0G3Re6TROhVakY9DXuASFipZStIRRuuEoYMCbL9Yf/+nTy7+/3V1N69vD+mp4+fnm7F7/4L07y9Py7g8u7j46czqsmBMX545O0MPXw7b9hIhYY9zZ+MH1TdDKBjHwyGBCMQSLzeHMpMvtCEmN2OY+RjAsu2ZsU9ItnWpiHsFVxBxrJMA2kg+33KTRqgJDi5CdRIBhZiJCd/fgonEZyVaZ0dEn0yda3SBbbMuoE0MQOeJMRSIjze+mpbrVZk6DTJQQ0xf03X0hnZLwu56h1tw6Emczu52TiXxPEJ6Tkxm+JiZGKMVERVmsUKVYNYpIkQKliHZd6XpRR35WigdR2b7Zf/znz199cHO4MhjG14f9a91+Obzs+fKt6/6sX78afv2fdOcXC2csMl8mCHdmUeWxzzlyqLuJimcynJnpcYqaI5ECQNpfDA8txp2EipnffiM0mVZmBhpYEKFB/CpMPOBTzKOt41+c3oO0kdquXoAOaSOzX7fbRcNcaYn5fOUNBSEtlfMwJmBLu5N9iAnFk6IIyDMRDrAKc2xhdTZDv8G4db+b4A/aAk8CsyJS0XQZjzqa1g7AKWAjdprfQuYMHhpVVGBUCrSo0RrJVBFVURUVTaYKEZnG6fOfvn72l5f726lONJQCiBgn2ISbT0fpp8Pt87KUX/+Dd07Oe5S49ICxNJQ5vAVhoEATC3A0FcGWVGBtGuOALR2AQJRO1wCBivMvdz7SJL7KSI4z924SR8vVmbAfKbCamlbxqJt8TovWOiXzM78hFccLN3LNWCIqfmcJzkjyIccyUrBBB4Z0vDblM6A3hMrkbuZEIUUFbWxpl/OUsEW3u+a+lFkaiWPGUUXmM6hzxDlX8auHELB2bc1044aSJ0RAE1GNoxR1/4BDWCkQiCoFYjQRkHzzxeaLf/N82k51cqOpoqjEBHiqUEfefjH83b/68hd/+XLYT37pIqLqx4WIqDiFUNUYhKIaoo2KiGjimt+3tqgrnkExDmLtDgOqGvcIqNHEdlKOXmnsOQASX/Q4EawhHJZhD22UoW47EDY1QiMpbAQSiUfu5BK8NlEDM2uHJiwHpz0C8qPDRSpAZOB2+8kLOPZM5JEbr/UvMDPG1AX9LBrwDzA8c47caezupAhjawZ/5JotPs9ZZzDpGS5y8BXqmEKoQlUb+rZUaP1qv3l2oLFTd25PXOL/hFRIJdcv6gd/+vSzn18O+ymMJcdcws01QqeqiBa3Juc6ENFM94WiaO6VVnTsxaLN+9vgu6NrjHBAcRjKERr4O5L+JilQOsUQ1Zx9z2nT30U8nbT8JoQinVt8SBEuAmrKwTHT+jVGmYpUOpE1DJnh6sjD0mWa/WTc9xNlMi+Jaykq5Hfjjludoh16tnOAMaVh00gMZMSHOQE4cgFkLJjj9NE5j/zPGYtqqJ/NtZve698e99OrT67LxNUKVnU3cjugqEq1HSBAAQkpwDTy+Qfbv+4+kyLv//bjrtf5UiQJhaow+LXFpWkOpLpE6nSISoHHQjTG49Pg6bQqDE2jS/U7cEyDzKR6QHGXZUr/5NEwRW4pFr7TDCO/4/8oRabJQj+FAOgCogiqX2dODlRhRApvCQYtHXPRwNUHY4wLEqsk7FgboDCjZdCmBjsRPBz88srme5PMUhsexkyjgdRM4wBAXZ3KelhDSsSPI43wgU6fTAyVFElBEY2b9xkzQZieLHspLsoqDJkTEaux/tZ7i2Xh5oBP34yHirFaUTk1VLACBaG1VeDVx7vPfn753o/vd/cWIBkEzJlhlpeSvh/dJgNlwlsYqCOC0oA5HCWIVA5oMVKEYiLq4SGSIEGlZxPwUpzEjAUORFaQ/87RdJkDqcP7Z669sc04SRIdnXIoo06ESPlymtmmVoH7y5P1tB9tvoAjMHb54RhyZgEukEbE1ZgGWAmSgGdRbEJxyzIomO3pSG3OYCRzRG5+jNmi8k/JcJk27/9tAm0C73FiDHSdFnFpJPDFSUXfSX/atY+qxc8Xq+7Xv3f3xOp2Oy7K9GJTlsX2k0XsBgSYEAMlQN1x2tdpsoyZGQ/yHp0dMO6bImKIurG09CsLnqL+MVA8bbA2OYipYKClNCwHEXOZhmJ2RBrEbZAE9agECne7o4sUHIWbsHRnXFnM8OJzBHumrR7jDZLLnPbLP/zW9949vaNHnzEsKGKPX67FEZqQm6yhxSTHtTC+FsMigvrRNT+SRhDCo9K3G5eYGQaSRge1PALNmCIX+jSRwQE5PSGO6uDedQKVoqIqpZPSQYt0HUovRUQKOkVRLUVKEYF0grNqZoaouGC1kE5QDeXIvAQoiHdefnq9ebOfqUwj1HIs9YkAzgY1ByIxpqVEMQYhGCtAPWJtQGZ2aB6XeOlHVUn3c2PPM+fQMsPOHHSRk974tERgFxERjU+9HKhI5nOEPC5wBQg18NnX6ecvn746bLMXY47K0uKwi+MZo5qmQmSolfmwLtbHHScjDPr3NRf3cefRDMzDlClqhsKsXTp9EM1BRYoFXyOOzVNytHx2DaWg0+I2q25tRbVAVVU1v6oiVEWnCgHW0/b55mo7DhVnq+47F4vlIlK/XvC9MzwqYWQd0AMEdpe2vhoaw4M7QCqLES0jlWJ+p3mX5I++7ijIiCVoFDJzDaZoEFHVLy/fSkKUsoMk/GQ8STqd19BoxxzCnFw0mpcDrJJJRTJw/3SmUITnxKhWP7q93IwjGlxnCWueojmNC4z0H2uDn2ai6Q9pApzPFlbVbqalDsw42OykhZjWrwASJ50+Xp4ULd71EiSvUb+W6Epzy+Y4AA1AV6TrVFVUpBTV4vmlaIkDCKnq8yRdL0JcPdv89KObZ1fj9a5C+PBM7p2gCE87PFrJb763/L3vdKeApeCggHYybEczv0avb0NA8T/dMTl38DQTaYaTiOQ4QpWYA6ZRaoM7QACFZu2M851LerBQc3I05zKBEakczVOXUUNUStRdxMtxooJSiqoU1a4LqT3xQZLsHVd5ZmNtSUhMiIc9giIUbxZxlgNLEItcvQm0yMA4t0khZ/mIYgbzyLPEkGbAlmaRyDI0MmEWqMgP79z/J+9996Lv09ssDTIVWpfQ4mJmPkT6LHPRBZiVTh3SROFIxrhCuPatKn1RCPvz/vF5uXNS7p+VlULDo+XBCb71UE4WuLPQe30bGADYvhmvXm6H7dSEVc1B9zCgLp16G0SYlft2IlYYGrUhxBHIhUDWQDCJ7EwxZkaKxJvjWNKuRwTeiPM1MuP8uckrYXciRaQULareN7XoSpeGqqBl9TLusvk8MiCBzB6fRvoI8SrYcfgEXL9vptpsmWxda+5VCTbxk4SemdalVYmf/Mj43R45l5PiJPZ0u97V6WYao1wjGkjhVVdpGCgSvY4tKabb87Lz8F1yBOK8oigac+oFSgj6TjtD/3p3905/siowW+9tO9phwELkyQVOitTK/WSHOg9IBZSoo+GYZGUaQ6GYuoJqmkFpzrVbepZeLFG8UQc+SaEKkSIGqyMg5lpIAzQ5KoNwbn6IAZEk3LQMtwqpmWOLJlWBcO6WEABeHBWXnNkutSXxzGn029bMCDGPR05V03XnfC+BMQ1EEqGa4oqov0fdLKxDhTITX7QJPqJO1uJlBD9EsWSuY5GkvD7sP769mmwu8c02jcg+FSKEVlOIGgspIp1Ci5SuiCKIBmhsQC6h2kMoYmbVaNUEsnxzwP/7bLury75Mkx1Gu9lNvfL+OU+Kni+LqFztbDJ0aWcKiGFx0vfLMt90uzcfryJUgRrbdR9x80wK0AipJCnQ+VCp4qdWItJ0uJAk0uubC1PmeJZ4Mo97TnJ8bCD0CPfcGxuo+idH2VbmQ63dNuPjfMmYp/woks1KiOXXj+MhiXY/DiWeLztoJQ1vvtUComSXAZryDCAczkIfawbJFoRbXoOETXVoj2kQZ+0CKQaQak5rpAikeKOPESg6c+0U4xjcKQsdZjCSYL27vHpyrr3ebg63+7obJlIenOrbF2XR6TDh9bq+vLG7KzkXOc1Z0oXQWwdnRG13TFGhwDS8PyAYITAEE6PFNLXC2lFiIBD1drRmi5Cc9fxPYej2YMNLZ7ParGYGkfjirGZDtKArmkPlHuwZfyuUoaMhNV/JdCsnP4oD5rCS4KA0Y5zX5sqqXyKjhSVawiQhS5AnoELQ2iQR3el5Lxaf5zVlePDmxyMB+igjAGjRDp0RJGrOYi5/zn0IEE0OYow2jqwNUbxfy6u1MRQWBemUb11scjRWt10FJrnTnz45HT6/kTFaIsjqgfUwcRxr1+HxhZ4uSlfKfrRfvprW98v3f//J+7/7ZHlSQj0WmxsNYrFCEHZNenPk/63wDCVrk55bFIwJbbVIxwFSsrAhIblFS3czIrji77PbWHPmYgErEGSHV3hfiQtLC/K3DAJIJ2Kk+u24i/poZzw3T4UZVp8NTyQ5Y2GcWhNlg3eLXxwy7gfnFK/8uX2ngJIgFleY8CkRmO0Y8xLnjgxOHE0lC/+AILORAEibHRdNDUkNEZF0JUxmX11MtlOHJmikN8e1ekLdff/e8NOX02EibT/ZZrTJ6EnkspPTpd5flr4vAuppf3fZ7Yh+PS2sxgnydiW6swOvG7tKD4SEBXjYM6YUeVw1aFSr5dmzmm/RsRBimudxLS07wkIoW6OinydmVzJBpkCEZGXMtLUYk85JkjANKMvqUKiZOfNHi5Q8XhFRSHBfyOzGxzp6t1vafnSY2SmyZkIkILO5QXoTQrOROb89lgPT2ObDJU2MY6ARyJk7N/P1xEWggiIoDggtJwvK4D/Vxluc50YEz3Cc3/HYo+RCeDC72dn1nrsDx5ETuerkrfPFUspiUYpARM57vHd39WRVyq9unv6vv3zxt6/t4HQ5uZaPuWTP3VxmYRqGBOHNKCk5lEIPe003aNwlOb5kKTkHSY4mwDUm53SabcJtSNu59OjngJd54MKKmxAJwsxIWq2OZM1LZ4YUZEAEXouPvs9YTOPO4qqe0a0tFwi0BKAJp/6n5nUdVen9HyoSqENkkTQar7ykwaM8tpGP1K7DV92d5nQ0hj2TLxxlySnoRTSPQ2q0cAKAWRBuycKbNubhP7LsP/MuGQHBVbelvLwZX22n3d7MYMS9k8V3Ls6mia9up89eHN7cDPdO+vNlX8mRGCfj6/3z//mXn/3LL8fbUWIK0/Cl5YkqM3lzwsNGtsLrY2DbbMbdz67J6Gjyqc6vpkgW2YMzZ02GHGYUXENy1COJkAawQcz8OpsEFwRDAMsFOgjinWx6Jk1hDZIR3ec1m98SZXgUx10sMx5ZbB4l8tY4UZh2OhkB2ExW58Ao85hEB0owhWYskuMV35svg0dZi0QsCh1IM6kjFS3/9+tC0jYAQQPSN5rN+qxpZi5Y6OWj01fQ213dDbaf7KzXiw5fXu5++qv9p8+nu3e6Hz0+vdtrTzFjnVhUOrDsefOvn33yx5/trka0SUprQ8tlYpKZlnME2YKsAUTO7ngRnZJHtQQfeQ3cQkMBL6mHOEY2F3aul0WkNhPIwGNAxt6gM0fTR1h8Qcuv/eGT0rWpSkSEHIkX8bvMXY+krTBmtO+5zykTGDPSIINOQ2ph9EaJiHdGIIlQGkRQpaO+SojM64ME3uDstq+Ko8T02JmaG8ZAtaSjjUt8B+nA01AXhmVfRGCVERsRyzYT6hweCJFpsu1Qu9Pu4sf37v3oAS+WtejJ7eFswtV1vdnz/Fy/+9bqyZ3FvdMFRPaHehhsN1USogVkHTl8ubs9TBffudMtC9Ltcy5mIpD9DumxIt5qzDmczYAet5UGlew8e4uPevAbXEQBJ+eY0VebCcbswH64HEli2RUEQQ4osYh9Mk1Wfu0Pn2iXaow0IPFIN7efyPEECtsyophhplSXbah+TdFkN6+WEGnuKLNqkNY2T/lRWinNfCUupxGlGHmdJ2J23ByyBnbS0DghQuaMIoOUj+00cAkuF0UAM2/Yh0iuznTHAKWIQFU5TNyPJkVKX87uLR/98OLe/eXdT9fb2+m0kx8+Pnn/7dNFLye9TsbdUKvKzX5QAVQXKvvKcTCZ6vhsu+30/rfPu875Jul9wZIDwhh+oGWjLWC0QU6G0SJJDk5GF08SwIgeM/UVNKKVYyHHsTgpSHPhqNiIVC77IvOlAPBVAixapqlqVlDkuB6S15e5X84W0FiXxR3LkXmTYUYZelrVsV3qXOvP4wcCO79o/Clt0U+aZjfbucXIpYrr1DMli5a1IjlB48uewkVEOGoP8d+2xvUEEYnVVYjctM3hDBhJD/1cVCkqZ12RTs5Py0++fefbd1anKkr2KlOtVbDbT1J0PdVxnOqhmpkYR0AnTn/6/PXPXteJubOCH9R7Tf2ER6toc1AjSGSVJj/O4ZzntWUK+a8Y3pRM0Qw1oWWeKc5HPLJBP2hOWF5UGk7a7LwIfy5QHN1D/Ny+TnaaetKKbA60Kee0uZ0TvVhM2v7r6BDxPiOfmK0t7ItH38rYkX40HyLZkms5bHc9x4QQK47rykfDD4ilguBfzBsWyXQ54xjhNRi4bsQZRUWgRL8bLz58M23rT56cf+vJ2emDxXa0t++d3FFcnHR3RZYLLWbjwSi4NbORFWYj+8JuP33wv3x8/cU6SWAbn+gdnBc3BKVlhgAPgGlXjcUhs4EjtJtpck5EJPgN8QLtLcYbiAW7R7aRThfhoOFreigyzXXJK81vlvYSs5hjKpJek+4SYBLTdARDbNfMnCE4dCAto+F/elrGsHlcwz/9l2wj1VwktcfI8f1fnhi2+Ns8IjOEryFpO2N+VedqzJyKzEAdw8BYxBdeG4kbo2VaFNKRpx9cb391+/je8uTu4vowravdO+3uqK760ouMxoUBkDurHlWHyfaGg0npZNmV9VAPzw/P/+zZOFRkJfbY/+d7J5CLUGDQ0MHmqw6vTd+guHPEoMca0QZPyXfmKl9Oe3O6JhUcXUxaQKwbJuEr2LPXnDAzRP9Zs4BotMhuC1o7TJ7b8hZC7KOlbyC+7yaa94jonmzl2daI2fRHHsXKzIPEzxXQzQSZ1B7B2bQDvY7wOmoUDMosbEcPv29RD3mMrw0eZy9zjbjpKpw/bhlScwE/b/ds++LfPq8j7676wezy6rAb7OKsG8X2Ktvd1C9kKiidLGhSCGBf6+lSTxZd3+l25GTc/tXL9ct9yrVJarwu0hrxvAdImKJauFejVrPDH4/PMdYlULT032cwj2DHSkMsykvgm6OxV8JkPoiIzabMsFMlosE3kee4GTbtJ40LLYynzxwjW0b3r89XsyFGySGgx2mCOVSEpp1WFGwp4leGsWNLCuttBweyiyg1CM45B9oPAV/u/3WjIiP+5X3kxzlL+UfCdJj+TDvNQNJkPdz8yZf7l9tv3VmcL6QO00AD+er2cLUfr7aH68m2xsv9ZNV0KTZUIfd7E5qZdYLtZMtOzyCbV7u8m6MIF2oeCTFvrUvBFrlIxiczJjmueza1RrjkaABSl5ijCZjV9Tbi7U83o1BFwtuDUjS26wZlDmEi3qORvsqUQ9BA7miUmVAVeILkR6HTouXDbq8ZN+c3Lc+D+U8kAWmXEdTUoTHjgPkv4n+ZOGVA4/E/0HCVsw/rEQ/I5JxCgpXbl7urz26214NfozXgagY3p/2te372N2cLJFC5+ZtXN7+4+o337pwAK+Dh6eJ00S0Vo1GJcbCTVXmzmcaKAzFABkYDvhQsVgrFONlqKevN9ObFlr5TD93tZoewr91vBgQBCcst3wLIvM8z+UMzQKRHxjSQGXfSJeeZRAqlLjUGxEiyYM6iewYMRE0hyasB6BAX48dNdMpkLgSR0MGOFJ20wKSW2YmUV5l6dFwzmCFOIhjNod4vjor5y4T4AkCixYm0xES8tmI6qRe+ZhNHRhWS7tfSXOceE29+fvnoFzdfPtv84kR+9C++f+/dU3H7ZpzaNzSySu3c94wsjFGP4fewrl/tbv7sy+8/OjtbdcUgY+WhPrrXn570hwnb7Wgm1/vJJiOwqyjCPVmqEBhGPjzX568Pt1s8PpOriQ8uhzqx9LEXxFHDRgYZ0v0iRiyuScCj+fRBt2Y8zFVyydAdPqwdPjGOjRxTfFO4Blez1SVFOYqhbfDdCYy+jQS7nJIol0efgBuZNlMJWxLfvijW7Watw6ctt3/RZnnI2AuJWxGLZZZuSRGpffURo7Ujg0GzSED8PoXa2iZaDp/mleOG1PUi+Oao5+jmAUHh7uX28O9ev1gPf/fJzfZQB9Hf/c9/eHK3D+Od013JbeW8ia+SvqjIYjUiWUazv3pRBpyflFoJoy4UC8iyXB0mE+FZV4r0Rc7H+no3icrVrq4PdndRVGRZdBimr67HIlLJk6XU60Otpp3MPIpmSOWrOWnUR5INpK7kq/0QNN6pCGZTOgauRloyqvlhvMHCGbXDQ3Jq/7+2y/JP0saiVd78HWdoxi5AwMOfpCQYU62xsVBwqiO6EpJcLt6iuedrtlfYnPcCNImF3KKWlc7cfooxVy2ktlcI0EJmJ0iU8hIS8/1MDwNSXdX1qBvYPeuZPEpCNs92n/3q5uWL3TBymrj9f14++sn9H//B240S+G1G9wvQZtnx2ZIxGXByO95+uX73wYmBt0MtwrHi5X6/2w/DaCSo2i/6btHrncWJ4XY37g52GGEdT5a6KvLiZrza4dGFdCrDRN1OdbJ+1SFFyGZwjFxNjriMNIsKLcIsG5yQRhZ7q7RsLykuGzqFH1qUPyiUIIiRFxxhltEXb2agZITiNJCUZGhGokOLuA20cBSeWsrVVOmGvyIZpHLyA7xJTZAPZPDrlQxaiW7tcOETMzy6x7DJ0Xk18Lw5N7kRi28BrWGr+QCzb+UoEMg8TiQvv9q8fLkbR1ajEfVgv/yLZ9/9zUfNP2LIRKzS7T61n+gtdzpE4+L1/p7gwZ1+t59MZDvyxW471MkG1spDrZWw9ai9np6dcNXJMFFkqoRyKdgc6ucv6tkK909L34kW1KGytgA31wR8azuDtv0+hckMkD7gmzvmhozecG2edpnMBpFxKQfWzyIibbVvHLaNGAPcm8zJtjyVJFhC1fBTUiCsBiFVXKxofASIPt/Il3PdQ8yzCGLTltzotKFPBmZ/v8ku5nfK/AZpGlimhdEAACAASURBVBMYnP/oQvPeg1m7l1nGiMCR/AnDrfLAbVISsVv6EKdBA3cA01Cvnm2mSSrFKs0ghvXz7bCfmoGBElvRJRtiEx0l0g2SMnH6/Fapq1JOOi3kehjXQx32PEw8TBwm7Afuhnqznp692u7MRpP12gwcDVR5uq7dQr73eHmx6gqpxOZyPGwnp4qNdAoj3ZNGlCPxidhuBC03BYxcp+WSEmm1Z4JHYHxElGfvQoJEEqTAc49HNhv1rO9ZZmEGRh8PHDelSxSCGM13PSCzMJnB0qM1srQ7k/oGhPEfbDE1LjKCj4vJqTsmhiX0xByiUaeEYuEcLt0LM0Gm9wwl+mbrXljRnBCDubg/o7h/RUHz7ZmMYPWgXsqd8zMt2dHuNm2RE9HgCQBgQPFb9h0Z5TCd345n91fTxMOhvh6mV5u9TeNUScNEjBNG41RlMNtv63YkVQ1WRAbjZmfrHd+5VzhNV1tZnUipNu3GcTdl3pjcGw1e3JeCVwjULK0ix07afwVdiAzcYkQiP9C0jxksbAaxjMVo5hSTlC24ImwbdmXqC/UFPwJSWCmQLubMaZODn2YqlWYwm04UjDKgedSXMCCDtzq6t4mlgpWG3DKi0OViJHxVv0dVyb+AWOUfAcpJo7agKhIMJIavRY65YQDpEykWZZeMT02/1Affufv03132J0ql6bI7XZ08PlFfKu7UJnc+J4VGr98GPIt4PmVD3T3bls1wOdjlbthshworEEJJjuQ42mgyThiqbUfuDlgP9e4dM4FV3NzYYZROMQy8syxPLsqy1/1UueH+eqDFTitt9WMY2WwHDKregnyS/UCZZmse+ec44kvc3FfVSIHRU0vEIogcURCqrusHClIQTMgPmwy2Ceme5TpPpAo6t+LYr58kVA0QmFBDXSiIcC1znhj77MYOEGw8Netc4R1+IZIKhP/pG+8IhcWEYrH63Uhl+AGSvUe7fvadxVZzYjRNmu/MNcWXiJwztuVkaGaqfkwq5ES79//Ft977yYPtzTBOPLmzuHhysjrvxt2Uwp0CNfOgmeuQrINtrg67F5v9L68PH70p26HSaEJWgVDEQCPHsR4mGHGYZDNwO+Awol/YNBZWHCqrAcIn97ofPF6dqJnofuT1wcbRdusRYPXedgKeXiVKZ8yUvFc2xE5SwXlWJTDcIpcU32ZbaKRvYpsUOLtdSfpHaObVOHdwu6aPWpPx3ImdzND/b0SnkW9mMBZn8c12YqqP0svy79NygeOZpt9IpLkQmEl8HDBoAo3tZj3vYXAM3y7cySOztGEGjQ2Hosob+ytRY3+Q1EgC8JK8tkIGM9P04fSfixopm1e7E+hP/ul7y9PuYYrT86aJcJNSHzcRNaMZWblfH66ebTa/uuGXl8vboQMWBlH6/dRaKus01dE4TagUAw7VtiPWexwGVMFKsdvZdsSuYtnh7kq+/XAx1ipatvu6GabbgTBMo80c5KiU2/hohrqG8EG5mkc38hvTn/U3MvPVBkkeMIHU22IyEydbcdenrQ1vpgYtrwNSJIeAFvIGOnqKAZqwNJEit2cDfWHWLHq5PcaFR0rt5DSStBAsBF75YUpdnnTCNybKFR65B4NHP5fGGzmQxkWybi0RDP3G5wtgbLAbbqHpnUw5BOKP55Ac5al+/tNLg91bFBLqpouWYCVXsTi8Ve62w/7mcPnp7foXbxaXuzNB36FTlOLrcUQhE2hWrcowoVrdj+ImvhtkvbdxQhG5uCPDgPXBRLAoWPXy+KIMo0FsO9hgdRjVaBNZ+lhRSxZfjRFG5UNkvgbsOJ4mtbEW3tXX1eV+mynMUpE7N3l0ymF2aRUJYEdWzTkgBy82zJw8GGBOFyxR1Jzbd5Gn5V7Y88R5YhX4lpJxa0/wGBnVghDZ3ArDltIOG4NAw/BWPGfCpi/DY8LXnCkwZjCQacYrXz6vRmhy4cggWpk8QDfxfW5/VEjd1e1nN3tw3I3Ls8WsCUhOCUETG6fd1XDzfHP71e32V9d6teuN9woWvfQFRVRLAeo00YhqHCsPA7cj9xP2A4cJqmbE7R6d4PGD7sXVtNvyZKmDwoBScfcEdSBOsNlSlKPJOBoJ7fTkzsIJsMZDIazxzjk0MsOLMVOzfAepd/hROJN6wlUG3+mjrR9N4yK9U3nmhKkM4AjiAIGY7381Q0KIwxEUSMLIIi4DZhEnY2jWi9wQyMbA41pDSfNgn0eGUExNY2/xIPktsGVAdQaZK/TDHJ07Cs1az2uaYlKzI6U7SX9kmaEt+dULArk4k9zEQ9AMKmZEkcVUX352s/5ygztDubcsy04LSJn2Iwce1uP05nr87Mqeru32sKx1RdFei4oqc+kAp2pT5VhtmmysOIy2GbkfuT5gmGK0phGLHg/PyuOL8uJqMsP1xlY9emJxhjOV87OC0bqOVkWsUkQqu7OyOOvcgy0ifwuI1uZfooJJF0QDk6GZJhyFwMYF3NgkmhhCD8iY659FIGZKwogaEeaVLXBWbC7wttEP608jYzx6ofzkDx5r17bGDirmUTzwo+3c3T72YHnUDxEW5GQzvuVUIpq6Gsx4cSG/p62jO4TeFkYbJDdaEu+nTCExQiDne49ex4juFk/dSaCKPIgigMrts92LD6/fut7JT19uPr45vNlhMttM+uHV8oPXy5+9Kp+8XlzvO7JXLIqWIklgrRJmqKQZqtlkHCdsR97ueLvn5oCbPXYHnCzx8FRPfEaNZwvdT7Y/YDLQcLLAo7NysZJFV2DU2PiBUKVhd7Cr/XhysTh7cJJtnZG0ZxwMhw9ynuCDmB63rzmaJO0MA2ig58CRCmHUFZRwNTzFq2asmW1kjYJJATspqppFAxc+YWbjZCrSMexQ01ottgJhSt3+QLZMXSKoHptAMLPYO5xN508QsqbHuYV4qpr8KtOG5J2+SbhKVEmYxaO2k2qWJuYzmwSfdNB0YFd/MJZ4fhhXBHMupoJ73z5/+155XO3uSu1w4EeH6cM3FHTEgnbYW9+rdq5DSXp5nfIxNBCZKqZpGisO07QbZDtyO2A/oF/g/bvlrVX34O6yApfb8ZOvdgOxG/jtB4vHF/zi9XizwaZisaulFE6TqHaFFaiAAJOhU9k/21ZDA7IEICSsiVk+94Yz309LyjQAxzYmqXpzhkQ0I0PaDCKpdqoVxJ6pJoglmNJFyEj76HoPWl6ONFxjhyafZoE6adFs8BR4Dbt5VepU6WP/Hg1jVPmBjILmB/DoilZ0TLEFs2sx2IR6nS1M0STvQYAaO+aLMjSRFM9Qd9Pt0w1U7n/3LjKeZz4KADYZjTdfbE4+eP1P3zvthT6QQ8WyFFHZj3U34mZbuyX73keVRhg5mdRaKQKzyViN+8EOFYcRo7FT/e7j/u6ivH33dDdON9tpO5p22ouUFU67bnXaTdUKcOe03F3hwblKteWyX+/rsu92h1qtuhS1WohQ7v7o3uPvnDNUoNhwmqxBniOozXHKmDQm9AbJshiAHL6wjwiIPs1WzbcCpedrVpP4wBuRENAVAhLMn9ITtfuokjB4HNmsPP5pngdEbuY2QDjzEkk5XgKBwXSlRIeW0rYsJCl8rtxMhdhNnG2XXRyrbQ0XM5eEHHUv4egUPiqG2O/Lvc43ZlVUm15sv/z7yzcfXC3fv3vxrbNc/ZCiKrl5sX/98eV0Nby/Ht+axkq73ZmZnS86ktVsHHG9q4dxutnZ4Wxx5727ouBo9TDVySw2eIN0oou+nParu4t31oeHT7enq05gYjwYXtwON4MNo6lyPEyEqmqt+Or6sDtENHvvYX9mOLlYYm8nd3vb19WZjiNGw8EwDagVu/1Eo9UYQFHfM8ZprDpmBW12GRmZI8s8+c5hzTxYIDOG9hBETw1jrD29aCpdawbyZz8FxLT6e4CDgjWkAM5Zv6WxuQl2TBRteQoBDTEsOH2oERGoQakx8S12S2wYHw9lFIhYal2u+wPxKDXVTGQbiUeIMk3blwT03Fp5DrjMDba05aCgyOZw+4vLr3725vBqey4yrsfpYGUZSz1Jo+Hmq+3lXzy//nTzFqd33zm52U3Xu/H2gPNV6dSe3kwvtvV2Xwt4erG4+L0nP/ydty7eOvPRGYZJCAFKr4Coolt02kk/1ov/6+nyfJJlGSe73E2vbvfbgVZrrTZaGSfuxhGie7M6oQIAHpyVpcrqtPRE7TrS2AlMtGhR9NUWCwyjDVfjuK965qm/upmAtNjqnckKkP9zWIrm/JaSZudmbpYRiMHIAIFIOT1ozukXAAv1JDGTgXhiUVJt3wcMpsBc2MwMUzxu+ukcUdoapcYZW6NAIwaSFxcsgfmIsZz3Fnqj9IU0cwbwN4qW3HIuAMCvwea8A6G6xnvNLsl4PoJh82Jz+zevbj697vf2vYerixP9i8+uL3/6+v5vPirLArJWPv/5pai89U/f+y/l7s/+5JP11dUXUp6vhxcvhp+82+8O+Defj3vKfrL7v3H39/7Fd997cnZ21sedFunoe19IV3yrYZSiUlAPHPfjqisw7Hf1ej0S0oEUHVSk1lphE0nWiYRysofncrfXt84WyipdsWra61SpC6mHKqowIW0y6VbqG+40yT3AHf5Qr0AVRixzHt8Ilyamubm00kAqim4w/iEyrXQZDJZrAwIenbY79ZVUfNNcQYjGM5fjKvPBszHpZuwYh245c7MskKaiHivQkt40vvyPxuajNImoToWtIbdSDOONxzyGDblZmqEUNG1Cm6ACEbEWvcMYEf4Gs2myzae365+94ovdWx2+9d7qzkn/2eXhrHQv/+plVXn0Dx9q0WcfXA/b6Tu/+9bZpj7utHD8+evD7vffHR/tH/+grp7dvLo6lHeW3/r1B5ub4f1/9Na9985UlBW+YU5SQIdTidyPFEIh16fdp59cXZyuXq0Pm12tNJLbA0ex4WCTYDIbK6ZJQNxZyeNFd/9O35MQud6bKA97K4rNvhbtdsM4Vd1P9TDJYT1Ng/ULRQU0ngOdvTVo4NTQzIlJWp+HrPaFiiqZf3pw8FqRpC7OsC7nZMmE4rDzWQgIzRVV0LzTKDhs0zAdOkP3AryfNjlU/J0SSNLvLGS33mk37pJ17lawP2JwkRAKyXhYJueWTaSjiSYtbJxUEpuRp6VQMhZnlu1mV/fT5sPr4e/fdNe7e0u9OOuvd9MHT/efvJqqye1+unu5f28/3rl3+uIXl7/2z78lxqd//eq//fSTrk6fjXq+tx/+s28trg/j/zHY9+7/zm89vvftMxpKUVSLXmdLniJqVmN/AScqhf3rwf7i6Qd/+Xyznh494LPrPSD7gxmwn3gYSYpZpcAM54vy1nl5dNatBKVTVhuJ7TgZxGjVUIk6jmYcqk0GEtPL7f5mXJ514odIMp52EQ9eTZ5FQFxybXMZHzisuJjF9BNEEPLO26BoRqMEDSQYNSjY3AYUvI5IwTYyjNhlPU1SolHOZ9HYzRrbLPDPthDhMnzA9Y5cX+Vvkb7badx/oJr6/m0xNBbPoECzZL+W1iYZbybUZ+oZuHXcAqYgRcG6mw4fvOk+ua63h5NOJrNPXhy2g315OV7euhyEl5+P6//tiztvnfzGP3t3ezVcvrj++P/+6vR75+/9R+/94Ly7+/h00Uv3yc3w++9+7/sX/rQAf8iDMSw/kugI3ZGQM9Piw/X+4795ebueTor4qpMPn+8ud7atPJjriVTffwU4P8HZUsW4EeV+gGqduN5a6fUw1OWi3+3HbiH7AwiaiRh4WzeXh7tvnTC6GuKh0YzRZmVKgj69zM6tTBJhEttcNJXBQttNAiVirIgigWuRRu+fRK7EbAs/4/aZ/k9zGw0DlBKX4elxfAwh/bmImdehSfVH5Mhjh9eeELQavmtd1Nidw6dhEPBN/CyfgesqVm4IkmtZpfHS3O6hVWNDwkNWmfL5oo1wDqYfvjn/7ObyZk/jZvTGB9uNeHmFojDyzqks+u75VV08shdfbJ/+8WfT5fjkOyc/+OffPnu09I2hDTL85P6iy0fABSwwzN0MuVefeIoDMTOVQsFhP+2KdndO+6uh78rVYJ/dHL7acjIRQV/EzcUAq1IhH76evricThZK4/lSLk70VGRSG3eGgv1+MnA6BFGySoXywM3l3sz06Km5+aSmJCgOLcn03XWzQQHtHQmNQRRi1mwyBR9ruCcBRZRkagxNr30lFTKEkUU+gZIcm/kFxnMrA88S+IJuWXIQ77/mXNGEd6klAvpTzDXicojwQMgX8dSf6E8jYYGkEfuCTNBhubh1xDsekw12vAgq4AW7uvz05uT59vOrvZGlFAo7GKDXm9oViGA/gCKXt7UaN6/2rz67HV8P91dy8uMHJ/dW6VYERbroGQ49KZY3ScYGze5xp0Q27HF7tXv5dP3lL2/Wn938hyeLy4kf3O5v9qjeSx2LI4yUyeDKgl/6unKzM0LeHOxkaxdLPDgtqyLLhez2HCcvjnCkGGWqNMh0mCJ2i1HzqgBALcpGjDlpHZGzvyRXyzRRGM0Enl2aEDUz/4hwMcYB4kFgrGnowUxbqbHRw4ikXwvXMcQKkl0g0Fwu9EzPtwslQTGNR4TmM4dpuVk/M8ploI3vUIRtKYoQluLanEE6YueTYIJsRuqQW4AeNWzGgw5kW4efX46/vFrbdPe0X3TYDdzsRzMqeLKo7zzsX16PA/H8yorgdKmnVR7cDoOIFFmuOiY5hIlbg09UVHIsqXZmLyFyjnZzuX/6q5svPrp6+tHN/mrqqFD7Y9tPjPhgqNriqw+ktWeNxysIDTAYvljjq3V9dCLvnBWonJ+SLKqy3hsUXbWpcv1mqINJr+l74aCkacu0mF4DzjKQd2hWHA6jmYnocqnh4LHMrrV1BLOOWCoRQSN0hZ1iFhnSjtzgrBk0Gz65NSJ5uwDSBU6EeSFMLl1Q1Okhck1CPNI93nMf8Y0d2QTXBMj4hXkIj6YPf75d5JyRkqRaw8zdw53CJpPP2a5OH17hs/Xrq8Mf/OjeyVK/er19dbO73EzDaOMIM05mp8uyPUwQ3L8jP3zn7HIzPLlYvL4Zrnc8/Pz1xffv3Hl8ktyRdagku754Dhz9eqNNIqpFi9WRb17ufvl3rz7+m1e3X429kkRHmhHGwSRbO11/j6zGwS/rF5Dc7smH2ijjRIVOsKdbvthOKjgrcu/M7i1KKVxkb/jmq814mEpZUFydBCRaM3xJMFuEhAUtjoKA7G+H9S9vbm+G2umbl/tf/4+fnN5doAXAaEYO001z8fgCA8Sql7GdMIaMkDx/znMt80CmKUUnnl9q7ODcoeELAuNy1/NQrbIw4LHLmoQfPMEUkplBi52ZwobihVB/IzGWXE+XnzVaN2epeaQAfsfO0R7u7IPL3XcerO6e9j//4vqjrza3u2kYMFaOE6sJUUvBspcK/M77D371Yr3e1eU7uDjr3tyO9WDrN/vzRyu35Jvn20//7Ol6Oz367nnpynio01jHkSpclbLo9f5bp7eXhy///vLm0/U0Sa9GA0yYT4pmaW1YESlizLzbTkSyZJlSVuxXgLZqA6iAEVcT31xzIXZ/IfdOpVY1oW3rONjihIGsaQnZQzHn/wkO3nvN65f7v//XX955uPrObz0a9/XDv3q13zw8Pe/dFEgBauX8aE8kBoFiNNJA35Ar1s5Z8L6EA7ZkVrwYRTL5BnMdShiMiHQtQoQruwG48CZJ7w1Ua6tImNFMgGi0bgjOXGGXpYIZINke+5h0kF4jCEgLbpuT4XlalOIAEdb1+PTZ+osXu571V8/Wr2+nOpkZauVEmUyYjxk+W9iD+4t3H6x+ebM++eH9P//p6+0B2sm98/7+O2cgrNarT29e/uXL7cc324kffblZPx+VMhmHyvvfW/TLfv16f//d0/M7PQ+1E8/9YVo8P8up8bnXVquzeCSewY7odW6UYbOWk2GUAKRK7Hk+AC8PvBpx3tdVHwJoMiDfHCiwJdJfeo8iBL7rsFmtu5vxg//9y/pyffbDuzcvNi+fbt+/2v/DT69//uXterLDyF21Q4VVo6Eozi+WJw8W9x6fllUXAkokF4lbDerC782s9Rak1ONMP3wIkeRSICxFPW5G0UcoCE4SvhOarXrjswjpUorhiIEGcLlkgqRYPpiawJZYGtXKzCa9tcrgbXXUbJkNuac1jtEmPv/b1x/97FIMn7/Yk3Th0TfEsIoaKqaC7AsWWj748vr6ZrI3uw1Up6pLkFInG3f1zafXz//6zeHz9eXWhpF1TTMZjSq6Ktg/HTeYCjHZYafbyVAndyER7yWvRpRUCxj96Kix9CLoag7UsSAi8fjRyOl9ZBEprsPDJJyMm4OcTbj3Yn/7and2t2sLcAmzCqsw1jqxTqxjHQ912E67zbi9PqwvD+vX++2L7dvvnZdSxsvh8z95/tsdH/7s1YLyZjsuDP237yxW5Xe20y+e7W7fPXlwM7yYTs/urHQRGOTSWYaSYM8eYA0AFTDWuKfESMZmBMzEMxvZSikda9WqUJoIm2v47Ma+CuQECKFA+XrPGZBEz5OSzALao0sjR4kufy/HZY+gpEHOylvWRxGATG/GMhHRq8PVx7dd7ggNKAtJCNXUtGhnFJRS2AlE9Hp9mJ5cPPrxvb//02fb13VZ+OD+0ga7+mKzfb1/9tPXh9eDmIhJoUwjl4XLpfSFpFQW0BYr7ZRTFas0qj+3xCL792pNuDcBM4tnlEXSGZl6FG8ll84EWU1AQz6TdxZQWCMR582E1VL22/HpJ9fDoQ47G4Zx3NlhP42HOu6mYV/HQ637aTyYDbSRNhGT02j7vG66R9e7zWjj9PrB6hd3Vw/eOv2j7bi+v3z16w+lk//g05vN+fXhH7/9rRf71bfOpQh8KY2DZ9aWfM+JbP/xhLCSkjF61hFSVWMrWsVEinT7L7bdsq+F0nWnC0zEJKSqP1PSgDJS1iNF9kvpLvrFQiHCEtszl6LiK+BF3L6i2DEaF4oCUETMGFmll7FEUGi0fM62+mP4LErnTt1UjCLVfMf1zXayYXh0t3tzMy0X6DyXRYVJpRpovm4nnlwrldY9OXnw/Tt/+6++Olv4Ck1OX91+dLmut6bGE+XpqpwtsOhkrEoTUWyHUM0G0wkyjjaZxyPUCEyOPSEhzETTsdS3LVRPaFGRcokEgYpHpYlTbxShAJOvaHM3FxAYI/XDqzfTv/3jTznRJnCqrPDmQTFxOJHc7cQDSmRzSlIOV/XDP3m5FCnkx7/cfvXp7o9+PH7rd598/t1zLPVkP/3F083Lf/Dozkm/eRgVqRQlGFmppfDkqwbCq7yI7nHEkBYWcp5lPwezb4ikWfcby3OjXV0dzlcsRTb7QQumqpPZfrCiOFsu9vtpsx8owJ1eVh06QREIqOXevdOh1sGmymp9MZUesqichmpnpfhWwqAStciyqEysBQsRHWCKWmidlFIWYgehxqbGRBGr1FplP9my09NucVZWp+XJarkowzSMqugL7wiHyi+2KrBlx8XCZxyjUR6eCfTLn7/ptna2AohH+/Fmb/sNVh1Ol3jrTv/jt09/+/sPL067j5+vv3q9udwMt7txouwHvNqRUzWiTg7p8LXEICzKyS5jZtmiiFRnrGF/7tWadcDG6IIOSCzWuTjBm62TFUltOCEemPbYfjX07q4EwCIQiMvmzm8yflOPjNj5bUec0y5HrgrKhe5+8+GH3zsbO8F+HH9+9eLxyd0Hq4n2/KwzcxKDiIO+zwMFENIkOyFSIGuWCHcgLyFAfCM4Ny3SH31lNlXrIGKVfdGxcr0dx1o9WBXBSVeWfTGrneDxvdNxqIVFDhhuRxEtRclpuq2dCCcbD9NiUQjre12qjiNrN6KIguNkqoqO56erRZHSaQ+5uRqsk6nQldLOZFL2gmIiRZdLHVitYhym/pxyZicmi5Plpy83RVBIpa2U94QvDthP3I0wq+cLPDgXMxp5/3T59KPXb17uL05lrPzOA7046a42QylYdHJvVd691//29+79ox9cXK6Hz9/0y0XpD2XZEybjfpyIWllJCmoNeSmym/xHUdTq62FgzKpxfqF6PGXQ5UC47JJyOJ4MlSgKq6hpjdkuBwrudjjp0cQtZGxNCQvIg7t5puxJENKVE+XtwSAQkf/xR8vf/Hb/32yGf/l6uH26OX98cv/bd5qanxsO0ZV6gpgcoZzam0VemFyMIrmsN57ULWo1tmyzSppVgtXMbJzQ7cep7/Rk2Y0mJyvopKJaAKOdrvq+180Ofa+ny+VhMQ2HqRTVVX+27EvB1XaySinSd+WiiKqSdhisau1KJ2PVir5omUxUpMq4P+hCu74bBXVfuw6L0pP1er1f9J1VsugELBfdCDtf9RTc7Ca5tbOzhULuLftXBoGslDBKZdehKAymimrYDngkrMDtgV/93aurNU4KZIEicr4oX16N1dAX77/nbrR/96vLv/3i6sWaqpiG6XLH3STDxO2AOlmt/jQD1hp1AoeiIvSdgsaK7JprwlK84xFTmujRMgOFWWTZvgPKfkSnOOSqOQZAwARnHU6XAZuWmYOXjVNTBQHNztGKqEb5ibrCYbSd4KzIquPr5zv8nx/+F4P8w/fe+R9+9ODJvdVgNh1gio1v/OJcilEn1JFSjRQdMaFiIpeCTqP5LfJSKWYdsTcO02RaolZFCOX337n4wx+9+9/9+Udf7NbdaqGrZSeAGYv228EWnfSdTrWWoosip6uy3owovLtc8nQBZafal7Jaar86gOi7ThV1qqtl36nc7MZaw91UuOjLdjeKal+KiI0Tq1nflfv3S69KiKE/WXUe52ut1aRTLBfL1bJM1R4tT+sEUVTj2Z3le28//MH33vmbv/vl1ZtrVFysYBXDBNbI4tY763rsKeen3c16PFtgnFA6itpmn5I1MYz19Zq7oQLYjLLsOE62G2GGYarTpFM152G1guKt4pFLVssuw8wuIyeeVSwXs7yqowAAHONJREFUbcMEZyNjwJX/1o11M+G0RFAO5kcIsCo4X4YS6fVyywyMhrYlFoCahzUDgSIoikXHVeGu4l4vDzq8r/qf3jW8jcfGf3Rx9ufWva+n22ncbMc7d1ef7bbPhnHVdQvtCuTVZnc+4ax0dZL1Zhh3NlVbLLqhrzzt9kPdY4JwUbqV6B3r1PhsGjf7UQlVCMvdrvz3/9Uf4R//J8BbH33yX/9Pf/vX3aLXRafelVyK9p2JdNM0qcqdk74vuj1M44J9J4tOIBhGU5gR48SH58thmKA4W3Y3O64WHciLk8WEWlS9y3bZl9WyI7noS9/FuuCpmoKni7I+1Aqidp4NGDBNLEVKETP0ROm6w1CNU0flsv/NX3v7/Hz13W/fp9ib15u/vTYAJwJ0Mf2V2G3x5Mn5otP1zc36QC0AcbvPojFAYjKsdxymqoJqHAYxoppvP+VrmWCEuVYR8QpeVw8TEYiXmDlbQAqFAWnteT1uE0VQLXSjmsZnwDINJRBR/r/2vqTXsiw761tr7X2ae+/rosvIjMzKrEpnOV1uJINBYAZMQDKeWCCGgBAMMEJIMMEgARPzAxATJCQGTJnQCMmWLMsDLNuAkQu3Wa6qdGVmREb72tucc/beay0G+5wXKfEPUOyI0evue/fuu5rv+9a30DJOWwhBHVrBdq0dH2BQR7avfIsj8NzhBUYQ2jR0vKIQaLcvbP6O4l7xiwPuHIC2+aWDNGKx2Ao8qp9JNHTDi1ECTjei7mHvp+tms+qutlMrTe68mPVduBlyuUI55Ed9OF41+31ugvQNT8m+Zv3znXkp7vjxD09+4d/+LeCngQQMP/7OvVcfvRfIsWrFPEwhbdME4q4JXWjGnM3MGKp6umlBnoubW981UThpgVMTUIzcyQyBoWpEFNjZmYXbwFH4dNMy/MXNmDLgXsyDMDGm7EHTPhcDt9wQEMhK9iDUxaCuMVA2N9UmYFKOLD7obz3+7Cc+uv/R+ycffe34/PLwyafnX3x2iUo1MISwWYeju6d/9OkFzIfsxXEcwET7hC5gm+eAlAoQHBlEqHiOm5flBjhQmTu7rd9vc5/N0QW3OgYsOBlQgWKj/yeGoU6qzdfulkgWny89L6mWgXXAukNklBlSm5s4M5TlUQhoBcLIBmKK4lGIyLuAVcvCnJ1e3aSUcMQgwj94F3f+GsDA90//yEQmffxyl9S3pRyS7/YljaZWSs5mFNnPt+OrIe33KbqoY7IyRcnqKNQJnfbxnXtHnz+7nrJyF5gdhOOVCAUBfuEXfw74RwD8N/8JvbU52XQ//sPvBwhFhpk1XegbTsXdtKiRWxcj3DadtFHU3CxH5jYIA02IMG+ImpYBTuYNcxQfcz7ZdPfP1kUVQBQ+2zSHsYwDXeVkiuM+3IzDfiw5e8kUhQ9JpdVGxAwwZ3a10gWqTzQRWuFDcTOPbF++uNk0dHXc3T1qjlfykx/daQN9+XL77HmWiHtHdHTUffjO+ve+cw73VBAFY4aQXx/8zgbbEapQAhOKAvNGrfpSVshgroQBMq1KrNfXzAyKOcfNuP8SIG9z6AweLcnxNnXOsfAropZbqf7gEAMxArCKWDe1sUDR+X/9OYGwYggjMI6OZEoW2WMgB7YHDMmTIgty0knVDExoBU2gVIv2AnwIvGzi4H0fEwHgTWxKQQh057Q1dyMLsRHiwzSQ8Nv31i3ouJez9XqfxnFKbta2vO7bx+eH2KLphIOZq6qvNhKYe6b//V/+15/+u7+GJ7/5i//hv4+ZJutGPw6rwEGgTlM2OBphYguM0EoIDnAfSURuxvLOad93/PwqpWzrKA6Lwqfrtgkcglzu0zBpE7hrg2oR0JTLcb96eTUQfN2FYSp9w+tVc9qF/ZjHqTSBhVG6ikBpIW/dwBRgAhInhgUS0xLUALTsR0f8o+8fnXbx5pBfvjpktaN1LM/JAk7XwuQXh3zneirFs6JhVH9VZuwnnHRYtZhqSFMsDOVcevsCW9Q857dwOM193BzXFjWLOrIjLPmU8JXibLmXtNwwWn5Sfbi6w3hhyeAOMFpCH9FGEKCKXMCEXiANqgRzsXAEgOtrPTkmYTbAio8ZxSCOnKEFImDCuqe3723+2d/+Cz/7Zz/47u8+Biu+8z3EeL/ri5sIR5ZU/KpkMO4e902Ew4uakNh6JUzv3l29ddzc2/DD09WUisMCoYnEm8YGu9ymVCwZrvb5+pAubiZ1UqPf/e7LP/zn/+Jv/qu/8S//3l/8x//6N35w3RF5WHcU2GOkVSNdIw4Mo6573rQyFm9CECYODKJ3722OWprGq+fjdNI1XYzbqTSRuyAP764ub4bDmI9X4e3jJpv3LIeAcRxJy92jdkhFjuLJKuym0vdhxX5h2gQ2syHnWw6L4FbIgwuaq91U3ARMRG1gcyuKD+5s7m6ahinG7ngdh+TPz/eN0J/6obsvzq9vJi2iv/3JyyGBCSyzpIwYbDjf4/4RUoZWJlJn4HSR+r7u+CqyVStunkHUOaiwgQXBwI5kKLc8P15fslnC9PrSggC+dYj2r9zC5etbQddAADdMhj7gz/9wl4o+v87bqbJqyAW2tBFw3OxdKzBLMECXz0YGDP0KP/mtB994987P/tOfAR589NEn2O7x6/hPf/D44EpCU7GUFUYObDZd3zdTysx0sR27KI2QkgyT/u6nl2b2zt3VN97eNEJtlDVkg8CncjcGRMG99fsRIIc6tmV6sv3Dx7v/+j+fP/vPv75an7w4341DbiKHszWfrbs7m5aZVS1GzlnbGAh2tUt9GxsmEe6gd1o77fjRSWwYKU3Hm37Ttcfr5mQV4Aot33y4OlrFOz2/uskh+H5MgTxrub4pqSCpBrIp4+mr62HSrLbuQ8l+KOWka0TIgTEVNWrQTHly0DiVogjCJbCaHa/iW2ddSjaYiYi5N4Ee3V/vk/767zzPyccAaDlczDHsaI2UYIrAODmWJ5d6nNFFjAXqUF1eaZqdjm+vBhGEwISFKZrvRQVdw/Lxah9nS5k/50eC2Vzg1+/jur6AZhLYHMtkIRzoBW1ElLmvTAUEfPw2313Jp6/SfsKUYTWh35JcgBMswwBiSAQI2VEA1GoPiIo/9/Fbf/+v/hh25/jsB7/0y5/81idfODwXIy+365aCsBBNKV9t9+4EJnOMmoIIU7l+kq73KRs+u8zfezGoloZl00kbSQhJfUh2tg5vHTdHfdh08enF/vH59OJqvLje/8df+f3s4e3j8YPT6XqXws//9Y9xbw0S7CbcDBj0epd2yXOyR3dXx6vmxeX48nq4e9S2bdhnfXDa3dk0L67Hz18OIcrRqtm04fxmuLMWncat5stLHSYlpqwWmC93aT9mEEfhw1COVlEIRW03lFLMgKQ2jYcmBhGocyPUNfzyelDo9pCmbEG44xACrTtxtd0wARRFRRjVHoHko3f6m6FI4CfnI0UMGQ/v09ffPbl4tf/yVWbChw9Xn19sLw+4swERdAlUukjxahs43xifIxAIWq/a8sFb0SoIPBtL3Sp25hxqjuwYEpReh8nXAo2FPKdaPwlASIpckBxF8WCNx+f22at91rmJrmXfbYNZs/Zmg9NNc7PPr649GwpgQCNoCH1AAH7j/zxdd+3Pnx3hJ97/Kz+NX/kffzJqdjUOgUFSl5DNQLSagYhESESYACkVlC3uDr+ZbPsqk3sjoVJMDB6mkrK5eYyyNCcQOGDSxsdXo7sLQMxdR+SHf4h+Vf98oODJFT6/wfUEM2w6qD97cjMMaSg2TlrU+kbawI8vhl/79vPrQ/r620cPjtshFwbawAYMU3FAlSbTKGGcSlZV9QpeCZMaiLyUuRVLxdw9RmlEjGm7T9k0FctqqjpkhaFtQt+EVgJgubgImVOMLMC++MtX4+XV9XvvnG2O2s+f7r/9ycXDB+FH3r9LoM+ebc3s+cXwY4+Of+0PbkCIjDsbTBMcSwG3lPOGJWwsmKdhxudqoLqNdnaLbhiE50hToYpZhMAohrJ8RABisM9tAS+X2HzOvA82GDJyARHaAFW4I8xaVDCjadB1YbOSzaobk/7Rn+y+9eHqw0enqv7lq+H3vn+1PaCN2LSAIwYcJhw3eGeFlxNiH8xps2k+/vpZEClqBIptk6dkXAtR6oLAiQUhBAJULWetjIcTAtfNxswC1ap19SBBmAEPQqrqYLV5gLxtJTCmZGNJbpyyhd//d7/98bub0EqZbMx2PVoq/uJqOO4bhY/JUvacy6RGJNv9OCZlYbi9/2BNtHLwbizXQ8nFCSYEZk7FkpoVA+cxq6lFqXUQ2sgGcjddxvkxV+W+LzrkbOok3EdpQzOl3LAFphCEhIR4nnADFVVyhNh0LGW66fomtqKm6mXV0cfvnW1aEZZvvnsSBKeb9ne+f10jSmgA0Lrzw4RJX6vkfEGkbuEJCXMyrTU+32LxS3NAgBLG8rqN4Ar3V5J50dMxQQli87R4EERCCOBa0mQIcO9IiOnFteYyL0VQxQS89yC+dadftbGJ0kQWITe62A59xNOX0/FqWPfxznH7o18//v1Pb6aCvqc0er2vxXAzoCiuppIL2n3+2jsnJ5tGU8nZpqROLsI5ey55jKGRIOyqmZibQMxcCUpTKKmEIEzjUIgcbknNPTehtqcopTQsIbKp56IpF1WbimazcbIxa/g3/+3TVSfCpObE1EVZt+zOIVCuVlxmFVWqc1JmHoVEyA1BfD9ZStqvWiO+vhkDUxt4RrfdguAwFbiPUCGwcBObGGWcvJhltWHKIErZ65wjEYFcmIXZrJhCGMwwdVcvUGYwGKQNENzvHPVX19NuGL/26LQl0mx5yEQkVGFx6zpx0N0fOu0uD2FIbYd1y1c72zQIAZoBoItgoFR41uZkSgytXtrLVBDhdQGHhU2aM6kDDqKZvsRyF8lBggB0glbQBYggyiK/BU3FsyEbtge9expOepDInbPVq6vhxUVxx+5gX387HPWNmqVU1DGl8uJyDIFg+PTJtu941fI4WdfQlP1m7y0DNGO8h4J9woEgwJjw5YubtuGcTc0czswpZTeG+zRMRUoTBEBRzYH6Nhgop+LuEkLW7IAa+o6SWtYyZbXDJJGZXA1BeNVEOMKsJi8EYRCJWbaQDfupipGJBVOx7QHqILiZSxAzAyAkoFm8ytX52pyF3cwMY1YiMbOkyFnnesINpKloIBBTcScxhjtSUQNxyrkY1FyLM4OYTdWZc9FspRrzEBAEgaSJaITDPHhnzELC7vy9z89jExshMyvZhmTVSqioVRk39zHdaU4erF4+ySm7FUsZ3tKobg5hJAcZshGRq9OUfZuxDojBg8yyJTbcepAYXt8kLJjIrQVzzYl9wCaga9A0FIH1SqZsMDQNWYWQACJKql0PHTEUnHRy2vEPXmaFf/zB6fFq//mzaZrsjz+/OV6F/WSHSZlp3dHJuv3WN7q2CUJw8UCc1WPYTWk8JAwOYjBBgMGxr801Qww/eLo7WTd9F00tZ2eiKVsIVRQBNx9TYojBi5qpOyiVwnAkg7szVG0YhAQMBOIEK9kgZoop6c0hBcjppg9B1MAsTRO4xFKGUIqSAUxMboU8F2ISQi5O7JWIpzp7zCjFHCTVSMaAgqxZiERhKEIsYfYLNlM1ZxaYZVhLYg5S249Vy8SBLTAzrIBCx6noNk3DaNNU4KqZp1xqIezkLBQbWXdhswqbVlZBGvGm7794dnNxfbh3t5tyAagUHavttZoWWB38PKbt+bh7thd2M2yOuai54+v3u5S18olZYea5eHGv784YoIqiEKk6G9hyxW5jVRUFMcAyXy/mGWhdRTle8fEmAFJUV63shuLwIJQLk+Rx0mzuDllohqcXadUgFX/66nDnpCPGlK0oboZSvASGMTYRWXnKw6qltmnWXWBm16LsJ5vuw3fpB18Ouwmqi5IVs1y5UheHAS+vDo/uHTnV3sJnkzioSNW/kaoZvD76PP7lcFM45awpFeIQG86aW4nMUlSZUdSZqRR1goGLOUsIwmZOTqumCzmX0AYBUKWdRHCoVflc3TdTtUlGjkBUzMy1DhcIGxMTIELuZG6aZ+iTyAKzQ2OY50frPyawEGDkrGaT01DKMJT9bhpHDYwmMAyteONc2A3uyuoYdvn8Ri9jCQH9Wh6craixL57e9J2cdDKPAKEybKDFJIyAveD55zsdchXP/Mij1fNNevIyqdGjO+viPhW72KYp65Bh5roMMG06Ot97U8EEmtH8ZUB/gfgdAggQCE3AukUTEJlFvGuDGhrBNun2UMZcVFHU5yZ3Qeo+eNg/v5xeXtnFzq1HI7Td+ydfXF9dletpboSPGjQBzfy+tCFj2MGpTAXF8Pbd9sFZu9mETR/g+O4Xw1DhwK+I4VRBAjI8P0+nRzk0cqv6Ja8KC1UDuRGzO+rrTkuZqYacNBVVV3I1bwg8FWUxNyi7uReFEJnZsB9AaLsGTQPT/SG5WQhM8GoMCCO9ZfFqKAPVwZJaJJOiUs0EdxEYXM3g1V5rFlXWpEtETF7UixZUAaNUL49bnMky6LBLwzDlpC3x6Sa2DXVRhLhe7KnobtLdpLkgsqh7gatif5XbO93hoNe7w737q+pXRAATFTVmgpvUiolw9WQon9+cdnKz08OE3VAenraPX6TH5+Ozy7GYF62l2KxRr/dg1MWZCYu6a3EQ8VtsduHa+TXkRnBXh2Z7ejG6eQicMxb9+8yczmJBx9lRvHfaCuHpxTAZhow+omG6Ps+T4qxDKlAgFahBzfrIqAPljmIoBYeC7z2dnl9O791v+74R4a89aB+/Srvky+AGbtvgrsV+sOdXh82qhxsLMyyIuEGrQ5p7VR8yeB4ln/X1TsItNwY185yt0m7iZGYgMEhqT2rYHwY47fZjYGEhVZ2Sy7ceNQTAjRjVSg649YGpQP2tY888xkdA0aqYdDjMTYtNuTSB4ZaK1ZfYzcxcq7q/YgFuagZzrTLgVK6ux2lSYQ5CQlDzXBENs7oGqBFEwVD0ZsRU5rfgB2+t3n948vmXl4/Ph+dJuY3rhgWein/xcgyB3r3bC3t9+f/yT33zsydbWL4ebczYDmWcyn50B2peVkOM86UhIBuSwRxRFjZpKe0rj+S3LSoAkKGKi0EE5kUIubydVB2Lp4LTa6QNhKahR/ebwBCWXS6pOAxtAJEXJxi6gKMOxZAVZf71fMgYCsa8IHARfUAXaBzL/pCaKGdHbd/icNCiM7ZcwZRG8OF7q3unITBFqsIBQ12KQFaKqTu5E0sdq2KCmamauZVi7q6mOes8Oae5hgzNBQvoOOWsWtRczVOxnDWX4oaUNZg5i6kBWYUhIu6mIIExkVcDGag7eMbD4U6paBfAdUrMMKQyZh2zrRsOgQLPT2sUb5jd4U7EdYbG1QDGNOgXF+Pjl7m+jsJohNpAqwarlvtIgUVEi/pUtIvyjbeaMdvjizxM5f2Hd6520/nV7vqAvNdhv715p//aSdSxhEDkKCVHDgYF4ac+PPrldcwTibCwbwfvo/ctHyajhVk6W3P1Z7gZbb+FOiK9psBfR6/X8WGeFrTFi6bWeaoQAvHyVTXJ3gptlzBWwcp3H7RdZC1+ncqotBZyYCpoAxr2zBgLhCmIB0MxmONQYIZG0DZow8xwqaOoVybt+fm0P+RVJ4/uxacXeZfgVZFGUMemjT/zZ95+fjV+8tnVYdJFwG/kFJnMnHiux9xIbX5LMbmZqzkB1YiEGQ6eIz+oxhqe9zZVHaHVFYAAzBwg+bF3msAgRxCusdJvJVeGrKbFzZzcWWgZOi5dE6KIA2YKQIhjoEBco4g7ETMvmnZzs4I6LVOMdkVvDvpqm/eDsUNBRUkNk+JmwvnOL/c2FSdyIiqGqfh7D07uHjfQshtKaIK7P3118+wyAzhrAfOb67KDQ9iTqftbJzHUutb9V3/7yd/5Sx/93meX1/s8Ji+KoUDLgk84uoA+8mGyVPxij0nBjE7mQTlaSCdb/AR5AdUqUqaVTQe4yr8Yfctnx1IJdPPXF67GwDp3+M795vQoqOH5vnzny6lV33Qc2McJTQDTvH1sKFBFtplmqFGztiBZZ2Kg6ELzOwm7qxfVk03sG9odbj1bAMezy+nZxXa7L/uxzPsKl3nbYrO8RE21eC5qZmpQ1Vob1OHgWpLSMoQyWycQu6pWL0EzNXdXd2Y3EDHMDaG6IBPVCG8w95p0wUxGxEzGXCesnQBjZxdTreUjOcDWNoE5DJPW+8tsplbTSzXrFnF3ZPVdLrsBhzGngsPoY+XkFtApMFiIgIuDv9zq26d+1FHbxLNNfHqx//6L/as97p2Gb396eZi8KN46xqaRWOyQ/fr5mPvQdkzFeDHrMyPAXl2N+1FXTXWcgCtiVzWVALCbsBtVaZYldgF9xCqia6mPspvsfGeVwzCCVOG/zQRo5QCYwEAGRNE1dLyWoz4K8+W20DJaUhNupXruHoezTdTiz/blO0/SCnS8AcOJwYJUUBlqZSRD3+JOS1nJ3VctDZMVpaw+lrr8GpHRR0ShWgNMwFgwlel0Ez94GB6/LPs8B9Fc8MlnU5Dp7poe3mur/VFo4BUiBSKRm6u6LfJhmv2noebFwUREns2JXG02OXfLLCZz6+wwL3bLntRtjR4WiHuxJ5hdPApIQCxwFkYt7ufdXabOMDOYcM2blK0woVbvU0EXeR5on59lhisxF/Nh8GGy/Wg3g+UCJooBqcyrfmowdZApsuGzc7t/hG8+6m8O04vL8XwLBS5307xqBGgDAR4IXQAKNOtN0i5yKVbYzLwY2Ojf/+p3Lrdl3c/10yri/XuSzPsoZhCxLy+0KIWAafIHp/z2SRMidYGy0bd/cMAi+6mBpJr+qaOAGC4Ed0hAcCTFfvJnF/kV51u60xeSqkLB90/lrbNA0Bd7/+MnqXWcrqvmnooRs08FTUAkFMF798O6YyJMybuOA7Cd9DC6BOwPfjPalFEcuwQmF0LXzP0Q3A9DuXsSHpzSk5eeF/2SA5uApuFc1J2YUSZwjWcgLakWAUZu4LrTkGful+Ceq93J7FVky9AMHDCtxkjmIC0gUgfD1cldEaZU3JjmFQ+zN2X9JJFWM1aH0uIcIkzuhZl5sX8G2NyMUGze4FqsRkZ1EJNXBjAle35TdkO5Pthh9NqVNtGzIisATwYYmgZnKyb251c2FDy9xul6GlO52OWXO28DUlk0qI5xwrq1lJEdTJiyZwWxT0aUXc2rsZF4UVdyDsKArTt6eNpcHcpZH0hgplc7347mzn2LVcNtJGZTp+vBQXza+/nObmu1eR6JIPBZqs8wRRC0AVlxOVSn0dnWBkt6zV7hCTf33WjffZ4tY7OpbrScFMx+SEgKBx6ehTD64veKrOBshakobUcNAmIcr9jUt6PvEwBERusQplJI4fvsQ8pHPbUtyvQ6po4Z0vA41VfT1SFEr1dwzlm+TjrVEsEJqJP0Oi9HBGZSzR11sxUpGdXLyG5KRHNNRUTFiB70xAz3r/jYzdELzEtm95k8nluqWr7dLjusj3c7pVidmHz5Jeexc0rqY3Y1TF7NERY46laVChDQMjYtOXA9ejGAsA5gUDKfrBbQy7AGIQIdQ4FkIIIuHz9ZcYNl9IxQiu8LRfKDQh0N0VmPrM5EwgBwM3k2OBCJGvE2zFYhh+xmFAW77PCvPrULfbnAVLdSjq/2pPMTtfxpVZnbivcBk9K+uDh4EcDVkbhcR+IIJw3tiwegWhklq+YrnozcXbiCKeTu5VbQscyE2lcetxOadG5FbGHJ2gC6ZdMWVNAX4BCLLYPP8ravvFrzbbz9m2rPPdtELllxwRvmgmhxt3pz3pw35815c96cN+fNeXPenDfnzXlz3pw35815c96cN+fNeXPenDfn/+/zfwEaHmaMo7lu2AAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy92bItyXElttwjMnNPZ7jnnjvUiMLQBMgGyVZL1mqRJr3I1E8y6UWfob/Tg8xk3XqQZDJSErsNFAEQKAioAXXHM5895BDhrgcPj9xF/YHs7kJd3Dond+7ICPfly5d7xAY+vD68Prw+vD68Prw+vD68Prw+vD68Prw+vD68Prw+vD68Prw+vD68Prw+vD68/v/+oqc/WjADAJGqEgikBAYURFCAFMogBQgKMEjLP/ZDBQgACH45EQTEUAUTq9qt7XZEpCogJqhCiRgQezPUPpt8aPYmAkAEKJRARKRQ+z0B9nMbAcE+pI6iDLL+3v9WryfYzWxksIdhQAk6qexkOYaU9P3dns94fdaEyEpK35u/egtS1XnG6J+MTgmkNodJxsdxfy/TQYhBLZFi6hWAqooQEbhBsyQohQ7dMsYuUFAohcjEBKAsgN8aIkpkS6IKoDxH+WxVe2qbIyKKHFR1ylJGb0MuF9qgxX5uz6Pq8+uzK/ZR9nNAIapMKBdAkEXiRAtqU5tDDPFf/JefNV1QiK0oQOUvtkbkc8Rgm1kut3Pb8iUsxlkWje2tAAPEJFrvVkZCRFruUCyAmYqhmD2ayRBBwVzWEv4nCEw+hyTqw7Z5sjkHbFHczOyJuBhstVQyI7H/YgBMkGmf07fj8+2y38n/9eWb9ifxox9v2nWoPuRmWi3b1odBUubEXNLcSFBcF+hv+3e/vX33u4dxNxFTXIY05fSYhTQl8CqIUGh1dd6lXuKSzz5eP/loww3lhPVZ261iaIKZD4GLHakAqmAolBTiWACBkhm7DVJVCLQILVT3aVJ1MzS70vJ+EYUoFPZEKgAgYlfYJ5LaC+aXKlosVMEiOQ0p3OJ5PB3Pc7NpY9OF2DEQqtmYxRRPZSUEWz02iwCYVMEAEYkhkqOQAZKCmMhsz83CYBAFoAo8UYEHAykiIlD9CYgU5iNlQokKAJabEAgQgiq7xZu1iV2g9D17c2t22CsGwkzqb7WxgxBIKLZ6tlo0lLtlXGyaxTq2yyAAOYRTBXj7e5nyCJIyUwRSMte3GZIk4934+HofmJpIYRI5YDpkHVSToiUO3K3C0Kf77/aphzIe3g7bmxQ7UsHpi+WT56uT58vlOpYIokpEECiyKhNBtAKZGUQJOlBREJQVpFBVtA1DyI2HVA3HAGGoalYPKwyFmgmZPZkFSvkZlKT8RRVQARAImHhUkUChbWMsWGQBCapE7BBrYFRsr5jHUXhyIzoKQxbo7KkMG0hBzOWGRFQ+AeKQWZ6FHMkI5ACjBdCoWpGyA64hkbItI/zGShXNSAs+2qXVDwDiEicqknF5FgWXm4uCsi67GCm8fLbIGw4xgA0Ni6VRCbOgOlvqYFzw10iHxx8AScb7IT2O06Qy5jyQUE6j6kEhOPQ5TIirPA5JtkoTJZW0y/39bVzS4jSOhzTsxpwyfXqyWAaAiYlUlQE1y1YGS7UyGHPRirUKZjNFECkVRoQS9At1KJNSwIuIRBSkJGXSQAoBzGMVQmI3sukQggIh8NSQJsgkColmEGb1IHCJkhYf4HBSAgwMQWwdSQmsEI+tM+OhanMAlzUp2O1AwzV62jMyz7HUw7ceBVAi0nkIpIRQYJSdrXG1+hoTZ/Ar74V6OPcwCiJ2lkFkbxG7jyA21CzixdliWCEEdyNbUgKIyYNXYSw1qBdTcy9RY7OSRIU17yX1iRTTKGnSnJASEalmEsn9TlQkZzABinEAkvAOFGgcd4fHYdznfp8uP92sL7rAwdaWjPJSsCBg+MJgISEBfMIM3VXVmSTYQqmBMMxi7UpVu1KVbPSFCJSIbU4Ns15S9Qkuts4ZkWIIOeU0SQQXFlvIOhc2CWKPEHYnMCkUWuKk3TPXEFbduTq7uZeCmYy4mlGVEENMFeXY0axyJoYqkQdl52WVZnlUdH5W8hdURkhQ4sLu3epg9MsM0cdRCJnZtKUnTqFFdJwkZb3djTrSCQUn3uX5yd0E/mRcwli5DExkkMAkChKSlDWBI3hCYAVoTErKBFFhpoyMrAIlUc1KCdAMFk2q+Y9jaOmwTofbaX/XHx7Gz3/+dHXeReZq1DZdYqNQKCnX5y2hwkNqSfBUA5GUyF94izAFRfbIP2dQUgHDIgQbTlZ4UCYGJENBgTlSUGokTkOK5KmSByf1RbWhFWDwiQVbuGJFRdoy0/ZGdUuwoXPhpsREHmapPHD56GI1RsFQQvbRJ7qBVW5mE3qUmhrIKBOEjH8xWI2uoA5lBsrK+s3uyM2mZDpmI4V7jCnf3I6LF3Et2jRUgmKZm/LY/E8cx+FxjqEEhkrWw9Xh4c1+3ElOikgqIplEZBLNIoEBQAW5JG0l3iZVBmWFDDpNeXwUzZJGhCZ8/vOLcNYxHQ0bHAo4FXyfzYUUammvY7461SGwB7VCKW1SSzSzdIvmyUZVEGA0KAuIBGAmVhJWcCTN2nHcHfo4o0ilMoBa0K5jcdQqmWYl1z6zRnjcPupDlfBhVmHLquqr7hyGa8QizGAAh5mjNNgeyW5X6beBGgDmwpbgWUHxx2PabkNAyRaUlS0MV4RCSU6IiJk4hEDQLFMvNYYr6vPUqYNlNP7wWkN18SEiqI7b4e7Lh/71VkdNAhLsep0yQaGC4MaSQQoRQCCWUwDIgOENBCI6PGh7Og27aTik1UmrgSyQKBVMZaigYO0x+6pJi32WWF5UBCp7LinMujA1EoMNcbNSLevuVsmBSFRZVcxuC4flyDnldWzHQ45EMIJmqMZHZGv2zdmAgKJaQGcP+Z4plOhpAFUTg8JojKNrCT6OarDMgI5Whxxb7XKu0U+Prip61ZExHlPJ2THo6DlKcM0uEhEUkCEhIDaBItsvCBojr9oQQIsYx6SkanyMWVWIQnmOGgkKHlc/ZxQCy2SrN9306WGKSbuWUqYYNDARA1kFCJRVkCySAxkcoAGaCiBpCySoAJGRJhkPeezT4/vD6rRbrqJPkedwUlJvd0McezBmnFO1mbTp0xIq1G1SDEI8NhKp2EIZ2GpNecBKypqFjMEpgZhk7FfC0qdoPy6xqwaOsowVEsgNvOT98HweBCpikkmvljoUxwErk9MeX+ojuKkwWqQJJTV+6YhmaKkEJi7jND9jchGy4J66aZYRODOqRlnGZLm4jCKqkoVEH6/6+++2U9a4jGcvlquzxeqkCcRP1vTRaUegP1yufoe91jSBysDmXNVX0JVheN4qIOaiZWlSTfuUM6aEnAECRZ76TKrLSJmwyxihAWhLMqcjkIEG33sRgwjjLt+/2atoiPzxT85DF2oeDiVlYYEytAijJbec9XLPAwoXN0RgKVFVVZmQpWRJqsdO5GtmyYL9WohYlZlFhUAkEA4k43613TdC0WeoBBZ47KQSkB3FyprZL8pKlgshdbpnhlfMsBptGZ8eXeQ0zB7U/vGgY/amrKy+jibLeWJRhmtr6HDm8pt7gn86l7va7ORe9rfD9mrf3w77d4f7bx4er8ZplCQUzsLiovv055df/PQJdBECLWJ7ftLSuIPhLlsYqSUR5xU2QnbaWQYcCgsXCDQy5SlPCcMo+z5nIWbpIrWRulb3BzQgk0snQCzwAdH/nADTOTVBko4pP4Q+BNo/TmM/LRoS5prnAEwsBk8Qtz9/lfABm5gyOyrqyfZs0R72i/hfHlygULbkBqpKWuTRGg2VlTJTD81D32gTazicSZN9kDEO9gBmPlF8uRgZAwop7yuKkfMw51yOiBVVjjgYiZYPmCNduTuLOucBGdjxUShXMGv1UVJL0KHkKZcpyU6hzIQBqI7b6f7N/v7b7e3v7ndvdof7PPY6JWRBVpEHffg23f6+3/4nu/SDZz+MT16ct6BADGIQmyAFVWVihXIRro6AtQT06gs2WpIkw/seve572Q05CZpIIlAlVRkn2o3aQwGK0AiMs0GwQIYyizXTB4Cp1/02T0Pqdyl0IbCgCRxKqc/YFUiVC8unWdeBe4KX2sDMomrikGhhPqoyZ4hkdYCyylwUOUuKmExdU0WJZywE7IiuE4lKrCjkoF/LSnX2qqZl8ybk8dVIuZNKTyDtSWad1goJcNZQAw6ZaqZgInU0tphvP4QbbinZHMkZbIhZMr0C5GaPpv4UJgWb7BJN0D9Od3/cvvnlzf1X293VkHdpSiBCIGhh3Jqh+VH/8L9fPXy1f6GrzZ8tFMqROdDsNlxCIiziK0otiuCQ9j1yqFDJun8YDoc0ThKZJciypf0oacJu0EnUDUsFUKABkk0/JAACStAAALALQgaLPr4+/P7/eHP/7vDss3WzCCcXq8vPTzgQKWsNKHpUFSzrBia4CWm5ZtZ3TIcCVO1JBSa9+DNZuiHOrVy+sYkwI4WCA9MiUOSNosZNOqoyV3xy9jcjjlZtwkFJAbY1KuGiGiQAMkXF3mLauBT6SOD6iZVFFXvye5CJ/LWoWiW0Cr6eBfExIHqttlh+0WhkyNv3/d0ft9dfPY53w0pw/qQxii6iY8Z+kl1Ph1H2QsOg77/d/w//9lf327FdBD4PITCTOY3JMFJqZebXxl9LTqvzZFgogYaGpY1jkjZiu1cRZNVAlFmRIUADIugEAJSKq8ProlCoAgIEIBKSQhTDVgA8asr54fHt9slHJ5LpyUfrEIJTCTXFk7xuAhgYQ4oJlUJ/iWNSBfdSZtHCzAq+KJRLLdwtr0gbDNasgIBJzSI5gNvYtdwSR7eJY8GiBkExUm30vIxGjZg7k4R9ek0Jne7NPKnoAVqUqvL8hsQlvFa8c2vV4/DKBeGdv5qAYoBXAM1+zIRKxC1sson3pKRIfaKcd68O02760yfd5YIlpWlSiAooqY4TbUfc99gecNdTn/D29f5/+l9/8yd//vL02SmzOwIZeQapiQHG1awExuR1+hIxzRfKkmPZkgovOu1H9IMY3mbRDDA0mBlBMyhBMwpNseczmSoBHShAE4hUCUgHTfssK45tuPh4HdtaGLG3OAM2dUPVDQF1yuHdN16CRkmjKjmymOnyFaMKrvaQJaQEZRFhJlHNAoIi0qHtTpomloUu4oGAgqGlEw2nlaR+kc4kCbVPpgZ9l+bnP50rzI8126jzVp0z59KGxC6CeAqJYt+e8JQ7wcqyhQpWpVRdJir3NUOc9unwcPgXLzb/7V9efP3t7ddvJ2LEwEI6ZW5ZAiMQFgEh4O4g20SP98Pb+/uXmyctg5RVJKsE5rJYgTjA2JqqM0Imn5WZsEx7ObzbHwY59DImi0EyJZpEkodsBQIwwCYZAWDX3BXIZVFJodmhRwESHO7z6jKCIUlmJgGfTyImiOXgXg+11LsglXEaNTZQSizF9UvsqUkplyqKFAlXUatchT42xGDKLElFFs3utF0ulpFKbbW2AVnRFTV38/UrK1oYpAGMOnUrrm7jJyJlGD9SxzfB7EGeDjvaAVYCp1n+rDJs6ePwx4ZHzGLUWis9WsGwhFwcKbQEILactkkO+d/8Rxd/9unJq9f3kiVSZM6iysRZwYoI7QLWHVKmMauADv10ugmrRbRMXyQwQ8FJVRhk+vfcMDUvMsMq3FDR4eqgV70IUlJmiqrDRJMgK2WoJZJSMk0AaAmTlgrFZD8BApCgSYvNZSNqCgC3r6dmsVudd7Hl85fr2LCPRMUEAPWOpVn0U1sAVgiByRp/4Ey99iOWQrL1ggiO+7cMnMRz0PJPDIgampYaCmj0EeBKtQqj8aVywLC/q6Mnm7hQMocihXmoNAthgxBv0poZfrnWmRaV0jjVMGo3UbKKJ5fSI5GAXSygcq860mpZbP9WaLUypz+b3Wa6G9bA5TruDsN+kJxJkcHEIJWcBYoiVXdRFy26CJ3w+H54/8dHGTMzLZpmtWgWXezaGBpPlpnYez7Yk2vvDCAm0CDp60eMVjClfkA/6pgsfQMDDbAIxdQMw8TzfvtJBOKRlze1nAwoIy6hk0z9tLsb3n37OA3pe9Nl1urUp6wCVewt6+qLarNl0yzki1jWuzRG1JUy7mMpWaETomL3ZuI2clhQH1Llz4ALvh53veGm1OvJbUZNOPDARSjk2K6oRc8iqs6m4E/pJue+79k1FTZQSFlVWLTU9j0qmwBsjnZkxUbj5lFW2mcGqJq24/66P4tI07QfcmQwI4tqhqqEwMTcZxoSDklFuQmITASMt/nXf/v62y/vpl7ElE4uI1WuQOostCQelUOSqq7eHfh1vz0kqHJAJBDQBOoCRYZxlzEDQHdkQ9EDQHSDs+gpjny5mtpIccVpkv5xjE2IbSCyHqeS+fraFOZY/MMhg5irfdmFZZXYvMSmUasm5QJCqd+X2EHFWiAWuavEA1gLiS8tOR4UwwZ5JdqY4jHqVjWyJvFFMgqY71Hy6mJrSpWgeTLmIggqt5I5BpYf+qcXSeeIDTobAzCH/Tm3mG2coJYNUcqnLRMTQrg+yCFZ2EPguBv5/V4fe01CWbgflUgbUhFJWV79avvt7+6GIctR52AJ7FS9xR+8dKAUvUYfxpfvDxcdn66a1TJaN1hseLlACBQIiwZtQHIhI5D9yarFquAWlgtlmS2sASCYBl2sQ9Py8qx59umm6aI7m7u6N0h5WLHOhprpo1RhyhQ6bvjSHpmFdVLUfmnySGNLACspeOefEpOpqbFce6SteFpgCz6rkAVPLKt1jDXrJBWUbL5SfrdJ11u9odlIkyfEJcY7jyc3TvZmkZpnEHxFKz6yELwZzH9TOGw18ZITkzLb7CvePUx/8+XDl9/tIFi1UHDOsh8kijYt5awaNDIdkrZBA5CFdJJ+l8pGCi7UVOdFcPOevaFkLiJ6cj38ZN0+nHdPbvsp5cMkh72QCilxQBeIGTnRmKz9EC0Tq4oKCEELjJlfjh5GM7AAkoOcCnZXiZ9DMgoOUUlAyAtMdJSu16X1HskiclvFlywNEykc3XtCxVaviFHqZfGaZplVFicsmYfNDc+KK1X0kFrprrDmqpEWsHVRzIzeahBFaFMrv8CVa2J7SvWY6ILSvDaOXcYDGZ6+1LipcycHz/DvDoSZc1izgC3zUR+czfDyabf5kydTpN2Yb+/2LJIkb3sZxzSlnHIOjCdP17xe3B4Uqm2gGKgJgIIjf/bPnrTLSDWg1BSHLBF2+KxxB1BSZupWTYx0uow5iyoC4dkJ/6sfdP/sSViwqmqaNGVhR6xJNEtZJFuDBGT/U48QLpQGFSgwbvXh2+n21S5NqAJn2QWEUm9lp9fVb22uQOrYVfpX6Iil2Wx6/l6Rzf2ZSh9J5XzergLMvygbGTxuVSS1Hq45X1OHOl/pGUoVczuWFqCBAzD5zBPrEaOsBMYyCac0ON4cgMJ27CIC6lYYMzP1mkGNBR7hy6jsk9RnCk0XPv1Xz1dfnA9pGifdnC2n0I0ZsQkqDIQYmHOmNK1aYtJlw21LMVIM2i15fdYWjGKiUnaA0YU6zVRWCP6QDOC246tRbh77q4dpu88MiYRA9KcvFy9XpBkimDIGJ14HxQgkYHRecAxpcPOq/ULZf0WK2MR2GW0aPDMxm7MopExHk15jgeuTdSZtoWsNWj1KOmIVguzOrzWAlfRLS11JCWaG3mlUSM332L0HAj0K1h4uy7hKyby+yVGqONnsDrDlKTBg7NLij99Y3fSds8JDMb4nvxV8AlFpzSKq5fPatQE4cTxiUUSL03bzF5fLrv3Xf3b5ZMFrmi5Pw8+/OA+BCMKQYd93Ol6ssOrAhBh587Q5XdJpRNME8wizszI97JNDIOfXPNucEqPpwqvH8XdvDtu9TFnSiGmQ2ITPni1frANUxwwQGqADVowFYclYMVoGAS2h88yAfbLJ/3OmOwCA2BIHSLZrdPZg38hjv2D3cqqcq8rsxQxrLHBUdYuZ+RKBvHmbnDaUkOzoripEpCo8q3XeOenxrMBCCXW+1m5CVB/3aMsczXEQNTiLc9bya6pDZccgt14ij6gO2m7d9oRVTymBtAyqNPjCmZoF2fLOEtHtYwJvPj/5yZ88+fTpogk4a/HD58sff7JhZCYEwqqhTRM3LVpmhaClzeV62YZl0qDCoXgL5vSpgm9ZGqYSJAqcCJ5e9/I4vL0bU5axl9OGnq75s6eLk65ZdCFEsmC6iOgioq83jKMCST2pBAgIwBJoAbi+ai8GmjV1q2Ab3Hwp5shFZVX+iU3U9fJHYZ1jzbxsOt/A0RxQ7wmd0YxA3gYJJt8TRYjklWp4BKWyXbRQaatGHM2sIY/6qN25zEiLclxjdHmMIwkTs1n5kxufPCph0rGTlqheHklqZC/t984LZ2QHFVbq9IKofhrCKnaXS95NT08a6ZvPLldDElAIlPsJJ0t0gTjxlFSgGkKM3Lb04jQuVjEQBQYH733zwOFPCQ/9pRmPiM62wz8f9O9Gvd9PyHK5Ck9XdNqy5DxMScs6IAtUMfp0jhnqeeV4BGPqpMT2vFWlgwCOOPusXZ52TRdCIDY/caMlV1OtWlyWT8BMktW7b0FAFb5VQWBF9tqjt00bcbRwpmBWsc1rZEkf3AUCMSGVRY8zTJEnEk6M1MOO/4cQQY72QBXD9LYjPTIPr3boPEW+FrYThyBFip1V2gpdcNvxQip5G0qVJyu4HkV6R0pVgmtuZvzl/y1s/66fPp/yso39mP7w+jF997gd8/VeNi3vh9xGlqzZClfMaUzrCFk3zbIhJmZmogwR2zI0lzIJtSRY+y5Ff5h0xfr6ZphSbgOeb+h0EZGnV9f7hWYRigQidAGqkFymIioGIHnDGQGTKWpGzqjs4c2lHgoBJGP3KLu7QbJwKaMTLOEnS+VY4X09NinsTdoCzxulFABLflp281hNFPCuAOuf99Bj2ISS4kppri890lBVKMVa0nGL8MIixFeu8C5PBT2QA+qtrDX1UNs7bj1wqtaReJS/+u6kEq31iOCa0ZaOWnhKWgHfUbRMCKgA3FHjdCUAVF3Ah+poBiLShy6+vT28vz3sJ3m8HjKRBLo4a3LO20QhCROPokSasmDMXRNWPz4PndMVUhWoQIqQCPeDGqiK2sfQ9Dj+8qv7VzcHJuqini64YexHXjU0THIYUhBtASYwIQtGNf6N1jQOBweTalsTNRTBy51UWZqiv8u3r7YPV8PZs9XReRJVCZgrdF4Rt5+Ty5OlmFlsRktRyXcHsEKsQoWiIOp8VzWfg9bNuVAmYmbJYsDoRKYAs/qK1fAs5Jmdh4gy2lmMIbgKVg2o6IBmPVorocVO1ckfihTiPNHcRGvQKzZKVuAvBkPFIOGZdUU4N6xj/Y+OwE6hmE7axyR3h75XUBc48DJwJEjGkHUQmsj22zMnJQL95OyLf/3RYt2hckZAfHeQM1+romvppCmsBg+78eruAMkMaWKIDAYuTrtnp50SH0bZdDhtMeUCUbUDYNnQ8oggtcACWEQQkLWsJNlGI2cuOqpmpJThgYxADLBvFPtevxLc+UpJAKXrntSb0+seNRcDXNc4mu+igdIxCS7ABgV5hy9MOBYne+Q2AK/qWMj16OkhX0vIP/KSMgY7FEGr5ObQ4hGugk7ByfnYhALUTrwMQ10rQ5V1PbmREpoMJavUXPzBjaBMpnqqpCBMi2ZaN00TOFIbeN0017s9ZWDUPqFdaAdKwKRQCC/4R//py83F0oKR5e2FuqLmZSiOWTK84u5KeBSdJjlfh0BdGqWNoWU62YRlwzd3wzDp81MaFeuDPvbICgZSRlLkrOxK7Fz0TLOQxg51qD1qqpuni24ZKZQRqbVmCKSUu8EQsXl33qu+/deFTY8dqOBQeiBsXyhKd5nIzLi9Im8RCZS9XcZMW1WKilp5lWOOB0bAqvQgtXN+vJ3K/cBFkeLaZQcXFcHcLaOOxRebXGw7glN3Ane3wj6hClLX6IpB1b+U1NM3kJXwSh5JSavRVXPPDfBic7puVeXTy/VnL1Ym63LgLmokmgRT1ikriOK6Ob9cUlAm8pbaKkEX5ke1kujydSGDTIfTThiLGE4WcdNx1/Lzi+Wzs+Uw5K/eHQQ4X/LTNX98Hk6XRW4wVjsKJinEwswoeeOGOpIBsJY1u2Z5yZ/89Mnp5YJDefgCve7KTrwN00pjm8Vpk/fJl2w2iPKuORDZ0nuGdZzdlfCtgJ8rAyIws4rW4F6FpxJ3tOBA8RbfXVQ2zPvAa7J37AeYDWW2IiqHCczqiXq2BhdSarJQzLfYRoFLOvYGOprHQskA8u6DgpyG+dYGUMZGxiqnjzar0/ZkFbqA9/dbCZQCQkTbMgiHSaekSbX0/jICMwcOgUMolYYySpee5oYNgIiLFxDlpx2fdJHJ8sp+kl2f3t4e/vHb3fsHuTyNm0U86aiLHIgCoWVYZV283GnG1BxZmz1ydLU2MiIhRsQ2nFwsluvOUJZdL581JhQu4mxCZxWlbC2alYLCTuD+SXWrVI0rc/yoqZbtAbWHhYLAzKSqscahIySqvFl9d0Btvi7sy2PcHN6czpkOQs42Zy5A9cwuc7+KfQ6cpqm4NKOl2QHO4sqQUPkhEWtlItDSpwmqzluv8x5NHyGhv1yuf3TxbDvtp9y2zXqV8076rIGhgjEpgEE07fL+ev/+2+1i2XRnMYTAbAwmwylMzZXqGN1VoICu2/h0Gd8ciMBMU5bXd4dDj0PCJ8/i2TJyoCkDIssG5wsSxZg0KUSogWI2LCJvU2MUBWQAGGifciRKo774wdnTTzbtksvhcu6jlQAZR7IUr/IJH6uCSKQ4o5+EVqbTsi1WZPLG6AJjtgvBcgOyFNu3HljAVCsHRw/JZoikNTmv0AM3CfJV4oJonmmQdWmi8jQqjZdQ6BEOuYVSGZ5zBHxPSnF6bcd4zRhrBseObIXJCaSUOmzDTWkYOsoDvOlEq3yrlFve/8Wz9S6F77bDKIdJspY0ZsqaEu0n2U1KoPBu+vv/8ev1SXf6ZMEgZppnzMGzEoX58DMqqZcG5pOWIgAwUQJUsO5wuuDA5t0agGWDi/wlh4gAACAASURBVGVYR91Osu1pNylYl4SWeT/JHhDoGgjABBBg1G0FAJhuZfOj7uWPzn/6n310/nzFc42HlarraVFblMXOLyg1IOM6zgTMOuy4jVItRqVKIHhna63Ie7pd01T2fsiKnwpmlBYGsEC5+ICjEooRuXxhFkTC5YQj4hmb7NO1JDnVLCpB8xUpWkWllihKiIc6PyhpjpclLzC85bnSWpjXcYStDmh4O4djUqgddAZLpwSUTlr6l8/DId/+9qofcsqSRbPSYaRtr/sRHHmxCiHo8H745pfXH//orDmNVPqN1WFYPTKZFdvwuZ5oSQG0bAik4Kw5qakhFLhIzKpKSm0gifbzEJBzpkj4/EVcd+2bd4eHhKRYMNZLut8qFN0yxEAt63iQfaDm89Of/1c/OHu+CNETVgNxKXxHnABVwLcJFqMGZkGzcbhlFo48S1FMJCBCrnKG61klNBVSVtijfZYSc1Rn0Y4qZZF9WzkcZpxtFnemGg/Nwnxf2dxFzSWEurjk0dGe3jiBIV4xN2ehBBf9jizYUMnG4PYMITJnm8lCdRCQlpb2IxZA5bPswaani/BnT/NXtxl5zDSKHEYcBhombRbULQLZPbJ+83fvfvDzpz/5y2dU6ipahGiHamvgcLt2d2dAkNcRAVnykHIgUqZsJy0WDdM2HeXA1IbMHNrIL09DOsgStG4QL+MwkSj6Qz49616sMxO1zEGVVPaBZBGHfcqvH3vW7qwNi4Z9x4LA0kNmF2J8JzLBE0fXwoCqo9UpohKPqthrQUj9OIBawDRdTatt2iT4Fk0mCj/76+cc2cgrSsSi4pRz1kKV35fLvGXbrKAEMt9z6b8g5tpECxyVEeaUwxyPaq9KudqqI0UawdG5PyYWlyNPit+oC23+Y/VDJguhYx8V/H0+d8RtWLzZ8SR3uzRM1CeZMocuLJYh2EGPCgGmvfTjtDpplydNiGFMMiahAGYrEPhtAdRuiIL0JEMef3/3+DBOWWIITdBFExcNwTbyE5HtbCJl5kXDTzfN02XXRNpvJ44MRYxYLUIbkCYJDZ93YaFYn7QckDNRg7Qdbv7h5var+/5+CsvYrBsKzm5nubpwMSMn5Ns7DYrn0+6snFIFAAc5x6DCR6jSBnj4U+u5IIBkkrapnbgkWcLP/vp5iOxjKcSnJnL1OJ+at7D/0m9S1rA0hBScKu/m0jOjx5ZLOm/CK2fSWrgpdqpUeoC9wd7boUqyUdbRQdkzZSLPIxx8q336LBH8PLUa2yXJ86v9ieDVzWE/iEbmlkMkZgNXylmHKYdA0/Xw9S+ubq4O3TqGZUyqHJiZmMkDOtWpKVsbFMSYDjL87m7apZwzU2y7cLaIXaRs1Ssxgs6BedWERWxyAgWOHQuIQxSlQ58yaDuIEp5tuiW4bUhAh1FSwJAw5pwn5PtxeLW/f7vTRVicdaEJRwVh42dU7cL/WhzT2hztuDT4L7UYpumwOqvyRwuvOgtbFnlVVbO0HDiQ1U4kI/zsr5+FaKjjB7RQvfnsCfMWD4eraolFbrHewiPI4BpOyuBmMCuk0TVaomp57AaG8l9HhuI2N2808CJ6GbZLF1whjX03iEExO0sngopO2+nhm+3Z6/0GMox5zEpNRAhQCJiIU5IsiJGWbRRAJ7n/4/7bX94cxtSetN0qcGQOBb/qCvgpIWV5x+3Y//oWU5YsIVAXw2bZBOJpylMSp2s4WXWb0ESi/aD77ZhVhqzbcdr26X4vDw/52eniJx9tNg1n1UFwmHJSZIINUuzcEaZ8n/pX+yTonnZNF2qiBaqMyilPyZl8ZeFXHhdvgGNV5PhKJyme6h0JbJKk4cCRoASlnCX89K+eh0iOJQ4+qFRyPqq4mBWV5HAOE9DSx1QQzY1zxkUDD9a6q4aoxl5bmdkCa3XAbRm1o8vxDSikvupwcJunqgUSObAqXGDxz6A85uFmuPny9u3fvOWbA4te7/PNgH2icVJiBdGUZJp0taC29VYABYA8yN1X26s/PCiwfrZou8b3Bh8lP95jC8JwO9z//TXnbIdhLdqwWUQC+mGakigRE59vulXXCCg2MbbUj+mul1fX4+sredzJIuInzxafXyw4INk2diIGTZAp55SyEol4sCAKIv3r/TDmxbNl7CLY+mHN6b2TpDxQ/Rt5kLR6pjGsEgsNajzezYZalqBkqx6HFSqIxKEk58iThp/+1YsSNy1v4yK2Gd3Suv5V2vMxVknU8a2Gs9m1XV5iNx+PfWZfXlEAqW28ILUyYYFULRhJ/lEllKP2Th2lPYRqiPCPgkMduTkSoGk3Hd7urn51++5v3u6/2x1GTZO8epgeJvSTObOA0I8KoG24aehk2Z4um64Llh9CkLbT9W/vtrt0/sm6W0Wv3FSqZsBKpIDg+g/3+jCpImVZtOFkGZn0MMqYUqDQMTccctb9kB724+1h+vrt8N2NPO4QAj55Hn72cn3Zcs4YsoAJGTzKNKQpqwiyyDQpqVLkLKqQSEEnGd8Nw5QXl8vGOmxnyDmyFq+gzJS/ahfFZIr7UM2wiWeVE0DZ1OyQB5AiZzSEEBhEUOSk4afGzzwQwUFlliDg7TslI9C66W9+D1VeVqOHXc01kIBtGTzUGQ6WMw2qKlYhjNxwjMJZT5BzPKJAFIhFqyjmeqN/tFs9vGxbfjfeD9s/Pl7/6u7q378fbkYm7ifZJ7nZ5tt9NrFHQDkrka67pmn1+dnysxfrF+ddE7kfJWe1T8yi21f7+5vD2ccni00scEaGhs4SGLEJ9GQ57qbxus8ii443i5ZJ94eUk3YU9tvx5naIDV3vp1fvhjxqn7AbwMAnH/GffnJ2sgyTamwCCxrmhilDDyqJOWWxjXSiREFTptiQKigpch6uBkO1dtnUIPH9EEjVfw2vyyaOalWmhfopXK4wVBGkwB7cWNQ0FFEGmhDM7FLW8DOLmx5T1M9Od/5VbAR+1J3/BhYzPUopigx2FHKpcnMcab6+G2U2aKrBsAZdruoJa9yl6eqgbeBondPKFF4uly9Xmz7lUXJN7ZxK1v4vVSJmnv1hzA9fPV79/fXdL+/Gx1GUmGjM+njI+1EDA6AshWZ0XVh24aOL5eVZt+zCu7vx9dVBSvnMlB9Iwv5muLs+XH5xulg3hDqRR/DBvDrvFs+WD2/7dHtom7haECvGQca93j+MUGpVx0neP+bNJqxXYciaJ332LP7w2YKT3j8MXeCnyyZEAvNhyP0gmVWg+4PsD3mctGk4i6ioIkQ7GSUGTNq/2Q9Jls+W7apxalXLMPNKkmcKKC0yhldeFXBwoHL6GcHTz3pBMUsQAVmkATcFv5CThJ/+1TMOgeoMzVR+Ti6o0htCbV6s86hz21BlSuVW3gng3w7BVDdilU/y9MJTxXKzOGRcHRJTaLi57ne/ue2zNJuOWyJQw/TD0/MXy812GrbT6EjoobVqf1xN3anFJNvf3N7+4ib1aUqSBYAMSfe9iqJrYxMoBMQmbNbxs2frTy6XJ6tm2YU/vt+/vjlAMWWtvFCVVJEl9w+jtuHZF6fEqDkzvi/XNKsmXiz2D1PYTsuG2hjHXbp6P7QLPlmFPOjNPi8aujwNhxELoReX8ZOLFpMk0XUXnz1ZLlahH2UQOWTNYxofJxGEhkNLgFJDKYMjNZEyQZL1Z6j0OrzvB5Hli2XT+bE9RwW/8ofWfKC2L6JSMHKk8KqmtZDMRkjl12R30oyGOIaykyInCT/7qxccfd9U1QXKHUJpfaipYkn1UKzLOW/h+eRuTmW1aRa6qh242lVsq8RiKtDJVtztrvf9l/e7Q6I2RND0bj+82+dFbM/awKyEFiSq7/r9IafvfcjsMcfb/Knq37TP49t9vx0PgyiQIdMEELeNBg5NG55suk+frT5/vnl22rZNaAJ98373+vogSlnK3BtUigiUVDSDDrvp2U/Olqftkb3D5cKSEXTn3erTE6xbehjPA6VBpt14dtLmMW8HOV2GZ8vYxLBZtJdPu4uTDhmjyMvLVUMskDHp3c2wy9JP0nQhT5IiJkbTBkrIIlPKOWnTBSgLVFRTQswIUXdvDhPR6uWqaYOx2TIuX8uqoXtFG0XHLdpGETaODlWr5kUEiMsbgKoQqe3iCVR6fTX89K+fx1AyIzixKAMhIWNVR9hQNA730yMgxMzbyvoysWPNjHjzgdfH6HnM7JZ3w/jb28Mh9e8OKQlvuva0a9/sHx/7cNbFdSTQY5quhv0+pQK4fNTeNI+/5CSkpUTGjHbdhiW/+fXNMCQKrAJmLDp6ctKdrsNnz1Y//vjkoyeLhW02An/9bvvt+70J3XaunqgqVFSzqEBUGIHGhLiOL390VgRG5zI2U+TssVk364/XzTJ2r7b9boRSCGH3kFrGkyZs1k0Eb9bt+WkD4M37/vS0PVs1Vzf728eRIg9Zt4eh76duGZV1P+phL7Hl3GdlXSzbttHALBTSJKKSEwBtQKq6e7PXllfPV6EJRlC8bEFAka2rsbjheZbg+I2ixZaGs0JODNSsedD6AYUiIYZoyGl5wLMQggfkyo9qkbzYBrxGOdejqvoP39sDX9USvnzFDSZ9J0vdZevlouM8UQEKV4fH39yNbWhXDb/dHyDtSdsx3fz6Ni/i8vkyBLbFrsphUDQPw7BNvIi2G9u8IBTGoCTet9PS8nw5vNrtrvsYKYSwaPnjp+tn54sfvVx/8fLkZBnNmLLgm3fb37/eimoMIQSrqNpR6CJCCoiQQDliEgz7/NHPzhbr1r//D1WsKn3LZm5MzS7tfnG1f5i4C7lPT5bx6WWLCdOUu0U8f9I2HK8e+qGfLs4XY9L9kAJxbEiJqGFJrIwpq4YwjrlbxAz0ghgREiPlRDSJIJFmTYGCoI049FP//tCsmsWTjtvC0Omo6cv5WYkGpUqurnl4lASgcx2zxM1iaVpCrUIbkPF+BSSZrtF4yzV58ucUqwajuXpRga9c5OBUUjyf4pI61HuUyO+zX7CzopAZmYmwMsn4/tDvpvbZsmW6/+ouM4eLZf9mOz6M7ctNe9KVUF18A0/6fPjfXj3spu6TNbGVN8ywtGTqnv0F0JO78eI6v7nu14t4tmkvNt2Tk+bTZ+uX58sYaUqSRMdRvn63+/rttp+0a7hpKDBnybabA0qqIva9bgSQDqPomLrz7vkPTmy7vi9EbS5QKw/wbur/w/vtl7dxzcOQl0nOny3ioiEOq1W7aAINuRd56CcGZdEY6GTdrJZxOORhlBi47cJ+n8ZJKahkFdJtP02DUEBIkiaIIgnyJCGQMrJq2zFDaVR5t9c2dE+60LKbBODszDM2+Fna6t2KUm3J/KXIapZvqe01mbcZMGnDoXaFZpHw0796TqHqCk7m1DfSuXjhORTVLMUCk3r/vb9tJly2O6mkfd4rMZ/Ld0TWUB7ZTTkyItO7w6iim3a8HaarPV0u46YbvryR03b5fM1NqM4UoR//cffLf/sH+ZOn6082hSwWOyS2OWQ2vWHVy/ofH6bttFqEZRdXbWxb/vzF+mLTEPOUNWV5PKTv3u9fXe/v97lteNkFQFM2BFZAs6gqskAEIdAoyJNEDvvd+Ok/f9otY6UUNB+hAiKKkzZf3j3+zatEeRpwFgIfUmjik/Xi6Vm3WTVIklO+6XNowtl51wVOh7Rqw7INuyGB0DGg2PW5P6QQaLWK/ZSJKXYBQk1AQsAiKCGLfdugJtVx0CbwOlIU2n+3GxiLy2VsoysSx+TftrWpGV/peJgNyyGvtHDp/Futjg8QsSAGMrU0J+VaAa3UxuPirJGoNa8ApcGktEtS3RdS/EJndJ2LXjVvLUUKy3VlZgLkXT2Ggqpxl8JJs/zxmbzvH98dmhcryuj/uKVN5C70/3i7/e5Rsxh+Q7HOuv39/W7UeLHQMjiyBpw5QSpfFkabXaZ9unscQOiHlKE/fLE+XTVsx+2p7Ib06mr39m7/uB9VdbUIWSRn1O98EEXZ/1q0WYxZAog07/64vX21KwzVKmvH7HMS+ur+8f98+7ibbq+GkNEolqfdyyery/O2XYYG2p00Q8sSCaKX63hx2m02TQvmrMt1c7ZpqVcGui6cX7SbNnLWPCGNmsakkMQ8QA6jIGvDUIL0mhJxRBOpi4FE9zeHb/+Xb2++vJNkbY3q1LhgF1mfR1Wk3DLmM9JQGB1VmylvL0+qyqU9xNc1Vtg0E3MdxLUw7471UmvB1LqN0uK751f+qn2G/5+flJ0Rakdlm7Rs3mENvxIU9GY3DimeL9qP1rvfXNPnp83H6+kPD30gHYQfto+/eN9umuXlyiJS+zC++eoei9iuY5kXUTAx7Ov8yLIPEAWRk8fpoLjdTjePw8uL5Rcv1qsuqGhWiEgWvLrqX90chjFPGW2DromJZJqmrDB5SsVO14RoZsKUoYnaCFKVQaZDdtLqTmiOn3T4+uGb//mP6fX94SEtmc9O2svT7smmaSMfspBoE7mf0i5lJOmasBDSlmnVHm4GXXKrJENmUVZdtQFJh/0gHRNhHPJiFZpI292UJpXICxCBJCgF0kkRlZVzhgAj9OHV8Pbfvzv9bLN8uvielcxgoTRrs+L2ZF/gkGfzKW8sRPl422T5IZdEo2yncoiqWIYCaFQKEnNcdXblsOHRy+lgMSkftW+nVWjdZFDBtQiA6thrH50WPH73uH+748tl9/IkvdtN+6SPQ/ryGoepEaTf3tz+4mr/bi+jcMrhu+3j4xAvF826hd+qUAynqvaZ7Sjxfvru/f76YfjJxyd/8cWT01Urokk1TUJEj/vx7d1+GEUECtosm4uTuFmWSl1Be1LjHCoEpmGSoBIDqSAwx7Y0EpN/KgE65fSHu9f/7pv3v77KU24YF0+6p6fN+aqB6Ddvtq/f7kV0q7Id0iLGi9PuxdmyAVEWHSQpQNSohoY1cAbzlLVPJi41XTg9bzZLOzKBFqcNAGVKJCkjqcSGrB9ESack4whRHn5/e/3/3Gku5xI5KFil1gvjinIEtklb1h6DmTr5qnPV2Wu64yBY0o3oq14I0ty0b216dncDvNIEZxNoO6ZQO7prtuJ9k2U7Ywlb81dy0BHTrLm/ut4BYcLzVfswDd88HA6peb6UIU2vHhoV2glAEoRGHX7x/q5Pq09PVkw3v7nux4SLs9Bawm4uaD2O7GetEkFX+7x/GO+30w9ebD69XLUN9oOkXKSmEPTt3bA/iECy6OkqdF24ujv0I4iEQXY8ioqoiigxaRaSrG0kACLSrZrlSYNKBGxuRcZvt2/+3bdv/+79es2Xm+XmaTxbxU3XgHB1PVxf77mLpyfNdzd914STGM7XTSTOOeWEsAwLpiz5IDIpEpXMvTlpxodEJF0kmSgdpkQhJ837pKApYMpgaFYQpLFjiCOmUaYxccunq+b+H2+f/fSiOwlSfLyCSIG0wj/KF3qqN6TOWEIo35UoUtg2VMqx8QVKCAooRUWt3xcmqLD9l+r5p+NUbS+CK8NF9vBqtndRm8xkXwdX8KokIoYHpQXRDrKf8c3iNRGWTfPDM2q5/9W1bpp42spXSUGBkIEpM5Pobuj//t341d2OsO3zOGV0XDGk7Nsp/6KYvWBzn+4ex0XDHz9dtS0Pk0jGkDSlTKDdIFf3w5SzCGWVH1yu+zE/TpkABataAiYKZIU1q45JA2vwrxJZPu3W5wv7TvrS+CXgq37/t6+3v7puoC+WzRPQ8yeLQIgEMHLE5mIlSd5e7a4fp09erC5OFuvIY9YBPA5TauhA2u+nfjtJIF2wZoVqzkBEaEPapnTIaEhJkZUCMet+nyjSpg0IJNCmRWxZJ9FA3HG/k/6Q5Ov73ftDt2nLqWEeCxTWNub4IAUx4PuYHGoI9m0o4uROdf5aART+Zkm3lTbdPgVFv0M9oK3Yk1l5NSmzNirfQWvXCTntLl87AK2lTfXjv1Hfi9pVbfeTUpZUgDmcNPz56SnR7h/eT4PYMTQlF9GchADkUfSmV4DbMAiWz1Z219JwMVPIAixhkuZ+Gob09LQ9XUVm9JNMood+nARN4LvtcLsbUsr9pMslPz9rH/t8/TCICECKXPiZqooAlEQkI0Y78lkj48WfX3brxmSPQjb6vP+Hq9u/ey2HfLmJF4FPIq+YwOAQdv34uJuWywjQu9shNs3Fuls3lCaZAg45P/TjzWPi2LZAIoyam8CUJU2iLLRiGYUDt2ukrMR6ch6Z6GHIsSEOUBEEokyABtI+aZ6mSUBA/5CIdPt6e/6D09Lw5zQJfmi8aE0wPWqKZ4gzd5rpkl0mlboccf9C49XpkVt12aKqsLRivrEDG+P7HuCA5BeWK+1/ZsRaWNosJ9fbaQ00lSXSOi5+cHryk4twczCxznYq26raaRSimhXDJNPF4uTz05Jm+pOWQ/mJLOte9iK7JIL1IoZAKWsS6cd0GOXQT8MkN9uh77Od0P7nX1zEwJFxaiIFCtdUtXO2CIBkYrZjcQAQdeHTnz8NTc2eVEXSq4f3f/sGh3x+0nxysdgs2xfPV10XNl3TME2C4SCnqyYTbh9SF/j5pkmqb9/v3z5OD3266dP2fmISjegh97uUcg4BWIYxqIJFJC6YI4MoMEcw9dlS4pRkApSZGEOvOkqzYAQek8QGp6dhtQzj4yhZqmrhqzlHt3JcTV2ZOYQZ5JXVdYsiJ+rH4RUAsRRvJ/j5vqpzrxHUgJNo7v4wWC0R3ZKIMhStOaseJwbwzXr+DKp+igZm850jqBZZhmkZF1+cLj/emJ1lkCoC03K96NYLbuMg6BNtB2l+dN6dtaiQVwwMxTkBQJa7qT+kRcNtE1R1N6SUsTukIclhlGHKj/tkjak/eLF5smmv7qe3t/22H6sr2+NLJjGOVs5f0bIrftM2y1iJGYFwyPv/+5pududP2s8+2Zxu2svzxWIRN21sAtIh7XfTJ88WT1bNvk+P+3zShinJ+116c5get8MwStOEk5N2HPPdfkIbQchCh4yHQ3q4G1JOkpC2U540dKSjTttRSUOk6aAp626Q8ZBCoKSqozQBaGjKSBNolHXLzSIUEdl9vXCsYmPw4qJ6qlAXTufOs6KfWeuphyit2ipBEVn9S33chtwd63qpl4ncyN0OSzKLQslKiaXospUdoRQ1/VsPdG7ItGtcMDc8LKQNRUY5bZd/+ax/HKb3BxBOT7t/+WcvPr1cf3uz/w+/u/7tN49plKByetp5UlLoKcr3V1teQoDGXZrGxExZsBvyOCqR7odpnPQwJgUOo4igacIPX64Y9OZut91PTBCw5sJ0s3CWjFJTV59HlcBxE9tlgEvmKqC3u+0/XC268OJyfdbFRRdPu6hDJuIsMiY9P+nOIu3uhsfd1HTYLOLtbkqkq5N2GNJ2PzTLyA3f3B44UtuF2IRxknESO3bMWmu1odCGlAWq2rIGENAsGSz7g4I1iapSzhqHxILDgNMVOKI/SMesdohtIfq2847s3C0GxB6kkDZSCITL4cglIHn2B88FLEBR4XhmPv4tnrOuofZ5s/mVHOM45Dokwmtj8K2nJcSWOoTMF3v65fF0DpjGDqSAWbmPJxkaKH52cvIffxRO4vmT5X/9n3/x3/83P/7v/ouP/uKL08Wi3U60y+iV3//6envd25k7PrKaMakCLKr7KTD1Y55SHsaUs6Qs+1FSzsOYD2MeJ8kqHz9drbpmO0yrLqQsWUnFvigkq8KijJOB4t9JtU9YnnVNy+qEmaecf3+f74Y2Nh+dLNbL5uJ8wcyRWbJsb0eKOFs2GGSb0pjl2ZMlBdpuUz5MUNn3eRIgUxZNo/Q7Gfq0XLXjJBzCYhMRwSDtMDU0qUIQu4DIkyJy6KIio4kE4qzKC+KTSBwCMREig2PYJ7276yUJIEWC0UqZPHS6LEVaqktmexZOC2z8v+19yZIkSXLdUzVz91hyq63XwXAWEBAQXADiQh54IP+Bn0oKhSdShDxQCCEIyswQg2Vmunuqe6q6qnKJjPDFTPXxYGYeOb9AKZfuruisyIjIdDXVp0+fqp7zvPaYAtIB93qbY7Ohyo+glnxZFKzFLCFrlzpbyrBGXml+DUQTyjugbF0D9WOe6dxWRqiDAgshUvtUSy6hlbIruekmbH56HY6f/QnDv/7TF/Gqf/v68WdfHX713XGc/WKjfZTHfzjc/eawverjUEayrBqAysFIJmZ/OOUgHGJ4OC3lsC3JF2PK7sjm3PTdjz/bPYzLu7u5j6FNWFcRlruR3QFmkpC6+YVI7ohy8WIbQyh3ShTpdr775W02vnyx3V32IhJIV9lsNSe4SicSpvx4sodT9uQvbobNJiRzy9Cgwyb0s9BoxLDrg7ATpXCeDMzHUSkyJ1tmmyZeXXfqyJMnUoJIcswwMi2QnpaxDcGBSZjpAmyI5HrPHG+XvOTQdVi9AWoxs01ScUFBvC2lLMisztURKYsQGw2Bs5MT0ok6/LLgibCGzUrfPmHDmrCiAbhqOVCeO7a0ralySuP5m2t5Wkx2qfrrlrV6mWGFVv0sgVvKvqDGuJDYdzd//OLL0U/J/vKv3//Xn739z//rza++PSXzOcW+o0C/+5/f9dtw86OrbhMQIAFSWpGq/8E0+7TY5T4u2abFQIYgTh6OGSKnk4H8x19edp2+u5tuj0sfRQW5CGjppLiRkLoTBZWINkrKGAa5fLWBlu13iInj3949fnO728eLbXcc06ub7TJmGi0GV8Rt2MTQBby7X07H5XKIz3dD7ES3vTkVriE8pskCguB6F/KYLdnkyAuhHDaiitPJul5jLF0BgABRPHkwOGgOKGZTNX95Fem8vV0eMp3oenk45cl4sRjtSYhpKIkU8TU5XFeWoeaERJu3xxZtWYEaRap7PBuck1F+D5ut4a26tCriqAyeNKwGJb2NlKy8x+rxyiGQ1rpeHrest+nmVr5E2TYHt6yALXmosKDkypte08i//s39L359+O+/ePd3r4+W6ZDTYhAE1ek343f5m/TPX17/ahEPDgAAHTdJREFU0bPt803oNcSyaUGEgDEnF8U0+6y+JDfntlcVeThNu003LvbiZvPFi83DMb25n+mcU6lk1sE7Tjey3FAHtHQ7CpN7CKKdXL3cEwJ3iA7vx7v//VaML7/Yb4fQBxkX88n6i5CSp+x9F3a7mIGj2f5m+PJq8+z5EDYxJ2b3KbmPOdDFKIm0TBeP6vBhF/oOfQxjdkD6bUyZoqJKRmWiq/S9yNER0EUkZ6cyRPXZofI4k4IkcLdOJCRz85YoNjyOFg5Lz03ZDuGNIwPXtLQhE3jB2sWyvNpXZdQgIohPyVfUJVGNzfg9muFs8MWZVj+k1XTQ+Pyi0eZKlKKYbxsitIb7tVoKiJe5Gn62VHlytCDqJo/pd9+P374+/o//+/6b341WZ+rTHccZnRqAw7djOLyevnm8/LOXNz+6GvYDAjWAFDiDcT/Eu2PadGHJ5oYYpOvEzA4n72L89NlmTvz23fFxzFe7mDJznU8hDtDV3EkYKRTRMjwUlqEdNs83ly835SZE96vXj/dT2r68+Mnnl7shHD5MJLWTTEpy2YToIoLbD9M426sf7F99sqXImHj0lBbOCyczdipRYudCJZTuQ3JxyGJmvlheZuedUcQYTpONk0unBEMWUYExZM6UGCBEBo7kQ0IUTCP3+wBxn1JevNzUso6l0RT13llxIV6dUPUs0AbpVjhWTK/cuea2SjwUkoxcM8HViArh0UBbY/FRq0ntlRsMrszGSmWIrwtBWzZqRNkj3ZJNL2bJ8kZlR22jbZuiSc5gjkw83i9vv3n8+d/dfv270b2lJQRFaEwOCG5HjmT8xW14/fjin738wV98evW81z4EVUueFs+LTUvuo6ZMc49ZYwhdF8bZPn02LNlvH463h+TE0IVpzmYWNFDEM4xOMK+oUWHElFCK6jdfXPS7UIDq1SldvB1740//0dX1EMdkcRMW8+lkz68HDzoAFN4/pO/fnfrrHp1+dz/fPSyHcZmTLQsFoh2Ddl3UCKEKd0FMO8maQ6KzV0sigi6GMOhpzEtCpojRMvqNoCMnSCdcOEQ5jf7uPr15oANdL4NKJ3AVLp5nO6MYPrGCFooL7yktGpWZGucgKwDgFcw1hqEsGi4LrykodobmUuTJKKLGNpQXLAOCtOwtbqGoEnNUSFmGp7XU0+QjqzMsAoo6G4uUNiYLhXaBn7NarlW2wnEApPhs796evv7q/vXbU/XXkMZVV9xAZxZu+o1w7hcc/+rD33x7/MN/94Prz/cYumg+znY6pmnJfQzZkMz76IBsh0iGoPLtuxOA7OiUXZSyjbVTIeFwklajSS3GZocn9j26Qa9ebUOoIqtX76fpw7RTfb4foGopmSO7dEM4LQbSGZbsp2PK2+i9/u5hnqaUlmVOtiQu2bKDpMbYh9B1MgydqEIlDlGDMDBn7/qw2ahSDcwJ3SbMU3Yqo5vCZ4iSQYdBYpSHQ35MnAwa0Su7QZJznFxPeTqmhs9EqqnVbLGIq86oqnosXRHbU+Msd0FQZ0GZI9S0AUQZzFVKpEovU5ULmtOV6NVC2Wmp2JWE6kmxEkRpGRCCbab/WiEHZK00rllwJZ0K0K/srtceofU1EaTssnKmo715c3rz7siGEqThSvp54KQb7u5OF1vtAgK8e5e+/k+/+fTPP3n2x8+7oNkchFPGJbv7afKhI2k3+8F8GfpgD3w4LVHCdhe7GKaUS6+NE07JNQkQIRWSiTQzKjRAomxvNiVjGbL3b8avvz1cXgzD0I1zypmL23YIZqrKZfHv340LCeEMQKDiQbgU4SSFrHM33JMhjbOGOfV9HPouSGAM3pGetx3zzLSkRTQtnHJeSFeSGBIlAKYQicq0YDIeHSFgCAjEkgmBOZDI7MWqQCnz270Fiyf0WKvhrF/lufTEFjbR9IllBq7TSS0eMJ4t1s8Dsgr9LVK2K1evwrXWVLxaDYrFmrwYptbieHVNFWdJs6Q6crF8qtqm1Oy6payoYos67g1Ccj6mw/spJwqqFrhWLtDyIaCkFzlhDNh2AvpuK/Ndvvsvv333y/ubz3fX7+abbZ+NECc9mZn5vHjX66bXx9FiVDd4RHaeppwSVUEE82zumXTC3TsVCuaFILoeGkRVt5dD+UQXj/n07fF0Mm5p2XPifhsP71Moc6IU96M90r+/PQWVYd9f74Inn5LNiTn7kj1leCk0Ow0K55Jtmi1G7Dbe99E7EY++0BZD1JSKRkkoOD56H+ADUKaTJ7rIaHY74jAjdrjYSm/sVCDSXyJFVVWSQnHx0pOCNYtcEZE8tawqM1vJDYLijTRrs8Dda7GxANmIEhGfwvNmbuXtCYeLqtBdWowr6UTdBNuS1DqVhU4Ba5ZZnU6NltXqi/FUykKdFG3/21xoS6kJeOb4OM+HKUBcig5FvTlCX2siXh35smAaNKjPyaFhSp6+enz86vFbIEaNQXa9GrHtNRkXc5qI6IeHKVvJof1w5ONoyXwbteRj7gSR3Qsts2TkhO2AGASC0KPfRzqVuPwwYs7Xn2z6rgMxdHr/mGLQzSa8fTPqoG/vp2PKh8e82XfXg4I8zTYvXJLNmdnopiXNK/ppA0h6xryMc4r7Xd8NUTv1XVAhDUrsrjgbDkczReyAIBlOFydTwGnGo8GAneCik34jw0aPJ6dBBgm9gvAK9isZVWkmesHxqJR7WYretBy1msMnxd+VmKdIIYAEhUPGWS11VoMVHCh1rV5LC9E8UaPNmtiHgCitbkdsBcwaV+Xpn6iySwrgvk5qKCu81w9Sh7aXQOuebHxYfPa63Vae7oItpg0jRFGsAcDkumVIyYdN3O3j7cFVBY4l+7LwcUQ2bofwcEz7bcfZltmyI2WoUDSSNs1ePpwR2ZCIxLKtATljXNApNp1SYUQY4rAJ7jIk796Op1MaKF8+G6RstQ+y63R8XBZ3Md4f5g+38+aiu7jsNOhpsmnJU8pL9pTpddW4O4QudDfQyfKTpSkv5nsbtn1gEAuac+qCeMLd0Q8jtj1CJxZpLtpLzjwlPiwwwb7HZ891IFRkWaiQGHHKXGZrlFRjMyoEKnYnJQ9oJiCtda4GqxrTihMsUYVCcVoJgi5QQOJqQOdYp2uqWuJgsbjVgIqdtPnqLAG01ALOonFd2xLO0bOVuZs6tzTQV7bXz/RtrXs1Va6bp9HgLrL2MJdspqYDKPMECSmOUNVFJ9fOF3POuWHYwtuquHlUuOMw2v0px6DJfN93Kg4JQd1MzBlUAbpJJrPRvM40PS2gY9iqKkyEKnHTaScguil1jyaQQbXv1d2n0aTDPPvovsCP75NQVHFx2Q0bTWanOY9znhemwppQKxShuNMIYwFtLIEoT5byknZx6KMHMVGZchr9caIouoBpZlpAFXfPhscFY0YfcbWV5/u4jK4By+ySEAeF83S/0FvXYwk8rLoyFmjiNbur7mbtWau8Wyvw1YSz6moori4titU8oNBsbamsN8FzwWSV0pKVU6tGXfhbnEUSle4vYVRKtG8UnDRlJssU0RrMayyteXWpSLdqP6qWjaSZV4+nEK8Dh5RicIC0ysWFKP1FmC1K0ARZPIRMo2ejGeHeRY1BxCQEERAqOTHR6WpkaI1fjuTG2KmR2SxnMRe4a5BpIR27AV0oyFlCp91FpyGA7A5pALa7fs52mOxmE5PzdLDDYc4bTe7zMe33wfttvw1LRlryacrz4pbJdr4gcAZ3GumEWRnGX9VNbshmi/vVXkIXqMogs8qi3A8Chzljr/Pi5pgzxoyuw0UnzwadHrMlbi60H/RuNpvcVea7xTK7DqQWrh9shfLqeZ5Qs7UkVSiExkbUiosAEK9S2uYC6YwCVkqrvZqsM7qrfAsE6S5o77CmudWEV+RHkF4/TaFQaswXsprL7z2rvXzLQ8har26rNurHgEbdfbINzzdetwQBRf7UMtXauRDk6mb4o5+86IYookad2KVsc/bTYvfHfBitIOY6/milnoFSTKpJCD3nGiSyMTvNzTNVkI0pQwWbvt51OjVwc9GpAN+frn51R3cL+O7dOM+WzdnJkmxKfjwt08mMhqibXWfkaUyHY5qmlHNJzaQlN1VN6aVHtNLyKOLyTGTjcfS7xzmn7EFGjffJAyEOIyTChZlYXCYHiE6wi+w6OU58mPj+3t8/5qwUMix++v6Uxkw/36azaouNsyDKYnijuLdPWJ6xPole6B9UR1iOjQDuzuiC4KRqDWMo5Jef42ENvhWX1Y9QOVfUEMg1NZRG4TWvVDEjQBSGT1tYl7Ug6qCWJQROX0fE1AgaOn3+4+v5fjm+f8NFRU0hlhViLL6Y1CAa1aHXV5vdZnkcAWGmzBaQl2TIpqqes/QRDYXWHoYuCMCcPYjGon/MFKU7F2MyyeYQOOU0Q8A+AKCqFK5cDNtO/Nd3l18fAngyfX8/SpRxtmnQMfnkNvU8TL6Y5SEm82yWc84JZmUsjBT1QnUEDjIbxR2t9ihOkmJANrgjU+6P7kiXuzAazHUbfEqcDRqxKMwwJ4TymzfMM94h5yQ0dMb9hWw7lYUgj2/G08O82feNtayTkps/q4sRiwtg8WLFj4gWPrZOVmbdu/vEZxW7UYjE8iytJMKKo1YJeMFMJV9sILFmua3OXW2yWGuLjqv2DDU5hYqfB4E4ipVBxOX8bDaTZM2jS4Ntv+l215skAsf20832ckDgcj8/fjN7hy/+4mW/jeOb43y/fPXmgTFvrnW46a4/Gy5yL98c//b1RAoo5u4eSAsaSgbRJjhpEJhTBNk8Z5Eg2WmZ2UDXoJgWB9B32veFhpaotonh5UZevj70j7NuujvBXnRx7K77Y7L0wIcp3Y/plPOU3YwEfUx0d1epC9oMCOXGsbpwGmEGK7wlpeQBRpqJGTORnclg9M0QgoqJZ8ecYYRlSCmiV/wKFyxEMLnsZTdg23UqBIioSrl/SKe76fqzfflAvlYnUQgjouoeBSux1thTtvhXiaZ1l10lm7xIb8C6b698QRrTXtCTQItm9Pc1O+W5jaitrwu4sKp8sVbim98Cq4xDZA28bX5+MbM1W5C6GawYYjkRooBvVIJy3MoP/+zVix9cOP3v/9t3+sx+8q8+/fGfv4qbaLPZ4tmcpMbQbzUOnSY7/OLD8B+/mRYXwp1mrhoK5iUQJLjD4AIV9ZwkZTgYydmwZFqCiKQMc+w2sumDwmLwnepVL7uIIbpO+RRgiw8KvRxuT5aPs0RZFh+z5cRcSvDuDoVT1BVS5+gillNPAY2O7I7sYuJ0AFLk6Zkwl2RMRDaYITmSc8k5W1jYFrUKCCyG3H6LGrDv8clluIhhvwmBpn1cxixRs/vkko758GH6zJxR19L4CqLoYCPvUeuaxYhqXapGV66jRpvmomCx+oMxshK6Nb3Qc6Gy+XGvPBlW3gR86q1qNsnV5oRY902wpQveWJn2bxncy+bFCNZaPNaCO1t5VUXCRdxcD5tnw8sfXV08H17//L1H/Zf//qfPP99rFyDod5G7Vu9ahw6E0H950d104TCTMGd270vjsMDLFM7CGrgJIax91MmQEj2TgDuycTfgaiPb6INiF2Ub2ClEHFmS5MdRppT7GDLlkOZklo9u7k4lDY1IVMAFQTrBKvYth5NOIcXI7HD3XCqELeXMhkwmR3YkQ9l9KI55oZnlBBisfFQil1+gQxWXO/lkE55vtCP6AbYIE+FcILfHfJckLZwPydyFgVUTW5B+Qeilir/C8oKpqvfiCqjQCj3Fr/iaOIAwghF80uzYNGYVJbuIlj+qu6z9oTyHz/We1jJrE0bCz6ZWDkDxixWjSfHDNYiLt0gt1btW+621CCck7sPFzbD90eX2snvz97ev/+b+n/zbLy4/2aooG1HMkgWVOpm2visBAhweBO4gxRyxVD2K9gmeXYWANb2KMxmyuQMqsun5bBuutrIN2imDEHSFqFCDhiAxxi6ICHP2D/cnc3OnOVhqKnCtM4jhZNASrOtFwunuID1TCvC3AhxcjHRU75WLDzMkX00ArFAOhmqORbcNRQT2g766jDeDdAaAWdQj0n2egIfs748sZSe3hvbXPkQ2EraSameWypsiu3JPeJI11OBYI2R7zUB6LO7RWWeekyvF4Wd+lq0noAotGmxd0foqX23qcAbW3j8WiUf1YJX0OHvMtWpefkBZW5vW1oOq3nU4sb/sH787/vqv3v/Jv/ni6tWWa9ime3UWaBVgKSghRN1sIh0GhAB3ZHgwdgEiWtoBy3Q0c1JpRnMjddfr5QY3m3DR6xAAOEulUyAqsdM+hhAkqjid7pZoTi8qhaovNohEieVWtYGkpbygpXbiFCPMUWfDlOpWS+e9rON05Fw3JaZcKiLIxPUF+i4cJ8uO0WBEUAQgExBsN3hxoZuAbOw7AeU0ZYDs5TTah8nHDBdkh3ZtTdxaK18bnWq4q5CNqP04UueMlKPdPN05Cy2Py6AOCiWCDsRadkJLDOWsLmrC7TWVaJRXlRDW9KO+J4nWrFdqnUBrIi3RE8169QzjaoFLVx1ksRwWXTBICD0jG69B/+r0w3/x8uaLfYm4ZXupNORKaR+k2a8FhBhCAA3mkg09aI4YROu2RgniVpuqueux33dXG9l12imEyObFkAWMfewjNWpXev2Nni0Z6eVJhUzUMtqyzVKCQ7xqXEqJXB3uubCMQpae+PLMorGp8bpWIxyLY3EUwoUOJ4Lichty9scjJsPkCFI2nsOJAOx6bAe12ebMeNPFoI8Pizl3+zg6kxVrAkW6bShLrwodUQB8kcjW5KQJgcBa7fSWqRUeBGtBoLwA2RQTpZjBSJy/c5WNFZsgta4HRs0QUM6YiLSUsropFIVHQ/2Fu2CLv6xwS6RyHzWQtzcW+T1YWTLhViyvV3JO2X/728PbX9z98Ms/QD1m/sTEVz/YAjKEYBji/sv98zFRJB+TPKRQV+WskIAghiAvdnK1CbsK0eEOM5o7KUHRD6ELGoJ0ShLuzDk74VZMqLbAE0H0zM3J+utwulAkiJthdVqlNg9zqcxA05i6w1GaTJGs/lPDgCIItj1StrsTpgwCgyBE5AwKomLfI0LcPBtD0NNkseO8uBMyuzk3QYNyNkiUzWVfk8rWblLBUWGIi6S0HAR3QLwG1zWkVtoMtUYKsPb/lnapis9aMlGyvVL/AQAtp0MrQK81R9YQXPnSWgpoFfeKluoXytOfiCW9Lg4szqPFfAeUSrIe+1bPR2GTREFkOC3ff3VY7pZ3vz68+uGldlIrU9W8vOYN52yFItAoX/7Fq0/+9JkGwftZ/8+Hw3H56ruxZLNDwK4P+yi7TkDklMdM94KiVBRdpzFoUEQVUOA5G81grAFGBFJm6tfpeiCpTeHC2jxRDmpZtyXFjsr3S5PceBHHNDzhKFZeMVl2kAhFhqSIAhAPj5gXxAA4jKBBBKroAnaDgEiZ3SB9J8eTI3ncqDum2QXSRbojQLsb3T8bmm0Yyo0ozGfdduaV4ay1vmIehfbkisvWhNJbrlqOHZUl31xjplbf5HVIiztUSYcrawFy9WriDZ61qNx4sDJzqpht8S5nIOfyNFyi4fwVE6MBxBIySyCvrm7MPNk029VWP/zy9vBPn19/uitW740lkrPN1/ki5UzYYrtnGwnSQS+ebzvR+810s9NA6QA65+yPyWpPrKDrQtdpAELbZQb3bECdgFAAiYY63Ky8r541ySVpV31SgUFRFjjhTnekdjfY7mMqWKb+omDEU0+WHQJoiZiGTFCwGAh0AiqygUQXERWBYELcigqXhSnRCc8QMGcGFVtoygDViP3L3fYi8km5poa/lZ5nmZjRys7lZ2zJJKohrtRHRVektHK1EIjFT2qVgUhtUC+aQ5WKuQqeQhV7PzEdwRo1238AwJWtKvr0CQKBt46TlVfGWmGXhunXER6VmoP74bCcbpd08v3z2J/s8G66/GSnRDcm/OphVIaXW1wOMqgHrZ+MAohNWYs47pD1wzjfn+S0fLphTtmMVtythL7XPhZjCSosLA7ds9d+RgJBIECdCirQslFBIQxrwz6L32o5GAhzL/mDOc2RneYwag1MpJFz1uxOQBQBQjI7MrEYloQycMwMGpATdANaQTZFpVI5gyDoFDFAMkgOvSpwPBCR+12Ysk8H77eQIDkDERoRgavP993Qne3MV2tpyKTcUm8KCtZKEGtHMWpWUMNrM8NqCXQliNi40JowVsxP1t64FSU1IFjfoJTXm1p7tZi2jrCRKeKAtLkJUjMM1PkvVSoOaSehJKVnDq+W3EsUWZxGknP2Psjh/ejZo/n1330Y/+Hu9mFhUF50dtXHT/fDq1247mMXIPLiw/xF4vj1+w+/m04fxg+HeUmEhNjpdlBVSmF1GAGju9M8OyHuplj3QLIs6tCyL6WueandDfVX4KUzlk4rx85Kz6e4Odwko9qZQ7SMMEsEkB3ZvYxXEUfZlJccc8JsSKxGVopILlgy3BEFAkSF5bpDsmTTQSARfS+e6KKu2HRiybIDEQJZlhIFxc2hMuxC4y3XEFhiXuPBWPoDUFvyCxKqpuaFwzoHTtDJytl6kTmQTX/WvE49j+X4l2ZfiipLKf9MfLQUV0CK45xalniskMqsVA5XWiLRgCAq/1ZFk+uzVrK5Jr5e7q9nt5OpixOnGZcbOb052duT//Ywvj68v52XxTNMH5N/d5x/eXfoVK6H7c32usO8+Ks/fP6Xf/twOpyOOQQNFxfoNMQAuDo9W4bDmd29MeAERAVl0ULJMVSglQKsM8frGaQANNKsKry9TttxK0gWYkV2QSGRXdwB5bz4lAVgNuRyFyttCBLJMBnMIc3IuliRseX6WAXB6wOJUFQmrOu178gFYYvtXqPBya6XHrAJjBI6MMNV6HL/3Xh4O+6eDzEGsjb9NtqiRUh3ImhpHyim56tZ1ngKwKmr/IIuLEwWKj5rZJU7JKx1heKfCleKGoRaJEQdU44iBCq177X9xFEbUsprrMUmadbFxu7Vn6PpcMvfnuNq9ZPl2xfzKXtyiZfxJ692r9+Nv/wPvwkjr6JtRaKwRwnkSjBn2vfH8e2YAt6pvPv+1AUMIVxvYhSQTmNO7p7N4W6FTq21tjqO3lZ6QsACvgSKOo+kKatIuhvhpHuJd97ulruHKoBwJgfpRjFjIpfMJdOlkheFBVSChDly6RUAAhEEc4AAVhj/0sVf1sI7EBEEIKKikPlCdJFqIpBOZQjiyamhi8wLVBgiYJLKXTV++Pnd9Gg/+PPnn/3hs6LMZ4O9FQmQTcWFxnyg0k5NoVp8Q3V/heyokbNmijFNuYReAaBezmspdbYFs+VsF8l6owvWnTog6l7EknjV0SZaYmMthLPmC6xj0SEKsYp2pMCPkrKV8Fx8aHkTF6jnIs8nAUT87OvD7cHgGHr9XrCPftPJTQ8IVWum6YAIAyT2uu11G8Vc05wnlr4l8dpwUXLG0tSE0CoiAnFhaBgoFAa8FmO9WgWb4tQLuA90OsVZ+Fcxo9PNkZzukhylIp4Ns7FwYw5kRxCU5W7uSF7EEehbY1EQZMIMrpWBXAwgFBBCCZVKnIZY9OvIC4MiJVeHmdNVVGg1MKmyG5BdErDMnr46XP3B7uaLJBWmrzay+rMao5rlVbpDuJbYWxNd8YNe8lUEkhosu1x9XhY7VJ8iJQK27szGYEt9KC1uNv4Yla2vxTo0YZA0FTirJqLRs7J+3/lVK8XUKIrCblb6T1hGS063y/G9E+iCmJdBd3VRqRBBsNPakFCqEMVHBzBEGSJExIzZngT+WiZDFSg1DFk58bNstP3MZwa5/kXVQVU00pB/Ye9qZwYc4i35twZjVsS85mf1fGEVPTTSp70V12TurB2tEROrLywHt+QrxfjO+dT5sbd7XQpcZaPM7lW8uO755KVrXoD1U9b5q40YrJ6v3v5aTiyPa0W8sAah+rmP18fr4/Xx+nh9vD5eH6+P18fr4/Xx+nh9vD5eH6+P18fr4/Xx+nh9vD5e/79f/w9jZ63pVvxpwAAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9aa8tWXIdtiJ2Zp7pnju8ucaurq6u6oktUhxAUpYsUqAAAwYkgz/OX/wbDBswINiGZYAQxcE02S2R3c2uruoa3/zufIbM3DvCHyJi5yn+BOOdAl69d2+eHPaOWLFiReydwOvP68/rz+vP68/rz+vP68/rz+vP68/rz+vP68/rz+vP68/rz+vP68/rz+vP68//3z90/9vzNGdSgAkKQEEAiEAKIZACICJVYqiCSKEMgh2kUFJSUoAIAKBQAoHsN/ZFgqr9lOwQ+sZPFAryyxOgBPaLUFwSTFC1WwYUIBDVG7aTEOxGADBIYfekSmTfJYXWL/tt2j+ZSCH+1KR2SoIKoKJll1tmBUQUADOpgkAg2C2CiIiYiQhjFiEitsv71fzMqkSq/sjwMSMhJa2D549ICoUfW0fFj7CpAShOjulaPpikAiIbYoFQ/a3dhfokK8RnT3x8GBAoq0q9HUV9FlIVEMPuDaRqc0JalKFMiUhF/WoMFSWARErzm3/yzvJsxkrCxHZa9oklUeWYozq6Nq42OVAFMasqVInJ5jQe3Mc3bAJK5NNjZuZ/9SOU7as2fUTE9mUzShspVWIGwsr9AqpErD7xZnUEjhk1axBxF1A/fww7mZHELRMpgc1WSYtS7sv+1XbdtSLIY1EGE/s3mIhBIE5IzE2bKOF6O2qDOgxxk+aRdaKJ/B/gsCD1J7Hbrm7hfxIAVYDB5qE2zT4+qkRQUbHTmymo2hhDFARRvwxU3T0VClG1r9ix9iUliKjYJEFVq62JuHWrqECgJKpQlFGbgm7WkCLnwolUOU6HcSjNfN52XWuTwQRRMPssGiT5VKiDhAELMyukDqK5vpmDuk3BkMSwzSCF2DGoWhRBtdraNN9IKTFBw+gr0JHjFTEHHGACCJBPHBjsMGJwSKqqKgaUICZIIJI5THyboFAmNqtooMwks2Y+b1R1HFEEKYV9EcjMLlGTqO1YQK0UMFHiGglIQWzTT/YIAWYAESsESmRwSqQ2QagABiIIkkIMbaFCbCZGSkJqFkhQ0QZmT2ZRblAQu5yq+DjC/iZqtqsqjlwqYXPKKgQRg0ZARKhCGwQCVU2AGsaXpM2os3mrKqkEchieqaiDUsy6AhQh0eAXTAQPmoFh7s4EJvt4aAIRqdsK2JyY6mTa1wAQO8ARKIKjm5hGPAz/N7siCgRDnDVM4uAfYag62Y1Nq9+FGkIyEZP6cxGBmeypLXgS2OLCN87s9584ESDuF/7QNocOkgQpFkrE3NQBVevdqz+Mj1KMGAVIcsQKIhDABCgxhIlYlUiJmHyYFk1apoZ8uP2xYwbVoUOR/OSJ7Ab84UBQnsYtgo0HCRsgjpDEYPdkBODb3MBvH1Ivyqwe0NlHhZQzhKA++fZdMJFFhzrrfBinatiyx7Cpikhm43fwf1IfRLdLBCuy2yKw8QWNmY0/KjOBxo8BC2sGFWwx3PlgNfCgQ5hGrf5aRKtVMJSUbZIMsclPWIM5AENcm/2UfDLDguL8TMQJ8TFfdFg0c7SnM0pF1eh8tigQ/RDUwy3t62YdILYxVRAlxj+7e+c3791nNwklBkdAt/9ACq4uGuck1AF0FyJ1YDCo4XpvE/uxp4DbXmUkMkUm/xJsWjzauLVpQ47WRhlIqc5jRSkL+Own9JMqERTC7N7qaG/DYVSHjSOiQuTEiYNJeaRjBNd3uwxaBnLCYiEDygwDQQZ0otsVeCrE+D3a+IJFddiMt893/SanGa3uL+bHs7Z1sz24I/bI5mTGDdStm5Aa1hIR28CFiAgpgZhQtLomcfCIb9B1Bsnkqu75pO7qBoIW+y28E0hJCSxAcgiBEkhUfnZ1qTaqFMkQid+4jR47qxN1x1AlYkAYrBAS9pSBBG5EpJPxqT87YJmeB06qORmIACGNrMVGsWI01eyjYYdFharakGtEgRibuI49oloIcmOEsqVMk/krkR3PIAHYybcZCoGo4l/1iwMKSGTZByKgM3nmSs544tbCd/0JfYDcuR3kiVhJVG6ebB7/7fPzX1zuL/teef7W8t3fe/D+b99P7SGSBaywoRjiqcDETBCgQQKKkSNLCJgpJbMrylCFEhOb18ZIT4lxzSGJEmmgjQYiaHxLfX7d+NRR1wEWxKSCmzxqdTCnOs6+/Xki+eAAA0/JIxlhuyQc2iX4oyOPu4jaYKg7QqCs57YgARMpx++gZKlm8vQeRI3HOvHIAUQgOkj/EaMz5TcxbCBWwzL1p6lBzEcnoMJNMNxR3b6hALjihQ9VRH3VmnuEDTHFReyx/XoGAO6w1ZOIANKbzzaf/m+/nr/YvMm0S3y5k5d/f/XzV/vFevbWD86Y41m5DiCm+VMwBXljJIIKFYCZiJkJnLhJ3CSzOnFX5gBujTuN6fGMwEwxIKMewuHJcBOocI1wJ7jpkRmNTw05Whp3p0B8x4Dq2KwklZC7zYaOo5Gzw/M40xyMRoY8BUcMDxQeNdQ0BycnYKZcsjuqEpE2zMREEjNtkKAxg8o1O6wSTZW27CoKrummyVbquFpHMOBMucZQBIqzAz/JZMoUVmz5ISGezPl8hAQilqDjxt7NsUzSc51luOyf/NnX//7N1Uc/Onn2cnux6V9t9fH1+PGL/h/+w6cnD3948mARKG8R11iAzaQTEGZBSebDnFilwCQIZiIk5mAT8WzOFhTsogP5LPs4m3RitBgykZfQZczmmeqwm6iIeNTQGwOHDCTsXIh8VklZyMELqm55gRqkKIiQYtEzRM2w/6AmNsn226pdwTUW4wFEall1RRqfOogCjbsMHZiDcweKn09BqqZYh2SWJnGiDnO4l6XpVPGCAgYnU4sEz9kZa7WqMFGqVhSSBJyOh7xLB6wcnlvAVeLLT67fvtn/6b961O+Hq4vNUcfzlpetdlz+n8fbq2e744dzrvwpqCUZixBRv/tESVWgSpyMBzn2m2VXxhEMtdLS4HjOGrmGQLNHJgKLACBmqDKZEIHIT5yCVOLtAGFG6ySaDSEBsecuQIpriCopK6upVA5eFuAROtzE51TI0gIqHk/N1FlRmFjUnkw8ojq41bkHEFkd+aSysifQ7ieYvMFlRarMfaJRYUgTBthAOurULMZv3LzeSFVF1hh4I1NxuoD7+m8QDlNZH/XgqtO1q1IyWRszuX/ePLn99kkz9MNml4csY9YxFxVadXR/kZ7/8ry/yWqyKTnxBNR9wjUEgGQifAQ2hcMiZHIxjch5KojYBppASMRB/AyoyOMc+eMrWUyJsSMK0cWFI7UQS34im1d1NswEE2ds/I3ZNjShjo+s6R0eUCjuwafJL6ju0QdjCzJJy2MRkan5jvqBDRE+/cxMACfPyu17HOEoGJQDmTp5iMQysEsmugDU2hHikSJoB5P65qBPFugGGz7Ak4lY/sdMQdrsJ85b4xYnLLUvsmOIzxRHeCViblOX8MWr/m++2Hx1mbPgesDTTbnuedHhqz/7+tVXG7tQlUTcU+MiqGNHzAkgZtfhbAKJfKZdbGWLu3YLk2LMxAi50CmonUJJ3VAiIQjvA8ihwJIhg8SwnOm3Wv9uMMgBhlynVuugOUD4c/kNkwmHkWyGROfIClaf2TopEefi/HDKNPkU1WGEoiG3KSY2qkWYJIwYalPJD9hxjIFdxZBP3HycWllayhGMjPHEs3kSbWl9RMkYaB+uKaw6cPvV/FFYWRnTNz28Wh3WiBqIk67fXXc3259/dfOzJ/2cy3LWXm2GrSQmLLu0OKXFUWO5rpcZg/ISIERQGMVPDYnAbow4WbRJbWq6FIA6eUDNZw5CypRsuMpQ2QwBNrz8jYFF8A0CwR5tis+W9lTx35OAwiBhm0MNvBM2hCZWFRBMQ+RKib1WqgSIyy5ixV6vEGnERpHg2zX61t+5QOQFBQRTcP2jcXnGzIKUDhiVxW/nZTEJPmRECro3WzxYLH9186rIFHpriA57cmTwejYm+uJxNeJoZVkgVK250mHnySwUBsETAB4YvR/sDseUHrx7dPLk8lvzplW9e7K4f9Rc/pcXqw67QVLLv/PdO3ceLh0QXYeMUhaIVKGamJpEAKVa/CQkCKfUzliZlbzAnBgRsYwxRMLIWuOCQtlKwoiyLBSVZdaBVI8sZmqA400c4kNMUDGuzlAxq1IokIjE/ZSKjfAUscww1VmvdUvYDGlk3dDAJxxYs3Fsq3YpCRRESbVExZeqcStAVdEisKVnAMzN3PygCrVaYARND3PVlhh6b7F87/QsebVAA+/4m5ENB0RAJ1KlgZtuze4AHv5tVMkkD3XSEGnuQWkIEQU8gDPXuoKxDj1atXeOu6MFvXPWHXe42ecGWLd0b5mWq+7d01nTkMvQB9TSBoFAqto17BIGMydqGmqYuOHUECdOTExIias5cjJbnXh2VPmNn1HEQ7t9nbwrRszdm2rg8VmsXllD71TaCvvxSFiZMLwj4fC/iFMwBKOgfm65CDaDiTOE6QMQrUdNnnFghnGj1dsrnrkS4t/ylEijL8h5kf8RUKWET65ffX17MUj24XKG6AlERG7DQ64phcdhQkDRNwOfExfLZJyZRqIWGXBg9fRFTGMMy3MdMElaluP5k89f/uPXm245f3U57gpttuOiJZ7T/t6cGja/sS4Clw8DUFTQtA0fxgY29OHEZNpbYheWmsQVmp1RWBsAgaHw4j+qFI4YejKmAZcmfeY0JtCUMy0mDlqe7RPnDRy19l61CeMtKkXIffdQobUnhpoLiKntPjMWLA0P3boUBHWJxIYFysoC9dKfemuBaxaqRJF0KgA9APqgVv4rqgwDYa3+h6OealHZ5AK3Kq9I+ONElAhrFzdwdxEitsS88kZ4D0VIZRq1XLhUFf5jv67yOAV4BmjGQUqsDJzOF6cffvtmlItBrra67LhhvtzrRpDXM/3wTMP52IBy4pieH3cNMxMzEjM3lJhSYiZjg2oQZajWtolhwRYKFdE8lDLIuBtL1mGXdarXVDYBD1LVMR0aJpAiEGsoTuKAZ5PB8dgU/HRywFAm7bfshImptly5ebubUlw4oIhjogJlA/HCyYUd9iyS1EOsrs3M3CRKiZrETb0tm8/ADDULdfHfMxIJU6M6Uh65AkRrGc1/ZbxBve+Qqp9TQFJNYNXr8QQXJOO4CuL12s5VHQwPQ53/NmaRCMBR283fuTOerM+OhkdH86uLfid51bWjann3mE5mFOTDncORWyAQ0YapZZ/ERDGxqAq+RRwlYlVOSRomgZJSfzu+/ORqe9GDkPu8frTO+/Hut09OHiwo1bjqFCmqu0ElAgo8UqmrclL76pxuQSyOxHQJMVszTgyksJL3ObK1EUUsY2tJJKs3IeweTCRUu0SngSGTei17MAQVIlIRCun3IGMHkAAlZigzN4AAKZKsSOd8uA1TVODYOzUBughnlS8wWy6mXkWIClQwiBowUUcgQisRhLxCXLVyUy81RBIQsWooRl5eVYJnLAdG5iau1edZv9jePNltjt8+nj++pFRuZaAZpbG8Ej56a12ZRAWwGtcoEZOkllPxwnohIfE8g8PNFQoxfieJqUkYBEM/fv4XT1798nIcZLzp86jtnYu0bJ99cvX9f/PuyYOFlUQdwkKH1SmmBOwd1ENBJsBT6DtTQal6fqRbEzayEvhQf6plbmWwkojUAB4JnstZlU4pqffrWYAUC6HEpOLFH29ABUVdHhD/OxMRmmA2dFDimApIXv5wh6l+d4B5FGhHYj+yvEK9aEmRBR9WnAhRUze/gkrFZVRSVzmXWWTUYJLdIjkKmr+TN5XXUCJR+CEVub3etxf9jPjJ5f7lrs8l3Q5lRHnxy4vZo6PuKLFFMIkHJIUFQObcFyXzQZcTvMxnXTaWdKlRKJWiDXFRufxq8+ynL8fLoQw6jgLF9uI2A3zEuchH/+rtu2+tmkYpiF8kapjyUoQ8ZOSJXSOITCo8Dk5b2YdlQiEiICpOURx3wujBi3QSMjTilZKS+EmIElRAUqlLJUWmJES7jBIaTkFgbPBDKoASU/r+v3zYtFF3ifh6EEcsME0xfOJYfjhHaK/pjB/zzZ8ZKnngj3NHj1t0UFlAIKtQRzj32FIPAylT8mqDyx8Wcip98/9bWH6+ffyfnuZ/eP7Ouv3yfPf8ahwFqjhK+PXHN+nO/OTRETOxBPVgULK7gAJ5J3NGqolAHRwncwGvIGKIYj9KHvPnf/3s8uOr0pNk5Cy5oBTRjOFWb5/vRyrb62G5ns2POjg/8wBGACga+qgOsytPiNyvujoFQdVgK66YUP13DCMATx8olIqIixX/4gtQNyhv2XYACPslr2HVTmciTcYrKOzfWmwUzFSyNg7UDnbRiOFPj4rMIeu4AhRNfH5dr3pNMd2RKBKLiZW5YkKk3szpjWSHdk2wLhAzFdWwf7dnDq3bfemgmQOgadqRBPT15sl/fnL584tBx/nbq+89Wt2ZpW3WXV960WY/PP/zJ4tld/qto/myRQtQncnKKsP9oxhiDm9LZZRg2dpB6q9FcPvVDQsppGGgIYxQYmXVrHlbvvizF4/Pzs/eWJ88XFLEJ3IeKwcNTrUoYW0cMQTRShAKp5WyzQoi1CGSPQqabKzLtWzy9QAHBkZEYq3tDuxqTbIepyIQW/ZcW02IYLXOLNIkdm1TUW/IzCd9/18+5Iacu3FksRUkwqHg9oKITBS5mR/nAcWLSwFy3kgGLzhWhTy+SNOZKXIVJaLEpp9VJES9i0AW0zn9147P0W3MBM7afL29+usXT//xcsWKnI/nTIR9ln1fitLRvDnfletr2Xy92b3YjftMHbfzRCnFnZMCZZ/niRKlGq3Y1b3oTCRP6S393I5ZFM9/cUEXw3fvdQ+O0htrfvuE3zhu2qR9QT8iqe72Oj9t772zni1SwGQwTT5Q2KeHjO4pjmFzrwIphEOFjan1uSOKWKSwkjqqWUW5wbm51oUqIPKFSiAirsEOXvayrwSrgwcczdqCK2dXwBahgFBGacwITDFxpzWkqB8zYe9cJQ3HUohLMELq5Mwjmbm1L4DioAIUlKwik0XkGngr+HEdnTCv2mrvsTt6bOHJVtitKlE7SnsxtI8349f7p5/e9MO47HB3mS6ux/2CX92ORy1Ou0aZV8fLz77aXX55k6/7219ePb8/X3+wvvuDOydvr1NHIECiJYaiyYICm9mBhqxNmhQm5iqpqoz5x+8svn+voyKASNHbvryxTor9r4bCTHmvX//Diw9+98Hx6UxokoICjQGXD60q6AOjtUEtgBUWAr3hQhxGjDFpMFaA4KVXa98gkIo3L6o3TZLrR34XnlCQ2DSTuNpl1mrto564icfTikpQmEEx1NZEoUFEYarFNXvGsC9D2WiL1WBAwNTPUXlA1X88CwEfsCiLufRPEgKgllXjBx77KHwOVn+dIivCyIigqonJy26E9W0++XKbnvXDZrzd5K5Nl5u873F2t1t1OL8ZOsK8bW5GfbqRq0HPjjsRFVESjE/2r570Vz+9uPeHD976gze6WfJBcG0IJM6KAhOYoMxMZD20KAQCulXzxo8f4KfPzq/7pJpVF02joC7xqiVVFMHRnDRr1yV1VAqGHhbkwzHJECAg6iCRj0aE98JFJHsTRQesjqgSoMQgtTZuhwxvGBREmLWQOllvtWoC2NM+1BhtUu2UnSCqKO4CjhSNI6eHKFul4cSE3dw9569urAedZDESQU8okkxPjI3oeA4Ipw7GHM3urClFI7VHDaqOn84KKy2pwf2wBOqHHO3ljU+25cVeVRKIEn3r/pK03O7KBfhRi0drvs305Q5PNtJncKKjORU1MEdKIELZ5Jf/8eni/uLhj+6qVOBUgEWFg5WGwRlwe9GfbJUt8frR8vP/a3+d9O4ivdwJI68XaZX0dJESlZtem0Qf/PjB6niOaKsPm9banxYNCtWmrKxSC6WkqNk83EBcDSMm8nATC28VOKiDq8RShWqyzu+gRCTi3Mva1GyAyE3LUgMNo/awTNUbpDIpuzsFoQkYBSCRvjtF8O/qZEUeLv2XHkDioJpV21B9Q5+dDoS37fmDRpWqsvjQFSxO1oaGb8bcmlyHxmHC2/IiD093hjGiuWRJid66uyoCQHpCf3v71U6uBlJQ25KIZlEmtIk4WBApRPT61zf3vn/mQuAB2sd4eDbKtadQQ9IGKekyy70Z73ph4M4MLzbSctM29GDVnK3y22sU6PnX19evdvOjtT+Rr7fkCIg+VZj4etR41CVWH3Wz9qBqbqPxLUcpz2jYV3PaXaqGdaEWGKacMkB7Yv+mQFtjiLMGW7ceyZ9DmsS6B0QjJhqzYDcE52fTuvJ/cjlyb6txMEY/TJUj0/GSudY9EjDdicEdE1ujJ6pxOuE3fXjqe6/WRTEiQWVcEACUlBXj7SD7cb3oGuJcVIGGgCbtx8JEveL5nm9GZClKKEVB2qZkjYQUHRtZFUT9830ZlTuqQrCyUiEFJe+CjBTJiDS5WyopCa8u+jt3uotNfrhoC/TNtZwezYrK48vtyVx//63V+a783y92Tz69vvNo2S6aMIY66goFKx9k/G5oDu1OvNRZUxXXlCqL8bFTg5AIogBJ9VqvWZKYDCsGReLt2UI1DzY7EG/htUCrIfrZYkWLWFPlS0khtqKLfH3FxN7E0824y9o/FDeNwNqansRKAJBFjbAqH4Dp68Hb4l8Ka37WCP7x+PXmpmzEYbaGXMCKaBy2pgRQsysixMAoBdBZm7o2zTuedQxwzqpMCjlp0zzxYsarWTtvuWupa6hJ0UsINAnlos/7YsHHmaSjg2g0jvhzTqHLG+ghGG/7YZTzzXjZl1ywnPO8gZayH/Wo43vLJpM2XQOVkit2aSy70QiHGnb3zQmhylTUBqCO+gQK5PczjX0Ej4CFSgYdZ8SDHOhwoCN5hIC8Hwi2lL1CbIBHvW6N5ExRiGbvX3R4puox7gjqAT3+Xn/j7gDfSiDIWTxINTGqngdyJn0gU1Q6eYB15LJF1Ert0OBtLupEnLVnMDvQNORcynYsKqoKUYgoMzVMAIZRsqBL/N5J99bx7HTVzbvUtdxwYuYGBCB7Jx3RrpTdGPgSya8GQTnUqjRQN7qqUkN6Or/YFxHsR9FEN4Oe3+6v92VUurtMl0P+dFvufvvk4Xvr+bKJsrt6AwZgxOVgVAxXAqo0dpxwKkEUnhvkDRPbgnMWmuKwQgI/Dgh7zXmNwGmYIir0SPXy4FcHOEC2GYzF/+keLM9Ra8jVA7WiWhhVzgHUYE7V5g4CqoRs7OcKE+HgHM5SnVLDUdbtK7yVKufy/MvHmSKq+mhyhKxD5zO8GfX8dtgP+Xafi+i85WWXmsRFdNvnm/3YDyVxOpvzvVY7VRFrFlVRFYWq9mPxLqSieesLgt3fKymPKQyHmsa6shs6W2jizYDLWzx9NWz6UkCDIgsGob/5ert76/j7f/jGg3eP62JWgJyaOj2yR2LvtrIsiDj6r4NGmV9+4y+Wt0RJyE2LAkq0TlY1tUrPbNugONRr0WpLXyBilhfG5ykBLCNxWmXD43I/7GoCRQNjbRqxPQQNX2gfLaHBi6SOJ7m9KZP1L1XQBKxyS6EGIRhM8D4F4Lsl1cIvapoNVeLmGyFA2WETMQtuut4abzFfi15thkTUJlovWyLNRftR+rEMOY+5dC0vWp6xMpUjyJWQl4dFBSyqIqShyA3bbGjGpJH2ESzpi4wddNAl7k8qEOLTVrt096h50DXrJXbQXdbLXra5EDfycPWjP37n4bdOUkvVNX3KzEWrBuZ8CNZzXe0mlpCzo5jRfq2WDiJ4HAxmFtVL+ifCHKBeCPBJmNw+TqWq4jVSxNpz1QrrhuS2aVX9qCdo3rDWQO26XmDh6fxBEMKPKyJbgdT2ziJices4FHr8EbniU6w+qLdRw6QLHeobFdGU2anH0LrNT5S9zMWjjufxhhSapRQ8Pt/cW8+Ol60U3Q45ZxHRIsrMD9bp/LbcDpnzOIN2aHuoKIqoSIYrwKqgRCjbUZWgol67JyKoHMCEi8nElo4Qzcby7kXfXg7Pv7j67GaksRwvuKF03UuRcrMvDfGi0e88XDWnM48ELIBHQi1KiWoQoCmykNmBzZIZokI9efQk1Ig4YJv7cJT7/cdB7nTi1jaCBj2COLUg7LJCwoSgEvAFghYQVCK+TYEYJm6TRnoAoBG3w4q1boXxE401/A6+Gr0cYVfec8vB3zz5rszfWj6dJ1QwZK26ZHWboB/AlGeJrWg8jE8VdG0ilKIGqqOAWZ882x4vOlEdRs2jjEVzQZf4RvKzy7HP2MzSSpGgRyn3hVUZQBZV0aLGrAVIeVd8AyfzFKMSroCKtadDhYRmRRa9HF/s9JNLfbzpd2Ppczfoy91IkG7PRQqUZonnDYax6Ivt2f/x6/Hh0e27x3j3CIuGbeGk98WYhdR8zCBEbOmyP374phEiI06Biwd61IFYC/PY6uM2olLnRSOBdJlWvHHfOWBNOj1CijJBhGBQOwkTbvM6oTFU0bjVxTrkenMGFAcin0b3ExDkQZkI3owULkM27wekimLfBkSE8zuPsTA9weyfmUGm00RtVF3mNUnX2XhIx1FvVwC0l5KYLzb9WDQx7YdCTGNfmDEWgeLZVV50fN7zrFGorBgXmbPXXmiEJuaGWSAKlE1WsSAR+dzEfAkQKTQ+33S/vqZXu/F23Ge8uN6+uM1a5L0Hy996Y/nTl7jZDWMRTrTqaD1jETlezdbLRrbj1c/PL/7Ly9X9Bb+5at88kkdLOptTRxLcKLybnWGLLTTwEqFNS+RglVnXifBaeNBmRJ0JqCDhpuZB1Sc29kILF3aUZO/uVlclvBIArs2YHk418G+izwptfIqcPwbQkaqQ9Z3VHHqCbA/eDm/M5uUcqYShskSfpxKSX8VnyLAhUNOO8jXpEY6iZXuKoJX6hygIRVRjFQBGybvSMEHTZp9VqW24H/GatP8AACAASURBVPNYJCUiSolzP2Si5mbUE+akpQEWpH1cQEQsgiTmXFRux5JrQQUaYrI9uGRc/+RZ/qunqz7bOpQ9o2N+ez2Thi93+cFR8y/eP/v8YrPZ9YuGusSJcLHHuw+O1qLPX+0045RYX+zLs+34dy/5pMvfWtNv3m3eOlYSxBJlCfoipFZbdAc12LAIFC47hVAKDwlb8q6aSkCc2hwgH0Glcjw1BoggyB56DI5E6/aYGtc3Xm3oyiwR96AkJLBWjSgtwesaJL6fAgI6aTKCKcdTiTWE0Mrha9idfmyNK+wUEEGpYGv8LZO3vSA8v9DYycb4vlY51mHZFpsSfIdGs4GbcX8zWOjf7HPbMjOut+V41T2/3C1n6csX/TCMgOyWzQA6abDPWFLeCPdIojKMRYlFtEkEQrkZZYyFsoHAVdPbPr65/c+Pl/sxdWlBlLrUF+kJRYXHUope7vJM9N3jxVOULGVUzYIHdxb35g1dDY+O5+tRKaMvQtBStOyGq5++oK+u9b99mz46U/bdcShUtQiIMc4eOMkzZocodYFVgx2pCqYtam2zTzilCkvx2Cpxkdq84ZeTMMnK7SYAgOXrVm63q4qoLdAxDyGBNN7QJrEggsHFIvNUMEPUsOCFR4rFMR6U1Qo0BDusyhOR6h7kEmYnEUL9MBtR3wxXnZ9pNLUd7MA8tZOETo1wjOHFfns75KK5yHLezLt0fj2ul93V7XC86l5c7s+vhqFA+rIf5SKnsyVTllWDoR9eaTco7cY8axtAmZAYeTOWQdJEdHzmVBUFu19c3BU5WrUJKA1lUSTiIg9XsxEqoHEQETkaVRbzp7tdodSS3lvP+l1uGtrsyj5LlxjQdWqGFm1Ji06wL9u/eHKz6vDOUdSDKZi1jfWU2Tr22+ok5222bazHVgShFKOU0Mrf7GFEJew2aIwDH8NqnAKx8lLIDt5dZMgqIZN4f4japaMu5pZPgG2PWvuSYjg10mmX9CKXrdHeDSRoYnBPqpYFl/msQuJcliONcm1R6814NI2PFbgo7lKj/6OqLPUm3CmzXj2+vdnkLFIEt/tx3+dZmxKDmNpEnz65vtrkcSzjKMM43o6yF4KWWdLTLp+modUy5rIfym7Q7SAg0r7oUDDtO0g+WaLlejj66nrd0XrWnC3bNaesOs960jZdy2zNWw2UOBOvu3aReIE8b1Laod+Xq9uSFbYqNDV0JeV2l2+H3HU8dqncjOnPv6aLwar4ttEwKalQtQdnKAZAXpjx9AwK1z5BKhZFgsAZRarQ6OXbWsKZNCefQ4k455Exqube9CAaMWZSDxwOJ9XAKHkT+kD80M9qvRqhswC267HLOyqBJxzLFuoCOlEkJ6hUb1E88T/IGie6CCXb5tfKnbaVlo+Au0rlxL6ulKLm7z6tZTfePNn0+7FtEzPmLSnAjLHXruVffnm13Y9FZBRBg11f5p083eiRykKk5XTWgknHZbotqUk85NxwS6OUvTTdAV0wkSBL/6vzk46Pj4/mDctunO3LsVBRKQ293I1jUSERVVXsKXfSHM9nvY4zTWshbliKgHTeNVxQKPWsV4OMSv0oLdODO3MQb/7q6eXvPhjO5gH8AmKIkw7DIaPROMwJAgUi7w/oE9TtDeIoixvkWyyCuLZzuNXa+pP64FQv4+sorCpv+FeTDK/2BmPyiKMNVR7tzeDEvqG7h2PYltDGzg7sRwFnb/FYbshUakOZqu9gW5lmGJaZ0VRjdwao1ZYmR4r7NhlJYdmJ+5F7bjfinfns4iQ/u9y3zPdPFo/uLvpeXl5d/erJ9ZfPriHaNdjvecx6u8spMWkaqJlTWabctc06yQdnvJHmQnk/ps1+nEmze7qZH5+qy8TQIttn21dfXPc/ffJ8zG+umzeO5ydns9R3u2ebWxUohiItI6VUijBRS7oZS8dIbWoG0g7aw1b/UMNtQsolJdqMsoMsV+2du8tCennb33x5O7Dgv3kLi9byYQtew75cPd9ePtlur4dmnt7+wb3VaXcgFNRkPMwHILDtaGqmEGmET6fxd9J4ZYBOoZqVVG3PbQ/E4geQmxtI1SV5AROyKy+xcZKTDUXjebDbsAV4xCo2J+2e7ZmYFphLcLkl0oIwDsTSo6jJTXqNpxQctm6sy5bWxsrIcE+1bc7E9HkDMwvl3qbvHcCWv3R0etwNm4zLoQis1vTscvfZs8351T4XiCARmgb9qDdbGcu+H5td18yZj1s+U0lJZ8xdM17viZXatlHV7Ze3J99ZQ5MoFHj58UX39+cXj2+fXu73o/zs+f6D0+E33pg/Ol3rssGQF4TlrGFARTFrSISUF3NIwkXJW8F+m4uYMI9ByqzhBBIgNYRMy+PZ5b7fbvb7vtwO4+VP9qt31quP7lKk2lePt0/+8vHVL84vLobdvuxH2f9p+fEfv8vVQkzTstRBq1VFBuE7yIu6MFENwSaXRMUL+mTU3lPa6S0DsJ6ceI2FTqJr2Hct+kwpg4IaNwR3BSGytZwa1Mkzx8N2Tb/6gelJjWtexjwINQSOFX1wahH9Lhp2FZkAbKNjWCZrj+XwT1AVtg0cES2kqMyjpbRoTHkr0DZxP5TbXX54Np936eWif/zqtt9IYm0b6kctqsOYL2lMidYLfm9Npx2KliZxR9JzYqColhLEmVQKffzL86/++vFiRkUgKtI1X+1p9+Xud0SPmtlxSqKlTa0t16UESgmi3HDLJJs8Q8qldMyzFkNRVsmq20wl57EozdPFph+HQbQQaSJQLs//8vGDO/PVvaWq3nyxufqPX/720ezj9Wx3k2/KmAU6iopqAkGZqAi54jppsxphzjbzr3zZ2butaq4m4HxevQNSPcGoSpRg6rkBLGyzp7huWgf25ZkypJmoJQLVLAOMNF7ZlTFbf+Encaii4JHRZhLxTqtKZkd4/loNiyJYVpAnPrBO4/7sKBaadOUVFKVisuRVFufjxcv941eb86th1+t83gxjWXS86OaLLs1mzVj0ad5sdiUxulaHkaSgYdJRt/tyul7pflh3Sll23tukKsCqoTTx5tm8LblsC0AAY9nR2aq72A6/ftl/cJxmDXJWkpwYRJC+cMOqpP2YmFPBWUM9N4mAous2tQ3vh7xtaUC66YfrTcmbcd6mLtnOe5q46Ofnz//n8fhfv7d+a/XFn331YF/OHraquLzJ+xHtmh6+f0JMVjYxkBEXCjTKU85NXFiA2P6hoYyEnAvYdyzvsOXmntrZC0kOJH+p4ZCC+JNG9dNbywKHPCCm7/3h/dTYCs+w08leA5o8hMb/wmpqtzfq75w0uin6fdV/eeOUVQXxzb/XHV0pMYGUaAJBqqJaZLWRHflWRXeeDunFfrOXq+1QVH/3u3cS05AVkMS8H2UcS9c1bUNFCpM2iYcspbhgc7Mf98LDmPuiA7dKmguU9OTHd4/uLeaJfA1p4q9/9gJDMY4wFmHC5XZYqDxo02Ys133ZldKkxCBRaVNiRhYQsO66eUtKlFpKiVezZIu/ZLQ9HOj55e5yO6YktnZ1P9JtXxqiZT9un223bfurv3i82/SbPv/0s6vLjVCDD//kW9/+5w84Ua3ZicdAZ+fhnCEHaJWvwuNxgE0H9Mh9K3rqw1IxiUmBNUFxCKooSExS6rx6CCujpo/+8H7TpCgYUkxhiGWRsUzfoqqhhWRmC1wpakuYauEcLyiLk/kCE/L8czI9X5UX9j61cMRwRICM5mhr1TKdHLS6zcvrvNmPr64HJvzGe2ci2A+ZGUOWxy82u2FsE68WfLRol/PmaMHrRRoF+14AFMHqqCup/eK8rFctMfW5nPzzBw9/92FKWDDbcqfFql0VbS+2UordThlzS5QSrRNGJRVpEs6WsxnTrOFlk1qllDBPPGopoF50EGGmLJoBER1UimqrkCZ99nJX/OmwL7rZ6/GCl22Szfjis1vMu/7e/PG+6Ons7IPTj/7NO9/5vUfdIsVkg/xNZ2EEbitTFqqTJBSGBEwZKAClyAac7Ufi7+tVPPGtvNvOLOzkomhiiFjxkYN2UcnaQB10DYk0auYUll1RyftITFPARK/cEw4zhnrbwa0ODpsS1PhhNMAgQmkAr/NK+8P+aVlMSDGqYuu6qKVZQ+NYStGjRTNrU5uwXja7fb7d7/pBxgKV3DaUEi+Jsuq80/VidrUbn73a7Xt9edV/6431ux8dnby13A7l3lvLt37vUXvU6O0ID6JEwA+PuPno5PMXm5c3Y87y8GQ29HKxkV9fj2dzvLVqULTLOuuSQDsmBVrwWLQXbMci0fIMppJzFmSRpGCm47ZZ/tYb8+/fvfrJ0/2T65Soa6htmusRlwPGvi+n8x/8yXvH9+ZKlBpOrZds1Pis7RIV+zBQLYmbVVmcM6KitWbNU6XJMi2NuroGCQ/2FFUHeBU8ZBRVwPMHhUKjFxFVwRUC0NiPYuWATqZWrwea3vLnViCuXESGYd8kqks6EYvF7Urs2EcK8YXsWgVr67WEPzpqyo1o1YVlTi53uJlObqoKjNCHzXA3jR3Jo7OjWYt5xwQaRmHQatkOtzIWGbMmFn/phBI3+uB4Nu/ok692/V6eaf7D/+Gj9RsrMIg5NfA+U9fbdXc7PP/0evvy9quX/XYo95d8vc335rN37qXrfX6+yx+/2r9zumhnDZKvKCoR7WdClGzRNnXMmzFL1qw6im6zMmFUzLv58Ucnq28dnf/k+c1fPZ433YB0d4U7i/LiRh+/2n7yN09+6797v10k8lnzCYitTQAINJIoLTYlgWIeN2PlptuNpw2iU21AbMSNyblO7OFU1DqIKjoqbLeGonUpp68vML3OdpXU9OEf3E9N7AFk0dJJUMxnAA6qAKaINrWgS56FmMZwuImYMnz330Pq5oxrCq1WVPEdOz1uhvTs6RCiJbdmDnaPCoCOtsNH17dPXt5uWu7ePz7KNE+8z/rquicCM13d9kUhKqpCbJhebNFl4mY/jqWoCN74vQfrB0tmphQzNJSOkz3+fpv/4s++/PLxbtHovVWzHaRkWbbNnSblUtaLZjlrvujL6Yy3/dBnLaR9ke1Y+iwdYUm0aHiemEVniTsCA521xHAqqrfrrv3OWbNIizeP8tFi++nl20eYt0mBJhGBzr+4xqPVyb0lfAlzcCVfxauqBkkqE0QdQlpUM9UlIpVa8akqLMV5PIS4WfmBigpzWgUBMaulYrZWgod7BldKSR/9/n1qnGl5c4aHsGjlqfKG06ngckHnSCca571TTrNqcjDps27QiLyCnGxGdYcIvl/LZMXTLdQMSA/PD8XRdrz/Yvvp813/nXsn37+7/+zW+luYqG1Tw9Rn6cdcBEVVovjnqauSQscsZ8t28cby7J11pFGAqGaZw25UVPH808u7Q/6td07evzNrUE5TGvbl3nquRMLMzF9t+t2Yj7qmATFTYi6ldF2zy2XZJeoaAqjxBUAJlAizxJe7fDmU/ffOZm+ujB7cfH07Ms8bkm2fCx6uZ2+fzN5Ypnw9pG+dUJcqUZm08hDMgrkfxFUPTVaqMkuK76lCSTTq6VFOV5k4nq8VjTKm/TACZ4j2CutvNmkjuD5UIUWbA5s03df7J6y8RDwRK8OPYGyBLHD51IKkGpxpyC6IypNalcIXulZeF9IGtLYhEEEgsalUXdrvdqpaO6Fc44MSIWW9vOqHovNHqwevxrSaSZHtPs9aEqH9IGMuRNwmdE0as1jgt/bDpqHTo261aJvE+cvb0heeJwIkSvoCZRUFtW1684M776N8+MZyN+b57Hi/K9c34yaXEdI1bQLdnTUv9/nHd9JilmYpcSmrZdcqfzb0rxLzWLqGSbWoNkSUkECiNJul81nqvr128Mjy8vPrk28fy5vrq797qp9d3hHtGhwvmrTtr7640g/vELPXepyRO1uqZuANi/DlkpVyqOrUdGFlAEuqnG9RGGqxaTCrZKjU1WzqAoZZmEm6FBNkU+RWCBtINA6m1ljtAFvbuhVVUq1pqLB126kvzosXL3sRgawt7huFI7EFwyZFc3KNHwLfrMHB3RpKRSW2FDU3oTBjo4Bu/dZTQGK7qDa3w+dPdntO7VF78nQcE+2FRGTMuNmNX7y43exGg7GGE7UQUTBkTKIoUphS10AJ47Ndfz3MZ/PobPaXoda3QH/4o3v/YqUraCny7Hx309JZhydX2qbuxXY8H7tBU9Nox2mWUsPUJCZuWPXBqnvV55ZIlLJkEJUCZoWSAL3og+Nu1yaxGs6uHO3k9qvbNG+WP7jXfHDGP3/ZbPbtmE8T9G+f9Ptx+PCeLlKVycjbDwUumXI4MADR4nAi4otGLHMPQzCeG68jtiAY+Rb8J4ZGCgSjcHOdNoCzAiXEu9Aj6YWqNlPiEA2yU+ZXw3ngitjti/dSeFYY6W1UHbxiy9GUR1Yfj8wgbspBUqJrADCe54Vdt2lSzy/IpiCYqYbOQ1gM0j65HW2HoaGMOxmLiMh+EGK92o7bfRYhgbScQJqYmUHQNEMeCyffNSIr6U425313d+Y5iZWIJLBacTTjoxlvz3eX2+HqZhiLdImP5vqTp9tf3Y5KvaKcrbq/vtrLCz1bpHeOmgdLyqopJZKxMJ/vxuebYZd1L8U6LOYNzxtOWfRyyILzz6/HJ1tc7F/8YnP+dy9klt768f37m/F+g1khJb0jMv7s2Tnz9of3Hf8ig5OIe+bGERi9RSwYnGdn1h5rlfAqvNUORini2w9aOV0I9l4BwxEP01Kpml0s+YvLVKcGVAK0UeeAcNDyzNOKQ5NM4ezR640OV95YESHbdWGpYZFcavauRKodBrU2QUGFnGpSeInfkXXs1egb75SfJEgFSMZyWkqzaJ5c5atPbs57mrc8ZB2KLFLDnEWKWEu4P42xVGFQ10Y6rcoEKXT7+Pbk28ecgt8EVtiYXSr98nLkyz2AUWRQgvJqlr68vb3pZdbqsqNdX74gbYmebuTvz4c/eDg/6XCR8cvz7XWWzSi5UKPy3rJ85wgd4zbjf3/MqeHjv3muY9ltyzzLcL2dd9w1XLJ89edPvtb837+/OpslifcC0N7CfiVolajFmo2YurpEyWjmZGrep1rUUECcyZHbEkTAREWC3QRDdh4YXUMBgX5yF508mtuhlL77e/e5IZp2Ko4UxqhPWBqhioH+ZLGx4MTL8c0SOiYhl6ayQlQYotMfbl7+Qz/Cq+NTUmv1gOAUNWsFAbg35kfPtp98vX2e8en5bnPet01ipuvNeLRoL276q80AUGL+JzUsD+1WkohtcPb78eS7p6nzTTM4SwfU5bdj0f/3b1+cjv2ibXPRTa8X23y+Hb/aSgF1DeWiLUEEreIR0VUpO6XjVXpeyvPdMBYF8TLpeyv6zlH5/ikS4f0j3Az4fKNXX22k6+59ePLy+ebp9bi5Gq63edvLsC+U+Hafd2MZijBzUbr46D5OZj4MUSkPsn2wzSmYKgMzNVI8BwscpMAwqC21t38Kufzq/oaALcN4tyaDfFGQgNzUIu+LBFCKpA9+9y43aSol1cwwOPwBb8fUHxGFDoOpWP+jNaWcDvFxsN5cjVUnmC44WYzDYOyogriZejL1bbxQT4xZ1vc/v3r88/PPL/bDyeLifOBCN73s+0LMzHj8cjuMpsQYZan71tXpCZGFiBT9Zlh+cDxbd57lZ+0I/roRAhHlVXe5nF+82L14ufv11fj5zfhqR2dd02R5cpnfn6UP7y7embf3Gh6K9KN+ucmP7nZnR835Jo9WmCfqC24yf3GLx1t8fM2/uqVeiEB5lGbdfeeP3n77nz3oHi03qm/96N5Hby7fXze3946eXuw/vi6fKz3OtF0vRKVdtLXYC9QtmmzYSKAkEIoQEXwNESUJKlJlcPzTA0I3NzQQjUKAZ3gaaojXnmyJoBadcjiCAiVr48KdO7NbjGW6sZewU3ZPGsX2LVJmXwujvmxWDhcCOBIpgSHiW6CJIJoTSUhsg0rb1E9ip1/TqxHtSxJbc3qPhuetLouw6NvPt1c/e/nkctAHq9uj2aNr+fCtdRF8/GRzcTNcb5ttX4htO0aNeosV+cBMJcrGEeLRKDbn/fGbR6FFQcUZovXH3H24ON8OHzfdNvc04IjSEeWjru204UTLRNtd3hPNx8INXe0LN0qMN05nX57v970qo4hcZ7ockCXZLI4iBCaSsi/NPC2OZ01L6/uzb/3wbmoSSukv+zdPFv12BJRnLELby/3Lz25nx7PZsjFRo66EktoZ69MZrzF09aJCE0lIat4veSBtWCQ1GxZfRezL8Cw+xroslYjLE/WBZ5CxZkAbI0SePMZagrg4gevrV6cCrEOU5X1mE6q+hEUPxAgXavz5iQSxMosr8w+b8fQiwmmsDhPPdNjfzUIELb7nn6o+2I3Ln7/a9CWtGv3Rvet/vDpTPH61u7OePTqdffJ0s7/ui+qMWRtM6rHfnr3uUsX6+cwhBS1z3owiSiCBsG+26XukqUrJcn013Pvh3S8ud599ebPfASpKI6sQ08kiLZvxnfX8znr+1izlsp89au+um/sn7Xv3ly+uLkcBiBJlBVq2iEyJODPGzKo4/9l5WvCjH96ZL9t2ngBF4vmDJanOu85dljBft2dvr0BsMSvqdT7b3tBvjYr+Qg2o1OIl+3qB2IlWq7mYN9adINQd0Hm8KhHKlHr4AmPrKUeYqutaBnMKKNL7v303Nd6RjRogqzlFkYiiQ8xDjoZEawlEBesgV1FLr5XxGhzrSk4K6ceDY7yyYSqix+HuO4eIbbb37ssdfXZzvGpuHh3dfOv02d89P1LumjSWMmvSfJb6sczaVESZauigGE5V2/LT17qQCBTKzPMP1ssHC1eTMjoLGxrpE9PR/eWLx7e/+KsnuXc8VBCRFtBukMutfno+XObhbJnO7s4/fHf18HR2/2T+4HTxXz+/FgEzmNA0mLXN6fFiOW+W845Zczb1iW8/v3n5bDs7mc1XrbNp2/fKZym8N0QNz+VUxasBZjbOyz3WictJ9l1YUdT6GRWq4qmOHegymxN5Ryi7lkR26Qf4kR6VNPyyVqZFc9HGVQJh3zSNqxQH8hVSaq/8id5tszqNjDditKFRiCG+Ap1I/QzG+cTQ2xVhZhIIiTWaCQgsVKytAzDoqltWeebtaAkgibbbvDprx12RN1ZDFmykWTWJaTFrctHVLN0/mS+69unFdjtkFttsFeSvQ0UE45qTEKC8Sot7C7u0qia1TkHf4NMWbW+vh0//6kkalJi5lQISURD7IltWUvzXr2Ux2/7p907ee7h8886sz/Sjh6v/5S+fFOkBfvTGSWJ+dGex6NqjRcOMr1/u/vzvn1xshgJF0+4+vv7J49v3/+idtz4845ZiZQBCNfIkj7zwrZVukoqoxi7xttNYia12Im0Ou9TJSCMTUNRT1sKuu3yx01ut3L3W5E1VqNquqfZqymiU9FKpNrbtlahygTKo+NvVOGKXmBZsYOyFq9gpwSQKj0LRxujQY5MnsF1PpnQxRoSIxRm+hUJV8f3J/bnio2EPAMWWgkSYD2WTy2o1G7qya9Pt820apU3cJEpMBNqPeb1oCWBCKb4js9EWi/lMwTuMuKKIguZNu2h9oYdhRNyU5WF5zJ//9MX+2d5uTEYeS5GMUaRJlBolJWZazuXbbx/90Y/vv3G6WN5bbM/3y9P5uw8W1728fW/1O9+7v+/Lfijbfe572Y2FtDw4nZci16ABRCkt5vN/+F9/ffUHu+/89r35auZWVKTGDvOACDIx697tOPF5CcMJJI/AgLBWgypxN66r8H2oDBeN44uqFQa0uCaqnnAgEC/0B1OhnMqlt98/0gIMufSS96Xscu5LGhWjZhEuohmSRUUhgChEaad6M9Kooyh7okiwXLeu0PMA7s9P2fOsieG5OOE25Yup6q9gq8NJRSH2YApbQySO3iiSGt4NRU7nzxfd159et6/6s6N2MWuY6GY7nt8MTeIicrUdcy4gSvHCL2uicxUZAtssyGjqqll+eErJdtlFKpo0JAJVVbz68ubX/+mr0mdVLUVGoVx0P2o/YMig2OeWGcsZvvPG0fd//y28e9K2zf759vnV8OR80zCubna77S73A+s49P3Y9/t9r1JANBTsSlHS4zvrzYvNxafXlzf98f1Ft0yRD9r7SSJeO6WyHRZtwNTH1UmXONvGFPUs8BlkyJTxSCAdHIjEDNUhSxwLpV6xJhYimgDvNQIRopSiKlma/PHNg/vLh6ezrk0vLrcvrob7Zwto2eUyb/h01WyGUYgLIKBRlAitUtmWLGVYMO50s1kjiamBErVdOprPdpIZUhIKEwOpKEbRljFnF12gIJbpzXpIpsgmEgYSE7OQMkm8o0CVgCIYFXOmJhFx3+EC9HzetMCeafdq92jeFJGrTb/Zlavt0Ca+In5w1q3mqUgZRqVEjb+50DnxQW+Tq0aaixRJmkLPtM2qnAWPu/Hrn77AgFlLSJwbToPs1AYY2wH9CGKXuj973v9P/+dnBPq3/+67WLafPdv0Y1l2/GDdPjiZ3Vl3x/ME6JB125fL2/5xO9z2mxmrZmlaLle7jqlpePOzy5/38oM/eXd12oWK6VRcTajXimgi8T5g+AskEN1aEBFTPyWMVao5aPRlhFobwqztvcEiJfR0aw2igloo4KJCigI06mZqeaYoQbQUbd65c/TodHnnuBuHQVbdyeLo7sn8ZrO7uN533OSbUgZpEkGlUaYi81matXRT0Aq1G8xFmAYFwEjM3SytVpz6fjfklOyVz1ilVLLkpDJPiaiIJFBOWC7buXImWTepv8ml4TJTaVJiaZU2rJ0igYjRdLwTwSCaVe90NAdDhGlLVBLtFWU35pt+s5eXlxsR7Pu8GaRhbttdX1Yiuh+LCIkKE6cErkJ6SEJqcCtaepFtRsMgiCBngaCAVDWJPv/V5e6r2zYBmhRS7EVQCTJiNkPTYDtgLJi1CqJNjy9eBdQ66AAAIABJREFUDP/jf/jVz768/OPfePAPX17/9ceXyt1GZ892qTSpNN2do/bddXOzL7un2zYPN1+PUvYsQoVvt1tbIQmlq49vPjl6+r1//VbTNWAIxN75UJmAp4JG4zWSKI8PBCkgCuYVHB/+JakwVQsGgKqKKAcuuhyrnhLBS4Fu3IZnHKKrihS4VlKK5CzNrEuc0vlteXG+aZkoST8OicCJs2AQJeYs/qL409Wsbfl2MxyvutP17Oqm99Wl0LZpUiIUwm6cg0hJBtiqIVDumJL+f+2d26vlW3bXv2OMOX+Xtda+1K46VXVO9bl1291Jd2w7iYkkJMH4IKgRA4n4YFARXyQSIkm8gHlKUBBBDSj4EpBAXhQl4oPEkGAjwdww3elO0p1055zT51LnVO37Wut3mePiw/ytOv03SE2oh9rsvddev/X7zTku3+9nhF7PXSPzbMzUEIlo3zddIyIxXo5tlr5vx1Jud2MQC5CTANHklNg3mUf1m0nXl9qtUkQohyVBx+qgXTl23pcpUdTokglFbTfqV9+bJsPZMf+5Tz/447eedsJHq6ZrhJd84hC7UBXnUozWvLFfHbuyay+9Io12wVEYDylvv3KDKoBHeMDdNUg4+oYmjWBihAZygCiON3J6Jz++mX/tCx985e3rts3q8sr9Vd9wm2U7xa7Mdx6cPpk1iq77/BD0vZ+697kvPj7fmxWFO6dgBUe405Pfu7jz8ubhx08DxIxSy2NunRJxjAlVxuDhh3LFIZg+5KjxrHDmRAiJaIgtwBEKOGwxmD/TbriHghHhRIC5w+EN1Q30UGVbKp1mERTOhyc2ggBmrFIKjcQCC5tL3Dtbu7s75UyJ2SLgTtzMasxUCV2SRATrPo2jatjmKCMiJRGhk1Xzj/7t30H+MQC/9fM/+D9/601Xa7PsZ9vt5yUgcu/bPBdTi65htxiLjrM2TWrbxCxmnoj6VhLxZOEeBJhqbiSllExPmkaMm5HGqfhsxGhaaRwAPvvR+2+/e3FzeTvOPsDVTB0W2PToDd/0+smnP3rnnSfXX/rqftNOxxvadNI1nLgONScA6/XqeNMG4YE3x3M6v9o7l8zp6nqfJe6s+yfnF7dPb+vBo+7qUdxrNk45mLErEYz9DAdWGXc3dOesIejNXrvrabXStu3bxEl4OxnBv/WTL3z3T/w9YPtff+o/jGNZd3K6TonR9enyZqzpipCLIHOY48mXnj486bsk68xTBDv2Q7nPmVt+k0qUyEJgigSEtywEco3jttHwoNipGWBqKDiGHBG/erI+344ELk28MZlxJOIMnt2mydaG5FyK6WA6ezCQ2DYcjLGenkSZsDLpjZ/4tC/KEKJgp0z8+unqJ3/g2+7+hb/0G7/4S2ndpyZTZnJyIu7aVPthAriRCHUNe1CTUlHtG0mZCbgFUuI2c5KlgvHnv+31epMB+I6/+9Nf+uN/MMzaN0ndZ+3cHUzu6Bs2i+1Y1k1OmdXRChUzIFZNKmbq2HTHWmJfdCg+TtpkTkncIrWpSTIX8/CEhpMH/HjVFA0zbxva71bTdq8K5m/MOPDoUf/t3/KwW+dPvn7vy2++NRXs9jFOyoQsS9gegT/76N7rj46aLCkLAaUoMaTj43WjEadtemeY3dSDLFzdzZcyRh1e4Y6W8Yk7uNejF0CwXfGLDb30oP/i2zuSEEKS6BohimEqAH7zi+998OP/cjvq196/PembV+6vZ43dNK1W/QdXexiE42+8gs/cxe2Mmwmfu7iVPxlPj9t1l5o2n2z60pS7q3w1zNN1sdFXXZOaFOx9k45bKRq7yT/90oNhmLfjfDGPXd++/fhyvxtXIvfPuvuSGzEL3N2s29ur92/GdZ+O+/Z2P9ukd49XTU4fPN07N1tMm64d5lJu+HaaSed1l9yjTXmTU3jwLJdb1TJFhBB95vWzf/IzP4zNDwDDRtYpZwlH0QKGR6DErLbpc07J6+kXHk4S0aYsCYkl4F3Lm76tBTIm75v2O//mdwG/A3w7AODbv/Ob7n317atR0WbOgqKuTm2ivpVX7q3urPNX3tud306zAxF92xW3Bg6iD0Z1WELuEUTIko+6pB7mMWo4CMLkODnivknDZOuO96MJwxxS590zMtOqY997OHKD7/vWj7x0b0WEl186un8ml5fWJLRp4USYL1r+R/dXD+72606GEuo4u7fJjC4v069mtauboWg4vIq8zVAnYBCgBg189FR+5FO2dvQtBsP/eJz3oybh03XHrkLoUn542l7sysm6+cSLZ1e3N3fXzWsPXvijd7bjrLPauksMmsahbyRz9IkLNJ/gBHT5JE4Eu+24urey4qNrxrhq5XYo47682OSSkkgzmu2209mdnIwaSSHKGtc303Y/qOo0ke/nTBKgq5u5bbZX21LI97Nvr+bptvhu9lXZj/Nxl26GYbqN29vS5mYs1YfI066I+50kn3h09+Z2enyx63saZz9uGm8tMiPiY49Of+Lf/TrQAj8PvPDpj54lNe+7lKQxs6KehSzII9pMCAHx7BpOTCSZVXXVkmkcdbltuMvZXbs2v3B6iiZ97b/83K9/efiRf/qzwCc+9bf+xdl//mfzZMX1tG/vvnyCvoEQmPHqEbJ81+cfn79x8caTfdNyarEd/f2npWvlxV7euShlwipLGeZirolSluOWZ7N59rPTfDtacSTxSCaOLkEIHj6PEwEU3uZ0cVuKIYBvfv3sI/fXUSwQmfDCnf7qfBuHWTu15KxATvCI2/2829N2Uo32ZuoBu39CTfI+O9ymYmqmHu5kAbdDcAeow7SO6Vvd+P6bXj4Zivfn+s4QV9upTejI3LjJ9Gdev/Pu5fTu5fDB9e7p9djk5nNf/Mr1dphUTm+z9k0gqJR2GbvualDDSRNmcMXpcfvNr5/u9mU7KYGaJubiq543qzzMXjRa4k3fm+ukCMzF/UtvvnN5M61WmSWVeexantWTUOrT091sDiR+ejNZxNFazGN0O9qsDDaVAufj4zYFvXC86fp0udtRlwDvWy7zdDtNqaEC82TjPLUrEpaOZLMW4Bw4+7mf+sX9sD9e9WnWKOZZyEAiTCxwm+cyMOXEqqiYCxHzokIkbm1DjVASPl5xl9t13/3GG/HbP/G/Hj+9+NhL7X/86R/92z/zs0B6+EOfwO2MwcCMsx6SMBZ0GQAub3GS7760aSU2j46x16+8eX52PyUhB+74nO8JBT29xXZUC0qMrgkmKW0whUmU8DL7CmFqYuEE1xgHNXciXA/zXEABFnzilTMrvh+LB4L4wd31H391a34o3B0KksR0vVcnFsLtTodoNDhJvF20EdvkGVGS8FTgQFg44Iv7Ax4oiqK4vjYM+0/cxZtvXX/tHLsLXCmy4Pwa9zaYNS5vJ8nyqZePWqH3rnbn1/77b53vp0kEVvzt8/3l7nKc1UjeuVB4JInPvoLba7xf8PgSl3vYk1vTkjMdScsUq0yOMIsIHPWpyVLMzcPM110uqg4Uj3WTHBAWa12O2NVZuJhLkka4OHb7MjKOV33fUHFL0symFLnJ6cWT/mzNr5z1qybtpjHCE+No1Rr47fP9drSx+M1kV7t5u1dHCCUh/Jsf+4Ef/8d/9cd+9Hv/+b/+3C//3j6ZllIwz6FOSahEsSABD6rmbCWIkTMVC4pIDe8npUJMnFKZFGdHWZImNH942WY6+vhHjv/KX3zN//cv8Pc8AP0gjv8Qx5dABgS4RlcrOVuo4cHRxe8+drP102FX/OLSpnnuMo+zCcXlPO8mndXH2SIi57Sf5XZfamJdNCqznSjMokmsit00T7NaYD9hGI0Y7jg+yimnp9caQM5CHndP1psjTOM3NmsRjq5t7m5W63VKxKfrUPVSrtRdmJMggKnwVMzr+ItAODRAAQtYYJ5RDI8Nv/sevvwUzrie8f6Mvqde+HawYYaQ73T/7//bl144Wd3ux+vdNM3x+Ga8d9TMxYdZa0NplfOTyzIrhIDAr7yD336KwWGGveNTwm9+sAcTwEXj7lEToSLSJQH7ZFrTTPXQYTLHVHRWmzSYBRRZ2AlGkZakEzeDevhQkFM+PV5N47jq2icXQ9dwk5kcXU6X28nV7p6uXrqzEqKuZW4T7vafeu0OhoJNi1WDaYY5dkUv5q8/2f/y55+++etffvX7P9sw3w6RsiTTqLOSzdBIE8lUY3e7O+raVd+Ge+1SDlNRR7hGQJgHrTy6oPCcNoKzm/1+HHtAt+fvH//uiM/+Dq7+EKevAA5c4gvvomVc7O3JTtXfOt//1leuV53sZt8Ner0bp9lTFmaaZmszV42JO2kpKScCTRZqpu5ZuE3J3M1iaaiQa3E3NyP1SCKTWgAvvnAkZLWtn5go6HSdz05X7763j2UkzNKFaJIwuc02DMMwFG4kJZ6KEtMqJxLAPbEklknVHeaLGCcAc1igBHbAf7+g1UaCU09+0gJaEkXXyqxxO0fM/vk/uXRcMoEgIphKFJs9YtZYwr7wJvGjeyQEdVxu7Xq/TESsvdPzy1HdixtLOr/caZgwt1mYSWSRLZQIMydJ7ioEArOYmQtxzlwLC0QLeZGZG5Zwffz0xsix5+I2jNYoC9Htm1fvPt0a8YPj9sWz1optunzUS98yI6biIvKxB/2mldM7vY/6B1+/+eBq+vp7V//pl3/vpS+8+/jx5SdPpzSOZdVKxXcQsN+XpfHJPKulubjD3Cq783o2NyWWNqfzm+F2cGKEW5Jy1G9XwG9+YXznnTck4mYsR/k3dkP55KNNcXvzg/Hp9Xy0ku2gDnZ3VQtmPtT6plISUU5ETG4RBGEc4LO+WSfT4oSbYZxKSSxHTU7CzOQaFibMbnCCmtX+XGIC4mjVLL0X9nHS8CjF7hw1776/P/RbiajSB/3qdt8IZcN4O21N275pGlaPmQZidofqFGReU4dn5amadArubeisj6YX7xp1j8lXK7m+Dcn88O7RumUQWSALr9qcKx6m0uEZbnF21NYj2B1ESExD0SfX869+4fF2XNwUJMgMLQ6CGBbJtfvs7rMJg5nNMKsHkyBEFMBUIT9cRUMkzOoGkHAVf1bhDCzczOpsehYiZuHFS+uJIvxinK7eLQwkHqt6D4GrXal3RxY+APGcwi1wPujF195vhNo1pVDzVNvFAEGYmcXNI8Jn3amKJBGER1EnkHlsugQgc7ywSaAQSQROCXCUafiTdwY3Q9hj5gh8cD3xQQz35EpBEHIScrNw82ACiNEnZuFwgwVVzYADEo2wE223+6mUYjaqRsTgbjl3jfS5IUDVFVrM51KD9PrTQYybYdqNLaGOoXQ3uOPsqGkauAGpPs8ERJeJwk1BTO1GYEwE4chSWxIcKQhcJ/XU3gwtKiYEsOrw6sPu3fOhGSJ0apPsJqeTFOAkzQ9/98uvnrRvXc9vX4zHq/yRe+vEcbUvRZ1Bu1KutvrZ105njw8ux1nt7lET4N2kJ6v9r36h2swAhgglxjTNTOwEaC0vh7lz1MeluJOZORERhxuBHQhXgIu5macktaNmjpwyM+a5hHC4CXNiANRkIbJimIoSs7sDyEJEBGYWMgUITETETPWyhIWqR+045ZyEksP34zzOlpiNfPGTc23NP+vnuQsRhbqxqgtRUYuIeRjBtMoS4eYQIgqPYsSisxKIGURQ1dnCiEQghAPtMgwg5aIuRCJGoHAKqrCxAymtqn9da4HZHYJom7zKqVa8GSwZwgFAGphT0ZiLF/OpWL0uBHxwuX/0YNUx+2zh7hB3W7Xcd7LbGap6kgBCkwXuQTAwJWqTRJgHwo04HORqHh7g2sSORZMSAVCgTQCwN3QP2+7B+vq9HR+1g885kQNNTlPw8ap5iHCnJlGTZG3QpObEglYkCVtYzlSMZotGIjPGYh8WAh1dQ4lh6kFhCDr0NQmsFsJRS3lF3RwuDuMIjYDBibx2BpgZCAPbOJXJWGAeLDKMhRMlyZkxTooISUmIXD0Iru5e59ZHGbSqmtWciNtOWFIJd7c2JYCKeinTFtOsPqnvR02mUchr66uqw6olhRYnk7uFu9VeQ14mgQdH1IYtRZCFI6R2b2u7oaLNLXLOnGQaZ4InZj/w9Dw8fPlugjNT6rIHq4UA6rEf1UGuDo4mM4OKmUgkIiAykSRQkJs/U0dNQ9lPuh20eJiTWRCBzaU4JBDBYCanRopJ38nN1g4uCALAxMVMKsgvHBwUpgaK4CQMVfNv0FMtJhuPRZNyvMp3N+04e9q07f01danL6ekbV6fsu0H/4O2bh3e6cGynQqD9pOaxHdTc1byYq8YX37raj7qfbT/5bGYGD3tyPY8lnnX7TzZNwxRuRrS0F+FAeNisQcw5SRUKCEE9vLhzTKbkzkyJ0mrVski42qwe4R5ELMSmlhA6xxiTN4kp3BBzWXdtMOtUzINDlMzDPaJt0+w6q87qvkdKTARzWzU5p0zuBK7SydptSapeD2mqEgpirp8dsVQcLIIRTAfqHS2ynMRg4hmaeGnRq5dlnAB53R2hRU3lINikgBObKjEzyMwqEMsDNoVGrZeyqsGDAaZgeHLKQmGRYFW/x5lNjat5gbje+olwtSvDFA64kQeEEQ7VEAIz+YIqCYpIVVnpSHIAmFbtVjghTAOkwmzuCOI61BOUEsdB37lMJjko5UTw8LTNHJeKtZE3uXMqJE+2erZufun/vPXyS6cnq/Zzn3+vmFfNaTjMEVgCsgA2HZiEuubycqCDBK++Qr34p+tcDQ0eywAnorDgRQrgXorPXmWm9aKDvTZbuTKCh91ARMRYyFquxShgqpQzCQlTWKm7KDx8FyOzzLMCRMViKRbGME51vKYQuYeqOiEsLqbJY1o1zdGqC4IFmjb1lBMTEkLNqhPFKcBVpe3mgUrwJIa7BjGHE4eFI5jE3ARws9qalMOVr5L0KhA4UO9xcLQYY7m0DGeiqtPxcNT9xb1haltiEoDcKRBCWHcSDuZaXfUaKQAu1SzhPk1aSswKJhSLcBTgeqvDOCdKZRliHgHHQfkeBzewg7TUTuViTKYqka0CgvqOCG2WRboa1T+zGDxrNmAR4c7FX5ykm+y9i9uL93dTyMpx3OfjVfPSvfV29NshiNAIUKu7DgD3Tuh2H8w8F+9ScmfA6wRroYWa0zS0aZO5mUGYAlKDkAirFmoLD4awNFnmWQlIIjVaqVWcihapm/tBz1274MyLmtoTsdUH0kFEVW1Ru3huERHqMUxK4NyKmrU5EbGZxwIXoDLPJjkC5mjapkpt0zyOuU9NEgKZ++LLo2fiEueqGgYq7aXOMZMIREg9A4PILUsdtuEpwMzM5FHHYh9UiRaEEK5ediZyErg7BwAmjyQcttiKwAgq5Aw4BcCeCQUhH3qcPUwj4LUuFJElFvknA0AJJMLHH3UnHeFwQ1uVnHNI9b0vZi24x34u8ABHBIfV4BcMQ4S6JwoD2rToYGJR25AdZKREEaqmNo/l6XuXe2h/3H78xV4Snd+WD66nB8UA5EytR1E0GfsRxTA62oRIlLsY5/j4o5MbjXP60BCxpBqOoz61qVKMwxWUgutcPUDI6g8sEbstGj+3UkG56rEvGiDzqvICAOLKoljo6BGAk8ZS62YSO5S0mKzG91NRLeq+aEOCYp6KVNUFkbmDqWHSed5u6yNKIlymOdUTJMxBkMUAspwvIiyLC6om4KgYtUVH705Ld35BFlUH30FiWaMwVHaucOWA1kICLKzelHKgQ1bvGjMigpdku1r7iGk5GBghIFrGExDL8kGIyDjb48t5mOrfuJwylHCyaprERAu8U2RRONZLsIyLCYqI3aBFtRUOciwgAEcEIxJCmGGxaiUxJiK3KgQP9oUA3OUkDAubR5vHbWq7oyzepu1tscFvd/H0Zvj+zzz669/z+i/82tdyE3PBrixsqWK4uvaccHyS/9p3feTND4avv3dtisOVRiCI6WzDQgCQmQCowWH1QSQwwrkmT+EzTDXMXATh5OEBCfPJEWYTgmkBSgoREELMTA1LMbWICj1NpEzMRE5GgYACnIi5bbO7R0zqZsGJk3uJIFDiegOQFxuLBcX2dkyJilrKwqlSNcJq7a5yprga7QL1KyzhFkQuXIeXL1ojosrvqlgVQMKDTAslIUSicCchMGGmMAshkDDsoJCTui8EA7CICiSrGaxjeVFQmEVFOdXcQYiWslVFmAGgYda+wTAvIuZW4I7HV+MLx8kdQkxcTQ3wCFOrAmVbjMIYZx+nqV+3AFQPhjQKrSYcg4cLgZgpfHaYoRiYIicwoZFF9z3MVBSuxaZdNSE8uru53V3ejrZq5WMvbs42KcLNom/jYhseyLn2shY+xOmq+eyfuufm17fT+9fjVJwYLdP945bJItgPvo8qAADIw6rn1oOIqFhZZPt1lKB5hUsmDhcOhyGYkD0a4ao+BxAeTGwR9aoKL5RPAVsYADMLEBGZByIyiMnDjJjZgxlwdlBRJUKAPdyDubg7JaJqqTQOouqMgctBQ+/uXJN391T7n7yIxiuVgiIiDIAsFetwr7epJRb3sFA3GsMboZSFA8TBiYkP5NPF1erVf8/V/eFQjyQkzBYOQuJYJHs1ioyoujFmqBlFbPq8H20oH+pI3TFO5rZo6ReN3xIcUmYURUiEw4GiuN7padc4fJy8yZzYEzNRtT1YAjJ7l7Gd6mYND0yGydEQxjnuv/ro3msy/uYfCXNHKDoX9cHwwlE6W1MWebK1aTd/x0ePLnfz0+tBDSd9ZKFNSwG62ntx3OzmYv5trx1RxPn1cH5NN2N5d6BNij4tOS6CA0ZECBeiOr2yxmhSnZv8jHZD7gvZnYgYIcTBzqCGq0kbHjXaW9wEQnAoEVcup5kFAe7M8g3kOAaIBEJLa1UW77kTM5MDQqGqbsElQs2SwCusmAlELgGRZR4KIZIEAJYgMHNwPWaqN7V+ZGYAhOuwHSJC4hCWoIgw9WgEnKilhFjmqCKQxAmk5kLsWGqJs/ptcSK0y+ZjMAA8qwfitEutLHY496iD5Qgh7uEVP+u2WCIWOzAD7pE4pJbCg4gWSOG65cT11FmUz7OiqCfxQNzpxesoBUQspsJwRMv0sQfd9W5QX74uDHWY4KTnH//Jv9y0+Ud+6F/dDtNRL13XXl8MT671rSfnZrhzZ/jqe7cx7b767vU7l7afcLrCR+6lTcMedD0HyNZdt1W6uBx+5f++bQUsWCU8OJZXeyrtijmE4EEeHlW7WqETYQARGUV4SNXmE1Fw5ddUZwgtiJCF216d6eQEP4DgSQi+FDs4s5lFkJOHVmtBNTZiMffFYtKjQ5h0KBmTOwGKZWLuQsZIDHAE8zJFQziYmIHlfqbF3kgBuBODgpfhZ2RMzEJSU/AIoliaGx4ehYgagTuJcISrORMWT7oHE9pEERAIAHNkxp1W1M3N621jgSzUMgHB9RCSBXGliDAwU53GxRQnvbx78aFlvlZfzUyoZjAHhBII7A9P8vVOn9ws9Ll608zqU/E+UbBxwMMtEBHMdW8Pc9403OYIgAhCEAIbjlpsjrp/+Pd/ntweb/3tG3vtFPfFFbydMBYE0A8lkT/Z6c0Us+Izr68+er+92ZVJY53TeoWHp62nFROfrtutcplcCAPjcrSzFV6+N5T1UfIS8ERkFORgQGt1O5ZRS0JWPwMLhLk5CYNlAQwHLEIOifLiSgLFwR9QxwgSE8FtObU8QPzhNF2DLaSMqPrwQA3dKg8P9Iz55PBDHIZAShKJF2tu5RhQGFjoAGtgdg4mDkIwi7tztUZTLW/GgSp7sMIEiDQRL7YfCoMLDi6J5ZFyIqa6YwcQEEFi8oi+jg8gIjQexkQBEg4KeN3lYRHesiCBCYdrgJOVPJu/UN89AWOBuzVZLEDhWlOa8KNW1p28f+0UIAG0anssCZYeWRBxJCLUGC7cAWb0DZ+s0jvn2maoAYScwAImQtn3m6Oaza3alDN3zcHgT/CIadbff3t3NeNbXl396VdP+kyzRZq9bZiId7M9LeOX37/81AubZ8ze2uJlZjh0mosYIRM7Lw5aZCEHmYU5iFkoLIIi6m6fK7PEoLW0wRRuRFFj1aU9GjUSJS9YWjYgLyAshABf/HEK4oU8VsseB8Lyci6Dw+CE8JqJR4Qvv98iCZCFzBdAwoFwrfV9hjPCwR5eRxYoE3n9tQFiP9BqY3mHxCJMHLzMA4AFJCwgwgBXD0e41XjcBQADROFE4bWWTYCHC0c6cOlrNZYRqBNoUVPcenDX4jFWDbUJt6j9IDjggBnManuEEjHEKaIYE8V+tgXBetCQqUVTO8ceEGIEcdiCZ4oaGYV734Qw2oyUFkvKqsErG3t87QLjxJuMOxu52E5qEAYIiWGG33/r4qjx115Zbdb5yfUg5EddmhDXg5rHWFwd+5P4o8t9k6HjYgJlxusvZApHmVNO1ZluSx8FBLh5dTnUZ4xB5iosjLCoMdahDAqUcHck9prLExwL3gzuxoyaMtZPM4wXJkAdllfvwXoo+LPxd8/6Rx6AWywamPqALTOikIoqk3hwtXpXSRZTqFfvZMDAcJba+3Cm5GGJZPEzg8zB5Mq0IGK8Wvk+BNPnxMXMHYsfPyyCc6Ki4eIHc/2yf4pY7ekUW4zSVKECVFONJWes2yMLF6OiJkxqtR6xeHAioIaxYFJbNVl9+Wss3Azj7MMEENRADg24YzvgZiip8lzDKijcluItgapdHYlJZCnV17I+E6Z53k2W0tA3aST+/Ft7LeiE9jPWHdwBwjCM3/fJ07nY184HU9/0zdkKqZOLXbne21h8Nh+uxqlrV03aUkFA6thUxFSi3qzqVTrEdVvCoUxdvNabozJYPMidNKzCnBYcaW0aBE1eTSTk7</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy92bJlR5Idttwj9nCGO+fNTGQmEqgCUPPY1XOLbRSbNJrUMpnpiRJf9Fl60wfoDzRQbNJo1pSa3dXd7KoGUIUqDDnevOOZ9hAR7nqIYR/wE2R5UIVEnnvu3rEj3JcvX+4RB3j7evt6+3r7evt6+3r7evt6+3r7evt6+3r7evt6+3r7evt6+3r7evt6+3r7evv6//uLzr7REBMRAIIqmKBKRFBVJlIlIgUIAAikUICgRKyqICKFEuJH4s8JBCIoEQREEICBdA0ClJD+BcrvCaYbI18DpFAGKQEaRwBQvAIBqpo/Fa+VnoAI+VL5d+KPoARW0jRYIo1XjQ/FBIV66M7PXeWdXlzvdInlibW1UVIo4jSV+8SHIUj6iabRAURQAZFKvEscJ1wIa+/XXr2KkA8aJM0BMVVGvSE0XM3ZNszWEFQEYBjL6UnTP/nx8wMCqig/hpZ30/+nV160+NsKZUX8J10z/zoBonFlJf4MIFJJI1ZREKtKug0BClGoC7NQkwW1zCYOGyGo/fGfvWtqS9BkMkQEJSZVEOc1IiJKa49sH9H84o8VwkQgilPMILASESmE8oIogTQZYLwGIV8BRKxQQImLIaGYClH8XQKYIEQkSiApg2FS1bQUYAIJURwQKStHMwLiMykpcRl+NBIlYkBDL+G5e7iZdZvwVx+/1Ef66HtH80NbBgQogaOJZqvWYsrRJ/NcqiJ/kEACWo/DZ6vtV2sdnXi92/idU1sbNmCBsUTHLZ3U87OmXlSmsbY2vvdUUTWzXBtjGZY4+lx0R40Glgw/OaiqJK9kRVBhECCiRBWxVwkSjSnONyQaiqrGIUsyNIWqkMZPkKgSlEQFSlBVqGi2RQWgKiQq48afD/O6Nrhn6kUTbXDsxVa1MQ0BhqHgOJdpakDEqmCOMzc5MxTEETbyBJs4w5RMQ5mYCYL0ZpwDomhurFTgJtpmRqWMC0zJ1vKPURaXyMRZALiAFRdsIlKA2RQTJo4PpPFagBIXX4k/AwFgkMJTcE2wPVcVWWtozu3M1DMDYqigmGdG2myqmi0Q0UEpwX6CD4LyKHAaumCDKLGQVJatDyJq2TBCtxHYsTXwNaFT8R1b0gBTs28Nz605qJb32qqpEKdRWVWye5FGQ0nArYoYikiFQaLKDJrb2gd0YRBVUlLVhIQKJdFAqoLovKIgEkkfUE32pDCqopKjgBpRIcSRkAprgBFuq9pb1I3JIcDbNDlUnDuiSY53DJQolnxfpwBCKXJoWXAAGfl0+hGIWCnNOgqiKcDxwxKNChNGglNwpT3YSxiVFzGD3BSskeAseUYKFkxQik8Zh5Tskkij/VG5FBGJGmZrxVZENbNhZtZozNEDJ6DNPqkgkHLGRQIhxiNio1BiEWzH8dVmuNq5Ubed241BlIjIBg2j2zoRofbGDXeue93ZeU2juGE0B017WDVLa1trVtZt3Mm7h9XSMvEeuyDNg0kQSylkanyeFCkRNIAZgSK4l7irBFYOceFYIQAnhImxk8BCyeLi2ijSonGcfxCDhEGEzo0zrlS48CRi2IIi2R3j2k/YEgdFqkLEk5VkwkSZlpQYmxZDQYVLJPzYC4ca71TgcbLjfWtGAanEYxKoMWmBP8qGuBfHAeUChMlx8t9y+KeER0wk2TgIqiQ0q41VM1/UOoOt+WtcjjIljACppBnEGdBi78mLIvUS6v3wqrv+fNWvRgPyTsYe1qhXpRChgdgASuLDOEh/61XARmvXr7fjqmXT2MXDOa29d/rgu8e2tsQEVUg0aWKCEEgZmYERQyLvlTQ7o/j8nxAwQyVRYqgKM0kMqUyUY2J8Fo0TkMJQ5GQKZlUFGKociY2AmPvghiEYl82KlcCWsrFnHKIUt6CR88RZ0EwJ9lYLxWYy/8mLGm0x+jhPiUJBn4gN2ewmMKTMlgpkZFgqqUa+P2mOYpoWGVzyiWxVCX7SW5PVRvjKHDzyUGJSDQISNNbMrHn8cN4dirUM0jLIHPoT+imBIYophsaIHx08EjRyqivnnq12Ny64EEBu1Fmli1m1G2TQ4IN4JTjqhtEaMkTeh9HBWA7euw2oIls7N0ozM6H3zVF99nRJljNuplSCJcRQqYlJRNKrKJSXQJKWMDpOtFVSBZMKmEkje8prAhS2hsQKcrIXiRupRgYhSgwYC1fBEPtRFMJs4urZTDiQL65TzjQtKvIaRxiJw5vCJ5ePZXuI5hJpP6agFhMiLqAXswZOdhyDTk7PCliVnGMC2ELO9gM4wAzNFynBPl1NSGOymeyScgaRZjA+mqqKCqf5JROfZYrmGYTLffNd9+6WwDJREOgQhotOV25ZYR2Mcz6oqFA3BFV4Re9QV6RMu51qgCftAwenYRBirS1aNmEXdrtddWAWivr59vDerDnknJqlMKDMMS2OtkWCvAQpzigYrCxQaDQpydGVVYRZRQ1DNJPNlGpKedT4gEYgMcAByimAElRZiUEVKjKjc+JhbIqtFjlGKiErGiBO81mmNZOlKWJFI45QPfkLFJyhLdPhPEJmEknYE0NKWhfK9yj/jwljxppsMxE+Cv5NQVABYo6LHbGm5JOaGQRHYGcAqkGUiWHA8SfIARwkCu919P71dUdHfKbGkslTTNCk9BARQRJuKzhn6zEsUEqwQR60cv5i5/ugIBUR1brC6LAbQluzZRhGxdw7GQeYGsoITkSIiUVkcCQSYExQdJ3v+i015t4Hh/XCRiwAJzgtCxIXXiN9oKw+ASBliWgPFUQj0UiEiUnBxArhzNMzdCXnheRMl4kEhqAE2QtXANgwDFtDJrD3oSYLEDNsQt4It5HpcuJuBcloMgNFnkoFOJHrBHYTv8rkvZAnkCJrW0SaCWD60X6CGdkfxwRBM8GNkgYSGEqGiuwAKXDEQB+5Qr5+jgQqHBBG4d3Ig+yGMICaw2p2WAHElYFhMgoFg5jBwNgLBkXMMpMdpicAISIrqypRzKyp+A2mFebgsRrdnbu8G2MaVFkeexGluqK2MpVVJmLmzokq6hpsTJDQj5G1aBB1ngKEiQQYb6S66tc3fbuwprKmIlNxTuVZYxhlKDSzhayrJciPXAPEKprCEkhVkwGQUEpa4+9J5H45v89ZqolwWGTNqEkBzEQVQbVmMw5uftAQVKE2KxYlE4wokml2EkmV92nZNJ972mXRMSlniuUi+7YaUTrnodOv0/7nCoWOuJEwKi4ecrqS1MXJCzKEUsHgRMPUg0TRh3DZyaudrN3qeliNvprbw8fLqjXVUUNzSxWHQFbVGFNVasHDGGJGkemngkyc0+QoOffiImHnoK2kDEA07NxuOwYvTvR4WUO006ASQiBi4wZ0g5CRYRQ2UEVd6ejIOQ0qzsNrQh8HVYOqwe3r4dk/3mwu+5OHi+VZszxtjU2Am0QV0bxUyLlYUloS6CValrQm5CVIdKkw2einIlmZYsTkXhXEHBVvIYEUES/qTup8Q1U3BFUlZoCSQhvNQ5VzeKIksxaOlkIUJ+5LUqwkSVaRIhYOz1N+Nzn5XuaYIiFr5oLxH+VEnZL5cUJ1NXsUMPKGhILIOWB80kREYuBMIZ2HQFuH2x7Ptt3rbtO56+thGHxdmfpycA23h9XQWF9xc9gstK1mcrCoz4/q52Gnifbk4apk7M0AUFSr/EYCUgVBIeoZy8b4lozTZWsbYxR6dTcOQRU0+HC3FefFjfCKbtRqKyDSoM6TU1hGZcgJXEAIaoNK0Od/e3N7th6+c/akPZkdiDFMTBJF8aQWIoFQBt847Bz2E1gRErfMcJUlck3xIrE+ydBYoke+NEfdBCmAgoQZ0m2PqL6K+ShABJuWP6qqE+spBkMZ4jSHP9pTHjgrFAA4pjGFZtFetkjQpPJg+myGoOSKhXtlvkbF4/axqhg1UZk92sPH9O8pNQ6KztmXW73ocNVvr/tNP4Zew6jXm3HowtGB7daOmbZe27ntl4sX2jy5d3T/sHktXbpqIqvFqAuDRJ4rBsEUd4oGPwitR7PyYVQoW6aud9yCiIYAa8hQqlPEDMkpKEAUdQXDCEZNQM0pLjMQFG6AqTB2ojduc9vt7ubN3LBh21CWI0hZWYqvKiK0qlJeKagoKYMFSil3IhUUPTLCTVb7c6wFVIkBYYWQQiXlECoUVRQCmAzrsJmNGzJLBKUKBNhiEnkKkQ0gLqtmxsZgIgim8F2YV4yqRXDP2JcrBHGImUXlhwWoVAX2ZJq0SBx/fzIyFG2CIznVbFPIq63YI2uUnUVHlZuhvuyGN7sm6DsH1dzqWKsXuVm7q5V0w1BZigWt1V3vpbu77t+8e161VmdxxiepmrTcMjL/rLZk7pkjPAEIQbub4eqLVTX6D85mxuj1ZhxFRMCMxvLowm4QNjRnlZpno44Cy2hbGkfiIEwYgpoAIQAwgHqEIDAIHjcvt1Vtxz4w8+G9FsZE+TPZUsL2JGNNEIRUs8sQlueeNd0mIaHSZBoAiFU1aWyMaFwEidlXrEtEjYNoI3Cj5yGoCKkhIjsl4/mSSlFaSyPjiWZJNqMY8/fMM8pFU3zMYS37QYq26Ukje8vWVgAyYVI2oGKa0eeS8SNWX6X8cMLabKPRF+PdBbIZw3a8F8JPvn34o/cOQ9C/++31Zxfdq1W4aLji8c3KD704oWHQpsEwyt36xvXh6HwpT5uYRkRMybEjshZNqJyqcwBSil94pqmYVN89sP/yp+c/fP9o2/tPX2x+/vnq44v+cG6918uVZ8aTe1VQHUbtRx1cuF3r6DWyLFH0kYIrKCuEQWE8CLp54Sis+s0gXmxzvjw2mPwvhT4lStXuaYFzcAQBpCrMrIliaU4vFcoxbYVqKhIQkLmKgJBzBIkXFZTFWjHWom4IfvTNoiaCVURekdUSmpYerAwTa2WULkGqZT11zw4mdV8BnrJWQky1sWfPJbzFKhAJkckiD8XSRrxUrpmmxCLV9VNIyG0QrDmNKp65l1Q4T4yjyvxP352//70zvHuM2+EU3Qm7T42aoHrAlalWQ7jdBgeMToNKrQi77c1VaE4PJRwyiBgK5kzCCAoTzZiYEjsoCfDkMhWdnsz+hz9o/vB3HmJucTvMKrrrwvUoAr3ZjD4IC7ox9IOMXg1TCOoCHGCBikEME9IKEuABSXIWALgt8HoUH1T08N6sWVR1RaDUgsE5kmXymCMVMUQos7BkKQwS0qhITyimmX9k7VfS4yV1QrAv2cbCABuimW07t4Tvdm5xDGJYKrJCAdUo4ec1zLEMIIZSkv9yVrmvlSHbSubIcd4pFRWSS2nMsTMwxrqgImv0Gd44a8J7HCjelYhiW8pExWLtIykhTFNEFUto7H99377/3gInFhqw6434mmTBMjeyrEhmYFPVlq9oHBw2PTxhdKKr7XBlvZMUiRlZZokTykpiwIDkPGSKrkiwar79cP6HRxVaAydwQaFKGEe93blVJ8YAQD9oP6iAnKN1n+IjAaMgZNsA4JH+CkCyTN9vQSy2Hde3w1nnqqqJ/CLJj6xZuU0+nNToFBoE8Z0UaZIRpEpV7GwCcstJshOJRaI0xapELACpKjQmBczcmKo2h4ZfbAYJgMJiMq8iFGh+tIRbqayZC+65XqgTZUwfLpJxTk6jw6O8Yr6fP/z1XqOS6RBT6doiQtJGOeUVkX0QyTRwSsgWo3NuYVIiMpUxc/zBzGBhsB1xN+J27D2pssZVk0AKo8qKeWPEi4GOA65vAxim3fWbkXSuItGCAcTSHpEyGU3lh8gbU26MPANG8IOWEQSrAZb91r+4GV7fDbe7YbVxzqGujPjABou57Xtdd6FiwMCHyZg4mRQ8SKE2i/Sc/20WTAzXh4zkqmBiodQ7oFAqsTJ2BTKRxMYvFZq0suRCStGnuOTRcY1jpEzZgyYWyCAlUgFbiFLQoExqeTebV1XTb533noi4wELOySdtaGKCWekGuGSFJXuORjLFQy4EPjeTJahLalxsqywmVph++bNUxIv9ltaknH4UnpcVahRj+5puTEyz2pxWjM5hDFDCog1cdYFvB1530o8agjcKDQIvllAzGcIwat9j83rYXHRWtCauglhBpcQKJhjDzGRMbC4gZiLiaHNMcZLokPA4tnNZwhi+eLN9ft1fb/3gPBG8aD+oV4jS6LUfRLxaBis84CeZLtkcQTkH0Ih58aduFZTMfFmJSApnlITGCV45pykAuBCLlMBMTDjL6hH/mDQ/WnxKytl26orJmpcCaokbww3bpjKzRb09WfrTQ7Jwo5OgNsfvwtJj3MzIE1eTVSEMEwkJcplcUzTP0E7FLfbMtcAXJnvSaQoK/CVgTW+Uqmv5O01vpAZC3beqZOwMUWLOyh+RzkE4aPBwgVWPN+Nwp//xi90nz/tnN/56A+fBSgStodughmEMkdcgLBDpcfV8o6PMZxUsg0mVBvWBCEyxGLCnaaLgGYOY8DMfTsaARQVr+9eru7UTpcHpEMjEBzAJFG9XGEdRgQ8YZcIwk5cRgEmhOWVQEe0coL3amk3DgEbJkJg1lrUFYGWJHonMlVN9gAiUeJqmkgBBmaZ6ZtQ7VEkgxLGkmdq9JHMgQFVjK6Sp2BBbQrVow0wHliW3XoIbfeZQoBzgchNi0Z+SY5SmVCmWFavFsaLAMaNk8FRUSBZBxVvSUmQ4S7+dDTG5WSRqvGdkAJQTSYp6f3LO/RFm64+1dE6wRySdH18PCAZqLn67+l//z9/+v5/evrrq3eAaAqsGhXqFwLJRIQkIAaISfe/qy83dZcdE1rKtmC2xsTlic5w1YuLo4VxGhvOgj6+72/WItoaXVze9tXh4YB4dGqMYgwA0Dtj1MjpVCQn3i8Xu4ZkFCDBQU+IHYIEaqAES3D3vXnx612/GHLLz/PGkLaVGqThtrJydNv4VuXEuw1b6dPrtSJdpAkXO8SP+BQqJkRTCbKwhshxMaBeVkB9HZ771x/eNjR16mm9RhkCprwgZj9NSl7QqDY2RlftI5Zg4XiZKLvsDntCWMqlPYMREqdqdfyEvmhKnpjkqGUGqWRgipWKA8VNRsExPwTwG+dVt+NUVXm/+/S9vPnm5WS7nA+jNemBFXbGoKCgIdl66gUZRS3w6o4MKQ6DdNtz/8ODeoyUZImIlOM2bD1g5jykHlOQEAOpXO//Z3RdvenY6rPrnb3ai6oOEIFe78GYdBq8qCKLEaCzPWJ8c0nsnprG66VPKCcBQQrVYeDWKzBumKCRGucHZo4Nmbuu2muZ0T0yilAwk1J3aRCn2mU28qYSWkhnkYJooeXb/mGCAABEYImuyWLXH8EEITu10Bd1Hr/1niewQOfyl7COnVKW+k2uqlCMbhCL87gXQ2JiXXDLygDS2mNZIKhpo0kooYXcJjtHEYpcnF2JGUI3iSA64hNSw42dWl9XVVX9ci2E6mFXfOGseo71dj8MQ2oqCcgjSVGhGuhI9rHC25NaCSecb+fROgtdI/pHmIfq+lG5g5Owmr46GXn/58c2rz27+5P3l33964b3eO6rPj9ra8MzS6cIczLhzUhsQsfdaWz2o+eGC7i3tO4cMuN/ewYfYi5i0DAs1lNSKom5EpYN32Fx2q6vu6OF8mcwjei0k18ZSR1wugMYeodiOxqwqU2qVewOnIpRm6SuLOqmNXUWLg4kKyFCs5Mdyr4IJQQhMNoN05kmRc6AsajYGU9pdSsDLFDwVnJAyhNwTmSPl/h6cdI1oGQRC7gLP/41cBke5F4gUUhrG4i1jX0ukh2VC9oMo5dKTg75S+tZJfdyGHz+ZffNB++75ovf6oJFfX2ye342DhyJUxAetnniywHEri8YApKDPbn3VcKQjbAg+d6xEZ0vuTgkRoh+C2Yo5atY794uvVkTm6b32g4cHZ0f1q8vd5xfBBWkrrgwx0eiUvKpXZ6Bzmtc8b/i9Y31552+QrClkNkYhmVdJCMYYqwJCL7evd+//+LzkZHEmpmw/Dy/FgijIcCqLRwNTQazZp1VP7WuxZa/ok8mtKernogCIBYmDTdvgGBQgzCCoTQPS/GdBzgksU26RaFpa+FSiTg/ASE+U8obUblHEy9yyWyBvj3vl+0STSZadTDqifq70F1+IM5RGlJuly7j3ojMRYJjuz745Izg/XLw+aauTp3MsqncOMftHf9ePryXtfqsZx3OEIC4kruXV2QZjF9wY6rmJDhF1pOxbyXNyvE+rYKx5+uHR/autrsd/9sOz7z05xJMlrrrfPltd70I3RllK1r1WqscNHVZcG20rUoFhczKT04XfrDBkKhYnqBgZ7wm2DBDDtsyGbWWQiGlsdUiVzagwpRiXMEjBsfVIKGpMomU3WZauQJoYfwwtQCw/ZYEpxt6kAuSWSkl9X3G5Y6HB5t0CCWGStj6tbvrdvbCFrHyl3rm97DuF/dzUMV0YpWc2NYIUS4g3SqZO0RNSeT7t+0gbO6d+OM2UmSLUZwtLOwf2IY1AMLq8N4Mf0IkT/rsvt+shfO+9g80u7AbZdoFAlsgrkeFWdVBWwAWSoG+2SnMjIqpqMuuJbpMGlMY4JU4RRpnpeyftP//Zvf6uf/yjcxzNcOeefXH365e7N2u3GcLOBRWYQMczHM/sYQOjINAYqAFVhlomC43GVFqRJNocwRC8IOSpJ4GMOnbeu8BTK5AC5V9ErCQa9yEIJOuYOQvIWZ8SxR7W1I4Uy54o1CBpmLE3KG1QBaJqnVO8vI9UhHJxP9WdUOyGs92kOc3JAZJgG2salBtMJrqOveBF2WKmQEa0Z0/g/G7seU6oneMggInSx8icATYL2zlRzeE6pR9ZX8tpOwggXmjA1fbf/+LuH55trtbu//li9/1nG0v81c24HcBEhjkAhkitinJj4ERvOnm10oPvzO4/XjbzOsl+IJAw0eR1+fbgskr6A8K/OrDwDR4ucG+Oi/71p9d/8+vbF7f9XRe2o+z6oEGPWtxb2pMZQ+RmG04XRqCiIYgGARFqgijCVF2EA6AwmiyvysA2rrSdWwm5gyly1cJ7qCzEniobFzi2XqM4sGpK/jQWdIXAGrt/0oJqjqogEsW06nuGltY0a1i2MCXkZh9MGhphUrgLFsbBSVrP3PYcQ3gxUKK9z4KQDTjtcc9ReOonQCqLUhqvluwoYVjiFqlpNj2wxhbzfB1KdLcYbAz6a8WnLza/ftP/3fNuFDYk22fj/QOz7V2I8MvKkVuIUYRBaPT+xVq3AR99dHz/6VHdMDNPzx8TjbQxqIwMSrCKP5/Xvz86vNigEjw5xKvt819e/uKL1edvuuttWA26Hbz3WjEdzfh0xo2hzYgAQCESgphu0N5pzGo0B0fOkOZzSUABDxDAQNWSqdhWnDliokNEFOWz2FW8HxKT6eyJpZnGKECSF6LIhJjYk4YiolHKLTTGaSIiiAaCSfYsUZFIoIBYvizYkzE3Xielm8hZR2Z0oKmLoxhxLvNlLlZsPW4DyelqGnPCuZQnapqcvVHkREE1x9Ps22W7B0pOTBzdhHI6DIL+hs2XbP/gw+PvPz6YsVrQaqev137e2jifbBJCRVq5cvx6o6/XKhW9882j2dyauO+ZMhvM3hrNmRA3LxMBH1n6/UcLOP3Vp7foRnxxc/nx5YvL7eXGrzu/HqR3zo9KAmuwqFCxiKgTHM/NrGJSOPHbwQeBzVRBC5IBDWFGqAGbs4GobpiWq9rUM0s0JVYxrHNOCSP9JyBv8YrcIk721E6HQndpjxzn1IMSL1AQkqKfU4a07KX8lsgQgWBzlMwhriBE+lw6HSP+PEus029E+IuUUBM1mCIapgCrWbnPv5SpxV6Ns+AqEkSlYmVKgXkf/HJgz0OZKmPxUgV9FLg15uqd48PfXv3w8cIP49XWXw9yswm1razh0cc6EkKgCBgjYwSPCKfvVWcPFxyLSwSoikI1HT2S4VQpkRglomrw+NvXV883v329PjqS7uX24nZ8vRlvt+PgQwjeBj2stQYRaFYRFE5DY1FbUlWB+qCbUU8OUDtc7TAGQFNeGZ/IxDIAQEAFhMjYGIvTpqpNLL+m0rIiw1HWyxRIxU2llLZPETEFhrze0QRiDpqIUTRbKYWQvO1NFSRx6SjePB1/klrD0hEuWoonk4YfC+X0Ncwo2FbsMuLXxOEygGkqz2qy9dg2sGeXyVNpsjjkvCLH1JylUpmEYogJQfO4MjOkhJs514xXE9JXZ/PXSkfL6o8+OH3/dBlPUnmzDp2DxHJA/B/Uxw5pi6aiRx+d2prG3ueeQcSjBoBMU5OvFUjFZ4T/5avN//aL69MHR3U7e3033PZu02vvVEQ1kGEcNOZ8Yc8XZlmxZZ5ZnlmuiduKa6LbbRDoQYuDlhoDUhieClBxnMgBNOR42p5Ui8OGmUqA54RrXGJUnkBk7N57BwokYaFUDiPYMGUKkpZb8wrlGaeUiMbVjQUSEY0yXZwdmxc3GSfnLeJKzGVZ4za7VDNTQKfmhZQhJhIWU1FlzY2JxbjKUAtVT2XKDK95uxUoUc+I6VTgLdkoEFtWsrHneUKqx2XHBWeEBUCXTfXNd49/ugl0yodV8+VV/6obPSSakAvwQhI0KO2c9F4AWh6a+ax+/ZtVvawevX9Un7VKiB3vaQFzWMnxhgDtrbn96OR/fLj4xocnuN3R87sxqA8at+wSxKZMSCyhYrWEirmpiYi6Xl6v/Ch0PKdB6K4LKim1ZEKlEz8rGX4ACGAL14V+58UFag3KxKKEB83LuvcO5VpA2i0Yjz7S2CKeAWjvXKLU/0NIm56SJWpSdSB5PwAzi/dqiGSyswKYmUHmfkVlzUF2inkE5HbfpNcnBsGZwsW9JMlwc2c2CEh78gvfwrQ5M484cYZim5oCME2GFs+uKbkmUbE/LnkAZTG77BJwTC8eLC67VbV1K+8fnLeywsuVcyKj0OiVDRbHi8GLZW82o/doKr3+zeruy3VzXM2XzdG9diruR4pCeZMKMpkkAGgNOITNx7s5RC4AACAASURBVFfr3WCZ28ouW7fpYRiGiUkNKUFrToffhKCbUboRN10IpGeHPHjd9WIJ8wo+oEdOujWd8iUZ3hQIQPAYRyHAVLbMdpmxXPqe4o2WCyQji++m7ahZP4PmQ6gSMYr7byNFyKEjF9TzkVYKIjBPtfYILzZhf2E2FO1LmSILyZuTE3ppwV3R3HySg27mfPlzlDbNaJYhsr2WJF1y5gYUgj3Fz5xXEIpRFSUhntuV2F8itZoy6XRjzjachv5yVnf32+py9+HRIeb8l5+G12sHY09OZotFc7Cozw5nb26731xseye7wWnQ9W83MDCtcX/kiCmKjjEuJHKcBOoYgJINEOF6M3z+1Wo7yv0ZtRVGx8RGyUAVCLFkGQ9JCRE9oB5hMefFzBLgQmCVgxkA9B61AHm/hpPJ1GIvmiXwDMfnMzCc8/WsiYQ/n3CgaR1IkehkNr9pb13elxSVtPw7REhHU8X5zYptWqSU5IskOJKUtiVEC5KvBsBOi5nGnyxOAM6tGSnIcRpcab7N2LeH0VME3bsJlMD5WLwcdYqCk1GR9/BS07ZJ5NsX2Eu6yKSj5f9GkRH5a79X/hiIbpf26Y6v+uCCKkAi1axZLmcnh/W8sQLpvY4ubDs/jMqky4U5O6oXy3rBhkOM86Qc3YaLS2dGGlM6vrX6f50tcOVmr29OapNGyQiqXkNsqDZEnM6pYyUh0qbhyhKT9o7SYwhAcv8IT5lFQZav78J61NWIAVDAMOoW9RHPjquTx4v5QV01piAW5UXPLUyZj4jGP7IRYgqMOWObCoVU9rNwwgVJ+yQSYlJUuRSUusGT/TCrE8q5m43q3EQV0/Ile9HEdaNQQrlgn2ukSB8gQFWj5lpIFpBtqTC5Cc9jPE0/QNmVUgAtwiSXtzX1hoDyLgma8gfKrIL2eFv0t68hLP0NVzdvuufPN19cjK/vxi7AObWdY8ubzq97/9Wb3eubfterYTx9Z/47H57eO26s4Rm4uQva0C5TgZSPFzahWUxTKNP2tD386fl378+Wr26v1p0XHTwGL6LwQSsiJQ2qorAkUYVlZig50cHr4NOJNMeWjxbVcl51vavn9hADtXy7CV/chGsHU6E5oPl5+/CDk6ffOz180FZ1qjvFZmbN8lamsIgOHDQ1oqXnEBXKTCfRlQQEqnl7x+TTjPhmTNQkRRGhibWpKnM85S+epZBLZ3uCQTmZco8+5mSL0s/Tto94bmNOUPfsK5dcv8atYkUG+49SiBUmdpP8UZWjR5uUIiSLVaVySOSkwu0xEgKVUk2cmMnYP6vt82+cD7MZ33P0fLv5z2/6rb9ar43duKA362HXKROswbsP5//ydx999OiwrjgE9SCsfF0zSFYtiS1aMBTI0l6sl4AJS9E/6/x7kFeWRk/bMaz74LwEEVK1xhhCSIfkieakXgEXZPQEwlFrTpfNdu1Aql7a2oRBZkRtw/dmtqXhilAbY44Mv3f46Psny9PZbFkzR15FqcW65POUdj3FZYqbTrL6H101oUvWW0FSdoeULCJG31gPBQuJxM0EGtu5NchElxRxG5UaJajNopjmOhdKsEtAMyV3OdAj8+E9JSwHRGia+RhOOb3BUYMxKYImq8xkX6N+khSXyUwn6N6LyFll08Qnp26C5IFpuTOxUE5tS4An2p60x0wHC1lf9k45Vlb6IQxeGJi3MMbUNf3znz780x88OF5Ug9dhDE7E7aTxYA22x8qpWxpqTMLLcjhUXpgD75cv1zs/dF56ke2o/ei9qARVIGgQIYUwGZPb4EkRT5d5fFqrx+16mFVkD+reh6a1N7f94UHb1nbwYTmrfu+DeWuo63xvcK1EisXStosq1emguYCpaYamPY0ohzGWtDWFrsjq4gEbOaxMTBmK0ouhX9u5wopAUna7EcWDN4gNeS+xY84m+GGU9KCAQ6JZxEh9S/v2B9J4ulnh7wk5Evyh1M1ieNV8xGE0dgHHS+sUgbPvJEUjBWFJKXcif0oEkTiR02a6lA3kPRQZ1ThNQ064iEBDOLpyza3zr7t8cI0YQy1zbc3ZcfvkbHF+0vzTHz1493wBVRq8qsKBgmCQ4OHc6DbAzo7HDS0qsolQZ/NXEN1U5suFfXzVXXXhauuut247OAmhYhKRoAQRJdQk+eAmBJFFY5/eWx7V5roLOgh5bdsqbCV4Wc4MQWeN+c6jxbuL6snDBXt99XK3q2gN+fIfb6+duA+Pq6OaODd/xYQp0YwpTqAcfhAVXJngDDq1becQFLdpZjEjZ2dxhuOFywkKpVGjUKN4ypASWWQIyVp/ouOZhucBomzAyhBV4mvm3CmlSG6NUqyivWpNTDYTwWKZRoRMKbP4qaU9dnK5TCGB6Blabp4nIRkekZb/1lzOZVVAVy5c9q7TYRCTdmVaUiHFh48P/rs/ePLgeN42/PTeom3s6Lx1ZJk79d0YQPBbP94OzrntjNfHlb0/O3g4tw3nRJiF4wShqnnt8PxmfHHndn3wTkysHBjyIp7IgGI1kqHW0Hunyw/Pl73TYXQfPVi8s2y2g6fWXr2BB9rZvK3sB+eLp8fNzNJsbm/e9OuF8UA1yL1R5OeXV1+tu++dLd47MK0tdAfIYjdprJgmvy8LQ5npCuXoQNlSOYGaZq5d4kRR2+NlssypKsQUOyyZwMwiSqo2GWperz2WpJk95pwgBbto7nkzBKVccUoIUuaoXwObZEAJFjXLEArkJrMoR6WOdpQ4T9m34ucpEY2cXyfsSoGVC7kshZM0RWUAQrg9aw46T8RsOG9VNYdz+9/87pN/8oMHbW2gxAzDcIFV1fkwjOJFbzfDx1+t39x13eDuBr9uuHpn9vAn5/c/OGZLk0krZqOEi93zy/5Xr7bXa88kGiS2XEdaxgQT9yAxlo39yQf3f/xgaTzdjuHZi7vuurvYjF9edYNXr3JQNT/7aPHdp0ffOJ+v74ZV769W7uVVv1YJhganUBwAfNFdXLy4/M7h0Q/uNcdNqvXmeY4LojnU5Tp5JmGqpVWIsk6TM81SN4xdQBGW8vlpkjSsSPxUKR+OhdyzJapqc/ZIeY2QxNRcz6Yc2fcO+dK8iAVeMiRlmTbXi7QIYPlgmvQblAJZfKJ88E+6bjxkAJOmll8Z0ySSCcoBOzarFVIYh5H3XgHT/VWX1V1r6q2nho+XNROpysnB7KcfnPzJ9+8fLeq4PduLqKoPsuvDdnBB5GrV//Wvrv/hNze7YSToMKqo4Mu73da3h83JO/NCKgjoCV9s/dXr3eubXT9IZanSALas4hSiapgYqJiWdfXHH9z7yfvHvZObfvzypv/rZ3dfXXZXG9l2mNe4f2j+2bdP/vij07rm7cZtXfCE4PSwtYuWBicVsHbBwiysNZ2/+Pub2ys3/52zxZMDijs/SrtoJt9ppTNKZcBDUlvT+XJx+zlPGwjiYkqJcQIpG5HjAbnpzLakfmg8CoIhpZ82oWDSyXLphnLqmHkVQJkKlcwgbQIjorS3NFO2qa0jS/MogS7i3pQOFftTEENSrYsyuc7Be68RIPXSZUuUPYiUrA+VPHZqS+GZAZmdk8NZ/a37BwR6fDZ7cr744J3l6UETcS+IhKDDGK7X/Wo3dk7Wu/Hnv7758mKjqqLkQ/CiKsIj7v7h6tnj5fL0cdXaEuHH2jy/v7j8hyufxAEJBIhA1YkSU0VqDd07mJ031fVF9xc345vN+NnF9tnd8PwNVFEBDx7yD989+dHj5Y9PZ/5uuCSE2tSEeW0OlrgbdA0aBoGoinqVwWHX+eBEPrt7czf6P5ajD46MLUdnUUmYUujaU8YFRTmL6UNarOi75TtJtIQizWlFjp4JCSEgg9wwRNEcSSzyUiQk4xx3k4GUlGLiZcVr928St8mXqDvhUBYpUkdQyScy55++FyDSqpKzpTtM2wWSJxbD2+dnJf1JktAe7iPiH1GOIgyqh/DkwfLDdw4qyx+8c3C4sLU1kYwHgfPSD/7irrvZuH703ahfvN5uB/fwpK2NbfthveUd3OggIjToi59fPPr+2b0ni0yDCIbd+0f2zz88eL3b/P0Ff/7GCis0JPSWivl81j5qmm49PN/6+w/azvsXV8Ndj5oxr3Gw4D//vcd/+t0T8tisRgW8kzlw77ixoqtenQdYh1G2Plxtx/WoPeT1euiDOKHh8+HVICJ6+tExW04xpyRxCZI0UfkUKfNEUszCp0yzQMDEumNVKom/k+1qrh8hHydPxISyDyWn5fmLbiZ70nhaDxcWnnw2dslNVLKMf+943kQd9x6y5AzZSjTuPG5Iz4mvFEMGzv2vUik8Y2kqZl6Pgy8ZXnn4SU3bu0/G3ew2SWl+EviHH50etNXRwh4samuYoV4Rgrog/Riu1sPl3dCP4iR0g7qgD45aEIChbqix5mpNIuPolEDuxfbis7uTh3NTFY8Qauzi3YPF42Vz0u5E+NVdcKJBa9bW2o/uzQ7EXl32TaXvLWsJ4fK68w6LCveXfLSw33t6/OPHi+u78WLtnp60jw2zgGs2tVmtx5WKNHS3C59f7a67cRcUlm824+3GCRRMITCebV7/xStVnH10TFWu2ZW0L/13DqeU95tpZlW039udBNmyBQ/5zKQMB3EZU/gqyWXS64jMt//onE05hHBK8DhXkzi1P+a+BOQ2HKT6UXkPyVkpB6z0ZoqNe611+S5UEwyRkj5lswzigjqCcMRbgPLRsEQgtMZ+dHR6fzbfjOMgfi+jKnJKGUUe3DSC9AeBDgX/RKvHBzPDtJhVlSHDJKqjV+9l8LLauovbftM7F0QE5atmAAoiKlCVfgzeixcNQVUkNHzvm0fNrJoAPQ6LUR821buH/HB5cDg/7sSHUBt+OGv8NtyshqfLGqP74m7sRE8P7Dun7YOT+Xv3Fj95/+jqbvjqavjue4cf3p/XB011WHeDvxzC1cpdvNld3wzX68GBdkEU4IZf3fY+yhhCEkRVw3bYvRnMUd0eNXEPc9lBsQcMOX9DKpdTCVTREnJHffL5DHxaytQ54mnQiomNzV6eqk4a1Op/EYRy0V2/VrREVk9KTE+Gm9UQxRTugVhkj1wtHhawx9gT/1TUTO8b9IIedKR654MRNMohpixThC5OhZqoNlXWOzQNIdttJnp7KbjmA01TuoJa9SfePmzMMEptyRo2hoNIP8hu9MMYnJfLdX+7HQcnEd4rw8eLOgj8bmwrs+sDxcZHBkOFKajcfXZz+dV6edLufeMFKHZDW5o9nM8ezP7su/4bj2Z//dXmLz+5uh7Do4q+dVTPmZ6J2IYeaiVcnd9ffOfR8nxZvd4Ol7fj73z35EFrLt/sFkfNbu0++3K9YYSaguXdxi1OqtUQxgFhCG+uhs3WedFmVgUNZEhEpBf5/PblvxUQnX5wZGyMLLH4KcV4JFtLGbkWrS0T69j3Q/mbxNIBPUFAJBNFjysxGWAybUN2jxAWy6KMUoJiyxNnlPSv3JSW5DDei08xf0xCRMbRabXTbqhjwjIoRO8z+SAuKKDstIL6isXktCEnIH0In61ujw13zqVUiYvZJ/0vwXdWeL4m6kEY9C0x33a86x0xHTettSyio9MxyDjKqnN9H67Xw+12jDIxMbXETcWLme0GTxysJQIqS5aNMeJVoTTejC8/uXr0rZNmbrUIBFO9F4Yw3g0nA/35z97pRhHR5ap3Q7jsez/K8Xz20fnyyYcnRwf24LAed+6vfn3zzQfz909nm83w819cnrx3tGSsnP/qtj84bd49mc1b+nzlPn69WQotRnnRucXceh9gFWDXAxANAcLhy83zv3jGFZ++f8hM+etMKFUHKEXLTN9i4NRMwqfAmas02ewK4Y6ldZ2q1AToVN9R5D7HgvVJkUO6UoqPily6Tsp9DokF0DKxA6LWqwWQS5ucTpVTsGrFdB/wQa3owsuFixUCsMoR64bQkU1n6MWsVgHFN9WdjfrSBzJRyCj2m/KYfIQWYtaUDmHSdETTPfAPe8YgCjpdNLPWeC8+iPMSgnoJ3RD60e8GuVkPhmnRWjeK82bRVJYxb6tuEGs8GyKQMVpZuEAgEqWrz1Zj79u51TxqVaTzwggCHJzOmoMWo//O40Nadb98sbrsxnbZfvT06E/fO2pOWixrbB1G+fTF5vyoeXLS2gp3u+Aqu6ioH8UvzMLZo9oK4ZPXu//05e0IfO+bZ6vV0G0Hqrh2Ehx81MUcEEgZ0nv89vbZv7O2osNHB8TxuE4SEignBUoyAuTOxBL+NdeqEj0r39mWxJFYBVCNS1+I2d6yUPxOCY1axHT9LKRn+0UyG8VUkc8ssihtUzTF5AqUgDdNfFKZFaAPmM8VIchCdRjFD8GOwQaZqc6DkhOESDxRvOxDw//Cmpv12GGvzVMzW8ypadqmImAFKVhS2DdEPxzMjx8dPTyZHS6qWWslwIuEoAJVVRH4IE5Ugq47tx0CM3VjuF2Pt9th23trMG8NA0xcWTZMAFuGJQIgvafsXuVVugWs0jd8wFkDyz9YVi+/2j277eqm/v3vPPgXf/yo+e4ZDpt4Ft/2zc4Tnc7si8vuV1+uQ0U/+d6JqP7q2WrZmsf35kfL5pNnm3+42HiDJ+cHy0P7xW68XXs/enUS+hCGoF4lKDOBKShZYPfx1Vf/5tnd5ytxYY/7TOIVZSwrhpAPno6glDiPpqVEST2z1QgzcT40JRoFUyKpdmJMWfeiFHKyeJKtMnP5DIwTD4ogukcgswZb8t0C1RF/ZsBDKA2hDrogvfWCoK2IEYI1DipOiEXieRKkADXQ/76x/q7/eBBp41cjfm3YyfeitqdR8gERaTpOih4Eet8THh3U22tRo6r9GLadd0FENYiuO7feudGLqI4eo3M4mfmg/SiVJRekrtgyLebVbgxrRhQnDasRsqxmZo1NSU8Srad2X/qh6sm1Axv0cvey++Xr9e9/59GffPsMHx5hWeF2hChq4PnwcuePj+zlRWdm5vZ6fPpuRUS7MZhRmkGXc/P5Zvyb395e7oZ7J/Pvv7t4eTt8dbWL2lE8fZxbJqfq0imeQcLgqCIeP7m+6H34rx4ffXBMNWdin+orUnCCil6buJzKZE0pdOaW3BJklZjTN9DljCs3RipgC8DkrBd5R3lyyKyaZCmtANhUtU+cV9O36WVVBCg9xrGomlMAHBlqPNZOGwk2AEEq1Roqo0CwNXxqKIjeeR2roDAE/ZnlJ17+j8tuNa+QNZOcnofYY07TeEVjlM/9Ngb40PGxZVzv+lGYMLrQDWE3+n6Qbgy9c6utu1wPPuh2F243vfdyctAMTkYXiComjKOKhsaak2Wz6dzaeCZvmUYIE1UzyyYn1fHZU76mD5T+21mFR3OAUOnfvtn+ye8++dmfvINFjSDYOEAxCK53r0bHLe/W7vykfXJ/fnnVyaBd1z86ag8/Mlb1F1+t/+rV5vKun7X2Z+8cnDX2P7y8oopNUDakrfFOx4jllhFERg1KgCxqtFzpi/Wbf/Pl0Lmz75+Z2tLUBRt5Rj4QGakgnIxvP1nIf9D0JrKWiwC1RZArfbq5/wxl5Yq1Jjlqr8iYwl+uZyIVXYvUznFFS60g8b2kNGhuCAJBT0AaNIhUgn4I5OXQQEjHAA3hvKGzGreq3oVAHEhrpj80Bre7z7dODutUmMougFRUjK6Ywn7UOlKCQ2iVHnn20MvP7+raiJD30rkwjNqNvhvDpgu32/Hybth0fr0bbzajG8NXb7aLWd0P3vkoJZNzAlBT0flR64KMwXedGDYhBEhsocpmRqky/Q3mf70K6EaEgHmFTX98b/7jH92DNfhyDRUMgsdLnNXqhvUa/d1QG37v3QWW1bGX25e7B42dn7VfDuE//frm57+5W9V6fNL84HT5FPTxZ6uvXm5HQV2TDxg62XUiFdXChsUbIgfvpZ1xxVxZCh6bZ5vVv3vRnjaHT48KIGmmOrmEk2wkhbO4JWAP0lLuEEOXZB2ORMNEXDQ3UaceLiXNh8TEe+Svkc3qRWZl8ZZlw8LUdIWCfShhLP6OlEQ5dzypJTpSBBFVrLxcBHEhNE548DMXzqDvsx55rXpPnZ+NchT0HZV7LqxW41bjVx7oFJpKhqHp3olCMJUDAxU4DzhUCqLxrEPnQzd678RJ8EG6MWy6cTdKEO0Gf3Hbr7fDpnPP3mz6cdx0rh997NAj4tF772XemHuHzdGyNdYyUcVwL9dXX633iI8S8ETpXy9a1AaXO1z1+OQW1v74h2dYWuxGbMdwPUAULcP7ax9mC/v4fP7tdw9RMTqvG3fKZr6sLt/0f/nLq5//5mbr/cJWP7l38KOjdrt1v7hcC6Ft6eigCk5EpTmAAiriBQ5Qo8YokxpAnAqCh3Yv1rvf3MkoyMkhUl4oU7M9AGJOLYElGmVJQXPEzCwqcnEpWSlK+qqQGDeTLVMuqe8Fvr3CeSmPJZDMYksJWHGfUy5jZ7PMYy5FogZolWrRmWiv2hsAZgje9X5G5r7lA69r74LXytCBxWHFT4jmRl720qWBT/XWAsX7kl4ZVz7lX98ZyYJGH5pK+6DBSz/IqhvvtuPdzq+3424U54IPGkR3vdvsBlVyIey62eClH31VccWmruADb/tQVXQ4q48XbtsbLz6MpNvw6h+vHn/r2NjU9/VE8D+PAQeCzYCKwYTzJY4rvNqi89h4nLRmCPASPr751ct1XZtvLhvcm0EUuwDR9rjFib646v7Dxze/3Y00r947ah+19ZOjqrbmP75Yr3w4PLRGYBUaVKEiBEWoMQSBQxAYSxWYKyKo73V00vV6/cn10Q/O27NZQYrU1KIqZe21eE3MBWhK56Zsh/aOYcj5I6fktETB9C1Eebk0SxpRUcmZXsK00qVY4CmngwWsvnZ7nTBvj901wBBkDBLGgD5YJy0BFfVsFtAzorrzYevG9Tjrw6mT8zF8iwDCxXZcu/LlQPsQivz4yEyDoCqpQ0Ot0H3hRcP9KIML/Rj6UbrR9U66QXa9W3Xuej28WfW36369daOX0aF3oR/C3XawTNsxOBdiJ4+CfZB+FFG9dzhbNNawqWtDTC9//ubuVadQiM4U/2rr8aLHJzf4/O76szv0CktYjWgrzCp0rn+9xdZJ79/cdC8udsfLCidzHDeoDOq4YvrJVfdvf3Xz+av16bL56bfO/ui7Z4+P6vq0ecHhi763TJUA2yA+iIRxg7FTEHZOglJdMxPVhhqb0jk1rAG2pvHlbn2xS2tZNG9MOjzlVZ2yQJTyy/Tmf6GzpQJgzrrLV7pxpqrpPgnThHIWURYzh09N9rhnhV+Lm5H2I+/5U4SiAEZTqBW3KreKO+gWCifNGNpAjaGjysyh1Hu/GnUzHvTh2Ol9L9+sDJy+WY87FWUupp8aB2JsjOYFiCpEBByfRIBG9YxtW1tRGZ04J6MPo4cPUFVjuKlsbSiI3Gzc65ttPzgQiaBz4eJ2pwoJuhtDEBBRbQ0zNZbvn8yXM/P4bDFvq+CDMcbdDC8+vRYPAv2e5XZZY876avvrrzanixpnDWoDZowKwe1Vb0A4qrYbtx3CEMLpokHDGAQ1o7V3d+P//p/f/N+/eEOgHz09/sl7B4/Omp0LL2+7l6+3P//13UBCHjQKE0xFXP9/7X3ZrmVJktUyd9/DGe+NuDFlRmZk1gBNVTVd3QyNGonpAYEQLyCBxCP/wI/xBYDUQCMBahqqKKqorMoxpht3OOfswQcz48Hd94nuT0CxpcyMPHHuGa7bNlu2bJmZ2Vxgv3PWghmtJWeo741rTL+yTWM1KSyZzirURB7ejsrvo65ClmlhuUihSvksqfYioWaUOQdbqi3VNqFLBkr1SFQpL5d9XziIsoe4gC2q7NniQRcLXk77XNRXzSdfLK7OU5LzQ2UkBAnR7ExoTGoMG8TILvCFM04phZROoRvSg5QeJXlhAEMY08tbH43JSW2VSlWLr59ABCgSAs2T5VTRMjWqwxz7xkXWEHkOPAb2Pgw+3Q3x7uTvxpD3+IGMiiFSZ8iQOY18GP2qd8PEgdUQdS0aZ9er5vvPNs8fbZ5crl48XjvXcGID/fK/vR7uZqf4G0FwmmFxI/z88RrPdkjltwRWHObLB13zyRYgS3h7Oz3Y9XjcA8BXR6QUh/Afv77/31/c/uDx9o9+5/Lpo+6r6+lP/s/Nd+9879zXr8eXwwwyZLC6bGxrRKlrzWbVuCTEsI5ES56GJGA1ChFo1MAyDJhO4u+9sBYWKqeOZdkHKsA21c9URrX8souu9D2FrKBws5VQyoZbgJaaYnDVgaJS/5UIrZlIrRRkQ12MrH6gcqLltIt11rhVE4PMfrAqi0r+iNZoZ31jTtYoUatKInPgyXMf0wOWR6LPDYHl5s6/PcVd7y4szjqoGrbrrSA5H6gfTPLjVvTuEO5OnkVCSHPicebTGO7GdHMMwxQDI0adgsyBkyggBFiTZYJ4fTulpAqd5tg4ssaseoLqcUrrzu23zfOr9bOHHaAQHb86vfvy9ONTWH15hJf5q8MwyuqvPcbTNQC88TgmiGDl8GiNQ8LM68tuCPr5wxU6B9LT7fjNb+7/069uYfT3f/Dg2d59feP/+Mv7//rrGwU+e7qyF82vxnkKClVTlsUZ6wxFDccoXshQmHWKysR5wwHPyRnTbVs4DUmMwXrjrORDFkg1rdy7dI6M76FgOhvacltrKW2fXdoSYfXMmSrqUmcDLRP4dEkmlhhdgzABSnUUfQ3dWp0olgf0bLbZI55fUVVAb1RvQCMQsxCYSBuXOovesTO3Y7qf2RD2q3ZrzE4VAtz7Xx/T4+eX//KzB/9sv34ehGOeZ6JaGnUrJ1w/aHUdIMAlAcgn8T75xN5zYA5JfGAfxUfhxAo4S5uV26+aftXYsocBRJg9f/X2ZA0dxmCNMYRV20SWu1MQUQDrvvn8yXa/bgHYpH/529M/vY3oDab4869OL/7SA+x7tIRNg7XFmBAYM+Mu4qLBpkUQO60nSgAAIABJREFUUXnyoMFhxuB/G9Mvvx1O18PzB91m1/3yzfTvf/aWLZ4/Wn/vapMi//dvh69fTjEyVHmW5BOtjaqKF1GgJbIKgvfwgzYGLCwEmoMjCUqjBwSOZbXvyGIpBalqIeLr77U+fE7tq2QCC5Cr51vC7lJWoqXGUNiubNEoTuwc+rJ7qKZWpydUXqzWqrJNVUlcVQbXRKFMPNOFMQEUAYgWc2NHawZjgqFEysZQZydn3xEOrCDTO9MYSiy3Q/zT1/PXEfvL/jHj8SHa3w73Xx39EFXO92Ghi0uqufhTQLGB6V0WYpYCigqUMPh0muLo0+A5hCSixphVZy/W7XbbG5vFxsYQff36eJrTYYwi6qxpnCHgNKc58Lq1IcmDffe9jy5aZz5ZuX/ze4/wfAPFn/zxt7/7vT0e9DgmBEFvsW2wtoiMVwHOwBncx3fH+cVHO0M4fXP8xW8OTW+vVs6x3tyF+yl+d+etTw+N+UvPds+u2l99ffzq5tRuLAyMdXbT0NrBGknabCz1NqkSoelgTB44TiDTtIYFJjFEjhO6HnZj2kcrk4kLvOdPSnCqacDSUZT72LWKGt5zLBX5l/Mv12KPUAKcqqBI6bWKaDS3BpXGtbrnCwI1VFrql7GKdHZroIUlNZDSX5nxYLFRqjZooKRsDRudFEa1EbSgO4NTY+d108+sqon1zstvQvg/x3T06oP8r68GFfnTL+9vdu7BX728+uyi3RLq5HKtpCKV5Nvk+60VGn0yQGNN31pRRCvCKoLd2nXJjp594BBDEhURUSEIQXKibwwSy7fXp6t9N4W0WTWNEhHNIQ3e7FZN15iQ5NPH63f363/18casO2yauzfDddL2sx0AtIQgCEv+b/DJGgJ8M+DNOEN++Gx1cxe++vb05LL/+PnuF18euk23V7qZ+NLZF59e7i/ahw9Xs/D/vR7nlFJS15mo6qOEOW3WLVSZERKrISdEAlU4Z4TUNNb0znQgqDFqwF1DsnJu31Ae/Fm9EEk2FqPgcn5a7KhCbNJaZfwL+qKyLBvvPzPbG6mqqx5OsRhNjZhLW8oibgFEy7hSlL0V1UtKKVdViSNqWrAUq7JpU3G5msd+g4SIjSMVb+ROMbU2bNu2YVYZRV+O6dcBrw9pGOL9yb+6ne+OnlnbziRmWPv4812zaspXLB+7asSr6U0h3R7SundoIaxzZB9kDtw2Zrd2qghJtn1zmsLg4zCl0xwxc76xQGJIhcz1Ydqv29tT2PQNyDhrxjmNPvWN7Vr79n7yEX/wdPsv/toT7Ft8ffq3/+W7n37vCsbAKGJCojKcyQu2DkoICZ0FqYtig7br5kcv9l3fwFCzbp5Fme6jWdkfXnRCen0bzM38cg5fvh6CaNNbqB6PgYU40qoXiRwiiSFlIDJCXjOg88xtY0F6HJIaGj1bQq908nLhJduLVHsq6eACtAs0P6eg1enlGFIqAhmx1PIo1ae/R2/mOcjlyQXlFCk/SnmrimPziYmpM16yheWAS4Ugy94zi8OpyL/yQJiFv8+tCUloAEeUk2SoMRisecUsjTMrbZ31kHmWL4b48siHY7h+N72+m27uY0ywRBth/8Udd7ZduwcfW9tQbWlTyttWz2oTpCCsmpLcBb6+n2MSH3X00RgyhL61fds21qw6s5nd2HN38rNnjITak0EGMen9GI9jSiyGqHFGgRQ5ilqi2fM3b0//+h+8wE8f47vpP/y739wc4u98ugEUrydcdmgMxMAo7j16h61D43Bl5bV9snZ4vN4+XuXEEIof7Np3b6eXd/6KdBjSd7fjeBOaR/jZN0cl7La27dxpTGTMbm+Pd1EU6KxpSJNIlK6zlLgxCBEm4mJDnZrDqENMbyesOlBLd6M8HkPxCKWMSapaWIIFO6nW/6+cKt4zwnze56qUaDW1epXXcQVPlVBI70Xg0jBUQjadC+tUKog1GJZ1VVrby2u6kmVgVO2/DOKFAqPqVFb6kFH1IAMhgwmmadGQOAfHcgzx1SQ3R3/9dvr2ejyeOJMoSjp62MTTL267B123bnZXvRjJSrNFgCcgQwKQZW2dBXA/xMMYV61bddS4LjKrYgqsknzU+9FPXiLL5FNIUrkkklqyu7mfTw9Xw5x268ZZMoQoaJ2xxhii5/v+Jz+6gjO4Hv/sq5snzy9WFz2chWMExjEACgZUsTXoLN56CJvPdnixxUUDYzAzUkJQ9GZnTdq2wxSjDdvEGvB6TLcTbzeNTYqkKWoUxgBRTUqcZAzMCmcNQJbIQqmhlUNrjSN0G3t75Dlgu8Yk6iPG+6AsakyJcah5eu2Py+6lxnpZikaa4W2hrAqTAM3lSJGqwlWtXk2LXqN2wFENdoDWLWDVVxJQa+bnpj09BydAILY8pRILeb6/kJIQFe8H5IwDZIkAIeMBAwNFVGNJWnJsNXgcIt+c4uvr4ds30zjlpe8LcYeYoIf46n9dO6LdZduubPdgtbla5YGG1eVTp2hBRGBRZ/Dpk+22bwD1QY5TOE5xDupjuj3FL98cxonnEOcgISYWyeMNazuqCUm+fnt68mC17m1ua+Soqth0tu+anzzq8LDHnL54fVrt2+8/26EhiKIzCIwpfvGru5nwYOt2IW1bi5uAv7zHZ1sQ8G7Gvb8dwjjxFISz3zcEwPV2ve9vfLq5jV3r4H1MKs4kkTSDKHUrN89xHtUzTAMJ3PbGtsAIjpJjzxT55OXdCdTAGgxeWDEfIrM6g8JvVGodlXqoq8sLY1t5Da33cXFKFYsV36Vn4qE8GXkfilapILKaQwtTWxmQCtwKvKqzwd+L6fR+z0wtLuTsxOREoBjs0nZZmUAqm8bzXPUEiDHJIga59Wk6pXc306trP09CS921qkoMwIrpy+ntzXfbZ2vbueuQ3vzg4sXf+bjbNPnmsKAHkfo60/Vy2+9WjXMkos6wQlk1pgTQcYqTV4UmMSIsAj6T4MRadqJe3/vfvjru1826ddbapJxYQpK2oT96cQEC3kzfvDp+9mz3R3/wBKsWb0c0BjuLEb8d5i++OzpDHz/c/vjx5tlHa9cQvj2+eTvc3c/3o78bwt3IxymNUQOZrmvWrV11jgydRAJge+OwUhMDoe2kX2ljLSuGiGaDMIEV5IgaA8/koIq+syHw/SG9OWKcsNnBueIlwjFxZNsYnONhzgNKz/+CpcoxY3FjeXJrsaraS3KeE180xCX9JC267YXnqurP4sFKo/wZVi/WRoo8qE2XNY8EVTFkazCtHxL1LgAVZvUMnkjLKD9ZGtqVCM4GY3AKN/f+7fU4jQnVvLRu5c6f0wEMDFMa5nS17w3Mu5/fvr5oP/mbT42zJNqLdmOyUVTyaj8dfYyDWGt85HFOxzEc5zRM6TDExlFrO2PiaJQFxCkvFFIiLWsSNYn+8pu7de9++NE+DwgW0ZBk39rPnm8QBImPg/9bP3qOdYch4mGPtyOm9Ort8OZ+HqboBXfhjnpLT9vu9RGSnPLGcrSQhtDDKqzKzeRf3Z4OM6sx61XnWsMCIULrwKoxrXuLIHHmQMpRFZREleCMapSMkPuOutaOp8AWE6F16C0MKQug8NdjGDm3Ny+5Yk068/maxf4WFL84mIrF33NllTlVza+Vg6FA4BbepFY+C/Q6iwiXwsBiiDXhUDUZl9UQff6DogzSWLwhAK2tWMX9mcW/EQiat8FrbmmhEORwG46nZLBsninTN5a5+VA0FiHi/hTSQ1n17QPF/c9uxh9cbh71DuaS9SnchWFVOU7xMIY5ptbZXd8MPiXRceZx5jnybuX2m8YQ0p0ME8t5aE6GvMtQWIqsP/vtTd/Yh9seQGAxgT/bd+gNbmd/mMeZH21aKGANksILLprffju8ejXsLlse+X7wr0f/WQjbtukac5jSycfR8xh49jJH9SxQtUZI+TTEu5O31jaNa5wzTSOthQgC0hTVaUwmzpqSJkJkWIG2YlvYSFbBiX3EvSIIdhs4gxggBBYgRE6l5Jg9WDn17BMEqCef/75alRFdhuop9L2xQRABGckHnevLxY85LZvQqKI5kNHiPE1JIPLIyNJWQuXuNqY40uK/qMCu6rRyMb5wHOUeMPQeDqxfTUjKuL4iIyOFsPghjfczZZxaGifeAxBY8g8YwnHkw8AfPQJAq6jh5zcf/+Sx6QiRRq/NyMbzFy+Pb+7G5492D/fu6+vxNIfG2q61j/cdTBejiur9GL+9HqY5JOFCA5ny8UGFqATpOPMvvz385IXbrlxMAqXfebqGTzjEP/vl3a1SmtiJoLM4BvQWh3g7+LZ321WbJF3fTJveXPaus+Y0x/sxHCecfBpmPs587+Mw82FKJ5/GIEmE2YTE05yatl2t1TgyrWUBaWMgOmu3gyPjJ2GGsdBEURVBTQcf5DDjJkIZqx2QYxiZ1oiJyoGhxVsvfqq2ZeA9fLXEJSpWd65D5rKVZmyS/1TMTM96C1eC4bm4UAoGCwulOR7SkldAUSpVVB1b/QyFt8it5Foi9gLjllR4GR5icktWnbVAKkU5rJHHex/G4PKwjZxdG5R1EPm9skTIgBgpqY9sQNtNc3dk+b/3W7R978iae+ZozOFu+t9f3T57uHn+aA3FO5GrfU8EZ6h11lrqG8SYvrtJ7w5h9LkAW308UNZToHx2gd6dpnfHeb/ZqoqPsneAKBp6/Gz9j5+s3ZMVvCAILAFy/Wbk1lxcdJj4wdqerlZPL7rW4jjHwykeJj7N6TTL4Pnk+TTzaeLjnI4z+4QoUJW8NiBMPkparZxzDRriBE3oOrSpuZ1iZDQNmh7UkM7qLJRoiHqMMIR1CwcYB+MwzQqFJo5TEhXKVFSe/FObhUpsQoU+C2xbai+ViniPzjobHVXKTQAVuDOSglLd1ZSJ2WoRpX5ZBgEha7UrlNOlkRMgxqJhLRYlKC2/1aXVk9OFf0OuSJRG0QwhU+TpGCiJzZ0Kiw69AsXymwAgMITO0aZ3Irpb2dnbGGUcghVtrO2dkSRfvLyfQ/rh8/2qdcMcP32yuVi3kWWc0nEOr+7i7NPk+Zff3E8+GgPmGigJkjcOw6hwFWBRSPLuOD17uFq1NgSOB4+dg9DnL/a46LF2ODGuJzSY3/rjnC4uur63/vW8vlj1+/bRvpkCj1O6n9NxTMc5VjtLg+ejT8cZY0BSFSmkgjAUiCOnpKuebENsjSQ1UecxDiOCYLNBYpos1MKAfNKbEYGwbvDsyhDTHDgFckah8AHH6+nqsz1ZWzrnVJGHkUgJkyQ1/yqcQx6SVhM7KNejzpRbjm66MG3lxNUt6KtWLd9rHQdg5AzXsLz8UqYmQp6smD1URWi1/QmVAFnY4awQK1tn65PzJIfspnIyK6zimQBjVLlgf6PLHvny0vm7t5Z2K7PqLBkyoM2q+XYYX74bw35lDG17S0Rz0M8/unj+aOMMrbveWhzHdHv0xynenMJXr4fD4APz8RStta0zDhJDigkkQsgbdwm5gqFEJKx0fQhvDnPfOA4cx4h9hyEhATuHI8MoesK9v72e5xDbjmJQYSFHz/a9hd4PaZirM/N89Hyc0nGOR8/HiYeAxMoKqXghrxFWRRwlcthsHBmXSGxSViSCbcABo+qaEANIdUiIQGuxX8EpMaF1lBgiZBozMY6vpxSk7Q1AFX8a1HhX+EPNwycXoF5SgJLbqZS5slpLAiVCooyJEVWQK4RwtlLUEaE4i/zNgojyP4K69RzV8qrvyx6sCrmREXRlNqpZKkBCYlC2Hi+sTA3aKM16NQmisiS5tr6TluFoABm0xrRNs9vY7boDhAVdY42h45QalxLLYTDOwjnz0+9fPdp3MekU4nfX869fHl/ejDFJUro9zqchhcQENWCycEZN41RTEoM8ZL58j5KOQXH08dXdvO/d1tFm5WANLlfQhJHhE7xANIjS1ppBJPE0JLttms60jTn5NHs5Tuk4pZOPJy/HOR4nPnoZvQwBiSVXByTTovVwGVBGnERNWq9gnIbGnGZlo45gDBoHECXWKBgDuh4bwq6zyYv32m/suqNhVBZpLPEpcWC0ttCdClGt6CvXoQumkeWxnEJqbhSRQoRVyJYtUYSyGrWgf1W32OzCuxZ7pDrhtWrPqg3k4kGNqljY3fIUqtGwFs4Lyq9cRNGwadlOdgag1XANkZrOrj9aT69W4d0oUDJErHou3hMB1sBYdKv+4dWW57jurQ+ILM6RBQaf+iZEwRx00zePL1frzt6c/O29/+p6+PrN8Pp2ZpFnDzeXK7tbuXcH//pm9jGmpMLRWOOMsYaSCDJ2sKYhjayGTBQk5ZhkDnx78v/gx/uPP9uiMWgI//MOT9foGsSEKDcHHxrC2mKU9VW72bm+syHKFNJxiscpnTyfpnj0afB6nNPoxbNEJpaq2SyA5+zPkgKC4yCE2LTNIDIHbYCkMAZkiVWZ4BmNQSNoGzgDNJQm9ZOwJbLaGBAzH4I/xX7TAdW43sNmuQwuoNy6jgXWF4uhnBxlAyuof+li0vcaVlTrvjpUGI9aYqr0XEH4JRFVaPZFmYA4u9NiJLrQ9VpEkwVVLa9HKAhvse/lzQE1xqgI2c5dfL6f7+Lp3UwqFiQGJEpl8yuZBoCxpFBt2mYa89R0DJOPrDcnb435zXCaI2/aZrfhq93+l9/cN8786pt7Y0zfNZ88MQDtVs04x8bSxbbtnLsd5uu7idVwBJtkjCk7UDV7VliDwOKjTElE0Fv6O5+s/uEPN+gNjh638/2QLnKhyuL6Lrw8BekMg6nFemXJ6GEMo+fBp8MYTrOcfDzNfJx5CDJHSSwsYFUWUuRB6Zo3DIgiSdkjppLhml45dRaNQ1KEGVFQCs+M1sA5aEAQHIjFQIEU1ai2K0ssCJhv/XATto81L9DMnCqq4Esy8FflYgelPlIBkNYcic5GUtPKapT548MVl5el31VrVIymOJ+yKLfC+CL2EiIjeTnKe4lnmS+WMYzWWde6rHxfpjcvaQaWikaO1KWMhqZrVptmZnJC/dN1v2utVb6e/F0wu+bJHz5rt12493QM/jDHJv7sy9tWOSWZmETBmvK3mkNilcPQv7ufnjxYidJf+fRy8undYfZR7o7+9d20X7eX++5qa7vWpKSHIaSkImVjeC7T5S5FIkqqPmpj8Pufrv75Tx/+k5/su8ZgDDIo9Xb38fru3dAczK1Pr47TZJhTFJCyBtEQJSQeo0xzOvk0eD3NaYw8epkTRFUE+X2lVoEYqnWdHmc7QzG1yUNUW0cnC05oOwjAEZJPzQB1FzF7tC21RtdrcgLbEk+m3WOY4/H16dEP9rYjFaoGtmybM0tSiQrYqDKKhWnTYhHF7KiUR0t2ULwcucxb1Vwwg+s6qJYW11edKYozKnZFNROlBagt3msJh6VcViqmpQj/F3QjZdZPmf+jmssMraXWEFbNw999uP14q8fwzX9+2Xz/4vlff7r7ZGOsIyMUQQc/fTu8+sXN6dt508CBJjZ5CVpts5FhTg93zcWmu9i0Iri+9zcHn0RV1Vm727hVY4nwYNOobkC4vZ+KBMqQJWIFIIbsvjc/fGQ/v3C/9/HqJ8/WLx6vO6vjmJyl6ylNB56ZA4uoRJE5SmANiQPLHGQK4llikjnqHOMUdIw8B4kMz8pS6oysylq8h2RnJhAgMTibWl3xpIKUVfCa9+kUW0wM24ATjEXX4HJnO9K2MZa13TRpEjhwr9oTpjS+OUUfTdvomb3IBmGyw/jzxwktxczK7gNKQpLXSeVYX4jYGolJ8hxkWTQJOUKYzL5WUF59VSUlihNbYBeykyrzsqvI4b3gu/QUVzSb3WNtraymTJon0CuIICpGzbbZXNr22f7ixa7r3Xc/f7f64YOPf/9Rt2nPkdspdzbumu5qdXozn6bQ2SIFQZnVB0PELE8frj96uHpzN7+9n6zFx482q84aMnOMjbU3x3n2vN+0+429H5rDECSqqoi4xuqqNR/v3I+f9L/7rP9073pHrbNd341B3swpRuk69SJDSkl4ihqS+hCHoD7ynNgn9ZHHIFE0JQlJA8scJYmmJIkhKqJgIcnEuBQ7U4VIMS+uf8hqCc1MAmuIhKhJ4AOYwRaqiAFWse3pam0uVs6xqjXU5KXXmoRmleGkMYncxei527aLo0KNelXIWBxZCXCywP3yrwp8IEXqsLxANUVRB9XCGRT4T6i1RoiqKZsiatYJyXOKjcmLXc4kcvZoZUcnRGAynio8cS3pZ98meaa5ihiqPcyiUhfPFdauXbvuYrX7ZN119uZ/XHsyn/3BE7e2Z6dJIIVpbbtx7qpbPe3wbQKE1ILyJLhK0hh9crFyzjDz86t119rOmcRyO4TThPthuh/itnOswkkA9C0IjqCfXLgfP1396En74qLZd6YBgmIKcopkY2gaYwhCOM0pskwpzV6OPo1efOIpqg/Js4SkPukcObFERmQW0aQQ1mpARkVEVap5FX9WXdRiZMWZKRJjtULb0DTzzBgDctXSGSSBM1hbPNq5fW8aMuwjWZLGyCzjzL7DyeucNDI0xZwVKkBqinyxYuwacs5s7UJdVoeWlZI5TyjWU/OF6tUI7vzzKENoTZ0przBGJMu29c+VLpePhTwNAEtBKkdEBcoqFNXazZdBoKjk6VtV9V3H5RYgmQ21uG4SVejHF/0nd+mLU/r0bz9t1lYVCqba9S4GZKm5Wl2sbLdvp49O8d3gr0MYREUYREBiAyXXmNMYHuzaTd+qakzy5n5+eTOq4Grffe/ZLia9H+aRxZJ89mD9w4fN7zxyz3ftZY/OkqiOQW+9qDHOuVVvG0sEsMAnPnkeZ55i8jGdvE5BQuLI6qNG5iAIiUPkmIznxFyOUpiSZm2IyWgnA68Cw3PEVIgiKYTBC8sgUODh1qjScca9h49oHZzNWQA2a3q6s/uVZdEA2NaIwTQnY8gbvZ8wBY1AYqydNS4HR6lFj/wiWkVo1TkpaiPGkiyUtztrgkreaeorFFN0NWhJXgj5nickIhHU+FfWxSkWB5alWVQFJFj+jpY6pUpOB+gcXKuJkkpNPOodUhUomVcTVYnCjG2Si4THv3fVbdv6NVC4Xcor+RQEs242nzXr5xskjUOarsfp9TC9HuPtzIljSj6kyPJg2/ooPsTX9+HN7fjkYvXx4/XFqoksb2+nRyu7X9Pf/8g83zcPerNqDCedYjp6jWqUzHrr2sY21hBRjHwKPPo05XqRTzGxT4hRpySRJSUOQjEhMEeWyBo4xZThvIhChTjblhZVvVbyIns1FiRFEjBnLu2Mti936Bu6PqZhAhSNLW3flkCEhrTvyBjc3yey2G0dqx6P7FqaQIOXJIiKJLjYtbbJxb5sJkulO6u6awunVF+xZJjVY2VZIVd6o9BwUtcsqarWue55P092ORXR63s1IlpAezH2YklL2woWHIZMaeSVaLT8XmrkrnwgMuepZcp/4Wap5hdQQL1wCPL1r+9+/npq//azbMdFbgIjEFrUclLenhpLDbq16x71u+9dpFOYb3y4mdXzlHjtnCj5wHdDOozhxZPN5092jYEG36X4fBcvO7ponTVOFD7JzSgslGCaxu1a0zijoJBkihKTTEFGHwfPU5AppClIZElCMbFPkkRS0igakiSRmDQmRFYWTUw1JmpiZBVe4cVzlTAbmZZwmTg7FRBAFl2DdYu+oWGW4YDGghRNAyZIhCXs9rRuEaMKcxKFwCdJLMFrUk2AM2SsQkGM/rIzzhY7yw0gCqgUivUcO1Ga00viuAhrlzEcJcXM9ldroyVDzUMuNRMKJfKdubqKlghZ6VGxm1Ybek/4qOXtiRZjr/G06iBzPSHnAIXEBVSk8CJZxSEKU/JnAYGTv/FW9PDV8fKTnXF5K4to3fWj5e3zXYI6uUU5KoD+Ud9drcDikvCr2MKEKFOI3sfn+/Z7D5oLnfoUGuK2AxEscAySRJOSEjXWNL1dWWMsLBBYp8BTZB/ZBxkDT5Fnn3yCTzz5lERFkBQxcWKwio/KIpHBzJkYSzntX4KjQKB5o945EqFaWHZmAlU0Fl0DY9BbOCB4DREANj3mGaIgQePgDLa9aQxilEC02pjIPHmOEZtLO44CSNvaxEKi1Jntw55Ku1gFXTmCL+4AWNiwxWuUfmKt7VJLPKpS3EyKSDHMrLkEFtFELTYuQGzR+dQR8iVq0tKeWxgQLOmolEnghYQtP1dq6pSbT/S9ZSbF8A1VvWO+d5XayCZyYGx7992v7sYfXW0fdQpyoD0LGxpUpdQgak3VGFWFIAyhXTeAASk5UmMDxWmMfvQbjd/f42qNzo6OTBT4pCdRZ6x1BgRnTeds09jMtrDqNGtg8V5OIWXINQceg/iUfFCfJCTxiRMXhjIxBMqs1YFBJC8yp1JHymJPKo0MMRUeOJ9axvuZoWCBAVoDo3AKP8E4KBANRo+mgTOwFmEEWaxXIIWfJQHrtZGoIVGMZCwxw7IqxCglkZzAdZft9vEmh5szv5VNTlChDNWyZrW9TPZL2aIiWliICi1re16uXatA4Raolu1Fi2a7pqolpdPKlmEpmJa/rSuRix/M7q12B79X9a7JQ3FqVB3QYo85N1naW0gS392E022aOTx56NIhTbfz5qozqn+X+e+BTx5vO/cbwm9h3pFOucIvBVqwF9pSnGIcQrzx/GZc382mp8dre7l2PZkpwCdqHIwl2zYN0BTgVYoqIalPMkdmFh91iilEnUIKCZHZR5mj+MjZwpgliebjk9oqz0KpWIwmIVZNCVxoi9K0w1I8FhEsASjhMimYSwq5ddgaoMGQwAxtMDOQVYUOYS6Opu+QJ/fPs657ahtMiY6H1HamaZGYwwGrrYkJPEm7JhZaf7RZXbQ4p4eLO</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9abMlyXEldtwjMu/y1nq1dHVXr2g0QAJchhxyOKRmxmy+jExj+qYfqm/SSDITNTOSTCYziuQQYJNAE41Gb7W+/S6ZGeGuD+4eeRumXyDrC3TVq3fvzSXC/fjx4x6RwPev71/fv75/ff/6/vX96/vX96/vX9+/vn99//r+9f3r+9f3r+9f37++f33/+v71/ev/7y96/MNVSlACgQACFACICAoQYH8oQARVYlK19/z7BFUQxRcVykSqBAgR25sHnwTZofyI9hUwUbwFgAnafm1nIiXgO4eCElj9wu3URKx2dUrEgNihFAQI4Ffq16ukpPT/cRd+IiKF2ojUIlSUAKiC2C+aiGDnUfjowUeNUEWLgtluGX4sbeOLuHUlYti9K5SI7A58JtTPeTgFiIv2gYEQEcS+plCA59sF1M4OgoJI1WcJBKjdjqqdBOqf9TG067MLVz80QVVtUO0d+4hdJvx9AEoKRdXEBJCI5D/5bz7IfQJRzCFTGziyq2OQkt04MZFSDGiMOPudUcz7wfzZ1BHgUwJgPpYqmNimm8zWONmIsJKwDRFsLv3Q1Iyf/GrdOsw7AKLwGvsNQVVV5ukNS1S/XiLMN0t+ywpiAgDVsi28L0nJJwZqH+REnBiqSmAiv1kmZgxFBhFiAoXxgN2cSEjJLkKhTAwCKSkRVNSvwwcKCoXAXZPMEMJHfQZUw04RA2G/lvZ7AqDipgSBAGZy7sbqdgaoCmn8U/0nqALVLk5VoeqWDYWomtFB7Rt+ySKKURZdVqJpX3PuU7/MILtl8z6/B59TdqOAO7MS2TvqGBDmBYKNKNn004xBPoVudAYWAJOZbJt+s5wwVbYxbzDmh6LAXnMnToGDfjVk5mt+7v92LwNYScmcvDlOmC3FgSgsGAQVkCirZoX4nfkUM1PKJHGLzAowJSQmKVWViQ+P6vYRHkrNXhG+oyog0kAdmFloshG2MYSqquF/gxgAbjo2ColQlUiq2PtmFQ1NlQCRuAuzN4BUoICKEsiMVAVq0CRQRRxERQlKaidUUZCKHUlVIQJA7QRdn4iZVLMDfgN+igASvwGUwg4M8GwIiFgd+VgZPnlsUAAPWUTksU/JDUvBIAVS2B5ZsEWLFxZGHWlU2/Vp/E1wI7Cr0QA3+08EWkVEEiMtUphUAJTdnDuLavCFiH9xQGpUwYOA25z6BatCVatE8GMVJSJlIpB/OdxN1W4hbiuiKMjM3GEKTCREpMSsFQqNkSCKCMIgifBi0c39kM0kAsvZrdHObD6HCC3BWYJPmIkSEVDBDFFiCssNfKmiICKJKMaq4helIFYVu0ghhordbDMrZEeRGBocGBk1SzN/5HBNtekgJptsjXhGhiIWExtEsJEOM1Nmclu1mBJWzcTmtFCjgC1qtyhhRwg7cL9QgEhFiVmhNO3q5mZ/92I37qbcp5PHq+NHy8UqI/lA83xKp1fOS316AKcJqs3j3JCNHUgE2hYQDz9EzBH4mMNMzfEZpOzI9h0cB+M7FNGuUpQ8KMygZ2bTWAkIJOajSkrCygZ4pMxcxbEfUBIKpufHIDFrAZQM6FWUwaKKBBUPZyzkXyZmFjOmgPQ2LY4KQMwzQwWB3kpE2a0sqHmgmoDaZDYUUTDI4IgCtoHGwxXggAONOGgAxRQ4GBDkNmtsjz3oslkaOx56qFEGxFm3mdqhdZAAnBgidPdy+/XP31x/cbf5ZidDAVP3oH/0o/PHn5w/+cFpt0jNV+bswR2LiDFDKiOAzUbS7AZUg+yYwVNDeucbFifB7rkRARBkP8w5fMYCPGac8wMzVBiA+Z7zhxm8PdcRn12jbOYzgfxCSp4EqSoTiwFNpCUg9ujMgXJCLdMT5zZmZERQ9euM6OsGYx9HSyHsKkSVmKRyGxjkALD5Rayk1A5FHCYYENvIvc5B1/EOnutFtGAcxFyK8ATD1JZvOP0zyA9GbS4RfItASBYyEec3rkUJpHWSN7+++9X/8c3NpzeLSkuuY0ER2lzubn69ffHZzR//dx8/+eDMo+HsPH5tYRAexDiC6WGMYSZhqEA9dlrwZGL3YgKQmNmmXZkIzKwRmmzWHU4NAZigNvkRPt0uFcyQOIp6NIE2ktb4DAFC7LlC+J4Bs1mfu4G2G45IGlNkJ40o63/ADTssHKwsqAEy5hhKIFjmogzjlW6KpAArqisO4Oz+6DkWHESICUIgZT4I35EMtdwKaMKCuR3Qht1+wY6sBoc2mvYRjxffyQMMWQP5KDhIzCLN9uBknx1WX/3q5rP/+TeLl/s/f3fxZEWqshn1fsSLe/nmerr5fPv8H68fPjvKfXJ/9vyMiTQ4ot2WthjVBAJnPARiliKNy2mQOTKIJSSyLNqJKQPKYHenoBCu23BTWGYbD2xk55NggkjjrSDP/iEAg3V28vA91z0oslENYtcsjAE12BIlRsvmxQOffcYIwexrkfRpTKUnCI4JFElxk67ilGYrNRus+TTObq7BoTSMIEzRw8x31I+GT4hgYwdVMqJmGCHNae2COZhdY0qwLzVSbudp1kpKyuD5BHatm+vhi//z2+759i9+sP7oYrniUipUaVK82UzfnuMfXpZv/vrFO7/z4PGHp35QkLIkVWdMREx6yJAoiFGtElZoSWxYUdi7xX0iMBMly/XsCAwGibbL5WCuETYDP+m7M0CkqszuCkTkdJ0aLHrWy55CQ5mhopit15NZo8nGTxSiaoZPghaFTblUJgqfMnLWVDgzsjl8uXXBpDQSnzIX8jwdMUdpjMAzwDl8zJTCb9uVKQBMkdlEnPVhdpuId2aeGt91k7MRAiAI7huBKT4TsgYziCwHCCSzxILFPeUgTbn+enP/2fUHF/ntk7RIqgpW6ViWrCcdvXPMnzxK/avx1ec3LR8hAoPBSERmZPAfiAjEPhTGiUIc4MREFBSXPeAEIhIxJSdnRlgULZ31sx5KfWFrHNYKGKXT2VPJTcQh1YRRH632PSIYUWGfBWfWHu5hPABExDG6/lGbBQ6c4xhaQjtys+8IV0Yf3eQ5wpHhTAtNzlP9P4Uyz+G+GU9YEMMkWDAHhpm1xdDNKXf7IkCQ9mkDjobaRByIQXrgwnPkiIQ2aFQz8ia9HsAvgxhacfXVXV/1yXEqFTeD3gzYTqQKBghapR51eLRCrUoEIjUzghN3+5nZkUnbFKnfQdwWg5lN4IbCQggRKYJ/O7mEiIgJltCwK2MxCJD2e2DXlJXipAcOryCbyYNZ4WY/8LzZIr0LxcZhgqeFNhjhz4yEmMBmpn5VEY4cxYhIORRck6U98WK7VeeM5IHTWJPLcYx5wMIPOeSeNpARBrgF/QgRzExuwUyk7N4ZqEx+f3HbbmmOTeS8Ij4TBYbZU20cQxx3w6QWl9v8uBc2BgVSxf52POr40VE3Vt3u69Wm3E9SNQnl24mvBt6MtF6kzcvdcF8cXKjNnM+ZWckBxtpMBVMmMCkRUooBUzqYQPsCmwU29WEeCLdNhptHDLhHTT28QeMtSmRXxc1+OeyLmZh9homJsUj5D88vfnByzOzJ8oyRbBn9d4DuAPjaiIYXGx4xKOaeQnMPiNKD6Qu/dHAKmktW2EPwEuW4xxhZO24DTj7INH0M2hfM/Z0lwNHoMFmzYEIhmjXbVPZDMUiYOAaYAM+fgzgEz+RDh45ZZwKBE60f9BcrWnUMkaHS9U6GYRKVq/v93X5kcE7EhFd//frrT6+kihs2U1ASm/02BzxPuYZRhrczU0peGPKLZvuCMs9EgqAWENmhxkxFA4uVyCWDhtEHYRREKXzPBlEiCqkDaKQvB0hFKVOMuQ85O6E2KzMIUHWVwj1OOXya44AOdKEBcTM3pwEaoBtzhEME8woDKSkA096QPU+FhnxDILA6orq62FRc58Dqo251kkCjg+AZoceT6+awaJfUfNc8QJ0ruF+oxxpqxcp2E7PP2x8Jzx6vy1G3yJTAaySpfLbuFqwvp9ovljcbURlzYkCk1NnRfVZDtCLXfwChVkkkePXVdI2qnDgJSKvr4o1mMIz+hJc26yGGehmWTMyKI8M1APaT2EweKC8xDhZaORB8LowE3Ryk/t3NpUSSGAJbA4jI9B1Exb7oX3dhzsh+nEwPhDr3smrRykbHipwkaF0VoWjYfDuma6BLNgMMvIL6KMeFqpDlrM1QvKDXUG1m1u0s37HvA45gnsDs5QwCucJmbgr3LKc+nkewXzU37Z5C63CQfkJIF11Kusod1fLgAfddKtOUiFZUL7LsmO6A9//1O299fJryHKlbChJXGoeOckXL3R2VGKqUMxdDLCJmgJkZKaWcLOxDrBBFnrK3NNnUiPl8Phg+VAQ1pPV0jdtdUggxxNz6LQxLXP93h6YoaUFZUVvaR/G3Txp7zcCKG5ZvunopM9qqCghMJHY+DksibblKU7IPYKUhLLF69YEpz3FZGw55SqVQ10jN/KGMkPa85SW5zHagrbdc3KTUA5ALq5lJPSInDdUluJe2zg+HbjeJBm5ErYqjibBYdKK6XqROdLOv20mTJIUeJ1qucD1ht1w8/pMnR89OOM2XOjtDHLOJdSE+aBs2+715Q0pUq6VtAMDMKREzM3t3CxE8I40kztU65yYSZuJhala9TBYLPqQUBSCzeXLVPZhwyOXsbEQPHIRAXsGbfwkyNYIV4sRFw3oAiLbCcag34sK72JixF9ptiMTJRVi4MnGVyko1WJcVWigfTGaMh7cyMJPMobRJLabFOcSqm2MgQ1TWXWSh2coCiCJTCcQSb5ihSDubVDab7Aygv2UZNiJ8scwdkep+nO6GWjltRuz2uh9kwbLs0CE9PV3oeS8pkJyadxDaxMF7LMy0QfLbSheDKykrKwubXg+Gl87MUqzzxgeLY3LCy9v57F3y0Y6SnA0OU8RwskmeIc9HVQ88NTQzq/ZT63lDTE182wTeCli0I1UfAJPJnKoJItW0qWaCSDB9UaOULTwrGQaHnq1qQqnnvNraIDjoboMKDypMCkqNbHq3jk+BA6zZl0cLA1tELjKHNw2B7VCKi5mOHoUgaWakcqA4wOSYxjss5AUPBVGqj1Z6tixS7/b11SA3AwiUmIT09V5uRhlB+niFo+zX50ZNmLmmBrvF7HIxugbObBVyAhEzI1GK5gV2/YHdHKUl6Y0h0QGpt4t3bcX/zex8O+ijCUqhzBGBwC5/ETHldmnBUoh5zqfYk5MYMPWZCVw2Cwyk8OOHOR94ogUc7+X8blIcB2NE0duklQOlyyqWBBAph+H5PLoTeeCVRlrarMYlxQHZYk3DAedjftFNWiJ3yLjPeZCtyBX/buAhDe2jZmW/CIJDUTkmyNlyergeC0bV7YhfPN9ejloT3ezpzVZvJ2yJx/dOpU80fxcRr/ng4mxQWstbeA88lMJ0NpvUpEScwoYsx7NvuapkWhNbMITZR4yNDwSHsqNmJhzD65/j1snkSV+IperCqGt4nAgQp7CWjPjkN65JcVgFTHBGnCkYAc2j6tdHDYYOPgrTrl0uIXL5QFvpwac3sh8mi5seDGFRTMmlWO/1aFWWMEU1SYZhJdQ5kGnz3yjc+ijEhDEZAQhQdptSATGiLZE9rVKK0qjOQ+3egTna+MiWi9W+as84W+ezvh8nScA6U0ESQn28pvdPI7NvwTC004PmWScIrHORxD9JDBIv9Hg84VZTYyYiJqGmBbjU7IY8S0HUaIOXLr26951ip5L3+0gUtkEaeh0r0CrqHgTNoEV1nkkQWLhptlY0FLKyl5B3IXhl31tLrO5pecysvoYl+HGaaVivhQVbca4VkCUecKKbl7LR/FbvDnrqBMvfQhAM9/mmH5nhOb9tB6WIfGFMoUYqkfdvOXWcbd+KzoTIXigq9+ZG6lGkpQcz8oGg+ng19J0M5WxJJ8u020AUY8aQcJdz93tP0knXppFiSAhRdWlG30aK3MLNYBKDEicRZ+YKSclqKZyJ+8RsHMRaFqJvN45ieFGryCTTJHUo/arrVmypt9Fa57zBClhihB2Q2uDSweDbzLQqJRDqB6LfzdcbOBh7Y7hSDSCGkOUEarYqNo0cEUVZSCExcPpbeG+jT4ENzk+VFeI9nDZZ2ZZr+CW7+CEu6Lmy1mpXIMV7x6eZ6YvNtXpjiKUspAfh0jDCS4bRqhnl10DpFkIPYukBWTgkSM0E4JTAdBAXbVUmvXu9PxbajnXVsSRBj2ECdbQTkp8+PvrhmfGdKGQagqpGcG/Cj0vNnt55cYwUOXFimEKaoQBlEJMyIy8yJ65+cQxUZlTL6eZ70WmUN1/fv/r8VorkPtVSz58erc56Zj6+WKZMqWd4q7d686+ScqRMFj20BXIlYonikJdT7abMFkNTRchukUJGTU8NJEFiCyX4APQAhdjBIh8zjeQgHBidFj1YAGNBSVxkm+0QhOznU2aKBQ0I745I4j0BxER47+RskdNX27uCimgNVke6puBEbT9Co1McZyZ+2cHh5o/O3MXvWYMjNcpidAGzb6huPr/98j988fu93g/1ZanTqjNn2VXccXr4e4/yKku0Xruec2BaYdP+4/yn608E1a5LRG3JDFvvLhGljMSut1tnqyhz1EAMlgW635Q3v7n9xX/6Zns5IFNaMCZ89dev+1VeP1qtH/SLVffBHz0+Ouu1hQ7Mt0xo3UQHDK+Ns1EZlZCMwltFWrN85KDejxjkxuzRk8+DOTQ3M1hueOcsCgQSt1GbGlvv4vamcZQW3QAC5SYnhKrQ/tWoCSJkqRL+7vXzxFQcC+bpQUPv+YsxnaF8ekYZhjNz7Rg5ptnUMNPOSEK+Y4gAoEWGV7v7v3q9+2YzvtOvcvr6evfyugioY4CpHC+3V+Pi8YqzUdYoJwDNF6LjS4iaoI45OKgSocte/ITxbG9XVNPMYCVhJRAyU05pqsWvXnVzOfzmZ2+++KuXt1/cCzEPRZhzhlYi0tsXW6l8/v56cdq9/5OHeW06svNsQP2imgRjEpfPYZjFXAiYiQ2Rdy+iRRs7ktF2jaH36GY+G2HRrQ0mhcW3pfGAMNm5cECtz8TELa9Wm4ZD6Sf/5mnKnsSRjZijhUs3rVXbJMdR616E3e3nQHfgZ0HOES3HRjg8EHrkjHYad9xY5WRap6tEHO2n/p4TEFKRuiu757vbX9zsf3Y1fbs7oTqV+mDFx4vUM3LizOhYteiXX2ypT+uHy5S5yTNuL84e7NUuPS7UwoSojvUop5SZiRIzM5iZ2IHLcm1i+x+IsB9kLJI6JoIIvv2n6+ef3bz+zd3uxVi2wgKdVAuoQIpM96Kj1jLdXo3HDxdHD5aeWh44GofNW7rJGhWSFu0RCYDnW/Hv78QZs9Po6mmEpNUn55dZIAMacZjReJK7QKvTaUMbDaY250JV+8y1ao6TariwAWjk8g3FQ4I4AL6ZjR6oqKEN2sodJWo5DyFofSR8kbyFdmCfmsVh5yYx6Cpad3V/Owyv9sM397uvdt1eu0QqerykNXOXmYDTE96OdZhAhP227r69//V/+BKqb//xo7TMfpFW2fDyJjsImODTZE6CikK1T8wJPHdxmRFaE4D7fQKIVYlU0GWiAaoQxc3r7asvbr/+xdX+5WhielHkxFJVCcRKAh3r9qVM5farTy/zOj9+95S6Q4yYYR+ipK1W6jPMUay29T6Ir/iQzVEmKgkciOVTGSgHiTpoxL1YAKCHBINBAiiEbM0TPMNVImat2rTqGFFm0jzXPJoCDyvI/RbTOsjQESHogEaFz0TdxjKWsNDI9MxMlVSil+AAD1uG5jrHXKTSUoercXix2315P77Y6f0kBaSUllRFh6kW5nVXTxe8hY4Fm8JdElZ+sMY3Oxlux9f/6dtulR79+EFadVZPs24BE+fIY4Qn8KEEuRfkzpUvjyoeIDRigPMDkwDAnJMr+lL0+S+vvvz55e71IKP0TOuVN0tUm3ahqaiqcqXpjX7+vz9fHC8u3j5OfUcxemYNEdG8pXnmM2Y5qmrpWxSUwjiCG7uNGdtp0dXmmPkgj5CmnhonlBZJ7Q1HF/uY23iTcJ3rmy8zqHoXlSIHUEYIjxuzwfaJiA0GZs3B76CtjrBZ8oSpiW80szxwrLCJX4vrbQ12W9pJgEdpECDbafdPt7tPr4c3Y52qincWUOLtvt5thpfXw3San676sdJRx+uetgXrjjLRecLdQF/uSe7q6//129uv7h98cn7y7vHyqDOl2yM4fLkPgggouUhpsZCZ1TkvAcIS3AkWHAkEWEODVmbKpKp892b38ovN1WfbXCURM6Ci5yvqMlXR/aRjBTNKlVpUJi134MycooU9pjg4F4FjZaTNuEctn2YrW5Obkr8n3OpMVjSPkNbiKDWbYYE2zideiVJRW1LiVJW0RUXViL/B+yMU2XHEyhoKQlYIIccFBlxFfhxX3fIYxNJSlxXnTujGRakBhJ3UpdC5YQAeUQmsrLHoBEGXwjaJCDq+2E+fXk2f3/Mo2S4pqQhXqXWqY5U+pdOj/NX1CNCDFX902j1YUqnj67188GCRE711yq8q1uuUi3zxH7+9/Js3Jx+fPv3TJxcfnXEPNjgShSqjnTpWRzBqVVKFdYSCRMVR3fr4IJBky6Q99VcoNOekHTPRsJ86KBGVSR+e4MdP+w8e9FVorMqJpqncbuvlrn51JW820qnevNhKrS1wu7JmP3kR0UZJoL7SwEh3fC5K3haiNKKgxYswjMgBIjbPgoEBQMybuEGEsuely4Asw/hopFA0qcisgxPnMMMMkEqssDHAjQiByFYjvvgRPOGxkxtmM6F9sLG2xhU5FLQm3ATOcuh45q6pDS8RQaXo7udX/MV9FqpMynZKFkJiroLEqSScck/Ay019cTd9fTu9f5IeLPDkOJ8seFvxzU6LahGdhtoz1/u6+/ubX3+52f7rt9/9s7d4YWtGiVQ1ecoRRq+2QClG1XuuDJ1bCxdiUSOo+SqQkRKvz/oySik6jjjp6dmD/NHDxYcX/bqjlHJKtB/ry5v9i5th1U13X2G712E7xrYYMWItUEZhZuYXcyRwe0LUEgK4XBiL+oZTbrjB+h/RbCR6kC44XgspxNNdryA0WwyWdcDo/DfWkK5apC5yApAdOb0C0koMdlky70CAlgE4NRHS2BuoCQJuMM675vhraxSVkLQV+8xqZ5uEyx/ERE5N5L7Iiy0JRGopKqqJCURKWjUlwkQC4kRIx4vjle0iot9Oqn33pJNR8cur6VfXEylPosuej1fZGhT1vrz63749ebp++Mm5n58JrAG1EF+XZDNwyKwRjRZx3Q4cxBHl4DqDpETHFwvpgYrFQhPrIpOoSGVSEUGtAhEmnC3TeiF3W12uc2IOkwJIWSE4yIjUl4Q6zKApXpjbOGaexDhsZwwbs4n2oxit0xqlKLufiMesEC9aKCm7CXiPKxqwuZlRaCcWZbWqiipAubVBwjqYAMR9tW4zRbta761oLt6W+Vki7DTLzct/Djn0oMDRPkztfyFOuRUSoPXNnncqoqWgVImGVa6sWaDJZpXBlJgmFkCZKDHSKj8fRtrLl1s6WS5yZvcFkpRYBQKmQS5/dvngo9PcJVfGXYxkTw6sfKmBcURBwxG5sAagxD4ZTR+BEjj1/PCd4/40y1iYaLVIU9Xn9/r0mI6Ya6lDwdWIm1FEednxo99ZfvhHb/ULBlghHJICtzZmbVhP8JacZlIRUHxeQBTMq5le+ETMhUUTVg2+CaAt/bUtLASBez65rU2fVarPoYQAGRtyhLIW2p1mjTUIBwwsvKL1v4W3HNht/DrcN6DdvuqLadVbqw6O6/bU3NPxgNj3LkOE1zrI+NktRKRCoKLITs41ETSpCCW2kKBIZDdZFSAaJ3050TCCEmVmc9C2WqjCsitML3Z1qqlLrUOMovbVvMuzSBf+fE+1wDSnoq4FercZ2bIJVWXm4weLBxfLy+v7hyepS/x6K1fb4f8Z8cnD/slJ97Pnm+d3crbkPvPZceazxcnFwjPwNsh+1Bhc8/zD6Ic5Z9BQeMUUqqZ0WDAVS0Y1vgqKeqeSBPF2I4sTA61jgkI28BjJbKuYPXC2FAPB6JpzwOsBLTENe4tfIHqOAWsYmjNhL6Crlz0QReGYIPKtWQxm6cDs3PS02bhBnrM8N/tyOdTnOxWIFvI1cuqCiyqB7SKYSZVV1Rv8FCq0l1KqThWUbMqRIq9XwP1cgSoUO+nAq57OMGHbDjjlpPBFzHJ4XLhnhKwMnrcpUNu8SZjpaY8x43SdnqzTSc/vHC03kxx3nKSe93T2uMvEAgUT70oZqwcDshFz5jujCpxxxM4WbfYbIWtG1IwTDmTUfBwkKgcbXBlA2QphqNpuImZu2kBQLeWFuOQfSiO7FdisUoNWZ5kEaI5b8nBpaYblyHMjZ1xuhMVWX3UrOhB4G0x7E6QFdb9bQ9UAvUAvHBTyyY8vMv3mHqNWcVWoiHBiiBZVZu8bV1aAqjgBEQIqiidF0vdomp+qhJm4TgTiupO6r3rSeQ+GB/iWCKnqoS4N8t5SrxPQgdPo7J4xXoCKbm6GbtTE1Of0+Lh//6zvGEOV+72y0Nun+vR0CdLXd+Mo9dU6932KCADbZUMNvoIEhx9QcxxXXJ1D2S0IEYutZ9bmDMwQdcpO1RDIOK2zAAOy3zqZWiLgxm0/k3d1UOBMVKIjhzW/8QRC4T1t0DkEAgipwc1u3mGogRwMkRmkUYeII9iBZ+eiRo0PESFgr5mlnU/jfdnX6ct70api8RvDOFWVKgpCTibcA4rESOytE2z6KBTQZGvgmBKBGMwpThYEmwhTnYZijMA6QEyBMie2voWZ6UbfgosCEfARNyV+A1GSJijQ9fmWSZUgut2Pw1RL1ctNvd6W630dBuwmYcCK3mOXN9cDWu7hXNsM2c/d6FVMvNqein5iBcG1B49FCIRrNCiok/mW6wg+QXNujfgh5imACs2d/FuGFHN589CU/PbFUqcAACAASURBVD9h7/H+zjvS9LKWYkbqG+imDRvttz42Gsg556zhUS1gH6oeTeIIRu0+NF2N9XqqVYwCVNVxEggATcyl2laFmqzvK+qWiXzpvF2qiu9GlsmsjeaV/VZiKlpLtOS1ISIKkgNQy0xCSWdE6pZA2sogjaS2gYdqzvzsk/P8/unqNI213A/y4m746npfKC16VlYl+uJq9+J6dzvUPfD4g5OTiyU5UUT4IcJuPHiEJTvJgWsfgQDh9b4O2RWatuFis1qzDCH/2XNFw0gDsph7YCYXOPilE/VYr9nej+4PwEFeKUeEQ5hosyU/WtuvCCCGxfSQS76zl5F6uobWohQGZuboLatxOW0cIyFGdHNAML3YlrGYbZQ6EnMVUYgov77ZHS3ycsmlKBQpxyhb6HAYEr/Blt6wcoUycfWJ8Gq1zNymK1KyZQRodJX8Cs2zfFsW+6UX0dzvbMAJxq09b6DVWf/+7z98riK/uKpEAO5Lvbm+L1WJeD9M3PEypalCzldv/eD05KL3w7R5jX4td2yNbv2mVhyUDu1WlIwptPlsfT/N9z3Fceu1E0TgbJOvDcZiaaY2LIJfhegcD7WdhbxyAqiodyJL+5rOpJKaFOE34d9BrOZ0lDM4d2fya2gCNYUqSB5EI2QG5mpMpksFNloy6fjtVkW6lKrUUrVWFJGp6tXdQARONI6iiq5jtt4J5bi8FC5OSmT9+9ajT9bC4yv1QapPFmntuZemIuvboR9l5qRGVpsbz+HdbtTXHrYFv+32bdIsa+wzffSHj9//07fHZSaiRZcSmKj78PTk49PjZb9MlJiwU6z+8OlbPzxPmXWmrTbI1MwYzRtnQ1CH3LAgsmxaKeJsCMme/mkzSCNI6o7SNjQmty0EahgLcCI3Qxbif3MQj2GiiH4AqVbEXifhlcFH5k5cN4g4iHMRnREPcM3YMZRaoaBR85lezFHWglFcNMWbAED1fiqv9n3umHSYahUVqcOI2804Fln0ybS0viMopMgkIlKrGEUR4mZo2nXe3cCsBI09f1QJrPKHF/2Hu8nX3tZKr3cnb7ZcI4Zrc2ht7IjML+0dX0Ar8841PvQOOwQQmKuWV9vby+FqV4YqfZc/edIf9eiSPF7x+ZoHxS2lRx+ecmb46owYCx+e2EjHlVkccOpZhveRJIJvEBMzFvGs4U2zAv8humLnOVe0PMFJYSzwUzmIizNExSF1NhlqaZ8iO9B5DFZV8rWjiEQ4vhECZNSkmhFTg037JbvLeNmvFTgDK9V6PKI84MvTBcpKYNHxq/s8GvRiN1RAFTxOtUp5+mC9zDl1zAprGgYRvH9ZVBimlbBpaToU716AVy1MrWAtU5fzg0U+frV/NUpZJh3qdLlf3Y7Lo7w9W6qSshg0HNxsw5FkxuervZpTcnxMgX1dXQ/pzf7+y9unn775x119RXi45uVCcyKwDII91bsiQy2Y0vHfPu/l8fRwWZfZFWO24EcOMQdEIAgyTPmaa36GeqRim2dHxJ9Zo6Obt3XAd9dzBmgFaz+F/RC2E2jEoQoZhCuFaak7ph6MkkVaAXEOdwgjte3dZoIPhTCcfLqMOcdugGMzNgProAzm/6aQ2qybmGYsL6QcAZFoW2AFAqRo/erOFJmxyjjVlIghU62itOgTJ4JohXjipy3+uoMl2zDa1+40pUKaB6qqCPZjvR+ni/shD3VaJN7X6fWm7nXxcLk5WbaNN7UNXHAPFRCLMRv1vQgoKB2riE41f3l39A+X5dstTXKMerbMz87y5ba8uJ3Oj+p2kI4JVW/GaVtoGOWsS/jF9fqrjT5cbZ4djT++0NMeHcV1hwt7QUubjQWgBJD6p0N71cCapuK6kRlKa3zVEVulUQP3qpnSqTWbNUAkD3sSlAGYSVgUhS1uk2r2f0VS6Ntzc/T1NnVTrb3N8kgJkhC6WNOpzaVNfVdVihwsyB4fXLnnSZE22OlkX3BbVMHM293oy6dVRSkTJeZSas5GwlBFRGHdJ6JSRZZdtn0LBaRarSHF40CE9lJVKpDp5XZ4ry5QJRdZ3A27N8P93bh+c8LvnVRO0MBfpw2WsjG0RgyN9JpUiwy3U3m1w5tt+eouP9989Wr3qze7Zyfdn314qkS/+87RP7y4vdtVgnYZpUoRrUq1ap+568jP8Gp385s7/JdX3ftn9NEJv3OMo6zJOzEd9509acAZkcqBrTROrASqc+0fcODzkcYBzhtIorEe9WTkYKGT8bO2+4yqKisJhcwQmZ02wLFtFFQVlCVGEiGv2NGjnw5odQkj/hR7xYfh+tJnoxVuSnPFBApl9R3aQAph5ShLObs1Udhe5XqUbWXCfpy2w0iq1eolJ/mIeL3sRASAl6mYM0hVRbSILvvUdbzbCVTs3gUKibZX+yBIRUSRE0ZlrvX4diyi68v9dLcft2X9csuTlJxcL/POhAq1XZT8mQ0hLIkI715tx5+/KZ9e0nZcEeWpHi9Tf9Q9XHe7oe5rfXy0+L0PzvoFfXu5ud1jsyumniTC+REfd+m9pye96O31fjfKm7tyvE/pci8/e9k9WJW3j/NHp3h2zKc9Wqbvg2+xT5V8g2bPRoP4O/BFiELAv9NN1UbEYXYRn4Ua4igRWWnJYqJAWp93aBazjqKOn2GWgWDq/RpzQiXNKq0tyxOLgx0wKFiJxlpBpwBu9Y2mtYvBYXs6RT8kXKZXf46I+wDKm51UIcXNfamiUK1KhfDkD5/QL64IuuiTior6kxgAFdFJZNHxsstTlWrNyqLJ1hxzkFL1uCNVY5219kzPXm029zld7veKG5W6mTAWLJPOigJa0u6ZaEypCLZfXO/+8sv+ar8kPcpplbhfd1LqosMipc1R92Y7vLVeyGb8wdOTDppZAAxFAU3Eu6kId28dd3I9dKv+EuX9M5oUpDqVSq82y6uh/uMbfbDa/9GT/icX1CdVVde9ZlnG16tE85nlK964IEFWdLZQDU1ONNhUBCIVgtO3OZ4apXPVR5t2MNvNYfw1DPEClSoRZSeQLb7F+hh1uo4oUiJgVdR3DglZhUxVYz1YAkNzMA36glmiiSirAZF2MpEB+6+2KtjuynYYoSKASlm8d/rgB6e3n91MVatIl6y6KQqUogJNjGWXi8hUq7sUIxMYqAKQWAeEDUJVzSylIlHXZX74ZpcY5XJ3vEhX9zLUKmgk1jV54yqkIq19iqCK6Wq4+p8+X90OYJxyepBoedxRxRvoImOcFCoropf3+5Ojnnfl/GT16vruwSqfLomA6+20r/r7Hz64UCyO+01VSjQNKUG7nKqoFiHozVi3z+8Xf7mnFxv5V89onWzKNCS7gyQPItHFZKDV3vG8IBZ9HjqPWoE9hI0IjLO2S+wN3OLfFYrEGn5EVTUqXx36JBIRAJrV9Q/POP0ZBQ2lTI4hBAV1bTraATzHsJDERKq21l5VY5PoRqNFQWCvnZKnB+qbfdjJxqu9vB7Gsby+2Y5FiSRxUsHZj8655545MxepU6UOohYxiEiRE0217AZZ9KxKorZRJatCUVkJ8cCYCt2NU8eghenu3E9lNdW7Kqd94pz2qw6UDtMozLNhg+paEkFuf3GpN7vK3BNpx5VB0C1pTnS67HSpUxFa9l1Hd5vh/GS5TFpXy6vdjpj2FX3CB4+Pz3oersflOt2+3mvR9Tqdd2lXNYtOfUejrEXvt4XKOHx2e71M0794m5YccAAXXnwWqc0mgvFDCb4Mk6KOR/Mjnjw1UDe6+Io274onj4UcH6iDeEZUhFwCizO/mHRnVpRJbVGMCTc2bRTFl8BFdYWwqVxOkINgkpInlRRoxWGSbgkzvEd5BKZxqiqTcUotr/bTdnp5tZ9qJXBVmsYKgBdpdzUs+9RnJDAJTSLVHoEEIbCobvdl0efErDoRyFpeAVKx50v4uUVxvy+sSoT9JEUlA0yUmBjaHXXbx+uOUSKTiQEjpaYOuJ9NQx1+dXWU6KTjsy4TERa8I+0Sny55rVAwL1gyl6r5aElMi4qPjlf7Ou5LzTkzy/GqH+7GfanPXwxTpfN1ut1OiXm7n5ZdKruyXGXa1wfrVHhNFd3P3gyLzH/8mDrSudxoMpUiMv+wnBh2ixrSOi1gSRqsy8wxjuLeItc0VQWu8ailIbbWXGYWYZyJRBVJUS0tIWIRCdEr+hE8gCkBJgzLXJt1B1aa8wqFzjYWEA1EYulG6N2XTfIP0ww7ditu4nZBebW9vZ+6TOtFzpk6ppxIFSJC27LsrA+JqkokqlBBFdmNdaqyyKmKHIwtREUhpepUpIhIRam1TFKVtju93Aw3+0kEDCSmQaq+fVofr0umOe8HoCRUI2SoXY8q6uX+5Ho87vjxun/nfPnexfKc6W479UrroWRCt0pQ3Y6yU6FM17uxLIhI3z45YcWay0nmo0pHlLb3BVM96/k487OzVcc4Xvf7qd4N8vzVFqT9Mu9VOWFR9fhvXvGvbjHCo4lp4eJT5JxfyFtZ/UNRF/T/a1QNTPygpi0Qke1XQx6n4BK9HGjE8aRG+Hz7Qjlfo6UEYjmQ/QmUNRIBj4JOHGn2XoKa4O8BkewiY18OY1ztQjUugQ6KAV5OM41eOXaNcE0I5gHDt5ubz25T0mXX76apSCXizAqWbpnXO1FFESXwWJSZEjMLJtJapZSamVOisTSZy8m/jX4VBYRZx6HuJ11qHUjf3NPz6/3qYqWQ/VRuiKf3T+r5khJ7XLHSAeClXEEgHItg/0/XK5HjVV6ssgo0aWa+WHYyTeVoIT3f3Q8p8+00JaKBeVS82Uwqsljk42UPqqfd4kQA0uNV4pG6RGtwLdoxyaTIDKJulVKfrsfSEeU+XTxbSk9XP3/zGrr9+IFPX0T26PLwO7choHkFgHu0IiKKyxUC4djAgEIH8szJLSCiEVlctCayAHkNUEUcmhRGigqgTT9zHcVxCA1EfSGGdVy5+BISnEkuIYWCDqBNCbGns4Ze7uUGdjNrOocve57k5m/f7G+nPhuRpMQMwlT0/KcX52+fDF+9SH0qVRNrzjyWqoLMXKVORaGce2ZQEYH44zc1qrOhXoKAYdLbjd4RulwfJvn2Kp10LFqv99PV+fH45IiPezg0G4K3KSJApermdtzfj9Ombj59/cG6O3q4fPtiuVqk68uxXu/6kYbM26EuEkBQQgfKzB2RpLRKfD0MN9vh+DjvVRdCvEj329L3iZmoZxVwz2Uvx6ssIzbX+80OiwcLFX34cL1+uNiX+vp2d3+/H/9qoHUnb68jqniTtid8IFUM22l7vd/cDHXUfp0fvHOyWCaFLZZTBjtKm/yj5MHXJAYVlTYIQcv8eaREKlbsjmcjApEaughsxh7pb9ZQWQIHonWOVK1bzkQb54EhUCCYgBmZwaTjHcf7rZtjLgNzpJzRR2Kt0Cp7Wd6U44uVitzvy1SKArVgOOJP/s27aZGuvt2dCxYdD6OmjFWXpoqpFiufcaIukZBKJR9o11qs4KWsVK12YVoMoUsoopfb+uXlbijTPVH5yenifEmZIk2KhMoikJAofvP3l7/8yy+G6+1+UK3yc6anx+mfv3f006fHR+tF6o8239zf35Vlrk8eLjNzEl2tUoaWIl3mOtWzdS/bKS3757tSM315vasKUl0v8v39dLHOu/vS5Zyrap8YGEWGfXn69Pjk0eJ2M17f3N/txv223mzuh/9Mp//tx7xexKw27kz7zfTNp5ff/u3Luy9vh3sZp1oS/86//+gn/9U7lLwjQ0MbNFOIVNLHT+FPqDaS5OgYxKwS4E/Mi9AqXsKP5xRFqFMFkH73Lx5bmDB7gWcBZiqxT4aSNZGaYcSCJbcx+N5UIcVG7YksK7C/obGdoYNl42d+tkGmz28waSlQ1a5LiRjA+uPTt//gkah++/dvjiv1mYhpnISIMpOIDpMUkT7TosuJsB2LKijWWAOksM5SMzuZqm5K7RM9XML2lhqm6UXB+PtPFz99ks960/FCXyepkib0iQm63Uz/93//WX29eXZxdLzIu6mo0q7g11fTN1f7Iy5MdHy2uroe3n3ruB8lZ9Kp9j13OYGZMlHHBHR9XmW+mzCNsisKQkfIXR7HIkxVcT9VYbq6G8Z9vRvLxcOji7fWN3f7zXZXpjIVVNVayu3ldne8Wr21sq60xohuX+w+/1++4E8v+XYa9zJVqVXLpNrTuz95lJLrn2FR5OFJPXlFS6nj3UOeF9pc1F2DDnuwlSBDoTpoASvSj/78SUqkaItkWxOF/0oVvi8qnGExmVQYVbTY0BetnmDmMx+sNf1jhrRgcWa5lGjcTuPzHbOu+mwb4yoUq3z84Ul/1JOie7ln72KjoVQRVSURZaI+py4TwLuh+L7zcR/ibJNUSZStnLGALgkM7IvcT6r/7J2H/+Kd5cOVt9hEpq1ALZqr9Imh2NwMf/8fv5x20zgVToCgiPYdn6y6EfTN9f5RDwbRhDzI0VGmRJS4MMkkIysLbSfhRPtJFstksymTnHV5texOEwvzRZ83w9TldD9MQhgVN2N99NaxaB33e1Wxp667LYjcf3U3HS36k46yL5bdvNp9/j98/gc5ffzkaDPUzb5sh7IbIIpHPzx97ycXUTm387ebDeMKboa58k3+FHQf14AKbTaqHrJbfRRBuxUoAqH0oz9/nHMygKHG1h3MYpNYfCe39LA4LziLvCPM3y0SUcii+JZtHMaxyWz7OhEzp1Wenm97QWYGKCcCaHc39m8frR8u+8Tls/sgh6TQaRIQMiOlZHsEi+purHZQBkE5aBU1B65Fd1VYpIOmRKVSeXby/r/78PTtY9/IN4bJHbxKqtozkWKa8Ju/ez3ejVaGL6IE9B2fLBenq/zt3bAC1kkXlPZVVn3eQ+4H+eZ6R116c7UbmTf7OorsJtlPdbstq5Q6or7KyarTbV2uU7+ri+OOR0l9mgZZLPOL24G6DJnsDnxtFXlvFZe6++Wb2zd7vjjK6yyTfP2fv5l+ffvDt47PVunbq+Hry+31vVRFXtDv/Nv3zt4+aiUAlyTCyr5DsSOja8KnEXPfxQCO+AFj8aNvj+PaimsjkxIk/c6/fMzZT6DUdv8z6o7ZkFoBySPvdzukYp8qwybHnLbOzN6xLILjYBFlYeI9aeqzDBWvBmJkZlu3uKiSzrrF20fbl3v99R1MCAvRZarClDKjKnKiKjqVGhdKLZBEck1QLaI3u1IqatVaaSP65E+ePvuDx9yltm4ohEAFWKqkSRcpAZQS3VwPrz+/IVjtSatSKbJeJAAvbsbTTs876mq6GosQdoM8vx8r0W6cBFxES5HVsttPNREWmRddUtV+1TOj63OfwB3Xoqo6jcKsRFxAX17epYTMNppMrEUgirHqfpIM4PX2+mZcPDsd9vVn/+Ov9nfj0aIba/35l9dfvS5VQIT3/vTJJ3/+DndWIqWGVgj1oWUPDdUA1wxUvEgVmoibZlA5OgiucHHBU3NYfTr9+M8fp8SucsXWWTM7o1h7TRY6jfuQ62dWno4QGc9FAmK3So5YSnP4nP+MHQpjcR2DikzfbFmUiVakHxzLo17peDEs81d/82q9qQpU08QETCQiZ5k7kn1FTiSKUkX9yWXtifGQKMAC6N46ym+v97e7u42+2Wg+SR/9yVvn75/a7imHKZvnElW4as9sXrg+7Z9/fbu7GixIqWqtcnU/3WyHRU5P12nFrOA3m3FfRJWEaX83nh8vNrvpYt0n5vNlN4z1ZJWFaBJV4lRVFzmVUlLabKeaSBSVUSukSh3kepTr3dDl3q6JwEORoehmFKgmokSVL3e31+PYdV///Zuy06/e7H7zevf8cpoEyvT4p+d/8F9/sD5fzBgERNfJ3LZIVpvT6PwyS4ziZqhuFKpXlLfdrCKG2pfiL62ipdlZJAC+dgEHLXxubP6IVTRICwpmSMfwRfZhdf6Gv435YSCRiJDaIxkiB2Qw91xebLGpdSofn8jjdV4kUsXd5f7lf3m97HIiEusxBgh4a0mnhDejFAUnZkKpKlK9FUbdM+ZxBJ387vkP/t0HJ++diKrcDW9/dPbsnz9ZPVxEsLcMOT4uqlWSoI8Gl+VRfvzB2VBkfLldMjLQEc4W/HiVFpluRjCnMgkTylgFOg365NEau3J01C8nnB13tK9gcNXbUiqw2ddukW83g2a+vN1vBEMVJNoPtagKmDOVSX6h6D84k7sBVRUqoLHIZqikqDHl1893b35125+tnvzpU5x0dL48enZ08cnpx3/x9o//9dvHF0sjVS3euVl4ghQGYyuGLRMVD34WE1QRPZUy62sIofLg4L5Vg4kcFVo1u9X6g2DimeRe9DIA9H2+/SjiFSpYYZ+A1qli+YozqOjb0Pj7kBK4Fm29lhrFBeE+8YPFi8+u0jDcH62OOuoSne2H/WV9d0ljqZVQhAx6nvT8NOuvN2VQUqBWScycWIsmit2ibZyslVbNk7A4zs9+enH6ZH3104vVWXf87AhkT5eIpsIDl7RWzJadqeL4rD8/zu+9s1ihThOGSU5W+Z3zfj/qF1fDq7vxVdUPT/LZInORoRTe96tF7hKdn/QE4DjrOE1TPVksLq92/TLXqgJc3o99l/ZjlQl3+2mqakuxMtHZcX7w+Cz/2/c3L3e7v315cnW/yCRCqqjCo9S7QZ/vdF9xe7/jT7rf/WePPl5nKESUGJxgDc3eOqSRYELmTuRZgHXiFcUEU0Dgyo5Zo8bomKFBQw4zq2PYQoJ4ehNE04/+5eOUkisvLcIBcymzLU2hVp00O2qskYL6NxRrzxv0K6GI2tQYWWBcgB8RETF2g2yOc/+ji/7xcZ5qHmuCpioMUoEKVVVReXfN7y7qi9vyGjnnXEVsZw0AUxGKOEn+wHnbeEoBLJ4dnX54hkSLo+703aOjJytuq0EjmYmWQlUlrZpq7WIrAyGM95P845v1MKCCAAPRZZcY1Ake9x0TvriexkmenC6PFmnZp2Wi/qjvi5aedarCPE2KSY6O8wopMZWqPdN+P4lg2fNmO6U+7SYV1arYFZ2K8I8v8qOlvHu65bR/fo8qY5G7kr7d1PtBOmgZai3YvBymo/zo3RPbuNS5jtUZJaZMZgvxTYK8NBBQF6qGusV5RTLk+tjFRWOC8dvMzA+oZHiWPvmzhyklz8v8P5t+9sdTeu0q1LNo50DIsQdP+VB/MEzwNC+rH6gekYpGGMP8l52yO+sfvHt6+vaRHPcVpJuJh7JMtEiE/X7aT31P75/kd5Z6M5RvxzSCFj2nxImIE6mi1CAPrSFJIUq2Rd7ynaPjj06cj8K1gOa4Np6h0oIArcqCDnNnxP7lrvzy5bivNzvZDFVVSTFWLDhhkGGSZcLjdSeZX+x00fOqy5Ww2Y5YpJeXO1qkF1fDHsilrrqMUaoIC1hpuUjLLvdQ4tRnSooM7ftMUBx10w/PuUuciZ+spycn29vp7nJ/tZOLHoukU7E6GWrFi6/ujt85PrlYmcFQRJroD4zQIr5jj7pFIGKSFQWi010t2fTfs4+MzurtocEdmCkU9jx5mpBVobBGZIr9GDTEFP+Nr4mLQmZIC55Z+3ySQiFePPeUby5J2fd1/r6XU1tSQ2prDWDLQ8FYd7u3jlKp+Wtd7vd5nBa1XBz1R2t6sNZSsBHWxCz2PAwhe+QxKTNKEUuC1Z7rGOmGKKRE2c4iP0BqMXOuDjaNCKqiIFFljbZSKnd7VhLiRHVbMVasMqa9vEPYgZix7NKi704Jn77e/vzNtCBWrafrbrgZKNGr20kS7u+H1fliFJVMIGRihUpBJpVKx4z9KBerXodyz9gRNg+WuU8Wroipe+uI/tX7l/e1+/JagVIFhEWiRYdVh9NCL/+vby7eWi9Pe1igjG6hGHQPaUbCJKzP/c2NxovajZxBWzMv2Z4mFlO95tOypxZWPQRAIdljmzU+es+O2yRo7h6zB8EY5voT5gDrnGlFK6vXCIhtYxpWQKAsQil2fMEczwC2mpPGQ4RjGyULxgw96Ya3jsdBbn65H+7GtFw8OV6kpKRUFFUItRLTMFZi6rMSODEn5hGV1V2BfLtjKhBVkqpaVeO5N+Ex5ggaa1nD88VIjopYrAAEmpMA655O+/7RkbzZ1Pt9IS37lR4vc5K6WHY5JRnrxeny7y63t7vx/UercVfXZ6vN3f7kpNtu6sX58qur/dlROl5mTEgLohGlJyoqOZHIasEqyilDyz/uS/fji2MmqeJMQDHVur8bsMxjnYpAhJY9np0vFomr4H4q9/90vfiDx06FI0UM7uU+5NYXSwZnstXipsaySbMq0eDvaL9za5QGfn6IeW2BIvvyY38gYJh7i7Qh+UNAyRGXGjTa8OscAFUbxbcuFLhuJv48XJduVVWJoSq2siH2UfHnjlrvKyFxOek3D5b3e2HwxTIxayIGqNYK1Q5QqZRYbAPQhD6laRJV38IIBsceJVUVUqyBhsT7bOm3/but+zcckJYAeDtWPltsmVNKR4nWa373TF7fDq+3iqxbQpfyMmdWUKLzBe8GJeJTTuOauNSTLmWlk8xJ8EJ0M+m+FgbpWHLicVMXyzTsS9/nTnTBTFxXKf/444uX5ysRjVqfqGJzObx5vv3Bv/9BKkX+5nl9tY1qkXaZzztefn41vn+mZ53FI9XGCAC1g1HcmJlgVLA9FZgJGgRQtmYx6yc2WVJbliquu7lZKjmrU1+Fl0O99fyv9dIKfPGIAiSejBGpapC5qIfbJw7K7a4ohFVqPBOrrT4JKxdYTLILj6UDEVRFialm3q9yoXyyUAVbp5PFuU7FdgJhAMylClFi63lTVSS13WP9uQPOC6WqVDD7p6zFUuKZsbHjprtORANLVz2mdutOTpbL2/2zk7zuOJE+XXJB6hm/uZ5kpCQyFBpKJzodLzD1qRItclIizkwZKWUIHq27q2liZQX1fRqH2i/S/WbsFnkzlJTo/23vW348ybKzvnPOjRvxe2VmZXVVV1f32Msd6wAAHz5JREFUdM/0TNv4MWbG2Bi/WJjZWMJmYSHhBRs2IHZskIUQEkhYslgh8bAswQaEYAGIFUbGaGzzsuWZ8Xg8M93jfk1NVXVmVWVW5u8Zce8957C4Edn9N6C6m6rKyvpVZMSNc7/zne98Z6vGDC/af5RwcaBXZqP5tYMc/ToRucxl8cpx+/rx+v2r7Z+c7YeiZIsYYoBuD+krZ/7Dt+m0QyOVCZhCwY1FuN80645v2giKxgqvT3uDRoHbhCZ8qjuNe5E+fnaT7Bg1eXUCSN768ZdIaKod0cd6DJqQ8E3PZs0lfaILpj98zIhNpicj0MRNVRTADX6kCvg+LqOO6mtg8vOnUXpQxzx72Vv+4FpALCSTn0ox9IpUrKipY5NHDGpGWUtWv5EGENUNCneYWXOrPXrr+BNTe2hs0sJ0ZNKIUcZDXl3UAxjjNHiDcFvs031/ZyYzoUCIAQS0gdUpg64H/b1zfXvH156FtGnCyUw8+SAUgL05OR3cFjFc7dLpop2D2zZEYNaKAA0zMzQbMfri+6S74vnu3E87TFyXDrZ759Kf9Q/evbx+tN/vSndncfuNk9nZunW/1YVbrbTk3X7oHm9dSW/NfRqsNPE2NCKlmj4Y6nkCmtCDT4KfqdRJXpOJiZ+aUqhx4O2Ee+E3WKT+3pAR3KeMHyOtiXE3fBxlp31U5bhKNhYJzMectJaOvIZjZqpIh8cHWK9sIk+BceA2YdwANAqVePzF/CZ9cHdStUwyMB+0AL4MLuC+GAGrrim7/OG6D10XIWqqpm61f4Kmg3Bs4QM70ygXns7GCZKMboZjLL/5Kk03zseQXiXufvu0O3kSCE5Cml04ZMuLKIvW/vh8//ZlWZsv4vB8W0Ij14bfvxz2+2JKrx3JSfF7p60Wo0VT2sgMEaRsV9u83vTPt7YlM7iqwzwGEhZuhHsldSbqL/rz9663j/fN+XafSpN9Rrvzd55fHTfLk3b+NH3h5W7eiQMSZE5Iavydp+nlpb80vxFd+1SMu4lBYzY2ASyasBkm5DpuxJt8YUqafKwdf4JO8ykj1ZtPQ3A3OI/WfgbwOGIFVddfa/pM9QOZ4DYa5xEA6HiCjhQxAeTVptQxOtADPvokAjQB/xpeeEw/RtdXN7jU0cjTNgQIYDaiwRw6Xk/D3hcIcVJkYoYMSYVYzfaDtqEW4iuiVAemOMtOAFceDph6K+owEWA8NjH9+FOOdgM96gECV3/n0RYXw+duRzaYuZqXgk2fLzfp6V6fJxfhPrsZrQI/uTrMIhwUguxj99FQyrbMrBRQUX33cnh6sEe74bK3oYwqmEiYi68CuoJNobMB7f/+6Ph5f3SrO//q0+26XyzbkIsbicCKnixjAzn/cMNqP3qP3JHMFO5KClensQkWI80+6sUMhqkggBs94+hOXCH/VEkeiW64k2FignxMpGr0uvmkT/yTCtMdHvAxuwCCw8jIuRIN9UGMDg6YBpl/AiNPJ+101tYYYe6jndXNBTmP6Vs1+WObCOSK1MYTcpzHPgFGGqO3kLnvs4OZC8g1Mpi8mBeXIN7GZrNPXSfkPA5ApwmLjHzNeEQTg7iK8aYUf3ynjYinFHN8s3waXupuZjzdQDfD5jr9rwe76MZMKauZt0GY6WyrT/Z2vS2zlkU4CF/uNASZi7i5K310tv3n/+Kv/4f/9LXhq3+63uWvXh3OdwWotSOIkIMW4j+w8h8+9uMW6jiO/m/flffO99uzw/fIZ6ezV3/i/u7J/oMP1jn5S8fh6dpmLdY5X+8sEL19kT57HIJAWNpAgJdZzIvmpqmmivFww/hPneL1RR+jmI43YwRx9d/aqIMfj0qnCf/fbK/pzP2Et1X9BPncj730sdXhtN/o42ji0zwaHhuhcFMhGHPRqZiOkaIdQf4NRztVGW+S0jFOjwGjJt31G/hjURNNmlvCQcuHm5KKOgm7q6MavIPN/CphZz4Ui0GEyRwyhuRa7h+vz51rNSrcmS0/fTQCBJ9A2fjmYEyXMU2QNMAh6jJ93UFw2mzS+99dhyYc9uWqz892Nqglw/lBzwcsZk1gZ8Kioc+8NP/M7a4BWpHX5uH1Lvy3rz/5428/vi38vNiD/aBasyZiZhF6ucGbK7zU4rjFIuDZgEj4/mP/2iVpPVeYGXh+tj1+61bPdvZwiIKn28It7gvurcLZRj+4St+7zs8PuldP2R6tZuEzJ8RTHmk3Wu2JaPo4XmNsvHMY3GvAG3dnDX8YfUxuzsmx0RA3kM5vPnA6B0g9eHWv45Egmx7vDXjBeKb51IH18ZOYCp1TI/xE7U7P7OZw9pErqyCvnrReezkJIINJzQa07jgbdWN1RoHDmFGMnu+SLEb+pWECaJvtYE5EseGiHqSyYkosNwayNs7T9lGAEtndzT5+hww0DifFDWUII3el8a2v7/NNhga88rlbp6+uGvbNg83TbzxN1zsZkIpGwt2At15ZrLP/0cP1L3zx5ddPWg4Ms2x0uRnee7ix8/Of+Ny9r3zjMVgDQQVq9eII5tcE22OTcTlwJxYYj3Z4vJfkzrX5cp93F/1bX3r9+N5i2Of1xfDgmxdz8k9/7ha9c3m67rsfOUmP17pPl+qP286Bcna499Xz7iQub89nJxG1Q8oNPhHpU2G8ymRrXddHaD9FMjhq68V4FtBNmJtcmOA+euKOOO+mRuqY+oTHTQvoOKmJuNLgNIoFaaTKpV6PEUk1E8aUiky6EZ5SRp9Or7Gr+CbXmDD/KOFAZe3HFkkn8NSe5Q6q9SJS86dX/XE7N9hRS8lDKnaZ0DtAiEEOqcxbdvchWxDEENimDHdC8yCSjm/iPI2WqfUG+wTOxtegktw0pvN+k4G6mzTUJLo6222e9tdbvdr7YdC3jhimjwbsPtrFyG+8NNsM5fEVZq3MWioF81Z25oP6Z+8v33k4u3h+HZhNRqxa74fBrzJdZq5mBRUV29hTSURgN80lNMxEs1XoVu3pvTkIIYb02nL9bH/r5WUZXnL1uwRpg7v127K/Hi7eux72ev/otDZy3oD5aS/YFNLYq9nzxKI5pp5iI7hqHcxYb4VNd6SybqP2YvKdnTYVuYfS54CmAQ0MZnNiqDGPw6vrkxclL8XYvWFqSOq7XUeGGJim/T0lanBzZlZzJwQ4yMdRC6jsxXS2TjGiXpZWSO6kuEkQnNS1Rmbf9toXQMicesUWwRqlVBtvYEZ90lzMDL2qubUhcI2XLpMHvodFrEntx6T0mEnSJDypU9+8CjXdCa5WBQgVvhBB6erB5uHXnzavrs7XCcUJeHc9lkPWzwvcQ8B3zg5RqA1+axFuL7tFlFz8e1fpYj184c3T//GHaya0DaYHhJpt1XeDmOCFeXSTYIIC5mRw3eRnb191PxZDJw4LsYJfb1ppXl0BkCaOocgJwPwkzm7FW6+uRoGGjdhoikZeoc3Uj6TuN5tszEypemFVxG4+tUfRhOBqFkDTSVlf6xG9Ycw3H+wsShFOwO15Y4TspgQIM43ZHyWnQzHC0FG4FdsoLsTC1VCmaYSZjFCJjnqxXIyKATAS5vEMcgAMV2eQjqQaOcyIjMBMXLnkSqsQkxsYNtF0wn7IOmuabTYLiJHmEoRtP2RVb4RTQRfFnYasqlbIRVhoxKREcCGZBcCgU8Iy0czjvQQRwdSYyaw6OVSY8jGGqSfI0f3V6/P47tfPrTc3cnMz59rfCCZQVk/Z9kAItE350bqYUiCY48t/9PjucazpfBuoqBUtNuqxR6oH7oBMCbG7U2FStWLs5usPN48C7v7Q7bgYh/R+AmqNGKayGBjjFDHDQDbWzmC1lDi2H5obA47xrw3Gk2qIbjaO1dfAgFFfNLkyOY1t6NX1fayYmo3sNrl7+Pzt06J5u89qWA2869OMyIFipZQ0ZJt1oWvCZqclFxGKG2siOzMJiIgCHx3NiHmfenPXgMLETJ3Di2UCLxuh6Tx0L5GXEkrOCDwntl4RSBvSQBCaEQZyBzUOsDKzsqO4RW6Eg/B+yKtZsCDsVMyFeRaZudl4Tmp9yrGJwmibULy4ucG51jhr+Uycs+leQ2CjWkMxGDFI3Uwm/nAELGRuUC9lvGFmROZpKHrQN2dzvdbzdy5zsZLdFEwuTMIgHmfYG9yMUsJ+MADCFITahp6vd/1+XyW681YcYdsrG7PoCKf9Ey61DnUeIQ4m3qHY+jvrqyf9p378ztGdRTXsr4Xmes7dsI9TyfYGuE/1zpHSuAlAowbNx+ELehPObngAGzfbWCe0EfiPAW0MXqP5yzj3YPxsR9j1maBqDtDzbcqqNdoyszAfL4MQm+q8lfmtrj/kEISMc8pBSFgoOaUDCc0N20OOgkgERifi8GCuF1mY3c3MRYjZV4u5MLXRxP3q+hDa8Km7R5fr4XyzJ2dyi4EDiNzbriGyZHbt0MAxos+5eDcTAiMXc3FiNIzFTJKqZ94e8vEiMCOM/VhWXZDdnMQAxAeHuDY/CpiJMWbE/b6chi6TryXFwMGhBdmNhXIAETUZrrYhJ8Z9bpdl/ujJ1flw9fVvnu0O5tnMACc1DMWZ0DbeiHgdteVWHAAxPClStjbKLCCI1zMxiCw75OLqVuf/1AObmRaz+P2v37relbsn3ZB1s0/f+u7zTa9WULLPTtrDg+23Lvav/+Qrd944CkyVCBWnQu6jWY5+Ipus/Ro2pfRj3ulTxXSsDIzlJ6rNiOZM0FHOXvl1NVKfhiv42C9Mk6dMZUym06J28ItTOOSyaLlpBCBmBGcfzUNdmBeLVtWGZFFk1go5imkTqGnivGvahg6pTiwBmI5XkUDk2OcyZG0CN8KUtQtizkVVSFrzw/XQNowYyF2Liev2OqFYvujRBFc3YSUEEe1TDFh18cDcw4QpZ0s550idNAheigcguzMwiyEV2+zyLFITw3hWw4BpZrIZkcjBl6yzwk3Hl/th0TbtIbfR7y67lxSAwqSYDsXUsLXcxECDDn2WAAl8cho/d2+xONh//vI733u8ro+AgeIjKa6O3INIuwgJI5tj7sUA9q7B3RV3TZ2hMc4WOZrJYbBsYDgzv/HKya1F3PX5s/ePzX0ey5v35teHcr2Vq+3w/ll2QyrZZYaA5uDf/K0H9z9/+9Pfd6sJwoPdknAdsWWlav07OUBKTXHUI4vCmZBMfRQKOBdvIQv47S5eHxI5DYGfe5ncO1wcg3vIzgpRL1p4QIGrOgt0zkxk5DrKLkCOhdJgvlPN2cIscoyhbUFOLG0u6vBZDKpOTIFdQkwDZzVmOj5uCS4iXZR/8Gt/Fae/AvyXf/0r/+TJOjm8ZG0CtUG2Q9kftHJr5BZDMPfNIS/bIMKqllTNrGvl1mwuTMULCb368pE5ilkqWjNvCdR0jTti2xisvkX7Ps27xkKd2Vjo43q5h4B5x7uUjxqhyfbgZl6uGkR8Fmm1iEeL9vbx3NNzKs4sDaBDaplSgXpphJfz2dX6QNelnXNWK/u8bJuj0Pab4Vmze3i+fnh+PdEAYzXBMDIU9bArA2aGJkx6A4YZVisczUloPEOZqRiO52Gfyq5nIv/s/eOf/ZF75LjaJodv93b3uNn2KWcz87fur84u10xUtGjS2i13d7X6zpfP0+PdT/7Qqy8vm5eWs4e7vR6yFHRNkMgIxMQLFmLa7ctrt1fEMLerQ5+YStGr60NIWAa/fzS7u5hdKJhpFuMHm93FIbUxzliI6Ol6uzQ+6qKbX21yHmzIOouS4JqQ3dc5AUqgeQwdyVzp4K6DbjZ9iI3UqW9qyuxR4MxCZKRdE2IjjfDWrBEKwl2U6m/3l37sTZz+fQDAL/2Nv/uVX//Hv0VM+55C4EYoCB3NQjYE4aK27IKZL/rQCM8ig7gRMkcqGgjzGDZDbgILs6snsyHbPlsgBGEQ5eJHR7h82tRgvu51lTQGjk0gVJRGpmSwhqWItiH2qcyacerUDUR2OFO4dTJbLMO2H+KBVotg6gbMmtDnXOsxyy5kU7NipE3kEBDbMOvmBHQRgH/v6dXvf/OhJRNCwzVQQBXFYAI1pIykqINaHAhSU/BRVtBnu72IbUOBPYRmnyyGcLpqVQcRPxyG3/3qwxBo3+fqMgi4OlQpqQ9ZF5HbKDzoJilMCWHZNscRT9/f/nH+6Bd+6jMzkkWP10rrbosw74eivZ8um7kIiC+8//TREZGfX+yt5BBjKmVY7+FkYjkWy6rFBrPVfHaSw9XFAWFolzErTgY6mssshu0+B/dZF3eg+UJC1n6wMuiy6Ct3jgLh+aZfzJoQiHpdxOaxlpByaePYbpXcCBrQmHsQESZmUidhzGadMOAmgnnb/tTf/HncrNNfPV7+TmCsWt4Mvpo3ZNYEutwNi7Z119NVe3vZuPm75zsiUofDF21wbg59fmUVbJMTHAWhCXlIBI+CVdsY3AxMSIUgYxWC4de7fdY4i1HdStGuDQxXBbk3Ig6PTuouo9UCA2pOTKRmybSgCS3vUm6YmlirB9a2QsAyogtsoGx+GmcnKw3CRC6Eos6MIPL2h5fnTzdB0AqYx3ZqU/QZqaBtMI/oC/Y9cgHTjWoFAHYHPJMiZK+ezk6XTdu0274445WTNqW87OR00d5ahGUri241i8yEVDRlP2TbD+VqV55s+rPrYT84qboqC+n6QIwGePho/Vt/+OGf/4F7yy6cruKuT2rap0TwfvCcJUYRoo+eXa93w/V+iA3l3dBvi2mR0BhovU/5qV9vBmqb6+FqvymqllLJuTihIb/YFu/73V4FzNBDn/tATMgZkVkbmkXuYnjyfN/n1MUAMnOdzSgwIwYmoihI7sWolcaJukZUS8N8SDmG0DXcxpBSjm34y3/hLcAu//vfPv3SLwM/C+CX/+Ff+cqv/3bKCvdBbdXyGy+vmGjWBhGKdxd47Rjnm09/68n3nvUX26G4zRbUCM4u/CqnoyO53JfrnbKJq657dTchjoFmkWcGVxImd/SDtw2ut7o7HIj7PnkuWHSgOmeURYS7yMsuALWNk6zyb5VNdk2HZLPgjqLej5bOY5VMmNx9zzRkM+Ji8ZBwNEfboAkUJRTLu0P6xrvP2JwIzJO2ySpXDHfsBzCjEcwiDhlqEEaox4mjL1jv4GZE/ely9cpJNxR78Gx/fKuNgQMhChpBE1iEzUnNh4KhoE+2H+xQ7JBoSBYIYgYDqV5fpym9xXsfXB8v48/96P3FrGkimeF4OVfYMFgjIFKIPt9udn0GoQmxaaRlWJnt+8xM7bxJ7t2iIWEz7zppO1Z1EjfCPHZDHgbV41VombVg0YW7J6vdod+G3sxJ4iENm77vltwIg92DZrNuKaGoaym11tiFUCDupWRLym0MQXDchUaoiTyPaObtNjcPnuHJv/qd//h774V//7W/9YtfeP0X/yXwd/7cX3wHD7cQhwgawmunWDRIBUSYBbSCp37vlVlwu38sr9yZn232j57t7i+DAYt5E/P+ZEW35u2Q7WIzqDvgwjSPiIFXIbzXELlf7XHvhFjcgYbQNegCmDByGK6bnYLx6Xvc1G+CjoSXC9jZ+ZBsu89JLWltT4SZMxCEBQSAGZtt3ums8Dxlm+1sFmwRyzzsAf3u48350w2Nwjyq5dapKRHMmLUYMnIZlQVZITweoHA0DYyx6YHnGmW3bOPrd+YfPNFHF7vzLZbzUCTsSbqMlxDmkZuGX7vdLKJcbPPFJnXb4k3/9cc7yxpaEJAPw9AboxJeMMc3//Tpj7x5u2tD1/C8a3LRrNxSmXeBCcUCiFKJ216JSIgyM5EcLxo1m3VMLKZOxOaesqm5MLUBfbEglDV60bYNTWCYzZtwZ9EsZu2u74hQTJnkeBGN6NGz/S57n8p2KEPy4KBUyN2GZExeu+9boSAk5KVoYHJnIcQgx/PQr+NvfPn5kMtbd1afuhPe/uCj1x/8I7x+Bz/4o/jBA7DGZofVHCgYDIiIBGrw9mOcdBjskNav3llw1xwN/jD1Ly0aBg6pvLqa5c76rMnKjO2Qi4OjIGfuk6akwnzreHax2+0GP12MI4IbgYFcqY6tcgMxrnbohxJmpEaB3esTgAPO0hTDrlromKujESYwGFqowKIIkaxmiIqkG25UCISCgkEtF/3g4TMoACJ2Mjfiaa7AjQABbYOc0WfA0ReoYRYQBE1A22Jxu3v+pN/2ePQ0D/niapeGVJ5v7f7to0UXlm04mjd1RN+zbZm30gYOR/z6S3Ni7nUQkZ/+M/f+79tn1R6h33u1NQBQSeDhgD/54OL+3dUicnWFZvbFLDDB3ANjyGXfWz+URkiJzQByJleYkKSsxZxracltdygOf+V0FSx1AiFGoGXbqHnXhc+8vCSzz9ydDWUxj0xAI0zkq2ULojKUQzZmvtzmoKUkpQAS1hgaIvRJE2HeUi6FstR+TNmVeauni2YwPWpnW467YfczX3jj8z91/8lX3rvbn+P7fgl4ABBWC2ABDGivAQA9ProAOTbD42+fPTjf9kn3fd4O9v75TnMJgYqi+n0OybI5HFk1CJiFRJ5vEmBtF3/wrZdni6vf//rlcuZdkFEPZrUDsKpFnRkseP8sv3xL5zNpSUCl0lht17x+79bRsmOmXJwJJBX6czV+ECaRqqVvimkpqlqs7kWCgbf7tN5kEIRG/9MqhiF3Z5BRlWnUSstgQIET9goDoqJrwUCMcrTkzZXtMpq1fkuvFjNpgpzMG2ZmokPSoaDs/Iuff/nn/97P4Kr/r//0D/7P+xeR2clP5s2ffeP4w/PN2eWOgVTGCi7fTCkH3v7g+Wv3T09XbTZtGxKmIJJUsyrMk2LIKoAEJmIQCVMMZIbzbaryKfOipYZoaUWUuC/EEp5v+z7lZasgmsWQ0u6751eB+WgZf/iNk1aoEVot4u0yHM1iP6g5bp3ExVEbrrcDMy+7hrhRgEFZa8VBtah5iULrZIek6m5m4nyy2pUcHpbh8ZM7n/v2w+uLp49+++yLb/4mzi7x2m0gIp3hq4+xsbwfHl7sNns9pLTZ27cfbZiZvrte73U/pCEpEYKQEaWkbZTAVL0zUinMQsgOVvesBnIB5m1cLaiYFEPD7FR7EMHETgZCpUmfbnC1t2Vnq1kGyM3V8f1vLhbziEl9p+pwzcUJFASBOZPDPfXa90UalkZK0aIWmxAERLje9D7OKh3r/FarY9UernL4igJYnQDFqB0ySdG1WHYQBqd80oahSVmRDFowZCLy7aD3jpsmyCGrqsdAP/PFl8E/jVP5+S+d/eo/e3qyiKuZnCya9a4cBiMhYjHXah9GhGVAcCjB+/L2d84+9eoJC8Um+Nj1xaWoEYSDwxhOfSYJpkrgEIQYZlb5rEmAg8jcG212vQPPmAgojtwnYdkM5dl6f70rLLJOw3a4qHKALkrXcBDAPBn6YvNAoQli6ilncyrFwMwgNd8Pmd2ZuWe+2g2H5BUAMLjoxbyVpfBv/s9v/O4fUGC/2pZ/89vvHnd0//asmD+5Gh5dptgQg7IZnFMpBGKemiqdhlTMPAYCgZnNwFym9I3cbNZJ04SUEhibvjdHxyLsixlpcTW4uchYva+ay0m+g3mEOAIj56n0x5h34dAPzABRKn4YMjMHYeFRXBUYbgjFDpt+r4izpols7od+CEJm+OjJ9WRfXxl+u9Gf2uQ/bXVAhAOO4wavLnHcYS5YdPA2fHhwP+hizsuW99mNXUHuMKc2sARhRp8s5dIn+rXf+Orxv/sTM7/c9OTIWmJYDBnqAJRBEsY+Nzhejvhrb2IZ8DzBHAe/Pj90uW2zFnMzpWTOxAxVsXHKgFsdR+pU3EmEipo5YhA3ZyYQ9VYUrm6qBpAEqeZdErg2gztR1pKM9qpuLoQALlXYSrQfSkqeSgk56d6pH0bHxqKZWNy9qHZNmMWw3vVpyIvYqFvbBAfFIGalQC7Xh8d9YjI3D4JnTB8+Haqezg2HNPYsBcGQp4nZTkxGREzUCKkZ3BVaXRdrfTBIMKft7lBgKedBLWVVtyjMzuasZspExKk43JlRDG5UlFJxc7QyqiZH4bgDDlW72vZVdFEUWb0J3LWhEB/6XksJIkyIxB7EVQ8pJ0UdWWzOTLztPRXUEYtio5zKjQzjNIu6yUyRDdnxc6/hS69iGTEYGDjblbMdDsYpexXJZ4c5ijqpCVNVmjDTIdurt2bzSMRyfl12yQ9DnufQhL5tpOo6UtasLAFdU9XOeO8S8xkOBeTIhr2t0/KkqkhNvdRnwUIozuTV/oXcnbT2TBCbO6qnD7hpxNQdClCxQmAhJvZQUYRrKaYwJimqzF4ng9fxouZcNQFa4O4pG91eMHFtTQMT1Or/CDJIM1IjDmNiNZPJFYOmtkhTr9IG4tEkFLhpEhzVkixkOqoGbpRp9X+8GaNQC7rMBEAY9YdX99qjO6mJIYRd7+5gIsHYojzuJCIzV4zP+5N9W1XjczLjGG6sdquMl6rjy6h7HDtRxm6HWvgH89ScQ883pSbQqLJ3uul1qUq5MRvA5Mp0N+J2BIDi4yy3pwMSoWFkG7/YEok4Ee6chMBcKcMh++1VWETaDbbuSd22+9JFmre8aJnA758fhkxpxACAIwK3A4IgTVVLF5SmSgMm7apPQzRHKeoELz/xFGj01SOR6rc6SV7HyjxEiAD1iUWePoo/QROCqGrYQPSJScIv1ov1Yr1YL9aL9WK9WC/Wi/VivVgv1ov1Yr1YL9aL9WK9WC/Wi/Vi/X+9/h8jk7HamFKPswAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9WbMlyXEm9rlHZJ7lnrvX2hvQC4kmQIA7SGI4G40c44xREiWT6UGLmV71rF8k04OeZMMxjUzSyPQgG2k0EAkSBAFi6b2ru6vqVtXdzpqZEe56CPfIU/wJsjplXV33njy5RLh//vnnHnGAV69Xr1evV69Xr1evV69Xr1evV69Xr1evV69Xr1evV69Xr1evV69Xr1evV69Xr/+/v+j87QkHVlUiAATUf5T3QSCFkv0gAJWDSFUBIgIUBFLS8l75XPm9EkjttCD1PwARVIlJtVwCJAomVTBBFeWMdnGuJ/E7ggIEVSUiu4hdvXyUoAoiKh8iO97+xvhrKCmViwFQ6CBhR9xr2slqSHmmk3mMLYMVSuXpyG8QCqJyD6QqRORPCq3Dp0pECoUSDYlXKa2kyzIBiaDP2g1QAjdErArSBtODEGYhtgyBEigwsV1aYZNRhllV6yRBy52ojkNVjik3rAAxkahAy2iV87GqAAxVQKHjJSAAqWq9VHnK+jwgVTF7MVOQLJSoFQ6RMGUOoQxBzhp/7Y/ebJqoUGJAqf5tdgAFEZE/GinAPrVqE0lCGkBlYgECg4jcPt1cyg0SoExQgP1kCuJq1NXs4FcstltOCHeBYmPVHLkYGhEpwOyW7mYBlA9LsThigh3rtwcigoqkZZ5fcXih66vhq826O88nr83mJ9HOTPWm/G73DK5c8iULBFFxSSAMQhdr+Wy5frHdZWl77fvcJ9302jEQacgST6bxsD26O5meTNpJVFGOHA+bMGuIiRhKIKEy+GUMVM3si1EU41GCCohElYrZKzQgBEbKmlQgqkQQMyoVAKqiqiCBVhOW8o4ZmkJVy6egCrXPkFmhIqWMtZ4O0+Yg0kloZk0Z5r5LsWlD07Ih095Ekk05g8x0il0AIFIlUEEeAlOoyOf2UI6r/kyA+JSWXzjcMQAmwM3R57DaKTFIiAIMeIrlkWpxQGJyf3CTAoFoBJ/xdxSVxB1BiZiKJ7DbjQr3aKbUTHho0E6izmgyj+20IS4Wamc0nyn/KHNLhtnl5sqPhqkKUm2X/e7xOt/2Q591kFUny1VSSNvERmhYD33iTrt5oH4TVfr1bk1EzTTMzmdxNvC8mZ/NuClAzQVCykwbGAMF/8xEFEBQ1YLYpIjETNQohpxFRUtQUFGQajEckUzllASFopqfn7daHwmUlFSDwaNCVTlSHjIrtzGi4XYSic3u4xgfyWauOq1PquNYmWoPHXvzWJ5cHILKqZgIBVXL7Gg1YDOBagNardNszccNBIdJHQMmeWyyzxObuZdwRkweWYj27MxPgAKfxZH2MK9gAEDKkblpuNWQGg2RmcluQxVs98XFwNmNyW/XMNt/VXyINkN+shpu+tTnlkMacjdI04Sbpez6DNUkEM39OnfXafOs4zkPN4MyLc4nB5f94qgNc+5X/eHDRXsQYeEgs5LU51ZS9vGHij80yENg8RMlsJIY5AqIAQEA1hrA7KHAAmFmEQB2JEFzAAsLFQBhw/Qy9BDSIeV2EJZAhBKwiCj6IRYWGdAS7EZ7UJtYO5AIMlpZYVQQmzl1E4JBfPmgFmuwK6l9lGoY04oUbhH1WiVIlAkzoFMtgFS9wWDWPk7KBPMLeslhFM4BaDRugIiN6KhSwzSJIRzQdtJjhhiY2EGexyHYM2Mtk6ykZSy1gJ97TdNlenS7+ez2xYvdPDRDSqtNAtF8wkPizU6yYNNJnyBK6HS36oasWVSJljfp4F6aTHhx3s476bb5/vunsQ0AUAdBYfzRyJW7Upk8dzopEKhSZ9ucXC14qDrtc1IDApNqZcOONyX6GKorMamAiMCiYBogachNDoQ65ogAMwNloMr0GnCRQplIzTtFDdxGul+txJlazQMI7MS/4hD2eBiPIceNw+22UDYQG0xZmIPTKItDNa3wsxCqMbrJ14yGdUS2cjBzoSHOPrnyXVZqAnNLkxhnrYZIBAYEDKiDpbKSeLJhvkTuQuqeq0QQyTc7+XIVE9DjYrdNAlaCYtvJkKGKTS/brvAkFQWRpoxBAOhwLYNsJ7Ow26X2epgcrKfHk9M3F8woMD5aBpGoUV43CbWEx8dC3YLMQgBCUAgpihmolCSGFVQClJbhl2JfanlFARfxOZUSz1SZOBAiSEhTuSvjUpH2QqJ5J1SJ2cOlj1gJfA4GNUrgJZDyyKT17QoFpFpyTTNedmPggkdiNNocSc0BzG/NwvZIvSqUyVJRv0MzeDXQKRZcchtPOqo3M6hkt04tjQGLMd4Mp/Ik1XrV0FHIMom9eOAza89BgCJsM3+53l0NDaiNlLL0CVBNWYdMTaCmIepoOtHAvN5h6DUypFwdClG5xu42ra+kPUnthKcnl9Oj9uBsCgJ7fCQ3NRU1Zm0hAhAjoAZXSiACq0JJ2IGAVCwRBIjgnI+LbaobbAEt4y7i+fUe7QZFcOSgrEk0A5HIqPEY29UG02ax+C6R+wg8zDivhoMbGUKOtKv4zxi0yk8ljyWAuCSZFfbcQiudKtBnuWQ1MjYeOaYo6oeR5cpjlHQfMaipAwXHVyJ2u6sJNaBASrLrdZeHzSRHkUi8B9TmccWDuFoeQCV8mWkrFCHp5MVu9XRzfbPLQkOCKKWs661kAYimC24C2ijbPnRd7gf0ghDQMIYMAKEYr1LudP0sdxP56oOrs68dzk8mHAhEbKDuQoY9i41LCYHGZuokKwgqasHWJoD3RSg7q6eajMLYIObIBBXiAM02awopZsMhUJCgIYnkJO00lJEtbL0MUCEcFrlHNq1EJEpEJMWeyqzY7XGxJ5tmi4A1lrESEbHWmEdUWI4BAFMZJnUuVoCoCA9l5spdmo0WwyjXdGO3TzIpSgpZYyRVf/CIsp8Q7NOs4qnFQgozVR16TUlUQSUTYDAxMfwxlMptEZnAVU7pNsmgdjWkx5vNdTeJPKTUp6GJDCXJ6HvsdgpICMgZ213eDciqAdoN2mdMCAHooRlQ1aymZdx+1d8833SbJFlGNohy22qOTNUnQQQmBpgYDLtD2H3a2NWUyN8t8Q4+JTal5VlthhgM4qD1LbsckwbEgCCUhmweWfKAvdABciMaoQkjCu9Nn5RHK+lJDY4lOoKFjOXV+zUMMuBz3l5hz0I3w9IFny0ys1KgWBIVLLc47DjqxyrIEW0/IprV71FGM7kySTYYIGJCE/hgFqNg2oel7CWxdrqayxa3Km8Y/7PMqzzdILwehpvuINCTXiKH2ZyayIs2RcoX10Ks07aBSpe0z9oLZSDbY6B1hRRA+T0Ek4gQ+eqrzZOTm+O7k/nJdDZvKrd0auZKhhMaVTBDhEoiacKoaGXPKsTkAklNB+yBuCAqCi0r0yUWDESYSMoZCKIMJihL6AYw7VJRORlABNhAzalUjXPu+nv25aQENQJ6ZoAaJ3nEC4+xowBs0sBLga5cX8Ggov5z/RD2/G2M6VSedbwrnxxPC1663/HI8mg1WRgFCQu+hIZpMQknsUkcbvLuhjoY/oKMCFdPA+xJirGXwAkPETrNGkSJcNvrapsVem86OZo3Cvri+U4JDdOuyynrkJSUEpAAAQJAQG/mrwxqSLPqFug3Ol3Ilz+62Vz37/z6ndOMyTSEEADUVL8ogqIejdQFJiajyB6lyhgUbC7Bzz1S/dPug3CTUy3qr4nCJpFokbVICZyhGvpNBO+GaWG8TBq5RGyPIkpgaElm6hxqJeBkVQwDnxE/PKEbOZ76zwzWWrYhZnumMfb5v9UhgVAlNCIoRp3WwMkZKyxpAgDl4jrqxLFoqeOjmdGbvuUR1eGsPA8HDhHzEJLy4TZOlA1r/dksM7Wr+j/L29XKQVD0veTL7eMvV8ubnkBB9Wbd3ay7pIGYA+vBnOZTXm5zFighFMnBcqIyuKpAhpGaAJWkqSeFXHywmhzE9qBZnEynhxQjF1NQImJSFXbqSoC7R9ESDNG8NuOUzNxUipmRZ84MSMm2i5rlbExNr0KlgwX5mSgTtNs2A9FRo6IUAyjHqlnv6Rh7kpoPpM9SBS8eLf1lVKuop8RM4vVMF98JrO5jUOW9chejILyX0Mj0KrDfmX/Oaa5dnzwxdhnMbwNkQqFH8ArSI1GzkxKRUE6qQ1ZEZtLQMA0ofGukciVYh/J/3TupKTHGV4Wk4U3SRcO/+6vn80BPr3cvlsOT22E9SGAmyn3S69Ww7cDEDClFlR4KYAIwISs6IEEzSrxGVKS1cIAIri+21083seW7by7C8bQq2KU2BbMTGw6tcoAneGLWViIIxCMGVNWyf1dSSx4oWiZFWUgYbCWFKq+ZeEoQorUI9Un7pKJFsAy//Ht3Q7SRHm3LmZczKBMfqr4Ai2ZmYT5T8DyxRE/39DH0wqnnyL5HOk6wMtRISxXEDNSz1pMUEuHXJedz9T6UicmI8N41SR3FRtoeyt0yIaPf5OmWFzIR0eUwPNdtPGyaaWD2qq17GPuVjfiXtwoTRkka6KiTP/v68X/xB291XcoppywxUIixE+l6EUU/IIsVjJMVtKEWNBGAxn9DDtsCWFVClIIqNDRhehBjw046qXDEsaBGXuWpQckZJamQV5h1JP17GDKS31G7BdwaLJH1+AtAKeUU12k6yLZt4vG8nUYViU42yB+hII+HrDqbSkVZ0FIHN3pi6sPf42r73Nq5m79BlleXbNkZAblubG/XmOsRzw8gAVgVRAIEjCkwQUlJiKy+b6bk2YhDM40XcRsncrSE5qRpQIpCQhmgwByImImLU1dYqJOm7qDGvUspgqDShLceHPzR976Gdbf6iy+TEBG1kRvVLLLaiWQS1UkLZihEFMnjBwO5sG0AQASkTI8nChnQG3nx6Sr1kpM203DnzaPINpICqsHJTKVosSRUNW4UblECSWFXJVczlXPEQwWgWmpUSkAxTamURISUxLgVawgBE4p9aFIa+gSdECF6RFRTTeBAZlNhjLAweLBWjcoSK58641Mwns5kgkylUuWOyTQd8qTIGJpJ+eQEtYZFvxvDRQ/yAJHX5u1wRnXSvSQE5guE0YhHL3WdSFRBedA8yDDkDkJKmZQjAvHfJxCO9XVYiK24SKNKihDw3QcLbPunP352MGvunurjq8024Wadtp0EYFDkTK1S21BqhQc0gAKhcDJAQNnnmYDkIFeGegB2N4hxF1o6f21xdGcWmwm9zHsUHhZLhCz9P2V0xJqqrNKnCqIsApGckHYpJynyoCYRApEyM1FAUDbotppEIBWQElQpCHJkNE07ayag1baXPFdQHGGyZhjV4U28gGeB7s1K1WRGhk1UutNcRVOzRar8D0W9dMWhfKywezbdulgZeZVzD+qwZ2YEl/8LrXIrr0Uhg59KUR0gq9ZCChKBpUBWKE59JpEcdRsTSKXVaWjahkKhNbXOa89SQE3LM1kWS7Uhjo6Ivtny9sOrTZcPZ+HHn2yuN3lQ2uxy3xnoi+quU2JMJnyQseskA6KQImRAPdUqUg8I4FoAAkLSLJoGrK93FgEca5VqBloAVlXgipUVjAsG1Y61bpc3113q0/aqX15ukQkBmgUARSai2HCchMmibWehmcbYMBEzqyhCaW4DBCKBZdb0HEmQ+pxSptKvQRbGxnzJEzImFDpAVR0wA6v2NYZXg7/ScDOGGBNwrAro8aYyqRpnKwLucW5P9f4+jYfLQyzG/lic7Zulj/KZe0jJMJj9s6UwksUhAzEJtYwg3WQgJlE9CDFOA3OZaavOZpAGf4RS6lRvTNrjQH8Sw/piO4/hZj38zUfXn3y17AZd93KzHlIWZm0iYiAOEMXtSpJLZ6XIVbPOcmbZC6PqjC0B2Miw7uI0lsooEwvERU9y7GO1+mwlNTVagQii6Fb9xWe3Lz5dduu0fbHtrgYlCCEJOAIRLTEFbQ/b+en04Hx2/trBwemsJh8ECkSRIBQYLAfopq0KCMMwDMQc3UJGgcBhw60IXqUf4+meOVgvhsV+x0X1CmMRDU0ng4c/Z4ReENpvNvRaasGncqCnB1qkRsMVeKZa5oWwp435OY22FzsoOQVAjJRVQH0m64kBSFsiTDkwdyGHCALNKHIs8ZhLUT+rEmkqebJDWL13LaIKyXGWg6vtzy82Q9affHh1cbXZ9KKKGemdg9ilpIMwIUOhvOmlHyCA6KjT7ptJIWSNm1p54hJG0wbtoj06nxaFrORk6gjvVVaxGVM1+IWytQJAsm6u+yc/v/78h092T3vpkQZQ1kHQJe1UI6MN1LMoC8IQj3YP3sP56wclSyyjUETfyCyEEJFnlMGkFIacJeeUIrkbVobr1czaQwVnhxbY/PnVMQnO3O1nQx5T/8z8oAxrM6zANpLp0rU8wtVYzfTLV3coVqiWMBcuWtu27bbrU9XyP9VbKp0NpW0PQdRTMSImMDGTsFHLAufMBKJgnY2SkUkqtUClZqUdreDa8vPlv/rba+Schvz54xVyDsykOgl0Ng+rXpJAoLnDtjf9jBQHAQraZRXPBtR6kSxoNp4fBELrwJYH7TaZI1exyCiqWIQ0vdF64gEqwpICpILdcnj80xef/+VFuuiDcr9LQyYmpIysqsX6RUV0EBBhGoQjxyYwe7MXE7LUhmYiRQwABNJyyJA+5ehk3zGE9oygYEjNXzFSHGdS2DOySp4KK3afpALArDVVMNN1pmb5p0t3Rn9oP9GuqYIJiCUjsvyjSGda1G72RNVt1Clk+aEwWxSlseCuekZs+l5p1lAFizdFE6raogCE4Z0C8HTf+o2LzSpePN7+4K+e/Oobi2HXD12fVSfMMTIIDdAGJJE0lBtlhQbonTleP+HFJF6s80fP8zqXWKkZUECACSEwGmCVxyiegRefbV98tXzjm2dG70uosb724irFl9WDJUq6TqoqsrzYPP/pC1ylhnnXIWWIqAC56M6qUAxSAjoxNA4Y1kO3SbOjko+xJxzj1JUigUOWkKgLU/XvMunmrgYSRZuuxW2q8FV/NNM0sPO4DyLZS9bgkKR+JW8xsbgNHYmfE/7yVynhGWxZOCTD1BrAycMjqOKfRWoas14PtApCtX3Pusq0SGkIdBtUa8Qii/4WlPdzIK2pMxGI9HgS7i3iR18un25pQHh4vnjt3mETCaIJJFkka84aCG3UeYODiFlDR9Nw77B59yy+c85N9WyvR3WKJBgyAhAAOGmTXjc3/W41eBqsaiW7OkvkP3o89kCSBlk92ejV0JaIwzKNFBgi0Nr87zZD0AC0Wbsvl9dfrPrt4JVDtaUtXP7PvKeAFqSJxamZSrSuxR2lcnYSuGLv8FXuWC19N1+239sT+oS5qGCQY8zKJ21sYLQDlbwtei98FwP20jubsFPNG/V+9yvnsIjprqD2WcPRalxKcBys7SnlmNLcYGf3E7LClvi4VxVwNBCt/6Nvv3f82zf3fvz58j/83huSU056cbv74S/S1WqQTpJQBG1EJWsImEdtCdOAlmkatWV+uOCvruTRAAICanM9OkUEAqFEKXNLxer5zvPqQizIwMxCj7l2ecLygAXNh23aPNtwQoICaINEoiFRT0A1Mrdpruh4lZdf3HZfP5wuJiBnyS6+ebYhXm+QonIVKN1bzmAzU0OhDfXYulrj0B6H87moka74kdZpd3jxg9jIHrkyOOaZdnjhSOoVd7caQjVtcuv2M49H+T34Qd7KPa6QsU+YCK8CR8USQ2Exo4wfg4hKhV/t2eCyO+0/LBM9TPL2quvWuz/59bvf/Y2733i4uLjafPToZtvl8jwCToqgxIRFo3cW8c3zcPeI21DqQTRv4+mC5wSGoRcBEZgC8Pkui04CgQVxGlQy+dgWJdSnAiBrG6rByMdah03KqyElzVlT0pRIMtqoixbzpqwvMiMjNzJRUmC43m2udzllqgg0ToTBiQVUJlJE1x+KXFF9Wtn0+mJvoYRgtWkFjWBVAlUlmWwlNG/npsKKCNBKuenvhTxX/Q27/JlgxMjiBzFbe6uyksBivkdK8oTYaLMZQ7l/p3q1bFzoBGkRHIsErYXQV4dS61gr7XHMJB58tcYgy8ENfiPondvd3Y9uPvts+du/eu9bf/IeXux++NHVzz+/vVp1opSFNn3a7HLKGhs9iDifh6MZtySl9bDPAoJIZiir5ZjFFZIXA6wxu/A2QWyhWTiwwSsZ6/POfTjK2YCaNs0qGZqy9hiS5JxVSFQZmE3QNLTdUZ+zil09GmFHZG0I6TpfP14fPzyat6E4mXMllGLpqKIowMresj8KQDCxU+2htEZJJ9MOYQXQKpwRUTH9uoKyTkDh46X+Vtcx7BmTodNeA2NZvON5YqmvW7u5HWDhsMbovbNxfRQrA5m9+N9a7dpkaIsS8HAxQlZhN8xM5Ov32IGhoARApMwIhP96Mf32Z6vPfvzi4yebb/32G7i/+PSHj3/yyc31ahgyhgHrTpbbtBuEgUmk41k4P4inM1bSLlFkBmFIukvYDpqtv95epVrQARtB7yBXQIAAtlZ8WHZUkmMqJ/ClGEaYuCpTmpFyzpmaQPMpTxti5kkbArOoMBCBhjBjzBgN4TDgIIIYkjT3mYLPntFur++oqPlomQhmlwEIpN7wXnHQw6VlWjXcWFrgmZr5iVbEGFm1G24FJXqpzxDkHxmDcoEmH4sCJ96lVJHOl2GQU3KyWoBVuJlhOS6NfNjNp+riFvjYsUnqoeyfZAIzmKiMqRq6gRAI1nxeTHICOrvtfuudOyp443yGIX32P/zt//L9Lx5frvsh5SzbPt1u+/VORNFEmjV0NMU0Sp/SaiuzSVDFMOSUdTvo7Q651KYAcjBTrwfAmx8V0KzH92YcA4z+jyHSWzEZ9VYLFfdRFdGcpIk0aeIkUgjMjJSx3ORNp7OA4xaHEW0AExrG0QRtBBQ6weJ83k6jjtzFa8A20oa5ZaAjWcMoCKMpiRFGmxCFUgmdLhySpQAWa6t65ec1A1NYM4lHuCKzsnNnt+kqabjzlno5LJAb+nqo9nX7His9XS7ZvkeykYr4LZcYXhaBedDboxaFVZQCm4zElMEgCuCyAmMcAlUoj4q19uD//pPLR//mY1mlb719/Hc/ePRvf/zsi2eb3SBD1iRIIoH0oCXR3GfMIrfR+PnpPM4nDNUslERvurzNlvPkEhOAlgFQEq1mV/B6esInDw6n8+hkFFYBtlSvikZEKqUG7io3JIuIgjSLbgcR5SbyLuXVTlvC66dBs24H6RK6jCZg2gBAn0BtiJNYEzKpaGNBTWqDQQGd6NRmFPDHgEb1XkuHUvF79fvUah+Oc1o/WsskLzVRFFkH40uBQntssW9NJLUsHYQbb2Va9fxmvGwmW1qJnRGYkXBp6PAn0XEa1G/YGszJnk8J7LVcKxaz/SFSCMoOE05LLWSDAFbo83eOv/nP3vu1QeeMR48vL2/7bpBBJIkpJ4HD8UwXUxZoBM0Ch5KEmBihSnTTpeVOT2a47dALSJFgExBJiZAUBLTF7wPiNEwXzXQerbu82hErCYsLhlqw3grOpTmem2lsj9ruRb/tdddjEhUBw4AsdHSAO3NabiBCbcABiEkaxiDgAOzk9snq+MHs8O4BeUeSKgKgDGS2RMVMX70z0NEIBC8N2K99csmXl9lhNEY7rTbj+CFudVTWzhdTsGVqrqUVIKt1w7Fqak4I145Rc2U7sLIWt3O3+L26AKG0KaDqzMVF3EzdfolYC8+q25LsDQjAajhhNK486Wi1PlYKEAd+56A5mMZeselyEmQgS1AtuSszIRC1gaYhzCNPGmqYDiZhMQ3TGCLxzSY9uREBYkBkYkJk89pB0QmSuqJWaq6K+Um7OJ1ycBLq0YTLYrI6e0Yr4PotBcbsdHJ0d8YBQ1YCsuqulz5pJGVCzgqIKJh1ErQJyCAiMIEHXX18df1olbqEl7p1LM8s1q3OxaJFpBJelcbxHecSo/sCUpe8wXMeD1NWjC+Kbil8qJN2NxSDONP3S9NsUQ883SCMxdaX/isleoUtWfQKnp/e+oK49H1Q+X05hv2SDtimCRczNe2wMjytbZWoUbuu7/YHMRrnd2xj9bCX15P+4IPnnzxdvXYUCMW2RAlZOUAa0p4g0AgNgRikIt0gxNhlfrbMz1fSThAUlxtk0SwQoDHBzErs5e8MBCBl9F3qt4PkcU7IYK30ZBSuVGpmI09WKAJN5017OkUoC1VUhXuVkqOq6DAIk7bB0tjsA8eMkKG9dMudJCk8VbMComq0VTKgoLLyGOAaSypR3tMr7Q5dvy/25ehlmgVKqbFKHoAzcHgcNPxTcsAcWb+bsIe20Xbc3KtZjHaP0hBa+UgFO2eZdh3D5RGqSeuPdq7i/szE7PVBjHdXWm3LO2PHvcceoHZ12+ReEP710+XPPr+5WfVdoqZgEZV2D1UgKxFMOVNFEsmqveDZUj67Sr3qnROeRSLQJPIsmlUVfhMJDSFUvbTIHIyhk5y0CICMir7wSWOPlC/ty2QP3vDsdDK9O+NAAEREBVlAQBMIRAFhEqgpKwoBlbIKHRr4+FfO779/p523bhfjllDms24kAGIlOi7l19ip1VmrIuIGUEmS2afudRTRGMyUlAVl5flI5mgUVkywspDmwOBGZiFMnU8aq0CtCkjt4tjLfavUYIsPqh3SS4tfSyItJZVktqe06j2UuawX5cAIgZj3y7/lRotmECzXAUDoW37xG/d2WdP3H7dNaJtI6EVJwVk1iYhSqbCQsgplEiiJ6mxCxwtqI3eDXG1IAYGsd9QGnToH2YnbnDdCKpAFbUtDlzxyFGioDkm2zJ6sslsDqCoUFBo+fu3g/JfOls872onC1i01wLQt6ZK0IWTBoIrMClVFVoQzuvPu6fGDA2KSMTMS1VCkE+IM0dIJQ9DS5+hdEIUhK0DVLKTak4WtEYIcYhwAFUQQ9b0ryPe/GFdO2Wt0KzuNiyGso/hrUdUM3dUyD5f7pMwSlZIdOxQb2R3TQW9V9snwyKVKzEAAACAASURBVFdMh4nExEQXb4k4FjBjDszZcjUnIV4m3asQK4gwiQffffDGoj16vLy82YmIKJJoFmSlJEJAVE4QEqvFiGbm0DKJlnCjSZAFD07CO6yhoY3oo6c5MFbJtAwAHDAIJgs6vHswPWibJlYIr+l7HTXTDiz62B8GNNDB6ez07cOnH13urgZkZaaomDXUeLNXICiJJIiSiGalDJ0/WBzenXJkVfi+PuMWf2SZVZGwVUGxTLDHBAc7gwEl7/RV6/nVWousU29R1mBxDGRe6qpxCyW/G3WOUlksN1gzSpMW1BEfxuHcmoxQjpyRfYPIaux+ZpcvbBXVyzmI1qIREasKUxCR2nShREGZOZSAaosmvBBAbsr2zIXjMjEmij8G7xQfrVPpc0uCIYsoRDSrtsSAiooqAgigwIhRQRiS7LJmoYZxp6GzozCbtet1/9qimXXrw/PJzU368Hm6GHB4h4/emi/OZkOf33j/9OTeLMbKrR3PjIwYA6pb35QQR65JxpaP7szO3j4Znu/OsqYst1tMGcwqqlmRc04ZnVDKmlWTIhPxJJh8RFpaSPO++GBlLxHT1hGd79gePjXVfMmOVD3yjTK8BR8IKRMVtbXAGMQEUp9Rf+Dan20nKKY3pgX7mOcjZYKAx3aPB6rWoW+m6tFwTA9YbEWylm1LMBqZU8wKbmCwkHDpL1GHxvIXhcrFxoDOgDdHeYZbCNzhkF/84OKnf/esmUYBZyCJqCILUhYoaWAp7ZL+MCEEJh5Eh6RZcLpozxfN84tdG8Nu289nIe/y8SzOAs7uTSe8e5epJRqI9Gzak0xncXHaVu5QwKWaWjU2EzPMc8sWMEZgpoftg68fHV53b277vh9erGXdiyQVyZq0HzQJ9VmTWDuaiErSsh1EUTjFMzyLjKUnzUdcoeH9790LTlftYGYHJtvSwozAAsrIuJ2t1MwMAJU9NeohAHnS4zpFFVbrChGrEepLO2dYXDO6T0RWudsHSR/d0RIsRteg+NIf+CclQwcJoiFQKdu4WZu9UyBiioFDZA5cdmFKWVLZniuULTfI6Kan4AzaMm+7/HDIWXFx010th25QKxNCNbNSFmWoBKYAECMwCzQlJaImc1Cdz9swCVl1sZjcXG5Pz+azNkA5Rp62YcEUBK1ovt5N7s7f+s17hyez8hg2rOokWB3/q9sW0HC9tMQFBrXrdL5OpyHE2Ma2adrAMYKoE/QZg9KQNbtOLUyn7x3e+fpJbKOaW0JEGdwEssy/7J0pAJFk8ToBfLdXAo39VuJOr2MjzgjK+wKaL9d0794TSNQJnGUYHprFeRuNrT7F2io41ZBfz2Owpp5Lqjec2q3V0OhCVzlNkVgVtv2gh5aasZarszN8QsEn4v3mZPVhcg/be9TqH8z0m/cPvvP26XInX17t1p2IKKsGaASaskOeKFEIQJHTykL0g0l8MJ/eP53mnd4su64fVLTb5rZtbm936yTMxEnnbWgYzGDldiP8wc3q45vcZcvLCaO64XdcW56stEjVP2EroQZMb/pmwFZpiDFM2sl0Mpm1YTrhtonTgIYQWQmiEEJolUM9RU2NinzpuXrZYIZsJmJZq2d5trEw9kDpRN2gl8Hqe4IVIlW3NdpDGpTKD1VFzH7nx6hHQ6ojUeveRvX3JfdaZSCvcY0Uqy4U812v4Y22FtBYvUnLgczjZ/kVGLZHHFiD2laMBGJGYA5MHGwMzYALbSxx3hHCMAIANCS9/fT6Zx/efPTV7eVNl7O2jMDlvgmUoRRYI3PxfAaO5u1B0z6/2uEwHM9CZN1mEeWb291KUxZtmvDGIh618d6dGYb0yRPVNq06IRG93D7+Hz9cfXTz2j96/ej1RbkrL8wVsNJx21Aq/bZjgmbNgJJpI8ikHAkSAocoITMxxRgEUE4UVIAkGhc4ee/0/O2TZhI8PpNrXzYrZjRUsYMiRvpskFPbGfYoDdVd8qwZokjR2McM00PI+oe0EntvI6Q9CFcD7bGdu7J6VbbzMVcWC8A3ISQad4GGWoqFMV2mvbuv3UOEMcHR4scAlRo5yoJ6UkawHTApRAoNNbGkmwW4pSZv5pIE+NI38i66zPhwnZ48uX12ve16hICs1m8DaFYum5pECDO1MXz73fO7bby67u+fTW9e7KTL/W54scq3Oylbiv7W+6e/+e7Jg6PJZt0vt/nT260QjmZNG2TZ5XUHGWT3ty8+/Gz54I/euvedO3EefTxQEyJnZp5qWuO7M96k2ufAyNnMQVSy6JBykiyqxMysHCUoHbx+eP7u6cHZ1OemtMOaUFX7w5zz5LJvYdSykZS6BKZ+Nz5VI+eHFpZvO4xXDNPRbgtX5zEU1VvZP0k1+jr5Tulq47YysdRrjycjHx+qpylQ8VK0HZ1nbzMPqgUoGEfh0u9jW4oToSy7Q2AODcXIIRKH8rZytp2QxgyncoSyB3SBB9brd46vfvosK4gzgYlyBgAeRAXUMjFRw5g04Z+8f/fdB4uvLre7A14u+89uNk+vhmc3uuowC5hG/Ok/evCH75+HrLfX3ZCUoXebeHwachNudkNYDyJCSr0CV7tn//Mn28fr1/7xm9OTBlqa4i1wEdUyp6GPVD1gyHS5Q1f25CjDJUwhcIqRuac+pU0n/aBJlAJ1u+H2Yq2E47vTxdmMyja0ttpNHM32SxMAJHzj9+/FZr+vq9oXMazVWyt/L+DhPL5UJ9mbceBb1Xl7oGMUeRCHX9rkZaf5/ra5HCwlfTld8I0ddZ97e6rHUFX2peOWAOwL/GR3XriZJuGMCG2bwMROxYgDBQ4c0YQQmhAise+iJ4IkkrKAictiH/LbqqhPAJEeNM07p/Hrp8NNT6s+AKokUAGYuQ1oAt87mt2bNVeX3Y8+vfrrT66//8HN336+/sUX+XKD3YBFi/Nj+i//6Vt/+Prh9rb/6HZ3K7rcpMM2nk5D33CnyDk3IXAkZkpZRHOkMDzZrJ5vJw/m7UFrI06VglSUR+Vx3Ak93vLn67DJqpCirZbmYeZAHBgitO5Sn7QfpO+0Ww2bm023Se28OTyfU3CcVCBrDCEQawkljicyaASpV7/gRJ/KwopCfAyjfMaMhZtaVfsmMb724yDKqkf4Rq++d1AFMuNW9Xz7nLBoF460pAyKxCDtReilxg9xjWhkvGP+QZWcWP5Q8gImBCa2nZaVgGI7xtjYo3CxeGZmIVt1XQsVhRToOC5GJGl6Opkctw3w/H/6hd5sUy7TJ5ElME5mfH8an3y5utymp0vZANcrJAIYE8Z8iq89aP/s919/73T6i6drmsX1Kp0fTr722ix2+cun24FkTpBIHXR3PeTiIUQqmQTbv3vxaJtf/xdfO3x94WNa12aMLq2qtBP6ch0+XdMqq6IUx7Iad4sBs0kI3HDgGHG1Gi6uuwwMHYYLgSzxrTtW2i7YObIktUXlavwHROH9793lGNz21RHFky53WIMnqi6sakgzipUgE/AdqioyqpeKCrAQ+d7eXM2bTIZgj5GGdVRr2Zg38U47nzfNkCWpf10Bqa9aNySzf3PdA2eUSYynSWmioJYphsDF2mz/T4CUbaNQtnzTi+hD1pSRoVSVW3s0aN171zFcCbPzWfvmMdoGm4Q+NZGmUd84Xpw18enTTWKazOKzVdoldD2gOJrirXP61XeP/6PffRgZP/1y+dq9g+ky3T1o7p1MRHTZDVc58zR+cbP96aObJ1fbXdacczfI0OemiUXhzjf9zaNle38+PWk9PaqEmaCkWXmb8HgbPl6FdSbvRcmi5Yt53IkAaGCKJbtUjUEByoyH3zl745t3pget52VlgyqNoBDYYMZKS5qzhG98734IZY49VFULqRaD4uN1xTO7OloVKy1LAsxU2Mu26mvd/IQ0RucaK12uI8eiMh5koa/cFjMdNe1xM4kcB807SW5FVTRT39cKJYUom4brS32PxflAGQ20JSpfQ2HLNJhKczYTEVMJH+UtDiSqKemQc65do9Yzh7Gmg71NXxQUeHoyPXjv5OCXzs8E+WpLoNePJqub/tlVN2356WXXC85O4nGrr98Jr503D8/n3/3G2eVN98EnV9/5lbsPF5M3Xjs8OmufLfvnu3RxtX385frqant9s+U2DEqqGibN0KXFUSuZFJKSELNc724frdq789nZVK2wB4BICVlw3YdHa3y2opVw2Y2WAFLJ5QtSUBreskBELCxCAxNAOef2bvP2d187e7Dg2oNfNApBZA5lMYl/pQERS9Lwje/dDcGnfiQ0Y2M1oYqze+iFCkFa5rpWMsu1rRW6EkGq1jU2eJnS4arBmBAU8yE4sTOBahriPLaArlLflf1FHGnwEmT56k4l2t97j+BpAIJIBEWmGNiemx0ViYiUQjE9Gpv4QClLyjIIbL9wL1GNjwknmJ7egMCBvjaNf5pwfza5WPW3g55RmE7Ak/Z2M7x+b/bGYXtnHk8PJifH89/5pdPc50dfrf7gt19bEPfbvj1oP/zo6qcfX6+G/DzLzbK/vN01xwc9UwOwapdSt9aUZdqyqCojC/IgYT3cfLFu7s9mpzP4WFIv9KKPnyzD451uhVRL41oZHhFky+BFwElURLNIFojKMOQh6W4QXjSH9+btQdu0DINzhRCpiUE1qyvBTzLCN37/bojB99Kt4adMTEn5fZIqBhXbq6NbJAqbI6tA7yGTH+r1dBqn8+UUwEQ8j7x7qUnhsmWvgG0elsOQVRw7tJqlzXIxFG+QKQ7kyGbr1VkokjbO8c2c2e2cbV/tYmjqdzZkSUlzYbBELvqOHIFYqX4RQq3igr55vdUPrn7v66fvfP34y81wqGCm1bI/AuZCkVgHCbPmO68fv3N3/m//6vFv/Or9N09mOshf/vjik9Ww7VOO/LPPr5+uunbSHJ3P1n263vSt6vZ6oIaOjidNYJ6ENGgaVAk5SYRSn6++WE4fHsyOWxBTVn6+i58sw7OekhT/CVS+osK+i6BsYCCA2pccSJ9EoCLYdFkVfZL17dD1PTc8PWxjE2uEhaBlYkM5Jd+ULGfx/jMtCUjBeyvrV2ESo3JQa+6eJRhHJz+yKmQjnrk0X4j6nuxWPuX8Wes3vwi8nc3pPKDAIPmq273odknKfluFbRVbKiJIrRgU3VtJQQKCLXwnWN9VIYguH1l6IOrZD1BalhQQUVX725d1kJNJT8/3ntkEaePcNmqPb/s20XQeH9yZfvtkxgCptEmPF81kGqdE9x4ev3//6LsPF3/90eU7b59+7XhyeBAfvVh/+Gz74Kg5Ppl8+Gx1nSCJFovmybP1oy9X3TrFecvHrTSsgXiXZJPAJKTIShk9EHY5P9l+/Ocf3n6+hAovh/D5ip93ZGxfA9fAYjMXiASakpRJ6VLuhgShlKUfcvnOE/S4+Xjz5U+eX321GrpBfbJfAg5fVVX2toxALe244m/lUBPZiwn4okHT3ws+wYe5JHGjsFRCSdXkYCcDFYKAcTNosyYV9Sy0vAGGb2lJEEghEVq+yU/HUxJ5J24hFWZMytCyFEI9AntPSHnUejtQT5qlKDilw1rruGhRH8s2CGU1AQL7hu7VO22Q1UZGLb0tv/nma4e/8dbx7ovl+rbbXm6poRePh8OD9vj+we+9eXb3uImi00CPbrsc+d3z2c8/v44XzarL//i3H8wn8c//3aN41B7O4ntvnjy+WHUqZw9nV483q126vh26Tu4/DBgkZ8mCBApZwjT0SXLUg4YuP19+8S8/fP2Pv3ZGARc7SaL2/La7atG7ROwbTnZ9HpIczpshYbPNIDDJapvMRlSYSXq9/Xz9+OiyPYgn9xZFRWM2UsSAsFIuTZFCQCT3utLXYFpsna2qBZRshWW0KLM63Qt4FQwKejgaUZU33DLtHXIooQqe+99zaKe0dgw1CDNrKNFfxbYagvrGqQBBpULNHrPcU3BV/QZGPwJIMxBUy4OJBWB43qQQKp1nwTNzHzna31kA5Pk8GGhV71xsEenDL5bzjM+erC92aQ5uG/7n33nwtbszCEHlg588+8mLzS+9ffTRR9ep4c3F6q0Hh6dHkx9+cXt9Ozxo4j/41t1lLz+4Wq83idZ5Oo/LZU8tghCAwIyIdh63y16zRObQ0LrTKdI8ED3bPP3XH+sbx2dtQ9CcKWsmIAQEBgNZkUUDU856s+4X0xiYUtLdMDCHPqUhyaSJ3ZBACIzMSFs8+/h2djKdzCfzo5ZLL45TM1LKkodlL4KsGq0XrpQqa8h0I6c6WtWQAHCwDZq9rPeSgqaWT6hHaJsLJzPFkn2FHI2A6lbqCSpVBabckFusl9HtwiKWrKMuNnjZgKupWZQv37e1Z6FKBBFb2Fi+cLdcW0Q4wDd8rbERlmJgT4mmenqPmcQlmn+P6K1eLm6H988P/s2/++rnT1bffu/O+w8P/+DX7zVnU1xscT798v/96slumJ5NLy93zYQf3l3k22424R/89Fkf4rfeOfvdb5598cXtjz697jpJWxzfiYt589XlLjQEQATNSZN3abVODVFuA3baqSIgZz2YhSmhvx0+/+lzeevk7slUUZbTQSVDg1DZ9yDnQKttv9r154sJQFlTytLtUghoYwjMMZbVscpMnLW/zBcfXh7fm08XkYOvP/F5K6pDd7npN0P0uOx7cDkEKMCOJQ4mXLVJwEQDBZMFPZMrYV8bZHsQaKmyq68Y8LBbYc9gdK/mWpDS43DdhNreKmYrHgABk6+o9u/5iU3TKwbOozGrgspe5qWKDxMmjCESjKaVnFKIo7V3GF0EAcpeOjWr8isx6kAqQG9m/IPIt91w72iqKf/8dvvLb5//N3/6Hu7M8HSNF1sEwrp70g+XDHTpZtmdH0+/+8bh8830rz+/ofXwu79zd8786HL3lz96lk8nTcvHb8yaIffLXkXWz5QbHMzl+fNhu9HcIBCFGSfWMGiXdLEIUYQnUbbpei3T+frscEKEkhWGYJElF9Y/yPWmh1CIpKIiGFK+XcvxImoEoC0TkU4i56zMkKyrx7vnj5bH9w/mx606w2UiFaJAcRZ5EncXO658x9GIzJCMzToMVQP7+z9YJFUYLhgultk05KHax+MgNCISlZopyvxVVoQR6fYuazFcS4cI1YpFoVBkXN6wCwQDL8M7UyOhavZiDlX+ds6gnlQYkJYj7TEEUBUoBGpL28YnG/uWCq4tQP/JSvDB9WY9fPnF8r/73z/dDfKf/8M3MY349HazGb78YonDtlfpD8JWpe/z6Xzye18/aUEffrXcPt188/7RuyezTx7d/j9/87jLOfd5MW/mrOm2o2mIDU8O+M7dSWERZ29MskCy9kl3KnGCUGoeitxlZZGgm9V2tR4IHBht5LYJTQzRFkBQ36chlfY0HXLus4qgT1kkb3eiKiESEbWNfVtUCMgdLj+72i67YipaB5MURKEN4aDRKce9ISbsZ3eOgWQdPnD2XXmXenC1Rm7bcL3EItQdPquN+Her1caf8dtJua708/xBXQ+uU87sDSAAiZYFBIZxJYRJabwwmFSSskuH7he/imvY93mQli1qxBrTCjEoXia23zmMbxiWlYVFtefB8xkqI+GbOYvKIei/EizWw8dPl+cn0//tB0/vPTj6T//h6eKwRcNb0cyUiFZX2+//4sX1cjifxbdfP7h/Pj1c57+73PAm/9Z37h+I/tXn13/92RWfTnndUQMe8jBAiYYut22Yz0Ne92iCZu22ORNkwX2nmtH12rZgkWbedL3klQwJVy/S08PlwUHTBA6BivSaVKCqJE3kWcsqkkWzUNenNjIR7XoBYdLShJppE0TRRtlkJQFlLF/0u2XvKzaFytYfBTkCtfNJezJhqInaoyrh4cG8uIKXanlPvEzqarhBBKpRVNCTGkP811R2b7NcTOGXGvFKDUjg54cx7fIF8KQ1G0Y90vFM3RjKt+dC7HD7jvkxAbD/g8r7I8yVlx1IUrHP/6Fmavab0vxcziEEhUpxKfzRJp+t0o8+eD50+sNPbv7w/Xv/4p+9vbgzw5DlYnO56mka5gfx3//w6U9/9nzQfC807z08PDyaPF31mz6/+9ri7HTyfz29/YufPUvQYd3zNIYYZMjT83lmxGmYEMv1TnaiIqnD6jIp4WYt0wnPJ8wB85abNmrO3ICnIRAdnYfl1aYfcvmiQYUOQ77d9uttr4ImRiaKkZk4pbTrU9vGyEgZQ9KUFaTzKRN01jK7FC07bFeDJDHVfszjQaDQ0HTeROM9MHVuLDgqlS84s1DC5vZCWtd0jAzd8zUn/fAwaF/YTmO0rIKIx2XyRNJevl7ecILsy6G8Sgu3TYPFvUYh60guOSmoaCjiDaX2DVheWbEA7ZTCUFKpKMqlWiflAcqg2C8hZReP4r5ghYxfh1BW4grdE/3Wi/7DT6421/1ffHrzZ9978/yNI1x2mBAEfNJ++pPnp+tBAm27LKQni/bX3j7GJCDJTcvnofn08fL7P77YqAxd6tZCi6CLGSNDsL3eYBIpslx3HJQD6YTbBR0vmhfrtMs6ASQSOISGF/MmDUlWSdvQTHW1kYXqetcfHrRJsmZsdmm96UEIHPqcVrueiVKWbZ93fVrM2vkk7Aao5JyRss6nk023mcVws06lO6AfsL3d5ZQ5RAtsqMKOMiM0keE+7vEJ1nMJ21e/ShXq5ljxq1I1VFizf+39qARDP1iMRtkDFm6sBBJDGVTJ18K2wtdfw0HTr1AcRh1qy8GONW6NxhQdfvyDe9EfqmoLQwt8SkVnP7lA1QDcwY8K4zfVbURiEkWA/lMO2KWd4sOnq3/y7fvnDw4xYRw1yIpOHn1yo1nOHxxc3HS7Xrqs79w5wNFUvlh/9fny/N7sJ8/W/+sHL/7uFy/6lKcnMxzGy/XQDykQkZC0IR41MuS4aA7uLCirZjo+m4Q+xyQ5o++FIpFK6gTdoKXNpJfNRpa3mnpsNpmIctYh5SwybePBpCVC18tml9e74XrV3a77IYGU5rMmsKiWbdI0Bp7E0ASetQGl21Wwue76Lo9ZVy3wAQpqJswmmeo4OQrCS8RcR3ZubNizxZHpO5aYTfncjmesFlZtdO9vE0elJhCkZaG/wvZZFFKeBX5z0syJPYB7W121a3ejwqrE6aa61ev48PaHKl0wD1KUbwmv4VIgHiulJkj1YuYSVFMIUtwTPHy2/ezZ+pOL9Zv3Fu/++kMkQVasE5i++Pzm4qZ/8HCxerFhpnbezDj+8v0FTpqr3fDJVzf/54+f/98/e36zHs4Om7fvHbQtLzdpu5I8ZG4CTibrPm+2QgomHdYpzNomYrjq+mWOgbY77QNUZTJpFSq9HLQxHLdoqctoJzg9DU2k6jBNCG0bQjCRe9oGEVyvtptdD1WFHM1CEwKAIeUihkzbCKImlgUv3BA2y076PSZUczGvm0ejTMSkKqSsjNo3zqoayFhuVZXAZjEEEnLhrUoWCl84YCqBmMbwcssw81jjgalqGLMQi81auo5PKPzx+eIffvd1PLy/+j/+9r/9yy/CySQ0PHaJmxvUyuJ+g7A9uPOB6iFQN0PHKKiKErEKNEgRL4KosPo3pLrTBaDKjeW7kSxys+KbF7t50k8f394u03/wH7+LuxPkhMsOLe+erD5bdscP5pz02YvdW+ezv3ix+ZW3jkCq17t0d/KDv1k9T7nbDd95+6TbpccvNp8+Wt9761DiWlXXu+HxxXbY6OH9VqDpduB5ExfNbjXkrNogzoLepJsXOj1DPJAuaQ6ab7aT4/Z2lVcdJg2GZQ5M224oe+ERQ0VFlBhNxPFB2wRe7/osINLINJ9PZpu0G1LBh5ylbUKfUmAQg0QDQfqU+qTVA510F6WDS4q4R8aLiLQfD2VEpeq143rIsbmvTGZZQSfe6+Zhd5xPLYmkR7pi8uKErURvgu14V6zuTOl7Ce/dDvjhBf79B//yzz/+0b/69Mu/fdFvkrF/ECwpLoGwkj+zL6pphlbxwvQI9bSh2JhoxeMSKSHluwYcpEuwJrgXecO2mSDw3ib9ftYvnqz+6ucv/rPfeR2TgOsdAnAyQcqfPVlfrgbK+uSL5RuvHT48nHQpv/NwcXm5++Sr5Z9//6ul4JjDWROeXu+uRZ9e7oakt9fdsEnttHn2vDu9N52fRiKiyJM70/ZkIgQknd2dZqK+0+kMGhAb6pPOFm1z0IqAe+FA2w6zQwqLZhBdboZ+EAoMUM46ZBVFkbynk3gwa8sgNP9fe1/WY1lynPdFZp7tLlXV3dXV0z0byRmJomGJlB5sg5YNy9CLXwwYsP+F/5bf/GAYfrVBQRAtyDa0kZJIDjkazXTPdHUtdztbZkaEHzLzVBP+B0YnZrqra7l17zlxI77vi622bWXPVnXtjCql5JshVNZam2pz1IDUm+BzWlqW1J0mLAZRuAUMlYKKfOEyrH/o/UhuB4mFFQ02ZwrKlAR9yAQVAFRU2XTPk9PLo9SKyyq4MP1qyWWL6Um0Qc5v559+Nf7ozfjqpv/sVX+zC21Fr+6nMMYPf/eyXtW0mKcSpWkCWejQIrKkHJqka6KyiIK6kISsVoBE1FBufEpr4ZPEkSgrMn0nZL6wAAAo9Ero3wYoy3/+4y/+8Xevqo+2OMxYWQTFGKHiV5Z7un15emzt+211N8yXj1ZPn7Q//cXdj/769aZr/vAHz37yi7v7wIbFnyQywsTj4C+frQUaIrvKRp0dGVO7fojzYXx82amKzOyhxqACPMFVNq3MYUftZStClZPKcAWcWOsgbQNrjAhYJIoyq4hOgccpKnQOMk6spCowhE1n29pFZpaMe5y1leXaUYyqpDJGP4SMNFQAm52UJvqY5rg8wGtCsbZkfG9pVCiJ9AeimXTRt9INDyyyyGDLl0rtY2a8+YtFx8pRtayshYrAkGGpr8dvfnm8fTPu7qcvb4br+6Cslsy5lzc//sa27oPfeVxVtjwM8sPmspBSuAN6ULykKBfFoQlSOlRI+oTzdwAAIABJREFUSJZEmKKIbWV4XPpRgUIT6U5TJbLNGq0Ff9jHzst/+bOvXx/8f/zBM6iicTh69IwK/RBubsegSlX13W+fDQd/PMy/+d5qt/c/303f+9aTS0vO2ejMeVfrbrytTdfYR795HkemPg6OwoRXf38yFWhlbl6PwSsMSVT2Ms8qlZGedYYSxsjzKFdNQ6CvXw1q6W6U2qEWuul5HcUaUmiMHEWT7pOWngxznALHKD4qi5xmv11XTeXWbT35kYWRcpVAU5u6MuPMpNBRd9/0V9++MLXBAsklYynVdDsWDlWweVEx6S1EvwScfOdUE9vSBzytC1HQgpYLB0gCQv5dpgRiLZmEJK9nryCSn4Tt4/DlaX8/3+7Hz16drm+8RlXF6OXuGPQUfvXHL2+/PClr+uFUU/EApFKgS//McD69zIU6oNCSB14qkuMraW4uLjRDoSoiqioi6a6IqqTdKqK/N/JvzPpnf/X6R//7y9/73pVrHDzjboAXdHS8nb76bI/O1YzL91dsjd261UVjxviLLw7/5B9d/vYnF937G8/ywfvbi7Oa19V6XV9s287auJsiuB89WazO3NXVOkzBdebZhyvjlKF2U1ePa4XYDraGEk4HiR5tRZVnoxhmuT3ibAVemeOsh5MXVRYJUUTTGCMYo3VljCFVWEuGjCjtT37yYo3ZdK6pjZS0tojUztaVydPGBfef7w83fVpwUd7FBTSJuhLtKCe4RcmUPGIau5nnbiRR7i1WQIkFaimnAYhE09D5UlGk5ePsJLPV5SxOZmgPdp4eJrXNG4G5nw9389398Kuv+sM+5kBuQNBx0siRe/7ln36z2lTdtqaKnLVpP2V57VqQo2YmmpmjoMAytYsJKS1lQQJVEbVEovkzCx1VVVJRY0rPsyqI3gP9G+twf/xvf/zFet38q995iq3rf7FfP67j6I+ew8lXT7uN6LlQ1bN0urpoL9duhfY7P7jCugqDf+yln2O387Ol0NnTKMNhZhayhMqq5/NL18FUosxqrB3HoEqiOhmcDj6mtlMVKOqtraJUxtiaNpfN69fTLLCCuyMLsDv5wDAEsikTbQwghgIrs/hELKFEehr4NMxd7brGdLUd5rS+TFm5Jtu4pVBBxzfz9Wf7zXnbbmpd4LhCRKfeu5RgUSOLqSGRPCqKWc4ClUK0cv8yKCuGWMTh5M8MIdXVZL9JhQ4i23JiA9nUlqWLJWQrKTQK38+Hw/zFy9PxGFNwzaVzMAqNwYD05s/vftJre9a4jXn00frZpxfN2qVNANkrIkdmyFLk89Y7LosWREmApZwQUDGwkkZRqSZsywseABlVKWu0iIAfEkHof/zFa1j3yYvzp2ctRl6/WB9vxq+/Or741lnYuFdfHj/6aOtvw9m2Xj1bYRT69HxdGZz87d14vZ8OYzie4uhFgLZ1bCSISBR3tSbgHOCJ4zHSBXHQfhdcQ5uL6nj0hx1PCmpAs7qO4r0OBz6vIEKHMd7czd/s0DpQi8GDBTEmJ2YNYCwZMs7R7Pk4hH3vJy+RRYRUEQV3R3+x7Zw1XV1HFs1pbChMW7mqCskdcsCbz24vP9hsuwouwXio6NSH+9eDy2EQGdPm0sKEdhd5PzsZkdQiXuwjixCSxms8EL6UAVqcSQFppVe11IVk410kjZI6T6QCE9+/GV5+3e/3MWUFHoSJtBSWRJR00ttfHbuVkjNv/vww/v70yQ+fu4ay6rLUaSpg0oLAlJQSwIgKkSEhKWF0IZcqKlKeTnZqWCLyWy4YIDSq368cXveffb3/6Pnm3//wA5zV8vI4CVCZ59/anobwD/9wdAaX63r/XCdSzIIzO90Pf/LT259/eXh9P+z6qR+jjzBG66Zer+pVbfObtnEsXHV1bXlWUONg/PaJXa8qJex2fnPp/D6GiLpLA6sRGdtLdzyOp0HuRnjG5RkMobXarUgCD7Nva6tpNbczIrI/+d1pbhvb1M6HMAXlSVVxGuJx9I83bdfaKVoULUKFnaOmMpNPbXmYb+P9y9PT55u6tgmi+Cm8edl/89mty/qi5LJEfRjmRMU28vSNxYwIJc2Tbjcp1Eha47Z4o+RQ09Cq7FNKfF3m1+aHyKmdJQeV7Cn24frVeHs7J7Cdek+zz1zwIkAGw9FzHOrVGlR9/aeHi/c3V79x8bAsd+GUAs2wP3PpAigXSJpSA7BZTTYQgcnLJRM8W0BmqWRUKD4yBkr70xhO/t/98FtnV2uMfBoiajuHaBjdxn348VYEr9+Mn/9q98HH54H5bz4/3g5+XelvPG3OK3m9p9vTfH8M/azDMA4nzyrG0XrdNlXlKmsb0sZZYJ75/FHlYOaD59qJYPYSheAgDBPVGJyf26Zy+/1UX9hx4K7GpkZkqCIG7VrMPnd2WWsi6+4wvr7vAVm31phqGMlzSGO6fNTdaTpb1Y2jplpSbsQCY6myRAaapswzTnf93If1pgYo+vjmq8PLn74+/P3RlMudYimKYFTwveYM9oP8VkBKgc+qaVRFIQ0l8SBaHF92loKSAMxg5wHeZI+T6oOSBajs/f2bMYVnQ6C85jLPbl8WhRgio4jexyCz18nb65/chylmJKaFnWSiWWJpTk6VlGmBrak3IT81USVKyF9UU4tA/lJ+1Tlb8X1jMISf/nL36NH6xbfOUVvcT2dX6/vdNA8cWW/v589fnf7PL+++HMOeWRrzlzd925nf/mDTWDvOYZhDZCGYqrLWkooRFQASsdtNr28P++MQfBQRaRx1zkb4nY9R5yBxxuFOWPXUq3pUra0dMHMIEiKud3wccLEFKYYJqmgqNI4MoXamqa2o3h/GL18ffJC2dnXlVo11zhiDyhnn4Cz2x3AcvTHUVCaTqSIdWbuUjgGC6einPsagw2F+9fnuF3/+zc1nR0xwJRIUvVySYJR7LlKAeStXlWSOt8AJUs+4oGj6RQehIonIg1AqCZ2BHgSygnVQJIL0lEX2u3kevCOwUUmzXdL05lLfZkBMQkqWEKMSe9jGtmZ4OY93s3vukMU7zRVLC2BLakaqSJPiaIt8K8gLKTRhMuRpMOXdpQLYtJZXQYRG9JOoh7+7/clPXo+uQh9gDM5q7Objyf/Wbz7+i5/d/q+/uQkr883N8PS9rZni6n748MXmxUXz6nZ8s5/u+3gYY+9DP8sweR+VlUQSjEl+Qu/308mFR+ctOQdH2jiK2jgaJq46so25GxgKsPqBdYJpKAQ5TXjNsIKKYAydr1QUTWMkau+ZnCXCNMXru1M/hQ+vztar2pFRaIh8GGdrqHKWRWePN7uxq03tqhjnyEmpKnrCYh6K+cg3r479cb7+8nj7xa6/FStQgktvd/NWgg75o3QdC9LKNFUNSrFzkUNz7Mlpx7RtJDmLZGhLURct7g1vBcnlVmfeoiBS9jhe9zYP0gUJaQYeyKt8F22s1GAY1bSiuyIX3kx4b42iQCOXVKSLkZGoaBJCUlGsqJAmhpMCe76G2ROLqKpykXVE03o/UuB9YHsIf3c38lm7cjWcxW7CykXg4rL98ovj37463nI4C1Vb27/+qzfnT6rvfProyba6Oc7f3I93x9DPMkWMnqdZ5qiRRZQ06ypCpTQ+BL6+G8/PmqappK4A+D5Y4y4eye7EoqgaVK1VIyaoqzAG3gmIcLFGQxDWpjPjpDKJGjoFnhzZMexPcz/GVVudb9u2Mqo0+uiDzF4rS6oaxYjy3SGcrcPF2jhrRdgYY9KQLZQeSgUM5h3/7MdfKyPOQMZg8LIMl1IsuL0gFlr4Wn6hAMr7OMPmxF71111RsRoqSpUkh7HgoUwicqhMCKp8nGW16HneeWvgyFiYMjaKQDBQgs1MJZfUorFwpBaIAazU304Sk0xTTP7hwfWtHEVBDEIF/6uqURWRBzShSTHTJSVAWRtRhep3hCAyK87W1X/4Zy9w0cCQfDMcptB7+dmr4y5qt3LTzbStqq6y20334rKbA7+8He8O02mOxzmcpjjOMgUOTKxGlTgN7tS0RUBZlUVD4Nu78dTPkBgNojWV4Xjg4STTBACTsFdtG0jAwesxYt3i6YV5/LgyFnMvLdH5WQVFf5xvBj9HnXxsa7td1c4SgU5j/OZ2uDtOWR5ILWqEOeB2P0cW5ygZWYld2W6MwbqhdU0YIBOMwABUqqVdMYpsPrTQzEUaSKJ98Y4JA1LpJyhskgiaV3shL1BKOU4xRKJq3majCftn4oH8jEuUJyJVjhwmtmmKi0hiAkILK87l2Ul6tZZWjmBNADjK6HHczyySF9dqkQuTB3pQcfOb8CGhqSmSiyiZpJnlpJMm/b8UWSZHmb6Mde9Pt9Ob6/H9dXfxqAMzGjuy7Prws7/f3/Y+GnXGzD6uW3r0uP7eJ4/a2n51M94f59PMw8z97Ic5DDPPUVihAi4YMXuBVBslWcm+uZ8uzmrXVNGSHsWyzAoYTANqRt2RBJ0cbkbUFR51REHnWWtjzs9tfwzzRM6RUTqc5vPzrnFWumbVOiIaPb+5P81Rt6vmbK0GFJXGOYSjJ9XTFPspbteVs5ZFCeClzJrgnNmsDAumENVDKfd1JBLmMlzJIpZRKCRt3pRSzrp03JUpZcU0RcmS5qXummt2BTna6JJv1jQ8T8sSKyKI5t+SRLicxkoROSe1oSwsqS03Ac+l+aRkDgzIVVi3tGkttfXXJ2JWFUSkgfSSV2oWNpn1lNIFmv/KoA1JgM0hOU0QSNhNIDlvkl6X5LJGARmqZ6676tG2/vhb51DByOg9r+z+MB4Gfzx5be3pGFgpeHn/w/Orx831bjqc5t0p3J3m+1M4DvE4hDFoFBLJIooUsJg+zuxJIYAIbvb+8rExDnFjppNOsxqDqkGzQgiqFW569RHPzqhS1K3pd9E4UGOazpwmrq1dGzMfPD3pmsaCtGscAcMURXF53jhLIsQsY9BDP3kvxqKtzOS5a621xokBlDiJ9SBCW2lTOx9jQvZ57RxlEuaK4opyBwhG8hZVLQhelxuci1UfnFhyCMlAH3rNtfQ2lk1PCl0EsxKDHx4Ai5NAIgnVqrr8/tXrH7/io1cCYNP2D0IWXgyRc7pqaFWZxtLTx6v1tqMb/vIuMvP22ZZcnrObXuciFGsu/xYt6dUUH0RyFUfqLy7OLfcOUC42L0AyZWgNIOSIDPTFh5uvb4Yn64pAN3dzbGiOSp3jyEFYWNfPVk+erV+8t+bIN0d/3/u7vb/v59PAg48+qqau9+SrlRIcTDiSFSSQNOtaERWIuLmfH587r3Q7KnvAAQbWGS/ST5gDKqBRqJqqMmx59PB30bUgk9b1aL8b2Z+1VeWsqayNLIHjpmtWTSUiXnSOcruf7k6RCBebyhna96FrzLqtnSPhFJYMDFugrm3atqx5eCmKTwIp3IO2laLpA/zKwS81d+S7VZTWbGoZDZtSapaEJpPAeQb9D+nOkjEo9kQoZHZp3s71mGKcefJbj07Xw/3/vG5rQ0aViQxEjSVtG+rOXeWMYeZAk+DolX3otri6ck++c3b13fOFUqTNs8klpOaEjNUSlza/FjpTUl1BKra4uZQA0ZKMVVXKlR8CgtTO3N8N39zP1y9P37lar525Pvk4md5HttRsqwbV6spu1xURXt9P/RhuT37fz4c+jLMG5pCyPNljUuYoBelm7AJEzs4sKlQxHrWuxVVODboa/QRpcOrFK+YZTY0KOJ2ULJ88xwgwSLFaUWWMqpDRfuZxiJtVbRkCMIsKrCGQRkY/+/3J35+CM7ReV4Zod/Qs1K/iqq6syZpCmjdoLJrKikpkVVmkd6AsAXSagIjJ+crUiZ2GZmSCV0zwLQ9ExVAeMFvmGynMlO6gh9amTGDTcJ7kNkssK6Zf+KeoGiVYQmtomLWqsHne2XXjIvvrwVS4+J2nj777yDqjk9AUxiBsjLbm8bZ+vqmrxsHm5idJKYxllQlSa0wikYW7FIW/qGhKOeuJhyrK4uAznVZNIzx+K+r5HG6OQSx99On5cYonltccj1Ng0nZjiWnyMjHvb/zk+TTHcebJyxx8iIhCac+WCHEyMS3yXKH5eYOYQBRB84alKAgR9z1/fOWMRYhoV+CIeUbgvDQ9KoRhAAbaCtstnTU2TRG0xk6Gdrv51Ptn6yqoinBkBaitrTX2NA3jFEfPTW1qR8xy3/PMalTvj37VNJvOGSPWWGdDXRnnyFEyVn0Y91pMxLZpPm2Wjkp5GMrlpizTltLRZBSUEjFJ/3irguwBcpfHyf9+AF/ZiSbXlZIQuU9EluU7Dz9HXeWaiqimD/7Fi/Mn3e6vb79p7fMfPL34cGMqk90jaZuMqMwRVSgJiQFEMmdIz1FTnRNEkn2rqLGZiugCvkpMT5VEQEq3WeSyBoUqLGE9y3dZ/rmSDmE38yB88jis+Ljnk0Sv2o+hn0LvuR/DHHQKEiIHFuZkS0YJIIGQoGRVURBYKkkXcImbaWIUc/44CkTBET5Iej5KEAMfwAzbYPJoKqwbXF3V1RS7raOZu7O63822c/3R986oYpiCUG5LA0lb21XnDkMcpwAybW0JMvnYT8IMC1KDftLbw1jZrqqcM+Iq21XiKiJrwMyl3j6Rg9Sosn7iXL6ykhZBp3C35NMTKy3CZaFoKnnoFYq+mx3YWzUZSgRwnmpFRe19UI6XOQg5t0Xpkhe9WAlqUF3VF2fm6Q8uL56t/ef76/vpk3/9fnPWZAdZRGASqBGSNFtLc1GHLGtps2SX0GKydoWq2hIYKXuPbGhUkuv5NyhBWRWoQ9wM8SzKxRw/YHnR1JMPr/swVeojxNL+NO96f+jnweswh8nHOWLyMUSJSclWTnQdi8RJJataIH8u1FREgia3JIiKwNnOEm5L3z975QkgnCb4tCpRwQFWcbal91q7scTWuMqqM8M+eC/c8J6ln9NCICZn6gqsZKJUrYss4xS6thLVYZLjFOZZCWgbYy1Flslj14emoidnLRmqLbVNUp5UgRjzrp3EkcnAOnTnrdMl9ZNRWso/J5eT8Vh+jy9FihlHUOoXybW1EKO2xEoUxSKlbsoYjgL8c00RFY3CFEeXauJKtOpWlWvtd7/3pLv3P/75/Yf/8v1222alrWRC8y+SPEA6K2rFhN+COTmbv8DFUruRVZKlLi3peamXOHGhKnA389kQHvfzZpjhJbCEqnrdsSESJS8y+bgf/WmIxymcJj/NMkfxkRUUgmT2ni6NIZUywLVk9NJ7kxctQyAgKbXUUXIjCytiGesZIjYrkyp4jjOmGbBwyMBxU+PqrK6tISLmYBUjwzRmHKgfePDwqpPHRWtda0lMnH1ljXPmOARjUFn3ej/cH30U2na2a60xlpmnQD7GENDPsvbSVNaSqZxTRRRE1hCzrxGFsXAdzp93l+9fuAc9v/ijEr0yViBSVWNQGChokcxKVXQRRt6Oolju9kP+6yHVkIlE/r5FzkopdYGC1KjhidmYP7jcfPHL/bN/+nzzpEvmU2aBaFEBoVm1K0QZS1V1cbj5d6VUeJEMF3qcaUHWilWVBHWQjeez4/x48usp6hiOY7xn1I0733RnKxeiHId4GsPdaT70/jDG0cc5yBxiYGXO0G8BWFlijOkNK6KZQqqmHQMFnEnS2TVHzLQbqphaogghwBqcr+2b+3g7YGRUBi4NZGQ8eWSer826psPB67pyaxdEd3vfre1gtJ+on6AGc4A7b2Vb6WkkpbapvI9TYCjuh+nN/VxX9ummWbeWmabAlbVRvDJUMc08eqnTJFCCjxKjTF5YAMB0OHvWPHlx/ui99faiM846XQLJ4s+Lyppoao6VDz5MC+fU5L2ovMPyzU9+JM0cyOJAIaA5biP1QKkmYa60JxOJlEYnkJKyRwD+0x99cR31O3/wfgnJxVMiyyZv+0Jk4SP7LFP+f1CCJbFOU4r7l1w6QdVEXUU+Z7mK42Xgzkee4jCFQwRZu9q2VytXk/Usu9N8s5+PYzyO/jiE0xxnL4EjC1K5KYEWbstSRitI3p5MpGloeBQVgSSWpkhVSErggvcjZyNblqz7AAiePKJhktu9RkHrkEGkorOwIlVb+SjDSabZX15W/SynowTo0asXJSIWbWqqn3ShManUcfLx7jD1UwBwfTddbKon511bmdHH2cu6qTzzOMd09cdJ7w4zUDlDc+Bh4DmIZ7Bi9cI9//TJs48vtuedqQwB8xhzfrPcBsp+gmjB9ViQ+VuqRBkrtfiE4j+WYAQhtQp5q8e7dKYUJ1LQ3+JZBGmxhqqSQugQ47iPN/9wuPXxxfHp6lGTvU2+JYWsLr0viz4CTc0uQpLTCOk7M9SihO6T+mxFu+S6vH80y7nETqAs0yx7FoGp2vZZV60aE1lOI7/ph30fRs+n0R/HMHiZ5xA4ldgDQryghiK3UdpJmlV+4pJUUGhkRCFK1aJEaWt0WuobNZuXZ3BZ8ipAXWPTkYG+vGYCaoO2QeTcrfTkAiuHcYyG1K4gQY8j9xPXazPOai21pNSo9xBCe1ZLVAgfTuHuMEaFM+buMFxs2+dPOkt0mqIPul07FXN96E9jLrcCcBh4DrxuDUA+io8IEdVT8+H333vvg7PVpkkzrEUAhcuYON0hFTWUx0oVm6GUwKYcsNK49MWFJHspdaUpHaWUDBUPbbz0lviWrzygkMVQExmgUoabFu2RI8tiotAh3L08tee1obS9tlQYZt0YyBc501yamQW2sw8MB0U4VoDFRG0YTzg89ryaQzfFioVYDHQGeiWQqWt7vm1aZ1V1Cvxm509zvDv6wxAmz/3kp4AQQ2RlVoWyprk0bJJdU8YaqUjFEphIFZwNjpRUhFjAommyfpKYgEwn07ZXr0iL4lK/ZFejJghpP0IZqxWgiB4CVA4GqC1ZoigK0fXWTTNPM8eI1dbMh+gIYkkCaqu8NpYQ7+bTcb6+G5vKXW6b693pbNU8f7I2wHEOkWW7rizRy5vh7hAIMA5p7P3ktZ/kMIgzqb4BavH4g+3F8029rtJ9yR4D6rCEwezNVPNWRXBej4osfi8OruCvbFw5Uqpqnv7+VkVSBnS6MIEl9flrfQdv4fqlfpDV3s8iMnreNubNz3fPPr2g2pLq+6xPo9xZuq/dkKUmIsrlF6REUdI+RwJBJSokRJ6Zhyin+aznx5EfiZ4bXVsbmW8ZBmjbatO5ytp1RbWzhmgK/GaYJx+PQ9wPfvJyHOM0z4ElSp6HwJIdaHlbJr0ub29J9WyUhzdQymdpUXqIwAQFIsMY5Zy0hSKtYURIQgbBKEhgUsLNYFYME5oaRuEqzD2sQ9cAiuGkwejZuY0ep2P0UZuWYtDTPtYVTZPCqK1MZK1WzfRmnProZ73Ythfrtp98Zd2LJxtDehoDFJtV5Yi+vh9vDlNlydXU1hWLMGOOQSNEcIqAwhg4B6pclruTneWWIjjN7eVSQFR2Tg8lPw/JzWQ5klD2kl3PwizhoZwLmT48aGkPypw+5NiRFRQq2D6HNqNQEpavvunnoIc+Pt7Y8U0fBm+r5mPWPzyOZ2pPwtzVL0mvjX3TmDtjZqJUq34mdKZ0HsOvdvHNbT/cTOF25P2IIVYRaG130dCmoXVNG3q0aZ/UrrLUOlKC9zJ6vT/NIcb9yP0YvQ+9l2mKniWmDVua2KjmjQrQskwgVWKapN9FgSilnihmUmgUisni0jA6UKqgTGHAlHEPzAgKFoSEahRQzBPqFsOIsy14Qtrp7ieoBRGaNo8SnDyqFdXOKvPuXrot1c4eNUrAauNCCKxkSaOCxzh8eXyybS+2jXMmRomszx51tbPD7I0xq8qS4uYY7g7jqnXWmLZK3p1CjEnzdATDCKmnmhF8DBPLSsQkPqZJrXQoFodiLNmAkiiVp4w9BNHCT2VhfAtQe5vgZcmBkPp2JScD86LCVLNYUCGKfozCMwyghrViBhAZCpI9h2P4tKt+f5j5bvzRl0fPWHdVU5vLtvrk8Squ7F3jQmWM4tuRfvfji//+Jz/5y7+6P92xBa2g7ap69uzs46v180fNurWrOm3xIRWdPB+GeO1l9HGYYojS+zDPGjjMXjmHOimUkEjThNLlPQRVTjUrmtshc9SQ3H5HQZmjiQoQmElFrIEovMAzRGFNXiee9IuQbp4CisYieDiHqkbvMQdEj7oFCURhLeoGDogzXAuyaBsz94GNpQqNo+hFgbalOLIA1kIjjCUeWZvgztdtbVlkDrFr7KqpfBQiamujSvve7/u5a2rnYMkYQ/3IUXj2UZQcqQLWgRhRwYL5FPqDX63qytosjKqqwoU5pK50IhA4/UVZzCCAc6tIrpowufYHy1qk9P0MkKEUtkwmCTkJTyAuogaVP1NhbF6qorTQzLK4gmBOQU+RgHGUo5OVxaNf7R/fjF+L/O3L3WdfD6q0aqvH26pydvPyuFm5s3Vztakrh/3E//Xz2z/623F3HZxzm3X14bPNJ8/WLx5XZ10dIg+z3B3jFHjyuh/8PMfTLNMcomiMwqyCyGmmDhtKLypZEpLTVVgI51y8COWMpGqSykTFKAmQ4FfKSwYGE60qCqx9QNpDGFVT4tLmLWwQQUj/MQzQWDiH4BEFsQcDUwQcALAvaxkdAqf0B+qWPCsHRUvNyvhJ1ZGpIIrAohasykKiFJV9dFNgMhhnZpG2caPnGAVELDxMsutnAipHhowC/cTDHMeZ50CJL6fwQ2Vw2eH11G0OjTNWyVakAhGEOdLZc2fSPJSlteItYQtLJUf5J946tLggKr6ufLh8Nf3kg6L20MuZPp+Et1KLVhpJiSBBd1/OIoCgdrRy6GqyRJXBOImPGQAmIdpaVJZqR6uGrEUI2gccJwHDWFp19Hhj1o1LgnJg8YyYFn4LfFQWMCuXcqMUzjNyB</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9aa9ly3EltiIy9z7TvbfmgfUmPjZFUmyKMGWbloRuow00DAP+ZsD/0t/8xfAAA2q4ZckS25IskxSpJz6+oepV3ao7nWnvnRnhDxGR+7z+CUadh1d3OmcPmRErVqyIzA28f71/vX+9f71/vX+9f71/vX+9f71/vX+9f71/vX+9f71/vX+9f71/vX+9f71//f/9RU++v+TEAIgUyiABERREpKrEBFUQoCAmKJTAgCpAp4cBFAQC2V+o/Z7w7bcBUBD5R0AgIqgCABERFCAFiEB+GoIqEaBQIlIQ2y/sikSV/BBEgJJ93I+ndmSFEuyuoHYl9l67N6J2bQRS+w9gaIWUmirQhsHviJj8I0ogjStggFAqlCSuwD8LAqlfnn3E7scuLy7av4NdJfnXk1uZB8sPZO9QtbGxXxCpCNqoqKpds8b7VBDD64dUuzIhfxeIANH2LkX7nhRKivYHH18lQOyI0KpMxASAoVIq8n/233w3LTLF8IF8+gACw+3BbIuYyCaVFCBV5Ri1ZjT+ZlZSJtjpmcKMQAphsLKyAkw+4/ZHgPnExnzglG3a3SLBDAWffEr8K1G4gyoRu02QqogSQdyOzSZ8joWIm+X6INB8VVp1vB36Sj7kbqZKxJwoMYmCoGACEUOZSZkP01Rs6IiJVM1bZqNpRg0G2UUi3qYEhbp9uPk1E2SouM3BHc+NVgVghbg9CinEzqCq9ncbMLMEVYV/ZUCgdnpScd9T8TuDKgSqqqpQM0kSDaNSe4vCzicQFYDKsSw45Y5VAMVwLDkvcr9gBROpEmK0CcREGuYBGLbZT4EujmxMDcWoWSuBqIGL2kEIZC4/H4QAcHsDsxsY4AZ06rpEZJ9yoySDnWRopDZtIGaxE8CPklQUlInUcRoKUigTKZjDO8wCibidTKWojqUvMERgtjOJEjNAiZJBE/sdpcwgTEk4MbtZKpk7BlKyo45ZV3MIgbKQElQaZgGAGRAYquD5jwTzdIIqWBUEEWSGgiBVCcmHT1Xsbt0mAEDNRsAQBSWzobAbgbAaNCmgUBWqbkYgiALmuQoVCNw1RFRBIomgpNqllBNBocpCmgkAcTi0mYtQC3gtANoYmw2SqpIyWKEUYWxGJgaEidT+goi5pM1omynC4jW1U524N7mhqh/bvsIvwbwi0EEm3d0Nx9uhX3W5I855dZZTnwLBfGKI1R1GASYCA0JxFKaIaDb3UINijxesDUscm1T91mB/ImYSVSXiuA07IhMJFGzwbubmRhYBgoWF7JpUDb+hBGW4zcM9wa8cArdfGxm7LXNDZlU1rwuwlgYWUDHjhofYCOBxuQy/R/8XykrCSmrgCAjjP/YgVWJWUWIlgUMPJagSCRNl4qA15EAe/zrsREgx9qFguyCbGfMPBgmFOTQ0c+Izf2OWGrThNGISAIu0hprqXs7zt3b/TA3aPBZL1ZvX+69/df3y/3139+qYL6hjTn3+8KePnn3/3tm9xeK8J26x2EHaoi9Z8I5DwWc1zAJBeQjMEDcwanZpBmKOam7FTCJqI2PTxxTkZv4oBQFuMfoEacNW7I1Ge8IJFO2Q0KTkpNM92MIzG5MisYk0DDI6FEQjzAggcDszSJXs+tn8MZyTlNhCKikpBMZ6lA2BVRBGbFyEiSFuBo7DlD3W+9hpnN9MXAXaqJD91aMjCbsp+r2YFcVB/LTB6ebgqBTzZ0ZENNMmBjOrn0DhB1SD28ZkuN09iAh3l4e//18+f/OLaypaCx9eSZeoit58dvynF68ef3T20R89efjxZn2xTJkaIqqbvdt9zIDBHCtpAsAkRYNnqZTgdqoIjgcfEVUQExFDJbgH+1+M1bJDg/mokddm/caSCEzBGtVjRDA7Up7RO84BjxbOT2KmoNLChZFVKKO97EY14ocjHETD05TUL1VO4gmRwAKdOJGMCTcmIJ4igAnV4gRDPdpqVjcQxyooExuFVBAxNeLJTDrPSVAvm252rhsB0EwIIKag+yexsvloIFmDTrByDJcdL4Jrw48WNwFCHeT3f/fm+u9vcqXENEA7ogQIeNpO5Tfl+Pn4+jc3Dz69+OGfvXj04Sb1KfcMNlxXMzIKUGmXxMb6zHYAQJmNH1hI8PjSJp+M8ZPnMc7YPJoYGKnORyPL+YgY9sXz7khKzQ4j9jnOsRq0N0aMYG0xUlD3ImZSgVDMYsuSCZZZRoqhMf7mdwQBIqwrh1mBCCpiKRxF1uWnC5Lu1wRpNIfMbj3xzk6PbO41wM4ZhBDc69mw1vzYkEkb1VZ3r5Zzuo166JtjU5hbI38UFm72GghueOcja7jewhVsClhZ+fLV9uu/epMqCVBFRcAMZnMuJIAVh6/K/uW74Xr43p8+/+gPH6fM7OyJyQIizLidGJDNMkjZaA0RwEyMVCEt2wDDUgGDXiZKiW18PLRRsE+ALBT5AAFBOXh2P7RxC8KAQJoTF8Ns4cpKqsSWDMQYe/g0AmATJRALI34uj6zxYwgjMR0hcSgziSe0jcHZR9ygjQBZ4GVoVbMty0vh4U7sQ9mnO8aXNKiXB9TgLdxAiC2fDnrhDuPq1IkxtQ+04aVQrwybm6YAcorDFKZLJ5caoBbfG6agTPXLv39br0YWIpLESAswkShNk2RmUZ0m5ERdB7wdy7H265S6OIelt6RseaQrhT6eHIEgYI0Sa62W3nnsdlRlIqKUlLndoBBlI90I0PSUKSTBJlgQhS7YMM20CTs2W5j2EWCwGPn2K3DHsMSx+e/8xTQmV4Yse5zVgQA1j8tKlZTMA2I+zbKlKV1+DtGIr+RZNBRMDoFumsQMUTADotk4hs62Ykfz0QiOYCAnFtmJCZCWdUX0jJEP7uNJfFxexEdzOkurwKzzyMxEsH0EmI+qhJbXCkD7m/GbX11pQcdImUtVJZKqqx4d0zjqqNCKLuGHz/LzZ+vVDx92q8xhts7D3R2MUASvpoglDtVKRJwoiYqLYTEa5pOsoGyZp5jSFIm2QUQAh1KbPIuaCHbqJzVSox5/AQT3Apmnm5IONk3Dg7wqlF3ac1gKQVZjRsQgSQhQYoVAHUpUiFhjVNRzkACHSALV4qAQWh4a7wIpCTHEL85z9G+lAjmiWMPluFACh58R66mVIKCLmpZ1imQ8xwuO9IHbWWaoYmr8OWi+ZwQngbXdS1yGZ8xQvP7s5u7Lw0IYWaqCwKKakiRO1BOxrqAESkmfb9LzVKexGFV3TzWsghF2sYlWMJMA3CBUG6oymCE1FEFEEmDXQz4GVTTgW2cw15bUITJEjVEiRzBSryv48BvekEYCpCQtamgbcNV1ThdddzkMY8QiaCUioz2qSqSqzJiVBiWh+RAtRYUnKcpANdZNDlgS8dJSEInIG6zQoAzBFtmdKjIm5OBb7EA0D6F6ItH47kyqcIL1bexY50QBjaM4OrpNqccQi43BzGi2P5yciNlhIfQmSyks56l1dzXwhPWKCCQVlIRAmwX/4HG+HerrXc3ERXDWc88VyvzuGKBrqfBs1F7VIYS6ZFPMoOp4SsSkzIm1uBlR5D12BA4iEemFI57VLtyz/Hzz8IdDRnrjeWcToTUYv/3O9Cuaf6cgerZa/sH9h7+4fPPmeAQ3qJjTYRtFBc8avufNNuwCkCUdTtCp/eBw1YKrBho3tGmViSYue9SNOK6qzJQbz0IYRGBPYggiANKsoKsJsUE4TAE0ces0zlnahlBuGvVUWO56SuvCjRGQahdoFQh1bUWZDDSEiZB5fd5tFtQlFIEASdB3/N0H/Kcfrd4dym/eDl9u5VGmf/l0sVrIsWAkSmhD0/g1NaIUDkDu3zr/mlghlJKKsuneBHYHICZGIvZMFJFqkZU+4pQ8Z3ogIgjolOYFdz6JDA0jA9ndoRGk33D95eF4Xb65LdPMqQAn89BIgP3zroo1aSakTIMZBbyWZWbVRNw2JIGidrE6c0mRNvdWpPKcBUrETHmm72SaScuJRAhB/yhSiQhpkdD6Ncwo3MQzM5so2kVmZR7sXMBn2q8PZGoPMJvgSbXJp8BFJwYxqBalXpkpJ62Tni30yToBtEj0Ry+W/dvybJOermg/0aHou7fHZ2rcymmLZ9ZoNejUuBDmESCnYwkslLPWErZBNoaUElFC1DKVowzVaEVDLA+DfmcnXNSUYdIgjqHIzwG5TZTZjDbbGLQOoyiJ82RCVU9YHY3ApOIAa2mvqWatAwGOeB6WudXb57itJDhpXNCgOkGn5vBmGUCNG4MoE7KRDS/qB/06SUjM+sxF2KUeN4R2w9/idm4kVpQjOSGyp0Rwpmt+nSab+Z9C2jHUd77izMxYuYqQ6npNOTOrCmnH/N2H+bsPskLGKg/W+WcfrpLI8TjdjHIlxM837Amt8Wx2thGkIubcQ40SE1V3AWaqSqxAAleheDERc05IKTGhKjsMEXv5I8A5xoZhzETQmhJEEbU+B6HGSuJ6IuoGo4NDrJEAzyu8Nh4m7uEtgomV2kksPqiCmUXFRlSNcwUT1Jkhmu2rRKR1Z5/nhk4LtjjRtozHufbKXjmz0WwyCzGCE8LBmrzCOHeDOIt2uho+DjdOajkOEEJAMy3oyfXY/4G70fzg1utoxmGRMfiJH3y8oSXfbmsZBYp1R0/P8oOzXhWPN3nVZ4JOUkFgotUfPn78k4ecgt6gTfOcysS/ZGUjbjSKiV2rJyIwc6jrCoBJiRNhtlgEdZuhOD5sIgiD7RsLq+xqLCjQm9jv2773P3tUIedv7ZNx6V5NmKHFc0eioDIaXNsiMDXBL67ZQpHPo11Aq0uYk5D931zSLxtW8QjaRdrgzQSjbPbul9LoAp2C4jy/6tlkCzTthG6T7ZoQgNgslMzyXBG1+9K4Zp2pCEVQa4rfbI8SwQJEOHu0nM47eXdYd6lLeHyGx2ep73BvsehTKgnH7ThVJkKf5Hydc59O8IUjELWITzEUKfBNW6EW5BfO5DgYjEeJec55VD1ZsbpyhGYfEBNnm2TqbuVNfwZxhtnh3OSx04ub7VoYZFGvxZ9mS4ZcQelVTgpE4gxb2tn9mBqM38ORla1COVG1ibYCp2Gdq0MWrewfVhc93OXcHVQUAHIDIYNmd0fXqpvDnwgzJOwiNHn5yYO8F1Bm8HSDt+M1m2y2hfaGU+vxyQtC1kyXWwEirH6x6V78wYM0yU+f9o/WDNXzBY+lnq3zouftbjgOpWoFWAjLr7dlX3DRz4YbCGtB6ATwccJ/RYO4u6ZGROxGqs4pyTPK5sHkzo34J+xglr61MVgXc0HWn+NjLl4TgHpJ3hSzYGUmocmJ5VodwnQMhgpZHkUh/rdk3dvYKJQqQIOcIBJOsEKZVcQNkcQVOgcVI3om6Xp2GXd+GlwlBgJZI3cgt4HQ9iwrDM0wcsmWl7vRRO48AwJOAd0yGmqtuM0E/f4ouB0QKI5AlxNLIzgQeqmPlEWnL/bfo5w+uD8mXCtWrHWcllQSjftR327H/VgFVTi/nYivDhe7ie71jrPtDnzAI5VWapUPJzjuCX5t3g/FokEViGfVv6X85hk0N0yphqzooBBtKC3S6VwbsdERohCE4lBuMoFR0SapbGXwqBPaOUCqzX1MGBf1YbRyR0sfQVBlqKAJtjN8Rt8A1KEOLZlphB6kVoMV8uEFUTQ1AUAOnt6wg6LD5KQLKaSNMIPG083G5JSytvAX8SbisUVdu7cmljZ25BRG48OBLETzcAQBADB+vZv+6jIfhHOqwI3ou0lV+1z54VDupeNulEFUFDWp/vjZ8ieP6eHSA0Po2T4L3vWKaJFyMGMlQQWQmJkICSpEybpPkwNwx12H0yJ6mMbJrdkJTbiU0Ey9NqPhedRKLKfyJlF0RhoQheYQk6ykajUyDuWzhXukhp8KIhXn+mahnr4hADtUK7i3WXZiU+DphfcYBYI5j1IX/qEnbf8tFyHv4MuEE3MC3Bw57MkOQQAoET1cLG+nYbKuTvOCU+Oi2UiaqO+NQ0RN22iRhE8Sj+CDwRGb0TaQ5FYwqOVq3P71a2xHUrYKoCqpQpV2mm4P6Ou0oWpFufT47OJPvtM97NXKohrB2mIJz4qig5CdzcJOBYFSomQSK4M0mQMnJmbNiw6p8S9NPIeoEE0IUBU93o27m2E6FKlY3+sX65476hcpdU7Gw/kV3AQk40JqZVHC3H4320O0ZblTqgSZh+GJ/a8qVtAy91CYJGz2T94CIojPuCSmUYJCJBQzAlnxUrWFN6OLQpaom4FpSEicG46HXKV+4pnBuD9e9Kt/9dGnf/Pyyy/3d5YeettGTJMCXtbQGGEiz9jt+lh8rCyQtr4a43o+PTPERQTxLj+datkOw6vd8Te38s2YQUIq1X1DFIBmpsq8LXmoeo9HZeIHq3zezdSrlQ4djCPrbFQpcN+a6Zko52RNaTY7BitMSDnlTCAW8gJaZuJEZHk8+dCp6PXL/e/+w+ur39+t7i+qQI7T4rxfni8efnx+dn+xftCvz3omnoetudpJ17BRQEIU24O6+yoND5JzEFeFZxAW6+aVMTNTMstrcmsTDhB5pzuh62ZWIdJYlgCX19SsO4xQwvocHpRIs4s1jaEpXL+YAc1RbT+Nv7785nrczzEMc7RxjsGhWDsKufPFry0RCY5KUKVkciAoKA5i/q0Ji0il3E7jN7vxy/30zR5bpVoTM0Fz4lp1qtXm16SRvmMmOgy0Bc5y7X/yiPsUgZtaWkMncQ2xmCvQ2GILqiIRciLwLC8we8BgNpFMmxXmnKzzOnJ2LUUvP7/97C+/efV3lwq6+WrLiVG0TrJ8tHrz2Y1O8r0/+86nf/ykW2bXaS0bjvBLZm0ed5ndsdH6W5sVGsODwNEoQrZPBJkG1Yo7HpftH6Fgll6Ds84XbWxW23+A1xit4agNazMZ8mYcD+FKgOm0LSUhE47JCJ43FITyP0j91fVbI8Jig+tz1jKa8BMPdxp1DkJkRj6HwfNm5Gp0G9HeJ1qLlNvh+OVu+Hxb3wxUxOyJiJKpDAB3lFMaJy1SmYmYWNFlSpynwuMaDx6sZoeIqKPR5huoSd6vodoSbxMpukQpIQEgZqJQ3QTUmn+N7jBBmTkzlTaRgrdf3P32/3z17rPr8aYwdCromCzbu9vukNCdpd/9zTeLs/zBjx6mBbsOEvlbK/AEVXewDXRjIaFWv4ykvYXJ4NjQk1VjOvNFOM+PqIOQPNzhVSynbu5JJr368gbMErdKVBQ8ypma5+NDlGeotqDvsz0XB8zJLGJoywAQ+aM2oXpGdwCq4nkYN5uLnklqM2kZFQcFhjML1el2HL7aHl8dpjdH3BQOl0nJrzWxipCoZpAyLXuuQlOVUpQNaQDqkjIfP993mfp7vZ+w3ZYLdaaShKTpVq6GClDtumQYxRR9apF/q8kTTGQr6kApIaVUpFpJuVZ5+9Xu6ovtcFdLQQIYqKIEETCJatFh0HeyffnsenHWP/rwLC/C3QB4puJsxioJ5EUBYSJF9fbwNskCnqGvYbe1XURSJS3dMZirp6SsrZYUp68ICS6apwDTNWy2PJCx93D4kk9iQqXgwUSU/vBfP+fM3G4uckBCiG0Nntw0tZlp8AQ3EmJx5YWsXcPX0MXb0Q5EcQLi+WeTCLRg++t32794XT/b0tXYjegSusyZ2Vb4WFRNbEkgPJQxusSJGYQqUKtWMmmR3efb/Vc76bk771KXZkXOb8dRbSZr7moAQKIL1T4le+NJYRwwTLXbjIImEY5DHVQMda9f7T/7xev9zVjfjokaVydRFaAWrcIQjEfZ3Q5318e8yBePVymfSJfeJWuiGSXDN5fkFcQc7umLhEI9CUFM6SQNndPfcPiYdgO6ANFgVxEI4UG1iRgBd6cmE01Jxj8Uoh1zIgJQi+SIqRRJqHtAeK4GdfM4aA3LFOuIm6nBlS2XuRpYAEEvHTc1Qqsl7fPlWup3/PJ2/9dvu7EqcWZKbbEblEDF1gmq5mzL4tyXAahSSlhQYiJRmYpOKsk6il8e3v1PX27/xfmDnz89e76KS+aICRaVWpN6XDmpaMqxvkIVVQgGXXOaRYCvEbJMJCfiyVXY/c14/bvb6eUABVSXWfvMABWhYYIwasUkqpNOr8eXt2+ffO9+s3C4/CLe00gAeztY0DOCqX1OsWYNT32BkpuAFT7dMtWWgXp/LYLhUKx+iajkqwUiFLa8wL8HK1VIy4wRvUBhxNzuQJUImTxaecxw/tQW69lJeFYDIulwghiZZqQfDuFzukqAkM4FADPPcBh1Md2ZW91P219cpkGIqWPL2UVVMiUQcqKO5TjSNGmptYPzJgBQsY55IvQdTYW4o7FWtXI1gyYZf3X96pvD0//6w3vfvaAQqezqqcbiC3MS9qxOIKpq5MLGzMcqSIgzCSLUUAIIfWIkmoZ6e3nQ7agqC8L3HufvXKSOU+rSguXuoLfH8m6nX95O1zuFEiadhlrKlPsebYaFldSpOPvqRe/tATzYOewoQEFAIhlA01S1ObzTZJ4lMpCtX6vtDSHOiEtlwbKta1LUWh8tIFthiTzZrQQCQ5A4UQqA49yu1CXj2TxoBroASNc8XEeRKG+H0K+zRkYn2XdEWFCLVvCfv01GSO6Kvps6Jk4EsfUdACdRdIkAiNC65yMwFkkkfZcsbRUhgRbxfSVyIgKJ6EQCkIiYzja+HV79z1/0/9331s9WHjWspqJAcjsiboACFfdwV5siWwO8Z6bdeiMiIOUFcybivD5b1FFqxQ8/6H70tPv4wfLeMhEzCYYq77bTy+vp/pr+7uV4dafLjn7/t68//dnj5boP6U2jdVRsBwOaQ+S8UC5SPu8apwAMizGReoZkEZmjpxUCsbwRlgyoNz+oiqNFyzNMO5rLRZj9TT138Rm3JaCmCpnYAba4DOf4ZrMUl4NgnfZ3NVUPzTJVES281KDeWbL1AbYVDW023N5ieePM7wCMtxMDOZGKjEW6RH1KOTOAWsGknKhW6TteL3iqOo6ithgpcQJ3OS06JlYREZEitWOuoiLSsWcsfDVe/uJSizo/sRyeW0sFCASXW9uVI3pPw6ccQOwt8SIgnJuIcqYHL5ZlkRaZHpzxusuLxB1TR8SMRJSIVh09XPFmkUrVw16ZsNp0kXh5CkneSWqrWL81aHHBII7SNLv3YKZOJ+8kpaALNvvWboJGrnwixQmdcTPv0fVcluZQFWGJ4ufoVjPbrlqj6mC94Y3Eaeu3dMBVT6rdE+xYzfo8c2wjHxeKuGwlCQUnAr2qUixgng0MRCTHeveP78x/DsfSd2QVIQb6Lil0EpBSzrZaVNeLpNDjUEpVtlzAwlbmxGksUoqMk5hezoky+1KE4xfb6TDFGDGxgVlr/YGjbTBm8mVxSk68XZlqw3syQxT8ggCcP1w//dGDfsk5dbuJ9oXGSlVwmHRX9OpQBlFzyKLIK3r83YtukSh6ppmDx8LT9miWsd5wjbkHXHo3z24pQBtbdcJp7VYeF+3efBJaYLF8Jorh820RESsFpyBqzoBgyKTUOJGd2lfqEEEyXLyHYypCPzpZfUBzbuD0k9Q73+iEI7g5nViPZ0vzxER5fY43HImQHF/t6tfHYajjpEy06DIiIVRoTqxw/+gzDVVrrV1mgMdJS9Uuc2IWlVI0J/SZi6TDsaTEiUCEnLiUSmA61DpYSdlaIMjlF5gSFnDhiydjsG0AffSVoo+RybcvIiJlG5BqI5IX/OD5uv+n233R2/30j5fTkzX9+Pnyi6vxs3cTQZeJOsLDFVKm/jv9Jz990q+cMfttu7kTRfNhK0IFH8G8lq11gVgIcy0WFDtMmSLo3ByeOVqkbPDiR/RCz3wZXjuUmLtQiGOhmMJLC2F5Vpr13MLWHJ6A0cw1QvBq1tOkwxPpzJGLZismOGU234p6oVsxNdYQZYgYgKLTb25ZUERKkUXPqr6MD2TLJyRZ+yoRSJcd58Slqqr0HTLTVHWq1seipaLv0qpPolqlppSyr6oiJsWxTneTER2KdLdhuvME1UaJWuNPC0V2F774nCgRmMnX63t1W1XARBfn3Yt7+fkKz9b8B4+XZx3pVHuVJyt+ssn3F3q2wJMzen7BL4q8+uy6HKU5OiKOh+YX8c5kKGqw67rwzBGDmXgaiKDwMYOnnhPAEpmCEyACrH/Yg1lg19y8FuKVAzwbkXC0D4t1TijZBWfGSR4TuWq7M7Qr5th9BtHu0IQBxKEpVhVEQ2BIo85posbYwjCIZF/k8pgTqWq/SIlZBIlU2aRKZpbwYQfYPlOGlqJVJDNnwjRJIclsLdS6yNzlVEUWHRLzsRbrV5Yq0/VAeoH5wl1vlGCSBtMnaXYrCnp/odFQcojgIDSugJhTjkPBdnq8yX/wIK+YCnCz79aJz7ry4v5y3VMVebMbq+p37+PZef6n/SRVCKmd2JvOWnXHCaFtTOSYozbes6l55uLJ5yxH2EhGSUTmracCn63fzAy8QZ4oEXynQa8jtGlvW0Jpq6KqMqj6QlRp4YCb2KsOhRTcyXKLZswUzKsh1myeHmbV32Nwf1IlOEW/sP92NEAF08t9Hi0rIWbKzEw8iZZSRMIm2ZqGZ3KbmHJKDJoi05RK+6GMRSBSqnaJRJCYxkmKaJBmmq5HFQkHdCdVhZJa64z4nPjNaxsj37ORwrFsrxLbUMwxI1APUnTYllWiLtGDTX/WJykyVK1TYsWT827dpZ5YhC+WmRe5Tjhux4YfKu2kILQWHhBsj54YUbHBVwcUDWtTf6+ld//RsKvfsScSYX8+W+FEDeCaSueTEbhxAm8tas3CsJ8XUcNsaYPqtwqsCINDe5MvMHTpsEYgjFDo1xk3pY7jPmDkFMHjZ/xNi9av9rbZX0rExBUAqiqmSaZSRb1WghPyqwCBc6acUpcIqilR13GXUqmyH8pUBdCplmHS3XFUqaZ0ETBdHaW2Wo7aDlWx7VnjR3MI8mhNGusU4hZsd4tQqNSREdawyAiFftoAACAASURBVAl81h2nuh3Kbpy2Yy2JjkJY0LbU7WG6G6bdJEMRZnxzqI8/2IQlBCkDHDujMg0YN55LoDNXagFNo/KosTbTuog0JtH4U8yTE3ufaxvopqIh+rjDdvxUTcB1/DyBEYQ5ABFMvbrd/DXookY7HTUOFj+TfxCn3NFzM68fUHSpkGp0RLXsbCZ84Wz19og3g0JzopzpOJZhLGOxz2Ka5DjWYapVRFSqqNfeIl6nRIlo0SfvnyAwU626G6bru/E41Jv9KKIpJSt1E2m9GssozZxsJpsY4N7ZqCU0egBOEso2XDGNbVqC9qBf5w//6NG47HcTLnflq7vCFXmqVOR2qK+2092xDlUE2i/o+mzRrfL6rDtF0PiqXoU6waQGPdS8Vt0N2k6Otv48GGf4usbHm824HHMyvUpe84kb5SAX/rOGx+v8laiRL4oje6bLLnC18G46+UxP4tzRVSRx/3oSImdl0O/kJHicwHOcnE5UKABavtqnSQlaRVddurobD0MRhQilRDmxlXqq6FSkFJ2qlFqrqGqFKhMlJoFI1apChFJEAanCiY6TlCIpMTP5ihFAd1PZTxFTfETCxJrbNLpJTkfUXNAs61v32xC/tWozkDnfe7HR7z84VN1NOo21TjhWgUBr3Q5yLHosuhP6vO8f/uThpz99vDzLjWCgdbjMA3YSKAIG7Ny+UYkCaluX2PVoo0A+IY17G15pg2C0gINvSdA+PBpfovlRAkQd51rAocBFNUBQVdVMENVkTCMOLb6UTBTsxCs4qDWYNQz03a/EGxgiCkcjQ9udxhbf2YYbzVdNGNCx6Fd73+enSK2asw5TNd4nQsyUicDQqlMBswCqBYk1JUpUrRIyTqVYyunNoQQws676vOjTIqecaSoeTvQo5W7U5xtqHMbDUqOznlgGSYrKnJUYCaTim5u5+3OTu4lsoyoloOvy8sXm8m+/KR2ItSYASaSWiW6PKqivtlWW/cf/1UdPf3h/ddaH0xsmugPHZkY2z77XYsM2aU7inwnAcHZj2Y1HmAiICCsEvNKkDVzIeBeF4TV01KAKUJxkZQoGiQoBFerdIhr1OUAFmmEJHJMKYsESI4y8mbGNMp0qx9qyPyD2CyEQfDMi/XZq4FVqO41DP5SU6s3AN4VUp6r74wTCIudqvEJAZJsKkRU2bGenqioCERkmFRFiJEqZsVzkpepxlN1xVAWnpIrVIt9b94uORVC5QplQVWS6m/xiwjUw0wtfc42odZjBzSFBGyy0t1gEVaivIOmm0u3r4XKff/Hm5c04LiklXqbSsUxK+7GWqrXWw4gnC3qRCKvcMoBAnahE2pHd133r729RMm0XqvAaZYQR73Ul60xEhLawY8waW5B0sTzBKLGbt2N8Q5EAQSWCii87CL+kEIHResNzVALgqW+E87kLIBowEdX6IDV64kWx1wx8e+SAL/fvRs9mwuOrA6R8vk9VFJhKUWitqIKpSuwEAxWlFFVW26JUzbC11FqqM9ZE2hXtM6WEvkvHoR6OYxHqM+XMmbmQcFVRYkqiKDejSyd0IhCEgVFEHp/jZl02IuEomMUtu01m0fV2fPLV9uE3B70eru+Gp1VuEnZD7VI9KleVIgoiESXIWZ/SVLu//Kq/PEzPN+XpqjxeRwOQzUGjNirRYk3Rh6YeLUxPmekIQSsiunsctBgJtayxhX712/W79S9kfn5iG0Go7ePk+yZoLCRVbVYYuO6sTxWU23fGwvyc4dYhuDZyGxqstd26CCzt/b49Xxiie4wgeJGTPQJMc9J9wdcHVUxVhklKkao6jHU/FsKm61jFgrcqkVaxypGJarUKc1p31KeUOy5TPYz1OBZOKRF3HSpURgvxCqYknBIDqAJSjDejFEkpBb9tPXszzfYHOmi4tSMdW+CgFJm2aN0X2k2Lq+MHX9xOL7d6PfxyO767Hf7z791fpvyT75z/47v93XESEWgtAoD6jpY5J6hC0iBPv9hd/e5uB8iPH8qHG3q0oFWnqWnzpBJhrE1+kHaToBCNtUGyVTT2vhaHKkgj6ZHCECOkI7e54JszE3S4a6lEI3tt7Bx/27uaJmzrRbObtQb7CpkjKKOecE9yxJNIsdUcIRYu+R5biPzEbNZiaDhD6NIWDOq7gXdFgf2xHMYiAhVMpe6HoqpWwXFRV5UTAdb+RgA0MVRT5o6JmJY5r1e5VNRSx1pFuU9cWKwJ1laeJSKBWCWuvh3qoaTe1ihRs7XGRCMMUmREJm5GTkZQJRU5vN6Vf7yWz64X2+GMoBU54eooq5QfLuvrm/FfPF7+9KOLp4+Xv3u9PY7TzaEcJl12WPesAoV8/Oz+YpCe5Obm8Lvb+vjtcdOje7TavDi//uScnqzkokdCC9eNuDud8osMguWj5f4+W4+GVIuGOAiT9AduiBttmy5YC7CTlhPDcFhpmawnELH8qtVZfeiQvSLhqWGDyAaq8zryoJhwZTB+TU2b0wD6SCkVbXOemYkatIkKCcqXuwwV1eNUbYgqSEC66UpGp9Zi0lzBjmj1IqtMZIsd4pDKohWExLZDORFb563fmi1+cTnlZiy30+LewslwkF+NK3dQE4XXBzWmNijIVK//4e34779abKcFYZGIE+dMuerDZbq/zMN5/uLqIKJ8rGeJvvNgWUfFgyyCLvFU5evrw6NHD370dF0vj7+/nSD4YEXrnrrEej3Wq8v8d5d0v6+fnA8/ekAvzsgFseBVJ7HdjWvuvoi6s4+NvXl+yklTDxoJs+31AuocJaQdPngCVOPYHrtFT0zP0a05hKcEuQXTE3MNswtEmqvhvs6FGouP4QfBFopTHMOVZs94SXytjmuPBKK6H/HqaIdKPv96GMrbu/Hj//aTZdfhN7ctO7IviaPSwAoQ27Y7YQ+HcRqm6ldGpCqHcUoOP8nyGKsmqAqGOl4d1h9ujGqJxwaO8RRIIw6t3BUpGpQUuy/vbv+3zzdlIk4rxRkxeq5jPSYsE93WqqLPzpZv7iZlBmMBfj2CVXOiIrId69lm9YcfnOe7cZ352b1+ucjjVM8TOKe7/VSLXhBubsbd//WKfnPF//pD/cE9dAm26iPce553DSACiQo8mDbsirqtpYLxLJ4ZhoLRNSM1F7O7ZW++EMU8CBY3T+ydrAUuNC8LrKSKTArrcJw1LW5M0+mWOsdtOcHMTEO+VFVuGwPOGQW7VN7WszqJA6BaLwc+iip2+7I7TkVAisS0PO+ff/9BDxp/e+tJiyhAOXPyojGRbZpMXrwToBRNiTYpl6pVZRyrPctomDQYCQhmaMIEES03k9hKbiA20JcTJtsG1POESLUI0DrVd3/zqpsqEfqkx4pNB60yJBrGyj3WzOslc0XK+XAoD876M6b+fPX17X5fZKfdvQ4fPD2vQ6VJZZP3bw7LLqXEm67bTeXBeX9Q7UQ3BbdH4oMc/vzLK0L54QPEKkEnU4p5XiPua8TEhs9hEuRW1oKrI2GzGsI8tadkFWG48zRjfit50PUYLbbsT8TJdfZVxdG3rCSsfJIuoxXBIxuQk/VaAIgt48BJZavtzheRxnijIRmJKhNV1VeHJDpWqYIupzJWAIueP/rDRw+eb+rdWAiLjoqAgEmUiqSeEwjJ1w34dTAlVcpcpNztpsMgpcpUy1TAlPbDVKp0eX5sDkxaFhmuJi1AZ35kSEsq3nQfRhZ0Rt01bS7Hd0P68vbxIm0W3UqxLSIdV6EFVDs+F5z3tOkyrSmB1n3iRN2oz/v+ejHJMKypJqZV4v120KqHq1KJlsBU6ZbkONWSaXeUh/f7PMhjzXVDXGT4i5c3C8an9yk0j4bDBi+NkRFBqpOk0J5gxRqFb2ccujypaxotgjbu1gzMq1IEkthFTcgq9WoKHBGqQjVgNgzcFtyFdCyiILXOb6i2hmUfZm0G3ew9xBRpdzErxK2UA/V4GOkmIhPVY8XlUEVE0HXoMhJpTkjn3fOfP+2WrB3vxJdxjVW6RGORYapjrVOpUxHxJEoBVJXjVO72U5XaZ14t09mq3yxzItkP5e4wBalXBCIDNN4NdSgRSOBSvw27erh02LB9tNW5oIrwl3f3lZakXaJlx4833VL0OE04ljNRTYREk0gteoQo4fZY6jIx0ZP1atml867eX+Z0lA2l7e24HOtZxxeZv3OeN5menPWceDdML1/vpUq/yTtLmQ9l9ZevcHn0WCkarMyJY7QGiFY0WcTiIGSmcadJgBnRXGf3KfbWaZ9nMyANNqUzbNgvY0k8Yrc/l1MQ8Jq1QZPJ+lYNQDSkeDLmTE25Fd6BeOBVACdOv/OL9Y3dAtOMS5EyaPxmT9tCRDljP2AYKphF6f4fPzl/vgGoWyV6uNi+Oq6XqY5aq3Yd16qJkZlT4gRnqneH8XY/HYciKokoJem7BGjKtERHmN7eHh+eW2JpmxJ561u5PA43Y950hPbctZmHRdxUaFBdcz7BuJ/kn68397p7q65WqRV6LKsu3VOUKtqng2oZSp85Z8aoSqhVh60mQu540aWO83nXnQ1aV/xos8iAKlZEZZDzjmRfJ5XzdV52mRLdjDUpzhf53vlCM73961dvfvp4eL5xqt3iIk5in0bJ0gOjFz5EhVo6EGtOnH26ZMcnM96Y15xZeJe1mh242tJ2wXDfFIMU4yFJva4UCa1pwZ4nROjV2LrCemDUGmfcy1vugMioZ8XP+bhizoUDsuuhym/vLPKNYz0OJXWJQPLB6vFPHjKTQlKXl8/XVXV/LKs+7ccKJWZMRarIVOp+LNtD2e6n41jXi/zwor/YLC82fd/lsZQqJFUV2mW+vBuHKlb14LaVIkj35fDyoFW0MQ4zJpOTZu05Ui1AKsbDuPuHy+n2WLkOWtcX3cXT9dmTFffcgWiRtmPdT9OxyjBJTiRFLxadVrlYpHGoh20577pFx8uCfJbrhMUmE5EuE7LyKiloc951RH3V4/YoUCn4zpP1s++e33+6rD3p7SH/36/5ZhTRRuuhZMvcDH1EaTyW2zf7yy9u33x+u706VnGTQjREej+CQm19iQJqy7wUYRNQct9znqqqouLbbajGoqSIFojOKhszFZcwWr5p9udcjqLSZIE3ikjO0zD/Ca6dq++Bov64RM9toLYFYytpGjKj7ka5LUwoVarIapH3Q7nejR/8wfNu06m6mrEVWZskK9p3+e4wna/SVHU/jCootdpQ9JmJlJkXGYnTosdUeRiNuaTNqtuOw3asy5xBRITEIGHYBt5jkYrEMu9kHowlSJkNLovUl/9889Uvr3Zv98MXV6nIowV9dG/xydidr/L52TrzEofd1e2RgYvlslM8OMsbpHS/0215fL7Cfnp43h+vxpT6mzpITl/ejV1Kw+3U9+m4G6dlV8fSZVYRXSU9lKLQUp8/P988Xtxuh3fXd7f74WpXL7+6Vsbq33yCjgNmI1oBx5vx619fffMPb7df3R7uxqmm5YvVz//7Hzx4du4QInOVZyY0GtYRXF/g2BfkDYhlX9bRL+ybRVttE84U7TEYzUcBaA6ywr6PkOEleZKpsWGg+tJ4Tz1D0aWm1QW+hTrgNN2Yt8KX1nsKQ8skC5IdStHjWHfDNIyyyKlcDdNu4rPewZQgirNVdziOi66bJtwd6sUmL/usokWSZUlmvolIVKdKfdb1olMtU9EC9Cl1mcZBykK7pLDNfOzxcExp01E8B1uDj1l1q+XkpqZevd7/1f/wW72dlj0xaF95t5Mvd8fPrsc/fr54Nsm987O66enq+OTZ2bgbc5+6Qss1EnHddCSq645UN/cX0udX747dAteH8mhjj61MorWojtD9WHaJdvtJVY6TPt50/UV+e7077PalVK2aSDqul7+6rD98dP7xufm9o1WVy89vX/67r9PrfTpO2FUUlrFe//bu8vfbB0/PjLzNbDTYTAMQhyaGzis5Y3WB0bcW6SjyS6hlVlWsui6kZnsk0CQJQBYVaHaZHt/qFXO1ywQ1f1Bj0MIIrUQKYbU9EI1OhvLh2GxKnkd/J5ppkcq9/vr19c123B/FVikkkv2vrg8/etCvO0qkirOUhdAlokV3HMtike+2Qylps+LM2YUazyPJgojYbyqmKlORKlDSPjMliIhybMhsihuzsu11oc2tGxc9Ic4AcPlyd/Nq2+e0WeTn99c3h3F7KDnhgPQXXw8/f66l0qLrz7vMh6kqUpe6ZaKcABEQEsogqWcVLPp0f9UNu5IKHnZ5x7Rh8CqfM78dRVV2R1WmIfFtmfK6v7rbT8OgyoTad7ySfL7AsB3f/bvP+d9+unqyjo0D5M1n1+/+1y9+/nRzyOnXr7b7oe4HHSelhC5z1J2chrZQJl6lnG/XSb3LZRFAKZ6iEfwilqzDQ3BkDiHqqj0oBUo5YgW1d83ksNkLsYUy0ZOVwQ5tJCTsS85dQT5tWeGWbgtsIxtiIFH6YPX2V293Q6miCdRnTolV9PK316tHi8V5r0VwfbTYmhMv+q6UwsxjkZV2VYSJhUSru46CpIoAVFVUPPth6lD7dV7c62lCVfX9AMx9OqZ0Gnc0CgLOoxWeFgX7FFHc7WuVcrHuc9I+88WqqzX/h1eHP3nBq0znmzwRploq6Vj1sB8XmbcHQQaKjsfpfNnLu51ULFXPLxa0n+5tOtmND896HMqjdbc7KpEexsqMg+rNYapl6BMYmpj6nABMks5XKq9v7v7HX+9+9sH9Hz9KPe/eDe/+/Kt70Of3+ndpJGB3rNujAFg/6e5/Z2OEgCwamt1oFLWDLrm5WBnK2Y5vcuWVc3+S7WmBiax0GkpWKBJWA2qVIE+G1RPVtiPgHEhMf450wBMM0hOG6Ef2S9AGh5GyBSC3kL16sdn8y4c5MwFV1DSL4+24+/xuOlQI6iT9rnSJh0kA9JkWfSJCYhbRqWhVIVCpdZykVJFSq9riaWWivkuqWkWJOJ313cfnlAhAFZSq1QB/ldMm+U2Z3m1rM0TmyOB0AfcfrbpNXypK1f2xvL4+HEdR4XWfUqJX23q5Pe5vh0Hk3X7cFX13N94VPVS9PdbUoUIra+rzvopwkio5p/OOu7MOhP58sepSt+5YpCPWUTpQJpDoZ6+2N7vR+ogUlIiUKWdmTplpfXss//tnb395KUXf/P7um99dX22n17fjNzfjl5f7652oghO+92cfnj9aiKNI7BYeEBPlhDkONmw3zgWnZIiCSOveD+wKMIvC8Ezo7NAZAKnhkSD2fVQ/PLc9ifzBc+rlxtPIeqK9WHU8dF27VmM+GjvZ+RJR4i6df/fs7pfXcjVM1UsFOXO5nm5f7Zb3elJlIsr+vBpARLDoUp+TaWG1oJDcHcZVn0SQmHNmUhQBMS062hIlgq0iXnzvYtyX/PVegFJkGOtQpEuUll3kzirSrtXXuAZHgELvPVl/9LPnv/3zL8aiCiShWqSUYZzKUKVW2R5l3Qm43h4nZu4SU8J0Oz15vDrupvur/lhKKbJcdjLVRZ86gJe5HKayzF2RAVImmQiFIEnrpJjqGeGfX+2OD/KTi0XpsV4wAVNFqZiKLBJ1DC64/fefv626vy3Xu3Kc9rtj3R7K65uiCjA++JOn3/3ZU8qmWdnw6ykKOJ6EyvDtROjkTRaPYB1NniAY8UeTHNVwzNR/hEik6Yd/+jgljpZS8nIkNJZmO8UjUPReuxH5CsMmR9n74DGJojko4jER4mkw9jviRKQ3g9zYA6HBnJiIJkyk9z++oESH397RoWQmEWwP4+1+mooMUxmmMo2yG8rdfupSulh3XU6LPhNonGrOxJTGSYZSmUigw7He/9mT9ceb7dtjuRqP43R3LMMk3fP1gx8+4N5aUbwNUKNqA1Ut0gmSbXrMfO/x6upyP749mGLCRKXqdl/OV7xZdqxpxRirm+ki0eNld3G+2CiWy5wFPTER+kn7ZX55vdeU9oeppHR1M/AiXd6OA2Q/6Sg4jFIUIGLiNzfHr6t0Z0sdJwUJSBT7UQ9DISaxbRHH8uaftvvLw9lHF+nx5nKous7dw/7h9y++/19+8IM/e7E6y54nRl7p5hRx01+h+KpYOuSqSYj2jvLksjUC9MXV0jnDMJYBViJoGTWbPOkppsAlWi/RxHZqYk/SPHkmrrd1qu/lnSzLBLyF9gRFzQ7tOXCip7ozLXj1ZD39fk+gWmUSUxGk7uthN65W+Xic+FjWPY9Vh6G6SghAmRItU1p2vFzk7KsHUKqkRH1K+6HuhzFWpVAWDDfH+z96sPxPn7wt3+x/dxwI3ZPV/R894AX7Liaignjgn8lJGpEl2Em/Tp8+XG4+WWqZhkJDkVrp2f0+g353Xd8OcjxMn9xfnifqe0bR4258supyBXeMjqoqF+KsU63dIg+lLhKNtVLi41SR+N1urIQ61kOpsG3VFA8eb6Z/9aF8cvbuN9eHX725mGqfPePRqqPodsSrI++mun1zfPbTJz/+42dVTIxB6ih1iUxHlWYsxpeMMJlfRVIpjdSHkiqqgIhpFVYA1iim0xxmNYJbq2A5HAqQFJql5VdWG7PDE1sUAZwWRyyHI5/tKuO/hwjYnx3aio7ibbAWe7yP8Fu9q0SEjsEWG5FJpSKp5Kvd1Wc30+M1HYvRyS5RWqXEKTFSYgYRs4muTYoQkUTMGWPR/TARUWaaqjChS4zdRETnLzbdv/1o3D5nRn/WLc978s2kVOZ+wmjWU1IVCDR5VrC9PC5uDlVQKzHp/QVXURJ0rB9ucp10qPTPt8fHi/RBl87vLTnlnHnZkySuk4KUe7BQQspV14uuipx1aaf1Xpdf7QaTLytAicdRqeoksszoRPhioT97un9xtv/bb85eXjOhiOyle3k3SgXpxCOy4Iv/4/cPPjx//PE5uaLuorvO7hNU2aZBPNUJgV2tvjQjWXxEwkhsHlXCFODJhAQskpIvE/ApFyilH/wXj1Mm9eBoUNWe4pbaI9KtaczfpKqxe83pr4OhtQo7Igpb3EFIvRGSQXJb6vWg531+uqZOL/bHpytcQL58O9Coy9uaE3eJRdEl7rvU5dQisQiqt7K7iGK7cvpilsSWd9rjsZYvzjYfboi5W6TFRb+46LqFP1+HzKQoSiyIwp1CKzq1p9iRKm6/uOWvbmWqh6lcbvUwaWYai6wo94pMWDI/WqRB8NVRHnb5wTqvNx0TbYdSSbdDLUJTlbtBtMg95vWqy0NdrzvZT+uzXsbSJ04MUiqiWdGvMlTHxyv+zhmYeNPRBxd3XZ5eH97caVFcZO2s0qkgYNrK5XZ88um93OWT9CymQKM4pM3gGvDMPCzK7ZH2uc5haYEJax6rtEke9lVns1YBlFhBoDpp+sHPn1A2kTY4le1vTN716ooa2f79oOjbcFuiME77A8dmNvZ79nY028zUtkSKOwYRp01afHp+/sP7Z5+c92c9T5KPRyn15athLbRMnIlypo7ZmoKc4bnZuxzWmuWqSqk6lWphVOxJmSpK6J6tNh+d+YgHDEeWZDCmmFOnGPeqnfpT21V1eHfUr286FdvQ8uZQq1Imur9ZvOjyAFJgvegervp7q+7/uTk8XHe9yFFVQccqSlpVK2icaup43ScwUpcgmjqeRmHSOokqCdGKaZk5MY6l3n16n5+sLDujxPnJ5nix/PrXV/d1ZNKhShXNibuERYJeHafV4t6LjSn21NwGLZ5pM50QAbx4NJdx25DE22ydVdvKI+okbazs8R2qQNTy7fEqIFCZJKtXOgm2dj7w0x3at5dX1Rplo29p/tr6XUWVCRIP0DPPqUpJVVi5vQeq9ohiJQj1KS8zoMy0+uDsoDJ1NH7+jqssQKpapC6UU2Y7p1YxbkC2I4u3fxOAqZa7fR1LEVVbx5TYK16kOL7clkPN62wpdVP/revWwT8kzJa0i4o9icvGPW26orTo0/0Fvbjo3m7K1zfDcdDfv9w++eje/dzvxoJElNFXHKH/+G7/dH1vQaRFckdSwIkgyKvu9+8OeYOzRTcNQoukx6KLRFL7TS9DSaOQ0jLxjunX03H1ZJ1ar68CwCCq0KHv6DiIqijurfD8fJkYk+j1Z2+H718sHq9aZJO51cK7HcVSfNFmhQoiiaXu/qaIfraY1q3JLElF26IBe2cYraGgqJqdQwENndaz1iDy/jg0X6TowoJCERtPtlI+uZIpcJrvuxU7npIqeQMo2/omIWLLK3z9nYrZTF7l1YfnA7MousN1n9gGSD3z02mqVdElZpYupWwbYUOHSXbHcjiORTQnXvpmx9xl2h5tnzOavhmOb4fNKllE8K2U/HFc6g196kMfWhLFrtuWw0te97ucOmhPtMnpXp+WSV7d6rPV4kCYSh2FNh33CaXivMv/fDf99DB9/HiNY03rVO8mPuvKTcmL/Pkkl0PZi3Q5T7fjoqfd7XHRp3GYUmJOVJk0M6ps/pMX+aIXadvOQwTvvtjuFumDf/PJ8ZeX02eXRSpTyoky0aJPK6Xtb67HewtJTBSt3MpK3nkizsNcx3Ii5ibhCGd1d4gvbhRVW95oUQJqKiMH8kXi5KFWAGr7nykoff/nj1LbcisQArG2ZF5CRoR4Ko0njEGJQsVw6cMDE2ZZw7naXNKi+J11pvlWx8TEiXmZayIc66JYh4l2ORH+v/a+7feybCvrG2PMuS778rtUVVdXVZ+u030ufTgczgGPIKAgCIGgEqMv+mJCNDExIVETjUF94B8w8Y1EEx8IPhh8gcRIJCKgOSKCnAtwmqa7T5++1e1Xv+vee+211pxjDB/mWr8q/gVTM6l0V3V11d5rjz3mGN/4xvfZflBVD1GqwM8HWcp2uRuHpMzU1qGtQxQOQaKwmvXJJiTFnG9V7e3lddkxg5HzyH++L33aFCIiuHrlU5dlcGbaP+2bzXC7igerWgLdqMLtVbh/s3azbUIjXLNXFMSwN/twN7yxbNZVWEcWmsqTKgbKVlVy3mdyyuoh0rbPCLwb1IBu1ATvRtur7Q35sEp3V8+amXALaQAAIABJREFUOHNTf/j1E2W5+70vLz51zHcPesd43teGiigKsaM/7TLE1xGBr3uv8qUpOWaCBcpE+5pEXBK70VzA0TwsmFwb8axcm6Ntemw0RyhNjHGUW9HJOWeTz/6Fl4pv6VxvAdftp18Hkc+IK55tnj3D1TA7Kk5/wjW04c/it3wZi8DlXAnNDe0coACBA0tgOx18k0rKZCIzpCIXWsUYJRQ5TXc374Y8qkXhppFKRGSqC918u0+Y7wAAvIztJ1c05675QZRp76yxNTdRVHjcarF4bs6vhOtwfLq7vZKjCjdqutHKQSXLyHXkLlkkuhz0m1fVez1D1JhePW4rQYxcN8EdHllH1Ui147xLB4tYEa9r0eyrOnS7tFhEJ+xHTaB91m3SMXm+vyprAeWzT7sxv3V+/mhzdT7025EaOXrjJtXVjfPNnUU4iHxYEcyPL3f0pLejRps49W5TrY/pDgaxT7cOrHysNjmj+AS1TWTFedQ0tQhTA+DlS/ysH/DpU/dn0cxMyNmCWymspioT5eVgomcXadxS+HvBBA2YWfTu5f6biM42Wylel3BSEjYVnKSQoov0nrs7eNJjKWOtQg1hRlzEIJKp7KJPERpYFlWQUKYMbg7Nns36ZAyEwLWEAkSULDpm1es3Ruwl4eQi3DD34wDcJu9Tf/5rX24RmyAim3t+0MFhvH+zWo55FblQbEOEKm6uwmmnbz0d37rIG0uV2NZk1VTvjXaasj3pXzlqPn1Y0YAg1F0Mq4O6c6yT12ZpcKhf7MbcyOM+d2M2p+0mGbk78pBpNGsAQ3/RXz7adx9c2mmfN7n/5mn/5lk36tEXbrWd3pfQNpFcQbRug7vTZUd/8vTi++65SEFM5iw+Tz3K18ymB4eJgOgzLWfOFqVeMkwDxykaqBT7E3l77kmn8t59xsIYhvAcqPJsG93xXFswfyQEkJGzTZ2pwQvKRkbGTqVWm/ePrsGC0i7MRlPPRrVEz8qjmYRTviNm8N54HkQIcbJcSeDJg8nVPWUdk+/65O6Hy7pQI9WgiiBkhiHrRG4iMwPAejYO50P9UgsyKE1RPoOTcyc2ZeXrrcjrzr/8y5D0Yu/ravL8ygom7JMyoKpff9pLExZEplw0Jy6HvGXux9wp/ex/+Hu/8i9+7ewb7x20YXc5aB0/3I2nXX64HR5u81Z9KG0HIPCGidjVuLkaF3/09Oi1Q+ryu7/9cX81HEauhevIdeBlE+po1YfbB2fDvZfD60dVMibGmJ2Jkpmf99S7L3xWRy/WtQzXeentuaph+kFzqYYZ6HBTzKODadvOZyxkqtnn/ZRpnvL82gFRKAUcOVzo2a2KmfQzubDQM3JaCaKJYnQtODnF/BSq9kzPb7aoK/DAdTPLYFzzAwgzucjdmbzP3KsTcXFrIjBxjKV59Jx9yLrvcz/mpHbroCmSj1lRkqUwDSmbYoZQpnbKdr75k4t4FBGE4JNG4TQxcczy5wUtp/KIrKjcFGjSQeidfvvj/Q8f4bXDWlj2Q3Jg1+vVXj+6zN2g+06DkDvVFcuOOKSjNhDRw5Mt3nzi6+pBr8Muayu/9f7maT+MWnxeYDAG3V/4Z9f+2trVcKfFV57Ybz6xk//+0fv1xxJoeffglS/eOn3n7OFbVyKOxreXedVUH57ux5HevUivHuaWwEHMECIx03jQYDd6XYPIiGaZM58uBXq+VJ1H2z6/4ZJ2/Hp3ZGrspkRn03Ynpiag6LtOMecTl6KgKwhTPGKmQM7XbSnCca3vQs9NwY2u1exLzptwgmf9KSbcbE6G029EcRAswjz+bHe5RG6hFxlsk2TQDHaCEJt5YBYhc/SjXu2GrtcxKQhHy1qETY2EC6VXhLOaqomQGbz8lWYEUvftO5fL7zyqj2efBCvl5nXe9ln1Yu4VpsdSRlMAnJhO1P/ne/vuTiGKZRHUIbR1uBiyC1eMKnAdhZibwAzrB62Evuf+4c/+zC99nOl2IzeP4/94//zBzogI7OIUmALTyxVerv24ttdW+GiHwfBjd3HW+9eu4HtkRlxUFx9uL04Hv9OeftBd7jIRToahreQlty7Rr7+zrZlvLuhGG9YLcbWHn6qO1nGiWV/DX0ZTNWV49lanIIDBfdpLmoOp9KGFpDPbHk4NwZza5p8WKaqyuOgOLkBUcC+FVzFqkQJTEM0AmT2X3Z7hS5h7AQKo3Oll+u4zoXH6ppTS7pp+6GTEZF5MDGYdTwfclU2MjJSAixFwswKQEpPXVYBjs09PLrp+yEK0aKuDZV0FmJmDRVE0XlRt1Gk/bxhNzU0n5oEa5UFzr1VRMWFjZ59mKcWPubx5v06BrvBJ7KBoakCqcP8H7u236ZHb7u2TYadC5Jy7MV2OuHNU32irtx/v9r3+1Bdv3FyFMVs2yxkXXaqFo9PG8fWL4cw5BHcn8yxczNBA7IF9b/zHF8aEXcbJHudpMtozx/nb56tPrr/0tz4T23D2YHf6cPfxVx+/8qVbtxZx9c0nVV2dLqv80cXpiPfHrJlotMVH29TG2MjiRiuBC1ZPz2usXFerNueEwouaA9AmSJbLk3h2lfo8pXxuoXPKNoW+4VMr635dnxUpGjb4dOERU9ncKBwPAhe4aZpwlB3iSW2qBMvMoC2FgBmKmy1mARKbR6iFYErXrTrBJ2/tSQ7hKpVlAzNIoBgY5Je7dHrZ9aMSYbWojw+aOkyRn83dXdWJ3NyFKFaSVZ+VXERmnnLad3b17mV1XImwO1lhaFw/8vLnTZUuoYScuTEAnUKN/OXXDjT5cDVsO318drLdjrt9/qE7dWX24TY3zEx08yDUwZtIbQi5sAPd//BJWiyrAfjWxWDmwg64G880UH442IM9GWgSOXMyhxqKs6gANubl7cXyqALTnc8c3n59ff/zx806CsvV3dWwT7deXe/Pbh86hYq4kXHQ3cVw8WDXf7D7xF+5t7rVzsJmc+k1XYzXmQlwnSwOn1VvRR9ZfWo2y503M3LNDPOWZpmx+8wLnYszgsvnvucmySQGSLjuxa4TmEGnTn+udwjXvmiYR1XlH5NW6Nxkllw2tQA2mxLMTQZm0G6uPKfWcFB7d+ODmcHc2ioExqbLTy/341j0goSYZ6Z5kf53nVdViSaBQDUnJs1TyWkGVX16NXKvi08exDY8D/yUL+LcitD8yAH1WKqW6YE7AE329KtPvvWNpxfn4wfvb7vesqIb9XGnp72dXKV98t1gH5wPH53t96MRURPpaFE7+clOV8vqYjPArGzPEPEkCF9qxRlxLBcEo1hkzL2JI6ut7yxDEwgOQtVGESZGta7aGzULV+uqXoWwiFxxVfPiqDm8u1reXzfrON9/U41Q4Pm5KL+++DDV9z6tQU2pC5MVz5TPplUrm+rtaWOK5pc6BTI7CShnC3rS54okchXIioVsYCnSOqSswD77CKthK4ltFHIImZWq3ybrO3KzycAZRaJszBYCojmB1PxajIUcRfqPIebGyBO+xiYKB3YJXSaAiZLRbkiR+exq34/Ks9t1Vt0NGJWr4IVkm7MCcCIhJAPcRIiMrGzhlMsA2Az5eK/jxdAcVT7H+GyLZtcUqXnQOQEwNpU2E3DkjryIt77j5odvnQpPKO6TwRmlNmCH9xnoU8r2dJfgBLe2YgZdjH48JCYrpF8JpKaFIYNiAXfNqwID6lbszaGKTO6G4bT/+Pce3fjCraO7C5oN36/rpNLkW3nVU/llBKpXAiv1Os17cxNW4X8mweG5wnTGSaeWwKc6aOoBMAcXAToN2a+l4gkz0jstDoQbHbrz8XBRV5V3fSLm7J6dxmzuqCuhjH2fs6stJK4qqtgDgRnsXMnxOu5SgpsSNJISBfegsFF94dQQ+zXoSxTBCnPnwJWC1XMgDzAmYoRAGe6bLOYZTozgrG7DPmX1EMrciufHY0N2NVO3KIVzW8Q1PRDHOgC+2WU399nDILlbxebWP9ytP7FygRtRWRKZIJdCH56WbtzM1VXnvt/NlFSzZPquz7z0jW88PnvnwgyagTJbEwtzIQeiXe9bVzdnARMzKbFXgfa9B3EmIUITaFAq1lUTeGjXE2YHsRnK7JDIPROxq9pwNr77a+/d+PMvf+LzN6qG4fxnZAvcS6xeq0w5aELI5nUjTOXB9NUyzA7V0/9e5gFzH1wucSu1a8FTCTN+cd2b4noiUKJ5yojMAjcPAm5EyH2z0ZydWB0gSA2IcAMa4U1gYkamdkDe5ZLSYyAWl8t+YTqmlEat6pBhTeBaQkrZwmBRpNRcDhfiRm5Vda950UTuvetzXITDg+ZRtyeHOPbk+awzBzMzTABVcjgLiU84y3OPysfs2ayWsFqEOhZH6wn8udimblCaEWMH9qOD0Y95/8F2+PRBs2zYzLMdULx09ZoCQA61SUZX2aGw5Aob2IPjQGW40O3FPjX67W+c7Hs1hSqhFFnZLSI4sUyOD+buIFV3t7JVtToOMvGunJmqSABnUiYp3ZVLARzpE7ePkmkdhJj3vT653J1vhqye1cEhWHr42w8un+4//eXby6O6dPqYeujpY5951dMMcsrpk5kSSiBhLpdnJGy+D6fbU5/lvxLxag7x+Za1ibj6rNGcgowMTqbPRvVhzFrFOKgRAUwgEnJzW1Rxsayudn1gOjxq6xjOL3dBAnkW4RjE3c09jVnIIwkCopMae3KVFERsb+g1xpBGIyIW+CblFgvhhdp2l5By5XR7VV2cbja7npjdkHZ9JFBZuCAomTA3FaNQfabvCgAQE5uZYZf6i51HIQlhUcmiDdt9HkaNpdIG1Nzc9mNmoE85XY7jH18ev2wLjt2uPzpYHTL1GAIHVu/GrI5MPkavROLe9zmn6LWEz7x08/DWwdcvn/zm777/8PGVKsGdyc2Q4TAkBYnVAWHW2boWOCSmZcPrmoSL/zWMLApH4SFNEF4V+WjdqOLl4+azrxw+POs+dXfdxHBytf/Ww+p33zwBUR7dCBakjnb1R+e///Hmsz947/a9lZktE9dCVxUytKi3lnixeZxGmNk3QJEnKb2+gEjpUEDgPmVm2sLTDH1Mgx9zNuMEmLqRJE9kyI6aLVJRTiuZ3M0FiIZObYQ7uyYPy1VVBzIT4moYcxWFmd0sBA7Ct6rlMIyAGdnBYc2EIG1bhx///lc+/cnD3/jKh29/dDnB9q51Jaq46kZVI2ap2B1tE/bC5t5WYuZJbcypzxoDV3VIau+fXBCobSKIxjHnrCzFxwnMEGPinK08Li6u2KXdLrwQN02KlBUkbeS2ift+3A8pFit115zhwJC0Txoi96Oa6vbj7StVvVgLKfEwNlVceRzVFHRLagddXHaU8qKmq24ch3RzVdfB+9AtD5ebTf/ho0v3mUJcSmrDLDqO/QAJ3oRJVcIdCgj8eC11BIAgAEENIfAi8paymrV1/RPf+4n7t9dX27Gq+Go7Lu6u2kqGlFT9/kuLD0/aB6ddVrOUjWCEwzurJ092X//V9974czc//crRJ1bLUPG4H7o+18QhkAdmARmWkfuEyvlw1Ziqwq+G0ZiGPo99WiO0oNdvLgX8tOsO1u2l5m/tu8ASRWpwp7nbjgckLfF+1L7L46DBvYoyREPLfbLek5NXHBqmpYbK3NQ2wzCoa7YQGEGIBCIcQwgSolDOFiuuikiwixDVVYwBhSf98z/7k/jyvwbw9/86/v3Pff9mr+6+H/OyjexYL0IyIyrDeVrWcrlLyXRdRxE2d2ak7MKoApe+OARhRzK73I4X57uUXGRShC+8NybWKdJmNXhMdEkiioHaulkv46IKarYbtGhomHk2qBkxdUPOSTkgu1/2KVaiWStBXFZV5DGPQiFljZFVjVjGnE3NoesmVIGaStoqbLt0tjn7v3/ywHORwgcIxohAJpAhG1ThBjG4IwquAfdQkwg5UAeIgImyg4kOl5FASXW5CB+fbD96vE1Jz7ddzlrG3DmTIqvx0PcHi1BFPk8GdXOv2/rmOp/u0rd//+niCt/3l46ZaHs5HiVh5vWi2XVp2caK6bgOp2OKVfzcrVsXm/2mGy4SVov24ebq7HIUzlXN8dDbJpxnLIkPm7Y7Gbb7cdnG1aKV7XjD5WBd1VV88rRb1c3AGaCq5s0+p43rLr0U6XDVpj45eF3HrPpypsVIXd+PCUGEJyCTJ+cHy5CAOkQRdvemklL6VAKAPvvqS/jyX577fvz4D33qv/7Wu20lFzuPMUTCqglD1j5ZFcVNb6zizWUYkm1HXdShJDYQ74ZxXVEb6cOrsapIXGqzfkhMnjSbTzUpg1k8gjQzyIUpspSRg+rE3ieiOnJTBWZsuixEQYTZx6xmZm5s1PXZjFaVHN9a3Tho2sj7MTcLicyAV1V096apFg2P2Uf1m7cW5IhSYDS4eWAC4+t/enF22lXsEsq+sxuQFOM45bOUsRuQ8pTbJEyzNVPf7pO0EgNakbZilpCV1m2ohPqRq+C53zcxrBq6s1rEyG6u5km9T3k36EXbPt2OT81DVlclmGTNXR8FDrz97tPfbMIXXr95EInraswgYN/l2lG3MgzcxKBqV5v+48dXo+acbdjrdtsLAcx9wuOzXRXHx+d9D7DSZpP6MeUhd31KQ1rU8eQyKejyKi1iGDMGG9sgKUETKvi6jq/eWp1e7k/OO28CCEJUVxCKOXKoYgiM0XKv4yI2McQqBtMMdzUbhrSoY9tUTJaSr5fhb//EdwIj8DvADwJ47af/6Xd86+dytsOFuEsUW7ehCmygVRuawG+8doxVvXt49fvvnO4TTrcDkd84lBuozy770MjKqR+1G+DZ+2xeWl1TVctqTLRe1kIE8iZIFZ3ASdUdyVVAQYiZYyj8EwXQ1oEYObuZqxmTJfV+9E/fX//Ad9+r6yhCMFxc9U/OuoNFbfBCNGLXlDFmJ6GcpfQ6RJNhD8G6wd5+/1TIJRCVDXwHOQLDA7qMNCIEtDUAjFYoUlPAjRmbDq7qxouKFjFI4LNdPmzD6qh6dLY/XMrNZbNehIM2LipmplF1GK0f8mbgy50Kpf04Xu09+LSdNGz2fVnVMSjhD/74UYz0w1+8y4E3XQLZyzcqwAbLPrjCktk3P9he7fKiCVUVNFnbSM4+Zq3bMIK2+7FuQzJNg9c1SwjuULJ22QahvY2mfrCuGJCEpSzWTTxLHWpyJanw+Hyz6TNHKKkyeiSKaGrWRAE5URWWURZhkc37PmlWIm8XdSVoJFYh1JHqENBQ066wXL7zn371F//be5/79P2/+8//HfC9P/KP/uHD//iLQ26WdUya791Y4/UbE8wihBsNIi/z+Bdx8M2Ptm/cXldLfnzV7fbWsVdC99bxg5M+MB2u4yJUj5bx7HwzDDrknLMRKCU9Plw2VZCCTpHnbH1Sd1eiKKEKk9LUqJ6LBSdTzqZqTBQkXuz2Y0ZbVVHEsvWjaTYX2g62zz07gvA1m/Nim1zW29So+vESdczLxhrOKes7H1ycnXdl7MGYxgxlPCyCxjE4hlS6KZgjOcSK2DeYkBXbHoDVQduodxahG8zddiN/69yqjS/qvgrhYJHbKixrbms5XtQDwkblIqct5L3z7sl5OloT1EG2udzBIARjuEEz/vBPn3zh9Rsv32xvHTRVpKRelvVXi0pzSoCZ31x6yh6iWGW2AHkcRg3CVU1uXFqFXJmauYe2CkmzU2DmXYco1NSx8IGO6urmou5y7FN2wGCR+Wh99PiyP++SGa56ArlnzxVCUtbRkqow14HqAIELg2EEbgOHQOuG2yh1HX/vPfrH/+Zrp+eXn/tE+9Zb7zz4z//s3k//KyDd/TufxzZhm5ANbUQUMKMbcGuFyx4PL7GKcWxvXAyvvrxEE1PvVR5v362JkNWPbscyAz0L9vRWe/K0Wi7o5lFzsKzf/ujivQ8uYyUHbW1EBMqqKasaUs5mWC6qEBhwMzNVKUsBsNHd3KKImV91CqBPebNP2TypJXUnCkSWICCGOrxYLGrGmJWRovg4aBqTDrYjHVN6+/2nZYmxkCnnacuMoQORYQHjCBjUMCrgqANAEEFzABDtNn5GGa6lMv7g6faLr9/5oS+sHpzub6xCFaVUhFWU7/7kUVOxq3Z9+uqH28tdXtTh17/6MXtWNTX0+7IGMTGSHbja6B++c3rn5qtNVZxwPIgtamGyUEnlGJKNSAqr5nEk3KtIdfBFFfajAeBACNQP2PZqgdeLOo9jrHgZ6ipwFSmr3z5Y3DqoDmq+fXiwH5WhMQSGNXXFwt0+9Um7BDVc7IZH50NIqshGcK44K4ZRF7WQoU/YjypEIaLPfmNFYBfhp5vGhI4P65/80dfuvXr45i/+k8//zI+B/irWb2J9BQzAEbABMtbLSaY9EA4XH37t0WaXdrs8XKXTi/Gjp9smMMiHQYVpn3S7z9nQNuFLn3upbcK6rfbZ3j/ZnVwi+/4z90JbCbF1fT7bjGeb9PTKs+Kv3TtuljHt+mzOLI24gcYRSc3B5j5kHcZikMRMIgRir4WYwcTXsnvCFIIwwdaek465K0i6MAOenU/OU7cbudgXkKMAVGAtvs3kQiBGDVDAVkGMlLBLSIo6YFkjBmqOFue73W5E1fmDp92qjTfW8XSXbq6EmQoE8+hi2I36xTfu0MHBtx9vcj88uegvOwfR5+6tHpwev//4TGBDgmHKl0QQgRngePO9s+/8zEurRVTLdSUARbVuTATkbN2Y+9ECYRcYFIQpCohoGH2TUum0+pTIKJubyYKjIY5mmv30vK9jqAIRcRXsYrvbdcOire7dXLxy3PjgizpS4KOjtl7V3mVqI45qwLHpg6o19bzrRz4kd1gdqN/t6hizWXaM2WKUAI9hValu9v2Ts+Ub999A3pycnH9++z5WEXgXuAcIcImLU1wO2PS46PqnHZu/+WDz9W9frZv41W+db/d526euV2YiRlLPak0ULSsnhqwYd3rVdaPRfnAOOL1EE/dtI9suP73SbQ81JKBiKBFINoMFJqGS2DBkT9kKD+xqZ0TIChGOJBKmGQuBslph0EFgSkOyMeUCyzthHNWBOooI4NhsR3MSouudCHbxeWVQiEzcdRpRCgMKIWSHKg4XqCOgqOFtS33nQ0ZW7npdteHDk51IWNZBmMfs++THbfipn/8bwI/cxpv/5ed+wSHmumzkeFlFIXeOUXSvhRJZRJyCsLk5sNuM//sbD1979VAEUUKR4XcgqxGJkxFcAGQXspQtskgEHKruDpbCcWQhBKaLzX7T9eYOpsSUUhYDE+0f63Y3XOxSXYW7p/265qRYVLyoZVEzmatD4YdtvHtYJbOQ1dSQspbRkJqOvXWENOaqsqR+vs2jurpq8jpsbx1ckflHH9W/8MvDQUxDwh/9y9/4rle/ctjIG68cPbjY/sE7F29+tL1z1Fzsxm7wbJqzZ/dsJAw1DKPu+wR4DMzMhWwXhIjZ3bPCzVarVovpk7k7suPbT7J6zgY4mAECE0QQmELgbcYHH18ctLJqggj3g51cjubGxGOa6Mpmuk8jHEPWYbQYWN0iS8lGTO7qaZc2uyE0IVQiIjlbxy6MlP3k9IrmVQyaxoBlu4aKpKHP2icGOEOApaBhNIy7RyQVD+rW51XFqpbgo4IFalZ2mdpaFpU8uuy7fdp0/m//wS/dufMrfTc8eLxpaxaRZV0ZkA1Zc1NXDoVMw82fuIsfeNlK5TIaHqTT7bauq2ji2bIqTxQbyQwCw9So7IHD9sTMREQp5zINI5S1RTIvs7dpIzOEAHYmFnEhdiA2nNwebYaTHbl6kMk/jthzxnZQVQ3MST30ozqGZ5MH4pTVXNuqIpZutye3VSDnUC2FmIWV2ZnyV9962KcRCof/n7c8CImwEFSR3T446XxyjLOcnGXiajBB2KMQETOZqTKTGkYzZhdGEDGiccxq2qe02e+LMkMppaOgjC2ywb1cFqaaD5eBAj4+HZgGTTCCEIxgqnUETytpttn2APXJUva2karibLbbDwwwI4ArQV3JftTsGoM4kWV34ax+1aUiik/PSBVFFL9MZ9jUzGEKc9xq8DffwP012oDIEPavnNrXLgV9rgLHACE2Joa5ex3DugnCIAY5bh3WZsaeL0+vrjod1bfbdNTSmD07tZW4k5lKAIHqyGaaRzzZYzCMCjXU8FEtp6zJHZzyaE4hCKuDySZ2mTNc3cxAzDBXEAvInYWY2TQ7yNyzmjCEKJkFRoZmeNJMROrmbiFIWZSLEsgpuwUmdcqjwjFYUqdwtdk3TYyBAepTtnnCVkfrBzW1OhDgOauRQykHIqDrBjMtjEe4ZwdzMZWbB/7uTiSshUVNaZLhkzKjLAGrWj4vMyMyIhZmCT6mPOY+ZVW3bqdqUAcRAhcCZjHugANjxvnVIPAhaR1DEIVRZ+aGKsIMZsgGJi8d0eVuYCIHBZZxzClfM2Vg5iM8ORBIWEorWVgmqu7uxJTVskMcmb34+sChfs27wpiL2R4WNW4uwYLe0Wdkg/e+HzQK1F1AZhhGbYD9qEHo5rp+cjn0WRdN9eXXj3/nrcdV4Jur5nteW/7y/3r/YBl/9Eu3P3jSCRBEklEedFUxyJYVxRCV0v1Xm4NFfHiR3nrU5wFp349VTQTVVFxHi/V22QdzcldyqLkNowqX6tAAyuZBQgi83w8uk9dDFYKbMeUYQ6EHDUmf25FMgQt1cQRRMmdHdm+bWpiYxQ10vOAgKJkzaxmyg4iCPEdFmjdUQc+CqXRaBbWfxF/mBc2ZwQaCF6OlQmGYN3HLT/yamXCN+hJNu5M2s1C2o/fpmkgOmi0wygiYCEct1RWb+X7wMblOqxCzM+rs9OLAQUNVpFnAiOb3MOvRTEbY07IFFe7cs/UHv9p5yhNZ/Zqhdv3yf</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9Z5NsSXIldtwjrkhR8ul+rcX0KMwAhMYqcCmMRiP5gb+WtoTZkiB2F4DtgrNYYMAZNGa6e14//epVZWXmFRHhzg/hEZnNn0Dr7Omp6qybV0S4Hz9+3CMS+O713eu713ev717fvb57fff67vXd67vXd6/vXt+9vnt99/ru9d3ru9d3r+9e372+e/3//UWXH3WOoSACYP8qERSAghjIvxABqkSkUALVzxOgUCLKx4Eo/06KcqRq/TSUAGWQgpSUjk5FAFDeUBCRUj4jAMr3ovk+lRQKgOw+7Tqk0HwfoHJ6KjdVb5ugdkMEgPKpiAFVUd1pPxMivbrehw6rS990DtB6LPITEVSV8+2qKogY0HxtJVC+KyhpEplimCRuRCdRgQgEEFGAkmoCQbXcGIhBTE4BAD01DdAQEsjT6k7jG0dMareAfGUbAgiB63uSx1IVNpVKxKqah1A1j6uQkuTRUgW0nAqwA2BHqtpkHP5MCiVFPpsqCEhB+uSZiRbsfDYdKEGi+p/86/falpVAdbDKfIDy0DITEaloPkBBTCTIj0ic5xtlspiYSAmsBBuOYitmwiBiraZls2UGoiBiso8QH1kDMaBM2Z4EUCXzjzzU2QBBIEa+KPORiULzVZnUvCZbH8w1CJpmDU/H+9ddGvlnv3hxexnf+9Hp6qLJA052A6wqxKyaL5bNND8FE8QuludDNe3jdDUML4bbL2/jzRznGCJIaYyiSfeTRoEjYoYqCYv3xJ6RFCA+df1l69cNKbmW3/nJnZO7vfPO3BYKybAAhSqKEZhhZDMnQEWJoS03SXVOIf+FVCUbULYtUVUlyQaqqlACUra+7IMgpaTZxQAlgULz4VBVCE27eDm0y3aR7mi3bpkpQ8I8im8751pmkKEMGcoQEZHm0c22USY/zxKTGQVQ0CEfRQQCZ98vAFN8gbIRqxJTsax8QoKCydwuOyaUOH+AykftYFWnKNCWbTrfJGDXtoOp/opqykTId0/QYrj5L+JEO++9dw37xvcLdEvf9R6cJ5ApDxBcser6T3k0dUSGF6qEJNM26pDSyz22cZ5SjOqYiKBCIli0IKIpaONojImUNFEIMo5oG1lAxzGl5dyetY5p2oaTe4umc8TmW6oCYqhk8FQ1xBUpmAWCiioz6dK3qnobADXjyhilogQSVRWFqE2bGR8UosqqAlIVeEGxPNg58g/JT6QU0HkfmtT2jsmpZgNIvni3MlhJQfZPniiuUVGzHaD8SubgBjbFnMpkl8BHRPnWSYstGmIpwAU46/yTWW8JtcWEyLCH6wEHjKRiQwVg6ht2cHYA0nwvNbCafR/+AZQStd6R+qbl2LH3zEwW1UjMPmukN5NlcyfSYuSsLJQQxzi+3m9+dbN9tqcECEHJEe8niSGB0HoqaELDgLbTVc/TrAqVRDHKPFG4Ed6mxdpdfbUJAWcP+rN7i6b3NmYqBtF5ZgjIswPjOJmNqGKSUOhRtqVMacBMokoKsMWIMskgznaS3yCQglX1iO4UypH/BMI+xBWCRqbDuCsRPDEVfzff5ANxYUUx7zKTRpGMcJlx1XkvNEsq79Lyx/yD6uFco2WZZZjpUUHQannZe5k506w8TgeKVYCKyg3Um0V5PCUwqYA4j2j2jQJw2R+CEkQW3jdtc++iuzlzbXdkxGQmn/kmQYXsl/oImRHmgBVjGq/m8WrU20QJkqRradzqMEVVAoOIxhn7SU5XOfCoI/aMmQgQAVKklAREaSu7oO6rrToPEQJdPF45zk7OmdVBRM1tRDPK12iiBNKkomWgqVAuYxxKygLJhIjAqmI+yiUi57csiNiIkk2uAkwQOEcRIcREgQiZ/2SaJJ7y6cvVuUQIOyUpADXKhDoxmaMQpPD2QowMJwtTrdOuJW5m2sLVuAqXp2rKOYYW3ma3atinpETl4fMYJtUkmoQ8W4QgpBDn7cyOm94Rs1+4pmElJhYCKykTw+xe7bEzqUlwjhaNOz/reT07x+bJJRc6tl0qiEF0cL4cGjSqDmG+2oeXs04pJZ1mWbTkGImNIMxRnWcZZD/Q2VK7hkLQmMAESWg9Wg/neZiRgqjg5tmEfssdupPmNCy49wS1rIryk2c+TmCFVM845CekykSqXBBJkX8nlDlXi2pcgi8yixE1q8mwpnIYFOSwTaTsKLXk4edJVJU4u4ISyNc8EwXLqBpIQSCy2dbiCcgPBbaQSyQFfhjIcwmzzTz6bNNVaA4K76oYVxle8TqqUcrMryQIVLNYmdLt093wZMO3MZ23uyjkOExp+2IYbydHxI1rTptHP7g4u79anLXdqoVDYfQ5ZhV7RkkAk+41bfbz9iSdqnPmlvxtVynxkwwtCvRWrEDcpfBimDfTdheGIYpQjOIcNw6iGqKKQFUaT12L5cLvpjhOut2riDCRJAiocbgNOgsaQUjy8he77fUcA84fLpuOibl4KhVyrVIjXYYhY9ZcfqdsWoZMbCGMM/E/JMsZoYhIVCyrBGX4VBKqOUi2AoESiJjUoWUOSVNMvvXEknMnr2oMFuX/q3fiEA0znjrNAZGgYGYz+BJPmMyhMreuYodFFWUU56MSQ8vsHLGkjGdE2c8KzhviKjEDoko5t5tv5pu/vxq/2aWoJPLmNtCS04h5m7xD19F+0KsZ+3/aUo/1uyfv/u79Bx+d+t6Xh1T7l2x8SSFKMenbm3k8SWttG87wm8dEzOBqMFUycpFjceEsmoSJhBHmwKqLjsdJYmJiXfcuJXWQmbHdSVI5WzfekagOs8ZZBArAJcySes8paVBEQeMIqvF6fvHF9b33193Ct0u2hCvfv2R3zGakJedSJhIBqIBDJiKidW5MvWCFVHdRZZBk1imEbIn5bKpEjpwoMuW0hBvCDG6ZAR8pzKlfq6ojyvwsTzPjiO1ZwDrYH6QSbXOWQvmpxnEjcSW8Ugl0VOKdkjJbWnl0mhJlUT9LFVoPTKvYWmGECoViuh7ddsac0ph849cMF+BbpktHKuzIc2KS5SzzoE9fv3nxjzcf/NH9T//w0eqyY2YYalq+yETM5PItCMcxSFIiIxMWzr/FMXPYZZOb8nNlhZAJLEzcqXONTMLe66IFiPsGrvOxS683mX1BooqzQB6gAQDQg2LCqAj5qgCDWIQHDC/Dq69uLx+tfe/YuUz6MyuAFqWQBGK5WmZxhfgYtlGWpkx4oypoUUklGUgkCmWwKNhItzk5ASSQbMGqmRgxMzlW0c67/RhUl2ayCn/g2wa8yMHTUNMCXKXcahLUEQG3uF5MxJIYzoJhyTfBYKHywAQmO8DyCvCBg5luRkdM6HCTOFAKAc3SBqGGRuEgqW24b5yShjklMV1JRcZZk5APwBS/+DfPRPD5P3t0crlAkRK5yKzOcee5oWbZuU3IRD/P0zEpLswyj4BaVM0MKQ+jRh1fjOH5MM8hzto3dNk1II0iSUmiCtB6ahplZufgSX3DDackACCAy4or+PJEp5lUSEkcQQnzNr369e3lO0tJ69V53/Se2Wi9mjhb9YOigBSfPmi8BhMKqQEl+6+BgFrqxlVuz86YEyxSEgZpDq/lQwRykCmsXHczJRUll8ET7tM/vOt8dmmGYVuZ0mxwbDSPCaZ9FjmgsvksPBjlIuaqGpgQymTvGDBkzsNMICaGXSpfjkyCIDJxji04MJeZtXBNuJ/kx9P0/mlzO2lMOkUZJ0miMcl+TPtB51lSwnYvQ0CKBEjHOszp7J3V6d0Fu0yADXUlyMlIn52c3Dtb7HbD8zCe3O+ahcvPw8Xe8w1TGaistYCJM4gTEyBDvP6nm6tf33QiH102P7jff36/fXzq762bdesIEpKKqgDLnr1DFA0hKakneMoSAQB0Hc5WtB81JgXgCHNEFExz2u/GOEu78N3CsedD8nxgjRZODiyXTNKkkmcaOJQKEJnGa3SlhBrj6FRIfUnC6otKxQApyfpmuJimK8bqcknMRJQk+ZLwEYpZV9fMomnFNwtt2YOzmJpFMSqBvsQ4i3CmJCnnCoV9EDnjswHhbz2QFgsrRIfpWwnwAdkZegr8z5gvPuoDeyL+y19tXt1ImJUdYlDHWDQAUVLSpPtZIzQEqFL4erj6evv4+xekZDoHqSqcg3Ng5nXvztedHxgk4DJ9VTcpj6lQU/JLVkoFE0Bgz49Omj941H3v/uKs88waom6GtJnSb976L96OT67TJPCsMeowCTu6c0rTjDnpHDREmmbdjhqTZuIUIkZAAQHma7nC2C+23dI3vTu777zPWCVGQGzclJCF++rzRjuMuFg4YYXkgcjR1LKELPwzQ6SOvqm7pm5YJCyxD8wU4tyNwflTFeWsvIN8jlklQTFQyjZtbxtb08rrj+yAsnpZ1FHNZUsUyCt5RMavknMbx4Ixt/x8WetDzUkzkWNk6YTK9ag4HfR39tPHmPzKa9v+8FF6fju/vAnbKCx0suJFS+T4epfGUbynNoEhY6QQtHP09sltmKRpHQgue4ZKItrM6W0Kp0sCMRFZ6arqyaYhVMkmpz50VMuy7J8bvrjT/fSzk99/sHh8ZyGgzXaekjAHgZ6t3Hrvu0Z5jFEoJIkJmgTKcxKJRCDPOgIR2AV0DCI0hLHgnAJhkptX+6bn8weL9WXv/LF0kBWwXDMAMauArOJMOcZakSzLspCc0GjKzyEGaUauVU0vgBRmnSm3mFUSQ6R42UaxmUXmIEFo4UkAszMwLDNFrb4W5y2wWG0MornwkWvhheOUT307dc2WljkZGf7VeraZNhiVw5U/GUeD1so6SmTO5/WCx7u9RKEeqnCely1frNyywTTLsmVySOzmkPaTgjQIRUUQdQQXddpOkhJRW7mBKknCPIt0xbK8MjOzwbmWIAIu2RcpFMwoWg2Z+yo3C3103v5ut/zgrOs7vx0CCJ7gHYGQRJOqakpJxyCq1DQgkIimSERwjBhBhL4gUxAkgIAEBICAMOD2VTy7LzGoJqE6FwQVydMlKBKfsawc4Ezoz8oFA4LC3Y5+WgHo0AxhMyQEFiggB41ExSxDmWlseGLGnOYpLNCSY+LESkQ4YBKOUsQyv0UzLsbBwNH0gw5smfLVYWFRCzyhWGMFwxJlDjhX6V3GPwUBLNX46vHZs1Yqp3Ni79n5Vd+0TE9fbWOQeU6Lhk4X1HuKc0yQccZ2xJx0SlCgyWTeu2xATIcrxChhTDFgTmmK4jx7T8TGNzkzLy7MNRNIRzDGxkwEJiYi1rbxPzpzd3qOUTbbeT+nxhETzbNsR7mdZYqSkqhimksJWzBHWvR0snaS4B01DswIAlFEIAFyzIkA7OFa1y1cfpDKkLkoR8zm51xGL7MSJTZqg5IDcImppfhbJilfrNbratMKMRPX1ovMJYjZs1+4dcvnDvvthFx+J+VydT0mWgXYDrzSWJr93URhtrNn9lJpOopqgZLElhhrdDETS6lF9gO0oehqB6gDleohAGbDSt5MXz6dvtzQpM45/vRe/68/v/z995YPT5vOcUo0BCQVSWBWZjjm3tO6pcaTqu7eTuPtbF6a2z8EMaQwpJDiFCSquJbZcc0ts7FXH2OnLpsaM+eOlpwEEBHzEvIwaEOUFAnUNuyZdkPYzTEkzFF3M0Ii77hraZ4xzRoExIhJrzcpBE1JVZCEIhCRkaAIxABnbBNsXgzDNkoqDIpLkkauZsqVp7BZjMm79a1v5wq5HEBspyIufy36glrWR8QMYnYgZpcHgYnROm3aVeuH7RyTZLT0sDLlsZuYqVVRuXAt4FAUFy5FlwKBJWMt0EsmUUs1nmMhvcTWbFxU+ZnRQaq4CiqF6kJNCKThet4M4bLnzSgqc+fp4zuNhjaqvrqdnt2m20lJ9awFL/l6kEnQOKhgjjoJ5FWYrme6L0oSiVQ0Jk2DUKNjJ9c0xhM9dU3ryeU+BhFmmBrOYE+AK8KBFg2uDAnoQuQkSEy6m+Ni0UjQlNIYhaFnPT1K7vWWX9+qQhxDBMxgViJsdxgn9flWBTO0AWKxLUeAIpW5SoKb5/P2apyH0C8cey7yf6aKJAqU3guDBylzqZbWZbzJDA01PYBSEUWL9mspCBNJFW7z3CRyTAqOpElBDd+eLJftYtpu45x84wHyFWeqIRCpgjkrx2SoabGayKlWWekQVVH7K1AdqtTZqRxVdDErRBd7KuBVI2PRDI+z4FKTNbvU86VLSW9m0rfjrpWzRbv2etrSNKcAjiKPFvzD++0wa+v5L369+9sXyUUoI0ieK5V9oH3MuZIqnGDdkL63HPrwZrGTBvfd0vfOEZKK5rYMppAgDHZ5aqoGUPM3ALRQ/d5mkn341XV8upmbdm6Z760oChKRdzjr3GeXfju1P9+Pw0SARCGZwYCKNg69xxQsUEZAAQdiqGeEhBYQGF1DVIkpBVG2JqpcUssNO3VOtfq1vVMUDRUc5s2AIJcQFASVnOOoleQlzwAzVKBkSardnqOGEIndmseOXdP3NM4h+uhCSL4g1/8HxvI7asWUEh8tk6x0KpuaFTMNq4qpHRoiKnDnvhNTzZWVtWhkxcAKBbCEm+tbxQyJcnJ057L/b3948eo6eErekUpsGPdX7rO7TXwdHj7ofvrOwkM+e7i+vpnf7uZ/eJW6BtzQHJQYmjSFhCRZm3MMMLh3tCJhHXxwLXuLGtQQU2PtH+okqFhEOsgDOT/PfIbeG+fzl/u/+vX2y6vxcuE/ue9iSN+8To500ZB36Fs66907p+7JDW/2CQTPcI6gWLV61tLdBRzxk036pw0S4DKOA5IAoGWIYlIooCO213O7apqmcGcFcjlFCNVmYMlmFWjrrOR6aOmkQxUMclVDS0Na1i7ybaiZh0kMqqoi7J0SWkfNgrSjkcMJd0KyH4Z5El+ml2s1swZLIq1JfK4TlH5bi+XljrNx1kJTDSJZVTaHsTpcqS/ZnBQXQilsaIWFmsEepRpZeT5F+tMU73U0N3PTNUrYD1FEwPrZ/e7+eX/R8zSmL1/Mn97TN9vwchcdwTG6Fn2HfQB3tDhpiEiUYN1IOcsHkEvRpkQJZ2YNZhJYZl9ETotPlYzmO3Tb+JtXw7/95dU8xn/5yenLN0OI0nha981q6Z1qw7Ib4QinnT9bp2mCd4hJJMB7Wnq9WPq1p8slqcYvbgFACgop4ASeLTlQ0nkfTY84GI/ps7VJ+0CEJb/JpBBriq7yqWYly9SkwgGoCJ6HxjQosUI4B1shiArUW1sOETGE1LcsKpI0xOipRMqaJ5YfamNPuffIeoeO6+NHiFWtrf53NRLUimmJs0Sq1rp9eOXuEoNOJTVlp1iyKkqbCf5FiJ+FaTuMH99fT8wv3g4p6WaMwu7irFkldiKa6EfvnVwP8p+eDb94EVuPGIFZG0c+6skd160a6wi103KemJRb662XOPeTZo9nNeGyajmUG5cLLchqGv1yG85ejUvH4yw/+83244enH95t766ae6d+3flhCm9vQxIJSYHkgb2QqMQRSwdO2jm+XPmFp1OhHz/Up9u0OxoqBRKQiszhPOb9PO5CZWbFHkgyoBkTMQ5tjEQPv2SaZH+Swp+4wFs+kkrcFcvO5NCloiBVyVKijUIJ1pQ1k5wHlKQLRFm2K/WnQt/zbRuMHRpdizJTBrminBYlPxvKt+yJjn6W0Kt23UN+ICWHOA68VkZcAd/fDC9vxte34Z7oLDxMYTvGIcr5SdM1boqy3cf3z5pfv5l/cx1+8WIAg4EITBOSqACnj9Zd34BURVFkp1KBhkhGZ0WWfKwDyuzeMmoyipwrA7lbJQu340n3wZ3F/3qn+4cnm65zv/3+6vGdbrVwc5BhFEkyhTTMMieIIgnFmFLA0uGko1WD0wUvGzpbNNt9fP+ie+d0/+QWO4HPYQ7wQAAcwAQShAlQ1aRoyGJa4TxCKEpqtiHU8GitDRmbj4qjXLI7NTxEPpeqKQSMHEG1KFJaqvQEUi7d47lSTznNpKzTVhtSzSkvCrOlA2iZ7F0XiaBirpUzqw0pkQNs0KkoZIdUwqhbUVKItFovHUk6dMDWQ+WJaTHLPz7f/V//8flvv3sysMYoRIiKpA6C3RBebWLYx2dvhr/6avvNddjNumwxJ4wRY44aDvc+OXedecah0pHDSW5yKGmKjQCTkWsqxKDSU/M7BVkw/fi0+Wcfri6neGdJZ0u+s+7v319D9dnr3TCnm1263sf9nIY57WcJEUxoHS5WOOvhCZ54CHr3BK1H3/nOWWGkMG5Q8WUohDDchldf3S5O+7P7nXNOgSo8lQKmpZPZELKKn6uGesjutTAkILMTeypYQze0iLIlejJBspwjgGQwt9y21MvzbTKRN+Aqy0ryNbg4K0pTY3GKIwBD+VGie7bow9ofEzfAgCCfw2r0yJynUpxqZEdEAuVAKvGCmAB94+l///AeXZwtXt1cj0FS6huIuCCym9IcMIzh5W341fPxydvZN7wgGjV1ETpm40d71919/4TI8nW12MgZ2om1PEc2cOV8aO5MoIP2VKN6rQOQ0jtz/IPX2+Vu3goenDXvXfb+ZIllG6/2m2242YXX2/B2l7YzxqRRkCQ50EmPiwWdL3g7JlUBURIS0DbofsykyWQFByiQe4ciQCNoE8chjrdzv3bLU1fKQmU6iFTAhERW6yleleNMCZ0ENvSh3LBfjAx5Vc1BJjErUBFmUjkuGhJUErGzZXgFPtUEv4pLJcAfDWVphEVW/EocpJogFABSi941Rah5qYIYCi5xlahaWDWtsu4oo4LZXn1SA5W8sId5Om313fXbvnfUeNdGwTCl3ZSu93EzxP2MIWqCto1vvfVO5SQlB8n7n5+d3FsCYFIq7Yl5LVmOFTj0+dszZNEyi0hFjzXunz0nFxceivx31+ODN8OL1/Mvn27nkLxnNBxeb588394OYTfG2yFtRtnOMswaAxxT63Tdassaku4mZY+YZD/FMaRv3o4v99jJQTNTWIdi7h4jIEetMIUsMlpWbj8L5c0YDVgh4EgvsOG3OUPJvAxBuHTRFO2zYJ4egXqRTfOF1JC36gNEBF+CXXHmqloZokjNc21BApXc1tC5JM41JTwqtB2xsNzZYX1KpuxQlXcL1FbCyblsUKI4HZkhFIRAxN+/ePhqs3l6+/pWb0cZk4aIKUgUiqKjUN+oc6wkrecoyTOcor2gz//5437pMMaSIgqE4I265ksycn6tzNa+RLaKyGpLZbjqHCiD3p/TO5PERdu68PpqenjR3Gyn29f7613cjmk7ye2Y5iRKKiodYd0iRRCo80qsKenFCZ8vOQTZjKlr9KurMJQhT4WfKdAXF1RGf+F21+M0LH2bSTFzFrz40LqPusRbc00yN2jQcTG6/AsUCDFGav25Wk1TS1unFh6th+oRqSizZXkMSiCi5NVgo1708KMmfhZRmAG1CsgR3zc3y5DGWixLi3UVpnfocSvifrY4LoTPKEFlpPm0Vn0viJ3RFAr6W8d3k3voeEzYJwF4Fh2CNo68p9bTR/eWz2/mtMGipcslJdGQ8P3//r3Hn1+kkEooViVKKi77dJ4eAARnuADnmEu2XVITrZ6a7zHX5Z4r/Ycn2+3L7TzEBHeybDdDfHkz3w4SFPs5TlFEFWAHPulEgZPWTZMsPbUeLVNQIqZl7x302U18sUFXC+fF9z3yvWFSOA+ZxTeu6Zzz7sAaS4tviUYZADnHRCkVHMsIzGvyPCS1KULu+8gmZcvFLMXOkdW6L8xEFY6gRGId4TbTOQr5UlAqeQNKnLQ0U2tiYhV8O4VUmzmYaDk7gNIJDirNGKVGh6OjDMQKAannUPMlqmZa4jlVXAUpTofADn3rFC6IjGPKqyZWLX9yv/v43uLZdQDIM05753qc3l99+nsPfMcSUqahxgcSIKSsnBtAyz0SKxMT57oKBEdurYCtqqeS4uPpyr/96PThNv72O92dE//+3e6bF9djSPsgAg5JFfBEUGVSx7xsnUNqiRpQ6+ikY2LqPDvC06vpi5dpjCaVOQBqBSgF5izje7g1JFDT82LdeG8sUvIEKAkpuYxq9alQ6gWAEYFMHcpah1RqATYbTLVXt9TQLY4VSReVqALMiNFagQ+dzwRPoJrYG5UvAdpQji07OLIKVT7ibQbKB2ClAr5U4L3yvkN6YYuiYBlANW5UKnAANT1syVC5oI6MZyftD8KYi777Ib7dRYBWnbvsedn7puEpSrdwq/XypG8XU3qym5/83dX6clHuSYmYhYRS0XO0UpPaYMxsFFdFRTUvTMv+bl2gsDsXJj7vP324fHDSrnu3i0jsvHONV1GERA3TxMqUGnaOEyI5YmbxRATZjbpqeJz1aohfX6Vhhs+BRxGBhiwJSGrRkxXjFmeP/cWDk4sHK9eY95qMz2CxboXC6AGj5hnxCjgrVQ2DDnFTDgZlE5Q7JoseqiWrJZIyjSBmTpauQizhBPxRGgzQYZKRn8pMhgr7O/wKa7zNT1QooREcKbG+QNSRGlJMOgO14VX9i7XslvJIyVmtJpoXP2jurFPctP5qN98OaTulZ5s5RJx0tPB6unCnS7+POL1zsnJ9ZB3mhCA6pGd/8+rD373fdJxP7kDKYMlKWll7C6rZJ5VGdVGLCITDcFT3zseoUkPqk7x5s3+mIE8dU+Od5wTmpBhjAENEgoiosgqV9B5E0yw3e9nPOkUNir4DCwQYJ8xAo3CF/je5TShBBes73cNPTldnHRFbK1ghtIWQKISKjoqiBBbQspkk1AXCZll5b5uiPkO0wgosc0+mWeUiTy4JgNmlJGWVrZ3al+HMY2e3QTUqVBMgskoMjth6ju6HpQqoxD2fU+oKY/tQsSfKaFFM1jDEahum7Bw5V5GkM3zYHg9EfJP0758NV9s5Jn2+SeuOzvum9dS3HNh9E/36wm/HOM0pJXhHq67Z34ZhM/s7PRUi6RhKiCgrYwAqErX11HDtQ7HpqftB1I09atMOOyeim6v9Pok2rnzPVIoAACAASURBVGndigGQ5LVIxEHSrBSixiiq5Agpg7sKAexwtuYk2k4Yk7iI2xktgxRSOybK5TLRi0EhiWz5VpXNSTLCaoG0g0nlBd55sIuIkdfdmkJDNecjghSkK7q7mt+JCaL5MBVLD5kpxQqPmZyr12oBVnGk8qstn1cS05ZMSCvjfdiwR4puX02KtNRtFbZyuHxQC6OG3aSpKmZwJYupCwuKOVDpC5WSUYCenPfx/Tv6cuyevY1RA0vrmqZpr7B4sXPXEwRCDBENSVKihxf9hXQ3T3bryy47IROLgh1zyqJHdhu4jKm5tYzBhFhynaJkkBVHDokclLFp+R96f38rjeckMsdErc5R2BGBEniMaZgxJk0CrfvtIJGokHoiNlORKBDFeUsnLULS2xm3M5SQcj7l0Hos7rqHH552qy6Li/Y/rQNKNduB1ZZJy7J0sScoqGPWlR8TILUFoShhmOy4kmOUdDTzu1LJAjFRKmzeyJOvC0EqJsFitrXi1OJkjXrZdfPnzf2LmnJU/Du6EypWUlUaK8tLDahWq7ACTj6EC/c5GPeBGxAADb2j33mIqNPb++024OWuuZmu2lWkZp+CkqYkb7dzCGCiTx6tThb+Zh+efb3f3e3WF5210xLI5ZYcwN5hEBwzOzjHjolye7NCOQs0XES+Q/6Sd6dJns8eLn8yBagOSV7twzDPQ0yN8qy8mWQ3xTHEMYgmqXwj651QRywiMif0DT++t1CRcRRl3g7z7SjPr+VNwNBhed81i4aZH3x0+snvPji56M1KCkwVNcLGtpBoQzQcKjMHbCiIZ7mfysH/1aoHWpZ8EuFAvrLRSe4fAoiEmCQJgbPNE8hrlTAKJ7RolR9fS9LLXDrjtPD18rsxFetByYaY76YWr1Q176tjmKTV2Lh2AIDzfR1S80OwKms7jcCVRDZHLO4Zj1btLOfww7gLiXoHx3xzM/7iyc26d7/90WXKuzOoNp6a6/jV//H80R/cPfn4PPMQyzhEchbE9gPesfOOi+YJApt8RgVlqxJCZcUabRztHC4chyk1De+jm1IE0xR1CrKbZTumKaQut30bFrrcSslEned3z/su6vKkTQ5vbqJ49dHdO+3WXehv41PC2f3VxeOTBx+erM67hx+ufZtXC2e7sGUx1ZKojlumtjZdJiRYQBMpgQZHcbIm/IWq5MG3jQ6KieVehCTZFOQQOpWLAfqsf5uekXmClp0sWKvB1by4zn5ex6wHtlkTQQaOUpGD5db8s2St+bZrJqkoun0VCqimOmW0VKVkHAXLoQSR3T/epL+/aU76xFBNL6/3f/nzV+er7ve/d8c7N85JgYbJMbee/evxn/78+aLzD98/BVHuO7IdptR0PmZico5BXMplZb4y7bD54rxcX1F4zW3jr4JSjG93cRPkapfmiERyO+J2TPtJppA0IXk4sDM5S8HoHF8u208fnV2cNl98uZ1Ep1nOVw1Eu5V06+604c65z9bu5GKxf7w6+fiU2fnW1/vTTMdYIVZdpPwui63rxYHzF0OzzhpLDoyasFlZQaRMM1QM2ck0d81nodJFlKEy91xqLpOByPo1Dh0TOZzlPSgzZpYoqIfYWjT8AmW2R8HBfYogUkFZv+0pXJBPCzLX3M2O/pbORjV1ta0hrHZXMguKafPzty/+8tnm6fD43vKTR6fDHH/2j2/Olv5f/uTBnZNuDJJEpiDsqPHcMr1z3uFm+vLPn7p/QffeXyszc+G7Wuu4ZEuTC1ppzQPMxIs7k+KoYdMR5piejmEzpJsxXm1j55HUbccwTCHOgSHs0DauZVIRZiXS83X3/sWSI26u9mPouKO18/daSmP6+N1TmdKUlDylMfnOvbyZvni+H95f9+8uiJVENfuDqBJykmgqRols5vdQwLZtLGHHzOPA0r/1EdT4Wg4isGYlw8IAlWSbUHb3I3KkKYnmVnOUvu1ySZv9mj7hIPofCRCFJhUZwMhgXl9cT6XWOHswzkqZ6eiwgyFW2zogNyqQlMcuigzXM82vpq//7OuwnUXoy+e7l1d7qK5W/X/z2w8f3llIUiZlImYl8KLhu2ed25IjerWd3/zVC45y+dEpOdT20XzpDHBEhlWl6w/FjQplPdqbNj/dzvOvdqLX47LhzZRuhrDuOUTZTzGGJKIMYofek6N8S/TwdPn+5fJ84aeov3pyu2j4tHPr3l2sOh3jeuncysuUTpbtnOTNbdgCD7fh6m+vRlF9fEItUakBQUyiV1iBqIxbTjZLnQhFYrf71tJgUTR8quUl0BGakUVQpApiuYOdpPafqYAdYiRW6wv1lgwe4lsROErIKzkmldwChQsCVnKhonNZmbkGPimgCmhRoKnAgbE+Ou4gULKtKg4mV8g2yjLQ3JturqYKGt7s4zZKAjEa1da53/38/gcP1xfrhgkp96V4SuK2Y5iCpiQv3w4AlkzjTfj1XzwLwMNPTg/KYL7Lsq0DFXvPWiVZ0NTaZFD3sVACEc1L//ruAk9vdg5X23mMuhS+mef9EGNQEQDUt9x59kx3z/ofXi4frLtXm3keU9/RwvM0CxpcvQ3sCVG/+c329LL/4KKbZ4GjjrFmHj3Jq+H2L6bheyM+v8BZZ5uClckp4QbfWgJwxINYobahGFWltsCNFkPDkcrBx0lDoUlVCspBIBMb5XJUtgcP4mo9FiBsDC0Gmi3ZfRu1QilElKy2JAulslBuhbNTERWYAI72oiz/ZQmpHW4gzAVUFeDav05lyov6Jjq8nvJ2naJ6sW7+6EeP3r+37Dpv+9BpXi6tL2+Gq5s5iNzuwsvrAdCTVb9o3VdfbW4kdesP7z5aFzVI8zIx50qlHCXnt5BOxxPJNfHJs9Xy8MnZ7lfX9HQzzOls4caQNvu0n6JGCknJYdG6pW8+urP8yQenj5btcDtv5/iLr292c3p9M72+jdzQHBXC79zv//AH935wZ8FB/dr5xm0288A6RQ0hxSHGv34xPh/4p3fad9fccw2OxWiOb+0Q+lD+Kw+2QtikWCqLxpWIRKWmeuWZc28LU94VGRbwBKVmZBbBxFAxSct9/4/vcWMWVq/KZT9sA5pjBpzvv2zmZKyd7HeyyjSKflGhkFAz7rw9H2leoFOqOwVM2XDjoBvk9ywJLAyACqBHuf7Z6/lqapw7P2l+//N7791btZ1zRAINUaNoCHJ1O0HpbN2ertq+c0x0s5vHOTTOTTFtX+5noocfnDa9axx7T13rut5554jhmEA0hzSGxMSU91plwJZLHiq5dcS497Js4qtpLdI42g5xO6QxaIgaQavO3z1pHy/bH95fNOB/fL77u29u//PXNz//ZvvLl/PXN3I7Y5zUCT180P3Jj+791vsnd856iO728eXV+OXz/SalIdFuilF1mtL+1f76yXYias861+YuTT2CrhqjUEplhauVLKtKC5Klm6qRVUw5xDSrjpek33Jbido5Rznx1cJ1k4IoJfXZwHK3CErdouhYckSPcBA7Sh/vgVBB6woTrYSyUr26foXMLTLWfet1SAu4nINKllD00KLGkdouXArFJGdBP/vszrJv1gt3uux8Qw6cVOagYY5BdZwSMy87iGhULDp3/2KhpJtdmEJaNLwnevmfXzz7/OKzH99lT85x2zrvHVyWPYpeiQN41wQ4tzEXr7MMnRz6D09Xm9n/388218N2CPMsSVQEXcePzroPl63s0t/8l6s3+7ANcR9Elvwq4PoGXYuzFe4s+PPz1QePT9456WQfr0cZkt6M6Xo3c8Pr1vkgpLwNSqLOI15N+//zm+n1cPf3Hyzu9qDSnJWDWS7llKpykdlsOytU0nsgy/VpbOlUaVi0aoydrmRFuRlBVaAeNckgBTNECeo+/5P7rjmgVl4AeuDteSRLgCwLMAHba632zRaKby9zbs1aOhkC5SuYZlLSBKqtw/nqZcvImukRad6LsA5EgTmQUreLn+zk8eVy2XnveLnw3pEqxSTDmELSKKqqjtmxLasBKImqyM0+jnMShULDJAF4/Pll1zvvyTWOmWydORERQtQpJGXyjvOGVlQ0jiNeW5VtYmZZt/tRbl8O03YSUVHpmuaj88UHq4624XY7v90Hv+Czy+bNNrzdyX6HFnhwB+/fW/70o4s/+cHF+yfdhXPqOZLOoo0jjUIAe4pB5yhzFALIIaXkicbn+9vr2Z213bqjQ4QvmKbVSXBQ74+gpFhdSXYygh3SQ/N8PWQPB+YqSRpi58mErRKiAZIk7vM/uZ8F74IaAI62L6cSFkuQzJSRkLcLNeuxlJMc57/aZk+VepZKMQDmUjM4fBKcq9kFFtgMGGU2c8bnSkJRSmyqRHduwqORVfV2jCfLtmsdhER1ipKSRpUcp70zyTBvKp1EiCkmmaLshzlGDSLTNj78/uX5nZbYOVd6GylXDBCjTCEqgX1eLJAHUesq0+IV1oymBG4dP1zh3ioJyc1ISu+etd876W+uphdXQ7N0IO083wzxmzcpzbh74j561H14f/XjD89/+Hj9zp3F0nOz9lOyr4noRNOURsHEHINE1SSqzFF0P0claML4atxdTXzqu7OWDxvYFvYEVDWhSDV0pICUHqC6/rlSOC0yB0rSX8SCbFgStWF2jgskkuZjVFOCtyKFLVSw0F2+UwaVyLN9PIduZOKYd5Ovu/yYEaAkIyWNqCwaRfyngwPl7kk6nJ1wWGOUJb1sn8CDftl7/2y33aVoZxY0QxymuJvCetl2DZNCQDElibYiLnNWBojJi4sxgtUxMdHpsh2DjHMc5kkVcYhXL3bvfXJWNUtVMJtjWlmg6OCFw+Qsu3JXG4Gc1BDBL/3684s7F+2a8c1X1yetSyIyh5O1Xywb5/HmaqZl8/Ejeufy5LfeO+k8pqDvvn8qIb2d4sWy8Ql6E7ihftnEJIjwjpcE8TTBYUpgJJAopYAUE2aZv3j7bAjpXz2+/OzMte7AaKVsXkYlMTVrIpAUsYzUvvblqIZlgbYyGVJKRRVQrYS6TK6aB5a4BHhkTaVQPKn4b9cpWWumRkxke7JZS8URRQOOP20fqq5RIn8pPh3bJg4JLerfjsQzVaBl/85qvW66bQjDPmYphFXbnWyHue/bVd9AdZYkEUk1aRJVVURRAH0DJmZKYJJoO7ssOrfu/Rza3ZSmKCno5mpUEcBnLpufIMOrY3LEQfJ30WTVpogwBgh5mwD7wqQivFDD8keM3/r44lfr9pdX42KMI1N30s4i4yhn5/1i2axn/PGnl4/fW339zXby+urN8PTF8P69/mHb0D6enjWzIkgKUdDTqvXzGK936TamJEoe45yGEIRciLahS/x68/zfpDQ/vvuDS9e5ir1mNIYBVae1cWaiJCXfL9FWcwtoWahXjMm0eYsseYMrw3X7BiLKe4sSnGNf4pnNd0HIgq0lnSAqW/4VfDX+Bc0bGNjSTzpcrAh/oINdWaLDekCs2jFwZK/2NIfqHBAlXU9TVBlisGoFox8jrkO/6M6WnhXMROJGDXPUECUm9Y5jEhGIUt/AMXlG0IytJKreYdm5ruEpyBx093ZICQ1p6Smssow6ZudAgqTqCkHJ5lhqNGS7WNeqG6BEl0H+qzfTyZ3F5cK5KL98s3cLHxyGQVaO14nORvz0vbP373TXN9N64W/2889/tfnRp2cfPVhyQnPS+yT719NIuk+yvw6R5jlJ7/R2Tnlt23aOATxPURRJsr1ofHL77M9+o4J7P77DDZfNf8WyR1XoEWSI9ZgRWf9tiZIWmsqclOkhWOaPQsthrN1iATFYTOcm8XU2DxXJg7RcqryGVbBIiEzjlW0ZrdVji42Z7Mo1vNRIb1ptIV5atpJG0WrLUcYRUCVnitAvb2+YaNa8w6VC6Z2tXK58VHKgJLY1ExGJpJh0juoYIUlWwcY5do33zjFrirbaofEuprlveAsF6XAbJQmoIUDJad6OX2z7LgeGxtoPY6OWeQUZISG1TUSycEcqnvikb3A1/erJ5pf/8PoGiB3HSe+t+x99ePEu0A1p9fGpeuB61pa+eLq/d97cXzZXL4abm/nxh6dyG1+/3O86px27lZ9fjc3ad0u/bnjchd/swtVmBDE1hAgiFZUU1ZGml/tv/uxrJbr3wwtuG6JS9xQocvmIKp7RMQcrJXZQ3ii5pA55YpC/PgWl/VFLBQdVNzn03avlvtn+5GCqZqaK/NUyuRO8lPUKDTHedZyHFGs/8BbKz4SaRBgWH6pHRx6SvQcqtfEgd2bZYYokMkvKY0QKJ3q2T75xDVHjqfGsipREFN6RCGISVcxRFMqEEHU/JYV6R0mwn2ISaRw33vWNWy9aat1+O8eohcKogkVURGNSiBBlkz0WD436aH0WKo2rhhl0McxYujdv9//p/3l9rRqWNER8dLb8H398/yc/vXv5znr14Skc0W1aLtzXb0dW/eC8v1w3bUPPX2xfbcYZuoc+e7nf7sLyrG0u2y3rk82sQfsx7m+nvvXOwefMS1STiqgKnIq82j/9s9+8/eW1xASTUY/u/VB/Oki5OABNmdtMYMr8W/ShWiC0UoJJCUVAyNQmCxNs8P+tQG2Llgz/Dn/TQ8NSZX2GomqdsLDkpQhotkQ+Q5YhYZY1KpO2v9TqBlXkq/Zer230AqpAF2T/NuxGiUlu9yElyRpOiDLMOsc0B4kiIkgJw5wAEGOcoiNqPDEzQElk1TVEWC983/C0nec5qZKq5n0WM2ipNROz83COHFPO0Y3+WtpcNEFC9cSVyMdPduPT7b//5dVTlduWX15N758t/tXDk7OzHjOwcGgdJg37cBPTXvHJ3f60ZU/YR/iVT3O6mkLofb92EtIuyrPd/MXT3c3b4c66ocZvYnINd6ROwS6naCBBEKEAUpmf3179u29uv9ykmNfm1alDFfktdlUIys6dkxyDqZxXFg50qC4U9T6rPSbXo2w5aAmgP8RbK2llS6Gc8xFX8zNKZRXwmqscguPBQYpsbFct7Ks8IQPQE4FA9mzRvPpPjpV2F+ULaLWIjlIYhgCLfURUx8hfKrcbU5JkbS3Gy/F2G2JKUHiHrvXLzs1Mw5S8477lcUIS7Ts3zjLNsRGag077aCKRMoqunTVJhcIxuxxy8h0SIPmosuI4xxLHlKD0/SHd28x/9Zubv35+ywsO1+mj+2f/0+88WJx1WDZwhKuERvQmvLmaXnf86LwNb6br27AL2+60+/ST8+0Yv3lye/fh2nEblZ682r8c5v68cfvULf0zTdf7uOi0CSoIKVczRdiRgBOhcRQmnb+6vfq3v8F//d7JhyfEXDJi6AG5UUIKiqILKY5TD87fqyEoDRU5cc0fcbBvH8tU7QgKiTSvmqrRSXFgsiYqoJiIaSallG3RrwiyWszsSHQlhW2bVeUNT0KKRrFWXYbUJtj6hiqLlQotCKplLSXqjNuFSbHcJFYwI++tv+zcsvOq8up6/urV7dvtPIU4zmE3pt0UsnI7Tskx9S0Tofdu1fskSEmXvQ9JVaMXHXazZLlK8zeZqtqCOhS/KrBFqCsJSsjM3mwcd53k8p9u/vpnz/+3v3m+CaFj/3uf3vtffu/B4t4CQ8BmwpsRHUPx9OV+9FhetCum5UW3vuiuXo2YpGe3aDyCTNfTgkCsT67GzXaOQ3x02b/eTT//ZjNNCk1IkpJywwpRUSZhh1E0Bu09NdD49e3rP39y82SbW4dQX9WWUHhAMTqGHnKA/J08h3o3Vxm2MHBN+dtS8vqSytYBVfWVShwq4vZ/ZGtYrKUik5yyE3gNxDVRKIhmOQHbtgyligtRbYHziD2LZ+YEL9pHSXCR7JvJjAGUb4SmWsHQvNuFlACFJkm/iUyAQFTGKQ2jOEbXurtnbRS52sxvNhOTrpYtgWMn+51gCXaAkmOCx7JzIbXXu4ltF1aiSd6+GD74HM4ZdNc2s1JZPfLuEh1LyLc5yCjulN67Gp7/7au/+Pkbv3I/OFv9zid3v/d4fbZy48v99dv55KwddvHu984RiC66BrpY8LPnw6OH69Wi0VE6wN3Op6fte++eedJXr4evhrgfZi/04KR796L/91/fzpC2g2+cc4hJxZETEs9Z1wlR2GPR+N4jJhm+ePv8vF1cdM26s00k6n1r1iwKlNmyy1yf0SqIFlODLRPNXqVG3FTFACOHJsk2xqJwn/3xPefLmm+r8WhWOLhYIJW8tezCgspJ6t7MlDcByF84yEehrqAZAUvlUxEWLBPyQrbc/pmIQLaTA0rlqlXcEUy5aY9L2LXUVO+Nunw2OSgRplmmICHKzRA3u3CzD3NIXcOLzgeReZa+c0wYJ708bZnoehtCTKLqHREhJg1Ro+ocRBL2Sd793sVi1SBvccBW5BShOaYox3J6fi6TNFDaH7Kzf7wLp//x5c/+6slM9EcfXPzpp3d++JO7XZI5pGnW1Xkbgmy24zBJJFIHRN1sZga/e9p5x773zZzcPq3vLcKcnr8evni65VXTd80795aPm+b6ZvoPv357vUtQtB2PIW4HjQkuCjELQYPOCX3nFo4a5wQYJx1upuWj0+5OX2jzIWupq+dyIxHZX3GcHB58Tmp4pRJgiBQNZ+Jb0ZFVJMXkSzCoaziLopW/pkwPCS9yoYdMj8wrvAp/yTSs6K1aahqgmik7xbkkStoBC0mzcmIholWEgkY28OOSjb6XqJvjq4U/5n0W+IHzTdSUlImVFr1vE89e+zZGwTDGmyRX23kOkhJCklfX48PLRRDJ8hKAlDQk9Y5a75adv/Wp9bzonXO6+83u1Tebs3s9A9Dc1pInRVShIhAHRv3q0eO7sz4CwuNZf/D15u/+y4sA/OnvPf7n76xPzzrkThWlFNPitBWZpqhvnm8Xy/b8zK+XDQGnvUdQuNQOKe4jLfx2O3/95PbXr4eW+WLZsqczQXwz/cOrzevNrIr1iU9RhwFgpFlEQG2KDPLweY9h0hhFAWqxv5pe//3r1furZt2iMN38FMVeTIMuCVBG7VLqyKaRHz1/4XWNhFI7RCxdJLMcVavYFwpW0xCjYlLTEqokTjPemkUaX6GSUeal7jgIzcXyFb3iJKqL6kU4iJtjE4WjLEW6mBANhfOFOsXHcxzGWG+ojIYC1AaVV5PmPfeTDlMcppgkJQETnKNl5++edvfPFsue5yi7Ke3GtB3ibogxaet5ufBd40RURBadW/Wub9gxMSuF+PbloFFUkTPOWs5TNQKhkn/YtipakoScPa+i/uDLm2f/7psXL7fff+/yf/jexelFj84jKRZNd3cZgrz8zXZ7M68u+5N1e3sz0Cynqg/vL5e9hwgUPfPywXLXuy+e71+EdHreP7qzuFz506Ct4OUUvhpSt+SLU7/siASucW1Lyvh/2/vWHlmO5LoTkZlV1Y/pedwHefnYpSztCrZgQIZtwYAM+Kvh/+2P/mBLliV5tTKXS17exzy7ux6ZGRH+kJk1l/4Jxi0CnOYMu3umKzLixIkTEdojgy0jJvOOHME7JkeaVGZLyR7+9+3pw0iG1hG0HpgVGbSPnD758CsMq56uTlil54oCrX1G7Ynrq5mVeUHPrCgrlA2rQ2yGxS2TfeY0lJoqF2vO2NxhKyqg1n8NoMEQkqkIESDqFV1R9wTu1ByrOCZfveJLwdUp3umqY6r6FDHAFIK8aLCyVYQEJqJT1NOUClsbk8WU2TlTDIH7ncuionJ3WjrPIbCo5SzlgDjYbuO7s/PMGUYm9z+fl1mGbS2PFKem1rBHE/ehCWXwLPhWB/rLMfHffvj+d3fXLy/+y1++4qIkvQhIioeIKIPny69273463d1OMkno3eurDcTQOyiw84gmgT6I/vNpefdxutz560233bs5aR4cDu77tzaZbDtHUTCywdKokZEAdfCsnWMTdY56z3XO+eBDlGCm9/Px5/HqVwfm5kFq1rhOMNBKaZGVo7W67VXzo6tBrQRUUxdiRVuoOjQza9s7ayqvtILbZ/+x+q+apTZPteYlsPWrAUb6bJM1T4HpoKamJNovQlGCqM/WR8GiQ9Zr0T5L8xP0TRZ7iufU/ttqiaf8Uj4Ji6pagaKqYKaLTfjienh1ubm+GA7bsN92neesmsQkm6gG545jTGpMELWsqmpmUFAf6LAJ7FxWccw//6+7H3//UPaVmEJrb6L98sNAdfr1g2AzA+xyyZd/d/v+h8fN691//qs3hz+5xEUHAPcRWZEMgS9vthC7/TBpRhcclaUSyRAVPeOim8X+6W76m5+OBny977879IdDiB0fR0lZ/3i//OFxdp55VlrMBfjAPqDvSQ1xRvAuMA8DhUD94Lx3SGJm5kmVlhHz3WxZGuAvh8SeWa2W15Wy+6c33EpNu0h2Vl2H1UBERSa5GsazOzRfzfTZdz5b5spjFZdlpKXqt9KSnzLC6y9S7Ri1b6GmLUahTEEBOKvL0hMJISgYNrAfMxmZEklgIrxZZDkuKQxkBDPJGVmLxWrA9i4FQ4apAkwiNi5RFI45eATnwjbs4WKy4Gk3RFGYYcl5WvJ5TpvelV+w89wFJ6qUcbkPhymezmYwPev3f3//5a8P24tOHVyBLYpfZGgl1annoH5UzvAnb8+nv/1wO8Z/+a9ef/lmj40HE8QwCz4u8IwhQCJO+dXr3avr7qePc0qGQ4ACP414M4D9D+fl7344ho7/5Vd76cK70/zDu/Ow74Yop2P624dzJGVB2HlNSuAQbH9wKSFmUSYYRAXsIKZJfQA5ULYMnWYbHDirWhXJrxXFhqXKFABtQL6mfu2YV6M0Kyi8ziNtrI81SEftGKKYsn82OcMn00tWtuy5qxl1zAcRTI14NbX/h7stb9nUQ6jUrHVS7olNZEGtV51UN4532XVOmWgx8iyJyakdlvQuJc69idkp4X4JY/4XQ9gM7m/mdBrzSyXHVMKk9zSYF7UpyjKqIqtaElmSPJ3ztEgI1Ac2syz2eF72G++Zhs5te+8dUiIzDMG/OvSPsdy0CwAAIABJREFUp2V+mBzo7ofHp7t52AXW0l9ghsItVj0nfwLbihqATb+M+ut35386Ld1u+PMv9lDCOcE7XAYMHosAhinhJLjuXm0cZomzfLEL8ISBP4zx9LNKoJ8flsut6zt3nPIfbqfvP4zjFP/yX72+eun/x7j8OCfnKXjqdz6eZDE1MSSjUXuHSWwW9R0cW0eUomwYbtelWRE1CvaeNheB65yEQkA3wabWcmZzaaT2TOjW/6z3U9fM77m4ULz+Gl3VGCZEZOsclxWMtSkeZLCqP6SaUlRirXzO9XEb41zyT0eNPcEa0g0gc0a9WkiSFGegd7yF0iIXqntmRM1q0fPBO3M6MDbZNKktYg8TvZ39h3kn+tWvD5eO/vDD+f+c074Lh03nibNq553vHUB9cFPMc5SoUINnP/TUd4HJ1Gxa4nHMZnbY94feM7N3MKMxxnHR3vNh07+6HB7Pyxxl/jjdvRtvvty5QDAuR9gMRGpwzprGxrRJM2ij9lcfZ3pcjmbffXNxcTXAAZ4xCwJhYGwYnnEbIQb1OGYMBE8+sD0sGbjvcBrjPMmmp+Fq8zTl//n902h282rYPfKu5w/n/Lcf53mSm+ueF5VTjErZI51TOsP16AKdnowCTme72CoFFoHM0nkG6fGscwZvjfd9lZ7aiqrKoSmModRJfK0U3eCYNTT3SV5mxe/UT8FK9gSrtTsUp2S+6vZqLLRmHLauXLTWgFTd3Cd8LGMV/hZWa5UqoKa8ZdmmEcPIjLK5LOXdEkEd74Btyjlz3/FeLQR1zi7Y90Xfclx0Vn43crSF8Xd/OO03/P6n08PD/M8Xm69v5Ho3MMNxnWlAREPne+/ULOYwzimpTUuekzjn5mRP4/I0Yujc7qvLi8455qcpfnhYstrF1m+Cv7nYXO+Xt3ejjPnh/bgs0g+hFju0pp4rKKkZF0Agb/Yf7pdf38//9afzWfDliw2CQyAsClMo4z6hd5gVrwaMGaeEpxhd2GzCKabx7XwSE7PLfXf6+CjqXecT0d3DdHHRb4Drm81pTP/jD0fXu23PaiZEkZCc5WQg53cGNWbsdpwVWcwUUW3oCWCN1nlaxEzhOzenbApyqPqJQgUWcUr1T8VNr8xChWvtUeMeqpOn1TNqzbzJVMtzCv73Bi1b4FuiuLIUWiQm5OhZmmSrfkwLg0yNYKtBtLSulK9cYSHByGg09IwMs6Qe5pkzqGcKZpRkUKXeh5QGCocgTrEQ5Jg1ZR1zyrpE+f14WnLOWczwhzGaae/9fuuWKF3n2KBmKaspxHSc5WlKj8dlEb3e9X3nnqY5q6rSj7fjq6vtYdunrI/HOGc9DN47Iqb94F9dbh7O8Tzn0/28nJMd+gqO1bSuG6htZ9ySNSL866x/dUwf3k8/fjxe3Oy/uOwRM0bDZQ9mjBmdAzMmxc4hGxagI110v3VP9/Gnt6MH/elvL0cFb8J+8D5anHNntFE6DP7FzfAPP50+jovbuMk0R1WSWWBETtR3LidVqGfuCTkbM4kAHuYcOlfYKHbUs81ZjneLZPHOVRuyFeOoGZWl51Q5nVp0Lznoal30Cb9Vd4zYCsHQ1kY1v2fwz/ZZaIq17xd11laxt1WN2GIHWrV97SZt4XUtPCjVAadEDJsIyVH2nA0mClGv6p13BmeqiwTGkHhwsgdU5UkpLapzzKOMcxqntCRV1awGQxL87qenfd9thq0jjkkMyNnmJFPMIphinqMy0RfXm23wpyU55uB4Vpuj/vjxBDMmWrK+uOj2QxA1wILn63243IfznM6309PtdPVi4zzXtFlMq4RKiUjrpHnamv71rF3Ut+9H9v7bl9vdxiMZOsbjgo7RMzzhKeMxggyDhwsY2D8uMqV+CF+92R+yXfR+Svbq5ZYf4/0Sw8b/ya8OXWCvFGf559vpD+9OxiSEmPM8y7LY4cqZQKIYKffOZrXFAM7RwIjQ3QBRfXxKGXSeLQScZtjbMU7iO6etrlF8WnVNBbG1DBGr4rFi/0/S7fo8A1wtB6/fr+BdC47zhdQgMGxdXVSE9cWuWkVbq7Sw+Lh1ycGq82jUXY2ojfutXVhWVqwxkqNEHIUXkaDqVDtmY4iSz7IV7ZNujR4XucuWU55PMp7nacmqJlr9csqWxZ4m+ed3p/3WHzahbGJVVQM678xh03szi1lS0p8fpuB4SaZmDpqyfniY+8A3F5vt4Ledq5I3M+9otwk3+/7jQzx9ON+9Pb96c9ENvmlJSirW+n2KdIHsC7UXSWFIjK+/2P351xdgYOsxpuWU+psu/jx3LzfIir3DoUM2JAHgyDbO795s4YBR0fErsd02fLTThsMuuJzy/W2MY3o68f/+8RiTDTv2js9H8YMTKBmI4dih95rVQK6HLQidEfEctXcIBkl4inlZMAyU1E4fzvMpbg7dmjtSNTIqg1GtWENpIF5hmZmVxuGWJRYd7rpuwKrkuqWl1vYyGjwazVWKl7q2oKzlJ6PV+1VVZTX36kZLndPMqpayCWybxwUYi2JmGkBGDNbEmJkzQhYhMTFjRke8MeuzsNjdnO8Xnc/p6bRMUzatLKmpqVod4an43Y/Hx2i73XY6T9cb/vbV9uVFB5BjeEfjonfHeByjY77c9fIwqhgxmeA454dzvt5jPwTHMEPHZdQwOsPFtt8P44dTun83Hh+Xi5ueHVXGn9YCZ2WTYPyrbIiKKHFMf/Fn1y+/3NndZJZ55/oXfTrl05xvHIHs/pSu9wEfZgjwZkNfX9A+4CJADFEBsNhukrljn2w+p2wgJPH043HJoMt95z0togoMgXMysKNAoqoKBqFnZCVY513K6h0Y7BhhiznBeSSxJWNzSnHMK8Npz+x65ffN2sKe4pdWK9FVn1aSB22lIKw0ffOPLSSCzKyc1Fo+IBRCeO0CtjUscqPMGi9nTRO3ciRoMg7gF34OMFqIRmbyrCVmmmXvMmwK3E9ZtKyTIQIk2aT53Zjvz/l0XMYp5tKiWNZ4KUsBSgYCcrKHUZ7SMif3btQfbu/++rc3r282Kesc5WlcHo6RGNfbrg9OBFmrPjFnOY45iVg5YYTgSYSSGhNte3+1H+5GOd6Ox8c5Lbtu4xtN+ywtLn9xgP1qESS5P8dB6evrAWMidtTbeLeEjU89vZvT6Yfj7R+P2224frkBE95s8OUWHkiKxyVGWaKIQjPU2eJAznmHoecBuL0jzfpiP4wPE5QzAyktpxQ8E9HpnOKivuM+8DJnBcGxLVomyKvaKcndScYZzqEslcIo80O0Ff6s0a+m1Ws6uAZHXkNmdeotPpaMkqrbakxjKYwX32MGmK8JR2V+zayOV6os2HOsrVVWLlVRrNTJswicrLIe3DKVxl/CzIRQbEsUbOYV5G00c50T0U3KQSwmI7WnmN8f08Mxj2OSLKgjvbKBFWIKUUDBABOe7kYKkboNO/+g3T/8+HSxC1OU8yRRssGCcwZTtSlmM5XCAJJ7OC0/3k5Xu82XN773jgjnReKcsiI4Ouy7zcM8Psyn+3k8J9c5rTUJkLNWVyYAB7UXc5an+Pvvn4bBIzgosHd2O7PjKcr//N3jTx/nbuNkya86ejMl11Ov6o/L/XG+u59O5zgnmZIuWdWYgwuD3/TBETuHJXDehyHJ5SEEEzBxNr3MoQvkcJyzqXVbH6OwSFIyD0tqZuzJOcSUHx7yw1jnAZtgcNg6yJxrrmY13Wy2ZqsN4RnK11S7Pah13uefGLUfqJlvPq/kZgaQb29CjUer9CO1MLlae5GUWa101oyDa5ZPz6rHavW19QCosgCtXfZmjheYNzizu2waADFhYjUWgeBhyh/O6XyOkssTSuuhFrZaVWAsBXw6cmoqGaJRzXn39mgfHpfLfQie2HnHzjFdbLpN77xzRRJc/kkZP9+Nl9sueHpxMXhvKct5ymIGYNf7y114e5qP98t4irtDr20wZi1o1ltAXy2i98vbt2dxlAU4Z7zcIElWDFf948+nD388ffvdYXfR/93vHv7m+6e7Rb55vXuheX6f53ky0SyaokiyLDonmRMlIBm7EIaN98EJkAhuG1g1z4mNDochLzovKc4qMFJTQwSL1wJq4EgZu+DnWSJgAWyQDDV0Dn1g0rXaBGgjJtaAiLbsqY5LfQYKletoPEiBWjX7hKlZnbEAMq2ezwBvpSpaxi5Umr9R+IrVoTFxE140Oq2yu88xHCBTtefgiVafAIyE6v6E4gTFkak9BQPgepddGc6hZHYf59sxxZjK32HQMsq+/BFqEC29KKCivTQ4E6FABOv9/Sl9+WKzCZylLgjrAhPw9YvtkvV0TqqqagobF/ndT49J9NuXedO5Oct5Eu+ImTedv953H47z+TGOTym9ykZUljVr2ahVZhuofbkIi15d9d/89jC9jwBhzgCFFwMeY4569WL77c1uH/jjvrt/f+bAFvDxaewgDI2iS9IoFkVispiRJMdss+j4eE5G1HWh82ocsy5ko1LKYnOejykHXiLmCQhCHY1nEcMugIjqFGmVOenDDGOIIAp8h94TqeUompU7Vw2ubbetZ8l+Qd9i/bm16hPK5NDK4NqzKbZ9udbKA1ryAFhr3qW1fvSM9dGEGlWb9qzVaJQvSnTUZ4T2TGNSkQCYMSEbncjK3joHgMCOHowE1sElxyaawZ7tIfj7RUWkqL5KyFeDKRrIhFWCry3agzlShnOexyR3j9Nh15WYzmwxi4Ec01c3w0Pvj+NyGlOB/XMUUSOm4xjJ8dDzOGVi2w1u1/tN4OkYp3NKUSlUd07SsgEzD9wskrPuo0Jp88UWYjglwHAR8lPa7P033cEvKU902HfffnP40ze72USiCGvOtiSdky4iS8KUZE42Z5mTLSJLtph1PsVkRN6F4OFcdiRMAqKByQER/Q7keYw6LwgOSk3vI0ikjzOmCOcBQgjYenRkAfz0w3F8WvY3G6sofGUvKjX2XM1tEc4qDq9CWq2oHysx0fTurVJVvaWZwVefWXMFNFvDLyQbVPt5mzzczNY9r2jfexaaFl2/ralIFTZbaluSFMgACIsiEjawRTU6mtU82UPvJms6D5R+TMBMP7GzUn5TXVWIRMSqyEqnSHOCnuKm86DSho6S6V7tBs/LtCTnnEFT1iR0+zRd7vovr4a+46cx3R1j37vd4La9P2z6+ylPU1qm3LmgVt/zExhs8ZQCyIOgwOBgioGxSH43nR8X1w83F37+MXLPh8tAWy9qS4wwaEbOOmddsi7ZYtIl25zykq0Y3JQtZkTRKJYluy73Q3Deu+B0ZxgVOW+3DkLnpHMCe4QA9lBiW9QMx4hF4QPM4Akbh8uN6zyNs4w/ne7+eN5dDm2tIZeooaZkpaNECa4FKCvke4FxDZ5rtSN6biGv5Ju1EWp1laT5CqIqwV3rR00nTm3coq7NTq02X5UZJTDVqpNy3fWA2i6DOhAI7R2wOuMyYjQ6E3IjSSe8VRtEA9Fd4MTcOmJgZo04s+rV6jEpa8tZiBOzKsghJnnM6hgXm+44Re8ckQDWOX9/TJ3PajYE92TJABAx29V+uN5328HfPk3fvxs/PEy/+vKiTB/ab/ztGJdznMbsNh5WG34amUQwot5deo9veswJ54wo2BCERY03nGdF1uUhpl3oBrfv6fY4RSibZdEkOmeNCUu2JBazRLEly5RsjDoniUJRTQRZLScN0Xbb7LgzcGQQOx91HuU0Y8roemhZ/UQKj5hxWiAGZnjC5Za8mhP1gTrPU7TTT2f5zZXrQzm+DeZQk/lXK4FWFq1wZKjdAKvCs2Wi2pLFFmrXDh4F+ZbDFmNsoxVqLCz756yoZGsByQjcRk4aP8fJEq2b+qhyv2jVCqovUsUP5V8EMhKGEEeHOZtzFATjJtBFR7fBas+uVhWr1cblQu0wEDq/OWw/3KbEwQysMCHxMEXhzFLWJYsqEVQUt0+zd9wHv9+Ex3P0zJd7f9h2ovb+fvrpbsyK33x79atX26tdd5zTfujsbpzPsox5czDlBv4b/owg6T2yguz0x9P+ix3GhK7LY0Lvtlfh9BhjMrcNklXGfFZ9HBcEJlVRTYKYEYs/y7ZkzInGxHNMU7IpIYslRVYThRpizjHxbgPXB7iQUqIEVZrNnAcZ5hGhAxFSxiQAwRQB2DEuB9eRjtFSgoNegOTtaX5Mu5eh0RnVM1WAZIVPrQfbGmtlNVxS3SZQvwV77oGrFavnCqmZb2qDZ7KsqaqAMr6pTB4rIKuW1xsCoyYurfPg6xQTrQtQ1pKXPdeyaK2j1lS2JtdEyVMmimp2vdn99koWST8cn0kdrabcnCKBwJ3/4tXl+9ODRapjIUVvdvT6euicU1jwZDOWqDHLxYaZu/OcJckQOPYcM7643Gw65xx673/7zeWu913gofMwG2f5+HSeprSMOUXNKaOjFrTNQKU6WBeKPyzcMci0dxblPGo4eBIjEJy5F90yy8Mc70wnNU4ZClGLgpRyFI0ZU9I565RkijYlm5LOGVksCwTQMmdAEbNGSRdGrvPwJB2N0ZTgmYiMOziPuGDKiBlE2Pc4bEgnm0cRNnVkqi7DJ5neT4/vxu3NUDmN5ixKFUCp1Nkqw9XQfktJrRL4xaRqcrCCvHrvtUVLeGs9Yp/EtWcqrsrJyvAPVaLS19sGWaz8WY2l+rwYBU3noUp1OG4dY1SBI9WOp6oRN60L45gx0PbLXfowf/z+CDHXkwUHEC9ZkgG0/Wbbez7/NFqS27uTN9vwEhxfDPzNi+43b/bbwWtZm6DERCFQSrTpfPCuc/zhaRLB5W54cei/uBp2Q9h0nkn7zjuGKZ+m+PPd/I8/Pvzw4ZSF0pIkZVX7xT5nMii+vp1vTovsNq6jzaE7Tzou6fFu3mwCFkn3s+tdIjslOUo+xigOTKrKIpLEUtYl2ZJ1EZuizlmnqOeIKWJKFoWzmQoMpGZigEEMUUwsXuyU2I3G5wVOIGpwCA6qiApXtqYKOoaKLRkxGwPdzgbBZuc0YpnT8efzyz87+N6rrVQrWRs90QJTQ/bWyNDqyMjaqk2s1vcJB1dfQc1qfbNqND6pMjX7Kh7nWQZDRgrl0s5e1kIW0q1peNlga6NLqWK1zPUTbm9tgqrF9zIFptbOAJQx7LwkgeObP73ZvN6o6t1/f788ppu/ePX1v315YXT99ydvtkRdvlbvKJR5PoT94B2zManaIrodHME/nGOeExMNvdv24e44X+67Fxf91b7bD94U2Whe5Dynu/P89uP87n48zVkExGDvut6F4CPWMgv5lL+6m/7N3Xhx2buBb384766Gh2mZovx4N3WHHM9YTok6VrYYc/0TBaJQk1TDpUxJlmRTkjnLlHSONiabksWMbCoGMxSdiJSWIoMCx9FU02EPkDoHEFKCFYGGQRTBwzMUGCdMBO+wG7ALvOnYk3WbMHmRc5o+jinmMiNt9TBaBXcF+iuVFKdpVq25qOahGlymRi+qwZlZ6aioRQTfnF7NTstzSyDjAsFLNZyaezRreQII0uZyG5TgqpjWtMTRVlfAc39vxTUwlABdsWVJbWnVDIKBjsm58MXm5s+vd6+H23+8j0P/3V9/++K7gx+cT/riRe5TkVBQ2e+as0bJU8ydRx/YiPqOzXB/jHPMS7YkMnRuN/go/RDKUl4yQzaNSY9j+vg0v38YH04p1q266C791eths+/ZkSV1SYZFrsf05e34Vc6XW9+zwySZ6SGl3/98SkzTxvI0KaAwjWtEqTy4QrNYFl3Na4w2Rl2yLcmm3IxMi4XBgGJtBaKp1QB6nLDdWPAML5bRBSRFXBAVYMwRBjjCtsNFx4eD2ziCqAgk8NOYT0kXJT9GTSVtXNVmVgXCawEbz+Kg9tO256nhemuRcn24Fq+KRfoK3MonUEcjaAP1raOfWl2qcHAtG13JkOrVtGmyat2/CtNav3LpYaCWx9TmP+C54L6SKsLsDqG77q7+xWH7oj+/Hd/9w+Of/aevr77alymC2fPSEy8SuKg+BUZM6IMzjyUKM05zPo5xXiSKOQdYMUe9GPxh1+07d7nv9hvnHHl1ZDT5PAS/G7okJhrnmeBx/d3h6nrooP270+vb08tx2cY8QIfQhcCnRd6+O70lPqqdnvL9Mhd/ziSliMEGNWStY3JLvS+p5axztiXrnHSMMsZiXhYzRUGyKmEtdmYKKf6smVoxwSgWivDKsCSMCVGgAAkIGAZcdLjZuS2o37AYxZynaNHoPNmcrbwmrfC+jJjS53IPr5xZRWFNBIlaJyhmVIJcTQDwzD21lwUA3/yeNcMBjJ4nRpZDaFThGCqx1oyrVTcbl0EGrfkCCvwCYHUVRvmgSw9aqWGV4jgqbbe6UxDBnCO/8dubzXQ7/+G/vf/2372+/Gq3nh4hGns3mJQOeICF4B2pIYn1wYhpnFMSBO+2G4bRkmQRTRnX+7AfQt/xxSYQLCbNYuOSj2O8O8Xbp+k0pTkqs371evjNIfz6cfzi6XxIcSB4QhRNSgphNdP8JEaOxcxMvYeoZdEMiKpUBTNn0WRQkaIsTmo5WxSds85JxogpYYoahbKqGKAoQrfqwBQZEIGimlodwCqWxTTjPFduuETV4LEbcLXjYLTb+s6QFU9jUrOj2DjbIkgJyrjZeg6uWs9aDdcWQRvxXzkHK25uZcqaFq+xWMW2PhlGspaDyj5hayX7Fr2sdSbYqsltbH95Ea5bLBqB0RJKXZ0Ymvssg4HNYMRsCiVt8XXNPWsQt7aDVkkJ2cwQsj78/cOrv3hx/d1lQ301/C49Z1HHCI4du86DmZmQRGPmmORq389JclYmnpMAYEJwNHT+Yuu74ILnnDWLPE354ZjvT/FpnEXyi61786r77ip8eXAXLu+TBgIRZrFJTRTs0Kt4MmZiNjFtCZdmRRI1Q1aIFXGviGnMBKCc+yTIkhfBkmSMNGdZEkWlpFYmR6nBjLLZsycr0VMhFTOj8+gClgVTxKwAEBySwgx9wMuD33hMpzzN5HZhWuL9kwhjTEiCrEiAA/Yvdi5U/1EcZ71zClrRdFH6q66Op9EfK+QvS17agJi6oV216CpMzcyvacWK8+rM0LIZmtBq+m17CwFNxNvwBpUWlyKOtOfJjDXkt0KolLmInyxRbjG+ngQq94uMDZqyieJPgeUw/Ph6U313fRoBWAbOBEpKoC5Q8M4x1BDA3nFw7BzZaPMiapJFxVQNm973oQybpZikKDvGOacUL1i+uXGvN9ubLR+C3wQELtJhErMlExGC552nzpVdG2ZGYmRiSUxVzCwpskAMomJmoiRmqcjmYCqWFVmRBFHylGysqaVmhZRYqTCDmEFRBjV8GjGrWxDsLig4PqUMw36Lealnftdj8PCsJtT3nLNOMZ5nI4cscEzE5oFOoHu6/GpD5FZuorJg1eBqVlkJMQJUtXz2z0XNap3UOgMKlQ2zUiCv39MyL2j1hFqXldYpGqhB8VM8WPZY1jKorbRY3VBbAWXNctfSv1X/hcqDaAmuAKkpqHhHtPphOQHJNMf04z89nh/TeN3tb4ZnrAkokAJHB4rqjR1BYeOYxyhzlJhyuVU5GzNSLPuEbdPzYRs6T6okqtOcljmFFN9wvjjoRe+2vgvOCCaAKCkgxkTmmXYDeXaOADJHMFDp4MtqUSyLipgCZqTQUugXq0YmitKaELMltZQtSY5CY9QpYckm0tZSN+xfKAxRqNYH1XkQCBi2GDpbFnGGjiEKVpAHEXY9PEGFRG13wdNi06wAhoEt1pUVmmEdh99cXX65Kxh77Wgq3qsQBbBW5H6GXM/2QmvK+Yz3q6GVGFuCaOHUfUljWx2JfoH2yldu5fQaHMsI/pZlrEXQTxjcX5JwxU8S6rp0qwBuff3m2io33JqSvZEXm8fUe/z0+8dX3x381rdf0gDODmnrwqJMtIjd3Z+/f3e6Oy5mdrXvL3d954mZRMHOLFlgu9y4jk1jNlqgek3JU3YB7CwQe0cKnaS4XzDggM5R56kPxGArZBCxmJWUIkkJgprUzMgMUpGKlmK7FPWvqSklsSgaEy2iWRBVYy4Vp2eXXmxpDZdS4285oPAemw6dAzuMM5AtMNhhnkCMoYNk5AjnKGxIE86j5GzskSMba2BKi/mBYkb3qn/zl6/7fbAS9NBSzKbzb3fbyGqh7bmXE6tL+zTTrKmlNc13LVArGcxXvFYSwPYIbdNKQ/loiJ/qYA2g8mQVlLZdZmvwbrkKqscza6XRmmbWTKMSHoW6bb8AI4udIk/ybh5fHfrp3Tg+LIeth9kh63fH5Qi633obPCh9fJxP8yJCxyk5ptdXu1eX/XYI3vE059Mcj6fUIx2C3YA2edkSeSCZEFhNkyIn67wN5tihc+wdekdM5JmDJwYzkUFFil9WMaQMMVNBNkvN8cCKSo4VEDNVKFhVikKrgnozAnnnHJuqnpKotvUMVhFKwfurPzPCfoOXexeAw9Yfl/T2VucEr4iMbFBgM6B3ECDOCAOGwFOW09GGHQXP55OQw7BBXACD87T5k8vDV7sWfSrAt/YAjT+tmWBJ2lApsaZJa2loOxvV4AqrBSoWVi7fGBN6LqLXYuSnSWTxQ8S1g8pqJ0CLtyU6NsK/FMao1jPhykCtWnBoB6L4tjWfbU6vJBuqYuMpjmOKhJeHrlcdH6aLL7Zb0//4ON58GD+Oibb9qPRxTg8P0/un+fLqYo7pm5cXr6/6u6cFS+opX3pck3y9T4FRdrWI0dOox0XGZItoFBVF53A1+JuNv9z5beBNcJ0vGZEr50DMxCwXYA8StaTVyLKoqGap6ydBlhUGEyMtSYBCtN4FMxDDEzyTKKZEZhXgrxHTAFEoIIqsMMKW8edvtl/fDA/vz9S5p2NCQs/IC</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9Z5MkSZIl9lTN3D1IksrMYs17esjO7Cw53JI7WchBDieAgPxaHEQgEEDkANnbXdxisfR2dmgPaVbVRbKSRAZxYqr4oKrmWYt/AOkQ6erIiHB3czO1p0+fqpkD37y+eX3z+ub1zeub1zevb17fvL55ffP65vXN65vXN69vXt+8vnl98/rm9c3rm9c3r/+/v+jxdxdMBIKCiAAQoERQJbCSxt8AAYACZO/efksgJUBBDCiUABApQFCA7Sf/n6PtT1KgNgEKJWKoIq5JIFWl+K2SvbGTKSnrvRYSoAqOk6lfSlWJqJ6LSEmhpESsqkywy5EfQ2CFQotiFCZSURBARKpKSmAG/DACkV2LCCrAJAoG7Gb88lCq/yrI/iGoencgbh6kta/8duwNQcWGhFTlXlPVLqzegao2AEqwT63JUIL9h7f/8+FTEFSVAKh9rnrv8xgwrWOnqvPxSgpx2xEVKkg5ee8rVEr+l//dx02biVTJLIqJ4s7Yz2wfMZG1PvpDzTruGS0REamC1b5QApt5WOPIG2lnYIpD7CpsPwCRWY53E+JA8iG1Po5hgFpLzWisL4ncegEVqeNshgKQmyOxndyuqgQ2c2H24Sl9obsxgSD1vAIQE3FislFgSlC/T6ZJZF8KmAkwY3UTgxkhe2MgROz3BCipDy8B8TvxeSY2b8JQAdiYkqpWI9XoYBt/AWw0VfytD7l9rQSIXxWk4vYKBRQCVdE4LWGyryE26FBRIoWoip+U7KRmj2VUnqRr2/iMxn7KTZfaLiuEiJWEwfaeqJqKz3PEMDJBRInNPrynAkgcGog5QKiaioAMQKDs41KPtZ/5Oc0aKgjWsaAwsbCZQEgfcarnpDgOEBUF2MC5GidV+1JwgkPafHKbGRORjqUBG/woESCkIOKcSUAgZUCJGYSExExSpkKU4qZVyCYxwYHT7T+B2FBPVck7S5VIRRDzKMCdgQqDgSjqfxAgboQG+KJixsAAoKwOY25J6vjEcQ5SCcSCqqqqQxgUENWWIaJu4W63hmAibvYiBKgKBJqS0lDajhWkIEiBpmxQZ36CwTatQer+aoaTe0NH4WEdzsx4YPc1dxERk80MAsOmsmEY2/kNRzhMif0a5KeKRrgNhT36LK8OHtXewi+/5URJOZws7v/0ni0qyPEzuIMjrpKKEpEWUDIiYFRCMRVYN9psLIysBIYUgMmhkwC1Lq3TQMNfqN24zR1VULLmEDh8hPmPmEZUb/I+1MMcdnX7CmFQAThcjTcapEQkonF2ri6diUqcnJULVQgUMKhAwUQCkIhhsyEjEwuUVJhJJD4o5KNLCkDAREyZiGB0hg1EZgiKMTbvouaWZqyI0Q5Tq+NGsyGECyODx+jr8I/WV44ileuEn1U2e6zTFkF73PnF+UHeqz7AFdJsrO77a8NJnwnzIPM93EQlNmYoqszmw4hUlZndXwXmMpn1JSaGTxQO1mMtZjUOEWYXM4mjXQRxIgEEbQt8JVIbc+c0hKDNqI4TgXIEBgkpiEkFRO5q7XzK5D7XTugNMg/PCmGwGEZbh4iCSEBc7QMSHAoq0UzvdbsXlphIDPGOzDDSzT4s91hOUHTDhLC2e8NrBEdA7BxYiaPznQNXh/vPGJ77Y/ZhDf9C99zozKrcpdnQMRG8iYGoxDPL9+6GgDiO0zp9qRK9GN3oIoTFV+AzP0YCMLGiiGpy91cPhLXOwZjteAIJU1DU6Cnjfn7jQUZ8ogY6aVDf+EBgRISIFOwXdDiocZIFJ87tfLqSIRi7oVAEAgBpPZbhhjh/Gu5hPpGFdsYW/V9CcDxSGCUxdhDHsKIwhSMHEVIO66kAFp3uwYDNP3JiXhHORtb9TxAFqo4pzIXCBZEbbrhk/xBkfE5BRMxUYTJw0H1c8hDF2XrcgI8BwAwVHfbT3cv95tWuTLo+6x68d9wdZUo10qgxDMjswJC18sWAQYdfgd8yOziIgt2/oHpiD29BzDaRhGEERAP8Qd4LFq7ct/kapVcWwIQS1uez32IH+9fPZrzK5qFWXDSMFRUwyE2BGBYVVEwLKLY5Qeoxu1SzVxXywCqYB5SN8llIRIiWmFOudkykbrDOSO2+NCugFqWbw+SwGq4+7v7Qe0Pinu6JIdUQ3UHcgwkwQdT8XfCTGRPYI3CaAUYR8zv8SrS8zgO7dVNemHSSV7+6/fJvXtx8ejNtRIpODU4+OX7yO2cf/M7D1VkX0WpEvTb5w3n553ODoweCrTGTiKiywVJFUnM8CSAmZjcOJIcvt0QOqcS7kVWVahzkLhTRmaJgJjVq7xCv+lbriJTA6o5P67DM6gzEp7yCoQpWFtJ7EKUgVjUlQTwAFI9K62RjeCinMWfuxbQGNvC+sx+a4gICh2RhAQNRBplH9J7zeRIjrjRbhx0X2GBzIeCrjlKFLJ6PDielQQTcmGYu595V67iaf3gr6uTQ2SpxYp9BMpXnP7r89H/9bPdiIIgUADTt8fVfX7/48fWwLz/4t+81bUI4EKG4adIImv1PuzhDQSQi7mYJbIBkggPseDVEJQIxMxMzi3nIykOdfXOAvUeflZA41TJ5gTnsyboo/BIUDJbqcjTc6zyd1cBeXccUVtbwUy6uORT4jGdUJKhQ7wQ/qC8z1CWxEFOYSEJTqwTJzJBB6jDo7CXG1zoh3w+FHAgptAnHMXNUSDFLSFlJKh2ajS0s3hHN+UC4ujAaM1DvB4p56GhmA09g9REz4kyOYWbA9112KfLl37764n//vNlO33/cHDU6Fd2Pct3r5a1eb/VXf/rs5OHiw//icUpOJkwWJDLCaFS9On4G1SFlwmR2TQlUQq+cIdxaLYmJU3SXj7wTx8CPt+ZTqLSGaBUq1P+du16DvHkUEXjgthnOWXU+S4QM9DaNM+9IgMkd4v4YEv5XKdw2iX3tgZMqgZhVJLwnOZ5qzARSNidLghh3o6PKikmJKEcrQKHHuvo4gw0AZlIlZReAtPrS6G/DysoEEV6BzLuH9BHEI0R9kNDMVgIfo6cd+nzcqutwnmEUa/tq++zPvjqH/o//+tFFg+2+P4w6TOW21xd30+dvhl9fjZ/9zet3f3CR17nOQHKPh4pUVUmhatcuHRiVQEqMqYhSIkcgYiiUKSmUKBFDC0QEkjhrtbn75N/MRSpNjMkpWntj7kK4Q0LEd+5UZ1KCez41cCgCOdTpr0Qkbt1mm0KevgCR3NOR3QGSB0AWfVAhQ0IVzAJLuJmYXOoQBDCpcwViu1moZDMHdhwys9Rqe+qxtAb3rtPD41yq7Qt1hNnzETyzUzfCkOvVBPza1X6RaroO3N4YnbuuRnpq9yqil5/eDq8Of/L7D37//dVwGF8MAyktm7RsZZ11nRtO069ebMdDWR43fm639coEUMfETArR8ZgFLCRmIdXIarF351thtaqISjJvqjrLgJX0mjIChQdthvTEZOIsB1gpOJIQMdnVyMPsKaDQltP7i+WmyMvDzny+UpmlCYJCWTw3ZxPaEFwCq4zIaPXG1rMGc5hlOgM+VaeF1S49xPAmCc3fGbqCmSYBV15F4TNJiclpq00rDg/nAxOtYLtbM6S3qDSxk3quLsPMPsi1yxpB7qMFTo3V31XfEgNJFDSOQIAU2TzfPFjSoxUf9sNhGA9jGSedShEpIrJI+nhNi/1082wrom7ScKdh08sxhYIcBgeq9m92yUycXHukGlBYkzhaGG1mImIzRarfUsQ0Gm+YYuoyM0cz4K7cfsIWpliwwEpEVBUOopb5vZOjd9YrZoo2JHI1Me4gOTq41XLMtMo+CMzhYvwGYmDipOzgFtpnnaMhdQW319C03POw2Xp0F5wlWpIZDpXupAJpYiQIHIJHsDTjpfNImYQ4S+FmYXEejg4nP5+3OcKLSvescTZgTr39BsP0QIuMDDoUvRvoboJAmViVBuS+UJNoWfRn/+fnd5eHGmeEZ6e4hv0VsOrfGw65a2WilFLy+SLVbxFTYssFR8BDDAIzERPfC1qtPwHlmlc1lYsp4ipnL95CrrfvLoxNpKi3T9hL+evL1z+9eeOAErFzXFXm2GqGbTteo88Rtxzugt6C0UoSyU0qAAEIZla5UMh8pFH54G4qV8ceXtolZg2TqGlBjcsYiM/yOUXBRAgqZrMcHpyC6QQCBP9wHuEAGdjlTjuS6XHLrPWmDBiVNDd88u7R8svrtk0/e94/f7Mbx+npafdgSa/38mozlqK9UkN4/epQRvX8auiFIS74XHIt2aN1SOUNBAYLIxOgKSRlJlZiTkwpMSdyP2GI6yKHO0iTx+IuPdMxJ/gCWcJpOPywq0A2/ylcdIUCgpCS9CJas2g1mAiTgCKONzqJqOiooBKUywOCqDaxaeaXUrCSKWdRSWPiL5xn2/EKZojY1KmaFBEzu5VFMYgbWbU4rUUhFNQvACBmTYUFum9+GqJK4KA1zXmRa9/RPcG6QnUKRLsPax58OvQxGMSZn3z79MFJJ5Cbu8N2AJD3fRkn2W6H/cSDppwot+nio9PlUUL4BFCkmqzrqKKqcQCfP/ZjdpABERJzIiYwkVUbIDGllJiZk3sadwPOHiqQE/tJDDWJyfSQgCbyUHvGi8BRj+lmzxxDwKENmYyRnCs6Fjjwq2csKhDOTYnmOnqYT2S/UNTmmBGmQAG/O4/QKMiPyZ/EIWYFSJAqMSOjwmb1VQ6TOmdiY5KZ+2VShRBSTA91HKrB9zybqlHXOKbCR4CaB6NWjhOO2gth4mtyQQFUT+5vzk+aowdtIvrkyfKoOYjQtx6v9vu+a/lRpnGiXsvFcfruv366erAIeAw/QJUKUG1o4CeCPfhlxeZEUha2dJTJVpw4/MNbpWXRcQwI1AuFnJvN/MSvKLBUlcMfuQMxwBPCvfNF9DXLZSC5r4yphbOi1epCtawQFFPMUJOklue5gG8wpy5K1eAPlR4pkdXfOGILsXWHCiIAMn1RRUCMbOUhPpoejVrMHpagHPK2ZRvNUr18KBpM7hjgnUlsv6sKiLWcg6LeqzAghGopQZnYzYjuD3hFxTqMABFlOjpuG5bHR10axjaljx4ufvHVtE7olgzF5SEdrbrVRTM6v3OeWmV99/MU0mmNlejeX/cwmZNKzRU6g3TZJoQYM9AIWSky20TqYyhefAdYZ0BYAmzEmYM7CMd4reILwxLYqoZMoq5Y1+lMEBUClIQ0R7Tp6UOnzZE2srZKWBnCxOsUtDIlhjM1rWOCefCdx/kUI9RSFAsKGJRNIgiuN4cC85mcOmiAtGd7vErQ3Zx3WGXDLqeEMdRxCj9oIgJCR7kv2L6FLKFB3QMe63ViGwhZNsvHq/HF7Zurw+VmPJQJTbPty36kScrpghZduzlqp5POGErNZQXFILCQ3kMJZ2ykwWGr97aaBvUUsZW82LQgsGvRbnluXnYusRSZKnwqs9cLV0JNyb256UUR77ifVxV1/Vg9EDCOGNBj07wqMqSkZGXAZPIlkTWCwBCp8S5c2A34spYbQjmldG6kdZ6DQqJy5a06L88VRArCQhxVISXkGoPOMbe5ahe41G3C9WRHXAnWOMMLaeBhcKwZrzT+X3U9Iop0lkm5FMWVKjonEY0kCTTNpATV5kCAJr57sDh6dvvl1f6r6/HsdPnj57t9P00KneRmKNyRPFrrUTtXBHCI2YjwIuKYalERubDPH41y70RSQm4HiBEKTj0+7DRuHNZd5hLFBOa4Xq2TjZfP83Al3vkgISJWiUJ69lokBUlEauRDSZUaoYYUbkrWaUwi8Oy6TyTLcEI0fu01PyH8hVVoEHWKwFFdf6uygrhMWxAdoFBk75XqSTh8VJ3gZvXVxbjm5KJdVDzE5GKKYKbyHIRnDIdSzWtGrupQvcjUvYkhozJFasjgnOgejSG6fbLOP4ZCC+VhkA8fLg6HvBnk+fUhJ8qk+XvnaO/5Ph8tsTRHtCs8YLTZpzWDmZNGCKOaOEEEDCLOXUPJAgVEGsYsIGr1VBVUhtLfDf3dOPbT8qRbPehSk5wERw1mMB8BRRDqgddMvJPhT7icCJLDJ5JLu0SVPVofm1rp+XwljVQqIFavFrKs+xyPu8UHVozQBF65hGAjby44oNSZCTsIeaJSoVlnL1epadwlMJNx4HG3Xub01W4jZucUirHZTOWOs3XWgaWY5+IxiBP/+34V8wXNf7sJzETGVAlEFYMfRDoct/uzJV0dLlayappDL8QY+7JuSBIfHqwXj5bhhusMch46n2b+QfA2gQJN4sRMqgxnOUQAUk6UMqeOi3ctrMTCQZhm7jcexmc/vnr2k6vcpsVpLoOsLxaL4xbAgyfr5WmbMyGZqqv3hoEtc21m6Flpo88xXgRIxCcIXcQ6SsLvmhcMXCEy78FCUkfOfZPPLg88BIGGkfN0JxnpbsxVtxrzJFxiNIlclSHOMyZGoxDePpDFI6RvnZyfLruvD3ciaszKnDfNLpmYPS0THKiCJ5yyGFY5Ot0zwmpv0VNw9ikmqDPuk0fjx3YrLC223z7Pn29Wy/JkxbuNFNFGUdp0OaH7l0+a46ZiVkyCKO73aewdY+XJvlaEANEmm/RgzWaTCVSJM1JmZpCSNVFYc05UimmzBKjo9rr/+mdXv/6zZ/124kS8atKCX/3kShSLs271cNmt8ru/9eDhhyeUIhT1YHyOfjRKMyKgJ2P5YCVJEfFrZcV+ItI6emFPoVNGJYQqEWRePUWkkWh3eFO1kC+CfHYJtkZOouRVX2oc8X4soRHtZfhUiVAxqAnVaR0Q85Orl4sNTVIVQ6dxznvrbEL4gTkOCKdpf7NbuocVESNRFGs6a2GdBV0CzBOxS5ZepkcA6bidbl/s32NC1kIyJu2JckdTwWGZ1w9X5BM7cMFBPczeMQh1+VmlCVDNOSWOLoEmNv8uiRMnv4EUNpoTEeq8kJuXu9/89avnf/9yejNMYD2UEX1OSsAk2F4eLj+7a9cNMR9dLFdtF8v7fCACJ0KE9H6tnVJ1jbiHgGNxQDFFOrRRqtM8pHrDBbFyN5/oQYAcDJUJJUhVuEtGrGixgZToPQKJILQ0F61JCEi//V89SYkxrzBjH9MonLI6HCb0IvsyRXatEhDUONPkcwu9aw2W1+FEwRcojmEOcuaRGTNFHRhFEtPB35Knvg4PUQZu5+zl5Z+/+Pr/+OLj47w5TOOkd6Oqym6SN/uy200vb4fmpOtOWuZUM2PO8wBQbSzm/8xDqE69rBM3TSIgJeLEzKb0U2LylCRT4mRTYJzKri8psxG/N59tvvzHy5sv9odNGfcKRQJkAhXVgmFbpr2UIvttf3SxPH608gVQFuG453FX4X1ZZkSyIcaM7dVK7Mg5zRjEJNIRbpN0D3ksPYHZ+6FyIqgye8zgQdvMnBF2aS21a5tuI9q22c4uRSqe4d69xbS3lXAR+cSNh0iiGkFhjc5AKkEyK3wwSGrtVDjhuI7flWtBUI2ShTiAAtHYFoTYIgTxcGGC/uTm5q9fXl+Pu6ftNNEvL3ebHgxtM+dER4Rf//mL7Zv++//DRxffPuUo13bpm6LvED1kzREFRJUyU2JiImJLMgYBmz0tGCDWBCioSZlpUCVR3V31V6/2ly92u+2EQYmoTOprCFiLqBQm0f5NKdg9//R6dbZ49NERpeTLKR0rjM4QVFmJ4CTRx5eqEliV7Sio1+BbqHTOZpWSOUEBkyWslKIYI6aa+lmZtQi7L9VYWq1QL9PjqPAhVG8aSxJ8Knv5UQYQw2vyvtiQVk5ZKU30rtFR3HsjnlvxdtbUk/36PoN1fDS66DkVgzfT8SIed0MgQCWiJqvwjnqXXmQzpGe73T9cyjA9WODVpn+47j68WPSDjEUyo59kUHrnmF/87OaL7svUpLOPj024tgrHt4X76uJdYmRo23BCcNwQcmbJKjCcIhOSMyVmhYrQi19ef/6j19s347iTJnGTlSCZuV6AiERUoeO1/OrPvl5fLC7eWze51kC6Y9I60Q2hOLR/WL9FXb9GQVlM0UpfqBpfJTxKJnexeU/SWJdkxmIr88jsUCN2qpUYOgNB1XvgCOgxqoKJfFUiyOxMaxPcIjRkXzdQ+Jo6dSLpIl0glPeK3kuQeyNMkrivkES2wpAu5OE5gLSaf+F55NlFcYBU5TDp7SCXB3lxyFcjF93c9IlwccwN4zAMTcaDZWJKV9tBQY+Omv04vT6U7a/uvviPz4B3Tt5dN8tkcJoqyIrNADckSgQkJJVJk98TSdwvk4hyAgAWgJRKUUBMuM9EE3TYji8+2zz/0XUaqMmUBEvCxVFKCU1KUB1EDz02vW4OOg3oDtIuEmd29h22XVUji7xm2lj1MZ/sAXCW7Aa0VsbFuCvbeuKwDhDJPBYE1M0RTHsN8lVZ6710WGBfKM+WbEJ1WgIkvmdArOZBNXyYwF1krLma/Z24xwBsBfy9QMHP4B6xvoJ2hnOqmSdn4S5IuQ+2jQIo8jwUkYS68rMZps/ups+25WrkSXJmcHp5t3/+ZrdkXrd81uWhKBW5I4gqcXq45kWXlk05XjaU02d/9eLy2d2H/+Lhwx+cn7yzalat1cagOEb5/bGTyKIqRZGqoucTJZZmhB5eA3ZRVU2ZuMHuWna3A486DZpA7z+kD07T+ZJPF7ntmkWGCjaH4fKufHo1/vxlGQ9683ofDtMJVvDguaaLCFoF1LBEpag2rHQljq3GIUF9ImE1I7TbqAYIxtooh0y/Qwm2Qz4pSSEhZYXiITGsiZERhWMKguXRrY1qqpYZjHhYOGeR4ndwzURrtFxNCRGBR9iC0ONmLwzYFAjUr6AVlJLiomT4zKRCLw746zfj64OINpl3o+6HcSzD9WbcHsrA05KIWM87XaS0KzQWnHVpkbnJvFq2DxPtBzlbN4cXu5d/9nz7TzdH3zu9+N3zsw+Pm5YJUIsia3Uhe/ikKrYQ3W/dA7A5urZepuS8BgQk5ZyOz7vcJSkYCk4WerKk405POn560l48WCyavB+m19cgHQ4iX17Jm4PubsZSNBOpihemONeIFNM896KvI+sTdmK9qJ7cDHKkCGHO1wf6+AhAAoVUow6vCqF7e3d42Kii8EQ7UAvwzOZISMgA0igaFUUG1NexU0bs4VHlvpi7TibduVWNmu7HCgGNNIOio/xbPjQiJI7jqaJfJOMjZL0niFhRPNLtmP6fy3I7tYk3w5gTLdq061VVm0xdk2+2/eWNrhfjJ6fNtx6kcZrebOWj99ZN4le9fnZXbvoxMZ+u2gfrTlWxm+7+9tX257ebP374/h88Whx3RLZFxj2EnpWeOqh2I8EvXFRQ6L1Z6H0ETrQ+7aRJNJS2SUWQOCl4LLrdjltMk+hYFOBVw4uWSHR91HCs4qwcVytbczeJGoBUhxIiP0UKiITEES+aO/uZmdxZPBVslHx9ugOn3C+LDdSDgpnEdbIYK4Ds8hGigQQoWhSNET4FcmCT45Yr0Y7AlaBJTQwQ1NPCEX4SEAFjVXqjWR6SUw19qQ6XHRuZ/XiPiL21ztDV871c96WIcFp1uYgmRtvwNElmPjtpm8y7wyQqv97gzTD+7sP2+0+oSfTyIH/3etpP0jVNm/2iYkvOmHU3Xv3Zc+mnT/7rD5pVUnY4i+CASUtMEctlg0CBL07O7Stnn/GJEnGis0er5SntesqsqeHXu7KdqGnzapkSy37Cq71+fTeVossFP/5k9dG/eNR0iaBRJ1+9w323EojreW3zLgqtmwvZMl5Sqb7FiFbNUMqcyHEooRgsKMjMSMiC0aCCPtDJyiNFaM6rEsj3yULgkoTlOlkj0hy3UzkmmUtUhLW6XVhQ62gjcwBDNnAIO1IgcmVBCnyWh5cMJ+OQO3+miDVugYaaRum+3h/GCVNBl5h8yYHVTzNjnVOb06LhlBhAKbJpmguanm3xo+sygloTT9m73p25aXJKt3//ZvPDi/NvnbjKb7VDCt8VSmCBoSM4xSAjohNjUKymEzKxglgFTCePu4sna9zeXhynVaZp1Ju9/NVmf7bY/9bj1aev96/31LAcd/TwpClNajorHYuyGDjHvkdNAuoroipgSwVtMLUirjpxck9Sk+EzCLn1GjkIcmNGEYl8M1L/wi7JYovlEfVhNbUuvoUC+2oqcW3CV/PmYJeV9Ft1dBTekvpSKISO59CubhZRUkMxN6ozDcN7G+aDfbrapwS2wn/b1MCLK20jJiJqNmO+HVIpGEfu2pbTKFZ9RYk5J4FSmymv2mEqTEQtFU6/2ZarQ5lsDRy0KJXJkvdIPDNlhdJBdl/vz7514lpH1Zs8yrKREgbL7Cu0+kfAdp9gWyFi912UGJrb/GSVh0SrBZ6seJFo0WQFbrZDKuWjk+aDB6yqovKm123DXZdj8xBLB4VdW5s4kIVisvuEFnemBPJVSQ5xgXsEExhmY62yqgOkQRSR2IZmFQTckmzfM2XyUiCOSkHzlIj1rmYbJpkE9LKiEN2LA6qtK81JKq2rMqmiUA19DRNNiAjUeysVX0fTMMSBJEIkVMvWCqj1y4p43Zue+zKME8rIUt5bpZe7cotkvWM1wxaRcqIyqRRVncZRR79XHQuYlBMnmoUeY4ilQKlsv7orw6PUpSAHrhOolgj/5mlzD3yrJ5CoW1GEGyqim9f7sukzSeJ81PHDLq+7xDl9LugSNQlPL5bjOG72pddRE43DxHC1FBHnWeKSwCpqxUwmVHt6zDi3UTrTACL8DUdi4yZemKLV3pz7awSQxKoFvkGF4TmRl2zMNwuLMhTw1cSkBpsWJ7gRiOujYS9CVFeWhY35SR11o5Ik4Dbg10KHYHCztSCaE5+YkaEaEdQAywPiKouQI/5bkwk8aXrTl0mmqTCUy3TW6MqYJalv+8LItreFFwrpMJWpiGMpUZO4yTkTTC8jBFAZq1Hsvtr229Gnl8X1pH6TVUVyRiBzCy11aBGnQlUFMZd8nQPdJRIwCZJiFBWhqWDfj7qgk0IAACAASURBVFcH2Q1lGCeoFC2qfPR4yRR5CrehmSS7llE3WpGgwRqJRkX917iWWQRCojf2pXWcfGCC0QOxCkTrkPAMPjO8xeBWXjjzMv9lLexDbQ1r7FoRTtClkbBfB2iJyMXDSITIRfe8fpxlTpMZZt0DN/ej0Jo3vQdcNn1juZHRIe5Lf9kfxmksU0rcipBoEZkKShFmTQm2pM2yQyYbqhIzZ6bEVjxGREpIrot5aoREFMpQTFf9/s3BaYaHdRZkk85p2PkGAokrIlNAiFMiJiWix5+crL/1oDvJE6gvtJ/K3TB9dXXgnBcNI+Wvb4bb/bgddKuyvlgdn3V0b22+p5cQgUkQG8/9YB7xmczbeCtIa/wggcTxncYZ7AQhVZKBiJs4hbFWpojoA4qj/CXqrFoDYnxhFcV7KIGynzGwZGbK7ifDFjVuxMoumedTIfRp5/pub45cRsXIV6m57oFIx3qhs7XbM0IVD/Pt2G/GZioWZTeMScp2FM2qoESkCaJwCAcBECnqDQKTUlTXgxW+n6qBtE4K2/+URu1v+sABy3gIg0vAM0cnUjBwBwQ42LiUM8vSDNKT8+5bf/j480mGn15tJ20SbcfpptfDbvqql/Uynx4lorSbRN45/vYfPl6svBaw+hQ7PSlp3dhZZ5dk7TFAcOv0DKN/y86TyGDPOfs/S1TaHYu327I85EhqXuse8twX2gJBZ8UrKtfcUemcW4X1oYICcpUqNmrMDzvJHDhiRkrlsG5v+L3f1elmI8iR/sD9V8Q2SqGJ6L2Jm69HqO7G4uaushtKYZ5EhrGQlb5DlFTENu8tNvLwPKmpclp1PTPtoiIiopBiDZKbX97K4Fhe5xi/7cc9iEJ4q5jPCPtV73eQrcbj9P53Tj/5L98tx/mmLxa+NEQn3fLj8+M3G/QjRtXthPyds+Vxo3FiRxINJkF6n92Yl4kA0jIaka8w/+PLkFQFEas4RFR+CZO8jN9HzaubhSfEEYgTZlXT7BIxcD2h+rnCgzlHFI3Gqm2Sq3Mzdb6XuYF2AXHgDfwT5zfh6GYGGsGwzjsLBDeN4GD2PF7cpaHQuYMGFZHLAzOlNmUmgYyT3B6mXrA7jOuFFeaQqhbRUrROsWoaar0Y/s1Xg5MWobHIOE59mUQUovvPt8N2vOcsvAMMQhwK1Po42FiQ1HlWBoExSGQFj1p+dX395fbNdtxNZRJ0iU4X/N6y+fZ522U+TLgTXDxaUqJw27VkNE5IVRGf/U711fAQwAhBpIk1jBRB9DA7tirDqQZJUXsbeqyKejWZerWBui4N51Dqe7rELSMUjjCCyrt8qmZAdV6GSeQ+MZClyntzQbqlpGzHjtBHImtvq6KsMs2lYIpRc+gMU/MVfrbRdySxyI0T0LQrej10TdoXJKAIjyKJpkHo/HhJrMNQimKaVKGTr6BQIVLRnJkJU/GSYNPLAAWJqiZGEVadiqgVyJa7ob8dVheLABIAtn15HSuDCJpZaKxlQ/WnZukiNMjqduou97vf3Lz/s6tHRIeDXm5VVJYJ0zhs+qFpWBLd9iMmrP7Ts7zM5Z21Zg7aQG5O4QydlbnVVA2phlOViM8YESU8MyZb5WucnHjOUM7MSyHqdM3fkhPzOUgRh26qTq/aq0/NOV7yC2SEQcO375t1CYgtQ0Yot8Gu3go1g9PEYFC41mi8l0up4v65oQCr3Nvy0j91pg666vOE691wfbe7IBIVK3605MxUFERlKqIQiKrlzokLRLVobAXgldjeISJQoBTZD2XXj6suqwJKOqEMRaPOVGy74EAxuucoKzTYNgAcKWyX/SZpv9jQP12+/Hx7qnLapeNl+vis+/XV7mY7Mss+pZM2dS31wKYfd6O2wPRqf/a//Qbvn+zfXw/feaDLbIOjGuZcEaja4D0Vxa1K4HtMxW/FLIOd9IelYo60oZgVXjuXRBAQrs18k2ggoKVfrSJO60ICHzpAZouzThObBzm6rW6KS6H8E5FCQjmt2FaZgpM+iwBwr7bIupxmUSOszFgtcSVzkWqy30feBwwUTVeDqL65OSRl8KRAZiLwzd2w5Nw1aZqmokhERDyOY05JCxcUZy72hAYq6jlpr0VRspErU7lXgFakvxlsKGqTRSsy3Bs6DwpmYYGUZNJydxhv+vFHr/nHb15f7n7xeni6pH/z3Qdtk3/4cdqW8c123O5FF/RqLDaoyqxFzk+7dtH0u+n4s7vLn90cfnzZfesBv7viRyvqbLNPhJucQ3tPCpl+5aBCwa4JiDIKQH1BfEhsjn9C4tp/vRdHSo0l5eGZ7UxkerDeMwEEp3LQ0chUBcQYiVABNMdU9x30iAMSw8cyEGtX3UO62bBv7qWIIjGKqec/sUtVAUMg/FZMqdXhANVDA6TgUfiq3/VDOQxHVCZFhkDTbpxe3h7eWS5SgqjmRGDeHsbEucm0OwyxYtsuKWoboViSF6xUIALQKAUKVWoSKSkJ7r64K79/wW0iVTAbZgtU62NDzFZtmaONZpHxUPovNoefvinPN+3d0InmnN47aVdtvtmNr/fTx016etr+8IPjL15uXmymu+207Hx1/5JxvODvvXdyktPl17tXm8Pd3aCbPf38Wru0/PBk+u2z9P5xetApz0KpjbQAXumo1VFqoG+gkwVWou72ZE5AaZT2BJroHHFqiDSz49GoNhTExvB2Vftjxh0FrMLE9RQOkEOuMoPOZ61OEFUqM+foy6htqzgLosk5vLtw+8wX7czRLdRDHC9JsnNGRPzPMBAA7cp4N319eZju9qcP8gFSJmbgVT9teqy2Q5O7RZsn0cNQmLHq8vVdz0zLLt/eDUoscp/uqVtJ8J4iWqzkk11J33226e+m5RmrwusYPLivYxP01oIgwe7F7vAXz/g3N2kqa6KWkbucJhmZHnT09GT95fX+KJHsx/N12590F+sM0nEiTlhl7Ablrn24bnDVP1qmTUlPu+aulH3Bbpz6n9+UX143F8vhOw/yD8/z01WteYTFt668w6GnbuoKdT+nFQTJCT08mKlI5B+8Za8OAKqmVgdXM2sgFfWZWbUJdcfqAK8WenpCJZsrnHXRSLrcw8Q5SLWBklncUJDlvSAetngDDIhjROez1Qnk5/IWWaP8Tci/irKfnr/cffbydtlgyaqi+6Fsx+nlToair2/2TKzQcRJAT9eLXT/2Yzldt76rkgtOGoGhgooANkICLaIiAhQRZWaCjpf97tXBGyyzShGeAzVWtrjscLl/9T//fPrZaxrHRSmnROtFxlhG0sn0G5Hjhi9342EsvC+nq8WkCpXjBVYN9RN6weOzle6mhilzylDuaLlqjtp0vsgXq+YR8/K6n/78q/F/+rT/0SWGAjiYmrnYig+ouD3UZs88LLyVZeGsRyJ49ghR509952O1he/35Zv592GRCohbcnxcryDGzISgxaw7hyuNIAbkiQLPAGiEr7ZK0bEZFpjGQga3EoHvGcKzrlEXSKugbj0W/L9Cp3plEgBVKbj89e3f//x1q+XB49VhHPaHsh+0H+hu0ZS70o/l8q4/WbRNpkXb9GPZ7IajZbto0812SJQ4CTQRim16YasLSbSYyJGEFw16AbgoGiYR6FTuvtycfXLCqY4RqUQw7fGm0WZI0ev//EpfHQqpEg0o3LRQnZj3w3Sybh4fNcMkDdGi4VebIWd9knlxvP56t92NMqTlekGnWtaJ+oMU1juRXqF9MQbZZkKX25ROR+ky4WaY/sMXfWZ879QrHLQmah3PnB05iEekOQcQ7v1IXIsV1UhR2nfOyo1dOTV3skAIfqaBDwhxV2wD2rA1DU9oZlhr1RhuxSD3vuZoZ5dWg3kDiDmxFN3/z14RGKCKaXE4PE6NuqboAfIgNqbF5qvNz/+vZyeL/HvvHR0t6HYs277cTth0+cmfvIMlieL19X4sZdklEbnc7BPT49Pl7XYotn5QXVVSjYBdYxNp1XzWPvzDR22XlHQaFbDHgGH72aaMRT0Oq/OWKhIgEp/DzTD94s1Zk86X+aLjtkljlilx29LRorlo6CjxSU5nq6br8uPjTjMnoos2nywWqtqglLHvmHgv+3683Qyb3dQlbhjn6yazckrXN3sAJeGk4fVx0zHzn34ln29IXbWkgCLyUQgpJPBKik2MEF5h7J9ICXKPP7vVKilJ5fH2cJ5qWLPVRvzhCRgrZIgucjnBOp8jeCGoZA3AMq8tTrPigpF2tjGa6wFoXi7wFgUCawTQtUAuzDVyKa65zUvb5igJJPvh1d+8/sH50eP36Bj77bbvBb3S2HbrP3h68vEJCaC674fdYTxd56tNP43y0dOjYSrbw+RxMSIG9qnA6o9nKwXadOndP3py98WdPN8PZRJJKRNr6l/sh82Qu4WAEY9i05BjXKMtmhLzq+1JX9aJjrq8ZDpeyjjodT+uQAuhtmFNgGAoMhY0Dff7sTScJzlbNP3YiI5K/IjbI6bCDNBqRTyU5XGXRlmsGgCbLd3cjYuE1bK53o2UmO56+vOv9ajDRQfhmjgK32hYYZ7FNpuJKM4gKhi+uHxvklOIJEq+2YZWLEdlPiRhQwpCbPhSY46Qr1zRtiH2JVTGjtj3aQ+XK6rh4o1+Re7AxRDnlfEAGmMEVKkl2TbeMVH8Dmc49JfUb72HKIgFJO/lE0rvXSw6LjIO/TAOohOonC+e/MGjdpFzS9aQ3TC8uT1sD+PZcXe0aF7dHFQnX41FEqdWEXUGg2KXoITlSdMeN9AyiWz2fSkFBNlO+8vejqnQ5e0MAgOgDJP++rbLdHTUaCYwEni9yA/bRkSxSEOiu1EOJIMKSDlpl6jLPKqS0KOjbtXl45wujpsmYd3w+ih3bVqu0iJzamjFyCKPzhcnq5za9Hp7AHTd0DsXy4+gF3/5rHm+U1UViDg5doYW2QoRpzoRadVOnpcvqT0v0hbP+Lb/VP0VeRRgZO0ehwYgosqkXlfppDCSFUH45lkKiAC2zz1V6ALUN/2JjEs1elAsMdWIUE3+0ohEI0keYZGJa+GwrRx5/ogqDrLGVQR0O3YABF9fH47KeBh1nFQo0arhJlHS7rg73BWF7vaTSll1iydny6u7fphKSs16kfZDkaKhYFJoTByOmaWAgO6s3QmYaCx6u5tWC8hIm5fbs2+fIlVlMkAdKILD3bjf9PuXO/785slJ1520D47aLNje9HyYdJqoy1MpTW6mvRydtCzjapGnEe2SMGnOabcZFyft1Og6ZZDeKaaiTUP7QY4W6a6UDugVXc68O2xueqwaKD0+Xy7POgC3h3683NHfveQ/eVeOm6BEM7JUV19GOWynw3Yso+Q2HZ0vc8MR5nl9sBZoqGqQCjhkVM9jC8vbS0SSaspdTbu5jKgC8vpT+1lSKh4ZCJFqjkgkujOiU0TWsXpj3HPoES1HAKoCl9PswuSbmNllfeGNRoLXV2dSHBdDCoiWqwONUiBf35b1NGbWohD2nhoH8bw4U2KME04uWqhebfrE6eKkGyeBigXdTogtt+yzUlQhu0kKLr599uo/PWdFk5pE2g8lZZaiM5WLGMvQ4eaLu9f/9/OXX24ur7bTpAx9uMw/eLL8/pP1xemiLNLwqvS7Q5fzinh1vqDdtDzuqNcx6zjRSLqktFhot8hDP7VNuj7I3VhWDVNKbYdeVBW9aD9MyyZvhmkCaCzvv3t8/mixO0yb291+P2x249WLa2Y9+rcfUcMSPB2xE18Z5fUXt89+dHn16fX29WEYRFv81n//yW/98Ttk+x4ZA4jhDOAIPgSnTf4QYQseCZZCUDcUEfjqOLdR1FCJSLWQWDWZB4i+calUyQ+WUKgurpbvVyfnMyIcbfBk0wHdeBTqT84M7uwCXCg3FJG1RSqVSIpIfzf2Q9n3sp/ky6tyvZODEnJaPF5ww+VQyn4kRpsZ4Can1SJf3Y0p8XqRli0Pk0wy+YOGbOtkL0ZR0WIbXZe7adyO5x8fnX3nYtE1DMlNWrQpt7x+tLKoyqNL85iqQ19+9pfPDi92T4/b40WXmEbBq0P588/2//4fX/3kizcTCT/oDjs5X7c0aKfUdk3H3K1y6hInTsucE+XjbpHpuG33twMEOpQkuk5YKD1ct9KPORGYtmMR4kK0OGpPz5dDP9IwLLKuGxy1tMp0+08vrj+7tRYGJxJVPdyOv/yPX77497/Sf3ytlwf0gkGG6/Llf345DBOqhAF1RxoxonlB8ce9RXgQgVSERghOpOT+wQt03Y+FFBrkUcJnIyMiyoAcUU8NGZuupuaZRzNQiWaSzhlNRSHlSGaAODbKdT/rg0dkDxmKiAJkj0wDESUeni7HZ1vsyzjpiy32Bes1N8d58c4aRLlIC9bEmSCKlLJ68MXLRQZoGCepT99QFRVVKgVFhBJRlFcDyF2mJ8vbn1wuu7wwbafhvMihLQVlVIAw9tPl8+1XX98tWwZQVAFKTOsuTYn/4vMdqz49Ozo+7sZeSqfNIpf9NCbgMF2Pkone3A5HXdpvBz1q06QX58thM9Gy6UCdYrlMaZKL06X0U0l5mPq8yK83wzLRZjus0rhswcjoxNh52U5v/vQ3KX9r/d6Rb5KrNNwNv/wPn394PT756PQXz7eHabfvZSw6Kdo21SesumUpSuCI1hIeAkQk+BzEPKS7s+pjEcE8nNRLzfJb+hMh2Ku6PpJRI0VC5J7DW0YcAS8PU0uNqc6VAv6vX5SIDddi2xWICCeqdN9OGxvsqdb9Iz10Ba0/Pp6Y7/7iOTEW69wrrY6XZ3/wZP1kDaAdyrptyqEoaBQ99MOrG2pSahKfLNvbbT+W4nkn1SIo4sgpqjppk1kBZlCi2xf7r//yWcNp1eU2QcDTqNNhClarlcQSgRO1y3yQ0g8BAapQ7pp0smxe3pSfvty1nJdt2hUZtsOg6JbNi1e7rkub/TQJlPTNTohT2fYY9aiAVReJSFGUVpnLqLmUcZBlotw0g5SuS2/u+lUjx2ctgZoMRVKwgsG5OwzX/8vPXn7/8ekfPu3WnYq8/ofX/U+vnnz3/PFJ+/mr/TiW7aEMBSnh6XfPUxPqGKqLSpXGmwyhHjy44B4F4/U4qvpTzUWoKoNLxAgmoxoOhq4BUs2IGj1DrhA0qHrbSJ/PdJMoskSwrKFvX1s5nIUA8cQHrfKHrzGpBkpVv4X4wgFRovz+mn/vIr26Oz1rjr57cfrtBxefnKSGVYHtxEpMKMWFk7v92GU5P15MRW/3oxRDdOeZTU7m01UxlDKOhVNixribeJ1Xnfk0CBiqfNwtLxaIySlK2bI8SrnNj797dv2LS3MExlJ2vRwtSmnpbj+8GPR6PbQ53xTZb0vhtCgYicog+/14erK4ue1PTheb28P6ZNFCVqs87Itt6TGVktp2PwyFSBdMk6gKKx2JfvlmaKlcHOVFZiZKnFKSpkEn1E561A/T3371etJHf/JemeTX//By2AzPrw9E+vxq9/XVNBQQ8PB7J+/+9nlEaFVbCKms+s9ZtA3iVGuSgkw4PTNJTi2agMTyVgrBw4iHa0sqAOWwcA2PPVuuZ7BIY8e2KBs2S3SD9U2FyeV8L9zmIGVxSq9lNSfse8NrtUpfm2CSoyYcfe/0/ZNvg2j1aNUsMidnn7oZRVSEiqJJIDCUx0le3ezvDuM4ai0EsbjZsuijEJE/BFEVWkrZT7vNkNQWFqREmECLh4tm2Xg/a5TmWCEE4YMfPnz+8zc3v7hk9z0ioOeX25dXnDMo83Y/3SzTzUFE9Kvr7cPjZVLN0NxlHuTsdNGBZNmetXxLeH1zaNo0jgpB2/KzNzti3o2lIQiRECHRctk02+GXX+8uTprzVds1DNKpqKhOIi2rNglC9KNnr6W03z2/2/ZTP/3Vp5cni/ary36YFMD6/fa3/9uPlyctgk278G62IBb0e/mHe0L7RXWfSlAJYhX03eJbUVchvC7DDrelrypK0KLEKpqdHyG2i7AnE0NVfTmBF++oVcAbQoXhzyIrqXrBoqeuDewsDkIU5oWkoVZfU0voEPPDskRgatPJh8cu9AY30EnoZlgvmuvtwIRkj09SFGiZwL49O1uvkFJi8gIZFdvYLyvaTLtJDy/2r35+JaNSsv1/SEQXj5e2NaNaXsY6WrzE6OhB+/v/5r2Xm/3N5rDty25Ey1h13CWiRDuhl4fS5BHAIvMiYbvtn552OOj5Ii+FOKdpN5513Aw6iUjCph9NGCojll3a91M/SpHSpjwVYdKS6NGy+XzR/Cp3ZTcct7xokgClaClKpETaJD0G3f3d889/cX3SUPOv3n399d2bCavjdr1ID94/+vCHD8/eWdokpSjygFa3RxF4isILLSwyrPxATD6IIQ9+56CGGjMhxCCNr4JgqNUF1ccDOdWj6uYAjeI4UlYWxCMPKKwISqQUa0kJVmAWZUruhFlFrewsAgd7NBFsVTibhdsRQdTVgdGiBhIV7AQ34/GqSVfV69rOIZyYSFFgxTwGnAJhi6XMFTLx+0fp/eP8V8932y/uDi/2jcrTjpctXvc6NPn0k2P4snWdZ61t3q8qpAuR37po5YRvd+PNfiyi754tjxq+2k+fvxovd+NuKB8cdw8zGNy1adrL8aplxulpO6kslgvNPPbT6cQvrsa2ScNYmpQWifebsV2kvYyqdJjKJCS+DxZ9+MfvNL/38MVn19ufvDrdjW3mxAwVUS4ybSd8tSlXU9pc3eXvX/zuf/OhZxtFiZGbTFlVXIgQCiMw2DGgcs3BM5+qCvC854GqSblcvaiGZuCpquDeBo0GUCQoVK8EpfS9f/WIMyIj5D6UakGss8J5Kx2Nkoq68YuvNKMQLwCPGuIUSvNbz4iZ95w317DjbddMD3NhNeFaK26JXh+OXvZXm+HN7R7EiUBEtuVlYuJkqM4CqY9EVpev2f5+uko/uGhf7abrCVM/ntH07koXSVmxe7R4+kdPuGGAvbhZhEZqfX8gaIF8dp1e76+3/eYw2caVpGgbvt6M7x4vnixyw/z5bb89yKOjhhM3ObUNCmicppGIQLfjRMS314eToy5PWC6bBVFHaBY5i+aUWlCT0t1+IKK2TUrYq/L3zvFocXjnZNdjer3NhLHIbY/Pbsur7dSQ8lS06NVl3z5Znb2zzm1KmVNTw0QbDAmPWT2oKNhKYBXQKCWTqAidAwB/XkRV1Zzo+wIozAKEBumDKgSJiUBl0vS9f/WQk+/j4w9wq4+9cRuq+7eaTwyRhDRYF0CerKT4DrGsfK5A9zPAC2v9rcN2rL6seonfcyQkFMrN88PierjZ9Veb/p6BApAmc9BXM0mpImNRmHIrBSA9S3o7lKtVXr6/Or3q1y0OI99MMr538ugHZ2GfAKACLqVlS4xC9lP6ycvbq/3rzfRmN90cNJGWAhHIgEzQoqvET4+anJuf3xxI9XiZLzeHUbEvutmNgypAk6qoZFYSJAYpkgoU0pcEtIk4c2JOgtNloyrKNHznAWfGIsvT9e5oMV0e+u342W15vOKTLgg7kQzy5Vebs49Pl0eNamyUFjUN4dKgXvMDUjZwcgbj7MVtrO68YRTdH/Vrc1cDxDyURyh45qUErvZqZibFVDR9548fpUSGMiCluju8jWIo91pRxkQNr1r04+ruyWZnPFuSku/F6IBmQl8dy7hABS+7gnNFT5DYwYLmy7vhdZ+I933pR43TgYA2UzUPjTlrzS6CYZC7/bTZDb0oTVPT8OVes8rjMjJSz7j+4OTB7z9eny/nxpkHmbS1R1oKZNfLz19fXk9W2rkbZChKRCviXLRJNIG6LiXQ2VGzHaZPbw8XXZObrEVzk/pBjlatDuX8weLmZpwyM8BtIgI3LARuEmdKzAD0IIuGW/AwlGdPj/iTU9t+Vln5tOufHH/91U5v9+cLHosOkzLZgarbsunH849OU2ZbnBq0tyIZGel0HNIQwiLG9Fi9EofIOM2SgeFVLZb0M5JCoOw7JRgQFiRmqE6T1227Ak4h8zJ5oBprbDxWI7Gn4ETo6foBwZ/a6PxPcJ/whcShsSG4gIgFylCSGsmqSwaeMyWARPzpzQzQYdw93x02fZP4/YerJh9utoMIQTUlCtGYDM3FFlcJhrGMxd315lCOls3thA8YF+M4PtvxEUbw+MGD9//dB91x5+TOMVXs+VyiwsIAJOVbSnf9CEVOeHzMmwO2o4xahkSnXdMCi5xyk4ZhPDte/ORuuh3L+yeLQ5EOlBbNApTW7aJgddL9+tXm4dGi3w5HbT4cpqZhHTV1uSllIvCCMyhnStzId06S7ZFFnt0vLV9P0qnuRh0KAG4T3n2QkjZDkc31bv+rm/SDc7Kgjyohr4DmKr7MBWdwEzScqjxNvGqiimY1ZeUYFuaIt/MLjnZ2diKoZo8bqj5rUqxpInUBgyrsb4rts6TmDDS8oYVpZiGxGEihZKxSqw6s6qYTCO0IRJWBMsUUsq9IoXjdYzO2mUUlEb3/cPlg3b7Z9NvDSMSxh4gCamGnKMYiY5GuzYsmF8HmMH7+cv/o3WbVtg/GaTthuy98vKDvnjXrRmExOHmKmOayEvO73KXdg9Xl7nKZ9b2T9nzBi4Tbg2TlNqHLqfTStjlNpW0bKjoVOYyCoSwXiSbJmbToouX9fqJ+WnTN9b7vMm+GosS7/USJp81h2eZhGDmlBlQyo8ijvlxPRewxKKoE2l/3L35z+94fv3NQ9D99MRVZtegSt4Sm4ZXy/tPL3btHctySa5kB7uLRYlUtJPax1RolakSPUkmcr8Nm5Zpglwpadmyt8vWCHg9pQw1BtujPH95F1fJrcS1ZYA91du1mUoWK8NRhjqTq0psVa5JScUUrEDpaaDqeWRG84FrscVlaxQyLYUTT6/5k3anopHq3G0XldN0eLfLmUK7v+n4oUPUdIC3boSoiq0XbJCqCUfTJg+VVHq635Xo/NJlzi6FXPmsXT9ezvl38gTUqECVnThHMt4/XA+hJw7/zdHW69liKaQAAH+lJREFUyBmlTLobpE10tSu9clIBaD+lUabTRBspvMosQquMQbTlwzi2bTpB3qveTrJMCYkapT14GGS1bDZ3Y9NyP8odkIsQ0fjZrb5/rFl95on2d8PUT82jZfPBCb51MvzszebT17tBmcGki5bG6136u+fTbz/U8xUSfLQcMer7kCU8uV3xbAYqGyoKKua+19ejixeZRcQXob3MNjTLkJS+/UcX5nespgJwQqX+/CNn42YM8dhDjmigPnzC+JyFoZVy/b/tfUmvZVl21rfW2vs0997XRp9NRFZW4ypMmZJt7LJcxrLohC0jJBhgiYnxhAETIyQEniAxQAghBsAARgyYIIQshCwLMDa2BeWuSkXa1WZVZUZlRvciXnub0+y91mKwz3mR9RdQ7MFTSPHixnv37rOa7/vWt77/K83mXPMrzxUUTa3BzB18RKmGqblPtnq4jal4XXrKZbefB6EYJSXtxzztRuYSFOHuTVUBlrW4GVMdOTAa8jpQFFJitRzfPq4+fkgTRThVwFOcNoialN/L4YDUob7qf/xGvLeURSTysl7Y6yjZNZn02b54MrxzFZ6NA8FDDHsMDnS1SyFKl5IxX2zHUMvFoOzagBa10KDNIo7qYBamqC5BNFtW7bJtmko/tj9tXXSCenp/bc/6x4+urk522VG9tlo9OL55ut0PHshbISZa7cbqw7Ux6eGiSMWmUdNrWs0Js551Sisz7DFFmJchoYSJUuRdF8ElPtLLoPMy706IRnl/yJGzhemFME3E8EfZiGkvwBTMCCjNRKnxp6qPJmL1mmI1dy4Lgth4ClbAlJVmbqwQv3NnM/2TEjLt2hx6TqdENJiMllQN2PYZBGEym6bP1QoIApAQGQNCYAnmWY2FKXAQBtwEfGcV20gOD4KuCrxfl5rBZmcwTFr5j6A/PilQY8uf+eytNx6fu2oVwi6lwEiGtqJFiN/Zdn9ylk8Ga+TyorM+oV7FL13m8Xnv2e+042eOmjTkkWy4GgbQqgpBeMy2A12dDZfAdp06NevHNlbmFpmKKJbUXaBbffHwav10xw/XuyEPZ8PBTt//8mk8CncfHIarYf+wJmgGhQiAkNW/9ny8tfLD1g3G8xSwwQp8X37jkumKa82USWZQyOdUSNO473z3pjBHblaQkev24rqXuH7vpvpsZpoLqjHlKeIi1Z00P1NlPgMUH4mLL0MrZjRtLgWLQUKpAw3gAoFOdpPzjPj8v03mbXxdHU1xDgXjH9WTZ7Vu1D5pE4WZ1ZKbmZO5ziN7c71LpGYMDuIMYTYiDKN3Q7p51MTo21GzMP/oPb6/79Mo6zxWcB1XMTlfA+ZWaGZ693zwk93bR1VQJ8NlnzXbpevlNj3fDY82JsyJyM1vH1RX27GKgUmrJm7a6reeDz92q5bRLKJ3v0z5fLSnm/Ri1M1oeXKUtYq4DUNLSE6nidpu3FuEwzur86+ePnn3fLEK+wYCVrUI2e2DwODHf/z8UfI9ouMFi5Ky8zz3gy5j3x3zmpLSGejsfl1uRamxbZrGmyowXH+Qbkpwm5ZSO81o3FSaoRTkU1D06yBI10kLCFM0Lqkf155oNtdPcysycU/TdmaaMulHyikvchyHU6GgUF5RiCailacYOT0VdF0VwL3QU1MxyeURwlz1WXU+atJ+tCFpyfJSro853M3mqdDpzWN3DUI021IRIWfaDGPX6WEbjHSbdATF+/vhsJ5Uo37dk818ssGnipeczAxwrAf7jW9v/9LbqDjthrQdrA5oq7AZ9bTDZqtV5ZohQc42iUUOI7tjNOhm3Gb7g6fdn3992ffp3c3wcJ0Gc1UzBzGxe2R8ckmf3td7C3SGu43/6vv0zvlw8RsfvM8SF+H1z9/zIX34xWebnd7ck6cXeVmLmZ2tTQjfPB/fTrK3CHVgDgK3oanyYTOV9T6N4U2jwFZsQmf882V4c/u+MG7uNCkU/SUC4hO/WYLPxC9hsuiaFlcUkWn51jA1C3zNLmH2fXyZOvmaPJ3qv4lnmmbjZoQLc7Qk92lmqhBGU09gLy/u9A/mbgM8Xf3SzV6TcE5OzhnyfFAFCFHKFjNX9aknvGZwS1fhBFcppmqzBa6Z9ymtd7re5VF91QR3HZRYCx3jKMAufFKNzA/6nDrm5xoe9qtnxF8+S2/WnlIy8wS5Gr0zP0+4eVS5mTki4+5BvWripkuj4u0bzVsHze9+6/Tx1t7vbAHf0ASXgjiQE9F+tNcbul2hCVhGXGxxMeDn3vSn7/LTEcFck3Yv+rPvXca39sKL/v33u4MVX6zHwzfqWztfteHDS310ng+adHMRjpYUiZ/V7QE8uBeJ2NyLldQ00d72Ms/NT5qhTNzZdXDCNXc5Bf9ZvO0vmfnpfkyV2XTBpoBp8okfOSb5PlC2fGaYK/+55AcwOQXzlB4nlJQKhTDxUd/PSJX6y4vpyfSX05WYJE7XaMd1dTnnzJmkrTap+t5Ok47ZCvRY1tUxkZkT+bbXpMWXfeqRMUWIydPHHLteLzapS9iPeOOgOun1Uqn65GFBNMxKInCfG08DQZ3Nw4ykl66q2atf+/Tx8geOu7325CKfnKbzkb59oU/WWgW6d9iuan738fDTnzn+6U8df/zW4sHNxYMbTSXy/ukOhofn/ZXmRFZFSurFaoMmLSqpQw298/MOneFiwLeu6DtbzqVjUuho93/qtbd/4t7dTx4ef2J/B9Bh/NM/9cYy6/3I4VNHbUAgf5HwMNYPlU6HJMx5VLhzJXO3CHe4zVjY/EzpXEhPMWX++v1P3EdC2svcO/sn23ytMCkhAxGBTMs+YXezaanqSw0jF+hrBsbKj1Ce/7J9arogE79TVvVMUMh1gTlbtswOdVQahJnonzxzzUyEbVLZFpxlXijqxDv1ZMmh2auKmcgMVaDCl4959gaHg0hKK60lUurM0TMRV5EvN/ZHHw77bdix7Ayr7DaNLJafiIjNHKRT6eBlshZ8Hd9CoLaVi2e7zflwtvGznoYhRdAB2UWi57sdue8t+auPNhfb8fXj+saiOljEVRMue73aWVuFk7Xe3At7kfca6dMEZBfc+zzRixG+NbiUT88m0RQ5PBDpkOtlDIHDUbM8am492HPzehHSneX5aX/j7jIPWQc7dpc2mPvucuzO+qdfet6+vnz9z9ya5jRKQQUruoMpeU5g15QgMHGX9tHchyl8lXZvzq4lp850+kyhTgBvKYHgCCHDAogd6kQotu8gh/E0fa6AqAuEBULuxpNdGvG0kOCj6XaeU3aDsBloUqeZg0oJ55NSY+o2CxBjJQ9awT4MYOPJPIS3qfySVeTAPKU34pS0G23MJszu34exlHg5V6oUhJa1XG0psFMVvnXl+0vPxHlU05fRFMSuZWOAXc//TLLwGe52+OZZ98FvfxjePnq2GXQ0IhqdXijb1DqTCHWjvf+i+/qTDsDxgm6umiD87Re74/325kEVtA9Cx0u53Kn5RNUU9URZUWHlbpUcLg5zdXJzH9Lzb5wtDpu4EgJVtZR3PLbx8A0BiENFKypPj5vHVg7uLPLH9gumea1knGJWgRiKkepcjZW6dHryXjaO198MoxL6SrfgM3dScOTZlspmEzV3gN1d7t+tUpdXg6FPtjXbZe+Ve3iXvdNwmfx5z1d56JIzscGLnVNyGDEg7l5YpBnzIgWyIbmHSb1R1ExTejeCu5mzuau7ktnMmVmJolpk6SVvUsbi8Y46LRep/DJD8n7Ml9v0/KqvAgPeJ5tg32uscWooPMbQ1uIGEQribSt1wyMhq1b399rj1q9n6GbEEjMgJGrspQcms8ndi6O0d/fWZ7uL99al4VW95moIZNm8H6xPU1W37vXh2fD0Mp3vNAS/fxwjW2A+XIZ1r0PSoqMoGGZxjGAmYWd2IbAwT9tO3N0tYbdOcS9Wjbzs7X1OaICbzn3fdAsoUPF19+sW0l5mx/LOY4IlzIxovmpTJzdhai+70LkmZp/DGK4ZqfmDK68vIAI0WTjqWUY+Mt70yWFOUMOYxiFbW3EbZbvTIfUkTGfKjZCQC1jYmfZWbYyyHjsCpQBnuPAiA2oJ8D0RpoKKiXuO1Ih4Hk24IfAIJ+SoiGyMljkRHC4EdoWwkykhbFLY5GI+6yCH9aNtupzNtl1W9esNKXAHk00KllJacAyy14ZtPxDTqg1txWquDHdk983lcDOZE4ytmDZDZxzGCeaqSH4NI1keNY96R+ojqb78J6fjoGMyVWLyQGAhKdinuzmNafrkHC7gZkE3D6ujBdh1UYsa3Tqot6Ov+zznbDJIae2dSuAgxcyGy1zDJx+edt94/PDNn3ztzv09kmmca/6kpwB0XWfZLD3HjM2jRF2n2bbYJiCs1MTlT/6RAD5V9G7m7D7BuaApqdp1A1puecls7j5z7QR1C26QQOfrNGQt/xE7x0Cx4jqKm0ehg2Xbj16xcELaGQuEnUG860hkYXnXpUoYDGI0McAQTPV0En3koq4JtL+sI5OI1Szryx5B7txYdq7P1p04mxsFqpzhXtfMTL27DJny9CxlV83Y9CmpqXkBtYRNbbZVnNqMySRJxI72mq5PeQq3HgQgMriTB3D/4W71mgWhcx6lkspg5smdiVTIBJycMzZkynSMcDvFZyfjkLYnz3cfPu36nauVe4CKEIM3ESFwoOnTmQzrCBl2emkMfObeogm8qAWgZR0f3OT3n3eOyaWtJG8hiOAH3ryz6frDvcaMNn167+nVxbp3pTzm+rilJ8O3fv297edfe+Mzx1UtxdMyOBu5zT2V+xRfX4pQi9EZYR7aNZ93zBUPS/freePvQ8Km4KeAFmsed2ct+s+P+EVO+bZAZ4YCpBcVbAhBRMTcahKfO0Zh7K8WY8pDSqtl3Gur0KeULQgzSx2lityP6u7uyqBVWxlciMZRx6whUiTBkJsYDM7ZInMwjP3AdZSKMnnqNQbTbW6Z07MOQdQQmZQQRDSQkB8uqtyZuatZUh9Vx1H7MSd1Aju0tOXm5laIdCG4lnKUw+2DOqv2OVcSQuAx5aTlmgFEgdE/2cij7d3D1aHCOZOzZuuSEbC2xHWIanmrLspCe3t7n7l3+Obt5re+/PB//OGHm95d5x7LYQRNGDOErK5RC3jywYQaAFQRP/hGdbyQuuJVE9qKifCx2+073xO1VAjC48PV7cN21+c3b68OFvHJGX/83koNp1eDmu26weBWJgQrNJnf+53HZ0/Wn/iRu6s2+KDHHroWl+Jskwls6b7K8lgyBCKFMXEuwrxCNhlVTo37raq+GpIbaaRzzxkgEjZn8qROCk7GBlXn3gzZFRQIbZGbkk4x0NhpYTSYdTn3bARKScNyGZsgRHFUBVDHaGYkHkiWrQwpaDYlX61quEvgSviv/swnP/+LfxHvf/df/ov/ddGl4g4rzE3kbZ+LmQoIC0gQZuL1jptaKqGsXjbVt01c7dVCtO1HFjk+WjA8G2W1CUUkyKJyKnspLKul6ZLZkEzNCVoob1VXM3cwlWlNLzjLncO6jnK1G4Rlf1mlnPsRDNdJSOfkcM0xu47DgjknGtUi0WrZdrtxe9U1FTljWI+14Hh/6VfjRbvdDfrtDy4s5cMaqGCKIWFUZMMIsCMIdIBFNNWsCCWY49Y+fepuu9dGgFaNHK/qdZ/uHNWvHy/W/doNNw7av/DDr62a6mI7ENHVdnzjZmvm/ZjV9e07qycvrnw7WjYdNRM48M2bq4dfOds+2f7E515/87C9t1edbMa+H2nwOkqM7JGYqXGqIl9u8mtHqyhQYN2PvasZzq96GWwvyM1FfLOpz7Kb+7JtH643J/3YVNJwFJKT9XaRcFgHd7pYD2nAMOpxHUdS62V0W4+DwYl9EaqGZGnYudug266DkZsFZoKrBGmFnagOlJPHKgThOhDBlbiKqKvA7O749IMbn//FXwWAt/DLv/IP/tU//Q0w9UMKIVSB6sgHy5gNEuBGTWQC2laqwIsqgicETrMSoa2lH0wCV0xqntT7rN1o5IiRmTmlnAzqPmYbRh2y9SmNORdhuZuXTcMFqXNAVR0URO4ctasmrLvRHKs6hIB+nPsUONwZxT7H95aRGCBPZk1kdajmZInYia0KEo9aM2srBvzFxea9Z+vTs81eTXM6wqhIGWrICdmRFAmgBCKEMEGBRZjwfD187O7q5qoG6GARln0UkY/dWb7/fAOHwL70zWcE5Jy7IRcZnKlnQ1YfzQV2sJSYfD2OyG6CZVMdVNSfDF/5gw8efOGTe0dxuxle68UMy1hp4n6XbuzVTUBFsdLuwXK1auLj03VI6hxhNF5uTWGsENakUPRjPl7RsYWLFzuINnutmR12dtCGRRu3uxydFm21JVosw5CoHzz3eZn93q1VYJxfDXuLQAIeaBWXJxuHez8iFIl+MgcyUxhHZ4YwiRAxB+blSriUXkKR6W/+vb+G63P3ny2aH6sj55rXgy3bikyjyOl2aKtgZnttPFgEQvvkogdYhB3eVAHwXZ9ePwzP1qkzB7iJ4kOunBCoaSLDVZ3BPZCydWPus46jDknLiglhciIhmPswajYXAjHqwHeO2mUVt0NK6pEpxlICQ8jSy6tWgFkz17apAQ+V1EFYMGTEul4uYoxETsyuakQUA+XsHz49j9AYqHBsIDRmY8J2hBD2ArJiMyAZkoKoPAhwYN351x5tYgg//yN3P/HavoO6QR+ddfdvLffaGNmPlnK8lGUdlnXbxBCEUsaoqR9tO+hVl07Xw8kmj1eJVF1VAvtuMLMAXF6k//4H7/Wfe+NwVR8tw5DM3PqU05iHiCzcGAWhs4v1k+TPLzYhsiqGLqekMbARX+2yPd9cbpMJNvlye5Vzdh3ymBOBI/jUhufDsOuUHQG67VMnvZAMo0dmCdRWvKirk/OuT6mOsVjULlsRoVWW0ESRSEMe1GnVRECqyDmnyOj7JIK6ik2kYdSq4p/6oQfYO8A3fgWf/ofACsAv/aO//Dv//v+Y6pAd7k2I924s1WzVViL02s0lHhzgavzgq08/OO9P12k3pv0ltS0/v8hXY1ruc+rT5sosM8zWXcrmTmiiVIEYfqY6Jh2z5pyzmhrMTDgwURSp6xACV+bHq1YCCdHhqiJgSGlIuVDGw5jNsenGbhzHRMTEQkEKy0vn65EFQuTuvUjOpoCh2o28iN42JkZVFUxNDc/Oh2fPNnIN1M0IHQuaiG3GrkdVoa2AEdkgXrgwOLAdcHKJr3z3Ipv9whfin/2BY5h/92TDoDpQxbTXyEEryybstVWU0kCYuQQmJi3ieNUshGDZVRmyPr+6xuufPOu+/O6zn/2JB8f71S5pzthnMcQhmRDcE0jPtmnXpWRoQhWDRPa2rrs+E3m9iD08NsKBzL2uqa6qrA5xIyyrZtTU5/Fg2UQhz9424c7Bajt065DMlDh247gexnbBEsjF4TaqNishd1cOZlo571VNUtWkKSfN3EaOwlXrQSRGaiMftDJobOr957/2xX/9X94B/+4v/vxn3/q5f4ODf/LnfvqXzr7zoo7MhKoKcv8YBzWyAoyGcdjgu6dvvr5cRD9t6bXbR5fD8MHZ5mZDQ6LDvSpkDdGODipyP91QykZMUVAHDGVNm5mauyObw1HHalFVTc2LOlaVBJ6kmOo+jOn0arzcdhebcTfkpHatS/aXej7Emm4eLswROFzsEhjCTACT7ga96sir/XVHbe3LKrfR9qoRns3tK994kbM6eBqKIqhObAyAtkJSjLkAJEgZAkg1CaaaBiR4scY7710Nw7dPrt784bcON7vxW482jy9SrKqR6SJRHf3mvi8rrqPcOoiv1XLR5dN1ok0aefzK4/Fi3a+WDHcb07BTnlyMAcd3Hl59+Int0V5VCR2vqqyW1AfWupIqkKorua6adZ+cODCyCJEcrWJSb2ti5uLiYu6pMTUwo440jBaijBmeua5DDEymdZQ7i2q1qDf9wETJlIkPV5U6fXi62yXrx7gZsxvnnNU4DMmHMYOsrlAJNYECQRimuRIOhDrwsuZVG0/W8Z//16d9SveP2nvH8pv/++t/++f+LfAmPvfJ48+9CXQ46bGMU91rDgGWS3zjMSrG8dKe7d68tWoPm2YTn570R/u1kI/ZF/vLcWHZvOuT1eiADK950twdHTaxCqHqu0HtqqsjVk1cNqEOIkLmGMZ8uUsvLrunF7sX537/9ebF1fDsxPdbxAgGVi3qSnK2IXnhuuo6HB+tmIUIUSQnDG4SUEmIwqsayXZ1gyBKqnDv1Ih8uxufPb8ggDGvZyjraWbmmBkRIEI/AA51rDPMEQOaCodL7N9YvDjtznf+zUfd1e4773z3mMneO9nuLxe3DtpVG/YbAXETwpBVCd3gBw0e3FwcLLKjq6rwhT91+39+5TGZwpAGyxnz4A8AeMYfv3vyqfuHB4taTR1g9kXDQQjuEsiT7cY8pCwkXhzTJ/mMRq6SIlkWKntNvR9yNr9zvKpCioJI5CEum+BuVag/dnclpm/dWY5J25oZFBlOWK5qMPmQ+tFJeEh+se4/eLELmjUIxVDeIBXhRZR+tDETkRFZ7G1dxxtKY6IqLo3bQXc//oP3vvCTb7z4tT+8ef9L+OwvACfAh7i9A/YBBS4BBgZs1oiMwHh89e7ji/s39/L5bjvYw6fdOKYYWM1U3UHdmMdkDgxJg7AIhyBn69EcoQ434rIA6x88OV81sY5BzbpRLzbj+ZVddTAFBxBw43C5XNaPTi6TIggWLe0tJGXXmSJn4NbRwcffOBYWEAJzqcJCAIMLbpByyupuJoEZbE7meLLdpVGL647B3NkmtBIonzSDGWQwx7ADCNmwdtSG/QWCYBk4HlaPng3rAeFS/3h80S4kK987iMtahJANQ8qXXX7jzt7f+uXPY5d+/T9+/fe+fRoDG2hZyQ89OPjuk82T06vAtuvNCYy5CjQAeP/x5qvvX927vVLNVSBhDoGz2ZAyHEm9H5XIAwmEmYmdqooM9GI72sSj+pgzAYBUFYGl00wil7u87cZVExmo65h1+70nF8S8v6w++9ZhG0iE95fxhqbDRdj1ZuC9/brZjwdYPrAbQYR5qlY4uY2jAciqcBLhLmmfTEEMF1DbDnnkR6e96T1crTenT5890h/87O/BnoH3gAVwiifP8KzHdkxn2/PLftPnbZ//8Dvn7vzuo+3FNnXj2A1WiCAi6katIgcpBB+NWamowImGXDQUTsSBkUw/fJ6ZciCwQG1CQfdbqMEBCThYVberxdf3LocOVcSN/QggweYJZ3dgb1kTkDWbwcvzy6TJ06hDnyEUoqjqkLSKIco0/HVx1WHeDOde7hd7wUngJEWpWrzOC2M7QZsO7C8QmTmP91ay29LVzruEPjonM6c+WRWkqXjIlh2B6Gd+9B4e/Cyw/Ct/5z/947/7327uxUUTD9pQRRpzdncOlBSYyGhUDGG4wzLe+eaTNN4MkWMMXOyOhHI2B4ijQ6eKidkVIBeRwKRmptPe0SLij4GHgTbbAYRTAojVcTEkIVCy06vucpuY5XL0XTp3VQI1Fbc1ByJ3S4ou2+1VXFRcRQlZ3T0P12SF4XzMRVUhgc43aTMYAZozMa/qx8s6Lhi/9tv/9/e/zEI4W+fDP/oPhw2/fWel8IfPt1/7YFMFqcQ3A8w95Yzp42SAzKwfUs4WA4kwE2XzyEw8DfNlpbaWtqn7fpTIm77P5hVzE4SAugI5hFA0lQV0dwIpVLFouK1k0fDdW9XJ83FRc9JZNkXEROrKjDHlF5e7EEgIA7G5C7kTxWS79bAZc2yrumYD9UMK5ERI6qfn66I/MMCLueEsYihTr/Dp6rujErzR4KhCG7GssDqonmci94M2vnZEfe6InEW4FAmBQ2RmJNWuy2D6d//5a6tf//tR6PHZNmVzt3ssyZ20aBwQRLKpMBTYF/z1B7jd4nKEOzrfnnXt6As2JLMygwNicSNRIiRzgwkEE2WVhCWbmVkMwc2FQUQdkjlnzVPAZiqVhgQmSmXJzWg+ptRfZjcIKDBlNWJmx3bUNCrIhEPOCFebIQQuHKmwqPs4al1JU8tml4Z+WARxoKorYo5BVEcieX6x/uDJUBhZYQ9CX/zWGTO7u+ok4AI7E6ecy2BxUWQKExFVAgCW1Mgd3I3KUtZPC8G6wboxjyn3mvsxqaMSXsQ45twETrlIIx0EVSJ3JihghqYJ46ia9XDVXF6Me4sKbn1WVeRMo04U6bbr60jtIkbhvh+GMVVCRKiFweygTZeHXDytXJmFaUx+uTEzz/PY2KRl8ckQTBhmUENSjIrP3cDfeBs3WgwKd1yM42+eUDfKRWd9yu5Q4qSeFWOZOwbGZO68S3Z7v6krbiJfbNOu9+2Y++xMEgLtLyoChmwpEwnqCBCi42SN0dAlOCErdnaVDmRLLERuPpoBEgMBmYoRBIE8G7krmX8EhmSFe4jBdRqcMzc3D8xgClIUrpSTFW1RzsoyjSiLEBOZMwgCylaM5Q0+mjvd2hPmUruXBAVXSCARGkd1Iw7uhjInTZOFEUnBKYsooigXGfM6lEkxQQAxmfm0lcIme6tST5S9OFMMteLg7yRMjqJkLqtxinENE4RI1Xe9W5FmM9RmdUXR2AGt4GAlROhG33RWCzG5GtRhk+s+iHCw4Bg5cJGSQNWFp9cp8wHmZRcxzd4hbkYnV3kK+ZN2Yp6UIMBf/gyFXr0RcK8FAWV7rBrWGSOjEsqGPjscjSAKZfeDpSxqcbgZumSHi7BqWNWfb/IwUlKNQm1Ny5pjkA+eD+vOMpBtUkKJ+82AKEg25W4naM2zztnNrmWs0885y+nKX/vsQeBlqCNM3Pw8+YtpfkOEGFCH6aQqK3ULFav38</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9WdNl2XEdtjL3me70zTV0dVWjgAbYAEiAEglKFi0aEm0rLNlWhOQ3O/wT/OIX/xw/OPxmR1ihMEOyJdpSOExSJE1wAEmg0XN1zd9w53uGnemHnbnPbf8ER1+gu6u+795z9tk7c+XKlbn3Bb5+ff36+vX16+vX16+vX1+/vn59/fr69fXr69fXr69fX7++fn39+vr19evr19evr1//f3/Rg2/XzFAoEQEEKKX/pT9CiUihrCQEUgWxqhARoIC/HVAQQf3fIDAgSmAlBUAANF0AhPRhgoqCiUTBlD4LQFWJKF0dgL0VUIAJqv739AsCkG6Zhno0jvxGBY4eygaSnjU9BREpkK4CIrIhwJ4xjcYeUhX2V1JVAoE0TxpYIenqBNGj4dFXhqz5DzYCBchvDCiEiFXtOUFA+otCQYCQ2ryq2tjtkvZW9TGoEiAAKZAuz+nvNr9p3DY09WfJw0qP6asFwIdkb02T1qnuVTttQqCAIYpqGo4NXaIW/8E/fRoaJgWYSAkAKAIAAhEYUJsmBRg2yWni7cc6rhmBlKAA+wqlITHyh8jmJj0+VG2BspmrKgUgZisCCHnN0txAyKyJxwmDEHGyKV9YIgVI7REAYqRpzaOxRSIApGq2zVBwnldOtmSzT0rKapYLsHtFMnJlv2Cy/WQFBEqOqqyk7MM3S3PzsDW1OXKjY9jkp2mAQkXzKpOCSCMRCQhqUKCkpLYEybnVXI6gZvY2A5psMNk21O0UJJA07cw2M2lOk+kmQyJRkCjWUb7cxyXdm06LSjaHNkZVsgtCtBtiUU1C0RSUcMpmP6QHd9ByFyIQiEjF5ietgQDjbCkpgwREUF8os9/k4kLEaX3T0yaEsCcgZG9KF0gPZcaqmuYfUAQ3kYwSIBQ2X/b+ZDBCaW7tSuQgBBCb5ZD7hKallwQtAPn1iUklLb2tJBsOMI2G4muZjNbBRuCPduQpZvgZOQyIic1v7YlUEQjqdgyoikINvdWNn80/NNgUkxjumEUehwazNv+hmhMfuVkCKUfpI2AStggHSX4rCohyD0yK4YBmwmWgqMUQB1U2iFUlZkbyerJpSEbvM5X+z+p4g4wEpCAiiIciApgI6ZntDTbrI4aD0t8Mfw0ZwSAGGCB2/CKQgtNdLfaACGSj8B/6aN1EScjnzmyO2f4AJiV/b/6ozykRQSld3u4TklMRGZwE0gCwoiK6IJ1HLUUDbIAEdQcawx2MMgS3WHGLS6HtyPJgqKgWjcgf2XGcjkKthy4nJGQfoWxXaQXIByJANq2Qpyjfm8gXFh5hzSTYf83mpsnhjxiKD5QDhzQkYiJlH2JUAJDCYh1lb/SZVyKCAGweRn5LdcsSgEmT+SRUchZj1mWBOD23ESQSgIkiIVmApIVNiChfYUJijuxBBWCCCDn4pLdpNjWH1AxAZiHGCTzQgJx1HOGE8y2MEZwYqh7xoaUigGbQpsNJN6x7rQL1LMtAkbENRCUiZRwicvdy5uMgSx4qYOBAgJI7vD2AErER5OwzZOgrHkWVBMrjpUA59Blkmi2S+TWBNOrxipudGFyY7ZMzH000UeEknAxpxTEHTlTAJEXBlyfNfY1vVvvl9hCRB4bCAw2Rr3JaTgcM9nV2kwMUDBUgwCBKjf54JMh+pOYBBu8+GwpljEx//KRC0vKOlm3cN7ENAeBsL+OB5vsancp/HCm9qgLMzqbTWog7DzQZVHoWt4Jsw1OlC9HJITYDeJC2izV0ehCCbkUnVdFPwg7YnhSbyhaObILd4CwBygiT5kiNLTGlIJwCM9ngVUHgHCCOubcvN3wa/SOUaL4bdA7qntYIGIkpjklVpgMZFWzZNM+x07vslpR/DKiCRWOBcDqtf/m980Wgn395/WGMbdQuyiAKaJGXM2WISAbsIdSfiEHiE2+LZ8HboMWDquasicc8B0jeqTn6ui84r0lr7OiTEjcSAzsoEJPFG6lL3ulvJZ8aOrLUNA/uByDWRCgBeMqc5hiqnqdkbzHDZQYKyHuHONn0cteul31gvpoGjbi9PZQF7SPt6RBO6+qkDKphhqGggbQvCmG1IcDTiNElbH1SnpVQjJUNvIDEHzzCqP2ANU3IUepjBjVGshQiyYOCx1NPpyn5ul/Ec2oiS+lsFpyRUUrUEjs1r3ALGBGzj7HrMY1oqvDwYnpR6HrZvKp2636AiihIqcA404SjGJI5pB55BTJphhLYfIQM6IhI5UgRyNzSclWLJZSzGoKqEAKSZuJygk/LmIVJvlpChmwNNtFKxKoixBaAUzprsJQXIiOnZLKeYrk5JjiBS3pXQRpEJ1GLdYtI282AfXx4UrSr7u02BqXtvn+9HSaTAtuhfVOcXtTvzmPbxedR9vNq96CRWWDnT8QgZ9zkw7P01/QU8y42omaSEEHNVcCSJknN7cfIZRZpKZVxHxNd6CjA+YQ6BaQcmym7rAdeu74Nxq3Ep80slxWqkYYhdgPv2+H13Z5LHHbd0EsvOkjKXKTI1z1yD3EmwylRJlJFIBJ3yYQSKQkwkoO0eInUJbZhDpWMUKsQFmV5iMMuRpsUKMAubSU/dpmIyHSolFjJGGeT3QvB7yF+KZ84/7PfxLQjjzyeNMAiORRErEfMmaCl0mOlyV1ftcNpS9vlXu96iL69O2xaWR2iipDovkcfYxx6hPDqze58ErSgybyidRe3Pd6dhLNKAmUlkk3OAiihE8YREQHCmR6a2nPMysjsi0FCkoKqBXr3R9ee3PSQc0+ivMRMELWpSwbuaAW/WprVZMFpMOoXNWS2iVJQwToNZVnyoYu/eL5alrratLtBtl0UKEQEKOgoMf5KJIOJUY4MMsq2Lk7ZnRQgGTMnE8/SyBiQZJffmE2/ezpf9vFPbu62Q6cjPU4XZoxG5oHPQ+xI7UbYN5xwZFIldrWAxglT8b9aYmhJr5BrfK5hJPULKAn3EOp+eLqO/fPti+sDN2WOG1073K676z2mJe87nVRhuem2bVzMaHuI13e7i1kzRC0uJsUgzTp2m53ea2hS2LOMYI6chrMzj+NIlhmRp9bkhDKRpkSvPNhY0DjKmzJRI8/4wY5W6otkaGoZh2UNEFUmFlNezAItOPE4dE2QTMpMHGhSF9MqHPq4LarY1FJ02g8iApCqFPYohhbiGaySRTpnEabmJc4zZoFu2QlmjtOr9NgiAIFLoqum/s7Z4u1h+Gi93cYeOublzq48nzmiH5lsOm81wCICSBTExlbzy0jhGCSQEcNsUIWY0qKZTpvlAlZ9tI9Pd7q62w87ef52t97Gm1VfMR0G6QV1wJvVcNdRV2kV6GbddTKI6OdvD1EAHWKUt+tNcze8//2z8za+eHtYPd+VHyzorNGQgYXJWZrxFhuBIa0/aHYFhxI4U0gTYharcF/JKUAiNsZRMtUw9cctyjzQkyNjY8Qpf4Fb2KjbciaNCi8hKQjMJGXBTV2EiptJTazCEBUCC0WACg+RZDq+RlAwHEkkjTiDnVvyES6bgYhbyMhScxUFUFG6bg+fbw7rbtgOg9tEcjBJ9NRnDNlDXWF1fATMcM3EmbIvU855x0TI8cHSVTIPSG7CbFlteqeCmFUn/VB8snkteqZ0u2o/e9O9XnXTSfHkom4HdFGgIYLjMGx0qIvietNt26EKtNypKk1qbNttHzHfDgAeXzSLCqsuvl13Z79+VV40YFihyMoC8KcVTxDIn918JlMrzmiM4+IQkWOM2RAIKgml2TgGOYXPjCyFb59LUlHL/9KUMqnAhXZiiNtUivue+RpBEYVywRwCA8QMDkx2cyJiSvqZqb85NAGe1BKcgo5BHBk9XGv2bNOLSV4tzI4IDBo/2ezWfWyjrIYOEMumodkwDC3JM0/NVuuiByUSkmUDRX54Iq+7OiyOBgqjf+m9DDPqkfcac5irfm8vpXIJGvqOFP0Q1+1wiLo5xO2ur2s+dEOMNIgcOum1P52GknnTCghtF7sIiSDSosD6bv/nt/tFU5yflO2Lw/asPjurU2w363Z3AaUhIvvzV0qsABGmRXlZV/shvj3sxb1jhDq4WpSu6Om/aWaeDKWEDRDYOEbVNNlnYkia5DAd5QL1lYVTp9G3QYhKokUdisApwySEMriiJVDSIrlyojeOr0l5hZGmkSupu777YbY/vzXcBIzNHmnjvcaX+71JM0Sq7Jic6x0M1lwXOrZonzwZ8/c8plx0H+XvUUq2tdBswll0Nm7kb9FC9XIX57tIhLtN1w/Dq7tu2/Wq+sV1WzL6XlrRSRHKEmWgTrE/JBlT9q2K6qCIrRAXdSmbrbD0Cry+6y7bataU61e7eS9lERxU1PmlJg8lIoURc7izJqW7ZP7hxfkvny+u9+3vvXr75WFnfIugalLHGAVHG7SMw2fC1UunWpRRlMaPaJK30rSpR6UEW4YNY8IAG4AWxE1ZTKuw7eO+jRIHEYVqDk1FIt3JrjSLhimLZZOekqLo+kUK44aK2cYdAdN1E8mLWWDNGAlHeEAJKW0kt18DY/IKqWbbNmOhXK9TZHqL44myYEt5JORTphgB0FdB2eBbUYg2q4F22O77z97sPn2zXx5Eoj6/ids+DhEyoG7QD3GiQUSiaheBQ2SSPpICXadtJNYhCpFSNwgTBsHttv3Wu3x/L8PbQ/XuLLE0j/Ggsa5sFNfUcEdpqDZFOK/qR/MpE2ZlwXsSF48cr0ya8sDnIpCnbDpyf/+Qml3lhENTHpo+PLLt9CdLOWwZEuQhRXIOSqRal2HaVIdh+3bV9kPc7zs4y2NCYVcxP0qQkNRDHtcZrsMY0jBoBJIjjSWZogABlGK/qR1ujumC1lVhpWmzQhNyTVwdc4FsEN504EzXhaEc7d3LLBnJxNoiVcIw1VEaOhIyoL301/u7bb/c9h+/2q/2fTdg0wkIMVKMCoKKThpmwrYVUSLWvkcnFEhVVQQSoYQYlYCo1PYKQFRf3ezPT8vJNpaCLqQsyqZTTTZKjs40CghsT0zYD/KL9Vogt233at/GI1WAnKNm6glwJm+UVA1ronHzO4qsWc9UIMkcPNbnyZMMAwFyBQtk6VcicVEUCg5Ul1wEPnTDoe0HEeb8OSo8iHjEgbKZtt/eB+crSRbJk8WYM+XImulUCkvpzfn9AAJcuMAxwpADWWb+WexKpqCjpJnuQSNEHREezVTHyQSnvhijfcY6c0EqIaVi0sb1692z6+7ypHm16ld7IeghSh9ZoYERDReLNsaoNEQJqsKUMncCk/d6pZ8wtI9WwX51LZPT/cWyD1G1OCIhmc07DVEEghAsIKap6DV+tFp9ud10Kt0Q7eNHnpuZV8IkjIuF0cJSSDGqBnNAWLDygJBiqWuOZmEmM6ohqP8kSRaaYEPLIkybUB2KgqkghCSWJDUGYAZ9hbmb+QDwImNuXvJbJQgkCsBXUma3xQTPqhAHH1GDSaPwagCc75n+JGPdcyRb/rajYHNERNhB2G0GCpCM11aFUJIvbfDpkQwSyNANw0EkKgL99Mv1q5UMiqYOl/OqDESKaUNNgSjUdsMwSIziaSJEdIjUR6WgIago+gGi1A3oIqIgKg4RqyHeFNoH84/MdXOq4q4hOvpg/pVGlU3s+xjVvT7n1FbScioPgFUBUeT6qk+Rp5okkspLrMJKDCussnfdOLnGkejozN+yVyFOJQ0hgImbuqjLIhAdhtiLA5lHF7ZisnlVUjUNGp2l5rQOXrvRUVNDDpyUUlkvGlCGouRAnvR4jDDymz7PWTxyOB+NCqOx+7g1dbHBc2vKyOjxyG00K42GiombesBPcSHF3pKvWyHo67vDchdX+zhEWe6HYZCyICZmEAFtT31vHFlTydXpTRSIUIzoBdtW2yEBp/GGzVrfvDnEXrILWYOLDdNLO1BShioJZx9wbS/1TEqaM3YyQwAnSmU5lgLERF7ysCDNBAJYESJYiSIxwEpsdwd7UPJVTkYcMlMhInZaCWK1SxIREWlgKstATP2g/RBDchE3ggKAqHDq08pLzd4ki5xcc2rUMYlACSSWtGRb8/+MaoODNmCijgcuE/5I2ep1aVRkXM/sBIkCcA4sDO83dCRIoDQGfmQqltMinzJOSUkqi1nWaUI0YcNoy7C8aZc76QZhpvUhdh1EqQgkg8SIIcoQiUjZqI/KgKhKQIwcRRQaCFGghML6/BCBglE0XM4KDuw8xCbKAj/pSFQgOUVMfZokZPTVCblNqnKOat7+4FQUxGykgEwvY6gJYJ6As10mxRfP5dwriaFijc3JoRxHSaHpt5ZJEVAUXARikyLUUkWBMjEnHkakkBynR2A5RqSMLYbQkoMsPBaS9xmojSyARsBxGcEIKFlOqCBmvxsdKSGOhGwhJuuRxmlclbBB8GjblgAACE5MvCkJRMzkWoKan0MIYVGW3znZlASiRUNl4M0BvVBTaBMkEFUBIaBgKBEHrksEReqEh4BJG6aaqWQuCBUbzNQFBQbXePSrl4+/d85Vauyz/ov02KnFAiABJSaQ2tGUkFrElW19zUCQsJVAYFJDf/XwmPlJioEmMJGtS/qHFMRWkcpNQ55mgggQIrWCaQ6etnJGnTXHO4GAAoUihMAqUUQMpAElVVIuHBXYZYcMkrnzfexIybhlylfmWKlGbIXhPBbJ4reX+jXZmycW6taP9PDHrRxW5fXpczk7cXtNkO98Ng2HAU1VWDDyBgwnbQxSn6MIr8KniSIEDTJ5NHnn+xddp9uPNlE0sDYF35/zpCSA2ojb3bBrJap5RnqOGKkIqAIHEg7aD9h2aBV9JCPIBBGU01DUwZdLs2wG73KyZyalMbVh71geRdY848nDdJQBxC3XU7Ax1DAkXRvW153CLGlmqh4nXVDy4rbXnNNi272cI3JO1qDCAQUTEwNg0KBQVVJWFdXUT5uWfPxQepCklB0rtVmjzmkv0TGpt+p05vZpwZMRCI/VBiC1lxk7ygJ/5ltHFMuwLQ9CnU+qC29wS0pRIfU0WIHGu6nY1zFhWXAsNKqbMpWiClfvzqo37S8+3kCUGIsKl7MwqzhANz0FyLagQfTQg5lQUMeqijLwpMQwAMxaoAh4u1UVcIAqaMpXj+rJlIvaJsemVZ2Y5CJ6jqgmpoo5ApFvSLAOKCTm4YKkkwhTvxL9z5JXSvmSRyNJpRaBcuCwWJgmWix/FdPZLFmyW6mkWydIUiEpAGYKRCFwCBQCCatGFaH0DCqwviDPXrOQ5sNPV/RcxrDmKDnFaFLktgqzW4LvUgFnCZHTY0lKXVLJwfZ5+ay4Tga3CzUxxUkXxn7wTFXcrX2klKUekOZwfJzkUn4Gk4A7FRVZr4dA1Clq0vmE783KMghpMWtkUVW7QQ/dEBUq2g7oI0GpYCaWfYshqgaes25adKKqUAGitut2v+xUXOpy70HSv5NUaW0b5MgvMLUcaW0NXkRoVFfNOCHWRkejeYnPun1aNRpjB0xiT+ghLgv7TykFBoAo0yNNb7BWelNUMttJkjIY6rs8ONVvJMETUaEKdYadq6V51cwAAdvSZTw9hXwLiAxJUGRNHslWvJZPpNCgiKAjHj8qgCNTN6tylm80kcjLJ4Scl1hk8GCaWaIKlP0juVYgjhp5Zow3HiUPpKQx8KYI08t6NuG+jVGJSYsCizIQhbJkmfIQYzuEQbA9xFUbu0jTghXUD0Mg6nuNkDZqYOa0fRUoW9WiqEqmqPA5UgZptE17RypinnifPRJvvfQ3qNimv8wyOMUEe+yvJF/Zl8QMIYckJHrj3ezJpnOczCzJwUR922eedi9aINmyRBmGvh+iiEZVq2SmawctvFkMHo0zF0qhA+PmBiNTqT9H3CCTNpZJBByMM9qwyyVwA8kkX80ZXYW2Bc8UgcQAFGagHiVz/IFyHkgCMnWGc4SyJvAm8LOE2SgBPMggADI0fPrN2ZPn88N2BWggZkVgMGlBxAF9Sh0GXTTlIELQSYWCtAtUMB8KGSK01bqQgtELmgKnkzA0vGjKsrTE0hVjZ9cpdJJlUga5agk+59BouHXcopu2tYqXE3xdjaVJWqzjjcKG39bzlimxpoQs14CN71mQtgky009w5luQgCiqCrT9sDv0bR9jlFSHdqfRRcOFkWYTkdPqaNI9yLZ5Ud7zlHzGcSI/PTx6ZZAlyl6nRx6WNjtZ8uM4ImyVEiiOXM5VyvRU4igJFS+MkSoxiR61aSLzBnVqbRhP5CCYCCxcQVeHOgFogIaDVHspAzUlHs1DHQxLWKksQ6XclOhl6Afa9RSY501gpS4OZVAibYGmxPmEd530PQIBU23Oq27fH2278B2XmWakXrpxWsgKd1+h/YYwGLkqG8C4tosjv0lbaSWh4dhDYKKckqm4alN0BFPkNMylbVJlUhEbQBaaU1EAgnaQ3b5f7vrtYVDXp5IvcKB7i5Jz/PKnMAo6LtkR8/FdFeS8htX+beaVVQlQSEKkwxdBk4H6XkLLA8yU1SVfVXZhVaFs8sc4AA+6qdZuhs1u5Vlps3uoL9pRkOajSfXdMWZ+IiW/3Ax1HO7N+XJKiwZFSL+nnsAQZh4GZaWSaVaWdVEE4m2HbSdKBOIIFqWCcTIhCEqm6sHkm79y9eB7F1o6FQaNumTaUEmcCLjFqDGZz3pYSgytnEmsgKQGFowytJEX15+dvSklHSpjgjrXzfKC7Z3NjNwnNKt1X9n3YSoS1MvSAFNgBQ1RiDV4mQmkkzqcTrgwvOWjwanLEcjN9ClwC1HAyGuyUYlbkoFILgADkCQmJm1YoJR1V0KWbZDVR4Ai1DN4z4GRZz0nCGYv1vDhqG58GSr4SkKaQFmVR783QwbrER0Rpp60KkIV9HSqBLo9QBIMqywaqUi6KGT7xFVBqza+3sQBJD22ne4OsQCIcNbwaoJ2ELlpi0mY3p+kxheiPK/GwzPij3EU7i+UV9cy/tQ5ZEKRv8kNhqzTJwvi7uMO7SlEkW8aSJdKBE9Tf713pQF5K4z6Jdz9PbanxSMmCoEXk3JaVWVZlqEASR+75ATTkguiwpDMxkhk7blpk1+ajpxu00idKacC+XGzDiKa9mBaFqKCUZwnrzQaNTI6C+crdkaMevqbsdZN2M8gcUzPAGuBd+ziwjjVxgE4q5TWM+dBB6RErKIU5XC3x4CypGkJ4rDadretthF91IJBoAA9bcJpQ8uDrFtZtbLa6xBRBuWURjPOJhwCTSo5gKYnlRKjYKXEqLKcQmM0NDlmZJUW6/JjJETzeTRhKadEGX8MbMz2xn+TtQ9nPpSxD85RclYrTr4dUzR91tcx/YicFWk6TKAoeTYpqpKbMkQBDtCoFDApWcT2b6asDCYrkxy5hpMaTWsBHQsk6VaJu+VVV38O8xV7MiOx8F/61jaX18bHPRKasxtl+SZ3s9H436yBmV9nCEROTLJUogp3Uh+K5afmScT3zprn1aEKXAY5qQuN2vZt7Gl9kNu9iOB8ggnrUBXr3fDF3bA5kBJqBkQRURV0seDTSdi0kaFowul7s9N3pk4TMzQn9/DQgEijlJ1TJpvVXBLKioIFEouR6vNxBI2j9JDopxjFHsv42dRy8j0qU6aca4CKUr5a5h5mmQmONQqpTpv6fFHPp1VREPWkgAqqhk/rEIehOAok2SPyannItiYpJdu2fdTCYZ0vJot6WmMdVmSskR2SOD/hV7MGiEbS4AiXnA6UhEfLgzxXyCHZHTkHbGWzLL9IQgjb2OcpvVoA8YSPoC4dCApunsxnm/7mk93TJszrUAfMq+LLdU+qgVQF9xf8vfuTi3n1cNpDNp90UYiakhYN35+Hy3kQ0U0bowKK2bvV0x/dn52VKWiKTQF5BxRhXNeRBntkHWNNpiJJh6J8BbsAiFRMzFcvOkOTYgBJ7EzSPxh3VxlYweKswhIESrU0RHVIldylaiZuyZ5puIr5pDxbNItJSczMEsA94mJSnk6Lt6tYuAewHQJD5Ft9veENKbzkkwc4wegRZrOjTk4CaHzSPBMIarK2g5JdwWfY2rI5IXTmazYDXuQjK1kwRJRTc1kG3uSqSaK0bN/5HB9FUgvXnlpZAkOAMPZX9emPLnVe7f7yRkSagmcVnc+Lb140vVAfe4aeVVwzqsD3F1VdDVURrubV6SSQ6ubQrQ4yCLWdCvDw6eLsnQkFe1anGuSB2zl5VnYILv04+lEef6YaR7iQkdqxjEfynliCpKyBRq2LPB65W7qxqy2d81qDS1ISlqP2PV88DxfExE1VTidFVYbADCYi4oDzaVUE2g/qp64hjobhCJEqEEkEtgg+ap3JVEQ166jp0yNjy4AFTxC9V1GIPMWGaBZ+kcOhguSrZ575NT2QIlMrf2RjaHQ8AEqDVrVg4eHXOYbhdn5wBkiZMK8W313IWdHHdNwNqkAPT6oHi+KkCkyIqiLUDwLIvA7fuWq+c3963rBIP4j0ol0nXdTJo/LJD89DoMxqfKuIeASSY1dUJ0p6ZFKenjk9sQgmifZmmSHPnah6MDXoEg/B6QgcsO3vN6LnDR+j+dhGLEc828pNlh5myQlmZKRgoqZiKotQMDMVgUEIhFnNMcpyP/AY0N0gcgU906FMWfPUWA5im3vNwsjhxxffoCo/wdHyZxpgVpYtzOrzmvw6Ffh01KXNIo2NecCxlycqHhTGfiEvRvsoRk082y+pqipEwaoU5uXF96+6iEEkikC17eLu0G333SSAiYvACp5XfFJzF6XrhraPMaLtse+0i4hRT751evJ4liUyfwC1p8zyi0nrmflYjkUK70PO5N9ipufzecq9NpBIcxa+UsOztztm2Pf5GzHe+Uu6LPs8knM5h0oXE3wuVVXSwX9FKFAQEwrmgikOWlIRRNbb4W7ZFl9RNI/Io0+KGfBXdkAaV/NHtadITpSMg5NXkrcZ0Gh2mZPArTk1WVCeSzN5CyHHyZQJIClOk1LSNdR3xMI+Ir7/P2XNY5zOcg2MaEKzsTm5gw7KAUDe3B8AACAASURBVCCcVhqo7QUlFRy6od+1UpZF22vP0g7dctcuDwOUJnXZ9nHXy67VdRv3XewGEGF23lDwm2jKl11FNz/Lps4+QXm0HkWVTAxKLqsifoylr5evjZ3G5aBvFMGitdrsqB0vgdQSnE5BtHUaz01IoVcybiSnJQdAU/VSYioyEk8IJCoJ5k1x2hArXa+727uhgG/aS0zLU850IAss1XW0smP0coHDvUO/Yj7smBzgZ3VZNmdA7WN3Nkqk3vah1m1/nHwQOYc3u1TLgjPD8rM4ku8KE0k+4Gq0UZi4l4HOS87wqbZVZ+AkFL96VT07nd29XYmySOyjDEBdhBebbtvHrh1ut8Oq1fN5eSW66fpDL5suHjrtBqgocSinacc1O96qGmwo8t4xZDOw5XW14UiAJSKjRwwaGKS57xGkEK9mSVYbDQEp5+PmtyBR8V48P1wnO3IGEp+XEQLVJsk3FJshJ/FLARIViIhIFGkKun/SXM4Llv5uG/tWCg9ZTvgB12VAmvuS1TmnxU5S52MYeasnfm6X5HOXTEkVXhSmDE0ez5xyjZUBtxDXNoGjc13ThcXP1ICn58jryN4P6TqmjwTj2xy3yfERBeFxVf/W2eLvPL7AIP/z779+83o56DDEoVe0yushFiWdFHwTw9mMT+ZSlnxz6FgVUTadHPp0FgdFkY9+/+X508XJ/YnPSz43II3CCKgqp9PsdDwPwKcH42JYKJXcrALndkkflLTlBk4JnEqrJwAp5wbskMMct9LcjGpiDilG/SwTS21C2SBl5CDKqgpJp1WCoBUTNaGueLWKq30UlcLZAJnibyGPnLapsxmCskfBkX+PDNJM3A5yJaT9FCGdbOv4MSpbUPVyp81DIvHpF3aiDfmDJNZg3WTMWbE0K4HmBq3kfJQXJOde1hLjAmHu00zPRvMQfjif/mDSvKvh8p0TTMPyd37xRz97K4wi8ABpI253fTf0pxVPinC/4a6Xm4NuNkMkVaCE9j2GSELoouw63P7l4ef/18sPfuvh9KTmkogFfkaNhXElkPvg/zcIunN5aRtHhnC80g48TvXc1JA2OOb4MeoSakLPsQsnmQFj6Bzjt92GKZ2RaYHHiBalpmKgCISCisB1wXXFfS/7w3C97te7CIGfe5CR3SdfcXQku6qQUtqzRUe3houyyGUwUfIhK4GigY9aeGUgHRKfN+k7JGKkKZRZhZl/+nVqfmLPw9wpDcCymnRsgOLFaSYC5IeBHyn9gdCSEKCnoIH5SVX9+uniHS4XHW6+WF/+zfuYc/svPvqdP/z8ouHPNv28IjB13bA9DPcW1YIZA0Fo6DT20g/URgWhqCiKgrXv0SutdsLAi9+93v9iNf3G/PLJydXjyeyipqaw3YxmWlkpUI9ungpRXoqc6sGUyWQq1s8ipDmfc3jGEXW2rMBFKrGj9OFrkOrClAm/5+Fm0g57NrMj3TGpggEQT+oCk2o2Kc7nVQ1dxn6372/Wfdv1Ai1yApxdY/wnMzPHozHEAX7AXtaEvG/YwDWNmHPKBwc+448Z1j2vSBOn1nCihkAjciZ6k6KG9/2psw7Npp+gkF1W9JtCA3C1ar/3um/eWzx99/T9onzx+XU1nUyb6UlRY9Pj7nD5Gw/RCf7szT/7wy+fv9idzsvY01p1UuigMp0WTQkCdn3ctEMPCUGnrDogqrYRg0iviEKHTlcDTgs8nuFXF9Wzj7f6s1VxUl28t8BV0z+ZxMvmEIUqxrycCr/fxY+Cbktysp6c6AjSjyfRq4C2NJR5v8GW8+aj6kkWtQ1MfDVVTKAeKU+2VfVLAhBSFkhqA7b0y1IbBSEwzZsK82reFBeLuiHZ9t26i+v9kMJpkR/AR5HJYJZlREdtQnw3OSEnvSk7VB8DPME6ci+1RipLVA2rnDa5mgGL2pmTZlETuTUulzxVIOwI4IRL3f3dLSxy0i8V9G0u3+2KD371nQ8+uMS2x7bnZ+3sslis17gv+N4DnJTYtrhd/Zt/+2k7SNMUu6h9xLqNF1MmohC0FY2QnQ5t4K5DJOoFQiqKGGOvNEQodHnQCExr/OC96dOLZh7o2V17dlKegYafLflVe/Xu9E9e3OnDxfTXLn9cFN/6sq1P8LOTom6wEvRsm+ds+2Jeo0zTxZUfOLe1mU8ifRCFn1TodEqPjM0ocA7JzpiNi6d8zIUCJ69J4PavBVDPMCidDTSpGZMwa4p5U0w5nk3L3SaIraX4+W/I9Qa1gtGRIGMc23ZuCY6OMHIenp+HRsR1Q8q/T7VsKI39ZOwmYdKtl5SUsoijfhCc58KOgjq6HxTEoho4sYWMg0ogaoD/tGx+6Rv38c0zdIqbPZ5vcX/6Fx8th49uFpPyxz94iKdneLnGJzfL1eEXz9ZvlvvLaRWCFgGvbrrAVVNCGWUAMy0m1Ql42w6rw9BrhKAdNCWTTLrpEYGS8M4JLUoqgFMlOW0KDm07FJPQLttY8y9rfW9P33uL73x7hven//J/+em7J81/8RuP/gX1P1kgqh/paxOeROe0TKlTASmtphwrshKp6imZUxifpeP/ug/6m8fY4T5rKbGFT78UZW6bfpO2gxdMCNRUoQg0m5T3dLLZtmVRJLJTqJcERtPKpMzkHs9pTC1N71cBse9xyskNMoG06/HoC/CIyaOmaymnhQjJPF3ttAJK58Cr9fSmpgZWIrI+Ngdfs0ZxzQMgJsQC/E9O5v/h9x5iPsEu4vkGH97iyQmi4OX6Yl5GKppZ9WLXd//8F994evr//Ozmz5/dTSdhMVRdSd16mNYhRnm96q8WBbPGyEUQQtTIh9hvWnRD3PVoO1QFmFSVylJnDb51UX33vDqdlkxFfU6XqttB17vhdFE2SlSGexM+US6WHV7urrfd7Xr47YeTy5Ppf6X4NbS/K/0nHJOwmCxBCFCGRiOvWSzKERBj/1+eBYyg5CcB6TEE5NZH8rgETQuTqouuDCc4sf5dg4R0VFHqPkzN+wQCAk1nTQTXTcUFpcbaAhCg8BGlw98iEGAi2YhSsOhuhxIT9Ctf9IQsZPujeNLnebK4RJV5pHqvYoqG6pUIHgNxPpcYEIjHXBeK8nkcitRJb10NIKj8+/PJf/29x9ACD0/wp6+w7rDvUQAR7Yt1F3S5aR9cTh6dNIjyzrfO/vBPXvz0s+XPPrt578mC276P5eyqeU/p09vty7v4WoezKUF7IWubaXvtBnRRRVCXCIySuQha9Lg4q/7jH9xblGG77l6/Wi2m9bwp+nY4kHLgodBuiG/64W6g2Wl179BfXk0QtSwDtp3E+FTo7666oYnPL8q+IGt8VwgkyZxHh+y7mDgugy2Jkw7Al1GtF1lGI4NLWWPdlBSa9lS5nGCqPExpsFZyz1tss6ldRLWs69m06SKiKHv/dDHye6idJZtCnAuGngq4Mgt1sOHjk5FzEuphkHJzkPMwC8wp/0t4yYZqmXuE5JjWw6isnrEiv9l2G6hLAJ5NqfoWPQBgon8yn0NL1AX+4EssWxz6L//ibbisHz7b/N6fvPz233ywZ3p2vf/hNy7w3ulPfvfTP3u+7Dfdt9873WicnU7KgxQBQnR5Uu+7/XIXX0dqCgqBEqoolJhLAiMUQSYlAbppSYj+wQ/uPTqvuk47yMn5jIBONBTh2fX22bKtQ3FvX1Hb/9oH94VxO8S7T1a1yr/79GaLSIfh2fLwF8+WLdPZr99rf+VsXyajYqteElhFPRGwoIfR5pxdIAdDtWPxLcJqSri82c9zO8rmY9iZazMpsmS5y0yKkI8LSJcRDFF37XDohuW2vV62bTcIBIoCidmZ0J/uFdSPRs1ptxlf+i6cLKvmDpSMhyaLApp/YyfSaPa6LKlmYcJGbnPjCboRBPUv/0rUAMp2RJhvkLGbp8ju8f8fns3mj87xe5/h3gyfrn/y+c39Wf2L230lw/CQ34g2LzarKA/OG0xLvHfyN37l8i/erGhavXi50nl9FgoNKCO6qO9fzrpeqtAv93HbCjEVKdgwgbUkrkpUgftIyzaWjN/+5av3LhqJ0i67isOBhhfX+zio9vFy0fAg75zUjx+ebHZtMcR3759NIy7emX3nW+f/7qdvK1WF/uUXd2FaBaFfWmrz2f6Pn062BbyjmjL6e4JvjRaaiuZ6pGx4MPE/JPzyBIn8o/Ag5OktoMmE1KQ9t7EjvyY1jbSP2vW63nXN7f713eHLt6s5x5fXmy9vtutNmw4CLNQNmXIq4OAFEwtpxF1YbusGIYlB2de0eVLomKr2Hje19CEFXBk3BurZZ6bv5F0kimRo5mtebxHkg4xFvXvWv/KPFf/0bP4P3rnEgxlC8b/+87/+7jfPX7fDhx/fNrMKMa6G+Gq1e/xk8enz9aYdfuPp4exmf7fs6lm53uz3VNy+3YtSFfS33rv/vScn87r8s1fr/+nfff7ibr8f9HYd13sFIYiGgoTQD+ijiOLpefH9b5w/vb+QGPvdgFVLRXj+avPhq/2Ty8m3L+ezaVE1xbA6xOV+VhX76/1u1b3etO2yvS9UV/zyersT/OC79z/7cn0yK0+LcPfh5mGUT789G4IbylEtw9kXrEoHoq+aFOUA5LnnkYDhwCIgkpxE0tEOKoUzpqzRIlMYAFCJUdH2w5fXu3vnkxe3Wx0G1ahRGEmsUkALt4ecHpO3B2aeDiiDoiCdDBLT+R9JbfBGzzRqsrq1ZRFpTtibCjl7jE2Bhz71vAOOnDmD9XhNaps/lQiw735KXpo751SJThj/aD7/7R+8i882+OOXWJSPHp/+y5+8LIFpVVDDw6r78mYvImVVCNH1Tbvp49ntfsdYTKu3xeHBw1l4pYflgef1R3eHR48WfLP/0d94dBrC//AHH7/etKdN6Pth0+qmzdVSTGp+fFo8PJs9PJ9IHA77Qa4PzazcbPrltv/+k9P33pnP+iidVKc8gCTKdFZIwDbGF9vD61V3t2wVWEdclHR3u59GBdOui3PC6Z3M3vTTd2af6/C5Qw/5bsUj7u8RztNHr3079bdPUp5+K0UR2YaSTMfgLUhWZ/XaivEbJsc/IhSEsuBABQati+Lb75598+E8Cj04W6837Zubg6IPP/jxPQ5McPUJ4gUeeIHRjM7WldhzmTGrTBZDY65Ama6RUTTTKo5lYKv+Wjabs+gR9XMIJXNdJtdcciw3/IeCmIH/7uHZr377IRQoits//HK57qYNv932bzZ9MSs+fbmenFRtN8xPJ/fOm7/68O3F5bRp+MXPbu/a7u//3W+8frl5/Xr33tOzyHRRl7e3+3/2Z6///NlqEeOvPD3Tlm72+y5CoPNJcTEvmlInFb1zUr57Vi6a6ux8WpXlmzfbMJDuh3pavFruJ9P63avm9dtNWRXNolp1kcowq5hmRd/2gWkjtHm23qm+2baPriZVXfRA2PYTxmJeSaeqenE3/OdPrn6zLn+3b6Ortkc0zDMrF6Zcccp5mp/8AHfzHD88aub9sXDek/I9b02l7PdHXAnUCdZD3YXf/OGTi3vTtzfbxaS6v6jvdt16edjuu9Wu73oJP/jxvZR8Ops3hkN0tIhWEic6Fqbhh2FZlQ7poHXffmto5YUfl3kM5NK0CCl7RwiNXjnegzKhIxuAmklbiY1gxI9JUTB+vKPFRsABkMm0DNeHn3y5+rOfv+2FD4cYQSzSdXExr85P6n5QrFuaVEXFv3Jvcbg7fLjc/fLjk7qTgygPEkXunTXcyyer9qevNu/dm0VQ17aTCpEq1NNZ0POmmNaBmeaz5uSkOWy69apdTCsqGZNqz6xxaPt48WBxe9dSw3c3bZTYnNVffrbsokzL4vntbrqoaFE/e7U+KQMOUjXMkWZXsxlRs6h0kAaC/fC/3a4/O6uO6ImvwMhw4IaWJs3IVP7HM65jckP5OuMf7EQXP0mG1HkejF572VgOSsu+aMOvf/fR5Un1+Yvl2dn8/Fv3bt6s/uqj6+tlu94NfR+zAHa0znqERhi7A1J4cqMXL/7Y+1wa1PxB/51/u0zyI89WCAINOWLqeLCoW5v7HZnG4z1t+R4qR6OThvHfvnv5zm9/G/fm+PQOL9bY9Aqtq/Dek7N7s1qgl/cmsQpSB4m6v22r/UCBK8LV6eTDL9f/5icv3z+b/Xs/fNj2MmGandccaAJczsp781p38X//v79YtXE2rcvAp6eLx/fPLs9POCgT6qqcNNXr55vl9SGE8OXN/qMX659/tnz9fBWKoq7KLz+9iVHKgooSwvT85aZeNOWifrnvlreHHeHN7S6EwIM0JYf9UF9UOAyFYLGork6q/aD//e9/+jt/+lruWidhCZAMZtS7G8hplm0HVeuqF3ju6bHIz3dKx5Qa0qiJJb7MKVh4K4YVATL5UZCKiIhKPyiiMvOTv/kEH7z73e88eLntX9/thj4C6XteMRpWppU5p6VjsyM/AxQMpC+Us0Q0RcaRf9mT0Ci9ZDeCV9+Mw4Ecw021sYtm57N76FHFTRXpFMg0twz+b85P3n/yAAqIQARv9zefL//8y+XNphtu93G7Z6ZPP7y+WR7Wu77d94duKGfl9KTa7Ycvvrir709OT5u/8cOH2HbXXT9fVOVqoDKEMpSgpuDdMNx08fWn61JDVRZnNeJu1e62ZQhFyU1ZHpZdHcO9i9nyZt9Mi4r54qRanE3OyjADT5r6/tV0QUF7rN7uT07q9fLw5vW+V1DFb2926+Xh0flkNq/rWV02BRV8dn/yjSeLBePjT25/8uLu5rY/ebGXf/uqvz4c+aSa96YJQto1Tj6N1n2TOXSi9qZiuUO7bj6aYP4LIGrFo1R1UsBTCvWLCUXVQQSDigKPL4BH+Na5gLpORFURi7GjxC+ea7eGYgQ7AsMzUPWzWDCaNrko5pHNseeIQGUeCs/C3e6y7udYmfiab1447tuQ1GdlmaypuvqjsvxOUcu/+gWfluixaYf9dpiBUNevP3tVLuoATEuevnuqwObQ90McGHHboeJ+Gk6qOq66v/9bT/Bo9q//9Uc7aEOor+ru7dB3w72T5uWb9evrQzMN33yw2A4DhNrtWqF1ycxUFGHGoShEBtnuu+221c/loizLXi/nldwcuOKLy8liEvYv9ldXVTUpJqKHgvs+Xs7Kw+YgzLQ/0JbCyWxoh+7uwIFeP1s9Pmnafvjrt7vZaf2gDv2iqfex/eOb+LfubU8LP9nLVFXHMtjZw2ZVnI0DrouKfcXq8Rct6lh4UU0VzrxU4ruTFenci4jceq5Ge/pBYq+HPgIVMMfFpC7LxI4gVORIlNMYk2jzN7TndHTUvdwFsgSL0We8AdbsN4GfJNom6dttHMJV0xF+to8LlLYZl0SBKKpvnLXChOcIRHYEFwDohOgHm/i9V906tNN3F9s2vtwd/vKL5e6uPZ+XZ9Pq6nLx7NNrrUJg6m4OmNfDAGF+u2mbSTkwXn2xmr13/mhSYN19/gdfvAn08sV2c3u4fGfx5s2WlYhJCn7w5OTDv37zWQiLSdBBi2lgVWIOAY0yrbtu2y8ezrdDf+/x2Wmvs8vp7u2GlbRgjVoDh9e72EmN+nQRupfbq0cLIQx3exa+PJ9gkGZRSy99E6qH027A6VnzZrn74pO7i3szZRRnLNMCRNNW939003971j2ZibdJOfUlx5tRVjME8TZ510az1uRUR+1kSTt+wQEoZZWqEWZkzoDUyA5BodK2sjl0hzYCJ8AZcD6ZVkw8QDR9H8poGsmySFUV9jVVlt2ZWOLDzuaWxY+j2jm84pikYrXvCnKx2sgcYqrMG14qHnD42xfzf/zBA/zgPhZnQMCw/uxff/Q//vzl513Xp3fa1/Vptrz3O/mPyubp37mHb57i/nzWxvc/uQ2M3/uLVy/2/fNN173dUVOiDu26LU/KvWg7DHFSvHm7u7yYbNadKL9Yt0+vpnvmf/Onr15s2ot35odNv9n3ZcHVrNruBxn60MWHj06LSdi1UdtYTwOVgQiBULa0eDDZvDocVFZvDlcPFqHth7anQEqhOAmavrNC0dyfDLsoqkOv3GvV8H7VV7My3u0aovWb7cVZc/16u98PpxeTeVn+/PW2LIt6Xoa6WMzK03l1edoQ6WrXP7tuP5l1t5dlItEe23LtBb6o1p5gK3CsYpmyYYCQQuN4WIRmrudxTvzHms2Q0vk3MWLbHja7at8LUAEFUIYybcglQAqzCy8mGXIZw0z9SbkQxhYndayWw9MbO0be8DAfypuqJWOSoUDqlzQBjEECUew/3VSv2r+cLnd/evv4X33y5GLyjXfmmNbFy8MH11it2tcz6KKkkI5ItK0uJeiHXXj6m+/g1x7gbAoQ3m5xUj59d/Lly+aPP7ouy7q6nOy3fWz7CMQh9giLRbXuhgB6uzxMp9ViQgL89JPlX77Z3naxrsvXXyxni+pkMXvzerd8sXrvO1ddG95+vnrySxcS9fWmfeedk33XcwARQqfYDAfu+bT69IvlWVVEaL2otp+u+MFEC+6ud0ShOqnoEKggDNBhmD2a99sucCHE6EX6YTKrtGhCVRRF+/j9s9uXu7bsJ/N6tijrpqir4ma9/4uPVjer3ebQdVFD3czXp8WPLoepp1OAyVL2FYo0mpTTOXPzzMjdajRVd7w9AZZ8sRNtIbWTqx0DiVyTSDQuDtL2sW074AugRP+y3XcGm9DimFrTOCDynTMegL1QkS0ZzJ4BJHQV55Lp9uLt/457ju3QLJtZYFw/2332fzz/6VokKqDMzKSBAgedlmFaszLvgk5/aX71wUVzUqRiMIGflvz3vv8Q373EpEYX8WqLz1b45PqvPrm7WR5iFzfbVV3Xk0kTh3i422NSd9Tt3g5c8b3LqcZhvTxIJ+9/cP7y+X79+d033j/VQG9U55Oye7u/vDdblRx2cTYJm/MmdNKt2nlTF5v+9LTcU1TVkilcVgfQs7vd2UUzL8PnL+7OLmYn70yvd123bO+fTMqCr1ftvAirZ+vmyQkdICocMKiWl3V3e5AedIhtHbq2Jy6ef3pXT2o6r04XdVXQm9vdft9fLOqnl5N70/LN5nC97N5sumd/9PykiBd/+x0KkvxcBRKH2KuIKiEwhTJQYcot+daynD0YJlkDhu0CsuyUHGUk0XL4biFbdMtjiRQoWBN4SC/4o8/wowof33DsCaREChsCckHDTwpUze076R/rlh1bib1GZHkl5Y9bK5GrN6M4llyDv/KEqjLo9qP1aahm87g5DG0XCUrMRFIGmtTF6aI8mwQifvWL3afP1g9/4+HZu1MwlUT/5f0TvH+BRYNBcNfi8xU+vf3Z56u//nz56avVvutUabc7tEOsyoovm7bT/a5btcP5bLq82V+c15PTanm9Ge7as7OKC8V2QMWXjxZ1EYbX+9njeXnR6E2LgIurSRCtlKYn1XDb1rcdn4bI1It+/Onbaw0qMn84X8rQzCfL5aG4mq3XQwjUEraH9sUXy0dPzmeXk9tNu2iK9sVy/t4FgO7uEEFn7y12N4d9G9vDMF9UV1eLs3uTsglEePV2+/hq+t1fuV8Wutr0t5vuYsO30/J8UxVvDs8+XJ388AHXtF8eVq/3q5fb9dvDftkOfRSgnJbTi+b+t04evH9aNSGpBzoyIdMlyLeUWdJmxpSiojrKSG52ZCghBKtOaU/KRLEd+s1h6HqcTADGaT2dVuTqfeGxz1KR9HVM6uqvbRlN4U+BcW+zfZV9IuTZAtXA6xh54Rv+7EbmB761te+i3O7ntU7OGo243XQ363aIACkz1yXmFZ9Nqwfn1eOL5s8+X338r74cfvzw/tOTf3zWPH7/CqcTCHC7w2dLfHT74fPVX39+98Wbze7Qx0hRhVQOWxkm6ANt9od9NwyggqisOURpSOPZtNt2dVPM55XeHfoDZudNXHZRQLd7rguJquu+mVTtzY4C0a6PFXbbQWI/zMqri+n2Vdjs9G9/cHn3aqvQqweLVy+Gto+TWTE/qfbr9nDoH3/n3vJ6Ryf1889XD96dXz1YLLeHqii0HcJJ0/bSK6nqZBHafjg9mxQVb7ft7XL3ow/u//KTEyJsD0NZhPN5lcJbVBlicbgbbj5cLd9sXv9sub9p+x6ADkIadQBUukG3n/z+9ff/0eMP/tb9dApZrl5b5DLEoLyVPf/e61fWzGpfOWf7BJOSqwJVQuyH9fM3d5tm+2YDAVCAiMD+VXQoJNe+8j4+gtUpvZg/wuxILBOWkdhpBozxC7Whrh9aW7ACxKTpwFdvRks6LakOypHKMjSBiopm9eR0Xry5bdd7CUQhUBl4VvO04mHQ81kxu6PP/88Xv/afNf/Jr7+HyykAvNrg89vtx3c//fTu51/cvbrZ7do+RqjqoFEFQ4y71WFS1XHQQ4eyKUqlxawsmChiPqnitju8PRQnFRDKulDiQ8TsyWz7dldNQjir8xHts4ez7vWumBTUFLttv73r9/322W33uC7uXqzPL2cS4/MP3y6u5vcvJh99eN0v90+/c/Xq1aZr+67tl1t6+PRstz6s6+LVs9XifHJ1Nlnuut3bYXpvVvT65tX64moRGt7sh7vlvlCRoV9u2/RVck1dTCchMJUBdcnbiHg9PPvdL4YBsZf0DSXdQDF1UgiGCCX0e/z83z5/+M3F+cOp6aEJoMYsL5KSJDbiGSErJ8XMyRQjRVCQgoLnpEqsBBmGzRevlnXYtaG92dXY4raNMXpZIuOZEzwZv+PrOM9M2+ehGrw9LnE3SmfiuYRhsCvKqT6eAi/bUY7W7e3pgh20TYEQqATKEJiJSE8n5bQsbjbdeteSJgtFP+i+G1TRlLxc9vGnN/iHAdse13u83Lz++O5PP775+Pnqbr3vBxXBIIlwUDfEPqLtYj8wOMxPAwmXhVZMOki3jxVzaCoV4QCel6EMB1EqlApmDigQ21iUDFIqQ78XYSKmYdvzEDd3+w+fx19/esGx7/fDZRUGhLuS759O6r2c/b/tfVuPROVhZQAAIABJREFUZVlyVkSsy9773PNaWVVdVd09PdONp2cGg7CxPSADBiTLvIDEE69+4ZlfALwhwYMl/oABg2QhBEJCCAshkGywPePp8bhnpm/V1VmVlfdz25d1i+Bh73Uyh5+Aaj20TmZn7bysOHH54osvZiMFMiXoRsXnn14/eHuOCusueMfbJh482XONu2nC1UV9vD9ynSerjg6nDx5NSOF22yiOAvjqqi4tKaLC6tmYSmuOrB4V+tXaf3TWOFT742JVOxf6v3DqowYzpDTwdhChu+Hbs3bxcJTr0t1oQA/NUhbjyXD9AMv28YqHmXgA6IUTd1fJmR0E6Fzc+NBBcX61eXq9huuaWYYOQs8/g1y3Qq+9e7fjZee2MrtpB7TBjroquKsjMzabI/w9AKTHVAlAEiAOK9GEEJMyRDPNK1Ykimj40xg8mBTWkOs4MsYkyzp0QbrAPkqI8l++f/mb33v95Ot7cLn95OXmp2f1p69Wq14OCoW5l+WSyByihMCdF4otRtzX1pZKAYRtsIXRYyXAdmw4JiEKW88umL0KZtX2y405KKISEnI33rxloLL163pyWEajCILWal3a75xUR5HVwUgQYONGe+NHTxbzkvxV9+B4ZCx2p5vFoto7Gh9OCufi2flqsl+NKrPauM4FoFguinWIq7N6ejiZj63Rvfp0LDRGxnXtL5ZtacxsLFbRpDJlqX/41eo/fXQ1W4zHDC+uWs7SX9CzYgQ4ZTPpFeoEXBOGaYEdtgn5fhCB0+Cf+k8NcwecATkYgNlsmQmwf3JfJjKAA4okLvDr6+bpxWa57khEqaH1rXdA/S79AmHoLbbXz7nL+XNHIFersOsm5SGRIbT3jG3AO+NDzAgiSTbq3lzJQPlwzLcrBjQIpAASpiiAMrZKE16tnTVAaGuXlrVftcEHaVj+9f/48jcVXC3bPzvd/Pir9bpuBZXBXrFfJCXPEpOEwJ1j50GRlELac1URgpBRYAQI0Zpu6XSpGMUWlJrUdFEBFlPLRp2frQ4XUzUx69rXG783t1So9XU9KUydki3Uw4KMC0WpSTC2Dqt4NCvg2lFIFaL2IkGmpXr6dKa6FJ3Mj8bjSoNPNxfb8X4pjAzSdO7w8WKz6mBeKk3e+UIjClKCyHx9207GgAhKK1p3f3rqfvt/vdJlaTUut4E59bsYYaCgQUhDeCMcIEtFoHql076qG0S0c9HW58yId0KOCAM2ApBDlgzlJQowZ7hLCEERaKISZWRwTNS5ADfteuthwGABALT0Tavedhj7FS0kMOg057Jk50xz/ye3lUAG9P+OlyFDXQOYN2DtnrJbivIzjxw9GjWfb0PiUpMhlVAocY+7WC0IdHrVLktfu/R62W2bwIIg8P0vln/2Yt659OKyfr1sREBTZCJAYknMKoQYonQeQ0BhiMAVwqjUViuERJY4SfAJC21KJRpfn9XHh+NqT78823adf+ed/XUTlpdOEh2fTG7P6mbV2cdKC3QrH4v00VX7nWcLveoUKnKCXSgWVupoZwYM4aRApLRsq1nhr8P8uFxeb4H0YloCp7oO5bSYlGazDcsrV02NLZWsBBQhgHPeKiTSljkkdiGlrRNkZj6/hf/4JxdnDTypuOm4iylyT+kRBOAEPg0+bNgCBUAIpGC8KO6YVDkM9QwrljRcPOyIa4PzultGv4O2pB/ru8OqiFCEtUJj1ciqrvWrVXOz8QhCCgmFiLVkZ4W7DtZdOXKvsdjPN+VYmuvKjJ9A7luCQPZlkmWr8M7pyTCLxxksEQRkNbHma7PuJ+uxEWURBI2SJCTMCamXD7tY+3Xt67bfUSUKISZ5edt1XVw2vvZMCIUiFiHyKanI0QdxHmJgESFCQdpblKXR1mDwGLtIlQKAq/P1w6NpF9Pq1rHA8dE4Cozn1cV1U7fp4TcO1lfNcutZ+N1vHZ2/WBlNJ09mEWS0DkcTO5taZRRZij7Onk6bl7VFUscV1QEseUP7z2ZXz9eKwY4L3wbNqr7xAjKbF9BFQzyfVSml189X+yfTi1V3vF/4yFqjRoUGjSJEcFHWdXSOP79pf/Ta2UKvmsAV+MAh9XhkCkm8BxQwCu7sAEERTB7Q7KjahZchAxpuGBBw2NUiA46b06Md37V/Fudu6eDtpK9RI0KCpDghJMDWp9YnALGWilK3nQIaNszhsBit78gPgG9+oPQD4gqkH3zjIbXLX5Rx2KF52+t9ZEWjXdugr1SHXTIwPGHY/okE9ukoHZnOp8RiCLQCo1EpAJYoHCMjYudkWqn52ExHurT09GjkY7rehE3HIUJkSSxJJCaIKbqQfOQQGUEUIhD4AOXIWo0UhRQkwtXGJaO6hq+W3XLr3v5gj4VXrTdGzRZljICEHFKMkQGcC/XWASEBps6lJnzreLQ/NkQgkcUQaUq3XTUrbKX9VcddUgUqTd0miEbn4uioNGOlLQCkmBKE6DbBFHY8IopxsihHJW2bcHrdtUEiiyAQotU0LlSlMca06cKX1wG1aj1frpubrfMhJeCUJCaJsV97AwhACBqGxeRGw4MPj6uZ2XWVhx5TDxzw8NEunRFBhh3dqPc4mMPyrkYYjFFYUgJgiIBAGGJqQvKBFYHWZA2SQaUVZeJXv28g08SGRJGyvUkf0XtflX+i7H6H9DDbKfSQyuCgcUghJbc1d2doUzIDAKiSig/3mwfFNsQooogUkgBFhm0bbzf+Ztlt2zSp7INFcTAxe1PjIl+vw7rz2yb6BCEOtU1IEhK4gMGDAjEKjEGFOBsp3iZUqAqVGJiwbeKq9kdvTWISTtg1XhKMStOs/dnn67396vhwfP78lgT35+WoKi4+X731cPbs0SQ23LZxcVCqkUqbAEnQ0HivjJcOKwMFYUjFtNh0Say6/nLJU+2VtNcdBEHAVOmgxPkUJcUQQ+O01eNSNZe1c+mTV5tlHWsnLqYeCS0MVhatUijQxEQkLGnVpMuVW3fJOe58ap1wHOISISgEItAEWsP4RD/65oFSeIeIZYOCnb6w5GZ2tq87/mOOXSgg/YSsSI+JiogwEDOgKCIkVIBXt+3rZbeqAwlpIjXMb9517/sWEu10GwQSQOZKDOXjEEMF1eCVM0uN+5UZgP0aDvkZITse/B727SIYuCS5EzGAgBNF39pr1yFeO9z6VEvHEkT2J/Te/vzR/uSdh9PWp5dX249O16s2vVjHutvOrSRhgX7lo45JQhIfIPmkEEtNiKAVBZHZyBZaSGMbQwLwPu0djettWN22htRsUb769HpxONkbm3a/WF93IwExWFZ6f6/SW3d0WN4yzwFNgPnhCLrYBb64aPf3S23V5avNW4/mkyeT19c1A5ycjG9cPP1y+fTZXjfRm5t2PrJq003emq2idF3oEiKImRrvY6qTHevYeqV1YeNPzhqNnFgLWBENVhkAIDKKI5MCqduUBGKUpo2FTSFKiDLoWXHObAhUHyhG8Oy7T8b7VoaKsYfihSUH0cFD9f4A75mWZGFH3gVT3NGBYAek9jAVkiJSBMiburtaNlaJIVBDc1I0AIPovFIvg7Ysd2MKkFvgfVEMgqIGpGxX5mJuumfj2i2hyyBwH9Fp6K/xbplJfgcBEJBowX0b9ywISxQjME/ydwL/+jcfw6++C5MC/vDlj//oq5LSHz9fLzv+7DbOFM8s+AClBgBILC5ICqIJyqNq8vZ8tmW57XwdjIJqUQmnzbKuFmP2vL6pp4uqaZiAJ0YVs2I20d3r5mCvVJqkC8h09GgyK2w6qw/eW4xLo6KE2k+mxUUbb15tlGD13p5zaXvZ3JTq6HBcr11MPJ7Ys9fr4NOqCbcsLz69+cYHhw+fzlcheC+KFFpMbSdMjEhT7T2kNpYlFAomBb2+diGElDhMiyQyslok1Z5P137VpSRgNK634LwoEtPvUFWgGCDrqxACIdgpPvsrj0++PkfCXmtCBBHTHXNmsK6B/yKDy0n9ihnplwnfy9t5F8B2kZbv2ojCAymagDUpUqQIWCAxqG9+91iZXXsc89YAAehZR/3m26HszYhMRvoHZ4TZBw4BdOif76ahhqVNw1amHYcb+l7tbneWZL/ez8orJI1fD/yr03LxnUfwjQO4rOHjyx8/v24aNzNEzEaRR7qsUwholRjCENl70ZaKbx3KX3wQHk/IyV6bSgROwMJK0WhauibO98ebZVsYPS11ErGeq71yVGq+deVepZWGreMIxbTQjqFJttRlYdx1m7qoK3O2bPcORwcPRl0duiZ8/dsPVldtZDh4NGOEdRed53c+ODw/26y7CIUGRmXpxSdLQdGVXTXObwMUOkSAlDiJqnTrY/RJQLYtNEEcsUsRtXZBfnrefP8ifLGKtx0jc3Ts/CCpQwCeAQX6Fe5IoBGKGR383Pydv/bW8QcLZTDXBXTHmcgIVH9nOATGIXqC4D2RzAGpuu/6BhtlQMe8jlinByQTousIqSofLMYC0LbuduNuax9i0piVKWAYIYKespgVjoc0H/NCw8xtlDubG/L9ftMHDt3/vLDoHpQ8YL/3WcPZVPHufYUyDDkDFkk+6HhxoKE0cNPBF7efv1pdLH3TJQCsFOxpIWYztbdtOu9YIBoBXWLxCw/lazPQKAzAogFj4vm8aDc+YYieJhNbMj94MA1RlA/jseVVGM0KrmOSFK47KokVSRCTIG6DOaz8xhtEM1LAApFtoV0XSaTS5BrutkEbpQ29erFs2jg/KrvWX7zaGG0sABpat4HPwsP39m8vtkpT9AEq1cQgLeNUI0sXQxBhEaNgUuCaGT88aSb6p5tQf7y6bVPdxbqLmODZQh0d6oTSMXaBQ5IYOQsEkQAGlskvPnj8l46sVYyYxZRJWHZsjdxnHi6F5Q6jlRyisvfaNXUG8C0XcoNQcK+E7F2KBjmhD3HTBauRBYzudy+jHsJ2lhbuUZj/h8wNO/gEkDENjar8HQEg80h6s6NhqGnol2bII882IAzUyvs1AeZyY+jhCyDySRueWlrMR6AJzrb1ZzfPz9Y3G7ftuPbJs2p8aJsYA+9VOtjyovUjkAe/8ki+Pus3AlrEk9KKW6vKxjYc7o/axvsuTYyOtZuObWcBN1GcAIhbdqiwOJpyFxRBuV+GLiIJaDRz010mI1Dtl+jZlvZEwYsvbhKpp988WqM7/dH5e99+MKrMZz+5LKblbGSutL48XX3zO4/Muvvhxxfj/fG6Dsd6KA61otvaJ8HCgEuiXcJKReFEIAxVSduGb75cybzYnG5jm9jivoUPD0cEDIk1SlVhVYy0xsQQOYbAibkL3Ph4W4trIw3N5F4iAYbokYPcQGvtU7XB5jgzD/t6bceZ7lEG3NnlcHm5o8CIfZ+bgUQgCQggEWpN1mhFiIAa7jCw3qT7Bv7O3wxOcngfMGQNVIZhJA57H7wTK5JMQoSceBKi3GuLDo0zyWWygMh9YG6gNimGZ20aL0rYG4ExcL69WnXLjds0ftvFOsjGxcaxDxIjwDaUJY/3qy1QWsdUBzuxBFLehMM23MTURLYMc6sIbGWjSgkLFW6cmRsAREX6uGrWHgwm4J46mjYeBFSlRavN+dZUBRjqblpLqphZuXSzebUYF6aOB/Mi1FXJ4K/c5GBsSr0+bcqR0WqsfZwpZRWNLN026ScfnT99tt/FUBbWuugSrrZhOgFdqI7FdyJWorLLyCvEeO3mx6Nnv/a0mOqi0OPL5uCz5c1Fs47sBdGJ81sihUQIQIghcWJOiRnEvW5Cl2hiIHPiBXJKPVSbjEDSr7DPEqQ40BaH+x/Gz4cRll2ZycMzMtG7NzWaTvWixI0rjHowr4yG6xg1Qd8B0r2BsgAB8SDpc29gLt99lifO0U+yMndGyAZADe+Zq+RJg/4zuYjAO5b4kBvczRNkR4qARZcOAu/PK1iMwQc427y6cU2UBNwFaUJsurDuQgqoUZSCckL2F46KUtc/uL74o8t3fvmkIFp+se7EqMLE1p3sj9LKTY7GHChtYwqMhlIbinHBKOwTIGChwyZAZDO10DERtD7ZkXFnndnDlQ9jD1zBpgm+DYcnk+NZ5b643X//AJ/N0cWuDdO9SkS2rzfjJ9PioAo3ra6Ko4ez0HlCCEYvpmZdy1fPV8WEgkRbEhLetomFR7NicjjbdH75xXJEcPwrjw6+va+HUSFJs/n1RHd/8Mpvw5AzAfcZDoAoUhGEGZm1SIhL59pYjDVAj8T3EQRlxzAdvIlkMxooNpIxhLxgRXYF3T0bzWO4QyEBpNAe75X7paV10rosFIG0Pm4an1IS6SlrIkPH647xk/2lQN4ce9/f9K/6hkTGLACzf6aM5Q7pm9xBMLso3IddHt4WmQAy+DpAAphsw35pD/Yq0ATX7eub+nbT3Ta8dtgmaV3atNF5AWAiKBaF+eXH8GSijsvRh3vxy6266CRyu45d4jaGXp9XQtQ+kmNIglbZPUukiIC08iH5bQiJaWyqynRbhxVJaV6/XK1bNzoZrTbh7MXaVarT6sXzVdd4jADbAFHS0o9JbS5dve6S4+ayhoTWY5kg1MkmPl6UVuuitLNF+fKza2DQWh9MJyNTaAUpAWkICD++dN/75OL0+fKhhaMSTUhE2eUDCEI4qtz7B46TTxKiCIACYpGQ0EWOiUNKAgJA7FJoU1/954gxPKbPWnYuA/pG9pD793XpPXK05JkkyLEUdgFUBECQBIRJmXGppxWWBYgkkcalr67b82XXj9aRCPQbQGAH0t4DUXKVKXl4a/gG2Wg4u9udpQPcJQS4mwu86wFINk6AnsmeBzwRGAVoaMWzHPn0+GAMowK2AS7r61XnI3PibeCNY8/KRUAAq6Ca6vKXHsOjcT9EYUpTEn76+6/dOhqjO6TGMSlUXkxRsEvakhkrVtjctCRiLDU+dYrsrIiO18tOT+36um09b3x0Dm4utw5kddOQVrfbcLVsPWGwtnHx+qLmWbladm2XvEZXmBBTAfT43f2ZglgHOzay9QujqY6agVzctKkVfPT2okpcAlllhcVoqiPcNqIdVAQEyAn8VSuJ71rBAoCoj0Y8KbooPiGhUgoKTVpTYmgCNJ5dFAGBhClybu9g7zV2cJfAoEkiwzXtPFsahDZ3k3PDV9/rNMow2Ia5eus9DwsmwJ6R5X2qW3e17pa1Z0ZAvUP875Cs7GcZABCHVWd5XTTuMK/8n77o7W1MGGSoMnd/nD7dBBBG2P2a+d/m5mc23+FHQRP529PynZMZKEwXmz97sfrivLlchybwqk7LJmxdTAkKotKq6jvH9NZoN1wVQBjh6rTzr+pFaS42XsgkD9qo0UlFBlPipksuMk0KQwRarbbu5YsVVYYEUWS17g6e7S037nrZnLwz05VZrj0avfdo0vlQt1FVSkoVhJeBNxW9avzrVbu15DRYS/vz8snTiULqhMtH42JsypJGI22N4i6CwGrVliKqjQeLaj4ukwfnOVpdGJyWKACbThjFHFX9HCvzXSNFTy29vegiRgFNMLIKEZZN+vw6/uhV+tEr/uQyXmw5JOHAuQCD3knlFE3yVmceSjLZjTINNR1kNAFEMgYukq9V+m6oDBsQkEhQmCVG9iltunC98VcbX7eJe+Sh5znmQDtY21Dt5ZTxDqkF2fknGIImwi7/kh0uAr1A1BAeYWf63DfWmYdqZbdqr4eGc50JIvCQ6YM9Db6DZbi6iT/4aH3gY2uKi83GRXaRg0sEMCn16P05vrcYWOUgAGg0WmstxZffv7BH8xnhvsEZaVIYti4BtArrpdPzYr1ux4eTbRc7F996tl+vuumiQg3brbeaXGQytLxqXRems9F2ubk9W1eTEglXVy0YrUrtQlx+tdGF9iH6a68Vjhclten6i2WjsPEMV+2UWQtMRrpNKbFVhhPR2el6v7RlkhLYEHChb25jiNLvrFAa0oPp9Ot7vZR+D/2ICACDgvEHe6svlv42CaKP8uVN+OpGWg9NAgegPBiPkxI43qsTd4PZWT8oT9tCDj04bI3boQxD0MoRdoDhewvLWTQACCRETtCFsGlV51LTxautcy74ngyIIHmhOOa+6OCVeuMdil8E4V1h0Uc/HGhq2QdKziGHpG2nVTr0O3mYdh6cVv/NevYGDmVpfhKITIS/0bWy9cutLNcyHZlffn9ysq//wtPxd//c8ddOZtPCQoLZjMZ//gB//hCqQSa4/+6JMJDEJFeX4fKq2bo4G5kpClisa1+38eKmDSOyhRIvjcDVTatAZhMtQlcv17N5gUq9+vx2Ma8eHE+6VRiX5mhhDw4rtwmzkT2Y2aK0m85/dd2UswKaoEa6Q4hB0JrbrW8svbrsLnxYB754sfIj4wgkMm2jLjVpQmCclI1BVapScLFXOiCj+kIdJQIhzN6fq6kWwb6a76OLCAlgsVcsfvEhFxgZvryNL5foE2iEhYaqd0r9ffVErV0ZkPOX/lW2Px68VO8zBO6Vl4OPk+H0/54kf4YRmEVQekrpugnX627V+JQkMQ92lYeX+z2vWbdnaAcNzi27q9xjHRBU7A1t8B9Ccm+0JDOVeoQlq/xD/pKhW5XDZbavvg8BogC4QPzbHD8wxdvfegxjA7fN80+vv/fJ9em1O1iXP/fu/jsHB+8fFj+42l68O+PjAtQ9IK5/nFX2qKQXjWPcNL6weNvgwcSst/6m9aPS1nUklMqaYlw0285oXMym3dIXlYpssE3Tqa03dqaVZpjt2b1Zka6aycSGo0r7WBiz97A6/dxdnNaHk9IeVquNa2r/6HCERp++uO6OZ+VUf3VeI8H+xJy3Pqy7MZEqNCMAgdIkkZsuQaWNAlua26VzMaGAcFIAukBzXGWJt94RYebugCDMnk3DNxbrj29u1gkBK42eITrphYYJxRRkSpNLOxwi1CBQKwNgijiM7QIMfIZMFsxVqNwDRAYDy84OhsWyQ4EqnQuuoJQ4CRAgAeJOvQVJD+afF5TkmrO/u95P9gJYfSHday/QsJe2LwV6xyQIwCTYLzHom1ODpQ6VcWZgDrlYv10FByfJiCgzwL87Vn99MoL5DDC1ny7/+KdXn73etm1qXFqdbU8vNxqg68Au7GLP3Kqe2QJEOEE6NtYFeeW7al6QEgBsQwqBbxM2CVxKy7VjgOnIHh5VoQujWfnZjy6ffW2vKrTzKU1sUah06xePx/hkrpuoCzo6GhUCoY6jSuuDMVx2OLZd4yeVVgfl8rY5PJyslo2wtJEpdqYsrpeunNjl2pNSk4fl69ONd/HZk1kw+Prl5sHRCBjSxhUHY8cphNRE9JycFwKIEQwAKNV0XEIfDXqH1ie8g54maaiORzd/cnW8pw/HtjToYlp13MvLx5CWlooxye69N4DqmGdmhQH7O+QdFpDBAcwg7uBcOGczQ/LUd+F3WREiiyacjIrFqLwp2+3G1V3gGPuJPejbnfk3yJXf7ofq+fy7EC0Cw6ZWyN1QzHge56WCA2VIUHbDV30utluzkzOGHOkH3zaohB4r+qXppG3iZ5+9PLtsr5ZNHQURUKNS0DhuXRwXNgB3V/XJ8+Ld9/ZfatRW/dN/9Gtw3vy73/rep6+29ny5fHkLiEgMpMeV/fnHs/pmW2/dZFLMR4aUvjlbHx6MK4HF0ahghI61gC0IWDyzYp4QhS6Iwmpi/GULUZQXWHeMsll1SQBQjh+MvEurTacsPX4yv3i5KqyeH41Wq3bThsm8QgXLOnSMZmSvNr5tvY9Su2C0olnVpEBIceuuE4TEMQEJNIyzAprEk90wm+AgeZx7dshAt646XZ/M7dgiohBCqamaShKDKFrZ8040A0RBTbLzTj0+m1Pp4Y6HFAl24YgB+hVy2ekMXfQBqur3d0legpYEkwDgpLLTyhRGMfOm6yRKjCmn9KgzRsxZhgBhII1g7mgBCSSgIaDeJZQ8hN8cHPsaBeAONst/K8IM1twD6HYNhAEkQcEnAqcvN588v7ndOGZMgiygmG2hpeUkKTIiidKkUX/6p1fv3/pffG8e90bw8gr+9/lv/duP2+h917JAUSijITI/HGlycWx1Le7ByeTydPnk3QMgLJWiKCcPRrRNySdxTJ6lS2Zko+PUpPJgHBpHkcu9KrWRRcBoHBF2oWDYnxVXV12KPFkUrgm3lxtmmEzt+ena+7h3Mt1sXNvGsjLWynhabJZtiPLWu4vrs40zyVh9/nI7OSyKsW4b8Q0ngYkBY1ATxUKXIw13YatHFgYhH33RFn98MaqDjLUIsnBi7n0QcxRIkW0lyZ81sijuUmfoF5MiDFtCYCfc3xtZxgwGVb2+LBMAkaEYkXsgam+UIgIpSepfMvcyL4wxSor9LoehONUDrIWZ1ZNh4x0vaDBdyIFZhmI3K4UnFMXINCSX2bRAMBcZvVXm1S/9r8SDZqj0NtoLushmmz56uV6vO0I0mpKABIgiM4VGUU8JL7UGTakLh8eLb334+G/+/KN/8bt/+pe/+9s+AYiQQp9EI1gthdGK8Lf+5z8G+IcAXwH8n4//yT//veZzauN8YnDpBcGgConL/SKYqAhwr+i2UQyR5nJmRJgDm4nihD6lKKJCKsc2NYGUchN7dbYZHY/tHp1/tTp8NJ0VZlMa7+PEEFRmfd0cHY7qDV+crg8eTHwXN9cNAWqlm8bNjiZN0zWKbuvY+JQYJiOaTYqCZU+h8cwRkAT7NQpIvVIUXTTqj87j0iuFVqMgBBHu82ZGJJCkGRKCpJWXLFCbi8PecrMfyDcMA2BGIjv0HHLB0FeaQ9aWhwfyTgwREWIWYkiJU0zCMiqwsooVPtifhJCuV1vng74HA+bNowMnpJ84p35mi6GH9nZb/TJkB0pywB8yfsgKLTAIaeTCmPK4Vt6XID/DtWPALxUulCKlvEtaI</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8y44sW5IdtpaZbfeIyDx57qO6u9AU2ABJQZAETsQvEKBvFzjViAL0YIsiW91V1V33nnxEuG8zWxrsvK1/EI4NcpDIzMjwMLe9bD0c+F7f63t9r+/1vb7X9/pe3+t7fa/v9b2+1/f6Xt/re32v7/W9vtf/34skAQGAQANEQQREUAQFfH6HBGnu1t1cBYAiDeoWzAzqLITDw+ZUOEi0EGbZImGgmcYY1Q0gq93Ypf3iHx8ZYdWq6m14V3uYJMIACTKzzI6wriLZYneHc07R4WQLhGZ2DEerBTdUi0Q33E1SOLNE0o3nmRHekEowGAijkzPL7PNtVgkURXNmdbgRyGwAIgxsaV1JSO5s0qGZPTbrQkvdADDCutvdZxZANwCgsardrbJ9WGWbmVrhFJDSMMtqEkaTOoZVtgA1srUPm1Me7C73qCo1LKxm0a1T5jJatsLQIqUWQLmzEubIVDirFWGZbTRBAEhIICmpS2a/dUJLAMnu/uweEtL6l2jolhkB9G+XfbVXbBHw6bBWD4syCQipqREDlMBtcBv7vo+SNo9jlg+GeSdjs3BAgrG6txFzFoUx4vX9/vJ8lXSc+Xzb748c2whDUM8vT/djuvvb233fRuV8+fr0D//w5+v16TFPQi/Pt2+v77fLLijcI+xxZkTcP47bbZxHQpqlrLqOuJ8p8um6neeMiNdf32/P11ZLMqi7QYNobkBv4Y+ZZmbGt9fHl+drdWbKg26uFt3mme6WWRGepcxppNl4nMdlc9KOx9ESYCNszhTppNTXy36fOdyO83y6Xc6ZLVTJzfZ91MyxbZlZ3RFOmqjONrOqdI/sHsascvMIa8md52NW9/AQ2tzvj0kHwZKCzOpt2DkzYhBNEaS6zK2yz+4tvDPNA91Nqkrdvnllx4icBZqgEXHMNFqrnXSzrDLzrCTh5pmn044UmjDMrCBaNeKSlU7PKh84j4fHLmHW7DZlQapmNJuwVDvZBsCAJrlvY7vs4T4iPLDtg7R5TrTMwHYfVLV7eJi6AJ5VaSWgW8p0M5ASzBhjjMa+OdkBHmd+Njx72+JkA7Zft20zi627I2zb99hGODLbh3nBw2PQ3cyYgoHDACfdarY5xHZD7EEiIh73Y7/GOX3bQmgK59kwjuHdqO6xD9887329hdGqa9v99fW+XzZVy0Oa5lsex2Xzx3neHw/VAE3KTIEeQdDIBmAedOsjG2NEqGqMEe4f9yPcSI5toxQBa4NxuIMqN4rbCABW5cYYvk6YzVzQtkW2RoQR1eVOuodDsG7t3uYWgtG6e+wburohdAPbiDGcm0NW3awW2ZKRNqL7dLMGgt4tidVNKkZAiIjuzCw3uwxHkm5RhYjq8zK80XU0NYcPY8NkFjQ395rpZgBkBAws7pcIF2lOgWbuTT1t4+efX2aV0T8ej30Lo0lW3VCfc4YHqPDw4L6PzMrsdQTcLnvW7G6BT9crjEaO8HU4VSaN+zYym4Z9i30zozegXnd2v78/wp00d3apoRHsKjfLagHd9Xjkft3VqCwQx5kjzJ1m1iUnGsic2XDSjN3qVgn72Iwt0EgRlX3kGWYCOmEmVc2WW2TleZzvj7o/HsOtoMu2XS+XsQ83VPUxk4KaWdPMRpCgUTN7hJX0dLmdx/1jzi/PT6RRUHeh88zL7aqW0OpPAAM0ASdA/XZm4cxjjAvVAEGYsbMfc45ts65ukBCgFoSJ3sfITEiNmT1u+zYziQYNpYKy2mmGNQ5aoo/NUO4xqwl09zlru25doiTY43HuY1ANdlUxxnlPWheQOffQiMs8J7e95zlbJj+7IhzkPNvYKoUbaIjwPeJyu3Tl5XLx4H7d7MiZubBZZZ5ZRJiBRHUb7Z5nTGupSkaERQTMmY9++XK5P87q7qJRZlSjOjvLh5MYw6vzOKbaPeTGqp45cyaIGEGqqrJ1HDOHh6NENTJzZnXjnMUWHZ940vjbh2FnZrUgSGgzSKDBgM5ZaaDYBI9zSk3atsfj42E+cva2RR3z27fXqvy4V0T87qeXGJs5wuB0AAKG2wg/Z162APasehwzU9fdjcjsMdD5qOqX2/U85n672sIrxbGbuYEC6bSUKLXo5IKtNAIyc2TTTLIRrAYJ23wQMYbaNvMGjMgsdYdaxtiGEeeEiRYeBsoEcYBdnEV3wgSyJHKEd5NOJWSGgIsqzDMvYc0abrNqD6gRxllVmK5wB2iSmfeaJint43LMMzyOM4cbIDc24X/1F7cff3j5+vXpcr3sW1wuEcPNxv1+v1y3x5Hdfb/fj+O8HynJwsYwdzP3bQsaJFR1ZcF42cfH/bjso0sA3eVhT0+3fR9mILnvsW1BsLogGA2kkbZ2CqFEH0MLjJqNGOaW2ds+upHdmZ2V1y3Q2d01aw2KnCWxK9UNac7sBXrVaqDZakpmrQZU6u7qGD7cZta+jcyMMR7HkZl//vVXEU9P159+9+V2HXAOcwuqm0aSNPiwLcwNtHCHR1Srut2d6C3w8Tivl/2YOfbtfJw0OgGIBqNy5lntBjcaYEYjet0evUaUzKjqzARkBtLCQIOvlQ0kMWcRBGgAunOWm5uZOVFQq7uqWlB3gjBo4Xx3N4IUVBK6dWZfxpjzMBtqwASVux/nGR5Z3d2PysxzVtNCDToGKVIt0IQiSKDVw727xrZVpf+Lv/5524e7Ccict+t1numBKlT1ccxfvr3mzH2M/XL5+ny9XOKyucUYw0cs6GUxvBsjvLsNMndz24dntcFJ0gihJQlr2neruzPbwubZNMtWVmf28ZjH8SjJAAFVDUhidlV2VpqZIEktlUBZEaQ11KW1JHUDhnAH0QULmlES3Uc4yALDINjtMnIW3Si8vh+vb/dfv/369Pz0848/XPbdzFAgBOF8JEhJNatm5zkr5zxLrcoGZdQYo9SkP+7ndd9b8tgcGFtEeIkRrlZ1q3W7XdbuaRH83P+DNHPG8AgPNwuS7samhRtWjwsyo7uFGWHOEQbCSZp5mNNoZr5u5MUdwC3ocIaZdzUJMpoiAHJm7m7HmXtYZnmMx+Nw8wTPx+OYx/v9ePuoY04VzczDwKbFOeXuanisJdfmrMsYOScACdkd24iIgLF6xtjvj0lwngnw27ePx+N+u4yXr1+cBOFueeaEQTIHaWBDfblsw4PE29s9zKx6i5Hd+7Ydx/HR+eLPrTbycUw3GgKi0WOnZB44zwIKFhIy8/n5tm8OIGera82nc55uNEjS49FSjwhKpUljlYycs7lbmF8G4VDLyEQNd4Pa1nICo4ehJWc8zrnt8bifWfXt9deZ+vrjDy/PzzQ5ne5QZWHOCQIGtWwRLhyL0AHpBJ3h3sLFI0vVm8zX7GDY822/388507lXNiHSOkvSObVt1hKpcD2OKXWYtxYY6KABmmdyH7a4J/X9cdyuFzXU1YUpnufcNidtQasWCFQnOUiHUlUlwBqAG0oV7ijNM23NNgv3KTCYs2ZJ74/5cX8XFBHX2+Y+PJwyocxc6C4clWeJ5gDXhj92y7MEOf04HzaG/4u//sncpH5//aBx2yyzCf3yyy/3s7++3H54eb7smxly9nnMMUZ4GElals6zwo0yQN3rehkBGmP48ch1wtonX8QY5rSprmwzkhCKYnUaaeFGmiHcwD4eaQ4BUlcJ61UjSAgOEADdC2ywWu8fR0K0KAkOwkQSDiOd1fKInC0ZjDFC3TAEeBznkfWHP/46M1+ef/j65QlkmFWpG/Os+8cxU2t/buE85ghfhEvOSaKyu6q7KQAmYIwAaO7hNtznzDPz+bZHuEfs18u+BdwItNCku8nM3asboIf78PVmQfaaTeZmRtIBmkWEhCpUo0G1YtsILrrRx6KlzGKtVZGtyx40I2lGMwfM3Wm+j2DzqBkxugTD/TEfc66dL+Ly8uX5druO4UYXWmB3dxPAWGPW2CVzJ41NMJ2WVfvuAvznn7+MGATHNoAO97HFP/352/E4fv7p+fn5qaWqliC4ILM4c7YILlSgdVn/mfeN8FntJFTuMS62RUT4PPNy2ZwusKU853CHhMUcwkS8vd0vW7h5V89jZucIJwjJiEXz3h/Tza6XsTiw86zFGKkY7gudVs2wGM4t6Ea1MkUgACOMZlwNwbfX95LC+Kc//XJWXq+3p+erhZEAMM+FSbq6LpcABKKB2z7C+dn/Dfdo0D0WuLpdN3eLMJpnFcicOcJ2N3ahVbOAtG5I1XBnmFWmGRe2MLJTkKoFrAneDlamhLXkkpZzCszZc7a61XKjUSaakTJ+bhi9IDnJPCfg0MJ/C82USh9njn0E7Twf7v7+cX97PFBN833fn2/77Wl/HFWzK9euIoJmDKObxSeN0ZkYw9a/MbPGNiSQFZ9Uu0vdpHnE4/F4nOePP/309HSVRCGrQFe3uWe12uTI7NUjdAqapyzMgKau+6DT1idJB1VVHnycJ1ph7CqwZ5cFdw86oU/JAURmgrThL5fbcZyk7scMNwGLvZN6ZnaphW2QZi0QSzxQSyOuxzFPQLQGLchUVf96TJLb6MslPh7pztvzl+M8f/32fpZie9mfXriNrHnODBMZEJoxQU/7vLxibZFLJyAZTFCOUidG14yyj/skabRjelj99HIFmJmZvYXbRZ0tt+PMbfgsKeDh7jSy0GjAulrm5oHOpaMEpG3z48gIr9K2bVUV121k0kkammYiBXM0LMZ5zg3KbDO2MPZNAoFs66ptbDnLR7s057xeLpXnr2+Px/EwmQ+OsX35cqOhG25q9qJfRKxLLYhkFQQDe9tjZruDiH1TlqqS7vF4HBHebIOu1yHo7e3+ww8//sVf/iypqii0SpL0qVCZGyGCLcyZ+2U3QqK70Xicmec5PPYt3LFv8f768X5/C9sbUtfLl8u+xbfHCUidfAoDPk9FWbXmmQJofdnGx/s9wt9f37Ota359uX68n7fb1t1jjDzPIIw8j2Pb98f9uOzbPB7b83WeCUd2A7jufnw8bk+3bj3f9vvjqKzzOEf49fn6eL0/zpl2e/ry89e/+j09Oo9orQMLMlFXGlqtAs1IwPApxImSL9mr5BIJQE/PdDf3OO734/Ufz/MhVZXm/WFPvY/rI9Ocqgnj/e1o2tMFx0ffrvvj/f3pegVZBLuRyDkNga36zBN13Ccu+3FMH+PjeDy93Mx4fsyCLmNPnuy2MebjtH0/j3kZ0XnQt/v7/cuX5/v7x/W6n/dH9yLkii5ruUMqIF4//lHg4Lhsm8X2OM8wh7LUqMWzVKthqEIX3DOzUM6AewO6f+TttjuHcBL+OCr+9m//GJtZ+NeXy/PTtm37+/vjr/76q34TP1sAXEojFluFVhNuBgpY8h492AIy7/eP86gftpHVLRlxzhS9VUsPAx2Qe0T44hgLyqouLspBEsDzUF5qzpI+RUA2KdDaYBJy1jnTB7NXAzeoMB6EZGNztOYsJ7VZq42QWt1maHW1MOURx3FqzkHrylJbTeHzjUu0hUXUAhYuX6qv0N2CJMgoFmEGyGDmaNHIH/FxjuPvQaogGdsWCigJgrDtm4NjizmTIiGoCPPFUBrdwMWooQCHsQWjmbt7AwWoPwlb665GrfUxxnbeT7Ugij2z6FRnCw1gaXEm9uJmaRZmqLZWd9Nobf3Ierm5FEKn1tlmaDOjIC4WwymZe3BbHBK61cJZtdHUBuA8H9Hw4ywd9vHxEXhdF7L1hx9//Hq5bKXVuBRlpCRSmf14nPu+kYB4HhPmIFQNorrub/eqMsoM27Dj45gNM9vCS9kqwqr7OI4Iz3NGjMV9kIQWM2SZVanWYim4bz7VTofYUtUiGMy2uB9JoUoQuwXYLFXK3ZTSsJxL1kN3ZfY5MQKEWTAizG037so83473N3dyUfJGCkWil1AKdDXgTtDAz+WTNC2qGEaigCYF/O7C//pr/19/TtU8MSknNYJoCeoSALU1Fe6VikB3AyEdkLUSolowqlVqtihg8WHdzqB1L1qn1WiqSevqANiLf6SU3bFkpW4HUFnYtkX8LHm8u0kTKR8fx+s2rmedQrf4OOayCHRSVkZKZ5WDQJXUBgcX04ZGL8x2vY7b8/W4n6gTkDFiXUBaQijAWgDevn08P13OPP/wD78QfYnYo4c7oMtms0Rwnm3CR7IKs7VU4Yjx5cstK/E4fvmnX+kQeriZL7gQsH59fd1iEGY2Su3eUDzdtqcvz/OsHHmeBeqcc2bnLOATvHVLasBA5pEL7M7qajhDUtZiJCnpzLo6C0JrfXNWz+SMrMI2jFQY7bcBayzLD/zpP2+X8Xy9mE7AGlLDLB5Z3YWWsd3WphvyQTWw1uakBQBAKe3b/j/9D3/zN7//+u3f/x+vb28638KNBNF0G/c65jnrKrUDImf24/TzbIueadnKhFTtnC3RM4tCNmhs6ZzVUxo8S7OZWSCz0Y1zdlF59myvVLaxUW1znll4HJmye9Y5ZVZHMc+iEahi3PZLamw7j1/vAGFHnWU2uLY+Uo1uNsrJRqlVaAq2KAfAiacvT9fbbcSmfnt9vFWlB6MAh6tLghmwhumnX4gtuSTr6+4DU7SvV2wRY2B3N4u2ocrh+Ok5fnx28+3f/5/5H791XBhjCHNt5Y5BF70J/PMwKLQZQV/7oFk/Pe9uPraRpet1l3C5bQCut8u2OQKKsV/Nwk1Qw50pjS26u0EfI2Ey67ZFgV5vRlgYbkYPPj/vbiTb3J+fXSU3kwqoMLmE+vZTXP+bv9r+2//q5/usOeuYVeJ/+uPbedbL8z6cRmTpMZM4w23JXdVcfU7yNa+p+rf/5i+eL9tm+PbHPwjthBGwphnBpt6/3cV2mNxb9fox1PVxtHTiQ5Jy5uW2zdmXy5bqnfKw6h6XjeC06dv+xW4ExrCIGCRQ4RA9hjpNlLtJHNsw4+15PN22bTMnoJYY7mU1RlQmqoxON8K2zZ+oQFpP9MMQDYqeZ1GFBiBIHzVa2varO6rxw+9+DObt6abWcdznnP/058NxNhSQhA5HFbTuUyAlCRaGVoO32wXh93d56PWup8uUxtgFg8fwEf/qr56OwqPO33/ZttGz8HhUptxoZiTEjs2BNpiFOd18LL7JJRARo7Lpfj9Ptc4zI+JxfFJTWWUTpFfLfUC1e0zk89PFgKqqlhqNzmynyIaMhBr7/tsAqs6sNkKcjxRlsNiG2ygSKLem/G//cP/h+fIv/+Ipuxps4ky93AZvF7CqddYCd6hWqaUygxqzJUnQ6+mX3X9+ub08XW6XIcl92be4fH5qiZiQrw9NAj3P7DpNTYu3eRfYqrePQ11mFX418On56XE8np5ulTXGiLBtd4equ6pv1y2z29hVFC+XyNJ+g9oELU8N1N4tIcxb5eRli5Q29zZzp9Gq2902lkNdTTiY1qh+oIzSgFXJ2Fa8PV0vX38g9P72FmO/hEt9HKda55GGBM2FuF1MRhqHTABFs1q7pGY/XfdGz7OHdJr9MPD1Fi833na/DLeIA25uHPFy87/7w/zDr48jJ2Al+DA3mIVYkLJotonM83R3qoxmrrVsNBMcM6cgul22EVuo25x5TmZ7WFdTauXSVAyu7vxk5LUMTe4mNFulMoJmpc5SA073YAzvMin3YXTfLrvIY54xHCSoc57/+Y/f3DrCR4xznvsYLVFVxGWLM/Pnr7eu/o9//+s5a48o6XGcp7RFPI68z/mv/+XPv//d0xZjxNrFu83ik2ps2UJ10xiC6G02gEWnFSkyuPRKUzVaaommCNxsdzcq22BMCjSEL84HHNwwzgkPdrUHjFaQkaJjcS1btBTtmZZig2MblJbYufYKkKeAYsNAqFmVa3mxdlrJaRqXp22M8frLt657g8P1/Pz88fbalaD5ZuqGSUI8ZgOqdQUMFAp0IrbHzP44ThLuMuLXj5qp50tDY/GJw7BvW3b/8dc7Df94r//wD/PP70JPgMfxoNnws7UMpUM4hmNNAswKRwRTHObbtjlZ6wZyN6oyq9ITBDZ3SZkZ+3Ca6KqU+uNelekRw21Ryev3L7t7dXWOcKDNrWb55qUlVCa63ZasAXXhc5Sv9bnMsY/Y9/h3//ZfRVhlvz/ycc73j+mOzPpyi64+ZffH7O7jnPsWS7R92u1Pb/Z02X73w22M4U4tCVzLlqrPZZZGZfUCbd4CtJwUhNBIdRFGFG2hpymJhDt7KfDqMRzIgv1mXs1znvt2cTd0ofucHTFaZesljZ3KTkiCd5XErHx+vj4eqeyrL9PYRKV6qnBOZEONJoYznNsoZ+xbb2M74vmX+2PWvWGu8Ngul+3tG7OKhk9E50AhSlp0fhPWWKJYU09PF5ru//ddbmPbzir27MSc/n601G74p7f8f355e7ldn29BG3//bR4NiT5s2x2GsV5NHIEY3t2ke0BytxHeNAdM6ONxRHg46aMbtVgKwGjLOA4pYunHgLI+WRKLbUho0SOAymqHZfUv3972GGSPy1DJnQ2SMDdzs52zuwukL+cbWxahbsKcPsIh/v2ffrldL2YUGO63G7YR2f04ptv2+78cVR1uJQ2zxlKN+b/873/aNo7bjufL7ToEqBsCbQnynwe627BPhTsJx6JbRDKWUfw3JjTMyWY1G0bKfKhAaTbdQbooEXQ5NripIKC0BHIsN/aS74wwcxp6SfrEmV0p///M+OG2nT3vD1QBAoy+bayy6GH83RcPd7cBszPx7a5r7I9DcJBWglALOrtbLxgOBBsyLBvAOskbCLNt7KkCGOrz/fHji/2xsG/+w9P48VnXzbdh74/6n//Dx2X0zy922ccxK33Id8FVYpOjtKYRaHCxCEHDyeGEnDIS3T6zP96Py+YCs/qT3DccZ14v23XfhKVYkFCJWf3+nvuIBXtS51BIUoMsD0fxzNM89n0U1AKF7nJ3iCUZLatXazhBD8jMYLQsfRwnwP/1f/s7gZJJVQVQpc65WABAEqobS3MUFs+jX97x3/+rv8Tvv+IyNo9msGTGbhAOUjACXe3OlrFBJ4Qsa3WwW2YeUJPbJxOxYK04j3NcLiNiZqHVKXMKqhIlM69sA+Y5QXo4lsNk6f8NhIWtCIASKVjEpUoCGjAYDICbmbaNVYAWhcfg0lQLyCQJEUf3ILshJcy7+3icEM1MgrsNNwgGiwBaRtFMJW8scFBUKctJks9Pz6V0VglHPo5zA0Xq41TJX089/tS+TTdcL9hvxrVP2PL1NCj3Mgboi3IktuVMNALsGP71+bbtAfV51tP1Ys5KNVpdscf9OK/XSzhndmZnw8yen0Z4PM7awkijeRVac9vHcOR1b+XXL7uZAUjNbYxKdZWRn4oZsARaEARlbaBof/p2vh6nCe5hFNBnyhlmOKtU2YoRVYUW17ZPbzVIhGPyehmG60CjWgYt8Y+wpd+wALpUn0qheZWIdpOVoduorgLaGAaYNzS6J13uY7kuIJixtXhuqMTA2MKEPI9wW3zwMK1ggNBGY3dDmaK7AZlljjA7j2pwOb4NLRXnHMLyzNk4uxXB50u/XPYFhGDM2uy10Q+o0C4pz9NWrwKAqp2dQkYRQIuf3mEZpLNBurE1W2FexMdssKvt46jrNs15APez8alyl8cWXuKCsW2+QQYlYS0arHourglAo1Skm0yCAtTiOOSZ54gm3J19ysNyVnVXpg8b7gJ1ZozhRAvXy4I4AQIsMPbhUl+v4/0jz/tjjA1hxKdla7GXc5aCTgPZnWE069V3wCx4Jb496unS4ThKb+/zx+fRHY/Zx71i1FV4e7SRt92OLC8DcdvjrJkwgGjhyKoythk/dTUAqmKTCRJW0FiNwmFsQyQ6qlN0dTrL3NRmnPeHjddjv245q9WfFv4lU8jI7tQjj4jlGSVoPbMMdHcyKWJFMgBXdbvRiJxJCwSNTnNCEknBtDvcNRxgNFQpN7ffblMQpIodHoNJ6JzpWouZSJGEkUY1ogXncvJpfQmClLtbTpgIPR73nVKxRw/3px2XUfvml3N218LP7/fTgafn+ewS0oi2bihIeAOgGwsGuNvaLVZezgh11Zm1BcHbbQ/3bBGMgawOMwvrro+PKeOIMYZ1V68pttITyyPUGo6sWoccEN/u54/bxWljLF0Fm5OA7xbmDfhSX2TEMjQ6GU7sIyJs81FN5ePlNtwc9LHhOi5QSv104Qi62WUfw3kmoIwI9nh/HHg78Zj3M5e3UyzAlwqET/+pqWiQmYRkQbhCvkarUTKvZlaiy8Oebj9dtlGZ23AzdlMCC0Bn5b5FdUugeJ5FLkjG7uUtQKmqMPYh0b0p60p3uAE1KSsl15inaJtvTe9uJtANyRp6VL0dlEwwUI/OXiS9Pk0V4Kg6tby+gEEEBxkkGyINVmvyNzGIlYsBUKjL7bmP06O7+X7wz++2OTyO+1ExAGCL+PLlEiPMh7m3bDlnHXQjhTYNA2TdbSUbMFoL5kMqktXKrOFOerbUyk61qss2JyGwoDxVNT1Y2Q1cRjQwzzliLJ8gZJUSjODlutd7duUCF2i0FGGEyMjMT1s32gxVZUEiYBFet33QdgKQIvbuHsMpptZtwpk857xs3GIsYLYFSwHo9ZFVwtsDH/PbxwTQBsioarPPO6tFc0pyAxpig62EYAYaaAZ6qOeEDd98MDh2Z9GIFmgGtTMAzDzg3uD2aVJTVy8lz8PzLIhdsrG00waN0d5h5jaEQnWF2QpiVp0kA7g5LYzRknW1hJdbPI81gF20M4fJzNA0X4oBP8/xTwjLrFYBsRCT0OzVzEZ0gt1syERK5+PsmV3r9gDkqfbmTFuacFZ+3E+b53W7Dr/FgoEIoIAWwgEiANE80dYsN2OsZI8gG+HmMDvOWo4ASGN4YHRXtTxI2hicZ5JO9HA/Z615v9z+gsK8SuYLD/m2D657mp9mTxFzwgffj3q67vM80RrrrJFkrdYIu+y+9E1Roy+AhF7JaAlS78PqEs4WwijBJLlaaBz4OPJP/+kf3x95nNmCy1fzk7lshl4AACAASURBVFhWgGHbmQkaPgMo1NIRYVq5oqZQNIUNCmoZ9PF2v15GVkFddBdKFLBv4/Fxd3PFmI+j0NZg2ON+3G4XdLvreByXy+34+PAx5sx9G5nVzGztY++cZADsxqzazMA16LHOJBoJq/bS2vmxbmZy0DAgwAzInGuqrtGIJgAUotcvQQB67QxEwLDszaRR83EYkOIOrVBTkPuAHbb+mprH4wQQT46nm0SVpJSsW2bNRvZUK2LUrIJk7sxlhxfawJm9m3dXZfc89n3LWWBRtnyqVVq7PxlqzCPPY1727agy8650Ytws57zGdhzTQmZQd2WGW0IQNPtxf3hu53HuEXmeUDsRJsCoE+jrdfvpp2dw+dn0uTJopRQAUN0riQ8REn8j7yCr1sdxP2f+4c8fv7zef31/GLvbDIt1NbJMgwwqwSJM/SlGrVj8GgZEt+Tyz5ejAHYmueXMIGceNrbf8oI156nt0vcT8swj3DEdzcfHQ11j287HaTbyOOYyGqlmldt4PB7jJe73ednQXa1WtQI/f93+5q+ff/qyG/H6Mf/LHz9+eT1p9piSSlJD94pWdhaRGLFygkb06if12uUnFdQyUxmxbkeIMMLDcHSyA359vijzqiR5THy7n8PG/eTrXWYuYkT/8MNPEYwVoYT0z1jxExGu/J+ggjkodcsotAEEJXZVd0AIxyyTdP84t21cdluPGXDn5/BVS2DPpTR0fSYZSbNPqE+YQeguG5a1fKVwCuuZDjKzz4ObJNbqhqbvDpmNCNNvBiBgeREoLPMvOhbaWJj209EDkbYaprL619ePt4/5cZ8oeqhoXAFdSVD3SYgNGFvVvR44IVWs4IVo6kMSGN3pDCPI7hWztwUD2s3PmUR3E63qXvRUkaTQbc5a3jeJqOqm9QoE5axtHwK6WNUkoBVc0MXtf/x3v//v/vVPZnac+cvr/P2P7//0eg8bf/dffl3QsGnH4WYIDgBqhyFgRWvlsOUutkI6LdaTFCSseBoWiaKVJmoTs+v9/XEZum0yd+PKxSvcWtnVMFTi9duv5trG5fnlq9h0iWoVGY3uppu3lX4jElY0QFhmFwLK7DHWMzis1D3RKnDk56McjLbmCCBWtpkrZ4bOzHCZCRzQ8q03aeaOkoRwJ+qcj8u2LQ9aEP88ZFqwzzcOcMgPEgRXZBC/LW9totajBdqA37yrDTZkDS0822hBlf1xn9/eH+dMQfokBCF2imsXpFb+USuM9Cks/+YkbOXqbHOiKU8jsyl1V8mY3TZb7EWVkKDhPNKdrULBx/KjrqHbREsrSsExTKJUQDsA9OK+RRpFyiBAx2yzpvHpGr/7eaeh6tNhJlqLMBvhhhaHhG14wM9TIJwAbDBno9hRy6Zh/wyjsQC8RILJlVy37s7WRpFNuiBpApKto5jZ5YL8AXwFDDAQDtD1OSEBsyGUjORweilXCoNkVtM4Oyt7G1gGKnNGeAtCmQ9YZ2VLFq456S5zGEm3GCsaObuEIt2sLpfxuLeZnz0dQVfLRC8BRFZJ7C7+RqJJIFNdZr+183KXYD2po7TiDARBwD5j4uBSAlZ7ABR8Zv3y9vj2ep+tqWHeYC2Ps8xgBDbZ8Un3ttOiVTCnwdBwc7LRpaZNRMMGzNsKPoop99jY4AhPlQdE0bhfR4PWo2eNfeT67Baa8iGz9TPHQz6CGb65pkCYW6pWQp0IAe/3+X6fK8pVDQPMMCfOUhWhSjBzftnx9nFvsO1Co8SqpLwFUkkUkUIIy/pNAnKgQbTJx2IfCBI/vnz5+Hj9uOvIWttReJH8dtBNpG2b/fTzMy0cbHIF+iUYpc4m2b3FBrbaU5+MHWlOWgwDwnh52rt7OI3+ZYS6heFuqlaEux5HhXFcL2G2X0Li5XoZ4SuqAsCN5rLb1Zd4RI3hFr6LZmbmkop9u10i7OvLszkqZ/ckS+5ajlUujaa0/qoWuSh9clpa0ZnuJJf1U2YB2nqSyErkHmd+e/t4+5gzU6hUDa6R9nlKzEyqjevzILytnQ4Hs4oUBZlQpTI3/r9Evc2WXElypCn6Y3ave0QAyMoqnqphz0yzd/P+TzGPML1kn64mmZU/ACLc/V5TVZmFOti5ypMbICPczdRERT5xdwiv+xRwmy4i25SVCZHhQuQcw1jFSoKkGREnimZOI7TmnFUY2zaROq3AfXMRvcxNmJdtI6hQAmQq7Ke38bc/X9wdyAypjJfdbg/+j3/9I0IoRsoRTpUjQpC3RCXyPNl5YQCiqTKUlnCHQ+M5eBDNcoJoP3wGdZV8/fZeq5epNp3XKWbuWiv0tyKA+8Fffvmmotuwt5/+pKJjbH0RiMjAIAgxwqhpKs9V/NPHHZCZpMCqzjjZTh/py1VzDgMk2kxHESCzBHqe59wuKiWACCNr81FVwxBZIqzIp3/GXAU+7TwjVs45SJqIkLkCLKqxByy7qD4Ah6iw2JZTIBJ5q6ostsW3f53qWsNVr0qx57QBAZEZ98e6H2cGn1KStM3dBCniZEGHmGKl6JMwIi366aXZB8oFnf25LMrtflz2HQZ1Z5IKaeH9aaGTY+Xt41FMMVy2F5Up1iHCEnjxJOlm50kxKZIysjqGCHWrDFWBoFjF7ff3+PXr4Z5uXIskb0cdq85kZkGk4Cvylz8+TGSo2TP9RvT1CwXU0yFLCS+JFgFCOQQKAWgKsbY6Vp84kWdPZr3IAxKqqgURV5SktLoNaUmi8gSynQhiBGr4DGbbyl2h6uO51ZaIUgMQxyM+7o9c+cf7LSuNeH15+9tf/6RsTzOIrFCCVMy5CXieMaaZ2BiMYqSYSQGqcmSp+blqGE1FlhppZiBQTOTjkS/7f876bZQAGxSGEmgnTaqeqX7Xpwqe0cmcei45m+Txv//RLDke57kiMhSqjVnAE3TELGoJkFGiogCzyES2PaMECpSrZglYPddoFlkiwsiIEoAooeUz7CRJ/ddffs9D//yXz3/6+e1x+6go6iLhri6oSsn+v7e1soDFSmKf41yLrHbtEUJmZkUUmRFk9dHOx6qIzEIhWbJO5gpxRFG8zYaGXkWDwlJdApTABSgAyjaVEzT2OdPPLd3mfH17+R5LCqpY6felGssTR8BclBjb/PLlVQEVgxhQ+gw4036A2EpSlRlUGAkyE6bP+ewJo/Ph9X4+zsxIBpfp7byfa80xVJviUdBSMaGIZj01GdrQzFpniFnfX9ozulBVigWaVKi0eoHGv33+9GoufQJBCEGn0irxnP/RMRy27ZtQUzERKiuzJ9MoztbVJEEFoTor8VhxnlEoIaEGVEdHE0Tp84zrD7IK288BUFhoI6A9bTQGqibquZDK6vV/AW6aAKBV/H67fX+/rVNU5acv+5z2eFCHJjF7hjADxzNDENGrFFUxAKCioApShZtPl/z0Yj9/3txMFKZiwOPh+7d4u24ZWWBR/+BFR7pBKgGZZtz89i5OsApaWeoGET6xDuBTUetszQCltFAFroxv399vCxEQ4/TaR7nOfTAzWZXCfNTvv/4Gyhzj5e1LCbL6GUXSkFATZpKiUvLkZnhxVU6pbNJCTJuqrp4VKkZvHUmm2xMYmczMoS4gqiIoJtNGrJViw9U2U5EzKcohIi4AVaqjHCw5WSTncEDOk6qRNgVCrCpXAbIArkwW29383MRIST83SSWfi6F+RUL68yc6++uiVlW1Is5VK9obkQ1s6Pg5EeCgZCXUyiGUpmQ8r2oWgRTpuJWxCMU25nDPdbK1fmIlzawyidqnf6siSwwvr5fK7EugpeOKgnAVRP08Hp34MbOW3wKpBNVECHGoJvO3r+vffnsMV1OY6VCcZ32/5WNlJQooarJATVSt9E0hpSJAZcrYQMD0mV/zFoFMtfBcVTYQR4e6Wn/Qp88ciYDZ04JAIqp1sRKFll622aS1TuBIHwdtolJAJUhrt5kIUSBVrYcioTzdKOLbfv0iOn7eV6z77bZfriVaaEesu4q6oUrVzOVcWSpCS5SKqlsVxBgrdFOBQiyJYWYmxxnm9v3bLS8c7lmkgGpFgtb3iYn1TgBPTaMn/f63H9S0vispbY5LEqzP1zcvJRjJv+MPoNaqx7mSAFOBHpJE0gwQBxWSKamqaqMDVgkVQo2UEpGCgfV8mBh0DHUDVRBUmWNGJFg+vI+m68v1n8e47JNZKSlmY3PwSdrIzAmqzTFGZilS3fLpjBoq1oguNTPbyBwmu4v1xi4rCivy28dxLJo02SljMfMuTEKeibok0Fb8pkQIpQh4g0aUYEmxA5plIm5qw1UIk8tlzzzjThKPEyq2RHTxkaoqgyL7eHm7ipqqRJLV5ly1djwBSFE3AUEBkpBegpWS0TnJeDz8utun12vuWwIV+nK55MpvX9/fXq+Qqsh9G+xx2gyUIVJJc2sOYGWtVUlB4Rar0R6udns/h2Oam8iXt2sVifr0eoUIV/StLaLFijiqEjTIDzN/4yqogCs6u9ditvQN3IOZQmAugopFZpVH1BFZhUqPBl1KlVLUlJaVqkpEUsBwdUqABcoqGeiMmvSWC1Qw41zS6n9lBfEKaf5tspNUry/7PufYjMlkZNQ6H75NyaqePqkZSyCCyKqKKkFFDR/JIPlMCLBM5PXiX96muRGooGt9f4codpfNrcBM39NN0r0ZkSSlYqHlYIipKSQp/Q3rqb6a/dM7oGOtv//9l8fj7GXH779/zTOCaozrsOt2ThsC1VVfP6pU8nH79ZebqoiNT59/OmLxFmYo1jPsCBelmlV2MA6QHHMQrJQ4FxKujv7+mkhBzRQUsd3mcINZJZtTXOZmVnzOy2OOPvFFSyqHtaWRUNumAuDZyChPVApsupqZiohE5xMNWhTR4/YNuQAXmP7IJEq7C6T6BdQvn07oU54yiJi/vlwjeSDgmlVr5Ypee4DPJIz8WD+ECpSursIUrdICVFVa6qI0vSMpKgWYilFN1V1QSk1NZu8RTb19PFDARxMLO8arAosVPWdKSUoO1zZT9557qKZStblr2g4PCgr1H1/X//iPD39yRLgW/ng//tc/jvcDq0qAqFxhomSdxxFjzsrKzMiooDzNAQGFJry/xwYkQWBRpUrULtcZ8RCBqr68XN7zm2R1SnulK6iaKyLVFBxD395e2jhIcBi2bdzOBR3t51RNgZ/nWQlzaw7uuWKqCWrOoSauVJXjWKbKasshI3ObG1QFnMOzV55V9oyfQAXn49y2ISJKtlwrhsd5fr99/8vPXwA6KMVaK8GtVwIRBZoqqNm8IoFJmO8iD5JEktbDFAoQFlOpWW3gat9XUiSZ/VEDpeVHigESmbkyqwTJZHT6rinDrR6QjKbbEsx+tYokxCrbZd7KYxE+1CIz62yZsEhmW3qb0Kpm/XrTc2UkwTIxUZDZV5cAmWniWdEbhJVLbTBjEcmqkmTbiCQrXy/48jrN1FTOyF9/f9zv5+OxwDVECYUKa604RVcUTbJqRS6SALKKtbLQoVYvCmFPAoxQWQJs019fX89jiTygZurDJQoGyWKmBkwrbyFSneF1s9mUJdXNzKdv3/mwKhgISWKqbDZCRa2e7DfREqp6j/VnZjz4FHFFSwDo9To6BC8CHwqYqj2OQ1RUMcZQkVjVpg+qROS2z8ryOa+Q3on55sO8yFrRbgVrpKV59muTLKqpjpc/2UerqXy+ZJ5bYRHRhg+QAMREqZT++5agslcLJKqkqiIzmJUUEbFhUkCJGtpFrQ0yAwVju0gFS4mAmjydyGQtsU2xCkLmOnPuvk0jICEEYxFaKhQTiPjwiCWqkmVuELjZcZS5s8pgiSc1oS2vw8TEHpmN/muPY/swhHjZfJtmpiryOHl7xMct7kcis/l/UepzhyV0m/4Ah4gxAHForaBrdLZZ0bmupzovTXFXmqpvm2/7pDCj3t/vRlxcRWK4XQaH13Deg9+FQqk4v/7+G6Fq8qe//MXEMnMONtyO7AAERAWZGRRVilpzXB3kYmmcyTxtGNwbNQ1IRoBcsVTEICtim2JQlpznicJxnvu8nLGMsjKlcq1zH8NdxbXOEKGEH+dD1W4fd1O7P44x7Fzx9vJqOm0OZigqq5SZkms1kaynsJ5+oCJVDbkC+Vx26vMxIAEexx3QTlxXYSUjKoWgKItChUhWKQQddEcuwCzlYerKE6rMzghKRnUewaHMzKoK3t4/7O1yHOfmcgSkNFHTWdl40FFrlVk8jjnGYx0/ffnMjBLEceq2ZQRKVy2DJTIr3UYcD/oORxz5g/ZqFfjl67n/+7vCivz6Pf7+j49///VxP8jTecuhSPB+HJAgyocTKDCSpkL14S5QKqRQoP/8eYxh798fNN0vu4q5+dhMYe7++dPrcJzHmSezqGar9BHIwmPFSv38us85IaaqZiaQbZv4zIjchhPiJlnJnlVFm/TbopQBQLKEoiSryoxurqYsUOnmjEWBuaNyDFvrFKAqton7EVUjk0AJJIoZS1XjDBcRqjLFZq6gakbZ1BZUWVmlcQZfWGrmnkuaBraOP6RONQdAqZa3W+gqMoupRDKZTyhVrzoR32+3dwBAJCIrPTvHAPOSStIwgKCg5+V+yS7QfxBDALCqWIJGVqSwqqrUC+kipiAqI9Z5GjwihS7WyaXByMpVle3JESlmipQIKpsdUQKwlvQGXTNiiVqSldmGg375ixoEf/68/Z9/finw/ZbfP87zcXx8fDRi0eDXmav8MuUvb9sf7/fjXJ1UVRNVM/eXl/1+W0wp0gz+17/9/LLv//r3X8a4/O2//HmOOXyIipu9fL7++c8/v3/c19LffvuP9/ePzPUR8pFtc97Mxr/8y3+9vmw9/0jbfapI3O/3PF4yckw5g9+/fWzuYiJiVfFMxFZSqqfpQomyOmlDAIiV3TFQhUY+i/SNqkSRpeb/6TIGsu2cBaKy0twEkPZIelWhVmSjS9pfXGAWTA2WD520edmv16v78etR9W9/PFSqQwVtGzzuq22PWkiEGrWciqJ4QDXansni45Q5xm+H38sSLjbdq6SXJW1nLaI3e0tRgAGe1RtVATKeM1V/FdvjRlGgvBpeRHk63vr841IomzYIUWRRqyGYEP4A+GTBhBRUwoC2PhQEXFmY6k9rCauNYqIUyop4vx3fPo6qEyoETAUyVTroFYIqVFKzElI+5tyGuUU9VlEUIHyM3aar8HLdP71+gkEhrFJTUF7ftpeX69uf/vb+9Z++fv16f3//+Dhu9/vxuImoqO/7vm0bgFihKgTO8wDF3SXoZmOzDSrFy3VjPX/BEN4/7kXJjM5vUsV8VJZZN3EIEtJ+XsDMIrIo1nZEdYGCC+h+hlSREpI0s7FfK9fKmvp8C9bTOGYQRDKCbiQYiQ359vbpPe6hr28//5XD//aXf8nII1eux8f3j4zIyMyMdZDL1BgnbbdSqmgBEH5ICVmY6tfd9j9f5eXzv9aguFzsv/wfUxAZj3Usiq91N9VKUkH216qeaUu28GuiZFAoYqbQEofYj72FiriKVZWKFLPLDMSU6Kyin4gOjFYyIk0BZQWyCtDSPu5MMUmomch4/3h/YL3dHplnZVLG//vfb//f34+I/His37/VH7eKnK7Gql+PMjkocu8Rg/myj7nt5/27EAAet/O45+12GxtAWIl/+Xwp8nK9Mnm73fqB4+7kvc+VMcb57/8mEtuw/U9f9v1+eczffuH1su3XS5zH93VU5pjDXI/7WitUWeTb2+VxHGNorPr5z59UvQ1dTfa6XraMynrOpswE9LGWjyGmorqZqYmbNZJ8brOqVAeB/bIDuOiAyJyjQfZKcVcRHXO+f3/fL/taa98mz9O3IVGietWrDds2N5Pr5aKIx/3dtw045nZRtTPCxywxcXUfr9ubdjCwiVaxjvNAvB/HEranBxn5436tVF1qtRCHmAtUVfVycRDDPx3HOeY8Hru5dVFSrIi1VqbAKiIB9CqROtxYKTJIqtLMRHUqUDBXus+CqFaZAFNFTNw81XxqQUxlEFRVH26S54LJdV4qi6rQZ7uAqaBMx0Dt324f37+9H+dS0re3Xx72P78eVSXiP6wzlWRwHSnPNRlCxIbrGHO/DKnMjOM9atV2mcr68voFOJNmf/vrzwIZbjbgahFLVZ63H/m4fYzN8jwf90djSta5QLns++vL/vpyEbPGkgjxuD/qXPvmcSartjG2YR0/36dV1nBtveUHqIeVpe7TTExVlUlVE1UBfdo2p3Q4gpxugLjrOlNUVa1jPwJU8jhTlfu2uZrp0xbs7lW98MFl34rIWAq4qULcVYhptql9/7iVX+bl5bx/xMcfzIWixAMk47RaCmiV8kScU3Kb++Xl8rJvQ32qDhNlTIHmWuc6HydUtssFsMfjtuthCGSZQkA3lWIxOvA1HZv7Ps1NXWlmPkaz4FRY6BqVGK7uLgBzrZUgFbAnSPrJOYuzyFirTKSKz8Y3aLFEepBocQW5Aqin0oZGk+Fc6/v393WsFQeziOr1lJrt123OuU33MecwM4+MTD47hwrmOsaMSBEVcm5+vWwVNIH7UFGf2yjWly+fCsyotdrxVyzu+9jGm5kF8357/On6aq67bYCayTqOkhKVSM59VNYKmdc9Im3Y68tLrKyqfRutNc6pVTxXqLULxtQ4bUNmqVZQgLEZnj57E0FWsgvf1KgK0E0As8ZSCYZrJBVqkyCbeb25zzkjQ4UJaS5Bi51lRjEA5saqklpRGWc9Tjv+Yx3fEeft9tvLZVxfX35+9Up9rHzdZMU43j92kY/ALqtEH4e/GQ+bhcfr5+3Uq6zb+/d1lEZC4+vbUQ/M//X+h89j2wcqRZp9riEJcbiAQmoGVcWmgCaLcB2DZBUm6hlfYWXvagLmQ0vKdGCIUgwtxBgNw2dE5yML0mGish4ZVAmAmO4ZZWpq8qO7rsTt5bpfLlKRFFOT/bIbJOIkUVEqoipD9ahSWdfLxiq1Kfp0GzArI200WJUd2oOI6sB5+BmhnaurTObw0cUIrNjGzCJML9MbOdl1SzaUKG0Uo9m2jwZDiXBuc84yNVGZc8QZx+M0UzcXoZvc7ofR5vAGICZFDCufhitJMedaWZE9bXZGo5MBWTUu+/D+UuZ5rOJmChKqBvBY8f7+cd2/JAPFYK0IHSbAemSLXgCOtTJD1FiIOEcRPCxD4jeDxLnM1c7F2zqjViFqllPqHC4Km8YSZpVJuMwEzLhv2x9//PJl2z7C7tscyhnfI7G+//avt2PbaAJ1dTVzn9uY5ksbfWCKsSKiYoxRSsnV7YMqlsA6z23fIcg4mjaj5ixWHk8gruiTv60S0Y2RFRkZ5epkqk1mVlKN6+ScyF67ZkVGiT9TI02Ta+S7sCKSjCxWjQFpRIPkcKmOWMKSZdDu5nqsJSKVpaoRq3K1yG/KGuLTXVRX5jrXyny7jjlnh5IL4m4fj/t13y7XOceWZObjsntEBPj2du014Lfva9/GNmS4spDMObd1hijm8K7keBxrDt+2rZIrK4v2TKyYCegqgozFhJupaVUmObetbYyAmOlxZka5W5FqI1AGbU1SCJHctu1x5sqaY1SGY8CsWoiwZ5GoPtEwCRU1Q53sGEkrduT5WDcMfFtH1NLK8ah9bKx1medx0CxzZaZsuo5DcKL88Tg+jqy1wq1YZtKHDEqqUEUxwZKleS4e5yEwgVI4dNgIENBCaRaGNy7bgDChbm5cRKF7cvrvqiOZHUgDSt0A6V0YnkYIm+buXsmn38d1jk31XpQ2SGRQh13n3r0+Yww0tXdVv99du0RBtn103KObjXwaUiH09u4WzaE6OqbFYseB2qxQmUJ1d+tM79z8oubm2h0Fj8e279uY18smgNlU04z06W3qmnM0lxBFHz6GgzaGVcLh2i56ETPtH3RmccDMiBRRMsy0slTZWZ9YuWLptk3XSJQKiiogqapZHGNEJrUAmqkShYZHaLubSAz3ihSQcbr5VBTZh6KSx7l0PKF3QKG0qpAi9GQC6iIo193ni73uU359j1XmWEcc77m9Lg4lLQINLM51DieJ71+/6e2W+zUCYXsoxoAJCjlai8suyKNSKlFZ0ylE2RlZKBA8ZBXUe0AVGAoiwz1EzLpljG4euaT3E11sVfShTIoQUirdXdPZqx8WCZFcEfUkqZGK6rUDVqzOUKKyLwaJrjESNwdKhbFKVFyNAKimRq5+v7ciiaQzq0MU6FIQ8Nm6FSLT/u//65869GZmx7lMOoOhw6zrAECeK4V4HKuiAL0/QsUgQoLFM8rVMjKiIFJUFmPF41zbGACHDTV1s8yurQQIgVXGWsu7wzYZlWOMbio912ni5h2MlPMMoO1uXV/M40lVFRbPFc2I7hycKLrca2WqmZhkaUQ+AyzFIrr/QVQyocXb7cFMEK72iNg3t+EQYPNTdbteoeO4L6s8h+5jRGaSbnYkXYUmUfjnf/7Zt+mTi7Iej9d9BviPb/eoMDURKT4dyhAAqWDBTUpUCybaxLDOH1IysiQL9yPOtXwMNxNYx2AgKiKZNZ7LOOn2TKB9Cw3epVr7Og2i2qhwClTm2Az0oWMMFFYsJn9YBp+NFioqkKwG+LenBixEZmU2EZpPzwdaoREUIMN0dEcgKS39Ad7ssG0ONRHZVMWHqUiVknS3jJzDPm6HeTdBAWSiBEYWwW0zUmIVFCtq2zprrFe/qIn56LUW24q+juFDRKoSYlubfbNgeoGb6uNxAFAVe5aSiIg+7VlVanK7HSvWvu//6f4QZKxydwDDp0ipSiUeheOM6Vbs6aRhJbpWVfUSHVVVP2RJF5CL0DNSjpvj8oQOn+tx5veDcpEsD1Xdd4nQbUpVSqDkn//6+f/5b//027fH++34+2/x738/zdWi4eU2DECpSkfrnrE8UiQLo6mjU0cDmc+1VARjPstW1JsjZu5qjt6IgZkK4dhc4VkpkEFrz8cROU3NodAz88dRp6yuLko3KfUqnisVMuckcRxrzo0RUFPV3O4bFQAAIABJREFU9jSpKYtKfervIlk53M1HVbV96awaw7K6XkES0lvRXuyPkmD5x+24bJtOlWSRR+Q++fq6wQbYTjUocB4x2JJEieJxW9d9Ayszc3VkDJV1u99eri/Dzd0U8v5+Mx+VIapMrIiowpkR68un17UWC7VyZVzmzMrKHPI0cAv4/f1+uV6AMqEK3x9L3fc53LQKH+/3OfRy2SqdRGVApLKicnfPTGZZe2Irx7TGp6mougzSFFU5XBHVCUohABPiLDKkJM39+7G+3UrJ2OBfdmL4ZTOTfOi4zIkYbn2zq9rLZd6PJRDCXNGh4IKYCFA2TehVByhNluzTpSCjH4MlRACp4iBRdIEZBbJvqiJTqr1QUWWg+mBWstFlRbiDQF2G/WDBU5KsHCrVhZ4iIoYis87IziUraGTVmrIHqcwnog0AKipVB9Br8KooukRmJftuHm5JZmL6c33HQlVnckpFM8JfrtucXow553Gsl9f9cRy3AyCKnG7fvt+uLy8vLxOiw+Xb++MyLupQK1VViqmuDFAeZ/78p09iVlGJLKSZzKmq032APFcIEJnnARgktRglUsTH40EVFPfhEBxHDldq581Jcg71aY3nUlUXicSKHE+pDwKqaP2oq4xKCETsXMtNIYzkca45LeM/SfxPJwYpxaI8vev/7Z9/uu7bv/9+O7MU2C9TmD/t2/ViHweHt+GgXZCtcP3v0iUCYBCHcJfnTzF+zJDd2ozKZ2hKdPH5cHs2Spko2xSOEKlnCA38EQh2AGdk/6mqEBMWprmoZJaprkwT0pRZomK7TVoRCjHpahshhCZTXWxUVpsdxpQSYgyhZmJluBrIM0o8FUrQVLbLps9sF7Y5znXm09x+2tjOsyDIhLmCEEoBoqKVjLN+/+2dgffv9wrWifs9Hx+PP/7xRx0nMu+3U0mu2N12cyXv7/d18v5+P28HoLdv9zjz93/8fr3seWZlXYZxrU9vL+dxIvH7r398fL8d9+P9220zQYayHo9HZt0+7iSzKs6439ftTFDWWvduQln19etjnfn1+72C9/s6jjjPE1moNMHj4/77H++//f5xe6yoOhdtbo+oYzEL92Ot6hQJxXC/n7dbrEpmrcQq3h6H9OwCSzyxH9/fz+/vp/zY8+w+rpe5T7vu2zYaVtc+VxBd7iyAFH/E1/vTITATkVnQVQjKOhmByJEFIVWGmbuOMadauxAIFmgrStCNh12HopVg8f5YALI4mvbYtuSsMUwzh0us8zKdjbNaoZB1P5GIM/oLu46AoJjDfQwdPwxuWbxuc52nqR5nqJoK1HRFqrhAq7KqHkcQ+PbtVunHsarqOPLxSGYZxjozz3ClVEhmHieLx+Mkxfudr3hia/tHe55rM4iam2YkJDLUnkm7ntBwu93dRIVDaN18ve1z+vE45jYVMtz3ffv1tz+GeqwAYWqZYSIrQqCZBWJFmIq7ZZXtlpGhAiJWMKtUkQfEpQCTiqy2cOkzR+QmT8riyhOPiFzLkPX1++PlZWdlrFjbAGU4urNCskz1/f2hZhUBnypaUlJKKQC//HZ/fYl9GkTA/OPjY7gc43I77o+zbo+gcC28P84MAWROfPn8tD2hH9rPxjgRgfXokVKKMWfcP8w0z4JkBlWzjy8ghJIirspn+Ybl0xDIiFNtYz77d3UwStS4soboM7dCPx9x2aYwAGVUGs/gNmRVjlIxzzSJKKKixwxm5rDxeKzNLVZet7ao6xIDyt2PR7o3RU3OMwTKYmZUtXeTJVWpY8iKdh0PqROqSFILUsJyNACvqp+ya5UoJeFj2rlUn6WPY7pCIvJ2P99exVSz6nrZjmNlLHcryGXfVHVsrsDctuOMOcdwr4oiWFBXFTVRs05zQFVMVNWGaUX6mOt8CAQot1lMQRWFhWRFRFaODDXLSkKNFYlYmZQIcbMnz2kxKyqZWWeEj61T46JHNpBL9TyPnn/b9qNC7ddtYXTvbQl0gJaVDCXzERkpQSUj0854vsMufRM9wS94MgggQpiguv4XlIzzfAjFbJatqqXNMaQ3ZgoSiqGohAtSpFQhRSVYtZksVlYR5SphJhQzMQgrnwdr+9qTvlknBRUEy80AkmlW3n0K1GOFGyqbTfEjSljRbbUsirtImWD6ONYJlAgoUvlMSERWt0qqgFkqcqYAnc8SmKqIqavAyYIMstAx8Fwd4R9jrvhWfaXZk4JaZ57H4nXvgboyH8fjOMfjSM2WYSiiR3CtPKP5rW07kyLmZh8fK6JIqFtWiox9m1VJaEbOi7Bq233lELFjRffskLWiUjDGLCIjktxft1xZhXMlVUDJBKvmvsU69n1mRlaaKJ8WLACaFSxWqzelQI1+KzQAkdZ2IVKGlgivU7c5VtRwN7XHWddds+yMdRl+JlRxGfZxu//6+3tWvX8cj+NsbVkaD9Tuwe6ei66iShtDsiraJ51ksJRs9VREToiTYsKSSBqgoqbCYbpCzESS2W4UoQt6ad4uQDVxNdVTRcyVKgZxlWC3V+t5hG/Ks+8LiIi69W+pUbpZ2f0Xqmg97+y0ei1gSOMB3KPBkRA1jUhxK6ZgdqVfq+IkS8RfXq/J/OmnNxv6crlsl5FJG1aStm33xe31moVV/Lgd275tr3uAWdx3h2G7XP2ybdDHSu2QZWa7ICPz/rhHQUz2fcvkuWplrSLEutjQTNP1fjvU7Plm8/6BKgyPc7nLnG7WvrRqwI65SqESxxnqnlVuXsgiIjPvhwhVTKiZ1TS44IrQyKhqjiLMlc8ttDQytMlJhZaNS8UbCG1SC1RJUzXF5rqSqO2yiRw1pm1ut9vj19+/PhY/bufHjUSpKpKmEOmAF9U1KocaRUGM7fVR34VozVxwgnQr1rNEpqogWlCgslIIqGZ2x5A0+L7RlupPY/8TvADtOrOqGtOSMrydSLoqpsiKVHNQzf04l1b5FFJEPQsBVNa++fFYqp4oRwNcTcyBsvEkN7XLu4SqesZpIllCER3uZqXF0lVhgLtqrfzy6cXd9j+9ZvF2P8xHkW8vLxCZyifRVnP4MPPh9vmzZ9WcwzwjZL9edqa5fzzi5WW/XDYRvV7HSr69Xj+97aZ6v59m9va2z+Fj8yh+/vSyVk4Rstx9292Hfnp9IaimYvryso+hJgbFcInIlTmHU1iFjFQVFVx23y7XyCxAhwzTFdWz/T5mkW5S8CgCGJtWdYqhtQOQUNFSRx4d7DD0gU+Vio6R8XTRzXQJ7RnAxVRPs81lKHox2MQFYOnTG9GQyZ6AoQoRNQjzg43LayVcoFNjmTnN7MkpAiESlaowKoQ6/aI4zvr85Q2mc3qB00dYzm2cIoBcLhtVbAxzu1x3VyerWFKaWnMbkeljzi2bsaSm+2VCdOqIqDH8Y+X1smVCRMbWp6hn5uWyqYrtQuC6jaRUHm3yntMBvL7sqvLpOrtqq1AulqhtaJX4ucLdsv7T2SqXfSZZVFaZmSpULbPW5jBUMMECxzRzFRV3azhKkWvFNsxMMznGEM3hNnxU5baNlZzzmf/OoorYME01t1wxhqiozEb1oEP0bEMmMDcTlbhXCX4gwOBuuWLf53GeZhoFg64oU4ja43HfprraubIrRgRAVUUF6OZP/66YmqkqnqqEF7kqVwxKmeg+NMuG2bQaBoZsPorczB6MCjHXRTgZVZWrgoR06w+0YWDm0p6RglC7LDrWdn1Zx90qCwbA1AGYSLGQGZXuShopwwc71yRk4hHRwNXH7UigCqpkLRU7jlPdGJGR6tLtJwKsqMwE5XY7lDiPs5KsWueZ4qaaa5lJFiBh2hBd6ShNVDAp0GoOmYBZHUlTExNNVkRWwaQ3T3AqQRGYWlQ5yG0MMyX58XH79HpRtVXxfj+ny+tlMzegYtX2tkfxe4TIHKYidj7WueJ6mWtFcy1bBTpu58cjxjBVJeR+/7ifh6myqCrmlqsKrOKx1mWOrno4g12uCvIImpMlK+qMYNFNMiFEnE9NrQRKuI/MGl4qMqxnAj0zlWFqK6lRELCLTVVFzEZ5+5WlmlimpqqDGKiCUgTDNx8OwTTsQ4+wYbUNvZ/xwjo+BFmZ4FLVDNHbwj/ujxTGKRWuszcZABW0Sn0GhVEi/UlbKmOt0+YAaU03lABni3MlFLP+AFKiIx7bPrQxpE0vEQkRZflU7948tDFBE6KdmBfrhOLU6hMVFLJs8P3j3OakyHU6iMO4bbOeQGphYU4hZAU0KC5VDY+RYij0iPz06RoroxUdYBsqXQ0B69seIlXpTk9wVQWqonzOo6DCLBmbq+pROaiZJWqEiuECnKtuxxpuc/i2+xn0udn0jAKSghKh1O2Rc7qakTSVtda2z3XmGWGq7ZFbkdtwVYEakgKajVirkmdvJE1QspBPx7Jpv1Stfxkruj9MZRBlna4j4liBJ0i9VE20K9siIJqmIqpVCdDcRbu2prpZHhJvL/NvP11/evUiH2d8vowCpuvmej/5YhRILr1OKWBzd/CWmeRKHJVn2UVEFZKd98sj00vUKAVRSEkR1KyToLNghi5MAQJQgapIq2hnBlT23kLWkCprW0SyI8tISGRpDxF1rszlTyNHFKQg5qql/H57XK4XRZ891fwJEzkfJ0lRRWWuilisAXBQk8yugqdEsmlJprqYREXw47EU/eV0HyOz+ZXJkm4byookPVa9x8O0+7yVGSVtN3U3/ePr7XJp1sQz9CwwYTBrXvbKzOD9/lD3l/0zpvQIT5GdmitUqEJ1pc8DIoV9jOM8hZxua63r5gpk5RR7xDrOnKMiY9vMrG3cWkWpWqUdkhTivtZw66VdLiagyqpChVlTh60AydLhbUuFQdEFeCoUNZlQGPVJcmzQcS+DzNXHkE+XcUaBet38/aiXbezDbic/7fucKffj5TIPrGFiKF98u9iZte6qZaYq2qQfAdB/CwMMGoCApnBzSgHl1q6mbEucokuAzcB4OihEhZd9K3SBnDBzDH8m4l0JlIi4VUgp52YZ1TEqUy2BQFfFE2JQjT3Si5tZA1ERWTZGVEGtjzEITVDBMQyAi6waRfQTXl3a7mFSl21LVrFirWK5eQeAnmKsmFa5D59zQKiiGeccA61CmVTV9bqzl6kEAYWcQTV9fbu2Oc6Gztq2zb5+f79ed4OuCh8KMjJAjOnt5Fz5aNOR2/j6/l2Iuc3MTIOpnpFJPI4zstzUzEmuiOxkNp4JbkglNaP6vxAY5hFRmVUL1GfcTdRFo1YVM8pFV9KUIihUJbtsktVGvKeGr4ISg6zkKbi6CanTW9ZXEajCTN8+bzsF7/rXP73gj/vmEsVvv72/frk+zoq5jnd5JoxFn5SMEgpDUZ38l5JEaaC0UNnUKjR3TAKpAmgqyDIaFNj2rZLvx/0ZkBPO1Q/0J3CGlMfthECF71GoJhpxTltBkRSUQL9/vZuing3pTQlhCyTrBBGqOofHSkoeXY1EZCQox3mKws1P5Fp0k3WetcLMIFS1IlawP2rUU9COiKxSjyhysZnPlW9/fllVLtpYF4UU5HFfK6KzXFlE5fW6STtgSy+7gf9/e+eZJUmyY2cAplx7REZmVnXPExySh/tfDznDNy2qUoQWrswMAH949SZ4CjvIyAgzGHDvd4k5zVOyzqTEoCwMIeDrrssst8cSM8fIJtjEWUSbqlrmSIDWB2fQF55TKsAT4DSnovQrUrijag3uQzQiDCwxoyE0dZVSJGtA1BgidMyZTFBlXSH/qqpMCFl+4IuDo7VZBkRr1v8zr1x+WEe1sCbAAqkGYwprgnOqbA1a65yRpvLBULCMRjkyECoJGigKss6Mudh04fxINrExvHbNhELApGBBgFDV4g+7kln7dlYyBowhUBJ1ABlWU7hZYdlsySGqqEgSseKsQUDr1xwhXeOaDJGsyATC4HxmXrlfygJkENGY7MhmQRH1wYhgIAIAJFEBATAWFVhUgZyIrHEqRHblMyurN2aJGQEKH1CFlcgJIQEksTbGXFeFiLCARVIRIeCkeY3kUGZBm3Js6paAWLI1uMQ1LleMNQ4pqxCgdeR8sMaIKoDmzJI5hAAGZA0CRW3bcpmzsei8UzYxsXVmZslZyFLpTXCkiMucjEVjSNGvJm9WzjmzKqmSs8WaqyaKpJl1DcuxRlj4L5gEIJGxxljkrMuyoKXM2VujQCuGBJFUGUhJ0Diz9uNEsiY74ZpzIasmwfGqHdb1O7CaKyytv3UCADWE69yeVpHYeryuY911nEEIYKzBprSPOTrCyAyoqopACmvAoBoQIcAsbIFwnXihqmYB0Qxq1kEbi7r1fhRQiKgWkeeY1GDhvTGGU1rWADMUZUVDIMTKhiiTxJSFMXMK3qpKmlkBfEDOq3GMQWmS6C2t4yQRXgRU1gxxYFYRIGuImdYzVmRO4CxYsgqYsliPKQqCAhECIedpSaK6DoMMYs6z/JiLEwgpiJUsOWdhsAaTgiFVhZR4WaJ3jplVKeZYFEUCFlEklJyNtffHLMpFUTDA2oUs8xx8vbqSCZSzDENkERBpy5ANTYuwKGcuC0+IDhENqWCKLCK8OoFZgeWH+4RAVnQGGFRMLLxexAqomLPExKBSkAP6AQRd4RAimpJYAjAIgOvbHAQYVjWFrqpgzkJWEAkURREAQa2uAOq/0IMrCMT8eHcIGdM2hWeY5hsh/qWzAlVNAgDgnXVel/gX0gpMUrAE/GN3LIIgYlXYOiAFolUYa5gTrxpUkCSKGAjXkTEbJO9tVYS68CCamL0hQAUlMZpYVswzKXFmay2QWhsQNWa2zlpLROgMAhBz+mGXBZiSEqGwEYks4HBViiDaVbCoa98bcy6LoCo5c1xmAEyZ15xFUGJVBAEGY8AZAljRvbimlBjidZ9jq6q430fv3bSIKhTBpZTJGgDIrKvZpO/rGDMCRI4eXMq5CHaYlr5vg7PjNFvrliW+vPYpMyKtO3/vfUyMZHwwY87B25LQOkgRyVGODMbMKRsiH9y8LKAYczbGpJycsTEvjgyrGmNyiorog9VFQdU4q7AK9BxnSpEVYcVupsTOEhogxBX2zmtGg6oPVgWJFLNkYUJzH0ZL9rkMuCpzhWUd1mkErLMC83q7wHokIqLkPIzTFGHVTqooghKqRXSWnCE/J0ska6CcrgIkUAALlJXtOr4FQVRQwypxEWMsGgBUAiu6Wp4FMAtT1GQRQU1mSVkeYySLKTIRsUhwtCwLWpdS8tYAJkfrw5DhB7cbsjCQQlZQmJZYFCFnUWEVsN7GrKqMZAjYGMqClnCa5rIos67CKQKAzJJzMs79hWeAwrslRkSUnKqyUBXOmhVEIFjLkkhsBkYyABnWjmEaZ0O4zHkVbMzTEoIH1YTZe384XPu2RMkxwTgsVGnOeZ4iAj3us+mr220MIUzj9G+/PJ9ON0QBY41CWxdv7ydyxbqbAKvBW2fteVrKIgzLUBoT54VFm6rglH0oDsdbVxfLktiqCEQWVVnTAFSZyMUYSx/mMRrj4rw4SyqaUqqqEGN21k7TJN4DqndunGdv/bzEqi6VgQCNg5jFGTPOyTt0LgTnkAwCisKKXckqUek+gxvyHDUmHpPcHnHw5Ey6DtFZM2eY54Q6Xce05OytOT1iWVgAuU8aU17jV3jNJcd1KiPrN8isA7A1yEPFWrtmGylaRBBla4nUiHBSNEiqmGT9rUhm8MYJx6rwwxgBTcq4bfw9zwBgiNYB/bxEJEOwfm5S+TCMY1sVykxIKupsYM19XTymmUUzIAFVRRiGGcSIZEDgyAC4KhYWjcwaDEzTUhYhpyjO5SSKiigW9LGwijpHaUkFimR21sbEkRMZhQwWVERkiZmsQUARRkRhNpYkK6Aimpw5x8xifvDyReeU0ZCKKud1CW0IUkz4V+Kis8Zba9YdTRQ0ZMhxZiK72qDLwvtgzUSivCROMRsvKSWWwCxrGySKRGSIisJOkzAzMBpjhnkprUOELOq9TZENmaQ55YRIhD8i0UCBjCFD3rkMSVVBKaeExiloYrk+prYkBWBVVogC6opqU19TGj+Gt5NlYWa1FmISBTFIMaY/DguhsoozlBhFFVHmLP/6eKhKYlDRvit+4EGIkMA6JCAl4IRJmRUtIGSxzhgCMAkyGaIsSRCJYbUoAYJBkTXei1kESHlZVu4rGrOev0hgMkNMqShcSrFAAMCUkooEdQCiK+ka12FYTnlZb1cRmeckLM7bKKACnMUG55zzRiII66r9xtJhQuEsDGAJlx8Js5pFvHMpr9YusJYiASuuEd3MqsTrEtSmnEVkxRqt9It19MGJhdmLt5ZyVkVjLMmYM+M0L8Y6AC3LApVFldAI6LLEOKdM0NYls8SYraHI6oNTlbVtYlVDJuUfXGBjXcxaBhtjAlHvnYBaZ9CgMzYxxzm6KhCZmKUMnoFR0VqjIivEnvmHGOeH6EJFUSUrelyBz9baFXnCzEhWhdCtaYAUV/HGuhYQZSpN/YTWxcRTWs5zzjMrJ4a15+fVeu+MKpICrwhWXh1ngIoZlQEIyU53/bLJlsiFYruhGBdh1rwKdQgNcdZ1bJaBIBECq1BmELVq8sq2suvk9kfmNgCAKDhDzCIr55UAVFLOiVd6DaUsQXSZc1m4LGws5gw5a86yXqZGQZWCs6JZRYVBVJ2zK719Zeyv1OEV0bviCevC4epCRAFj1veYqBI5QAFQFkTQnBMzgzOqkvPaqAlZRFXLOdvV/qwYc3YWOOtq34uJx2kWXVVcbAwsCxPZmDggIllhEdUUU3Y5eB+XrKqry2NJOWZelgxkyFCMnLMigoo6Zw2QmFWJJKBgDJXeimpmQDSiiorWUczZB7v+DYQgAkUo0BKlFXjwA3uytuqsq1fUIVBMMRQIrOpQFVJaE1pgteqv+umVF/sDYgoq5LTpFIkzEwJ4b8Qaa5kD5SQ55YQLZxFJyn/tsQTAMSYV+UHJNkrKgBxT/t/v+M8vG7S+7cscc0o5S1ZhTjEJWlAmNaCExII/srCUjPywDqVVxbSeykiiKKuNQU3iGNMaKoeGjKyBLQREaAgyI4A4iymyNT7OS2aWNalQmRGLwloy0/yD++isZVaFLGrW+HbOEAWCc0uUzHmV0WTNCExoV45OykrGIqIluyQlIhTOWQE0s2ZWWRGSqsbYlMVOSw6FF1FnjM3gg0spW2tzZmT2zlnn1mtonKP11nrXUuW8I0M58TCyc9Z6460bl2QssWpWAKI5SRSpC59VpzmFIqSUkYCZNSeyOLPUdSk6GuuQGC1WZfDBkkEVQmsAkIxB0JgFV9WGd/IjIg6MJQAi80OjSGThxz7CWOcURFaSp2iK2VhVAGNszIkFVCGlJCqgKZOJDMmsK+okCgDoLMn6trBiyYuzPyLIlNfJTk4imhUiKiChsAAalJVXK4D6cR0mQR/cOmL1AEYNEalkIJPjYp3hxIi4YMy8vhsAKK8Ng0FiSKuQxGBCFEBMWZSTgk2qS+YoCVV4YUMoalhRf6TeIStmARFJrEZAROekgC7mbK1jEWtxnLN1BhURDQAsmTNkEEfWJFHvHMYYgo+JI4OxTgGts5yFSBWxDHZamP/Ck/N6PILPKivvwBKJCKIDiGaz6XJms+LKGUQFVqFwZGOMsRYElyUvKRkw63h2JX2SMc6Y22Pc9J01tL6s7o8ZwWSk1U6oSr4IIvjDc/UD7Q0pc12tPTg4Quet99YQgarzITjnrCE065G+ut/M6lInAlhTVEwIzhqbWYwhay2uwxUEay0ZzFnrMgChtQYIrDPreokZRBgAY85lCFVdApEQIlKOy+1xH64no9L3DSkbi2XwKpKWJefZOVeWRd1UPjjnXVWWzq4SQ2ARa621aJGch7atm7oWwKauyNC6tffOWGtC8ApaFt5Y670LVRkK74tQVqUJ3pjVoSm4QhqIDEIGaKuyKCtAMMZ4Z4kQEYkoBAcAPqwoOLLWGEIfaN1QA5F1FgCsNUSGLKCid4QAK3rCWWsIyJA1lFkL74nAO2etAVBDEKwhonUJaRBWE6kCWO8RYf3UUZJ31llHBG798RM4QwpgDRoUBTGvX3q/2uAMAqo11q7zKZVxmTkDgs5x4azGGSIc5mUcpqwKCsyCBOOckFAUxmkap9mFwpBhFl8W1+sjFEVivt1uVVWjwcxsfXE4nuumneZ4Ol0FKSWOKWfF8+WhSGjM4zEC0bykJSbrXEyKxpB14zgBGhaIMTvvx2lJnJ1zogJgGFSyrBYgAAU06/zL+ZBzygwCypwRMTEbMiF4MoZTBgJhSCnHZUYAG5y1VnSFGFkRTilaUmvXBlaXlA2iMRjKYNBY5zkmVABSVkKipq2d8yrAwJwlZTUG8noLroBWRBHNOf/FyEUfgiFjnaurEgCbrq2qcpmzcwbRBO+sM5mZiIyhnPmHLmMVAqOxBGiMtS6mXBRlTALCRG5eIqApq2ocFx+Koipvt0coC1STczbGZFZELcpmmrMAhaoex8m4oEKX20DeLYmzZF+W0xSJLFr/GEZjraCZ5hjKMjHGmEJZpowsbGxImX0oANySkvWFApHm1XGe0hTjkkRYs0jMCD/c0cJsEYwhEI1JLFpjqamrEAKSEYGVMnS/D5fLten6dtPNS6y79nS6+CIgmc+P97JufFXe7mPZdsfjpWoaJffH9/cs1hb1t/d9Unsb5nGeiqo8HE7TnKz358t5XiL5cDqfrAu3x3Q6XUJZ3e73OS7G+ePpwCxA9nS++sJPU7w9Hsb60/lyH6ZQFdfb1RinSPv9uagrFb2cz67wK3O6aurT8ZJyNkSH/VtZF5u+c4GaphrHkZlD4Q/7D2vNZtstc+LEcYnj/RqcRZDxcTEIw3V4nC9F7Y3JzLzb1JwW68g4v</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9a5Mk2XEldo77vRGZWVX9HMwMBiBAgARBCiAM3NWSlHFX2p+gP6M/po/Sd5lkWi1ppl1RpLi2CxCvefTMdHdVZWbc63704UbU1GAwgwEGJCBZu/WMVWdnRWZGePjjnOOewCt7Za/slb2yV/bKXtkre2Wv7JW9slf2yl7ZK3tlr+yVvbJX9sr+/2789pf3BJaeAorxNgiCYGZKImBuIEkrRWa8hL50KM9u2m1ob2YGQARJkgoxiblYCKX4EnG5q7vJ5uq7XanmXljM5snc3Ey1lrn6XApM5yV7qvfooZ7qkYSOS7YWICBIuTSAItl6RmakIAIAISkFCRJISBIIiKQSNEAAKQgaHxECIJAg+dEZWX8mqXs/g+N3AIApCeB42GjgeBdutjuU6UEpZky16zStR6TRCCUkAXhwMU3VJAg007ffuvry491l9fePy39591wdZqRxLl6ctfpusupWirnxal/3uzJV30++39X9ZPOuFFpxYFexrzDCDbODxFwwG9xRDHMBCzADHR98iGcv8folHrwGTMALvLjBzQnvHvP56eb2ePWHT/F7TzDtMM7++n8AgdZxXHDbcG5oiaVjCdy229vzy5t2fVxuT/147svSW2aGXh4X/g///Z+Y87hk71HM324mwr0upyNSouo0WynFvZR+qPxv39p95VD/n7ePf/P27es7r05frxPP0il0We3h7OY2z4VuT5/s9lf7hxfl6jDvd+ViV3dzmS8mHCZUx+yYZzzaQ8DtGaeOlojEqWPpiLy+Xm5PzUgJ5xY3pz4+8/WxtZ5Lz0gZITGh3tGVSMKgVAJGE6UgTIUmIjV8i5szkgbSjAII0m31KBpsHIDuRhAG82LjJkwYSCNoPp5txqn6G28eDl87XByqBW9+cLIAQXerbjAopJAReOsKFzNIZGIJfPl14GsAgefAS6AADhSgbv/fbT8YcAXsgRnYAfZPEH068D7w+q/yKwm83P5cAzfAGTgCHUjgphz2xYn9VIqBqeMNb0PTXJld0QTWaj7Nxetu1y9n/Nm3XquRnvjZsTO0KxQJ8th1SlxUezDZzs0N3nM2lJYkl6alhy1m1opzFmCGQgTRA8eGEE4NkQBBAUAxJEB88Oymn6NUS5qMXtyIqThAcxqYCRgysPjwLuYIZaDZ6oJGGilSKZoN1wSQ0OpmkJmt8Yl3QciMKG4wOkmaGd0ssQZwNxPYA0Z6KRezv/HkgMs9ripoF7eOo0CDO4Y3SjwHdhVPLrCvoKMF/vE5bl/i8AR4ATTgApg3P5s295q3nwvwGKif49o3wD/TET8EZmB/75EfA+8CL4DnwJvAm8DFFskEJNCBDpyBE3AEzkAHlu2RW+AIHKEFNwtOHdGRwItjcXJE2X31bzzdXR3tf//htZHmruwJSKKy93Y6hYLv37SvXE1e+PpF/dGH5x0I6NR0G5qMu8IQWko0KFvn7e1yms/LrkpadsoshLmfd0acHAbsJvQEgNbX9HYMRCJSLaJnHpe8Xm6EY6gJCXRJtARrtXlXANKth2r17BhJDaQToEWmmRFIaXiOGQlqpFPRVseykf3djIAMBpptzkUWN26/a+R4QjFPAaAbp8kfHip2BTCYwRyloApuoKMQAFLowGHGVGEFcFTDbsLhNeASSOBdYLoXxgyYNp/bAQD2n8PJfgj9j3h2DSOqwYhimA2owAQQSOgGp4ZiqBPwTeAK+BDv/0c8O+ImgMBjx8UEs/WiRCKFTGSiBVpgSUQghZ5YOnpiCUT0nj2jN/SMHkrpxU0r+8lynCrSiC8/nK4eXFxcHD549uLYzyZCAuE0Ka3yw9v46mPrsMvJLiYn1BLn1Gw4VDOwp4qTkXSzzGXBs2fnJw/lVs38lo00mrV+rNVrMT8HpoLqaIGe6tG6ittp6Uvky+vl+ra1Jd49hsjiZhxRKpQ8tX68aYIEAzXV0gFzK+5WaKVkD9IIJECZGdwIcnxeF0XRCGH4IteMunobjIWksZi7Gwkzu6u3aO5GdXmxYpyK7R/t8HBCLZDBHNURgg+fM4DogQJcTCjDjRwUvvJ14DvAU+AAvADO9zKmbzFsBgoAYP4ckezv8H/8CLcnYJSEAAEIRjiQGrcxBBhA4vEP8XCHt2/x3ovlpOvExVTm9wjLzb0QkpSRUiKUGjdzKoGUomdKmUhFJlOKzAikMqWbUy+7aksbVS1OTY+vrJayP8yJR+fb68zkWrumUtfX8bPn5++8deHOWuyi2qOJP7vJQ0kfiYSr04fJhC5a4qfvH5+f+2mZH1zk5ezzFNPL826yHiDx2qP9YVfn6rvJW2QXKJxbbz0jBUrkseuHL863HSQL4W7VuSusw3ndDALRz0HAEM06QNpCo5vVyUHCbTYHAGGtztcyDDAj4XQRoxIbcYs2oh1LsWIGUsQIf3C6WSTMYWZXczlMBa/vcDGhOooDjkugd9QCI8ZL0wDDYQcONxop6Q+BN4ECPAOw+t/qZHeBbcS2Ed5+qf0QN+fWk1jbDmXSaCQQiszQaJQgpYTnp30keqCrddwKiAjV2XvrvYUiJUlQhBLIFNbfB4RQZiJGuEoklEJESoqUgKVF8XFmjSTPETvn5IA0zbWUUhlLyI0yy47T7fnH7x9bqBhn423Lr1xMrx3wzo0EpLKnhRCSgSGYFIIRH1y3F8dW3PeT7SZ/cKhfeXJ4fFV3Uzke2/HUQfbMqfrDy9nMeg8zU4K0U2qJlGiFBEMKqXUdO505UpmbmanQ3K0QxemUgTZukOyCmYVaHK52HDF67Ri5xfI1knEtxUiaO0kWdzeaOUyEjee5UaSIYr6fbF+9fmmPi4q9A3tgAoSrhuvE5GuJlgKAuaDcZcYEFiABAD8DfvhxP7vzsGl78PMEs5/gB+9IcPMRIFIaVacyFVJqdOVKDW9IqfU8dGnRsUW6tQDPzIke2Vv2BKBUhpCRwvgow9UYKWWm7lwPmdlTKWQKQmYURM7VSWYq0orlw53fRtY6z7u5ou2N+wcXL0863p6MfP+2KTXNXg0JSXo4ew+8d+5MyhSJNETKTAFayqgEkUpFKm+X+PC2//jZcZ79alevLqbL2d98sv+91y4OuymRt+d+c2zFWd1bj1NTJEQUt1F5YaQvsdbCQilJqOucMiUJD9HMLY2oDpeRuXc3shpDcCc3TxvduhmBkTqNBqO502gjIprZiG0jnJEszi4WaJ7K4305J9CEPpKUgAIICJSCWuAOjmMn9ndOVoAFeAg8BSpwBnjPt+73AdMWzz5P+f8PeP+GpVCJSMkMozpd61YMgEUYwTtEEul8EbYoTkl3UQllj1LcS8/giGEGJUGNBm11tVHuAePYCUHrvyRTMhBgaT0PU41MJ0Kprid7vriNeWdvfPk1au3grgqV6ZbnjCWyToUGJ3uqkA92nsAH5zCiQyE6EAIju5sBboJWyGqFFIDW8/3r84c3C8gfvnvtxKPLPs8lQmaAsLS4PXcpIxMAacg0d6UIFi9mxWare6+1nG77zYuTlIWEsRg74KOPSYGowN7Ni/WeFDVQL20wmEYS3UKZ2Qhhbr7FS6wtwZpJvYABPX3jAk3TKWCjfR7OsKxpcVcxF1gZ+BuQqLvNzwam9zXgAIxfGSX/XeFvHy/UPg+EcQb+ESSmgh4DBAQCnRx50lwZAGBAIM0MigTJbjiSACdlpZFJIVlqidZSoKAtAdgAhyQbkRFkUkrKJIFrQw4DjZirl9M5DoeUYKSBx6U/nKf+PFJ5XLKdF0HFWee9uYO+CC+P/UuXE8Sp+LnLTQAf7kzAiyWHE0mQjQIAk1kV2sgaK9SpURdxzV0abyAij6c+wNWAIhQpCH1tVAgCmR1ycelLRc62M2MCoAUhWCZRPYmIpMyguZgbxjFSMLPUaAFgRg5cd/gYaIY1frm50YsZzHzFPNxJwNyLuzsFIoWQFUMaJkfdbTV7ogemgmkEJwCGXWz/OpLmHni6IQvxiWqsfPyvnxHMtIFV7wGv4/uXQANucP0Bdo7W8f4NXpx4CraOFoj01hHZw3oPIDMNDAp76sogoK/Ftrt7CaXIjBGUCdqIZGRqdFhEIk1KQBz/0eAJK/aly6m0lkqlRomo49KfHCZlSjqfl5tn7xbi8ODC9zs3K84Wevfl8ubDycjZcYrcYxyel5On8OGSAVWYEjKkcDmzlPrei1OIUkK2ossCTZACaC0iIuXMTKE4R87XiPBrxJcogKY16YGoxWv14dE2aAMbENxA+wdFYTOTGA69HWz1XGgUyISthZf5gDNIM/PRVXIEMjgtATe6s3ghtdzEVAp2Ba8fcLHfUp4BhrJD4eYu4w2Xe+DCGXhzC2YjSPi9kIZ7P0+fGcxuNnzLgW8C39wefxeXbwMPURxf+RBfebGhXH3DvXrBbVle4u1rPD9efXDKD27tpoEdhSdjjNznXj16KEmuZEuSIxfTDDnSgoG59jUjnJlE59Xev/Ld10uLHJClAKXOTY8mGhURtU7VfSqoRjPz4nHk0vHeywUkDJPzpn102Yy6nKxLNy1DIBSioLn4vPf3X7C0oGieaY6KcCgRCAiqtrSMEA0SOmIc1GlA5keBcIRAGCnAQFIZUibQD/syungjAaS5YnXQSjpFmEBphD8frBI1cP0N2jFwRW5pNoIazU0BEmY+nCyFBArNQFTH5YQnh80nRvgh0O450Hj/dXtOAgX42oaKHe/BsCNL3rWcn+1kbwMX92LeffsS8KXt57c+9QDTS/zeB/i994B3DS9WoBXL7tk1/uGdfOcmUEuJFj2DCQhpsFFNkcqVxNOaFgRARkqiobp//esP8C++WTLZe3qtKSWw9JyY+2LKLNWH87bed0gjq5OzvVgyU7V6NSwBYYSoERJ0Ua0JEYLBJdKc8uLfqfYG8denOHZMTGR2g8/uBQ6bCm7O3cvo9uBGGAsQQk/mykJi6wiTNEA0gTCXOcs0U5kCxdHpaMCKIZNA2Qj3OfBarPUqaRBgSqaNem5ztY8wWiPMTMXNaWYmalAMboZqKI7dCFT7e8V7bBVYbn4DYN6w/gY8Bh5sV/t0z8/uIIzxMz/NQ4AfAAQefO7q7RfaFXAFfG376wIswId4+gM8/Q/2v/3f9vwMzA+Mt0v0UBczM8KSOQplQVxTpUBiJEfAzB5dVfzF14A/Lok8N11UQTIyRWQ+2tmznqVUekGeoweU5tZlp5YfXIvAVL0auxRJQSKUSMGJq2qNuh2ei1y69gDc5sgrY5GKK8GT0CQkgykVShGQhZlRRNcZuXT1HHgXzEbZvjYTAEQBSZpkpGiczGk0M4gkuoRAtLDjAmOPUFv7SUlmbp70AiEgSyTpyTBSEI2ERPNRunkxWnE3JkT3qTjmguqoBvfNme5CS27X3rbCC8Bu+9cAvnLvYt/VbXULfr79yqfZh8Az4I3P8cxfyUa4vQSeAke88RP05/CCnR9ODS2jq2e0UIuInj2VmZEahZCgQR/QOBV//ZuPcPFHwB8XCOclLg+FG5kcXU93fPeFKs2K50L1ZIbRnNrP9YRcenph4WAdZCTXdgQSIFzNhiVvQz3JniXzfeEi9cDwhnsCz6RbAoO+FlOKECHJBGQmgFyxHiS08R8EDNpaijU0rYjrCFIUMzWoJIdhggN5Wp8yVA+GEeZhTlJdPDXlpAkAUZNBuiCZtrbJyJBtZAHcDcUxFRRHMWg4VgIBxHbNRllmm/f4xhoFcACe3ru691Pk5wxOPwGugbd+o0523/bAA8wVF44yIYjJsaRneuQcQotzi3PrS8vW4qxIcSAepMz5+KriL78GfBf4dklgsJg2mgjodukP5xo9bA+vu/PpthqydS87GnuL92/y/du2r07CiJaajBpAcK7ghRNXk+WiJdbS+zr1D01VcEUDzWjO2bmvcHczhnRuAqOmrdokZAQiE6M3FYxGiVibxOHZEMWPvG1LNGvbO7x10/bQiN1ucqMENwPUO5amFagFQEvQwYSlKDDXjG3FbV8LaDSgGEpBKaiGWla4f5zmleip21/9HtC625Lmax+/qLstFn5Oew4828Qdb/xm/OoX2DVaw2QojqwgUBIJDAigxbx0P9EYkVJXZOTQkhmq2+NvPQG+A3wPQJHUQ71rmmAkhGPLq4OQET32h7qvD908CGU4WcxluD7Gg4d1FDA9VG0tuMfLANCWQF8ym9C7vMAf+fk2lw43zruyqzDnxb5c7UsIETq1VooDa3I0skVi4O6CgOJGWp6bGTDu+oHnbDXM6Ic2pA6jeIBggt3xmuS5w51TcQKZQROBJqV0AHyVpI2M6YMgcPepOs3htgq8qq/M7Eo0TVuHuNs8Jjbodd68bci57Bf52a9kz4Br4Bb4KfAWcPFrudFn2xl4G6cFFAJwAw2uQczBBj6rUlW6SPZAD0kyRyVffzjjX3wT+P4ItyVFKZceu9kBGNRD+5LVFKcjwaS3UG+ZapPhwaOpL/2mZS2ksRqWxAyuXRyQgIQQxj1/OfvLJRO5n+zxoTyv8eJl37lNe9tPJHxRdvDRRT12RMiolmFOwLqyR+YKLAJk793gYRCoVPW1o1duINhourf2bnUzDVddRY1OsvIuFiaglcxENRMVUoZI7Glm5u4GjtoMvol8iqM45rr62VS2Gn8CLrY+ABvcMIRi+63TfPCLruuvZNdbRn4GvPtP42c/welttAYJDGDFglZECRtwBEBMoUf2BDXOih3+9EvAnwF/MI5VBtW1tDSuJzAiXXpU4oPnLzN6C0CC0d0fPtgfrvYgs6K4uVs19D7avLWz2phUgQMOxaHgLEyFKYR0Oa0Uag8ROnU9vzn+yE6Pr3aPr+ZR8yuRytAA5qiECNNABVfsbbQ6o8tdPQgYz9t8SBo1nMCBgYCgHeYyTZ6JANvSR7dkZHEr1YxMaHa6wTbSycEB4GLEs+qYHHPBfkI1lDskNoC+NY92T6s4b95GYAIefjEPuAawKcOOwM+A3/9iB/yF9gO8/cFWCgsymMETaZCQQCZCSGXE0GsoZY5q9tXXD/ijPwH+1d2xipCSnbsMKlib+KL812/521fzudVz15KMVBdCnTfPk7yl97yCsRiuAw+l4Y25Xc8UV1Ru47Pn2S5mmwof7ooPYD+iJd6/yXNo6YJkJqel1NaaCG40IrW5z/CxUY4JsE1zvfJF6wcYMARoSIJanVMDeAMJJ73YRPTG0VzaoGgkcwdgRjO6050+dBt3fmaGYnCHOTpWdddHlOUG0q5Q2XyPoLzzti9iz4EFeAv4HpDAT4Hlix3w0+yHOJ9RuJKXJNxBoQshABg4QI8Waj0zZVQxXh6cf/lV4M+BR3fHKgAEtIBSLHKyANHjjceHB3srdLgli8QWee6xhI7nLmWGajUz62ohw0qhMiEBQVRJRIISXhz7DmWePcGbsEPxw75c7dzJR6cekbctb8+RiUVpPtyLZha5RmeJttb4oysdcwIENtp2g/clM5NkA9mjBle8Ci0kRAysJEv1bWwABIrRQV/VtDQnDWY0hwNuttYoxUCHO8wQQN6PW3fAxJ3Yen9PcPF51Ba/1ALQBsDax8GR36D9FO//FKa1Ixr1R3GMyzvE7wlELqHzkgPtN8eu2ptfu8LTPwP+6/uHKwkOndAS2I87kVx6KsJgMlSvZRpQgNE0mNHMPC+tug2+PFe2eghQOJq84WQjj4+W88Hl7vnL84c3y3NwurZpsqnY1W6ad+VqsrSlh4ozh8MWyxzqAIM2WQWxEt5DfgkOPeLoaTUwQpOS4sDVVrmCjV82KvXi5bmeuruXQVACkBlhJqOGnqH4UJkRUECTWzHCuYkW7wq1gqncC2b3/4yqf9zTZUusX9yeAC+/2BE+BG6BR/cor0/a3+D6Bm6DHFw7eHNQiA5yLcMzz0ueInoARHU+uZrw330L+G9+7nBlVHMEWk9jGS1Z64pM9wJwcJJhg+qhk2u1Yq0UMyrFnhhqsVVXR4aQg4zkKhcJqDhff7yXdG5BYw9FxNJPdmNWaII4QhENWFq42RBkbngZV9WNABihIdrx6lhl1wZgE1Vg4IGjeBv1VTEL8BzqiNLhxYrbGiDJQrrRADdOhQCVWkKzwyiUNePCuebNgZ/5fY6o3CvI9r+KmOdXsqsv8Ls/An4M3ABPgO99ClDXEP8ZESsJMwqBJMyhdfYMIFLRderqLZPpxv1kj77zBPhz4Os/d0QDkDBJxyW0thPZU6clBkNjpDn9jlxe5c1IWi02ZPgxmj5Qa/QauVur3wlGtI5zi1LsyYNdcdNAt2gg3UlxHXUQMoeAc2im2LpWTxhcWsKBIk1Go2VmxnhFAlgpcYq0Ub9pu5FI1snnqZibYEl2oScSd9yC5fYiSPiIhFq1zWvRZYANXMPXYbWPuEtsaFm9R4H/xp3sC9rrwAK8C/xsk+9+0v4vvLP907ipiqM6nDBfw1sKqXPLc4+eMqAUe+PxjD/9rz4ZzLDFM0g8tsyUOC4wzi33OwzxV1AYY02GSJgzBcCmYoNFGApbrgU6CN0h4msRKaV0bpmhabKHl9P7L85dMAToQNJMCbMMeA4YQixyILkNWq4NJlGJ0V4g2u37cj+xFq+lVLNiXkoppiKTJWVEbEOaXCPeNq20PgoS1VjGUNRoPkYTL5sKi60tBob4eFNDrjn0Y7T3XR024tn+k2f8t20T8G+A/xk4A7ef8py/xXJeMYvxMUfUH9oGszVptjz1bD1DcuNhtt33Xwf+HLj85BHLqHxkWpoiVQsAhtCaUmt/R2QqixWBkcmt6i7FnHRnj+FYI2kiMeRJW0k1bnkiQ4OWuNxPreXt0o0GIEepPn7IBBgJo4yr4w+RnRFyH8IgkykkwSIRQFNa604n0yyKleJW3WqhwaRCFocTIwCTNjQgqxOTGAwBMIC0daQONLKOs8ztpI8Gc7Sf9I+ny/tasbvJkd9B+yvgf7mTwX7cPsCH/whg/bzc7i4AuZF+KbQ8tTyds2eSdOdXX9/hG98H/uIXvl4ZCgfJMtFTqZWoO/eIrvRUi4RXW6MagAFaQChuXq0QyxgGJ1dKgMqhqcytMQQy1SIH0lbdri6n9lw9czSC1Bg50pgAWAVf4Eiua/KDNmrJtr4AEOQDk12RiwJZqKAzgksfKEappdgqlARAQ8FI2pukak34o17ZnrlG5yHzsTHruXUAfo87v5sZqR9vPH9n7QA82ObLf87+A463QwIFB4phnN4Yg1JCT7TAOY7nOEek4KarnePffgP415/2eiYocuUAl0Cuk1RqqZ6pRMvsEREIqUcOrL8Pra6xujnVBuel1S0GzpC5ZU+CQgudlhiuFhLB/a6kEMpNxDS093CuM5XjNLjZQFqHAmxDzFbfSnJ0uWMQlRyxCEb6GI4aGAVUzArhJjdzyI1uLIbinIsVN5Fah/aGGm+rLsdnuGNO7S6H2j207JOTI/8Uk+K/nv3CuPXapyiO/gFIuK2ch68TYchcPawlTnFe+nHJHkmgFr7+9QfY/yvgW5/2DsomSUBKL27bvhocmVh6Hk+xOxjFjIgh5hoRSpssB6zVDBYYnpNYAS0OKmgrw2EUgXPLCACZTZEwY3FeH8NMBrqjliHpAZWEExoSEq1qsxXZ0haFCDazJCptMkxkIcxZvBSjrWAGEhgaf7/jPtd5JQ71RS2g+YD+zX3M6rlbca6R8yNYfNOu8o6wv+9nfk8T+9u15Z527Rd6/FPgw088+Hd4/jbMVuSs3GXMgZYFmrAEWpzOee6RCTc9OFT8m28B/+Yz3s3KBwhI6sUxHuzDZ3NjDyy971GHLDAj6MW2BGNciZ6pmm+Mk2PlhUanGesg82g0VliuZ5BMABJpF7spYrk9RxCR0ZPuqmM7DJVEphYBtdIiBx/lLDA4kAHCADh9FYnQKafFtKepThOM1k7Rm5NuWokp0gZLMfiUoWwzjDqjFhsKdTObqpdi2LQBa2gb2p+eqHd55y7a2T23++1a25SSn2YH4OYTD/6f6A1uoOBDfWzrMgrFmjQjseRx6a0nqanYk289Av4CePwZ76asICpBsEXOxebZIyRh6ZmpIIWEBSPpHhIHTADQirBq8e/uc6wSUgJI0biOXrWe584e8jHpbQRQnFeH2mKd0OyhiMyKHS2hTLTkTcMo31IMDUmXfIyIMAoAcpRCA/QfyIZn3ytybHBxsw1rTMlXpyIgpzm0jm8ajAOw3cS6IMaNuEmSN+hlK+eoTZ3hm5/9Ujn/P4/tf9l74C9oh/tPMNQUfu/ekaEHBESiCy2PSz83SSqGx5cV//KPgb/67Hdjd7WgNPb0pESCKZ07+lZOLS17ZGQmGImEpTAVP+z3YxHBElpnmICxSwDA3UBuihEZcTdXMroWpeRul4daaIPkIaFUJCTdLPney95S6xKFQT85AfZMOkCvxrrWSwNitf0Ei7NDxWjUYEgHpiHBVwaUtjrl6p0r/krZpmuzldq4i2PjNH3yatm2umd3bz7gt26/1NFPn4hAf4/liFpQ7iM4AIZzADE6gDw3LT1ITIVX330K/OUvnZIfN+p68sYqBAkBZWKJOPd1FVlKLbMneqoLS6gLCVweJi9OoKXAXIfs105gpYlWQexQ5CckJbTOL0MSpmqH2TEc1Dgm0Y9NH9zkEquIesw3jyUX42jMnIzFWDco34fHOA0qrkEhDen1KO18RCwbYzQcKJlx7IPgGqfWiVoK64x/Amuzu4Y0bb3ouAx9+9OABTgB58/rDL9Nu/7EI3+NQhRD3ag6Yf3UYyVHCyyhluclhDTi9Ucz/vi7wF/+0hdbeXRtiMHtEj0yiRQUOLU+29g4wRRajiZAGQiipGBwt2IM3TEAaxU0nDeozAFKrW4lYK3iR7VHQdzNpafOLQkq1aDrJZeuUmwdeDM4rRaWNeOBkEluIwiZGx00yozF4OZrnqONGQLzbc53bC6zMW5iPZCUeyLdDZmD1lMfs7GQr5OmWzBbg3Uh6PYAACAASURBVPZdu9aA08YEjP8vvxutwGfbz6k8XgDvbAFsSK0S0Apn5JY0lxygAcG5Yv7+65+BZdy3spVWgpjEcdGph5llJslzCy8JUYW+lnJDMJ3F2SWBpXgxnOLuxGtI9WOog1YBmIzIVAyO3QAgkpLGZp7idrGvPZeI9ZOm6NskZnXbF5sKv/Fo/saT3RuXpff48YvlP72/vH+MBjNBYjGtq6MIOhNcs+sQ+I9NHD5C5sAwmBDpUylGDWrNDU4OFiy6vCjvwtjgyga5/7GmILa+NjcQ4XfcyfAJ1P7fI5ZtqmwtTBFCJDBADaElWp5bDHXCG48mfP17wHc+z4uVNbmJY9VACxybppI95MT1Ob0IJdWTJmau4i1jX0dcNFV3WmSMmc2tSAPWvRdIyEmmEoieObkJMRQ8xFgp48ap+OWuvjh25XhLGovyds4//dL8V9+4wtM93nqIN6+gmD54+Y2fvvzKD4//0396ebMgtwEIDBDOZWbTrjK1cxxPIlTcdlNZty+MxmDMHxrN4Oa1eCmrRNvdQTu2XLm0UfWv3qW1G1hdaiVmt0G6/HwrfX7r9uTjf/2HFY423KlbhsILKQwmuOVxidYFaFc5ff/1X1r+31lZ5V02RvEoYekhlJ4iFNI0daYnetJpOWiAavQVW8paxsDbOglvqyJ/y5uCYOuCRaFLykwaRv4d5DcBIZm12FztvOTdLo5i/Oqlf++Nii/v8OUHeDRjApbE7Dj49LA82ZVjj8S65AdDtpbwUs7CRC6JkSCfPDhcHeaRGXMUfKmlx/UyhCaMzGgs7mPZqCEx3rdp861RT+gjcbrHJggTsC70+P+Cn918XOr9d4iXQxMGAKskw6AAhrBxLc7OS0amkU8uC772p58BzP6clTUfJMxokGjnBjHHfrVzl276bso5WWHVPQW3rMapWHFirc019tdR46qslctwYmLVpUGIVAoGrRuUN7B9bRGAuZYebazaY8+98+uP69VlAYXecAP0BgEZcOJQfv/x9O7xvOSQZA9ZrbnjYj9d90RmS0XH1dVM8uVtq74uy+gpMzvsyk07ZZdVCVYIQGNMIcCxpMG29njdWXe31jAEv0uUd8GsA9dfWJn9T20/h2j8NZCrPuAjbGosstuYgCVi6UtLQNW5/5PHv1CX8WlWxqTjmCcaWyrOXahsqQDMbTnj9ro/vkA5ay5l0IKH6nPx/eTVSKcZfaQg50DXcuAugG31/9Dd53qlhMyNRdSq7AckuHM3ec+cobPbvtrFZMitGvVBMgJhyILrdpjLm1f62cuOsWnR1l0/MFzOfj7DDcq82Nfr2xahqRSv5sTN0tHT52kIgBlap/glZipNq16TBiGFsRonA3JErq6G3JImAN9qtVvg8LuBbnya3Uc9nkHvrIqM1WJ1snEv3RGap2iZlbraO779LeDbn//1ynZ911Ak8LbjjEoToTGiaYXnYLQ8t3ZueWr9jQe7XS27FlcTx5zwtsl2Hdel6MaxNMiIlZBK9syBe2KtC8d6I8SqjySB4r6bcDrnociN7x0jnvVvlcTtEU+JK8fNgg+BE9H46On8B+kf3t6sEG0xOidacStGRvbQrjihc9ep5amnNaNghqm4FCkT0XuSBNPDVAiMjYTQKhpIZI617OsFSCFj8y1tyxkHwAGg/W772X37a6Df66JXGGcty9aMmVj6aUkpi2P/9Yv7MyafxwruBBG2Dmwo86rS3DJH7a49SWLpOYbRDrMvkV5STS3gBJ0++sgh6FiTpFZpyZDcCFttBKaSFDMTxVd0fSwrgMGIXTWJbizQ1cTTOZ69255+dY+3rxE7zMRFwZWNuYYPfrSEm5kNRnxXQLOrai3SnItIZG8ps3kqA7DQKnlfhU8AA7IQmTD6WJKpzFi/GCBTZlqLs8gVDlIiAu6bn8W95dPXQHwx4es/m/2XLZ3cGdfyX3fEeVtO0TINupgd//L3Pw9mdt9W/oubSFFSRiKjVB8KqzESOnDzOySTlhm9JRpQjaC5IcQYNTcArTQ2thGPnoJY3MYSAZAmeoEPimcdJlnXkkGcJ87VrOutq/rwqqIWPBQWgInDHrWjCCp4b7npOVUDrRh31fZm81ycWHoeijmSYQZMhTCXYCEZtSGvY7kQRoe7MUzrEDs2ZbD0UWUWQgR2O7ihB/xuli62Ku0OTsvfAQLqs+1vkS/vFWd3NrRAGuU/znFaIiOnavMbM/D9X/VlyqraEe84vOFqU6njKkiqbqSsWKZoNAng2N08AxRO+7Ik3j/27LBV/7H2A4O9MMOSeNni+N7pxx+cp+rVba5Wi81uU/XJfaqoxdeFU2UVGh6P7b2b/vDpjMeOS8MLIA2HHV6esDe8XNBoZvsCkPvCvXNfSnX2zINbMZivOxbCLdd9euijDIO0rpcaiiZbxZk0AJFjQSG4shlbNxABOA4VLdCF7LDY9ooJ2AMOnIALoAPxu43Z/nu0DgpuQ+QJYPRuyOFniXPglKceAHaT4c/f/JzY7H0rGOq+zZUJSGwt1kE0Gqh19S9Qio2iyoQpcwIi8qbl83N+sOgEawYJERj6NFIGlnUhMXdl3RzWe7TQcYlBNebGOLljLmWufrHzffV5Mne/DSCB645JgCMcqmAHDL0jebHfdbXDZDO5n3wu9NlpaC2Loy2aCBYLY8I65OYmRTKAts4egLa2lSFYKomUuwG0XJGNzc9M6+KMO93fFMAN0IAJOAIAbGs8B96x/53U1j7H7dtArkTTxjQBGBpq9ERPnPrN0qPLHFePJ9j3f43x94LNh1f2jiS0nKPHCoxtG8A4RDgm1QgPReTzpg9O8bIna3185V+e3M16yGxAbQmxFBaj+wA3CJg5MxVgJs4dS2QLnbsiFYHbiNum63M/7KZDdWXsjH+ysEi4bigVQXx4goTW0YB9+b0HevrwcjJZcqqi6dy7bGwtoyFnI8zSLATKeoKgmwVAjM0zGiM3EFdpcCljMqCaWSIyPW2l+ZzoiZ9+gMOMw26UtGDbpDh3gpwEbrduVJ/v+yX+me1/hfqqmB0wPbBCG6M8aIFz4BznpSewL47vv/bZOrNPs7WgXVXK44RTvefNse93vqsDjwUEz5xSjB5dt4Hnp/7hIk7+4MG8q1aNbqoFnKyFpjo2VKOSc6UZeijFUuwweRsqIPEcGCkbiS4tHQnzOh12834uhXj24ubZsf3Hn57+8EvzBTomxyS8DLRYp25///H0ZvjfHf3iEpZQQFFPp3MLmhW3QlYzkGnmkgcXQxdB25fCDlE98hx5SiUEeZ3qtPMWnGtMbwI/87jtkWKPTBUHGnECSFzNaMKpYQasA1eAtr0Ht/dWbNwxB9NIzL8BJ/kN2H/G5PfgWfto39FwslPgGP3cW8ipJw8mPPzux9dpfV4r2vYXApuAEZZShsChYgaluYdH7123yefn9vwsFHv4YNpNdjWbGwFV9zExeaiaCvaTRcLdMrOlMklnMRanm7fIMcBejICMbCq535Vpcnc3r4UXu6LMpZW/e+eYwB+/Oe3HbPShoAgcpwN4euF+Qh1Cg4LJPS8OS8PNKc7dSxmTceZmSje40BJTrT5NOOcozHYlp4jrlnCauZfp3B8l3sWSY8ge0Q0lgdZ6dUPvOBE/ew5zzDu0wJWD2lrOwaZzo6vvYLYh5Zi2FbW/RfsbaEHxdeZj67tX5qMnTh2nwHG5PYdSU3F878mvUZkNKwP84ZrURlW1SuPn4p6aI0uPlnrZ8/kpr7t8skcPp8tdudpxrmbGHsq1qaQTF7OPc7ibXNRpYQpzhZQ9cW4EeW4ww8U8NkPxjErf7es8T56CGfeTDZn4N167aAf+8INGO33/Kxe4Ih4X0HB9wjTBAXMUQIlaUMv6fYCxw2Hntwue32D71kKINBWiSOt+vLHxXyyyPZlqx3VBYSjfPx4bfmJERu+igz1QSNToiIo8IwqKQYFClIrDS0BABU7A9ZY9cW8F32jrfm5FqG9X+s5077e0skAfk4l/cfvbrSbD9hIrjzuADJwCxxanOLcg9Piq4M3v/NprFkqOHXQYBdpHi8Py3PdLd6mnbhLPbvvLrnkuDx6WRxd+UW032a4WLzaImiZlwgxOBijhtGSVRar39FXZb5VskSE+vqi7yQhG5oulpA773bSvxYtFzyXS3c7nXktJq289uXzt4vz375z//m37IzraC9SCCjyZkImbBSQm4mLaNqwQJPYVk2/faDSgfI1NyGvvU4EGBOFCoJjvoNO5L0vjka11AIXI3iQUk+jNeqHHgnE3IO8UWobJcL5GrbDhFrfAbswJfXzV43jVu00cvvnQfQFF23Yo35H097Xg5QtTqO8AH2yvq+1PAEIEzh2nwKnjtt+eeo+cCvndp8C//bVfr/Tc+IARybYFsNGy9XjR8eLYX3bVXXnysO5mzm6H6vvZ19055LkrBML2s7eIaDkEZyn0iF2xydgSAEF2yc2nau4cS01DfHnC7mBGRoqpqRb3PJ/7cWlzddGeZ/mDL+8fHW4PkwMdt8DrFV++wGWFGd5tmAwemA21gEQp69h0NRjQAueOZcDBCQ6wWB9tUBx8+RiCUp5bjx6nRT7WjXB8ZaLHWCVHkfBUKeZIyJEJn9A6jMixfsqAC2DZvoAyt8YzN6rgvp8RKB/3s9hAOGyYHDbKgZvv1i8Al/y7exyAbW8PQGAJLIFT4Lbh1M8tAFztHV/99hfZGVP6WK65qviHwG2wT/rHF+3Ycr+vT6/qfrLJORdOxaay9vinJqCPpVE0HZeMTCfHjiA3RuCUWYtVQ2zIyH6yUkypJpB8cc5j9x3QI6MnUATuq4H24vq0IPZzner0gxf2ZLrAhXBRMRFv7PFgRk/85IRmePMRzrewRAGKo1RgAgkuEHA6IgPdRl0AOrwjEhIKMb6CqgtIhkQgskPLOdwxlXXEr0OQBxVNJBJFSsA8BRmmQOP4kk2QwAU++u6mO/HKsAGqlS2q3fnZ821BH4AT0O5FGtu8oW7U0Djgr+dnAn50jy+/ezDRcusxO4799tR7hhumr18Bf/5ruhiAsc9xfO0Xt30YuZ4MQnzyaL+bizt2hv1Mo02F7gPvYC0eqRyzvpaDc6awm6yPPaKEm4WUY7GAw82MiFi50L7u4bAeengxtcjbU5tnVa/F8MaTi+rl5XE5ty6Um91+OcXTCjyp2BW8c8Q1sZ9xscNccTGjGKaxm3hG7tErygmTIQK1IzaGa6S8CCjuVTs5pEEZGbJM9QyOrVPrN8IahaCEBFGBdApy0+QF0bEAs+GSwAw8BZ5vyO1dVrJ7XPuoz/q9ZWnL9s2sjzbdx127ynub1UZIu/PCX2O1wr8DTvecbHuHSkSi53AynPqxhUIXF44//cPPqWf8dD+DQnCB62YgB7RA+2IwvjzF0mMuFs4W9PEtlAyS/29739IrWZad9X1r7XMi7iOzsqqzq9vubvcDG/fAGJAHSMDEAiQkmOChJcQ/9I9gBhPLQkIWRogG96O6KjMrM++NiHP2XutjsM65ddv9cDVVDR7kHkU+7r0RN1bsvfa3vsfV5K09eCMMSa3Z3GCmMaIoQlMjwLWHBtNjpNNgQ+UfININlyBhmXle44Mnh5ur6XTpd6fl9qpdH+a5+deON+cljDxM/uTmiJl48xZngUfcXuEwg0fkjINjJiaiEZjgN/CvIFbER8Bps+ySNrO4OkB7h02IGo0TEfdrv+8hRQojo5ERtceTLRyqFi/QU5omy8wn7oBhTWjgjfCEmN4DXu6qtelRrZRiRTt9IfZzs7aly15YZWh12s9ZPLooPHxVPgrB+HVt1f7bI5ylVgCxobK1mZ366TzGSDPcfPPm151m/vxqLCWiAYAMI3OBzYdyZdRkmojGFOzuosxorYBb3tswc2XSzJ0GtFZKkLLuUdRsylxIA8xscpmbO1N+dbBy1+rBZmZmr+/OT67n69kPTzwy1nWcl64UD/OT60NE3p3WeSqT2BnRcNPgRMxoN/BrtBs0oF12vuE18A040M7gK4SwrOhAJiy3IfESgOANg4jxZukvT8t9JEQJkYKhpHkgWjAEOmrDMwO6h9GNGAkOBGED/yPwPWK6Bt7fjz/sh53t1VYdW/vZUluABZvl7HPgsFfeY+7hgz/Ow2P+mnX2A+DVo2+y3zM2LdPAMnAaOPXLOjLz5uj4o2//uuyMX1RnZBSyAfTgCbw58DD5oeHgODQ6sQY0MoXJNpxNqrSf3X5YADECAxvaOxJCkmw2zOggTT2SBjObWuhSpo0emo6tXU3Tcrmsl3Fs7m6t2fXUSPWhZR0Sbg6TN7uclhtOuGp4MsOJcMxHTDfwZ4jfQ79F++/gx4CAG+A5cAEOaDOaYzIo0Ld5kUaclrj0c2Nr4N0lPl37uUcluZhUQrzICoLFyFKgS+QQ2gBM7r4dNwZMZaozcFkwGfAEWJEdDzIWjH2+bj+7Mz1Aa8t+sF4B14+2ND46bccjL9xq3c6/zun5F/uZy8++c2apzLEETgP3/f7clx6knn54+IKd2VZnACSMxEIEcHW0uVmjQI7E3RIAGjhN5vbAR2QK0bM1Kz86ANwD4FKIVIGxUtI4iv/MzT/3ei5oYTPBuJnmCbxx70TrwXX4VNYDdLNDM5GZOK9xBJ4eJ0TCfbuJtGnLTM0PEN9GAm3B/BoIYAX+Ejhg5G5f9nBdI5AUjHTkqa9Lx6XnXY8o4WiUkrT8JK3cKRNmEmXdmFCYmvGpVQb0gDUYcNWwJs4DTxx4BVzAFUmYQYGLcAXgAAxssYfxqGgeLqcBvAC+CTwHfljQC4D93vBQYQ/V6Z+7zl4Cf/0I0iNQeeeJEVgD54Hzivv1vESmbg7AP//WF4EzPqszQV3oianxyaHNDYfJDYrAynRysm3uJEnkOiSFWbk1YQxtRrGEUpUf0QwQKZWKjYC79YCbQYyA4DJ35yR7ejXFmgfwCHrkuF9kuLk9HGwGoSrGZpVNnbHb3vWBdtwwGBExoz4CJyADxzvgJXANfA1xjzG2RPAikCGR0taGkUonDJpd2nfnnVysVKbKvGhj8goQbR04tDyU+XQkMMAJ545L4BJYP8U3BQgnYQpMHfcdxTK4ftjDbC+1CRj7AL76/XvgNfBV4GofIVSFLfuW9jC8yp3u9gtcx35u/Tl03upsEzXtTMZtytRx399eeh/hhme/ff35lSZ/S51dhBl8MvPp1TQ1A9QaexeoiWzGyeGVUolyQEB7MOepsTsVCRjW0GQ5T9XrK4SJXhBpX+XbfuhSc9qBnMEZvGltHWMm3ztO2QcGj9fznJjGcLSVCgrMJBsNJAKwCZNBRAbUMTr8BfiXsKdbqML9Ca0DA1zQF6wX9J19EFnk2D2VSE4OZnmWD6AZgLrfQIlEwlwp27igOQSZCB4JjNgukQT6AB0p5MCLBR9/guOE59e4MQzgroNETrheIWwy0e2Li7522WUstaX9FLgGboCXAIAr4D3gBFw2MxNoP2THvuf9aphjAf4nmMjcDHY2Lp0wAkvgMnDuuu/LGlLeHA3/9HeBP/5y6qw5b4/29GqayveCPK8JqVXYZ6rRAlmibTM0q4MkHU7CKRiMDKm5zU4Jp0gnk5ajGrV68wgVrcwmmCcaOXsFXFI9rqd26dGgKXWArkA3TNC9lEYkwnTpOhraZcAaZiI67AI7Y7xEOyG+At1g3CFPyBUwmOGUWFfEQAqjnLeUkevIERqJSFWwPDZ/GiAVmZvKqS7DNYNVpCmSaja3vD0SCwFhJIwYgeaYDUMbODzN5XqCTCwd5gjhRFxPWOIzn9uNgtv3m0HbeR8fAe/v94Y3wACOwC2gR4cp9jrTL32Tt/VfgDfY9bfAngEwEj2xjtrM3pz7OsINT799839HzfjFdXZ79KtmKS09mm3+K62MqyVzppQBCnNjfV5GZjPLlDtpGIHBPE7WnI2AWbNyTlAPJMprwwgT3M0mw0xQdNLM3dnK+YI8TD4uK/qwbm32KdNpg3lOBgIyd1tSbQl4ggZLgHADAzqDJ5gBr9DvsF5gM8SNjdhX9I4s2wWNkVHhoFIkeuRIpLJEsqEKMNvChGgpUpYoEziaD+SMu97fT8NwNG3pDdULHht+5wl+fMZERGAYzoE10YQw3BNHQx8YhgCuD/uUSfvmNO/X0p8CAJ4Db4AL8NPdJ/s7j4C0+oSU38KvPjr/Ctm3tqH2s6LTjcQ6agAQ9+tlicx879bxR9//4nDGZ3XG1GSVSwjbzHPIcqgzFpmveoFIuAkAxQQMGbLYwDAjlMlhspSEHlufOZF0FvukHAlmEuLkJRc1r9iHUGve0O7OqyI8ZRmUNeUBtmALCw5glW4MWEpdN5CJlrAOqzFFQBfkGb3D6lzg1qrHQEqBGDk6RmiE6tAQkEpITpJlv6aNa1sW02TxlzKwMg/kuogHbfYQU6tkEHjCDe/VZQWIBIkROHVEQm3j5o6BHEji0PYbQDVh/uhArNbtJ4ABHwA/Aq6AJ8AM3O/2kbnDJQ8iq182YhcwNhl9qcySG5xRN4DTivv17jzWiGa4+f4z4F98WUUGoC2hUPngsfypSPhGiGddCyt416getHLkT/SaVkKHZqxfMiVxpC6htWPyihZBRbZIjMTstJ38yGIegT75Ej0ykZpmX5ZxaevcWKEFk6WJq5TgiAzj++/f4v6EsYIdmfCBtm5d0hByBQaUwLqPsIUxYo0MjKEYGqFVykQkUzkCY6Qqd0WARAqpkTJCaTJRFqh5gJVj9PV7wDShG85RrRwiSvWKS4U5ECTWgcu67T1meL2gCeZYB6I6rTNGR7NH0bCF7k7APfAj4Bp4D/hknyI8zL/Hoz9WJvUviwQg8O/BPwP+CkugGu2MbdB06biMcVpP61Dms6cN3/9D4A++zDqLkdLu/Kq0zTaPJNehq8YHGmSCc6MbxwZhqMqrjxyJEWyUaKMkkLSRCtFdtkvmjJxoZWBRLhxl5eLNpyl75KHRunVkH7GuY240ujU3RBcLtzezl//r1Qcz4IKAGGCAHTSICECJIUDwPU4BiJ5jyUhEaB1aIgPKtK6MVE9lZrkSCUIqkIqS/dMrZ54QK4kbfeRxMrSB789oV1gN64z//RZB3Dh++xo/vGxnaHLrfoygwRwRuBPeO+Cy4qrheoY6LoHJMRHmPwvTG/AK+Aj4OnB4hPo+PMa+h9XRefyVrKE/Af8Mr/4Cr86ln4WEdeAceH359NSXEZPj6g+ff7mbGYA2kplquynriDRjGBpQVwG3jctRjmEhrqEKoAnsTqKZoYoPlAHm1qMSfjGCBUYWw7bcFcoSyk0EA2qw+TiNWGg5BdBtpHpkH1lscppFKsRI5IhLtI/PuMp+24CjwQ0aiCLqEAmsCRCTBzgyzbiukSMztUrrkIhIjYxe960RIExZRpPFYQmoNTOgDLpVyS9ZSmdT6q9/FL+d5+PzFR80PJnxe4Y0jIGP7nFJyGAJI84DIzZ7xBLg3wtHwxgwAis+XTdGuIC57biudoKGgI+AJ8BT4BOg750Z97H6A+2i7+3dr1h/gt9a8IP//MmP3q4jnRAUI9cePWIyPH96wHf+EfDdL7fO/Pd/59ncnERmDdMZZbsCuNeECcIWhhJZSdOFZ1TkD7fILkLGZjY7QWRuJgRFyjVaM5uMFQHtwFTHpk3zPBmbTZwm5ojMYYkIzHMz5yWyC2k4CSM1IpY1EojUmrqMvBqyEFZhTaxCaqx56evdmj25BtY1UrysY+2jS+uoQlFPrVlpfhqZG29YQG7mp1mINFCigWD5s0opN0zNFHh7h1cf5+lH2T+K+KTrVfhrstuG1VUB3K2Ih4n4rphaEwo8a4DwekVJkat/atoHAI9n8B14b9e51E72kPL5APlWr/a35pT9A3zzk+uf/PiHLy4fv11en8bdMnqkG28OfP+Pv4HrP/3Slaf+97/1/mHyq9nKhAXVoBlDzESXMhnCEFMqrwJytzmGgRAtJdGaQ5XLW59CUqg4KDrNjAXyN6dTDUxZmybzFspAR1cMKRVrSjrMc2TeZw4qYCdpRI4N9OLIDGAIb3tWkMAYWkI9sEQusZ7TVmFErJkCL+s6MnpmT43UmlpDkeh1Ay03NW5XnpJJFKvDihVJjtBaQS3JZmhWYRYqtOT+Xq/fpKHdHieQW1NogBRv1lTa49OwFKAH4lnDeeA0Nu8+AkzMj4dUuQP3NSq43RGQh93OdpvS3JGO9jm0VX+I7758/uLju1OPzNlxaLya+a0PD/iDf/nFp5m/qM5+51klOpC1jRVhvzaiCuUCWDQsuDkAq5ic3Z8nUwKn8uuxcuvgSKZqM8A+ebfm5psWgU46aW0+HJo3TGaVkt57jHWYuQHnkWdogGm4JIZy6QnAzcVN6HsJLKlkCXPyMrREnvuAWwKntTe3Ia1jjYw1c6SCWgZGZkgRiN1/suYACUUiMnPvyUGOvS5DgDiVLBQQKxqGI/L2qn39gyurbqPgaSNGnN+uqptsFU2BtACeGJ5M+HRFDzBBwAQjDjXfq6J5uFEKWIDr/cHDEP3BQ16PGByfJ3rxH+J7L5+//jiXQdPB7Wb263/zXdh/+E3osvz3f+dZc7+e0MwrZGK7EkjFiSU5ezmE0Y1TRVK61fvim2kKlazjbIkCeFnX6GbmNJWbIs3KZpGYWE5S3holjDXXNSIyFYwkrEe+ldZEJ+S2KHvkunds29hFDGhNhRDQErluuqkBd4FLz+a2ZK4jesQSGqpkss20NCUpCU1e+5pSldtSlxcIDCmEUNUfkTk3Kz+HCpRtzZB6ejNfH93qipPKEB04x915JeBbnIY27i6F9xwAXq3QFjEFFwyYCxd8IIftGqTPCu6y118pte3RYD4e/eXnKLXvvH56etGWAeDDb17j2//613Jn+fyrqVqRugLqYZqEzQZ4t2LdzhYoYZMxhgSU5E6AU25mJtEisIaa+TxbayCYIzMMFDOpdDczKwmnjAAAEopJREFUBTkkKseIcitu7mbsfYi8jLhIqwHGyZkjF2hk9hGc3KXMGPWkjBIukbmbhETksoZrzbIQGhnSsgaVleZpBpWnkcg9WkOihFSqfIxye71l5iJg+9dgFmdFkuTO1swNXVluo1tfJ0aGJU7ndcQgWlCT7VAkKik2cBLWgYnbidkdXvMr/mydPKhF3gIT8AS42y+Yl33s9dDVrfsY9POsP8U/uXr65//x6Udv8c/+HvCvvszierQaIXIjWcD4SJhe1j1bfpiZBPYQMwBL8ThvntqkCLqn0WFM6crb5C2KXeOEyyRn9jQxrgwh9kRSEXFQ84JHiT4yhSVxHjpnwOiNFKLnihypjPRmUuZ+YjUzACMUUEPBonkeY4ZdRtxczdukOIUozB69b/ErNPjWi2GUcVECxJbUhxzBLTyXHpljKNKu5u0lm4EmSGOUOA9SKnaujYQep8s6Io2RSVVSZMUsl3D2vCITWaMqIoAgYiAMIOxhsvRwSp4AAt8BBLwBzntG8QObLR4BacTnWv8O/3jCy//0JU6Zfn61m9lvjwWoVkL0Zu+D2v7LNYqKLGMASEzRK3xJMmLyFhkAE+pdzXkok3RGX82oSmodITFncxgErJILQzqkInJyy55Fm75b8pIZSpMmn5oQIztyjDRiylIhbEzMh+12RPQHrLiH1EMuYOmxRsSAIQEYVW5GIZlYt08aR6aVfISElMmuMu8rUCcNcPvsndu8OVJkjlXTZAZlIrB5xCi0DJ3XTjCIdBtDbrDCig4OClcGGk4dIoKf6VRcgO1bGnevq6qzDvwEeA440IH7fU71YPeXewP3+Z0W/i0++O4XZGb/6tWuDz63OiQpqTmbwWlJbcFKZXkiKa3CfC89570ufdqsdcaoKbvNzUWfp7w/JyUESYzMFA4ThRwCwuFak86YeyTZkZSWHiP62xECyrDHhJ65bq7yObv1oeZlgSGDIhLkZOwDaw8nnRmJ0cPd6r6eI+qFUIOklWBJqqiEJSrLnQFlbISgAAVEplAOIyZK2wdMqS1DOVME1hGHg6FIICWVSAh5voy1R3N6IEJB49BmsnoEEDjMMOFtAIbBjX7RgalBCWs7A4M76F9t2Sd76OLbfUvjLn+qOjt/jnHn31i/wSIDRisAPAjmFp5JyPe8EHcqa0dnSs1Ag4sBZA+Qa5AoCqCaaW4E5FP2NTMqhQKBHEEzhpIKS4RByT5oxkMmMhDqkZe1m/plpLctvXpQ2aMrR26uUWtgiiwvltxcWDRC50s3Q8+KU8QYIXhmAjkylWqmmo3T0CoiSBmqMQI3L1oJYA90pMFKz5piZJTsszkAU/mhSZkB+IhoNkPKzHKFVDKV50uPSFbYWTIDoWxwtIQJ9wNPW/lNIoW0bYzegE7MRMZGsPMH5m1tqGfgE+BbO9v7ficXFY+tRqWHLy+R/YuvaK1kcKlilaVS8iypUp1JpnWkG6dmszEBGCbQnJGKVIKmPG5XMEm5rrliE3Wuq6xVj82UpaKQz5QG/GrmJSKHCPQYoeypy4gGI5Fiebv1VNYzMxvUSHndhDNB9tTl3Pe/yABXQRmeqVRI0SOzw7LIAUoMoiCrrFas3j4phZ4xNu7ZPnXeiI85kkS6Mes1Z9IsIqR0R6QgVM4kRCnPlz5iGH2rM6SB4MDhAAk/XfBm4HvvoRHFORYwhCBGwA2Nm/OyP8Cw2HH/V8ANcATOe1zr/Igvedm3wGdfhqj4iy+1JdLcpra5zW1M3vLWJjKyUOrCDkMikSG4ZSAlAZPz6NYa3GuuUPgRm6EXrVByMZAcoWYa5eHo80Qjktk3wbCGoo9cMjJQJ3mkQtmjLokakc0ZqkBFISBpWXtEtNZ6D3OrG2JkTMwbzz7yPBajMjRsi2xxJ4AIjQCwDQLqalFHdm66BwWyiu3BMjylyLS0as4ysTWrqczaTAlo9LysXWVaKWRaCE6gGSbgTcfbjiXQB55N+OSCFJIIQwSG4A2TbSyxzzBb2+cEHfgE+NqjLq1csfqus+IO2N7+Haiz3qrLVVEnHIbykOJIKNLIcuDrmRQmoxsE66G5mcTGbATLEFSJzVXPHAyoUsNa3dJ36V5kRQZEM13QpqltYbCSu+4u2SPphpC7BRKBZUQzb0YpBUcqBA0FValTRusjojhOKYAh3fr47k378dvlZYzWeJhMtTFtPg8qZVNKEFOMHdZQanOrAiNzA/LLY1mqnydlCibvPY4HKwgsFSOsRnGXy4hIGpGm/ato25BhG0YN4cUZ37jFizMEqHyHARfCduJr4gFe2sZQBWS83TMYuWtYypascA3tEO7/x+zsBwXN2oZKymRT6eGMY4CSuSBY41yuKMlm22iOSHNe1rg5mBkh9ZFGuFdaoikVFRWAVDKzbPSAusWWuZBhniREBg6TPZvlyJ+sGqmQzLD2MGOE6gkHovCTOgotlIWpKiRGZs90sEE9Yw+swFDeD02TmWFs3OsimoukNyjgJA2RdQlAqEYB5AaeEaUWMAJZyY1QJjxTBc24tzIVRxWuJROn85qp4rsgMt1Ug9NZkHAOGJCJVxd88wZXjsvACLTq0gwtMIrCWcpHPCI2Yn/w6aO0vMI+HkrtLXAAZuC3/t/X1w4aY5+GjTbZ5ppZ46MmmlmJzClkYmyR84KsufURSSI0TSxW5gZlb5GckNCBiIQxM41UzdTxsC+UeYIZcZhwf3f68OjPj+2Ti9ahoZSyTvGe4xAmIpGeCHMvJDSVIVGZmalEbuVoFYMMKOfmzdgDr9e4CE0Vii1wDzhIjJoIbCgYsyIMas4hsGifqVEuMCOm5tjjxDIz4cFIZXMWmyhNhuI+5uncC++bLSUqkMYGYZqwxsYUGsBl4O2CpxMuHUOoqJgERiJj06t3wUpPgJ0IqUejz8tu2HH3yO7lArwBbv4vvBc/38pfMnLQXlv56HEvojVAGQxkJs00GSuXZnKANZMjoPM6IjE5vaEVIzAFM7etV3NaTWnmhlENPyt6JyFzqDwTmsHI5vBGd/YRfbCLlxo9QZBa49pzpGhld73b5yZSOYJgboPIFMjMdPMR2iAxYHaskZehMELyYphQNfmq7bBWBIvumVl71+5Ib5YGjwSxCtX4P4yngByBsnrYMruFhEwaPdYeCdmuaJHIUDsYZuJcDMdNJ43XC75xg0+AkQgiiSAy0FE4MrbOTjvMoV/0dtZ79Ga/aa47tPabWGXqNj8qLP7cs3pwrwmgN2y/UwvAJK9GXkDg4AhmVsZzAlRKTpqpuQOQIFojBFsiofJFh5MdtkZlwsoJJuE4TI2G5iXChbtdzW0cAlh6ZA87LwPlbaGc3RXqMRo8M2Xlto7IjOK0CREaZQC+uWVjHUHp0sfXDrh2O6+xhNbIiWZOpywrVlJbnolRQkZUZ7kFZ3FT3ICobZ6sXn5zIZASaeFSaN5UhMhUWhoA2PkyRgRpshJVO61qXyBw6ZvcyIiJeH/CVLZWY9OGVLWN3HbdSAxDJuYNBXjkh/AwBq03/rKzI4ss9NXfQJE91rzkoyPygcIUj4psPzdBjQCZXhK5VJcoHqZN2Etgm8IkAEwTGwnJDQJbdV6CET1z4qZfasZmHsAIjKxLOkPQCALevLKhD1OzW8abZXLmJfrIstnuIw7ejofWR0SmNkyVGRkbVU6UNvAvJWQzX8dQUshlGU9mMfy8jEOMUVaOI+kMKcwgdcnAtTwZyB6iArszciOTRpSTmjKxByIk5No9b0bGtTcU47suGQKlu1PPSogSUWepzAjM3MhnmZtz1pJYhLsFz2a8vSCJAJxbqZWIF6VwMRDbxgbhPnAzAdqH6Ot+kC0AAQe+8nNhYV/Wqk6xP6qwh6rKvbYeyi4Lp92+DthcHec9rKSnJgKGFHtsuZaGmk6rFLtJ5UgRa1czHhrMq3nV1IxkpNZQmfZzjLn5ZJya1XXufunn+3W6xFevfFz6GOktSMbIxcdh8rl5eY5iA1nTKj0jtiCVEUGWsXIW0p6hxvz6e1eZua5DTpdmZxIjEyhgZictCqAaGdqGmwlMxmXkGtq0EXUVSdC3W7MKIBMKUtsLDHVPjYjzaa30R+7EEAUPE3BluATWAABPyHFa8V9f4Du3+NYTOBG5YWZbTAQR5R1DsMRUDiROK06BmwcmLffaetjhroCv/5ojgb91PZBEyhs1Hh2XeFRk+egSsP2xGdSchJyKnRJU7QsG2GTJAbnZ7GSlG24dDlKJoICeeXBzp/YfWnx6CBNhky1RGQ8K5RAnyEEIGONwf/axnl8nziPDK/BXNZwGDs28hosFo8pjM8JyViYxNnTUNluFzMwPZvvq7XwZcd2TY0jZhwxwsjAV2z4wBDKToTKhTYpOZGpyGpVgBZ+tURQKFUdWUCoz9vkqlYWNpIFaVy19qP5BSfHaPZTXbkhgGYgEgXBQaIQSny743nt4MuHFBVHnJhBEH5uGvnMT4iuQwIsFx8czzQeHmGJyPwO+DTz/Us3k63o77T9xPJqGPT4xY/8P2Dc5AdFSyEjadkZKIhmJpObJIxUsn3aULqyuaqRv3kihoZzNNhKt6iPMAJrkTolFWvYicGOr5NZ4dJvH+kPyKS2aTVczzqEUHeV21fsAfHIvkm9NYHMgm6gQGFlDpwQhFd7LVHzlynuoGa9naychNZQ1o3TAzAA1VqQ26SXNlNd5JTg1G3NXgCkJZCS9rhLFlkqNrLwY1KlasyiSp/PaY5eXipA2AkiB3Wt8BozlzoRdB96s+OoVXl02k6wHaANC7jJVS1wMq3DqeHr82Y0E+xt/C/we8N2fNX354ut+Jx2t+/Z5+EVFFo/K62Gru7RRHoaZA0ZUar2mySOyh0IqLn/FM4TSDJGWUt9+Pzm7mQkwFQtoUz1m0CyxJmo8n0JZa9N4aHZ1aOsaq03tSrrvx+NkqenVWMqpHzDjSPWeBYaB5bqQACKLJqcHdZLBo5AGIjOfTNPr85gNR7fZCObUSoqsIaayNpTSQ5lIE7YxU31QauxGUSPEQm1CG/rGulxbjmjzlBv2mxF0KgJv7tZMVZERvD1wHXnViCtHCEvsWRcCE2bIQDe8OOF338eBWLTJBUaxRbSZt9WN8jLw6dg2mN4xjUelUDOAD4BvAx8Crze7pC9nVTXf7XV2eLRZPpyVWze2V161Yytw1w4TJ3eUXoQESs+YmZSlwQSNUCIZaGbY558BRGoyE5Ta5GDrEFpRCBGpbgmwOU0cUu/hzYiycyKNh+Z96SCaYW5+O/FyKbgkATXzdcQy1KxuHczqelNpG9UwEyM0uTLIGg+MHJk/ej2ezv78SXNwGVkEu3kCxSRDcBKEi+Le7JUST1mcttjcEGiGiB2wrWYsUsaReSz6LEEwi5ubulx6lOgwAdP7V/7xm3HlQiPern1Jc2gbUNk2nuiJ1wsovHfER6eNlBaFmWkHQRIwnBJ3HbeGSCyJsgGcub+pR+BpOeQCeKS9++LrwUjmtB+X076P/o1rZuz3AAADuAdetbVHaqP7kWxGcesfRDorwlAcCFizIHgizNgjjZzM5omQls6QnDiBAiY3Nw6hGefmkpYUicnbGCHh5ZsLDR8+PX766el9y0/u1tmd0mnpa6QZBBgLHMlmNTu1RDTzCDh7bTx9REpuUS83I5lxf7IX536a7NLbD+8uI7CuI6TzuhnnLoFmm4mpAIKboFCK1LHZacetqv8a0gisEwk2aAyZ9d5FYyhyxDimpNlt7fHqzXkFAHW3E/npNZd1DBJvzqeXy9tLVp5PcxybHRu3YKUc+MFrQLhfcAZmA4EDt73NDEa0gvoX8IDoMMIFJ2bDTcOxwZ/sKFrhZwlMX0bo7D3wCngDvARO+21jfQRwxCMUQ4+6tDPwBvgRf+v9tgVQV/9um+tCNUNuG7aJ7ReO7cCqby7S5KA3GhjVA5VFAUkiEjXcLBcfsrr80iLAjc1tOa83Ewgzw+sl73uSRoM/CKuyvvBBRUWvvQgAsPEtCGAXDiC/crA10AxmPG0fGmSFPG6vjNzo/9upXE87BFTqaAkHa/cCIeROpZ580+YoMU30Sl1x1nY4QktlbpVZJnB7cEJXxpuDvT2XStMI0GSwCjsw4Wq2D5/M82Q/eb2QnAgHjl79mzbdmOHSFaGvXNlsnAwUmqEZj80mpz+7+fC7zz94/9aMy2UQev/Z8fb5La9mTM7J7TjhONnUUCSFNUBjK54+4Ga3B392RZ8Ji/O5//jl+MGL+OiFlqH7Ne8XZmB2HieYl+ZUFLcbGbY43jJa6vnpffzw9fKXPz194UJ/t96td+vderferXfr3Xq33q136916t96td+vderferXfr3Xq33q136+/8+j93caEKKLtrugAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9aZMkV3Ylds6977nHkllZCwoobL3vTTanuUgjDjm0ocZsvutX6BfqiyR+kEkfaCaKGomUWkM22Wyg0ViqUFVZmRHh/t67Rx+eeyJBoLsBavqLrK5lJcIiY/EIv36Xc869AF7aS3tpL+2lvbSX9tJe2kt7aS/tpb20l/bSXtpLe2kv7aW9tJf2/3fj1x/kITEbDrOezeHmCrUWpAB6ctGyM2W8svOv3t1cX0/Hqb77rGwSCYGsobnByK3DjE4ZCcKAtMmWfciWUnIiuY2jD8mHZDQjkd09WQu12miUEKEaoUBpcZzqk8dXaBFQiJY855QyW0iCIAIhAIhQaLlTARIhmDEiABIUBUEAQEIABAigQGN/Lev3EAAlGCWYUQDB5cMSBERQIE0E1f8OmvFs9PNs14nN6RWsIPtzjFQIilBgu0lDtv5Wx7lFxO+8fee1e+NP3r2qwGBMydzobm5ITjcbkuVMime7lBKz2TDYJqfN6NlpRoPMkcj3n57+x7/65T++90xaDlSAEZBoBoqhJkiSYIaR/N372zPjLy7LP1wdD40Ck4cB4uIl0vKVhQQoREC4+UalJkI3D6HWPwYgobXgf/vv3zob08PzcdgM/91PLo2MQDleC0Eybc5Iz5mbLX706ua/+fGjD3/5/KOnh7/4u6cX2cwk2Is5TjX2medDGpyjwc3clc03d7Z+sdmOw51tHga/sx/OduPF2XD3fGOkOXfjgE1GiyjNnAhcTWWeIyKOU336Ynrn7z9s18dT0SFUQZgFEYDMzLkdc0CknUp1ciqt9U9FAnC3UhqNJBUICABJdicTu0s6KXZXAURzQODyUJJ0IwmQBtDMCMFIEebOGiDhZmeb4Y07+a0zfzz45daHE/KBdBjcDGZWa9S5AXr0yn6/SaC58enlNDje+A9fxdkd/O17ODVsHWPCmJAM2bBxjI40AAkAsAMSkIAMjMAGcMCAADIA4F38xV/8T3/9bouG5fISACPMTQo0taZQADTDSPyb1/YwP3x49R+fn35ZEPLdEKNHBQRK/RpWExQKKVY3hUJABEJosbwohKbod0YooNPU0nZI29E32b766v61x4Cn46G8aJOiCRjcmBNpbvW6KieenY2nY7m/Hwa1gJ0aQN7d+NngRvSrMFHZPRkt4jRjkwNETgaAEInTVDdDIhEKaw2kGUuJUts0VXPWsviEG5hcEWNiJqOhKVqolFKF62NpgBmL4ny7MQBAyu7GlLxJRiR3SVUywNyWkCU1AbLuSYsTiaCcRoNEAjSYmff4TLiR7E4HEG4GojWYWXLc24/fuJ/PBx+z28ZyssFBmrv1t5lLlFQ2Q75/Z7Mdk5mBvLi3xb96iPFVwPFD4B+fYDBsMoaETIwJtNWlADiwAxzIwABsgAEgYKvzNeD05OODGyXvQRQ9DpsQgtDjvYEUJJ2a/ud3r+60UG1WlYUJQRpN1lqREYCkWCMbYNLNRRtSD5YiYSQEiWHNwwIBCmwpUjIYrYZGx91dbsP2zkU+HQ7leAVAqBYp0GrVsymuTiVnD/LBPu+YPj7WEu0imyc4QbCFwtQAhgw4HMv//fj526/uXq+aaxynen1qT6+mMacGbLLfv9hscxqGROI419JEAYbTqc2tlbnMLQ6n9tcfXB+qcrLBbZM4JstuTppEsrUWoaflFC24hDKaEzAQGAUYBCYaCbJFEDQiAJICuu+oOxFppAAQZjSAZDKDdX9cfI6kGVvQEwazMdvDrb+6zyS3g12bazAvsMVAMUJy32/TmJMlhxlCePMM4wNgA0w4TkgONxiRDMnABBDw1ZkykAAHfL2h1f96VLuCPnjvyaG2W8kOIIQGNUFNogAoIiAphCniUGPbYqpqTc01F7I/qbUAFATUFFJ3ue5oAVi/b6lkeuqU1CuZgISeNpKb0dACEXqwT++ftNuP427n7VhDEOjm8KvD8Xh1/dHz6Y3zzUCBjGhvnI/vXE5zaQiGE1AEmmBgAFU0oNT4xw+u3n963A3pfJ/2m+HBWX71/n5wnGBXh9nN6JbcxsH32xwhCT230ayApxpFmkNziau5Qr3eQTZLBncbeinDcLO8eAhYRQuJMbcgRRucm/1gjhAJGY1EL8FIkMZeyhkBMxNpZiBgNPebMLY4Go0RoiGZXWxSzvaVewOTYZM4pq/SLsHrUzUzd3OyBpxi0n43pJyQDTQdKmsPFAWXH+D5jOTIxJiRHclXD0vrjZ49bXWsXmSm9QfAc/zNB8epuVOtB2hCAVECu2cQlASCQvS6irOxBU+BOQST1Er4QBq7S3XnIRBYbvTyuHsXiX7WGCFQaNRau/WKOI3JBqeAea6vnQ3vXDdC43b0Ke+cebOptrm6nhwqtX78Yvr6K2dGnmVeXuuVHd44H959fpoqAuHGKkVTcaLJkhAw6jjFYapPOfOpmSE5zrbDq3e3j+5uH9zd7od099w3mUaW0qYax6kamRNb4DBHiSAspZ4CfOlfQJHhHmqlSqX2YOMkieTmhDszzc1IuUMh73HNlhcwMQCJbr04AxdPE8z8JqP2nsXI3i0YnAQRYDKeDyknKw0BwAADttmS89CqtDUOyd2sTXXMHma7MWPoPiQC+Np9YAMA1w3JMRCjY3S4r87kt8JVXt+Dt37b4qk4Au8ff/YxASfkJvTKxLpDgRaURfc4o0K9NIVATsYjAWnsRZkg9wREiL3b6fGK7C8HGNSM7KnYTJJ68RoUtXRMRg7OZEYjAJxKe3XfGzQ8uHehfVI0dwvfWD5dXTJCH72Yh2xMtsn+UZGATcJr5+MvL+cqtGCTQqAUQI0gPfVT11s5CGBreHFdro/zz96/NKOTj+7v/vR3H92/2IGsLebSkrE2HqZSa2tLhDMosudenrt7ymPeGpJytnKMy+dXaL1skEIVQINZGEViP1jK3Azp1KM0eBPVBJkRoG5cuGdP610z3UmztV5kbx1goPHO6N98uP/pR0dzHhq84NyF64oRA2nGcUjJzWk1mQXSaNikJVaVhle3wBmwAa5hjgSMhtHhec2Gt/Omr77F9X4CAVwDMzADJ+Cj7T7/0VfuHmp7cl2up5qJqdSptlrVpAiFRYQYS16IiN5J9/SawQ3UIEMInlweESH2NCEaFZCJweWU9q4WlERSsZSE6O2SG87PhwSFIdN4nNudO3Co1mrJaowQ5tZcGgYfhzQO+2eT0ZRyGp1FapLEbeKj8+HD6zq3BiEQlImMgFtkM7dQIDqKgJ591htSQIdTnUt7fnVKZjK4UUBrrdUAUUO9duqXba0FiFqslYq0PTvb5tHohuu5RK2QO30c5mnqQSrR3BAQzXrdoF4ek1h7zOieBi3O1eOi0UCaucFICT0DijKaO0k8vDNe7LLbiWSCnW8c5xmbBNn2qmXzIadkBDgkQ2i/HTBmJIMbThXfuQ8kYASeIzsyMCTkm+jVveomhqVbAaxDDgFcAc+AGQhAwF38+e8B2qHtTs9wnHBvh7ngyQkvJkwNc0MNlIYamALX85MX8/PDfDW3p1fzCSVbza6TM5wCRcvWqnosM+8uSIZEaIkcSyLlkjdXMwPB/cZ+8NW7qXV8RTgWDYx9ttaawPfeeZ+tgHj05mvJc4jTXN/9eD5ObRzdSZGll2DCJtuDrX90iNIUggH9PEbgzsYj8enVRCBA9mS+HCD6HaU1hADViFblbgBqjZAiQrqJMlhLTYTC2IbR3RFNZS6S2K8tc5BB7w093ZMDFMTWlpohJCNXX+s4kMFgZPIlAltPmSQNRhPlZokoohmSGZ0fXJXLYxvHtB38/vmAMQEGWW8i9gOH5J6IgMEhYD9gTHAigN0Au7OCEQVjQiaG2zHspji7aSd5K84JuASeAloffBd4BajABMzYfIxNBu5iqHh9wusFANCAAGKFQqYHuH6AA55c4aMrPJtwLKgFc7x4dvr7X149O85EVEXpNQZlQAS51ntcvvQlmAGfBLj+ZX7ttbPf+dFraek83EoNRtzf8L255iENOWWfSWS3EFIyyU/Cs+syZCfDyKlpJAVI2iR7sM2/jNIkFwJiENSdrRuGyxdTBLwFDHIj0AwutBqClcKptLElGkLy6PgVet/XsUEsDU104LGHca7XEhFDZmXq4AQgs7VKBhOUuTTlCjTEUtWTkG5wil7dk7bibGaEe0+qZIBgAE6AJsLJEAr4cD88uhjTeUJyDAZ3JEI6h2RCymjNPYGG/YDRQcOp4Rt3gDMgAQUIbDL8JoDxVkjzWw2m3arSngO/BGxtDgbgTeBVYAIugQDuAXtgBwioa6/aw56tOXcCroFrPHiBB1fABFSgAIfzjz788V++89c/eTzNLRkOBTUQRFOHx5eksKDXEnvHQLI3okYj7+zSH3z/Ffz4zTQkAoyIMM4lHu6Hd45t45bGEYdr0qJVHwZzx4SrWp9end66tyORnaXFkCh07EmbxPvb9OxQao9pIIlkOMvpa9nOi/6+RGuwFjCviSnBjG7K1NVUPLkZBBY2gu40QkJToAP60X2hfzwRJEUCiiHBL8bWInpkDOU8Cqq1mSBFx+t7qa8gbUGDOh2weGQnBoAexkC6LUjHAtKCNDpRhSaYaAZzG51n2TA6eo0/JgRgAQ8eBAjuGAyWsEkYHGGwwOb+CowdAIPjVgDjLZfiCpjZrSA3AR8AV8DFen9/ZAUMuAuMQAY2AIEGENiv4fC2BXBYf6Y1/87AEzzc4hvHB+88f87CwfPc5trmYARatNq8yqJFB2OFfoEHAgCNIpmc33hjn3/8Bs7fSMkcWoCQ41Tvb4dogloeUrlSIFoplmVuQdLS9RQ50z1tM49z2w8MkWQThRgc9zbpxdxKqAM3ERgyfrhJ93I8uWzXYCIozVXhlkwS3VTnOKS5n9+cHJAqS23Hqba4wRNgZq0FxegwdQQkI3yTcocqjOxwboRCtUaU1q6OIEK6PpUeKusC6DtNAFsAlAXliJDT0Au2BcMgBHPr2CZpTjhtkz0lZk+NhsTFybYZZmgCA4PjFAAx+lJ4jRnuKA0PtsCd1W/mW751E8bsM82m3cqYT4GPb2XM7mdHIANnwDmwW6HdX2+2xtR9v/IAAAcgA8+w3+ycbZMdkR3HytLQImqwBkpTaa3WVhpQUaEIQNG92QwXu/x7P3yIt98G3kytVndzwgyHEvfvMBNmzMMwkwiVedrfgZGZqG7PDtVpnrhxe1JrCwjsCEsIDjLpvvvHx1aFaGFz3cb4d4Gvz3o1ewKS80nFR5QM3Yc6yGekke4LLwZFrUGyxsKcdFhbwhqYIMq4lAf9j90v+unv4VwRL06nXtjVquQiTC2CTNYgA22u4bDs6kh4C4Ew74UIYWaEgSKTLZExmQ3Jc/KUWEU0YK5IjhYLg2oEHMkwJAyOIWNMGB10VOH+BTCsgbR9Olfe3LiJXredz4AT8ATvXeKNHYA1afbW9R7wABi+gIfdtgzkG8xofeuGpycwRutNj4ycXQFroRqYa5sqJxpUq0m11bagbE4m47ffPsMffQX4CvBGalXj0POrTSUyY5tUS8tDKnKLUufZFG5WxHmOd5/NNSJnHwxzRAv0jlgr5xXCLvnFBs+OLcRWo9R41vSLGp2LfNHiJITRadmVE5NbqVFrCOFhnTOMFqXFqTRIvebqmY698iQAmbrzgVz4b3RPJBQBrjBiT3kdMHQbsksL/i+g1FbFaL14Q0CJVNMn9b9AWgCblHpWdSIlS+5Dck9w90OzXSNE1E6yGzyjApkYEsaEnLDNGDIg2ADcXx2orRArP+Nkt33rJnsKuES5wnsHRMNbF8AFsAH2ax+Qv6ST4ZaH3dgRuMSHl7VWkJI56WYJEZSZWwBUCNFUzKBapdJEyAxG3Dsbv/fjR7j4GvA28HqaSj1HEkmihlTr3dE/mMswjsNmuzF3z2rVLQbHuB+eTW0qMQ7JjUUIBWFtoSNAQgEg9tkkPZ+aQiFcQ+8m2KxQ6VDBMNp+w+3gOXs/xac5zBFSBSIAotZoIYKUJCW3nHM7to7R07rzyNhjzaKmWHwKq9u1oNQzHYCUzNwlJqc7y9SqLQ/uAFKiAQsrAPRoDYDu3LiV3p04zDwny4nJPSVOwZ1lzIEhYRhgwERQGBxjxpiQHdsBQ0Zp2PfYA2AApjWY2XrK/VYO5RpgblrOI3CF9w+4rvhZwVuXwMM1kj38tJO1z3OgL2INuMazx/PjyxoBWHgYFsDAAFANPcdqlbeoVoVEwKGc/Xe/eYH/6uvA14G3gIfpNDcAHduUoZT2YOvvXc3K6e6DC0pNOk4NISOilqelHaY6Dk4DgRLIHpChYxlACBJFneUk8rJEina+97ub9Oy6fvy87ka7e2dMibXF+fnw2sV2GPj0EIfTPA7ebOnv1DSVoBTqoDwlKaL7UBNSz529CVlcbAGgAZr13l0NArsvBugEFwWRuBD7QbLTdGBAPfUZ+rPMaHQje3nmJIxGJuvxzFKy7One2YD9gAzcGbEZEIIDTlRiTNgMyI7tCBhowCvACMT6e7OCrv8M5XcgVn7pRpRxAA64nBQ4nWL7d0/x7SOwA177dEHW8QsABSirz/VXaOtbjL8iw87AJf7+8fOrkwAiFEmEGyIQILrCKaCAAhGttZ7NZIZk/uj++Na/fhv4FvA14E1gSHNpVJh7cjNqmuP+BnU6HY/X81xrixrRxOR4/dG9s7OtWpvgF0Ovpay0Dqn3ooRCCGyL/ihGtz0ipN3g240dq5BbENdzOaMb7d0nx/eenu7shrNtzjm36ImXYswlWosAqpY+E6FoTdYZ4i4g0EpAyAQZLBiUee9HtQh8zKUGJhIp8WyXSqURbeFJeu2FwbsX9jgmAWadc6IZ3brX0d2Sc0i+yWnMlpKN2Zvozxs2DgNKgA4QNIyOTcImY1wBMNsCF2us2gBl1fbglrd1P9D6sF7DvQBOwBVU8MYZ743bJ9e4DuAFkNdC/sZusm2PIxNwBCZAq//1w7j/eX52BXyMdz+uUb2DlgTJ7CaoQlJPMIpQi9aqaouu6HDjbvQ//p2H+P63gW8Cb3dXTrVFqdplGAWh1PrKWXzjTPNcjtbQkxPNEwdNNodgxxkPzjOJwTG3GBIhNmlBVqCQAAZoaCNZzYYkQon4wes7rUqSEFrlqenx01MIr97NbowWBWihCJgxGYpuvvkgDYvzCFhOf0f1exgE6b0QAxZ8THBKsq70S27ZbUgm6jRFRRfMwLrwjOASExfdmnX9mdG98zSWzLIzdfpTJJndndavNBwbqmPkUvtnxyZhHGCdCx+Au8B2jVLbNW/eQPy4dUO3HKUucEM7wUfc+xbuvYk3HgOXAIHzz/jKzYtkYAYKcAW8WBEyAWeAgN3Crn7KnuDj9y6fv3AS3pWkgjmpBEaoIgA2RYRK01yjNXVkcXD7xhvb8d99E/gO8DXgbn/F1IS5tDv7DCgZEXEv47/+ztlpGotYG08Nc9OptLm0U5S54uo6cJ66yGKayj5SWxrCXoHjBr/rXNPVYd7vfTOO+83mbJs3idktmWpp7z+fr0/lNHe/lGlhLZIZ0/LpuqpzKfOBRfSEVQq2CBT7OaGtSMTaFRhU0YJmWIhcABQCsuScrLOZclMvybiCa/0K6/5DwtkzqJnR3cz8WNWobeN9d2RfWMvsGPrvjJyx67V/x8kMuAM8AAzYAALGFda6ocPjVsjhmuYMeBu4AmZ4z4C/D7z6eaHos8aVITgAL4BL4AjEGlPvfMbPngO/wP/x7lyaORVwg0RYrx06q8kmKlRDc1WpUQUSyezemf/BH72Je98FvgG8ffOiCeBpDgpmligB89w2O+cmn7uPw8iUe1oJRbSoLSICFin5YLxqi16zxdL6dQmh06QIUKHrUuC8fzE8uTx+eDln97Ndunc+7vLmzUe7wX2q7cNnh+McpTbCzOU0ErFoJwSY1IMHIASJJhhDjNq6zCIt3kMaGYu0GFArzYCFY5KmuS56Mu86LHSsljRzCTSDE4YVQdPCeXXM1ryznGbehWV+fsNXuiE7UsJgC4RxZ7dKejrukIAHwPlaG3X32gMPPs8/HgPXQAWuAAceAc+BV4ACzF/YybrlFdp9BjzGx89B4d4J2ALXwCuffvB7wD/O738s9owBWEeMuo9I0YubaIESmktUCQgnx8wfffMe/uw7wLeBr92GhRPEqTRJxujStqnUHccOGTTABbiZweF5gDtri9PxNGRmYhZaKNghtKWmaCvgrgXrRA3cPRtz5gePr0ttl9e6OswAxiENyYxWI1pooAXUqpqFG0KMAGMBMrRQTlTr3QDdLA8pljaAhkVNRq4CRqOmFksBxgDmEopibgajL9QWoeRdXAsas8u9E10IIRFGcwNIZ1fuMxlT8pxs35kA86UUGxJ2eekxlyaxC1+3K2We1liy/bX94CvAK8Bz4DmwBQAQuAecgOnLOBmAPXC2vPXpgF98jFqxA8YHwPzpR87AB/g/331xPAokZL5ICwSGzCzQS6NgDZXaGW2BSMbX7g5f/ZOvAD2Y3b39uglQqb3b6nplHee42xo+aa06D2Mdhgqha2NyTiRboPWLXuyASu8Dkhgd6QIcKE1Fune+LSWePj+SiygjWkyCWz+nHbAFgNb6OIPmtuBgik73CyEDAJo5CdCN6lwk0BMnukRxYUkXnR5zMhlDmEImGcNBo/WJgp5aAaYubDQDGYoMT0v2NOMidHGz5F2Z7ZM4FiIBjajExsEEN6R0S2C9BXbAFtgDe+DiC7vIBfD7K0x/Djxci7YvawY8AM6w2eGbE376Ia5OGGegfvphHwO/wE/fb9GbR9JoTiObTNJCtwSaYm6Yq2pEb+O3I//wew/w/e+u5f+nLEmoodPUxuwQgphKzCUsW2eyzB09GghwUAwwwDEnEmaKJnMK6AJhSm1VWwY6wqK5xvWxbLLfuzOW0i6vT6XRjTIMBkAtIMrDVkgZCSawNQndAUUEgqkTAYRLx+tJhGXPbpbM3F0LWdR1aCKiRlcQdL4SWsA5gW0Zy+HiQLRFTEJKnWA1c5Fwds7O3dgHBtzNzVIizACDO3JGcgwDdgPGDhkMK8+4A3bAOTB+GSe7Ma6/HwGvrLjuF7d/Ao7A14ER+AF2W7z93/diZy0Eb+wxHr9zeXl1A0Mu4xPWwfiOXrGG5lCpMbfo7Xlye+uVzb0//8aaMf85VpwESLie6p39EIQDLVRq240pQujpOMJlIFHD+5ATOeaOLXEOjCYtciARtiosTBQgF0HUWiXR7P7FZiptmhsgwUqNm0q/MKIpYAtqwU9UFz2gLOC+MZpaK/G0zJfX3guunFM2SymNQx7cB0ue4IzoBfYNY9BDae8RIKxiIiwObotWCBLMsR9dWjTdPScbuoiDbnQzd4cbvJPoBt5ArHn9GVeH2wLn/1Ls9JNT9iUf/1fAe8Dbt9C1P8Pdn+D0S6CtzWy3GfglfvKL1ioNBL0HM+u9iVqoiq1FaTGXONVWKwSY4Xxrf/KHb+DR94FvAa9//kEHdJr7XAsiUE2nuW42gxbhZaQ+zQi0rspRGDkMbsZkPgtZgNAoqreHEpZMTsINkGpXRQLDkF65u/3w48Mi1NEiXWKffuutZ1eeR9To0vQF9w9rBoGGVpdxykCYrITqVE80oBkn0pKbuyVXxJ49YnVVXFeBLDi7deUQ0Kkzu+mb1dUuS8biwnPeVH59XMX6NBS6Gn1McENvUBfsflhrsj4Ad/Z5IMJv1f4X4J8+D4/9HjZPbjW23d4Hfo4PnphBolEp9QvMqC4NZGkx15hKTKXNpQWCUE787ttn+A/fBbqffY6lJkCYSutDLE5GaCqtRTRZi+oALTW0BSwIQghYckvJk7GUqpRuUqSAWBUQSxxSlMbT3EoLA1LyzZjO9vnFVUFv6xbtap8KAfoA0jok0g9U0VYp+6IH6w22IIrLWPMyhwkH++hw1EYjsy0KSy7BccHaQFIG6oaeB9Cl7VQEnKpVbj1VA72lXseiaHQ63ZbZpOQwYkjIaRVWpDWSjWt99tuzCnwAzMAz4ClQgQ7h2tpz3LbvAn8J4FapF8Av8JOfHqfJrKdKSwYYJbVASKWhVJUaU41pjhpSyBx3d/7DP/kK8H3gO8Ducw8udXHEVGIqkQg4QZuKWgSMDWFNNWQmxqrVChCgMyfPhqu4GYZZ/gKpCg51ZrLjDC+OpbbIZi0Uod1mPJ7qcaomui1q1X5MTnYAzoxuvFEC97hH0hAVZB8YpnsfgJNABSzhptvsMklOobNEd9z40qIvMxK2G3pStc6ZmsHNSDhBmoQ+f6WQTJ+cFy6i2yWA9Tk58yWkfTKDdDPQ+9tzsr++RS51JfcToK3qoC5ie+3TT3m03n/jFh8D/4SfvgeFuXVHMCeAqp5a0KTaYq6aS0xVTQFydPzoW3fx+98FvvvZ8v/GUhMk1tDTq/lim0BG0yF4PNXNxmBRQ9Yqfez5UH2WhgSYB3ZNaRceRvcChfTJ+GgH1ZKhtqWbDEUIyXjvzrY9u+6SJonNwqhensMi00G1m3lqLPT2TS7rUqFqbE6Ht9ZGCIRtz4Ox2WzVilqt04m0ZPwEzu3IEJcU3/FH0szpdE99AN3clxHfZaK/C1ICcLWlf1gPBVyGLvv5+UTec6MY+636Gdb36tqvYQXMBmC/evnnhpndLejuBS5/0a6vzenoCAOMqAKpdX1BK4HSYioqLRTMhnvnw1f+zVdXLONXWuoCCwqXh3qxTW7s+xGidwEy6zPsIRgZJMPYlTo2DtlNDYyQdRi0jyAzJL/RV5sIIpoioNRHAEUyJ7tzvnn2/FQaSLSmSplABwO1U6UhLTh0n0ShdUKc/SDQY2xbeQEjLWepORtyspxcc0afUxJaJ5WMVB8p62qyBQ2Bmcm46jd6o7BIbnvIphRzkFKVcmgcHecJwUXbkYHhnzFIXKHa36rd0KNdk70Dplu43a8qCm/zm0/w04M471UAACAASURBVPcJJe8lWa9iaFQJIFAVpWGuMRXMtfUBiyHjD797H9/rwexz0ebF0tL/Q6VqOyZ3tqqqdpjqsBmC4ZWBYu5CIsKkZiSUfFCf1gaatPaC6B81sI77AoAY6rCe+7JToF8i25ymzTBfTT3+KRCESwB7zAiFmPLGphItIIQZlxHKiPUdOykZRibCYo6IVGoPRKPDe7qLHowXFEMLs9SH0ReZpPW5mk8YKgSW4+nfU4duuli5CdgY9g7P2Dg2wC6vidJWIpyrrv+3ZzdaSK0s0wHgWhf+KiQl3XKyI/AzfPiRpfUMdhakp5KO/jeUGqeqqbbSQpIbH90dXvnzbwA/AL796w+xSxMg8FTiOHd1jCROpbVQayoRtcXcQlIDSqABIbrbg7vn7kbi1PpQ8sLvGBhL3bwMsBEoJbqWui8CaeuN/TZtxrTGDa6qCCajqKY0EddTa1JpLcTaVAOgRWcwVrVYNhg0DvR6tDp1vtJBIxzojHg2JuuqayaDEc4+V8K+Lyg60rFOa9+Aguh0B27+rThJCfQZqgY0obaVkYxbrVysz/kt2XbNy7t18GS7RrLeaT76zFN+Duxu+dk7+OA/YZ7gRG+fV21fL09boPvAXNpcowkENtn++HdfwRvfB773G/vo1K9VARE4THUzmoQSOJSY5maJpGBogbmtU8cNJiTDOPSW00qEunwEfSBJIhehLRcdSZNa69g81mjSBSd+vh+6zHxZDhWdG8DH1+1QFBEdR3BQQpOcFmpmRoOH3OBCdrp67Sh4B956du3+tKxjWdtbLG2jWZDJfGU0Tb35NfYRVOtqJ8i7sHbR8/ZACEwVLwoycJHwIlAKdsTGgbLKsvEZ+OA/u23WdNlrwRfAZmVOd5/RC3X7CXDvFrP5c/zduz1P9uYbi/oq+r8aqE1zVV/AAcmNr98fhn//LeAHwDd/4yGmWK5TBXl1rBdnuYtjp4q5RlqkOIwOVzAEtCbvgD+ZcsqGubMXXKENgn1LFhFCCAaWZYgAWMXzWPoEZbez/fD8xRw9M0XQ7Fj0/FAFCEyJBNy9RGMv0WgtwpwZlolMJoh9I0HP5UKEemlOov+J/GRWpQekiP6VigGpl5kd/GD0zRRc1uFo6UfkgHWiHTqFNoeGswQAraEYSmCDNar1wNY7wX8ZX/RFbLs62QAYUFa47u6vJunfAb6/uuBj4Kd4drmcwVUC35t5NLVQjSitIxrqW3A2mX/6ew9x/gPgB1/kENMyEwVKujrVuar1QXjEYapbcyKYUEOEnAuzBLeOZgxDSoajukopltEgY+0ZGH0IbqEK5hKbUWbsPUbTMrJsxNlmrE1X1/MyNS+d+vogs+R0IITSQujLoRCdlBDcgrJCumiQEdHZyOQDmIBao+NtRtjCWy5UprrAA32fBpO72KfWYUCL6EdOKoLma8u5/KcnFLUIN6AFasADrrXwb6torAEzcPxV2NL/N5vXTVXD6scZ2AJb4N6vfkcBb62338Hf/CNaW3cqcOleANQlabamucZUo9SQ6MSj+wOXYPbar3iLT1lCB+8hCaeKqURnGAx6fmxM1ULBKhpdFN2Q3KI1AyUO2RMRUltbzgBN0rJpcekGrNNZLShJ7KQliYglBhp1th1KiWmuIXYBndnNK5ivdL4vhDn6KpI+/Y2lxCL7YJLTUhoSt0YC1y/mnP2th3cDUUrUiFD01UZlmXMRwtSlAtF1HKgQAs0EMRAK62y++jqniA4EBuQkakMVUsOu80K9Cajr2G1ZHeI/u6XPYP1ag9nZr3jKXwFvAG8CAA7Af8I774PLRY8uP9BC1rQWLWJuMVVNRX1L1ZD5r3/wAJvvAd/9wkdJ9ALfjQqdal1UuUA7ljx4Tqisje6mEAbvpB6yEVLOqUufgTUw3ohXl3i2tMcItqYmWSyTZz2N0mCdEhW2m1Rqq7V3EVr5HgDYJCM5Jj7c5wdbv791Ki5P7eeX5fkpABkMK7oxZqeztDChzEHi4mw3Dsndx3PSrTa1kIAPnl4/v54og0EhGBUBmqDWZBTli0Z5VSpH1ytLNZS68JfAVACiGY4ztrHWZz17lnXJyvTFZiq/lH22k30VePxrC/O/Af50hULexc9/gjItPVHvdgJAQ6D1j9m5pjmmGiEZdf8sDf/2q78Ry7hlSr32ovXTztMc3k+DcGhRL8s41G3l0DDmIUIkhuSbxJpIyJ3mnj06ZCAFgYUF7bPiN5PcWKDaBqabFbELMBV9BGRw24x5bjMEM4tobnC3B6P/4OH47Yfbe+fj11+/gzsD5gnPD+89Of1v7x3+1/fmujQe7ERpcttkvz4phLnqzpgT8cHjS9L6AUeoArshU1oUSAF5z+/wCNo6hmB9pZzkagEL9eAdEa1FDUpams0stIbLGdtr4M46MBfAaQVOb/iof4E9XseAbzeP868YJLkPXP2KAbu/Ab52C1P9Kf7hPVjngbpLdCQDiFjbTE0lTqXVGpKy80ffvMCD7wDf+cIH/zQRETCXiQjp1OgpVYqOnNI17N2n5ZXz4ickLyZIuNj4OPh+TJtMrms1m3pp3EHZHnq1LsxbAM/almowGmhLYiUQy4UkAJsxz6Udp2ZLHuS90b91z7/3MP/e6yMe3cN+AANVSDwf8GCXxjSx8pMlIjR1AYctCpLtJl+dyuFUzbjZZKgZNdc4cJKb1Fd8EYGlxOzcmgJ0w7LaozXR5IoIa6EWatFqcNGThCEq0JaKxhswrp3mtAaPXgGdfZmo9gtAwF1gBgRMwM9Wf81rB/BZx+0C8c+1d4F/u95+Dv0U1y+WmuxGXdCLkkBrKk1ziVOJqbQacsPFzh/+8VvA97+Mpvd56lIJdLcgjhXb/QBnKIpE4M4uhdi5oanEXBu4GaVD0z4TITqNaBGjLcSi+sptYJ3SXfDP0tQCRvXtzBEi+4rXDtCyKzd3m1QDu9B1bhQe7e3183w2sCn86hp1hgG1QrFJvLtNF5v09LqyqyBhANytaeluBdQmMUoIoflqFuXkMKT9Jh3mBiwrOcDGT1odRVgyGaBQOPooWchqhInRrKWIEI2YA+OAmOHA2FuBed2bMq00FNbqelrHen+9t70HXAMTUIDLdbwgVp2U1pnhL2V/CfwXt8rEn+E//gxLGdM1D+g4dAdzuvz/VNo0x1wD4GD8ztt7fPM7X7wy6x85rWOXy7Gz1vNB5kR4X1HdAba+QdkZ28ypzjSH2mWzwUCjG6J1IdcnX6dWQUQ/cZts2dgXLLRQVEXAPfpgZofju/A7ue03jtDOm8SLTRcgsi9aXkKkJ3icIn081d3gj69DQF9Y5uSQba5qQDQA9uIwWzbz1GVVXStXQk8Ps60LtJdLQn3xjQQoll1CISnUx/Ui1EIjcTHyWgpFqRFT26CCDbMwFOAE9CVQuzW1aQV8G3AENmv72QGIuBWTjsBz4Bo4rXNK3c/O1sEC3JpS+VJAyS+A3/k0nPb/4L0P+0YwgPAbEgAAWqi2mGqcShxLaxEG22/trT96Hfj+rXb1N9o18DRhJUo7ClpKi9pyckv9S+6kIYwWC7qvFTuP1lRbePKc/Lr1BefLkS7SwpvUKRznNhQ9vS7b7OZMbpthIQAW0deCPlNQTrbbpnmO09wOTf902egBxxtRN+cG1fKi/v0LfXSIJNzf2M/NIpA6BptSFS/nuiGHzFoaaX2TVF+WJVILFttR3S7A1U1w6FeeBAVMummMIqKaMeLMcZbsxdSAOExlZNlkISoiwQ2Y0QY4gNOt+aX+8gVIwGl1tbwWWDd4W13RkNPaQMS6w6cAFyuphbXD+IKrNOraYN7Y+/iHv8VhWofel2J5/asiWFpMJU5zm2qEkB1fe3WDH3Wd2Re3D4Gn6dbkIAFFICKGZDD1jfvJb/RWwKp3sIYBGAUFrzfpMMcvjnF1UvJF6kigKZxczi9wKDg8O334/OTuyemkJxvcc+Im+5htN+ZNprtthiE5aots/tHTw1k2AB89LY42B8tHh2892D4/tTcv9hebmkKPDw3AJpu59cmkk4KEO6ca7sxOLct++sgdF6bUJMGXMMo+Utqv6r6LulMlWiowyFRbDG7ng59l4qRoUS1Yy+X1lA3bnaE2vAtsAq8UQL2OXCNQRzp4a92Br9BX17X6p8NYXcuyjvH2e+6t8slYvfOLLNT4bA33t/jJO8AKO3VQ4xP+QiViKppqnOaoFQDG0b7zB4+AH/56acan7WPgCXBIWqX/y/5v4HSsF3fEdbesoWut5GYEo0WKGKugOMzx/FQfH+uLqvN9HrJPtbUWPRjcjFJ2ovrRuY0pNSGg1lAVETqVdpj0JObeH1gfSHYfsw/JsrMGB+f3Hg6l4P6W+yEmYns+jGxzub6feAxWpDcfpL7xIpsagrRDlL4h1oDRqWQBhqCbbb6r4EPo29XQmYEQGNLyf/4AFpoAUiisT2A9O9VINLe5QQRSi9Z8AAbD4YQXht2ImHFogGEDpBs/m1fI/vYuql5pjcAD4BlwBOoa29rKJfRw8ASIFRrt0aGtyxm/lJ1w/BtMR7gtzaYBIJaFyYpFmtGDmULhxrcfjPgvv/UFCQAAQAU+Ai4BS/wkX3T3wOlUphJbLnq/pX4BKeVoubTW2rHo2bF+dCxTYH82vL0dx4zkFoJBKXVI09zVd/0rogWCHJJ1j26yqcTcojRNcxxKO82thUqg1DbV1hd4bLM/n+J6jrcuhvtbjab3JsFoQ9ogAH3wVDKe70cmP9s4VS6vyzTXJGycxWnA4Azrlz8D6HuLdKNHAKMTo8C6otyWTfk9e1Kdtm2iQy3w3ml+Kr1+f2fGyylKkVh3O0MhjhUnQ53xInAMeIKEMTDgVl2Vb+0B5eolvYvsI+NxK1zp0570MXB3rdVuEuiX9bP/C//7T2GEaSWabkk4I0ovy+Z2mKPUBmib/V/9+CHww98ozbhlvwSeAQZcpGVGqVcoMEClxNVxDg37LVPfcRjK0XKNaPWq4MXUHl/PB/F8PzzY5e1gVOTEwcVk86xEDGMCYFR2gqqV7thkP9t434tWAwe3Ej3egUBpKE2NKIVXc0Tgo+dHcztWNPDJod4fEq2PqBjSADW0Nqs92NlHldtkUNQ55qm2qgGgtE8+pDC3mWx92FUIYxMCqKF1cB0AFvofndYymuVkZqwCOmaGaIJ5TZFKqR8+O2RnQR5SGAof7bBN+PkR7tAOU8XUwIA6xUukzhkYUFevMnySrjZr0jysifJG9HHjoAZMwIfAvZUs7x72ZcnTv8XT50iEeY/nn7xIa2pYnGyK49xqyIg3H4z4s28Dv/uF3+LDVdZ7F/D0SdLoqH1HxaVh8K4rTKXlUtHqoeFyao+v6hHabYc3z9J28P3gntAqhuwka9O9nQ/JhmwhuFlTzCXC2LVAU8OQrdSYa7j5ONB6CgseiFPz0iBgNyaC7rw6zh9clfev0itb+3hqZ5ZehL/7y2POBkZD3NmPb786/g9/d7UbXCEMtr83lFqPx/L/tvcuTZZtx3nYl5lr7XPq1d237wuAQIIEZAAiCIJiWLRNmwozRNkhBYe2Bx554B/nH+CZwwqHBx7Z4VCEKYEEQAAEgfvqvt1dVeecvfdamZ8Gufa5dXEBuClr5OgVHR3V1dWPOid3rnx8j7l3j3ATQCaTEAHRIQG1SHhmbPv0PDLuShOrakAtcrHXeaF3SirlBKNLlFhaeISpmrl3mVRwt+JnwMkxEccVRZEQwSywlDDHShRF7ZjSUOech/Lj03alnt/4hz/rJjP7HPg74D964F/x94qzH+KHfw2JM/jnPOKEE861+an5cY7D6ksLkhdV/+iP3gO++9rjjBPwETADN8DbgBQQKQo/qk0BI7yzCPatVw96P3S8XPz5oTeRJzf1vavpatJHl7arpiI96FUJXT1qkTpZwj32k4nK6egeKEVyZtrde3enTNUuJxVVd6zBZ0feLkweiogkySVB+i9ftR89X/l0shr11PZi7mytr4JZ4mtv2X4qF4oU+i/AblKRXbv2ubXbw3JZFBAXDpwPEYKe8/7QfUnoOT3ZFjlytQqT8KKTv/1OPH8ud3eRtPhQ8ZDeJRjNrZgXVzV5dzJ/vtqdQw0qOBxxscfs0JICSBCAHY1Dg2Pt0FRLEGg+8AZ8/EDe57MJ9xZD5yKPwM+AK+Cb25f5Fqyvc/4SP/sQSNhJNncKBpzo4X1ksuPaT2t3DwBfejrhz/4h8AevHcofAPfAJfAe8BSDtLEtgQgqQRE/LZdzBePOebfEx4e1iT6+nt69nJ5e29VOa7F9NTMJQHpoaBDFJEeZorKsXMJ12BgAxFihks3lyXW5uaip1HAEP3jh94vsill6fg25Tiy9X9QyPb64uz/99IVe7MpXbuyaeCusGw+FBtnpht+PuNjVqagaTGWadOp6uS9vFzMrHxwOpzVC6YTH8E25KXalEpAW0cHFYx4qIUkhvvB++uCj5i5DUoJCijsP86qqxUhKCC8pj6osS5/IUogKdAUnnBoK4QoDRLEGnKgF65kflaEG3FTgBlg3zZV2nkIC2NYJ+bNvgfU3wNvAlx7QfV8nzn6Gl/8Wpxm2AVABQBK8Co+l+WmNU/Pj4q15kFORP/72W8A/eu1kltq5ZZNuMAAJZGX+Wxw6Fpib365xv/jz+7WpPL7ZvXe1uyiyK1JNTW30bkRrEYSo7IoGsK6tR4ruUIFdAWge0SkAVud+0sudmepx6YnXeHbbXhziYqo6hFI0Gj1oxnBOeyvTxZcv9ecv5+9/tFzvyttPdKmy39ll8L2CneLlXWsh16r7WqyIFQFoYDFdm5apFJEiZkbN60tEQVV7KjYp5oBAFTRRdF9I9+gBwW30ODUgpHcXkaCQWHtKxZCUCAnlEzPpEaLao4OlKNIRYelwIgym4Io5QEEPaCq++IgzBa4F8nybdKwPKrM88fn0lnfxK+DfAJfAW1vr8DrnB/j+3yU+eKwB5GyTye7Mwexh9tMaLQjw7ZuKf/Y7f5+Z2YfAAjwF3joTI0qyTRKiSAwtl+PKv/7kUIo+fry/uZqmqhfGyaQWnYqISNEhURYRgCJ46D01PndVBZAi60p3TFVUZEqlBuG+WinKoAdCcVzj1BmEE+hBE6Xsag1yXntCJKwU1Ovf3e1++vH9v/nFCbD3b/Qp7EuPJ+ysLfzBi8XM2upyk+TpsLR1ggDilKmoiUymPaipmUFRxYXKlIRTMl1c9kW9eXefO0W0FPEIOoBQFU/ZInGYWMI/TSrxKPTe45G6XEp5XPAnb+EXK+aG3tOKENow9yHv2BTF4ETuRorCgDDYCThucv/nwu4cZ2c1Rjz43Q+BHwB/DOw2wuZvTmnPgR/ixe24i/NCD0EEIuBs7ktjJrNcaE6Gf/KtJ7j8zmvH2cfApwA2NO84xUly09gk4KACZhdTfXIz7XZVgEKvpZhKMRGzZGHUyTTQYyAVdwIUITENpnwpGqLaeiyOaqgChQZkWT154L2hmNweG1lqSiFHn6oJpJiq4Hpf705tV2x2dt195f3ytMSjy/reTt55VFHsJx+vP7mL3TS9/diO8xruLKqQ9FVVQaV1793x9uW+M1aPTjb21qIBZrEX7YzuaKByzJIWj3V2J2uVGHrIQjIUdHGG0qgkVIlHVRDRO2cBwi6ugRcz7hvuuCyhBTUvJw9MExyQQBBdUAxG9MBeIB0gjh2XCkygQvrn28zzWvM8NhNgAX4MfAN4+/VgID/CD36M6J9BMwZc09EHN3Ne/TT309pbDwWeXJXL//J3gN9/PSY9gZ8Dxy9CLEtzeEkCNwLs4Nz1Zm8B3J16a743tKrLYAeoygqRi2rFPPszFY2gFdkXNWFT3Yh3osbW0KOHa++wUti7QM0S2wj3uD2GVfQe1xe19ZhbD4MI9rXsJwV3a3MErWid6h14Q+yncjvzrz5cVi3X+1pMC+TyeipVuHnNiqkIVbh0vri9RyTNScuk1cpUwp1VrBI74QJoRJAeEs62Rg8Xkm4hIbmDVWG4Q0B1uBQLxqRyVWPp0qkft47Ff0fw1vWKteOmtBchdAgqBc3hDaZwhRMlfxaY4UIRgdlxCtQDqkEqfIXFg17yl8gssckyHoC/Bv6z1wiCV8AP8bOPP/t7six3wskea/d5jdPa7+dMZlFV/uDrj/DOP3rtZPZT4BlQvijfV1oKKoOgniIa9PqqmGo1XBTsipgCgbvFGZiKmUEg3cNUPCiEJvKxcVaNiDTKcwpDtOT9zM3AposJoFORWkxFDoufWjyqcntaLnblYrJpsnWN09ovpsLgVG1fy9I7STN5/+2b5f70l89PJ+xrLZfFJmFBXBTbTWYVEOmqboZiDAi97uKiW+sejpU+r92D0GDELetXq6lwLICIFtF7X1ogQlUjtVDFXQUueVl2QFJ6BLgUq8GQMOEVcNv1F5/OF3+N/Xdv8I234scfOqWY0mJZ+57AVNADkWZwAVfsCKuIwF1DAxh45wDcwCrcYfHgusSDm5FbQ1CAnwDfew2w7o/xyQ9xPA3lGo+t2CM8Vo959ePa7mc/LH1pAfDmsrz7p78NfOfXo4wenjvgQyCAR8DNL23DSh/Qfpk9muqjq7qvdV9RVUxJ8rQSSN2vIbfpY8QGlSGmDwRD10jGMSMRjqB1hA6Fzt4IUEynEmtTDxfw2Z0TgKD3uD2uT653pnaxkz0KmFgU7KpcTFOEH2f/8NnhomrndDnZhcolYi+ym/RiZ1MVMSEkTHotjWUlutquql5GePNOEB0RARe23tfmd9DrSKnKgek7Nm9OAIqIYIhw8FQprhBJT1s1mOo1aBGiENff3duLkJNyfwMw8ONX1+YvGr1oa/1+7q3zRhFdVM/6fYQRalga7htMsQTujrjZAdewAE6bVHbuRu3B1cmN5HIE/m/gP/+NQfAM+CH+6ucIH5TmxP1FwOnp9tziMPvd7PPqTlaR7339Bl/7feA7rxFkAH4OHDb5rYtfQj0VJ1bHDFrRm13dFy3CoCydi4vSi8lkQ/pksBICwrCQWixTVxmuZdm4cFItZSijtAApTjglPCZwFTGEUVVwN7uKFRUKltXn1q8moYgJazUVJX1tHsS+lGrqEatjV8tlsRvEheJiX8pkpWhJZzgARaPYHAbuAyaYKxgNhsaA0FxcKB1SDHfuqmWqcgEsDZGxzVQrV9fkn9Jd1GST9c50Jk92uu/0IDxU0breR3z0EoucvnlZMHljNJcpop/Ymq+d11VUzFuYCqhQwa7AiLsVs2OytKXBzf3wPu/HpHAA2DTx5MFlel7M/w3wVeBrvz4I/hbrj3B7N7rLXILQ4WDPZBan1Q+LH+fePAR4emNf+hffAP7w9cDZHwIvN8HbR19MrmWlvOy8uSxPLmox2dciYNq1mmIqMGHaF4vq2kG6KaqpiLQeqgBzUSNEOrVJINwxBPdV0xtZhcXg7gKuEHiy95hKLRHhGqe5e8d+Z/upkDSlWkEFg61HEZhJeNSp7KLvi+ynYlW1FLUKtYElUVWTCWrXF2iP+3Iiyd5VPegSAIQRIqJgpz/r2EMDODJWcKooZoTQwz0gmpwoBERdQimIAEjt7pFyIuj0uet9jxbyixf9o//rFbS8c1Wu99qdy7GtjRQeZrm+kNaCpiVizGnhuFuxEkqowQSfHvB0B1zBFaUBFXi0UVr653cAsX3+X//6OPsE+Bm+/wt4Bwa4GURWZi0iEbPHxQ9zn1uPwFT4n/7eW3jvD19vNuvAM6BvAqUXX2hKvEDx9qN6ta/VFABU0rOpWHICxUwUWSmSwalq9j0itGFVKbF5rpha9q0BAaDE6ujdVVBUHMKUboRQojmCUg2thamelrZ2N+mPYwLASQ0CoVLNxMwSYKQiO+MO3CW1XIWonTtGsTQQ6B3idYfpck9//z7upL8yKz0WJ7pHhHSydUaAztV9jujB+xbNBxaOAQEzzHLhHkGhiAYhBtvVRLjSSDhd1SO+bCrAp4G50bRHFI9ojcfZPQiVwyzXO+vdGREiU1UAuJvxsgHJ0Y0hyvbo1RC6WohdB+42gci6xVYmtr5F2z3wr4HvfSEIAvgF8Lf4+FMAw+dLAB8iit25ND+t/Tj7YfHeA8C7j8vVX3wL+N7rVWYfAUegPBB4a59XFTmVt66mfS2geFAFx6UropiGCyUoxZ1D8y/C6jBdlKFukijYcGAyrZUKnDpNJEB1WbtvcyLxLGFFnfBhMTAkEdfeL/eVlPt5vd5JKmyZokEhISYMpVIFKf04idZE2giD5mGKCdiLvAeI6Mcid2IFste6inXAnAJID0agufdgRNDRA+7RHZtlLjB8kinOjSWTGpUiOhK3iVAlqDugeeyKpgD1TuWpyP5R/XiNyUxBd66tL0tPHfATOroquKwoiik1R+9WHBxVwIAFxBDAJwd8WVFvBi7Sb/HTA94pePT2divpNt1IfugO+AHw1S9cc0fgF/ibv8VpPXt7bEN5esTa4tT8tPhhblmZ7av803/8Hi7+8a+K2i+eebP7LNv8Zdl6F9t2svflckpsVVDEKYgQTeQ+BOgMdgpyKiZC9IhatPvwifeIIHdVJ4OAonJV1YF8OwmUJHinNOdWwzklt8ymqiItQiClQIG1e2l9qupFPdzcQilgBHsIwGrivafqVY+cbKtQ6TeBr5heKJrY0tYo9kzsFeUqtegTBz8E+RgKdCLtp0iEkwyTlB7CUPxK51zEkN6NIARForM3kC4QF9lRFjJcHbFC3nu6u30+qzCcLDEvbM0lU68z3CeRQ/eLyaCOHpg7Vg4q4RxDSn4NfHSL9wG8BTis4es3Wx9w3FLFecCW23cD/g/g25+H7lwDv4Wvv4O/+QCnGF+eawAygmvzpflxbofFWw8R+e13d/iX3wH+6PXAui+A+cGu4rwxq59Z2OJov/9b1ynMlHT+omIqVaUYig4/ONmU9mXbhqY+RXMBUG2otnLoX2BtSQlWVRmKdbvIOgAAHatJREFUDSKB1MWAB0xFTXtnwGqx1jFVM2g6ZpbhBSGJ5B2GJ+NjMXCvuFRUg6s4ClHJKeIx41GEE3fNXwoWxdIWP60+L/feFu+t98EVI+hERLQAHZ3szgH0IxUConffJP4GNTVyXWsiIpeX5eneLhr3kKLSXNJL9CjSL+zlyQ1I3dx16WtLL7uUhsPNDncnvyq0naAAr1akNApjo7jFYB8dF9zUjWdwVtDQBxM12z7Ot9aBj4AT8JUHofAe8B18/YBffIC7dZl7tGgtlhbHJY6r3x76y1O7m92dFzv8+T//Gn7rzx/Qon7DacDHwHEjEZ6N97Bd7lk7HlJ8f5CTgBTiRADhMKMBVZFWbwEEaSoR0dUiHSpIwCoApOM4U4KhiFGpTJ6zeoyUrYpiYmqdIMRUi9rOWEJMoaVoi0tgRymRq+twFy1BqgMaokUfP963+7lpRH4z7Iouckv5RZEdHYxw6a3HwtZw35t7a9HDg715DzqDAQ8yOBZoiCCiExBnenIkgXODBA8VKwQkgmZ++b6+tbvWA8vMdminhlK4v9EGMOgCjXCPeem9p0wJGHo7t3cu4e73c7x1LTjmSmpUtShAk8SLg4ET8OglrvbABMzbuztt87OyhRo3ukBepj8Cbj6/9n4L+B/xZ4r/+V/96Mcv7uYO5OAZa4+7ud+f+tpdRf7hV67wJ7/3ejdmJrPjg2LxDMzkA9EkB1r5TJ8kX0OmzAm6oyiS1KgiHqxFa9HVGdl+QsDoLgzvXUwJ1dZZTSHSggzkI66WbqxSk+yZJgRDAsh2prUWiZhUi6mYlOCOsQ+dAAU9onv+IahwX+qjp9enuQGAs0uDLiJFces6u98UM7UWbVmbLx0rpTX3vpI9ujvRwhl0R/Ljg8logkdaKYcP+DaKihYtmhNCyVlj97CqyyKvTh56f/3Yrt/dlaWsB4apmy1LRDjVSLr7unqQ5lQTJ08r7xcVugUQioVYOqohHFCsggogX3dFCD66x9dfAY+3ZpPbJkq3INPPg2/zGv23wFufp1gq8D/gL+Lr/9P/8r/91bNn92um6yDDA8GicnMhf/CnXwW+9zoSQMPWDjPQgd0D29B4ACrJH6t988uXpWj2hxyIagq0qKhKSdN5FTET1RSOR9BUBzpOZVAZRCBaTUzEIaooKk54up6amFomTZUikjQuqWIXxfYqEpzSRNpjJ9iZTGb7gp2qiAQkWeCtByCHV3OJqOIqdAyiZiAiHJghR+GdsjVf56Wfus/ew3uOKbo7AowhkOGUHvQYnLqNSMggzNLhLhmcydBGEJ3cFTWz40Fv7/XuwFdzv2/9GHEM3h/ktIY7VKQALXiaG0cqBITuDEZrfHcnOgEHXztzDjyCoZzVpDnuU3RcJSt4fcBYSdj32aMzk8q5y3Pg5RfUrxX4vfL7d1/+4IMPX8x3i889ukPAnGH9x998/NZf/Anwz1/P5OBT4BVwAso2mD0PXOKBjE0DFvvd9/a1aN6ZlM0VcICpBWPUIoHogRj7j8HPMBNVJRiDcIKqMrQ0KAMDLUPTWgWWviqAiokgOifRi6pV1QRCqIi6T0UnkatdUUEVVBMAjWQkKRxVlRHmTRkqAYkc6Qs6Y2EcxGeJfur91H1uvrp7uA/AT4YMukcP9IiIocLqQwtoaB85YVBKKmsguSkhCOd+si0zy9JwOuonn/TDQRnlohQC3V0AU6xrzItjCHERlM5I2433rxSK+b4FCNAACKFAFXgMrlsETBBA7djttsHsuZXDgy7vDIs9g2xX4PAFomUFvj199/4ffPjh87t17WGKXZFdkSdX5Z/8N9/Ek/8K+MPXCDIAr4A7IDaTl7NKUjyY6iVg6WS/+97+5mKo7elYJVm6RPWEWDLhprkKY0ZNYvRFDEDqnKWuaVbsCYslUgRWku2WlBYVS1GfItAYKvwCFB0Lh6oiEZe7sq9WRAqkqIiiET3YPJoPwYtJaGAhASoCdIku7OIt1t7Cj42nFivRPITRO7tTQsKjZUMQ4ZQgekQbzmMJ98zJmZzR+84EnEpAQOwmSxuepLGQbD2eXO+uL0oqdLgHiWp6PLbFIzOZ5VyOAsaN8a1Hhh73JwdgQsuMZ0B5sHx0DurdqeOpbSaH5536OavpdlVha/Ty/34P3HwhOU3At6bvHr72yYcv79cImkot8qffeXLxX/wp8M9eT9fIgdvkMgGXm4DIufbvG+c0E9vRfuud/VRNISmTYYLt4YPpeECmyYqiZA+4dYBIEafRg0pen4QEQIpDujModfACxVJ/UcQpQuxMGCLDHoMRVIim8bFgPxUla2JnVCC6RiyBHpGjEGdIDtYiCqjgUCCLzu5z97sWc8OyRqeuzXOLxzQHJddImUKm8VQi8NxJMJweHPeVjBROMiBOBEUV6Tm0KS0IGAJ5fFOL5qwd3gOkitwfVg+qpOJfkpIp5Hs7udrreuinRhUoWItAcj6ec3ACgAdUxxDKApeG44zKBw3mmWRwhkaWB8zQhEN+0TtiB3zLvjN//eUnd/fL6nx6U779338H+z9/bdDsEfgYuH1QIObkbN3izB/8ONlX39nf7GxfLbXZ88ocnDMRUmrNPCfpA1iKqgoDkBzTn29HjeDqXBt7ljkUS0W7lHqBiijFBKii1cSdIlZNiulkmhgv724qRSmiRUZwQ2QNHsN7HxYCQTryOhOADIlg6766L877jtlxWL2FtEDKrXjAPTzgHKbHFLRA3sU5nt1sshkx4KbJm8hyyUkHqmqtKgP7LdWGt9rl3swy8th7ZJAejj1fyBQ3DaECVfiVndSCT+87c7MimDIrZQGRJ9fJSeJlQIAbxe7iwVpTH9C8saW0h6Wbbh7CX9Rc2QHfwrfXrx4+me/n/+Q7T/Hdfwr82WtrzPwC+AA4bf/uw2qsbfmsnW/PEsydPUlk6hZk6U9J4iYFCoo4mUsRjFWmqIARqhjelKqVWDqLsaQgngoJ9wiVoroGlDGppQUcGSBD6V0dkQpcpaoCTmjQVcyphQgWMJwRJKN3hAo6nLII58ClhSX4AHCEixFybKFF3AN0z3ns4JaTjA56SAd6xPACZn6327gsLT9TscOxRnTHGrycbKs9kbu61uJiXwgEIxckQSq4NvRwTT5fhItIB02L4tICC5YepqqBAN1oYUNyHDkvFhBoPtSajw3PDvhS6h3fboPZM3XgDLJtG2+vbwnv7tfEyjXw3+G/nr731v+KP34f+INf5Uv8K89z4GPgHsCm7fBQGDW2J+FMPvUyGSxFQKECGDd/RIGlCrWdCXegOHtRRS1aTIMsgmRuqAFAd0xFJhNCUyZRgHQTX4MRsttZTbV+ZFIM0CBiRUwU0i+qtVOjqwu7J5U1tWMjPJysVEpE6EJ0RhM9Rlx22emYdFLgjJUawuKS6oskRRNZyU62oCdiIQiIR2C4sOcmgB5UUoqAlIBTPKJnF6nnpQoYcEXvXqxwKOJyUxflPGedhjCEI4QYbQRQDT3euy7Pjz0i2ctqDDg26yGFJxBX4A4RHIkXjv2neJKWdSuwPOgDzo3eQzncXPb9hrH+JfDf4o8fAfLaYMYZeLbNZrMunLf8mpizzG3zVi8SaOXxRU2V4dQBCBlisCZDwZ+UHqP1TVBGREgpCfTTYuHpG4yIKCLFhsV9rg1SrX3ppEjWL2mbmcMINSEECkKdVNMAW46KQ5ugQjs5OzpJjwCcoaEiIVAnSCzBWbADiia2Kkg5eeyqQkmE9whlyZdeRDZXCY8YU44IOW9jMFq3pGqK0MCAVksDYiEjQs3oQTF4j8j1FIPUAboBu/O09CBFJQKEegLkFI9KgQZUpkvTY0uKWPi4WcbV6UgTPQRS+wMtsBie3+NJ+ptkwli2rFYe3KfrJsKd58kvh8rnTgX+4vUiLM/LTZuSW1TJtt88Q5XOV+f4mlKKZiXiRDUtClMBh5/4luckgp1Q0MdMo6tqNenOCHGS4M7EDKSoSe/5SCsEHugc2Cqk+rDABE6qE4UjNyQrfY0hwq8pwSfNOTvWNGgkPAhjJi93KCJEGriAU4gKEIRydahpd4+I5pzMh2hlPuK6uYSC2CyCQpDg9URnp/4xBB4SEp4r39HWkIHQcGpvLpLhx1AakJVu76kVJxqkKCUtZWCi10Z0AoJsTwPMVzoMHTCHZDUXSBBS5jlscfXBLb68Bypw2GZm51Ft23CRZ4eU/Wvfhq9zkvN3jrMzpfk3LAMK0EvSnXqiUkhwkyE4+4aQFAZkX0TlMzedIOfGU0uu5VA/76Fm7qGA5I0BSBCZsYIRmns/BNCdpaRBVVCV7t6ZBqCpCG9Fe/AYaOFLRHN2oJDKjUGRc2AyKED0JMyR3gHIyd1CnPCgCNQDkrJaHS4EwwFSZVALlegM9zHbUAzAsMdg0QK0VBDnGA6rcO2eoiEp3u0Uhatgbd09xCRCoEwbUCr2GtXs+bG/PPIbF/V60ts5V1wCz+cvw0YhGLrzuWAzjjv0bsHNS1w/AhRYtwurbcyUh2cCLv99lUp/5cmR2HGLpL7F2XkExAfLgDPo3IsHPFgUakiGXYuY1EQpUAKdIS77KZNRSCiURTSEPahUCC+qJvixj2aczqhW1h5OqqpC1JjqpKkke1y850Aun4u1IUB6kZSCD1AJHJwnhhOzx+rsQg81y7c1ay/m9sTBlGQvRE9pehUHPAhGl2CIfmYwwKzaPAFDacPJMXcYLBowADplaL+FA+P5CUnR5FSptV1JJFGQKsMNqDV30gL5WCRaRCk3BeH86K4vne1+uXo83c/H8dxEiMuIp7JZykR2BlkLdbQCdTw/4jqHF30bJZQt3/jG98zPXP0HtTA7AacHg7GzTaxsCezcjpzvU2Y+SytETa0RJ2rqRgbG1ScogkTEaN6ZgaZESOapfZXEO+YgQEUorGW4IpmIlbG7cSU6qd1g90ufVKjanaaOoXMnrQW2QmgJLKQHO7gGF49Q8WFqNqr4iJxgDcg4AIcURkDpDIFHL2lySEYg8TeicBfPK4uUVNITQaSKC5JvwpAezCvPKabZmGeS1hyCRKT+fAYKc3IRwXUdfpFgNpuqApO4LHZc43RyF3x8t/6Dt/eXVZbuYPGIQoEbNBCajjEIouV7QHSFOkxxavi7OzzZ4UJgfesAKuBYF0y+yV39CurR/4dz3Gaz84No9vMwG8CDMd55RRGAFwwJ4zCzJCoGiYCTRWVTnJW1RzXhFkxCgYZJqrsjEAhNjAKMpgLG3LWk67hJjgxy0AFIC99V9RY9Y4QAkUCgw+pKBiRM5yARnQxycbQgAM+9EIXMDhRDyIznlX+IsqBfK5xoGipiELGsADIsJJdt4lSTvLbCI0TCgxAfjpNgotyy6gqKMiL/SBikZzrMJoJjMyrC1qK5b682kzwFYBKdRA+rE1TIaXHM7eamrp/6sAh0hQaCyMQmgRC4w3TsOvsGEXp5wux4ZHhkKETpY43dHC1wddp8Ef9DBVm2mc9TN+8BQOMh/woP8hm3XxLoJZxuVAdBo7gwgqoDdrczy04TQEq2AGEiTu4Mk6nkfEdhBoVSCGrjkN50aoLTTJFVnQisyE50X8vh1OaTQ5FEyMc3uxd36+qxFYmRjakHnL4GeiSZgD0gjBymkQGojLUYAnmLokjc1Diu7EM0G71D4DlPkbz3Bv8eBoSSY8uJEOoQTUWEBsNDRFzMZJvbBkNDm4d9Znk4HpgglsVHEzra36GNel0ogtvZc9i2dqyvlumdfTGsHjZGExswKza1WEmZyW2M0Iklu5mOlx2huClYiKsZMFTDqxV1xpSr94f8tl+nA///elbgQ+AD4ONtp1m2fcP2vX/Wfp7TGLYPopSCgnxQ6UAViAmDpjSIKAfnQhBbexZANan55lIGJ3cAPaQPvwelSKQpbCCMlk4CgCl21dTw9NF+3fdnzw5v7SUtkl+dWg92UhkFYgGB9KDnxCuoIVlQQhBBRggHASWtScYFjtFPHHqsEIVSaVuiz7UHI1ZAA+mLm34afUjTIrkAhkQmwdP2gAnrkHM15t2nfc2kxQR3EwROc0uilI2XgLnzvSiyeswJIFYsna+O/V3D9aSvZieyGtOEzQwvnPwvNUBlfF4UXVI8FwUQRQWq4DDjqo7Z8e2Kdwx4DEybnEJ2o/z38sp4DnwIPAMOD4owbIGFB+O6c5CdQy2AXkAO+Vnk1ADVUt9cVEAPESWpot25NqrKVAeGbJiTAz0gQOKr6EizxCAk9yU5HxDsShGVYgrAVHeT1UmfPbsLjy6l9zisjYRHVAFoDAFGhHWGExVBWjpQOUYVP6kIUmUIuZE1sAyOd7hoSaufbIxzlo+RvbIki80DJfILc0eW3VSkBUcKV43ZH4Es7SNiOMjmMoADq7Ku7mQ5kw0VQqnCfcW8+soA80GNdx9XEHZZ9NQSQalZk423TMfqKW/FKjCgO1ZCBBMhgjlwL3hU0r4QxVAyxz4CrgAC99saitto9+/lO3sHvABugdMWYXlX9i2M8PlqjJ8PMgJe0qkNwYBMhaTMq4tATaSkNSoVEmR3qnFSzZ16YjNUpBRdO1swupuqFijh1MYowZ5qCSr7XVFNx3sSUEUpsttNOmmLLu7zaV08q3lXlGwhRaRFOrwCw6cvQoQpPB65zEeEC8SAQJhj0thriSzYI5ZOFXSRIqKa1vLSyEQBUBJPCwhaRA8xpVJ9SMADIESQ7HuMGE2kEGRM7yGUABVCtJycAUGR4XgngrhU2QlftWTrUSGjWzt1XJhJesdSI+A6LsoxUxFk9++OoujAIbAHejY4irljr0idojkAwfuPN1L4DJy22UfWd4e/z7BjAV4CL4HbbYph23brnNLkQVZ7mMk++6AE0DtFWM1AcQ9s+trkGJU5mdX3ZKomA8c5VBCZPDySRTEVocqkkgw32dxCTLS5e7Codh+K7oRMxcpU1sOpiK6t9fDMvhTpIJzJ8xNBMH096SRcIEzUNQWtO0FT8YQGIrz3OumpUSLS4zxVrroEXEXpwTURkmC2Jj4MnOBkhQRdRXUT02cEtus017sE3CmbFPpoV0khTnNPK/ihk5mPhun1JE7cL9HJyhxu4//86f233tnd/Pb1zc5uj909qips41dmbssLPwfcTpwCx4ZdRdtmB6o4KfYFEnDBLn3ELje7gizRyjbRbcBhc1T5DXdoAPfAHfAMeAbcb2VZbLN+PFjhn8PrYXo7ZzsvAFTHeD24Zdz0P4FUVYLNaSajG9h6OgI6KIey9oQkiAirqipUWTRBsCNsc2ipgl213I223p+9WD/99O5KYs/12d2pi+Z/zIOpKxWR44IxtMhYIIZ5ew5gA1BFdyLFr4F3r3ZAzGtPkXAmFkCGlLZQGiMSqO50CiUYkrxdBTwiIBBnwFSCuQzgaOAlr0t1j5qwJwRyUhYSimVuznSECaGmd7FJ7LQcVp89gkhIaVUYcFz6zep4NPHQneEh5oFi8MhhyXg7s0ABcN8GEDIC6zZaO3YIUASPL3H9JeCtbZWeVgS6qcfvtqyWkfEb7tB74BXwCngJ3AHzgzlwPMAj/VKQnePs4W/NRYWWjIAcaY4ulUEWWKPTUr+TpgrAI1R082l3D2nuxbAzFRVutY5wqJ9KEjeIYgJiaJox9lOZqs0nv2yrKpXau7vWAItq8zBARYcSXO4Ox/CAMWx7AmMchs0pXYLxqOB6Z92VFmvkyFd6DBfOFHwegvWkWYJxRxAJ0BlVpOTk1pDtrXuoCYJa00KSAbjHbpe/zDY0cUWyrL5BQ2R0DsQEqcb79axOSqZnj7B14nbF+xe7Ii0xdjT4GOxiI11BiQ504tBxKUBADAysHNP4atgVXH8J+MoDSY7zDhRbhGELwdxQ/TpUo25YxbY1EOvm83IWCz+nLv/8jekPsBsrDgftnc2jO2K4ReemHFpETRcnw3V7GfOKyf9wEEvnaQ1TWCpUkSCzl/cAkBDF3BzSEq8mgrQqzy6sd99PDpGipaShXeQ74x6+DTrTjTAnCnxoUTg+PwbuHkHGddUIBFlNSUaIYOhqb38WEQNLQg4sq4Al/TcBVcnElleeCgdEY/NaABDBIExSaoke+QnMS1+9h4+6rprkX3JZISqHFhGRO1gyhDRgjbi/X6Gyv7TExpE5QgsM2FYMbkIL3He0gAma49SxOJpjcSyOU8dlup4/2iLpIRTsHArn+Oib8vKvPKlgcB5eyIPN5rotA+LBB+cfbft8H0uqn92XpIwFki8oQSlGNZ1bKJyguACsoq3TFSUxr44APGhZ6ZZUOk2MmubdAoiGdqKWoQEjAATVytVF2U3lcFr31/urR1enZ+t+svfJFy8axLKscVA8ug64ITKEI/1YyZAswzPPgRLwhJBVxamFgSVHKklk9xCRYrK2NGvHpHmXAgIFqrL7gHemFWdOqFOWq48ybQy0xrxXhtGFQjhmZ1iX7s7kLEB5NUkEInhVdW1xf+rjdQaz4jTRU49Ti+tTx5Oqd6uny6UzLWk+898iAMWhoQpAtIAHVFBkU/Iu2D8cmPkWZOcld4yGfAziMl2lZow8IGCez35boWJLWud0eF4G/FKbef4YQAeO+Pk9fvSq2OakJYl9JQjpARNoIoGGXADFqC4eYRRCu3tRqFmQnbQQ5gyDzJfPGRAU06yFWoSH7ooA7D1etdUUT28uf+TPzQDGzc4uy3o/CnJYgrNDBNhiKN9NkPRxuQsw3O/y8xfiCuWmVZbXYvfwoSQ+gHTdKUbLh5XMZJG7N0GIyIbxT8wS8o7L0j5Hwh6imhWYYfOwCuecgi1kOtmvnTf70uaYFIcl1s5iaYYnUDIEGhHSnXg540uXtUj3NC+W7SLiYKhT0B1z4LEm72q84wkSVGI3YbrZdup9y1h9A02crVXOS8nYspRvwXf1+bluthG3G9Zt3f4qfVDk4cF1iQclmgMnfHSPH7149f3nBeM7wHA6HbVmqIwVDSWS8isUVYGwR3bgiX4IETXyuLAUCNHFp6rOiI6iweEcEKnyGIx5zVYy3ntyZSqIuKgaAgXev5xuX65RlDSCknbEo9RBrpe2WWimuBguaBLJeRJDjyj76cW8LqCa7I0i5h45nXJqFnlO8dYHWpafOQEWleYj/UZEpHG16BgtjJmrhHuZjMz2IEjNinFZ3EeVgQi5X3yncqGQ4N2SEgvKQEhEZrUQFfbA6dAvVC725e7QPVC41WcZA0KI4tQRAcmbJis2GTdFMTy+3Bw5z8D889V5Zla2bZZ2zm0PK6oArh/sDG6BT4BPgdTOzcRWP58dz9nrHG0ybswXB/zkFt9/+b//4JPSWgBIcH5OfVZnSfU8layrmriJijAyjkVaZ/aMdJkj5gYypA1Lp8PSi0gpZiYeYcXS6kYotcbSA1yvL+pxbrd1PR7XiFh6IKjQcJ8XiUrpklEVJCkqFFUGzAJbZzCGUyO3wSNW5dL97w59X8+jGWg67MmABK8dG2AMANuoltA8TDUUPkjqeS1qCotARUFI9K4EevdL0gPdUttRAPTVXx3WIAKyU6wq+708u/UvX8jtHM+PvrYo6hQ15WzSTGbTCqytr92+8ewI4e28CrETXheZklM9Xnb8/FV/e8L+Pj11ZdDnTDAprELKZqKoW7I5Z6wr4LQ5G59ZBfqALhVb/N1tWe0l8BPgb4ccUNqeav1V47GHoYaRRz864se3+MsX/+r/+ejHH7+Up5dmKaMBJDIlUXubVUb25wLJGWROhERA1c1GZCxqEj48JkqasNWkdSo8x6Ck2TDaKSa1WDG7vT3UpBUJILhbGBBN5qRseAdG0k90gBjk3MvlIn6UzoAKq4iaFB3PJ4HNqG5csQ5qGvhsk4rsQSNCdXxPyScAxpI8P53iB7nkDLLaWN1aFhyAO9fVE0uWOLuLAg9cFamGU+emJQMAKmICGzg/VtWnV8VUXp56BKrQxtyIhsTj8X7ldcW+SIGYUEQMMBVT2H66evvq8aP9bioiCAeEu6JXl/XRZd3vyq6WmvRaxejDIEioTgIOIWIoxS52RSnzYfn0o7tPP3x1OszLuvaOxOtf7mxXLDEuESFpNwkw0lVXlh63K58d+ge3609fzj/7dJnXX9dqvDlvzpvz5rw5b86b8+a8OW/Om/PmvDlvzpvz5rw5b86b8+a8OW/Om/P/o/PvAOvsiSannj23AAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8aZBe13ke+Jztrt++9L6hG40dIACS4E5JFEVJtixLsmXF8si2YseVjKtSdhy7Kq4k40y2qSST8iSZxEkcxx5bdsV2ZNOyVkoUJZIiRZEgAGJHA41u9Pr1ty93Pcv8aADERlmZ/Jvi8+e73znn3vvec557zrudC7yLd/Eu3sW7eBfv4l28i3fxLt7Fu3gX7+JdvIt38S7exbt4F+/i/+8gH/iRp2RCp6b2Pvr4U2kYvfTqlyziXVs/5zpO1qnESQIYGBNF/UE/mJrZubm+GsWR43iEIJPNRFGgpJJScsbzxWJtc91z3TCKXcsO4/j8uTdz5czEZNloGSWSC53Jo9VQBGp00h30bMuqBEFXyl7Wm856BU3jdrduFO911wlLlCaurwkVOW8qTJKgt0EZc5yC5xEukkEPF06sxJFmjChlBBeUQkppCSENjNZKGcYYCBGcUiBOJaVUCM6FEIzHacwIMSCe6zFOOBdKKaO1n81SymSa9HrdOIqLxWIcRwQwlCVRyAW1ckojZowbo5QEMQyE+XliO9xI27JzYVRTMrK4Va9HwrInx8Z7g77vlZyM2+msVcrEzxf2zD8RJ6TRXOHCPbjnidrq2rNf/j2l+8PV+4k2L33zeSGEY1tREjke83PcKBb18GOf/uynf+J/+fqLv6/NICtsRVtKO8VsebPenBg9urqxkfWyW53TUm9VqjtcMWxUeOTgR65cPRvFScbhRx98upT1AWxsDn75Vz5TyAvbNt1gI9Whmxk7uu/pU5derK2vH9z7fmla166tnHjjNUqcbKbQ6mxKrQVzueAaoVb0/e/56aOHn9xYX/zcn/wTSuG52XAQS0gCwIiZsbGhUjWMzGf/5r+8/8HpQQDy23/yfx3c95Fj+2a3effd88cf2nMUwNX6FSYLSRQqLQnUtaVLUYSHHnvviy98NU1UrlC0bWticnR9baXe2DKpmpqeKZSqb77xSnWo2txqzs7uevHFF55/7k8feOLIzJ5CELQsy7Us5ebj2nrf9TL3H921Ue/t3r9vnH3ie1c/N1w4NlWYB2rAEIDf/fO/1wsXDWHFauqS4f27H2yGS+uLbcPNrl0H5sZH6tE1l1X+67977txr1yzbTqLEQAvG0iR2fJ+AGJAo1pZjy1RZgni26IUxo1zY9uTEGKPGtu046DeabcdxCuVyLpPxMl4URpWhUWO00WplaalWWz9w4L5up+FlcmEia+trtk38cSX8KEl1xs8ksms0CwdauOnUjorvZBMt8+6Odv9q0Nts1BNG3cefeEI4JE1z2axbQQnYBPYBYzde9QDwAJzf+sKVxdP79z+zuVz/rX/5H33fL+az7W63NORM7slQRVur7t/5O//0B5s+rgEeUP6rml0CWgZLPWz4eJTh/hvlTaB0bvMbf/kXf+BbQ3Nze18/+a1+kFKIfKEg7BZI4Zc/85sAJPCv//PPW5bxrNLGZvOnP/2/94PWS6/+zuFdB/fNHLWtMTtT3b4i95zKTZJdWNksFK8//0xldnljy/Uszhyjdb/XO3TkiUZjk1JeHalyZpVLWcsSMk1On3jr6OFDE1PTF86dHh0dzWTzUT90XOf0ye/aFuv02hsbvWyBj4yOUWJJGWayq47tEpN96tDTAAXw4MxPbd/0YuNLu8o/olF2sz0n7zfrCgqO56ZpbPSAcRx4wJnPTgAHM844cN/RBzpXT9ddz494mESx79tGCsMsyASME8YYJUYTZbTruhpMGsMZK+RzBFrJxCnkc/liGA4EZ8aoYiHf55YBGCVRnGaymTjMWo7lyezI2Ni5cxcs266Us6m9NT52sBeulXIT7f7F2akDFxcWR4pzkVrXNKRE3z/7synWnv3mPy2WcwxZ7SwlukRhVTAN7AL2AYs3RrQFnAaeAGDbznuPfdrD9Jsrv+M4tmNbhBDXcQT8waabyYqJuTzQAfK3cyUGjgNHAOeWwskfjI7zwHMEkzkAWAXuB0LABUoAXE9NTexqt9uer6bGxxaWN4eHxqul6VCfeuaJv1+LBidPfTVrq1/7G799dvnkd1757ZGx3MzQODA+WvnQm29d6IRbxAwmbvKMQH3rjW/tmHvA93zbTWbK10XUgJYJcRzB+FZrnVCnUh36wrP/7eTxN5565iPEguu7URTlCpX3vvepbC7TbTcb9fqe/fuCfjgyOn716mKvu2kMwn6rXN1ZqopMPmSCbqy3/Qw1OnAcB7CBaQBb+EIVkwZambBtzl1bXyMsRDpeKtiRXEwkjWLVqIdDY8W5bA4IgQi4D0CurBlMGAYExHJszjgoNaBporShxWJOKZOqwGjSHcSMEWoAo1dW10qF7KDXYYxVqsOu64VRPAgCxvhgMBC2PzExPgiCKAqVIVubtX6/XygV6ltb+UJheGhYFSrrW99jTKxFdUoz+eLUj7//s8Dg+Vf+NGq18hXr5YV/XirmS+XJIBwIEa1c60H3bd4Pw3Ag/+LQ2LBE6GEaEMA60AYSwOoGF/tReHBoeu1aw7HtbCbDKNVKG8OSUHcTte/wEBDfoMJNDADcTrL/IXwAeAEYBtaA/wQMgF8CCICZ7Lw6OvHtl756ZalWKVYyjfrYeEkrzePMG29+cXVpWZHaJz/26wBK5ZLgdnW4sH3F+mY3DsTyZq1cnLk5pVLXz/aj9lTB39xYmSlPXu2sb1d0B9L3fM9xGBer15YOHHogjELXdnbO71JS+b5jWVaaKqNULp8fn9qxurKaL5U4FUkcum7m2996DsYQSoxCEkaui1SH4F3LJpxmKuVyp9N48fyfAG8CKGEuxjWC7t7KVIEcGhnxC9k5ahjR3UKOu7lOc3DZcrkiSQu7N5Jtdl4Avnd0X0kqyQjVxliMUWIY54yxfD6by/kE4IzYlgBIEMs0Va7NfUfE4SCOYy/jJ3G6tra6ubm5uVkb9IKteiPs99MkrNW2gn6/WqkODVd1EvguF5zls75tWb3B4OL519M0sT0ShXJu8rHp3PsBhLjmVrpjk7se2vmZx3Z+SEtfKxYOWkHYqi2bjbV+u9m8srDgWW4by5caS8B3tt9zIFvHlwEkoTz++rO//8Vf6neXqpVKpZgnlHDOHZ/nq/DyZO+hWWDodpIBKAEH3oFD+vsy7NkbB+8FnpQoAXPA+4DnNswfAAhRe+HlPx8EG4NBfHHxiuU4Tz/x2dkde8MBVBpOjI0xxhaWzgEI+7qdBFYWG+0vbG0+z3UGIJu15mqtdvNm7KOf+qBtu9Qr7x4dBVBwshudFSZySRgwSrRWQdCTSu/bvevq0jJjvFQZ5lyMjw3HSZKmst/t5PMFpeKVtc3hoQqlPA6ibr/79a/8sdaKUmI5YnymECY9YgQobda6I+NedTyTLWUPjRwGHgOu9NBsp1HK2gKyj6DfiWO9amg/7hNDZLcjXTtXzJZthxYyu4fEPiACpoFxhdPf/NqlJFVaKdtxBCOEkjjVhHEhhNSGUaa1UkrHqTQwRCsQCGHlcjlCTK/fN9pogBKqQTgzQthTM7ODfs+2nanpyV6nk8SDYiHHhLOxseV5XhIH3UELJFYqhOH5Qmalfnq991rKW/eN/dxQbh6wgdGhzOHZ0cfmd+w6d+U7WptCwRI8Z9mqH9T7YZLx/diWORxtYdEF1Yhi1CaLD/vFfGNzc1AT9UYHlMZJxCizbOHl1fCMt2+6QMG3F7XtqQCwAQApYN1Fox5AAH4vhi0CRSAHXLyhJsYUC1u45KMMlFwCirkQaaddq9fT9z7+43GaPvnoj7mZnEzSpx/41PSOA5dXv9XrdR959BM+yxQzhbX6JZWoRNHLtQv9fndpY+Xy1as/+qO/6rLrt+Q/+eHP6m0t6QbK+Ylms0eNZhaHVt1ufXp6fpCi0+5QZlmOoEZarttvNNIkyeVz1WrlzLkznue7nhv0BqDsjVe/pbWSSjHCZKq0kiaxe03W3ooi2fMKlen8HhsjwKMAgNkLV/6sF2BovHm1m/cxrhg3Ojqw/7HORDdVotfWV65+U5LWkDe2tHq6Mj15s/ssjFqeIIQNBqHScLKe1iaMB1IZznQap4rGjrBsO0N6YRInhBLIhFpWkqaEGM/zZCqF4IMwyWQc17OHKsMgJI7Dfq8r5fTY+PjlfiuK4t7KCmNEayU4yWR9N8ecrMg4Q4tXLr7viZ+zs3JldRG5O8fTQjaTKXAnGhmanxt67NLat1JESSIHfQM1iItf3uosFfNPZnB4e+HbXZk6mV5MkhojJIoiJZXtO0bSbo1OzZY5dgLjwLUb6tfN+2XuRaYGAIACU7eXv5hiQUAADrAPMAABbOCHXXwnRODiMYbXgDOvvXZyc6MudTOMe5pEnu86YDuH9gJw4Hzk8V/9L//91/JWAUCIfq+/qlLS7vZzuemNxmKn258YHS+Jt+/KfuM3foPcIkV9kFqCpXGaJBGjZnXtytbG5r69+68sLsdJyiilhJbLeal0EPS1TGZ37h0EvavLq4WsYzuZbrsTDHrPP/dsGIVaK0YZIXRsOkPBJIk9VwyNl3fOPZCnSgEaKxSTTbxxdfF1paI46Q3C/sTYQ4lc2Dl9xOE7BiF2jTydLYzX6t+dmRvutGhtcz3NnL5WX/bzgYM8MPjOK28ZSdJEgsC2hUp1LHXGsy3BKKVpkmqVGhCtlFZpPpfxPJdxEcWx0SafzzNKKKXDw1VKxeTk5O59+6Iw1lr2uu1CsTwyNtpuNizLKuTzBrQ3GJTLuX2PTO3bf7TV6jZbK3ES2XZ57+hTo4W9Z9b/eCi7//ZBzXSjjYO7D/h+ZbW2dfnySdfNHt4xP53dF/BBmY2UnR8Hqjdfm5a8/PxzX+60+jA0TpI4SY3RnHFQtnP38OTIMwC/yw6ob5urd2ED2HlX4+8CjGEYmI3wRY4hIL4U/G5ZHANgYVIgC7RirBr02h2uweuN+pnzXx0MGqvri924OTvy9hp98vyry2vn3Xxa8mZjjU5vUZNut9cUwjqy88BHn/lfAXazMb1dDlR80W4FRssk6S8snHr9lW+Pjs/HCq1WC1pzIQikn8lE4SDr+8MjY0LQCxcuMJhMNhsFgZJqYeFiv98iAAGhlCRxWrsWB3Fqi2FlLKQFojMnNhYi5DkywF+sdj7fbtJ2K+x38cjBvzeeuW925JP1TnTi9PdsOrneutpYf+6px9+XxtlcoUt4t1UPKlVd66wDgx42fN+B0ZZgMpXtbtAPooznWEIAIJRyzigTBsSxRM4Tlm2BCak1tHYcK+N74xNjhFLf8xuNLcf1tmpb62urQ8MjQ0PVNAm77Xan24vjRGudL+bSRMZhVK9vJWTJy4U/9dFf+YVP/sZjBz8R4OKpq/+93V578fxv39mf1VIeHynjmX1DH/3YY/9qcuKAh58GPpAR5QAD4MKtjaMgIoiVisM4lGkiZWpI6g3pXNGanh+6F5lwY+m8G9l7FT4EPAQ8CNgOUmAcqI54D66Z1240qAI1CdpVydrqqY88+dO/8nP/Ikqkkmbv/gefPvypW6/12U/8A5WI73znK520USmPpUpzy+RznuuYqZHJO5byO3kGII36nW7t8sLp4997xXYq8/NzKysbWivGGQzJZjyppFbKcfxKdaRW20gSmc/nObeCwUBpnD9zQkoFGKkUDLQ2zXrg2X4+N0x5v9lsrK0tpTLoxv2XL70c4U3BOM/0KtWpfGEigxEANrzZ/A89ceDYTHnXdDGwcvUcRu6b3P3g+OPHHvzwxMj8jPMT8/kecCYDzgTP+K5tC86Ya4lcPsc5kzLVmgAsSrWhXAhh2RZjAoQOBiFgqtWy57lRGAIolYpJEudzvlY6SaLN9ZVsNj89u3Nufle5Ui7kc0kcCdeNgrBSLhLAZoWJ4pGcPyawG5gEkjfOfOPy4hub68vlsnp96d+umS/d7MyhbOXWvp2wPrZ9oDHi4VGgBRy/WTucm1m5EnfbSRzFUqWUYWgHskNJdYaOeR8AUqABbN5oHgPrwGmgfi9Kjd+r8FY8uP2TxTGQ48Bx4BIAQLbTtY3m+RThdgMDkfFHJmbuVgHxyQ//gmOPv/ri5+O+rPrzlpqyxYgCb6fdO1reqSfWmkGzsbq0dKHVaPle+fD9DyuDRr3uOC4lTKZhJjscDAYGxEA7gq6trjqul816WpM0TddWV2obV7bFM8ZQRgRlURgPTTmW23L0RBjSxcuXLMGXF/40jCJh7cjl/LmZowdHPt7BV1r4dhFP3pBlNwBA5AsMKAg8HOLs6tK3PZ+u5b4yhok+aqs1pGEqlUyldl2bMa6k5IIDaHeDIE6NMYRxGBijOCWpVJ7rgBjBGRNWGMabm1uVSjGO01Kh0KytuZl8xnc319danbYQTqVadF0vSRLH9dRWfXioEkcD3y+8dPyVNNr4UuPXYbD/4KFChcYJ6ffV5csXMlk3Q57YwpeBVhWfdvHQPQeZwwJCYHph68Wd1XFgGACFT8Ao5dCplNpiREk7aJOhqnNj3ioDF7YbAxIYBRRQuevyKXAeyN+lnN2Kt31sYzgKzAHLgASOjYtj49W3zNyby1e/fm5ja+fMvvsOPTNt33wQeSttPv7M3/zcn/19dSVu9/sg3Y3GmqHJ8JN3+lnu5NnSlQvnTr8Wxcmjj793bXV1fvf8+lqDC84pJVTYQjMh0nbHsUU+X+j2+0rDc51sNtfp9KRUF86dSpKUUMIZ10LDQGqttcl6E8I3NstZLNncSgZxc5C0vWyuUBYTmalLGzGAPD4EwOCcAo1x0scuYADQMka33Wwx5PlLxw8d2hN1xoI8W9is8dQvVPx+MxSc2Y6TpjKKEkQRDKJUJqlmFFGYGIu5FmPCsgXLZHNGp53ewHNVmiRKpu0WM0YPV4pB0Ou1VLFYLBSyzWb95JuvT05O9gYBjOq1O1Kmvp/N5XKV6vjDI3+tmb7RCr7gehNj4sHE7zJmzp06320PjMzlcBg4vBR97qZX66r6QobtqNzigChgx7J6YYodFI76zpnPP7r/PcA+ALZjx1HICCEwSpqNy0k2y4aG1C1D1AWuALOADwCYuBeH+kAXOHh7YQJYN1giNS7Q6wGAi0AXWAaqwMVtMYA4U4jPnn+B89KPfOSvDzu3zo7XOfO9i9/YvfOR19/82t69TyoTrJ95YXpofm7C7+haxd7z/Xi2Ue8yxrQ2AL776isPPPg4I+h0OpxzCqp0Ojw8FIQD3/c8P5f1vcWrV4Vt24ITKpIorNU2li6fppRyTpWSgnNjYIxJY3XmxMnqhK9jjwnPdi3heiRmRIvLF1vW/r7rEuD0th+ogRdyGIkwIHhNw2p1rMn8LuACcLiAgxmvSGVuNF/pozNUnBuzPn7g5/Ebv/63HOpmbBFyrrSRSdrpB67nlouZZqsrOMvm81CpVEqHke95jx0+fPzCRRgdqFQwRoyyBOs061SIfD6Tq1SUJmkax0Fg25YhYNxOk0hptFuNbL4waHe2hs5YjHY6vNVea1nfU8YYkxsZOrrVPO3n0h4uRtiYdj4EvAocOL3yUqkyUWF3eLnKMgXY1nTWLNG1K8HJWW8fgCROiDGaAIYQwqF1GsuwNXbLidPA2o3j+r0mMwBF4LG7CpuAAS4DBDAUwY3yCGgANeDTwJDBVwn8tcZKo9V7/6OHBQrvtARXyju/8JXffOKxT03l5wBQWlpdeqWSLxfMqDYRJbc1pmv9t715g37Pz7j79t9XLuca9dVde/ZtbvWVVkYDhFochkoZx1qbbC4rtekNBozQXC6XxmEw6C9duZgkA0pACCGEGAMQTQghhvbbiMI0ToKwH3h28fFjP0eYN1w+Oj/zwY2NK7vyRwD08R+a+LcVTCs4DnIB7Asrg/X65gBKwerjWeC1HZOzmoTNUG2uJWPWx7fFjmMppUxSFUVRHEtGje97ed81RuU8Z9dkherUcnzf923HTuM4DtuQidLSdRwhhDEKzGFO1na8TLEkpd5cX8tksoZQ1/OLxaohLJvLWxa/trR05cqVNO1X6XieHsln5menn94/+rHpsYNZrzQ8RaZ2zMaReumNf39t7RWJGoA2fn9yIjfmHLnZyd3rHlpoCYAEqOTL+UQtAy+vRp9XUjLOOWWUcc55ksRKG0puVaOHgMM3jrduHJwCakAXiAF5L1acBTTQADoB6sDgliW1DOwFntrmA8GhAerZUuH+nQ8IPA1sS54CA+DWaRU7ytMf/aFf2yYZgAd2P7nWWL+0csrQbrfVvOP2/OyZf7+A8sEDH7OFWypXwn6nkMttbl47fPQ9toVms0kIZZTCyFzej6NYponWCINekqg0lYxCyTQK+q12c2XpAiUkVQqKYtvco5RQJqVstRqTbtmxqv1WkMlkBSoWxobH5SBY7/cVYIADGXRfu/a1Y5OPhNhYWr3keP6gq/xMStG61q+nYWm0WqhU5pbXXm/WrqaSHLj+kmvLtmQc9vqDVBtHEBDmcZ6kchBGjFKL6/07qrVWFCqWpMTx3CgO875b6/SVMRZnShvOqSV4EISNRrtYysskAjG2xddWVyzLjhKZK5S3Gg2ZJjJNOb1urs+VrttfeRzIFw8AQA4X/N+qNc5Zlr3SWyhmNzgGGhu3dHjfxXUv+c7MjwHwsHHf0CMSr794+Wsrb3GttdEGRlu2a7QmlDJKuu1FILpXcKl14+AQEAObtytkrwE5wNXYougDBoiA3R4AyBvqL4BxwAMKN/6WfOwB6QNHAAlcBBZjFGzsvPXGPTTCIB7yro+BAX7v2f+z103jeCuSYbsTPHwoX8q/vXDTXCnDrYzruEmSCsYsyyaUXF648tDDj7c6MUCFsBjjlmU8P9vrDgyo4zrCynS6PRjCGbRBu9O5evliOGiBGBBCCbTWMEZrQ4gxBpYjxieLs7uqni86waXXz/1nTjVSEIJ9u58CZgAAj9p8+I21b3BQKS2b+9Vhn8N18aHJzH1rK+tvnX+z2w2HK/uHRosTk3M3H8EYbVuCc0YIZJIACKNEauJ7nmVZpxfWLy2uTA9lxgoeJ6CM2Y6/Y7Ti+04um2FcGNB6vZFKlaSyVtsIBmEqUyEsx7HiMCgU8rNzc6mUvX7EKGnUt7LeeCO9UIu/eteoA8BsaVcxv+dA5cdnsg9vRTyDv5vDJ26pzwh87PYzRoAsx/uemPtHF0/XYUAIYdzijBEKRikhxM/kbpCsf/u5j95ybN9Osj4wDOwBpikeAHaFWAUCYCewE9izHcQEzgIAigoXb7nOHmAIuAS8BTSAweraxZXu2ZuXXu+99eLLn683l2+WEODjP/wreX9s0DEba/FKbf2l01+/VVB+4fXm449+MImhVapBPd8/fer0rj2H81nr8tKWsCyjlZaR4zAhrDQOGBfZrMcYY0xwTnP5fBhE3U5vefG80UopzSghBJZlyTTVlFBCLItawlKKzY6Von6sTKdUrB7b++m2WWg0u2P8mZvS3Df60a+d/Dfjpc4D0081dWsjPF+uPACAYeI9R37inuMKQElDqOGWpaOYGK1SmUozlMvvnxmN0yBN03and221dt+eHTvGymEifZtRozigKHU9lyVcqkEUxamUMpXt5hYlRAhGiZtIlc3mbMc9depNpXUuV5Cmc/qts09MPMFRruHzQ5gBZm6JBWEA68DQ39o+nnF+/J1kvifm5u5vbD5HCDzPD4KBYIwyoo3O5bedZ3cna3wfZFKEtzjkoZCGSF0AaAD2jSjC9aWQvT29AYBBP0n1hWsnc65tkKSpmc390M3ajfrFSjV3ceH4vomHbxbmOfrR5kg5s9WVlpV3s+LUxucPjVx/x7grK8Ojo0EQ+55HjEyS8NLZcx/+2E/1I2gDSmAolWrARY4LNrdzZ6/bk3EirUQIPug2fN/t97qb6yvhoLGtlkmpOYfgFIREUWLbAiC2JXy3dHUz2L3zGUF5BrOAM0zGq+UabsP4UOHhenOZjjkenRobsr0b87m58QLegd/6D//GdS1biP5gANBtN2wu60dxdOrCJZlGrsUmR6szY6NcWDAk51nQklLicDTC2HY8QgmlNAjCVCpjdJqmuVwGBpYlavWWIVRrZbTKZ/0kCim3fvSjPwtggIt57ACWgU2gArSAUWBHJ1osOMPAPAB+b2fpO+L8uROUEtd1w2BgtKEWY4wwyhxn21y7SbJ3Uv9vg0C1oc6W2XYos68xCJLUtZ4HBPAEcAmYv8sm3cZlgn22QN6+0K/Xg8A8eOzBW2rDIzt+DEC862bJ9cilbeejYK3bHYyRnFGREG+rlXTXoUeFhVzW5gKUkksXz5aqk6WC22i2GaVaay0T2wa3bW3Mc1/5UrfTqQ6NhINOt7XJGVlbubZVW1tZWgAModQYSKW1gdGGEkIo4YwZYxzffmju4KHhv1GkBzWSm6oGxZ1u7sPT758f+/QQPp7B/UX8dRt7AWzpky+e+p0Ty8+eafzBHe0btWXbEkkqtVKglDChCU9SlfWdPTsmds5MlIt5iwtQKKnDJJaJVFJqrccqBZfqoNNQqQqjuN7sJql0HIdSGgwCQgBCM9nM5sZmp9O1bSeJ43an72evD/Zy840UjT4mA5SBBxWaAc4CV6edJ7dJdgNnb/XEfh/8+ReeTcKe63ppkiSpFJxTCsaoMRiEg9vb/tUk24ajp4BR4CpwXqXUYl4PbSACFm4X8ia2Xb7XdZLp8R+rjlT6ffR760v17Z4f3EwYuRmIqAXXHcWPP3AkiWPLFkmAJExUwjfkme0qPjW3M02gpDQqNUSfPHH8wz/8k52BCvo9xi1GmZdxR4cmI6UdRscnphnnAJShvV5PKe17/sbqcqe1xhgzxhBCpJTZrGu0ZhQw0MYAYE7cxEoJNSBf7y7nclO3rjW3I3d3JCWMW+3u5tW1773n8Y8CS9vutG0YY4w2NicxwCgFoXEScct0w/CtK72RUlbGKWdxFCeK6SAMU0F912NwqDZWEhYtFpiUAtmMq7RWSlNK0rnSfbEAACAASURBVDTtdTphHAvbb9aura/qNNWuw0YqRTt3Xey9paPAADgCECAxaHgYBmYBD1heaH+rWpjJ44nLg1d2+GWKo9+fEP/3b/2jyxeXPcdRKo3jmDNuO7ZtCaWkEGx85iax1oEysPkDZjL6Yntx3A/sLwoACrgMrNxhOd6COxk8VH043PlKO22eW/7e2StX5qeP7Bx+8o7le2nl9ReXLjzy8AcP731wfeNslKQGFhWWxdy4n24vSDxNUyVjziglZOnqpfHx+ZGRwpe+/JXN9dqjT35Aq3R4qAogDiIn6z308CMA4lQWiqX5XftWrl11bZbL5QaDnjE6lYoSIjiFMZxzqSRjgAGlVKp+I14u2eeAJz0+t9Ba2Fk89oP01DYuX/mu7/lCzE9nPnxHlZYyISbnO1L2CKVpKgVjtmMJIYTrak0GcdxsdTY3NzmjnmvnMm7GdfPZXH+QDAbB3j2zhPHVrdZqJ4wjSVxqjAmDME0iLmySJrnKcBDF7VabCy+N46HczeSItxWaFN++uGR34ivViT+Y9x5fC16xqZWHB6yWffTRviuT4zb85Zf/+8riBgHt9LoqSQghGpBSOo7NIYYm/UcP33yvusDoD5wuezcYsAvY9Vc3fBvZ6enJWvtq0R9RMT9z4dJ6rRnE9IMPfKYmXzt56qVKccZirkF8+eq5sYMHdu6YOn7m/K6ZsSu1rfpWM5PxUcDC2qu8WV9pbSwFnaZWstdqP/Xxn260+teuLva6vUG/XdtY6Xe2Dhw+YlR6885SKt/lTqlQLh0GcHFhmTLGKI/jVGpNCIsT5TiEgApBjNaRQq/OXQwpXGFYzXkTkvyVqetvo6MXK9XRjbXl9zz0M9slV5bOzE5fz4xQMnUz3vUglzZxIl3HTqShHA4XV2vNbq/vCOoYIRhb3KzpNDRajZVygolysTAIQt/358aHhsvJ2lanGcRKcZYOQN1Ws12pVuJUVipDABWCpzCbm9fDiwECGwOGKoCOzC8sXUxDosL0UuP5QTfYMTsyeagG3F/Aw4PrcUMAjbtz9t+88myztiC46PYG3VYDgOd7+Xw+l81YlnA96/EP7NpOHga+c7uB+f1gsEiw4141NWCAe1fdEymQVPPe8bOBzf2x8nQvNL1u48LmC71g8IGjf+ebb34uipceuP9DM6XDteiNtc7G5PC4TLON9Uuqu/TIE48DGCvfxw7PVvvrVxtryxvLyzP7j+3ev2tlrZbNlYaHRwmSC2ePP/z4++M4KZdyxoAQSKUY4+wWd++uXbu+9uU/k2mcpJJRSikoIcYYAmpbIlUaBlGfXDzdjh05P9EX+ExODAH4xqnf6ybNkfxf8czfO/VH8zNHfDEbxmHeHQNQLAytdz+fteVrb35z4fw1rZSSSsq0NwgtIRzHsh1bSdludcJElovFbDbj2DalTAg7ky9GEhuNXrfV4jZnlCpl4iQRjFeKuZFCzhOEc8KEQzkv5HPZbL7VaioNz3VTpaMoOvLAYwAEBL0e+YFHx/dMz+/b+fj0yNz8jh8amXZPHt86f6m53lxqJldta3ozeKnklG/EJfVNk+bFk/918fKptSv9JEnW19aVTIWggtvV4aHh4apW6oHHDty//6dv9EThnbMz7gRB4R0MJx8o/oAXAbpAEZgmxCxtXIwDOlydnpzYXymWT599c2V9oTI2bTvkkT2fyrjZU5e/u7z2luf0PSfb6rQ3N9fa/cb+/Y/knILggi8vL2c5aXf7Kc9++tjjGogTWSwNySQa9BtT07PFcq7X6gAgBFpDSuXY7A5xOOdKUiGY1oQQow0oI2mqlCIALItTwq9d6c5v5E9u2dXq58fwCQDNxmrOnX/+7L9xmP/o7p+754M+99q/yhRMgd1fqAJo3yz33Mk3T55+6esnpFTKGOE6ANGGZDNePwg9Sl1bSEXCpA/orJ9RMgmCNJfNuL4rLCuby21t1hbWW70wnh4bKuVzcaoyUlu2lfe9aikfS9PoB2A8DIM0DsNEAQaGSHlPbzuAGSAFRgGU3aM/9tE7FLLpr732uUrhvq2NjvA7T93/89ultfV6v9tLY+raglHCbSEE8zwhOHMdNwz6UXTTZGvf4kq9A8eB6dtnypM3psD/Sdxc8Ecf2P3etZX17x7/2vue/OD0yGi18pHjZ1+dyOxAZgeA80tvbKy/TFhyZPd9MmCXFl4jXO2Yqjbrr08UZgDwbqvZSJPmIPjgRz9ULNiXr64xymEMpaQ47Bx5+CNhqPKF/PZkRikouzP0/vuf+11tjOA8MDGjNDYwWhlQrQwEHEdQyqXUUunVlUb5Gj//5olPPfOJPraIZKXCmG4Vok4vVgOb+Xc9pww72U49HMy033rj5bm9E9XC9b7OC9bsNzutnhDcSEk545bNRRJFMYzRWndjA4OM7xUynsXAHV8bMEYd26ZF5roeJSSOonq7Uz+3ND81NFZNZZrYtmPbjp/xLcuarBbBxLV6xy5VnDiSqWo0twy5ZyY0gA4gQyy+8MWXX3ql/iu//o9Lt2Ufjj1z7FcBYBfWu5deeeM5wp256Z2p7Lea/UZLC85tW0DHnOrBYNBqtfO5DGdkbfPseufqaH7mHUi2AnRxDyPjbQ1M4RK7t2l5T6hbkxNvQb6+1WQ8mZ+dGK1WGQpZ7r/n0E8uNc/F0dlM1r6yeJbpFWZ5rX7f9DhhrFIYfnTPMWpfZz/btWO0n6T58shPfuYXCsXs+loDBMKyhGUqk8SmlU6j6Xkeu/FesdsDpF9/+c9e/eZzSZwQo5RWjBJjjJTKGKMMyfiO73lSqiCWlJD15f7i2aC9klglMz92v1W2g/DK2PiRqdFH2v12zrnbCUkvrL4UDOLvvfj1bqvGvHBiZBLwgHXgzJtnL9avxZ7nQulU6W4/ZIwZldiOG0Zpt9sTDJmMM1opCMHjOIFWjuOkSmV8XzAqLCuXy2Wy2c16pxer/mDAieKMEWooocKyHUcUsv7ESKU8Mn30/oc311f6vV4Qp4898Qgg7hK1/sJXvnn2heOm1724sPj7f/hHm621hx54+K5myNrlybG5iZFp38n+yR/90dpyO41VKpVWUklJCE2VsW2rkMsybozSYbs/OX/4HdidA6r3Kr8pXo9iDVA/sIP3HvmI23CK9U6vn/dyhQJv9trUFhzlglstZ/elfD0MI06xc25+ZuhoMT9c8sozQ9PDkzs9b2I7r4Tt3zNTrIw8+dRHnnzy0Y1aL4oS23I5ZxPT1QytaiDoD/K56zONvn3Nf/W117/053+YJhExgNFaKwLCBSWAMiYMk4zvCMsKoyRNleOIrOsL4czOH/7kj34WQMkZN7Y1as/ZzLkXyQCgMu5funhusNmcmds1PlssZe8HEOOVDuSZNza6W6HS4JQmUoEQrTU1WhoQGBgDwvP5TNZzHcdK4lgpwy2Rpsp2bAqTJKnvu3v2Hep0e3EYxRpbzZZMIq21lpIQWJbtOJbnWITyysyh+X1HALOycu2Rx+ZvmV0Wvvh7v9NZevPiiRNqEDoWbbX7p67UBmF67epqZiTZNXPo+4zqn/63P4wjpZRWSnEuZJooDRDqOu7MjsndB3f04o1cLllceGvn3LZ5/l2Av8OGgHvibAMLkZIu7eEuV+X/EASZCtuLUyNDjGeprRzsvcnmv/zG/7OytpEt2LZntXtb5bybyd2XyRfR7cDOXufZp37yp+b3HHjiPR8sFrNXl9Yo5YyzXJ7mXB/AYJBUSjkAYRgLwZU2lFxn2kat8V/+8z8rVvLDY8W4n2qdEoMwjhlnjDBCqWtzrY0lrCBMpEpLhbztONrgH/5v/+Km9IznxDu/QwA8OtysLdfXN7xCJpYptRvcX/LgehhrBd2VK3VjAEOV0Umqut0+KLWEGAQxY9yxGAwhhGgNDWbbViabFZZtZOJ6nut6qUp7vUGv1x0dHfJdN4plvd2N4ogQqDQJo1BJKWwboMXxXQDGJnc8cPQ+Jgo3u/grX/vdpBkxlToWz7iWIObslfWzV2uUMcbY2VPL9z+dLdiT91yM/vjzn1+8fE5LmUqljPFcN4kjDcIIyeUzw9PF8dl8e2uwcGmV2SZhV6sVynD/9yXZCWAE2LilTbrRWxTapyIU14PI/9/B2DXb50DIAHIjrB6hceKtb8/smDu4b/+O0lPl3KPAFLAECNgAvO3tC/zhx97X7/V27BjbasZCuJxzAl0tXvdGEmMAaK1d105Sbd0SSXjhha8ce+yjn/zYxwD84i/8BDPSQCdSMUaTVNu2AJiUihAjlWKECMuOk4SJ2ywm997awG1otxuKsGOPP5XN5zN0EpBAHygI6zIlNAiDfj9igilF4lRqYxhj2hgZxRScENYZRFLDEtyxHCkl47zRDpnl2EIwxjudtiV4nCrGrfHR4SAqNBtbJy4szc+MzgixsbkxGARz+47ejHsJ921jrdk53lgISxnHCOb6ecd24jBodmMCI9OYAJQmf/ifXvz1vzt3Tz/C+voyjAEhBgbKcMG5ZSGVtm397b/778aG/aZ843svn3JzfHiGlYtDm/XexF8RCDgMXMBtkcoeI5Lw1EUeuIr/OaplcjNAE3CCRuKXAUBh8+uv/PYP//AvVsQEsHIzzGMMZHBF+BM398iw8dHiAw++b2JiZHW9TikTXGTz1He3AN7sgBJt24IQAsCA0Bs0M8Af/rd/+7f/1q9t//3SX/wxZwZaxUlq2bYxSnAupYoTads2Z8IQsq2oFYa9+95zxP2B48H/+jf/8erSsibqQ0//rEW2z6Lbz3Np8fXVKxsW51GiQEiSSEuIVKokSfM5zxKi0+koQ7VhUsms5xggGAyUVMK2KCG9blemibDtOE473S60KZaLhWxWSRklyeVrm4MgYASDIJzedahUyFEoMAIkNycz1xk99OCTU5Pj3VZLGxhDQFDOew6n61vtOE0oMVGgD7/ngYJzjzXri1/4kzgaKKW1ksbAtm1CoJUZHhv/0Y9+DIBLx+4/8ozInxsbrx5/7art8FylI75fKjaArwArwDwQAidC1A1LSsKh1x0iw+98ogb6t/hNQkADBhgAjRu7Wkowq0DB8kaAAZChyIxO7i2yUQAdXF5cX6pmpwEQUmHWKgCAADmgzj3Pv//B+/oRlNSWEI7rFoo1YDHBaLO+Xi3lklgzQpnl8lumnoXlkz/86etRsK+/9JdSSmJMHCeCMSmlY9uMM22MUIoAcSqVlO1ORwL37993t1X5fdDt9UySzu47cnfVxRNXku1EbUBr7VgikZIzagyEsCRRjucTyoLBoFKsMs57vdB1rEzWTRWiMOz1BoSCWQYEnudbnFuWnaZJLpePktSArtV7wiscPbS3FwQXzr9FKY2jqN2q79l7cGR23839PHZp+ugzU40rJzYWL4XttkXMI/vmVCqfP3nJgMhUThf23y08gCjoMsYYI5RQwoxSWggbhvziL//DW5sdnv1MD+en5uOxueg7r7z69CN3J8reipEbgrnAfhcXXcaBKpAA2TtCdreD3r5FaguYAtYB55ZPzmxcXlyCOM/ici7rloZtoJi9YYjkcSQ/ivXozdHrSZ3lZNCknHN7HKiwf/Z//ObU5OjGZo8xJoSgzPT1xQhZh43nMjmtVb226mcK22HNmyjnR6YqR66lL2dZ5fhr3728cMli1BhtAMYooYQRZqC1Ib7vNFtd1+VhLHOlwuHHD+4dfxgg38e0uRX3P/q+Rr3x6U/9jZslXaw1W+e6ycK1hbVeJ2CMB0FIjYY2wmKccRidxLFKpQaN48RxrXzWTxOZyMS2RKpkksg0TWzBfM8VQti2GBoadl0/TRPACE4J5blc3rF4nJpCpbS5vrS2erXf63BqorC3uHBu8cKJjOdkiyM3hCJecXRodr9Ogm67s7a+eeLSUq3dA6GC8wPHHq0U7kzcWF1bf+U7z9sW11qBaKONbVsZ3x+bOfLMU++/va1vA3Ypurb4RpB2eoNrI+V3ipaeAx4Cpm5YawK4tqkuZSiAUSDB7bmKt+NmQkwCdIARoAdkgAzQv8Hd+sk3jzPQcnYyX8oxfudm0sv1E+EgqmS3w2LXwo7iINR2gSb7rf/4HzXQbkeMcyGs+tbi81/92lDp0HCpzBmxbYtxx/XvuRO1nmf7zi+fTJP1yxeXt/NRkyQFkKRKcJYqZXFOKI2T1HXcMEp27Jn4+U/9Q0D8gCQDYDOawowOj75dApN1Z3POzMryytbWehQmcZo6lmCMKo1+ECgpHc40KGVMKWPZImOJJEqk0ZzT3iDyXMexLBDCLYsxEgwiUOZ6frvV9D2HMkoIqZTLjsU2N9ZOnHpraWWj0+23O91yuTIxPZvN5dI4CQa9yakxsNt6JjcyM33gwZVG4y+fe0EZbXF7bHz8Z37qr93a5hsvPPet57/0zee/rGRqWzyKI6MU54xzatneP/gH//jWHr6h3xQ87M4X0z1jRe5mPKHuXgEjvMyvO9JuugRSgGWoD3AgAZJbZiYAtRs7WbahgSXAAJkbGRnxjQbhDcWr4Hs9l/ojM/sZz6dYZxi95QooeSM3SIZ27exmLbIYDbsd17Upp1hb7Rhoo1Qcdmd2lmd37Z2eetvRl8neaeB87YU/eWPh2bNXzgN879TDj7znI4RpozUhBCCMUVtwAzDGpNZhmLiOxQXPerab+/70urer/ez5N24vuO6kDoIYxqRp4liCM+LYdncQKmkIoYwxLrjRWgjmOTZjTAPd/sAYSKnW1mubG+v9IGSMSqWVMZ7nu47FKLEsUSyW/IwnONdGFYr5kaFCGoebtcaZ85ef/eLXn3vu62vrG2Ci3++ncXxDpATB6k35PvQjn/zn/+Q3cpm867l/8xf/3q2iX9vY8vL20898KAwHMk3iJOGMa0AwCoCy26yiwdtp2QDg4YeAT1W8+2ryAnAaWL611rnHxicBjAFTgALkALU2XgQGN77vogEFJDcasxtz3irQB+qABAxQA+rAceA8sKA05VYOKMreZXHvffDbOEMFtGkq1tYqhlS8HyGMIkvYxqRh1AykfODYMfduN+QteOa9n7z1b62zSqlwmWkpDRgYTTkXnBuQgYwFJ51eLCwhtbl6rvba2e8c2/d2MPjM5jcGQfvYjg8DmwnaFsbvdvNMjt/bnb26fClNJGM0TlScSM6UZ/EYKaPEtpntZDfrTaO1kpIyIo2RqW62e1IjCiM43KWUEOK6ziCIRkdGKMHqKhsMQs/zCUwcDkCssZEh27GU0mkqU6lrW3Wl9ad+5q+PD1f//I8/98LzXxsbGx8eHskX8kG3lzMg/uj1L7o9+r5f/aXBs1/69qH914e/G+ucTSdHqpMjVQBGK6lUkia+68U8FEIQSoS4rd/92/z4F4ASYAEzlL55rX2mVMh4aEv0xfXg+j3dYwpYrOOqgB8mrBdcq2F1vDDtYw9QANjtDhcHGAE2gTVA4/o3Y4aAHJDfThkaHS10aptXF74ZqJ5fDKaH7tw/BwA4AQgv687PzxIlSNaG4PTa8qrr+IBijGhWK/mbBXsUQCLNPUe3F935tSObTwjKfD8DkO3cRmgQijhJYLTgotMPZKo4555buZVkAHIZDBergPfq4kud2BjEwJk7rr+8fAl34bULf9brdow2YZwGYSyl6Q4ibeC5ru9wx7KExYWwGGcwhlDKGLNty7HtjOvYljCU93pBrd5yHZcztvT/UvamwZZd13nY2vMZ7/zmfq/nBppNAGwSAEdBnCXKtFQU5QqtSJYTKyU5lVScVCpOXKmkUpVK2c4f/3C5pEolLtoSZVmiRFGkZEoiCRAg5hlooOd+/cb73rvzGfecH68BdAMNSlq/7r3n7HPvOXvdvdde6/u+ffNmv78bhSEhNMtz7BFjOE2SOI6SOJ1fWFpcnIsE01pORpPVtXNYzP/ir/73ly69+fTj3//xEz/Y29mZZrOtzXWo3iaLwyOf//LPfOHjN7e2nnzh+Usbg4Z4Zyx/7eoPvfcUI84Z54RizBgVjCkt/+Kp//fi/p/e7cHfA8ABGADr4TltEIbGyF/dzbcAXgN4/j16VYd24EETQJUuGItD0WvFbQ4JwPj9JdOaAE2A8LaiQnAbLq13s3+lVNlspEebk7s1H2+tbwGcofQTOLgHxWvAQkCIFlmRph3vgFDnSTnI5pZSyEv3+9/4/772y78WR+/8wzxYBOSHj/3pz//ML9x+4UYcNRoLs/G2sxYRZLW3xAaAOGPeubwsGcbjadbrtv6n/+Vf397wqfWvZ+P9+d7K0RZ84PgjAiSCRYB1gD7A2yE2XL303De+vfPLP/+/H759ffj1NJ5bv3J1Ms2ssZgwjEAIQjCqa+kBRRF3DoajiXOurFTA8CwrrEOh4IxRzniSRMba6aw02nqEwjCczaZVSbzzlJIizymB+W5TW2etj5N0Vug4CRDCtXFavj3RwHCUYW9KqQmmvbm5gIvFxSMsVG8vRb/4pa8AwNEj757RnvrBU0prsBYD5HkOgAhBBLP7Pnz+ix//VQA+KnYHg9fOHP1wCTcjOArQA5gBYAvrBLoeGGXVxmC91UrWkvMA6tp042TzwTu/pAK4BhAiWG2D2EU/3twaCLZ6bPHkBK7PwS/AXWwPYAEgAOA/IYDuLdlR3+7vjBrNd3vqZHrzYPNaHN/KY0/3Nw7623EYlbXFQRhhsJjgIGUfPP7IUnoeAJIIn//ww3fSBgEBef2Nixdee+3Oi79aw+WF1dV8lkcBRh5pa52xAJ4QHIUCeUjSiBCWFYoGt8bIEvavFU9s77zJOZTmag7/qQFHCRQaLhloAmi4xWItLu19GxDSdla9RXvUdjLY33HaEoyCIEiigBAc8CAMudVWa6MdaGOMUs7ZOBSYEAAvOAXvldR1VWRZXlWVNtaDH48nGKE4ihhnxlqtFCIMYVpoKCoJAJyxNI2dI725hYX5XiMN//m/+BeHv4SAMUYPB6NXXn3l5Zdeunbl0tVrV94fqvqO7e6VCLz3zhmnjcEYEYypCP/eV3/90Ec78dKZo198c++PNycvXc7+DOBKAT/Ysd8i8AGABQQPrjUfuaf3pQ5tA2TXhi8id3tPGYDyUIZDwiWAAqDTokutdGlwsLE7uYH8+0FOQgAPYH/yKq3ZXNnbzpMkQpo+/cT3bz/0+GN//PQzT+8Pb5E3m/P3HTkSI2KlBkoIxRgD9p34DljShz98qzB3OwHkhz/4k4Pd9dtPe3322HgwHo+2opBai5SpMWAA0NoC8gQ8oZQTwjjGmLzw6nc+9/DPA8CVvacK88zcPAmF5Dw6UJcVX5hk2cbN1z526mMzup2b51Rp2s3g+MIRIYK/95X/LnwrPznYFMPRzcFAY8IAQAgeaduIhPesispC6v3hbKmbCsGoA6UtIVQqXVUyYsQ7qC2qlVLKBJw0G512qzEcTquqisKAUEIwd84h7MEDIth6b42Nw1gIIRhtpO2qqi68+Ng3fre1cfViHAofCYKwEMyoeppnl998PUmbqydPAflJGK/xwY5z7tDVCMIEY+eg2e4AwPXhsye6DwPsACyfXfivZvB4BhcNvHx9tEeALt8q0wQADYAuA3Zz9thoLE+d/DTAegHjCIyHDMOJw9S/gNUaXg7gSAj3H2vdU4z+Q1UO51qr79LIeMsOF1j1nevQd1vMPzaZPM0IWVhsC5i+/fmP/ur3iqz+1X/0zwDeXh5ZCDHTjGaGTsYHzUZ8MNzxMPEmPbLy7vr/n377W2fP3nf69EkA+ORnf/7qb/+fF9YPzh27ddoHG/9t3fj9H5n1OOJZVmGMMYAxVilDGfWAtHWUccFF0hCWXAD4/D68knSvrtF4tyiRrwk4Rhd297d2+wfT/eG67Y/qceUHFIK50w9LFFhjrl3dOnXKPPnkj65f290ZvDm31KS4EQQRowic5wQxRinGUSiyUlljpVI8jBlCxpYYoSAOp9PSAaq1oZRSQjJVCYqms1kQcECAMcaYBAJXlQTAiCBKaSC8VhIARXFUVrXgLIxjykJmiksXLnJUB+00DKIwipcWlsIoss5xHlZlUU0mYTd6P0zioz/6c++tMdo7h8BTipz3xrgTZ48BwHLnMMm5/FbP/1QD7gdoHutcfum1b12e/fjMsU9uFd/FLllOfxpgfnrg5Axm0xsTtpHL2XyntwDJbbFXHsCDAAHALsBup40mNWfQArgAcPQ9WCMDcL2ELHpHePvgrniQIOm4emqQSxgDnQFLd669OM369zx4GCG8feM3gvBIELang5fIP/r1f+yc/P73vrW7uf/wJz9F7xwyrYOdrZ25hSOtZgIAS3NzTz771CsvPPq5z76D06dAnn7q5YRRJWWtrDEGE0Ix8oCs84AwoaKRxvPLyflH5nBcXVz/0ygqt/pyNrKcsV4rmmXmbOfn0nb34usvPPn0ayKJpT4QQdxbXPvhY09s3LhRqmGjG7345OtFfvCVr/7S2tHlYmg21/fbjcQ7QwlFztd1VVTSOIcQCArGQRJHUmlAwAjJ84pSTBAghI21ZVVjMJEIKONaK60NJYCcK8rSOytCAd5jTCgldSWt94wwbQyjTCoZBaHzMNdr97rz8/PLC/NLjXbv6NETjWY7iuI0SYMgoGHyPpqd8Lu/89tgnVLKe++do5SGQmBKPvHFpcXOhyabF6Nm705YTAAAArpHFz45rLf2+y8fHGwhjGq83uCNvcEWOKqJ9MwkYZLSUEB6m5JoCdADwAANgAkKGXgwpI7xEoB8D7AWAyh2G3ZNwQ1yt2Xs6qnj1y6+bBTx3m3cuGTyHUqNSMJT55Y4jA7BnuA2ALnp5DIHqRUl/+v/9n9dufzy+vpz953/+OkTJwCgrCtGb4X/GMGJE8cPnezQVo4/8MSj3xSNIyfW3g5vw+eefNrrkiJX1KaqFaMEE+wBrPXgkfYgODt59ujJc8ezXE4n5WyqyilwThFgbV2V4YNse2vjallnD33ip7/wvGQk6AAAIABJREFU8X/QPj68f+2LsTgTrr7y3GM3pmN548pmqYZH722evnfx2s3Ll1/YrgrFGQkYLQ+mdVEajGZ5dcjhZoy1mkktdVHJIKAB4wggSRKCiUdECEEwth6iKGylsbfeGDPX7Uits7yklDB6S8zGeVsWpXNeKu2cLYoyDISxTip975kzve58p9Nrd7qc8SRJW522s84jHwUhDqL38bPX//w7T4B3VV2BB0IJJRhjFKfJ53/xAQTbz3z3ueYKjcLFu6Kuu8nqXOeerOp3FhAiqrL9bqulHFpb7RwJTqf0aAifBFgDIAA9AAbQALj+lj9JDmcaole5vQhzgLumJO6oW9zVyQCAIbE3e4MDD4SopONBOs1nH3rwKxzmFOyWcFnASjbcGvQHFy/eqHM1Hk1xXec725ce+vzRBz92q3Dm3U+KZO85uiCC5E+/+W/e0iLc3CqeODjYrWt1WEjmlBrnKGWEUkowISDrStWVLlFAu1GUE4wZxo2GiIKwKuu9XTOdlONhsbB45My55fNnTgPAEvk0wDLA7kF/ai0EhGtbrZ6ae+Qzn9kbbx1fOe8MwwiMVLquUUhZHJS1YpyGQWCd94h4D0Eg0jgA7733nGCCABEcCRqHIknCuU776PI8waTTbSZxTCitKo0wxgiDd0kUcE4442EYdJJmQDH2EIchARSHgaxlqz3faneSOE2SRhiGgAABane7gQidM2Druz69m7ux1nqaZdY4QEAwxghZ585//NNd+PkQPn8zG/c6H/nJkfjZY19eEB/uCNQV800RR201KHY3p9fxO1TF2ye7E2+9ONS+a/fo5/82PJS728rJJZEQQ43n4cEkHwwPLx5x+KgDCVCw0E3HI+rDne1Rvz8gn/vsJ9c3Xn7oY59em7+FJ6GUo7v8l94xTfCFV56coBsPnCkVvPj8pZeuvTzsNhKj1WRWT/ISAYiQe4+sNQBolmUIeWyVwf2lU3hxblFKV6tKcCNNNT5AJ4898pGTf7+XnJnCdcmGTfwBgH2ANgD5vf/wB9mwxphYZ37my58/3vm5pcbD3QQ/8aNnJ9M8JESXJQ85RhgRIjgPQuG8xQQLxgAcRuCcRc5Tgq2zDKFGzOJQgPfdTosx6p1R2lCCRBAWZekdcIabSRzFIaW80UgZ49LYXq/rrDPWMn6YrKnvPXNPp9MJgiBNY0IYF5xiggUnGDPOwXugd0mXf+N3v36wt1VLBQAEA0KIEIwQ/ge//puCRgBw/MS57/7wdz5w+sH3tr3TmhS6GJr79Z7xB5RJp/l4YtvJsfdrcCBfjOnbPqf+5pSWuxqPy7yacrbY39xCcvYzv/BpQG8vUloAXcpJlQ/muu2qLhGx+NrlV6aTKmbvzMr47k72HMDLh6/+zmc/11wgmdx7efRUBShMlVSSYgBAnALByMMhOx1hjBmlxpiyLGezbPdqhbLzC/BL9yx/bL53SurEeQZY3TP/EQDIYffG9RuzbF/Dc49e+n2AjZdu/vHujYmScjAcJGl49sjfBQCA6e9843e00oxSQI4xapTSzhFnw5CHgUiTOI0C6w+ldzyj7BA8AoARQtp65MEjRCnd2tojlDEmOOd1XUulkzSea6ecYqkMACqKKk1jggFh3Gw1D2mhQDBCOC8KjDFnDCHMBT+s5IJDRAjAGMRd0Yj761ff0No47yhGCGHwDnnPo1YjuJUI7XR6g/Xhna1usb1LePzOz+cB3HzwpbX4vznCP3W0dY9gdyROL119Yn3r+XF+mOUeRO8C/oEHyACu3rWz/zrbq2GLxlDrWUxhrtcDdHuFfg7gBsBcs7PMI3zy3NJHPnWODoejk8c/dOTI+8FF3raHAL4P8CjAg9vw7fs/2cYBzCa+L+rtG5bjYLM/ns0KpY2znhFkrMGIHKrUIjgU3WBBHGTZjf3WcFZN0vh0r70WgXlCPvrDC3/wqXM/tzV56cHzD9dmd718pixm14vH94dv5vlEVy4I6MqJWz33xPPfn+5KRmkgOEK+rutQUEuw8x55V1UleIQpVUqFgoZUMMYEE9Np5rz3iBjjs7wsi7KuFICvpWm1UqUNBY8BGPbaOEqAcMYY9c7WtSQEY4RqY8Ig8N5JJZ2zs9msKPJAcGtNEIaMB0AJeA+YAr47GuWbf/xtpaSxFhxgCoQgDAhh9IH77sBftOM7mPrP/vn3Hv7Sfw4A+6PK6G+dWnjkNir/2xHORwFeRt7sTf5yofW5Z55//Pf+/e8aYynBnV73vvvOrB5rP3j+y7dd9TB2TN9HLvmvsRlcVlDwEDVSduS+cyHl4G8AGsE7C9XjANDsffDQj73SVFt83/0P8b8RfoICXJ7CUy1gCyvBaDTRpuz39/LZzFo/mZa1lN57fNgtgDBGAMR7QBhzzpxHPKEG6t3B1d1dNRnu3nvmaNKUoJJRPn7qze+dP/tQCmef3vy6gb7Hw/7g2WZrLowj7NXaqd7xc02AywOYZgcZJSQKQ/CeWCM9dg7CANM4mpa1NZYKgTBCAFo7RoESnCSpVmY0HLEk9oCTOBCBmJYyDkLrXVlUQRwJxpIk9NZY8AQzWVfe2WajQSnhlClrMUZhEI/H4ygKBKNZNqvruqrrOI6994AxMAbagHdwSMN/j128uKGVNsYC8uDBOccZxZj+yi//F2+fUw8e46Z89aW/OHH2XBKsrL/++mhv9PJTf7D68IoHZ/30Tg92Ev5MwEcAFgDcYDCO0uFu/7d+5+tPrV/fs85hzPhGf7A/PnJkMUnX7j31kff+qr+tadiqoTLGYerTJsElyfN665Wr933oLqQbgCZAVVZjyjBaO3YHLMkaS+gdwIERXJDw5hIAgG1CCNBZWN3mUYIA1fVQyjwvZBoL54z1QIkzzllrEMbOQxBEQhStRsRDsbg6tz8cUpg/c/ykWkL9/d28sNpQjNx851hl0PX+9/Z3DzBzlC/0OktW4rRNvTJHzyzFaQrAe/DQl7740L969Z9Np9M0DPKiuCUf71EQBIV2THAApLUGByIUCIEzzlodhQK3G5U2YRQiDEWhGaNBEBRV7QGLCDMuFhYWZ6OB0gpjyglIYyaTDAC1W0nImTV2OBxxxpRRvW5HG6OU1toYY1Rdc84xZ2A1GICoAVC/NwDqb95QWoH3lOLDbAshhIs7qje8cgFymOEkWAGA3WtvOm1G2xv22ugjZ37jPb14SkAGcMHAG+vXh04iNmerwWyukXbOBt6Y3JZjmWf1cHMLvv2Hf6J/Ye++sz/7NwdlvdccTDXoqq4ceIccZqiS5cb61gM/9bW7rq/Xr76ytLQiraPHT97b7twxUL8LnQIAHTj3w1dfmqyOz7abezB0IMejgpHEk9l4W1U5Q0hJbQBRQgC8rQtNGRUIRXHQ7nRG04xQKgQhTBJeEb/sFM7zopG00zA6udSMk+Dy+rWqXzhnCIVZNo7C9kJ6fkry9soz1shObxWj+JBecePmVlmUUSACQQsEAA5jFESB8Q4BTKeFEJQShjEhGBGMGadKKcGDg9FEa0OoxBEPQqG0LWuJaZTNZs6ZOFqhBBljOKXOOe29klrqUnDWajXqoiCMzfV6k9mUEBKF3Ho/nWWNRkOpGiFACKWBAAClJBc1EPT2hocA8M//5f+xu7WhjSIYI0DeO4SQtQ4JfPrsHYLcePlszF5bXD0NavTi9x/NDnYo8u3O6vkz7yf/dr6wL8fkQ6dO5D947P8paXntYvnA6VN1XQUxoS3TLzY2+4PR9ujGunrxueX7zmIAfTde4N/I+tmGhnGuJlxQa82kGA37qq6lUvqufhbxcHt3S5WOnr7nQ/Gdlf67LjY/c/+vALzx7MG/mYwkwaHMm0U2c97Ocu0s1sZ6QAiDNsY565z1zk/zssuoNZZzQgg5c9+Z1nw0HEAaieF0M8urqpxVdfZTH//lBpw4dSxtwVkAeJX8+50+5Jm/sdUfTTd7C8v1LF9Y7J1bfOjwTn784+9prbVyWlaUc4wxD4SUUla6UoYS0GVtsOFhJDhXWk4zI7g+FAeNOPfgOOdWasYQAGIiBLBhwKyWCOMoDGbTsceMUQKAOcNaKakMJeT6+uby4nxVyk63Bd7Nsmo8Hi8sdOuq5lyUZZGoFCGspORBACQCUwJlhz1aTkdGVdZZq41zjjEG4CkhCOFPf+HLdzxosnji5P1GzirqdzeuKVVjRHsrd8113bKYHMrV4o999GvDwasH8nUG6OUrN3pHk7WltNPhqBWwoN66ON7a3QKA25xs/LfRQAAAmEtXN8b7RhuENWCwvqKMWu8vvvb0/E9/5r3nzy8fw4PtzcEOPnn6rH7/fc0O7FNwq4a19drku/vbkE1QNgpNyatKK2MbjU4YMUwIowQh4IwIzpI4OlR3EkIYZwkmIhAf/NAHGs01QDwryjguOz3PSDMIGknoALqHTnbx4LH1rTcd2Fk+ffa5H/V39r0WoJtlQTTww8z47tY18EC8lVKV0iptpLKYYMaoc1YrZbQRgUhiIQRjlIP3HqAoCsYYY7xWxjsXRREClMYRcioMRK/TBoS8c0Ece48IxsbYWZYRhCmlUirKWBSI4XimjMWYIoSKWTaZTvM8K6vKOWesNUo7rZyzs+kUIATv30YRtttt66w/xOcBAnDgHedMiKDXfvfTX1haDCwJ45gLEQRBp9ud676f4JADgMoeSn5uR0EU2Y6XLubiV77ydz92/oNhGrI4SJpJZ0H01mB37+Zzrz12W/O/FVUDAICBlebAON1qHqMsBKx4hDEB0NO7nj+bDqNG5IWkcwstWRkW371I8vLr3wf3wzNnHtwbXdnuXwcv6oIlwTzQLE7TvCyJW9bysjPWYLDaYoI8gDaHAr4YISRrxTlL42D95vWoJpPxTlX70UTPde556IFPru++eOHGUx873gY4A3B14+Zj4/GYMaiqimA/Hqi9jVmz0fzEfb8AABJ+8MKVN8ejfQ4ECDLGUIqtdUZriQGw5ZxpJUkglDGBtcNxgREl2DvrKGVZUcZhKJUpa+UqZZxvAATM80BYawiG8WgaxRFmwoMH8IxSJhjz2FmrlGGEIEDee6N1EARJzJWqZ7M8iRvOee+dMRoIJhgPx+PGfAGsB+U2RAEA+fLP/tzFixeMNRghSglBiBBMKe10W1H4buoXO37vYd2xqksRBM777WtXjggl0jv0pDzcKEEJWAvJme3dHy8uHSvz3WeeeAo7Wns8ngxwC6VB0yBLCCQtWFyjrXbMg9uDs3dtcTL5a0nIN+UzlirkYZrvSZ0Zq2kYdpaFc+qu55dVFVLeiBqUYDD+7gPapd0fICSardaFN58q5bisKu8QsnHlZ4Q5SpuC0oODrcGWbDeb49GoqmrKGUJonBVJGAnBvHNSG0owoXhnc4sUUw9qaeGkcWrtWI8Hbn9802j+HHrU+kfn5xa6c0en5V6n0+u1Wwst9OPHnxtuF/4tmdUD//psOAs499ZrrTBC1irnXC01Qt443+zNKa0YZWUhs6IOGQLsvQNCMCGIEVSWkhJCGTPWEO8ImEpbyn1RVlHAwZu6qgD5qlRhFASYTCejo2trDiggj5DHgKy1CGNvifHeWS2l0UbbQ3EXBIAwZRwjv3nl8uqZ8xB1INuC9OjpDz48P7+ws73lAMA7hGnABed89ejaqHyuE3UB2gD2DmEznW31d3ggltZOn/zoFwDcJP9BK/ns28cRHH97OArbS88/81gcMqOBEDSZDOvC26F1TVtHWiQi5KlYFqForZx8P30QqOESgA1g/v3oKpdm3/QYcdEgNLC+Nrq04BEvRI/ns/Fdm3CWyDLfGe7QfJa323d34aee/05vfs7aTARRaXY4R+CTbnOpqhzy1DktZ1pmdZX7gPEoCpUyURgY5zsNpI0lGGvrGKNVJUtbYwq+aMStpBUtlXV58cLN/W519sxDyvR7zRPDyXgyu7m51beSFTNtbR0sNBtps8rGMzR+/eY3Cpfroih3gkbEtfISeSVdXdcIMcapxwycmU4zjDAGTwjGGAkRYILyqpbaWO0oJc77JBRCMC+9YKwqa+mACJ/NpsinhNK6rgkhIoy63c5sMuKMlmXWbPUmeR4EgTKurussy1utJiCc51leFNZY66z3gBByziFMGmlzfePGaj2CoANxAnYApPeBs+d2d7bAeY8QJZgyFsfRV37pH9/1yU/za3/yb/9tlk30yP36//x/AwAAbiVnrxx8/fTcrwHAm3tPnl14B5ncCU7M8u+N9t3Gbj8JA+SUlE6PlRkYMSdaR2IriGMkbXLlJu+33Azgwf3Zy6gx936FAs6jWdWPk3YrWmGA+riuqxnWxhqC3d0v6jwGE/hSYKUkAnjviHZj71VGU2vdcHBdSSAEPDjk5d7eUFWIEZokTJoxox6BV8pYDwBQK+Wd9c5KKRFCWhuttXOuyGqB2qMdq3LZbqQirlqtdsR6x5J7pWm88PqTVW12d0bD8S4Lgv2DXJbZte1th1uYYOTd7u6GLOrnftB/4dkLdVUiq6qqLquaEOqcdx61Wmm321HKeg/eY8YYIXiaFeOstMYQhATHznmCkTHGak0Q4oJhzuI4MkYThOuqCKIIMHIeOq0mpdyBR1RMCzXLirIsR9OMYNTtdLI8995VUvcPBgcH+1mea60dAAJkHSBATIhm2rxx9RIAAO6CLAFg7cgqwggQYIQF53EUtrvvK3hx5YVHR4NBXtWN5dvnyqUTc7dwsLc72aF95jP/kDAyGO1fvXFtd//gYDg6GE+KcV33y/JAj8bSWnFy5bPL9DCFpnerx2tYv/Madr7xEfH+FO4sm0yzobNegGAAzaSRBA0v6XRf24yqu02KUSNhnKdRF9+4ca2qHHqPO17deA6T4OBgxzrR39031ZxXvbKaZdNhaS6NqzeVG0URmZtfZCw8jIIJIUoZJbVHgBGmlBJCGKHaGF07JaU2tSaDjd0buva1yncH10d+cF/vq2FKrly5CjbFuElw3Gw2tLNK11WZE4wZIaoSb7ww3NrefOhznWaKVJXJWlZlFQgqOGOcFKUijKWNOApDB6C1qeuKC8YIJpRFQUC5KEpV1rIqq2leWQBtoJa6qEoEznrwgLVxhAnOhQgDKRUAFUGojKmlVNpI5ZwxBKFOu8E5p4RIpau6zrK8KAoAAIS9dxhjjFC3N8e5uLV5ebQGs2udVooRRR4wIYxRxkVv4dj79eiNKxt1JTHB80snb/+c3IYY29zZU7cBHigOxxNflLIo8sFgOBxPyrI0Rhfj6Q8fe/Hm+igbeiMBAAHckNBnJD2Y3rzzazkAZLC7X+xUd+OeFaWeTfLRKBuZ8QwmFFKwwhUBKsR0UF985bn3NrnZXx9N9ytT0m//0X9EwD/2sQ/dfjjX442dV6ezKaUyjFa03yllY3IwwyThhFpjstlsOqxajUgpcMZrrRppNBhNvPNBEtS1ZowYYwV4jMEaP3+82TrC48Vlz+XOwSVvMEIxxejahq2X9wa7xWg4OXFyJQpoPqtWV1f7/UuNJp0GFAAoYU/+1UuDweDDn5774hfO/9noymzWJ7KSunSeeLDGuMLVxnkHwDkPhMjzCsA1GlRQ5jwEAbcOBYLnlQRwMQJOGaPYM1oUldPGIlpJjYh0zlhjlZSYUO99lKYdj1SdKWWXlhYEZ5PROE2juiqN0UZrrbV1rpY69QAIrLUAnlJKKI+isNjvx/MnAQAaJ0+sug898MALL71ECWaMiyD4wt/52ns75tAGB1NjtOBivPnSX34TLc83kyTFcUPTcH1jtxEFsqxYEG7evOatP77Q3djduXTtxvbmTl1WjZB77wPOkziIApHVxdLSfW0qQKr9zfXjrXsAjgsAwfH16TZA9S4CS1b0b9y4rAp7ZPWBE8vnbkulquW5DxelGo+mGNIowqute4aydEpSIBiZ0c5lOP/Qu25kY+NqIlgFJf38F39ube3Yuw6/9MZ3ajWgRHQ6bcz2GgGW1YwL5J1vNRcLmTtVW6/ZUjYcuior0iRiBDBhQiDvEWcYixBhJKXCmGCClhbbH/1o8+YmXLx+tSqcVoSH/cCu7PVnVb3FuRFRNR35cobzyZbVKg6iqy8Wgz2NEcYYg8GtXrp2shPBcRKMarvPRZim2qgaMWGMJRQNJhlBuN3GjFJKiXMeIXDOS3O4o5nngocewJqAEWuN0Qoj3EjjfDYTUZDn0mezKInDKMLg6yr3AOPhgFGKMY4CzglwijFGUkpMqBBBu9MjlGJMqroGhLzzSkpKGaOURQJ4AOU7euyi13vkE5968ZWXCKEIIYTI+5EXJ9MbxhjnAGNf1+W1iy/LYavZTAkP8mCRMaors93fbyZpb3GRRTwII4dpUcp7T92TeBky7ayjhAQxd4wY0zqydPZzn/1pl7wqs+xt5tJefZVz/l6WVBq3zn/wkdcvPdU/eNN5C873lha7dMECNKL5teUHLl1/fHvnahTxo63zmCaY1iygwjlq7jJxYhcdTDYxN/Rzn//su455cP3Jy865JG0wjrNyv5hpBASjxFrrnLPaGJO1201kV0Jmo2jmlFHeKynDKGCMISCcsayQHpyxnnOW53VZ8dOn1l678goiopE0gMhiuL+/7cvCyApVUmA7newV3TByara+Ob32iqSEEgQE4aQdp4vtteXzAB85c0/68pNvCsGs5oQ4qfQhFENrTQV31mkw1hjKcVnUnFMEqCgL8KAcMEY0+KJUzSASgVBSE0KCINBGh6HQRT7u76Tdeey91how1UpVeRknIedob2/v6NFjS8vLB/t7QvD5Xm9rd4+LgDFWVRUAIIQBobIsAhGwVhsgiJvN2/Zlaq+tLrUabWMUfk+56XZrNY8THlk3sc4iqRipphlRWgWBKKhtdLq8prouro0mIk7SRuva3ujc6VNri0vWoV4rvHbhuU43Ns5aDjhtG2W2tl9549rR++57KIrLLN9Mk1WAiwvBeQjusvZM4TgArKwsZ4WSajAc9vvTK2vL90ZhayE8ooKql57aHlzIi7J0FWWJdJuEYR4xO0NlDdGdtxWI+dF000mH5XsSH48//sP93f0wpGkzIJRGYlWwjjVQloWshus3XxqPbjJCOq1jp45+YjYpsyxH4Lz1lBFjjDFOG3uYuSWUKG2iUPR63XuWPrMQHml14yCcY3ECaK6z3JPGbN3c3t8/qAs72S8mB9Vrr42mk2h3043HkzyfYfDWu/Hw4P7znzt35GsAwcqxBkKIcWYckvpQCVErZQgCKaXRyhiDCMaApVLOOGm0dT4KuDFGMNJqNpVzzvmqrItaiSCIklhJRQgOwtBrSTHOqyqfzfLZxHuIolgpF0dxkiR1lWdZFoUi4ixOokbaVkpZZ4113juECGOsyHNtDEAA4ABDPdx9pwtbzZMnTmCEECaU/iRBrv/6n/7L+z/xZSCBdU4bPcnz0XTWPxju7W5euX7zuYsXb25uSVkt9uaWuy1GiQiiMG2Usk56KyTqShTT1lzQXU0XVheXjp07/4l2E5fTLM+7aXKYOrkXQABEt+1O/I5N4QkLA8prwrXxUwQeEeSxAQCH/MrSve14xSmyceNNUJFSvlK6yFxe5i8+/efvuhTGTClpKqDsPaP3jx79S9LTy815rQjnOOBiYEZxkBQmJ7TJQzq3GC4uN5FvX7j0jLXaGZd206quCMZKG+clpdQ6QBgRQj3CRZZv7+5fnjzXaXVPHL3v2WdeGw6rRho78AbVtSmPr55ptpt7u292uo08WyaefPQRlj+w9sqPr3vrMaJlqfY3RvAAAAxeu/hX4JxS2oNzDiglxDntrXNOGSCUAsIAgAhG7q18AwDCiGCcl2pluWetqWXNCOYUWXdLPtxYxxkXQWRUFcYp9RZVpapLgglCKE2iZjOta5llOQZPMer2Fs6fT1+78PpsliGAsiyrunLWVXWdNtFhMg14rNTonX+4mD9x7PjlK5eMtYzeZRvo2+2rX/vaV792K4Db2ph89w9/e3froiOcJ26S1QxDo9VKkkDpqiyr67uDD5w60U3SQZbVw+1k8USj25oWebfBg1AUXvc66WRc1Xl24eLeuXsP0Y4eoASQ71Gbl004XuA3ZnKESdBotooyoxQNJheKaMN5goB7cMSLhB1Z633k8iuvgC+AYhqJungXcg5Gww0MhGJE34VqXF9fv3Ht2rFESJllxTAUURy20qCHvNSctTup09DtwfyRha3r0uqx11XAeRTHw/HMOIcRuoWIQR4fsogo81bnM5lPkFSjvf0DrcdKepekSu4vr/Bz98cpX5hOs/vPnbIsu/jGzKrYieDoPa1BP9+9NvLer51ZWj5ePvvGNx/+wN//qQ/9+l/87jNeWQzIYyoYBmNC7kvFHFjGqDEOY0yRV96PZwWjGCdxVesw5HleVXWNEPLeWuswZVJpRnEQBkEUA0LYz2lZcUZlDYRHDrxzKElCWSvKqfXAuVBazWYzTPlwOivyrEwSzsjW1maaJoIxQMCDt5G0ERfRbVOnX15eIoRwypx7/2Lfe+zIWus3/od/CgC//Vu/dePKy0qBwjgJxXA61dqdO7GKeSDrCoOfZuXysdPHzt4PALksEwGZHoeMV6oEhI+vLY4OxkXh4xgBMIBdAFdBP7zDz/TY9aUslCy1mknjwPOb268mSeBAe6yLapIk7Yi1j6x8kANwFtV1Bcgj4gQheaGT+J2hazY5sM5LW787n/Fn3/ljWdfZ2Cfi6GL3tKplNtO1ImHcjpNuyLHRpVQgqE2b7oPnegxJSqhWKisKijFljDFGKamrGhAgRAAAEMlmk1dfffyNN549OLhIEI5CBlAszAtwJPCNvf2NyXisdLvdOXX0xFLS9nk+nYynrVan21mYm</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8d7Bk2X0e9p1w8+3bufvlNG9y2pnZ2V1swmKRFgQDSMJMCiZB2SJNWa6SqkzLdrkslyW6aFGmJVIqUiZZokSJBAlBAkESIDYBC27A7M7M7uT03pt5ud/r3H3jCf7j7YSdnYVAWX+59vun+9577rnn/s7Xv/NLp4EP8SE+xIf4EB/iQ3yID/EhPsSH+BAf4kN8iA/xIT7Eh/gQH+JD/P8d5JnnDvR7qe0GMzP7i6XpdudyUHBl6lDlaGUsr51zaL7T7bS3Nwmh9ZHRJE0r1ZFuty2lVFK5rkuIUlqLLBNCAMS27CgeaiXTJJuamb98480gR6VOh2GipTYtL8lizykK1ZKZMgwmhBqdLLlWodMKW90tk9uWYbf6m4wyIVNAVypFz6s2msvJMDNNZlgsHhBCdWcjCfspY0wqRQiVSkPDsrmSYIwySpMsgyYEIERblpmmWZIpzmCaJqNUSEmgOedCCNf1gkKeMy6V0kqHg14qhGNbhLJwOGSMppmUUpimOTZbT2Q2GKy4bp5oszZSGMQbI6P7PKuyfOvy5uaqEpwaqeMEleKolCwSGzmvPD83s7G9emtxbf/+6bHanKbi1Jvv/PW/8stPPfFYp41z51781hu/UwhmlE42VsNbNy+v37oVR4nUMiibjAvDMrTUg6ayc/yZj32uOhbumd01yJjNR64vvr650Z2aOf5zP/vf2u+d2ncuN1/61u+Gon3y8KeXl89+7YWvRINB0SxLPnz66f/q+557bn17oV49NDVivn3hxu/8m79PSOf6lVXuZiO12rDnG0xX6xOuZWrtuU7tW9/6SrE2/1d/4u/+01/7X7aW37JNqxV1FYHNc5lKlFK2yw0WSB1WiuWx4ni17nd69G/+3K8uLJz/9X/6i+Tf/Mk/nJh4Iha9Tx7//vfTsBH2GsubK0sLyzdvDAfdUrU+ObVrbve+xYXrWSqEyCYnJ6SKRCZ7vU4cC8e2GMVg0BGpMAz78PFHv/r8r/muUtagsbFFKAnybm/Q9b2akr0sUdxAkPf2HS+4ZF+j0V/bvmQQ1xJjN9bOcCcJ+0PX5TPz49Qora/etJgVRdHY+PjS9eagM1i7JBrLfcumMoMAzVJJGPUdW0E5tsMJGUax1gBACALfjeKsO0gD3yqUApEKIVKD0XyQE1LYjrtn7z7LcZrbrUyIQWe72+2VyhXHddaWb7muG6VZv9+3bXv+0SBBz7B7nLthj+47uMvwGuNjTyIuvXPuFQYv7KVrzYvf/9xPTJfmbmxfX2+cy+drx8a/AOCLX/sfHn3q2LT3eYCdvvn7x6d/4h5JLwLjgAngqy/99uXzpzaXh5xzv6YJS4tljyiju5kIUfiffvEf/afqlNbi4OuFbF+xyIHDD2rwlQjSwQTAgckeLgZ4GugBwb2NMuCFr//R2vLri90Vy87lg3q7uxzGYmR0rFaeGoTb4xPBMw897ZkzQPXOXey5H330h5/5wq7RPff2tZn2ObM44BnWVrNpGoZj28Owc2tx6VOf+ZEwDDOZMUJd1x0fH9NEM8bTLCPQIyOjw37TDwppHB08eOzKtYsbzdNpInI5rzJWGpuwx2cDTrXJST7Ij04GpTo0USPjgWPuMh3XdDOT5jLVNR3Z63XjKM7n/TiNK9XS5MTs0aP74khWK7V2t9tr99O2kcbCYFRTphVAiG1Z3OCmaRZzHpSg3DBNk1JmmKYQihsWIXpkpBrHied6IKCEmAYrlyue71VrVdu2KSWUgjEm0lRqlMsllSaW45SKxThJLdOcPOBKERYLoxO7SoWKgNHXWR7S7HaGRw49+tDUjx6cf3Ktcb476G4Pt45N/fhM9cnR4BgAoDcxT65cXiCO7obRvpFn7pH3qwDauGxikoJeXnqrn17TwpqsTw3THtGMGkRETA6sv/2L/5dJ/lNpBqdoHnacUaAOvAV07uUBAGBgYA+wH4gkVtaz1SJzAAL49zZiwOT8gXPXTvfDhl/ghbxLqTAtzlmWZmGQ82LZt9yslitrhASFnbuoVG72vhHVzZwNXNs+12gPfN8vFkszs/OeH5x87BOW67XbTQpGCAnygSZaK5okqciyICgAYNwihALM9fPP/+m/77a6pp9W6qOPP/Hk2FhVRJaSTqHCuSVPHHmuXN7LuHcw99fL3kwYp3umfyjTSS/cVioOArdQ5YYrtOIqAaHhW29eGwySpaXNRw7/+OT0CKFaCCWVNg2DMsoosxyLUUYJVVozbgqppEKaCdMwuMGFzDing36UpEJKCa25wSUomFkq15I4TtOEcxL4rus4hVJRK5ElCeMGZUxr1GvVUiFnUj9f8iXdVjInk4JM/F5Tb2yuzk09XKUnNdYuN1+Ymz+cika7vXlHnh0sD3HRBR458tRU8ORUce975V3WyIqoMvCNZHm7ezFJhWkZjFHH4UHJYKawA+rm8h79TybZfdgFpMC37zlzCzgBhD38ETDHMMpkFagDZorTdxr1kS4Pty4svDk9e7RUmlQi60ddy7CIMJIhiwbSoNIk+csXtr/16imC6Ts3sj/+4gvsPSNoAQ6ACCtc1cJBTCmVUvQHnZWbS89+4rlWpxtHodZaK1WpVeM4FFnW7w+0EGPjUzeuns8ViuEgDPz81vb2N1/60syeer5OFR+MT6S9Dum24mazmys4uaA6X91D/MTO0YhLg9avLV4Z9Jut1s1Br09glwvVQrHsB9XHH/rcsYnPnr72tenxE5PTY0xOpjJ0g0Rl/urCugZ1bFNJCUp912KMKqGiOAnDKIoFpSzLhGEwISWjzLK4bRqWbUVhbBos57u1SjkXBIZhKiWWb94EYdVaHQScEkqJ79iEQiqEUWwYnBHZTzoxWSuWaisrC4NebNGyFipLo9XG+Y3h6ZTxcjB6+tKXC4VyzvdCskkc00VxtXWj7kwxJMv9W0Xr4PtmvUIwFmOdw26r86dePnvj7SGU4bleEqo4JJSTUs0rFcf27370PxPPtgAGjALf6eJ1GwawCwCQi3HDxghg5XhCkTSwacLmtzXf2etfOvXWH68vbwEmo2pze0VraZs251Zv0GWGlSaylq8/vPvY3PgB0ynfeR6/7/lXGjdsrpbXTh3cP03pCKGpEBm03N7e2LX7gOfl3jl3lnHLthzLsjhnzXZbZVpmaaU6qrUCYYSyOIrmZvf8wR/8a2baJ058f0KvDoeNd84tqwRac05Vr6mPfHSihyu97Nxg4LbWt+J0ueiPxGnbtQKjYCcyDGVoKG+iemDS/zSA0ZHRidFdnWRpfCKfyqHtTY/V3de/fhaUKqWU1r5jpnFMiabUBCAAxrhhcK3hu0avnylFCOGm7TiOWQh8Ah1HYSokSxLHsdNM5vO5fD5PmZHLBUkUxVFs206tPtrY2MgFQbPZ8kwWDyUxjfbWgFNL03S7eXO88lCrtTFMu/3BxsjIDOFV22FJttFpZ4uLC9Xy+vGHH7b9sIdhgMdmc3ng3wE/8v6ZP7t0fW6SDrpKJp7Bho7pSKF1xgg1uLAp4bsPz/xnIhmASQBAF9gCNoDLwD4AgJnH5wAAFy5snTpSfbwGa8dqBPCNC7+URZbQ0fL6Gbp50fdKjJrQJBapqWm1NvPZT/zw+etf11FMXcXN91CLVfbg+ury4fmjO8eSjo8Hbj81Rgq7+92BZXKDM0Jwc/H6sRNP9Yfhys1Fw7AY49VaRWmxtHBje7NhmWx+94GFxauWZaRJpqU0bO+Pfv83vFzpc5//+dXVm+AD0SdZaFq5lHLBpZ+qJMw2GEW9dLJSOVzIFyxm7Jv6yIGxH9g7/XRje2WzuTro97vxraXGK3MT5ZXtpYuXTodRO1/Mz+fqBrVH3RMvvPQtgxmWbWdJSgkoFGUUoCYnlJmGaSolpdSmwU3OJCAFKrVivVazbbNUymsltUY4HHDDcF27WCprwrQUcRxrjX63A41iqejlcoblNBrbjm3BkMzSQseMEtOwSsW6VlGjuS4TqiQvVKNOr1Et7hkMu8NhDJqNjIy7pa2tLdFonx/PP6wQruCNPGpAEdgArgBjO5J3CrxKD1S9Xa985898I5cPcgbnaZZxZhjcijrs4x8/adxu/F2hgRUg/z20vAikNmzAAIZAATB2LoT4RqKCkrUPSIB3bfeVzulmZymOsnYzJVBSRoybec8g0LVScc/+pw5NPj41Hm71thyXhFFUyO26y7Pv//yTuaJ5cOaRnWPfAADJMwNes7VumSYl6Habg346Pbvr1W+/SBn3/TwhulwuDoe9W4u3ouFwZte8yJLFhevTs3PRMCqXK2dOn7p2+XSa9lLr7cFgc7vVMQ3Pcb1YxmPVvZbjG8Qulyf25B4OiMvJNccodtIl204SyJXNjaXV1wnVnU5EyECnsjNcbbdbcZidfLQ8ZVjAIQO7gOrLL/2JyoSUSmswziyDc8610iJJQLnvOVkmk0xxRgzOhVQAUVLblplG4Xaz6bmeHwQaYJRFcWjb1vp6w/V8Slm/32k2267rp2kqpAqHw62t7enpCWoq5YZpnKWp1BqKyEMHn37q+A9ZPLe8vNzvCC9ffHjyR5Qdzc8ebjZbqYwba/EgvNntryh78/rmawcL9W1c8TAHhH283sLFHAhQd1Feis4XjNrXvvbnBc/R0IwQISShJEsVM+gTjxx/n+X+QJDvjWQARoEh4AFbwCrQub16wkBSsizgALAKjOycrJbrN1bODrqKwknikBrKdwOJ2LQMyuxCzp6qz3Kws+eu97qEWWMj5am7PPvff+l3MhnNjO+jwNmFayPFMoCc4Q2iDCq1LZsScuH8mf0HT4bx8OVv/FkUhtXaaJBzLddJ07SQL4+MjRbyhaWbC7lczvP8frdbKte/9MXfSZNBlsmgbFmm7efcXC43MV1NMlIrjnX6G8Ph5snZZ4G9gE5g3exdVKIX65Vu59ba9qudfkPGgdbcdIZKMdv2LMuyXToxMupiHJgHigC+c/ql7bUG5Qaj1DJNoqVpWwYBI9p2XNuyMikJoUKqTCiTM9c2lBLQknMm0lRKmabpYBi2Wm2RyeGgH0eRJjTs97SS3OC2QTbX1mojNSi13WpPjI/1hq2BXM0XcrZLIGrHD/3w3trHOUqZtzK+Kw9mURI20lP9VrSyuhzH3W53M4kyywKl+UfmfuLS0jfb2Gi0Wqm53cnakRJRFHdkUjL29fD2117652+8+TyDtqgDpaM4YZwb3NSQE3vzB+afAtzvjUDfBRrYcVm/AuwFRoFJgAvEFAVgEXgZeAgY7+BtG3vX8Wbutj4jSK8s3jhx4MduLZ9Poj60GUdDxypEWZiReKI64prDXntoMX+jtX1z7SbPV2u5d000niu6CyvJhZvXpqd3PzS3OwGsnU61cB3f4Ea73TDN3NhE9fy5i4eOHFNSSyXKlXIUR1ki4ng4OjKmCXq94Z4981maOY537drl9bVF17EYpWmoWC0DMaTuUjZqMHrh/DtB2ZyeOAjkL3de3Fc46OOIa67Vg0kXadszt9vbjmULAsMwYeTrlYl+2AmzRGvx9sUrpWJ6bPQ5AMDzE3vE+g0rzQRnlFFQymSmNGGW5zNuK60Mg2cijSNBoBkxLJMZ3EiTrFwuDgeDfrtjmhahVAihNbIsdd1csVi8ceXKwcMHoeXG6nK9mrctI44S23aiMBJZalhWEimwaP/uhw+MP3Fp6xvz1ZlJ5xNwsDcAIAGG0R3xtv/0zK9odC3TJspsRJfHxwqJCqs107Obq2uL2w0xOV1NhgQuAozsmXnienShHYVh3LdNI05SlzGt4QRsZMYAMkC836R+ELY+WPOR22z7KHAdmAegcGUNFyuYcTEJmCFeutW93hu4j4yDiHlwSCgGaqD++Y/+XQDLa4duLIXNZk+BV4KZhc0zrmcLqd5euSyjLOzqi4uXi8W9h0Z333kq+ye//I8KtflSsVqiBLdfotXPKCS0hMZG49ahwyczwTbWVhzX84OiaxuFYmEwDNM4owTFUmFxadGy7HzeH/YjbvCXX/yzxsayJpoRElS9yT25JE6IJgq9rY3GQ4d/rDayb0/1Y0CtYo8D3TV1xjKCRnd9mOSuXl7kmkolBIllljFLddqRyV3ClG2XDFJyPW/E3wNYwFyG7tk3rkJJQrlpmobBFKiQWmlNKdtxKk3DACVKayUk0QJa+b7POIfWWmlGCSFUSM05cRynUChZttPtNINcfnRsZO3WkmEYcZJ0uz0hpOs6w7CvmTQMi1lZq710ZfWdubGH+2Jwa2uxHuwsE/fGHpyuWPQL+snZvz9Xf+rc6m+VanYiwnpQM+DO547nRsJZ54m6/4MAAL/Rv7i2utxaS7JMe44rpLQtOxMpJ/aJx/c6zjZHE7AB74MZtqOudhps3hf6AgCcB2oAAWxgC6gAWwQn8njKwBxQAtYVBiP2s+PBEwB8WgHw5s1/z1yimGXBArB78uhaa7U/3FQ6W91chqaGwTMVd9qh1rm1zbVSsfg3P/8/3vtUCiDw7DK/Kx0JxGFXSsmZESY9JaXvGKsrN0EY55ZhmNVaNYwimWVKpdMzc4PhsD+MS8WCyESapo3G5sLVs4qQLBWEwPF0re5bxDG4s7k+6PfDtfbpuXx1J3oCBMCBjc2L1xeurayvXL9xJedOENM4fuKHPvfk352aPWDZjh/ku4P1bq/Z6fV7g61B1FvFV3eGOrvrKGPccexMSEIRBPlMSBDYlkmJZlTHUaRVahnc5IRSksv5vusIKYdhJJT2PM8wTNexR0dHSqXKsRMPj4xPZEkqhNjc3HC9YNeefUIq2+SFfAHQIMiVzYOP7Dl67CQ0ArdEEmOidGg6d5IifdCsX5ycrD9c/68BAFmz2bx+tTFTLtYwyjEOlOv4G7cdPQCIe7S51bU9zigNoyjLsjhNoQk3eb04ZuMzwOOABVz5YJ7dCeOGQP19V98EDt3+vgLsBdDD4u0zHjAAcHMp0bgbVG2JduBNnL/yF9cX78bb5qZOWKZRKDp+zuAW59RSWoK1e8OV2emJL3zup+97MMX7ON8bSNM0syzeaq6efesvyuXJWKDb7VDKODcYlY7nh8M+0bpUrgSFwtraJgNMy0hTJUX29plTYRRpJQkhWmNrJVy+0eoN+5lOAn9ianpvbcS82P96H+cUzgKNEH+sYhJ2toFoYtfs3J7Her1kc3P70vqN9Vu9keDpSmF+3649U2NzhZzf2mpqMqwj38eXgV6rv2CZjFIGqDhON7daAGzLNA2DMWqYBgE4ZdDKJMpzTdd1iWGmaRpHkeu4ExOjlm2WyiXLYMNhmAvyURTngmCkXjcM3mk1oyiWCoZhVqoVQmiWCS8IaiMjoVwrlINHnjx89JFRgU0AkxOzm+L8ewXZ38RaHR8FagAAY2L82U8f/Ds5PAccaeubHSwA/m07BQCCfFWIjDEtZdbtdYfDQRgOMh27BXOg7sxSAOwozh7QfyDXADzIkusAD99zOLHzEekoRRsA8BrQBw53BvLlb35b4xQQAyjx4r7KyU8c/tnjs5+5c3O+RI8d+qTKTNNAocB8P8hSzk3l5FLLSaDuX9wfsNgnYU/IqN3euHLpbBJhYnz0+uKa1hpaU0J938uylICUysViub5448pgMCjkfSgM+r0kza5ePAuiKAAQBd3ejKOexa1UZTQSYc4fnyjve+3tr0YlPVKdg3WqF0drm0kYRZ6ON9s39uZ/6JMn/wZD6eL6uaOHnk1U3zCb+yrfB8wsJl/x8xE3NEf10uafHqjLMNpijHJKbINprYSkOd/hjAqRApxSrgnNFEzT1FDcNsNEpGmSy/mebQMSBLVqdTAYaBAQnaXy5o0rldrooYeObW9uFkvFaNjNkiSMY8POAt9TWRIOsu+88UohH7huJbDyRQsWsssbL66tXX/2+A8DyxsqG6FzAICcCQPI3RHs8ZHPAzAxBoCpq012PsNvVjEF7AVmAazcWr95KbRNcEI0tFTSyavylArG0+ZgqRbcCfCeBsxN9Or42AeQTAEZYN6j3oB3U0ANoAaEd4hYJ1VgBaDABuACg12HqgwRRABuv7/rHUznH5o++tCu2ce+9sKvP3bk+2+snAuHHZfVYfJmv7G4cWN2bPK78azZy7JssLa+eOXiO51W79Of/UkBtFpNRqhhmJmIg2C83Wm7rsdNxzDY2vq67XqlUilNMiHk6sqtTqehoKEJlKSUZ6nYXO7tfWh81/7DjcYKc9XXXv5yKW/fuLIyUtjfjfwDxYON2jdG2GOWGx2uPgaAoQTgwOhBgAI3t3ARKAC5Watcm98joIFbj9R9oBmnQ9PghICFhmlxZpiccykEo7w/TFMhhdCVnK2kEpCUUKE0pcw2jUKpkKVps9kpFALXdbVWlOhuu8kYG/Q6g/4wSjLPz5UqVde/yblFGXccOwg8t+LwerE3bMyMHT13+YZtVR6epd3oPHPaf/DCP3ADs5gbaRTqhXLdM1plnPygeZpk39cCKSG/gQsVjHAkQLxw/YyWTEmdqASgjFNNqErN/fs/uSe409UmQFrYilUP9BYw86DuKbBwz4q8DcRADsjfVq7vAA8DHHgT6ACfAPrAR4ESsFXGEQDg5x/U83swFoxOjB1dXHw9EclWuzHCSpuNBuWJad2fhb2fZ431pfW1a8s3F6vV8XxhYnZudnVlmxBqWabWxLG40lqILMvSsfHJdrMJYji2YRrmcBCmWXb+7VNaa9PgqZCUEEYoKDIpRibrw2RpYuSgYcWry9d6LaPf7Zy+9E2tU+NIPFn/6Jz3zACn6LsrAgSWOPKAD9SqOA5ogA7gX2/Acy3LL9uohrjWXI+FFCKV3OCcm1GcKZ5ppQdC9ftJIqRjm61W17IYJ1Rq+I5tmCxO0kF/AEJ6nS6jhDBmG0Yp76/dXMj5PuMsicPzb79dKBZ6rS3LspUUWZraljU6Nl4Z2zU7d3Al/pPNxuVSFfvLjwFjj85+/qWLvxn242FPmjPx3OyIZh0LMztaakeubdwo4iO3DxPAIpB9LBpoSVgcFmA99fgPXHjzN5TMAFCqlUSnIZjQK0vv7Cnu8CwF6kCzhMdLFBnOGw+Y/StACyjdo8wqwBKg7rQY4LqPxwAAywAHLgAFYBwAUL2y9UWLqUq+6LOp+4o17sVb196anJjbai0f3XdyafXVXOqM1yYKFYOYarx85LvxbHN7cHPh2oXzbx48/EihkCtWxhhDp9OxLZMxI03i6kh1EA5t0wzyRWjRbDZtxykGPiiLo2h7q7G6fFVrDYAzQgmTSmultU4ajYWgbsM2lxcXXLNmOlybrVhdl0mwunZDZktqisy7HwVCiXWG6NzaS4SknuftDp4DSju/WgJLqk6769n2wiQ/sS6yctUMCl6vHVmmaTCaCaWhuv0hZdx2HVOKNJOu73JGTIOmQlGiGaOWaYIQJTJKoaXI0sTWbKgMlWX5YML1fCFFkLOXrl0pVytRHPuu22k3hYRWOorirXQ5sKe75obn8C29WCNzQMEwiqbTKxS84bA7HMTUtsa9h3ak2sPpAMeLqAG4Ff/5lP0pwNrEW2WMpjhdRuFC7+sHg/0Ajux9Wst/rpmCgtIwbUMLkSby4K6dkq0O8DqwH7CBGLCNu0b9vdj7oJMzwK3bDuarfYQZXivCFaAccR8LOfwAAGBN4o1ec9mgMhNqd20FOPBBPCuX671B46985u8AODT71Iun/qjRvnLk2NhWqwt0dgKcd/CeAoB2Z6tYrpTL1aXFS2+9+ebc7OzmVp9SSkAU4Lkm41xLZdlOtVySSg/DiFNqO3aWZGE4uHzhrBSpbRmUEqW01hrQGoj70MLpd/pXrr4axp3xyWnXN4PiCJhiPAwHYb1WJKy1Mx6GIbBerIaZaiW638FZ4DJwEYCHEd91TRaP8tkuzjl0/LE9/31QGFUKjFLDYFJJIYTJOaM0n7MD3yHQqRAS3HRyWuowjrNMMMaVFIQQwzQJIQREMktq5uaC6bn5wTBM4lRp2J5frtSUQr5YIoQmUXjt6rVr194OhxtCq+mRRwP30PL6tQhXh9gu5Xb/yKf/y7k9s3HSvrb4ehJ3MlwHVjJ8J8Dd9MuU/YkQp4BmHfvPbn6H4+lrPWNjtXlu8/cAJFJQRjkzKCWUcq1UmmUAqQc7nmPhttYJEryGu37i1Q+iwr1zC7QkVoAuUBnF0SI+AhzleASYMe4uvpcY0l17ZmZm9+6ujd0bQFnLvnPn+2a0CGCmNDFfvcvpQwc+0el1ry4sqdhFcv86ySaP14/vPQmgG+osHpoGL1VKjc2be/efnJudWl5Zl0IyxpVM83knjIcU2rZcbvBhGHU6XdsyTZMP+721tZWzp74pslRpRUAoo5QQg3MNSKGLFZfZKo2kVs7s7PEDs59sDZd27y5uNTKt+cFdJ8b5eB+vWVgFngSCAtMquJbE7rmzq3ahkjdza/jzHDxtoexPJHAb7WzUPcpR7Hfl4sK5cBhJpbNMQmvXMSi3INN2NwKlpmEAJAg8zonreOVyMUoSCqIgXcuRIuam7QcB50YSp46XazcbMks1lFY6XyhsbG6VyxXT5P3BsN/r2a5z8OGjRbrPRM3BmJcTHBZAA7/sYX/VOdZKrhnuwM/nVzvnc35LYcFECszdFviGgfPACYBXfNfEI9QaVqoTQ3Hl6uqpL/6rL/WafQ1AgxuWUhlnzHO9x5/+9G19kAPeBsY59t6jMExgHXgLWAb0fYrkNhHbgJGhz5Gl6DF89PalHtDgOH5b41iA7RDYrAI8AuSBG0AOYDk2fqc709CATd/jZODPXvm9xsZ6q9Pvhe1u1J4Zu9e3Bfs//snfXttYq5WmM6Etw7Rt0zD4ubfPf/qzP9ofJMMwJKDcYAaXQS4YDsNOa8v1AoBsbm4maWKZTArRbm5ffOfs6urVLJUgGqBQiuxQzeBxKqZ2F+cfKg/iJB0K7ljMN/udrXzesx27WvM6g8GI+wMWMhUAACAASURBVFgX1yWkhRRwJJKF9c12w9hqNHRaGBl5OBZGjp7s6IVB01+6ecuxypkpAzb+/PNfDvttSCmkkkJQSgiIUNCgSmnXMaVSWiPwHSVhWmY+H1gml1KY3FDQSkJImQnBOd9qtv18XmWZ1ooxIkTGCPFzQZDPD4dRv9sd9tqamNU5I6ZrIb3k0902JvpoGDA9zAFdwPYq2s15u90jibtFSa2An7qHZDeAKWAUcADCUAPgYMbDrrpduLpy7e1XbiqhNbRhWpSAgHDOHcex88PxERtoAwVgvYNF+26fO+QoACPA7veTrBF/zeMSMAE5RE9hYGMOqAAArgMd4NF7ljUBVIF9reZFx6XAIMXi1auvVctH30MaOC+f+dLy5uL0yN3y2GY/XVx8Mxyk4VA2+41bzSsHZ+/Yo+AFf1ogH2cgSoJoy3KuXH57fs/hQs68ttjm3AIRUibFkq9Atxub+w8eIQTM8AihBLBtJxrGja3GzYWLnNKEgFEKQIEA0AC05oy4RcIsPTExnfhqq3m+NhF7bsqZ+1DtIxIiRg6o1/CTGr1N/H4dBxjyc6MnzrUuu45hW9Zqa3mudBJANOBrWxcf3v+Z7fSdCeNZAHEkCSGmaQyTjAJUyzRTUUYIIYwTQiiDEFIPex3D4FIaW9tNkzNGiGWZhDKRie5gwKTKMkEI2VhZJtBBkHNsmyBWGkcfOrayeqvR2DIty7LMLBNUVrZWl4m7mY79xiSOFFEGbgA+EAO3lpbfPjn18wBm6HvmBsDtLPX79Q2AQ588cuhP5RcoJYzbnNE0SS3LANFK6fK7S1gGOMDjhQfdf1/ATOIGwy4ANfs5oAVEQOAjYaB4Nym2CTTfG1EDUHr3o3ziyuJXuEE9y9u/534rsIuFEw8dvnxl9d6TTx197MWXfotqorXTa6dadmLgTlyEvvPNi5XCyKAfAjAYVVpevXLxiac+3o8BEIMbzDApEsMwfc/xXGd1eVHKLE1C03JsmzPKh8P+5vpaHLWVVForAsI45ZyJTCilGaOWZWiVJfGgmHcUTeOsu7/wmYcmfuGt0+c3tOZ43L9drk4QLS+FN9rngVoBh2fn9trW6MP7f3SudHynwXzuU0/v/1kXk1PmZ3fO9LstgJq2RQmVSioFIbXnmlIKIZQCUVIYDKnQ0BpaDQfDJEmEEIPBgJuWaVmmYRCCYRhqrcMwcmyLM7LjK4RRrLQIh8MsTRzXZaalZLbdWTg2/6PDJHNRibEJxMBB4BRgAgGM3oNp8D2AEHDOLdNM4oQyShlllFOKVnenzmdn5Wp9L12xe4xCoAS0gAtNdX0TF4CzwDvANvAowD6gg9Le2QOdzSwOh5trm/ddy2MuT/Y+uu/Z+85zy+AIu70GpcRzrT9/9V/duURH6vspg+vYtmMYhnlr4fL4+N58zmi3OpwbWkuRxfmCTxgB0ZVqbXpqulAsKZENes2w3+t2263m9tryNa30znqdCSGlYpQASLMUhBIQP5efHjtummPzux597OSnd4LRc3OPjpL7CkTr8zM/1Nn2EqwDoxPO2Hj5QHvYAnBPJuSuaF49e0pkgyDvSwlCQbmlmWGYFjd4PvAmRiuUIEsyxohhWo7j2JaRDzwA3U43ieN2qzUcDhhjrXav2x0KpRkjaZoJITTgul6cJFmmKKXFYmHQ70tijY5PHtn/EeBWFG+vtTYcPA4cAUYAC6gB0wdGv5cSsQfg//zHv8QZs2w3iUOlNGeUUUJ2PCrl3JM2KP2luh3iNeA/AIsJ1rOkK2S/hfUMDeD9Zb36vYePnDjx2MZSd7vZ/66ZLnHntsePHinmuG1x3zWUio4d+uiaOg2EAOjkrn2EgHMKIEnCM2dOHzvxaJhCSiWkoKClUmFsZMp2/OZ28w//7e8JpSmQJGGnue7lgvZ2Y3NjddBtWNa7dfSZ1IRAKsUpIYRSSjKR+YE97x3aV3oyV9q2/HedkVJl/P2jLmD2xO6/ZuEhAOu9KBmqsjd6M/nG10//syvtb59v/iGwcqfx4w+d5AbL0pRCaaVAiFCIk0xkGaOUEBiMeg43DcPzXE1YlGSD/tC2Lcu2GOWjlZJlWlmWUUq0hmlw0zQpo71+Px4ONhtNBvXWG68uLS5GcWJxSgk9euxxD9NAWB0NJktHboc90cblHU1joQwkd0a4pH7vu2aHdrDypW/+b+3WDcuyZRZnQpqm4Ti2aZiEwLJoqXqHu39pZenhI8D3AT9o4bG6M5NjpUxHBh649r5/i8vBx5465jvuZu/sn535xbdXn3//PS158Usv/NK//OrfW+98/WOPP3Ho0BHX4mOlkudXasHIGD0OuDf6X+ZKyywlIk0Zozdv3fBztXLFv3jpBsBtx5MqrVcqAFzDdMfHf/jzP14sFHqDyPYCqWmn1bZMs9/dzrJESU0JtNaMwLLMLM0YI0oSAITRRK3dwJ9M4UcMTNXZ4ztDHMcTDxRNig0TIwAsMnryoUcAXLtxWYje5asvVwvT28VOhU7caayElIw6ltUdhgZnIs0Y0bbJDc7TTBBo3/dAmWVSmxu9fk9ICRClKSOYKJc7dnSxN1ASjmsMhrFjW3GcJHFomUYURdVyXmuilYwiUfDsetUXYidfvu9o4W7+W+BiFFUd56KNJzm+DwiBJY1VAlqgbeAC8BjQ/4DcNv7t13+z22xlGY2iTpoJAEmauco2Te5yvu/k+Hz1jg4L7tno1gTI96bedqK5A46PB+gFZBHY/cGNN98zSPrk+PiLl5ZuUW1XXef1i39w8do7tjfxU5/4eQBfee1XGltLNiv67lSjHY0W4tJoYWy0PlYtn7lx/dSZr5s5t1q0by4tsl/4hb+VJmESdrMsOX/mraee+fRgGP3u7/wzrcnExHRre218fBSAkJpSUigUACSpKATexNScxWmlUv32t77R7zW1JlkmpJRaa84p5VxJTRlljGlCxnZ7++eLeTw1xLYEWeyuVOzaB70ou53ZdyxrJ5K8sPId3wnKufFH9/yUS+7eeH3t8vm33rI4U0oPkyzNpFTSNC2AOI6tQaNEOq5vGMw0jZrv1Qq8kHOiRPcGoRKCqCTv8rVmL+c7/d6QEu3nfC0SnUSDOBVC+Z5nu26xVBGZsGxLZNkwzvbuu2sXN9Po2sa33r7w8tK15saaTMQwEZ3LC6+N16cIGkBqwweevT1/D9Dfv/+H/2LQazI7Wb7aaW93pRSGYeZyvuc5JmePPzH1qY999rYDsQIE9yyg7u2alwdAY53ck1rdESdgAwoYAvUPrmPzgeGdPQEAqHG95BRubm4urix98uR/Uxk5sL6xBE+UvVKlMtXsbM7MnKiWpx+afeL5c1/u9Hq7xicSJTc2tiDYRz/yE9u9ZufaKr90+pW4tRENelBk+sCJStl/8/S5sdEJAtHeXnvnzBt79x+Ko2G9WlBKU0qk0oHvADAZGZuYAqBAOedCqjQTlNBUy0xopiTjHFolSQbObp2PVvdPVac7Ai86OLEv/wMA3t64cHTkXithcG/tSHs4KN4OEyZbKqatoR9h/j0i+cZXv0gp1UpJraGUVIozbtkGBY3iKI5FKnScJDnPcQx+aWFJxP2Jem12csxiqtUN15u98Vpl73hlYatTLBYoIdvb2zaywDUZM6UEYcww7O2tLc/zGSPDKNPt9r0DKJtOefzj8+MNDwL4NLD+J9/6yvqN5OI716d2lSdmcqMjXm6n8vEDSmG7/eVBNMzbpNNsEwUttWXZlWrZs00h5aMfe/Q2ycI7FRbfAzJyu9LyHuwMwMeDswjbt4MdADygg7tr6ycN/1qttMyJADBZGJ189mfeuPzyn13/nXJ18vD+Z3aVj6VIU6hhtzNeHXF47mpzyTDkxvCCBewbOVZ5LM8vn3ol7xhhJJThfvbkU6mCZXknHvmolun29mq1WnF9QwsDAKUkEzLLhOtY9w7wp3767/3qP/iCFMLkTHPKDaahldYMoJyrTHLCNm+oMy+KQz+TCeQ8fAJAht7K6jtxtFGfCGaMk7dFcBdFzwdwfePs9Ytv9FrbJx/7+Mjk/SZ2v9WP4iQDGKNZJimBbZlKaa0FAYZRBqJN7lXy/kjgjObMOMl6Ybi4sDQ3PbZrpLLdGxDG5yfqzWEEM6hWK8vLiyIclEdHUiGUUhanaRp1Wk1CqGnZROtKbRoPgOrCurz8R1dPR1fO3UojfuzIx5597PMATl96fWJ2YXnjnWgYP3nwp67denv31E4+6tsXNzZf+KPzre2maxqr7UQKbZmG45i2RV3bdVwziiIbe28rnu9SRvv+6tnXgac+uP0DUXnv4X0GXGVudL7uxK+99duzB58csffMTO3ev/dwQN4tyz57+U89wyCaE+1QqDAcWra5e/pdrlfKc3y9sdUkqtWPnv6+nwzy1vJa27Q9xpiURq1SnZj7SDRICgVPKjAKgzNC7/eEr1w6xQ1OoLVWUiqpBCGEAKkQJjhllHOmNP3WN//4kz+95hC2hVtV7DUQHDn8+MryjdPfeXPyiYPsA37uS7dOt7rXoNz5mWfeeyW7sPIng95ACuXnHGhqmGYmpNJKSh14jtTM9anKMoMRJcWt9cZ6Y8PhdKxanp0czbuu7VrFwJEKQiT1wD27uDo9Ozc7Pbe2dhPcdAwjy2S318/lS0E+YIz1+t1Bt2+4y+8f5JkL+O1f/3frt7oMLElibpj9Dv/JH/88gOP7HwNQm3nXHqJcv/DKl6OoWarrm9ebzY2tza1m3ncl4NqmwUAgu91esdSnxOWWfPWdNx4/shPBMd//XKALLAH3Ja2v4t0cOYArH5Du/MuiuL2xnSsbHzlxYMcirLvv2gDL4dVJd88j+54EhOEXsvCGn3Mr1eKIN7F7+m4wmR0/uKfd7yfc/ms/8wuO762urlPKAG3b7MCBOc/x2p2+7zn0ti9C3+uUvPDt//DK819NwgGhSJKMUpJkEkpnSpkGNw1mOw4hJJMIB3Gz3b96eUjiqZnxXQBubJ0/MnV8fuoh80GFyI1ssYW33j79FtFe1AqPP/xJAKcvfqVYKXPiAi9/7fnXepuZaRrQKhUqyaTWimrFTavZ7EZxwqHLxZxrcdcwC75VDDzXsmzbLOTzlsnTVIRRAiUyIUyDM2Bj4VoiUiV1v9eTSjPO4jARSvmezxkRSTIMh+Ds4ZP3uy9/++f/1+Zmj4AQQoiGVCpN4vOXLz37zDP3tSzlRuem94/M1edHnnnh6y8uLi0kcaqhtEYUhYxBKpJJmcv5jmVSliWDyMlNlgoftH9JAxMP8hPvrAwG0Puudd7fKwqlAbMJhwNU74m/YqPx5/CH15Ze0LpjuwGNjLH8lMWdfRO77PzuO4/mW+0tanlPPvbM9HRtY2vAuUlALNsbqqvr/aTk7ybybkWy0OD3vFQ7iv7ipReSOIQG55RyahlMZFJoJaNEce64DiG0N4wIJYzh0l/EuRy14refeeTRAcTMyKx9v616FzVjFqjb/qmwIbTSZy7/S2ro4wd+GgDQXM2anY3IsgyZCS11JjQIDMaSOPIdTytJKAWB7zqlgh+H4ZWl9SxN0ywJbCvNsnohb9qWVIppzk2Da4poUPLNasmWCmlmZVpRRvyiGyWZivqmbXPGpILW8r5x/sNf/pXm1jZj3DS4VppSajEmpbx+5WoXW/kH7QcJyDgATSwAlNI0zTSIYRpCCKUVNw2l9Mee+8GVjfPD6Obq2pcGg8ePHnzkQUK61w9Yu70V9M4u8C5griffdi2ax2fuv/UviRSejRTIAZdwt8AJtuW+9vpfCBG1usnHHvpY7Kl+/+zM9K6kHRq9Fg3eddq47QXz+w5/8rkfAtBsNk3DYZwZlj408hEAje1BuVYHICUYA3nvL+d3f+vXOq0tqrnl2DKLiVIg3LQMpmSaijTLpNKM6iyTBheFwHVdH6A/9tf/FmD790aZPhDu5z7+hTNvvHX+1ItJTOLhAEBbX8vI5Quvrgy3Y0JMDRimlchEK50KYVlWHEZgzLEsrVUiZH8QaqUnJ6aKLm/3usNebzAI0zhilHueE+QcW5hCYmu7uXfvLkYJo8Q2GcBACIgmORcAM7g1Utw7VWPee+yYzfDcN772FSUySojSjGhFCCfM0Epppc7f+NITu37ug97t5uJVgGiNNBOUGYZhRlmmQSghlJHZvbv37T35xX/3Kxdu3ayMd6V16fh8DQjwAcEgPMDwzwMoW1NX1t84PBp9F+f0e4GFQ8CLQHqf+ry5vSljMkizxx97FCjYgJ0bBwgzGPWsO9v4+Ke+/7/I5Qq75ie2WpHWVCnFQSZG3v0VOhbjDJlQBqf6vUmK/+df/PrK8pXP/dXPLly58s5fXDdNDkLTNKOEgrBC3ldSKCUBopXiHDnPC5OsUBktmPbtof/HYaO+3b4J7hx96BMOxoDmtUvni3WeDgIpCaeq0xsSgDGepmIwHLqO4/l20hmYnDsGHYSJUspznG6ctPs9oVWnlw7CQcFzDCLLQrZ7vX6/l4RpnCS5wPFznmEYpmFZtk0JI5TaNjVM0zRMyzbKrkvIe4Lmdffwv/mXv33mzJmgULp65cqbp8/evLWyMw+U0sAvAuc+4E+goKQkBDs+k1LS9e04iiillmU98fFnrq++2lxrNdstw8HaraYO7b27jnjk2AeLigDfBA7fG1ETeN7EJ6ZH+/8fSXYbo4ACfGB5558TerhlcPfgoROb7cut4UrdhAK64QZLo6AwClhAujPPXCo1ObOPAO1m2/FyEBm3xE6v7V5SDBwABqcAhsPY996lSJTi3IXX/u9f/dcAUvG7b718SWSCMTKMUs+xhchs14okkVJxRmzHJoSAUBDteN/L9sO7eP6l/7Bw5ZadJ87tRWH3gd1FHNr9Wdy4+j+H/YHFeZJlYZQKpRjjaZaKriiVgnarHTMWEDOMkixT+cCzLD8chl6Q9/MF2+ThcHhlbavfHzTbXSWyUs4b6JVywfdsw3cd33Ncx7YMK81M0zQt09TaNU3TNKhoLvHyzF3ZT+4andwF4Mmnn/0C0NpYXFxYvHL9JqHkcP1TH5A1BwDGCKGMkIwAmRCMvvuvRw8//tzHnvgRABhHufLlfCk+/eatxq3et1555TNPfxeeAbCBxds8uwgojiJwKYAP3Lq9e+WD0LiT23gfYsAAGNADmEg4t941HqSiH5n/qwB21050sASAAtzdHQ7eDNQQtAxIAGl2ht+4fu3HfvKnuwMogAlhe+5YvQG8BHystb2Z9yYp0+9ui/LuWn8vv/yno7vf9RB72zFjNEskowAIZcQwGCVUKQ2tYMPgBmEIo2R69+Ef/8LPfte3vR+vvPg8Y/rn/7t/fOdM8Xb4R0glMp1ISSjXyHzX7mstMkEo8303TZIoTodhRDkb9x0pZJYIxlilktOahsO+EDJfLLtBSWAtjGLiWgPJeEr/X9beNNaS8zwTe7+9qs6ps95z9+6+vZHNnRQXUaQoUYsVy5J32dY4iifIGDZmkswYHgcBgiDjAEaAIAGSIMgg4xjjGW9jRV5larElUqIocW+y99vb3fd79lP7t+bH7W7e7r6kNHaeP/ee2k6dqrfqe5fnfb5eUrhuUSvnHBnOQFAa+F4YlsvlEm/vNiqN6vjR8i0XKNsBzwf0Hrm5MXm0MXn08Wd+yO8qLAAAwRhjhAkCax1ClDHf87/4pZ+8tdkDR392uf/VyaPV3a3e9QsrL3m/98mnvnBX0uEWkpvyUnBT02AFwAJMH9TIeQfuKG7ut8tb9/3DKfztUHaEChvlAcCj9X2FmUIbS9NOvjHuNWmDAy4DjPacRc4m6LMf/TFOYbPfJ5gy4VEKCJCFiSQHRnASj5yTldqdzuxnP/MTn/3MYwArAFOrlze01tpaZyyn2FrnC49Q4IwihDDg3qAflnkU55958NFDtck78rEfjKef/uRotMbviup/cOnPVZ4bB+CQNgqD0dJySiglYG08ijChQqC8UI2yhxFKpSSAvCAwxvb7AwDLGMWUCgcz05Pc89s7Oxi7rCjKfhBnUpTrBCO/VBr2B4N+HErnRwkGaJcH5anjM/6iUbpSq+LggDrSj4K//PM/xRhxTo3G1iJEEKXE94NHnnhWvOfIAwDM1Z+erq+Dbl86vSNK2U0W2t2Iu6rXZLcKSnUACzAHsAmAfwTFjf0/ZBdAAxQA6I58ysVzC9WwMTk3C1ACkAD2lhVO0ONbyfWp0kkA8OlDYLY3l7rTJxoAMYAl/+b/+XeAIUk0RkR43mCwaqtbWh2ren61VolGgySOK7UDi2hyPd1dWb5ybX5p0Ot5DOeFJIQA7PmySGnDOXUO50Xm+UGWKfB7ZDJr1DIOhw464AE4cc99x+ZOMLE/u7YMUPhB+fxb5wE5baxRWlCMCRZcZEWOrNVaIYSzwiCESoHHnE3TnDBS5HmhTBiWBeeCUS8IEEbW2mazVeQFY5gz5pwDhBglGAFgKi32yw0R1oep8cuN5tSMA9tub6VZpqVi2BgZUW4BcjncIV4NQAPYOwjx+/Gd7/5dltuXvv3XYLVzThuFAHkexZhxEfw3v/Xb+272XlKgRGBqvFkvjbH7jp1g0DjIzoqd+Nst/1O3Fy4VQG5hA4EGmL6jmnQ7erc7cCWAOgAFIAApgLy1I3bD2UNjBD2s9ArBh+/IHof8pp2Y3TOnL3nUNzITCJA4in0Bm5sDhAhCSOtsa/vqd/9ykbgbO4yNT84e2c9kAgA4u/pXAKfXRm+oYeXek5/8mV/8NSE8RIiURiojtZGF2itXE0ylltVqaLSpVLzmDCmVRHlfVPxDgQAik+9fMr/9BsB4q3TIGuuszfMcE8wodwDt3jCOcwAnOMeYcEqFxxjBlOC0UIWUjPM0zQf9wWg4MogAxtZYY0F4XqlU8jhvNuqVSugLplXR6fakVKVSwIQISlVMhcVicXVTS/XMp3+J+iyoNS5fvfTVv/jjt7//bRUleZHtLJ1Rww0X30nYuoUXv/tNguF7L345T0ZKKeu0cwDgMMLGmNbUe4nNNpzfvyODh09NfcmHT1ztvNx2Xzfw+v61Cs5NlH/qrt6kCsAhDGMWdh383RBeARgBdG5md1f2bdm4Gf3vNX4CwAhAAawCKIDSrVF1avJRCveCXer2u+9/07Zl1vO4wyKphAIjBAA0SiFNU9/D4KTW8TMffXBlyYTv2x8K2kHVfxpg8lDlxu86ceRQUeQeA4QRRsApRZQwSgFMkktjjPCI4BQoziI+6pph62oV3uP7rqofHGbPAvTfz2WeqN1Wfh4PP7Inmuqc0UoLzihG1lnkMCFQ8j2CXeB70rg4yTwqCEEOYURQrx8jhIZRiq0qBSKsVTBCTDAmzeHZmSLP+m1pHZTL5SyJs7QwFjBCSklbyLFmHRDJi2I4SFauzgPAA498CgCaE8evzJ9bXLiKCc9zWa9ViyLlTEwGAeDg7pD6U8//OAB87GPP/9Zv/tMizy1yhBCCEWcMMA736YKOHZBZjADC1tgEAURgDmDtJukN2AGNont+/WoXVnNoV2E2dy51rxppZr2fAChuvixv1awowAaAvSnBFwOsAAQ3B9ybuQxXFNGon60Z9H4v7AWAdp7p1sR4c3ICDAFaArdFvvQrv+qJvXBd7Q6u1CfoVP2+D9DaxQhqpdu8q9NXTl955w3ByGiUEIIwwZQQIURWSM4oQng4iv3ATxNJceO/+IXf8G73P5bbl7VYurpzbjqcPrDYnBQpp+/1KQa8CgBvnH9p4cK8sXYUZ2muolQCOMGpMyZgOKyUGPcHwyjwBSPI84M4yaw1hFJKiNIaMEUAgrGgFERRWq1WouEQEGitfc9L45HvCeuc0UppyzjFCLfbHSkL5JyRyeaVN+9/8sm90aSQ2ZUL57a2VofdLmZkd3u70+nMTs4QjgEfnE340z/7w631VQDHGUUAGCNfcMDYOru6/a6h8dTYCXQAuWMHoOpDxcGAQg1geQTLAk4CwMC94iFxu9dbAtDr2XfioguIjJPHOSr5qIyo8sEBqJvR5a1SgQZI4D1/ZgRw4gDSEaqcu/giq+mo70hJBOy2ETxN1xjLuu2s3no2COcABYAF2AJwGadJxrkwqhA+gNitQAMBRInc3Nq++wK5uxcBPH7v42HJdw4TggHAWmcdWOuM1tZYbUyUZFbbUuD99M/94/07Xkn+sOcWH5n89Cz7tJbm9Wt/sNL/xl4kvB+//2//53cXv1zAwv6Fr3z7q6MoHo0SZwEjCDyWS2W0Y4xVq2WldBSnnPMkK6wxeV4Ij5eCoBaWq2G51Wr6vjcYxNIYT/gIuatXr0TRCAFYY/r9HqfUF0wI7qzq9nZ3trf7/a41stPtDofD/jDa2Nr5y9/93/fOBBOESJClMsmia/MX1laWlDKFVHI02pNFuRuvv/IdJZWx2llrjMYIUUoYZY88+ex/+gv/7WP3/vjFq+8cdLGrBs4BjHPA1wffvhYtV+BJgGjL/VkK27fU8AAAYACwBvADhDDWfhK3L3ReWBusZSAFVByYfQ3Mt9C+SaI0AMsfQKicmal317ROzNXTr96x6q3XX5o/s1QtzwEAALp87vtr8+9013b662vY98sAhjLaGq9MTs8ZmAGA9s7uN174+t3fcf7i/ML2AYVkBSKOYmcNAlRIba1FGFXKJedsIaUn+CiOK/XZpx55dP9eO7vrZ+a/1oWXAeDpuS9VKie2d9vb8HewT6xmCFf6/a1odF28R3hfPTP8batcnhcEE18w51zJ9zijeSG1tspAluV5lgIAo9g5KKTkjDhjtDbgDCGEEIIIiaI4iuNKucQFp5QWUjlwsjDU9xUQozSAEQxF8XBza11wanWBkC0cHoyize3tL/9f/4ORu/efepxgoNTTBnOvdOjwyVZrAlOqtZbdg50YZ6x1FjmnlAYAjBFGOKxWPvHpPW1YeOCeDwFc6sBfbpoXARYAFMDLKayQG6yKbKw0ZZMSgIrgJbE59gAAIABJREFUB6tLSzJr3v4NvoZ1ABF4lZnayan6HCCdRB2lXQGjgyhDAJABMIB3AS4CzAHcd+CZA0CSIp1JjJUt7P7l165+dRT3elGX+jdoNaceOtZsBYMobvdGlGDACCnQFILD4Q0P/dix2XL5Z+/+jq//zX84/tAzxz/3XrTYgT8bg085QIzYcuClhcQAxhhwYKzzBJPaWkQQuFL1vWsRwfIb1/6svTN8+NT0Wv+crfMQjm3sLjUqjWyAurV3mvAkAAZYJwClSuuZR38VYGnvKbyUfmXtOiKEYUyF4IQQY2y1HKg8L7LcONIdxBWfMUqNVYIzQEgqRcAxbOM4JpQM4xwjRwlpNqec1WmWI4QAnDbGEz4hHsZaG40odcYAgO9zpYosi6QsikI++OgTE+Pl5XOnjbW//7/9L6XWjHPGD0qc02qtwYUHgAGQ5/lFUUC0BeGd99XzvDiOGLmh00YwNg6efu6z+0dZCXG7HyPcnqhKAhuLauUY22u6bGMIauzR6uTC/M4fS6WdoXPB8wVcz6DPQXpQxnCYQgsgrsMpgJqARxtNFDVeW1m9yENSbxyo/lIAPLBPEPl9MRwAEGkzAgbizUvl6fsBAFT/7DvXvvDFf3nbEZMEl8jk+ES3n2AASyiZOjR5x+HGx2945Z1O9+aJ5Nu7S2de/7v9m21EG986/6+Ji3yPE4wIIQCgjVNKa2OMcZhSwXlYrgz6V9pmd2+vEOaqrbWTp0IrVhktMjj//Ut/dG1hcXtph0Z0+fqVEfythNMAtXRgapUWhYkYMgXdb37vP3zva8tbaxE47AU+I5gg5DNcDvxmrex7PI7TNM0JZVzwwBPOAWUUIVRIjQg21hlA1hopFcY4y1JCKCCEnBNCeEIoY63RCBHPEwRjbSEIfE8IRrG1Ki+KvJBf+Llf/dJ//htP/dgXR3Gy2+m1d7YQJqVypVYbq1Tqvl9CGCOEsPAIpmmWQrx5x7W1DowxhTLaOgBnjDPafezZ/e1DZ7bSUTU8dqr6a1suuTiaX7s8OLP8R538tYXet653d0d2HsGR2dapuG+s9gD6EvoG0hz6GCRAHeAEwKM3MyAMIAuQ5/sIo3AA39wTnNoPA12AtduZHRZged/H63t/HnvsM7nLEBFBuTIa7O6N79cuvlWfuDMnKspHPf/pICwVSlKlVK+7c+HCgi/8Jz/8DLudXbaz2/393/u//9l//ZuV0Bfgffijn33zB3+7f4NHwifOTZ2ThQoDnmYFQoAxcc5JpRDC2oHWzvd93xczhystcqOykcEVXWijetVa6FMdZXascSiZsutXdwbrp72aHQ0Tz+uEtnPp4rX1tSvvXH4pzXd3F3aurV0fO1QLS5AzjFFcqYRpkpbLQVEUSmlOOecKOZukCeZBqeT1BtHeKWV5ijHX1hBLnLN5IQWFNBIIkDVWG00ZwRjyKAmCAGPEOVOeB+AKpShlGBfWWM6Zc/jIiUkA+MxnP3fyxKk/+je/Y43l3PeDUqVS83xPeD4lRCkFhPAg4LQKYEAPgL7nMgtGRgDOAoDFnHucUe+OyPTRIzcjoln0hdkKwEOQQ/+t0y9yESnct5BVmnXAfhpDo0bW5bfKvNGEowDbEvRdWbJVgJ6BzPdbcd6X4ADmAW4rYRE40oHFsdteZvh2MaJbVOYVQgLlXKvRWNtYX9z4k/tPHvYEf+aZp29opt6AsXKt1z0taLUWViil7Mr8m+fPvvnc859jd1IYodlo/Nwv/HIlvPFG/0c/98vn3339f/yf/vt/9d/9zq2vf3js8Euti06ngZfHuTLGcMHAOWUMOCCEOMBhuXzioUmAnS6cXWqfdiiL2mXKXdyjKTGEkEcnP9LfHV2NFipTx3/scz++sfPKfZOfA6hfXDyXRsk3XvhrDNia/Mnn73n40cfeevPteLQJDsAaipEexAlnClyUJpyAA0oJJhTnhbLWGGMJwYxxSlmJUutQKShbCxYQY4RinGiJHfI47Q8yQAicA8BxmjPGjFZxkhMKGNMkLxDClLwX+R49efz4qcfanR3GRKlU4UIwxhjllGKlFBAOxAcwACUAvE+AGEqlcrvbRQhRTDFCFlC9VZLwwuKFuCIenD55IK8aPKg/9/gX1rtv5XanUoUuLA97i0cnj5TH/Ek+BxACnAQ4yWAVAABSgNHN4CAEqHAQ06Eehe86KA4q7R8Zg8oHVGP3oTp9b4NEwaHGpODQHbnY0sP33Q/QBDifggzgcQDYXHst6SfaJPWQLq+tYAd2Y+3KxFF26oEbtMwoTW4dklJ0z8nbYpMv/me/1dtdfvfytZsLxkYQjaLYauN7nFIC4DBCmBCCECBkjZWyyIvixLGnAYgC7eS4Sojvl+rVehTFWxtxEcvvnPvLoti599Hpf/Szv15BR+6b/BBAHSCZPcWssWk/15BVZykp52+e/1avncajmFIEWgmCpVJKqVGccsYo4+AcYcIXnGCMCUUIMHKhR4PAI5RTQsrlIAzLlXI58EXJ92thudaoMCakNoRQqbXgNCwFlFBCWeB7U7UmJiwQfrkUMHJb3uiXf/WfU84x5YwSz/NL5arv+54fOAsABIADcAALgPbTaR555HFrAWNMCEIItDYTh6c5fP7og09//ZW/Bjj3ATd5tvnkidbnjR4hlx5pPHDi6L1eCB1YgRvmBTnAxujtxHT2RaBVgBGADxBW4GNV+Nj7sMB/FCMDgP6R6nHedLEbQSnsZ/L61ZX21iIAADxEAQP0AaAxfQ8mZHd7cOHi1WjUp4vXzrJm+9M/9cnJsAIA1jlG3q86AQDw8D2HHYI//L3feex//XmApwBW33rzjNaGeFRq45x1FrS1glKjJcFIa53Lwil/4dz29OH+aLBeyFFzDIz1qNNbO6M8rumQ3n/q4xb3BsnWTe2uvbf0mde+cwVutk194hOfemD6cwCDpcPzV177I2tMNFKUgaiWlLEeYEyIBhM7q7QV1nJBS4Zqoz3CjDVpmvqCh2WhgAnq6rVaIFiaFYxRhDAgRAjFGAjCvmCYMkpZURTtbk+USy3kkijR4Ap8pw7tf/mb/+orf/C7wvNL5bAUlBF2CLBzDlQBjAOQu2tQ/8lnP//Vv/krBAAIEEZc+F/8md8AAAFzWgkH0z90rjBKGxjVCEwDbHBItRJf/+789tpZQhupW7Eujdru1L3PPPPs0fFmFeBoTy41+K26uLh5kf9+wAQA+cpq1F4fDjcXjh+da03dODi/ORx7pCY8Nz7Z6Pa7Za9Gz5991R+HKrmRUMYIefwg8bZ9eO5TP//tr/37P3npG7/8ydUVUKvtBeeMEB4nyBibS8k4s9YijBFY52wSJ90eeee179jSwk9/4h+frPlndv80S1PuJZ5P81h9+Og/BYD5wbcoCwrYENDowbca8LnTKxvtlVwqncv+Mw9/7IHpvbAfvfX6W9aCNpoDIAOYICAEU8C+UEYzgjHGxhqrLCIADpw1jBCLCUVIcOoMYOFhhFc3diZaTWmdx1muNDgoB0HZI5RQILRQinPeqNUyqarVqu/7w1G0f9y8BS8o+X6JUkYZ5YxaB87aeNgvBwUEY3fzqgkLJycm2u0dcBacG5+Zu7Xq2KFj6M6WkAPQog9F9hJgB/ARD0p/8idfOf3qYppoxMz0sdAhs7UYnX9n+dKF489/5slnnjhyV2Pw39vIAGB2CN81kHWzbUJgvFk9duLeu/pSRwC+X8cTRw/fi4/tro/o5sbqqfqTlf3dlAc/TXtl3RIAfPbzz80vfiXKo+8sdGdmD4OlxlhtjFQGgSMYAVhn9/hmmBCstS6klFIOuyOAKQT+I+NPO8DvbJxGsIF5sieXur2zCqQ7cyKYT97tdTrPHpk8d/adfqdnrWWMnHp0bu88Xnz1xe0rPd8XTmuCweQ5YSRJpU8RZ9TdcIOcttbzBTjjeaU8z5xFgEBqlxUmL1ShbZpJpbXnB4gUhFCTFZTivXmGtEOCMiFEURTOAbKWMRolie95lNq7L82pB55cvnYGwHHOfc/nBBtrnAOtlemtInAIIxYEwN8zoI8+89zfvPAXlGIE+NDsewNW5X2f8eUru28cG3+U3egrmQnwcK/TDsPDefzn7fYgzwrMEPMsInjQyxGwK5eXrYN7j93fbPzDJ7i4hY4EK3XhiJ0+fIi3Zof93lhlfxvYPEALoFJtTFHgADzOV2i5Ovbk48+xHz7h3jjAHwM0AY4vxy9Nn/ByrbGtU1KWMbKA5q9vZ7m04BCAAzBGO0AUgzEWYK99BYdh7fLuH/Ny/VjwcYCxWmXd83CRbLzw9r+u1Sfuv+dYE318WX19fXMx6aPlQ2cs7mujCUZjU6UMXweAtfjVjctLBEPJD7QqdJoWSpUDUSkLX/D2MHIAnHODsNNGa+P7rBT4JT9od3pGaSq41DbwBJYqkbpcCtI8d0YLIQLfL/JMy6IAjrCVinhYBEJwxru9nrE2LJUAUJykd1+ak/fdc+Hd74eVapZlnhBBEBBCrNHUr1HmAzgAesfo+emf+AXuBd/+u7+yFv3sz/76reWzrT1v2NyhsFJApx5wtq9SnhqSoq9P4J8EgCRNyj6/51CrxPl4q8Epm3fL5xa3CqN3uqsvfP3rn//ch5v1/VSOO+oHPzosQN2DVk9uYuskxEripdVt6eXTE7foEUf26ocU7pfZ5TRrY8spo/7RE++rDXk7MEDbwdUHy8eXJq8kWUQ47XeSaJRmuQQA6wAQ2psCAhPsHAJwlHIhmGCMBWLscCMzZrTTPna0AIDBMOPMp6illHHGltBYBOnyNUnIBOXdOO43xqjwOcPouc88jYW82P/Dhv/hslcf2FFRFGWPRAkQwoxDjCAufEyLku8pa51SzgFnbK8qhQlt1srxKHIEl0olbHUsTVgWjOBcKnBoLCgzxp21WmbWOUEIGG00lQYAOcG57/u9/gADIgj1O6o+dudrZ+bwvcPeJsEOnCWUepxZhFSeMva++q4f++Tnpqcm//alF/ctW2svvJOUBveefPwW+ULCme1sY8Yft6QJMLWnbQsAIbk3BL649Vca2SwdPfP4Q7NjFa2MEP4eNka9+jE3MW16ZnFncKRZvwLQuNnR/vcxshQ2EVAfxkOYtuqCsVaCS0f9JB5NT/zMvg1vvTt1b9hRqdpc2aFHj95Tb95Gz9jrO7/1UcFwafSDbnT26Ex1EjiCKoCdPck6Ox7gaH1ra9AdgDOe4IUyDmOCjbHGaEMoJYTVy+U0T/wgqNXLzul2e3O6+aHleD6Xbx6ZOTmOxooJfWHtDMW8k0Rb2+vJUGrICA6a5QfbNRs2dnQGIKwsSGv21Djco+R3kyTzBbHaZFlCMcYYCU9gRhljhZQIY4IpWM04s0oqpRjDDhGDsNW20IZhhAlR2nicj+ICCLTb7VZrzPNEYZVUBiNkrIlGsdLaE57nc6V0pRIaDSoafuWP/89f+xe/ecc9eOqjz371//0DL2eUsqqUnFFrzGg0bIbjH8BFO3Hf4ztRsm/BIWy1yuIBdGvv2Rk/7D8B0Jr0MQB04VrzvYbyo8emDm8PXjl0ZGplvp3HqdJyc6d/7Mjhw9Ot40cn8dRw4pjPkAqaeyIJP8o0ZO8LD8IYhhauj8xmnPYxUJu340QbcmDdGwCoM4gJIsqMHj95P73dIcO3t2gyqM5UPuq5YyG8A1BaNMuCdJI003nYHSRJop2leZFYYyhj2lpprNGaUo0JKQWeCDxCGDg3NtuaPRZuLidx3pVoczgga6vX69WZJ47+8sOHbMf2NzZ2KmEtTcOF5bVqaWpzayQL0TpR0p3KZz70LyJYDWEWAJZXr0mpKBBKwA8CjBwm2AEMR5FSWivJCMWY+r5HMHYIG+ecVghj6xxYY41hQgiHlDapNKJU0cUIYaRlDgDWaK2KDABhoJQUudZEIeSPhl3tXL1SVcYqdXB1/Kd+8Ve+9pV/V8iiUa8LTvMij5O4OZEA3WP4uAM932ef+tj+jwTzxthsbV+dmwAHaNwy1uadqgWkVjn68CNb0FEnDx2xqpisd2empsfGG67q1uFaWCEIaakHe/pQ/xBgCCVsWYi7w11jlMPGIELLFPn6+uK1E8cO0IaZGp/Z6WxYovGRYz+8X7kElcPVUz6Mvbq2ubK2e+Haen8b54OAuxlBa5iAcyA4NdYi58BZzpi1Nk5yY53RWgjuB/7nfuonjnk/FmflQSIL6ZDD165fXt/cAHAM7pvCzzQaNaUyHpAH7v+QcXBp/mKcpK36LGVoYFfojQSBKWSBrEmTZDhKtAPrEGBsjDXWKSWJs3mUYIxKgUcINdb2+qO8yJMkKQd+WPK0MZQJQqnPRVj2OSWVaqVSLgOAH3hceEoqY02WpGmacS4IoQCoVAryXLa7fWMcYeyvvvznB16ovCisMVLJOB4lUWStiQeDmyt/pInN66256enbMvU+jN2aFvN2dPb+rGzNN4LqZL1ybXmp00+atVoYcGNyZfNa2CjxBkLBdn99KX8th7cAkoMO9aMga8PFnejCRu9clG8qJ5Upcl0grrwK7u1ePngnYpM86Yw6uNmsxal+v2MvZ9+43PvacvGNdXjh7a2V0J+QmVBJCckxbW0vnTfQA4uMtRhhAOdxIgRnjFkHCFypFCRZIRjzfPrGO997c+17o3hQ9WcEndPSjNfmms3GkvqLve86WpqMs7WdnY1ROnC28D2/uzPaXNsJqxM1fKQH6wDw9vx3dCEROIKxtU4bm+W5VtoYTfZU/pyjniCUEIKkzCnlXFAE2Bqb5CpTLstknmfG2EIrjhG2aej7lGJrzKg/JIwTJhglCGOCsRDcOpRlhSc4Z9RYhxGyVi9ePX33tRpFcX1sUltrtEnTtFAFAjzo/0jyi+/dF3r3IHtw18kQlgGggJ3FxcuXLl1c2tzu9eLdbn91e3dh6frCwvW0l9ZsxSTEKl9p2xtEXbcCcEvsc3DgYd8ffgseuDd8BjHE/YAJHxFsQAFxPABePvgpave2pmqTZugwIZAmBw8EV3e/f/X62U5nbWtj+fL8/Pr64vr21TgexSNqHKF+ro3Oo7KVgAHlRS7zIpdSKR2nuTFOCJbmudFKCB6WwktvLVybP9/pbm52zjkYeBX00COPMQaLV3cHcDqGKwjY3LETRY6KJKmVyUzLH/ZG3c1B4LUAoAakDy+cO/+y0so5kEpprRhBYG1aFHkSA9harYowJoLFcTqKsyROiyInziEMXHApC6ksoVRpJ4ucEYTA+J5nnCkKaYx1VmspLbgkLQihgMBZNTleE5xZCwQjwYk1kmKi7Z0kOQCohOVP/vhPG6XiJCry3AHChFrr9tOcfigmn/n4+6+8lMOLO/IiAADkVXgCAARMfPa534ASRYSVy2GtHHKKlbVJWlBF+ovDhSu7KicEeJSOhlGq3zOv9j7qtrJw6YeeWxvOzCcv1sLpk/Wn5sYfnpo63mxNCS9ADEXpwVT1YdbLcl0J6zRPs2bz4Cfm6tprWhda5yUfFXk/SwuVRtpJ4kApw0TgC9jttItUNeqVTrtjLGBMtSmMdc4ZQilYB+AQAuI5WjJayqMzD4zibqe743vhsdYx3aq9fPFrr5/r3nP8yLWkt7U5JCRr1GeySOfJYNjp9TeTy/DKmx/2DLs8PTUBma5XSlobDEwbnaYpxtRarMCpNPdDSinljBaF1kpPjzdHcSq1AWXAWc/30qSoVaqezwAhSlAaxVgEOpfI2Uo5sNYUUlJCEPfKAU/TBIzSWpbLXpymJd+L06IopFSGCeEkoIPqJrOH5qJhF5UCQblSqr271RxrlJof3DsJH9y6sofNZGm69CmPi/Pb33xo8sf3rzoyc7xzLTKJVNQVuRmlsXOoCmQYR7EP9z1cYYQZCGr+YXqDpltkoBygm5Ehw3B/AhdKB0tW7SE5s/A3VLBG6WgFpnzgBfK1ZyIeRXZAi4NDAUoExjQaSZxnKTnoBy53LlTK3nhzBhz0h6MgqPu+l8sYI+4F1UPjD7UqJ5KBtIUzEhjnmFBGKSa45Iuw5O1Nu1xI5RxkhTJYh5VwsAlby+2mPy5HeHVx/c0rb/QhmZk54RCdLX0oS7wkQr5fGw6Uw7lEVLCSc04V2fbqhcFGeO7FpLOeYNCc4kJpo60FpI1FhNZqdYzxcBSDQwjA9wTnvN0baee01giAgDPGeh7HyCHnCMGMMSbEXonRaCVlEZRLUmnhec1GzRM+IYQGYa8fFbKI48TutU4xPowiStmBRgYAj33kE1or5xAhdDjqK6WGg8HdJOG7cMc90AB3ejyV0hyAB4DuMDIAOHXquUESn7927fTZM1cXFnbavThJGSYUl37lC7/+9GOPhUGtGc5Ms+f3tP4MbG4NN/HtLPk9I8tgONAHDKnXo1eStOh1+0sb55fdBQPUQakACZpgysvVg/PAVFCHSb3ZwPagIQAALl4+PRzmHq8CuCzvbm/tVqvVsOYbWR52442tle2d61onWkdSqSwvwIFDLk1yKWWSZuAcQkgpTSkpcpmNUJmN97bSfrcze3hydmaCeunm5sYkHHmo9k/GGyfeuv6GlNg6ohRqNqaMCbu9gTGaEkIIHg6Ki2+vvfiN07kegc5lMur1h85IwSjCmBDEBa/V657nez7X2hVKaa200VIqTIgvOKa8KAopizQtkjTHlCptNCAAa7QhlBRFYSzmQUApY4xneWEsGAtZUWhjs0JFUcYpqVbK5cALw/eVnwEAShjzfCVllkSYUKkU2OwDtj/wGHfzDcsHKBffwPr6+tZWP8uyIkvTNLXaloUni2KUyvnLuy57ouE94Yp6cmNwjAkcLbHGIN/z1Yp9Thu0h8s7u9eHOgaAeF/QoBSfm/hExbt3c3vjzPlXNuWugsrS4tKgM3CF0fpgK+r0+jv9jRQNyCc/9enpqTnOb3ueNOit0dXd3Y3BaLcXbSOHojjxPT9Jdoe9lEFQqni1lid8kkRFZzkB64zWSmltHWdUW0MwDQKfMoox6Q9GEzMhLxPtJK/obmeYJIMCBoNBL0f5kbF7hmbz7Pl3alWvkEkSdXxRpgxJ1envFFE7K5e84UCuXds5+Xjlkz/xyO7VfpbJXLo8V7V6aLSllOdSIkwQxoQQo22SpFxwz/cq5YAgEpQCsDBMcqUsgGWeJzgnGOV5kSQx5yzNFRfCOaeU2utz1sYyIWr1RlEURZ4pCxMTE9Y6qSSldHz80KkH75wq6xZ2t9YYF9Ggp7T0/HJYLldLJcTEHayN/79w9p23Xvjrr42ipEzcZLNWD8NWo14tlaWxtNHa2lnaavcoLlfDIxPhXuqBA0CqF5M0qgfTAN5tDXleEcXbm7sLW92Va4vvdOPt8bGjBBDyOCGeF9SMsaOo2x9sYRa0t5cgc9gwVMDOxtrE5Ik7zu3tt17NTF/imDSq1aee/lgY3sazO33lO1vdBa36/X4XnOd5JQR0FK+miTWSlGpU+N4oWc/TeLhtumsRJ7gUiFGcE4o451obRokDEJwjjNK8OPFQY/aeStioWYw73W0i8jyVRFUlHiZk6/jEA4urS0XWkZnLsmLY3dYuRs50t2zUjcOgPOglvGLuf/Lojz3+pTffni8UKqR2VgtPaOswxoUyUZppbYTgnNFRnBKMwrJvHTiLBKfaOGuNAyBgq2EZIQTOUoIxQlIqymgUJeBs4AeUUkpAKRXHCfc8ipG1jmBUq4VGmzRJrTPOoceefBoOgoTL3Y00TRNjFMaYca/RqDNGqV+/GRD88Brfj4jNze0rV+ZXr15Li+LQ+JSR6eRYdXZyvBqWpTW0OV6dmm2Oz9x36r5DjVq7O0JANWYeIwCwG1+YaNzH76rZe1Crh7V+vsz8EiGMUp+WvDIpYyTiOPJ5mKWR0pk0uXUS44IAw4aY3OAMTRy6s6vg/Pm3MzMqVEF/9df/2fTUbbURA/LM5ReUSawbOsQ5LRuLHYqyLIv7IgyNsbrITG9YYKREGHmeVxKsKCTGaK8drVYOHEZS2lwq36eeYJT4pQBXw4nucKBMkUbEsV7St1GOK+XmVT0vC63Bcq4H29F0rYWtvHJ2NNjQGCHBxfR0zR9TFX8W4Bj2KsYOS+WAOKm1ssYZo6Wy0lhKqCw0Qo4xQinOc8kYNRbSNDPWWQeeL5xUSpu99mGtFecCXGoAeYJno4EzmnslRkBKhQkddDrOmTAMbZb22p16oxFWKsNBP8sOagfS7wKd4yC7vTbBmGBsrN3rae11O+NM0PI4gL67dvn3wPb60trGzkSjlqZFOD5xotYYD8tbY+X++rVEc8EhbE2I6aMz49PVeh0Lv96sDA3CiG6sbNTum8tNuyTmSnCgBioQqM/NPDzKBt3+yigaAYHJI5MeiLn6CQAYP3r4zOo3O8lVgrABYayWxurEkvxOnbF3z50r8lyp3Bqg9566s7h5+tzLPNA6tmV/SnB/kGwTPJB5gSwfbzWZF47VprrdlThpB77AhBKsldJpnhtjMN4j6SCEqFSZ1kYbU62EM0fLTz/ykA9PstbwjZcTzsPh0HGf+X55bfn6ysLWcJhhaxqN8d6KHm3uTt9ba28NZWw4IVIVvOpah6efe+oTAHD46LHu+jqjVDKGEEqzHCMwDiPntJYAXJs9CVObZTkCIZUliFkLzjmP09xCLpVXCnKpjLGtRiXF0B8lvu8bgovRQPilOE6kVI7wkuc756TUQvhFlhqjMUHlwCfkoOHPAkANgOXZ25x7hiBrLMEEEEaYnD175vFnP/6jiXH9ELz8g1eLLG1VKt1hfPLIrC/42auLnSRxfmN8ekZrCtihxkRzfHpueko62Mn7qhs1WxONoMoJ2uoOGJdJLlQwZGDu5gjlcCG3fYQCIFq7u</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8V5Rm13Ue+J10059D5dzVGY1u5EACJDIIigQlkkqUKFGSLWksLVkzaxRmPPaSZ/Qgrxnbs8ajsCzJsoKVGUSRFEgCBIgcG43Oobq6qrvyn8PNJ8xDdTeqA5IfZ+F7qv+ce8/d95xdO+8LfIgP8SE+xIf4EB/iQ3yID/EhPsSH+BAf4kN8iA/xIT7Eh/gQH+L/7yAfu+8BAhBKGBUEys14URjaliCUW5ZYXVkGZflcVisVx0kY+hcW57TWIIQRwiw+Pl0JwtDJUBhBaFooDFmeLZO0023uuKGaRDz2ZbuzJlPbtoQglTBdm5m6Sesk62VPnT6Tz+c2aitR0gC18tmsm3HiOChVimOj45Oj27/77SeOH1yhQCKVYNx2uFYmSRWlRHCWpMoSTGskUmmlCTGUEsEYE9xxXK3SKIoJoYRSGGNAOKe2ZXnZXL/bp5wU8vk4CtM4ErYtLKvT7jHBKTGwY2FbftScHL7po7c/sNy6wIh+88hTmVxpqDzb7q5G6VrQD6MwJYQYwzjLeq5jaGA0lTLJFQ2ocJ1iLlOC8tcbzZmp3VSYoM/OL56Ipbt0ekkninFGGStksoYijmJC6d5bRh556HNdP/r847+Spnp6wvn6d55YWXlTaal1MLPtYznPbW4snlp6sllfz2eGs+7Q9tmPVqojBGg1Fu+4+4cqObF5qL/2v/zPwl2zvGBpcVVBlYp7q4PDpeJMq3Xu2NG3rFyPY7S23i14ZHVjzfeTez/6E48/+uO//4f/+tTcG7Yo5PIDvW6979e1iTmj2tCR4X1+0G01FyzHGypVfT/x3MIv/OK/ufuejw4Wr2apMIFtgV7FZ3/x13/nOq7gNmUsmxHZXKbVapWLlWyhmMb9Nw4esm13fHTAD0K/5586eeSVF74tpQKBEIxb9sc/eWcQr7oFZVK3WC7dfc8jyxsXmEnHx8e97HwRGQuPPnPiTzfqS5XqwC27fualN/9qdHhHpTzAdOGVg0/evP+mNw691mzNQSS2yI6NzWi0t+/aPsO/BOC7r/9ff/d7L1MK30/yucxAJddodKNUW5zYltXv+7YlhHASrTvdUOvU45RRkyuV8/k8jOr3fG0MYzROtRDMdR3Xdrbv2XvmxInh0dHxseFTJ44TFRWKRTtbOn7i1NDgUJp2VbbBXBYm6/fd+8/v2PnJLtYklnpqY4p9EtANvHh64bXhys71jaXVlbOtVocxK18YJCzJuflGZ2l4MnHcQhpnpiZ2lGnmbONMPr9rStwX4Nx3X/uL5gZ5/cmzqY98LiOEGKoMcovX6nU3Y//L33zIxWPXCIIEAEABfmlEAc8ANwGVd5UgEfAm8AaQAP/TVXM9fPfkhcbtE7MJomaaDIsHAaxGi28efH5+/oTt5h+450vffOL3/GjezXJIu1DazonXap/itucJy2PlH3n8V95LhF0B7jhesVgmhMo0HB4Z6fe7xWI5k82OjIy89ebLpfJAsZDN5LJRmAhhnTt7AiCcM2OMEEIrE/v22OT2m297cP7cUdsG5dzw9QvnNjKO12qn624QpV+tbUhDZbcbddOzD976zyOsJ7H4/gtfm5wZOnXmtYmx3PTE/vVWvduO12tnPnHfAzF8oA6UhwanstkjMEqmhjKSJJJQlvGsnGsbYhilURRCS055xhVJYiqVIoOmlk0IkQr5Ql6mKePMlshkvXKpmCsUjDZCsCjwC4XCyMhQu7YGQzqtpsWZbQtqRCc2uRLjrjN3/gnmqE6jvv/m3VPsk5vnXcE9d0/fA2Amh/7sm68deW5544jCBaMsQvLVqp3LZg304IRz5PAhy+LTU9vqG8emxj4GxK1mo9c0O/YOBzVNYXPG3IznOlbf7xcGHBez1zsgC1gGxraMMODB93GyDlADRgAA3wI+uXUuh2q2cA6oWCgPCxeQAHedtBusBfFKs7Py1At/GMglZlM3azNtuYKNju6xvfbdB/ZHUXxi/twHYjIA7Ke+9HOe44KQXM51XNsPAmJ0ZXDIqHRhccmy7XK5IFPV73UX5s8cfeslxojW2oA4lmCMaPiz+4aKIzmZmspQ9ZVXnqSKh520vrHiS//jOx/JZJfaoZieuqdcnNpZeJjDdTCQ4c7ebW65zFfqK/fseWi0tG/HqFuL11IVDY5sM5T1cDoP9uapVxeP1kCISlOA+mHiuZbj2oxAa0Iokam0bUtqIiCFJfL5HBiTUsVxlM1kBgaqSknXdQcqJT+M9x/YX6wMKKlCvxdGwdjkdKFQbNQ3XMdxHDuIEs6Ym6WDe0gmWwzDTtYqWqjcd8sXPUxs6PMZUriGBUZmhnasdo/eecfnpyfHVzaOjW0XUrFqNe8QnSsOZfIqn7GG8nsc7BUYtbJuvXVSB25jI2aM2ZbtOI42Jk6SfXcVMmNRFg5QvuaM8h/0UAEAq8BZYAjYDdQ0XiK4acvsiLKXs7gLWAYGAAqg1j+4sro0f3ZFSyRJDJJQQYpZO+fmPvvov9o2PD2zbaTq5Rnha7XO9slbPxA1nFFCmTAqqlaH2p1WxnVyubLr8NWVVdvxbEs4jud3N8IoPH70oFJKCEtrxShVRkMTZqexXtrYSIYr93Q7yyqOgm4mCGI4bdm1jrWPA9kH9/z0Nc89B8AFxmccIA9MA9tu3lNj+JTAeQe6h1oLLwXdwHVtpVQcCi541nKExbRUGtCgShkFqsAsixtIbtlRksaJzGYcz8kwTm1LVAeqnU5XKu37Pcvx5k6fZlyMT07WN9b6nbbWMgyjXC6fyea8jp9K5Qo6MXpLq7M+wIb37NneWEv6aGdRHKST19u9N1pYevSmXwKGgXoYfe/M8e70jvIIhhiqeafsYhI4A9y/ebXDRpJQ1DY6QShdy+VCcMa6vR5gdh0YHAIH6sD293FqCmDvdc08sB1YBWaAmQb+bADfBH4AQA3fG8D9BH1gqYuT+UtydCh7w9RYdOjNE8Qk5bzTCaNcVhjDm/3OP738lcfv+qyH7QBq9e/0uvH7IPIKUIBJmeTz2UQGBGCUlyoVGNrp9hiluXxGpsr3++cX5tZXzzm2MFoTQiklAIzRjNgOH4hkc722uLqyWiwM5ctuZSxXHuZuTnOhG+25Fk5cepxReCnC3wJv+DgG3LEz9wlgenMuRel884QPBpRzyCSI4oAmSRIGEePCsoSUSitttE6UqjW69XY/Sg3dNPO1JJQoBUqJY1uVStl13U63xxjNZDwhaDGXk2kShn6zvjG1bfvYxPTk9HQhnwPg+742mnNOjQr98Nipp6sDbMf0ndPluz+69xNZFAGsJyffOP/ni9GRrXs3F5wu4TFgGABQHR6688FbfyZj3SCwO4Y00MA4tmjD5597stcJbYtxDg2jpAagtSlWs8PWXuDWS8Js+b1OrfU+rvkosAP4FADg+x0sbmANWAKODOABQNebDuCudNoAApwDYGFk1+xdOc9m3JqdusWx8jft/sJNu35KJm69+cLBuT8DzgOYGJ7K5fJvzB178dTR96LhbbAv/ewvWFwXCp7vRwTScQswSRTF7U6XC5Zx7Sjw67WNN197rtdrAYQQAkAbcM4AIixrdKJMrLi23GKUTGybEY4oVHIQTdtO15cD24k60enx3P0AQjzN0F1WCz5Nl5aj4XwIsEvGx/qxCy+AWL4vq9mZHqxzqxe4cS+camkFL+MKzvpBYnQaRWkYyUTqOFGc0ySKKTWMMspFxnMznpckKWPMGNNqdRijggutdda1fT+QaQqjCONLF5ZmZme1Vu1GjQuRK1a67U51oCJckimzTr8/Ur3h5LljhSHXRfapt/7g/NIL7d5qsVo7dPq5Pjk1lLkZQEjm8/SGy1s5XtxnYbTM9wHjDRw93z2Yt4VABIxuXvDyoa81mhsW8fqdWKZKKamViWVaHXVH985ksO+SaX9ZUR4HBq53ak1g/HrjZ650DmwAG/iyhBzF9gwGgBuBPCAAOujuAbyqsx/ARtzN8yKA1459O00DTtPljebwwIzSNE7bkfI5kUlMG/7G8eUnz6/PrTf6nJfu23/HB+CzL37xi+VKzraznXYrjhPLdlwnu7KymqSRI4Q2uttuzp05eebEm2mSAAQEhFDGCaeMMBqHaa5QHB7f3es3kyCd3X57qTIeJcszU4ONehLF2vXSbVOzFs5x9AXupdhZon5DzZ06sdw3muUyFllhaAGlTry4ujI/NDTF7BqAbbmf2zZ29/Pff0rKNOfaXPAoSRkjnV5ACcvlM44t0lSWSkXGmGVzKbXrWkIwgArOpUxlEluC+X7kcmPbtt9tMm4XS8ViqXDy2HFD0Go2lEyIMZxbSsrxicmh0Yn7735gdHJbK1qw7Wg69xCQ9emxdnetuebHSVguVKuVoeXua9J9g9JiFjuuu61Z7O2Lt4aICxSABuAB1vef//65Y2thTyuptJKGGMGYXTJD2zjPyGFvAvCuXEYCuWvWXgYSoHQ9JpsFyKWfatPq4vAyuBOoAMcAAXBAbrLgZTz9+l8w2z63MX/3rkcO7L7nzRPP1lrnQbxm48Ja63DW1UbGftRrddsEA4ak+/b+0F07b37/TAaAauV7nmuMadTWZ2Z3VsolMG7bDqU0k8loTRv1xtypwwTKgFBKYIwxCgbaGAqAYuqGyoN3fKo6NKWRHjv55IlTr0a9MEOHc4XBW+8sFfM7hjHuYDLFAvBl4FsdLC4srVokt3yhWd/wLdzTgAQuZHLuzOid5dwYMLHarm3SF6eJ0brXD4IwklIlSZrLeLmc59ksTZUxOggjQ6jt5gEThpGUmnMGGBjDOKOUCQZtdLfXt4Q1PTvrZvOdds/L2J1m3bJFGMac80ajHkYRISSOzFK372Ik6tf3jM4AClClSoES0e9Fsj9kW5VJ58bp8s2DeGT4UhhiGYdqOH7lxjZkigbW17EAhDV8GVjttdrQjBiilFRaaaWVQS6b+8F7/+2B6s8AVSAGDAAgAQ4Dp4HFa45sDNh2vaPcgSuCVhcNOBvTr2/8Z+ACsA2IgcpG/MJVd37mrl/eMTB928xHAEikd962f3bb4NrG8V5YFyQjU8UsxgWKJQHaKpcG9w5fl4B3A88XC7btuo67fcfOpYW5sckZqSRlzLYYoSzod9fWVzqN1TRVhBBGCQhXSmmthRCMEiKoNKvL+pszU1WZ1OrN2p7dH7EsHWtz29h9AnsLA4cYPgIkx2tLNw6EFLdHJqzkxmt91V3vKqsB0G6XV/JTZdcyrplbOJXLOb1Ao7gMWIwSavGgH2pJBTUGzBI8Ubrfi+M4FZbFOUtTaVsM2YztOIV8ttVqa0oJJflczqiYcsfycjBGcMott7a4mMvlQGgmlyuVBlaXlnKFclTfSKJwfn4+Vym5LTWeHyCm+NbSQRkfHxu5rdvzBK8OTfmVIXny5BuN7smZmdtnnIueQYjlsbdduWUgBrYBlQyfNnhuCPuAzwzgNgDl4vgKWUtVSgwAkqQqiuOwZS7dO7+FgSxgP3Dqss69EkeBfVt+JoB15ayNtwXtkdsGZ4AycB64E2h4tgVsAINXrnnRm+4kywe2379Wb9c2/P37Hq8WqmcWv2dUaFueIyxbiLXm6gdlMgDUy3hgrFGvra4ub9+xq1gsapW0Gyuh32+3Wq1mfWnhpIEhBFprKRUhhFKaJFJqBUI8x7Wt8vmzTUpK+3Z/emgkt3fkluHK9sNHDgrcBnglfGRz4yoDA68vrQCsRLbvKH9qoHzDjp037S//PIDzF84ApdXe+cXa8Runb+9H6o6JnwLGgAGlNGPEdixjoKVkFEGUSglDeSbjZBwrjhNKQQlSqR3byWQyhUKOcWoM0lRKBRAipVRa15vdKA4YIUG/6zqi224HYRDGiltOoVAwhNQ2aozwA1MPA+O3zvz0DeOP3jr7+KR3D4W846bH773nB5KUpqpfGSJB0JY4rfA1iaPuFcGtMWDkrfW/O9n8ZqcdzdfD49FJjf7mXK8bwmijlYYhhHHOlUqVunzvMHAYqG1ZbRcgrjyvBWARWLpy8Kpr9m1hsiZwI3ArMALcCQB41sPENUz2NqrWdorxfHY8m2FrtdfmFt+EFA4rDxSmpyp7Ol3C6Xu6ulejD3DbyeayxfrKyqkTp2+65c4g6Kdp0us0hkanautr66tL3dYa5yyMobVWhDCtQQyjhBBKCKGM7t3xcGGQONiTQa44eI5iJI+Rm/f9+FUPG8fH6rr/6sLXpqe35zE7MTJ+bml+c+qG3bdqqKQf3zjywwBuHpu4fJdSkmgjbNtECbQyksSp0UYBxuI8BRHUJFHUbTeE5fhhwLpUJakQzHVdEMRh3O33KaWWZflBUNuoR3GUy2a1UVqpsN+dmJx0PK/RahmlwqDf7XYAq40jRdzo4aIJsnfo0wApkJ3ODSLw65Xy/grG5+ODjr1qcGHqCtGyBqwcGBo52T8YNGjQHe2iv0L+ww07bv/e088tLZ7jnFMCaFDOZZIITrOlyxLLA4rAuUu2f+96xtk0AGDqykECSGAJKGzabRpHKKYBBrwJZIEsQIHNDFH/xaNP3LPPALuuxxKdTcH20X0/tHD+qEyCbnDhrv0fafmLh868OtYZqORJaH1gpZkFOIxwbWfvjTdPTE7nc7mllb6byVJqt5pNIfj66qKSKYghIKnUnmcTwBgQAkqIMUbR1MqQDOBC1/HqIG7bXHqIXec1bpp8OyrtAKXxO4D2Sn/59MLrnD1zz54fu+r6//c//XvPsR3H6fV6BDDcTrXKZT2lEUUJZUxrQ41i3NaGUAKjVLPZzHlukihQls1kCeFhkmitgzAkhPTadRjAaM914zjmwtqza+/8/JlGo2lZLjHtRqNxbPGpVLdumtkBOACAlcvKq4hSIT87js8DmLA9FzsvK6ynD37j+WefcBzniz//gx51d2cfQnYvEAMWQM7jd7qdJqVUK6VgGLc4oSnZDMqkW954ErgcqNs01Q8DWiFmF6XRO6EFOMA54FUDp4d+ATcC64AHnAW+AADoARmgks91V/ovF7MbHu69Zp23Y9GE5LbPfsSxHEPOFgulserAxOjoHXsfme+dfVdKrg/eqq1NjI3allWtVsMwzOULrm199L4Hm+srURw2aqvKGCkNIUZwCmO4EFJJEEIJKOMG6o3jf3rgpo/Pio9DJ5IWODSuzqK+C4q1xvELS8cmx2ZX8PQofuCKzatfEIKFUWRkqkEpI8qQVGpK6VC1QChbXatBp5bletmswykoI9RJ0zjo9XOFQiq1LTijzA9CbWC0DoKwWilRSjjn7XZHG5KmSa/bNUo6+Zxlu4ToylDJ6FLNvCnJkRHsBiiwBmwH1lfS9Z27LqokF/sBpMBf/tXfvPzSy/NzJ1SqKCPPfON4qVT+pV/7tbv347JbV8LDQfcPNlWAAbEsSyvNGWOMpXE9wksO7t764nV8o4o7gEFgP9BjWAC6W+IddaAO7AYQ40UbZWA3cAbQDYQVDBbwcQBABRBbGPfkJt/bzKtmqxYy734wX3jsVw1AgOdf77ZbZ3NOOZQJwLflqu/7cN8GHRwcS+MgSZIgjHq9fiGXcR2R89ypmdnVtbUw6FqWkFJLaQglcaq01oRQLgQlJEpSx83Ojj8yK2aAkNDzC+3Dr59/5QNRMDo1ECWdheWTRw6/BbQBeXkqjWNtjCeYIYRTwhiLE2lUagkulZIyzXu2Y1vZjCOErQz1w8hoSQlzHItQMIIoSaRU7W4/DFPbdRzbCYIQMJQQx8sGQSCVYYxlspler8/szNTszLBzy4h3i5+0LTBgJzAJtDaTFqFsDJH9l8lr9PFTP/nFP/uTPzp+9K0oiKRM0jhOUun74X/7o/+29R1zuDXujMFoSpnrZbVUjFFKiTbwPFfDBTa2Xl/Fp7aYULlLca+tGAbqwLwNARCgBviAV8EIcDmkx4EC0L1k8+0BxoCHdo3fbOE2YBvwHhb9ZoxkbOJWbeXPrh5vtVvPH/tKiv8uPqsMDjNuaa3iKLRs1yh1OQJz330PUSHSOCUEluC2JThjUmmltCOE1Eqmym8lz33j2KuLb51XfzWAge3Fe2+bvBvA11//z3O9Zy+tpK777E3YWJsYnd2/69FH9/+vQLGJy2JZAiZNleAilQaMxonkjDq2ZXFCCJXKGGOynuc6FqDiJJapjGNp2bahLOO6UZKEQaRhchlXCCoTSRgxxnQ6nWaj0e/1/U7z4Ksvrq2tp3FCoSkVDz30wwBeOvfnQ3augp8DhgErxmvAQUDOuru2WtB/8V//HyuqTxetqsc4McQQADJNA7934fyZq14zjlcZpa7npUkMgFJCGROMOVmRoBPjjQ9yai3AA6rANuBWYBcwANwEZIDCJWWyCFwAGLDnksFnAzMAgAwwB0TAhXd6wJn1k5f/nhkafPzjP9XtRvWN9uJC46vf+9MPQupFUL/fZExoJWFosZAV4m1v4vDJOUYpF4xzJizGGeOMcs4MjDYaILYQRpkjr544d6I+wfKvX3ht88Y2Tnzitp/PZ/a2cRSIgOBdKMhjfNvUgZtmPgIglIktPaAO4IkXf9+AOJYltQIIISxJUtuxEgWpjOc6SkMRi3t5yqglLFuwYjHrOI4fRlJq3w/TVEap5NwigJKKEMooCYKg3/fjVCVJkstnCUwUBEor17YnJ0YcOwPg7pkvum+bycMh7BpeBBaB2wE08ToA4PxYNbn3wOyDt+385F27D8xUBYMxxmillEri8Gd/7n+4/I5ff/F3R7cz2/PSJE6SlBIQAsY4AcJYF/Fx+zoVQe+CHevpJh+vAD2gDawAACoS6wYvAy8DLWDiyrs23VIfCJ579Ui9f7SV1DZTSddidKj65Bvf2DoS+XJ9tbW23KqtNP7sm//u0MrBD0IwOIwyRnue1/MjsmXiK9/63deeOaS1ZowZDcKo1qk2BgRKGc00F4IyZgySVDVqHYPteyY2q1BQxB4AqZY5WgGcSwb1FXj5yN/WOqcmZ8cOjPz0zoHN/zO43LrQOJ+p7NpQf336zfMgxPdDziiB8f3QdW3bshijMpXrG/UgUrl8JkmlUjoMY5mk+XzWjyPHEkIIUKrjJAhCizNLWEkaJEmcJhZNQ8JFvd7M53NxIovlKmGW1lrGvu9v/X8YCLGkgVcOf51q49ou29MuA0CSQQqcBC5Ux9LOOSc1tFjM3brb6QXxYq0HwhyLZVw7iX0AHVP74z/4P7gTxz7TSRInscUtx3U4p6mUjJLJHddG9t8bQ+KGWJ2TbD6DIhBvqs4QBzWGe7I7xLPkSkt3CzLAgVv3r65cWFZEl7bPbzHgAHQWum9O5+/LoHrL/o9tvY0z1vPDVJtOH2FCvv/MP970hVveP8HcsjyjVJwS13Uvj87Nn3jt+beiKNTKUAbGKaMk5UwnUkpJCbUsy8s4caLjJAHhrz1/KpV/X87M/OiPfNGCBaCN82P84gu8fvQrt+377NanXohe2ajNLZ6ru2zytdUXpnZag9kDgAvAK9mnF5965funN853pIRjMWFZJowJoRnP7fth1rMdi8WJUDqlMI7F0lSlcezYdjbrWbYygJY6m/HSOLQFS6XM5XJTM7OL5+bqtUbR0ZlM0dAkk/EYt8IgTNPUte0UbrvTWVtvDA9dTBG6GAdgu81Y9pq93pn5WnP5Bb9lHv7UXTYlALUsZ63WAPjoYKlS8B65c98Lh8+Csp1jlaFS8eVT67/xm7+e8VLuJZUqaW/0e/2AEJroVGntMJtROjqbG5xiwFlAAduBt4D3m8+x2YyNmS1B2rdcpOfDC0KU3pnJLsJzyoVSdOiNhfGSzlxRLlmYzt+3+VdZXGERbpupnJ5bSCOZEhbL9tTwdavl3hHsX/zSL5VK5SAMLEtwdtFP/Mu/+KPVlQWjIRgxWspUMsEoJYRAKh3GspDLCEtEUZykxhJMJ7S52vZbzb4+LcpRxd3mbPGQRwf3XPXUAh8/sfh0fSNcPruwdOYYpa6y2+XcNCA90l3sHjr++nLgG8cSxBhCudQmkYoYqY1hjKcShDJGaSHrZh3hOHaUJLbluJ6TSmXbVhSljs2J0alGlKRK6dGxiZGREUBlsoXq0KBSspDNKG38fqffD5lgAFNpev9Dn7iK1MnKtpmB3TvG2Hhp7/RUZqPdev7JcwsrayljTDtpze+HSbVYyHnO8EBp++TYjm0TlazNQGrNNvE8L2M6zbjb6S2dacVBbFlWLpfJZjzOWWXI+YV/9vBQ5nNAGVgHBi+VJb4HOmg5uCwULts5w0CxIEoWpfz6iamtGMt4bteft2wvm+NAqYf1s7WjA5nrpOclzLe+/zt37JvgjHUbXQjv0Qd+bv+Nd2X5e3isW8F+49d/jXILMFnvonabX1h87oXvfepzPyil3232BCVxmmzG5QmhhFDBKAi4EGEYS6lyuUwhn2WMP/aZn/qBh36y4m4DsOLP5axrS/behiikrpuvX1irFKr779hXHUsd7ARiQM7VjqyfVZDgnBmlw1T5QWQJJpPEy2U7nZ7vRxwqn88OFjPGGKkVI0xYzBKW7dgylQaghEpDev1ocmrK89zAD3K5fOh3E6ld26KUxUmqw3R0YCBIoiRVfr8fxdFHP/bwNZTmgUGgCOQYzLbxz9968z17d95WKI3U5mtFAmESnQacE0vQTDZXLlYotB+r7OjMw594jCgsLy+fPrJAlOaMutnc8PBQIZexHOfzP/1I1r5nS0H2+z22LUy2CQU0gAxQBsoc27dk098FxZIXFauFNF1txoePnnn1wPStDIUe2kuN02VvCMA/vPgfa93W4ePfXVg5fePuPbfs3X/kzFyuVPIy5Rsmb6FADc+u9F6v2Hvf82E8ny/2w6CYf7ud4Knvfeu3//f/ACBOe8feOCGYJiBxktiWSFLlOkIbbrSBMUmqBGee68SpNKAP3nf/5UVGM+9RrzdbeiiuPrNSXkqVv9o6l6nshQcfhyTaWduLgtp3PaQAACAASURBVGVtjEqVJTiRqRDcaMUoTeOUUGIJKg3NZhwv41Gg0WjBSEKE70elcoG7tjGGcZbP5Gr1Ti6XtwRbOn9uYa7nOlYUhmvriWWJOJZlIQSD57pRHPtJlOh3oXdT0rwdfXBJ6eY7P/Ls/DlIRYzsdFpKJtwPs5nYcTLT+3dvv2G/lRvas++Wz3z+S2+88vTf/PWfh0En61me57qOBW4N5x7Ysv5163/eJxgwAGhg9XJx7PuBk5cqDoVdHhDVtWzv4JkXO62navVmmMT5zxRbtflmY77ZvFAt7SkWBubXVzc6zfJgeWZkdm7pJMenF8NX+/5yFHevk7a4BjyOk0wmZ1sXidtoNUmhvfn3/Kl5IZhOU86INhCCJVJySv0o0prYDmzbIgCh1BiZKYjDtSf3Dzz0/rfH76+3mrVdB267Z/8XAAWcafZ6yqL5wihwijLm+6GUXBuTprLX83NZlxoTJzLrORQkjNJOL7AYY8JxLctxXD+IZJoarbWSjLlTM7PnFpYWF+bHRkcybibHmU2l5aIbSiO4bfF+0M90rDTRxphUQyrzXiTfCrwO5AAF7KWsdN9P/vLf/e5vW8bxLB5FYbvR0byw7557KpO7twqVW++8/9Y77/+9//u3Dh87XCpXGYyTVV21nmdD7/q4ZyNkHWw1t5e2VJ6FuEKw0SvbCN4P7mD0EFAAhnZOxOutzJ07bjxXPzNT3XFw4buraydnJu/LZLO3zz46v/r6iblv1kUyOJznttIybcb+qWMnvHy/Ui4C7UtJrXcEjZJU8LdjGYOl/IOPXxSDS2dXjNZRItNUcUql1hnHoZxSyigBDChjhLEgjArlsZ/5lV8dHLiOX/lO+MM/+/0n/uHZMJWPPLCZFWHAjmxuetr+xGz+ccE9LVWapv1+EIRRFKdKGz+IlDZaqzCMiVFRnHb9KNYAZZbleJlsvpCPoqhcrlarVSnTI28dJEaNjo3EUeRyvra+fnrubL/VHipkh/JZwbmfSs+2KxnHGFKqVD3XAV68RKACaoAE3tpKdh+vARtAAzi9OdLuq1aog8SAWtzN773to5XJPdfVXP/iV/8323a1SrVWSgbPfPMr77pDx4CPXclkuLK88fT73+1r0AEAZCBuBgaA2CYTk+Ubz228MVPdAYASe3L85vsOfG7nzA4Ah098r91rZnhBBsmp+ZOpah06+fVSaZhz3msqIHzP51EDQq/YEz4oprtY36idznieNsRzbW1gCcYIJZSBEM6YsATjrNftw8hWuzM0Pj4zduPwOxT9XRenjh3ut4JMIa/wthQpYReA109+TSVagzAuCGNKG1sIyxJao9cPhgcrSspWtxdGabPttzt9A1DGmo16u9X1w7jZ7vi+D0CmkhCysHCh3ezkhTMxUNo2OcmpXV9bjdrN8UJm+9hoPl8s5zKcklKxVKxUcbG6BMBhYADgwIGtZGfxEeBeYBbYuTmyc/+O5mp9db3WS3Dn/Y/N3rjZoJFcb/f5Iw9/kgv3E5/5glPIMLv94mt/8s47dMM7T23i3dT8e+Gyl+YBElgDfAAzgxe7S26a+tiN4/dodBZXD9XTZzMeHyuPRWmyZ/QGW1iE44EDP3777KPbp26fHJy6pjzzOuAUSvDLGj0CHBnns/ZQfmDo1o88Wl//E5nqMEoswRIpLcsQwpXWrutIqYRFGeM6SjTrOuDAu2uBK7Bn7y2R3/qlX/j1q8YvdJ8mcTaKkzSVQZQ4gidacSEopeBGME4pczNuEssgigSjuaynter3Q05RKGQJZUkU9Xody7Is20landgPWCG32tjI2bzZqBmjK6VCxrE9goHBkoYyUtnQgEniaAsh7xRf2GS7zcx6Ahzf/9iOlfNrrmffdc/Hh2cu124IyBaID2YDzmYfBoAf+MxPrDX+3ey26fkLk28dfLFS7kr65Y/dehcwB0xdbpW4Btc2nviAADYAiv+uRNAW1FdryyMDM0DtKjNx3T88NTqcJ0Oe+2qzubJzxy2lbHnf5O5TKxcLk6rsFhQNsLo1Ab+SvhBEvWpuyoHnXCotIRu15kD1Yqjwqno5AL/yiz9GkW7U2rZNGWMghHMqpRZCRElqWyJOpOVYv/E7/35b5YMFVAAsXliYmpi+/PNY6zszpXEbuUZT/pff/U+JNL2en0SRoFQZTYUVx1LJhBGA8jhVMpXVSnF4oBiFKaW0UMhyTuuNrjFSxjG3LcZEEMaMUUpZ3hI2UlvQJI5tSwxXqjnPMZQawmyL1tu9lp/Ug+Rf/uZvAwBOXxZXV+IlXJnw3oIA4FfuX7IpJIDilWq089yRr9XPnzt8aGHbruFcIV/ODX/srp99l41a108M0U9cWQjZBGpAGei9Q3nt+8dRIAUkIK98uzcBF6DfeePrfntpIGfvnnlIaTpUGoFhsLfW49Tfk9e5syU8exWTdVJYDEoBxhCAEEMZd2wrRBwnUisjlRaCUcqS8F0s6Gu59yL8pLf15w2lR4AmUO60T2pttJJhlNhccAYtSRwlfhC4QoARAqKUpoxTSuK+70cym7HbnTYXdibjGi2ZZzNuaQIhxNDo6Oryagrd8yPSiXvd3kApl3UzjsUIY2EchL5pN5qMst1DlY2FFwanKwbnCMavpw7eiclw6eLQBG3COOwc4AAWYABzJZ8V7r3xp48X/7bTkffct/fs2Vbgv4d9k6MAngC2+qcxMAQUAX1NI/EHxZjBSYKBq8rdUtC+Xn3+1eeXl1cde2h4dNdCZ2HX+DQEQK7yMK/ubL0WNI56cZJcd+7oG69WygWpwAUFIQDljIIgilLPFpSRTs8nhPp++I2vfvmqe/tYAhDjzMnOt667+MEjb+6dvfGa4TIAmRAYLRPp2NwW1LEtqYwfRCCcUggmQClnzHXEZtlPEMWpVJSxvh/GUZQmUhNOBU9T6QdBKjVAKcFgdXDv9l379+waGhgylARxEsRRt9fdaDTWNxqe6zqMnnzu5ef+8p9e+fKZw0/9/fLp7wLdS4RtphHfEy7xMv1OK2xcWJ1/tbl8DPABClz9f7h34ke+9IV/G0X20MgwE/jKt//Pd1nUu0jAOgDAB14C2kAWADAEtN4HYe+CEoEEFoHlSwIYADgqh8++aghmxnfu2XPP3Xt+TMbUiADEvcY0fG9LkRutbMt66+jRA/v2XTU3Ojna7QVJHBljCCFpqoQQ2hhOWSxlHKdBEBZz2Wwm88M/fkX1bIIlgzhCJ0i9xnrrVPK9XQPbr8yj4ZYb38kASt949RkllYaJE5kYo/1YCO4IqrThjBUK2V6Q9PuBbXFGoSk1QLPTLxE020G/3XJdZ3h0GAYG4FyUi8Veu020YRZf63XX1ldVmoRhrJJAEDJYLhJCw34Qx3EQCWPAOQsj0m0HGxfWT750iHFBCQUllmVZ2cIt934C7mUf/rqVdvlsKUnDIE2TxYX53uvPUsLz+UImW9i56wae2+owsj3jty1ET7c6jdNzGy8e+puP3PSj73RMGwg8HM9iAqBAAowB5wEXCN+hMnYrVoChd24tDoABIAA0sH5ZC2vkp4Y+PbVj+6Glf0r1xpo8RGzq93i+6F91lO+jaRns13/zXzmu+yd//Hv33nvf1okF89WFk/OHXjhIobXSSmullRDCsoQleJqkiVSUUmXMvpvve+yBK8oNnjn5x2cXTjql7qi9a7JyV617RjvNLDsP5LYqo9/7/X+TmWgMZK+IJj955D8efPqElDIIkziRAE1TKaXyXIcS5DO247oa1PfDjGvbFudcBGGkjSKgBmSzY971XNsWgnMDumvnjlq9nkQR4yJfKDIKy3JzhVy2UFjeaLX8SFG71fP7hrUi+YNf+lk/IQvzZ/r9fiJlKmUcx2ESR3GcpjIJw1iqgfEpgEIFkEHit5ntXR3FYGLp3OlTJ4/OnTwWBKFlublsoZAvUQon717Z0+YU+YBbMcJtaammRu669oRq6ruCVvP4hIUxQAACKAB5IAT4ZvH9u3p8akux0CYiwAAM6AAOIICzAKIQnLsgF7M4FHbRHiBgI/ndo4XdOTpWLg/2wlUT9lx35pItNA/0rtfkdzV4tVx64+BrKyvzV02cv3Dw7GLDczkUSZXWUjFKpFZamSSVluC2oSApoXTX7isE4etrX19eXikXSu3wSOJOWLglIcH6Oifj9iB6lxtZn3zhb1rttfWNzN7Ndm6YueAbxG7ULnSCIEyilHLGKaWUWJ7d7wdxQi1KLdvq9PwoMYSQIIyyDg+ROo5NqZPLZKI4kcqSSq2sbMzOTjqOu7bRPH7sWBJFtusGQZjxHEiZL+TjJFJpOjk9HceRkqqnSA7i4YcfKw5sv+OB7Xc88DiA8/NHX3zqifXzZ4iGbVuOZdmum5w+Nr1jj1segFZRv+8HPXTbtmNRxmq1+oXFc+tr636vGYVdz83s3rPfcbxSdciyLNeyHNdFGkNsNW4cYGqQT+X2Dhj0QjzlXv2NlpWsqVgXnd/LlnQJaAErgCOxwpG+87eDGoB1peEVAl1AAmOXNC/aod8PWnZSqKn1ifHr+HOr0Xya6sHcRBg1B6ujwOql7zPoa2Tb9cEBDI6PGCP/699+40s/8qnLE+XCYGujZltcxooQUIok0UyqVCljkGpNKXNdbgnR6l7Bo93ehuuSoUlTLAx18NZq6+jJuVNZVh0q3wHPruOvq/hsgre8DBNO9v79v9LAsQpuAEjR42sdw2mWUSpsy3McP4wpJZ7j9Nr9xKRWxokSlURRqjY/ZiaU0USljFEtFYxxHItx1w+SIPDDMHEdx/PcdqsltTLaSqJoZWW14NmUghDGOaQOM9mCSiMhmrWNjfPnVrdWzE9u2ze5bR+Ac+e/HfcLtZXW3JHX106dGt9xcuduEkVhFPpRGKysLOTyZT8I67WNTrut0khLXR0YqZarxdLQ5OSEVNqACMEFtyGu7xK5qAJe02wY8h0Pu4FJIAUEMOrya9PEIVACxgCfY/TKsiu9nD4xJi73YdiXmQkAIIE+ULyk6U5s9uelKenVWL7qDYxcXwVXHRY7pTi+UHFdFdiwJNxNm2H6utdfCwpgYnB8aGzqrVe+vnViX+FuzypXygXL5pxRo8E4NcYoKbWGUtAGruvlc15xyADo4pmLK1pzk9OF7YPjeRZnkaNMESPStqzPtV489K1GOz6+/A0LI0FL5/MVwHWQAfDm3BuvvTr/0rOH6rUW54Ixxjl3LJFz7ELWLeZcpVW7F0RhYnHh2ILACMG1QRylzEhiVLvT6fX66+uNbqdNKWGU9vqBEFxYAkAYRowLpYzhdjeI4ygkBBnPCaOUMjE1PmZbaDca192jmclHd++9696HHvuZ//Ffj+264cTJE77v+363trG6snK+78fNTq/daoW+b7QCUK5Us7lSvlDNZjPasFKp7LmuATGXNvwaRMAOoFQmXt3vLCevSrwArF2abV5z/aYbOwoowKRYAC7XyrcIiYC1SzXMl5ls9ZKGtQH7UvJ+32ZSgdKsS518dRwo41IX4JXP257DYNHek6PV1QsdnSokc4C/pQjgPcB+67d+C8COvTc/8+RXN7rm5n2bYWgFjJ08etxvbzCjozT1g5gQsukHSKkMYAizLGtgsLjn7tJkZTLA2VPtb8zXv6ti0axFCXQvbbZUT8YKkp4+sTo3t2QVwvY6zWZKqwuNV19+qdVcr/XOcEaefPpbzz/9j4kJRkYyaRfdJrKOTYgxqXI9x7WtOIr8SCZxJDhzsx6lzGjDOHNtO4xSSkApUaDamE7PtzhzHWdkZAgGzVaHc0YpBaGMWSDUEiyVysAorWAYF5xR6jiO3+vX6muPffpz77JZbx56th0G+/beYlm01Wq0W+1Wq9Pp9hzPk3ES9HvcsiilnpcdHZ0oVcrZbN4SwvKy3LYYYcaAGQmRvWZhCQjAAZYTlhptF/goMJvi+dXoWJ5nr1SLKcCBGOhKnO5gJUTiwWuoOY+WFqPnStaodbF9Zityl9zSTR0aXWKROlCXIkx9nXfd+tq8naf0+vbWAtAwOqzXNsBSk9hW9n1pzE1c5MfRSgUUb7z4tUd/zIziYSDoY+n0ybdslVjMaE0smyexJoxyQgEFkDhN4piB0jt2fA7oMYy3No4rxZPADFarnEWNlbRYKvY73XazUxnNfPGTvw2gg5cKuB0In3rh2343PHPywoXFRr/TuOu+m/Ye2HNu6djysY04DLKlvEq0bQuSqm7cjVPJGLEsixjl+2EunxVSKCUZdaVWSkFpIo3mjGujwjAUnG7U6pYQnDGjtbAdHYZxEgvBjDGObfn9JDWqVKr0ur5lCQKjQKIo/NY/ffWTj/3QNbvUPnV24Z++8TWw6Fd/+Xc2h1bX1tNUMyYsy9JSxXFoYIwxnDOtTbfbppRQRj03A0ogHK6h0gTCAuIrXYHTEc5rjHqY7KAbBf1eSDbks1OjS6lOxp1rKxYFcB6YBBwC3U7bA2IAmNTm5IXea6XcZBa73+GsnS3ibVPVrgMDQDlPEOe+f/T0ySgO3eFs5vpCqgOUhFvdtUvolPN86R3c7evj7etuuPGWMOz/9R993+DvDZ5rRwHlIpe1YUgqZRDEUqYUxBCitSYESRyncZgGwZmzS6e7Z09fOOY4plK2ZnbkHS9cWVlT2oMiaZypVoYO3HGx1LGASaALvAIaapD2Rr/ZXNl7x/bZvTuOnP3+6mK7udqF0VqmniNkx+/XWmGc+GFKoC3BKOe5jCsTFcYJAdHQFmdMCFsI17Yoo4JbWmtGCAWiKFIylVLqNIriOI5CAqO0ppRwYRFQ3w+5EKmUluVYlj1YHb4ek+EP/ui/EFJ5/LM/+tkvXjTfVpdORWEklaaECSH8fjeJIxiEod/v9dI0ieNks64pCPvSD2EUHJtShjS59CnQTbTaOL8aNT3sBbIFTEzk7tk7+IXx0QEKs7J6Vd95H2gB4WXTm2FMK7XSXwYmpG8tr57J42ZcXZ12GQ6QXhnrGrr8Wb9aq9nr1VPVP/zKyeveXF9rA5PALuoe4PlZwH339qKrwFM8KXA/wD77Ew+u9V8jmeZXXz+5a/fuc2eOtZsbgyOVhBqbE5jNgBQoIZRSxpAmSV8mrWbzO//4V3d/+sAds5862vxHyw6gpcj0CZNQzu1TP4apwlvrX+7325cyEyMAffrYiaW5Dqc2YWZiavpzD/4sUN5V2bmR1Ode/HPKSBwlOgyJyy1HtMJYcE6F1e+FxmaMUsqpLQWlBsY4nOWzbiJNIrXDWbHAgoAzYQlGXdtuJp1yqZgkcRR1bEsorZNUSikpaJrGYZRyIRijnV7PtpzxibddrV7kry0cqdfry7XwF//Zxe+7rtd84NjiufbcsRUDCM4lgY5UHIeUMo0UBpQypaU2JooiS/DNCG2REpZxieDQCioFCy5FIuTSxrmww2d2ABct/ykAfr+9vHTCsy+64gEOz7VeLOaLY2w7u9SJDWwA3qzz8wBOXPh6GrUqxevqu3WAAi6w8g7JNADYO/vRN+N/UIEI+u1auzlQfNv5WFz8ftROCsWLTmvSne+2W5SwctlHZub98pnAPNAHGit+bXTWNQRhP5OxJoSJHHF2ZaPd94Mollorxpg2GprCbEZfkEqZpjJJgl6nRjCwo3y7g/7p4GT9/yPtzWItva47v7X2+E1nuvOtWzOrWBxFkZJMSRZbtmVZHtuG0UHi9FOjESRPeWgEeegHN5KXvHQHDaQDpIGgEbjRcT/Zllu2FEuyZIuaKJHiWKwq1nirbt35zN+0h7XycEiqOEhiOuux7qlz7/nO+va391r//2/dH6FQnbwH0ANoh8O5MtzAy2/ub59ex2X4xA+/cZ0DNrFB2X7yE598565aeu3lb3of2tanFoN3JjGMqsMQUQgliAgRiUEgZIly3sUQpcSqaoTApSIDoZQQvcJura+0rdeJbp1XSo0nUwAhlaIQekXHE0UfBYoisUDYxEA+ZqkdHt37q3//b5/4+Ce3Tj301qvfOzzcDiF+8hNvd3uic0fb9c03DqfjcZpkPvq2bZUSVTUFZg9QllNgNtqG4IlijKGpayFwODyal/OTJ0/LNAWO4APId1eC1SfW/pvv7P+HP//a/7pxMoNkOuhuP7L2e6eLZ17Z+zMN9VPnAODwzuT5SITSeFjALRaNrDWAt9eeR09tATzj4WAEPxrAp977FSPACgD+nCQDAIBRqNV4v+2k9s4r31r9/Dv7VL/34x+92M3Wn1p72z1luisrcjYeQ+Mg+cjK7QUNy9+F/WdWz91a3rt5e3fQEwdHO/e2b8VAx6NZ2zpEAJRCCiZgJCEwxgjAgNIYozvcX1Kv7v8fF9Y/C/CZRPssqZzzbdx+c/i1R5f+gc1jVd28Mrl17ebRaLaVqDfu392eThtkXF7vPvPY276aO0evXf7Oba1tYklIFKBi9I5ZENsiASWZCAUScQghxiCFAGaFwAITYxRykuoYY6/Xnc1rhOhCTKwWQkiptZYSoVNkaWIMS9tTUgnXxm6nOxqNWAAjRO9u3bgyPNi2WifWoJLAfPO1H1FoALCp6vFoEoJH4HI+adsaUWgtjbHaJOPpMVEQIFAAM3jfzOfgncmyrNvrt3V1d/vOmbPnMc+ACXwLOnmXv/Lck/8YnoRXrv4FysH6mgR4YwS3qjH3BwHgRYCJknqQLVkwCfQAZgBTgC0ABpgD3AKoAU4AbGqYT6c3uPviEjwIj10YTqsHarlH7wCwHmxOnNnd/WvltVzrDpKfgmG+8Tdfe/yp333k4oM52oGcw5Drpv3oekP5j/6HZxNz1IGOhpUjvNc01WBprS79vetHe9ePikyHQCCEFMAMWksUkhmEUFXbdjKbpOkzn3v61MNbzTw0GFuz65q2bUM5m46OZF21h83tz579raPqeDTeqUqnlex2+lde3aknPsv1x375lFipN4onbk6+9cOvf7+dhMAMRMjU1HVmNUslBSJi6xyDEFLGGKyxidVZmlqbeE9CKmYAAASYV85Ye3h43B/00zRhhkhxPJ5keb7UTROjfESlVNO23SKvmjbPszRNCEAr1e0tffH3/gmqbDKtDg72Z7OyrNvZfJoV/RhD8M5739Z1kmfWJlmWa61skvzWP/onl574xDe/8RUJJKUgJoHoXVOW8zzvGGOSJOt1unVd1nXdXVkDLEAKAHxfu2Zj5ZH1wSNjf/320XWatp28e/JckWfF/nx4tvhSX34yh9MAawD2HW86AgwAaoAL75wij6d+p3Wubz4oBJwByHd+48Ih+z4YjBrX+9FXWdaFCD3NKl/du/69w3HzS8/+g/e+8hjgUtYT7Ehn76vthZ91MlCnipMTKGPUWt50vi7S5en0GEGOhyMhhHMEUklglFg3LgRKjTBaFt3BZF7nRZIXqVQ4G7fO88Pdj105esWT29o4u9rbnEyr+wf3vC/fmrw6Hvm6LTLbXz+h1gcn+ktLs/12/eTKp5775Nxv341fP9/74t0ld7zzXYGQp9bVUQhFjKkR1qZH04qIhBZCIAHEEJTS1poi7x74w3JeF50sBIqKtOC9vcMss1VVp4lVSqEARNCCYogAKK3SWkspGtcqBCYKRAAsJH7sqV++8Pj5C4+/R2Zz+aWrr7/2zX63G4i8a2OgOD6WUuVF8aU/+KPFZW29m5dl2suIiZxHgRRVt7eUJqkQipjrukrSbD6b7N28sXH+yQ81tC6+jg19/u54u/GqM0g2V1QLU/u2/B8+7H+lAA9iYE6eLlZ/xvb8fQnxIVKiZ5/6g+df+nfFig2lv3LjzfNhyNB+4Tf/iwdeEgEaAA9wE4Cz7IPNrp9ZTlM7E388BNBHVTVrSghNXqSb87rUsmzaiRSAyCFQjMG7oJWsmmbQ6VirtJLM2FvpP/bMufu7l9um8+03/hxEmEz8fHT/3Onnnjxxthi84pt6NJkYo+czS2CpWuNev7vCNhNb5073V7b8UbsqtwBAinw6K8m7xMj5bCZASikFCpOkug1KCSZwwUEEkxghEAERuN/tSAqRKC+yTAsGAYYTrVGKWVn3ej2lZCfPOboQWEjp2hYAOnlmtWYCYpYCl5aWqqrMiw9WtuCxZy49//yfZVnKRGVZ1nUZQ7z48MO/+js/pRv9q3/5z2fzsp8ZgBhj0EYHRmsTrTUBCARAobXpdHuH+7vdfj9bOvWzigJ/8Vd/e+PanX6vf+7C8urq8rLR85/r5o8wf2BVzAHKn8M2+4XRXU7zVYBB4oreqNJlHd4x+l0BeARA7s6en0/LMPXrxWagfG0rB/WRsPPq5vXxYKU4PpoGz5o2XFMe+dv97orRGoVIjChbZ4z0jnWRMENdtYNeL4aojUyseeTjlx7qPnvlrZt1U2epPbVxbnx0542rrz566fcA+ufSz0M6hMHSD27/h1NbD1279dadWwf37h/0VpeWzkyee+5Lp9WnT2/88qIp+73v/1XbNN08QYrGGiAWAtMscTFE4mpaWqOFkCiiUhKYAMh5D0KA0hQiM3qGJhICGKOrqgkRTOP6/c7q2up0eOy9F0JqASGEqnKRyBqNSrnG12VJFO/cvvbkJz/+wWv01NOft0Y88dSn1c9Yhg7uHzVtPU51NzNCICAAoNIqEjGzMZYZYgzMnGXp9p2bjyydeiDJmqsHfwlx640X33rhu6/eun6zrGut9Mry4Ec/PPH537x0+uzSQpa3eDXBbQErAHaxvdufH5x4z93xn59kACAkoWnzdHkYqrtXDp9+4t2r8QjAfYDerB0KKaq6vXG428n7ayvL7fzQ9n+xxFXd23mrbHveew5pkcmk6+ZV3VQ8H49D8FFpJpJKRIkUkZgkQpalVdNqpW2iy/b4iHd9qKezMk1OhIitKzO7tTd9vd/tL4R4Y3j98Pjms5/4Aknxwg++WxTd5d6JXqfcH956+OSnCeYCllqYVtUcKY7HEyVRSC0VSWPquqlJBOckgqtbqfRCieGdIxatJEt59gAAIABJREFUd9YkzocYo/POmjRNrXOhqh2ovKqnSmCvmzEThSiVAKYYoPXtbFpZY/qDbgghL/KyrDm4g/3bH3qNnn3usx/674t4/oUft23jnDsez/vdFSWlQGmsVUoTgxACEAWitWY6GaGUoa5DeaDydxMiGd7mL//Zn2zfOTw+HrWN8zFqrWPkpnX37hx89nOPf+JZvnTu7cKegNV35K99gPGJ4v+PwvH9gQIIWwdDZXCwpLPOgwbvLsAdZZQ0sHFyafetSa+XTeez7voHRYQfEopj0kyVspqDLss2zQdSxOHRoS+5U+TzybhynilxIdSNTxKbZmnbts4Fo3Wv1zm4NfrG1/9TGfe8Ty9dPBvZn9xa39p8qAzV1fF3L/V/B2AQ4PWtzUsvvvz9qq6kqds2uXtnr5zPnvvYHwHAtvvxWfPJN998OcaomSVCCOQjSSZjQmKtC+y8l0DUxjTP8zwVUnjnR5NJnuXOuTy1UoALaIzxtTNGS6GkzZUMaWrJeyWFtrqcTbwjpYVAKTC2bRuJ67o+Op5sbq6Pxo01H7Vbt4i3bt65du3N/+crfxo5IkDbtqiSXrcIMQKwkMommdaKIqFAa3SvN/AhMNHB7s6JCz9deKqhuvz6zbpxRCCksFIBUFnOYwx17b7/3cvFsq/iv336wn8LAO/IdF+fw14BlwAeVFUd/6KhT78gal+qGkUOSdpN198nxS4ctK132lC313v0Uw8lnJOcfvgbfSCUNSmizdM0KCUxMyrU0IR20la+yNN6PrdW2iQJVZOlwgeSUgIvTFKkMuysJtP5wYWHHru7t3fz5rUmtKnON3r913ffOtqbjlaun9zcev3yW9Hr2Xw/BtjcWC/H1dVrh+Df3lcsm/iD+//nzcvSt05pESKFEKzWbetipHI+F0lmjHbOqdQSMzOVZSulSIyRAp0LAYSSoq7rfsi0MW3TJpmu61k3z4pOwdFTpCRNp5Ox0dg2bYiUprnRMhKkaTYczfb2D2LEfn/wna9//bkvftCS/v744Tf+5M+++p3JvLTahOBjiDHGEIP3WHT7Td0IpRBxAQUCAKUUE5sk6WeFUmoyHYMfgX67rLq1uYkATVMj4Fqvc+7kujH6zVv3xmWdpkVZeefr0+dWAJ4H+DSAAhAATxfwFkADMAboAcwBqv9PPqAPDxYhko+USKmz9+8SDDy9ttzW7d2BXQZYZx6L8FHvTLWyniNmRwdThUWauEl1OBoeV9O6qV1SaE+MDJGC1dIFZiYlRN16QBFCACVBMFSd7evDLMunR2Fnb2dltXfn7Pb5zXPRbbd1czxsICaz2dRacCy2Ns7OwvY3rrzR6+R7zY1o5i1dVnUx298tcks+SETP1LQtgGhbD+SMtt1OMZpMlDZ13RJFgRA9SiUQ0Vgzm86jslLqeeNCqLWSRkqZQpLYGBwSz6azNM9QLjZPqJS01roQ28Z3Cp1Y6wMvxqpcffPFD82zJswS1fnLL//He9s3d+/dCpFmsxJA+OC89xRCoCgAxpMx0VZW5FJoBmaEouhQJGO0sUlVz2eROp2ODw7wp4eAR5767G//xhd+8P3vLhXZhdMn1lbXtNHdTvfvf/JmVZWdblKXoarmy51NgB8BFACnFhyGA/52gjvdt9tHP0ekf+cDVYwPDxecbIRQrTLtbDbsfmBxXIZP3wm7YPsAFWL2YZqADw/5mS9t+DAuR8SkbGIHax0U9fhoMt2L0QfvHADUTQvATeuFEHmRMbG1ejqviyxfW9u8fW23bqdPf+LJrc3VWXtfy97q0onTxW92++nLl7+n5YDYOl8bk4UAMcyP9/z1N3eNxqS3vbPz6uE1u325KodziF4I4UJoG0eAiEJbo7StmxaEiDFarZ0PSsm1lUGIMTITAzChEE3jet08SVNk1kqyb1lI53wkQoToWh+Cc6510RoNAAy0ub4aiQGgqiutFTJneR6De+bZD1JbQQkLAJceeeJTzz4EEW7cuNG0HgAjxRDcYpSCFAKBz505m2WZNkYKrZSWQobgpEAANEnWWd+S6VLRtaDyB+tnpzYG9eTw9MZyJDo4npZtuHDubKINx3B2ubt2Zjnp8ergxDw0ViygL5slvHR/fGt/djda3xOnfi454ReYxRfRwL2dw8uBWyEQQJYTv97/EA/puLqqwBqVVrNxrIVKPpKrT9TzeHxQ+RBV0tiUp+V9750vVfAekVJrWuelUMZoRKG0YmJtNAPUda0tzeqhzgDT5trNN69dvWnzMHM72/ffAGi68Nh06onrbk/6UHXzlV965guzqr1xZ0cKNEaWVXn76vSbX33pytXLzrXkaldXx8OxFCAQQiRjzOrKkkmSuvFSKiZIEyukOjgeB2Lvg0SAGBkgSWxilURAIbRWkThG8pGnkwkxIUJd19qYvOh2ul2ttAJ2vu10UmZOEgvEVV0LxMC4t330c6/YiV/7zX/8x//zv8g7XSHFYiAGAgCgEMgh+EiJTdM0V1ZTDGU5PTo6nExns7K8du3yj5//22uv/fCNV9+4feXVB990/cyFnYPj169tHx6Nb965G5o2M+qXPv741uryyeXOzr26v9wZ0a3p1L2DMoUAGGMynTXbuzf34cp72/P/OXFcX6+aSVOVTdPUbRnCh79hLpbK6Wx/57Bqake/kBTxdqi6bCjkg6XAIEejad3OYxPqssqzNDGyRiHmjTaSGY0SWsvWea0VERqjV07h5kVVLG/OmsnewV5/0EDdgOscj+7eo787KT62sXp2Xt3ycSn6cP3WC0dH1wGm3jcCUSt14/L47o3x6mn43K9//PBV2ntr5B21LhYpJUkSAjJz7Xye51IH5ujaULdtnibEFGLQSifGtN63ZaMAmkZJw9ZYBjZpAiDndWO0aqo6L/Jp1djU9Dq9EDxKKXU6mpTdLk7nc6NUmum6aY9Hk263s3H6F9+gWX72uV/71a/9p69QjIgYI8HbI4nYh6C1RSnquhxOphzaEOLde3ecCwdHkzvbe/f3h1XtNtZX/8d/9t89/OSn3vEW4HK/G21y8fTmxdN1v99b6mbT2m1urHWKZEY1u/58NAe5O6Hne+JTAIAg1wfnifVkfnBwcG99rflZ/sWPGOvpuav6uyyJIDK0ID9872W5V6wks+G05TYrfrETfRHCmGRlLe/1VpeKQdOMytnIJJh1tBRKKlHVDQrIkkQqudQvjLFM3PiIgFmadPpZr2fWN5ZQqCbU48lwNBqNDmfT8fx47+gY9oywezvN8f5xPZ9MD1qtmqJjmqkQCFKYvVtVZ4CrZ1YvPfpI70THixxNqpVqPDOISNT6OJrM51WNiFJIBNG0rZAiS5Jet5Mm1qYJonIuVM7PqsZ7YsAQ43RWlnUlEENkAvCBkjzXSkulyqYFEARQNW2IVNXtcDIzAvv9rlayU3zUzvDKqieK2tjFJAUAVkqkiY3BC6kBhHP++Hh8NKp2D+evvH7n+R++9dJr944n0Sa9vOgcHo3/l3/5b66/8S6W1lx66FQ3N/d2D1qP9/f372zfdG356KWHbu0dfu5XvvTQyh8Olk90+8tSuGn7Q4CrEWZLsrPSWdkYPJYkGcABQPMz0MaTj/KJSqh1oVVmGMlRHdWH14fn82ZWl6NyWLXHZfVRZ6MoIM0s59NROR3atMrTXp5sUQ3OH1ltiQIARCIAACEVQBDBuWg0D5Y6Tzy79sj6BQsXvtH92ksvjI1KpvPGKGwm+fe///3UvjGvQj2rOqeL+RGNdvxqP6ydORvrYyEEAvb6xcYFm+UWfQZaT2ufJTbLM/AVM0eKzFzWzse6W2RFkUotEQURKa1DCMiSiaUU1mrvggBKrFISAZUAnE0nJk1bF0HIUFYLkFYWg0BM8sLmuQ9hMp4KKVdX11xTIUBizRNPfe4jXrg01wCwGG5CREoIo7VNTAiRGGaz+atv3HrjjVshAgAurPxaGeIIiJqUl2Jv7/D/+pM//eN/vml6WwDwq7//T//VH//3vuEii0JFJYhUFcWsLOdhQgDQh4/dPb4ekPtL5GA3tOVR2fR6S1vJ2QkcDuFgABEBPwDr2wW4Pw1JV/08YMc9+k4EsmnPxwqREAF08NDoDzS7JNtqWguhZpPoh3d7/Q/xaH0w5Gd//bSEBkB1l9QTj10glpMh7t46VIB5mpR1HXxgBOej1soozQBCKQSWUj33xS8myQkNotF0eDCMwdqkV3Qt2mZ15fx4WNdlOdmfgoDRrkOVptlKdzWL7KYHpZaiWMfNC/b8hQtPnfynp8499d1v/I3SCoik5ADo6tZYM6tqKWSaGGBwzhFzYlSMEVFEIoohEvgYrbVaQJKkkQKwIKBECQYExLapkTkrcq00cmydq5smtQkCRSKj9erKUl23IQQh4OlP/VqWfyQVQrl//MKLL3kfiHghIi9Sm+WdpuX7u6Mfv3Tl9vYhsVBKCyGJqCynxJGZfesYgYmFwOPj0ZlTG6fPXwIAIbWU+c6tq0Wa5N1iXpezqp1Pp9Px2HbXTNId9E4gri93zyk4I6GTq6x0bS9dk3Ahgc0UTiGsAFQfOHh2HBwdHEz7P1tmfQw/KF0zLu9LZRApNbk1RgCadCP7gIa7avYUqaPxISro570gKol9+TMesj/Nsy/83mdSDesr6T/49Yf39merg/PXr9/Ze2t/a2O9atrxZBqZAAQT5XnmfZBaIyMKrJr6i7/7O32zXoL/ux9+69mPfene7j0i6PQMwVF3IF3Na6sn5pNZNZlIEfub/TMXTz108eHHPn7RhTjeG88n9T/8g3/29Nk/BIChf/VHf/tikiR13TRty4DBeyllIAZmKUBp1bookJmZGZnJOZdYU5a10korVbchSay1SWCWQlpjYgwhgjVqdnyAiARCALkIzNxUZQy+yLOmqYFi0ek2TROJlcDT597XRakAKgANMAXw7wgf6C++8h937x+GGBEAAZQ2wMlkBnsH1d7BuGkCIiIgEQuJUkqmOJ/PgvcM3LQtMAFDJDo6Ovz1534JTQYAp86d//a3/qpqmkk5Ox6OqrIBiiDTrDt4/vnvMKuTq8s++NHwyIcsTbeMPK3lOsARwG4DdxXoBzh7C43aMUAmYalfnP05SZDBybujn9w/vgpMxtjBYLlnBtZ0uuK8/gBl8v74dYW6nM2nh1PfANV+5cTPV7YBAKhEZw+defjs+fx0uradH45Gu/0sl0IRxdlsTsxaaUCBCMF7YrBaBySBGCl+5Stfvvj4Q3nWrcv53sG21iRQhzCTAjvZfOlxOTqMv/67n5jND/cPx8PD6mD4qr6FxDHr1zqTrkyqkYNNYPjmzVv3gKmpGuYYCRVialWMQQgsK9/tFgCIyIACQCCiD1FrJYWwiZnPm5VTK1KVrnVKydaFPE1tYsuqZo7GZkqK2LY2705n86YNSZ6lJmGKMbIQom3boot5kUfXHuzefv8V8m+CPglQAFgAfNcLOZl57wMTAytC65xpWyUQQCx0oBxDjNHHGGIMWlttTJqkZTmfldMsLRxFoiiEeO31q9/53guf/+JvA8D//m/+9Y9fvlwkGilYazdXVgRAf/0Uq+TS48/8yhc+BwDzeZOn+c7+QZGqe/vH586cRNAADz2wCBMATODNHliA+M5UFACAEo7zn9Ew0LJfla5tDwjW8sInJjfStnSQifeXS7xrXGqzbkqyghrFR6PUKmN1Tc1hFb/y/dHO/SObxqqCleVBZs28KpnYpCpGSpPUBx9jTNM8EhOQ80ErCH62e39Xi/jiT7623DuHokpTlyb9uqyBesaIk2fProiLU2inbfvyT/6uSOX110cHu8fdXv5rv//xjQvDr37/f/qtz/yLz1yCv8bvxuiRQWujFEoUWkFD0jnWWglEANQKiXheL06s0gVSUkTmpnWJNXUVYoxCIAqOxGliGxeIKCm6oa6NhKiNdXVs64AopU4Su7a23Do3m01d49NExujff4WCAN0FkO8MSX3329RaW+8Ns0YQjCgQGBCIQvQxBGYiImBmwKqchanX2mitGXg6HWptpNQxtG3bfPvvv7vIs15h07Qw0vfz7lKv2+t2gyyWtx46vX7i4mNv95eKIgFIOrPRK1ev9Hs9BCDovVf4IVq4XTvumfegWxkOR+XOTAzL0VzbHJCU0XlR9GAdAB5b+oInuHbn+cPDY4rol0ORdYzfG9j37+pmR0y9GYHzHAHnNX6kI6carJh5OR69HoeTanmtkCCI6hjAGJMkycyXUkpiBODZrBYSs+ApMgBppagROS+XMD199vR4XM7aq+trvSef7jVV9tJ35x975GOD072d7eP+2UsDYLSzsyc+JUDKWG8Nnsyz9OJDTwuOT1z43Zdv/HnRtxK4cV4q3caWCLupmc1Km8git4jcti7VkjhEJsGxcWS0AnRWSWu1axatHm7rWhrtnGQGAVB0sjTLtZQVCClQAOssd54iQZoaIZCYAIVWKmpumprxA/uM9F0OyHt+tLd32DSaQUilKQbvXfRBaoUggnfBewJGBkCOkREBAMrZZFE31loTBdfWiEAh7O/dW3gD1tc2fuVzvzqbHkI7TrKuEri0+cjaxtZnP/1pSN6DVsi72TLEeTmuq1GaZe+bD2zh7MYHShwIqyfzzoKifGf8ynQ2bw/r7spqb/ntbtXplSePh9t7oxuHh/uuqZf7Kx3Tfe8bAwAM96t6BklXVk2TFtzYDze9vj/P9vbKPNeXzjy3NL+xeZrvbh/uXD+QMSVAo2SaWAaBCJFhXtbdIg1xMbkCUVKaqxLG62dWNjZ7+0f7PoZLj154vLsK3cFPwg/vvTXt9TbvXL8ZKrOxtVSNqNorBOuHz64qoYKj3astirCxvtURl45uHFx8+InxdF6VpZxPJNK8nB8Mq60TWZZaioyIUgojjIwBQkSr8ixBBAmkpIgUm3mttUqs8T4SOeLFiitzYKmUStNZWUkAobQCphDq1gOQUiKwqKsmAjNBU/9iBOYiJuMmkhKIRDHEGIP33k1nI6l0J+/qPKEYg/fEEZEZlJRGGxudc8G1TR28WyiINte7Tz12frRzfbB1fjRvitX17tqKKPeC44C2WF5HhDbUUGubagA4OhoOx0eNr06t9rfvHlzh5tzZcz6o1c6DD7if5XhbPF2HpKdNPJq5ZoA/nZkygLW14uJ4us/SxRiqWam0/aCVs5xNyykVbYIpKQGhmbUwtr+o5SCffu509O20mh8Nd85sPcSluP3maGGmCK6tW2+TRAg5n83n8ypJbJqkSitiVgo3LhbPPvdpFu7+/XtPPfbZ9f7H794aH9fmeCpUvZHqflNyoZa4Nu1EVkck2YqopTACFTDOZmU1a6ajiSAhQGV5d219oz9Y6Q1WBsur3d5yf7AiTapNWuQpMyXGRKJAkbxrXOh3MqFUWdUCIRAoCVJpJVUgEkJYoxGxrmujtVbYtM5qpSSgkIgi0VJpzQiRaFCY4H3TBiVVlprgZ5unfjEA9U/+5P8G5rZt6nruvBdicf6NVTUbDg+rcrqgFRmjtU600lJpJaTQSkkppEJEJv/4pZOfeeaJJ594RAgxn1T3DydFaiofT2ydcuP7vY2HHr30SCCKDHVdKqRqPHzj2hUZZzfuXGVuhuWxMHHmphw4BpP/FGW3WPwOAKoHcPHHDq5KqFtwrFEouXd0dXnpzFLy0+77Wuf0/uw6yogs0Os4V53u+dS85wB+5fJP2rYBgQFi0/j5pEHorC29O0W0BJAfzHLlXZMMuohtXugbt++tdPPpZKaXLKIJxCHSgvJaVjWAQCF9DJI0IgDL6Cx57+ckm/UwsdWBM+WmbxIQtp8pKY0Uihi8937WOu8ZvBRaMSrBgYgiEVPduOnsrpTS2ASA0yS11jIzkacQAQVKVVfz8fGB9/V4PPE+SqU1x9o5qdgozYghUqIkSMHASkohEACkUlmaNc61DgKBZmYikixQ+hi0DK2nWek7hbVWikZmWQ4Qbl6//sxnqp/PXP2rv/1mVc6tTULwQsq2nk+8X1leS9I0L/rOt66pm6acz8dEgZkREN957hHFEHz0YX1t8PQTF9ZPnAmydzDlLNY2MacGS1lRTcvKLp8qsq6MRBQt0mh4eOv29vrm5qOXHik4DMvZzvEu67roFG2YNUGmsARLg/cy/fDBGgfD7XF9t5c+ZOGsxPmJzrn73Ws7+y8v9ZeWHjCkrK2f2jts6lnZVhCiu3b57z79qX/44Gd/6unPvvrSNwk8x+indTsLeOpBSe0irTnCqwgs3pnoraxNikSBkJvrG8OJm47YaNM0LQXSujNY6hRpEiK1Xq4scZIabVSapALl8vJyz25ee+Go2+0mhNuvjCmCFjmyJESUgAIZBDNJIUBrxRhjRCGBORIBg1QKI1IMiBKFCD6E4JhBCEHE3rcImOZJt9MTy8srK6tNVc/r+fHh4f7e3fnx8XA07XW7SkophDUyMClEIYQQQMSRCBGlxBjBxSAQGAUIGSPbRJFgigRIxDSb1yfWV3YPtp3RSglA+WFAr+ZBef7XvvxVZmraRkpJkbTWx8NDZhr0BkIra4y1FrgXgvO+bdvG+6apa++dcy0KQIai07/w8KM6Xw2iSNLi3sFQTyvvQ8MhMhibcOw3gAfzyWw6o0Ghlc4yWVjFyMlSJ8uLeTOK0NZx4j1W0+D3y+mV7/WW1rae+fw7f+aDT9KqgTkQ7IyuR7qDUsV4Lwaqq9Hr177V665omZ9ffTqBTqfbmUw6jXfsFQrp/DS8d2e6u3tHaxmVaEPgwN1O3l15+6H54lsvsKwfP//JFHIJJx+c5aiMHkwrs7UB6yezlZXs239+d23tZJ4WWZFnSSqVWTA1msZR9EwMAqwxRps8L1Kbp5RArZlYomOIzntwQSmtJMUIjI4JpERrjdYJMy3KXwDMxMQCmARqFAIAmFkK5UJLPgCKEKJrmxAiM+dZJ0kypZO808vzPkqjddY2s8RIZUzrfOscEVuUGlBKKQQKRO+dUjrEwEyI0sfoW6ekLqtqwW4I0UeGvcPhqa3Vfj+fzUptLKP4AKDwPgADxHeN4LduXCVmoAhExiYhBiIyis6eWf61L/2XmxsbT378MS3gv/6j/+rOnTvBOwaIwQu56GdAt9P95c9+7umnnhjPZ7e3b5fjQ511B8WJrNu7vXeklTZaDwbdvXG5f23fpmnl/f3Do631jSQ0N7dvjuaJNSx8W4VqVmquZbN/5KesQBwdHZa+ffjZZwBWALZ3J1c73b4Gweyr0ntiJsVRzcbzsp5Mp8MAGMPxbH6IoMtmcvLUOaLYLZZr7WoOQDJAePmVv/nkU7/x7rW4d+sVqQ0o5aJLUpUPsqq5t9CLo5Lb927sjd/YOn3iYyvPyQcGtystTZGYptIHd7gwvTObF9OkyPPM2sQYiygXYgTi6H0gIhSolQbAGAKQCBHAEQIzyhh96wIQEzOCIQzIgpiBMUgpkAEJGAEYAQgChZZBaGMwCB8iQgSBFDl4D8ghBGYMIcyms3JeaWu0skopY5LTZ85vbG66qhwd3ZvOp8YoKUTrPBERsRQspFxopkOIiGCklErFGNMsS41u6mY6nQujtRKta0Okl16+arQkREWKiY5G11YGTz2QZOU7k+0dgLl6+8t1VQmUCCIiA6KSYnmlePLR88988mO/89s/pcg+/NjFNy+/FiMppaRNKcY0LWySbp1de+qZx63R1WFzfDxZWd1cWl1NEtNLbWLNhdNn7u/v7xweF93+mZXz90fja7d3RuNxbtSkLff94cyr9d5mknd1Ow0uhLoZHY6HY9ImARTbxy/d2zt46tMXD6fbt3Z2jNZry0VwynGQRs7dVIhUc9KULUbj2gYsubaqqlk1aSQqm5pmFnwJ9bSNGjThkbv/7ie6ef2y0AIUR6hE4mTPhLTcGb5y5tTHHfi1rVO2gLv7rw8Px8NevaoBAAKQBKGeeuSCkZmrNVbKVWp9VWttpFJCKCmlQASBQIwkQCEDLpxqwUcGAQAxRmZGgEgUiCgyM3PrEWWipFLIjABMMUSmEEKMxAxCMDMQkVJmwWtiJoFSSiGVi9EvPHBCCgb0IdbVjDlmeU8pJaXIi7zfG8jltbwo7t65fnC0b40WkQMRAispFzI1RAHIzCykWlpaOzrapRiQZYyeIiFQZJmmKRF1E8PMpQsErJV66YUf/caX3s2zEw9MhHAA+//+3/1l8EEpARyapmQmIfDxJ86sry1n79Wg7ty/IYQgFAJVmhXetYAiselnnntGJWZahofPnc2VGh7ug5RxEBEDOacgDLrFnXs7g+4gT3RbjqfTqbZmOKuR6tLNO4N0WB6iwoHpouG8nxzBcDiZKe3R6G5iZ8PhvbdGso+Gs7qcj7RQRpah8d4xoGZ2bZxNalJRKevennap3ZzH+6O026nGs6PdUTmppFJZbvMsv7ezc3JrCwC2b73c6S+hkbNmX2eULBHqCOQTEAnYhlS36K/784f7d19+6QdrvYtL/Y0g58fTm0q5VSFSyxgCAQMoESPFGIUEIVkJIZUAgEgUiZWSiBADUYwLIQwwMNNisx9jBBDMIRKEELzH4D0wISIKiYBt8BQYgFEAAjJgpLZ1rRCSARhRCLTWInBD5H1LREIBEYTgKFKjaqzBJDrNUoEiTdL0xKkksUW3d3iw1/qAkd8eKyYwxrgYTOsCE+Pa+vp8Pmmqsmmbumob16RGWysQ0Rhj0yTRKkxmKIRzzfbN+r1Un3fX/+kPn//q33/rCoICBGTuD5ZDCN6VRZZmWbJ+svsA4P1eXVaIKIRkBKV0muRN2yirNk6sFqpTzg4NUz/N9g921jZWDvd3bt1qIykr3GQ2r+e1EAHTbGllfSnvNZPR9</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8aZRl11Um+J3hzvfN8WKOHCLnSSmlMjXYsiVLRsgj2IaCMjZgUxQ0dJkyBVXdNDU0FNSq7qZp1iqgiirjApeZsTEeJBtLliVbY0qZUs7KMTLm4c3vjmfqH5GRipBSsuT+10vfWrHi3nPuPdPeb5999vnOBd7CW3gLb+EtvIW38Bbewlt4C2/hLbyFt/AW3sJbeAtv4S28hbfw/3eQu95xN6WUcU5BGYftOFmaeq5HGQPMwuICZ1Yh9KVSIsu7vc787BWtDYihhDLOB0aLWmfM0py5lkNqteFcqlJYbnQWBkZMWKg4Zvil8y8muSyFhbGhIxenv1MsDBzcfV8cp88c+3qtVJhfnpEqBWF+4AZeIUl7g0ODu3bu2DS088//+n9cPLFCKRFCWxZ3HUtIJaUihHDGciFtzkEglFFKwWgCUEo812W2TaHTTFBCQKCUppRxRrhlVyrVlcay73qFcqnbaholLcdhzOr2+q5rKy2oJ5VRSid7tr/jtoN3nbp0NBHR4tK5ocHNWgVRb0WzRrvVzWNNKQXFYHmHokmSNbUyBnl1EAw1x+UW9/I86nT6O3ceAMPSQjQ3ey7q6eWZPjGUUsI5KxXKWssszwmlt73z5oOHbt86urNe33HzgR1zc62/f+izi8uXh+vloDJYr22/cO5xYok4nW42e8P1Xb5VHZvYPz4ymebRyvKle+/7idC+JtRPffoXB4YS0OZKa6Wfik3Dt3nFgShbtszI0vwc9ZqBs+nki4/v3rntmaMvJGn+kQ/+YtH1//rv/1un1QrCGufu8vIFz/cIyYUwWpO33/GPlpanzl9+hjPXc5w801vG9n7q0//+8G2TNnljevann/+LMChyyyKE1KoFymjU71cq1XJloLEyf+bc+cD3hwar/W4vjvPnjn7n5PHvKq1hYNmM294973uH0Au2z0SalqvVex944IUXj9VK9a3bJgg7ESL08cEHn/ujXjRTHxx/1+5f++ITv82IededP7e01Hvm5H/bsmn0pTPncxVZvlYZHRvfYfmtfbsOD+MjAL707V9/8HPnCXSciGIhqFcLC8stpeDYjDMaRxlnxHZdoUmnF2shAodRogvlaqFY0FomSaqlZpwmuXQsy/cdzwu27dpz7vSJiYktI2ODp44ds7gpFsvMDc6cPT8+NpplrcRZcQMu0HnP/b+wd/Tuc8uP+QP9Ihkr4SCQAs2jMw9tGz/w7POPLMxdTUWyeeyOXPWSbMFzgiRbnthpPHswitnkpt0M0WKzMVTdP4j7mzj27af+fGG6d/ZoM+9S3/MKgT84MCSNbDbbXmj/s3/5ER933khGBlgvTAV8HXgHUHhdyXaA48AZIAc+9Yq8Ho5NLRzbP/xJgUvPnP3G23f/PIBvPP+Z0ydf4NS3nKDfa8CkdpimfShpP/Dun3vp4omZpadsOwhYabyy9Qfu/fgb0q81sI//1M+UKxXH9TnTIyMjWZ46jlssluuDA5cunee2N1gf8D0/SZIsS5/+7j9kecooBYjrOMaYsOhv37X9Xe/+8Vz2d+48EqWZIBcvX7zY60RJKnrGemnlm4tzCiwWgg2N1w9N/MjYRNVCuLBy7vZb7p66evzgTQf27t4hFKJeptji+275QBdLRVSBsrJap5+9xBiVUlo210obA89zCoFnW5xzppRghBoQRgylZHCgHIYBsyzCOKCDIOCMeq7r+0G5WtmyedPQ6KgUqtNugujJye2UmDxNGKX9fqS1LhWLxgjN+kGZWa5cbp9d7s9320sj9S0D7DAAgAOF0eItHsa2jdxVmxRZrrrxOcvpGKLKxXJY0fXBipD50Ej44vNT7U5vuL5ljI8bJArdF04/2W+LWnnQd23fLdartWKpaHGWZvnw5vDggSGGbRulI4EZAIC7LpECOwDne0nWBZ4GxgAFzAA71+cRnG5mS4P+EYbKpoEhoATg0vKTzeWlbreZ6X69tjkVCeMglNq2p0Vqe7WxofCW3du1ln7Z3jR885vSM+44jsUtpXW9XpdaGG0sixdLxW6nKRR81w3DMIljKdTF86d63aZlc5FLRiljlML0e8vGLp2f/kalOpSIzqlj3ykXqywvNFZm+7n5kW33xrVRy3QoGwv98SpuAhBiPzB30+aDwLzlmcnKLcDA6L6hJ8KHlpbSRfRzpZfYk4O4evbcSUYJo8xiFNr04qxU8G3LMkYZBcYZo4xanCriWcR1XNt1ldRCCqlEpVKtD9QaKyue7zq2t7jS3LRlq1CIoqhcLmdZojQGh0dbzaUgCIMCjZNcKhkU7aHJQaiw2T1fdkcnagd2TdwJYDo5NuHd8oqxG+c/zPYPXZ595NCW97excPyFhya3eGmiBmsDHP7th/ZlaBXgaFgU2wvYPjHynExOJu2s0xSlouf5vu+5zSxjjE7soXPipS3WYaCyXjrApjclznWYBnygDowBL0l8huM+YMtqno2799UGAQOcAfauJlqcKsheP7MFadCZTPQs15moV4RmH3r3LwK41P3C5mItj0mS8zfbGk4IIZTbXBUKYaPZKBTCYmnA4nR+bsV2PN+1bctpJyvdXufsqWPaGArCGGWMKqUAwhyZi2YuzNDArubKPDO2lLwdz3P0bVN+dv5orbLrjs0fBDoxptcqvQL0gAQgO3eNrP3Udu7ePFMrRsPoEKY1lhuIXFr1vbksF9yyHNsObZtbTObSYiQDUbnINbWZZVtExcL23CTL80yWSoHvOYQYRkltoNbr9TORSSEIs146eTwIC5u3bF1Zmk+iThLHcT8Nw0LBL7qeK4XkMFGUO046Pjq576abuiud1RZPePtvNHon61Y2suV/AzCMg0J88/zJfPvewhgmgVEJh2MEkMC1n37c8ZIeaa3kUmpCmGM7nusm6aLt8vtufi9AgLmNevZaaAIJMHajrGWgDgCYBTiQADcDPYWcYwEoANNAHRAGlwkoULz+Zpb2s4TFsfRconJpOwyaC5r1IxydOnZ48y2TxQ8DswvLZ4Vhb6CRG8A+/lP/hDGUy4FQKQyhhNcHB4XM5+cWQEi1UhZ53mwsnz557MqFk65rG2200YRQxog2qNWLW3eNGtZZmc96vf7A4JagQv0iK9YjRVSlWG/1zriloQATFgotfIPgFMdloBdh1saeEGVgZFUKy/pqv5ebsFhAhSCby5Kr57ozF5azNOfM4jbPcslgjDFJKpudqJ9khFLOGbQxKqeWbQxhnIaBW6vWKKNRnHqewxi3OCMU9cHBhbl5kee7D9xECd20ZbNRamVxjjLu+X4/Shi0Qibspb27dwfu5ER911ihAAwBOLf0ZDM+RwLirdODE8sPjQQ/dP1Wufrtkz8xwI8A5Q5Opuh6OAD412X5hS/9MVjGtZ1l2mK27wWO40b9uD5R3r/nw0AIlAANJN9rWvSAxmtoZLB2MQ4IoAFYDTw+r+ZqdDMgAQXsBOgKogCHVmfMVQyPjB478XSWJkXfdh1XaP2TP/q7SY8uNqa60cnBGim4PlBnJm1EjYtzc8WRHQF9Y6sAgDPOHYvYNuv3Mi1TPyx1mktJLkGpy7jRIk+ibrczdfE0pVRJBUIYYwAooaDoNUVrMeYFI+N516m87cg/nlo6ttR+PlHzNR9TV6c3TQzMLP91uf6AjVoFdaA5gzmG5qWz0b7d3y2vWXKg1FxsS8OTPkc4OY/UxsCR2+qnvjutNXzXBZBmcZrnaSq0IQZUaaW0SaLY82xuO4TQQuhTRrJM9Pp9AtLudBkjFrcoZ5VCMHP5smNbWsuZK1euTs9s2rqVEOYXAsuyGbcti1XLNbeWDO+rz891tk5s+87Rh2666aaSHX3rqW8yRwReVdovHJ9N9+1+7xA9BKBerq0fyr3VB673ZSH+ZieaH633x7EXGF9NZRaJ+4mlbSN1t9u1bRtGK62plQFY59d7AAANLAHDN5LaArD1RukvAAfXrjWwF3Dm8fURfKzGTgE+UAYuAQCK9XVrDglwIMTWzaP7hio7Zude6Kc9N3AMWCoNqGbGm55tnJz6G2KEiPwLU5c83zzA3qiSAWAf/9jHavUio36jseS4gcW5F1Tm52dElrmuZbRpNpZPnzw+e+VsmgtKqQGIIZQRRimjNMnkwGhh07YDnW5LJFlxILQ9qszM3sldZ8/1HJd4Ybp/6GYLTYouMAlsLSJblrPTV1pxbhLYxJv2MAXw2db5qBvvGLszwmnAGeU/VAk2PfrNr2ljPMfijEapYAT9KGOcVUoFx2ZCyHKlQinl3BJ5bjvctixKqWVZSgolctu20iR1mWKcJ702t93awEBQCK5cvJCnWbfbVEIQGGNACR2bGCtVhw5uv4UGrBWdHRgoTRbfZkG09XzUX567ugJjFQphLhdya7FDnxlkexgGbzSqyYC1OXYvbaUTDTR8zAFVwP3iF/9qZSbNekbkSsicU+q6nmJJeSJdVM9sqdy1tq68CnDgOLBz40pzFVeAOvBqD+lpoAxUV28UHqXYClRdDDEMAEPAt4DDwCIwsf61i8svPHHyr549/dXt2+46uO32kU2DswsXG71Fo8zFKyc1aVk8y7PefHMmTW1j3Chu3XHnJx84fN8bVzKsTuGeGxqDfqc9MbHZ8zypZBCWjFJBGEbd/vLy8tTFUwaGEkop0doABqAAMTDcolv3V95+63v+If7b9tLMM899YXBoZKDmF7FjbPPC+Gi2sFD28ENAQ+JFju8C7iJmFhbbNq/MTTeLpUIVH5ZY5qgMjw205kU3WaRsoJVM1UsAoI0xSve6ETiDNhKqVPQZtzjVrTjX2sRx7HuBH/qm3xGZcCybUAatDYxl25SAMaoMRJKFQbhl195Wu91udWyL5SIrl0qdZrNSKfU6HWWglem0k5Oz5zkXMu+PToxnaDioOh4zmkW9iMktlOb76wcEKjbGrk9S8zg6gsPrRtUD2lL3Vtj5BIUa3gGcBWo6BzQzxiitYEyWC6G053sfeue/BgBcBkqACwwAR1O0HTxKcO+rRLblNUR5+7rry2zNsM2bRwzhm3E/UAU6QLUrnilat11/dFv94Lb6wTONB31YAJJU2LafZzrNs1xcAXHD0PVDL1ep4zYNM/t337pv6IbW9PVA60Mjlm2HhWD3nr29dpMQqkSmZM45MRq9Xmd+diqJ2koqEEMIsS0OAiUVpZQzZnGa5u2r3b8/dPMOv+QIKe4+/OFSeXQubtw5+q8m8G+ODH8KsIDhE4t9gxLwAa221grDlq8VxKbqIQCnZk4A3CG7bS+8eOmlLONp7K+2jxBi21wpmWWCQVFKLc6V1v0oMVo7jk0py0XOGXVdr1Sp1KoVY7TSmgBBEBiZc8dxw0oQhOC2kHppYV5JAUo9zy9VB4wxYbHMGE3i6ML5883WSpap3UN3UQydvjx17NIjp5afWlpIq5XRvYdrpZHmubPPf+vsF22U1nlCuK5kEZ5fS5NbrHeWsTSBEBgA7gB2VMrDBkZKAWMIIWmaL68sJZFceyUHqoAP+MAeF3f0kb+G1OYBAYi128a6rD5wHiBrhk1tIndvxgRQAiKAAo2ipfHymuwa9tTes3pRrwz/6Ps+MVivc4cVgsG9299T9Abz2KIyYMRzbPjlkTenYgAATiioZU1PXb5y+fK9997PLTuKeq3lGcasOI4by0szUy8ZGAKilZFEUttmjESJtG1FqOX7Xq28eWkxClh86Na75pauBNi1q7Lr75/9zckjH1hf09ahsVPLl/fXZ6psYKi4TySnhgZoiMMAtDQAphdfKhbCg/vuiXX/lsKPrL6ltebE2I4jUqGVdLgdJRkoJ5QHAeeUJZkIPIdSSKE5Z47nFQtCKymlUkopTZkUWZqCIIrTwTFhMZrGPc91W40V3/eTXDme74eFdrfX6bS9SmHf5J1A7fZtnwBmgW1AK0u+cWjTP1rC144df8ay9dBo8XzvqR2F/RmeJNhhrzMkAfalON/V3ShrGJ5JquYvHT+04/YCJgD0+n0KGKMBwqhFGVVKgFyfARUAoA2UV9eMBTyAV6IPEGBxbfG0ivVuYgjsWHd7CrgJCAAL+AgA4Gngfa+jEB6KQDH0i3RQ5XlnoTE34FYLlUFlTDefb/R0czjZVnydAm6A0wvnqR9UikHJ9wOjqeW4vV5PSBH3e4VyJY2jhfmpLOnYlqUJpFIwRBsNDYsRQimlAMGhAx+5fcc7JzZPwInu3nXNzt9z5JXx4jJuHyrd+fi5L2UwFP7+oVuF0KtZ42MTl7rP7xg5tC38wSK2D9NrgYB2B1oZA2o5ttEKWgshlDZ5nsdJqpTOpbKojpO401yxOOlHcbPZztOEEhIEnhf4jutGUSqU0tokSbI4PxfHsWW7rmsTAiWynbv3WJYdpQJa97tdkSUzzacvdL8AuLgWNa0c2vRjABnE2w4c2FGtjI4VDw8XauflQ21c7uOFjb3suKgP0nHPm5u0PjDKPsS5d+zCnzfNM5/7yr/vd1qcM0YpJYxyLvLcGDM6cT3gOQk8AqyOSftG8oqBEAiuB0peBQVEANYs3CIwBXwVaANm7Zng2MX/0cwffo0S4tV/Q/Wx99zzC0ODwxzdvTt39fTUfOuKy53AScbqbzqkt3d4B8/i1LbsHbv3bd40abtOs41CWCpWh1YWFwphuDQ/LUSutCYGSmvPs5QxxhjAUAKjoXk2tfLgeH3rMLs/d2cVGANiTBVv5EbU7c31Xf/8+u3BkVFg5bkL38mksv1ksvixVzz/n/6fXw0D17J4p9OllGmLKq0LRV8KLaVknGdZTiFty6PM4pQYmE6nUyx4SZICJCyVQKid5krJLNMAol6HMUaJCTwvTjPbcTdv3XbupTPNZiv0gyTqt5rt6QudobFqWjztXgtgRmtTpPKYS5lXxv0ACnzXWqRqFc8Dh7C2LBjGTwMIceTtW48AuIB/21jsEEq0VsYY27YoYChhlEndXyvBxTVvLAL6wDywB3gYoDmIjXuA14paxUAOZEATaAENiRrH24AYCIAWsB0AsAz0zzcuQSazi93qxOH1QY01XHNXtm25/ez5Y547RHTaSxcDp4JCsmPb5Kbxon/juN33AI/7XZGlNnH9wOt2e9Vq1eZWfbDebzdmZ682lmcp47lIDYxtMSGVbVnSGEIpIQSUgmB++cxEvQY4oruPlfcA8LH5DTdgwLDa7PSjo0Objjd/9+bqp9fnGZ1TSpIkpUZLYxhluTTIckrZQLWgDVmIYwPNXBoEBcuCMZR7TpykedQHJemK9D3HAJ1ORCiMQZal5VIJMIzxKIoNYVLJNIoch1u2xWynUC6+67ZPLGUnFsTzFevpEiYBAnjAFoAvtfW9+391rXX1jR059Dqd3I5fbsz/C0qIIYRSzhiD0YwxymgazQBXgKG1cAaAtsCchd0AgPuAaRs9AOuCak8DO9Y8sC5wFtgDCOC8QUAwzrG6dbEF6AOja2+VgBcGq8O1kvA4B7o30rNr2DdxRMMcmLgNwNFT3+02powtVvoLu7ETaL2xYPIG0LGJbVIJJWW/20/SzHdtxyI2o9VaPYq10opSIqU2BgByYZRWALUtC0Ca5WEwsGX4gSrYlP6zavmlK8mTV6O5N9WC2DwX9VfOTz+zqfqOV2TlWaaVCj1bKu1YnFIqpSRGu46VC6m1rASu6zkF3wMluTDdfqSktG3b9VzOqG3xJEmV0lGS5rkOAt+x3SRJVg2yH4Sddrvf7zPOHdtud3qOX9i1dxcAw7NMRhx14G7glhTzQB2owOq+2fFdQymPfALDuO15rhSSMEIpMdr4YQnYAqTrHiYWblsXqZ+4vjW0htuBEFia7z8InAIMcAVQwHaCYN3DM8DourCcDewukYNVvtPD/UAdmFrNSNC43oDri4tVJQNweN/bBbUXG4uLs52vH314KX9z8l0F9QKPcyfPM6lVGBaNUtfz7rjjCKFMCcEYsW3Lcx3boloZo7VjW1JpaLMy2/7z33/wiZdmiGlWsGOLd+emYBTAl5/9bIT+a9f7Mg5OHrz5wDs+dP+vVTeEBrCon6GEaANKqDREGZJlwra5Y9uMEMp4lkkJEni+59mMESEEIxBKc8Y1Ya7j9PtxkuVa60LoUUayNDcwSutep7OyvJzESdxrnjj23OLCkhSy4Dmu5x86fB+AK/NHd3k/F+D9AIDZDM8CXwau7gpuBpobm3/xDQ60zCPGmOe6SZJQSiihjFHOuWWLGM/gmsVaxehrlgIAyHAMsIHBkfA9wJ3ANmAQ2AxUgBHAARTwKBABtXVmUgHjwFivtwg0gCWgASQAPNSub9VbwJmZp/sv+3MA8I8f+HTUzReXWtNXlr/w4GfeYJfXg0bdBmXc5pYxJvRtzl92Av77n/4Ro8S2bcqoxRmhlBBwzrQxuVQEsG2LgsxeXm4sZpvY5LdOX/cu1QeOfELC6uPk69R9afFx4LKLzW6hUCJ1AN2sM9c8BjwKnHrkyw+DUM6YVAogIJBKO7YtNTRgW0wZpsCp4xkQxqjNabHgU2b141QqFfVjA5PmwrZdAmgpGWOcsySKe1GU51pKUSiUHMeSImeMMcbGRoct+ABuH//5dc3cTTGZYwnoAEWF2RwXU1wAMIe/msIz33OIW6r/m//hlymB7XppEmtlGKOcEUoYANcPfdz2pvbLHdwiXl4orCroKq1jaQVPA0eBFjCIazNvde3Ja5ItFLa+ePbbjeRsW08DZ15d/uT49oce/p31KQaIY7Gy0J2daSZt85m/+81vnvjSG28wAG5xW6vc8zy1IfQs/+i//9b5Fy5rbSiBVuAcRmutjYAyGoTAtS1DmDJaCHPpwtTiO955x96fvt6lLqKl7tUdxdXt5ym8ymM7euKvLy0+yYP7N4UP7K6NAjaAolNqdttA5cTUM1On55XS/TixKYPRSZwFvmtZFqFECTnf7QlBypVQCqWVivuJ0pLSQpxnnm0bZlPOVRrFUerZNmPMtq0sTWMOrmLCvFa7XalWcyFrA4OgtsWYyPrd9iunxYZcOHryz1RHe2WMbzu+I7yjY1oF0nThA18ewLK90Qa/GgvZxcef/IxXTpOOleWZENKyHM9zGKO5kBYj2/eXvw+Px0IZ0MCzgAV0AQf4egfn0qw0g7PjTgv4gdd+e/Po5qkLp08Ua3Z5c3HjjoM+duXbt2x51wP3fWJ9KoHQWjlES5DAG/OcgU7jzbkQ7Ff/1a95jiOV4hbnaztWTz/zxGMPf1MKKUXOGZRWtmVppTSMEhqUhIHn+55UOs2EAZmfaR1/9uwLz52a2L2l7FcBOLBrzjVP+dLsuUpxfH2tz87+0eLs3NWL/bTtnDv7Qn2M+Pa1yaIcuBcWnnr0i2caS32ptGdbtuOkmZDaBL4TJ5nn2q7FhaZZmgeeHQSeUTLP0sDzy5UiZdSyLBiUCn6WxiDEAKVSaXLbzn6v3e/1ApsVyhXKaKlUDMJit9PVRvueKzWiODl05O3r2+nTEOGF1HTLVceyo6995bkzR6/sOLDbIbcBHsMksHX1F3JDRJn5iz/77agXz1/O2o22zIUB1Ua7jm3Zts3ZtpvKm/fXy2wrkAIecPpVy4vXAQHGgRFgCzABrAgsdvog8Mv2B1//Td/KMzp95US6bft2kPXTNBkpbwVgry0818CkeW5hYSVNkrvu+sn3vu09K+nlzQO733BTwX7u5/7p0OBAP44cx2UUAJTBn/zx73W6DUaYbXGtZJ4JximlhBKSS5XnqlDwGWdpkksDmzOHeSo3nm2Pby9Ip12yN2jVK5QMwFjx1rPTj7Xb6dyFi0mn7fnVhF2ohSNADJy91H7x3PG2yIhjWQRGGQippVZEKUKplCrJNCHEsXkpdH3HclwnF9JxHNd3tdLc4kmaW4xRijQ3uZBZLsYnNo2OjhOosFQpV8pK6dB3hTJxt5PmkjKqDYxSt2zUMwBV++CWgbuGC1HN2XNw73bpqGcfW3jp0slEiJHBW4FpQK7fGwBmrrvwv/+f/w21MtuXF08ux91YCWG7TrlSDHzPZvSmI5s+/P73l9m9gAAuASNvUMnyG0c4xh2Uqu6AsjN/I6vxRqhVQ9HsLJcKJdsxXTx39NKjmyqvJNit4htH/zzqP/e2m/e043bU6V+af6mvstsOvstBsoinw9fcB9sA9r//u9/Icsm45TvXAtPHjz3XSem//rXfujp/cmFmyeE0y3OlDaXEEGJZ3LGZARhncZIbpSuVouf7hNDf+I//ddPArlUlm+mcK7oDr1PxyKYJKdPG9FyxWNi6b2B0ouxgN3Alw8rVhf7SJQmlYQBjMiGTLLcYl3nqB2GnG2VpZjNTKRcGKwUDk2WCU8osbluWbdtKKkKpZfNcml4v3rtvfxB4zUaTc5pE/SzLbcviFs8ykaR5oVTkFldStlodpdRtd97zWoIBtgDO2MAd+/fesmfnwZHBSQAG7rdP/WGqSgOFobUni8AiEP7Bf/ntuN/UKdoNMXV+3ubM4qxQLI6MDAW+5/juhz56xMKtAAccoA7QNyIwoM020GsBxIC11siCjxtS5VbRWUfNHa8XEq9I+8nlY5efOLz9vkhGgjJn7YHvnPkz6nrTSxcvXHpyqT1/044DQ8OVM5dmR4YGlZEj45PT/addTrv0SgGT37PR3LbtNBcF/+WmP/7kt3/pF38ZAHcLSqlECEJJmuSua+VChr4jxLUREUK6rm3bTpSmnNvOuoEaL+16/YqLZAsnX+XMSIi5laVtk7cDmE8vuq6xLd1pNzhcbYxtWZk0nFGttMWtLMsoge1awtDAcyzHsSwrT3MNAyCOs1K54DrEmIxSNlAfWmn1jDFhEPQ7s7NX+5ZtiyxdVrIQBgCJ4ygIfMe2JXJipFCvQxNdDTVdH6VrwVsC/559/+tq0hPP/0OttoNby8Oj/MzJs2mn31lJqsWwuZz4rsMtUgwDx+Ge6zIKx/f8DS7UG2eoll+VsjrH5UADYED4vTmpkzEAACAASURBVHpxDXZBRK00E0RF3nyrsbQ4ffHSuUyRj37g0y7o/OKLly4fHx7cv3niQLPxwtFLZ/Oku3fn5jAYnlmKh6yx2d7TnfbcUNl/7TDcuu5lQgZBeJ1KNLN8eeuha3Pz9IUpi9FEKE4BQjjnXCpCqBAZKHMMwsAHJYaAUTowFhxb+ptbBn/kDY0VACCOc4LSXff82J4dtwIAFvs9MuQeGhosOM4VmZpeL2KMEUKzXPT7SRh6LidZLp2CTQnpxxkhxOKcO55NjO0HSRRLISihMJoyVq0PmrMvzc/NDNZrYeB3u5FWMk1TpVGtWKViqRcljVarFPogXGisX2u/BgLgK8AdwA1M9dsO/QCAmRXVXgy/+eW/vHTxEoERQhitGTOMkCxNUqHq9QHb4panp1snJyqvY3t6GZ7KTbFA1hMx1jPMOhv1xt646flGsD2oNAOocmeq5O2Z3D16ePe7e1IcO/MNyzUWrzoV5/7DPwnga49fnZ+5yn0yXB5Os26aRMenHm3HiyLLnCyYjZ+dX4qvXLw8NDZWmyB7R9/96pp4mmaF8GX3Yry+VVTHAMT5dL8dCaWUkIoYRsmqv8w45RaHNiAkl5JbrNPp7T349k/+858q34As9Zr4d7/xL/KkPTYxtqZkAIa21G+lGB4NGCcPSqSEIM+F1MhzRQjiJIcxjNF+Pw49O8mENqZQCCzKmMVd1zXaxHE0Pjqe5km/H5059YJtsYmJ8bjfA0BghMizNNcGjDFCCKXUcRzb4lKTsfGJTrsLnANWLfEUMALYwMPAy1wrhWUGCZwGBm+obeMD2wC0Oz2jFShL4oQwagwMkEnNiVZKEU6kkCeeeHrifa+jZ9928H6HJOuTBMrWy3dX1uncm0UO2MAmYARo7RjZkaWNy+155hc2FXcqJeevXrz/7k+H16ZjdHqL1M521vfEjf5Ma0GTYlgILlzJzx2fO//C8V73y1oZ2yEH7hw9oEZX0nN7J+8dwJ719VEAlG7wDIbZfgALs40g9Ahlvu9KZSyLEUMMIcZglUhICImThFN0+5ET8kyp11l5vRq9TkcrE5QLZo2oAMDCMIBvPfq1XAipjNIg3DLa+L7DONfapLkcHqzCmE63H2ei1U2iKAUMCFaWlrrdnpB6pdGM+j2lFSPMGJw+c67T6XLO6gM1h3NDiOvwNI2lNpVyxRDicJ7nealcqQ5U16lOe607Gwh9DJ8AhoHdwMDG4OoGxFFEGVNaxWlmDChjUkFpQykNitVP/s//0i641F964pnXiXmuRom9dSnS2hAeetMk/XW4LikL6DisUCvbW4edTcWdAO7a//4P3/1LIawrvUsAvnn0D11HapkMlSdu3n6QO6A0X57WF47Fx757eWWptbpt44Y0rNjSyGaj8/yxJxeyS+vr4wSGranZsjhXt4qtpcQbxOTWm286cs8TD/9dHsssy42xMiMd2zY209r4gZ1kMgxcqcAoLQ04Q+zNGe1NW7ZVK7WPf/SfXh8wiYTDW4qe9f2iFEoZLZVhRhJoowmjjNrU4kxK5fm+0iqOEs+ziwU/lyoXyrGsUugrQ9M4inpd23G560mlpFKO4+S5dAJbSVEqBoSSNE6X1FKeK0KIVSmkWcooTbNkHcfmhqZieo2MujpkDjB3w/C91hqGSKkAMEoZ40pLQmBxbvvG5eWwWDr+7OnBoX5K/uQdR/ZZaAIV4MjrjtkrfDgCJBsV8ftD0oq6g1746o5wNg9Mbp2snXvxVNnnLnMZtd9+4PDMcn/26my80L55ouza9lI7nlmJXJeBIOoKTfXMynlL1oePvLw+4I778gqgbu0CMDp4TWM+/MGPPPqVvyQUhBDKqL1KaQFhjKa5EEIWwiBOsvpg+WM//AtvtnPvfd9PVCsbxuh885t7qh8YDI6YyeHHrSdACOdMS+FYzBhTKPhxnGgpO+025XaWSQOEgSelTJLMsWweuLlQrVYTxhBAGy3z3A883w2EVJZt9aO+7XitTrdSLdsWc1yv010BQSfKoEEpybLrm3svvIaeTWy8tW+oZCfPXQEMoYQQYrQyxjiuI6S0bfvmw/d+8qd+9uT0Q0Y2tDG1CWtlfvr0mcrBPa8X8ZJ4jOOdwPmN3LIQ6ADJuoj/9wcR1AqR6gRsM/DsOl1/sug755a/fPrMiSSnuzYfATFphuGRm+quGQ64lyTd2dOO7WwapcHl+SaNjUK/k2dp3phNx6sbdq4oZ1SbV9cNAJ//288WAkdrAxAGA4BS6roOCDEaxiDJMs6ZyPVzZ19Bw4rVy1zQqRsWro1URK9P2VO9xos8c/aM0VoIkeWCMW5ZllTodHv9fkRhGOOUUoByzgmMTJIkTrUWrVanHyelcqlQCCrlYrFQ9H274HvjmyYMiNFGKeW4juf7hSAAIYxR1/U449oYx3WnrkwND6zGJlrAViB7g1J6NR766p9ZjBFCAEMAoRTjNqG0WCp/8pM/C2D/xAN7b90/uWPk8JGbygO1xcXZ1y+wjXmDL72KwDgFDAMK+L5391dRihq9gJVfZVDLTx997DuPP7K83B0Z2ZZYbDGbLo/VoAUrVca37rj50D39THdT7Xvu/h1je3eM+a7FUjMswy1WpTGzgUJHRR5pA4kb4JYD7y4WAiE158wAMKCMKiXTNHMdS2vd6yeUsSROTp54duOrLgMDsKxfeOLyI8DyRj4CAGhtBsvXYk7NdEObOFxoraTyXduxqGVzpY2S2rJtSohlWQaEMeK5lmNxEJZkWSYUs3iv2++02nGcKMIJI1km+1EipBC5lDIPgkAZUwgLFmfGmCzNjNZhocgYVxqVcmF0YpVZVQGKb+DA92tieeEqCGEMlBJGKYBVSsgHP/IT15/ZM/ZjP/7hX476Vn20kuSdv33wt4HF1ypwAJMEHGitJUwDApgAIuC8fpks/v1h++CABUTAhbXTUABwdO7hSC1Wq9WJLTvfdeCX9o9/lNsayMEDwACqn8xdXWwsNKN2Pw59Z9+m8a3h0FZvcIB6Bc5ay/Pr66CZEJzisW8/+ur6W73LjWZbZDmMMSC5UAAIqOc6SZpmQqZJJoUolSs/9aP/ZP2L5/pfv9I9mqNpZNGlheNTj/Vx/DpXcxV7drx8xr/qlteIoFjAc889/YhUShtEcdrsJsvNLufUsSgz2uKkUirYFpdCaK0phSFQmrS7vV4/bnXiRqPR70fXIhSEeJ43UKu5nk1BbNspFUuM034Ud7v9MCxUa9UwCMKwQAgIIfWx/08T0ImzL3X60dce+hoMHMcihASeTTm1OPE9b3h89zvetv5QySJQ3jny7qC2YIetpeX5J44/8tplm0XdWKcEDeAmoAzMAqDXaIyvg/T68K6Wtq4NCmgCg0AF4NddwMvz3xJJ5dCBj91++0eK5dV1WkrNQB41gQwIATa598iBnTuqIfctYzPmG2vYqZbtgFEmlGw1l9a3gIdhLUrFN//hK/fefc/6jOOt/3p5aiWK4oLHu4lSUmkYrTS1LM91kiS1OIPvxkn+Qz/2Sor2+fNPqMzHkQtb7A8Obv6Rs/MPRSIKrceAveuJCb/7u5964GOH9tR/GgAQADHgP/7wlxYXFpRUSSa0NpwzkYtIpqHnwZLF0KWUcms1/s9gDBi3LApjoOHYXEqlDImipFwu+i4RGr7nMcqEyKIoCQt+FvfzXAW+Z9k8k0oKURysLy4tKalXz6V+f8g0Hv/W35TD8qkzp7WSlEFrLYSyOGOESIXf/De/ufGNVVvu7SzcPfi2ZqX2HWQ35GoDmAMmh+ht61K2AyvAJUCk6Ll42/dqnVq3M7Z+6WABDGgCUbvdKJfHrpPVKLdu3/ZhCg9ArzzbxVQRmx2/ageREm1mrQpxZrRacHSWyyTptwmEGxSohus61Vqplm0IPtBi6H7nsa93u6802r3e1MrKpWLgWhZjlBFKKCFCKam0EJJRZru2xW3LdgrFDdsgXz/9h8vLSRC6K60LLZwEkhTdhcUow/C6HmZf+MofpTK9cnWV0AKDztGFP7kgPoc8yNI8y3KbM0oJpyQIHK1WPzJFQUir00viRBukaSaEiJLEc5wwDAqFsFoKa7UqCFlcbDDGbddtNVsnT7wo8sy27W6vm+cCUhQKoet6SRzleV4sFkSa9nr9JEmrhRsexvzeeO7UOU7VL/xPv/bRj3/MGCOVjKMYAOPEtW1CiWW9Yql4dd31LWXcd9Oue+646YM5XuF+AECOK68K1MXAIOADxoWPDVwxtfHJi0B74/arWseZW/1dbb0ys3hlZnqlcyVeXG3Ylc312+iasHbVfmClvQxgqDAO+MwKr83gabbQbMRpZjQyKftxEvV7UgvHsYbr1Y/95IalIQVw3/3vh5b/6TOfW58xMb6ptZx7nsUpWVUybYwSanVGy5UmoJ7vF8NgpXMaiK5TzaReGpvwx7ZHowMjLqaeW/z8sZNPzU9dAtw+FqbxWeBqD8er1dFSdew9t/76Co4DSODcNHxb1Lak4JSCW7bve45teY4duh7RWgghgUxomadKacemjmNpA04JIdBCKSUJIY5jc+5QTtudHgEJQj9LUiFFmmVpks7PzVmOY4wWQgFkpdFeaTQyIWyLt9udSy99D398PVKlnj956uT5qwBu3bdr1R99aeYJrSQhWP0gw+rXbizOGGN6wyG5V7DN2j7GgbG2WO7jQeCldVk9+wbmavX3sA/YBowDF9bSuzHOtvGddU9uwyt97wwvf5XoNHAZYKXykEotlpX8oc1AB+CvCIVOT59cyC9a2JzoZt7NIBIAcDdtuXV3xoOeMJkyUZI1293FlVaz3VFShrZYXwJf/SvXRy6cfAR4eQbcQn98uDYvyIIWmcVomhtGKaVESWUAo2EY8z2vUHQntpeBoIerISbm8VwQ9ArFYtktJqrRZRXHJZVipT2THHviREvO1jf7y/FT2+q7pi+eY5QDIlmJMGC+/ODnudtpdK+atu+4nlKKU+ZyFnqO5zpxHDQ6UbPVt2qh6zhckyjLLM6lNHEaF2yugX63D0aTpqAwYRj4gdfv9wkIYcTkJkszx/OlyBXhUT/1HQ54NmeNZtu2rFqtFvd7Uf+1Zq6XMTVz+plnn/vRD33cZezQ/n2vyH3wC0/kQmilOKdGK0KZ7XBKmDHq77/xn10/eOCun7lRqQVgHpgqW9ZS2g3dOMfTEbIK3vm6HzkjORYt9GO0Fc5lMhSSpqI1UahtfGzVFq5S3NrrAoQd4M7Vg5z9OBusVCuD24EMuPjqsw53H/jp1Yvess773fFhD+os3N0Hb/3ITXvwB//XrwSBQ40RMuVUaInBzTv9odV9WH1tL2D1/V//9f87y+L/8/f+47rC0347TpPU8xzOGTEaIJQSY4yUyhittFHaFMthod4HTmai/8Tc71y48riIguUZPXU1vni+cWH6XLezwKmZmr9y4sIFv6rb8zQoF09dvDw1dWVhZuqvv/p7rW73v/zxb5194Ukl48ktQxTEEF4uljgjlsUc2zIwFmOMcmiVZjkYt23L5twY4/sOQKQxUhtDqTEmilMCwyhzbNuy7TiOiTG243DbUYqQVVo+pcogSjLOWeD7SiqpZC7kc88/9dpCBWC+9MXPtqP8Rz/0mp+Ym51twRgYrZW+HqSljG3dNvbD93/qgbt+pp/0Hn/mc696j61aOBuWxawe+jbGKtjRxtfm5aPrKPvX5LJ28dKSOtfACoHvo9buLfX6TSFiC6+kNgEACkB/46rfA3JgEXixOhh4oS/ihYWpl6BvuKO/AmRQzw8MDYxvs9vxYtK7Zp6JD9v18lx24zRORZLm2vJqE1svnjn1l5/9g0e+9qW5K+cWZy5cK9RlIBSXXnr+dOsP91buBlpziWiuzBcdAq2VMpwzITVlDqXUQBEgTbMsozBkW/UHAenx8bR7zmhGQcMSyfK2jDl1BtvNhTRODty+/b1HfhWAxCmOfRiZ/dbjD8XL+fnTM1MXF5O08/Z376+OVOdmZrsrmcxzGjoasA3J+ommJslyQjS3OYNJ06xYLLCcaq2V1kJIi3BQGA1DiFYqSRKb85WVJqOUUCKEdFxH5EJp4dm2MSYMvCRJ00yEhWIcJdyypJSdXmQ7ztnzZ3fveCV9rycvPfy17549/eLoZP3grtf7vpzMY600iDFKM0osixFQ13c37bkW+g69wjtu+3gbD822ljdVthXwNuCSRJthkCBcQZOA9bOkQx4bsEcanea20ntfVcl1b2xMZN/qS7OtOMJxp8WWltoLt26990af5MC1D7UAax9tAWADi8BhAAHQsb58YXolihJvsFC6wRbDQNZ+wvF8ykKgXK5H6w3tRz7+6Ye+9Pml+ek4apeLRe7Zjz78YJzkw6PjQ8OD3KJKrmPC3HL7Hc9851tf/ZvjtZ/VQDC/5GuNwLPjfg4te/2Uc7Zqz5SUnPM0SyyKuNP5xje+Xt8mpckdXxX8YGDAWl5emLvQKRe2MsoL7taBuqgNVte6uw9AF9+Ootho2lnp+zX5vo98cHhs5IWTj+SR22nGlGojROBYzUZXGSMtmmbC4oyCEGYVi0GWiTQTvmdTSjyHu64HozSoMvBcV8mcccYJ0ixTuTCMKZElcUKocW0rz4XtEMe2kyzrdHqu56Vp5rmuZdv7dt28XskS1fJYZamx+Bd/8YVP/eKvZB/sOtgQE3oF/o/f+Q2llJKSEE0ASpgxRmtz6I7b3nXkeuQsAgIb5Uqpa+G8gaXhrcjWMD8EYAB7Ye0GMJv/6VxnqttNNlJunga2rc2DKSDH/MMzyelzjeP7a3emvdTolG2I5b4a3Y2soeucOQgphGorqY8+duK+H7wBGX1uqbN156qnKIBofaCkOlL96M//s3a7+wf/4X9xfJdQ5ofF0YmBwZHR2sAApSxXgqf4Sxd3AWPv/uEDbflsUI2eODq/b//Oq/MvpkmfEkcpzSgYI4QQGBBCOWeMUZmLvpbtlnfl3ItDO255x9afv5j8jeslrfaiRG47zOKF2zZ/EsCTVz63tNSaXOf7/t2XT/QauWu7MPqmA7cf3vZhAOOHD3Rx+dg//D4MkjjL0WeBw4A4zn3PBaW9fqwJNdq4riW1S6k22jicBS5PJSPa2NwiIEma+Z7LGS2GYUer+kCt3e7kUro2V0pKRVdPgOZpqpFnQgS+n6Qdx7Lv/6Efvt7CxIiTR59aWWls3n77p37xVwA4KK7/Kt11z+M6OiuLNmf9LAO00cbnjBGmgP23rafiBQB83OHTO4AswbnvnvhqyGqVvQ0HtRjpKiUr7vRarWjb6DX/L8bRC51nA6+yxebsmp65gLaxc9I7Ag+XF7+RJu2RoRselFoCKmtEyNc8STVa3x21n2aUyazXzVBcF6U++uzny+5wsXxtMb509SjRAobXRxTcl4XaWJjzi7XS4HB9aAyUuEEYhgFlFMYwyriLJeBYjr+YXlnwS8hyovOAwE06xrXd81cWozjV2milOeNKKwIDY7Q2xhilQCgRKkn7TSCe9PYQ+InzVKuVMbvh+BSImlg0wu7LxSvq71544fk7D93ebtlnnp6HNv1+z3atu955/djm1a998atKGiGlzw20tmxjiFVwjOacUAKjQBmh0Nq4NoTE/8vZm8VYlh5nYhHxb+ecu+eeWfvaG9lskeKipkRToraRxLFmRmMPRrbHBuwH2/BgYBsw4AdjAD/4wSsMA7bsGcx4JM1AsGazFoqiZFIUxUW9VXdXd1fXXlmVlXvmXc/yLxF+yOruqupqklKgHgp185zKe27c/4//i+/7IsWgEGZVrUnNtTM0boq8MOisLM6XVam08T4TgdoHRaS0RuF2bpMgIlpnM+WaGJMPSKjNI+BZjubTn50CfOmjSV2PJNm1jX9AiFoRICAjKVJExpj+Qv9YxwDc3b8xnT/3zKN3cDk8/9Mff/6V67/7h3/86wvL2nP9sedxHj6xunhmd/2akwxgB2DuIN1WkFmr6RHafgFwCeAFAH9meXG2vKghTuFS+3FXhM57Sfb9oozTg+1YjbhTtG++9rUXPveAg3nz3a/fvrG5sOC++PEHvJWlkwtQHuzucl3LQ71xOPf00z/3S39tuL/Z6XRiiu1ez1p7RL4iIjqAcgzX96H+wpnPz833gBtUcWtzZ2972DShrELjo4+JlEZCBAAiRSTMiKC0ImWKOdsdmNfv/9YQpgBnOPQz07PajCbrlza/pkG3B6zU4frGN+p659KVb93c+N39w93JeNjUVWfgFlsPlvrvvHZp+9rIOZc5S0ajIuY4Cx5SKnKbZa7VKlp5lhKzMItopRDwqLa3ViNipslY0+u0N3f2gg9V1WSZI0IiMlpZTd1OK8tclmVzg8H8/AIaPb+4YLUCIKvNaHf06MP/mx+dZI+30X77N97x3o9npSRGQq0VCISYLn7iFMDx3fHun/zp77678f888V6fOv9LX/7S32vZY2dPf8zC7gj+aNRsKuxsjbYAdgBeUgwrvbUcWgiLANV7J4MGwANcAhgC/EgLzicIm4fvRLj96O3fr7bebycEgcuPNXB75szW/WEIwfRsyz14d2l6/63LV37lb/2XX/zph+mrrZShEPrmcTsjxqbdaWljuoOBc1ZpjUDBexbRHiiD2TKsAEwXT0iAwriwtbWxt30YfNNuuZhYUJRiTpwSEwqLkHFG6163JYBPPfeJvN2tp02QdL38fSICKqTpjQ4F4t5s9kefP//z3zwY+nID0Qs33c5S0bnHVbOwMvjsly5+e/3/fPHkv/3W/e+9+8p1hZhnTiFwU9dV3e+2clA6I+997QMpozTFJJnVSpvMOBGaVSUIpgQ+cprVs7LWygyH48GpE8po771vfFnWg36nkxsEaHzShmazsj/o1VVjncncwmg8slkG6SMIBU+Ixxj6MB3WVV0FHwkBiQiRiJQxf/Vn/zMAWOz29/wfnD527km3ehDPX/xrAHB99FvDg90fPfPJzvN7oJoGDhykVXMR4PkPXeEAPgNw9T04rWNgitB4mHwEB/x9lo5BsB+SIywOludJxOp2VTXp8F01OHn39pXF1Wcevw1MFH1mafl6NX1c0CCciqLligJJaYUAkoKfTEYhsLaweHlre34uzuIWJ2Wx31TNbBbqaYrMvkzKaGYWBO+jYXZK2dx2evPD0ShzWadfxFSNhg2m1gCX13dvKGNPrl081r9oi+6rb3yLqLhy8HY5g+lMlFoa9LPF+eOd3jU/jGeePvmjP/bZuzuv301Xnlv78t2l9O7Bn3vvW87M6lppw4BOYdYqpvsTaw2QYgERiDEZY4w1edYKPkwms04njxFcTu3cHhwMO53WrCq71DLWSkrWEKToPShSptDGGJBUlZVShIBNaIhIK+rNf5h6/0PFt7/7Te99CAlAiIgTA4IA9effV2Uq5KyCtR/YnJeye+316zcvfctzffrZjjND9PSjz/7kR1/xQQPAwOfPD24DPI7qPSmeIIh6/lMv3rr9cneQD7eHb77z5urKXTL4uRe/+NCPVAC5T0Or/hygk7ceAep8Mx3Mz1sygVOoq4hojW1lLRG+ffOmfvPdqcqye1tbs8kk1Ibrtqallgmtdr0fp0aJT5JYog/CnFgms9m87YGwMQYAzzx1/ic+87lvvPoVRfwnb/y2MW779sHe/Xeeeeavz8OJj33sk03dVCVqjRJbinKu+3duj/qrPN6jpbW1ljrOfP2E+hQADPcPp7PSaUoxzsqpRjKUkzHGZlkRlQJOElMUwSzLhCMCiEivUyhIEaDdKQxKHaTb6zirRHBSNUtLiwjQK8vom5SiVqqpKgDpttvOZVobFtZKFb1e3TQ/RBnz5PiD3/vnIYSUGACMIgbWilKCv/MffmBLs9Tt9Z9sNvtBXL785j/5J7+zs7VXN8FlevXlhWdeOLU4Xzxur/FIPIxitH5o0dQTYrHz9M78a64f+6YDzcre/n639wC8YHid4FmA2b3Dbw73D6hUi90lltnymc77+7J1bWNsVVV1VSEkSTIdDXcTa1KApDd3754+eWZrawRsLXQrP6zl6uLgDMcgIEZrn3zudANCDmLikNgaF1MyRrvcXnj2ZAYLjS/qZtJudRYGp2/dXp9Mw4uf7gIMVulzUDRQuJ3dq6trJ27cuios7U62dOxEPb195Er/I8eOPL3g+s1LMQSbO0JweaYBQJF1tqwbH4Kf1s45RVoha02QCABTikKqYRGWJgpqYERJSStXlo0oPR5N5ub78wsLk4O92kciZRQGHw6Gk9zFbrdFRk/Gk8l4rI159/U3n/rEx/8Sn9BkMg0hMKcjFQUhKk3tYrA890FirQw+Ksn23tn9E9Wc+Wf/8LeuXb05Hk+YMcYIgKNRfbhfPfeJ0+mn99STtAgAMoKdHjwM+J07oiP8Jd4FACSoKSvmiqWNu1v7o4PnfuTBaYDgEwAMoMflDmkcV+V4Py3OLy6Xu8Phfn/tgfBzd3vTuUwpUqRRi3MZJpmVs1BXtLd1eP3m22UZyzEFUe2+sMD40JejKacYYkwxSkoCEhIziyK0zszKKndZq5VtbKzvxOFsejCeTJwzgqntestzF27uvwSwCwAAzS58d1RuzM13u/3Onbs37q7f7bhVp/t/9vZvA0CABgDevfNqTIzMk/FoPJshKlRaaVVV9ayqUwiGoJmWoQlF4RSpxDyrfO2bxIIABCwpKq2cs0qpWRNRt0NovG+YY/QhpaQJWVLThLqqJ8PRbDYVkbqa5XmRFYUAXrv2lyFy/S//6/8QfPAhIIBShABaIQB97qcetk283fqIoqmC7fHB9j/7R//wjdcv7+zsVrNSSZxrW0NSltXBweiNV278+m/840cv2gV4B+ANgHu9x3tE9sOeoD98CKQg5RTu22x2/NTyoy8SQLTWtbpuabVn8tTttg6Gu+8nGYBorYNvQggx+BhjihFJ9fv91WMntMICfQeVR9DT8bQ3WKr1F5xZEAAAIABJREFU3u7Wfa6l1+0eHuw3gZVSVdU0njOne/1OVdchRGtVt9W+e2PzD776m6ZFKPzM0+eHo721Y8fWTpxYv3/zLfiT5+Z/AaAq6+Hi3MW33rk0Ho3n5yHUcuvmeuOrzz/7KwBwyG8pGt6+cT35YLUAU0ySYvKSnDPWmgDgQ1DABJS3slaRAVLwoWkqorzmppVnKOKZtXEqNcpZpQ2q3NpUtHKIKc9dXerxcOSjOxqhAgGDb7yPZVWNJ/urq8uN93PmL7BxvvX6d1+9fGV7e/PurasiSROBAngwWUFrpc8+9ZAf3cFGuX8nsDf0SH96o/69Zjp74akv3ni6ufTyjXPHllbmu8eXl+YGg92Dg6/+2Wuj0TjE9MdffWn5+D/+K1/899//yIdww8NkCT7+KJV8AlA8UYX1Q0bkUNazLOOiaA96H/bTWyhaCz5s9xcHZ06eTcEo87ASBxFRGSsphRAIyRp7dO6OIei8yIG0M5Zsp7C9OmxzrWNZpSB5no1IFzkZZ7MkeYZl3SAAACpFiZMbqGKRhGF5cOJetfP6pUuTyazT7X62+PQ9denGrZ26vju3sPDapavJE8Cs1bIXTh7furP+7svb7dYDjX+Xyu9e++r67RQ56kghpZSSs7apfQzJN7Upunme1XWtnPFN0FqVVe2MOVo8OMI0Bg0UYgzBC2CMqch1WY77g07mspRCCsG6DHBstK3rkr3PsoJI+xCddT4Mt3f2tHHKmFtvXTnz3A+2jfhXv/k/f+vlt3xkrYhTijGmmIAg00ZAAGBx7dyFYw/V43Ofz827w8P1xflHOIkY5ezCswDPXnjm2qkTa5965gymcDiu9aw5trb2sQvDb79+NSVpmgh6CvAKwCcBEGC+Dz+5A1+NcKjhPoADcAD4ng/6Y330v0AwQwzSYGRuAsiH+09rxU/txT+Y06sAXW1m4IuHiR3aUAroY/B1RUggokm1inan19PtAWvQW1uHljC1qxiHVbVfl1VZNRqJBYA5NB4RGt8AgCKazSrSKsQYI0jIZtt8dbh15vRa8nFvaz818c2tK8ePnYl+q/HZ/hbkbmUWRogNJ3Guv71xZev23vy8f+nmb5dhb2l1lk0Xwvh2r5V7HyyqmfdlVSnSTYgSA7lYFHmSpMk0jWfhwukQg1JERNbhdDKLYLLMVHUIMRaZ0wTddqaUSjHEEJqqMZkF0okjIFptnHMiWNe+XWhrTBIwIiGE1175xhPz7Dvf+4ZEePWVb00O98uyZAbvgwAGSSkd2d+yYhJIRmlF6sSJx6lsy6vnFgaPwPElvLPWPhLPwamT5/tzg9feun52dWFzc4cXYWVh8G989lO3NvcVcwA53B0DKIAK4DWAUwCtSeXHcHM59x0YAIwBvvjR+RN+GKi2gpvMED0we0Z1d/T2qePUhguP6aw4KNBzAA1AB+wjdLczZz7xvW9/DRBARCs1m8YUY4rJx6Q37t2zWppp33U6rc581rLahp31qSZVVTUhJIGyaqwxMSZjnFIKWIzWh8Oxn4katO7eudNaxOUXPyaSxs0thdnawskl/WNLT13/1//f/3Xs2DPOtmsz7bZPVbPy+p0720MiIIS0de/PQ6Sb33O7WxtYRYVsNE2mKTEDEoGQtta5yXRmHKOAVhiQlKJOpzOezkJK4KNAss7VZdNpdbTRWKNWOBuNTKszG46dNVqRcCzLICI+SOZcCDE05craWl2zD0Ek5TaLMSgiH59spf5jn/0iALz4+S8CwEt/+q/+xf/7u5wYFHEIPkYAVkikEEW0NkWr9Utf/uXH7mCMCtXEtgqAPYAFgIPiISXtUve5v//3/8df++//61OL8yeXlk4cX+13u5Mmnl5dPTtXXL2/DapJUB3Ovr3QGgBcSdADShx4t74XsuncD7DH+qHqgf3ZbUSIMSJzAJaG2/Bh8Aymh7MOD/OWmQwPOsXxh9cz1DZxBAGtTWKu68ZYl5jruqLxweTw8KgRU5b19ubWzemkCROVoreGilbW+GCNMdYgkNYYYnJWs0DThLzno9nvrljTDS+99PLb71zRLg0nG9959Q8B7udAVUNCE+Pqw8Mtp93ZM8/WfjodHyqlrKPhePrG9zb//KVXq7CvSLiZVtPZ4eGhUUCELOiMnl8cZHkrsmhlOIFxWgS29w4DpxSTItAAzOIyqwgAxBitSJHWLMACk/EEEJCgrmqXZYPBXKvdcdZYo4JvjKXEKXcuxljXFbOg+sEfyad/4pf/4//kbxtrFAKDIAgCAiIhOGudNWsnzlj3+OY1+PSP2weA01H99LgWwdf3O7m7ubHtmbZ2dm+t39m4f3d1qb+yvMjMhLDb3CnrGuAFgJ9WsDIwq938+HQ23S33E+x8uEXxF42ETYxV1ZRVMwuhjik88ccGbnk0Oti4tVuHBuzj74JQhZgApJzNjpBXpXWn26fgMVVkHCFks0maHKbQBIaq1W61WzmgMlobo5mlVRhrjPcxxCTC3W4xfwyXT+oTF9fy1mBUH06a8fbGVGa5Tzt7cA2h32/PT6frVTVWYC+//fU33vwdwEkMSZEocJe/u3/vxub5Fzq/9O9+cnGtiyDM0UcEpMwabVRMPJlVLstaRaaNjinNZpVSiIQo4DJbZC4K1U3jm6as6rputDFJRFlLhMEHZ3Vd1SbLGck522q1hEWQEtmD4bSsytFkmlJqtQoivbd/ULS+jwnKB3HyzE+dOL+WOAkfaUVFgI8YBtZlFy48BTC7F/4pwKv+ETHSh8+cU4D7AB4ANrbX90eHB3uHOzu7h5NpWZeJw7mTS7XI+u7h7lYa70V0Y4AbR34tGbVX1NlecYIDHsDeh1sU74f8cCfQU8XPM2FMQYQRGfWT8yw3/YW5RTJAhB/+T7W1WtPRLA6tTQxhPBlOpyNdZK12r527TjfHOxs3a+/nBl2jbc2QEpdVRYTOucQpt1ndpCbGJqTMmVaRDxYGvflObAa7h3uN9zI9BJr4Q4wa7t6+u5uXhG5r3be6e+PDHS6pezLzPjVjhYiEarw/Pf5UpzM/t3Zs9VrvsKECTbLW+5C0pRRTHWI9jKDIWWe09pga3wC2ijxz1gCAtk7XMUQOzLryna4FAGYZlVOjFClTh9iyzkfOskwbiwi1j87lEaCalS6z07L2SnXarV6voxWeOn36h/lIAODjH3vq2lu3MufqJhEzIDmjiyLv9bpf+MlfAoDj5m/D404Qj1M8ANoR7mw37xxzXyoWOOu0jcoH/V7tq4PxREjND2wC/MUv/8qv/p1/6970K3Pt1kTuYrwrWmqeFkpl2uXZufwDtDY+Xk7Bt4Z1OZctfp9EBAAPdyIAWYKIgswYyTxRbAl7+7v5XDb1Bwakx7c1PfLE5uZWdnfv+KrRWitFrVYXRHa2tzUIJR+3x/f39vj8uZXd/Xhy5ePrr7yU4i64XBMmgBAjM8vRGiMSYnKGB/Pd888vnO2dd3DWu923L9VG5aMRunYWKv2dl79LYsfTSsUqd93hJsz2m26/WVg9yWFTKQLBk6eWl88Za4oWnaTsftXczbKs3cohVimllJKAzMomMswPiAiJQCkNwErpxgdFSuuktMqsiTEaEmcUgCiFrbyYjEc2w9pHgEopOrKEybN4dPYuikI4jUaTPMuXlhYnw2FeFFqr53/0cc/vj4yEiOKDZ5YkYAmtNdbZ9/kzTwoC2HhsbqaG5465MwCw3HnxP/p7L/5P/+1/tbe+LhwIxFmrBJuo/4P/9D8HgH7rY3vbB0bXq/Oqlno8q7Z5s+jNdfC5h1iH5aPkJSD4uMveuLf/9ePvTdZ5wluBG3tw6CArijmp90UCg8hHTf1BEytGtsPhIUwvnX769MMvLi8f396+xYkZeDQaTicTYB4NRxTCJFSHLQfnn5pbXV7q9PIrV67s7+wN+j1jLB4RtX30ISUBRDJGW2MSx+mknG//2AH3a5j12qtF3omse/2VxeM9169WVk5Lyi25w+1mY32rHMbBynKvd35xbfDpLz2V51mMwfbq3nL24hc+28XP/ezP/aoiRUTGaONciKmpG+bU+KAIhEWYa++NppR4Npsxcwi+nJU+BNLKZRkAHQ0dA1ACUhQZIVqtGl/7qrTWGaObqkycZtOJr0tNaK1t57ZwBkmlFFJ88jf40XiwB1FQWikBOOqbEymX2VZefOrzX/6+lz9xyMMH8P3f/Hf+7r17d3d2dsqqRpbxeDSs4r/8vX+9s9/g9IRTT63OfwHg8xle6HWXI+sOrgH0HlomPzwSpwcw6Pc+9aF//yAUnJuDlQ4sLQ+eaeX9Xm+p3Z1zxZObCqyjBNre3stdYUx2//6fPvxquz+XYvChmU7GMUVrbbc3GMwvUbt1eqHXffri4OdefG5UT8+deF4SS0ydTrusGh8SIggIgCilUkpa6yNCTt2EvZ1Jl1Y3Z80771z/5Z//9xQppXKtjbFeFVuDBbh48emVY2sU6u485/NgW6rVWvv8z7z4/E88o5S5f63+q5//7852/gbA9N2bX0EERTqkVPvILFpJ03it0HvvfRNiBEBFyjeBmRvvm8Zbo5rGG4V5ZusoLICk6hCVMa2ijQQikltbDvdmo2FVN8E3Isgg44ORb3y7lc1m08l4vLC4oEgn5q3bH/Zpvwcwfc/FbvoeLnr/1bfeYBFOfKQxNlojoJD+2NPfh5Txg/VUv/nr/3uryKxWjiizisHmvYX1G+984+tfyzRhStVoeOfOHV+ttuGnjs39fMMAMAQYBnj3ods88oVpwcfa+gdIBt/d/7N3J98d1pvGuUFreaV9ZnX+yS6NQ78bVQCA4fbscK8KB48p+WDt7FlUXHSL+cUFbe14eDidDPWgPXf8xFzei1NITdy7t3XJKsqdizEMx2MEtNYIoEL0jRcQp3QiQaHKN3/8ta9cePapELmpDr778h8uLfSqJsa0qUg6tpw/Fyb7zZe+/JzQxTvrO/du7R9Wb3R2incu32M6sIXqdVYvv/PdH3nmGMC+VgvCXFclsLCAUWRAR44A1HjW1hIRi2giBABEZjbaAGJm9KRqTi4uI018EwgwpaQoU1qlSQREY60ijRwFYDyZ1d7nRbtVFCkyM2RZFkIjnJyzRquNu9dWTj+aKH4TbPu9UVzvl1trwUOMfGTUcgRcK2Py7Pu79/yAiTW/9n/8b3du31wbdDq5aReFMXrK3f7iMZH0wvOfULlZyufubWxtbe8t9gfWUkTl6DTALYAz5gOfx2oK6xFSHy48hmg0MHIfYb6oqH/r7kvOmm6/X+SdAto5OIYD+tC5WCKKlu58J/paa5xbfRxuPHf6k3e3X0XgoGdNOWsN5vqLi/pguqH38zbTn/3fr1ib5uaWEWYL83POmBC8CFhjYmJjVVU1iJTlkCIzMwC0WznGZjbeZR+uXPnu0uL5BON2PznTrRpPaq3TccsL5+agODM3m73QvPL6d6Kv7707jFNeWVn8yb/xYncw/f1v/dNf+PH/5lPn+V/KP+eUjFYM1miypLSBOurImFmbmBWiUpCijKclEXZa2oeotEKEsqqtUU0TmVkpYk5AKs/zWdUIYKvXD3XdNYiZIwkpNsErRN0q8sXFeR/CeDQiQNvJmrp67KlxUGQ7AAhgHy7rm6rSWsWQtNHAgERaaeO+P/Hn4Pt4+/zmP/q1alY//9wnx/u35vrtosirhucXTi7Mzb/w8We68w+6jcePrQwKfeP+ujG601tYXlzQj88Wzqf1dCX7xGMHghG8XQfVN3r34H7kSKTydrH4nmP1+cGP7w/3tg/eqeoyhlR2634+H2hz7kO/8HQnapkE5hB9DM0k7HY+xEOxC+LDYRNrPW/J1XVZ6cGCjRH37urMqrXjxd7e9v5OGbyd67WLPJ+V9RGWBUDj8awocu9DYkBhrSmVln3W6reXTjz72qtvQHb97Imlzzy7dG9MX/+de5/55Pn+UufS629/+hOf0WCms3Iuf0qTO3siV6xz63rujGroU8+d/9al30DwmTGzyqNSiQMKKkXD0azdbnUKG2IMPhTOsKQk0ZDEBIlT44NVpLUOTc0iJFzXJRlbN5g4ceKi3cqdqwgBCQFFGG2OiRNju5MBS4whJjbWckqTyczY/cceGbXeb1Q/cl6blRUiAiCBoFaEJALOfv88e3KSvfbapfubm1lv/lhnfjHPD/bzMN5tsJ3P9ztLJ5+7eGFhbTkGAIDIoAlagzl/75axrWOL8wLyYYHTcnb2wxhKD57tmRogOz534f7s5mQy2r5zB06rRXPEGTYLnTN7+xvTySjF7XJYjfWoY0dzpx5ns+1vzULNpg11qvI2jOO9NXiE5LIL19g2pINVZBSC2o066t0dNrp+9sKnt/bfOn1yaX/z2ngrFNaVdZ0ZlTJHpESh935W1lnuQEBrJYLW0tqpHrZnx0+sDfrZ+sZNY+3C0vkOtM91i2+luHV71uuujvf4jddvLC8vHGxKanoxqRNL85q093H98iEiLyytnF36iXvr608/z9NJOZ2OJ5MxSZgMx1UD7b7JtVOEiZRWShAV4nRaGas6RSYsiKyVCsHHFK0xmXM+RA9BAJrgLXNmjDZKOTeelplB1IaSpBirsgHhjsIUeTabEmlDUNc/LNqJACKMiEfnDlJHSs2/sEPHqy//uUZAwMGgv35vs/FNKx+0pWqCUHup2+9nnaKellm7AABNkIQPh/vnTp24c+/uzu7m0uKigOCj+Al+pPleBgAjuDYJ9w+me3WTtG6/94K9sPBjo/29e4fvRF83VNs0k4n+8ES4spzF0GTeqJZEgJ3De+fXRvqh7bgKO1mmtCusybUygsFjpbe3NubmepevfoulPrG/0NbtqtwuLJZVQ0QxRWcdIh4OK8Sjea+giGJMgHA4Gf7MF3727auvRV/96k//F9e376xfvz65rzNlzh97Qals53a5lJ3DCe7PUvIakAiIkZiAGauyEo6zye2iaKUY19ZOJoGynFVllaKvq6qqSt/UkVkRzyYTbbCuGh8jQaoaJpCkqJrVqFQCclqRUgIoAABoDImYpml85gmYRZzTCkUAgNBlhoxJKU2ms7XludCUnlFbmzlz++qfnb74RKntB3Hj7t2jGU1CDADaKIUYUvooJ7mPikuvv344mjprTqyttJ2OPrZzM5o1nRaOJ9XFZ5/Ji3xje7fVys9kFrS6fPkNlmZ7d/PMidX9/fvjaqQ6F5omrfUertnDUT4JXENYfugE+lIJKoOOBuq0+7PZcHv/lo8jMA8wEQv42ad+YfzmVhMmHLwHYP8EqJY5hsBYC2IqmxBjGp3h+ffOphWs54Z6/R7jzFBGYEVyp5QmglZeCJpOWw0nauX4+RivxhQJVWAUpsQCAmXZGOOU1iEkrQ2RcraY6x2vx0H7XvRuL5+EXWXLJfQ2oW1lymhHpFKSmGKo6xCCCJAyFigRpcgAwAIc4u7urtbKWMssWuluu8PAnU4HRJSxSpu6nB0e7Pq6OhwdyJSAxQaelJU21hgtQMxiFYpCQtFKE6EwGKORoG4Cc0rMFnRiZgQiHWIwFOoQQxnmB22tVQzYbreR8N763dMXH0c7H4s//frvI4A2WjglEWZkYRCQvwidtRK/u7cXYwoMvR4cVuXCYK7r7P74Xsx6ebs9V7QnsTm2OCccvvfqG8dWltu9dp9as9nwjWuXbE5d5Jt3rxV5J1X2xMpRpfU+ybFCOP/QlipTOCibGtxJhk4Is4W5E9t7d9669jV+6gur6sHRR4Gem1vc3al8xYEBRC69+c0XPv6Fh3/t5ZWl6WQvQOQmBF/5Uhx/MDQoh5MZ6MpsNVHqCVJUIFQfGJ1nVmMs2vn8YncymWxd381cXteRMtPrLw/mdJ5lMSaXzxGCs0ob5axT2iwuLGjfuX3psN1d4gauvnpPEii0iQmItaaELILMcCRiI9IpJTzaWRiIgJRGhBii1poUpcghemAghSlxCB6EC2Vyl3c7nX5/UDf1Ylnt7W1vrN+eHeyOJ+Wgp0RpILKKPLMGQlRaiwgkZhFBRGYOkbWmwEICSVK7yBglchJhABhPZytLS1evrU+c7ffbKeJHNIg+aEkd7OwCoVHEWiXPRCgCeZFleetDF74fw8es/7/zJ1+XmHqdduHc+v0dZ42z2liljdOkQ4YzjsPpZKlbjBqPgCF516J+b9CfzsZhUjYbRrfL8sAJpPx98dI2PDgW2EfrtssGjK/H2/XmdHadVFH7CgDKanjl6jfvZC+3WovPLH0OIXY63dFBHhNQskB4MLwN8EielZNDJFKEPkRk6nfy9nsP5o1730M3LnoQheuZVHsSqrFv/OHuSAsMKu86Op0+Nz854D995fDUyXN53u502pnLlDZESgR88CnFI7jIOauVzfLMRGfIcWmYWRGEmOrgEVBrxSwURQBFWCttnctyFAEREWEESYkSxoRknOGkhQUwKaVDbFJiQYwhhuiPNHRFqzDauqywrjCuILKd3pwvR0SMWjVNqOoGBIQUAGiliYAIYxNRq8gMAIDIKfkkzpjxeIwITJRiZOGNzf3FxYGx2DT1ZEIpPVZWB3ggQ99+32mnqSdW63FVAoAxWilljM6cM+aJ9Vnz4Y7TGN4sSL+7uT58a+/82ZMq659bWbm1vX8wrkXAtVw5bt64/JYQDNr5/e3dxbn5rgo3t243fnA4HJOv67ocTQ85qTCVWQq8c395bbm1SgDrAH2AuD18pWG/MrfGKSauKh9iYh88sJuOxsPZlo/Re/b17p5U8/OTVr/o2I7SSitjKXHQBBjQX7vz9oVTDxQKV69emU4Ptc2YVJLU6ppOp1UDZ0AAgGi3tu6rYaONEp/iSFd1mVIjiHqum/c7bS7V1deSg+Ls6YtFVuR5blxmlMYjx0QUThJSEAYiNFonlhiSCMQk4iMAiFBMPvgocGT/iBofEBpYUoqRCYQZAAEFRFJKKXokbYyJkIJEPBqNJ5yCZ4HECQRj4ulkMplOrLHGOm2c1urY8RNLK6uxme1u3h1NDrRW3VZRNp6TiBIAQSROIoQxJQIgq6w23nO71TIamhkPxzOVW03omyQib755tcgzJI0gxphHu0Mbj/kd39/7Sl1Xw9E4JU+kiABBUkoxRa2fSPfYAug9akJ2ZWdzVDXlkVO4cp0st5qkcHpxYWk8HN3evN/vDU4sDNa3d954++pwNFbsxzTdrTf2RveXW2co79zZq0il3HS4LMNwo9TZ3u5ef9gmF9eWFptQXb16c384XFrc6HeycgYBAxMEPlBQpIajZwTjy4oQal9bVVaTMpvPhKEZ++nQY2BjLZp0/dbL7+fZ+vVLSDpKYml04akltRu/fvUrn734i4dc9udXRNcbO29VU89VwoZQ8qxoka7006cvatWKleGAJCrrK6MNkkJQAARASAgigEyoUT9QwLIEAQDBFBOLIEiMnJhFgEUaH5BIKyF1JEqClLxEeV8UBCCIwAzaEicWYRFBIo3GWtOkxCkiCBCCYOBYlqUwF62OUkor1el1O+2OmRtkWYHrN3d2N0kBohIQRCCkGINSGpEEGACMyZZWVjfWbwZfG9RVXTMnJQKkiqIAkX5hA4PS2lhrrb7y9htPP/t+np18iHF/AODeffNejNEaPaxm1oAIICpjwBnb7T8R15gAzADkPVJ1B+DppaW3XhndPb6yMu/s5ub9+cWl3Vzv7Y8GRa61jA5Hc90upDA93D4cj7XWGzsK7W6NB73WfOmrwGGuvTBptrlu1AzCfkB0B5Ny5o+denopy9z+cFuRMpJNx401toRp6Wu0JBF1oHrox01lW7lG24TmyEMfmDgCJIVshns7EkBrYwqdubC7P1mc76RmFlM5WFxrUj0L264rrsdCoaoPAGBABZMPrblesba7eXc2qnganc67tiBNmmd9JocJJTKDkMYHOkQNMYrWpBQBYIxJRLRSAJCYmeUBOwcARJj5aFcVIJEkIimxbxoBBhBCIkUiFGNIDESgEKOICISyQqyRlEIERCA02ojjVMUYIzODhsTMMSBSTDGFQK38aBhvlhXZSlYUWbff397ejPHAhwACMSUi4pSUVpqU9yGE2Cpa1rnQ+KYJ3ocQo2I4Mim2zhmXdTI3q4MAzqaTOzfS088KQIAHelp8b4DIEKA6GI4QQBtDigixyPMsc84a5+zSCf0oY0IA9gDcGIYFZBqW36+ZiFSRWV/PNPNof7fXdi+9eqduoJ4OZ5NpnVARs7Ht/mI3b5fDw/s764snCq14Vu5ubY06rZVBvjRrJuNqH0a+2ilR5XmrRrLzq/2D0SETzc/1+52B1blob1B6ulWmKgSGEjTlqpH2nJuWfjRuiA1iSrEBSc6alWMnD3f2RrNDn0CCzZT63rf/xcnlExub66Px9IUf/bmEzZWrX0NR7JXRWfEealgejq3rFjgXyjvleBarlLLgPAs0uhqzc3y0zJBCiYyAhAKACTlF0ZoQMcQEAMLMIoigkEABIqGAACSGo5raGBKmI+v8qqq8b5RR1jhCEkQRFgZjrNZavG+CDz6kFF2WZ1lGBCAiwgJAiEQIIohCCEVRGOeUMoiQZZm25mhZJVL9uYUsz1vt9tbm/d3dzRiFFChSSuPRUPeUmFN15co7CqUJgTQa61hpRBQWwCODeh9CAzpvfC3KVH4McAvgOMAIIAJMjnxTyrBdGLM/KgXUmbPnm3dejzH54K3RzFpELpxsASgAee/PFsA+AHXhJIAFmAEkgBwgTsfVfL996+aonIzv3NvoZCYlbmf5W29f6Q4WTp06K7XfOTgoG37u3AWLqbn2Pa2nWbsNkmmgvc3tCWbFoEs5ouL1ty4v9F1ulSUsx/7W+iGRTMOoHgMIHFtca</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy7d7Rl130e9u122u3t9T7zpg+moneBICkWkJRFmZTkRM2SvBxJiZUlL1vFirPiZWctr6wkdiRZkhVZpqxQEimaFCtYAAIEQAwGmF7fvHn9vnvf7feeukv+eDODmQFAwkn+ysL31z377L3PPr/93d/+tQO8h/fwHt7De3gP7+E9vIf38B7ew3t4D+/hPbyH9/Ae3sN7eA/v4f/vIA88dsSyaZz4Bw5+9P7jH1yrnu32rxGd2rPz8bWNi1evnPK73W6n1em0lJSFchnKlIZHOu221kornfI8UK2ljmWilQZgWVYUDoyBkmpyeu76ylnPK2jS63Q2k0QzTqRKuHAsoWVkCINRLFOmuXSu2woHoS+EbSPbC1uMqziOtJbFck4bMfAHJgbl2nHpoGuiUIcdNeglnBMlDQjVWhvAtiwQQ0AphZSaABqEEm1bVhLLWCnGuGMLrbTS0uLCce0oihgTxVKRcx7FiZJJFEVGKeE4gvN2qyUEjxMppRKCz+zdFUb9QbBIIAjh2UyRWi3hlCZL+9c3ry+vXIG2DAkLhdFj99x35sJrVOhiboRx1vHXOrVgeHRi7+49vWDr8vmVT//E7xw79uggGFy+9PwXv/z72gyOH/3k4rX173//C53GQIZSeNx2IRzNuTBa9dtIZek9h/dOzxcOzH+aMnX2wnc2a1vjkzs/9PQ/2TfL79rak2evnz3/6tBYPho0Tp7++tmzV5Iw9oRjs9zQ2NAv/eJvDvzWxNjRUgEXLi//r7//60Dr8vladpiUsqP9fpDPDo2OFKXs1xvJ6sraRnXjwx/5R7tnD/7eH/xWMZ1br19UhDPCg7BvCYdQWSyOZLMlaeopnhsuDmWKYnPd/Pzf/5evn/zOZ/7sX5P/8IV//dhjP9P3e/vHpm8tcS2qj9sVADFw+dKV1aXFRm2jtrlmKD127OHJmZ3Xr1+VSqsknpqcUiZI4qTT6QRhnPZSRkVB2Jexct30jj0Hv/PSH3HmaKtVry+nvTxzkiiKbYtDI0k0gFIxt+NowuNd9Xq/3lqEcjNkbmnzHLX73U4/l+XjM8PC8XptH4nd63dGRgsLVza7raR1lWwsdzkDwBKFJNGUM8cWFMT1bGJIHMdKEwNDgJRrJRJdP8qmnVw+q+IkUZIT5HNpECK42LFnj2O7zWYzDMPA73WazXS+mMtlqyvLjutIjUarbQu+9/HJbNFt9y4RuNnUsMZgeMLK5+cy1u7z51+q1Vc4UtXGtaef/OSB8Y9dqX+53l6cnJwacsoEV7/47KV8cfSpo/8QwIsXPvPw3p+6jRWv1pKNIfEMgL/5+h+ev/B8b4t4blpikBlOLJaxbbp1PSKW9U9//eeBGaACAOgAuXepUWJ8Z7mzOmYf8JwRoAvsekuXr1/a3BoeTufxwCa+ZWGqgMOAAMTtnQxAgH/1+7+iqWYEgzCmsCxLjU3NHLvnA432mUq2vG/yIKCA8VtjuZexpvNF5It3rCnqwK4AsABKyejoWDadkipYvr6ya9+hVrPupTIyjkQmU6qU+v1OJOIwihmhw8MjmxuLpdLQVq22Z+89r59+rd5YsixndHRo/8Fj+YIIZWNro8c5oSZVHCLVasMgLOQmc+KoJud4Snfr/U5n1ctEnV6UyJgQUdtsT87awyOT83MTFy8sF/K5QZfLaLVLmC2EEDRODDWaMWbbjhDM4qyQS8kgHFCHUhZF0rJ4kkghuOvocqnY7/ccL0ViQohWypQrRS5sx7bSaRcohIE/sKlRKoqilOdms2nGLTeV0loTSrJZxPHqcGFvaSJ/YOzxK73PR530oN9bbX5zYmryA8f/WwAvn/uPl66cbLRrj+//+/MVABJYAdiR+/tG5xJUBUYO7f34nXvsap26sZFEp8vaSNc2qeagrwJXpZI4tmyW2XV0Frj3tlHvlmQALDyx883uG8B5YN+dXfbsHvaBpImT3bDT6y4Whu4D7laTBAAwPH6ktvGi8IgDR+mECTuJTKfdqG5u+vHmvkkfmGp2esXcwe1R7L/65V/bNbHzrrkKdhHAhZXTBBlGiCVoKp2t16t79947MjG9vr5ECTPa5PNZ27GjOA78IOj38/miMSaJY8JYHCTjk3N/9u//d8uLS+NidHzs6PH9uVy+2wz8MMlm8pYbP7n/p2dmjgdJcKjyDIC15sqjcz8hcu6162coZem0bbkyV2E6sYq5sWwxWLrqG0mrm9H+nR+M5cbG9Xa7GRmlHc/VCqA0nXIYZYRQSqA0CUKpDeI4cRybMaqk4oxJrbWGZQkKbXHBBPfS2UpliBAThRGITrme1hCcxFHEGZNJTJnQxmQyns2Z4oE0XW+oEUVxvdNtbjVbW912u1ouTx2deGBTr6w3LzMRDsJaOp0aK+6lsAB6rvbtrf6F4aI/6nySYQiABes2ea8AMmSJR6YU1Iuv/0mj5sMwEzvCjdMZh3mxbQubDf3kj/3jd0+sH4gMEAInAQHkgABYAXxAA7aL481g2Wa5krMLQISTHKPbw85vXpWWk2FidOJgvXEpDOtKSyWlSpIgCPygJhOUvInTV65vLid7dz9963nsM3/0ZwA25SBNLUBfG5woWOMBWtcbX6+kj/W6fUMgZdLYqm2sLz/2xFO1+lYURjDGGF0ulwZhP4kTvzcgBCOjY1cvns0VioOen88VVldXX37pa/ccP5Qt64R08kP+1np/dW2p34u5xUvD6fHsRy1k8qXBRtxZa1/d3Gh25GBx8VzkD7yUzUza8dxsYSjrDistB3730N4PTI6XiZlu+YuzszMT4w+eevFlzbhjCSUTRpnjCMYgpYriJAjCKJacCymlZTGZSMKoawvbEp5n+4OQMZJOu6PDlWwuTwhJZFJdWyWEV0bGGCPGaALk8lnbspTR/iBgnDPIWMfSruXzmc3NRru5JiNQo3Sc6vZaS52z3V6TQF++/mIul8llhwuZHdXBUkTCtbWF+ZnhHHAtOlHg979l13NApSWvZ9n0pa2vXDm9eeX1RuxT2xIypLHPCKHZUmpqdveOicP/H/EMQAWYA57r4rSNPnAIqABDPbxmwy7ZXDrtNPY0sRJgK4Wp7TFfe/4PLp9/9cjeR3ylM+mhC1de8FxnqDBM4QbhQOmE0GCiOHZgev+emSPMflN/8gD4/qnvPX7oIQAAnUvdC6DWTuZLH2sNEmHFKokZpb1eY8/eo7aXXbr2ku1kPC/lOg4TvN9sy1hFUTA2NqGUYtwyQBSGO+Z2f+3rf8wtd9++R4i9tVL9/uXTdU6RyrjExFHYnx65L8GXJZZq0u1vjVW3Wg4fde38I/f/veVrV9c2Xq36iwW3YrO0MWZseK4xONfo1rw0I3yrWGRz5bm5cuVPbUuDam1g4HoiDgJGwYRNtDGccUIswbSxUq7laz/RWhlkvFQ65ZVK4JS2GlutTjeSplwqEYLKUCWVzmljHMcLfd/3QwNMTE6q6kZ+amKzWueCJZE0A7a1rii1GNeB36HOcBgGcRzFKpo8MAsgm7PjuHFtsX76zMuFzPyHH/w1uXN3PWxlnZ+cs18GmsC2laIAdmsn+nFrTV3IpqYD/1lKGAEJwkhwYTGXS5hIPH3/p25jSQg4/y9Itq1NrwN1hQAwt25k8H4AIZZW1zrD4yhi8uYi/c+98jvczq2urv6L3//VUqmiDUkSGllhEA/CxDz9vl88vPv4//W3/6yczRVzFcbZ7c9jlbm4NWgd3/vg9vVmGKS5yDspAM1217K44BTGXFu4cujIQ41mq9moM25zTocq5URGly9eWF1azucyM3O7Ll88m86kZRwbpUHF5z/7R6DJ6GwlSnR/sGUipmKPeT1mywwbitEPxVrMRmbYM1bGZPMjleLofP4RF4V652yn3W50q91ea+DXQz+8Z+/DvX5reWGl3a5OTs7uzk8YDCzMvPDSS0Zq1/WSJAGMzShhFIRwAFQIS0iptDKcU9vi2lCpdCGfGxqucEY8zxGcW7YdDgZMCNvixXIpSgwxJgh8rXSv12GE5vIFx/M4FxvVWjqdSmezmUIlSBpCMNtKFUteymOtVtcWLud8fGR3OmsVsuP9sBMFClTli+lsZf3a+qVW88pkqRLANPBsBlnABk4D47d2wrWQIDdm7/jWC38ljGsLSylNGfFclxE77rF9D5Tsm+fXW82mO3EOUEDmh7HtNSDvIg1EwBbgAuntG118dir7YwwDYAuYBACIpfYLfiDrtfag1w3jfuD3R8fGR4d3xuGgmLeP3/uxLLPHhvTa1max6LSjzYw79ybPfuO3//nQcHlmaAeAU4snidDcsQKltObN5qZjWZRga6saJ3RiYurrX/tCFMalyhAxulDK+/6g1+kTYHJqOgh6a6urk9OzoR+UK8OvvvzitWtntDKHju3R8ButOmPMSdmJlmPlHbaX8fvR+PiuMZIG6i5Ent8XiCUPg5p64+KlF0LVJ4RUN1u2A0GpP9iq19tSqYceHC0JyjHDcBAovPTys0GvH0tFCRjjXDBLWEoqGUVM2JlMSikdJYoAlHGtNSUkTqTgLA6jem3TdtxMJq0BY0y32xdCrK+tO25KWKLdarXbLdtx+v1BIlUSh+sbmzMzk17Kc4peu7kWxbHUgdL66KEffeLgpyYn9p27eKa2uUFdNT18dKg8cWTy/vV2PQi7y2sbcdzt9GrtsL7evDZRlG0M0pgCOPDyCr6dwy7AtqBeufTZK0tXz7x8OZvKcsaVlgC1LUtK5aT5I8cfBvI/jDrbGHoXJAMwB3gAA2oGNQIBTACQ+A6FZWMWcAKcFtix3TtTnq5WLzQbgyiUllCOJ+7Z/8EHjz212VjOuXaYLI+XJq5cPesPdJSwbl+PVubf5NnTzzw08OsTc/ddXLw8PjoX6WjEKTmU9/2EQtu2Qwk5e+bkPYcf6PX7p06+EodhsTxSKGYcx42jOJXKjAyP5PL5hatXCsWi63r9bjubLf7lf/pjJUOppZtjUrYdl3Bhz81PaWjXKrZ6K1Sr8lAlTcaBmRghg73RW4mt053mRi/oxEqZhFKkUrmYMzefL4PpoZH8dGEGSHEc2Xa16r3Fy6cuMW5RQm1bUK25ZdmC2pxZji0El0oTEKlNHCvbYinXpkTLRDqubbSOojjwg26v32q2CaGDfk8mCeWs02rZFndc17V5s1YdGR0hhLRaneGRkVZntdp9PVNwuWAF954PPPGrQ9YhIL3SPzE1M5orjSndDrFQXWmdu/5GEvvN9gYDsSxPa5VKm3an2ZX9Vq+dzaa24vW26sZxt6VbRb6nh4uvvvF8dWUpl81lrGwYRXGcCC5cz6WUZEZxZP8M3tRnXcB+d5y7C33AAhaBy8AEkAZGgIpCjyIPXAVOUdwroKo4k8ZRgfFbujNNCmFCF5fOUKK0YoTSMEhy6cq15fMxcefGKhvVRYellqrrq5tbrV7/wPybrjH3sjl/sPnqq58X1uzhOa+bbDWjetquECNtx+GUbm1tlspjQ0P502cuHDhwJFGGEF0sFgf+II5kv9eZnJiI4iSM5ORUIY6l56UvnD/baKx7rsUJ9QdbQ+M5ww23Vbu1EfSjsHttci5fys4O050dRDmMWxg/0/h3pUJ+jMw2omspNx3LrSRU5bILlp8a3T+Ia51+I4jbzc76cGn6+OR2UGC5MN6wHCuKIssSjBDKmdJaG2JZDrdsrbXgTCYqiKQxhlHNCbFsy8C4jjPo9wPf58KijBpDtNZKynQ2V6kMXTx/dnLyoG3RhcsXK5WC4NT3FbdE4PtJlBjjDtrKTonhsfEsHX7x8p8f3LVrV+EpQCAPgxrB0E290/naqX+T6DU3pR23ksvkh0dlvVGbmChqXOr0go2Nrb179nQaIYZhIbNv/sEFnLpe727WfCkTrYzjUKW04Gx4NGPQJm+aZdl3ZpIGYsAHrFvn4G3YNpu2fcwbkDjVwoqNMIsKMFVLnq+Iw74fwkMMertjfGTuEb/fP3v+uU6v2QviJx/+2BtnXwxlLSu82lav3l/i2llcXwtD8qMf+KXbn8o/8ejfbWpTpNthEezITvkS3U7AiCbGSJX0B51Dh493BzIMwlQ2Twi3BSijSSKVVOl0yrbthcWLxVKJUoSBT0Fee/V5SkkcS8ZZGEhuiziMueMkcdxqNkuVqUxm34Q3D8zfdEiuunalN9j41tWN9mZQqmTTYiQ9Gkdh6CdXr68t7N1xJE4SqU3Jm8jkbr341NzMYZBzlk2UMoYyx7KCRCaxiY2iTA380LFEJm1zwft+lCRS8TjR0nEKYRRblqWVJgSghFJitE5ns5lcPo5iYkyn096ze9eabWsdN2r1QRhzSpWSSSRBRSZVgtW+vvL84tLrj9z7aT+JN/3T87ljAAiGbhNvrlQYjQ15aPqfApefvfR7w07Wy1AHmQHY/tKhPaV1hsfHh4cA2NidxK/1B4Nee+D7hlHKGBdCGKU0YzNzMwRZ4DJwz528aQClO1soEAHXgeJbeNYBvgE8BRQBAiwB08ACxwcqNzq8pLDERZ9gZs6bAWDBUsDVxgnPcSZTBwBk8vknH/3p73zvs83exW++8FdhEEQmoeZ6r1uXwKDb7vYH+3ccPLpj7x08A3CLZABCgDIkUQDBLMGb7U2ZJI4gV68tUyooBaG0UskP/EDGsTHJzOye6sZKECalUl5KJFHU7rSvXzunNTQ040xLyZhk2jKG1bf6QeSni2Iu9TBQvfnM1htr3wbPbW5tQJFUgXvF4XtnfxbAicVno616Lpc9d+WVWPUdNyXj6zQ1VM1+YQQfAVg2NyOEIAT9fgQYx3M79Q6lNOXagHEsFoa+JSwCbjEjQbKZDGXQ2vR6A8ZILp8PBgPHc2wnBeDQkaNRrLqdNmOs2Whw252e27l45UIul0lnaW9xBUCqYA3tmZoaP3Li9BeYNnEgbas4IsbtzAreBtHxqXuAHwMA7AoGamWxed89u8rYFYMBhOGTt/cOOqy11fNSQoY6DBMAQRA4tpdJ2bPjB4H9QO8tjyi9pQVADjj6du1XgB+/udEbDvYBGzWsDN2wwHxAMZSun23R2VfyqRvxl1ZUo9Ra21y1x50he+c9Uw904p5lqUIhtbh8Cia9a8d+y2kxZ0BCwi1+7NCh993/gbsefLfbEsWxDGEJFsVBrVa9cPaNhx75yCBCr9tllDMuqElsz21ttGxL5PMFYYm1jU1GYQsx8GOl1MkTL0VRDGhKKYzpbhmhp7f6V6WIPFEoFMqZTHZFnpX6YsFq5HGwjrN9v9doVb20qUzPDXqdJHK35KXBQK6tLGRzO2PZePKBTy2sv0qhF65dTSAHplUlwQg+zmhoCaq0AXQYJuubDcGY7dicUWU045xRxjlXGg4HsR3LtZNYSSmZUdlsaXSoUtuqObZrCGk0Wrbjrq4uuK43PjEe+IPmVr3X7YWRNFpn8nnbtqIwEgXkh2xfX8lms4cP73bd4RE6DoBSviWvlPn8bbK8fqlzenfumVvXx47+1Bh2AGUAXfy1RHsEu7Yvt+G4VhiGgueUihkhUiUyYTGLvDytB/60i3dn3b8TOsDxm79j50YyYFThuXV8bwyjQBUQwKwRC6+/fubRRyTHwwDK9lDZHpovvKlHc1bm/U996sVXvnRNLWhDB0HLSdmB32C2yhfzjx4+4Dl3s/9unuUsa73VTGS/Vr1+4dxp1ymNDpcvXl0GQAghILlcOoxCRlg+ny+Uhq9cPhdEcTmXNoYMet0gjK9dOQujQYjWBgTd1qDbirO5IYIgDAOX2lo5rfaZ1la7lQ5HJr6foBAmXQabM+dw5WdxU4NLsfyBxz59fvkFFcvRlB6dP3Kluwhe8H0TdtMRXyqnvr28ucoYsywahzEhhnHLS7kwWkoJwgih0hBOmCWoNspybD9M4ijJ59KZTMooFSZhuVTsdAeMECF4ksh6dT2VyR6/777axsbo2BiDXFvWUZK4SnmuJ5jREVu4fD2Xcx07N5Y6aOMogJcvf67XW3762KeApav96zvTjwAMyOS9O2JIY3gzQlvG+y8nf1QUz3KUKTTwfgDLy6urlxKq25wRRjmBIZRkRrSdH6zXz09P3QvINfwnjvQwDgOzP5BVXSBzM0t0Y28BAJeBHUAdGAcC4PVRHAImgBOAAfYCC7O7x7O7tRxkeOodZx9LH3jmqV3/9k9+RTjMYsrEiWuGmXEdz/v22e8+sTdTLN5Btbt5Vm8FYdBcWV24evFcGKrHnngylOi0W5wLTrmSQSpTbjYbtutw4YCgVqt7jpMvFqMgVkovXb/a6zYNjIExCpQSo9WVc1ePP77HKTJBvMQEF86/Vipku1uktHffWu2Ve4firbEu8Y9rOrh9JSOeBWSPTpWaaAEAHNsL9mZnA5gxDAMLwGq302CUEIAyZlsWYZwSaGVAaasdJEoaY7w0g9ZGK22MAbFtIThNp1My0Y1Gu5jPep6rZJJLu7WNNc5Z5A+qGxvVam1ufqebyqTTacYF48JxRKlYKIyO7Hpg8uXX/tp1yPOnv1opXhyZsJmznLPYF176X4bHKjpmSXFTOMRKNabEXUnM25HJilkLQxs4wzFUwTIw5Ym8kZxyppUE0cQYY6jFvImRPQ9ObQdpz49jBrAACdRx6095N2Jg9bb0ZQLgZkp7F1ADXgXGARfYDXiAC4wCe7bHFpEDPJY6+w6TJ9tT2bA+/PSvPvfiXzosJoaHSeiJ1FZzi4oed8hdY+7m2drK1ZWli83G1u7dhwdBPDE1srS0ybng3AIhrmMrpbTSkQoyE5PtxhbhVsqxORf9pB9F8bnTrxpjhMWllGCEEGI0mCCj06OEd8bLe68uvE6ToN+wOv0tr8jqm2xhKNSD+XvHfxKQt5bxxtrvD43bY5gB9hRx/3bSN8vVwsYbhfxQ5GZs7E+wqCMXlERRYglLWGLgRyqGNjqWJoiSMFaOLdqtjutYgjNCaNqzLdsK/LDb7RMgGAz6jBrCUi7P59L19WXXdm3H4YwsL149k8uoOKCMKRkP+j3BxPDIyNj04SLG9+1eW1n/ztTsxJz3cSBbnnr9e5f+pr3V1UF6Zn7PXGl+gGqos6AjN1/ohITgOHQ7FWyoHl7Iw2gcBaYAfPTpv/e1L3xVK0kIjNEwVGnVr6ugG9yMYtyj8c0e/BymeziXwRNvx4MTQPtmcBU3GZbc9EAT4KUuTBYh0AROAC5wGBgDYsACVl++8MWUQ8ZHZovuOjD2lvlvlGB88+SXs6lcsTB66ODxl05+nTN88OH3vXrt64yJrLfjrjHsd3/3d98kWbW1dO3y2TdenZzdyyjbsetANpddXd0QnDNu6SQaGqkM+gPLopWhEc6wsV6VyuRyac7tdnNreen66deeV0ZSQimhnFMQojXSOVEcZoliVJera+vp9Ai1ObVCba12Wn6n4XBK88UdNjIAArwhsHBl8zJjpt/XBW8KCLbPCAd0tfdC6Fsk1cvRyWvROlW6uuiHgUx7rmvxWINSdDu+MsRxHM+1kzjO53NcCNuy4lhyTrngnHMuBIyScew4llHSJsqPImZ0aXTCcbxE6X63pbUqFArNRiOdSg0GgyAIstlcz+/Yw3TcnWr66zPlAxT+AI0r9VMptxyHamJmstFaimivHw92eD8OnAWGFK5T7KPY5twiUACgcEWCediyoc9VV0fTN/IxX/ziX1ECA2MMLMuB1pZtffyTv+GKbY1QI3BDLDm434b1DubaGDB3u9m3vdHAVWAZANDkkCESAQOkgF6IJY57AAY8m+BaojIggQIreJWbKTIAwV0FQnOj8+PlqX07jpcyYwd2PXp16UQ/XN29c6zfoZOVWZA7Ii/09ot+v10eGt4xv2dl6dz58+emp8er1TajzBhorVIpB8SAGMGsQjajDfGDgDHqOk4chf6gd/H8G1ollhCcU6W1UmrbPvC7st/t1jZXzp1+KYlVtmxLM8gUCvnsTKUyNrPTemDHTomF7TVwNAe4Xp7oUi4HqHbxEnDCx3e3Jbh7bK9M6jTJd7HoWuXDk79SLM5rpbXShJA4TsIwdh3LsUUubQtOAQx8X2nipXKcM6m00QAhSiaUEMf1CIwxRFse446TzpSHRlvtTugHlAvH8YqlCqE8lclZwpIyvnzx4sLCxW5vBfDGRu6rduOLW2c2O6/XNheSKP3Ug08Su9psL/f8KzLpAj4AH19imLlNxrNAfV0/x5C+VP0+w4OXW4Wteuu1pT8EsNHY5IwxzikhjAmlpJQJASl628pMA0PATgoLeAVYBE4DC0D0dmy7CyFAbvZMM+z3cBTYDYwCmt1QWg0gL3BobGR678Tx2dKB28/li81v3Pp9bevSXbMzoFDYuVnbaGz2uMzDN3d3ePSZo3OjuwF0fG2UsgQtlUr12vqBQw+OT4yvrlaVVpwLraNc1h0EPrRyvYwxeuAH3V7PsSzOadDrrawun3ntu1LHSmqAUEYZY4JzQhAnqjQm8kNuHCVKkWKhNDo1bxSOTP3I5bXXyyMo0591YW/glQyWGIZ66BImBlu0taHbUW88/6DAzgTPMdAANVsMp9yJPDkmSeRist9Xi1dPDQa+UlpJTSnxHAuEySTq9ALGuO3YRpt0yuGMuW6qUikmUmmttNaCcyMlt20v5TEq+gPfS2f9XieOQ2p0FCee59XrjWKpbFmi1xsM+v10Jv/YA88AqTQbL9g7hryC5bi2W9lZuc/G3tH0fCO8CqYKxUzdX4Sz6mMpg3sAG0gABjSBToYcAdzx9BjBfu5G+4Z/PMp979TVF7/2uWcHHV9KBQMhLK0V58xzPbtMJoZ2hvgKxwAYWPAIOHAvMAwUgQFAAALU3hqYDXBCoAtwQAEwWKmZepo8dku3ALsYSoB9y1ATKAMMmAFi4CrgAE7Z3X1rzoJXXmxeKrh3qMwvPffHQT+sd7cEswXj+cIdbgodHhYvn/mGBBhFJpPNZYuul+p0wkOH7t2sd8AsbVEAACAASURBVCnjggtKacrjtp2Kw6TVagZBoA2t1eoySQjRcRg1W43FKxelCmSiQQhgtFLGmG1JxbEkxi4NjxVHRzQSP1oPwkbGK794+a+FIN2mu2K+CFQ3Nk6umksaK1DZlNkXhQxMq8QdIG6i2jQOMLvVVX6gLl08f723ul5vALh48RXOmGvzRBkYCa0TqWKpNbhj25m0o6VUShNoQigAUJbLpm3LSqc8y7I15UEQtpptY3S7O2g2GkobRqntOBS622nt3LXL81JhrJWUwaBXr9UurH71cvMrEtcAAFMe5mcz7xeoAG0gOz12iNLCLu/npnI7I1RG8Rs3TzcBnACK2+fmdgQBQA4PAt4s+UdDxV0bqzWjARhh2waGUUoJBYHyB8CaAwm0gQZBAXeYejnABjaBW+bgm+rExRCggWXAAmwCq0C2TbcYeA1gQOq285cBLpBdWTkFnNA43VMr/fBtHIJq9fKL525ouMVWNQE4Cv2e2to0565d+d6F797Vn+qwND/9UBhByQTGWK69uHDpwMH7PAf9vs+5oIzDxJm0p4HNjbX53fvL5RJhtm3bgvNUKi2lqde3VpYuUoASMEYpoZRSANucszgzLCYinJmaKg15moSHp/aNjQ9z1vqRXR87WvkZh0wDh4+O/oRr9jXMGgcrsr3cEQr8wfkPpLBfJ5ZLJgB47rTg6f17H8pk+IHKRwBEIbTRQliGwCjNoKNYxlE8CEJjtFSGwSgZtVstGfvGmM3NWrfTBTRlzLatVCoFQg1IEEaUkGZ90/f7WinPtS3LgsHc3JzUemNjw3G9dDoFY9pbaFfrZ9a+uYLPAjEFAxaAELCAbq218PD0fw+kPDw4jo/cKe3t8FURb4d9pWd0QjWU7bicMqM1F5wQGAM37QGiBQk4wCHcrAa7E7cb7CTAhZu/p4BJIAtkgD3AYwQJcBHoAPotHusNo2py8mOLK2sXLi001rtpJw907yBZePnBfR/V+obfNlsYEcDk+IEoiENf9tqyWg//tz//53fwbPXMSspL+f0+41xwmsTh4rWF+x58tDPQBDdSH0DEuMhmUjMzs9evXgyCgYwDygRjhoD2+93NjZUk6hkDbYwxhlLCOUsSKRPFKLVsYVs2Aa0MjYeB5CyxcXyY3r+5EQAHgGLlRvB6Olb62oW2L/sBVrjbbde6fQBAWUxnMQdgXNy7o/C+LOZKuJHWaG2tWJZtOTc8aakJgGzWo5QBhFKSJIlrcwPGGKPQUqlEyiROOq2OoYwyZgkBYwa+r7TxA9+2LM4ZJZRSdPu+AUnikDE4jgMqjFFK+Hv2HZGSF2ADXwQuAEziS0ANIMMTb3XQ3i0YgRCCcx6GAWeMUUYZowTt7haAAp4EduJNAv0guDfko4ELgA8MgEtADHwrwGY1eR24cmcJ+N2YnXzC75leu7dw6dxd6dQRZxeARw/+6O2N9x15vJd0B36r0WlASqLvMNHo3K5jlCOTSbsO44JdvXhux857Ug5a7S7nQiuZxINM1jUUcRx3e+35+T2VUlkmYbe1GfS7m9WNxtbm+spVGGgYAiITqbQmAKM0UZJSZozKF7MP7vjRYfp4pjCazrrbz/74I//dnYFEjIonZmefzNlzFuwDxR8R4FFSB6Cxsdw59VZZnLx4wZgklfKiOOGEGm4RLii3tEYm5UxPDhFASUkJsR3Hth3bsdKuQynp9XpayV6n4/s+CGm1us32AASWZSdJHMcxodRxvCSJ251uHCXZbK7dasaaTc/uemT/Ty5WT251rq4G1yX2AfPAa1Vc6+FKiNen2dxblnm31fy2+Gf/w29QxizLCf3BtoFLKSihWuldex4FhoACUAb+i0pqqUYfOAk0gBzwCtCKTWS0AB76YWMr9x6/P+wFjpsGNt6pU4LF660rAM6e/887JyoMiW0xP2lbQvk34nYwWOUjUzPQ0NrIhPjB4MzZ0z/24z/T86GUMkoRyuZ3znKKQMpus/Xct749NjrlplJxErcb1ZHx6UZ9q1ZdCwZN27YMMPAjrYxNqdaGUaM1BUGSKDffa2JlFMd375tP2dth8VWO6beue8g9dvOnIvLlkrgXwGLvfL8dT+UOnWt9fn/h/cCNQPXRPXu/SkkSxzangVaM0kSZOI5TFMK2ozByLC7SNhPMc21l0Ov5UslyMa+8FCMmnXa2mj3BGReMgwKEMUoo7fW6gqLW6peK2dMnXolkwijLpT1C5cjoBICxkd3lkXgM+8kNtbGD4JTEZgY/DYQ35A8B4EL/9/amf+yH0uFzz/+m1C0ueBIGShkhLMe2GGMySdwUa3Svjee2ZfU6IIADP3TCW6B3KK0Z4EqJLPn2u6wpOnDvQ+36RgistvClhdV458Sjta3arvL7tm9fa77eaJ25fPHK1/rhUKX8zONP/uWXv9oM1HB5Np8veBB1LORACBKeJEkcEa0UNK4tXBob35nJOS+9dMKxU4ViWcqQUwBwOHeHKj/3C7+USqU6PT+dK2RzQ9WN9UImG4X9MAyMUTCagFBKbIslUhkwBhgDytjVi63SyKX85PeZSVfIfQC2S+p+INiHP/hLAC5sPHtx6VtH93yiGi/uL3zirk5aK2ngCKEBSgmkEow6tuCcJsokUqa8FCGwbC4TlWjNKDGESqWpYIN+GMUxIa42sAULwiib8aIwDoLAEjxJEsEt12Wm2w9jqW1eyKU44wAqeAB44NYaqjidRPlqnBQyAJwIFyikQANIjaYB1IFhAMDGbQVkb+Jz3/wXrVY/CTHotrQ2lLIkSZRxLEKstHfwweK+yVvljUfeHT/eCRawn8BN3R1dux013FFyMsXY65EJl1Ziz0qfPX+i33PXV/+2NJQ5OPbYuYvf2axdH6nsnZ8aafQ7a70Oy4gd5Uqkwurm6nOv/02pPGyNptI8of1+Y6u63qyt1jaW1xeuPvLIE2trta9+8S9PnzphtNlYWwQQxEgSBSCVSgGgjOZT7vF7733gvgfmdu3aWFuhjFLKY6kZhYGJE8UoA6WMUaWU1jDSe2Dy11x4k25tRX7nYuuNW+8RoPmDZRMHrbSViuJgxLo7o3dq4TlKmS2YMgBhiTJSamGJMFacC86FJlwxl9sujGGUuLZwPac/CJXSSSKllFqbbq+fz2bCKCJGK6mhIsskrVY3juM4iSkVoxOTaS/leF4s5dra2u0LaOn+G9f/86nXryxeay6f6Z04/7XvvvpXz33nuwIesBMYz2PqNvXzNiT7/Bf+z6RNqKWipNNpdQe9PiUkl89kXM9x7Q994rH3P/zT/Aa93pVltg3/hjv8tij9wPK1oTsvLcdybDJ3cHL2woVLj+z7uQ/e/+luv1vI7F/rXyew0pnK8Ojs/P7HR8oztV63MERGRosWM1SF6yvrByYfbDXppQvr/NJr3w0b66E/iMNk3wNPpdP88kLjnkPHbdutbV6/fP7UsfseHvS6I0N5rRRlTCqd8W58AeGlswD2HXnyhW/8mYRUSjPGpDJKaaMN45wAUZyAsvWL/mp3ZThr+jg/yX/rhmuPxpmN7xwc/Tvv9Mb9uHrq1RcyBTo/+kSjv3q3BICT33vZGJJIaRSgVZIkjmM7jkUI+n0/iCKlqS14BAI/DAaBZQsv7RmVeJ6jtbYsLtuJNiaKk5GRYUbZRnVDqLCY8yyRlkoJy7Zse2lxqVIpU0qUjgb9O5KwBZouzDzTnRkIWC4+AWxumfOvPLv1h3/6+dmdU9OznluIxt3r5I5Q7R2Ik61up+eOsW6rR6AZYcKyy6WS59pJkhzaewhvjt37TpO8FR7eaibewtt+9XmXrr0M7AQoMOLlR4ANRnyX3TBXnnnk0wD+4ht/QoX81FO/td34QvWa0orBsR0J5hv41fZpADNDBzB0gN2/e0KHfr3e7En2kU/9nDLotAelodFcPtduVjOZ7K69u4mBbXNCqZQqkUrc+SnLngP7vvyFvzBKEgJKICxOQEAIJYRzpo0RQlDY508v7nw4lMzK3bQYFoNXLl96Rdu0kprB2yEh/bWN7wdxcnjPx8cKO5q44t7hh69/9UvP+n1/+xPpvh9RSl3XklJRQHDaD6VMZC7tOTbXiVQqSafTuWxaKuU4DkDSrpBJLLU2IF46N7djBzGacj4yNm7ZlrCExZnSptNuaMNAEYdRNlfes/+uSkPYOCiwA2gCZY/s3LXj+LHDD81N7S9ldmXFvka0eeLyZ5ZWr4VhIo2Xdrf/pS9f2Dh56oVX11fXHVgb673qSotz6rqO59mFQtF1LANz/N5Hbhmj74zFmzG5bTSAEHB/2Ki7cFcKq3Sni5YBQqU71Y1zr197aefEMQAHdjy0f+aRK7UzpdQwgPnpw3tnHtqon9ozO3dp4Rp3yP7d0yOjcxwZAHytWiM6qbV7H/30P3AdLC7XLdtNkohAF8vZ6bn9/V5YyDpKg1Fwzihjdy4I/+FP/p0QVBMhlSKEJFFMKIUxUkoQwhkTgimtF66eX1/lo1O7buXuF68td31HvLMOP3P6XHWlFan4q63PfOCDH83ekfVfPnn5hXAQEEIsi1PKbccKwySRUitj25ZSxHVcYitb0IzrSNtKlNyOFViWrbVOkmQQEm47ySDJF9LdTiuM5NDwyHoShZG0HIsQ2un2cgU7XyxZlt3t9rqdLrXeyYL+NjABtIHKXRGysr37sX03gukdufzy6efq1VY6nawvt9cX62trG8VCpjsIOKOCAjpptTv5fI9RzR31t9/+6w8/+cvvJB9gEZh9S4EQvY12b/3o/P8hFhdfnx0ft62JsfAOy8G2KbAMTF3f+NteEM1P7C+JSjqVLucrD+1+QNyM6rF9OyZbfuDkKj/5M7/MLGdzY5NSRgEmQrvcGy/v6rS7mbR7q+SW3BGI2PqDP/2X185eCP2AUhNFCWMkkVIrLZUWlnBs4XmO1oiljsJkcaF37tXqqVMnJ/YVz1W/VGudHy7tPzb9NN4BsVg6deJUplSRg3h5bSmI5EjlRiFALfzyye+udRq+ZVlGaz+SYZQwSqCl7XhbW+0oigQx5WKmkPa2k63bJRu2bQvBtFKMCzfl+IOIUH74yGFCzNK1K2EwIEC315NJIriQUvlB4LopizOjZW/gc9s5du/Db13q37z02a2WmymPX2h8cTR1DDgHmLdmgRyamxjevXvH4dnJo9997sUL589GUaS0llJFYUAZ0RpSm2wu47kOZQlVlh/G42Mz7yChwts13q7JBgar5K0Gx385uNv0bArYLk/fbsM5TnVx88LZxWc31r4fDAZHdjy8vLTOjPfAwcNWevetxfBeMHAyhUcef3psJL9W7QhhE0Jt1/aK8VD6IT8GMcmtSaUGvy3z/vXnn188v5YkMSHglDJObUsorZVUvUFEmcrn0oTQOI7ALEuQcEtTP9wxOaIRDLrt+en3Hxp+/w94t9nS/nzpu4Hfl83ox3/iF5Yb527eqVGnwlmbUaqkgoExYIzCGBkqbYNRUMoUiOc5mUwqiZNWu0tgDEEQhOl0ilEKpV03vXPPxKuvvLKyvJxJO9lMyg8izknghwSkXCqm0umV1Y1Go1EuZKUhytDbUzrbaOve//ib/9Olc+cZf00rBWJGxr77oU/v/8SjO4HRHxCmCsKEUAJF+oNgu65JJVIZIwQ1Bj/7S//43KXnr13/Xtd/9ZXXcf+RJ34YE95Wdc208TWNxRI++sOG/xBknH3AGaBmkBDsv9VuY6rZemlxYUkxHDkwf7F2eXiMT8/P11aTsax/S7Xz4vDY/O57nnjqQxpoNpu27QkubE8PpecADHq9kZFhAEmihaDsNpJtbNaf//q34njAmeWl0ioeQENrJYRgjDjSKKOTRHFBEqm4SQq5jO24lDs/91//AwDTBx+40jyHHwiCoZ/65O/87Vf+7Xpj9cLqic2ty1MlGUFurDVK40NbzTqlVEIJIaiMlVJhGHuOLeNQaeK6Akb7QUxMnzNmuR4BnFQqCoIkjlOplB8EgT+IYk0ZBKf9XldwbnSQxFrJOAwZJUQIASCTSVFCBBe7d+2q1jcBABqgQOPZlz/3H//NVzxGdlW85iCq9yKlsbnW/uz/cTLqsU99aB7YvBnUuBurS1eMgTJGS8UYsyx7EEsAlBJumY32wrF7Hv/+97+3em15ZLofkfOPHT4IHAO8d5DW23sJBdxztfXtdOH7Nu77wdL+YSgCAZAjd9Ysntn6CuGpyanJ2Z33zWW3Yz3PAdSyCZAA3W3fln7445/ae+DoxHhps9bjzDYAjBwt34iveI4NIEmkEFTqOyzDv/rsn2YLw7/9r/7nww/vC8KIEEooiWJptNaaZLNuNu0ARhujEiUEcRwnCKLJuTcTwPPF/XgXsO3U6PiOvROPPXH4F+pJaMD8luVhVIZGyqTd7tW2WkEURbH0g7DvR4SyJJFhGFCYvh91B2GkDECZsCxLEMb7g8CyHddzZSKbW1UhrDhJlNSM8XwuLRj1w0Rw4gc+JSyXz8EQzonvB24q5Xo20LlZTxUXU1MP7Bx+6ujOjzx6z0998L5nHtw7lHUooUminv/KdSB5J5IBMEYTUMAYGK207TiEEM55KpX9+X/4T2aGJ773+mcS2S2NOpvV5srZLrD3nUkGYB14DlgDLgBbNxuvA6M7Cwds7H7nge8eQwBHXLo1v0JPJZm52QczhUwme4t/98OgWLIADjSBGFimCwsLk9O7AHQ7PdtxBeNOWm93rzV6XsoCIAQHkCRv1ru2u+Hy2tXf+PXfLlhT1LFgTJRIzkgcK8apUopRKpVJpKIgrucQyggI42R4/G2/z3lH/Plf/PtLZxeod+MdKuJJBw/tO/AhhiEtE0ppKuVSRqNIGhAhhFSq0x0MVQpRnLQ6XT+It9p+r+cbYmDMVq3m+wETotFo9trte3bumB6fUEpeuXwtjmOpVTqVJkZVSnnK6KDfr25We71eGMWc0SSJKSEDf3BbXKB79OAH8pk0JdSy7VIxf3jvjkPz40RLqWSn2XrjSvBO7wWAMUo5JSAwRipFKGeMMc6e/OBPDOfHCUoPHfnFn/n5/+ax9x3ZsWciRvDFb/8JflCscRwgwEvACFAGXgGuAzNADegC71SEvZ29eOs67zYPAAAz/UG41d26lVZnyBwe/UiZ7Tg8+0wOMzdHOSB56mgkPcADlgBQf9Dfu3em1VHawGjlet5oOQC+roB2sybjBPqGfebabyrMF7/3jR1HboQYBlsJIURKCQNCCQDHtiilBDBagxDKKEB6vv/Ao3/nk8/83XeW1NvgwplX4yj80NM/c1f75Y1L/iCMEtUPIso4YDzHYpwTQhljti1SqRS3HD+MZBJnMl6SyIEfCuEUClnbdsIw2mq0TNIXFATE8zzCuNbGD33GeBDG2/ls27KCMB4MBp1BBGOSOBr0faB2c29ErXWq1U+qzf7Ji/83ZW8aJFl2nYedu74996y9qqu7q7fp6Vl7FgyxDyiB4CZYImWKcshkSEEvFGWajuAPKxy0rQhH2OFQhEK2JdpBM8QAbAKkKYIgCA4AERtnX7qn967eaq+srFzfet/d/KN6qa7pGQLfr8rMWy/zvXfeveee853vrK1s9kol5icqLgVrjLXwtT/8qw87r7XtXWuBEowJIoSANQgBZaxaq//cF376/rAKO16Jjrbna9gpb13a/NNv/bt73/5ISAXy3uZg5t4upANwCuARexcAALgKcOsAURYA9gU19htcgwRFbG92x+8NzVc1XLqf9+TQ7BYbu/LO/ZEADWACgO0dCn/yMz+NAEajEaXcdT2EFcCoB60sh1q1Ho+Hvd4jTuynP/+zP/2Ln9jjlmRDJZVCgJQ2nBEAYIxhgjmjjFGC0WicGF0OhqN6q64BRnD5w6/UQRx77LmlU88eeNNCbzi4gRFGCHHGyqIkyKiy9DjzXAdjGA1GAAAIKal837HGFIXUWmOC86IcDkZ5USBrN7e3QmZa9eqJk8e0sQBQ5CKIQsZ4JaogjBmlnucRgi0gz/XurKxMT87f2215APrS8jd6/d2ZVj1Px73d4W5/NNmsPHdyNnR5y2f/8S/86oed1yvf/GNKCWPUYZRSoAQzSr0g+LVf/58PjGzwZxaX2NlPq6c/trB0mt7qvvPIA1p4sy8sfWBP8/eo21WAlf21F/sQA0wCVB6lCjO6R759KL5w7u0Vk1XblZM1fIzA6f2h3Vn3yXh8nz7UhjLuru4CDAAygJy+8OIzuQRCHYwNZbyzfWWle3V+8lPNBkReI4nj8eChCPh9zKMlgOqlm39tQBFCGcNZUVCMpdTWII6JNtZ1HWWMwwgi1Jri7QtfXjxLTlZ/jCTd5z//+UbjoWTc7cFfHa6fef6xX3z16+cp1cYKjBEnzFgLmKSjmGBkMEYIGwOYYARI5vlkrTrZ8EZpOsxMtRopKTIE3XFxZD44s0i3CmS0KfIiDD2pVRSFlBDQKMsza4wfhI7jJclgdnqiNrE/WHXsM8//vd7r+bHFw67jFbJsNeq1ivfyx5snT6QRMsdPzMIH8I1v/jFB3s3rFykhpVbGaoSI6xEpleOGS4v3/YqNe2pCbAp+dap9G9oMoLM6fkT2qatfdY1pOJ+7tw7ux7UUkgDm9gUjdjfzH854JwFOAhQAZt9gAaAAAoDOo4RFwXOmjx46AnAoyy76H/AVDzfvOt/x8L3OWlfJ0tqtidlZoIsYA2xt9Ky11pqyTErdXb2satFdOw2jaGZh8cDhXr/2ByW8u9bb6eXj00d/4md+4T9lzMEEK2mkNgCgtFbKIIws2FLISjUEY2s179CJhcPVJ+/7Nztw9YNncgATzRlA+xUeYLF+MoMEAJQsrTGylIRixihCpNsflaUBAE7pHrHGdZjDCUb41trmexcvjfu9Q61oOqREla7nhWFEKJ9uVtoVn2BirfI8r1ptuA4rpRqOxpy7rVbD9/xKpcI4y7KcHVxhjpWlvHH7Dgc90whNmWoj6/XG048fdx/FifiTr33pC5//3InDgSpFWQpjNCC8R3azxkxMPyCw9OHGgZsI0L4zuhOPdcf86Ri+vf+zkNiIfRwA9omi3Z/AxMbu4Hb/ewCjvdcxvJ0XQwl7BfTth3XU8nvphwDgEsA5eBjT04cAGqU+p83ByngL2b0/V1UxdhwxORXUagGUGgDwYAyiFEZro0uA9OyTz559/lP+B9frfXjxxH/C4Zn55otNrwIAR2cOSa0xAowQRpZgxBh1HM4oLYTU2kilGKfGwJ2rO+duvX3/OJm5P832Voqvf9jXHZjTNVR9WAQArbWSkjFKMC7K0ljjUsodwjAKQs9zuJLSmLsbEddzc+msdZMfvPHOqLdzZnHyE48deub4HMVGa9V09ETNB2OTOKEEF1k2Hg4wYa7HCUJaa5dzQihCeNRfP/Dz1npJorlxI2EtCwKlTZIlRuncPDRsd5RaWPniz/08QHXx+KfAGlFKqRSllFHCGMUYV4IHT5T3kLDoEAAAdiaqkzNTE7YUAOWq/N/v24EHH/uwy7YD8SDOB8kwgzsAALDhwaQfeOzuRljfGzkGsPt0r2YAFj5I3J2oehub72/u3Fm+3jvwEQIfAJR5Ix/fYg6vt9r1mVke+OC7ADt0c301iGrWKEpsL7k2De3D8wfzdx+NG9urkUcJEITuFq0TggjGpVQOZ1qbbn80OdEUosyH9IUjD6L/i3iPqC6X4++vrt8kRyqg/Tn/7IHjx+kgCh4EvimUAP4ff/13lVLW2iwX2hijDCbIdblSKnAwZ4w5tNsfOZz5Dju1MJcmAymFktpxmMuZ5zCKoUhzzglCiFlzZqExqjqrq+seVCKGjRdKDbIoMmkD3zdaZ2mapSll+MDP86NaZ31b60arHdV9rjCpthemF5Zk5S7x6c333n7+6bOtanA/U/mv/4//CQAowZRRo7VF4HCmLRqPO7//h//L4sLCc0++FPj778Le7Z/3oeXTEdAcYHE9+Tcr7vIh7wkAPIK3qw+FxzYB2gCrALkLDmFl6E37d0sKZgVcaPDZe3ow5F6spLKPEbQFEABUANYO5NAQmzL6VtonG7f6CL319NMPMXJHg6vVelWCF94VSegBTqHUwF1aFGW1RoTMvApXYsfAMQDodIcbqzefefagA/5ILE0tEEJUKQAhjEApi7DV1iIEUiqpTF6Ioiii0P/1f/oQZ/zVO19t+qda7Ylj0c/oqW+FuJmIzn2G4H186Q/+15/7hy/PhJ/Ze6kBrnX//NbVy/3BSGuDECYIXI/nhRClJIQEvieESMucUzqOM4fAd99+T5ayFIXPceTx0yeWrAUhRKlMkWvXYa7reNSRrkLGNl0ydXjKGJtLayz04hRkDpJP1sP+IB71BgdO3/VIQVEQho2ZpdNnnggn7xIlFmt3K3Wff/rAk5PfuHYDGWWtMoqUSnJKCCYEkZ//+//46OxRALi5cnX60Ia/j+IG8HoXNrVGU+QnAEqAy4/VvyDgxtX4XxrpRZWJKt1vZ9VN86cz2Adoe+C1mp5WD9x5F1oEDj7MAACQAIQACgAD7ALIh4uN9xBIKHe7BQJ85+o7B+zs3Xd/4ODgpU/d5Qhev/CWR7EfNJrzber5AYBhjDbqVaie5HtTpUUXL175oJ298ebb00vHFxr7M98lACe8PuotI7BgkZAKU0IwCnyvLMu8EGHgp7motRZmWg8YKW93/+XO7taOHC2xmWZ96WT9C9d63/E4ArgKcOb+sPPLX0+z0dXlt5pPTztwEgBy6DJHE4qtMa7jAMZpWgS+p5TK89LhqFAgRVmWChDyXI4wPjo336wFUmTxeGS1HA2HVpUO50rrUpYOoxghzrjSME7TvBAIY0yIxwAAec0KBmSQqbYqhyeqmB50Kf7Jb/7OrYvvHHn8R3omAQDAM0ojMGCt0grvkXgB/Gplz8gA4OihkwDvZPBKAT6FhEICUK/DU5QcAbgNkAA8CwDb2bdpUe90RtXw9j3KOwAAIABJREFU/jy051jTCC8CHAWoMxgxtoUQtrCNoLqVvDUdnnnUr+oClAApQPsj2WkwGitCoFpxy4c9g3PvfiUvypkjTwC+m9M8furQYKvTG455XVOELMUYuQEG0sJ3d4KTE9V/8Mv/8IPf8c2/+MrU4ulf+0f/6P47t+H3bXpSqthlGAVuUghCkNVWGyuVZoQ4jmOwwoDtvgUng62t7bW8gLkplstBCm8H8MLGzq3IJfWoHkEMsAtwCODOsWNLFyaXP/v0b/bh3T2/emyu7fZGRmNMKaGMc2aUqYW+LYUohNS62x+3qr4LqCgVZ8QA2u5sbW2IJE12R7kBe3R+9nSltrG9vb07tEZLVQ5HSaktUtLjTirSRrXqep7DuR+EnLG9sBxlDBPCqL3113+ECDn89Gfhnp70j2NksLrVQ8gapTEB0IYQigBpa5976ZP7RhUJbBuYHImLkYN6MOh3bz3bfhkAAJw9DQQL7ynZl8pnhM3yFw3cvCnOtRzfAc+HIxEE9wJp1Vn6MaCnAPrX1r4aF6PKMR7A1D5a2x7WANijdPkO4uihj10t/sSzYTKg4/XzlbknAWDcWb5+Ze0Xf/m39o8UeVafn/UCGA561BoDCCYbHgBkpfH5XXOgFADAAFy9dPGx03cZoeO0m155HeCBnSlFkvE1TiRxeZnmGGOttTJKlkpbQAgsgOO4LucEkn//w3/1dz7+GwDgQ+upM2cM0LzYjtw6hfHN5LXBIMkKs+gUl/t/FE2UMgufXPzi6q03tAEAyBOiwuQb3/0ajwbjOAYgrus5jII2DsOe65jIT4XcHcScIgsB5U5ASFGqKGRjoaUEz6s+tbBUrzijfv8vf/DaOJeEMmvNcDQSUrmuR8HqJN9K1yv+VjUMQ5f6nhcGnsMdx3HDKAzDiNKK0dphaO3ym/NPfyjT5CPwb/7Vf2esllqBshhZTKy1Vmv45Cc+c3+MhMuxrkyTsxXn7Ab8XhvO7A53frD5v81NLRV2Rxl6ZqaN4NRUded2/8bzp44C5AJS32EMtA+tD/jve+ScrhuaVNE73csT7d32QTubBpjYr//9AVzfi3RUwomskAio4zmDQbfS2AA/2t68FdYPeq5O1ARou/5Ovg3kP/u1f5okgx/+4K9WV9ZOnDx2QOel2+3/4f/75TNnzrouA4Cjp1567Qdfn1w8O31vBWzi3TFJzn3rRuTzvChKZS0CsIgQZC0yAEqB53pB4M8drjz50pHMuSnIzSvdr/Z6u9ZIa0tEip00OxF9VjJx/u33Ll28ZdmosznOU9Lb2b56fvn6jQux3V2/c/viW69vbF+vN+pCbGS7ThpnjWpFae063CiVF6KQyloLFhi2BnAYBEmWu5wYgCIXE7XqbLN69cat95ZXx4Vt1KuNZtvzPcIYo9RhBBGcZkWptdBIWBIXJi/lYDROszhJkjiOx/EojuMkSQpRFHk2e/zJA8IRPwq+/a2vUYyFKAHsXkMq1+Fu6L/06UViCaAAAAhMR/hujKMCT3M4Mts8c2jq+Vtrt0Q2LGTGa6mPcwX9ZKd0WyEHgqEwoBVYH449TI00AMsAADCqeTOt+gRxHYYRwIg+VPI53jHnA/SIyqB7uB/Yu7zR23ZxEIX13W5nZW3FJxlGtL1QqVbuy78NAdwkvtzfXJZSS4nJP/vN37504fVLF14/9djzhxYOxhWDwHvqmRcr0d1QUKMSvH3+/XfffOUnX76fG0Et9uSFd98gYKxRcSpLKR1OEcJSG2MMwgQQqVbCw49PvnT2iQyKUXp70BukAyvLnCBSZJYzw5xwY22j01k9/dQLX/jEP3Emb794/Ivzs890sneuXVjtbQ96nb7j4WNPto4/driz1d+8OtTaeJxgC0VnKLWUFobjhBJEMHFdx/PcLBNSStfjFBOCsEKw2e0LS8KoRhlFmNYir15vAKAwCNqthlIaEHI55ZxLJbVFhbK9sUiEzUtTSp3maRwnw9Gw2+0ORtmp009SzwMQ/fUbW2vXAxcTxwVQoFKd7W7cvOBTQ7yHFLJffff/XL60JWVZlgphYIRSihHCc0sTzz9df+377wx7/cmZ8MM4tDPto42JGd8nFcdJYDgcDEGGU/U6wGMYEg9evG9kFi4iMAAhAAIgAATgMMAkgR7DNIAmPVifpwI0Dw8FUz4MWoW9WlSdm5xjlBaap7lYeuJz1coxgKv3khDudufVfmeQJgJbsrq2QaUsuru3H/vY5GNP3gvmxnEUPWDxhg8H0/75b//Or//GL/3el/+vX/0H/3jv3Jd3/rq7O6i6iFLGOJYSA8KUUms1ICSU1qIQRd6qHx5BOU+OXBapy5JoEhdFHicDIwNQ9Xduvlao8bEzs5958u8DwFL0aYBpgKs0KJFFoBEKJGkovxG8f+X1fBxkWe4wrkVJMBiOEOAkzT2XGwtFITFljBJwsdTSWkAIPI6Zw0tMHLuXwUa+Q1v1CsJsaqIllcYYxWnpuIExKnC5MjrN8jwX1mqjcXdcAA8V5aI0xK9lWayp6fV32bg3Hg/Hw26apUncX1g4ut3ZUFI7nA8GvXqjrXq3vebEfbv53reuZ3mWZ4W1hiBCKEaAjIWTT50F+KnFJ9/47rf/+syzL3/ETfZg0vMnc/hjDLJdr+UB1bBD4O0cUm8fLQzBwj13vgdQAbgf7nqCA+wjdNzHo6vkH4X6XDQ/9Hq5jVmz0V2+WI77x07cdqPD9xTUAAAmJp9Id1/tbG+tZNuYEHr10ltuu/OJv/VzdbrnXcKeWOtHwA/r773xnZtfzI56nwFYubF8nRDsujTNCiVNKRWmBBPXSg1gwOi8KJR0r7x9GYfD+OhmIVLPQ57re465cbtHodmaP3V2/uUYrl5ee/XepmlvGsh++MoVhIjWxsX0Jz/7hZnwJXPk0qvn3r/8wztlKbEoCQE/9ISyAXiYEg0WoUxpbawlBHyHaqUoBWttkece55WQS8tcimvViGIsZIkR9hyKKPH9AKwhFDWiwABIpdIs3djqqFI6CMXxuBBOFIZnnn05qrAyH1y68GaaJtVqvVZvOK7f6Wwz7q2vr3S3tynBSquo0kiTURj6zcZE+/AzABDwUJUbymiCEALYq933o8Ynn/k7ADBdeyFL3vxRbnVS+knWP1RzfT5RwEUDo8sXx8PeN1/62Of/7GtfCurIIrm0cPTkUgQw+Sjh7Y+oq/sb4SBAmmYKRGcwxmL01BNPuNH+dNwWwLSFxAvQ7Nx0r9f1nRp56vEjmDpnz/yCS13Ym2TJQTE+ALinAAgAELan3337OwUaT55Yv5Nt3by6unMjbVQ8VcpxUiRF6XJGKAVABIHSZjSOERhKIKjbT5/57dnKC9K9I6Uax5mGQkvvhSO/AgBXdi6PhmtzbZdAQ8ElDNOv3fjzc99fKYoiz7KnnnvmxTN/FwDuJK+9+s33434OYDgCuqcdiTADcAKPYMwYdjg3xmhtELIEYwwII0Qooxh5LreAEcaM8c3tTrPeUNpyhwkhslzUa1EzChDGhDsYUddzKUZFKTjDADYvCkJQf7TLORnFY0w9x6kog5Mk29nprq9t3bl5tbu1kcRDUebGAiFsdnZhbu5QtdlSyS52a93OxpVrV4y2nBGMEMFACT71zCefOH031oAknp59RFZ0z+O5/wKTInCBwxMARygc/d1/+4ff/sa58++c+9M/+cqF98+tbFxfX127eO76OBFOFdejxXur5wF0f4Qil4NI4b0e3FEmz8sSa+siZ+nUU4D3H2dTQ0KAJ3JrZn5ydnGCYI/udLamZj9Rcf+GDnsGtIE/orAIcPbUE7XjL1QVyPPn4fipw0oOwUKcFaOk0EYTBMZYa+yen4sBaWtKqawFU+6lODYWyDxU2u/LN6VWCBILHQSTcbxCnJgDuV5+pbO5c2axe+PGud7uLrKWO2xi8a7H/da3VuRIuq6jlcTIllnuhzzJdEABgdVGY8wQstaC63GCwXeDvBBaGWOstqgotSjyQupxnAMgjLHnOYSQohAup3f5YAg7jhv4OC+KIAyrRW6sGY6GDgdryjyLh8MYwARh3QA2RmtZGm04JXGsZqYnXNev1luBX5maPTQ1Nc1cB3iDugAAjVpNawPIEgQIA6MUgHz25c8/uM7p+ofIXmxm6n2fnt0L33twZns08Kt7YTN/5XZ3a7NbiBIjrC0Ua4IzYfW42xmnIj/0i7MEyodZ3SlAsKdU9eMigKWB3RBiZK1utSpHJ08m3S5prXvovsL3iT2Lnm6/COADbI2L92lUn3r27McfOYPtB4YXMfwhwFsA27d2L4QNZK3hzLMAVjFj0PVbHSEUwoAxsgB73X0pRspaBIgQasG2JprL/f8bV0ZH6YsAk7IATuqjePyNt74UVqqfOvHzJfTf2f2jXm8ry9LtKTV9yEUUUUumDnluRQKU2/p82o05pUHgm1KILFXGIED1kDuO0xnECCPKsbXIWKuk5h7nDvdcf3e3L0VBfd8YVK2ETMhMKM91CimNUpVKNQi9oihAa0UQRrgsS+p7ke87nGmtpRTGGlmWeSFKkWxvrjker9UaSZqCURgUGFOrVTAGyqvPnP0YY05UqSilmecBRlDuAm8BwLGlJWMMxUhboNYSgrnjTzcf+EZPP/1ZAABQEnbZA50puLp9SRTxzHylTe7671PVT8bwSgQ/AbCdpAnFNnBwwJ3Qd9NCbOzGhDFH0EuXL5y/fOj40dnQgX25lr2HdrRPyupHB1YCsrxghKZoxHH/2s21Z9sHdQIAAMAB2MziXY5CShCfP3Sw/+ajcAWgABikUD7Temlrrjsc95UWnc3RaDBO88J3udbGABBCAQxCe9ZmOXc913Fd7gR+ZToURscrmszErnszSSQAJqhBsNusTUtIV8ebG7cM99qVKOLcwYi73MHIHDo5RV1zZfi1U7W/tzC38f7519M0rbg8kwow2Vvqmes6jnRcqrRVsrQWXMexxoCxiEGjGibYaow83wWjC2V8z3U4yQuBMCGUBYwaZXWZl0o7LsMISSmz0mAM1UoFYWQMStMxAihFnmWjIseDWk8bi0FRjDFGrcak57ppVhiDJianEMYIE2ARALm/ZLXnjrqMG6swsowxjMnJpz697yJ3cHVyL/9zz8h6BgbXe2+cnPpZgMq9GWivOgEi+MStzW+vrN/wXfbMx8+6xDqUB36Yl+X33njv0p1N4EBrcHXzzdbcS6GzAjB1L4m5F7L/8cjcKWwY0C6wyJ3c6S9r4jigd7PdsvwgGQkAoLDj0dZaMs5vLd/Gx46fqtYe2lGaD1B2b4z/8luXv5KABDgbQAtgx2+UYRQpk3V2VvrdAcGAMMF7wq8ONdpqpSghnue1Wy3Gueu6laoninxjfRlUVRVyY32tGkwcmz/7U8//588++5zrsrV4JUnGWTru7e6qrAbFUZW3CAPKyPHHT3tedKr2dwGgu7OTF0Ul8Kw1UpUYDEbg+B4AAIY4ybSSCFEEiFKKEFhjjDYGk0xpUZR5qTVCruMIJY3FRWGyPO/1+wTjvd0fwQgBklLlWZ6nqdY68ENr0eTk5OzMguuHjsNkKbQse92dOB4brXNRIISian1yarZeawyHA6UUwhgI+cDaRCvVyAJGgLSxGJNjp/ZJBu9uv/+df/sfXv/qvvHNtXTNGrW3ebwTfwsg3xe0847M/Oxka/7o0SMYIYzwziDe7o8o5ROtBmWoNhW2Z6o0ykrIARRABg/YOz82ApjdHt5cS9/a7t1WEkSZxvmwl3RKKAr1iCXYRRPjImk0K/V6HS8df/yAf4g/sIguVf72Tz72z0OYU2DPDW6/uXNZZEpkLpQ1U1YICZJcZHmJMTZgS6GklFJpUUrGCGeEMQqApg5PLS41CQ6lKde3Lo8Gw9u339nY2gJgTZhuVecjfxpjt1qPpMDDgVi+vr07jGvTzA/95469PFVt73E776wuy1Jmaaq08nyfOxwzqqQcjBMlJWgt8lJL6XsuxtgaSIUohJBGcUIchhEYzjgiyOW8VCao1BzGGCe6LBmjAEYWRVYUWmtKCUYIrKXMMRqGo4Rx7nuVyclpgmF2YSkIakWRFaJQSvm+Tymr11vzC4tFkclSAhwsdt1DrdYAaxFGFGPKnOeeeHb/Z83W8c+++Cv7x1eD1qn23QTMYvT5DxaaN2onjh05emetw6m7vbW9ur45HI5PHl2cnm5UG6EXVRFxd3rrI1gFqD+cbvpRhG0fwjBZEaXVBoHFSitrFHaUdct33nrlkePnWoeEFjS0dHbhiP7IdMM9kAzQrs77o1yVqkwjm0eOO9madm76mxhRl0MuJcHIEMyZY6zN8wLqNaWVw7gXuJ/53KcmncYyGaaFMTIvkjIttLJ7z8FUDaaAZLfyi7XaRKNx+Mqlq6PxnSD0p+fmtm70Xr30RmPaNhoAAKoskTVSSCGssZiB0RY4RhhBKUtsrSmk12gGgUsokSXJ8wI80EK7noO0KYSsViqeRVJpz+WZkNVKFIW+NYpi5nhekqQU4aLILcYu8wBhbaASBUmWJ2np+EG9EsSj7Lf+238BAP/NP/sVh2LucIIJJdSCrdVrlLJCFAGqgNYABdCHgp8zM3O3by2DxY7Dqw83c8h7g9knPwMPowaPTHsDQLa3J9juXq5z/dypIz7nzz5+crLV9sMgzotGVJtzK45xsHGHyejS2msL88MmHPYeRGg/uonnQezCxbDmaVNqU2qslCyzMneJdUIWfkjq3QvD3rjTT3q43ojSuPyQI6v3tn9vCFcBhl349rnNy4Uo8xgZ0aa2rlDSGb67sXMtS1KlJIC1xnJKGCOAiLUWI+R6bpbljsN933njzVeXx7e7vR2H1JWqVOvVifrcx5Y+u69n0Ybrj7e2e/3+blZuMyZEJtOkOHri7KdO/1K1ehJg85uv/n5e5BgsRkhpC2CEKLVSRZ5jBJgQbYF4jjHGWDMexYBgjw0BFo3TIlcgSpWmWVYUUkqCsUP0XjMoq00yGmHCMOUII4wxJcTxXM6YEJIS6nBOGHEo49xp3fPcMSJSSUKYHwSUMmtBaxOGESFkr14OpAbR219QNDM9QwhmlBBKl5YeKrr0Jg/K7n8EuvZ9AFAw2un0bt64s76ze2Otm0nb7XW3tlY3NlZ94jaUP1hNifEr3kSSFJ3unQw69w5w80OKTT4ULXi8Hs4HYT2IalMTjyFKNZQKFPOQxgfpUnsQYuhRd7AVU4SgLHKIHpFwOL/6rbWdrbj/3bwsvBC2u1ub66vGICg9xpEbkOFIFR1Vxsp1WJoVRSmMNlLropCc8zD0sixTWnNOA9e7eXFD0aQUcXd4bnFxKQzDucaJtfz9Se84gfHN0XvHqycbrfaNm6tSjFqN1lydvXt+2FnbZmYKAKpkcK14ZXt7E4E1FrTSRmuKsbKQ5YIiTVxSr1X7/QFz3DTLNRiGkZIlwRghzB0sCpHr0uVsryeQx4hRglEqSokQwsgia0RRAIIsF57jKK1EkczOzqaFBqsJBkZZkeeu52FCVQbUh5/94q9++5tf9jw/8CNCKQBYY4EAsha0soCtNdgLQJc276OwDuDXa3VCEOfMddzDSwcIXh/RvmkAsA2w0LMbTXQUgLTRiwBAofq3Pvlf/Fnnd8u1oYdxPB4bj9ACNJBTh6essteuLi+cmouCqskkgxa5VwFqoQBYQ3elDt/dIxp9NMZwPdHDiEw4PIigIZoDI0ujtS5MNuo86j/kzmgzwpOHZ4/SLE5a7UcHz1a2z0mJBNeMovG4L4VGhmsQHrVCKD9ohC7tDhNZmFq1slsKjCl3HJUXnFNjDEKwJ7tnjAFH4zDt76hKfYIg2FjbFkVhnyD1lv/6rT+Ih+jxU0fe3/3B2uqGMYkfVSrhXL2SieFydy3B4v2/ePt/RHwU+m6xyxsVJKWRyKpMZrkkmBpELMJ5UbiEEkIYxjkCMFBvVtK0EKq0UiGjueeIrIwiz+HMWKAUi6wA7trSaCVq1YoFWxQFY8z1vcDlSRpzAnmeeV4wiosoCPJSKa3zvAyrdeoDAHziUy997zt/5Dou49x1PMdxCCXWGK2VVAojpLXhygCtovDuRT527JjDXc55VAnDIFNwjgIFKODR3MP7qO/m77a8U010/J3NP3t25iEdg8NLj/c3t5BBFsw4HRoAhHAU+G9cul2bqbbqPmioBjOn2p9g9+QNEUwYMPcmtL85unFHvrK+s6xMenT+05NwzMJOM5xGgA2oeBT78pH1VCzXwrOmNxhTVYpHso5udt5p1KqjcZnlYwBdbzaTbCBE6dAaoWErnLYg+9uDMi61tNihFghCBqxxHaoUSjNBMM7yHGFaKmmI9kiztzYskv7zzz/VG+xIY/rdeK59ZH4ev7X9WpI5g95wOFIO8+JYWbOtbRV7LQQjo3V/pxN5U8vn8u2VUYApQWSYF1ppwFgp4xPcqFdHSRYnOSXEWOs5DmG00x0wzpTUvksxJbnUjFOjlKWYUkIYIRgDIoXSGEGeZ2EYpkXf47wSRcYYhJClbn+UVIEkSWrBVoLQWkjStF578GQyShDGYI0FK2WppWScWeBaaSBYKWWT2Kk9mKgqrfnjS8cHw+7UzPzi4ofJiwwBxIFads+7m9s5YGQAMHNk4cv/7k6ZCUIQw8AYjcIwCmu//Vv/YmJJS7a81U1m2i+wBxqayWZxM3KbEUQAmwAPAlvdbLUo9XztoKThPHtxl47XO+8u67fTySFzDMWWgYfBYQxoZOBRcKhnEQqCCs3Fo4Mf7116rTlpI782HBdxscvHJKwEOBH52MaD3WSc+IEEkmIqlFZ5VliwBKMkLTAGpfSeki9Y4IyO4qQc0+qhqf52Zq2mDM3NTW+POsPxuAbHauz59IRaWV1uNmbrVRsnneNHnux0dru715NRSgkmBI0H+sb5W4PucG62jQdFkanxOPcYBGFYKiCYKGsrlcjiApCVpcqFcMFigqw1lDLP9Uols3FGEMLWSmMD3xeltkZhrK3FAEgrXRrr+gElhDE+Go8RZpTSwVgEShWlAgDwtO85mLBq9UG9wqHDR0RaWIREkUuMKOWu5yGEAazWylprP+D8TExOJtmo1f6IWeQRfdCDD5fO+/53/6rbHRCrtFKcs3qlggzspignlLPD8ThAYm11beXkvAtQ20t3hiwcjtdQZRw+vGJu7Fzu9bpJa3zq0P4WBUCgcnLyc0rx9c650Wj30NwzDnfi4c0wqDnIsxr389WGd7BupTfupVqPdZ88/vjphYVjvn/QP8OBvbN2KU6Hw3GfkWBntxP4lSTpxsOMAG+0IzfEjkOKGLZujZAFjGyWC0DgOK5Sak+dn3OGMBkMxy99+oVDxxe2dm6RMF27sz2KO5YU/d5OSrZmGl6skgsXz09OVMZxLxl3ijzHVHluMeqZ3saoGgXZ2G6td579TPs/+qXP335/O8ulkDbNRLVWlUoRQgshDVhAeM8Bj5OMsbssRUKI53kAkGalVAoAfN9zXIcRXJYqS2JCcSE0ZsQoo5TSWrsO18Zaa+utNhiTF7k2MDs7p7RRUnJO683poyfupnFOnHj2/fOvN+qNMAi541BCCWWuwzFGRmtjgVBGvb35LN0j3mxv3u73e8fOPD89+chU5o+H/++rX37vnfMyHU00KqHrtmq1RqWC/KZ26cWrb0vkjUYxI9HS9GlCg/u1F6m+HcfpdPjEw3V14FSdJN3qjTa2++vYCYjL+YNtKQGXZGlqDScoiMf93vBOmRZQAtbQ39mcmjgoWPTmG99Li5FCGb1z84axB8l679z4/mbvapruxomghPs+A1Rud64nY0Ih9BtWmrS3ta0LUiQYW3Ac4rlBnBYYI4SAEkIoKUtJCQFMHM5IuKpdWDqz1Ol1ctsvQYzWxlQHvcHG5f47k/VjnPhrq7eVgCyV+ehGtRESTPJEYozAkmE/njjkHjk9Oe0/U5J3LdOMW9coJSVCoIxWGo2zEWesWg0ZZwhjYzRlVEqlFGitrEWuy4jC1GjOiJISWcMooYFflIpzFseZy3EUVTFGWisthRAiGY8IAUYpxoQTixwuiryUcrd7vxkyMBdjRChljFNKGUZ7Gw9sjQWEjd4fwQ9AdoG1JyYmr1xlTz/xUfL9PwouXLq8vXorGyXH5hZXZDZRYdUwQAiPBeLTh4mL5+bnq66RRluirty68fix0/iumRlCTLt9+IMTZx3NP39s/v2NrysN6zsXlm+n7cnDp6efKaC0ABGdDPGk40nfq+yk2xassUZpIRVl+mBgbziWunDH5UDTkv6Xv/FfT7QfqizO7fj89T8R+RhwZiwljCgzInyYx4AUC2oepZEUtki17+vKUrl2weWECiEsWN/ztLXVyDcIF0UppA4Y5pxniZ6dddv1qcFb/ZHK4xHzKoPtW0VcpFbjFeiMhmmeylo1HK7ntYpranD+e9tlgjDCAFBv1p59dmmqtgAwzfya6Q78wMNGGGuU0hhLqUAqzTmXUmEAjBEhJE0Sx3GMsVmWKWOtBcaYliCECiJOsVOWJeOOMUZZ8H03H+zaUvCwQsBKrREmyTg2WlarlTjLdnZ25ubmKeeDfg/ZA26vVVojhBHGCAAQtsYYhDHC1iJKCagMaAgAwNpgB4vzC+9GH7G1/Jvx1puvU7A7/ZEG4tXbz508fi7AnY2bhaaIMHdqbn52IWy4XqXmcmZBtetBd1BcWl5mzD1+bAGDquIPlnw+wNz00jDprW5c34nXhU2mpxcb0AAAD/MXj/3tS1vvZGV3ojm/21MgyrJAWiiSH4z6RiEzBuWlUEbjWuMgFem1175DeGbB1MLDoV9nThJna+N+gaxbqVUodSk2Il8rRWzBy3oTWhmtVCGEM</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy82Y9k2Z0e9p3l7lvskZmRmZF7VVZXV/XCZndPs7kMRWnImcFo5JEgjiwbtiXAluEXP/hv8IPhNwP2iwEbGMuARiN7ZA1NkcMh2SS7uVQv1V1LVlXumZGxb3e/99x7/ZAd7R7NUAO/GvWhkIiKXBDnxHd+y/f7TgDP8RzP8RzP8RzP8RzP8RzP8RzP8RzP8RzP8RzP8RzP8RzP8f93kG/97S8ZlpplWZYVvu9lorAsU1e1KIqYTFVZZSBMlrIsQw5CSZHno8ns4aMDXdfzohBpdmNn8/GzQ5EKw9AVRb2xs+FFfhxFmqZXnJIfRp3ulRfMb+/e5goP/UAUaeBHZ93L+cxfX10ZT6eEkJ32ZtlxiiIP4oBRFgRBXuRl24miCITKkmzousRZGKcHz57KkmqZ+tPTw1iEjMqmamQ5NXWtO+zGaVquWiSjrudLTJJkPp4Ny3YVNNtZ3WotNz0/tHStAEkhJL1ATMGISlXwIs0yFAUKAiDPChQFUJACBS0oIBOqq2qSCT+KRVEAhFBCwUSRS5x3u0NCcXh6urvRrlXLiRBPnj0bz2bT2aQgBQVlnGV5RinJUui67vuepumWbpklZWdn7ey0Px5PG42yEOL8oluumKTgcZr6vl8plUfDKSGMspxSRhlWV5Yn06luqo1mxXPDq8t+Qchs4rrzsF6vlGy7Ui5PpjND1ziXXNc/OnvGJYkRKRH+anMzz7JQBJTANpzu6IpRyTFLOXLHKJUsO4qj0XSc59k8HoEgFzmXFJXrRVFQhihKkiQReZKlECIXmSgKIM9lnVLwLM/SJGWMAsjyPMtyRlkB5CInH977F0stuyiKLKJTbzIcjNut9sbquud7ZtUEUZAKyDZQABlAUSTTi+5/+9//DyW7lBXFfDr/z/7jb//vf/J/Xl12VlrLjfryH/z+N6qN6vHZSZok2+2NOI4nk8nR6dHb3/gDQAWyaPyMg/4v//JP3vnlL167c6s3Guua+o9+5++ubW9BYshSFCSYT93ZrFlrAADhsNcBAgSIvUf3H9RL5eF8/PDgWX/W608HOnfeeuWtrIh/8N47Dw4PtndXGGHRLN9e2xRZ9NMPf3Fjc0vWpP/mn/6X3NkFfKAE+EAMMIAADYAAAHKAAgAEkALpYtUEIIACaACAKZABU0AGdABAGZgFk6f3Hx68fHdfMfeB4Fe/+rM//tP/qzfupEXcXt666l2laSzJat1ZSZLAdpyXXry1t98SPL69sfWvvvPji6vejdtLiqI8+OTIqRhbu61Bd/rdP3237FQuLwZ7WztZEUsyc31/b2cTJN3Zb29vrX/00ePzs77rz4+fXvWuJnZZa9Qr//g/+XuziTseubZudLuTgydPR9Nhw26dXB3903/wT9Io/fDp+7Iia5J6fPmUU51SVq3UVmqrzeXqSq15dPn4g0cfDYPzMBDI+Wpza62y4Qfe0L+IIiFR9cnxw4IogR/kReTNIi4T1WAiYlkeiqQoCClyFAXSNC6VS3FYBF7IdUtN47xkO17hr5QaJdu0DAe6bOoNwAQsyCFQBgAEgADRSmvNO3dfOD8+1xTJ4/l0OmvWq4NulxY5oUUmAG1/84aRzSbMruuw9Xrc2tsHGoAApmrlFpD84e/9rmM4T44ODFUvWVYgomHvwjI1pbICFF48bbZXwU2AAW0AQPQX3/+jN++8tv/a7wGoYXbz1bcB8p1//b8ePD0O49mT08Pbe3ujcX88nKmaHETh6vIX11ZWozS7c2vv/pMH3LGBACgDKiABHCiAcEEyLEgGgAN8waq/ihKQARkwAziwfE01vdx4460vfvan+oPB1J1mAqqu2iU9issFEdVSFUQQlP6r/+I/AiOWdBtQT06/C5Ct9qrI4/V1S7I2ao2KNw8uLztggebUtBnpTTsiF3mSMpmfDzrLjVpapE/PTo4vji3H7k3cnEav/MaNNE2yIv3xL3/49W+9Wckr60o9xdo38MLTy3OJaj/+Po2N6Y0Xd9o3v5lE4qpzsbezWQjSHQw4lxqtClcyZ1WmoV9eT9m4puVLM3esUCbyIMZ8OOtWS3XPH9dqdcLzySQOfI1YVDPVNAsKkXKmMgrPizjPFa4uL9fq1Xqa5JcnQ/Zf/7P/cH2lPZ3OJZUa3Mh82CVzMupJBEw2AAtgAAc8wAAUgAFy4F4+fvjYtKw4i9eWWgWjw9GYM04IKOjmzTuAQdUC0ABn8a4EQA+IgABQrs6e7rTX3/3ofdf3FFl5ef+FKElqtRqkNtK+Oxublg2aIPNBLYAAp9/73vdWlpadWg3QAR9wAKumefcPHjw4ePrx4UPXnRPGusOrOE5EHo+8saIpKY2TUBx2Tp8dPn52dF+X/UqlARjXZQMg/X+sNDwAgAuMIrfPFQsIAGvBv88w++l73392dhqLhFGpYpcMw8yQ7t/cuuwf337hhZf330wzfzg+7nQePXty+c3f+rLv+1xmx4fd3tWUy6jVqqoiR2H85a++dP+DZ7Kag8YFgVM24zjkUra3v/SFnR1moNVujPveF966+/Jre2985YX9O9tcppuNVXDadYeKQqtYatlLS5ZtbErVFV1IIbQ4ov7O7oZmqXvbW07TuP/o/vsP35+Lrp9OOxeDLNAazsrNrRtL5ZWN1loi3HsPf1EU+WQ6y/KIMiEyv8hJ4uelup0KUWSJECRORBCmkRcqKmOc245DOa83yldXPbZzc4lypigyI9SuLY8Hw1LVGc9GU98N3J7tAFABH8gX59sDEiLmP3rnp7qpi0J0LvujyYRTSeSpKsvNRmPr5iogAw4gAQTggA5Mcrff754H05GhE6dUNWz95PTk4OjIVM32UnPvlbuQ2kCE4Iozzs1NkARUBUxgDkg2Kzb3NsEAwL+6L1sFYGt0RjNqOxZyNnddL/JElqe50ExZ0iCpcpYU3f7EsczRzFcU7fTyvL2h6urKX2bYGZD9+gD2echADghA4soqoCzoRT7/Q73+j773ox985dU31lZahFBV4dVy9cnxUefqynOjjbUNNx66XmhoWs5EtebUnOWrYWd519rZXd3b246TXNaUSsPOBH70vQ+urnq2IxFC1tdXTUt67bVba5t1z/XUGq1V7dOTqywSqYgrFe302WWepUurlWWprIBPAndZK0ugAHExbyqVGl02CXOJZ2gUiEJ5zkg2Qffx0086nW4q0jwtRt2oWq6urLWqdUszlCgLgzCYTqd+EBq6ZWqqIptFgSgJZYVkRZxEcV4UIknDMMpzoSgyl7jESFYklOWnR1eSydjaDe304vzo9IwxpnJ+fHUkM6nkOGmceROPUaFpEghbZJkpAKCAmL73q/fBhaTyJAv63ZGhW45tybJsGMaNnRXwJuABIVAAMeADCYHI4rRaqULTwSvp/GK1vvzW668oXLu5t6WVNoAykCGd8NIrAAESYAuYATJgV5dvgUmACtA//Tf/Urhec60G5WarJf/gh+98460v39698fTsWOVqQTLTUZIk6Q2HyKSvvf36t//hN2mGnZ3W33njDdM2ARngn6OaBqiAwDWL/wYUAAU6QOpOPlE0aUHQ67QbAVemQbMie+nFvTu3bgahBwmaqhyfX8VJTqky82bnl513f/6hSLJ6s/z08Ojg4uFHDx49uH8+j2evrt6EVQRu8P3v/OzsuDudBKEfWLZx68UXXn1jf2NrdWWt/OJ6S3LY4dPL8Sh854cf6Lp28PBEVsndl3dW61VHsgrkOcSTJ2ejeDSMR1fB1YaxOsDYRJUCR4PTRIiGWr0cdodBt+JolNF6s5Ln6aA/9NNJrS1TJT++eDYKRkGcGpqhyEbspY1atciLNEsm01noR2keB0FECfKMxInIkagyI4QWeaGoqqLwOEoDNzEsg33ty29kWeoF7snp5f2Dh91B1/X9y14niF1T10RKSrU1gC9ynw4ogKoYcjSfPTs4atSWdEtL44KBKIpKKSjjd27tQKaAB/hABDAgBQiKgCRhEgZSns3HZ7qqmStbJV1mRIiMOPUVIAMiyEtACnQgXFAXiIAYCAH/4198RxWuKse9zlV/NELi1ZZvp7Nn3/mLnxi68ujksDceizyMReiHru9GSUwLQi86FxvLq7rK0lisbtwFVgECRIABFAABGEB/DcmKvxyrkk9fJJwiPDy5PK/V1oASQAEKFEAEdIElxyzCKLv3yQe94eA33/rK+588ISRzbMMwTMewX3/p5UKQIsPtmze/872/ME3dLpe2dlvj/vTg7OjBh0+fPDzM00LT+Hq7dvcL27ZlAmnoR05ZsyytNxttlVY3mitb9e39L65Nx/6t2+317WbFchwY3WQU5KLJylMx31lvu37U7w1jOU5FUlNKgJ8pMUFWk+yKoc/CsNubtDYavus+e3ge+IKy4uaLm7W6M+xPzk4vw3h2fHZy3ulkPKisOiJLL686eZYWNE5FIhIANBESQcI4VRUlL4RIM0mR00RESSRx5HnCfud3vlQtV7ba65okJVE89wIv9GrliizJoPTo+EgtYqdmAAZAAR1ggACyJYfff/CYUZ7FUCzGIDHCRC5IUby6vwujBEiADDQAB7ABB8zkhi4VKRxHoQzWErABySg1DMe0IdkAAAHgU05TC1CBBsCvs6c38tM8vexc9EajvfbeXnuV6CZDNOj0Do6OKk7lcnjJOPfCsEgJGMp2rVLWzi8HFxf9hl1eb9Ts6hLgBt6BJG8B8r+T7/4Kss81B5/x7LobLROpVKuVgSYgAfniuwxggKbruu/3/CguOY5pOGEcrbaas/los73BKH/h5vbyytLR+XEmMquqn5yfyTJ3Z97V5cCxVUlme3trf+8bXyqtGK++vLu1sVxZcl5+eWdzeznw48l4XqrqDbkyhhvCkyBdDaZv3L21qjVDRAXgJmFZMc+jq+PDq9XWyqrZGvgzp2EsaWWBmIM51K5IVQLGITf0crVsz4Lp2UmvVq/oukq5XG+W8gxxlG/trqWxyNIsjoJS1eFcS2IxHY+TzC9IIct2JkReIMsSiVJNUVORpyIhlHIGykieZZSjAGEvvd4uaN6qL+9tb7x048baSuPw5AQAKYpCpJqkDkYjmcS2KiAJIAYmwAQiUDSFFvnp2SXXeR5lS/WGF0ZhEGiatr+3JTstQF0IB9IiKihACcoK4EAWwDpAARVQIJWAYpGArqNLAuRAsXigA1alKfU7V7+4/9Flb/Stt7/C6q8BGqRsvaxvrrW/+uXXf/HhB5IkRSLOsoIykqRhzawXIPVadTSdhZF/4+Zer//knXu/3N3SCdZ/Db3yhcbxV0lWAMaiSpOByiIKxoBYKCDa9apt22qv7bx37yfvvPduGPrIC6dc/v1v/latVvnVh48ur85Xmq3Lbs+LvSdPH622Wzdf3Ol3J1ZFNTW1vdNsqBVF5yVUNVg1zTFgaqC6rZaqOqScEyKDuwgv+9N77x4KNevHo+Oz/ocfPxsN50RHHBY//8njXMpJlTSrVdDUhC7BDEEpCFAQUAIJUHzMuazImqFpapKKUtVCnsZxurxakxUGCNcNNrZbSYxHHx/MZ7M8K+IkFKmUi6zIQSjyPGKyrGgQIihAdENjlDLGKViWZ4SCvfEb+ze3b+mKcWO3rag65aRiViul6tpSyzTV5nJ54k0lItFcyFlGkUGiCPxoNOYUcRbd++CT6Xg+nXgoMj+IiyKXZcnStaWN+iIeRIAL+IAHZEAOECAFSou3jQISkAEpoAAmoC44eh1OCECBGPA6zz7ujoeaov/h3/8H1Fn7tEVIuwql5VIJBQmz8PTsvDvs5SQO/TDPxQv7tzwv+Dtf/vKNrQ1qYL31ehR1ElKsNbYWLCk+lxCvScb+CsOuQRb/CkAs1lIAOZABMkCB/Po0dq9+alqlp8f3fn7v/X5/JHFVMWi1VD08P3n/3sP+ZBT7aaVkNxrVcrX00ccffP23397aaNdXSts318+O+2fnnYcnz9a3lgzUgXCKqUAyR2BDs2HnhFAwAyUbpmwgoWmaiYOPL2ZjjzEpCpL53KvWy4omXZ73KjUHEuKE6JKZQIxy/6PDw0HsrlnrQBmIXQQFyNNnZ1Ecc1n13NgqK9u3NpbskmDxeDgf9sayrpw+uwr8KQFnDHmRJhGRZJkzOc+zLI80XdVNh1JWqSwRcF23ZdXgTJZlJYpDtnnL1DUlSHwGxfX9Iqe96dRP3DCIwyjOCYIomc5cd5bOwyDykmTuB4FPKHH9ZO55URJ1u8NyuTKfTJyyHaZJnEaaqd7cboAzIALSxVlPgPRzaTEFAKRAtOCfvKgCM2ACCKAA0sW7bgFVq8wfP3nEOF2tlKlevS7n3f7jP/7un51edUIRxnl4etqZe7MkSmRuNOvrbjClRHn1hTueCJZW7YpdO+8cuVNvdalGaGNBEbKgCBYx+Nch/7TW/H9far5YUbH4bwFIpmUA0R/98b+YuyEhPIjF+eXV0UlnPHDPe2d/++tfWd1YLjfN8/OryrKdZUzRmOkohJIH9x9v7i0trVYvTvuSIjUcc4hJkEQykxXICrQMBQUbinmJmimKg/OTx/dPXn/51fkomM5mG9uN0A+fPj6+Op+4s3B5dWl3d1Vlel1yYoT3Hn0wnw5nwykYtqpLBPMEoY2qDCVSPMoly9IVVWayJGvys8PLDLR7Ohn2JtNZgEK02qve1J9OZ7mARLUsLzKRibhIcwFIK2ubd156kRE+n0/9IPBnc1EkmqalImF7t5ZkRZJlmmTR3HNBuWYoT4+PGeGEkPF8pMn6zA8NQ23Wq5QXaZbpuu1F/lV/RECq5cqz4zMKqmg6iGCUebEfi6RqlXQkUiGQp5AUoFjocPoihmERFa6JmCzq/euv8SK6FAsdIQJ6Tx598PGjgzAMGpWqVS0BDPAH4+N/+84Pw9inKDqdvq4plMrzWcBlHqeBqkmOU2qvr7z3/i+nI69UVrfXN9cbzXd+/m67fQtQF1mSAdKiZfl1Xed1MMsXNQAWa0k/9/gaIdC7vDp2vYhx2hsONNUwVH1tqbXUqFz0ri4vr05PO0WKzlX/1p3Nil0iPN9pb8QiCebR+XlnNpmN+t7V5eiTw6PJcG6V9DWtMYE/Eq5GNQ1WiZY9uIN0gIJomnZ3bcdo00q1lIkiChNGZc3kIonTVLT3KnPXF0o0mY1Emtzc2WyvrdytvkSgAkUOwaDGCDwSVCpN27Ka1aZmm4POMArEbJK6Ey9LcXZ8XK5WKKTpKASILOu6biiKIqsaIbmqGQQsCudJkk8nI0mFP/WiMGW8CNNpnhbsxgvNuevngnCizufzzqBnSLqp6aGIZIWfXfZmvivJUsWqiIwUhDIquXO/OxzHaeJ5YQEqcfmi06lVy4JnqqoXGZVz1qjWHMccTycyJZxkmTujeQr5uh2LrvUnQAKUhcSQAC7iIXgG+EC2KMvwucQ0f/zswe29m0vL9Y31NiQFmAEX9x7cb1Wbqqo9PHlIqCrynMoIo4RQ5EgoY3/4j76pc1WXJc4UVVabzT1wrd0qgS4tkh39XBj7qyQTiyPBFpHsOs8mi7ozXbzadNFfU4BbVtreWl6uNd5595cizeZT96x39uTkKEoCUzUb5eWfv/+BpDBD0SmhK2tNx7KZzCenk6k7j6LcdcPmUpWAlWs2WE4d6s4CSeZR4dvUAGhP9Oaulwb09e27AHeoLdt8Mh2fHl2dHXfHg7GkKrs3NpnMdkutFElFLVXK1WWsmrge9kQATZGFSE/DU8I0k5lVVMtwCppJpiwrWhqlIuXzyXw+93VtLQ6LPMsN0+aSmpFif/+FrCiS2M/yNMuCNAmSJFZ1RVHkwdWEAE7VLlccFGAvvb4hFUpe5KlIwzhplho7mxvb69uGrnIlb1RqRLCcFPNgmqZ5bzRIYnHZ652cn7luXCRUpCJOxGg4khj3pgHndKXWYBBJnEichUHoB3HghzM/CoMw9T0RzhWaxOFApBdEdCkGYGOIAYqgmMxG3WnuBXJRII3zcE7UZBFsfCCdTa4++Pjg/Opsq94qLbdArksrPZ+F6/srRkX1PK9eaeiWpSryfDafzEagBaM0CZOt1dU3Xv/y3u4bzcYKUAUIqACqiwEU+TUFGRZczxdJ/DMdJF8Q7rOiMwe6wAzQARcYnHVPnhye/uynHxxfXEZpIKnSqy/defu1L/X6/Xa7perqfO5Op7MoFMdPTi1Dv7m5U0aTlpATzEYzWVZuv7Rz6/bezZW1lOfvvvNJuaxblh5FSUXaBODQqqNpndFQLcs6TMDSwZyK3ukPT47OddPcvbX+rdffWNHqCtReMu2O56ZhWNfLRwLQPiYp8gARk4pdtm3BjiECRAH8ghBvHnUvBqtrK+7M39zdqZTLg97IC+aKKgW+Px1PJ5PJbDpM88Q0zVKpBJZYjpXnYjZ2KeGGYaqGoukWIZRnec7VDBxMzfK0iOLk4PgwCuNJNCEsq1rljdXVSIRJInwvnc3i3sURijyJU8G5nye6bhR5Xi7Vx+NBpWyLLFd1pT/opoVgR1w3jcn0tNJ0WCGZtuwnoWoyu6xTRlNRVK1SnuakKLK8MBSrIIJIxBVx6kNWeBgE1PdsS6cZLTIQThzq/M6rX3p2fhEGSdQZqRUHigSSbb/4CkBqlXOvH9ze2x+PZ5qkXJ5eHjwLVU2tlLTZOLrR3gJai4HVtfS/viiw+K8vyIoFsSRALEIaA5LP9QQpECE7Pj09jeN0c6UlORj1zn758YN+f/rk5Gw+DxTJzBCrsnJx2Wk1lv7gm79PZQwHY3VfqVQqz84e6xXnd7/228A+IFfgrt/aSm/Fs9StSTagpRin4eiV115wbH02n2d5lul9Bh2gBDBNpQQViGKMDwaXF2e98XCaxFm1Yd++syEQS5AAVpJLzzoXtWo5pL4GFdAApYEsgK+AWWgDGhDP0B0Fs5Jen49cfxb406BPh+utjZ0X26enJ88eh0URDfpuJnKZM1miWRZzykN/nhe6phsosiQRsY80ySj13DGNo1hSZG7KdiBcIHenUZblgX9YnONj/eNmpaEqMpalSBU5yVVZkSSWZSLNSRzHXugXUUQp1WM/F3maZGEQGu3WZD66uupqqlGrlVdWl9baq1mexkHEOS2QaxJ9/5MTm2kFMiJweTU0NNUx7V6vl2Ncrtg1qySipNfzG8srMrN83zvqjiqWJTHGGaM01/XSnTs1fzwjBUWaQNOvMxRQMLRf/2IL0I1Sdnbw88vOIIeIk/Sl3Tv/5B//ffC9heIvL8bkf6P0/1nWZoviTAYYEAAMUBfpvjcZP3j46OQnP7//+ku3ry7G/fEkSaOpN3t5//ajw9NqqVyp2FmWcaYqOkfGv/jGLc/1//XR4eOjJ1bP7gyuvvylV4GXAQpkpnkLaEhATerGOJhjkOViPp3u7KzXUTFt88NnnxSlDcAGwjmSpXqdoRxh+OHF4/fffVaqWDdu7iRRvn97yy7ZGqzr8auN5JW7+ykoA/UQAp4CWYJBABU6UAaGOfIy9ESPBLyVemXen6ysNmlGiaDP7h9dnl8mSZIJkSQBI5Kk6CJhmlpSdRpFSYGMgoVBGAQFZzrT8zTJOJdILic+57phRLOoajayIh1ORkxOOOVLqlUrG8865/3piBQ0Q0IIsQ2bZ7IhO4xzReVxnudFGvgCpCiKlCoIQ89UzSiOWst1u2LRUnExPmOEIyX1SiXyE5LmK7WmnMuSQoPYbZac6cwvL2lZ5uTIoDDDMAM/yrMs9GZUZrKiViqcg+U5zfMijlKJUl4vGZyFw1keUWp4yELIzmfUGZx82On3vvuz9yoVe3X51fXl9d/6ypfA9xeF4N+IZNERcwCL6u0aFMgWE47ZgmTTw8dPHx+d//yjD9eazfWlpYeHh0vL5avL0c321lqjUTHtF2/cOLq8fPv1lytORa2yRmkfqGsV+tZb4wePP3n7S1/Y3dl6+PgQuAe8BnhAFQDQB4SCxl989/vd8eW3v/2tOnYBlmK82mpFiEwkQNLpj+80dq87mEZz5Ru/u5Sn2b2fPbhxZ30+9lFQkOvBdKHAbOK6vw5kLEfoTuHVYWhwYgQC3Ry5h2iCsQ51CcshYqVEDEV9tfbSUXz65MHpzB0G/tyyStVaPQq9xkpDpFTT1TCMvJNJnHgw6WTkSdSWGU8zJEmWk1QpnJwUbOdmk8lxpVQDYX7hijRtL7USIYIoadVbmqoyiUhMTbIkzzNKijxLFUXWNc1xDNvQ6zXL1jTD0htLld3NNdlkBbhpWnpJFjSbTOZKrookueh3+tOhLxJbMySFjyYTIhNJQb1cPr3oqqq8fWOnslQSPMwjABBFqpsKYdA1zbLNLEnTLNUVRVY4ihyBP555eZGrhIDIYNcJJAPShx8/+qN/893LYa9Zdv6Db3zz67/xRWPp9YXr5N+PAgiACAiBBFAXz1+3nz5wf8E2ALPJ4DByJ4EXt9prTdt68OxAVSXX9ShDlmAeBOvNpSzHzc2NN15/uWLppqZrkvLxw2crdYPLbeDwT/7V93c327/9jT+0jde226tAuPjj14KiAQzePfhzZuILb74YhhlVAg2ZB5dyVMm1GYlMo3lNXwYKDr3MrCovDaNJ4IebN1ZX15ptaQmwP5NaAADSdXfPsWTAAUqAwsEowMAI0hy5AlmHwQFu81BEpsJPh+fnp+ez6TxOYlmXa82qXTI9b762vdFuryBHkYWSXKiKNR/Fy/WWCJMYc8pz27FUXQEYe+GldUWRQFJFMrhERBJPJ24Yxpah767tbW/diMJkubRiKuZGa922LElWDEVXNR7EQV6QctWpV508l+IkC+K0tlQybB4nOVgWzAMplWSZsIIEcRinQtIRp0kYJKEfzj0vDGIuQZbUMIglJmumSVJiO6Zqy0TPFUU1uEqKnKuKiCJDUWWZRWGUx0kQxGBU1SSpUYdcBSWLN8Zptaunj5+ULev2zv6bX/vNdIr78jQAACAASURBVDZh5vbfRLLi024XAuDAtUPkmnbXPBsC/QcPP4yjrmNGoCbgdfsXy2ubunkbpH559lGUiIvO5Uu3bmuydmN3rWRamqzu77Zzkk3nw9Wl5XKtIpJg/4W97uWwd/X43Z//8quvfzHPYCixZoZh0Ds6PPfiTskuA2eABSgAXavd3G5sVSWrqtgChQLHwJJFnOsa4Ecf/2pjo66jed2FpPBShFCx21ptya2yVBljylGwT1M/W0wsADAgXhSmBeBeZwMO20RVgwooBIWHKVVIbz6JgnQ68GRd3r21W6s7aVwwxgiyPBNba3upl0xGQ9/zx6MppYWkFRmJCMt1zWCUhB7NIont3VnVdV1T1cl0nCXCdeM4ShxHK4REKOWMKZK0ulzTNUWRVdvSLdMghAiRqirXNNXUtBipZSqWpVWc5o3t2yfH591udz7z/HE0HI1iEp2edKdjz/OjOBZxEmcxFE0ZT2fIucy4XdLtskm1omBCYTwOkyiOIjfWqZQlKSsYTdMiyymlRZ5lmVBtU6mXNUmSJAmcgxLkMdIEjAMpoL360v6bb76+u38HaDJzcyF0/XsSpQtMFzt+Xe2FgLfoKxNgfHj6qxu7O45TBd0DZIjJD995d//mLrAE0ErdvLX/YhK4b33xlbVm9ej0YqVZXdtYG04G3jwucvi+V8R56KU/eu/djaXm2t5dd9g5PD5rtRr/3f/0P0Mk+/t3LnvHnLJKeQ/pFGwIhIsXtgxYBFRBGbCBBMC1PfNy3l2vNqVFL3LiXp4Pu7op10kT0ABNAztNzxnLFGhAviBWuuiyo8UmiL986krX4vkgG50dXh18cmiVnGqtJCt6uWpxIos0RlpYlsML6kdeMHavhldhEHAq27aTU9qqrspUyfIsSYgKK0ky1t5sUEan7kiQYOb6rODtpbblOKoqR3E4m80JofNZwAmjEkdRqLLSnwxTIUzNsjVTojIR3DINrhRzL5iOByKMqUAaiygUSZyxTGkvr9qWHUciDhMmcdM0S2W9VLFlmZuGkWZFfbVkOLKmOSTI8zTjBDJlMuVarcY5LdKUM56kSZHnqqZClRCJIkmJxKHbQAYifUqyLAHlYBZIGXAW8q+8GF79O8gBb3HE5YVOSwD/c4TzgQAIK6Xrca0ugicfffjT5bW1jUZN0jYACvQzt0sVaWurfXl2KauKKknzuX9yev6dn/7FzbXN9kqLZNRebpvNvb3tFb1sg2g/+dFPGOPPjk8vet1vfu1tTosfvvtuvVQpGfHZxWmpohBCgCgMxpLUBHRAAINrkg1w+t7DX3k0fPDRs9qmkTL/k/OH9w4enp31Dh6dK5rUrjQWrsHMYjJDTpGST1eqAfIiWtNFLL9OCHTxfA3YAowyNVrVldZ2yzItRvXxaDYaDkVWOFqpWW9CkNCP59NxkYssgW3XLNNQFC7yiCua45TXV1ZXSjfu3nm5gGB/6ytfuOiexnEsSbKl2STlpZqdJkSXNdPSJ95I1xXH0uv1ihCZ5wXzuTd1p5RSXdMN1Ri7c1WWJJkjJ3M/IKJotWp129neWtFUuVYq64baWq68eHtdt3S7VDFlfW2pZjtWQTNB8t1bbUljgRcWIcvdJI1SPwg1LmuKwmQVtgFVISonjPCSxWUO24BWgqYRU4dqAkDkg1+rrAaosRiPKgvjtbrQxj7Ps+tQkS/cQXShJxWAvhDGrnmWL57PvElnPu2KLFtZWebyiqTZAAnGHyfe/N3339/YWgWa3mRQXmnqTuv45KRSKd9Y37646kV+tHLjJsIIbvfh/QdnR2c1BXdefPHGjd2qZn73Z+9urTdu7u9UVNPR9Kk732yviixnjKS+pxjXp0UG3A5OXEyG6J2cXZ2fdFwvfPnN3enQc4PAcPT19abIxAu3dwxbryvXlmMTYBSEgZBPD1IG2EALCK5dzddh79PdgwbYQANY+mwQx5CaMHSmXZz2Ht1/FIwTESQVs6RKUuDHy822Kssqkz03AiuKjEtEARftjVVNl7KQxIXf3muTlPB5PK+UK3EaI88rZlUpG1N3zBWFMWdv46Zyqc3n00apMZsHpZJRq5mXV/1p1yMRvej0NEMThdhqrQSpliUIwqjZbsVIgiRScqnVWlEYyUTOKNE4UzTWtLQsZjVH4zIv1bXOaBzEgT+LLFnPo3QSuzKX00TULCsJkiQLTAKQInW96dxXFVXXFCYr4OliQJQtnCBYPKMuZgy/Tnf1F0VYBMwBBVAWBbL/OfOjtNBdOZAjDc6OTpq1prl8bSUqAQI4BVS9UgPKX/36CqAD44dPD1a260DzlS9+a3j2vqFILMfh2fkep08ePfzlw08+ePLod7/y9YeHZ1EUJFHaKFcrptW9nIA6a/U6KbU/tYD3zh5ePFleqZSv7eVIM3QVEBU2Qb653tBU9n/8b9+TlWJrc01VZU3lHNLO7kZapFXiAPpiLTE+LfYZEC565BmwCqwsJmbZovW5jmrX7uUUCAEZqAKRhGTcG71x95WKVV1fWUMee2F4TC9mUXQ16F91LlkhZ1m+tLai6+Z4SiVJOT1/ur16e31zzSlVvP6M/fa33q5X60HgJ2EsK1KcBNNoWmRZLCJFUtdbq24Q+LHPGBO58IMwLzLHsR4+PVCZTDlNoiwMg6dnR24Q+fEsyXIuM81RFJPLXBZplieZokqhEO40Sn0RuGFWZKolDd3ZaDgNh6nwBcmy2cxTuESKTOK0ABglbhAqhKRxnIlc0w3dMSgARUKegUmLxKeC24sTmSxGqMpflyWDxWw+WczsJSBdpE62ONMpQAH3ugwHEuS987PzJ6enmq56s75dMhZZtQQIMesPhkeFmCjaBrC9tdMEtoAMRe/09LxkGu99eHD31pbB8dP3P9peWfvWb3yl4hgAfXR0cnByfP/p0VLN+U//7u/B1EgioFwb9SRmSvWVipIXv7j3yeHRk9Dr5Dka5q4MR0IdqPzyk5+9/MVbr928U1dro2QkS/LpWX/u+pppMCppYEBMPjWl8gVdSkBtoe8kwBCIFq56CdgERkAEND7nozEXxVxpe2NjqVk1NWU8mHx0+Gg8nwJFnhVxnGUxLWherZRbK01N0tMisatqGsbD2cxy9CfPDohB2JfevqXo0syfJ3GSpCIrhCTLBERX9OGsa2qOqpqXV92j8+MgiNMsSaMkFsF4POWEba22W5VG2bLay63t9ZW15YYX+J3eyFYMLrFYCMZpRouE5UGaeCLmFq2vllSuDibTII0syShiEUcJpzROMiEyU1NcL0wSkaQCRTGZe4oiiyw3yhYcCwAMA+x6p1TAWrBKWngwzb/OuiiAKRAuHheLfPr5X8diu4vFdFIAMdyDi86Vrql7G23HNhzb/sl7P5qOLpvLJSB/+slPwzRubewoqgmiLcLkFHEHIlUlJRV5yTRXluuQNaXA/o09o2z/j//8n5uq+jtf+erx2ZUsKZ+cPnv55o5VfxEkAftsOEG9zqFSdVabTUPVzi56jdpSPzwpG4aHuDNQnEpo23rCIp3K0zhSZOnx48P+1bRRqa1paxRfeOJ+UFNMwFxsznWA9xaOAb6I/QBihFeQrtOCAtiAtzhs88UeDgAMvKtZ7o5n86th7+zqjGTk4dmj4WRIJQaW2VVzY2+jWauUq5WtW5uypuQQuq3Laj4cjNm3v/3NeTCdTqaM8SD0IKSyVQ5TT5NNUzX9yO8PBrZuzoJhu9EuWzahdDgYcio5ht2qNhu1crNeXV9elrjsB7EfBx89eXBzdcv1A1LQRCQclMss1wrIRRjkRFCusDQRjmHKqqxwWeasKIhj6Y2ybZu6oSqEQlOkOMuSNFNlxTI0InMUgHlt6/3sFhZbZLdiodMqf9k0gYWyGi78ieai5L/ebmVhdDMXV7mujW7XQlp35k0MQx3OJoPeNEkyy1RKutPe2AUzgLDaWHMqNWAFpAo4QHp9YSdxJ8PhaNCfPjk9jPMUWXF8dHLztRehLT3++JcfPX1SLTnrS43h2GNK/vbdL/zo3r1oflniklJuARaQA/M0HXfOz0sVm1Pp9KLzwp23B1fnF5OzH//gPUXqv7T1VlmuOXRdgp0FoabISZTX6o3dpW0ZNtCqKdtACpiAA7SAEjAEsFhvvtAIFSAETToXh6otGCHAmRf1ZC4BFYAseikGkJk3cJNgMhwXadqdXl72LouMRGHiBt7Gre07r97OWRoWWSbHiqMPe5PKcnlrZ5fLyIuE/d43f9PWTDAkcayoCuGCc4mARkGia0ae51EUzH2PABKV/DjMkEpMNk2j2axpmsYZKZeN7c2NlWZtNB4cnp8Rimajdtnv+56fiBSsmIxnIsojEemKYahGZzjiKkq26eiaYxlclsySMnPdIEpVRRrNvbPOQJY4k7gXRIlIwySdTWadk24+d02dQsxAPLAQcJGPxdUJTcbADNK1s3wOxAvmfWZGur4SfB3qVED+nNCf/2XD2fWhL4AonF/qjixiIYOv773oVDZFONLLDngJaAIOUAZKn3MKzQEViDpnRz9471e9wUCV1HufPOwORpO526rasTu4GPSDOE0L8eKNvTyjF4Pe3tbaeOZ/cPCgUV2S0rlevjYmCZlzmbKTztm9B/d7k/5HH/5yMhvlOXpnk6989a4qbyzMoTNTbadxeHx8lbvxSrUhSxwIFkM2E8gX2ux1II8XphKKYgqyCVRBly3HYYQCGlCT+WdlXLHw3HMgdgP3w3sfFim8xFUVhRZcYbqIAUZf+/JrpYY9mXiJyBrLtfFwcnY09T1ds+lSpd5cWmatbbM/6feGAwoEsc+4tLu2oypamPsFjU1bURSp6pRVpsVZ3B910whrq8ulsjX3fMro5trKUqPG1JwrnKbUVE2S05nneWHYmwzLmjWeTmRdgUxs0y5Z+qDvjkau54YymMzZcDS/uBh2+uOLi9FkFlz1p93BLE4SwsjUDfwwCeI0TZJUIIqT0cQf9sfd8/7laef84LR/dnXx9KI3mPUHs0lvSoKRrocYX4GGkK4vFnwmr1+7jK613M8oJQAKBAtSfnY9XbvOGpKyQrKE5sQwLRQpMPMm86vOwJEpUa87MrEoX67taBGQDs4fPTs+X27VqUTe/ej9t75wZ39n+96Dh7e2944uupdXvSiKVmo1klPG6J39/ceHx1SiFceRJYkRVlleunr20JRyIpFcJLHkb++s7W63n56c1uu1J4cnq1vlF/ba9FPj8TxKIs5IOAvXG41Jf7q6vMQYASmAfooz9uloYfq5kyZ/Guaj07/4tz/f3Nta7IkFVD4V0sKJGM9Go54hy5B0YAXQgN7T8wNJ47ZsizyhhNSNJUaVUr3a3trYvdk2ocdFlERJ4IfBLDK1cmP5hdQf6WUmELN/+O2/lZP8pd1bE38+9WeaQlVF0RQj9KPl8nKzssoLnpNiqVbbbK1utDf7QWcyHYs864/7nLLDy87jZ6eHJxcXlwOSc8c0A0+409SQzJKlz72AZjRP8nBahPMkjJKhNwv8gBN1MvWuLsedq/F87qucL1crjNLVpbqty4yyMI055dWKrSvSeOYlsdAUvtwo5QUyIRhleZGncSJyEKAoihzEdcPz025/7CVuUJJD6POFUzwB5n9di0A/16iKz00/C+H+9OLisVPZAa1TuQxugMmIo5/94uevvPlFojYBeWHGvB6DJp8GjGL48b37T87OoiA863VeurV3c2/7z374486wJ/Ls9q1dxiWZ06+/8eZoMguT6Ojq7FcP75/2T0BzTvibr70EZc+qrBAlAF3jauaYtTD1/vydnzVaThjFk9m40a49OT1trMoyZgRplM3kHOOLcdWuLdslXlBvGqTe/OLk1IbJzMrnzkO4qB8oIMDzZDLvnDxurr/yuQ1JgQISp2bJsDioAm+WhafQBgSGUSO9URcFCf00DdEbDuNMTF3Xy2bVdVuT1Lq6tFSqLDnVlXrjrHtUb5KlernbGVyeT9k/+8//YLnZ3GlvTmYzUmSWo/nzqFlt+m4yn/qlqt1slOqNklmSu+MhilxXtaSIkiSUqTLye5GXijQbTiazYTSdunPfD0VaZMhBFK5TSimlEudh7qUxjbKUcsoyVohCY9wwFEqoqkiU0jgWmiZThmatvFR3ptNg7gWeH+qaFkcJZ1RkYjr3r5VEPwjjJOWMq4qkqqrEeJKkhNI8L4TIRJZ5XjjujPzByEhHJBwEw5FcMhdMmi9cjfHCB/uZLyO5/mwHquD8/FnDYpCvfwzAJA3mY3fUWltdlGLxov6bAyPEvYePP/jBj38Ui/DVl148ubhSuHT3xt5Spfno4LDdbnmhv7e5YammZZtBknzw6CFknhaivdHaWt94+bX9N19/Bco2oAHnAFt446Lh9ELW+Rfu3PyzP//x+tbyCy9v9y/Gd9ZfJDBmk3nnZOjP4jDMNM2azoezWfD+wcFZt3drY1Nb3lwY5W3AQDoGSxeGzTGQ1lbMX733qGEGamlnQbXr4BcAFJR5ncHTw2M3nk6mbqVaUlCyCylKM6Nqr66uvHfvV4qtxFmgmBKjhBl0VVotkFJkPoKcFZJM+8OBbijj8Zz99jffLNk2ZUSTlRwkiP0gCLKUgcOP51EYv3z3hqyoqi0fnp4ojMiKvLOxoSpymsALgopRblUbMld8ERLCUhQ5y4qMUo6sKDhXmuW6ZVgEPENeFIVMJJ2rhiJXSlacJOWywRi1dU2R5ds3N+sl0ynbcZTEScop1RWZcWYaap5nrh9SApFlYRSnWV7k4JyJLBdpnhXFpyTLsjRN8wKkQCxEGCbjWRAnWb1Zgra2sEyqiwj0mbrxmVHxszJZMagrmxbY9dUmBTCZ2m6t7QImECw+vuXakRYCxXQ2eO/DDy1d0zVjc2t1f2vr5ubO//2jd99/8MjQNEPX15Za6+utx0+ORC4KVqyuLr/66td2tm9urL/WXq+72aSkVRaf/VEHbCAGzr//iz/73k9+HMThaOo27drdnbsf/vSA58zgqmXoqrFVa9wq1drUm51fHG7evW1rhk60y6vuYD5tmpIkUfDFXWgmL64FXSs4CYi1VFU+/vDQnTxtrBpADgyAFPkUhAOa7GiNNUcCJDDdqQO5puoUxZODZw8OH4zHw4KKxvLS/t1tTTOSJDYNLUdxHvQyXjiGdXJ0GbjRYDi1ywp77bX9NBdzf044bbdXlhpNbybGE69SMaIozWPywv725t5KvWFs1tcrju3Ujf3t9Rdu7ru+t13/f8h6jx9LryxP7Fz/+ecjXpiMyEhLzyqyWMUyXY3u6ZmWMAJkGpKglkbCCFrMQrvBQICWWmijhVba6g8QIGhkZgSpp400VdXVZeiKZJLpI8PH8++z12vx8ktlo9+C4CYyCcZ595zzc+fg4+++gyn9/NFjYywXDCEsGBOCEW6F4EFEow7vjaNukiCPtXZK6TAU77999M6bR3EUODAU0V4avXP/iO9u004GdTmbLZW2nSy5mMwWqyIvS2ssxdhYp5RGCDvnCcGBEMY6qRSllBLinCWUDHpZwKlU2lrnnWeMYESVVMlW1EJi5jXXiWt3e9XW3IbTDHg8BrLTytQEQAwQAXRaR9bmTyvV+sTZFfKak+idd9/qpPHkOi/K6no6++WnXzjkG2OHw+7B3vjuOzcvrqbPjk8ED8cHveOL08O9mwCRgbMnL74FY3vZvVY5HAGcN/DFw6dPf/bXn15eTRLS7aP+773zvcHeu2/s7lADB+NdiIYAHQCYHv/NZDqpynr31lsgmJMFJvRnn34y6Gdb+3cAAgAJ9RqqJQRB+72KNgitSLcO7h9uZdGj33372Se/xlh3+yMwFrwCvBGqUBF3og6HupxPJw3Ko75wyBTrmoVCkDhNskF31Ot1eMA4xRbwt18/uji/+ubLb5XVJ08nYRx9/usvyb/3pz/tJ9kb797pDzrU0TSKIh49evY8r5aYOMxtvz+6uT3e7g13egOC2Hh7JxCi2x+EKd4adT1Dk3mxKtaLVZFGYZQGDjzmIk7ivJmnUViZJl/rVVlWleKc8ZgYZapaLZbFzrC3f7C7k8adOEbjMYAAnR9/c/ziclZVjZRKGysI0dpEAdPGOucZY4QQ74FgBAjW67KWSkolteaMRYKOR13GyLpSGCGE0O2D7fH+dsQZEhhI0I5TuF0OdOvExC1a+7qRZGOyitqpbmOQYa3CsQaw08vTf/3Jb+/ffw+zu8+ef1I05e++ekJRqK1L0ni8M/qTf/tP7t+7Md55J+DJsL9lSH7v3ZuNqr59cDaZXUYdNZ0tnILZZLq/+zHACGANUDx58fPqyuxE2/udg7/4+d8wLYyGs6uLBGyp1gc39yBOAb0D8AQgfPzNF5XN86o4ur0FKA2yYGvvB11OYuG7o52XeI1uQEoICCABYAHy9l33AFK5qpNE0FW7R2OGUiCkjTXZYEAFQA6E1K66mM9GvW5pK5PjLM2+c/ud77/9PjM0jtNUZAlkCkypKgReSo08Hx+M779/Y2unT/70P/4jxngSpwdbg+3eaG+w2+/0Pnvw4GzyHGPCBdruj95577YjbrpcaWS6YVrpmoV+kA2yznbYRQr0xfWk20kbJ0f9TtJJvNdRwLc7PWsxBrYuCiW9csoaF4cBQ6TfT4fd5OT0gmg/XawfPDyZnZy59UwtizDEZSnPrmbGuE4Saa29B2tdHAaMEowRo0RpW1R1XjYYIRFwZ13dKAQeeX85XU2Wa2ud0hpjYj3M50uPINoathNV1NIvr9zIttXGbIDKDXOAW+rm1Yy8YbRcO9vlAOvZ9OSj778FMHx08ld/+bNfzJbL3/v9Dz764Mdh5r7z7secuyTGAAJgf0NnbQ86yOH5VdnI8snps9F2/+7+u4MeGe1mFFatZqTIPE6G4fHplZGmVvJsch6L2CHzBx99P907AhZtEk98MXFysXP7wyBUe3fGxFrC+ObBHu3EAVgab7pwBUhDyIGgFpe2ACnA1iZUizBCo96gO2Zo4/6KAYYAQ4Cw9aVSQNtYr5lnp6eTLz79Jg2i27sHgoneaJzEeFasHJiMZjXobqfT7Xe8Ew6bIKbj4Vg7RP7JP/mTu0eHzJG9wX7EsiDICEHn8/Pj02NZKx6zXrfz0Q/fSMMk64TduMOSfpIkFCcAIwBCkR71k529fhKEQcg6nagum2cnz/ZHN7mIZvMpMhgDxgiw8QGmTaGLsi7WTSP1fL4GRBerPI2jZV5Wlbqar799erlcl8Y4a01ZSQeum8baaOtAG+udL8rKeW+cF5wbB0rrspLOeUZRWWupdRSGnThopHHOJXHAOb+YzMvZ6uTZSTGZ9scc0Ob/ddritKKl+Vgbr2dbM996M4y3GodXlHwh5ddPr7/6n//lvypNfvvGrUEnvVheDAZ9zsio934afwBQKT3XSAp61P5sBlBqVYkIF1Xx3vf2724fASQAtyikABlAf0OF4QBZ7C6ursJuwDk/vzp/dn56sLN7eHPv+uz80ZOvs8wL0Uc8wuIGwCiK9gVfziZVoxemqkTEIS9o2AHaAxAAOTQSxIYpZ63PdLN9m/YJ34DVFGDcrg4buvMKgG0IUAJ2vlrN1pOd/jYhuKG+G6YCaaXkt58/Dijvd7uBZRhH1PLjR+eH9w/KdXFncJsGiNy+uaNL+9bR21Uja1mezk6WZtobhXt72yfP52VRdzvxd7/7Rsg5QA9ItwX9GOjZ9ezps4vzy4vlbFpeXs6ml2ul5WpSjjpd7xzH/s3DG7e3RxyhUZxgQGXRAEAviaVUTa0DzuMwqOqGEjLoZuNRP02i2SpvGqW0AUD9ThpHvK610qasJUbII08pxQhjTIx11lqlLXiPCTYWAGHrrNI2r2vwiDMWCK6sWayLxbpqlFFK5/NZsz7LF8+zwbzticVG/LNR/rQvXA2waHVBGwtd3ZKhBcAZpVyy1W8//XI6mw+303xdvnH/VkhirHivf7gBpcLgtqBdgKhlEs8ACKXbyM4Xp8v7wwMUbox9ewAU4AKAthb5gCBEMdu/cZAklFqmtCnqOsjocNS/mM4ePH1WzCe7++NW5C0RNGXRWEWqpoq4I2EEfAywB3ACVgOzgLqvuQP7AAUAAcgAopdrwcvnfMP5aoALgJVczyjiQHy1PluqldSyyo2S+vbBwdHNH8aMYI5omN44/EGvuw3gEA4YkACPA0QHUZ+EvhP0a6jI//Df/1MP7osvH0mcW1HXJM/SmHpiC2QVPH9x4Sr/47c+IhAxkQDWAI1drrAzv/zrLz7/5FlMRLWW3351fnYy2co6d8Z733v7HURdJuLd4ZBR6i1arPP5sqwbNeimdw53D/e34jAoyqpUCgMMe1mvl2FA89X6+dnlcpETSglCQog0FtbYNAmjgA+6aZqEGBAmqJfFznkAxDhnjFCMg4ABQkkSbuY27xDB2Dq/yIt1VVWN8uAxIbVUyiIHfHu7GyQbGeqi7ZtzgApgBcAAFEAJwNbNNZCColc6LdHqBJ2E6y4dpJ3w+mL5h9/7/WLptkdb5UIdHN3xZoLwRjwyuZx+cXzx21n9NAhzrXLOugCEYllNlVImSVOgmxiYjSYHWvzdAtyJ4jsAaRyzO8Ph3tb+D97//oOnTweDzocffJAkfH45Z6lKog0RZwHCOL2bZNnk8hzAqKYM4xggB18BFoBw+7ewFifbMB9TgDlADkAAOgCD9puGAToAlAoOxAEw0PUXjx4+Pz7RCGnbSO12R8Pl5NoHUEwXYbrpDxs9lWpgGWQ8YXv9ICXgNGjyn/+jf0dqNV3OL85mP//F519/+XzA+x+88W5VqidPH6/qVVlrQcWw26PGchEDDTGTx+cXnz9+Mp0tA8p63RR75A30Oh2M6WS2KNYyYJFzeL2uOp1YcDEadNZlzQTjnEyWq3VRNco0jQ4Ee//O4fbRbm9rECKsjSnqhiCSxKGz1lhb1pJg5MHlRYMwMs4tV9VsmSttmzUtyAAAIABJREFUMUaBYBSDUpYQBAD9ThIGPEt6yhhnnfPOgbPGG+ukVEpqTLEDX8qyVKUsSuJrIQxgDyAKczyZXFLuGSkB1hvF39dPH51eXkYZCunmNzRsR7Sa+EYpZRp0cn65t7N7Obm8vL6+f/8nABnCtO01l7/47Bd//pe/mF+ul2f5zvAgTLYB0unZxb/8f/7cEVwvylGXA++3YqTob4+DAJADNM8efTsp8+FgUMq62416vcO8mv4v/+LP+t1sf28LIASYAiiALYCk36muTqbfPn2e59P5+sVo2Gm3Zg+QtoNpBNCHcjJZTKWqyqKKYtouoSFA2vbTBCAFCAE0sssgivrR8M2j+2/efXd39x7gMCBAMIt6g5ZuXkNTgVTLybKTbUS5gMADOHo5ufrBR3/48Yc0Gh6Czv/b/+6/+bO//Ot37ry5MxqFaRoEaZEvnz47/tGH78dJ2lzPHNa1L20OGUqiHfH0dHpyNYtptLc91EYfn12ncZgEQtW6G0dA8MOnZ1JpTHF/1J1NVkYXo1E6ma/zqrHarIv6i4fPwrNTQUWl1HSWW+uFoEkShoJ68FEgsphfzVajXnd7q3c1mQlObeMwhkjwbhYCQozydV5Y6y4nyzgUXFijNQJwzhtnlbbGWQ+eB6gxCiGNiddLeTab46eIMnHQH777zt1PP38SYEqQeHx1UlT1Vqc/yWcPzx4xJupCHu6vb+1/BHAFkAJUzl+8OLsEQ3a3dyjmjAMTXkSbRUG2pikMUHjtfvLxh1EclmXV3/57myL65aefPrx4vKxnP/ne93VZs2TSanV6ADXAFsASQD148H+8+eaPwaxK1XAg62b209/7DkAH4NqC7g3Sjz/6kYcSwXOAFGDcQq2jw0N56523m9X1148f/tlf/OxHH/wo7t4GWAMsX8IcwAFKiPdG8UZbMCnlPBYeYNCC1eOWR9kkB4RFYwQJt++OAe62WTXNdDoZjrfa4dUC9CEomovL4d4RQH4F023YBxAUMPmv/uk/PnrjH7Boa3b5bDI/B1xRCo+eHRult0adVVnPlguJKyn1e/fuXszOJ7Pp9LqYLoqmsYejrFzJkAdK6dW6LKoGjEvC4PaN8du398fjvrN+uS4Ep0HIdrZGt/b3QyGOL64ZI7I2W4Ot/XH/arbKSzldri+uVlWjKaXW2WEn7feSutGN1AAeYzTqZZGgUpssCWqpMcKNVIt1JShx4BqpGWVpHFKKlTaDThJyWpSVQ4AIoRSD8CKOuWBR1mVEgIG1nCtnApxcTuZfPHr4/OK00e56tlpXdTFr1mWzqOaLfN3UbrUsA8cHMeNRD0D/za//zyfHZ4P+4HBrlwT7lJgsSaaTha31zu5BK8DcGIzFnZt3b+7uXF3Mb4xud7p3N5Vw7+b2bz79lTT1xx99ODrYDHNbAP22b26I+Xo0wgD3AadbKd7udztbIcK3N7DwPJ9//PGHgnYQ9AGGLVzc2+AUWNQAhzRIdnaz20e3eRABDFotGmsFw9FrbbrhVLwWudUA0Hbj3qgmExHWQbgF0Gs3iQbg+ssnX51enqK8Eqq5uDwJQFbXMyCcp7R2ZV1ZzU0IdA0L6iOTr/6m0fVvPv/s0YOnf/Djj985vNMbpg+fvPjzv/jV0Xj7V9OvBAhw+LOHD6TRZSEZ0JXOEYLFHL7/7h1E8O8enl5cTbQyURZ6ZKu6WZSFXa1WVbWsytWiEITOJ8Uyr/K81tbVshkNtvKqqqq8aqR1CMADAmOcREowdj1feOgNe+nXs7PJXKcR66R1UdXzdaGUsQ4oxhgj5GG2rrwHa733RvDIGC0Y2R11/sf/6V989tXpv/XHP9690dPYbndSRJklnlJ+fnw9W101tkIYo4CsluvFak0zxFmZBmkkxGpVTq5nNm7CQHCTAKD1yh4/X73FZov1+uJ0cZafSGtf0LOPv4vefvNdgKjfPwI4a6OHOi1GRQFiwOr23t3O1k9bvAqBCA/Ge9PmfOsubyNqPm31cBig3yJ8PwBAAD1I30CQP/j2X4231rr2F9NZ0NnKxNsAE4AdAAMQAFy3f37WospR61vZFFD5Wqoch5cwykbT0W0j1aEtPtXu3RpgCZAA3GjjnqGNeIq/8+Z7xLNyWSyrfL0oVFEbbSw19/jtIA524s2SEXSNJf/JP/qHo8H4L/78L3Wjvvfuu2kvWZVrwogDe7i9+9e/++L0bAIev33nTlFUz08uv3n0fNEsswEPgb5x88bWsFPWihGEwCpjqqpKeLA17F5czx4cnz+8uLycrrwDbaGsGtlIYx14zwixxuTFGiPqnAkEB++k0taYRiprjdLOOxeGYrZYG+uMNVWtG6Wsdc55Y5y2tmlUo0zVaEYQwRhj8N5tDbLD3S1j9M9/8yUA/S/+wz+6dbAVcuKQpxzXhbq+nMxW03VVVKXSWiOEnQUWkCIvjbWudoe724N+tlZrqQzCZNQZEBD9JI2Z+O1nDx48fPrWnTcur2fDMFqsq0W+Ql5mnQwgAdhqF9hXb4YGiAFcEN8DWAM01cXXdXFmqsn7b719795+Pz5qA6ZRK61j1/kvY7GJ9No04hnAC4B6NByfHJ92OumTp+dfP/62PyY8ahgwgEuAst0kcoC6VSttoLsFwKp1NJXw0p6OX8swfAU+v/qgVoUbtFNj0DIly5f6x/IFGEUwwVEkIqEKvbs9JpSPt7ouJJ3xDcR6pZpzIgAShPvkn/2X/5nX9ptHDx88efTuvfu9LDw42D2/nj56cvzk+OTF+flskQNTtaryqliV9TSfr8r11fVU1eY7b7/diUX/xtbu7f37O4O6UWWpjm5sCY6uFuuzy1knTsuillIihALKjPHe+5dEIgKKUZYEWpuqkiJgxti6rge9zqCbFnVjjalqqYylBGdxsNVLokhQgpbrqqylcU4qA4AYpYFg1lmMSRIF2tnpuqHR9v23PvzRD3969N0PBNaPHz1+cnzpsXfWW6mni1VTu0h0imXuPVaVRhxVqwY5ZGsTUhFGYlHMq1KCxwELoXZOAnhLABNElJNPTo+72eCH3/vu3dt7v/z08+1eJsIRQK8NFaStQkQCzDcjUVO9oNjWsirLGhEfdnCSfR/gAMC1qMdtgBig1uhyqa8tXQVAAU5PF7++nJ2W+bqTfXfQhSCOf/brX3zn93bub+0z6AOw5xdfW5pH7F4LB16V8EsO2WsC9KidFx3AVltwcVtJGz/iNQBrhWvw2rv1KrsuaB/OFYAHLtZquqrKCAPiHYrMolkMbxzgOAgyYUBRoJwkL3NJVE3+o3/3DxkBh82bb9462Nve6m0RRBlFXz548vDZs6vVFHPwQNayXNTzWXEpXV3VTZPLNAhVo1bLHBqZADqf5g+fX67zoqzlyfn0zVsHYcgownlRCcZCJhillJJGGUapB6SUBeSdQ0HArXPGOEIIJiSOIsEYgMOYLNaVtY5itLfde+v23tHBlrOuqJqiarQ2gjNMiHUOADvno4DPluV8VWnEO/3t8fZ+t9cPaGRc9PlXv3v88OnR+AaySCq3WK+KIq/KClnCIaEYjDSCs4gmWdxpKvPs/Hqymufr2uQOKUjDGFNytVyuTF02crJYaC8pjqvKTibL3o1wuprsjLZaEcfmDcAeTo8XX8ehJ9AD6FBWAWYifj/tHYUpRcQBVAC8xRp027migDSErr948Di3VxAXO+HuIDvoZCMABlgCDN56u7+bbgHsArwBsN1N70RsE2oebsyq/KWBfqNWL1sz+hCgC1ABLNvxUbc2u0285sYqZtvU6Qpg/reTRHBrVCkBytIWSdJZ1mUcxB7Uxfx60O8A7BAg9KVFj71UlWpF/ut/9o/XKr/O598+fjZf5LKUzphnp+cPnz/eGvVG/dQiW6rSeUOJAAQA0hNjkMEYL9ary+n84nrBGBuPRpj6k8vrG1vDNImKsp7nVdVIzlnTqKrWUpu8LGWj87Ja54023jnrvW+kMc4aY621UjlCUJaI5bqaLlcEkQ3umsYBF+zrRyfn16u8rJtGeQDnvXfeOrv5l7pRzlvKeF5VdSMBfJHn8+VsMp2kUWe1ulZav7i4WqwLACJ4gD3q8A7GbDjYFoR0osAaKNZlXVX9bpJlMbVYN36YDY+O9tZNndeVcZYRVlUSqHXCKG9WsuwlnQ/eeq8lEjbrfQOgEODyqvr8k2c3j/54wxX+65//r4cH3wfQLUZ19hotIdvuZgBqAsXzi8uj8U1f0DjcBEn3AUqAIcA3FdQLnSdkww69Isf2ALCDXyCYAPQ381M7s9O2kzYt/hcDBG3fNK0yYPMxABZgCnDWxl7T9svwKs/m7Ddf/+Lnv/r1k+Pj6WKuQT99cfLm/bsUvwol3qDT6eaLVC/OyU///tvjw8HRwY1ABN88efbVs4ffPHv+9hu3emkaoTAKxNfPvpGyUbrRjXQejDEYUc4oQzSicSGb3NS/e/Lotw++/uTh16UsR4OhASWNcwQw9vMij0S8vbVdlmXTNIFgFGPnHaMEEWydoQQ7670HQnAg6Lqo8qqRxhhjjTHKWGvdKq+en1wv80oqZaxXxoCz4C1C2FhnjZZKWgvaOIvwcrk0RmOMizJfLxfXk6t7d+/zMP/20fFktqqbWlZK15Z7EicJFxRj6ETJ3aOD07Pr2WzpEYRpaKyjmPWzXhwni2o1ldOQR5i6hhYOWRbTFKdOYQe+buRWPDK1OV497ECARR8Ag5nNT2eykvPJatyJWbIF7unh4ZsA67aXPQbot1pq30b4fgtwedU8/eSrb588uMoX5ftvvgHojRYC7QDI5+WvtnkmCCMvT7oEAJdnz36d9QRABbL8zVe/y8YLAX0AB7DflkgDEAKY9hDMxrazIULK1sv5yl+4Aauz1tCawd/6zM5nv13Mls+On8dJGrCAYOydvbn3FgACqAEG7S6yCY7IWIzIT37/u5jx+XT15YPHRNPx9sAbl4bpz3/z5TdPn3/y4CulJQGKwAPxHoPWNQKPMKGUMhrc2TsQgq2qspYSwNRSN0pfluerul4V62Wx5JiHPIpDHgmy1c+SJOGcJHGQq7pylaeIE2GNQwgZa6taIQSMEkKIbDTjjCBEGUEeALzRxljLGKUIwoB6Z1dFaY1xAFoZQMha11jjlI6iOIrCqqqrai2bajjcWi3m3z5+LhtLKc3SRAAedjNCmCMAyJZVfT2bM8K1MSKkCtkwE457g/xyuvYWpLHKNAS5+XwhfRNQPt7aVkpb5ZpKP350vlrXs+s6iHmnGwIsr86vIhE9enZ87+AgiRiJE0D7AIPW4y5bJeOmQzmANYACCNcwGdAeRKYTdt567zDiN1uqMQQozma/OD+5+svf/M3+zb2VmaZ0vMlGyHob1UmFaHdvmFpsGNzYACsAnTb4N2pHMQdQtwKnjW5lr9W1b2bnJUCzyb16LULw1U2PKo0YG9QipB5cJ0uTIL4x3s3rRRLtAPSnxc8ibgG6AIuX3xC7It/76L3p1frqbGFqxwmLw7jM5cnxVWOlED7g0bpcYYIJYtpajDynnFAsOAWMvPdaqYBzjNBkPi+qxnptJHIOX68uV3ld1RUljBMK4BB151fzslJ1IxdFeT2ZFFXDMWeIOOcoJQjAeW+cMcYbqwmh3oOUDQGUxgITtLc1ePf+AaOoqJqylt478G5V1N6D914pY6xxWosw3NndTZNEKY3AOy2Lqpxez2UjG9kEoagr5axvtDfaWOurUpZFXVY1IRRjjAGB9xhhR3WaBMgS5ITHttRLIGS9WnoEsilylSc0CUmsJSAEZVNaZ/O8vnNnv7KLXnfAY4a9HvZ7/++nv7g6f3RjjIHOltNvg0gCIIAuwDUAbt8bCZAA7ArIAOKuuNUdydWy7sTvtCGSS4D6cvb0fPVCF+ijex8qaSO+C6AMnGAYtb1YAxYMOi365VpbQNC2vLK9UOPaq3th69PkADXApKWkNrN/BSBbIcmrf4YJyebV2d7RdjykW+PhMOpc5JcgiojsM1eZqqEib/2Ly9mLp+RHP3zvYLfnmblaXF8sznggLmYThHAkqAN/fnmpQUc0qk2FPYpEwDnf7+1RLFKeCMYu8snz6zMlIQ0zQpAjxjqnnZK60c4gQhRqGqPWdTldrnNVEEwqV+nGxzzIksxqHzAWBFxb4wEQxto4gjElFAFBGHnns0QMe50sCWQjEcZVLTc4LQBQSotacsoBQFvNKCUYx2nW7/c7WacsS4xxXZYEcFUXcSCikKdJDAC3j8ZK61orowyjjFGGESaYAKDxsB90uXKNqeReNkjCTl0rhMBTn8tFJxiCc12xC5JwH1ruEPPMMoQRJTTkoqiLxyfPdoZdSreyXv/rR5/9Xz//83k+37/ZoZE0oL9+8HB3vN32r347A20EOcu1/kaQAMAziDpxBrAP0AWoAR4DTP/qV3+9f2t0c+8WaDTsvLFhhBo/ZSiT+XnjC05vAEQAEmAKQACGr4Fem49o11JoaU3SGgg20Nomx6oPQFtNaK/VdxRtPr8AGI67nR5PeqwTwSFAb5AMI3IHoCJUI4owRu1fFEdZQf6Nf/MjxhnycDY7pRBcLa7iOAVLZtMV9kQIWqnKKI+RFyxNaFzKOtcrY4Eh7q0TEAoh1vVq3RQ8iBE4R5RxDiPvneeUAzbGSqtdXWqpgADBmggepEnY76b9LCSMGqubWgFCxliMKULgvScMa6WNNd0syuLAA4iATWYrqYzzqKqls65RWkqltaOMEISsdZjgtNPhQYgQBYRkXV2eHM/nM+d8EoUY+aqUURB6D8YBo9RaW8vGe4QxqmXNOSttE3bRslrPLpbT60W/ky3MgjCsQTLKHbiqXuz1DgIURyJWThUmR9QcHfUGWfcnf/APtrcPdsfIFoiF+wC8qc5/+MG7d+4fNWs17t0Ig2h3PAa40T4/VZviQQGWzy8/Oz4/2xu9BdAH2HnNtPeilrOvnj18486bD795Nsp29se3AXYABgCaodyY1TcPnpdVMxzG8JIhGP6dIpN/R07XtJhFBdAHiDcqS4AUwAOsAXoA6Wat2WR8tML3qs2D9ggOAA4AKMAIIFbwGYEYcINekhMGQEk0J//pf/APe0lqrcnrshMMOIqcQqARB2qNVdJrbZkRCe+ZWmeiwwWVTu+m23d2bi6XVcB5VdfII+UKK52zPgh4yJMsjGpXMI4RwoywMAhjGnNLCWJaae8dAKplY523zgMAQggAEyycs3XTeHCCMoyBYNRLo/m6cMbtbvW11UEQEIKk0g48wdQ6b42RylBKCSGUizTLlNGr1dIYW5W5kg2lFGGitLIWgoCXdQ0Ov33r4N7RjcfH50abQESEeqkVEziOI++UtnoyXzx++MwKR1IkQWLPbIlT0et0e45oGrOG1tuDsbINikxdK/D21q0AQCBb56our6dxd7vbu5uk97ppNugPgIwBRvCyx70CqDYnFk4Ld/bgwdM33jlEeM7gZnszagOi7jE6Hg/CNBzePtwfdobtGkgAcgCGcZiv5/fuvw+wAzABoK3VAF67T0X/TrVtVsK4lXwuABqAoA0Q2WwAHCBuZ7VNWsJ1G0YkAPYAGEDRqoxM1ZwKyhAcAuy2t5oKCkB+8vF3a6lnizzkAQPaS7KQ0SQM0jRaF0VR1hQDR4xSzEPCAmrBN1KN4uFPP3iv20nXZYEYsWCkraxz1HOPKPN8mk+l9YhY5yzlpBtnh+Odcb/rHPLeS6UceIKIdl7JxloPCNVNY51taumdDUTIGK2qhhIqOI3CgDJqjV6syiwOtwZZVSvnQGvjACFEMcGcCkJxFHeiNC6LcjFfUEKkrMH7NE0IId1er99JEULaGGdNEodFVfY7MSEgjTVWY+TTJETEearjLTfYycIsEUMuhIjDOA5C58BRRwInSVX5vIEiSLiSytTer2BZ5ufz87tHWaPMZTlfVKvxYCNn5QAFoE123ybqgrcpMptHpQtwxBEeDun8siAIR6Lbcjv99iGZAvQARhgOW9IaNtpxgAYg6Q93AfYApiA10Lp9CBuASVs0ADAHuH7NxfnqbdsgZHOAVctTpX8npmRDCaxKaDjsAYQAu+0ftTFdNwCJoL3NccEWB9ksIoJ89OHby3w9W8/BYMGJ1qappXVIGUM5TcKgrBoghgZgvFlXeRiFCPtVnWMPw0FPe3s+nShUYxdkrBOSGBGzqKbOWYQdBsK96MRpFPB3D25t9zuPn18ihJVS2hgAZI1x1mljGEUIvBCMEJLGIcKeICyVxhgnUbC/M8jz4mqWl43S2jjrASGMQFnnHCKEOGs5JQ6huq4ePX721YMnVdVwCpyQOBRpEqdJxAkilCGMEMJVI6/nyzQKe50IMNXGIIyCmFBGGAPVGM/LbBiFIlErTL0gGATitgTtlcGlK6iVDjMkK2UrBwqHXERBBAQePbieVetSS2XlwdYQwAHki8lXdXEaJqxtha+SlMt26csAMKejXud2hMW3X/1muL3B7jfxWPlrdeNbLmgFsACIAEKAQ4DxyzqmpD2cNWlXy03IzUOAWQuRBK9lXC5anfomYiNu8Tz9t7kBADgu1DwiIYLNfdVJ6zHeyEA67VqzAZ9f3b7BAIT84AdvL4pVLCLBAuQQ8qhupDXWGttJ4k43KJocWW6wNkbf3j547407IWMH2ztVpcqyVlorr6rcjAYD5gJwiDjGKAlFyAg6yA7f2Lv1wTvvvXf/jdPT82+fX1aN1UpzQR14jMAhRzklFCuopZcAnlA86vUEw5VUCHnBCXgnCEqSII1EIMRqXS7yCgOSVoVD1L8pAo6yIGWMKOtl05ycXjx49OLOwQ6lOIliwWndSG8txpCXpVKahxT3mmyLLub15fVaKlm7Sowr2q9xR9IIcKwy0kVEqQqvrxuiuatdEGEe2GigB0eWJzZOIMqwIJFTENLAU+h2Ium1rHQ5bbDEbx4cpp2NTTdy5KLT3QY4alFc1pZX0/6+F62JNwSYGF0kaQbItkT4xnC1avn1su1iwxbBh5YkTdsOuFkeWStAX9Vwxl6+WwigaFu2f6kRgkU7cvHWW7/x2uj2W0EASk4E2ujMYNmuyZcAtJWZvAq3gjabY6MMwOTj77/PKCGYBJTdvbnvwRNMtvqZEDSvV0VdOIcrVwnC3r157+1bRwSRNMmMhMW8bJRZrvP5ep7PpXOeEoEE18aHYVbLijE0jva8Q9r6pnRfPnzc1B4DwgiliWjwYmUmBZrnbm5IU6GlEQXvS95TLqoglbRTG9BSmapRWZKMehlCQAjSTivlkPDBgRrdo9hBNbPUkdmiwpzXZX16PUkysX/YFwkghwihlDJGMaOk30lraYwo0jvr9NCJjOicXF6uszENhx5Q7cjSUYcFql0la4kdrZYQ9fDed8DHMyFoRa+KfIk9s7OwnDbOaZW7bjAu8tJpZ7Xd6nQOtnY+futenBAcpAAdgBWnFuCgRRCKltvJATBADNBtCSsAcICjpHML0Fa7G/p2Eh+1o9Wrihy0ATZ526qg/ZENo79u80QyBqI99l20jOe6rXvbvq+ohUKKtmhUS3puzpXuAGQAm0Fz4yfYBkjaDovbh7B47UBMAAA0i0LAkbcuEGS+WhdF5Zw3xvSyeKmuTyYXXvNhp7s7GHuLvnx4XCuttEGYzpdL700la8aYEF7XWvnGNN4CTlEoTIC9O7+chGFwfjljlHLGuCCMEsHpwe6gVxLjd5+eXmnteeDjYRgPRBgw5MB5Z6xCHgvqFCtQEXlkalvzHqapJ99ACHj4JmFpNHlelRdgVogS75FTqnGhfuNHw/4wjXmk1pZYLwb12fGUUjyKBlrJoqkkO58+mw5HW9sH20nCRdzJ4qRB5fW5NYaFOwVQiSAyBCPWZAN+4z1CI5k/9/PzwqkuxRwRqmqkNefdNEBQlmtn7Covwbt+mCCEfv7ZY078D34SQRi8hDqrpxBlAGnL//RaW/wG4BgBnLXZsKgVcbj2zlX+2nGMsjXBJ5sbfgAzgBBg9v9LHV+e0rYtF7lxnkKL1o4AVm2A40au/bxFjDcc6Lw96DFpJznVRkNseu5XACHALQDRRvua1jmRAiQtV7tslQQV+dN//4/DgDeNTkKexmEttTRaCOq8XxW5lJZR5pHvJglCUFR1IsLxVjdvykU5V2C0l956QH57p5NlwapaV2UlC0mAEE8xJhihLA6Rd3EoOmmktZZKI0BlrrBjSmHakcF2Y5GTc7w88ctju57pqqrrCa+vqVyjwUFQxfOpnyz89PRkPTtW2U2cbpPZc3V9UhrltDEaGch0coDDvheUpH3x9vd2tm/0RILKqro6Lxb1arqaV5WpC+2s4DzQCqpzAM0Fp9RRbplcMt8wXyS2IsZKzglnAYvQ+sQlzR09CdYzNe5tO4PWK8mZoJxXRSWlCTgTlFtjnLNKw2KxrmQltd4ZJiLC//v/9s9fPDm9ni4X03knwGeTB93O5tfZBQgB1gBzgGU79ZsWmAWACiBug48AQLc75sYXM24FldBufxtesgNQt4CFbBXbtC2sYXvNDbVclgNYtK/sqo1A8y1DSgAmABZg0Mq+KcAWwApg3mraGoCiXWk3m80UYAmwAigBxgBLen41KcomYGz/zj6mWBqzG3W5IErau+mtO956ZV8sTxbNzHt8b29/vDX42e8+ryvVj9NFXmrvkaMssB6sNU6jJu1zwr1ZaY4YpzTgZHfUW+TFumjysqmlSpP44fPzqpaccsIwF9YWanFmVVU6rCmjRDu3Ao5ANipNg9mplTTHxOKyQ3USj1w0FNcn5fS01BqCVPG+8cIORv0kFHHS621zGpF8Jk8ezSfPyutZ7i3CjngPa1UIyolgqmGcOsbE4pnRtt6+6</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8y5IsW5IltJbqNnMPjziP+8q6WVXZVSXdVQ0iDc0EEYQpH8AYhBFjhsz5omYCH9Af0AMQugWqJEkq65V58z7OIyLc3Wxv1cVAt8e5/AJyTCSvnHMywt3Mtm7VpWst3cDn6/P1+fp8fb4+X5+vz9fn6/P1+fp8fb4+X5+vz9fn6/P1+fp8fb4+X5+v/79f/OU3X6k/IjOHIHgTzaAkKQEUREAEQQGEJBBSAhBSug6eexJYyMVEckgjSQjCsUFCFzIxgAQMOBqG4MDJKALCJZWCAACq/3H+pX6g/lvX25V3DVsSkAMirl0CYObOlDIkaQ8kACDnhyIJJmA4GiQcF37zthmSIIDtGtlhFEWaSC6Ny70bAVEUBTOCJARSCVDz7wRFGCjm7TWBlLL+P9UDkNDt+QTNH6jXQhExJGhxQ90TpSR+/kvSz1YPEnBbJwCaiwWRrJVCvny1NF9sfQaJzPrvy80SEBJMAajPqZsPQKkeGEORSlFQc5rLjeR87SHGUAojIYCcX9f+2//+v/k//+3/4srxfIZyOdiyNnJAFEQhKav3rnp0SaiXk0AGvnsef/f784F4dcDp4AKuXectScvIb98wknvosulpRxcWw9uTN4NDXx/8aNjg333slz0IVLRRqEeu1xuaESPBhL/6Zfv2q4eTL9wff/Nue9717ooAD3fNlnWMuG5jXPoe84WC8/3Wrlkd93cg8RffHv7yT9+uzYzK0Mfvz7ltZjJYM7i1u4f1zbcPTkaCBoO8udHM5k6jBNLMQJICzWChT8EgKefyWirrTioG64dSUiKUzSzE697deFwb615JSSkAyiSQmfUkL2GX9V2ZSCUEgWYUhFTedmpCEiGJpkwBBojIVAqZAlKCBA1xhI8EZI40EzigMXTted368zau2+iZblyPfli9OUmN1L7nvufW47pjDER9jUGyNi7KMRxwI0CHFgfZoBT4kkqMJsAIqLayJIIYDfddbkhoJA5OUHtXM0TmnsjEwU2IC+CGEXBHM379ehm9N+mwGGRrwxjI2zaEwQQQKYhQwjD/TEMzfPP1l79a1Z4vf/ra//C8//bH/pSQuqJvgSOVx9qZtwf4WQSLYGI94o+/PCyWjWxuabhbPHkg5eRi5sa7+8Pp0ABkykgRi9HMvFnmTL4GiqSRIEgoM5PeaiOPTKNLmZUZAKFeLSRIledSMjMCOK0HGgibaYpQIiECEQJaKG7JiiQkB6nMSGTilmvtU5zNl1BRbYBSzopDKJOplCg0SApJ6eLcS46gpWApZDjTTJTMciHaYmujU7UH+lAfEZERMMCsQh9MmKn9h3/7bwwKgEiToqeODhCoXFiZb6Zb1INUxiYhGbA6W8MY6mnnnodFbjAgCQAjtLQ0sLk8gcQIjIwejWhCAKLkZmTMqkykYEBW4s35L7zlpJ7y5u5jj076abWHA6JDiZAacTAIGFlriQQkVGAIEOGGP/3m+Pq0EIJCQoZI89aINJDN3NiOjWBCIBKiGJprX9fLxlDSjAT2nplxMGf9yszIrJc8UQdBWSIgRAYkd6sPdOdLUbzVN83CSUFQzgI4F4Ws/JiVWaFaFxb0Sc2nliSaZabVb6SUYmqClU/fpTQjDSTn1hAjs0eMUO8ZmZmQKaUe2XOu8rZrDCkRCQmRGIkUlgaDmmLQmMomoeJvZFsaUAVWnGX208PXX01I0Ki18bDY3jXESClBUJQCCUQaydpU9rOAve5ajAlINMqJeijeYMzt+ZGVB1AQplZXP/7wIVr6tX/c+nno2rV3yjwiRsgEAQsnPlgMNJIywA1mFO1XXxyNJG3Wr9Doo/nBl4M5TSGCxoQi4EYV+AFDqOUUUmLSANkNQO5RDz9BRqUQKTPrVU7QWRUORI/aZgCRqdasSuosJS8oFSJMzLnNK9A4E1UKSsFYaK0CmXmDW5pYqVYypZSUFG8o7waGQTMHlRRgdec2FDFyDPU+9pE9FCmBISGViZT60AhYzuKTwEhkzuIDsVlG5f4KKiIzHci5jephJXuJtFu4VcBlYGk8rvbhKbviOvj6YOkwkiYMPA/dDYBcHHuIE6siMu8Wy1ErQjcaAMN8J5ip62VfWxWa+eLw8eP7v7+Mrw4WEXuoc81Xx2++/mLv+bSN/bpDin1nDo2I6BioamQGQGuL6xbLXXPI3d3sKgmeiggB7k42o3NEwRfQYIJIA0IwSrfAMZI2C/Lp4KmWGea3Z5ioW5DIKp0kVMViaTb7q4S73bKYCItKfxBQGzJRO7ZuAvMzCpnRbntz4gQDgUxNIAlDQBZZgM7MMmW4RXIlMyPMSBmREgPKUIRG5D7GPqKPiMxIjVQCqVkcM2cn8lI6QiCw2ESkLVP0RAjNM4cD2UMH2ky/MwOlZAXLDHbLNVU8G/Dl6Rj7uQ+4aQuOTDfR2BzHRgEGuqkZl6baJiNfeiwActCInK3Sp4ZoVp36l1vLm1IKjzsuI++Ofv/2TYx8c3/nzfdBHNqAf/jwTPjXb1+djotGZKbGiN773tvYujJpzdzdzAxmGWFtdQokYYJbo8AquwSYMifrBn2iK4Ap0mC31GD1dpIhEbq1n1CVuLmkVP0D4LW1BFaLKaUKQN6qXTVeqsJ4i4iZF6mZtuzWcVIUBKOFIrLyHedN5cSDJFhIrhZTkuq3cAOZ1TogpcwckX1o7xmpVA4hhMgJeaG5+YGJUqqNdYfdkHH7xbdfnZ8v1+tVhWUVCpmaETBmaGbxijLWq8PsnhOkHPz6lb+5u+89rnuHlOKtn5oJTEBLHFa9gdfn7aPQHoCk6IaXXHdrqWc65XyQT3+AEBKoFMx5PB6O4qbchy5pd3fr8XT89a//oW+wP47Tt18txwOUZsequcjUGA9v2nrXjKDS3JZmpy+PJAx1G1pXmUXMCqhKW/wEnCaUBAX5LAlC5eYEdGv/blQDCAZmF0DKavVTksw4gWBVQEqy2wYzzE5AqRvAkxFIIBSV8uqvWehNFqN6yIQmoq61B+ZD6PZigWoFCmzMLJBVZqVUxsgeGmOMQKRCzArLlyDDxDwvq0OCmEFWTXZr69H3bJE5ClgJSYXorDRfSZ2q+jD/zMrKZKQILG7NsDaSyMioHskYI0jWPWfzjGJqIJgbAnXTAGX02Wm/RNitQONWdjA7EMTclnP/GXm8e3j+8FNvB6Uy83g4nO7v/vB8efx43r9609zMOMMC9NYOx3Z61ZqZuaCkeLg7nO7uJFEaYzSStplJhYthhIw2W+5KGhUumNmsosJooKWi8vXPGA6+8Ggza5A5U4tIOpk3WjJFIlRrXdlGFKnMF7AsIhMZuBF0iIJdsCzYw2qD5w3YrBKsOiwYlXPjCVRtMPCFQgIzMUI91Hv2kSMj617AW7gXDoEE2exVinWxiR5hhBma2Wgtn3rfr/1+dVZdiko2hdduizxrHFE7kbKCLILZZG+XZlEtgklCW1oRnFCI3nkLK6HqI25x5wY3ZHyKrRdilrfu4ZbmAFBi1QN3mtjgp8PxXQ9WvgQiM4HrlufLdndcZjdWTK2ymVVzP0LNjIbD8dgOLUZkj9bcwJw9rpmb1WPc3khWXqg+wiwl0NyRhbHrF4mJ9nWjUTXJUt4q5KRCYZBOp9Z3naODN3K8EI+yeMzM+Qn1DrIw+PyGyoEzQkgW2wJEBVj1gD/rYWfMKgUFIcMs/bptjUz0yL2PrY9r7/vInH02CdFgCcx9BxV6rn+5VaEUTLAFzeD/26//zX/+r/+TX//Dxz/8/h/X5pZyyIxtbTYrGDVZGTgNlEEoNgmzl6bBYDSkMCInkWw0wAkzsBgdqdKPmW67UsfaF/TLNqIe9LZnyU+d7mwFAAEPBx4WXocW4+Hg93en18txPa7PI0Ok0pv/9P75+Wl34P7Eh/vTRM6zfOF+8VcnI4BUa5biutyZGwAza4u5mbCbYWnuJCkzgna7BwGcec4IcVlmn5iJTNFonHTMzzPQbN8ntGUqV3d3OHl/WAZ03UZpDPUteSNQJj/BW3lIhDIyX2jO28PN6H/pNIwIFTU7EVlxu5EYIyKGlA0wq/KMlARkcGRse163ftnGtUdMgEySvtCN7mgO40R/Nxg6V62qeXMsjSTbb/7dX/8ff/3DP/z6N4dmdGMYc6gHlbRbwfoZ02Az5OpjYZyJhwaTL02jM5TVoNKScjCTanmLThXmmdxMFvCpT0gEYbWfCCaSk7mutF+9fIFTQqQ7vZmfjs3NTvsYe+z7wPP11f3xp/bYE9fLPqJq3yRcKn3O1oYAWR2lhEwszaFsK8YVk/ufgswtym4FnSILbZqVMDXT8ywdRcdSE1fNp2eKJIhmXN0XN0nr6gIu11FAMGeHMT+qfhuzoFVDVyrBxPgTJ/4s4qrUsvqKKo1SpJSKVGZmZGRQWBrYms1WZ2L/kaN3bT22HvuIzARhZmaCNZtds6CIQKS6ZXbFJ4YCAJaGg7M5JbT/8X/4nyQy9kYxA25KQJkjfTVWL15ESiEJyIobqBIqBlDUFAyedIeiyqlYOoJoYFLGJEOyamcIk6ciCRrpt6w5GYKKvHrxdet2AxBCJU1CbiS4QAcHpIiUcozx+v54OOD5jNFH37al3fFWj0AdGjXpkmr6jMaY6wEjxxia2P+21pyFrKoeOavGSLSClUU4CJocuylHYfRCh5pdAQUptEuLoxUTB5733PsADS96lFTbWJOpJlMFg25yFkllct7abFdm/SsQVX12ZMbIlCIyMzKVMSCsizWuZlZ4sHoXCRHaI/roex+RCRNhzY2LuTnMSQip0YbQe09wj8xMEgkosDasjub02cpzbH24M02ETK06XkY3Hgq/vtDPZL1bgcaJaVXVpuqoGSu1F6cjzqdOFeij0orhJK1adVCkNapRJFwFn2fJf5Fg6o3Pmnzra9ywOA6LAeO4NChjRGstItalPdyvz5d9DPVt4/0B8CoabjwsM1RYPBhb3oIsIWRk9pf6PTu0ubVmXr0pmppBlzdeDMigkEZLKBPuVhx8AkoKylSmHNlBQcfGPmJt9nC3Xnpo0rwp3TgeKlM/6+9m9tUtdUyBH0rISiW69ZMRkRnR+z4iRjViJULl6utxXZalNeOE9kgC1VFGSeaVJOVu5qu35q05zQrmhlXHC2Q3k8hMSFqcq2ttXsBiUC2TJA04NERqoTjMMTywOmheeXcSjCoZtHjUlz36M3BAAziUIQNCOUlAVY9W0DdVtNJLkSGwGhZHC7wwjbr1ySpyNZFAM0TBYckdq+Ow2pv7VW69jxEZvRsXJd3wcDq+910EoiMFnxi5kW3yzkUuGGGZGSEjZbUULyaP23Lekitf4m7i0E8IsqpVPVfdZkS6+2RBQFIRhaiqCwEhLJ7S6Hm+DhkIS030TwmGDGh2Y9XBMnN27jMpGF5QRuloL96a5tYMdyshbVt/PG/7CKWW5uvaDsuyuIPMCBUpksqIERgRI2+dtZNuXnQjYUYBJq/aPtJb0wjYYNdowGHhoRVKpBIj0Ur4dObaakOmmy2wplwJb6x7lm7oni/VpJimnFEoZuaulJmVeJKSlFAGMlVxrwmFvIAChl43NtNqOjZcer1J1nZ8of5CMLsJ4Tb5Wzccmh3XdrpbQb9c9xHJ1NjHsjalkOPuACec3ae8oUwtCycmmyQWxkj3yfEjSWPmqMSZgs1aXtTEdOxwfhyLlooEyRGAhmgUYuS47SQlBEqcSOeFeRYOix0Wv+zj+dL3jIWe08MxE7kSESivVtG3mSwizXhr/ksxhGm2kbOxNQPph6UdG8jcrkbg/ZMCubgfmjc3CSNyjPpSRqiHxogRGZEl0JqZu5d6qrIKFBkigTJjI5xmNprZ0bW2WxsEhdAH2v2CHdpG3i3VkiYsXGiQKde2TBPLhJilRuLG9SVomcjMkdGIDRDoThOChOAUGgmGEtKIhDAiInN0Xa7DXsHpi2N1rq4ek6wr7FwVqQSLwunT5QWsbmvjYXEjlsXGQArNMklJrS0PDw/PH89maAYiG1FK9nG14gDaTSx6voxXD6syS+4UlFmtA6tNexGvq4t/4XYq8jMzxWaqftNMqUnyzc6hatL06Ux9ASDNjqv1zKfLSGUzF5kx8URZiQS43VgpKmPmypc4LAscUJaQyQgVVKz0lqI7DdYtaG1dXNnWpTX36gn6S0glesSYxOysHLCCBgk6oAzOXZNKcIRyZAQjo9wSS6vWRBBC3Edeu1oz7YSRrWRjRRosYYSPbEYrOhGcO/hWOgp7ZERQxvQFEN/vU0cC0Dj9L9VqOw3AuniKQBr1fI3z076aHVoeDEd350h76ZhuNVQIgkIGWkMKbjJibTLm2syI1kghMs1werh/froaeViWZYERdwdHDDdJTLNjm3qXAGUhq5hsqOXoiogE2o24m/xX2beABFo1LCpBAsiqUdVavriRrHZkTlPHZGCrRayM5cpMXXqG0syAonfnz5eXcEZ6cehJTiIvbeo34C0K7eamLGhGMSkkrnuMYc3VO0QubSVsaQ4gIiPVx5RPRypijMAogUkayAwzJNIwJJ+xl4mIHMoxEKE+cgxR2fzFvwkl9qFL195RPrNQJtm8OIziHEwc0ajWTFWNaVaFo1x+aSNGTrrDAQzha7q/scXdyH2kESOjtpzEw8I9cNmzyJ3Hpf/+e4o6uq+Og8Nt6q+VBhIFMkABCTUo4UQjmqksYiXsZWYgFSHxuLatISPGvi/O8667xcVukIMyud24KE03p9GzEKzUIyOv6/FGSs+SBAXKEAEgRUegqLMXqEkYmUWw5SwohdIn45qoXWvgqO8SznvsQ0YHinGQGSSNkPNGud0+AdKLBXdSGPai+s6sOfm9YoJvrGsP9ZBkgLcGA52WyhRGhKaLDtWsRSAzhtRD28ghcYADi6G4spRKJ8hQ5DRuUFialExOcnkEtqHrjh5oGX5sdoSUaMQCdIiWTlDhiuZTUm8G8+mzDskgYwH0FxKVb1+trTWAi08osSx2tzYCX9wvf/vjdVRCliL501Onf7j09BONamZOlBHLSmnLKZMAaIbMeh9ohtXoVuQ63V0pw4hQpgw6HdcRtSa47kjg1YLBBGmg86aSNAPU96QYocxw4/PzeV3LtEJ8Smgv5sLZAehG5Y9MTHz+IroANCEBx2TrNdvUsiNUljKCvO5IVb0uJ2PxZ8ib3VoOA+NWuTVlgMpkmDSLVCi2QvBTVwzc6FXcdFaSzcoZVBsT9NobkZmZyZFjRO6ha8/nXVtXF4wym0JYmbN1A6lubFMGqITATA2pB7Yx7Wjt1f1yWJbLUz/HsNWbwVdx7xiiUiPIxQA6fVYaJYbJag8CMpk0PZohXkcweSUik+KXi70+rUP4V3/+5d/8/u97FPbiCAkytz2yB5upseScKY3RsGv6JW9fPd+aE42s5CoQzRzoIyMzYyhydYvIrffLrn3AgIejX4CdcHJxm4RfmaVC5l5N0OXanx8vy5cL4SkZCCkEt4l5lZV6EEjCIoo/F8hyR0+SdO6IzJiU7vQgkBKLOC1rVUAKsSBdyswqCXHSR7BJ2OomLnIq4re+v1Y3bgZf3CS7GVuVGHLW/iIjIQUUESGl0mlKRHKkRs8+Yg9ce152nXdcdkR8MsxVDLijNTSDO5vRDX6rDqlMMW4KgTmYaGK+OTV3e/yw+2rWDiNCSu/IxNj7IY+y6hNpTIAjgZvVvWRgIUvpjwxao9MwM+oPj+OHjx/Oe/71P3ykQC+rJswEsDli5CjQMtVoEFgdMFzHp0fDS66of6IIM6g1c3MqR0SMURDawYgRo2dCwtpsWaw1/7DzfjGzKe1My1TKkZGE4G7ffPM2cLlR6shCQ6VAmAlqaTJBBbEnA1EeGSfKRmJGGq/b6H0cD2sBhxvFm3Ejt8yYSLqlFKFUmspMU/Itb3RSZjWeNbOiLL7shmAZkXWnAJMvEyATBN1oOKaCUtm7InKkRobTEojMiBhD5ZvdR+5D16F9VJBNGocTU2Eh3NAaFqOb2Y3uTCGLgyQJtEUMZKLRLWOsDnN8//H65Vs3RzZPMoGxjYg4tnV17EknlsY+MCJHpsgRYZxYVMAIsaXJnDBjpCA0nwK2G3tk3HhqSafDYUTs1nqpBi2QxuahyMi1TaE9bvrtC6HOAkuGo/tqHFHrBEhGQ0ZGICIFNxwWNnM/tEvk6UCb4FkAlTm6uDhCoZz01OTkIUlptJvLQgCZkGX9atGnZZEQpEFWSBhcym2P8gghlaDfQqP6D/OyPlhJQ8X9esMY2Ec45m1EplJxY4RuWkTdnhXuz0QCNkvg1BdJ3lIcQSCSKaMkRWpE9kgK6UBoZPTIETFCQxyJnohkQtNRV34yK0eqCDRnM7i9FDom5siTuW7GJxgRQ60HhmJ1v1/sw0V7H+3Yrqk7WFNEB8Levv62C/vzY2CPngJ31X7KrSeZh8XdWxItFVJExm2tCv++unOn0ZSdI3MfEtQDd8f1mvpu8McxjO28Ll3cWnOp96uH1th9ZKGisgXf4FHVDDPzStZbH1Ia5kxQjBiZKRwaluZmrtT56dmxvr5banipkln1gKpWDxGTxRXNK9gmJXpLrJxOM0UoMq3I7ESh4/qZUJT4arNzvFmEWJ4HTTHB8DIORcDMJL57uiryzas1ExkJKsSc6oBNPIZPJsUp/6WJk+qvNjRuFiOzF5EaFDMRc24l3QylF4cicrL/pFww46LGSJ9SsDvdvRmQcspJI6YMwfpYDSGjiD0Y4WYJGLMZFRm2tLuljbH1yPvG3/WIwAIu7g8Pf+T3f/L8vOnwELF5bhHPboOKTJI4tGa0m5MPhhwiysdCxgg0MzdJfWQf0YN75McNv3+/fXjaIvNpy4gEBmhBOrZDc2VGZAbvYEemTTK8mgNBN2cCHSRyZCgzaFa8dmZExAjcHcsz4uddSPzww/vt1d3Xr0+tOQuniKnMmhQsIsbIaeDBjZOa0ZBZk0mUMlNZjnaZlCFIihAIMwxMjJUJibKbOWuSzRBstpGc0J3OMdIJW60K5ayTn4STyqyUpE/kzFQXNAFS+dZeOPFUWIEVL+0LqdTIMTNjokZLojKx+2K8c5cjr8mdoyQ1WWtwujHN4Mby3EgDYGQOIcVRkk/QBLeEJh/ZmHntvPNs5HGxj8/jq9fr/eqX6/5W+fabX33zq3+58+6ITZcz+2Xx18rXGbvi4nE9LEvmSImJZaHAS59kBKQXyk2pIe2R2473W3z3lB+fLh+erqOPZoIopZNAuuBmVCyNdAtx23IXT4z1E49VJHUNKlrhgp6hlPnk+Hro0mMPnIAaGL5c93VZ9749Pj4/HNqb9WSGbWSGMkySCCdhSSTQatsUSgNYelkzRkAI3AwfZoiIkepjem9nxrpZ3Eo6mVpVDV+lOmG18TWdPgCRkHB/1yr0MqdFrMI/p8GE05IlConqgm9jnBOLpab8oFRqtXIqzP2Yyj0yQ95MN5tETADezNh8aUAbNOvuvOyZSoJOuMnhhnSyyD6CI5WpFIv6g5Vh80UTloSGiC0tj7k639757z/u7/d834cBbIdvvv1Fvzy++/Bj6QDMfo3tYIBD4aE7ZdvHFdlXSyTMVL5QQkFFiECGurhHnrf8pw/7d4/j6bxp368jWpFO1GpYHQk0Z6bWxRuxRWbXcXUpP264Zx4h+1nVLB9XuVHL9FIkfkh9RA8Vhn269Nev0PdcDuu63n98/Onj4/b29Z2U0UNwadpKZTI3MslUmqw8hkRZBiZToRSUUd67fQiZ2z5i6nF0MkWbewHT5fySclKXjj3tfs0FNzJfHCWAAG6eyByIoqGm6JKoBG5S1vTAzSMypQBO9nxawQvyoZj2+QzSCF333PZuZjZ5SpUJmWXF8WbO5u4N5bojtfcBwlEinhkIZaG7DGXmkAmQ1d0Rhe5viZhAu1xGO/jWo5kfmt2tWKBfnnwDEHr/7vF0/cnHI4RL17anlMMIQ3TuI1OZIbhisfV+KeIwxclNQJE4dz3t4w8f+x/eXx7PWx+5OB6OvngLBaWRorE1z8xmRkdE7OTzJbYhs1jMDiueLzDnOgk1Wfk7lpYwIy97CulmhEZERBbXv7r1xD6wXS6ddrcu1+X44fl8Pt+d7g6ImThSsindRhXHGWRC4bG55FjmQJ0YEe+e9x8/Xr59e4oYNFuW5mYw+uRRJ24zm2aiGg36/Uf97R/2//RP9fXbFVkd5QR/VkktAchpA8lpWywXtqUUc4CgeqmSz+k+ebSSHku4asZWQjulRB953fv50nvobp0tT9acnABrXojS3Uk4eXDS3PKycURQdKYRGYpS0kJDM5PdHI8FCUSm5WTtALT3z/2N+9bjcFruFoMse9zfH948GJ/H5fL05RdfPX583vsQbH/evTowQgHmyMwMYfULWp53ugPGxYOEuGV+90F//+56Pm89db5sTj2sNLPVjQ0fn9kjiioaqdPaemQB7fM2ti5RmbxG3tFk9jHytcPJECEu3tpSbVxc+w7BzJSKPjIjhQDWBsC3rn3sD9mOp9ND3P/0bvv+3fOfNI+RJKtCUWKbdi/MFuCTlLsNIWQabNb72Lb8+PH54+P5eei0sJmt60270s33ahZRFTZjNECLc6SumwAsjZlgTelNNU+hVMLMwcgbKuM07SAU5Tk28AW5VXuxj9Q0j5VIKL/ZMku1HpnbHudrXraxLMW/pQI9MlJVMc1vPgHSATYvh18j985IKKHIlBQqUbRaXVWQ1Z5IkGIVTsoEI9oWict4cr46DqPuVx8RD42L29OZ7378ISNGbFcOuttdM+NwZgjIp3Mc1tWNAkMYIWaOzFfubthTPzzmb3/aHp/35/NmSCOaW3O62dJI6bAaexK2LlQWyublOlIYIzlZBDSDmdbFPl5yiL8wHisQzILLYbHLrtWd7NPBX+8iAWFdjOb7npn5xandH7Bf/e39w8fnp9fHp9jkh1c3/0GdtqA227q5hNoGusUAACAASURBVIo8X8fvv38+X/sr4Wx6varS5tFxXJanj9vx1Nw4LGhA+rq484UCw0j8X//Y3z3nH7/Fq6POfXlzv7hFEVy3HgqgmDQ3pcbAiJBoJtVQbnWdKRoD1YVUnYRSo3rNlERaGjkbIqAc9aPruo/r1s21WHMTwVLNQ2CD0VhlkrPcEWpOwJAy2HWPIUQqIiMzh6KkTIBkguKcowOSMjJLGjdDS+PqwrUDh9baofWgbZEjwYb+3N99/0/LYsevH7K10pfKE+/u7IDb3XERFeVPIPvI8z6W1h6v+f4S2957348t3b05+pAbF0cz9oHVQTRIi1szkVwbN7KPIWE1HBeTeE0ZDM7m2HY8uR5kAhxYMAj0MfaARLNGSMox5tZe3WkWI6C8P/g3JztfHHG87Nff/fD8OnXgquUASJZGy0w6IBt75IgcqRxO/urt8ruf9n/8/oJd+Zqv1uyDm9QWJP166YdlsQgbtGa3UZvaDbxusXV9/6gt29ev1ndX/PK1zOKmsRZnW/dPIUfULoFxHtBSklP5NGrxIvFi+5996xxMz5QO3qzof4pCpPYx9i3EXJsvjU6GcgSyTPFkBVmJWVPgIEFGqI5Mysg+RmbEUJbBiVl6d/K2VT7Nh34ahUihucmanYiM8Naedlz6vh6XSyj3fLO6bcNLyndVu5RBUgi6WWRuY7j5zY6qFM/baGF/eOzvn/YYcb+YWQN4Oiy9j+vI5tYHthHN/P5oSqWyuS2O3qMZLwkHD85vHtrTlmOXG0EdFztfYwsTsiSZJbbVTudt7B3Pcdrex/0qgT0iEwY0h5vFCDfcH5djy29ft/+n5/3p4XL+6XFA+7bSW+MKrUG7Do3cM8q7hGQHIhGJ5+frZeiy5bsf8uGAIQr66ovF0CXrY3hrbbIANfeWksaAmf7Vr+yXX9g11jev7p/+qX8MfPeIX1B3i5R8ccILijLeSFV8NfGWpnI6iYlqHqrZBAAvByinHLI4zGCsqoctOEb2HE46rYyKBXmyemYWvuctOEqzYYYgjIjes9+m0W/Fws0sMCsmOI0PhoGs6dOZFkm1u8NBzei2X+N4b794vbw/63mPd0OXa79rPJFUWoSoQkWzvzHcHRzwUTNGOYkcM/XIAcVIII8LV2tQNLeRCWJ1jpRN34wA7CNBLZ5OT5M13t0vzQHp1BjyNNsjIyHR3SJzqA1hRF73vJz353N/OCyi//h4+bMvVgIaPQEzmMHNI6+HxU4L3fT2Dm9P/iHbnY7LvTdfXtv54AYMdeyRkRnJnrmHLnvumZdd557nLpd15HXDEF4f6cbHx/240O/WnrqnARFhMaJ8LpEqSO3OX7zhdx8HMv/4bfu79/HXP7T3V/6Lb/bTOl1kpRPMjmMeR1X4bM7MIqd6iuJ2VHxFGSBlZLMaJ1X1kTQuToKpvvXxYq+EMDJGlAPaUdCM1K3/raKlzBG599yucd17HyMq0RYOZqUxVtdXt2+aKtccPZ1kH9uHzsPqCxWL2CMzXx3aVfjFqf32Op563hcs72HSqIetWJutMkrfqCESUIsR5N7nWRqr59azSPGRSWppPiKH5rF1Y1R6FGBujCCmj1eLWxdkvD8QG+R42nofmYbvr/luz8PHuD7/o7VlEL/88pe/fX76L76O/+ov9Mbzf399+F9/ffnbD2huJGPE61NbKI9YNP78Dru25VWL1DVHk5S9J3cogcvAnnENnrcYiX1oi1SqEUA6CNMQnq45Eq+OWLzVeIcUKE+eEcgRUMKWOvpCjxf80zspP/7idb51/+mqx+thRPmFbhr5DWbNyjnZwBkdM4eh2LSapy0qVlNRIAk2JqdM7EuzbY9t7yPDjc3MDFnFVUo6abdJphkTApxzEv26j/M2zte+7ZEZZfBqVXdpvYxQyUAiijgDIXs5Z2piXLWHo/nqV8FGv45xWDGC2xivD+3VavslZuLrw6eQB6NFyoqYz7KmFT89p6UPiyl0v+LxWee95msQ0XvmcbFXR3ND3zPFk+tubfsYoK9ubnhztyQY0SVfHGOIzKctfnwMQedNIwHhOmTEF8I/y8sR1+/v/uj3u/2X/+zuv/ur05+93pnLX/1R+9Xb9j//9fMXp/and3q4868e7GvbWwwIw7LfIcEhW+Wjq8vUMSKuoS0V0j40pFEzoUAAmWiGGn4ksQkC9oDtMZRvXh8mBVFa58hqx5o1g8S2tvwX39Asv3u/3Xn+6z85JvbVZr0sV3vJdCPn4BFfxslvdrIJhGroTFBGwmeLrCStAD4zDquvi2XqsvfrNtxscVYTuveIQJSBnGXvqqaW1cxmqoe2Pi6XuFzH1kdONxLawmXlsi5gS3JPbV17hyyQBoTNCa7JOdbdt9PpS2B73K+PXZH29shTA9IU+Xb168geuUJI2Yi2ruP/c6BgjUYk5KWaMyHn2mzD/va0jjF+fD8upbQRq2HrqRx3R6fgmHPWKV73Ee5KDk+zGpbTnjhv48O1X7u2jksvDQeVY04rvnQeTW7aN3wf+3/9l/ev7i8X8GGxL1+t/9mf3H/7xR3MTo3MdSehJGzABCS4Sc87cs8QLtd4GtoHemQK157XrkuPbWgb2jv2QAQWx7ljTzjK/473F9xD375alsWMyMwS2TKzRk5iZFCOaMTh6CKbYV3szZ0l6lwIC5Wnb9pylYrMyUfNFk5TL0+0JjPq5kEzZXAaag6uxU2Z7r64Adr7uFx7CIvz0NwMvRfLlqEmh+FnQ4NCEcsxdO1xufTz1vdtZEynuBsOazsc1uXQmlvS96HFxmbYtrk56pwQvNRoQEL74s2Xr5b86fnyu7/7PsY+dh6aE7nHAPKyjQt1cjIz91BLaZ45JcAJNFgJRYLVmB+wOvYRXx9498XdFw0fH7VJI9kzzjuet7FtcpqbIvPDBZynvOa142nLRkvVqaeK0HlTnU4DQYITIWw7TgvvTavRIJdeN/3xq+WL47WxZfTrtvcxvjjYq7vlCotoK0mzPoKBLvSR167n63i8DkTsfVw3Pe157XHe47LnuWMb2AeGEIEh9MAeMMc8P4rIRAwEsB6auwlUwnxi4pw2j1QyLW86OBafh4QBN1vIdIdRQFagpdiKWiFfpj4noWd1EJAR0+KoaTIyGpROLe4k956P533fg6aqmCjvcUJ01VEgoGXGPECEAvqIvef1Op6v275FmTQhmqGtvq7LutZxoS6yuZyNGEzflXEzVOoT9wwztFPL42E9qVl7AnwxpZDgZaeTx2bWMjjckApDtnIbiTW2CchIK3LupRib9QwIr+78F219+JpLs0vP91sY/cfn/tv3/f117EN7zx4QsDoPbR6KeY1Y3N2pwKWnG5na8OLVmXfvxEqM1B15cL458LqP54/Xt3/y5Wnh6cOHd4/X83p39+rOhR+eRouMkZc9nq95Gdozzlt/vMT7bWSPpy0/XsbHDVtgVGwJPTD17DqNlyBhxOmIxW0LscsdPWFIUCNkNX7HpOROAgYEE0H6FM7f3C/P18jMMs+QN9NBrack0B02J9pBMzONQTdba5czMFMdb/prHQGQBluaLYaR+XTen667NI/9KivDKI2JZnSZgTXPUOw7MqLvcdn69Rp9i7LAlOljWXg4LIdDW9fWmrkxYYsynYeG7Aq7mTiL5JgnzABAU1zOl07BkQmeQ0XTREiKRj2b3s05KL3u12+/vudU8Yo0cTCNdHDMuNfi1eKlWVsOy5dL/PL1+nDkPkTjh8vh3//u8u/+aXt3GU9bDmBEBthHLot1yd1Brs0vGRFoDfuOzDnF2Ry9xp0Xg+Ga0uAVyMx37z58v36M16++/ub+dFic/u4a+PGyR5y3vGz9+RpPPc6h8x7Pe5z3OG86dxWCL9NV5jRUNMIaOti7+o6//POH1w/r3/zDh9XtP/qLr96dx+8/9Bzj/HSR8rLJzZuDNJUSRFBWnSBSaWTAmUmcVq/DlzWZTRYxwQmYbgEEQNmam1mozoYtikq3k5gpJOvMPIh0QM3tsBik58t4uozrPtbFF5/K6AhEtZS2AAwxIqFcjObIUEb2HvsWoweRzgoyLa2tx+V48HVpy+Ju1OwGb8mLaRMfzfMSp3Ogxs/+8MN33z/HsS0fn56eL523M01NKP8CKTcejOb4auibL07r4mKWqisF6swDk7thniqiw+LXPV6fsNPOPb9/3Kj26uiHxofWEMfHLf7Dd3HetDiNXucvG9AjSQvFuzOUSfLQgJw269awOgR888XpP/6zr5B4VDz17anb8xa/+e4jjpcfnn/z3cOxGd89Pb/X3Xdqev543sfTwHnXJfK85zU5QgH0AYEeABAEFnzz9vTw6rS0hUhFBO1vfvthf9z/+Z+87gmO92/fHl+flvfXBGBu62HJvr173K/bWE/LKN8DOA+aLcQGZgoWkQl4Ip1zBHxauTHtGiwGgxwpUm5udXiODKbIvB3OSNKCL6e0wlDpSD3S9szU5dK3vrvbsfnaDNC+I5WilfMppK1nRpBytyFkjKwT/pElolccNbf10A6rLau1ZnUoTlX9LBooIkbZMedIGG/jt1WB2q9/9/jFq/X//u4p5mFYdXJ0kYeVkPGXX979y188WPBw8OEUKu+SAmkvB306lZyHpD0c29N5L7PbYlxdl94z8/WhHRb7+sQ/f7t897g/b/zpqjoMcO9cFxH8eO4jaAwAd4v98zfr10f/978//81PMsO6mExfPBzf3B+26/5hMNrKVW3bfvN+e/L9nz3oF9edZqH8iPyu5/bT9amjA8l26bxcEaF9YBsgce9qwMmxLLYt/vDq+M3bO5qdz9vT09mXI0mEfvpw7UlcVQeTjCGAdXBF1b7Hy35YmhncjQWCb2c1JiElEiE3y6wDR1I3GzJvbP+c4csbi+FuNShqZNRZX3XMYbkvpqUgCTssWBo9vQ7UuGxj70HyuPhxbYurD0q9gJybdXHfs4/ejKe1NVJl8BLcsaSnMAYgtebrasvaluZuDf8vU2/yNEmSZPc9VTVzj4hvy6Wqsrbumin09HQPCIAYAiCFIuSFvPHPxD/AG88UHiAUQigAB9sAg+nqtbbcviUi3M1U9fFgHtmddckS+SQlM8LdTJf3fm8r8ggZBpL0CPf0iIxtTSsXxdx4Fila3px6AiqcKlSUF1uPiUKpxK7qLz56/pOrK5vMqrz19SlWyBhjpA6102a6GaM0KuUw2Y/vPQlVvZn05Q5XOx3yh/CYq/7s5fTjU39qCHhPJRmZQp1MTODJRlwV/LNX0//687sq+Ccf7f/l//fmm0cOOeP9eY3oh0lm1VPzc+sKnohfPToTnrmvRZQntt8+9qcjXj6bX93uwm6/eX18+v2bG8FOkIJumAANNIP2vNnjh3en6305zNN6Xtp5nVpfF7+reHe/cCqccHWop9Ufl36Y5KFvtvvx+XrmzmzM1D88NUMZlQMReuEXUBjJqgp+IHT+cSUwprM64IOQJD289Uyymv6R9XmRs09FZtNdkakIkk9nnskeYYpatCgxQBsQiBIKUXe0CBU8v94dZmNka946hjt4QPgSVLNpKnWyWlXNKMgYy0sAGAZjd3TP8E31mX8qhNsmMlK+uKu7wmpmw6kmKqQYith4ZO/m3ac3N7vDXPaFzffgYh1Ijw2XO0Zzw8+jkCSh3BcZXNNW9IdFdxIe8eyqXE9D7JF20H/+5f5g/Oa9nB1vTvnu7Ofg2se6HdeGv3yh/+BlOZ7bLz45FPK/eTX//rSoQJU/vDn+7X7666/uQB4mU8HTOdzKWcvvj743fqR5avxhPd8vc0p5djPTpnMpd4f6s4/x84IJOBL3g9jrSGIhHmr+ivHj/fnzl1aRT0u8OcXTCiTWx/a0nufCpcfizT3vDuUBQ8vJDUGhqqPrHDrP3OSt0NTLKDuShnTw8r8O2DiotvGCbPrQIYDMiBa5tp6JUsZ+KvPimxWgmM4qhlHsDHlc9iTA0bMFEZ49IoKeQg1PLD0zcZjKfldNZA20lNMaPVyINdAjrZgVrZPVUtQUAgZDLqAdpjtXz9493DctMrbpEba97SaQLx9dFTN6iIJqw7okpCZgKir6yeF2v5+1FLFis849S0qKmBKjathgc7kpPAmDaMG+aGteS/0uimT+9NbWsKtdOUwmyEOymh2q/PR5/+7Rf3j0f/edt1OAYoLbvfxvv7j52cvp/tiXNe+PrZrUInczjr6hKNt63pVnSWHKXAw7nBqJq/vT6V+/6fY6VBGTUTgpTcvS9czYV/t1yF3hL/c4OCThBARhsCt7qoqT3D+12/26N6jg5Hjq+PhWPv348O///uEnHx+q6fcPTURMkBFjuai6paIAwxiOixJ3o+AMC8oQ/2WCoJlFpnAIt2S7FCCbp5wClYiMYPN0Z60mm4xkE0MLxETqWD2IspMprcfx3Fb3YjZVE8nec+2eSe9wz57RUrrIPNtctXl2yHGJ9w/96dgyc+BsrMpUrUylFhswom20BCp1oLg9Mnw0zjqVyOEBu6iTRBBjcq1S5ql6EsqioqZC9JRdLRCbDHOtrz56UaYy5lcisjvMeiytnzE8vYPAhtwgwSnMMLGi/Gq/M7J7Lj3fNvnV29Ou4JPr6ZOb6broyGfwpKh++Vy/utv91SfT23P8q9+cfveY//jzw//09c0Xz+q7Ryr5cPZv3jdVebaTufHNCV+90K++uDvMxTOECs9qsq8GIHG4z/aH1+cEXr3U28JdhUq62stdeXVVfvhG/kAi8ec3VkTnuZ4eTo+1/MHzu6eoZSbz9f3pTrMIRPDpFT454N3jeSr49Pn+1MM9b/alKNNbZo7NtIqq6GCo6lZ5pVwMSZSNrSocgRUZyYGsqlUzPjgFGAO7QGpKMDPZuw+JF0GPy359m6ll71SkKbRI7zwvvjpVZC5WDSQGbTwCkUlneiY5TWVSVfK8ROt+PMf5vAxXjAhr1Wmu81TMbPxb8oM2HBhj27FqU+RknAdoSSQjOzWDMfaRUkRYQ0pLJbVWrWpmGpQdZC5lqiKQ59N0BS1OLVqLAijJOy972HwoB1OsbpOZqRE6F/aMxXWvzPyE5RH47Wl5emomfLkvD+f1v/5w/C8/nkGpwE3lzU5u9/jytn50Y/syRfLV7fztU3x0u7uq+uPDGl5uDnY+8V3Pz59ZKRMobx7bxy9ffP31J/enVpuOEptluH9MRXuwyXntGH6RUoyiAF9dxfNpqVf85g3enPBtxrwvpXBxfPvgLLDD1U4V2VrwyfMxEImieFz4+tTrrM3jx/dLUXt2KIpkJBI5LBmS42jbBq8QSR08lyR0ozjACQZ7ZCkCZpoMyfYotQY7XQArlpunkBk5TeUigyYhSXFPDxZxBuYiV7uiRM+MdOZAD6eK9RgHjGSmJEykFLXh7oW4x7n11iIzdhah4iFWxGqdplqrQiyTyEuySo4Fv5CBTAXqZhXWISIejNKB2xplJiHdpUh9XsymYruyyS8Hv8FMhfn8cDBB2RdR8OTlULArHz072HwTvqAtpNhUoNqaw3Np7sz2GOt5PT62s+BtdPe8nuQff7x/+8Q3azwu8dDiUPD1y/rls/nmyiQzPM9riOKTa3t2PSV0DTLxya2dO+/XzPAX1+V2VyLw6mb/05/9JFQ96ZG29nMSmlWqShRjYvr8xf4P785MaaAJjk2ur+Tx4f19tP/xlzf/6t8/PL5FvMZZ1psdQnEM/PzP9p727oEz1IX3KykyT/zhAdfE+wV3kv/p90/VdFcFjFFFjdYvA8FLfyWDCgvIBtb744d+OYWGSXQE5YzzSwVJWVuIwEwZGbYZNaeqdqE0Dk/k2nxpSXBSqEgLzJ4KxlgRCYoooO7eew6KAkLBFMVkVapR6JlPJz+uXYA6lulIE9Gq06RlUtOySXYlh0IpRjBFRkYY0gxVdSo6l6IKQClkKjeVBRJISO9RXnzyZwVMX3eyJl3JYhKJHl4g7eQ/HNeSlUD2zFP2dF8azdbT0pZzj9XNPMMzg9I9evjQmzvZOkuRq7l8XOfPb+one31z9h+fesf20KtmuDSP1mkCVW2b8JlPyZL49bv2+3ftfu2vbquoTCYi9tOPXu2fX717bLtqvptMQUrzkKLzVJbmHnx1u/dwDywZprbT/J+/1seT/e//92myq3/2i+v/418/tQVa0QTfP+JHxy/K9GfP67unZqkHywfIflf2gs+mPK65OpNiIibikZk5V1OVgfVJMhwAIjl2jx9kPSB7YBRXQz+oigkybCwJ8e05k0wxRTWFSICIgSyGqIIfZk7aI89rZHI/664aRYeZuPXhHJdaUEQzwzs8M4LpHMxkVVUTUUlBbzivnsGqYgoBhmZ+tDPVTLZ6cVyWg47mQ0mbGSICTRWpprVIsctia2Qp/FG8hEW17He7KkQPzWhOzSgm+93u3PqyLv/5/uG0PL3/+2MyJttQNkN+7iST+6kUZVHuJptMdxNMZtOE2KkFMw9TcfKr57vbQylSv3huD0v+7ffvU/HQ4j98fzRVE62qV5MUYUPWAtUMiKUAAcXVLEnuVfZF9nd3d6+eLc79XJqnJyedD1M5d/TuSw/V6pHN49lh/927p5psnvsa1zXLlaFMr+/55rG/+qQ8LfLDg//tW75fUCoelv6L/f7uqr9/wF4RHo+pa8hUJwv/aN+fXY0+kMWsqJpJNbSRcpXp6UQND5gltonlWKSoBD4oTrEJqMagUYEgIvLYMxK3V1V1zCEQ6Z4QwHRYyCBEAGsLj5irTXV8tVKqToaqkkHbRvTZ24B3SESGD+sbgayEkoM/ghwhIaOg3B7roUnKSKtFAVMRRKeMUKLm7p3KLHVD+en29g1F7iZh020zn0gGpTCjVLhK76mSpUjzlApIqbVeXx+ssNqCCKiBWa14UlUzAyLP9rWUTUhOajEUU1O0EFGPjMm0Qh48f/UQ3nPpKcQprfd+KGYTXp/62aNaeVhtLmEms1OseDAhkfm4+M5gmpG55u7Tjz9W00LORfc7a11pWqTMHvdHdvcEd1XnInPRm12J3ltkRvub37V/+Ln986+vns7yeHr8Fz853O3L//n39//1TYypQFHsZ/3pR/P7oy8tTguhUaoWy0ORXrEr0snmFMFUtaoUk+4UMAj3BDcW3YYLHyAGAluL9eGA2DC4Gz0IiOT7Y3t+XS5dw4AqpGwd5niUB7c7Ww8B5kmLajExwb7o9aQKtIjwDGZvaBcPaHj2RCTGsIPIg0nzkOgmKbYl7Q0qVoY4U8SVkhQrMiavuCgIe2PrXgVphg/WfISwgCkXTEp+6JpBkMXgqhWgSBgyIxLKCFEj9rWKok9yJdAIMYWKLVs5IaJSZysqIjRh6+5JU5rasoQnBOoJVb5u8X99u/TIpefzIj+9K3OZj6tPhpdX5dT5fo1j91PobPok4Zlr4NyzRVbFl7dVhMfGLz57tbuammNMICdXM5nUkmQLBaopmVMxU1xN9mCF7otLRPzm9bqbdl/car+O376edOnref2LT8qXz+LX73C7w5cf7Unsd2U/yW/e5tsnfPVq/ujajj0fH9fbKzy/2b15bENqV0zVYKqX+EM2H8B0xcDrDe+TCpl1+NPk0s+BxNZAKCGC7nGYdC4lmbJlQ2GblQxgHraWIlK6EwpTmYvu53JVMFcxMgZ5ADGSv0bF7kkPuIjNKoRHtuRMyRzBe8NfID0YwQiCDIck2cOmtGpSFKKRkSkZaJ69Uw0ezBRPiUzNspV/ROACI9neJ0aihC/nXD2ZPQp8Lijg0lbovN/fLJCMTtur1lKokKmaJXbGnkjSROaqRSngbvLwyIzWowhVMFmZjPudjXdGVE2R5LcPvQinKjvYpLDKZ4rI0iJOHUvk08qnlavHZPLFbRmb493h7ovPX0K0FogzC820qhWT1jn0olMtSU9yNn2gi6Anl8Zzx/NDBFENwezhqOXdqe+v5n/+VT6u/b/9s/nLFxWCZfXzwmPPqaIA3ePt/fr6PT59Kde78u6pD/HL4EGbDjjcJmARGcMMXJg9jByRDvpBhH1JWoEnP6R/TVXnWgBkgJdLtqgByEHE1yHdGEA/AlKEtcpVlblIGYTw7uc1uw+fCHpk7+xJ1nJ3VefJ1p7vntanNc4to/kGlwQ9Rja2KAxMkYEURviiVbVOUBnMs8gIpw/jhee5QzVqUc1kiBlGHlhueqXBmGUkS4SrTbtaTqsGdGkhGlBVhGlOJlrLVT2A7pk63HyZU2FrnFRmw1QIGOhmpWqJiMVb0VTxYihF5aILVdlAQnnGXfBhybcaNzu82Nda6UkIWjLd1oxTy55yqDY8ipT6s3/w+W5X+8C6KDXFILf7EsGlhYloNaKbqilvr6ag3J/9XYgHHhbe7vj+FC/3+NXr+OExhHEuuDrHR9f211/pP/jsZq6agdXz6ew9+Jef7w/76dffPd6veHGD2/10vddqm0rAxuM1qnmkCOYyfO0jG0GF8IQohfSgmgzX4Bi0imRwy0wek3NVZGztqGzKsoQot0LVRJwpkZkc4FK1MZmPbBltjTXcHQwmskeuLqckrdxczy9uJlXcH92jvX1srQPMIphMZmVRFIEMr7/KkGHEgLtkiK+i1gEPuPtorhshnWCYihWKZtno2FsOAbaIkRTAg0XKXkW7kzJlcDJNBIlSJmSv6sVGKTsaorF/y9ax9hST61mqSoBjjtiSqjqX+USHYOkBUaZaYR20ZlASa5UfPEO4OO/f54/HvJk36v1j4/tTHI+97g67WaBO8v2SX3392YsX1yIopj7iVsh9tapcG017tZJgTfMCzzCR2115dTf/4e2xOd+d+flt/7ffxL/7Xd5dHX759ctvfvvjXOPtk3/3mB3lZmejkro/9rdHX50A0+PuoBTZFbk+lKJ6cyhLz9H9+AZ8Gbvija4y1i8mmZco8HHHqUgOkz40OWZkmwfZx/O4LdLHfnrgG4etIitsYGkTGMgNYBAH1LuoyPF2ewAAIABJREFUDcpnIragrwiuwZXUatdX892hzFVPiz+c/PXT+njOtSES1XBbUWbMqiaQ4ZsnISmiRgaFI8sa7pSeud2tQAQWwhNqWWsUU1EaIWrD5EIKxoMk6IkSrTfTCC+qnsXpyTSrJpKxaMbo+EaNHxoIpmLoxcW4dKaxquQWGIZixRFAcVKgEaSxRm7LPhKCCDwaJrFa8VyVZFDeL37sIms/H1dEvnj1SiqeTsvvjuvPv3j+5ZcvTU02KQ1MJJNFCWgXL6bFsgdNVSWGj4GM21k/up3evmsP5zy28vULfvMWrSugT13+87ft7RNe3uHTF72YC6YWfPfYPfOvv76u0/T9u/urnb196mfKp5OuzttDUdVh+JFIwQfxDGIb6lMpoblJ22VcjroZx7etOVUxlgXD/D2W4hxt5fiuBy4qh79tG090Rvc0xTz0shhbUegW0Qo4emANnHqugf1er2fZT9qbv3tq3787PZ28O3psWXe9UAkTbuKjIezN8TeHkg4iEYQnPejJiPFabV7Ds+XsOU2cwOFIVkJNR7j1uPcBFM1TVZtMhCyFnpIspiX9rBIpzMxqG3INHPnzkpC5cCoguXa6bdEKTmrLJJrHbFaKFaEJS+F4cU21mIQRncVYSz15z2AkymRXloX5+JiZ8vza5l25qfyv37X/7q8+O8wFgCc8mMzV48KQHEJnXtw16cmBpApCwBdX9bs3y2mV90t8dK0/+0R+9ePD//MfHorGT17gi5fY77D4cJfEaeX7Jy+Fu2qJ3JUS0H31uWp3qmYtNpVNk7i0iKDKlte3xRsRKePNvih+MPg5Y4A79D9QkWEfCcaY7TrHXkPojE23KAqZJp2omdnDu2+6m1EhVZN9HXwwE/RxtLbgseW54+xJlVP1jFy6v33sx2U4GIfZG0JkILa6kRtT7cKmxJZQK2Of4eNRS1xkJdtvWqCPtoMpYiaQKkqJIUUmJSU0SluPk1SO+4kahMNKeMtAzdGYtu1l3IAnAmRiMDKnakvL3kc+fYoogamomTFzP6tHGiCSAEc2eeLCZt+45MYCzbGJAMQEg4nDrz+5/rf/8f1///NXn724bknJ8KBHmqKtKdgilQcqL5OR7IMXl8zN4YJ9tf1sa4+HM5P500/051/GXGwyvH3Cb97gt/d4OhsADx6XfHk3/fSzGxH55ruH20N9WvL2UD9/cfX+3MjM1B55mGpmPjy5yJYbGsDGAv3gNhyNAIhNRwFsyFBeMKuSjEhESAsujWPZnUPWRhHB1VzmSUDsilTRLHzqPB4RLe92MpvOhhQND4r28HPPhwWPq59dA+qn6B6TSs94PGemFCUqTLcjLYDVsRaYbXEcJDYoEjf7Xhcd0U3+gdJ1cfsJ4InW0uf0GKYkUZWhsY5gbNcuyzZPExkOPu8JBBNmQprSh4x4KJKb0wSRCGbZUt9FBU6pylpsYI7dM1XKuFAoW2AFCZViODdfek4mMVSygIr1ZGueoFFMKII/fP/+f/iHn/75n33y85+8vNqXHhkxbhgsbVB/x6BpYMbTtxjv8AjPjMQgvoLcz/b4EKeOhP7ss9xXEeHTSd4+7c/tRMGP7717NJfrw/6f/uzm27frGvn8YKqemc3xdO4YYneCjGJT73luzWSEjA/VVSKRA6wo3LRmsCH/VzUQkMG7HWOyMbhlizgu2Z0eYYZMuAOSZiKgCWvB3d4y7c1DO7c8O293ZVe1Ft0EIcDqeWp5f+a7U39aM5AmFsoeEAkmI2jK/YQwuI9zCEmcHdYpwK7oYA4NGjFVk3CRSDjEBZmSssUb5+U5i8DScllzKj4VLZpmMrTWGCe0UMBymHe7yQBVExDvs80iU0GmecRsUgxj9COqBqFHj5hLEbgnfPEBjyymgExFitnj4gykoccWzoON0a6rB2AqY9KbDvRIpiQztoAPqMkv/+Krf/gXn8yH3S//fP/RzZyEqZERjuaxtl5ESSTZgt3DI1uPAcRoPvLQB2uCSZjgFGgrv72XHx/kixteXfEB9vaoa+K8ogcmw8PJv/nxKUL+4+/e//KLm4+ezRAe1/M8TVq0QPaTnXuqaFG8f+qCLB/C4bZF+AWsQYyXQuxipc4YVPwEB/N93IwR7CEjk3SCqMHBlQmgEJFNoLNxaXx3XL991xaXudj1TveTQrB0It2dPbF0nlo/O9cAk6kdaqowGQtHqFmVNIFpikMUo3N8bEwyKDvTguGgN1jJHLISbnqNseskLqQ2hEASa8Np7VOxoi4CohTNMXyObYCXpVqYgOJVtHP8lJggwWIwGyCgVNHZVBXnTE9VgUKrUIvI5tqQACNz7R6Z1co4ewZ8wEQA6UER9SBhCelBJDV10+nnaFEw73f/4h99+erFtSiVOeRcyezOpcffffv4fG/XuyqCQRKMbY2dEdk8uof7ABRu+q/BJH98Qs/28TUAPJ7x5iGe1iclxLHBoyi//fb0737fH1Z89qKL1B/u29VuOkzl1LJWm6oem1dVVXF3U6UGqRwC9m3oiYgUUTNuEeHbRYqIwTgUjuRkQXiuTu8pYDWBmCgVWJWrpwA1SAZY3x3X3/x4PK6Y9/OuyK6oEw+nDHelq7AFF8/mAxYlBHsIIktR6JgriYADZ9AhY81KQANroCU8g5X7KioCqymj2UHJRMQQBvvlIdveLG4H23lFMR9L3QiYyfhAPegRx56Fg/BO68TTmsVMTQRSCieVoGyePEoPtM7Wt2/edJD02TOFaNy2LBB4wEzcB51F0iGSJpvaz1SYkpnFFEwxqQIFR7u+ZF2jd08x3D/1u72OjLrueWzx+9fHZenluiQxMDiboFdlhI+MSO8YvNktd5Um+udXdZr6//KPcDUjEka8PQKAOZYF6viPv1574/HH7me0wOHq+q/+/Nmbv/n9xzfz87urX33/qEUi2Tr2syqoiiKKEUUHYssPBTbujpDUDf++VTOKgQMYGzuJQIAgyngYJXPAMlSqydK5eoL64/16XuPccukZKRkJrYSc13iMiDXmGleTrc5Ti+Ma7tQxKxZJ6njsLnHSTBno9QH7RKZEblFfEdvXNxcVzVEQGESYRaSrIBGCIHteJtIAAHcsCltifPitx3BIDEdLJE5rlB45ZQHkYQ2mFEMSa4RJOsU5sBGMbKbSfJsPQaVR0CHgyN4ZsNjN8EjpazJzaF2SWVTUpKh48OxUcJpUhL2njzA2IAIyUG+l/Ju/+/bs/fX7dZ7qL764fnG3a87j0v/w+viTl1fDkpYXSoqqVtNqtmCQ3zIyRwjuOO2eqT6/i3/6V/jLTzEZbML37/DuiNOKdw1vnpBH/M2/aZ0QxQ4wwa+/vX+2k2pSzV7fH8/Nn8/zsSXAXdmMIVYorkAOF7duqfeULT2WvFQNYxYztpmZF5yI0KBTQVVmAMJM9FRApopD8rjGqeXqeDg1kt3ZyZ1oiC4hyGDSLGcTks35tOTTEoKh+BijCaZoRGRIv5yrSR2i2T4etQ3TjcXxjiSwy5wCqqkqkixDIZ1Ck8x0RRAfhOPD8NwcEEZmzzyXrKYiSMggPyzBohBPaR7L6oepKLx3jGJpaQmMgQoJdM8kgpiKddIdVVgLdFNtDyeyCOiZplBJlU2kLMMoTRmN1NiKqADQYgiGillFJAIoitfv7+tv9e7menX+v3/39rOXu4/vdr/54fHz5/vDvPFWN/2BCBi1aHWoIjIGWUhFE/3cMkLI+Okr/euvpB+JCU+Ov/kDTgsY+MNbRMeNAhNa4jFQBAfgk9vCWKvKx88PPz6uqs0Tq3PtAZSluYgUoRsNm3V5yFgEHB5A3XRmSgYpkuM/XPbSGExMNVWFGINofRMZKViLTC6PPVvnCZvMKIiz5+w0eEMeCndFi4lnnlZ/WHLpMhcmUBVVYYpAZhEmAuguPcFIz4yQTMbFBQNBEqeOSB5q7mseKopotfzgVSiKYlKDLlgvDWcCJDzBFZG5uEwWZjkO9/EAeUgJqlI64Ynj2oegKhlKqKEKzAblCKUYhhUGEhn7CoGopKlsLG9irnJeM5l2ARcUFROYQUD3HCwkCGqxImiemZxLITNSyRim7+6gaJkKYWT+9ofj7358NGB6tj+kmgxYIkD0zE2dorqrNtUy1Vgbl+aEqGrzxRU/ewlbb37/u9Z1+VHwGLCCd/d49yh3wWcFbnh03CmyYyc4rdF6LSpv7s9PS88NMEYP3j+13TSUYMODKcm0IfMZoQBDkCaqQxZDcGMgYBNGytgOkaCKFqtFua4+XMBjLsMIkayGU9BDgiJkjzz3Uwbzqh6qKGRWNufi8bjEuXkke6omTAWqZjKrjPtNREg056np44J22buPwElekifPDk/2BBK7mjacnBhyj/QcK6nLpRnYsnEEDkSDKrvAFJQ0jN6aDpQ3Ry8rqo3CopjpVBnR64hGyI19NPa+IlZK8cw/4WqOsJBhs2NEtogimMuoRJgZVnQAc0EOKrEnAVl8kNc2TbAnPKVlZILKuVoxAwRpnKpkzEWLahAD9RxbZQZRRMAEpagJulPUrnZowUyUYr/8jJ/uBXp3Wvo3D/f/+bRkgrRz10ONLyvKGq99ZEWhCg47/OUXz5a1ff5y9+rZ1fLdg4o+LjEmObtJVFAUDjFaSpiYaOpodiAxfD7cwsNGnAHFBCOdc6Qj0iOHJrEWbOxNAMOeFOyxyWmqisdGqmqOU6PHyWSuN3sVnLpExnn1pxZJGdHFHiICU5hCQROdK3ZFzKQ7709JyMgM2DpHbmapkBHBCQFszABTimUmurMRa0cnfEx3h7Z2W11sxuDhxe9CBVwIoelIkhQIuLrtJp0MIugtMt00Nr55UE2V4qJCGU/9NiGRGKmAo4kdU7si2E9a9FKQbFR8UaAUhUjBMAO3ycSqjpvU+7iUxxueIrUWrcUmQ9RJZNpPBjo97o9tKmqqIwOGRPcc87PTEqPZePewJKlKhdwd6j/7Ghr1uBxj1l8/5v1jEcVUSi18nv1WZBHsBGfdqC3DNCZI7/Hm4fTmqdVSPLM7mGE6Uq/FsJHkNYcTUVQxzL9xSTPMbaSjG1Zqg7ogtu2TegQjgPHBZo/0YAt1j6CMnmvo6QdEMRJvj4C0SLndT1m5SBzXPK+EDGckxgqpJ9QpImpqhrnqfrLMVPGWPDc0RyQyRxgyRP4YE+iJUweJ1TjYpT3QE7Gl4oGC8cUzt+tOthH1OK+RAh2LdAKKYsJdldXDkOHsHpprgk6tGxhHRBLQTE9I9gFrGKMPGdeBisCkOwfoUUVHxuiAdCkx2uLB3lOFCWpVgO4hKlXFqvUgiaJcugTZPKvhMFum7OYiynaOh+6npdt+UoVAPLIN5HekR4rw3Py0RlF5Wv3pvPbwv3ilH934hHU979dp+t29p0sxub2Sn340rb9p2fkUWBN7xQORxIvncru3xebPnu++v196siSbMyJ31UyHrCEhQkOS1FFXqIlue6ctYmy85AJkpopeVKaC9LG0zkgOwVZQItAju0uSTuk9MtFzSNm23SiAcHz/nqe2fHoT/UonzZFxaRe5kukQtArH6ZjsIU6lDHSjqFJFTGHKkb7JbccECkKQRAOio/h22g3d3Kaj2EJesP26+OJH47NNPQSiSIEBmii9eybnIgwBWTVFVA0XHD0JljHIhrinqjA1hMmAMCOGE3U/Yyry0AjBubMoVBHBYiMqYVu7XgDmqCZTNQ+2nhEcl+FUNAn1BOidIlLNdGJ4hkePbN096BmWevJYW7dtnEFPMjlPJROvn5bdVK7387tjRsme2Rvf/fj41MrZs4hZUsibJdZgTxLaMkHcVpwCzfl07usafjdHojmnSXrwtPqz/RasOkAmJqSNcovVBikbghxT821aNt5pEsOTjC2aHRxJq+MeoCfXoDv7uNESkbJ4eowygYMeOmq8SLx7wl69qvYCUIqijgEeLjq40XOmdCBXSaIlquLk6AGnRm7Jg7yMwYbTXQEfO2xFSwwl5uZMJUYs+CDSJ7ER2j78U2V79kbMkI1TTVAicioYzzlkQ7KIIMcWFDnkQALMVU3RexfR7jQkhN1jNmbi6RxFLcm5TnsD2ccz7skh1YpgZmqR1Xk1aTEdoC/ZogxkrhqRJixmPfLh3HNb5oinr80zMoIJnJuvnS1SAbMRjCC4WNj2s17v6g/3Jyvy6uN6d53vTrE3nivwVv/J1fRtrDeU66dWXCJH65Gz4sERxJXh80+vailV7bj428elZ75+aKpYW59v95dURagIFAU6iLJlHBUkQgcEQmV028k0VW5m88vbjg2gzYCMFDOSTkayO92zjXVtbuPoncmusge6ohBmMJO1sweZMlXuTc0oIqPFHxOAADMurF1HEfbEqaMneowVJCI35sqHWlwuZb4pIBh1MsatGhs8Y1MG4/KEjRHd5oDAKBCLwgQQlBb9ioUkMjCgLIRulukcZemgVM1hvrn8dVeGYA+Tje05IobCVudSzbpSR8S2QlQopmalexPoVHLbY6QrdCoKEc9QSEu2Hp6gyPG89h5JG1vxvET5LS2OS0xl81scpmIjg3akvBcdEPJdNWes4VeipxO84n7B8kM8z/hplb2RKY/OlvDEVkMpzh0t8fr9enddP701VTwt+esfzu6sRZ9d6aZvFGwLgARHOE1ul1FR9IQwTcTHH7ypuMcIZruFgDEgHbUrkwKhiVTj2tgiu2cL5GVM6I59wb4OQRisYj9LVXjieOZp5fUed7u4mm0qbmI5DlkRcDzggw7kDRhRVO4j8vcysB3PmfwxAg/cin21MRIcNsHLdblpU7ZjU0b4ro59PMZcx4Zm05BEUQQJoU6lLN19jIHJnpxMJkOQQajobiocAaeqgDDgdIWUAiZbp4rUYoJceyo4GcfEf6ikRKKaRrJFth5gmaqOFG0b4BNmLVKt9M7Hlt7b02l5fl0U8Iju4T2SclqjFnQnwKlakDZyXwBVLRIiMjyMcHw6T5/cld++Y3J5eBI9Z19xa1JEYcjOljBBDCgVoIrVYd2fjme9u+merx/PP7zjXLGfU7a8VB0r9QEaTEoRhkk1weabSBHZatKtFE6BEdyIyCkUxiCiXIiMSpGCHTWCa8uFQ3Iypg9bQ7erNlVM05BFg4nTyndHPDa8X3Dc4dlV3O5kV2E6Qha3reC4t0fSr8c2Qhpqubwsxf9k6jLWE/jjO/FBiYLLT8p2OY55rQiKYC641PQf7s9xp6EUk2IKEYoUM1XWwbVhTCaCcXSrR5xX7ueMoJDjXRZBODOlRcxF16AAnak59seDxSeRcOfAPKtIpJhgUC1FwlRJhUJEw0NIB+aqnnz71L54yeFLFYhHADi1uBvbt0FGSUG5qJyB1QdUUSYzUHaqXxzqV7flb7+vv//taTrHy1ko+rtTPJ9svL5ty+lFJwIoFUJVxUd3k8NU3o09JRMvbqZBKLtIy1JGUpjAhuJZhlFABjpHYqQzjTzHTbywSec5lB65DY4oo6wz1f3MHprICLaQwYoSgad0joFFekrruXjeH3FsCCAcb45ojui82sVuYlGUImJuqXqB9AWx4f+2tL9NzfThCZPLYfahwBzzC9vYLZcfwPZg6p/IhDCiTxRFtz9180hTyourWkS0qJBqEoEiFOFUJYLdIxIG6aBZRqcWiRBG1qJDMbdGXLZAaUrJHGt1iGTKqH+4JcmDRC0ym7WIiDTQQZOIpJPhCS0bOgDS3D0pDAAC6qXAXXpMRUfSptmH/aGM9Jwku4/lYOKxnx7si8/mz2/KfzkyscUXvXWYZQHnguOKTnRiCTSiK6KnAG8ez/fn9v1DANjvttp/TA1FjIytPpGxnkAZzBKIjx9iighGhO8AAnADnXHgjoXAwGOb57gomSk9EJSkiOSkOEyYivZgD55aNMe5sTmbY+nwRAwoIrbd3dJAoHlaQbVU1WqoNhZ0QtKAapwr3aUp3bdOU7bQVvzJ4bbNYzU3OWT+yRP5p0dg5sbvNUALICiCEYlChSYLs6cqXCmqYFXIiL+DLjE4MwgVAZa1T0VzhagVxWTSM3vmkIuJsqoEw52mGGh0Ha4eGXmJim08KFK0RURgKqNfpKjuhVmsp6zDgTLDm3ePMdUjfRwFV7vyw/35+fU8F0SGqUVuIUPjHbON142XyfK+/+5HefJ889h3fQiJRQQeXFP2k+wCEAbhiUdHS+zusJvkMJe//Mkn//abd+d2NEUEXlzrVITMYZX7kw+ZEJiaqiiHVY6bv5xQGaumHPk2mZGAUvLSSMiw54iI6FRAopoVoGpczSgmL6/KVOzd0/rmKUbfet/5sF7A0EOUuJlPcaioFaqyBrsLwKJpmlOR8ZUVgygUUgVzQQ9w8HU3WClER3e8MRnHS+wjzHlsOS712zYHudRnOXJOEw7U3LZeY4SmijIOFbUxFU4dxkPI0uO8BCCimcS5xa6oKYpISxaR5t49i8kSSbIaPYRD9DLMjOSoVzplKjJNWFoWZVDOLcy0CKaiQQ55gIimR0SMHsOIZHpkGeGmUEVCZMBdf7xfPn22EwlgGNoGESlGl7ybSo388+hvHv3138V0o/uuB2WDVAPJ55OcHDuVomI6uPOAYAEm4LQQlL/97bvf/vjw/rypRqexR+OlxRr7M35IMeLIiVeyqGFQeZRCKCQoKluWoED6sPpQirGqVJOkFktT7EwGAKGHOfRqV17dmILfvYXJunpeTSC4vMWS4GUQWhSHGYcd9tMI3VZJRo9z33R/1WiC2ThVTDacSQRkKps0aFR72J77MVaG5zbxH2qfMeka6szxA+AWTiWXvoFEdHTFpCiKWjD4qSXCtZgAkVFNu5MZVrX5cAboEpgsb3ZWIB55djLQDcWUxNpJQIUtSeAwyWxYQyIxm0wVCg1yNxVTMaRCA2iO6yqiA6yqu2rNvTmxYeukjlmvqJpVQ4xbHhARU768ndub86n5tZS0bB2lQEV8UHFEqsnXxqvkt4G68O/fxC+eUSqUUlQasS/YUyCYQLs8OVXQif0sGfyLL55fXdX/9IdHD1QDEi9uTXDR0W9pWyAEShmUPdt0mgKK4FKljcH/sJpBFR5I6oClF5FDBVWdEJFdlZ1hLgqow6TWqyq3M4yOu/l6lsfF3zwx0dqa98etfjeBGOYJu3nwH4fqT4a+oQsjsQQiUQVTxWwoyqKwSp10N0s4uzODkiiKuUAEw5C8OFYHA0HIZW0wyKbjKUde8sSxrQEuiixM46+nEKAM8khGiCASJnDgtNLDi6oVyJrdeZhkiKGHVTWpLTCWK6IKRDWdJzUhmfsqs9CKHSZtTg+C6c5xUGXDXIfEY+SkDSWiQDKBappUkiZSVLRU0ZBB/44EUUxr4qPb6f3JFw0zAd10Cs2BGS4q15mfpx/Bu0lX8FC5N7ZgABU4JyeTnerZHfpHYPGk2O0RycOM49JfPy1/eL9kIhXXuw2vIpf50mAvymUKcDEJD4uwDNLe2Iv40MEJFPCN66hFqOBcUIsEAXJXZK5l0txPYaWEzQA087g4oh8mPjtMj2sRac1Lv+7PyjCLQIEmaJs4Yvj3RIpMQ6bfuTgihtoenVgUKpgKroocSqkmUSgtsqeQs2FfMOzmqyKJ5lsHMKZ/GI+XQkZpKGN0A71csuNj4BhKcxuFFBA9sugW4eGC8QaPSDMPTkVWx+MaMi5gYj9SQsm5iqn1TIF0585ybGcnE61mIh4oJtVKMroDishBRqaKlrKtSglAOFmZC7tnS7aepdr4/j0REeMnPQMc9EYh9WFZk3h+VQkOBH8mq+lL93QnuCvyvuVf3ukk8sMaAo7Mwip2VW1Y/MuHcbZgUjyt+OTWfvLp3d9993BcKQoFbg4yFxPmRdwvG6ppmzdtavjRhUPGLI+yMc9EFJpCSDAjdUx3J+NcWU3oFNBUTWEqteh+Nhc5tzie2rIuRVIOVk2L5EhGU8VcsCsoIik8BhhoG02ljqS6NM6UybT0fFqQOmTDw4o7ZBeDLG8FSQNTjJwNZtsZ6blNKDh8oxjhjZeT/LI7H9VRDBvVONITo2njxoBGSSKDLcMTuyqgJmPNIpQWHPCjBKoOLC8FMjKOMtk9V2Yki0oCnmYihxlT0Yg0k/HZCdDCinEU7HOxYh8WriShIpvrIagq4gHQM2tRhLshRqjTeHcj1WQuir2p7V4/tKs5p6ogbMCFgWfuHhnAU+Sh4JOdvV9jiFso8qwIhUV5Pen7NiLgttLk2bU8nPn5i/37x6ffvX749h5KTAX/f3tXtitHjlxPRJDMqrpSX/XinvYA/gH//9/4cWB4jG7JrbtULmTE8UMwpbH9B0bFgx4kQcJNkIzlLPHpqQoU4oBMNOCU9M62HprXPTJvqjBXU0hkL0DlcDitUyuphlbkUiQ/RbVJwQVggqpQ+Ou+v6/b0Y+iNCnH0LXH+z6O4XfnuuFTw8dlluEiuphaLviazA8E41ritsi1xOvKPcW4CjNRUkfEkJCuQAlCI2etJBzonin+PFXT3gE4jR3mAERmt5vdzpyxxQRJcwlVAOV+eC10J6FC+eXT8rrZ2zaaoZjm3tqiOexIGNhFYJBi6IGmUhp6yBixVFGgewIqDEFESJERnDseRUhs3ZlnJtHhE7UgZQSUAZFa1N1bMfpwyvA5kBIRUXqEQZqZXWzr/vXu12amk7x0WXv2Wm8HB/iXixahkwX4c+Du/LnapWAbce+xjkiETgg3DMox+MunD6XVrY8+UAS14FILEJC0jEp8hkz9tM5yRL5BLvneqRo9tAjjYHZTAlFTNWM1KcZWpSohemMMSh5Td4Behc1CwWxt7oevw/eD6+EjWFRWcqwQ4bVCiKoUYxFl7hGDhKQGWBt4MVwK985ZTyuIb</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8WY9lSZIe9n1m7n7OvbFkZlVWdVfvPZwZUjNDDbSACwjqgXoQRAgCRL3rQf9P0JOeJICQQIiCSI5IirM0Z6Zn7aW6qnKLiHvvOe5mnx78RnMAgfoBQjkKqEQkEBF5jrnZt9kFvj5fn6/P1+fr8/X5+nx9vj5fn6/P1+fr8/X5+nx9vj5fn6/P1+fr8/X5+vz//fAH3/msFDeaIEkRkgSCZHEnkJAyJbiZO81MQmRmKjMBmNFAEUYCIGE0EBIkkSDNbX5FEAQplUCmABHmhdXLsvhhWW4Oy+3N4fZmba2MzK3n1uO8jREjso/oI3pkwACRJkACTZ7DMjC6ek9BmVmMS/XWvFVvtbbi3lorZWmV5m7u7mPEZbuct32ktj4SrK0CAOVmtJGxJ/ZMCUgAUiYgSARU3JfmtXotXkshDKKSW/QYg5ZOkpKUQyNGH6P3nM/MzUt1K7DK4qzVzA3GzJAgBUijSSmhj8iMETHGyOtTBY1OwkAQAEQhlcx8fvAwAgDMjaSBAjMzIiIkyEiQTtTiJNzcrbj5uqzHtqytLcuytrrWZam1lVJKAzykGGPfthHbadsufaPoZsV97+Phcno4nc59kzCLZIws/+Dv/53jYS3FlMyMS4+IBNBqaa06MTJGj4hYlnZYillJZe+xj9i3DmJtxd2MZgZAbsUckEk5Is2tlVLczS0jZ4GOjBgIpQQSrfphXe5u1tev7r7x8ctvf+P1d77z0Yu74y59OPU3D5cPT5fTfn46P2z98Wl/igwazEgHTEizrOPslxOfHuN8jtEjMu7W8ulHx1cvDi9ulhf3NzfHw3o43h6Pt3d33haUhtZwvjy8e/fl23enHl89nNJ5e3fvtWT22qyV/dLf9Hga2SPRQ5mZww2UzIC21Bd37f6+3R7azeHgWjR83/VwOl32s5XRCguRQ/vWH5/OHx5Pp9MWssWXm5t1PbR268sBy40fDkttlCGUfexjDHdzswikctvGZbuct8tlu0SEFTOTOYobjdcaoikUkf2iMUC50Y00h7vXUowO2Rixb33rHUKpbkQrflxKcS/ubku15eXdPdcXwAvgFfAKWP79raoDXwACDsAKPAGf4/LTL9+/y9RIjZHbaSuttdZqcTcyMs0jUjRW96UVgBF9YxBalrK2ZmZ9BGiAEQRxXGut1UhAkkgzIgUpyfTqS6mluJFRFBEx0tLSFYlIQaKZhG2PNx8uqYeRPI3x0cujl3Lu/XGPrW9jbKEtONy9tmJGKzKHkBlEFJMLJGqt2vdB6eVt++and59+dPvRi+P97XFdDrU1Ww9Yj2gLagMqlnbHFKNtnYul4fb+1muJ2K1gabVHDzFybHtuPZTG9GateHUjLdcbe/WyHZoDBahAaxc4sa9F1lthMx8jL+WitEgrZQGxlHp7d1wP3m5KXdSOZfECMDGSZDMrXs0NPqpiBCiw0dEWB0CXmeAykgCNRkshE7ljs4gdhAFWi7FASjc4zegtrTjrMCNrK4QdFl+rOc3AkRyjn7anGyeqgAIc/z/rrAACNqACAwgg4KN7D4R5oQmdBVJEkjT32ahZUNyKmZkpk7TiAuRejPbLb29mpTgkkO7m9FAoUsCYXWtOYikyLQkzzWkrAZxNO4lUKrH30Xtc9nG57B8ezz//6v3tsZVqMAQhy/AQIpk250GBARkRUoQQSIlWysIkavVqvL9Zbm/Xu9v1xf3N3c2RtcEKzGCEhOgwQAlDKVYyW46k3M9eam00l3l4Y0YN0GwkUsHFy2JLYYHBPFuT1QAC6EACgTQhoKQAqSv36LsCznZobAR1c2iHG1sX8wY4MvvGLlIYW/Y+egodBjJ69qE+RmYCKl6FNBdcQBpBI2AglNIAZE7CyWTi+gIiRpp1xSy6GKlUGvs+zJmhZCkFmTidL5dLPPHp6XB6eXtu9wE44MDNv6fOnoAL8AF4AhpwAb788uHd4+VhBNw8Zed9LyNUIoD58GlmIiBovsXMTKRkRkiRE6JgAjK4QZCQIfPrX40YGTm/g5khkcwRLEAqIxKQ9FyspGBSZhqJMfIpt73n6bK9e/BiBieNrOLCWmnVajVA7CCz5whlDECpTEqil0YX1+r39+3udj0c13VduDTQ548EhAwogYQSkheW5MGsaxPei8Wsei3mnUyrFirIHGEBFbPqhkD2RAUsE0iAAHHJyB7sMYaCSqVGaOt7ZGaRF1BurnawushasiARewYkIAPRs2/7yARSY0BDkUrJ3Ws1d9IKLWHK+apAgkrahFoyFjqkQCKFhGC0iIQUGW5mhgwpOZAW2JELkbBtG0+P27b1FPq2MeJjut01wIAA7v9fRZbACTgDT8AGKPv29uH929OH07aFVEsz1tAos9+QHJ2w+R4YEqAkUsjIlAhKiEhRSkjA/DeCBCKTnEUWfURmkjSjpEiREgbpyNlNvCsmZIVIm4ULd5MQERG5ddbN3Z2OWksZZoFRzVtGWHctlak+coyIPjTCSXe2Wkq1Yl6Wgx1v2uFQ2lrbsqAUkBPJA4ICsonnUdtS7pdcnqI8bR8Gz+ApSMjBrGCppl1KFhU3aSiUxcwKjXI3E0QRGIAUHdqxjxxAktpHSEgTyeJwc69mJcMHzQgNJZQZMXIIIwVQkvYefcuxRWSW6sUXNy/mXhkCKJIQSEKEEUmRQVanzDTxfkqwDBByJw3FDACVY2hSPCYy+rnj8tS38zYyIezgdqmPj0/37QnLh+s9wt1fKbIA3jx3sq1vTx8ujw/n89Plct4v+xjFCjiKaWgUURMtgvNuB8wMyiRICXltvdr37sWNzFQCBCEkMtJSkSlCyitdhSBQIIhMEYBgzkIKlilkBjQiaLxWLQQAgqjRJYkjSSABFUtg5L7j5Omm2ugYoRwZfWQPgFbLaK0s3lDrnt6zd0mEzDjvAQ2tYl3A5fnBFWAFAFxu8GU987Fj6Enoop7e88O7/d2b7d2bvJzSvX3ySXv5grGO2tQWerPiTptsNEcoovfQQN+xQ2lBGN28wNyMRGK4KZDzgkuSZkEMIWkiCFGSAjkyM+fkKE53uk+6LhrcCgnIzAkyMnvK5tUnAObIMZI24Yw1d85GIsKBzD5kkJR97zk0IgwwQQIUIxIhxIQEZ+Ad4MDxeVy+Az4AZ+CC2C/7/ni5PJyfzlvfR4+h9BAAz0SU6qUUN8LMIkIAlJhjUeL1V1Zm7KKn3A3QBAWzPCLnKJSRktxNKRHGyQ2YSCYykzTQSJmZIMtJukWaGd0MYNr8Vs+vZcogE5z0HKahAKNUFAsRYOYEgvRdl96tl33UFdBxaXf7du7jvG8HCgm2hnUFb4EGNMCBCkzQeQfs7XC+reOpx9ODfvS7j7/zz37xs5++OyyHpbXMuL05/OmPvdT45mft+z988dl3D2W10mjgwIge+x4jcozsGF27Mt3MWWmFoNEgRcSIEDLLsKSgVIzMjE5ncRJAUkHCirvTaFgWL828QAwlSDjLVbkgMyRqjMxIgEhAptCIjMzYQ0QzJ+jElTeAoAx0o9OMpMssjOaTy8NizIq4tgEggQuQQAfeAV8CF+Ay9u1pOz+ez5fL3nsoBFHKiCQTyjF68TmuJc0mNYUXYy0FRCQyZyenm5lxdmlBAt1p8EROpADI3UAISIicLWkQ5Ky9SDM6rThSJGCGOWFLcXcjSFooMlCrGRmS05ShhIChsUcIsbtakVXWCgrm5oYe0TNGzxwi9XBe3p8eWyugbsfBySNVJHCiqb9aZPMcgNrK+uH9+V//s/c//oPHx/extpvT6eHp4S2Jhw/uXs9b/J//4vEb3zj+F//wh//J3/sMxi3zcrmcL9tUBHuPkRE5JBW5SGfJVIaUucegpSykYCKhkWPEkIKAWnEaaRSL0RuVrAvdQYOYkkaGobiJcjNTIkJzSu69RyREoyO593G57DHSjKyoTiskGZE9xugBGAQzK9XH6BIEuLkZFdp7ZAqcpHIBDBjADpyAr0b84rydL733MfoY+z72HkhAcJoMKUXImBlZdMWSmBqqoEKvtbTioI2ICAOSoBcvJMjMJDjVHZKSpRIJQW4UGEzoKsNmykwmHyPgxgFWm2TTDC7yWWWkKJNBbl4dZsScwBQ0gb5Syj0HkkB4eqMd3Z0UCBlmCWUq+hiPp9OHp+qmnv10udTqx9E/bau9MCCBASzA8bnUBPRJTv7kRw9/+eOndVnW9vT+3VePDw9CjD4yA6CVZTv3P/q3759O719+w37466/2rT89bafzpgwYlJo3l8mkBpBBwiRkRmS4S5YGAUrL3iMi3Wl0yI2uhAJmbk4j6SBTyDGiR1eyVJQsgZCUgYzsfWx93/a9jwHBrUjctzife0YajYdcKtKLUvsYT+cePY3GWjRp27wQzqmP9KHiSMQzpBkAgA7swEPo7bvT0+l82mPsoyMRESMyEyBNcDNKk/WYZZnM12iZkuDmXuhmXgoASaXYCCNFgCSI2dXqVZ2lQmM2CKRgzwUrYVLSCeQUoakOhyYUZXGbAodEKUdOVyGd5ubmhDD5aYpmzBwGc/PomcoxVBLDYSuLmxAkaiVppbgb3LL38+M5Q/vp3Fjq4fzUpY97Px5u4AQdy/0zPtuBd8DlZ3/65l//yy/Op8vDw7vPv/jy9Ph4OZ8TGvvY+n667MW9LjeR/Is/2/6Pf/Indx95QqenbXYOLyrFWzHCYiSUUnaGuXNeUeO88aRAmWDGlDutsBRQU6tNGWlwUFdwQEzcDoCgkBJy5AiNMfZ9nC+X82VPpRlLScJ6z8zoI42z2CY9yL3HvsXl0lup1UwCRRrdLUrGJiVCsoyuof3C9QlIoD4TzIcPp8eH02nbzyNz1uhIpUBaMYNEpAQai5tZFFAQJ4N0pwHgZAXkdahZcc7uOdHa81/BzIxIl4mkBNeVQGjyIILFTFSMnBx2EguUOovVTBGYGH1SbtIkpcJUZrFGJEiKNHNRjozcApxyUwdN0/ES4dXMaFBrdljMmPvYcB5nd6k+XU5Pl/Ob92+P68GddN4cjre3t8djRRWw9afLP/2nf/bF51/u54ft8vR6yftXH33j5d3d7ZqZP/vy3R/+9Ms3H05fvT+Prn7Of/q//eS7v/LRt753OJ/30UMSYJUADUCEFCCk+uw0objD3clgQWhIVBIJpVstrqkADCWGFDFIWDFCtGnuzZekPkZ0ZCoiY0SPHD1GjMws1TNHJifajgiZlSIvsALEs5yUpMD5qyoiMslIdakY3enVe+7vt6eXo6DsgAF95PnD6fL+8eHp8jTGoNm8OUbUpd20Y7GixKVvkSOYJPaSJVMwQJrQaz6hlFLpMDMzqhSfDGH6ntOkhOZsnL/r9PuulBGE2WyBVopfO9YIITW/p3E2SxJztgq8clVcG2fw6qFGwgj5FO3oMnopQkYQlono6pbVrdQr2nNjdZjBJ6uSYuvBft74+PT0/uH94bCsh6U1O4067IWXm6VUcPzRj7/48R/9FPvjf/4ffu/v/d2/iW98hNvXVzsl3+MvvvjzP/zF7/7557/z+3/2r370Z28+XL78xfkf/09/+l/+ox+sB1JGhIWhGEUEGIZEKV5LKV5Kdbu+FYmKET1jxIjU9CpdpdAFjIyIHGNIMoMXLwa4zCEnUz1SGX2PvoeAjOwxi2zWOjKlNAGZmamloi3WFi7N9n3eTC5LW1upxWFIcRs5ImXWqkjzolYcrvO44IlLuyS0jf0y+uVyOZ0vW98FNJg5JXkpH9+8/PTFJ1bvAMO+XfbzuW+n7Tw2L6SUs4YEmYhMgdn7ABwwEmYOxMRwgH5p3U5iei0tSvNxKY0GoxvNzI2ZkimNRvdpHhRjYgrA5LNFQKSUk5eaRUQqFJNVEEEzJyDCjfTSIVDVCl3XbkHSWQtrsVoIZUaa2aSBYpKIYmDWBUGzVtdjORywrA4Swo9+/+e/+PnP/rt/8Bu/9d/+18Bf+ysU4UvYwMen7729vewdtMz8F7/3x3voL3787vM/f/jrv/lKYEZpxVsxN6fgENyuohfcZRQVmghixOjPronDai0V7vDIUGJ07b1nspgh05q7USkxRWTmvkffR98n2c9tH5GRkRM1u9l1dADV7eZQW7NWURsBLzVbdTjX1dvi7hwZIxUCCCtmNKWSSmqPjo2X2Ic0Ru8j+j62ffQeZkyGw6ova11eHF5YfQ28Bm7RYm3nFadX8dD08+I2h10a6UYAI9NkaQnAHCRnqUl5FfCvs5M0Q6amYAgQJmbomumYrWUS1Ge4Rnd3L9XdKmdqYBgx/QNeaz4yMUBmZMZIQWbmbgUgydkSIZiDei6ySWNZqy+LOZGZI5LMEWMMWSFTXr0WLqsdb+vxrtzfrfe3683tCnfA98vTj3/8swP7b/32d4E7IACbsBd4Dzxi31Hy5bG+WPybr+++8eru52/PmYi93y1rptnqa1tacwf6QEZCJJiCyTgQ0lAERipSUoo0E91Lg1erDohJMCKjg5S5mczSqMwESbhGj+2y9z0zrjkSAjPKUNyrFaUIc6oal4OtixfahECdYVRtpoQ7zTEUe+99RACFbtWKcQQFJXRVkkeGkMMYVmQe6DEyMizroBf3KNYJVOAWePHvtFx/+OSbh2LXKpBmOxM01dYAGQVT22JOwmvP0hlx7WNGp09WLShDc3ROtgFgqoqzYqy4F5tzhAal0sJAkpFJMSUk0zQYTktkpJRZKirmPKeRErqSpJfJVRNJM65LXdayNgox9hyRibFvQcLpBCutVj/ctJu7dv9iubtbb9baik+y2WN7PD199mrBt149MyyfIj+wAg11w2E5tn2p5VCw7+dtu7RV3/vs5d16ENytHNd1LbWYR+Cy9W2Lre+FxGBQFEhlDhlIFPpkLLWUpVa/4glmTqsFZlbMiruBGRBz2ig5pMR1UluhgRF9hNGLFWpaMWapWlCrt1qWpdRiyux7j4hMKTkyPR3IETkyAEeZwhZsYmzBWQqb0hAsMsIHRuipR8i7q1YsNaulb6e+HB6xPAANOAAAHHgJ9pICMyeo0i/5YiSNU2erRrojIIOmmnJtZ9fgmZORmPh9ck0+a4AzqTYixnj26MjiRnensnh2XdVZMIGphOg5f5DC1FOWWozUnMgklDPMNiUR0ty5tHJzaOvRawHlF+t7jzGyS5YYEZNHHNiKc13LzbGuzcwzsRtCin2/eOncArUAeA4pTBHkE+A96lfA+sXj+1P3j169+vTl8U9+8uXHHx+//elHx2UJwVhWr8e2oK1IO9j+pp/O+7jSKRAuOuUpgzHNvJqXUqoXg0GIHHvPERGZuIbMwOdgH4w0xkiITg+pFpbiCSnhpM+ARMJEATQBbNVq9eqmyL3nGGMOXCUINzeBYoL0iWxIolR3t+pWHY1RRjcmMUBay5rGMAa7JauaZ8uBD+fTuPzso5cXfPQeeA3cP1cbC5Bgsedc3HMS8ToYef2frFimYgrvMIBmdJ/aMgBTJpEkZtFmZNJcz0geMKJWTi3Ebd5VXQcr6cVNyudwnxlIc2qCsuk0SJJlhGIiQSPF4izOWuBUrTys7gYhE7zsGglIW48RYSALbqDarJUyk30xYkdAqT1j9O9/7/bdv/kCyasNCgIn4AR8wF/+4e/983/7Rz/54rzFcliOh8Nv/8bf+LOfv/vbv/4rK4/GkhqQyEQpWFegIL1yj4FULEupza1pp4qZaEZetQw3N89Uj7730aNrQKlQMjU6nYYy9W+A7saBKYemG8ydStZanMUMIgIZQmq6EK1Y8xKB0Zni1NtGjELSGMpMjD69Jiu2LL4s5VjYqhVakzyDihyXQMK9HtbW/GCse26hjuEiY4+xx9PT+f3D4927N69ffIUXL1BeAA35vggwTJMHM/o5hGlDFZ//zegJA0okg+TM1notLkyiSOA586Nn6ZdXXmpmtQD0Vkuduj+pFDQdELn7tEerkNIkvmastUylLRUIRUrAGJFzXAPFyuJeF3pJAr0P0t19HzFSvfdtB4g+AqAKZWamVutSq8kwmFetNPbLrsv4rb/+3X/5l2c8XPAXv/Pws69+/sW722qf/eATZP7P/+QPzhHZXmy5j4eHY+O3P/vWf/xb/8Gvf/97p1/0u49rpJL7pfOQR9AgmwpwZFxyIG1pRAORtLhqN5j2rWdmRPYRCrlKJYZGpiQNqZqMPpu8gFQoRcELS6EZAJdBok3RrTB3RcBJMB2EzOlmjgwjwCye7jNmKzy/jFbKWo7HeruWI+WuYiygj8QY3fpO2tKWpSyFMTIZ5nYgSWVaN5OE7dL79vbp/eOLm9uXd/dY1+3dYzGgVLuqgUQGjBOw091mTdBmOloGwuBmtdhsrPPaR1yZKK6dcEprnBIrDAbW4q0WM0xPO6UZETeaMWkmpVxIQjmBfy1WvUgagR4ZSnVw8hXJzJpbK16coCJz3/u2eSJHj33rvce+pwQY6VaqHW7q4dDWpRa6hROuFJI5lGdg4zdfvfq13/oBPjzh7ft2ePXm6YvXr4jf/Bbs/tPf/enf/JVv2MuP/+RHP/v86XJzewi2zz79dFwe6bczbhJCBpGGHYCQ6n3MogjbL1CBOro46IkwJgvc4XOIFDq8CCo0A0vfY4SrNLZmxYqhZOTY5tUGgJzRMzoyAU2TpmRSMg6aVIs5YZDBjD77aGtTJoX5hHhJyMyWstyvd7fLKys34AIaAkgVDFuKyQiubWm1wKsVG7Emou/jsl1GpMC1HuqhGjDGeHx/GudeSn338FRKKa04AQkpwMKCdNY54X6pPJOUSJGcGXLDNaY2n+iU0wAYbZrsZsjkdAWmmmecvT8iZoZdmRmZV/1X1yz9xCLFSczLyoiMzN6DRPUyFw2c0xAFgQgFkh3nfVgtkQpNJT4CWI/L4Xa5u18//ez+4xe3h7UZiTCEK8beZZ2IUlGr+698/zu4O+IHnyzb8re//QLHgP01gD/87DO7WbDoh7/x6Q8DH756+oOff/j09asG+E31WjydqcKKqBiEiC0jBLAUwNVjH0OwQcJgBpoKOKefEg6omJsbK9boF7uEZ/XleFiseHoO9pGInqJNtGqGUswMgzlx6jWjZKy1FpTDWrxOJT7GkBLmtCILkekOYMYjeVxuXr/49PbFt1BfAQegAEDu6IHaWxttbdmH1QXHBcVWDuzb+XTa0UekZMXL7eF4XI+FdrpczngCEWn7QCnF3MzIgNAzyakwkAApSHEdZJodeK4BQClxIiVlzPCQyAlQaVJMnC4plaRlIiJIcHDqwEpGKKZxCc60ra5/VKa8sRYjGCMmGJ6FpatGHKkgnLAI7GOkc9ljOTgMNJqbFS/uL+6PLz46vvj4+PHrm/t1Xb0UOXdLIbtnV6QVLLV49fbyGw2ffAJ8G4dHHL4NvJ6jrfiKQXzvOxg7/vwnn3/5+cOHx+P9ty21vCpmPiKZ5nbQqNwMMU5P277H2gprkaUy1KO0SsGTBiPcVAwkvMqbW3WvpZCM6GtZkHIvXgpNXREjGczU6DEi3AEU0sxRfcZ5khDN5FYXX+uhLW6ulEbsGUNOCd5akUXvKRnDEYdj++bLb9++/Bb4GrgD6lWVsMRCUCgFh9Vg8IZSMC7Yd8QA5LRWa6QKi5el1mZejqxklYLkYUcpZu4G0DJltCRnYoCEdFVmJBOutEcSlZFJRWBuFcwsJDjdcS/GSKRyrppkoJQ5QyFp7tpMFyoiRmomKGcFgbDZ/oxGzixJcWvFRrFJeGcseoyIMiLKlM8DslAkMuTNS1UtqbWsrdzcthevji9frrfruta2cmmqCFOYxXU/y1nWWnxpWOYj/imwAr/yTAjy+PH90+df3Hz+Bfbx5s++fNyHV8/YX75eb1/UFKPTssJqdLMxzvv2/uEs4HZZ6+Jw9eyBpGTQzFmQNHphIWAs7lat0g2m4mVpy7T4ExlThMiMCE41O2XGFEUzmq5ZwZzaeA/BZDXLUszZI8aeQ2FkirUs1W5Vckq8tfWP7z+6ffEp+BI4AAnsz8rOjhhwBwvsALRr/Y3EeeuxKTqe+waLCYykFaeZVwEqzsONpnpnM3tOTOsNRnP36UdOt2CSzGsQMdl1/XfSmDF/igCYzcgkQdM0QabdSdB8FikMTktpjIxMYhoCutqmIonp0T+TCul5e29AGYEraYFSY8w9kZApk24o1Yu7GmpNI5ZDW9d6OPjdzfHucDxabVq4GegwJG0BBNZauVTUAgP2Hf4ICL4DBG7w/qvf+ef/dw/7Gzle3PjnTz2tkGP0J93BbFUHwjUQwmVsGbqMfYyo1Za6NAcMRZ5ILz6TXamwq0lmShYvlXUq45h5KyYsoJEjtuiXvm/7NkZCcjfOq2hOlZzrhUY3c6PJVGhEeg9DAluMS+xpqukyr7Y2P4gl9x7clmp36yvYx8AnwAE4A18BT0BiTwSx3MFmhqoBAQyktkvvcQmFkLUatByXtiytWAHdKg7rimPDcnh9eixTGoTgbjaXIn3CMJuhXiWBNBMwVwfmfMMULnhNdE9JxJ49ACNj9h0anO4z4WIw40wlz+UBc8MM2858+0yE8ArmphWYIq55SQFTPJSZzTRRpiiNjIHwhSNixsqV9FpKwbL4cqjrshxLO5b1hitHQXHQMWUYA0AUQ33+SgD1gMsJyxvYPXCH8vjrv/r9H395+ek5L9rkZd9HkpfT4//4P/yb/+Yf/f3vvL63dAkZfd/Rx5hJbsIRGpAZmnvSS3GidnTgapdlgGYFFajwApubSgEKyn3s53E5n/fee2ROvbCY00BWpwGWA9Kgg07AxUL3FHvm2E6hjBw7YbQN2dDM3LOampeVuF2q4fgx8G3g1bNk+AvEG6mzLmg3027AL1sNAk+nh4f3I7e2lrZWd4tFJlCDrAAVYrPrUtnxWKaA5e6g5qQCFTOigymGJZ7XRuZgm0Lx894gGaSJmiT5Ol1xVTbMDD63p4pd5TYiIYruXqFMYsEAACAASURBVGeEY/y7+ptg1s2n3Rm6RjmnpDjzD6SBMFoqMyylPUYwmuo1zSYBqtWMtq719rjcLmvzZeVCO6A2VMILMjA6MMC5PnSNCiOBLvicFA4MJG9f3929efrpeR+J2nyAo+fD+fx7v/dHf/23f+vTl5/cVktTHzEiAR4Ox+OymEE5LvujYpTq12UrmMNrNdZy5XRByOAO9yk/Tp8j9nHul8vo0/aFkaLDvB5qrdUb4YG+9957SGmFraKWkrBMXnokempLhmCUMyCyZrZWj4c7wBGBYwU+fS4yADfAp/Az8SWA5805AAE8AgMfHt6+/eLx8XFZa2v1eFjNtfct9t1MOY0bFdeUMQqQZWp/z7lWJ5FJznTbL8vLrtvmRhMSsOLPm0gzuQRh+ke4Js+u0bnnirtGPK6BEBaV+U7NKKUXU/7SkZwIfpJJi0yjZWIqaky7TprZhcW47gdku/HDTWu1GKxUs4kQzA/H5fawHtpytKX4Al/AAhYYMQjF6JGI1la0Bl/n5MNl4Diz8Dn+8f/yO3/wJ/d3h8/fvPd6f/7kxbquYNkTb9+d3n5436N/sfH2rlTLbe890r3UsqzHOxQitsvY975RaFZCIgUja8O6wh1D6In4Jc3RdWVGykgNMI2EA5GphLlXb0s7rHURbdu2AKL3vQ8zaDGsRq+RTDFG7dkT3TxkMa9gIlASSpih/dUQ3i/P7TMB2q7EEx0IbBect/7wsPVTXdrx9uZ4ONpK5JnZyyFK2dgKrEBH1BW4AVYgy5zo03MgmddPJciYCZ1rrnG+fpqTKHAWd9A42SEl+WQRmlxxQq7MnEHxvCYknwvympQEVaqbcaQyYtuukRDac1HPZYoUSJDFHbgW+9RIxhjzZ7SD3bxo603zYoJIO6x2WJa1ruuh3t6st229WY7wFSwAURyc/j0hExJe4QfgAA/gjM2BjnvH+VwOL//Wf/9foax/4y/fxr/6y//1q5+G+umS5x1fvHn8xjc+evny8LSdf1b4yWK7uKWqUTQUQzEN0Ck4HajIjB598QpzlAqvKIANDIGa5YVr9B3F/NgOJcbI2Dgy1SkN6dozYGRhcRUL57BxfXuoC2ll5h98DKknuqVCSOWu/Skfl5vqx1sc7p93Mx+f1yYGcAK2573fMyBgw/stTr3v+2m/iFrWZT0c7HhECcQ5lKmLNXoDUJAAKrADAzoXmrl5QrORCDm9NGWS8OdckD9LNW5m1Wt1ARmKMQpLKRbhc66OkSOljIFJAWZDIwxG8/LsihZbFi/VRXDrnWqp7TnHYu5XITITnNnl4orJTmYifIyc4bna7Piy3L1alrXUVuaSxdqW++PNui7LUm6Px/ubO7QDtECEGawCBYsh0veOBNCAFTBkRwgJbI79PXrgu69x+RgPO37/y//9J38aN8vDOU7n89u3796+e/8f/eavvv743h0ftlO3u/Xm+L0f3i+3K3CcIwMcCw/aNxYlc8+IUGV9XrgiADTOnQpIv9w3AkmvTd5UewTsMmL06KlpSmUqNdR7H/uOQGExXPe95zoHBURxr4wlhSmEK23DdqwHlsShATfPBfEEfAACWIEOvD+fPuz9YrSCZVysnzK7xhiAUIq3VmqDGZjp7CODmUyPPJBQQW4wIoHHpzLHmc/lET2rpWRxYoaGRTO4e3WrzcpSWqtlMZpiCFpada+eI+aib9+z9zif3c5730eMZwPqao8TRCl+e7+uS2ExKWiwjvFsai6tgNi3jJESMhNzE8HdDPMrY8QUd0vxw225uVsOx+LNavV1rYfWbg7rstZWfV2Xm/VgyxF+RHeAMwUEVIDwwfQCu24RI2CGuwPu74COn/0ujp/iBfDmR/jjL//o8fHlJ6+i+U9+8dXbd19+ePtI6O/+p9//3md3p91LLS/u/KOPV9Cet1sFGG9fL7cft/7F6elNH089BzVJ5dyIGUAgJ7U0GK9B/OtyxBQhadcwfJBJQ2pc4jLOXbJ96+MShTSr6dPubfN3oLGEmzcxQhrZCReNhrR92N6u8AvADny54c/P+47hlvV8vjw9nfbYm7WCQw63rE4j4F5aLaXWTNi5D7s8jdOuniZTGsIbmjuiQx1pujyWa2BxbrqYJn80o+QAIBOT5m6sSz0caj2Udiil0iqKl+p+OCzlOfG9X/bLuZ/P+9PTdnrYnk7bfhljCESpRqc7abYe6+39sh4anRnDCi8nRtXNTfNKLx4jzfbzkwaRCSbcyDJD9RnDgmEGX+p69Jv7dryrh9vaVl9Lq25taW1+eox787qUFdZARxJJFH/e5U8ACMGJeg+8uG5AUcAF+NM//P3f+7VvBn71h/jOPc76wbr8/MPpy6f3Tw9vtscPMeLFi/Lbf/P7ujm2Le/vDsvtLbACcR18Vyc+gc66HG8/evt+veSXBxtygcIYwEDsYECCOVCee5yAnjkyMwb2se/7NqJnXpdtIvpQj47Y0sY1PZiwhCEgyqFqbhXRqeKGWqJClkl3pgfX/ozxd+AD8PnnX3zeIxAeHdvW932UUr226qxlaWwms2aVnAPlaXsKStaHxzCGGIEC6zyv9tVS6rIUZ3vopzIfQ46U0TOtlAKl7BpRmniJ5m7rod3cN1t8Wb0evDVfj22trbWytFaKSYqe22WcTpeHd+enu+102k9Pe9+GiKWV+XkcJNdju3txuLk7uONy2c1Za4GwLKUdPCPHyMe1RJ4TptwlTUrsPlccwh2+1PXWDzftcFeOL8rxph7XWrwUeG1zFcWrL4bCWV49cZncOVBw3RIbHZV4/avA6+flxPG8onj64z/96ffvvtd+8Qu8u/zkJ+9//vbh3el8OT2+/+rzvkW18rf+zl87fveb2MvxSK6HuZkHAHh4bpl6Fjz7w9PpZ198ePPmw2/88MXheAArtrH3/byfd13kXEprdVm9kEzuW98u+2ZCJvYtekQOkXC4F6fPcHb2TIUSqEtptXSzvCrcU8pMFhkoeoKxU0Ip1hav9ZfjMoCvPv/FF2/ePrrD6DE4RhhLvb7n20O7bdZMVCjH2Lbt6byfti0lVJUDrNg+rG9mgiMv9XLzIiLr2jh8LzMpkEqTWfP1xte1pnI7x+lx27cBEpAXP9y3w93iiy2HejiWw81yOLR19WK1XWsIECPyctpevLg5n7bzuT89bWMEpFrd3UIyqK3t9u5wODTSzufzcqjz8telLCvHiG0Pmp2fMsYWwzk/MoI59UlRS631xg+39ea+He/rcuPr6kut1bwVL1YOSzu0m4OvjRWq2ITtgv36qRKwgWXHZcfe8frXgNfPsHfOuwBWPL798Hj+F//mR3/3N38AxqeP+ZNfPLz98qvT0+MYudT2rW+9/s/+/q//8f/1e3/+86fvfvdb3/32J8urI0A8Pf3lz9+/eHl79/EPJtua+7Tn0+P5fH566tWOWG8QRN8ul/+HrHfrtSvbrvNav4wx51xr7b3JIut26lwkHUuKrMhxgESIIweIAf+J/AS/5wflLUBeDeQxQJAochIgsGDFliVbkc696hTJ4t57rTnnGP2Sh7EWDw0ThQJRZLFYa3eOMXrvrX0tvjtvq59TvFS9W45WFmFE9rWt+7YTCRlnUjghqBRiJZ4SxBhTC0pSqTyVWlkLMYPlcFjmSZlya0972yws3C2w9WRnrSUs9r5N5S2wAv743ddfv3n79HxWYSYFWLiCmLNMMi91OdQZZUYQbB/y7fP58rTuDJ4WZVbyTBPbemsu5McHdGJVmpbQYPVIRWqVOulyX073dZqqW7C2bWu+OZNAcHhRTi+n091cJi1V5kM5HOq8aK0qwkVlKlVVmch77IdyPFprfdt6az7Wmjr2eAhiFhFVLaqRUSY+dCMSZGrhOnNr/fzctovPU+vVAYyp05VQxMG1lGWa73U5leWoy12ZZhq/jQJVYC7lNJ3u53uVMQBjtEDr5r25ZY9jNqjCHJ9/H/gC2D7sl26d/N/aZf9P/v7vbr86Y2+4P5U/Ov3xDz/5w7/8yZ/9xc8c9PkXn/7Rf/V7z+3yP/yP/8s3bx8P8/ziYf7h916cDse7h+MPfvDV9z87ASuAcZjBVu9r29cyT++ecf/ZjCJokn3bnv3i3XTjBjdrUysiMlCBqZLaHQpW0SKkFTxlsCfDPC09BcSsVad5qvPhxTRN81ynEyDARfbm9NTW3jOa5dbcGyzMXRN5PJlSsR7vnp5aj9aiwxk5T4s5CYlMlUmUZTi4QAnPdd+ftvXctq1ZUT3KNPPkYwHbvPetU2RrZDvlXEGr7zqf5Hg4HI46HUs96DzLtOgQ1G99T6ll1ruH+dWnd/cv58NxrpMWkTqXZSlaiCSTHMykqUpFNGvWmf0w9W6928C6MJOoYMim6Aa3YTEzVsrQCOgAm0mWXjP5Mtu8NGuhhSlH+wtRhkSZab6Xw/00H6VMXA8iCua8CmCcZ60vj/c030FPSMbWYA2Jrdm5X0jQcl9qme/ugB8C/pGvf3gC5F/+6b/40Vd3v/cHv/316Rtw4u4V9oZJhH7+T//k9/HFS7w+fPvTN//TP//fy7L8vR+/PN7N/9nvvv6Tf/Rj3L8ETsAROAAOBPAE5Pr4uF4uQuaGn37z7kefvcJpQl+3c98v/dL3nTedSJKYiMo0TVPVWaoqND09kGQNylNCrUXvZs2s90hwp5RaDnenu7t70oErK8M6xJwetnvb99j3fD73beunvUTOlv2y2nE5gKiHEytYIoKZMzkCzBw9+u677JJg37Lnuu7nfb30dctmGiJESoC11rb1EmlLlSQhxLbv2Nxgj++f9NX37h7u7w5HVWWuooWmRSJJCpx9PpW61Lv7evcwn+6nOpeirCy1ik7MDCcXghQSBQsISSAWEbnCnTQp4spSGCqfzIzktDTznpYS4BSSolKqAEh0FlGVOsspau+UyML1umTVmO9lvpPpoHUmUkhBUgLDQEXKZakT1YrptvdlB7GDLBMkVJCFsgjuXt3ocOPB3oAGfPPuJ3/zz//n/+31q+N/+8c/vD+WN3/z169+IADj6Xn+7OW7ff3TP/tzSv/Lf/t3PJ2+/PKL5VBefXL/x//F7+D+B8DpRu4IYAUmtAtqeXp82pu3fXfHustf//zN777u798+Pj9fWrfWQarHOj3Mp7vD4TQvyzRDJziQBIvSmhMDFGod1pz2PaxxBnpEEUIRrYW0APPtjdiB3r3t1npz67ltbd9926xA9Gzm4QcRqbWIVNFZtMnewoK8GSeS2ko6Ni8t1khPS7fcsu20dd1dGMohPRlIA9lUsdRFK+/UerR17VvbH8/P+vlXDw8Px2lWIk5EUGhlSiSmYMynMs1lPpbjoU5H1cIyXHbiPSLck2MuhSRGkfn1awaL6GH9yubAYLGMTSIlMqV137dm7sPnxOCAB7mo2PDLT7wc61QRoSp8dziEsUd4CZmzHEgnkGammwdLBkGgwqXoxCIQIAy8wwK9oTdPB1/xgNPMU623P/QDJZfAGG3Ey0/kv/9n/3T5/mdXTs3X33r/5s1fX7752df/6R/+4C+/fbub7U/nP/7Pf/zy9Ytm/HC//Pi3P8Ppy5uiRm8cigaU7Xmb731vRmkJhJvl9vM3b04IbJd1v2x784wXd6cvHh5eP9zNxwXzDExARQHQcFkT6B40SZDvDdZhXdJZ2QHXKgFr0Q5jyX1tIZ/P7c27x7fn8xpG2bNviUChGsbrOSJpmSkiIKWI1mDaKC13b+IxJr5IRIbxXpyvKLXkTplzT+7KLIV18kIlgo6oU51Op0Op5bk/f3t+f3k6Q3zfTF9+dny4W0QlMvferUeprKJSRSdurerE01zqVGoZFx/AaSD06GasEM7WIQQXy7EtyXSL7t6HR/uq5gYo/GqGFjPfuw/6CALErCzzVEuplIDmdNCD1UKFBYepHpfFO8zDyLdcWZM1Pfq6OziISERFtMgkWjpR9kb+jGAY4tL3ZpbRzUJCVac68VIBAs7ANK6Y60QNfw+n18tpB07AOyD58yOwnPDzP/1//uLruj0hBfnppy//m3/8BzjMKGMkewcccAVdKbAN7hzgT5cu1JlpvVwO8/J0iQzf98uvnqaX1PZ9695Px/nT+xef370sDyfo8Vas5Vr91dCaJ7v3zmiRFpl5VTuDWQiW1vslsjA5EIn11+/efvv0trdt3x1B+2bWkpIFnM7BCMvebO+dDRZtbbu7dTMf1gSLbuweydF3FuekIORgBnSJeshEZ2UqnUjZo7DMc9VSlAtCvKFtHtzPz7tOi9RFPS0i0owLaWFVlgJwqUthpqE3ZE4MHlz6lQk6NGbeeydl6p2HFs09PEZTYh75wV0cmcMa5p42ytFjDBATKFo8vLqNoT9Pef+i1kmr8nEp8zSFk1tc2i7Ngp2Q++7KRCLKWmqZdSpak7Qj3u8X9HN0Z2e3YbUSUZmnepir1AIZ88ntho0ot63LYBc+3G6fQV69HL788X/5Tx7/4ie/5N3mw/JP/uT38fDZbYtwvP2LefvVDNhxZZvm07kBePe0ff+L468yCe5m7y7nZZ48kxl3h+WT+1O5v4PeAdO1d7l+Y7BSVWbvaZ7JwhQkShlMKWG+W+++C3Xi/bgsLHxZt3fvvztftjAzy4ghFrxykrxFGrjEZVvjuRtq663ZHnY9STJiaG1a9ux+SYiylFHVQyaNeRGW9GyO3qGsRBxrrH03Dnm8bN7MOzbv63NTD2/WzC0pSUJYiBPpCZJCCmbFYAgyIYOGVi1jwLI9gnpzHcPeuFJ93D0ywsLCEoPkhkgeRpXu2cwHtioSbmE9rJuqBnxBXaaJWeoi5VhUeZrksNSqhcC9hV0stAYc6cwotQpDVFW1lBLBZrGHebdoZt2pg1MmnR6Op6lO06RS9CYCGfbMJ+A0RLO3K28wmD5AWWdgAx7KXfWIFw+Hf/QPf6Svvg/MwHgClpv9bmwCDOjIDjoCLsLvn5sK1t2GvC3SGdxav0zTYZnJeaoqROAPPa8DeitcAhMGF82FsisxpVpGt4yrjzrC7by6+3Zen1V0a3a+bJfz7n04GomGU12Y3SNiX6NfYg9aXbZW3J0ovYN80JdIq2ZSZDS4bU5CWAmEwbZjYvciJaZiz6nOScG7bz2o0FQwb62tra/bemnrtnfd28oy7C4Bzokn5IgFAAGiyUTEwZDB/hAgiYLYsvuYChs12ttwKQ75IUKIZQIHpZt7Cktm9sjIMHPzPvwqmRxuvZtZAOnOkRxg4ZTCWlMZPMHVGsDgzkmKKjXCKb2UOrRqLCxCkbzvnojebd3W9HCLvgcFvzpMIqWoMiki0RxlVNUFUOD+Ntfw29334ZAb+MIJ+Obf/+SbP/y97//W734O/eTWVJbb2y5uh9B4mQksUToQvce7p3Y3Y+/hHnOl8+YsCYpz94fjaUI/1kmkIOIGUyag36rWgTDqlhbwzEjkWEURWcADRgyKNOsXN+6C4LXZ5bxv625mlESshUVGmVFacbY0975RM1/PXYmL8tVCy6QiImwexME0fvHoPZu77T4Ax+ulLEdeFjF9unBz+G57JgotBUtYbLb27AE3M+3WqysQJJAkYTADGRmEiMGywGDzRQ4dK4NEhQA26+npsUcSXESFIUpFiAQE4qAUQg/KjMyB6XBr5pHDnAIfx6MKVFGUVDLhSZTUgxAaPbztyUSUkkbDZiFj2j8EqTpU5ujdPTKDVWgqxTg8mnMqs07KosJC8kHwNN0mqAVYgfk2pKXbWTLOp3G9Lpc3f/Vf/8kfogysy+kjRh/dqnNQSLbf1Nx2BoWHPZ17WLr5eWtMyHCkA767g+X1cZ7mOs8LqCIMbEAi/Lqz4uHbdqfoOV4iRpmZJkITRETT3Um8IwK+oZvvzb2F9+zNM7lqpkJFRCgRwtDK+5lajwhj4DhXmmHp7klKsvAYWOw9rzgjR7h7t3Xzp/eNk/jTu6nOXugSfc1u4RbD22WKJuBIs9x72N6aEqBCmUIcVaUUHrZzIJUhRDEYuhnMV5YtkyJBkZlIQ2SGO10lYZAQKBMNTtcQobn5IAJxIIhJ8mrjI0pSpEOEp7lMVWphMEAR8G5o1vJKmmFh5Ri5DKJ8pbaI0mAaBLlWSlKlqCJWi5lfmClbpSqiyRnihPToMrJLYMAjUID7WxPwkYbiNyJSA6ayfILyFWDACZhuh9+Hm27U5XfA+fqsKvL2TcvYKc08fv129ch1cxXOTFUZJoct8fLFCUUhAge8ZfQW1twdMT4iKZyU7t1GaxVGcCZWIi6sWSIlg03Qdt/2aJt1DzdQUhh3i+idJlYalDVy1USKejTvPYRhFq3DzCNi4sp5ky1E2JYRJAlC9tZ7M3JUqZqFrzd9mEdvbuaZSUQ89sbeuu/NrPeuVaUWzUwWLYWKkLCEj3EUZYabJ+IqlMgcnEUfFEwLt4xISgSnuSkoBK27OCWTu1nvvXuYmVOABgZNhSNjRHWkoGgpqtM0icq13Rg0aJh7WARADBY2HoZ2qIhocE1lKSzJYIcDKErJkkppureOBCeRqwhS3JkMGdQnTrnedwlcPjqTpqtW4jpi/VBGvRx+CPwO8HdAvdXih5+A27RsAxTYgR2IF3f11+9is60of/24ulvrfpg1kXNlEF+2/dw7DhWq6J77vmVrse/Wu5sjmEgLT6mQtPBI7+HhOxFNApAICCIBck+JoXI2YWGPoBDWqmm9te5VwjSKCYkUIoOpsgjaHpbYtta7MCHCy+S1TEISGb5zv/RAsCYRTbWECdc8zYfjYZ4mFk1L33fvzdzcI5AWyWOAA/b0MHQtKkUYJKpJBCUQgmUwH8MCRAEfwFyww8KDIwKtubt5DxojNcLgdfduzGiBpDSz3sO7eaQ7BhSeuDAniIblQpilqJZSSyGiocGy4TymzET4mJFT0mCYJMgjlam6uDsP9Q2QAx3D46P3JIaIzNPEKVrItTcOkLMgxOT65A9AgQpMN/HChxUnbpU0nk1PwK8AuZ12+Ej8EzeP0AS06817eWTBmzdv//3ffS1azJMSl63PUyWgFFZmczyvq6+bLNVbe9wuLb1T6xGeBpAymDRAAyc9Qq48khEdzATPpEQMFxqGNJUSUKZhRWAhR5p1qkmUjijETKwjGyoHRQW75aSUnMNJycSigmDKvq1pZtCgkgArlJSWaZnnqQiC97aGd7c+UjG89yG2p27m7oLoPRQxLEZJSXzFGuRVcn3tEkFEAioQIbYIa9Ejeu9uICYFi3AiWUCUI6TCI7tFRPTuvbsbzK6upmE/KUUyODIGqCMDbkk07JxgUFzv3MEKFBUVVvoNjS/NOxt6gwsTwcMJyUNIZ3BLpLCwQpgJEjuMk1RYgJ5Urq+ogVLagXcAAZ/ems2PC2h8q7f+1G8/IT461cY/3IBnnC/P5+1X375/ddJ9ff7rv/7bolqXea6lm63NkFSUGHSa6d1q/+5X3/3g0/myt/fbpbOlBl2BfERVQdnDPLy1dmm79TZE8cEIA4MBD8qhKEwgyIOCFPMiYCoOPURr44lBwkDmOEUQgQxKcosE93AVmiYVSG+QMnQR8LTLuUFDqzCL90QUIkGShfe1reu+bx5mgQScKAAeHjY3H9FqGubpyQlcyShXOf84eoaFV4mnogWlcAnK3Y2jMxhKRZiUILDsCWT61bUegSC3DMsw8p6t+d48CcQ+TdWNXAOM1OFShpNFjHIhYRk4AzApQVmKqCqnZ//g+fcMSTMfGO/dOtyTwswyCCST1FqqVsmIHj0yODhdYqw0rh2lAhdc/m8cDsA/uK0HcLsNP642uqqQr08xfPRDH469BKQHr7v3nt9+dznO/PrT13/+5//6uMw/+OGXZta7AzkUm4dZnvb4+v1+OKD7drHN2Vi5EJMUUAa8BSKt9bbvrbUWEZQ5Tm0HMRgckQYdON9MyjKBCGXG8LqW1No5nISIktPDmnf37uP/lKxlRk/hFGJhbbmvHZLgbL317Fvb0WkOTgrr4LBt77WjNLd0b75vzXsPJDJZQZzm4T28ZyD3i2l2+O5cFJlBaXk9yQIMhqRSprBMqAvPVWsmzbANvZNdPcaaDtsCm7UEIQYggSXd3K1HGqWnd3jHNYLMw5Q6u6pkQTqECcgcCiWRoEBwmbQws0BJlMAeMVS/AU+wkNkQyAEZzfvA4Hh04VIEqSABlQzz3VrrrlSUMCnfHeerqHo84ScB7oBn4JOPKuZDAeFWWPxRCX6owvwPSs1NhUudmj+/Pff7GS/uDz/44fd/9pNfmBkSvTcWdcc8yWHS6dxa+LdPxmXdbEvO6kIi6eOrxUkeYW1rl2138zQnsLJULQxNQxKcJLunjrQQJk5IOlw0i4JYxLjtET0D5pEtwylapEUEhqgBkAzktrVIskiDG+z5ed+2PSnSyNSZc4DGnteUtU4EVUeSADaCN5LNwJzWvXfzDmGK3TUbwzhx7aM9kscHKgy78hNVRKIs0zKXBZmNTLy19CKkIsnR0cNzH0K2HCMLJk8O5eEFdqbg7Ok9mNkcwQglrpIpmcO3n+5JMBhBBUzsrMLsIM/0cMI1BSIIYFakBQpIyNO9p6d3d6QQw0EZFJm99623p8u2r1ZlORTVIvV+iPcH23eHjIHZZx/JEvEfHVR0o5rTbVSWH5Xd7WCLuKz98XlNqNbDxdrD/eF73/vs+eliZmbWdpoOJRJz0VpE2GH72mbK1r1zQbbo1ksZUmeKCLduvbXWbbeIUEgRLVQql0wm4mbN1QQJTov08BhGVnEhCsrIDIJzhsMitu6XzbbWd3NiqouwpBBFxEgV6h72tO22PT1vvXVKrZPMyzWhsJt3X9etk4oWnitn0773bhgsi967RYPnVEpV8aqqqIqJEtEDSCTHmGvQFbtCTMrThKWgQiscBdQyNFGgygIKTmkBsdh6RAYRWaZZuhO5aLCHo1HsFI1IiVJVWaCqUqCVayFBQNxzCJd7Mg0Q+thVjei1+qe2TAAAIABJREFU6B57jwAnoEqusALSIMqR1hPBSE7WkjOkJvHudr744/PWLA6lyBQSAf2gdJ2x/QpzuTWe9aMW8sMVGcAC/Bj4bqgCP2oRPj7PHOjZrZuLyCcvZrO5u//avkuSu/u7fXt6fj7f398fhYlwOuh5taentSgjjp6T5+qeFgbAzMakMAcNOTN7tq1zMhRKWlIn0jofIqlwDXZKT3h3b+ktLD1cIsmS0TqshTuFY1vtfPHzpbfmeW3EMI1gS8Sw6DKbp7W+W2veMFVeDmU51owkTW6ZgCpUUYsyhA8aDiZzj32LFrA1MmwpRXjMx6PAJTzCcT3LMhNjcExMpEUmXqrMQmX8NtwQRmlkyCKkpVJEydBw8czokdG7tT6e9FxYENY8NBBJGjqlKkjAmrxIqawcFJbkkgHcIsysRwhxBpwi3CN9fOxEmWGSLKyVqWDY/MIpQpiK8iw8cS9mYT36zrZJb3GZdg5lVOAO6INp4M+7tB33Deg3Vxnf6ga3kho/ut8K6+Pnf9xedTbMcCLMLHtv29Z/8e3juto0TYfj4f/75S+WuZxOp1rKq/t6Wfef//K71u2T+7uUbY1D4B3GpDncjAeTSYknKiAgxZAZWHI61uU4L5NORaon1aiR4da6t3DjTvveGtvEjCRjby331dtu7tQ2f3607WI+XstCyqxFWQfxO4lJNPc9t57MQ+NCRVmYSRkMwCLBksIsUGYtEx0zy+RmrtUJYW0fDWgpLNOklBKdPIihRCzgwOBXjHgIKqgEYUgEc3PkQEphTElFhCCI5FBNLVnTs5u1PfbNiFBUuEoFFCYZHKRCE3MVlVJEiDKjG5LJkW10IZTjjy+TCjgpDOZp5oYMx9WoR8xF+Cgz1UIEDJFIhCtKySyRCngEowmZptkeDtu/+GQMZkdeJOTh+N3Pvn5xv91u0iEQ2m9D2jEqq8DPb+Xl/+GlGb9RAVnvZr3bvrd1bee1Z6BU8TWE6fHx8vqTeyY6Hsphoj//N79+/fKwWzycqgUul9AyBW197xlBgLJMqhOXyjUNvUBzEmDR8nA6nZaZRDKdIeScnZi0DCYHgYKi006RJTx9323bbW9O4H3t67lbzwgkSIIJ2MgrETEscZhoOgg0lm1yo4YstWRI21I0iKUInEKEmSSSEAiAhCihSrNwN6pNxuSCiVRZYZQj84FFSVWUmYkzkdZN6GrC8mt5jSw+nqoihJkwGrzmfTdvCScKDkPfY1tNhQspp4BJWQmmRIWpsEylSBFwprmlUVJ0ij7C8jiBZJqqFghR2qBbjpQ/z0xCgDiVi5jWqAvXSOvwvjdrmeo8GTIhaWFu3lsPT/d02yYZj/qHEe2BcpyXGe/f46F9NNG4AIePbsYPK/a4HYTltir4MGDLAR8Z2t/RczNzbx1ILYWJny+X5+fLz37yy8fvjpn5cDef9zgdaya9PffgU6ONgKnM98thmaaqLMmc7MKdYpaizIdZD0vVwslpyAjfHN2dgoSJhZXKYZq9WW+bG++dHh99721k6m6b9W7uOSgk6ZwuiOwGLlGnlEnJBJRlknmqEkByeIBIwSMBTBhE6GaxJUEiIymSkygpMc9ix4kzKTIDFNDokQZmrlKmWqcysYywMaNMhMM9Is1CiAcpoxRGSo6cOA+zvq1tW/d1ayFXWpBch4GqqkJsiES6j7BREFHhIsyByAgzD4P1gHNRLcqllmmeDstcVBO+bhvOSGCEXYRnCkTkMNe51CoqKeEeLXyPthuzRXZNcuoO2/reemvuFqEkvQ/RjtxkGjZ/ev7lv/v6ywe/9ZXjiLKPetLtoxGu3dbnfpt35K34yG3QhXnEWt/UVMmEw+ngPb/51beET3rg+59/4olXD8v9aY6k+uZpbbUu8/3p7mE5Heo8FVHNdDfzviPNlTFVXRbVykHRqO3urdtu6J1gNHMtoiPsj1PIFY1s9f6cbUuQ95vCrHkPzytaBaV1kCW6paCaiVVKVdFSlMOtBdgPR9WS0dENu0XrjZSVeTBfwaR1hKiGqC6VaPJoIczMqRHBScs8352Ox+VQipjZ3lpL40yP8Exr3VSrVtFKPAiPQeZubmbr2s7P62VbewBJyUQgFj0deKrlcKgE2Da2UxwJpIrUWqcRleJh0dM9MrgWfbi7u79fplKHA5NVMrwU8cgBM0lK4WQRVZ2nUqsyyMO8hVm42d7WBNiJdjj13fdmZsjMHC+MbWu34MgHYAKWf/mn/++/+atf/He//4+AMe9YbyvLcTkO0MYAg31zm7qNaAFcD7MwMKObDfFd+o3XO4CWqaW8fHn/u7//vTdv3q9rO5yyBzzyy88eluN8ed7Tuxu/un/96jidpitv3rN1rHBr2VVTRFUpyTZPZ2vRL31bN9/X9M5sxTSOmMOHUZ84FT3IuII7eKi3zWO/Ar2DGCJQKUURHokRohGRrCxadF6ogYi6FJqWnCoRZN8IF2qb+d5bUnoykzLBNUskEQ/Lv0qQZeTeTYlZi8613h0Pp/sTQPvl3PaMa+6XR8JEGDTPleYFAphhbx5pbvtu+5DhejINMDsSUJFSptNhejgtWviy7hmy70TkqpPqVHSqVYUp3DjZ2EH8cHf87PWLZZoyM0GeuDKWwaIqLCNtYAhnlWiaijD3sLDsvZlfIyB6NCDTyaKvfd96D0QpOs8lgy6XDXgLLMBPsJ4fv3n37dvHbgacb9LtHai/ma5dn2X7rRvgj5bo4+8MMMzCnZAjMWRrzW1kngxaYT68OH3y2Yu7V3c//be/MLOn5+fDxP5iXp/x63fb23dP09w07r988Rp6AAHepcfavbcuksKFSZy9h1u2re892t593ftls76RoGyXfS1b4dp7t+6coIAiBZxuZpGWvaHvEUhI8pTCMU9cKofDkSpdiFVJNZPgFiQByVJYC80HVVZQ7B3VymWPqzSSBosIYSDloTkkIpLo6O4xgkS5qB4PM44LIiZrTxFm5n3wTAkZKkxTwTIhHL2nm/ce7pE5XMQjj7RzkjAyhXip04vj4dXDSQ81uxedwvjbdxcRVVEmmrTMU4nwqiWBZa6vXt7Lwx0IWPe2tm3dmwdzekBYpzoDxkRVVQtRpCoDCLu2yz0tyCEDROPhuVvbWttbG+EHykSB795fkA3kwAsscv/Kf+93Pnv37gnPb3Aa2Jx+k2/oRy/9D06CD0Nau73PGMzYnIVVReUaW8LskRip90z08sX9J3f3SPnu/qnvq7l/8+3jw5Ffvfz062/eP5/XH3zvflt3lAPmA9bNzvvaV49UnkvRDPFIStt829Muvu9tbd33LWwLNzK3te0XbpNMaZluJdN6izbEy2NdM6LhyZ2YaCp6ONZpZiRkYmWWosMhWapArtGs5uTJCU5IQKXQ4agQ9UTPSIrwDOOR7kvBETTeWt1dCphZl2U6zNPxuNBxwVKRiXVN+JBpXFHbmSqAMIQAQribuVu4U14jz4tKEJEkKVNQRzDTVIouM16cyPPLpLZHGCJQhapgqVKLqJQ8TCo63x1wOmCZYIZ1f/f49Os3z555mOdSRUiXmWtNM2eC0Iiyc8DdLTBoAOnhzfpuPcODMty9u5urauVSMQu0rQSa890v6OUdUHGc7++On71++NlPv/7+H3zvVlj4SJTBH8nL6KMfotthRoBGknUbxF3z9HCzsG7unu5J+cXrV5/ff0qBn9ZfffP4qKWdXr948eLuzZvz19+8/d7nLz99cfi//tWv/uGPfwRmnC9723sL1TJVrVK7k8EQPdq2detpl621zbwFpepAhhZ4t9WSOnE4At7d3DJiJNBTJBExK8NEeJ7K8TAvSzHLfktEoeCiZV4KQbaL45Jg2rcEApnTTESFlJm9lELwtOzw0VW4J5ljRAmam8UAY+tnnzzc3Z9OhwVTASkocA20BYSTkCO5mIanbWjnw/16IxCGmpWMSITKzFDVTMDHGglM0AmaWOaH4/x+0dZs4lCEwCl5mSY+zqgzTjNYgMS6f/fu/S++fvPtuwuBHh7sxf3dMtUyTeG+7Xu4u3vvDT0TZMjMaNF7t3Xf131r1olTBEXoMJfXDy8e7l6eDqepzGBWKsDrtf3sgA3ojz/99c9++e7rN49ffO/De+vjLRPdvt8+Es3Krfekm5+AWZUstRLtMYZ/e2tDkiWqAnz5+tPXxxdI/ntf/ejXb79hpvNl/fkv3x0m+f6XL7ae/+LPfy40g4Ftg5syQ+tUWKWAtSYherfITrmTWbRna7tpsgpE1ImDGUzeQ0B9s73tmdEjHCYQZii7MIcGUuqEWgtSeguLbN0tWkmi4KrTVDSR7RowkK1H35HhZq6a3WPvHXBmSoEkZ6RHWrMwIJOTI2J4m4VcX764W+5PmCpquX1kKSKqYpaJ9OvSPq6fOQNITx+xanSlvoOJIKSqZSrJwtSjUykFFrgKCVwoFuWZda5aCyhtksqnGXd3qBMwAR3rc3v3+M2b90/PWzdD8rZ3t8j5yjNSpt287W3dNneLMXhBdLd939feetuTBwZUatWvHl59+fqr1y9eHw93LBXjsYTj4fMfwd5CFxF6Ou9vv7tc1u2jIqPbFak3tT7dXmM3stBAz33oFTK+efvY9n5Z7bL3y27mAyR7zT17WE6SAsfr+4f17GbPx9Oh/uCVefz0l981p7Xzq/sZ2w5CeBRw0ZFAzYgEKC28uboUF39OfwZ25lKneRJiS/RrKkOmu8fwAY1EMSlKbtGS6pCdOYSi1sIirZmZBYWyHCY5zEuhAmd365v5Fr35fnGmFNLedi0UHPu+E8WgOatQjxzzdbOelkxcVaaJp0WSXJfjjLsDpnp1cUXAY/CeVJlAlk4kI+xgcP2x1LrVkcWNGKnrxDowtKpSwWRCIEom666XDQl0V9FPXtxV5arKlCwqdyecjqin38imHU+X/Xze2sj5Furdt32f50J6DdTtvbe2dzPr7ugAiDMoM4Mop1lVuUx8qNOrl6+/+vwHn7z6Hu5e3kSzoyyegIfLtz85fMHHLx4e/8/L3/3s17/1gzcfScrwkUr2w40pH1lO/DbpGH+VttvzuQnz8VjrVDy3vUUwdGjdA5K0X7bMtO7hUqr86IefffX5w7v3+/G058VDdCn1clmFiCEs16iZQUcn4SK01JKmF1ftZYnFGQphV2ImBHfD7t4sjZhRlkoRQ0xo1jlBgAoX4sMBvFCdmD9YuN3nqUxSsos3So/Lbu++2c/ve1vD9mBgjV27slCLDvJSRZkz0tzD0ke6cVpEiIxQwDLf8babQhn1g7Umxjq9lqJ3xyJMROOrPR3na2YRZtyRJo6Jp8ezexLltExXCuPA6CUpIwgW3tz0vEEYJMvpbjneYVIwYzgRakW9A063wCnGvN0fjw/3J3PskwvLVHWqha6e3RGgGwkS4byCvFmUiDFB5qjJXoqcDseH0yefPnx69+pzHD4DXtyY5LjVWZtn/lf/x7/+4VcvXn9yV6fj87l9LO/5SJeB2zvswxoqbrv2Dwv1qEW0VGQI42lv69oiQ1UicgCmvdsuPSPc2sPD8YuvHn7rq1cPd4tIkTL/zS8uT2d79XBvLZJRCg3ZoYd7pIjWRTHNSzhzXi7roSxo7AhWBjh6mntv7t0pUplJayKVU5Jat5FrOuASdcFypzSTA4PhI5KZdV5KqcV7Xp7Nw5+f2vm9tUt4TwFHoLcI78zCKtNcVJmY+m7RB5phTILDI8pEdeHpSNNJqLICV2zs9Zsw5nLIIwBUwcBaM2OaoAtwvKpP74k9D47euyozqyc5Bh+ZnNzce+veM8IiY5KplIp5wmHGNN0uprwF6E03s+QCvS+fxY+I7u5O29aGFSAplSUQmRkq8zQRwM5aA8zzVLQyEA3N01jkMB2Ox/uH5cXx9AmWB+DwUZ+I23/9CUmPl/a//tlfvXnz9m4hUf6oCfiwHZfbz/+g2rCbK4k/AnMAhS9ry7TGfNm6iBRQREQ4cU03YIRxZDM7HOvnr0/f+/wOh/lUIqWdHvPp+flUSnioSEayEhOtzcysFEWdMU9gTNaP58u67l7TPIjQPSKi79Y2A6FI0cLElIKgyEQhtW4WiUSZ6PSy3r2cQ61nuoEvHO7MqSyebD0uu7Wtbxe3FmGJSCEQcw61Ncuh1vvTJMyXvnuMqZtHAJEErhPNi+iC+Z7mA4KhKPyRdSdBguOCqQCE+uGakJtDer5tmg3zVuZdq5AKwJLRh9KDkpMCsVtb1zWDTod2Wo4vTqIToHpTseZH986wCd2au6pyXD4haksHODPDk5UiYNW6aas6T7q7RRori3IpnOQcIEyH5e40PxzmuzKfUE6gBcjbvlJv/iUGXvHd41efPnz75v27p/7+uT8/r7cq5P/oMPtwko1dwsdF5reNJ1225mZCsAhmlkA3G7y/3pqWUrQQ7GL9iy9f/P3ffoXDESBQf/O+PT5e5lJmURApa71OkaImIoJFIAwWCFDqXKdlmZnYxlQsW+9JFggIEycYwgJIBkkPZ0oQWaCZH1TqQctCmEU812cjTmS6D36Ge/e9+Ui8Bqgo93Ri5siIYLAyzaLHUictleBr3zHe6kGgoqolysSsoZVIgxmKUv4DSyoEXFDt9uYfi7zyUZ81vnPA8ox9pvRxA5Kbtt7Mw90zBhSztWbmzGDmZZ41OrYzpg4h0AfL9XBw8G++ZtuGDJl1mSuYYYEIRFh4JFtoDTUvc3SHM1OwgzIJEjKV42G6P073qHcoM6TedLAf6ptu+MID9Hd+64+4h2+7N/t2Wl7clgFy+8lxawX4Vk/7R21B3roBBgIqRWtCmGJKN8/Nu6osh8PlfBkiZRC9v1wudvkHv/+5vPhitLHr5fL2/XZe7au7QxUh4jpVvDjhsMBD6mV5f+7dptauQO7eIzHPUxXp1q27MGBuI3X4FjTIhD5ERZkhnMJSOCyoph6SFydFv7IDrtBxZQrAIjychlKBI6+hyAOLnUTOJIUhyElApbaprptYODHYSZi1MAmI0ZoxMwEK/3A7fGyv4JvQZXyOejvY/Pa5F6BABR5QggBwJ3M0MBEFa4pgORREnWqRQi123bPGSjYgZQxmlDK8KADQDa3hvO+7M3FZZgxCOHesNmScRLhC4YkEaiBQJHGPjkShqfI0yQKaEYIesAY2sEACJLcDSYCXV6Q0L8+X/t13T0AgPkQxfKizm9rnKvJeb1X14YbdbmsoAsmLh3nv2Xt06yr+elmWZXr/eO69qejj+fz28elvf/nzL746nT77BFgG2e/x4s/nlSIfphrhBEFR1BFbAUzGfN7PW2bOrYHZ9xaJWmoKF5OcnCm9m4UlLFlKUREeSU8krMSIqIE5zXRHsZQORTINcpj1iHBRYgEQ4LjS+YOuoR8jSzEDBGZkOmAwN1hmKJWlTHs3dJPkIqLMIgZwRO67t4spzitOl4/cPnnrp3b0DVuHAyJgRlWUGXhxY80vqM+jPwZ8hBcGeXiIspY8HeoyaQREtJQC9s0vLaE2EvI4QVIUwlCFW9v7uq7Pj6t1HJf5EyVWRga6b23v3ZMSJYmBQixgYUZYwjNgKSQTTTUngGPrkQaIEJEqimIkQohAFFRvz4A7oP3Wj7746S/eP6+//OFXv33jSX04aOPWaRbgAqy3o11uQ439Jo10gF7d1zePPQKlzFPVZeLvHtenx/PAWZ637eu373757tf/+P9v78t67EqO9L5YMs+5G6uazV5GGlkaSJZntQYWYAz8MIb//4NhGDbGxliWMVJPd4tkLfeeLTMjwg95b3Vp/A8MBvhUJAsEK29mxBff8h/+FDj2w+pLebrUdfOBMDAQToSecnh9T/pzwFRriXAVbW7uriKqQoMTIMQGRGas3CyIgSASHnJujADI3SkOKdLJdFxlCFG0Ft4QDShQ5tShMuUQglApYR1oBXc9BigI/dCFFataEwmCImjg4ShWpKhoyhrJnbFt5h5Efnla9fz4fMqENwfI/pWLSYFNeLrM07qslSFJeJeTnHb4DMBbYAAOyBXpDHLASDyH11Yb3M2YOWXKnFpzlh4SYFutdTEBadKUBEzUhJVZyCyi+DQt53mFQZSLlxEZTGBv0dYoJCFKGIg0OHHIVZIaTppkoGFHA1dtU5umpWy9t9Cc85Dz0IW4whDBaQ/cAXeAAhczuzsNx/1wnp5ve6R41aV1R7FuqY9bh8e3Q/YyNADgN4d8WbvTAJji4Xn98P6pbLUrwUpdp2n+4u1+98X9TWncPj4vz+etFP96lyWqcHAYvN16QoMHchrHQUSJGRFe0SNax5wg6AZNR4RnGMdSSoSbQ7NQTrU1Q1ASCU3SEg+yI2Fyk3WudSbfiBqGlBVggnkLcieqYWFw6/7oDA5hCUOGjpoTC7mEE6ACKNlOh2PKu2GUzIuXlbHathYrW3l+2PS79x+trff+GT6XW0M2w1dczg/T84fHaZo2Mh5Vdinfr7tTEhzzD60bpSttgdjDW0QLhzmxCSiaByKat7CtlGneytQAGrLmMfHAxAQm4hgoocXT83R5WoOIlI5tHCmj1bWVQltLlRPRjnUU1gCbUTAxB+CSoAOyNnb3rdTLtG2LBTDkvO+h9hEiLswkhlPHhPstVde11VbvTol/kDO9dHIvK4EK1JuTj9zaiZcutoMgjRKPiXyUrfq6tofHyzpvbm0YBiZa17XV8tP7F7Bws3l+fFrP0yaEz3dZGcokHaesFTTDHVuFBbFQShBCs4ESeWMCsoKB1rSLHjzloRl5td6TdbcJdETdyYUBVSG0Lepml0dbL2arSwMAJlYGTJqFUmTmUJi7gFS7NwcFRWYdNQ8pZ03W+hNLwjLmYVTd70ZSkLG32sxr9TL7Wlyfpzmr328HRAUJYCjPmKeneXpYL5e2ljAOUEsisW50eHzk3QDR21M73nQ+vjUrzdZS++gBj1KqI9y9WFu27fy0rk9VIh0O4+5NTjvVhOAIDgW12R//MM1PhZPKoPtlkrFvtAI7TwwdOO+VhQi46ZwIoGBIsDiThVWr1cJ7oBmnlFWSahLN2hE75psSsx+gMi9rq6219tt/+p/Av/9j3wN/tQlo1yCLH2bMeDUQBMBIokK7FMvqT+d5nTerFUBKoszTMu01/SztrzjLeX3456fHx3krdacp8TU0XlXBgq2hWm8xa7HmtssJjhtWp2BABQQgNCLlxLWqSnI1tGZhZt3ket22UkoaOWUIszeptZXFz8+2nrcofhi0y7I94E5MzEBShIOCBcJESSQJh0CZkzBn4qRm5M2be4tgIpEkkkNMiCVU3Q5Z2uhp3hQSMop3Fqxs8LXO56f58rxMs5XGpYlLMHQnaTDS81Luni54u3+1QmaA4RwuQRqgHk+xbaVVax4e1sxq86fHenk/D5EV6XgYMjIc7kbsAbJa54u9f3/Ju/F4d6yNmgHMaeAkQ7Bx5iQMWEUAwcZhIBdEUDCMvbJXEkq7MY+ZNaUhp6HnLKcMFYiC+YbVAWjA2lojgluA+nlKrzr9F+SlvNpmxu15lVfHzgGAZTck5tC51a1Za27GQilJVH++XP7yix/fffUVsEcxfFfXb8u333w3Sxzffl1dxTVh8FAYwd3d5nVdlhVASqpSU2JcY+UZwh0bhxOUstqQqodFUPXgoAhyM2tupYW5NaREYTCnusbluZ0ft3XaGEjMWSicvHJzix7DBeSsiYJCCKwhqQfBUbCEkzUyFyoWxVttlkRKhFgLCiNnpYEUwR42D7MiBQaq7ENZods2X76/PJ7naas1EEZmiKQ7zXtOe8kazFGISkXerqBlq7AWFh4Q1sRSjbZpXZYwI4AdVCvmjaZnK0vsRtkPh+N4GtJgCOIYhiSqT76w1qU8p4FPw+mLuy9Px0MXFQacehQHAuhxuhAnMjZDLUZgcoaJGyurjEqsWVU1SVKooDtxJ71mQVwVcgvWaZ03RuQhp6yv9kivpZp2U6C8YBm4fZPXmhQCJI/JvBLC3MMszDhlJq62lmn9xV+8wddfoRq+P88fp6eH9bf/8Ltv1ocv/+MXtt9XkuKZLPlGHr6Wep7WZV2FOGdbC3ISZSahISUJlmAIoYa7BLJqqOmQm9OYzLdmjYyjyZgdxgJWgK1G3bzzgywkSDkSh3CLfnKTo5J7ZiIhUnhlcmEXcSHuq8lugLI62BxbWMBRMbWytSoZkcwZzBIWKcluGHVj28hmK1wXr/EwzZd5nWttVqPb+rEQNEIQSWTc7wdKCQ0gRzhahReQhXtSiYgWRg11QVuoGakwBVmNOlGdyWrs7oe7w+nueJdyLq2x0Gl/GMad+vTxsO7H5zf78UdffHn6/GvsdvDKpcAdIDghDGHqruGAgJmWcnmel9KUVZiVr1lQxETdw80d8bJEitsj+Hi1/fnOp2/n1TZv5XB4c7vM6DZ0v4Z48MeXXLxSRm0/BPkMwktF1/yX4h5dJWa1/vztXfrR5+AR7y/1+8fvHp6/ef9xC3z55ms0aUgSsjZ2ourRrC1rm6a2VRcOc65mYyZNLBy1mUgQjHBNx42QZsmBCBVokINiyDgN1MyrNRIHh6FttMWg69p2+yZCKWnOWVIKaESQULgLhyboACFpjVEFVcKJAe9XLZmHAV3dC3eGx1ZrC2i3YpEgwNzCXIS0RJ1bSVsJFneU1a0pmSLC0QwBj6VWopKi7oeBiaGKIGwFtYWV4EZi4MZkbsVKtNK6QIKdieFGqOEVVsMqUk7jONwdjzrkaV4DoTKoDElLTsMw5M9Ox3f399jdAQN4RTO4wAUSoAT/4ZECiAG3Ok8N3vJAOZEI1JsoB4eEDlnY+dq8B/+gGcEInLGUe919+PjwtMx//ot/BQy37v6lXhDafmmVV8Z6L</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9aa8l2XUltvY+50Tc4Q35MiuzJpKlEmdKJYK0WgMEC2g32pBsy4aBhtE2YP8If7V/iQHD8AgbQgstCBpbalGURJZEcayJxWINOVROlfmG++69EXHO2Xv5w7lZRZEUxW6rRFF+C5k3X94hXtyIHevsvfY6J4QkLnCBf3e0uHGAj/74o0cHzMzMvdbq9ezsLP6Id/YCP7YQAED4fi8Z4CF4CLVL5l5KuYizC/zdQwEABBRwVZXdMxe4wN8lGtUpIO1R9CLOLvC+4L0gA1TlIs4u8H5B3uOzizi7wPsDAfgo1C7i7ALvI+TR40WcXeD9xSM+u6g3L/C+4V0+0ws+u8D7ikehdhFnF3jfIN/x00WcXeD9QmuACgDwIs4u8P6iRdtFnF3gfUST0MCLOLvA+wnZ8dnFuHmB9xnv9tQvcIH3BfLeDxd8doH3E++G2kWcXeDvAxdxdoH3EbzQzy7wfoPv1ZsXfHaB9w1ywWf/Hvj2ay/9qHfhxxSUCz77ITFuHr76yguvf/vlH/WO/JihkRkv+OyHxPN/9kd1WL/wled/1DvyY4fWDriIsx8OB/uHgM/nez/qHflxAQEQ5G6C+sW4+cPhuU9/JnX9h559tv33C5//4x/t/vxDBR/Vl+SjVRAIgH4xH/1vx1ee/4Ptdu3mb3zrldXpQ9+uVufj5vT+8tI1AOer0/2DSz/qffxRgd/zA3axBfBdViMv4uxvQRlOb9+6Sae7p2jj+WknNp/1U56WAFC/9lfP/4f/0a/8qHfz7wH864qYb6Zt6iMIq1695lxu3XpbVI6ODq9cfqyLSaCFRjde8NnfimGzUqELYgzPPH2lVjk+29Ra3755Y3N8686944cPzr76V1/8zM/+4o96T//Owe94BOBjHTeb9Waz3W639+4/eO3bbzz22FHXdev15sHxw9XpajMOMYRZP7967eonPvGRT3z0Y2/duDEMg/tFnP1tePDO7b5Plq3v4uWDxcPT4ex82oyllG/3z1weN9thGl5/7dv/iOKM3/voKG+89da3vvXG2epkuVg6cePWzWE7vXX9TafnyQgXAYku9Scn6xs3791/5/43vv7C6vx83E7Hp6uLOPuB4PbVV14OIODBhWWqOa832+PVdDgPShPQnWb2vR/9vd/7vV/5lR+v8fTd2PLvGB8J+I0bt/70z57PZbp8dOnO3ftv3riZcxU6hW5uDncCpGPtRQUOefvW3Vu8e3i4b9XPV5uLOPtBWD28P0x1s8mX51K1xKgiUA1OVJF7q7J1jV3nLjdvXv/gB5/5zs+en53+kL9lvXmwt3wMQMnnx6cnj1/70N/9N/lBeG9k/I5n3qscjTZO02a7uXHz1jeLk16rmyEkRJVavRq9lZWEOwCIcKiqiofHZyoCXNQBPxi0qJgKw2G/vLTcFL1zst1MJVc72fjgA6ACMfDffu5zMcblYj6fzWZ9euKJx2/fuVfrFGP//bZb/uAPfg+os7579bU3z863H//Ys3nI9x88qO7/8r/6F1cf++Dfz9d79Pido6R/10unJ2d/9LnPv/nGDQmU1kUCVUUIgmZejTRACAoFwjYfgCTcUN2rXeRnfzN+97f/tdaVOcfi2fXc0t03T67fOnFzd751834l3SkARNw9RlVCVJ2uoknljTde+9jHfvp7t/zrv/5/37hxY5xsyDWIVOfLL75izskwn/W//q9+87mf/qmf/ezPzOdX3v3INB2//Oo3QfnMp58D/r/Lxd8ZYe+Gl3xHkJGAeb13/8GX/uort27dpFiKgYKpuqoACnGvj7hQ6I4gsjskNFUFhSBAM1zE2d+IBw+PA7NV20z11bdXcmsVowS6gLWa03cnRWBmhJsRUIW7u4MhyoN3Hn7sY39tm7duvvbKK6/cu/P2dqyrTamVKam5leoQ1uKbbVmvp1t3/+TFl7753E9/fBiHL331xYP9tJzP3nl4Mk584aWXf+6ffPYTH/3Mv+/X4vcLsnfXlwXghDh9GIaXXvrmnz7/hfv3H5A261OpkzsCMGY3qyHuPqqACUC6uDtIVwGdklQg2er/X3SN+8d3Hjx451Mf+xljDtJ97xveunnjnXce/pPP/rWTN4y1lAz3WnwYpnkXZ90MbqJKUdCrGwmC7i4qqKyoUZVOqIAxdem7ftGX/upLr337zVpKLp6iWrWpONzzTs5kJ2rmFfbN12586/UbGqQUv3OHGpBinM/7b7/59nozPvPBp+azx//dj8R7dPU9oyQBVDeA05Tfun7zres33n77+snJcclTiDpOkwaKcCqo1ZyQXTiBDoGLigYIUB3u1CBuTH2IrpnyjzzOjlcP//z55++/c38+6x8cH89ns735/JMf//R3ve3O3bs3b97+rjjbDkNQgrRarFgNOuYyTnmcqhnN3drwQjrphgA41KQCgIub//lffG3/4OgTH//ku9t0dzNbj0anilQHQDodDKoAqlnfJYWIwuFlojtJsMA7E8kH+8v1+fD5P/vSL/zcZw4Pnv7hDsN3Edh3Rtguzgicnp299u03Ll06fPv23RdfeunO3TtkGUdTxbC1Uj1GNSccEMJBdwPgAoEQIGpui9HCAXcHoBXV/B8/n/3v/9f/M4zTcm++2U4nJ+fPPvMBvXr5e9+23WyPj4//+nM0txjDZpgcMu8jUTabmhTzqI7qKsVJRxCYy1A9qkCchEpbJIfb89XTT1z7zo0+PD4uRhFZzDRbFAxd35nbh56+uh2Gu/dOVPHYtYN5171x/c52W82422BQVVHRxXz24OT022/cOD8//xf/5X8BLH6Iw8DvCbJ3R0k63KqN0/SXf/mV16+/CeLNt9525pxLnth1MpuJG0vBNFUVBSgKd5q3xpKIihDWpA04HeYuQje4OwTkP+r87Mvf+MsQZTGf56mu19sY49lq9fGPfOR731ly9nEEYHXartfm/pWvftXGstpkJzq6IjrCcq5XLu2PxY5PNgCleFDp4ZOjoM6idkFJjOZRpU/x6pWj/cP3cvnVye3NelNrVdVszNU0hFqrE/cfnM1mIQRRxflqWHHYDtkNKjQCIkHFzDfD9OZbd4rZ8cP1fJ5CiP/pr/6zLn2fK+eH4zCS9uabt772wosnJyfXb97ebDZTNjoXS4lBJnotzKL+KN2nkwJUQmgGAipQodtuqRY62G5J4YSCDtF/vLrGejj/yle/+sJLL6/ON6V4NdJ9HOvLr14n47Vrj8/me3TrHokOb9+5txoGACH2+5f6V15+4Wtff3lbalBNXcyjdYI+pb7Tccp934cUt1M9Xg99Co8t+/VU18M0ajjan5njbDtd6lOOoZ/9NbI5ODr61Cc/8bk//8q808NL+9dvPRTRUlhKHscRkK4TMbl3/xQQM4dAHCToXg10tOLDyCAy6/uvvfhySvE/+9Vfw3t88X0Viu+8pcTueYIgr1+//ft/+Mdv3bhVaybh7iKMEUKWzBAkiFiFG1VBFwpJBhUSqoJHBiBReItbQAUxBAFFIABJ0X/wfPbCSy8991M/9cO80zj94ec+d/PWrZPTc5pth5qrgTTbidUESsVXv/Hqa69fn826+WL+Sz/3s//Bpz8DIMRAee+OC5/81HOHR5f/p//5f+36mIKMIxhkO0zbgQfzNJSyzeV8m6u5E+c9V9vRHRW2zdXN3f08l5nIg+OHL7/69YO9S1/4i7+4dDA/Oth/+bU3+z6drvNiH6QLFO7OdkroDoC1eouCEDVFcRJAzkYCkBARXd397Hz91OLST33qo4B+jwb2fQfK9wKOxMPjk7PV6vVvX3/l1TdzqTFI6hAjI+CGmhkUZpKrqyCoCOgCEiLqzi5FEcnVzY0UFRcRUkREAoIIRQV0c4CQf9hx9hu/9ds3b9z+YeLsxu23bt66+fqbb52enuXiQcTM2il3h0g7caJBQOZcU5fW680f/smf3b13z4nTkzMnt9vtYrFjoKeefLpLoYuxS4hBFFpJBQzYn6VtzTqKqAYVI6QxD9QJqAQRiqjIw5P1//K//YYGunHRhcVMTs/LeigE3rpxr4sCkgKSUVEpCaJBMnw+Ew1iVahU02JGgE4ISwYAVdRMIOwtFn9TVK03q7ffvn2+GT7ykx+8dHjYWkkE6Zim6d/84Z9++esvzfoul5qCtIJEhbkgTw5CVOguEHNXwHYkKG2wdGfbXpsJTBHBu6zWtFq2GCPE/2HqZ9988+U/+dMvbNbjZjUR+K3f+d1f+09+9Qe8/zd/719/89XXx7GoitNqoau4sSUKIuBO7BKlxqRdF4Ea1ATy1RdfqrmWsfaz7rVvv/bpn9mVouO0VYHVMjjc3VG6mdApUTWqG7oYZCH0XTYigKqmqDEGEY0qFKnV3EjAKyd1mbzClsvglGFbRIKTQSUGjcnVZdanYlWFIcj+Us/WPo4MoZWchOx6jiJIKS7n/S/9/KcvXz4C6iOJtQWZATg5PfvjP3n+G698i25XH7v8iz/3mZ/40AcuHeyVWsdxeu31669861vb7bTdblVBSAxOSDXm7O4kRWgQqIi4WBsSCQEgJIUEWpkcAKBdzBoFBhUh0FgZaLsNmez8fLv6xgsvP/n4k1evXvrLL38lSvjsZz47n80W3Q9r33v9xmvfeOnVk7PVYj577Ojol3/pl7rwfWSq78Jk05e/9rWnHn9ynMZnP/RMn3oAv/NHv/P6WzeG9VhqFQYQqvL004//t//yvwYw5EGFfVpsp82LL78C2Ndf/Mb9e8dTNkBCQMvGFAhBSml0BjeyHQkgRPR9L8JqbuYiIoAKABxdOnjmQ0+l2PVdvH7z9q237/RdEHCaTJQSCDAgLGf9ajOVStJLpYqWXJ2IIRwe7kXVs9XG3URDiEoaBNOUVWAgnBSoSGskCKQ6ValCgYYgU26qnGiAO+kQSjajOUWEEN39c3S4/I//6S/85Ic/9OFnnwFC4zB3e/DgeBjz7/7B52/fe8fMu6hjNkA+8zMf/ae//Avf+MbLX3vhlYenZ3mcNkMOgmIOIEWgsQ9IZ61tCERUmMGcVoVowyCdEoMAdAACFbRvpioEvJUCFAWhQqKULP/Hv/o/l4vZs888/Wdf/OreQf/Og/t0Wcxnv/izP//Z537+e4Pj5r1brPahp3c94/Px7Dd/+3e2Q7WKJq2o6qzT//xXfvXypaMfHGffeutbf/XVF6z6NOXlfP7P/9kvf+5PP3/73i2hna+YswWogUHFnVevLUPAmAuoJEqhmUFY8lQrQM/V3aiCGIMIzMwdpZo76Duah0AEqYska3uJ1Naze8T3j1Jb0F1VQ4RVOpmimLVuMVOHWoXupSBGzHqlSPA4m/dBNefizu1Quj4K4G7baVJKtkpAyHfLtxR2YyIcGqDQulMLSIqAGhQOdz84WDxx7fL1m/eqWQg6TVUUqnrtyuF/99/82sc/9uH1Zjg7O9ubL77x9Vematdv3ZnNe8k1Mb955/ThZnPl8uLocO/23XvHD4duBiE220Kimgsgyq5DDExJakUuAOkOVbciZqiV7qy+S/elVQECEbT0VwRQBNFGvuSO2Oic8hQ+/jPPnZyeH5+u7t0/3mzWpXAcfRhr34VnfuLpFGbvhsXvf+6P/uQLX3zpm69FwbPP/ER78stf//Lduw9LcYcHcZIAq/lPPP3U4eHhdwUWUeTRDc5+//P/5stf/tqUq4i4czOcv/jNlx88OJkmy9lQoaJGSiu+nZQsWmsxd06T10qSVpwCgQAwa8cAqo+ecbq149KuVWlnT1Xc6Q7d1eIkFI+OIIHZXGKkVcQAVXGybVCEZkhJoqpok54QFN1Mg8isT4RBOet6iOScF7O+S1FD8moisNqSZUhLtoCgwcwEumO4XS1CFRUId21GqkoI4dq1o2EYq1ueqpN0BpH9g9lTTz1+//7DL37py7fvvFNLuXnj7RDTcm/ZxZSHwQwp6qLXs/XJw+PTWivBrpNqPow2ZXPbFYYCiRGE1Aon6SiVQVArnHB38+bI4HsrabcknzQH6SKqMWqMzX4sQFA192oW3W2ays2bDwh3R8kA2M/Cm9fvfuH5L33kwz/5zW+9db45v//O8dnpxpwq+MoL3yrmz/30x77x4gt3b98WMgVxN3NzQhCcsVVJv/E7v3Xn7jtmQ9/1pA/DeHR46dd+9VeuHF178403T05XKYYyX4hisx7alT5NVJGkKqTuCmkROB2bTXWTboaUMI3qDidUNKhlNxHCIRECKWZudCd3NgLAIdp0RQgwn/W1CIW1FgBkNHiQ4KSIxxCg3js1AJR26FuyF9p44bBKVe06VbUgUsynUvqUhGEYS1DsL2cAN0MWwazva8kyD6qBjjFPZhVwFYkhhRBEQ85DiklUSskhJgBulssUgpgxl3Lj1t1xmqxY63U1Krp///QPP/fFq1cOhXK+Gd5++87R/n5++KBY88ZhyoVgces0GXOpXPZdrhWUFKRkEF6rzGaqKubwAjOaw82NCAInS91dqUQbDne8wVZiNZKGXLp0sLd/AMjJ8fF2vRaRRR9PisEp//3/+D+kbtZowAmrFJWuk76PQfoQgoYowFSqVRMKhfN5N+sj3WvNpKQYqsHJoNUZRSASP/HRZ3MZr998exqHzSa3ZmstDDFcOlgu9uK9O6e5uEYJqnt7KWeWApJWoYpZVFLcXUSqmTtjBLW6S0wi1GlENT86PHDU9WZl1UshyZhargUz7hra3BVZEAYVAPPZbLHYG8ZsXsiqipzVrKTYkchlWsxjSHUaKeIhaClWTQR0QzUKKCIxQlTdZTajG1SlVgaVFNJyMadrzlM1W21zF8Ph/sF6uyZVBIRMUzEvoIAVGhQqGqY8dLGTENwM0qjOcxngXszmsxiilupuZkavdFBEVBFTeOKxo9m8r8X2Fl0fU3VbD4PACBmn4mQgHj9aimAYrZgFwWo7bqay3WQnVDHrNfVSC92FdBKluIr0fXCzXBlEU4xjKa0Tu1h2e4s+Z8tTEUG7QjTNLHR0Pz4+XZ+dxyCzPp2vp1JyVCWd7hRROkREhG5SCl3MzGPyEAK9iToOiFfL4uv1aO40dL12XQfSxFIUp3sdv/biCyod6Va9VJLFDRDUqRyfrI5P6Y72jJV65uxiBFAr0W7a6Kxm7u4GF1doqSRAWM6iyjLa5aPlBz5w9fR0Mwzb7FPzpUyTRUXqtI3gO54nXRAoJEMIMcYu6TTBxapneKfKmKACd0ZXCK0KSTOUYrXQ6EHE3EFxMCgAtepOjCOsuqjOuliqu9W+Q4iSc6UwqkxTOcPa6bNOSSUoKsogKm4uooSIiEpo7BBjEkUMAUAIrKXEFOfzlGIwQ6kmgi7GdjYIU1WFlCmHkLZjtchqZgZ3JRi0g3ExSwxdVJ0vYMMw79NsnnK2upeLY29/IeqAmNUQ4nIWVVVEzepqU2czTSqLRe+Mx8dnZu6oTzx+GdQuhXG7PV8PheHZDz0xTOXNG/dqLrVD6QKMXg1NuIkJ8x6lSs6sRgGEEpQi7jR4cGujl7cEheSYqw9eq7eByQd352wmopxK3m4cIl0XorooRZpCRELgdLIUF23ELzCKiFdkdw0CosV8obXUqqVaZuZGVRcREYcLFEF1u91O0zYIrRG7KEgwkBJUzEXFJcCdQaSLkrpYipdi7h7UzVGrx66ECAirDWbQoLWqmaso3avTzCHioIq0JrI5o7PVB6VSIcte3VvewGo+6+L+/swMMfo05c0wdCk9drRYrWup9VFKKaqBEqR9T4CQoNrP+qjSz3oAbvM8jaUWVYkxdZ3O0cpAMRpdolqMMYAQuKYg1LaXYAgaBV0XzFxUS2GFyy55VTpTkNCnSNegQjOrAutCjDEoUK1uh61oSlECveSplJzLJKIaWHOplTWH9WY6PduG2N+5e78aAu1kO4YQnn3q8sn5sF5PMURPFg8PdHFAgQ5bKZnbDXOmGZgZ1Q3izhjbAASIN3dBrW4OtIIErMW2FNBy8VqgKn2nkFxKFRE0W5I7ICqQQJi0jispMVKgTo8aGRwVAEvxnfwF7qo8IZ0xUVXpEKCUKkQ15MoYooi6V0BCVEGCIIQSgsbkZQLBGGV/0Z2ts7tXYy6eK8XFzIuRRt/JYIwaVEWaCNF6KU0c2RE6Y4yN+Fs7D4JaHRBQoDTzYhZETeR8vRWxoGGa8q17qxSCOZ0uUDYZYScKOAgViSmEICLIeRIJoJtXVUIoYgDNQMIEpeQYgwvdvJoFlRA5WAkC220weAARUtBhrF0Qq7VUq25n69HrFKO4mVNwPtJMowgQYlHZ1FpLpVl1iDhVxdwIoZFA7OXug3WtrUQXFajY2WaMMalib2+5Xk8xpb0FtkOZp3gQZ3HMrGeekroxJDm6HM7PLWffpcxCc6qJBjVjrWZGIY2tYiLMq9BNpCIEOKFKAcwd8Gn0rhcVAQwQUd+5X9DKO8DdRLsZZ7PgdHeGiEdCMkUgFIMDEGfo6BQYSV47Wn7sJ58eTLe5lrKQeah1KlncWI1iNcTghtRhmmqZmkodckYMmr3WPOaSm7TRvKAk3UBBMGgkBfD2V4LAW2NvJ5eK7JwJBF0gUJTCEKSa03UKFiaZR7CWPiFqLI4RMk0Tum7WaQzBnWNxShCi1TkagqrUOpkPQYVGc7FSzWrqEaK6AQjV3B1BxY21qiijhnGyEMNiVklkt75Pi6DFSq1iZmmRrEzng5u7mc8WgVKq52JiTqWU0YszzbTvRbzQmSfLxVRBVzNXFWvyhwhFYhaS5u6GGHQ5m33wA48dHw9TqbWy1Gpmb987mXXx8St7i8Xs4ekmnhzXlELqLIikDv2+XLki643mSRS6EwWUQHN60Ky1c9kOkNDdAaUYAI0BmoSGlCSPboY8cSeKC4NivpDtpqmnj+QGsO+5OLBxw8VS6VivKBJadWjVZn3M2ZokaJUxxSce2z86PHi4rtVo1QFZLubm6fT0vPqkAg3SJLNpclBiapEi4zhVOl0cULV5wmZkKVQVr2LWPIw0hxNRUbILQNUgQaS5dFwoLTzfVU2FoFgMCnU35loT8qI7PJ9Gc3azuUzFPJdSAen7hVVzCN3NRQRNgRK6WzUrDhNAJTijW7VSNIRuBjqqGSAaNQj7TohKSlKcVzfHcp4uXT5UQQykc7MZWh++us/mKapUd/dyPo0l19aqp1MRt2OFKJ2qrFYV2BUZAUZCQaCxxZRdRERbbsqgOuv71PWnp5sHx+cAu6jzeaeKxbyjY5gMoaQoEYY4Q99J33M2V5rHqJcuqVXmyYeBeZSSCTIGFaVU2i7IgJ2yRHdRacZKcadXrteVVQHk6nikuLhju62lki47xwAg8GrIA8/PaxxUhPTYNPrqkqstUz+ykpxGJ/iBa/uPXb505+HGbVPNpmEMIZydnyuo0hJqEbFZp0Hp4qqB7uOEQBSjk2aecwGxN9NhgptQdm25IKIiZkar6BPpFBVn9exOKJs/OUi7ITPbTZnNmof7kXLLqRpWsi25mvmgpdZacoGglLLdTqJRBaRbLaoaVOFuNFBLrU3yTgkinlQ1pWGo47jrAoWkXcdCAUV37olWM8g4Tn52HJR9D3ObsnWd9p0EhYOgJDVAxuq1Chwgq3HWp/mM1ajSPJ1O0p3ViFGc7KLO5joMlmJUdTMfM4VIKS4WsU8K5VTq1SvzqKqCYq07KjFqLVXBaSrx6Ch1XZQEgMPogORiy73U91RFjBiSDxtZzON6U/soUbUYy2TuUCA0NbWZyg2EJwGtNWQe9TEAFZLSJmC1oBRll0K7csrkECjEKhYLrY7qZqJNcK4t3wajRnMLKttpGoaxlErAzI10Oh2q3J93fa+Hy+5wnhaz0FSJ7ZBXmzJlH3MtxSxRxWeLeYrok6VIhTLQyEpacRGmKCo+7yJBd0FUujcG7xNiUnfAtaVnlOBOcUYPGlApm2yJG6XPUygll1JVkVKzcbtblSBHez3ZhRj6GChwZ4rJfCqF01g0peOTs2YAIVCrCSBBFgGsuuzjaiytE5rmoU8SopY6rc6G2SJW02Go1djPlB5URQS1WhNlqiOqTNU8uwgODveiDqvNCHqttPdanNw51CoJTNmm0VQVwtjM2fTtUNarLEDXpb1FWHY9khTj4d4sxdClMOYsolE9hk40idPH0Y0Ccw0QsWG0LkgIoU+Ouai4QkIQUaqiZCjYsmUYqIgCEQSV9WaM1DhPbU4fhNL6rABdSKpCBAIpUwlRS615YJr65hIrW+1SW5ehXr50qEGmcWrNloPlcrVerzY5drNcqpubOxzWum7Q5f7ek09c/YmnlvsdrDBFHadaq6234/x8tApA3W0aBovJ3Y5PV09ePhwngzCISJCz82ELE6ILUun9fC5Brz12JQTdbtelFIUL89m6LqP2fYfAYax9DEOu8/3DnOvq9Cyp0i2oxihmtJqXiw6MEHFHrTXXTBefp67rtmOuZpUgECenD0F1O4y9o3pLiUAiqLQOdskMwiuH881UVSVGRSf7MaQ+DANOTuqw9REGEUDLiPPiBEtxtNQlIhcjkAKyU0VUII8oYRxrKa1TRydE2Iqd7UAFVdXpXVCwsTFLdlakGK2yFqmd2YSHp1O1uj/rpyypp4HS5ThNVr2KBKHUTDgisF5XEdnfhwj7pClhWDNEATFNdGtFHwEBIQEKlYA+qoB7s34Yc6dapPV0tPmrANFApWoQUPpOy+BOnS2X29W5D3k270KKIr7abPdmKQYFJ6FNUw4a6Ha6WonAnUHVHGZwYhyGEPRgf38Ypmo8OTsPMmzO1rMUK6IYcrX1ZqT7vJulFDbDePfB8dGVK6enp1Mu8z6Was0lSiCPtQ3oWxEoJxMJiocrUTk/X+c8xigkc3YBVIdWDqmgVo+r0Z2llBA0qOwt59k4jUVU2/woFSWpKlbNBaVUiJyttzvRCBCzlDjrezPfjMMu3xAEUYqYmzhyMXe//c7ajARZ7MFDzmay3k9SKxgAACAASURBVIAhxRjcqhMkgzAb1xszM0BVAVAgDgMEndbqbqg5u7VJCMiZZmxNcTpDFDcCEIWoikgKknqFwcmcXQV93+/NU5dCnzQIXe3oaqi1rDJYbF+SB9uMQ3RndEC8m4kERZNsySlzsy5cRnSqKtVh7qXQKugIoY2FILGjJ6eKDNsyTTVFrdVFpVm/pCW76i0tE6GqzhGkIvfxfFUjU+DYi1aRqHpt2UNkNL/3cNOk/U9dmt/0eHpy/uQTlx8/mmcrNHe22RzQEMpUzOuw3k7jUMa4Oh1UdP9gGVS227Ga0xxU97gZJwfX6/NqNUWVR8qV0YMG8+auEZCqAjCAZ2cn0FBLFYVKoHiM0tp2rQMjGgjWWulUFTpjF+fzXtGIgUGlZoN4UK2+W4qilNJ3adfBJwBUs6A6jjW7w9k65Uo1cxGkoIxKJ2kn66JROsCzz5Lvz7sQw9sPRgGmbBq0S2Lm02g5O4SqpO1k62bm2Q7etPf1ejSnVXNQmp9M2hQmeIUIRDSqilBFzIhMOGMQUkB0SeezLihFIYHRpNK3gx0sZe8gQawW1sooAgqFlEZSrnWyNipnlZCNRJ9C1zNEmHEcxFzRhBQ0rw2C7iSQUoq1nqp7mnUSIMKmFFmlgBpBIgQOq41DaY4yXVEZCSt18Bo7FfPBfCAX856CImFa7K/fGSZLZfQn9+K946Gns5qLdVHnKSX41av7qY+NkK4e7Y21lnHwLjgr3V1Y6wSrtZZZHwFPUYOKQGJUMRgRVVOK7qy1igAuAu+6RPqYs7boAEU0tkKcCncRjVFINfc2SwPKIEJncQddRUutdCK0khWqIpBc6jTlZZ9qrU00hwdCjBBVGimoxZwuoq2vQ0HN7YJxcQmq7joW3nlnOrrUtX52rYzOQpTKUpxoRAB392Yao7u18UVCwJirOWu1ZpIUERXStVV6Ke4kLRcIGVSCMnWh2QtUwmLRqyIkzPpIY7Uy75MoYgpTNat1mjyIR6/0AFY055B5JaVZG/JkIHUhfRdVjIEqUhNYTIhSm9AKVcnVQfFa21jfrKXW/MeyOz8iCAqKiNPJtFzkqVJcIes8WdBkHoOO1Ydh0qDSxRBUUy8qD3MgIRqPN9t/+/V18zxdOZoPw+SG5V5K8Oc+9aGTVd7enrSX2vvBcm95gPVk9269o6E73O/F/OTOarGI80Unju16BADnUGxr1dwrcO3waDtM03AOIrZa3hhjWDQvPCEKoTBSKYzcZU+CJolBWintUM05m1MkOEgHwVIMAoGmGNokjc123BklSYgsl31KaZpyKbXQBCJRQkwgNcBDEdeo0U2qm1cbs/zkM9dOTze5lL4PPC+AXzpcPvOBJ2/evrfd5mGsIEkxGnaxjJ3blRIIN2iKaijRzR0VIFyl66hBU9QuaVA5XZXFQlOnQkyTdVGLMUhMnYqUbDw8PLh6+dLpanWyHaN66vR8PdXsi7leOgjFPZbqEukuLOx7Saq1emAQMBeaIU/W9dZFKIKBfYe+UxHZDhyHR9cA6KBGbVlAqWYUddMUtU28aqt5kEIYEDVJjNFgUqMSgJRq1eLePM66YRqNvHy07+7DVB6erFLUg4Mr26H0XRBg0YdLy+7BauPFHzu69JEPP51irNm8lkG2xw+3qZOyXd+66+fnI4FnPnRpO0yYNom+t9y/uly+ff20nEsAYogpaQpwmJuNw/k4ZBXMNT1WZ0I992mteW8+g2p1aghe65hLqVnQOgKgUx8l7M26UErNOUuzYIlIE6t2/iKrtjO5OSmiXT/zWszrdjst5qzVVCUGTSk29cvMqUZWmgY0Uwka2z322JX1uky1nK1K+/3Pfeojn/z4x5cvv/ryq2+s1oOKmDu9pdIERVUIaXKKmZ+erFXFKSFwsey6rvX6nOJRkTqZL+TgUheSCsSLjBsUY0RKyxDVgmA2S33X33j79uBDiBocuTCpz/Z02ceYkEePtVILxWGBYEgxqZib9DM0B3AuPo4lLlLj3BA4FSYNXYTMmo2zOaWkSQBDUYRKspvNNdY23uPdViWhKhowbLPlEqMQFsEMUMAgIm5Gg50er46OFuv1KuesiOvNuuSx1u7a1auczoqzTNZ18Z3T4ZnMq4fzV6/fdhfp5PEnjlQZFPuJR5f3ZDYrLuPp+bAeZrP5sN6e3j1/cDpUc0AoPnWFoHlrDZCkCSC8k4tCKuhSz21nZm5TPtwdbZZsy6zJ6i4iu3qCjzpWoAYJEFGkEEJsSg1B8TYYEBAEVY+iHt19O2YAXQrzeQ+QtADx2DnL1Cz6whBBiqoKwl98+SUzC9DqtlhGgfT9nOSnn/tk38+e/9LXTs42zVPu3E3HMacQ1V1FVDVGdSIFWcw7CabidC/GUj0DM2eKMYgIjaIaZXYgC9FSNY9MEjVAie1m22QmCWhXUYgIwYs5FeYeqzEUN5cE2Q7u2yklUZUURGMAPEDEMQw1KETQrFepR4pQJR0hNFMvc0EICCGYwIpJ6zEJQKE4nSBFJQryNB2fbpTsuuRWB8ioquBhlAqem8GZ+iiBXdK2noX5OiiDpmF7HhSr06HrYpe61Iez8+3Ds9X9h8fzWd/1MQ+179PJeptz2TvY60TyevjUwXTSzft+vh7tIWuAqjey0X430RXuzKVG1X4WA8TJ8yEHY5JOtF0jImjmojYXuHlkYM5a3QXSriLVvosqaP7E7Tierkane/WdQbBRn7J9yOqmebgktEwX1pqW2btOFWK17rwDoNVdKi0BGvjUpSvnZ9uHx+fVKiif+vgHn3ziakppMZ//9Cc/GoK+/sb145OzXGpLB6k0cwkQETgF3qXQDG19V1vdIrpbE8jMQc0bR1CMHpQSRKN2yR15tkx1Uig8KBFSTEeLvaFODo9wCa5MKqpieRqjeLOeQ0StenGW7CHoGEQBVQlRnfDsSNJHCUHppoqoGum5ugBdr6rSUpSwVVWCLjRrrmiwZVSkNPM73YPKrI/boSqkdloL3H1JV299ZVT3YchmFMFjR/P1VNvM1JSkmr5zvL58sLx2dTEVVs9jzpcO94OiGDfDKPAUJSCuTs/TdugUL5yWTlHqdLzJ65KNQngQDUFLNaAJyCSoIv2WIDKkmqlqW4MJSrqoQlVImPvOIAC0XLutjtPa6qXEZhWjw2jNoBFiWx6grXPQunlga6GqgIzh0fLUQK2mQYK6VdfQ5HF1OpQkoS4qUGYbRWHufR9B+cAHnrpydLnrkhN9333y4x95+snHV+fntda79x7cf/DQ3VardbYaVdebrRVTtS6A4t58ywaIxIgOYoKkMlW3scRORRACUUGTvo+Lhca9mEsNsZhVhW5ztiLL5dyMl/b7XHS9nY5m89VJie6eBF0MU7FaW55Ld1eXoOIGq1VEQpBEgYQ+IMVIZ6X3fYgxmLuIEB6TmAdR7dSBuBuFABcqhRCy2XklF0tRF4s0jCWGKDFoU53J6nS6QkgaOZWqkNSFkE375KzTNLaZk1Mtq+0gCGdrU0UIcJcUdW/RDWNdzFMI3E8pRS3VVpt8th1KNRXpZ32tldS2tAWJGLWLUtxq8RCkd5pbDjElhWiQ5sIVhF2ZRndRhVODAhDutICmTLujegWpygq3QlXGpCnBCfPmUgQN73bvFNzJIIZ2caYgUKXTjNqcQxKihLHUasadmVvPfO0ZqZNuLknTOw9Pm/QPYBgHMz8+Od5uh+VyKbAPP/vBmNJ6vX3w8OE4DbVmJpl1Uoo5HRrMJIbdAmYEVbRUTJNBRIxQBzQoRKFCEMYSE0uhVcmsLRa2I+lyBmkcMWW7dnQYmx42ZtstyWc0IAgQpInF1SCCFBCD0FmEquyCEjIMRSV0vUJYCrZDcQcRUmJ1mDedGXAgtGWxmKISUtY2n8egSG1DiqNLy81mSEm3Q6ajn4egba6DxNQaJ6Aj9NL1fUol73fzLrpXs2ouKYYU4+0HJ/MURWQ2m7VZRX2vw5AhenBpyRCmUpu5VkVDCm3uTt9BHaYsk2nAwV4vDlZfKkVYzKNqjFBoc9DlWoMiaDSa7nJP6UKo1fp5P4xTC1Y3o8BNS2Iu5tWHKkHooDQPORE0Os3hMYSdKKui3ugcfUSz5FOETgm1n8VuppttyJniTCHCaQ4BAuRgb37r5t23btw62N/b39s7PjkZhvF0tTo+OfV796ZxqFYvX7l8eLCf81Cms5REoVHBKLW2hikUYnSxnWOwFiN3M5qskJHFLGf4MpVcY+cANaiKdtKplvl8HjSULE7LVmoh6KKMH/nQlX6+gBtEm2/EndVcdXfhNnNjUJn1YT7rgoiqhhiioHqbH8qp1Igy034qHLb++JW9zbY+OM1XDpcpibeREgiq88WsVvfsly7N3ZyO83VR4OknHnt4crq31JKrqHQpAuhj2luYmYkgpUDzFOOsi7X6lcN5NcAZVQ+Wc3PfDJvDZddk/ZLH0zIKAZFFH0g9Hy2XQvdqDgneBmgRDaSjmNdq7qYqYy4CqGiXoEIK+oAYZDOVICq7WXEga4rR3ISw6u1SGMeRhhgIh8puKYAuSUzRqjuihIgyiSIorJkJJJEelG7S7u0g0rotQpeoIc5CNQZVJ1jZdWn/6gyQvcXek49fOzlZ3Xz7wdlqvb/olrPu9unpF5//y4PD/SeuXRmG8XyzjjGtz9fjMImw5Knk6dKlo9XpgzKVWR+SJhCpaWxN8U9CFyNU2PRhM5i5BJZMDdqUs4gQADEJQdQlBJEuqM6W81mKM6smKtP0/1b1bk2SJcl5mN/inJOZVdXV3TO7WGKxwIorkpJJBjPdzPgHJTP9G5le9Ko3mfQi0kyiSIAEASywM7vTl7pl5olw908PHtkrPc2tprrqZBwP9+/mft773bYEhv3L/+ZfHI8bsySQSTF8OyzbYt39cumX8w7mMQazrE23bYkKVPIEgJnNlH14CVAj83L+7Z98eDz9cvnX/+7HX//yw88+3i2LMfF178S8Nfvtj58ftvVP/+R9M3l+vfyv/8dfC/G4nu82Pdnyq198cP90d9weH46n0+G0bX2MTDp9WI7Lend/WJdFVS7X/W/+9tPd4fCrf/LYWsNEUKdbmkBL073v+z48Yu/48E5U2D0jw9RAWbrFknhMVwWQiSQsqlztpLB7LK2JUPlAiZJAZmom5dW+iYXIM4loWey6e3h45nUfKvJwt63bcj7vqrqtRsTnyw6itenwuI5hzKfjmonLpXukKq9Li4SKoKIEivkhLg/cupqqmkpbGvb17e60Gf/qFw8BPTZxz589Hlfy7bRscmKRj6eNmUyFiNRkbfThL34ZqMlkgsbM1FprJqoaSCGOhMc083i4qtU70PtQE2FRFVVJYPQY4aa2bc1UACqdaA0fpvr8+sr//f/4P6i27t7r6mS6O2yHTfbdq5u5gV+l/wGI7o/b47uNWdzTPTxyHz66E7OqXHff9/Hubnu9ujDdHdpxa8KUIFNR5Ze3fe/xT3/18fHu8OX5/B9++9N5DxNbF/n8fL07rcfFmtHX13G+9H14BJrJ94+H++OiqtfhL2++u2fQYWvb2o6rHg9tNbVmS5PrHtfrRRgJEBmo4PUUZVVjpKiaike4p4q0VmYCjsyy3M2TpBJIE1UVYjIRNfaBZdGl2bq28Izbq1YIxWlbg7Bf+8vbpYJY1taOx6338Q8/fD4elr/45c9E9Xy+9OF9xPlyfTvvpvKz794RaB/96eVCIFWpn3CMHOHp2T08oqktxhyUTCQUoOvletk7QN89LqLaHXv3ddmq7YhROrHi0KiazXWxxZSYwtORGVhMS7FHLEQ0HVZ9RCQx1qUlyEfpHDCGJ0hFIqJ7VtRe714u+WZKN0dnNeiicr1e7e9/92VZV2SqiEeY2X71fXT3rHN+e+ORoHRXs+8/0pfXvfcRoPQoWYFH0vxBcbn2H356ns5lLo0Gi0gJG5nluNmf/eLjl9f9h0+vxOqBEdE9E/SHz2+ZMXrfexTxp6aqer7uGYiM6bFkMjMCbav+2Z+8J8qnESqSxO6+D0cSiWTk63kfYxTQZaaBFNyylMCsospC5ElAFEn/4fH04fGuqajZVKNFRGbv43zu3V2keIHivgMgK2HsnAap4iVKzxOByPj+493zq72dd1Ub4QQ6X/rr+Qrg9dz/7d/80FRBuFx7HwGAkJ4U7qySSekBphKZErA0S6aI+P796eF+XZflvBMriTRP9PMgxvncvzy/vbxcImPKq4lFRZnNhFkIGOE+gpEsHOWKZIoR7x7W02F593BHhG1bzITA++4klIEALpf+9en85eXsw0ekqdaFAHBrYs24NJ+gTOz71TIzIwgUlMLiY4To6A5KSipulZi5cksJHvGHT09MU11ap0eYUG6sSnqIZE4m5pm9zJSUpRBZ7f7UROz//H9+u/eanYAAMYnI8FCmBA13RNQ1mAGmRBAzvX84tibC5BF9JjjQl+fz77/gct6zGAeAp2CfEqgvVhZQMrOKnA4t9tzdI0JFExATAgHfNKLWRwao98GsI/xy2Uf33QeBfIQ1IaLWVERGdw8HaGlmZiIMQowYEULkmcNjNVEBiP/udyFiEUkio/twd49R13k61UtJWFqrSSISpnJTWaD8Y0zU3T0RmUvjve+RFIGeRGA19UDf91J0AlHyHmWJgCQNFktVbe6j907EiLj2kUnMolp1HU355fXVPVntug8C9VHYR9GJ0scQyXXDxqJizawwxmb88/fbj1/2z1/7cI+k3ruVrFVFSywAICOmNf8mrOZ5MdRQX38lEQVCVBkVQUCcxMo+AgQhEqFyTdY3URYQmsrDcTvv/vnlTIzRQ1WBFBEgVTgiql1QFWbKTOFMzwrnWUwfTquKjshL74H0kU+vl4qlYOHMFBazqs0qRCoChI8OpInI0g5rGxLWIKLCwoxkjrK4lQgH+Px8rpegwMDw3HtnEVN29xx9PbSlgSnsQEgFFWo7CoY1S2vMRCSKFGEZw8Xa+ToiRynucdNoZKQanVarB85SIXUw5SbiSBFWRvfiF5qqwfPvf/8SiQg0UyN6fuu9Rx+ppkJ87UOYM3M75rZSBIjTA6oUDlFezO+Pq8ppbXZa+K/+9sunp2tSIFlNWS1LPJrZ+/781vfurWkEjTFAtG3LGP7uQe5Oy2k7edfIUDURYuaH+7aYvbxexiBkAND/+r/7l6qaCWGKm4MbN3VMRS4VQCTM1Y02swlq35q2+pIJWRIw/w3PrJh6blzmUH5523ePEmOpGghN1cy8xAl+S3Aoix/xjSAVVV7XBtCnL+dPX1+Z+e60EfH1OpgYQDMl4qbCfGMiiJA53w0iFWaRy3U8vV3VWJVYAaKk4oBImFmaD+8j3VNVM9PU+vDMZKZmVsoKYRWZHvcSfgCo7EImiPK6NFEWEmZqpkzcPYene4rw6F7zHRIVSyECqgcsUr5/ImpGzKwMj7js4U7KtrX24fHw05dzMpuWXJaZ5fXSM3LdluGJQpWIRIKZhmf1ixUPCeC0rsZtW9aP704//3jIwJfXaxba0lRZ9hEIj0QCZo2Ft21lYjVOQEWFWTTN6J/+8k9++vSyLgLk48PKTB7++LCx6OU6SotkhWgTQVihZXabCRTF8HNpOnkmzM/SzlV4KIkisjQafCt6dTZLX1LHcRGuKaGuSUplYR/ZFs0iCoUJrCJixCKj54hc6vP7FrBC9PK2P71c3ZOF7o7bz3/24R/+8SdTBQUG3ZznTBFAqlpmBlJZhFlV6pv0MYSlNQVlRM7URICIh0Mojse7kZGFKjPXm5B1XpmLDi8XiZgAc+0MTz0EQKxMpUSHUIwktWUxjCSWbVWPbGtT0fLxMJtQgliJIVQ/GzOZQiQRUfCZCBnDlEVoMd0OLc8egKkej+3t7CqiizJxVGBM6Z+JQcmgSEpPM2ISIJuQGfvo4frpk9/frfen9eVtRPwx1mhZW1MZgevAvg9VvfZdRTLyGn1drUSR29a2pR0Oer54a3Lc2nBfFv3lz+6+PF0TFBFSWKqqemRGuEdhZhWcXK9ndbzlgyigqBi+4oBrGDYTUVWZ12RVr+JsmGcbOtVBqipsam0xItSzqFzACHfPMTwxdxzQt59hagM9IkFpov/lf/Gb//a/+s+JKYH9OhKZkcNTmPbhSEQEM1v9ecLl+KiJpHCMdVVhCmRpe6r8EcOHV0GNSFXxUXrGmSknwvrHQaCGAVQY5zeIJIGM8IiIKPOjqbiHj8Es7hHuACKcmEoyLoXDE08OCOqdrtfI4DFIhZuwe3lj9XhY3h1XMVGRl/O49mDmu9PhcNyAbKaqhW1TEtVHGpERtJgcVkFyEh/Xdjw2VWvrcjouD8fFjJvZslidh09POxO1ZuvaHh6OJrKuTVXWdTlsi6gmaPd4erp4hgk3k4h8frsw09Ladx9Ov/nV+2U1MzEmSkolYWFlSZ6eVdBs/4sHn5JGEFEi1eFMojRXaGXEt4aDmUSIWUAQYmJIuZ2Yi5+pzJwS9wMZCaaUumAIIMosyyaYb/dxsdbCghJUMigfH+4f3t2fDut+iT4GJbFIIyqY15pVkEnvvVkde6IpeC9RJqW7CCHAQkQ044l4guHuUJWiSZhpWZaMoBnJhFtTQXPFDLOKiKi7E0NZKCfoSkQgfn7rAC9LA9W3rfQQIuIEODHTIIHIgRnVAGUK8IgUgQciSVXujqsqn46LvXSU+zCJmXofJHrd92YtE5lBDKMMpA8CMp3PDGvoHvd3h+Nxu16ur+ddBH/6/f0vvrv7/LJ3SikTOlMfce6Z6UncBy7XrsrDk4nVNLpryww+HlszjSQWenx3ZPDuo3cH8cPd8vHhMPoQYlaW7p5RovBbd1XtDeZTnnZ5JiSLkooQU6VjMrHU23Nz0DJLsUYzQKU+lVuF+lZUSuCJRB2IzMigUnXLJJ1QWQBajSGImAqkNlNV/fnPvv8X//zX133UTHzZOxMVxjPGeH29jNGFebKQpdQBmQoAYQqQT77j25UHIE3rpgUSHp4ZFYtnqtbspuu+JcRMmAVElJmqoqxmam2mupYhwhPVOTDRdLvf7o2CQBOJyERmBhDu88+NSurree0RQDPdtmVd2v1xqQfVh1+ucdjW0+lgKod1LevxsrSaAZmYgExmob3jugfAzPT2toNoXdRUzrs347vD0kxL4FQK1tfLIBZlURMzUTNTLeK6bjWP/Pr8dn/aHh4O98ctE8+vl/Bs63Lc2v3d9qffn2pSIRCZaDHK7iFCCOJaCSXViyAZMvUsk1DLeokq+0QlM4uQEeIAkqDEyfMSUeKpwwI8nEhIJqhWfX4CQlJdO2rN4K15v/0VkVAhFfGMGB4Js8Nf/uV/9r/97//35bI7JSWoMSWJgEDrasIKSqr3JyAi0wjHs/qWAnCWbJ4H6OXtwrww1ZAsvEgmYgziaevib7f6rYRXz8YgZmHOuq9F2957ZmTSiIjRRW14LEsbIzx8pcWHJ3JZVerIVsArCIAnMbNAjEUW8Rijwz36CDktzFwJhGo2PH7/+dUj+h5qMroDRJxMmeVNJWrGBFSyk4AikyJ89221x/vtdFgo4+5orxdXU1VB5nDs3edLyEygzCxMtC0tPCL8Gnntw0DPz+4R96fl8fF0ufR977XN7uPH08cfNxvDTa21lpEsIpLTgVoxEDzjB2/ieNRHxCqqJMSOuGnPIcTCFKULToSQTCBEijQlYRMpu0dm1nifAVZEuLKAWIWYNcquWOIIAITiFuvnEGZi2vdOlMfjcV2XdW17H6fT5pEiYtT2fRwOzT1Fii8iFUmCiAj4piZnkRu6XLmiYDDZtoZTgClopCskovACqnppypJz5ChFkEw+nYUrcXOGC4kwUkTJSJsZkYhKRqpphQLJPGBeNrAqRQAzCKBMBuUIBDIHmJEJZHrg/rQSQUQ8o9nSmpkZU4+k1qyqLEFqniGezrxEAAwhIWlLM8H33z3A8+28b1v72fvTH752jyjcalnALM00M/d9BFIg7gPEwqMPJ06iPG3r+ezHrV13qMnnz69JUFk9criT04d3i5kKMUcGEYe7CnugaNxqhhIovQpLWS/qb264BlibZEAYQvP7gFJE+FZJeEZ9cII8UpFJpeS0YvuJqKlGRQaKKBEpF5QsVR8A97CmwjSjA8n66LOJMeXKRKS6tUlV1/VmGi3zI7iELkSkKhX+aHUVMwlx1tkjQlIfXqBpwIU4MdvQHq5aUrGbkQuAzGShKs6zthEiohS4YNractkRAfexrMvbflbVSBoRfd+bNdV49+7ueu2jXxPVhsw6kk71WaixippSJDKRyOPaXi7DVFnI3esnr9Bd92DmmVwJYoYzauie4JUwgHVtl0tvJse1eQQznQ7tvJdlL91DlUE4nY4svZqQIqyIKomIh3smeveH+/XyNPae7x5PlDk83s799Xw9bst2WKwaBRUlJrBkhoncRoHyYtdEAL6htB4AfPoamDhyfmy3CfWWgln3qgBZGYQkJCSgOnPIzLJY1YUlrGzVSaCqY12kJUtR08xkUr4Fe/jwuF3eoxJEaNTs3PsQZe9uzW66CWKRasyzZpcsLVw1hyXAJGFkSmUWp9fx4nEDz8xUxUa6zHEmK7q/5iSAQDkcZkbFfwspy/v37z5+ePzbv/90vjhzjym8JVVGoi1NWUWysPgxhXckDI9kYhFIchR3p0wsp2Nj5m2xdZFzl/AA0bq0IJgqM2cWT5PfWgEQRSSEERSA6sQ5L9c8HtbD1vY+hMmM7w/6dvUKRCLmzAjHde+998t135ZW+uFKxPPwCHo7X5l5331ZdGn69Hzeu797ODSVu9PWe9/3YZkQrQ1kWfNTICa4TXQTM9yQMYBIambOqKokxWoJZwYmassQYoCQYKnPj6owJKWxIpNVcTtSANLnvTXRhwnhUIEQnmCgpoECqT0YwPBE0v390Vpj9hGpokQwEyJW09p1ZU25QnmI3IMqfAYaGSWVnZz7fk22rwAAHElJREFUTQYVgWVZeh8CBbI1qyqYkbvvlCmmdAMYZ9mYT4dFhYkig1nS8/Rw/Ge/+fV3333306fL569/AAiIYo1zRhzSHt00np9fK+Zq9irgG9LMIiBijwwvmkFUeB9xf2qfnntbmplU+aeJIUJE3PP/Y8vA3PDFECYmPl/2RRdTfno5Cx8f7rbex8vb9eG0fHn1HpmRxNSsEZEom1kzZ5EcM0O19k2xICL7nh8eTy9v19fzdWl22BoRjQgVOR4PKpW9LZWuQ0wTh5woxkSU8I16AhEoS64ZkSCMPjIykQWViWr1Q55Zmk++NctVhW4DKTOxSE16WWfCVJqZCHvEuLFPmYhMU0HCi0SvyYIwRgxPgNR03/vw7N2B3PexD/fhvXciEhWuEHsWuvXa9fOo8La1+7ttXRc1Vuaf//y7//Q/+dWytsvlerlcM9M9EgjPMQYAVaF5DooQpdvkRZUuzUTIrDgWAEtrd3enZVkzYlmWZmLNIjIywp2IIkJNVK0ERlV+Cp2bJ4RnOn8zUWMEXfZ+ufYb84He512pQqK6NFOVovIqDFaZc5K9hKTwGskjI1/f9uL3fvr8kqCPj3fbZvcHJWSVkut1T6SPbM1Od0cR2dZ2PB0O28aixGgqKhLAy9tlabo062NcLn14VMTGGP7T5xdLAiFV9dtjuzksivEhqkI8SzCBWZlZqqqJLpoJ4wrPTSYIk+rMSq+3UivMmufkWAQIEQMUEao6I+yYImqnEAVJIpXZlN1vuDy40gOKAewjyoL2cHeypkV5EYtZnd5sS0MgOVW1tNG1Pc0jmWlt7Re/uH//8E5Mvj49ff700rv/8p/8/Nd//qsvT/8qnMzM3ec0zXXz3jhfzLoxoWe6kSHAzDAA1RaabV3uTscZOz0Gi/R9vyWC8zTT9y7rrU1g4gLdUpiCmNMBmhMVA3349TpU2IQPq1aC0PU6WL2phpfC2CtFu9YzqrBpoYYFMU2lHZBqPLqfr+P+0N7O1+F5d1x++fP7p/PnPqg1awsTkQ/vozOpx2CS4d6a7bszwwOHTU3k/Yf7H358eno6j8jjZiIK4Lq7Cj0+HM1URJQIEWCWREj1YjlxohuIhiLzuLqQfQSSPJTJQcpcyP58yAgCkZKAk8BEalzr8oSltCWtSV1UXOFjU6pKdY0WiwAgk0wrRbJi9ySyKmlcrnt4SNNlbX2ud0jJecsnsqnG3Hw1KXbc5JCZuaz2cPcwxlDSy3kfEc1YWR8e7lUlInxEIJvp3oeZDe+qRjfqt1BGYaoXYx4tglDpI2ef4e7n8+V0mmxJglRrmsYYI1VFa4XKLfCNwCbv7u8u+3697ktrY0SVIqIUs1LL1ZNhImVchquKmbBoYx4+hEWM6lGPXqonJiSViYaImcNje2g+/P5+NdGXt31ddbH2dtmXthzXZR/XfU9txsC6LSzifaitSNKmSByP6/UK9z6Gr8tawVsPD4fevW5ParQuWqocK4hhjlozJ+uW1ViWTJDQtyFzSshERUhmRvwtBIVqQpSJ/Ne3+/af6rqsDyn/qCKSioxUnSxYfVkiGWWWRGCCeREJQe1tIGYfIyKWxVTluC3DAwkSJUoG9zJXVAVTRSbXFSwzmZFFR46f/vA1kJdLBzKFlnV9eTmXA6rSTAJzXfC2rUTswzODpi0NlUFMlMoc09Cft3KWlPTpy9d/91f/4Z//s9+o8uU6QWMzY5V1nWqBEbks9vHDY+/92vva2l/8+tdvb+e3t9dtO+z7/vT09e7u7v7uJKrnr1/XRohMZVVpTXt4H8NdzDIi+3ATBSMDrATAA+4ggibYJDMJfO3Ru7cmyhyR7x623v2yj8f7gwcyK4NNA9l3J+F0EMNaGzGYefQhqu5R9kFk3h+Xyz723a/7OB3W1vS69zFwPJgqWxFE33bjMktmTHLm1kaCK2OdOImrZnnQjP1DRAhrHQoRKui80Pzi6lU4kirjhJgyMnLqbUQ0E+u6JJJJy+TJoIoMASVzqc2SmI0ZgAMZgODrl+fnr0/X6/L6/BaZPkJU0keNupNSpypj0yRbDV/xDGPEYbsPes5AJqtpRnx9eh5jXC7X4mZFNCLWbUO4M/V9VOYwKl8ECTAYkWAhj0l+oB4SMxE93J3ev3+XQPHCmZnIiJSK+xu+toWFP7x/95vf/Pp8Pr++vq7b9t133314n+7OIpl5uZy3dd22Q/j4nQ+/vNVoPDyZKALbupbXvA9vKh7JUn06mwlRmiDAopwJJCcywo+bvV365er3d2vv3pqq8PkyROm02deXHsQqKofFRN1c2UpcoK2t24rE0log/uo/flXhvzxsLy9XuqN10Yh8PV/vToe7o16u/fVtN9zKykybwi0z4hsaX8NjARLzHk2zRjzzZUrhQ4Ajpd50ZCaJTngKIOYUERAh5pEWlSppmUPYZo1hrmHtxsRrrTRRuQlu6p8JSPq73/7wP/9P/8u7u8Pvv7wxcWsKIiS3pnsfwjxGEKFmiDndJyrRjpLOb9f94qdtfXp6lhJBEv/0+XPvd3U6ex/WbIxhrRV6t64rUXjMAp6ZxDaPdc6enaoM16RD/P7945//6s8Ws3rMQJjZYTu8nc/MfNjWiDDV1trj48cPH79DZgLKkoq2LDXxbNumQkLsAikmgxFe0CuIuOS+SzNiUjNVSoCZ3V2lGAvRRGHKKkjSbVGZ80y+vF2bWj2kbbOn50sfXk2tu4vp9bqLijbu+84ipnLdexkaeh9v16Gqn5/PhDThax/b0hL43Y9PCXq8X+5Om2UEkWHKevgbz8NTd3ZbfcQMFIyKkoPdGEEoS1LkLEI5Kes6fzTXFs8ZYDLYQcTuocKZZGrEnM5iXAVjGnHdRZSZeLYUE4un2Tvi2v0//vbT8dDAWqucALhng2ammizrAve5nA/zWi+GNDL8Nf/63/zNu8cte5aDsNmyv12/9kgfxHw4rBlY1hUZalaYXGXSzqk1+eF4PG6tnkMt+kRlJZnW76zA68tzs0UI4T76HhEROF+uixkRu7s1W1qbgqMKjylmeCp0aKqHGARRteEjwX3442mp2UxVb0RQJEhUM8FSGB5PXdy01IMgSng4LkJ0Oq0Z6Y5//PLa1uVPvzsQ+d1pPb7Fj19falmWmpVTtW4GSq4QiOpN596dwO9+//xwtxwOy4PK15e36x4vb/50Ga9v/XQUU5Us2TRLKQyLC7pBG7O2VRWp+zQjQpQoStFQF3bR26o1zZBU7UHePhfOWYiqfE4k4JYYiNJBLIsV8oqYEZUJCFi0RkhkQXHKAYrA23W8XfvxuKkaE6lZ7VQWZoDHGBNYKba+nskNskvkD19evr5dTSUyROW4NBA1k548HCh1KXHvXc2mbIDII7VwEeQYdEEQcb1mphKJxey0NWLZFovR/69/9W8uvX/6eonMZVkqtevudFC1PsZhO3i4toobShOewW4VAT5hHAIhbwqavXsm/fh1bzbdCX0M8RThbV367gXZJFFmVA4kg1Vrq9dUFRLhfBnL1u7vlt7zs+w/fb2cL+PPf3G3mHSPZuoefbgl9j62bSHipTVRBchMb7vbS2WCHz+fD5v1vV+AbWlrs7drjq/jKenzy9WIWVWTkm4+1XoJ6CZFuJW0OcxXAM7SxB1qECJWBVJFAsGYtSeBGuxv42pm3vDpOqwZ67pk5lyr0+YNHqXwpxmurCXryCoYICZVrlewKCaAKIkbRxBlRmRrMgaJsqn8cYKd5PTMbqHaQODxPFK40nTwla7FYRwO2+GwRTFpEa0ZEtaau8/NOYJC7f/mt58r/6XAljnYEFREhUuOW/Z6NmMWDyTSjPs1mkYfYztsde5LQxt1fgFUHkUx/cROECJjgMiU9qR997/94a122ZppH12Fy/NCISXUpYL+S8JU0RNFhxNdrt7UxpDr7sfVbO5fH//2b7+eNktU5gMzOEExxlAGBJQaCISQ3AwiWhPd8Hx53S/Xfn+3ZeZ1d2Woad9H990Kv9TkpEr3pKmwrTM1P4IJSE7sBekxp9TCxTLBwhJTxXDrxCceQlVEiGr3EuYXMGg+UtxetGIOKhUhipyILLFxQfVMQPKI6UiQZDB55sKiTYihqkxMG2ckRNNHUd1UcieulRn0TfpCc3PcNwaEGMLCkdl7OYFBN+OCzuVLFYRIDHilTTEouL6vJIHIOZUZ5BNwSyybbJtJm01PDe8i7H3ghu5CmUCRM1STaR64BGqpAptUDoiJJOXbpfLyONxbMyZiBt8CSuZ7Xgw6V79LkwHOHAnKFIJ7fLr0MduYHM5fXzvxfMNZhMGH08FUkxgJj2hmmVBWVdnHLQUSvLv78KeXSwbu7xYV9kg1bijTQvWtf2SXiG4G4DlAMZeIoxQcOTexC90W302RI5eYjBNJQawkoKjdAUyL8k3hmCUrGqN7pNQ+p2RVCSQzr4tWwuBUuWXm3HZIIuIx9/3M5mXOtsRz/sLeXZijiFoCTYUZiMCgiKwOyCefPAtsHXNm4tJ3NCxLI+J1aV67IQjuUSGCQL3KU9de7gQSnl6r2+JYnuMCmLm2WEjS3rswt6aT1WMi0O9/+GSMtbV10Y/ff2zLxlQqSHx9evrHf/zDGPv1OtZ1MRmNuUdSUmVECrOazrWQTAC7e3GDwvSzD/cML7woEnfHbWn6+nolxghaKAlS1vMEVGWMBMEKs1Cph79ta3i6D2YZ3WmxmHtC+QauEjPeLvF67sdDE8bLS56v3kzLTGWRkLoDeDaec/JHwWWYKog6C0RiXC3hN3GaMqcKlTCJZITPWN9EEIFJqBgCigkvkJq2pmaNMFiYYw6UwrL7UOapZis6P+chA1Mkaq1UtY7CAsbwOBAlsJhGYlmIiGlMjtBUIqcFo1bGK3MQ5gvwbe6ZdPjsdvvu1qx3L42NR5jKPBf4xtFNAzULlY1QbtMOQEnQ20RlRiy0WGMhooZJIKSq1l1+Pp9/+9u9qW5bY9Xvv3+/v11S2Ls/f/p99jcCHRd6eX1eGrfD3B4cGSYGgkcs1qoqCKfZiswajLZlkbTT+7tm21//+98ujcKTWJsyUzk2qa7s0ccVtC0GVCZo9c1spgBEpbEB3BYUqSVC4Vm20xpvI3HpuS7eg757tC8v2PddiJam5h7MUVBksXa3l5SFCCVEq6tFSIVQgIUwRXqAQVaWv6LQszal1PaSKRwF0axBYFMRkxL8qzCaoUyJddCRfCMgKoZTmFkL7Pi2+4bMmCAiXFTNtrbW7JZKnN/UQUSsqpOIxFTvlnYnb/cdwLM3rhxdnis/t20ptrYuMGZzDyZ4hlDR0lz7xeQ2RtONs65m6Ns/1syDSKceIFNFpMcQtdL0ZuYANZPe+0+fX5/f9sNhWXN3lte3/vHxoKpfv17ezruovL83IiWkTD1FqghoZrgyoY9Q4YgcHib0wx+eKdF/eFqaiXDvrsrrqm/n63HVgrEOqzF3ZubM3l1NjdnLRCBCyPNlbMsyIssXl7V6KTl81IdVwISyvF3jF98fGHg9+7WPClgawy3nLcQ3lQxxaR648qkqqquyn7/VZ9r3XhIoAocmEYreR1alYWXScj6CInyOY6XTr2YBNCIYFDm3IhQ+zDwXUxBT6b+TUAkD1QoSMcCLqUjtkBOZ9a94LSampKwLPT2pdISJRFrdxESRwETBcOP6y9RGSbVeKDxG8dNVonyMtjRhykgmiAp8drF1905BHhPdOj7UTwxKTyAOx9aE1XSgbr36hYmZrtfx/PJWyOrrj1+Z8eHdIiIA731c9v2Hn17ckxjbcv/+Dkw0c7uLOQEHsomBslTpqnJcLEc8v12F6HBcLntX4aeXs0ceN+0eH98dvn+3PT7Y8+slYn6CRBjuEDVTz6QIFl5MK+US4alackvmW6MFfBMoXzv6wONdY/Zq3ImxmJqImlakj2QZGIlK2VfHj3AbQm+in1vLjNKL3nhxqtpDBIpacxxc7StVYMQ05VJZFWX+QcUYDg+EE0tEoEin+oIZ5vhtLGEWJKjka0ko2iTCSxReI0x4fTECKYEEig6vGljvOm7CsXkoCtejrMy8pZlquMv8ZcFL2yInzFwDXJSGUCZSoMQ8o/PKV4eqZZo0wFTi0qR2G39rOKmMDxBGRIMGZQLr0t4uiBhCGSO+vvYxHMR3R1MhEWpN6hMoikWEc8SFIgPWZIxgISMe4eXlDGLKbE3c4REvr8lCn56ujye7XEdTyVrYhxlGVpnILKyqDIyIZooMNSmtQ6G9iRtnXUtwOT3i91/2n304LqaPD/HWIzyHu5XHTIiSWXmyegX31Q0gInpTW9UNU2hTDT5MqlqdryTKn1NepsIcqTwk0wdwy2etmyU8wLdPCwiAMgAIixinz7s45mQ4d6lY0wz4VNEQKadmeBJnXWJRQYp1V06X/rRgFeA5/BZGy8QJBxhUwr4oYjIBgomSBcDXvZfltogKZLJNMkOtfBXMBKeUqCsUwULfLlMqfEaaKhuJ8PAkwpRdqhS0m4mBENF1W46HI9GM63k+94iIYk48//Dl/Cfv121prWn3AFGM5MaiXPmHAFKz7ozW7HLuSdivHUTdS2gnhGS6gQdwItmaEtM34Uxr6hEKZc5lJuCzmbJoRIYHOJNJRZ0cEwhHBtzj88v+9aX/4ruDmjELC0zVSsTAjPxWiGcY8/TD1YunZXtkNlFiuGcSLWYkbMKJmhI4APdbZB+xmgCVfcZJGSOn70R1jFtFAQ33IlvKi1I50FlDXbV1zKosbKAwwai89MyIpPr6hCpH+FS/lHDNsypms+lQLyWSRxJT/SJcpgaa16Ems7AqI9NR+1JRCk0gyo/EhWmXf4hyUbtdmqBvYqrbEF+viBBXKGMpfFSmDNczhWrFySSFj8fDdlhba2ZaOJx7f3l57ddrbWd6u/hPX9/uT8c6vCNCiDOjohgDULF1Ux8+PFjom9SvWH+qZAnmJOoDI7A0rcFqsebko/ZeOqRGu4HyV6vIGGHGkTEZ+3DV+qUKE6seQUf3f/8PT3dHO1+8yEbNsIgi3QlgnZMhl723Yt8I7KVharVGToe7iqSgMi9qujVT9wgPgKypqc6JYbIvwM1+KUzWlIk8KNKZyMwmv11IUcwqJCKq9WFnuRMQdN2nJBpJdfiFZAILUvsjUkXzttlkWeQGmCWDSn+xNFuaVYgXMn0MMl2WNZHuLqLuwSJVp1lECZH/v4wnj2SCmdUPWdULxFpZtjfIo0jD6ggjU5ggEpHVoowRpkxIM9F2PGzL4Xhc2sJC+7W3Rdd1lc6nUy5NEcFCvY+XS7DsFehUKFcd6cxgkvIkMws4KHLbjLgVfPBwv4Hs5eW5wt5l4rogwD0AsIhRRnJmJtiMhem6ezOZLoPbn0TMzQzIAsYYYJFyR5PI81v/ux9frjtArCrhXCh8ilYqxUxrEJECZ6qT3TY1s2Kww7NiLMystPsIOJycmHlZGm5GS7HSq5UJ7Y+tsdzyrU2JSEquNdtKIcQkHtSsTjwxhmfN3tU9gEWZ0UyETCsjF3Pqw5wvmVhNhNmkOjQwUfcYw63ZYV10LiAXgrSmrS1AuvvenSg9soZkNasPoG52pZmDnJn1tOSmd1UWMJXApObsw8KrijZh4Omtf3lzES1nfOnXmrE7AFhrj+/fiaiKZCIirVmlv3hma6uoNmXKGGv42N/2jIgqBwPoHjVhmS1rsyRiThPypHePD3en07730c/3Kz3c2+nXf9aaPn1928cQ5OU6TOGJKL6FpBmFZ9YmZyWdQH192sIitaOdQBlzO9EMBuFv1Cz97g9nEb15c8TuTpu2NoEGtcoEECJRO6yLmnUf6QBygPZ9ZxZTzWlAyYo+UhFbRKqKME1+kwiJShEusS5AScWmGE34ojDOggkm15WogC6uE8+zmUtrpqIRTly2ETRDs7ITgOhmoSzLOHNOywEBRCCvUd9kXVY1ZaKM2jpJ3aOPWgoWwb7aVvSzGjFAwpmZ4aasLMLUPRIopDXnQA07LEwCShUrQuy8ww0noeNm7epUw3V3JgoPlhyOWlq6rcvSlqL7WEBOifRIopw0YCqk9r5TiO29F7ppotQmee8Bgkd6BgBEpEc0a8u6mNlVcO5XuebxxO8fH7/78Pj68vb16fm699e3Sx/ByunF97Hq3GBfgAMnzKwpi3Bkjj5AtDRjIRUBJ0OAnC0wSWRcd6jBREQ53K21djgeVc1Mq3qIajNLRDoqEU5FgmAwF/fMPgZArZmZMqtO8pxQLsuZCoAk5umrQSYFYXh3z8O2UvGexLVR6sZuJxGxyGaSGZweIKHWtqVRw5J17NxZhM2MWYgGAWPQrUnADWhAob4sc+KNyN5dlFtbSvleiEbcdgP24YEKPMC2NYIUYZCZhKRMUW5cuw2DmLd1LcRRhJs1qktgllpmgqhmJohfO73s7oPWxQI3mlhkdr2skxUgqmmRwLJo+OgjzWyMPiIDZGbEOhAedOnpkU2NjRa2slgOr2GNRdhj5n2MMUbvY+wRHonzNX/49PrT0760RRDpIyKvA6+XXh8lAFEWVsEMpy0mcoRzSHGjhboXBikqFflABanViAceHhhOpsbq7rasW+0mGsNVzSNY5ZbmQgCZmWojQu89kTy6ipWDKObYMuVDk4IvmmyU0lJZBKXr8yS1pqKiU0hT7B0x3TzJrVmhWRHsTs14bZuoMgOpE++elY6JkaGEJI4pYmICcwWTF5VZ27gAGhGgXG0TmZLMEggwSEyJaBMBYe9juIPYVLikE/WYdQZdESGTtu14OByI83q5wofot9CtugyQRAoiYk8gIxPKsh1aeA6Pevfmh0SV+oIa6DxzmnOSet8TxhVmce2J3LY1M89+3nsAMEFkqqlIJY7Doz59CDOJiHJGbQAqcgjXfXhgWfH2dr1c9yr53kcfSUTLylR57ApVEVEzYI7ZVF5UurFFAFS0mVVOCohmRgrVEkUaI/pwAJFpz08v67ZkzideN3HRAXLr1VRNTcbePaLuuTFKcAiehnMREJkQJsesoixwD8HMQtuWlbcNiRGeQUykprhthqx0tYLMMlmUl6WpakEVmTfZPxHzXLRyY8HBVVjqYE1ZXPGKYEIGSsNdajZVYYC0DBoiqgSYqdSOkMlOMt16+Hl9fwMlMRe/1Tc0W8qYUEAvM09hAAgcY9RiAyUgmQ0kwtOYHfPratrPzIhY11Uqp8iDqS7rMLPz21m00gzqqdO2Lde95/y/J/cwOU0ACeXKriD38OGsIiRqJpKijMi9+74PUV2XTU/LyNe9+/Xat2UBc3iyqCBFhBezqdtDEjGzsNx2mxCBVbn3KNlVSVRqQKFG7hXNmXa9XsYYAKsxXYlISEhvdQNJotOJmcjiZotwpCmbY6r8wdlp1YHH/GjoW5TVjUicn9YU3QsLZwQx/TFNmGvCFxUOYk7c8ILiJ1QFpawjECiiHA6YIAfKUDMJEwBj+N6HiEhTYUFGEmnWqwFkJf7luPESTbX48qKqMm9yopqGE3vf3y77W6utaSICYZJqeKclE8ycdZGkiygVxJNW5lAQ1zbWAkfK7nA+n92j+HVRiUh3n/Gf7pF5d3cavTbPAQl3H71vsRAqHvbbgIIJLJUYghDhY4zSfjYzUwWTD+99RJyvcmaRSBRBhEwzgzANkLKo6hS4FK5ATCgPBBMj0XuhgfNsVFpsZtBkChKZvff/FyZIJTFRJmt3AAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy8y4os27IlNoaZzekeEbnWfpyzuQ+4IAqkLygEQgiK+ozq6gfVVleoJZBADTWEROlxS6p77jn7sdbKiHCf02yoMSMP9xvEno1FNnJlerqbm42XBfD7+f38fn4/v5/fz+/n9/P7+f38fn4/v5/fz+/n9/P7+f38fn4/v5/fz+/n/++H//D3f2PGKhkNhNFIgHAzAgIkgjKAZpIgACiVmZmBMhClqgIEQSSMNDMSVQIgVQkEJJqJdBoMJJElSQAEQgVw/Q+AhGBmgJvT6cZ1YAAEB51OwtavEwBRkiRIr0uWXAUCBJrHZYtt63vz3pvRSAJ0j/WTJdKYcx7znDVnZjJJmBndjKQBSCKFylLOmlUOdwuIKDBgDg95AyHCUKa0OaDKAswkqARlFqBCqQS4I9w9QBKkUKQACiXUTEkFEUAJKAiSsK4NJgowCKIgyki9vmQVKVQJ4sedrvWFgHVzjCxB60kDTrhbd5MwZo5RBRnYo/Xe9n657ft1367bft33bbu4e1bNMcd4PJ7Pb8fzfj7PHCqUNHN+e3/Gv/kv/3Mzn3O6h5uZGwknWwSNANe1udNISaV1i9CahbmZScrSrFp/P4AW1iIIlDRGlvL17Ak393AnPNyAkVUqilkqgMKUJBlobgCcRmdvrYVb0M3pQtAavFt0izAPNae5Zs2szFKVoYIIKFhuRKN/vl5++v7TH75/+/7T9dPt2sJNDlrfNrMgDQLNHsfxfrzfz8dDzzOf8hlh3lt4s17QETYLNY7x/pzjTEfrdg3EnPKOds3thn0HQ5am0ebTn/eaYwrJQKlG5pyzEiUJJWLrtu/ROs0NplIKAqqQqTzHmCWlKjGHVCqBxta8hdNAJ6yEUhXNKBVImBKQazCnIK7aFmbVesGFAkmDVVYKFEvV3G6bX1qr1Lf78X4/s2Dk5+vt0+3TH77/8ccf/oC3H4EfgT8At3/Rtn4GfgX+Gc9fvt7fn2Oc57gfz//3z3+OiBYe7mb0cIMZATeYmZuBRlAQyTCUkFmgGdHCmgdISZSikBIEUu7WPEhlVhVQBGAGwNwsggQjjKAHjMjSnLXuq0MQaAwzkKsjZgmzgiZV0IPmNAqQkQaIBrIAqKDSmAWk0yLQjN38sm0/fLr+8N3bd9+//fDp06frdb1FgKFtcIcIGMjrdb/qrTSe9f7t+Pqsd/gJymNEozNaawbcH8fW5zmk0w19a5tE69Wv2na1C4yAmKdNN9g8zpJkrgQto1cQkMlpFvQQXR70QEkpQDVTBBzmW5M4zzqfCcw51My2ve+9tS18lSZyDQITRRKEUAWlKckyCVmZOUulyqwE4DCjjF4zz6mqUq06i6CdZ4bxcomcRVrvbEE3IggASGD+iyI7gROYABHWetzz+V6Pez0HZ2ANNBEGwQiQIM1ICVKtpw5pCiBKUqmIOUuaZvZ6ugSBlAzILGkaUJBU6ypWP8MapkQIdAQNBKAyZSFrAhThhdd8BARUlkqpMjJTpFcW3TDn8wlaRmNYlTIrZ9ZIpBjReptbC/nmwWP2oTmlVfksmQHh2DvaBgZgMAM3wA15xc/t7l8OnaXC04OtR7dmpqo00EgXxkRynqQ3i2YRRgNUJdTEmHMWZs3JURos0GDW6OY0M6SKVmClUuKYJVRJmVOVMNEAUCVlVUkJSmYMlwfXy5glLYBBiOYwIz5+0qo6kVRqzhQkqApbRDhRZYaSV+UslmDAnFNizgJkQgFOzExUoYQsYADvgAMCNuAEfgW+AHfoMc7zcR6P47wfj/fj+TxHmMHMHTDzFiYyzIjiX++WQAG28AKNKEjQSGTOCAdJiHBJpEpUpZXcCa2SFQAC4AthUJVFM1tAjEa39edQknFhJ5rxAzvKjGYGyICahTTYqIlZmcgW8Eisa6UyBbMpZc7zaLPPzNnCb8/9cl7u4/TDnQz3fn3DfgF3YAMaYMD14wXNdr2/xXkfmarW2HprNCnPc9JgMGVBJCkkQrbBN3dHJjPHOOucmaMmcmrOHDSGIj4QFWTKOceUp5h4AdTKqpkJVARcrizJIIYZgtY9wloPD5lpIVo3NxpBwFQoSKWZU0VCElDMzKoaMwU4gICBIJ14wXPIzYx00o0SFipuHmZAYsxSFXyNAgITOIADuAP/DH2tcdyfz8d53o/n+/NxnrOGVAoD3Um6u9PMCDNCXA0IKhIAw4xmEqoSBciMcFvXCRVJ0WB0aCFMrKt0Q4klkNAau5CBZZUFEM0boTKwZCQIM5i7hxmMBglZ5WbuXlWLnlSlUjk0apZyUC1kgRagw14tuI6zJlKzVPW1x+2xbe+Nhqxs7lvvfY7FdgAADmz/YhBcgLb15n6doHsRAFRElUbO56nzKBSNkqtv3nbCM4XHcT4ezzknxFmVNWaWqliUyRAi8yyKo2ZpIAVLSHJl5syZlYQyrb+QMdyMQWd5Mw/SQENqVqmKrRFwkoBVZVZV1Rw5cqIWe2JOPJ7nHBNguDVjkUZUcc55zqwswuDWmgGokVqdwozSLK0ahRHoQAACHsAAfj3Ov3z5+ttznuc4R9YcOcbIBAATg6S/6JStmy1gYTKpAIJoYREe4TNrThAlyN3cnWvsupzmTtAIlKiCVCSNVAkqSVULocIMlTUBOLzyxbJINwkEXy/LYkxGWoQvHmx8DWGpqgrKs3IROAOjsFs0N391UJZolCorn8/Hl0eLYGmOPJu3fe+I+CECeyEmMIECLh/g4wQSiPAtQGAIY2CMnI/z+PY47u+zTneoB1oztBLwHPMY+Xg/7vfnGHPxqMV+159eUBncul4gLEnRiwSrBM2sOYurocsJp6ACZO5mHuaACajMnJo5ZGFRVkzRUJpZOfMc83k8R2ZmuTlgOerxnHMUClu3HuxhZarU/Tmez0mhuXezWhAKsDBNQchS5iIaBegDnK07dp/zt9++ffvt8X6O88xRqcrKRFWpQFqYsXnA1uTVggLrWQsCuNpci6BZABLMPXOuKWhGQQ43YwsjHdCckAsy4YNLQ1UA5TRJArOUSJUkrJkYZgqoVpfXzDKyaM1g9gIfqNK6SpI0ZoZ5TeVMUZgKo6++LyQVQXc30ozhYJ3P8xs4Rj7NWnu055xH5tvl3nsn2K439LePiXAHHkC9Xj1oYj7zcX+cX9/fv3w5jju8YusGE51VeX+Oc47ncdzfx+N+jJmk3Ll1B60SyjlghnKf9hJjZM74EG2gMpJmBluMB2JJmpLRRBgFIgsGLQD2UkBQVZAyNWeOMY5z3h/HmJNENHf4SKhqZirl4aTMJSgrx6znYxJiZ7VF/ORhJmUqU7noqeqYZx136w3o60Zpfvvl/evXx/39+ZhzLs1FQFaC5s4WsSpnCS0CQZXWzBEIs8CHzgQzSkbKzSAH1/BekxNGguZGAW6slxaDEqr44hKU0cyYmVlACTYLau4AzehkQiJfMhjlJiFUkr0KNksQFrJwC7JSWCjaQE2OUzQaKKMHzGlkOPbNI1A1j6OyRsks2uM4vty/3fZrDze3vrXPb5+vt365GGK82BMKGFPn+3l/nPcv749vX+/v96lHtN7CvUc4bZzzzOOY4/E879/Oc4yaisYwQxpIzVUJxSBpr/p3mpEEvQSkVAklAYDuHibOXDxokX2400yohe7NDEZkZs5ZqSzUrJnzHDMrc04PVqFQlQSkrJll9GhiyMHM12NkmZmRlDRLqarSXDTWiG4WfM7j18fX74LeG5Tvx/F+Hl/u71+/fTvmWaVwW+pnhF/79dL2Zx9RVS9+b8iqEvw1clYNvU6pXL56uVsRXiqtxiGQ1NIOl+r6mqavMUzKX0RW7rb4mF4cA/a64ywVQVIq4SUmCnCyQFalXu0MElykgSLhnlURmmlQFSs1TnS3cMrkRnKpfTQDocr5zEwBPJ/Px9f7133rl8ve99inl9+9fWp9CxasQCLnY55HHu/H+/MYx2OMo+ahVtasX9u2eUPVmXo+xzGPcc4600SSKFiSbkixjEUzNOvh1rx5GIyEUqXiyBw1qxZD9xYeCJIpqXJMZSYJDw8H+aLINKSkGmPUPColqebMuUamykSIkgG1Zp8T22atc9tskVyatWjNbdsi3ERm5jkqRfPFCeFm1ljMr8djssx9ZD7nsUSyx3HUTLotvC/DpV3+9ruffnj7cTwyZpZQZLiZmc2ZYEn8wGmrOdec4CKBwPIBlOIij6vdLWT2oTovs2GJ20tINzejuXHNijKp6C4zczczVhoM61dLWm1EpWLSrYofKjoFZdlyCLJEMtwhFGa4uS8mYWY0g7u3hu4GlkqrcZ9jggSzygrZGpPGxn5pl6ttF4tGmAF5zvvjPB/nOcbI0hyqE0gPeY++R+/WgjZH4ZSe0IQn9/ACVTDa1mJhD6XK4Ax3c5ojWACQVYXKyjnrNaQLEdHQXC+ynlPjzDnT3FGyxmi27BpIVZgjz7PGOVaVjjnmnFmisJ68iEoCZeS++b5ZC2sNhI1hvak6t2bb5h4UVj/T6mSkUZBYrKzSPOssgefSm+c8j5znLFWA5dW8Ne9v/fZp++SXP/olYubMVMQHeQSyKlOL4gospURWSWgtPqqHLnt9DcJgS4pdhgBBrfH7qjN+CDukLU4giNBC+O4ebvKas2RkLcOKAITKIsGhqdLMWoZLmCF88fhlYCBMCDrMlnuxnrG1zbpTUs4alhDPWUbQbH3nvvnlFrfP8Xbrnz/tt7ftsgfMgZTyfjy/Pu9jZNUSlGlqVtiabWzuHjRLszKfflUPI2J1DYrWW79szY0qjLFMJhOKciaUmJUTWUgpqwRywdEGb3SnFWAaKsxZVWhGEw2GWu0SNFTWeeRxjEpVFQloiUOiWzMz+NI/wjw6LpcINyPdqSqo3Nk7zEAXiXOMc+bIAtjCwymwEhLKirCZkqSkVai8w0fVnM9UhcPNXIFBTAANuAaWTUaGm6hMzsQSV6Uy+nphSJtII7FQRVWZvRR1AOKLnyyHFJqrmOrDEF2zWASrltyYJWEzunsL97CcWKaeEfM1hqtgVkpqvQVVmYVlWfAlDdHJWSXJmhnxQu7yffNti32nGXJmVo2ZmTUTLQyqxghn3/1ya58+bZ8+bW/Xvm8GW3zqeJ7H8zzHGHOKMqVZ0pIBo1uPrbVw982901uLjJYcqSOhLMDj0rZr780csPOs+3Eez1lKo9W6cSRqwpaOtcRbD/ctmnsYsFy7EgCYmZm502B8GYDKs5aKTRCiL9FRmkJRzcxhKKKMVY1kYwvfWuvdDXiOMWdlLmDCSk+zZY5VwZ1L4OQyp42UN9tUXmUsUkbgnkerSsmBhq2pe4UOvH95bPsX9BGrI62JWMv0Ur0sVeGjUkQVYLNqmTkFe9nmL7kZr38MxtXCSquq8mWFLECdxcp1ynwZUC9MDEM5skpJowpYqLmW3lEUINCNLSyci/4YbP4LMWZdhpG923Xvl6v3Rppy2uMYVTlSVaqRKlSv/RZm65vbZY9wFGYWUHgez2+Px/35nFmEUR5lVdYgcxG2xXbZttaiuTtt71XcRj5H2VROFWSbxyX6tm1gu7Vi3o98z6mFImBwL1hPO5duFbTwCG9hpJjKOescmcsJJ0CY8QVrjOtNq4TRKZmhORk2xlxSaJgRNLEEoxXhwa1FuBlwnnOelXOOc8wBLxueCaYAyuwlBdiCXR5mndZ8RoIaVkmkwmOHy41wKb2ao3PaOfLP91/P5zRv8ZHLUFbNmQsYAaSBlGBSrmfIRSkNJNyNUtVy/vHio25ueEUGREgpCsVCQlRKNL4sXFJh4UEzd77UIrNanLUcLgDI1Lqb5CtQYqQ58fLEmFiuC9eL52Q0i5ATRl12jyCI6eMYfJ5T4sjMUYLENqu8We/RI8xQmaOycNaZ55jn/TnPZFlEDzSDz6ILcraIy75d962tq0cJLhayMKU5SjMhosKJviF22Nx8mPwcJ2GtW9usfCbXu2lBawwzCydgY86R8xxD+cEUxDFnkIx1zwE4rXzdXHiYPAxEizAu+5IQa8BQLLgznD0cYE4SVlWZykwAtBejnxOVRUSYd79scem2mSKiSa6ymXicU6Mc3ny7Xm7hTx9x5ukFTUdinjnnuD+fY8xYw68qP9APRLhxNRsCkyaVmYczzMJXgTPFF6UknG7OCA9+4LmZJdWavxBeMge1PHLQLHrz5hFuH3WzXlGjmy+ACwL56righ3V3ElWoWq69qmqBOro7rblvzaPLmHPmzNz2NmfOqjnneUyBIz+U4UaRLXxvzWmcpkUslPMY4zExy093a3tdWuuWMY1oILxvcbts3h1GMCtH1SxVcUV5kKWpfOD5lruvlJBotKwaOcsQTnaWFZmAqFod2uEqlXJm5pTJGzAZpco1ISkn3dcQUclUkNLoHnQTjTKFLRWBpBVZp1AAFCQFW3EmrPZR7iWrMJLCh6zUDFvst/a2xS3QTTQ0WiRpI0dSma21zbfWPIFUdu9L6ExN2uEeOet4zlhBoFrGsgTCSbrZh4lthiquSJn5Gv9YnamWnWbmwVi5IoLllQmjZmE5V6shmRNQafW+9gEwP9QTvSRYwknZy09dmp8BFmxm0dzInHOIEmYmATdbr2IEu3vY+s81Zh7nbH3B5DFGjjGrpJVFadb3dntr+xbhYXJOx3Kl0/KJesrVNlnjdo3b5hvcSlYJM2vNvW0wgROqkXPqSKxAGfEShiV5FjGBEhJz1KwUVZ4nBzSFmTjhMpEJhwWcYKmM7B6yJXxZwMacLG7sm/cIk6tYI8/XWMGS3eAGyYoy0jxMVrSZQFk4mtOgl/ZgoNCCs1FKsyVYFjjcGBFv29t3lx+2eGt2BR0isnLWqcmyw7I1f0GH5n3zrJo5z+M45piSM26XHtyCC1y6VdUaYLYamSBVFqhyswhze8mwkhaW42ozBl8holffWq/NK0q37PAPnWNZiVpj0D9MpHoBw1qBlQIIE4uvvKMAOGlOWzfRrDTnnLOquUMAinRf85tUVaIscZxzS3+lJyCVcio2Xm/tctt++pu3P/7h06fLpbmhDGUQxgAnNKItezbisl8v2w7rH38Al+4HMyhRdeY45jFx0FhCUXQPc0snQtkxHQacGrNQ8jBzpPKcBRQdrDW1ghWkEebLaqe5OYPXls/zOH06fO9b25qs0uqZZ82pMinx8rzpgSqZYMElapKMcLe2t4huoICRuVTv5o02pZpmacaZA2Jr/cfbH//m+7+N20+IG9ghYk4cw2deYuxbez5PybZL922D1aX6/fF4f1SmCjDE1rfP19tsI0QAfBUKsSxbAiAyIZUW1VgeO5b58AIHRmB53S8ZB0W8nMflDkFrygJ4CaxLcgMIZco8M5nKFbpSIauquAZuVS1SIrKqSG9h4SZpQeEVgyVUUimrkvAViTlHkRUnRjY30m2lOJvhdtu///H2+fv9x5/evn+77N4DHkkla0LTc8JpQYuIrW1929E61pwSkUAClXmcmWPomDqe+Sgb3oIuyQxeg5XovqG2OmjQ43ncH6eZ3dpGr2Qx1813FnxVLo1yk1EWbB7erLlD0hY9s4zm4eacqlODSSQza4wkFRECSY9QoZa1ypIcEbZF31q3RlKzbM4TbuYU0Hafx4CSKEJb8z98/uPffvf3fvsJ9h2wYbW+KMhhBTayXa5vgKM3qHC85xiqpNR6m5lp5tHNWiyRfBWRuwEiUfkKVxRpzpUNecE4aYVFlvCxwnSgXhm6wuqL+aJHeHn9izSgqpQvreKVMatSsSRlLtdOlZUr+blMhVcejma0l1K8/FYb4Rr5cryASs2Z1XIMFZVZHKpCZkXzQHhk73Cz661//rx/98P17bpdWt9s29WYoWlMmkwWYdYstr1572gBX3lxQ658Vo2R93Gc8yid4hg42UUfZk5D1SrZIJumHVml+dvX53HOfestGN0GMmus9mtuK5fndGcYaGYOj1iDhED11oQisViBFXRWZpVWr9YCzHpJh6scikJ05gG4GGJXNAN1PDAzYUTB0PbeZI5M1HQ+b33/6dNPfvsR9gYYcL5SLRwYJwRERwS2K+CYieOZ53g+jtQAk6jVKQwuWKliwe6IFfdHrR9XSqxEL619cFu+Sg3LquKrq6mqXiKevOw1/yBpBQyWP7TiPXqpJPC/2ghrtoZzSpmVq92htJIaRopmdH/tK5QE6WO+o6pe0VVSUmZiqJCClLKlz3mUqbWYG7eI/dL6Hm+X/fPlemt7V4/pkMG8IIZBcI++BVuDv4Y7RCDXFeScz/OcOVCLUcvZKFmBaYaYkyzDRAnHHNIYOc4xQHbzLYJUyHMtPpiqKjUBhAXpFBzRLILhS3o2GRKepZw5R83nOJe2pyozLORKc2cIhqoli7rD4AgTCZ8yJudMHXUOlcvMzBg9rs6ekurY/PZp2/vlD7CfgO8BAH/B+Bk5AORIjwu8wQ10IFbVnKOO40idRZG69AbadWs92pEK+8BeK0idVSu/Y1x6fixV7CNlU/URzjZQlATnynMn6au3/fWsbOPKRr4KU/IVyVv60aL0y0RYqQqaBMlWjmPxVH+9BcsYfYnDi6bIIGl1u1V2TMzS0PTAnLnyHQu87zujxb7HvrVL79fYr37ZqpPGLVZnTq4YHLm45Br3+drbQKlGnSOF7GHhXmXP04ppgEksU9GmMs3Aypwzx1jmHhb2mqMs1XuQS8awmVP0Nd9VhOAIR3dzeMBXfhPAPGve5+M4z+cxsooCzCzZI8zC6ISjmDXJosNkcgeCxiHmPDFzas5SOqvK6VvbHB7VNg+zm1u93a7ofwf8BFyBCXyFHffjlxa93Rr65RV5B4AChfP5/u3Ll69fW2e/tN4bNiiLmMQAFM3djOEWHkCVzNfijxkkM3uxvhXRTC359dXPXuX0yumYvWhEMamlbfOlzvEVJVzRWXeualvONkRRDqpRWVkF2vrBSyZ3fyUwsuD+119I2loOWC49VyuVauQclba/3o/V8y3MyR5xu25vl32P3tkvdgE7zGEBFuekRinhZkyQMEfVq84kFHImqK1Hf3HvFtYlTQytXMUQU906O8c5147E1vbb28VoxjzP58y71rg0cGUL3bbWLYg0lVBGGixWWA+2Wkke4zzmGLOWCwOjyXpsEdFic4+qGjXnrJlFUwVac5gDfo7SUbOesFx5fJBebtmu3W/9evG9ZlkQn34AfvyIFgfwA/x+fRtz3hEbYFjgDwfOgcf59de//PLbLznHtl/2fWs9Suc4J3MiUKzwV7iHr1gsSq+gLI009w/wJOql88NeeSyu2CHhRveAzA2pJUoUa7UqrVlc0l+fumRSAb4Kxl/+J3pJbvWxVZVZL4F2FbFBUubLPjaaWS1b380o4SUC1zmnNV6ufd/aCxjs6mKL2KLdrvutbxffr77BO7DqzJEFZQ6MGr019B39gjI8J8ZACXCozL273B29LUdwuyx5dp7H4/E4alZEtDDAzjnnUcvLbu26dyeroMf7XTW2iIJDkiG82dbROkCeE/N1Z18odSGGVKUwabCimKoCgfDWW9/71d3HTJ3HkWM8RwHVIVm0kHylDnOOWRM+aYQhy3rsxQlLeJob3q7A9aNdrbMBn4FHxIp8r5DDgfeB9+N8Pr49vpB1fbtdrrfLpcPGmWVt2qa22W6MFxtcHYpw87Xq57SP4tMKSnxI/x+uOO2jRm1pHguNEhJoy5CDVeklK7zszhchBcllBa9VTicF7/TmlTUr51knpxL2qrRFbD9WF0Fzawi9DBiAzJSQEKPb/jkub71tvgTi3mJv7bJdth6X6/Zpv771S7Qd7ABBRwQwkUvks2Bgv4AXOHAQyhxzxXicXkoYEQFztHgR/mHtHF/GXaUt6MaRmTMf5yG2ti0RyFc4GmFwoJGmY5zO4HLPtw0kPHDkyxleAQwVJKddYjOzkTXmgMaSqZUvRAzRYabwCpYr60xUoSW9GRkAjZtp1JiIQkKFWfNe713tEo7P36F9AhrwBE6gAwbcgXfgqRJtAA/k0Fe9//qYc57ncY7Turd9v12vW28nStTQdJ/W5gzGylTUK/toNKy40l+nEhZe10vUgoNry5Awt3Cz8GhOo0pzJgF3KzVVEpypmcoxZ36ssUp8Cby+omcg3a31aM3MeZ5TJ9AhebLCzMP/aqeW1mIwHfaxbbWWoZAqFGLD/tZuP2z7pbXm3sxp3ePtcr1etr6122X/dL1d9ivsgjTQ0AJtQwSEduaoZAXYgYZ5Igtrl8EM4YCsbCVbXny4t6W9zZw1y0xbozsza87z/fEQR9971nXIznEWy7t5kxxnjZEF8w+NESDwAa8/cOgLQzjdZA7P1DM8HzUmXzdgbcvB5pzzOHNOl8HMwkGjmVuUpPJgo21ZUk1IKp/KaZNRuDjaFdgAAd+AL8A70ICAvnz98vV+vEszuGHEuGOOqlErImLRWguGixQwoRMyzqx85IySqpAUKdqrBsQ1Jl/qqpHm9sqjUQTdLcyiW2vR94huFiaopppb6yFlFaEaZx3nHOe0+3E+bc6p4mvdx/TSKcKu135525Zl4M3gZ00zosr61iJsnDXOzFRVwXxlztauXmVm+VQC8Gbbxa+f+/XW+2a9+7Zve4vLvu17by32rV/3/bpd0a7IBhDu8AACDHgCHgqwIQWfOCeexxhzdXuEvxoMgJmoxLYCUYU5zpFAhZtRa4H6XMksnb98SfHctiZmb+at0qqUc861OicCJmQCBSVWngMG/6AgeHk2LNChWUIBSZOQM8/3o4yWI8/nRLJ7TFERy53/0Mzd5IYWXmMJS9aMpM9pB1p9APwBfE3848/f/jIHXNs88/39/jgfBLtdmA0znEEazZq7t2bmx5HnHE89nnUMFAuc83jMWAJrpsJ9gfiUoV5L+Qvr0+gfi+n1UsLNwy/71i6+XVpstGCERfjee29rL5OZ9bifz+d4vB/bt/b+fjwfc56zgFhxoLUP9HsAACAASURBVGZG9C2un/brW/fmUD2fg6Z5ar+Eu0UYpMdzCsinBFYpnCADgLGIGtOM2xbtEte3dv0U17e2XdrePbxtzfsrVmHNo/tG67DAMCRgBrMXdCSQxSLOiS93kDjn/dtDwuV6gQfcoQkWMjHm+twAZK0175EqcCX6TalMqZrDyKzn10c+0rburV8+1Js8q9aKW5mQgk7Uy4MHaBYLKQNKzamZmSrMmc9xjDGyChLdUsnMs5BPacLLQdFcsCpWQlTAIlgLqNBdeyVXihkG9ETTx27EA/j5n/78T7/df2V5ThvnPM4JscfWG5t390vQIYRIY1Udz+OeB1zTzoyasGXVP94RWNGbFh8pVkKVKpRAa8Ewh2xW1ZIEpQXM+h6XT9t2cd9su0brvu+xbX1r0XpEhJNzapzzeJ7fvjy/fn0+7+f7/Tjus6qie29BUqW+xdt326fvrr35mOnt4UGlPOJyMRBzan8O8lEF1cwqwMNfizApuZFh7RLXt77f4vpdu7zFdW+9h8OaR2se5j02R2MZBJzCc2AKcwKJG3Amnidy5phU2XEKnCOf57xu3V6x9xfbhiwLylKOZhO9QQZaRI/OxZdI9h5X7TKdSLRqjXv3HuzNQTxS0PRo1+ulx16p83E8xuOZz7Jy961tm2/NWaiRx3M8VVKxRr3W4ATSwt2CRfGsSVUKBXdrzStigObLnQaZ8PJXeMKQqEKERbPWHQDwBAbw7csvf/rzn395jqM1r8mcqmJYdN/3uF7b2xbXoCulOcfI+zm+Pe7nmDBwQ+wQeTxdU/c7g2T4CiO94hdZuT5tIALt4pdrN+c46/F+Pt7PWtKHcbv16+fW9uibXz5t+x77pV/2aC3CPVo4TIBS45zvn4/v78fxmO/35/Gcay2vha1lk3C/vm3X6x4R53G07p+/e92pfnGwzmO+fzvPp45n5RSTEb4+YMGNNCkiNttufv3Ur5/79ZOvum8W3S3ctrZf++USe/dtQ8c0HOfzPv782+mOHvzTz/f/4//+y6XzH/7u8w+ft8u+bT2q6jFmc9u2BucKxC2kiLXCb0SVaEs7bN7MjMgx124hb9drtDk1u42K2rf+ed8/X690l5IPNu9v+6e+X8AwzTnHt/f59XhMP8x5u1ze+jXcwRrjeT+eTACG6VVQMcytwboYNGFOiSWje/S2R+vZ3GHbvl/3LQJzPu/HOGeqckLHUJ7c5G22McY5vvSWgD+/ff2nn//yy29fKyvWFjlDCm8R7N33S9svbXMPTR24H8/j+Ty/fnuMka3FzhBZMA0+HvX+9XzZ4/b6NJ5a23UR7p37td0+t8ttAzEelTXvD1UKru0t3r7vbz9c+hZ9j77HZe+XW/Tmazz1aL2F0ZUaIy/XdhyX83k+j+tKgfpaexdocHc3ixZGOw7fL8uxppn6HlLd70cmtu3ct45ClYyg6M3c4MTe2/4p9k+xX9vlFvvNPdjM2lrq8fi0XT7tny9xdTbAceq3X+7/w//yH//xTw9n/fzrl//rH//0559/m2P++MP1v/rX/+o/+1d/9/d/88Pt2qLZFo22BElbn8IAATALYm3rImGGiH3bH+fxfj9Y6c3cbe8RrU3OilBo7+3zvnO7IBpnfvINbPAG77BATdc87vV4zOFHxRw5xja3iCABRbnBlaxi8wgzRrYd5SXTmDNrFoVoZtEvrW/7dr20tt9uN4sOnO/PX9Pex32ec4yJM/U85nnEyCnMLPX+MPn7+/N+jEqe5xzI8K03VhndHWHr801e64Z5jvn+fH57Pp7jGBPRo3t34zGPHJVjznxG32J/a9bM11pbaSu/XPt+7bHbfo3t0ox4PmcizxqquL7t3//x9v2Pt9unbd9b7xHNL3tvm1lAKBjocmc0c1hL2y8xZ47Rx6w5J8kIwwoTmNanjJi5St4wM1CgsUdYsJQ0P5657+d+SePHppRg5gx59+3Nb5/79qm1jX232LhMaQdY6BafL7fb9Q3xBut45n/8D3/67/6n/+ef/vJ+3L/++vX9n//8yy+/fnk87qj89u3Lf/OXb3/70//500+f/pN/+MO/+S/+09sfOligXiVVWlUFEtFgwHG+XD8SdLMOLw8IOQFvRDO2hqitB51wIjrCsQnlgAEGGWY+38/jPh6P84EDMSEE3YHeL5fWvbEhJMtZQk2O9PReE+PIOedKC0OQwrfr5dOnz7e3N9gFaICA6a7SHJWPcYwn74+8fxsUPmsH53HO6+Vt79sxp0jzVjxXTnlOAkLaPHP4OOyQps57HvPb43kfz0c9T050wmVNmXkcxxxHa7j0Fp//ePn8w8Xd6ITgZG9xubTo4cHYrG9m7v05ZIUmCbdP29vny+1zv7719WFDLbzt5sFiEWVhHrSAmYxozhJtAi4TWraPXOxrf05iFTQ1NJPFIIAwi83NmBPmufD87TZak0q+SgyQo11x+ezbNWJndFgA67PPoLXKtbd+6RvajtaR/tuffv5v//v/9d//h9/C7f7+9Zffvnz99v7t/YuvsDJpGsfx/N///df/8X/+337+5ef/+t/92/2PP8AaJJwGDFjAA9bQA5UYA7Me5ygR5v1yKc3UuQKf1pxdy8wcGlboOdASCNBe4kUVHs+vf/7119++HMcYU6Bve/tuf/vuer3tl9u2974BtjbANcaZw8jhY/IcifPUeVIZWan1IFu0rcH6x0LvAGbqPMd5nqMS5zmO53gc1WnHIyGcp4yne8DRt9Zv8UiriSOTNQzl9fSX8z9srA3jGqMOnsOP2Wd4Q5/wNAiY9NyjBa/xw9++ff5+h5GGoG8R29b6FuFWkEzupK2I2/X/Y+pdYm3LrvO8f4wx51xrv84591l1WcUii1Uiq0hKNEXblPWWLTmw5BiGAbsRpBeklzSdfhpBWkGCNNNIIwgCGIYBI+kFhgwoMJlYVhSRFCmKFKl63vfjnLP3XmvNOR5pzH0obdzGwcW92Dh7z7XWnOP//+/ngeA0bvNqM65XeVilLoMihUWHdHnKXJiJg6SD1iwCbtFMW2hPUgUotGspPYbHpr5U06pd62SQujh76r47CkoyrIRpcBMQ7cYxSW7NnQNDyMrzQFwIMA2DBzGEiEhKGjkl9Aef1sPD/f/++9979GxfOIT1cDxcXl7Py8wk8zKXxOHwooAlptb09/+v73/zF9/9m7/9udNpP+buhcKQkAqQwBXhten1cQnwaj3mIVmEhpg1I/fEKVGwGOncWiPdOhcwOEAFBphibnV/nI6HZZmXtqhqWQ33z7b3zs8vtitZrTCUkznHFXONptUMhcCiRrVBVVwzdxCLAAL1alDA+goD5ml59XL/4mq/r0uLRlphDQmC4DqHq4kks/BwyZKIRYkyegqUHRxx9BkBo7bQTKe4LAWhiWNUVpWBUjYpxo1L5pzXm9UqItLFvdV6V3BC+MlYxlI6Aw/qttTGfWkPKQ+SVkygsk6lpGHI3TYMRpAv6h5m4SNSSyEA6ISlCg+LMNOlmbt1HlyfIah7H5uoeWudPhKuRsTCnDWPpYgkh+aRV7s8riUnZElnmxEhTd3DFyxGytkDXqtq+I1+mrMMnHKITKobPu4vD3/wh588frqfDtfH6XB5eX21Px4Oc4Qx8cV2rM1K4u16tT8sAZiFefyLf/3v/uY3fx67u4BACM4YEmQAbgETMGOp18dpP9WUyy5xGbtLy8JoaRZEwplYYNHMHVCKEgROSBkCLA1wQrjrUpelLTnJ7d3u3u7iztkZdhvQcBqWgsCKAq4LLLVoFlE9tI8HKDNboh4h0qbTUvNqIODgsby6un7y6tlxOSyzhkMXa4uFUSJ27cElmHptbVFhYKrLXBc3t7DOp1A1dQNCRRcQSThCACJyIiTPgzNV5NQ10DQQs+Qha9O02smwSeZakpTcR00SCDMNOElIlpSImCHgRGBI5h7HBXUmx02sEo5OlWlIRLG49WmIhbqbmfbo6im82e0VEUHmMDfrHrLOhgwI8WoczC2lREEksT7LibkMvCplPRYCm6Jq3S+uASJvqsZCIEmcpZScSxqYRAl7q9P18vHHy1988Pz5syevLi/319dX13uGv/3a7c/evxOABT17+WrSAPOx6rwo4L/65XfeunfrT/7wT7/2d78JZAgjF2AL3AO2wEegERf3l4cvpnkZmZq17BHZEcaIAZKFGcxO7rJmIZZ1XqGsISsggQmrDOLcDCwdCbAu+dZ2c2u3xXYL2gCnrcBpPiyMlNKQq5lCiZlPYZTgyGFVTad5QVRmNTuWnM3s5fXV1dWhaTNz085RQ2JywC1MHRRLCxzMpbFgXhYzdwOMCAh3EgrYZEtdFtJuBO0+ErIgThhYHF59rj5kZMnUQic7zLMmJA9qgDsYYItOZXBzBYNTSN/aBzEjFWIRZuQknACHAUxhahFhYQxo04pggFB7QE1Ne6jdrLk7dWcFyL2TXqOqKU6GI1O35k2NQeZq0BFDSUmKDGPKIqnIekzjWBjkCsw+cE4BwET5xKRMLCIl54CYhZodlnm68h/8+bS/PkR4hGfC+2/d/ztffee3vvH+2Z0zNL+8vP6jP/vg29//ySdPr2B1XqZbY/knv/71z16cNT38T//D//J7/+A33/j86xiGG3kosH+O7RsY19n/TEPNluZJo3AEkydiSEe4kAOJkzBLWWHYgLfAAMgJVTcmrG0Yjuv1qjHGQaQTK3vIHw3gzizrw+QQuINA5GCmlITClUibBhwc5LZUI7SlHRMnA/aHeZpqXapHuIFBAEkmccBtMW2LK6G6VKssp2iSVwKIAikxi6iGky1q1k6ua3cPIoKUJLpWkYjiydNAg3ksugRSmyOZ1XDyMHM0DUBVxc1BDvIkCegQLOqR0MTdYHuSCkScApKkqXZUSLgrcDTrhp2T2ZmQEomQRXizbvfRCDOYWzM1dzAjIgJNVZsRUTJyl+i2jtSBE5ESLHtDPcV42PMo4hyuKWMVIOkWDSZCa2HmFjbN9clTO1xrXY7zdNwk/O6vffUf/e6v4N23AcfxGlM938gXr/bf+eGfT/tXcBqFf/UbX71/52zcjOO4vfo/fv9//J//xX/zz//LNLwHfAJcA3tcvsJWgF0ijGsuI6UxkBQMkENDm6s7C4KRRXLK4AIegc2NRA3AAIHIWPoAIqWBhjQ4hFWRlptl/TMDhTlZi+ZkfWtCAJETnZ4NgLOwW5urVTUmqc2PU52ntiy1T/6Ec2d9sXBks8A0mVdoxLI0JkkABOZhCEmScgKjwx8DsOq1uVrUZq26G40lbTZp3LCqqSDz1EKrVqZcj5F6eC2xEIWZEojg6BeSgCmEuzv75BUkdBxjxw9ATsADQhLWaO4WqE05eoKCWZBTN3SEG3GQwsMY8B4FNVPrmEr3k2s8jCkkce6nOjLvlw5V56zs2jA3MATOrh28QCmVmxwAiVCATM1Dk1MElZS0xv5wdfnqRYn6H3/zvV/7z/4h+H1gD7zEugANPrz5pTf+i9u//cHjl58+fvZvv/OTs7Pzqv7kyYv7X/zMWw8e/Ml3/t80XQHA06cYKs42mGe8eokLnBWaNqv1RtabwaKpa3THqId1QA9iGDI1HrlhcEABuYFeNURFc060zsOYJZW0Xg+cBmggKqgzHnvyx05eN3ZVU2tqxjAPJ4qSmTi7dcucmIU1WtRra21xV7Pqap5O1g2ULE7BRpIoJT7M5ktD6JDyekxhoeboqaiBciKFuXa9gairs+rHfZuPth5Kke0wiDKmWKZYmlqzhljmg6fOR+duhaaggAgAJnhKkrNkoW4eJELqqoGGU8BNmJmjJxkoAKdw9E9YI3IIxE+WHfJT0okAhLlGSHeqBkL4JEUwdUMeuWDIaRhSyT2oGA5Thy4NFR4BJ+HEkD6ISCIOBnNmcGZh9nAwFZKOdBAXbdOL58+8LX/rnXu/9o9+CXwXeA5MQAY2WCfICD2mSO/cu/PO3/rK19/74r/69g+5jHce3MM4jtvddrVCcuAJpqtXGhc6o1aMFwBkt7o4p/XFGXAfqMCVLi8v2zMjuLlRALG05kriOdOEdZcR0+k8uDS4JabttmQZKffvBNFUl1a9NTMNC4DEE3MIqVU1baatNSKjoMQdXSORyENdU62+HK0tVhvcw5XhZA0aLRIJ2AmcKQkHuKVgtmWyCBdYbQSK1iwlpsIcBHCidKzNag98EYW32lxdggYeTqlLiSBv6q1pbRrOtVqioNyTnT3nDhIREDGllJB6xFLI/BRV6kw2Zieim6i6A+zqbm7NTQMI7zRkBDOruTtDYBHeWm1qGmbWmbpqQUzdmcypbwVESEoZUpZ04/ZWMw4zj6aG7gRlFUo9+9aUUxL3BAYLjHqM2EXo1u49YHkaH2y3mKarr7y++qf/yW/itdeBA5CAuzfu0Kf4yaNPPviExR986QHO1tvPfebXjlwjLdfXw5bXJX/5nQc4C+AZoo054ckLeGA8B2bUtr54ALwOAKjAnRSrSRfgktg8mMFmMG9i845FBBj6/czQZsyLm4F9GBLGAiI0V22TNY26WK2mGkpgkShF2MVg5qZuao3JhbsNghiAsFqCeJ9xCFOiaOEinFM2xbKosrplMwixkBhOh3RCqMeyqFkk7gc13/AgIomkqusMreHknCAiY4HnYMh2s9qsxmEEJavmdTFVa9VNdZpaggcjEgsYHRV2etwxE3tiCDpxDxYUbohgCvIQBjt7WGgYrK9fbR7odn50O7apRRBgHRit6q2qm5mTW1+nwgIAnHoEngYW6bJV56I5urDfmyRCEQgSZr+pYfDaQ8gs5EqNoYZbZS38xqH+FPgclqeED7fnfPe19Zfv3cLr2xtb1QXAgAKXj/7Pb/3Rjz8pPPzOL7+Lt97Cfg+1z33mTuOyzPPxzz5YtL339lvYCFABGpY9vnAbWOHTH2G3xsDABhiACVgBb6D+IOLi+sjb1b6UEBcQXNHCjjrvYgCW0zxsmac2RUNOJCnBK4JU7WqaJquNVGHmGn2DlsQBOgEfTE2tm1CDhJyJ6SYK2/3LvSCEGB3zmhKRBFIIgzKCLIhFJAEnel+EqyshFFQk3IlBAemcWBZtmA5u0agEC1NIZsp5XA2rYSiJtUHr0kz7qTbcteqSYBbNApSJERTudEPHkADZz5zWTmB4wEMCTJyCMycP9LFKa9bUKLhr28FBFCwID7MgRNPofMFW3dSanmyCoEhCnISZHcGEYO6lCgF2s94AghNksp+3WOR0s0OPeXo4q7VojFichGX4DPBzdPkj3PsUtS3Tsr1Iv/fbX/vqN/8JHn8HeYLcBwh4CtQf/qt/++efPvv61772oAR+4T0g4+XH2B8oZCw8If7ipQ5JHrw2dBwrEtNVwxu3gR12e+zewq7zlAUYAQYez9evjovWNjxf/P4t322GImLmapa6yTcqADSrulRTYgQE3ly9NZ0XvZynyVtk65ACdBIJQ2FNrXmbl6W2amaIMLJQCHe0jvccmXeUDnkwyppYxIGkkSvcIxF1xjK6A9Ud4Rx9i9wtqZoTJ06uaEt02cLhc6t1bnlFKSUzCuMerYpAM5vnZTouWsNU3d3CGJG8qVeNnojmoIDDKTkHEVj6rDXCA6fxqjmBcpLCuVAiFg2frRK0cDAzJyYOhdqJ6UWnep6wMFiDK0xZq82LGgBQLqkUdlXiTkJgeGgLIlUzRGc+drUfxCQpFZHMHERu6kFEZBpMsOYhzsbAHni4vzqub3+CttbjIhu8//4DYD58/6PNNx7gjACgPqrf+tGTJ0/eGO3NXcWb94CC+VMcDshBVWFToTYM4fCz3YAwEPDG66ejAxpkAFZAnGa2EOAllhfjG/fkJx8dD/syjI+eL2OS9VnJmZopsXdSK8xr06mZ4+Qwawa4zbUdaz20eUFlQZLuynAnUsBVVduytFoXNQt3JnIkkFI4MQXUyYm5oyQ4Rc7ImShHOARUorQaCLATE7SFqmr0BBCFYWmeyMIYHpJkntSZDTbNrWmttsyLBZLnMAvTQNK5tqwK0lrbctRlrrgBYGu1FC3CQA4YvH9VFuwOkYjQOPEZvW/TCckTCDnSisdRBiFp5CXyAg2PlJiEnLS6TDa3U1UCEZid2MOVTNGT395I3T0IFqHeGCIcWRDIJ4pCmPfCqIjsJSfJPYyNRCegsjvIeq6SjIM7RQGKwysMZzYbjkfwlpoDgUHgrx5L/cxf/OX4hYIPnr364JOL9z7/a1//e2gT7t4D3gQY6Rk2G6iRTWCPWBLNV4frzdkD0E3U52KL509wZ8D6s8Bd4CkwABfAEdNTrG4DZ29/9vDw0aOjNknpk+e6WpX1Shi2NA8YeWvqrapaMCQlrta0LWo6L21elllrDS0sIdzTa2YM9jBvWqdp0aamGo5EsspCJOTsHsHJochm8FNaiNwAIechJDHA3KxN4W5mpPAKV3hzN3fi4NyHKFFV40g9gb8opnk5zIs2BcLUWNgc5j7VSHPwMaWhb8ZvjsgOd64LElmSEHKBEXVgMRMgHoS+/jxI+n/sARQIUeJcUDZ5LZSaWfLE1ogjCZOQoSFqdW0aHtFpveRBJhLe+nzWGB62RATMEA0ixJmDJMBIiZncnN2iU5RJSDg5C4MawtwZZmjm6mFBzOlMVoPIZd0H4vqw321oHQX7Ge2KjhRnjGGDZuObw0/bIX7/j/7Nt3+0zMs/f/czOP88cNVDRYAibXEeuNwjNSDUzbxdH64ubg031n2ALnDnNWADbAEAb9ycAF5itQLeBLJkef+L+z/70UemuLzaf/hk+Nx9ArTW2tTnVmu1cBKWJK6BqvXQ9kud56p9qB0UZN4mtKzCFL3VpDU1bbXWRU1NAKaBg4eSw4VCzKxR5fCByeDq4UFqGuwiIQR3c/cQsohAzGpL1Wlpi6oBqUgi6vq2qwfBI5alWtX9dJz2zdyTpDJKGZjVGsGsztVl4rVwLlyy6MLzEmoUjuXgqWBMMbLxiTgWJ6qgq/dAHIJ7KoZOCXTKKRdaFRqECzhlV41I4SDKnTYUYqBJLaqbR99ZmUE13ChHauawFgv5DCKmSBKSIEkkeRooFc7odTshPQzMDUTsDlRweIcnqUUzU+8QVv/c598Fb1785P+urM9t3k2HcWG44LW766dPmjJwjlfXV7M+X+aHdnn/8+e/+uAB6hE4B4DjS7z8Ht64DQ8kQXNI7tfZs5evmk98sQUSUAAB7gIr4BJ4AqyBcvP3BtwGBqABw/mte29/gT/86NlxOjx99oJw8dp5JYc3nY/1elrUI3MqWVKihvlYD1OdWjMiCafgiOYRro1Z+ISuMmdEGOlipsacU5IcOUNKXjGXamoxECzC1ZTdW0jTcHaIRriBanVtYQ5dMM06HfU4qzl1y2Y+wfGdkUAQ8UBYra02rY2Q81rWm5yyJCURq2olgyVS4ixZhgxnCqmqWkOYU6Zx4LUwn1rQiMhhS0SQB3qMJ06QRAYjiyQaCo+ZBjiDTjMzMyZ4EGVKoFRbZHgyVyOgs4rUzAOUJDGg5tUjeQJxjjRAGCzOI8vIWYLDYYpwig4wNjKL4GAEBbzXgASadcUsiPTyz39yfveNs6vVo9yum+Jzebh1GwUYXtutPtyUAdjh1eOlRmje3dvR3e1ZZowMGLDCn/w/SAlvfB7tJV6+AgVIQu0w1U8ePd2eZ+QNMAIjcAUMwPamZuAlsDutM1fwEfhw+fC71yi6uW8Ytrtta7Vpff5yv5Hx3iY8mJrP03I9TcwyFMkFilptXmpV81wKQxBkzTuQvUfDEnGmLMTmZgT1Vris02o7rtbDOkkmyklzINxbbRVGrj5VndUSkIktRXNbZpumZg1mMR1t2usyRcCFJSVikZSJOJKABbkgwn3PaQphQfSBV2845ADAxBzMxBAh4cTj6MRUWmpqzTRths0oa1CoKexEMejPdSFh8CnbyeTRgYCJkcgZ4FCQu2l49Kob6e09asEubJJQkkfT1lrU2c2cmfKQBMjIKZzChagQD5xSSpxZAm5G6nCKXrjRfUQNIWAhAVFEa9HNGh3I25f4/3d89k2VjfIt3y1k4BU++xoePwamafHzO/eBcyDCExq7scM/InylLXj5h/jw8O0ffvh3fuNv4PlTPH5xff1qt15VjX2zZ6+uPn387Oe/8cbNYvIf/4dvvfvW13H/i8ALHGesC1BPXSq8xdUVzu4M43tPP/jwMH5cy5ooDeNquXpx0KuH5HeGcWTOIDFY88mXRZEUHtq8ttZYmJRLZmZSDVNnpiQ0SCopDcgUoglpGD3pKLIbV7vtOkkKQsCF2Y3cOEuBcZAKGim1ydXcYM3aNLV56XzvmA86T+oKDzL2CO4QWMmwAAvyKhFRNRk3Q5iHUhLRCreQzEIJSYl7XWpHjkRQP82i5FRmSqthNZZBVZtaWH9KdM90YvRUpQSCmZppuCUIB3t0MSjYPQJJUiIJOIPcQptqVV0sLMgpjKzGPFu4jzlR9+52YwUhgRNTTj2WAkTYUjVAxrYEdUA+EMSJUklygs1ERV+NhuhpniAf5Acvrr9wsXtne/Hxssd0jdUF3vw8EOfbcwz3gecfvnqlYW3R3tT14/1UIV8fHkPn99/a4enTn/77hyXKG1+611prFodjffj06aePn/3q7l0ggBff+9Yf/st/+a3/+r//XeA+cER2oD9PR+A2oLh+Ar++eny9X4b91XIcnhssSdJWze2lx5Ndfn1HLJQEJbE5gd0i1LVWbaYJMoxIhQGCoqS8G9frcRySJAKFhMKYKhlxrHMah5SHxII+LNIa82IRSMEQZvA4DNXa7K5zGOS4r/t9a2pM3txrNW3ak1MBhAs8zISqSY6RSNSSECcMQ8bgdlNN0wvy+BQKRCBqM7WKgIUHBwQUnhKlMpQhFwJmNLPG3X3PlCSVPIxDySlFuJkxhbZuyxAzqDqyEIlIMAn13ZSZNq1LnY/zNNXqBiFCZdH/iAAAIABJREFUHzpzMKWUkwhOG40wdU5OQcKSJQfcOzpHw5uqUuaUM+eSxjKMq7GUzBSLtq7meiMPD+rQIB6GApYYM77y7pvXV1h94QZ3A/zczwHAB3/w6eHlTG2uUzM1j1u77dd/+W8Djlcflx+8/P63f/DlL38Ft1bAkoeUN8OTy08+/OiT43F6/mr/r//X/+2Pv/OTl1fHf/D1bwBvdY/OTbB29Vei+H5/vIwXh3o47JfWjtO1pUYwdbg7gT96fhzSqGYQyEDFOJjMm6rPVd3aKf7slqVcrM92eb0Z1kNOJQPu5toWLKFISJnGksoolKJGa9C5WW1enXxBRi6SIR0VwuTCFkuNtocdoOYBa6oaZhaLNgpwYkTi/j5k4iYjqyqoEHEW9sGZ3EzzwOOKOdDIvaHWVpvXxBTi4UxBTHmQIAch3b1zPqZ0fcBxmiN6gSblkrbrzW67HoYBEUutS53duhXPDaqtWUqFU0qCjt8zJTMPX+Z6OE6H41Sb+WkeTUE8liIim1UpRZaqmFuAQCkgzLnksaRMRBE6OcNqOIvwZr26db4dxtwh6iwCilqXiGjq5gEIuVMPfQx5HNOLqV5gwO4X8VevGRiBIwIvry+PtnSV+/W7t37r1/8ecBt4govV+rPHL9cvgfjHP/7Ju19/F/du4XB49vz55YvrX/ji+7fW9//9n/zkS5/9wmfu3PrN3/uPgAwoUIAR6Pyc3NfZ4frq333ve+vz14NC23HyqyihtoBY8pCBudWH12WAKTzg1DmhBv9ZtJtFiMdcdmV3Npyd5d2Qc86JTu5FM25EWjLnkiDewqp5izbZMs82V2sThcmAYR2RWJo5Aexi6qRIzkJMhi411ObWrc7kiXwYpOQ+p3XqYLuIgLBwHgTOFUrGw0jDEDmTazpOrkdfWjcZNoqORReKCA6EpDtvvAam9PSFtqbqTU2ES86rcTzfbXgcsFTVBg837SYyBZWIklIZR+QEN9TqHu5Wqy1VtamqExw4KeREPJSyGobz3bgeioYnzk3ZbGFIkiGnknPJIoAxaqFkjvVqvHf7fLddca95c1K37vPmXhdanQRSckmJmIacUhIL/6vbGB5CnyEceQuraPPV4XBsi7qvVsNv/fIvAHeBJ8BzPHt21Olj/+jlw/rFew+wVP/po+9/9NH1q/m/+m//O2xvw4+/8rc/we2CgZDvAwuQgDMAN3J4fzUJfvb82XA93Xrttf3xxZIO2jTIQSkT87Kw8PU0YrN1PkpKDDdQBAYvDi/CF9uz893mfL07G3bbslnldX8La3O1ozYNtyEnIBFDw8NttqXa3MzmqtOsy+RheY7liHmVxzDU1mBBDtJITHA3dVe3CtXQFk7BJYiRhYaBAVhIcO+doJTBAY2wGiRITJKQR16PSZuotUGzehcV0f0+HlAPZ7IqCbvbgAzw2+oWsd9PEcQi61Xh9YhSwEjHo5l2GwoQCGdCKQklo2QsMzr+VtXN+ypIiXvYzIWdApQSyW69urXdXOzWYFqVERBvl6rRMX+F0zjmRFQkm0fJcn62Pbu1Q06oukzzNNe5NSI2VyIZZLCRYZGylCQRlnNiRlUHPgbeAh7jxRPsJ4yM7YT1LXzmbvoPNE81JflP//HvIL0HPAee4Or59fXxcJwe7y8Xqcv21ocvPj3q8qfPPvxnX/sVbB8AiucvcHUNJ4wFZUESnN0F5KYd9gowYAO8GLPkaF5fHQ981Ou0kuPhaO6cV0QSHmattUq4u9tcbHI181nrwgtnKXm4WG9u787ONpuz1WadR8iAtEIz2y/7eWqmjLTKA1EyhcEtYq51ieVQ56atLlaXaNURXusCb3Nq7OKtCii0WW3diQ3AEQ64wpWdLXNajbLelN7RK8KQVHLkknMSZklyKiHRhQIMJIewlDKmFakTh01MMI1wN2V3JkFbok+DVti09T27hz6jstW42mxX2KyQBOTMuMGSgYk8QrrilrrZMdxVtblZhJ+oCB02Kggh7+4Kp5LSahiw3WBIt0WsoS12vV/GzIVoyDRmSSLrcWCmcT3k7QarAQyYH6b58fOr41SHsQwlM1Eu5SyX2hRwYXInd0Pf3z95gvvnMAUIY8atFfI58Bo29ouf+dy/+eF3//Hf/yWULwFzZz5dvtg/fnK1tGZOz6+PUzq8/YsPsCz33qTvffDdn/++7F8eP3hxub0tZ7G5ZTvoBsMIF/DqZNs/vsDlFbYZ1/WjJ090/2R1vnr45PL8zVtubTOSRZ5b04ZAlJyFpbYl/PzOJsxsrm2xWr2lJBfb9flmsxlKXq2RMpyhDdMyL9MyKzOPZZNzCufm3sKa6jLrYrpom+dFF4NLcg4YJXa1eVnYBGbJA2qqZmEUIULSU42dbwgqmVbjsBoLMbVqzSPccxGOVEouJamRaiMJD5onpx72TcySiENYcskncIZxdD3UvDbrVBoB1jjfrQP3hdW85IzVgJJ7ZXhnjzETE/sJKQFQjzES6FTwrqqI/s/BxCCTIpTZmXhxbXFqYssJ44iq29Vwti5WWxEk0gQjt1zSdrvGqmC1QikIx7LMV/tHT199+uRlq75aj7cvdutxGIcSCCZqrbq7aVvMQGQIvLrEfYWssZmRd+AtcAfYAHj7N37jP//aO7j4CmDAK7RPLh8+ffr8+vt/8Wiea6vtan/88V8+ffsbX4QMd957487d1R//6fd+/NHLi035xutv3roVuI2bltNnqMCjqlf1en+Y5zYkPHlx+d3v/Mndu0h3zG212gkTHxcRodJiMSYh07YsR0Rc5+H13Z2Lkeasiy7VNSXeDuM2jynlmzSUYdHQhYOGnBLlLEmQunLtdYlGqOwNbdZ6VLLIkpgZxEasHZfpFurzVN3V3DpLh4mFQohcTmVvOYtw0hZdNKqtATEMnCWt8sD5lDjpdSzHyVzN3XNpRFxbU21ERAxJvYUc1rS1aEtNwASMAAEDdjr2upuUMA6nA9SJCp6E2RFkEd3KjThlIzgCp6JkwqmJiHpBXerHxZSTL0cvwxAenTIKDcAyYzemkmTILOSJsF0XnG2wXiEVgDAf4+rw5MXlq6vDsqh5cG2tWoyI8F7ryYSltfk4nepphH76+OnbXzRgi2EB+OZs2F/v4OIdADe7eLx89vEnj1+txvLJw2emIYl//JePf2duWG8Bg+Odz95u5vdvrW6/fhubHbC5abgmlLntLj+9enn9/OEHP3rsUmieNnfk7W+8m0f+6aPj9dGGhLMNLUapCM1a1dxDF0M4XcnDMuxun4kjOZNnMeJGzoYQ1Bnw3uTbmnLQwImIONg1mBjuVg0axdNxJruGTySUZCilpB6fd3cOINxM1VtrLUAkEJLs0cKEwTmJmXqIcM7JPZp5uBFQimyGcUgjQ0JDl9DFtHqdtU1gd0Sr2ZCo78px4oaBmaxZf9a1tiTUA8p4WlKSsC4IRkmQvu2w7ldkpnEsnRJuHqVkMEGAJBhKWY1taaanEhSAJMmpJUGKiIS7Z5cki8U4VbihKYN32/X5el2yJCEQj+OIsx12G9DmpOHQvCy2Py5LbZ3fHYGlVtWSRDpg2szqvDSzzo2IFh8/87eXZxh6Dtv/2iI7An6jSCbgFvKtz+ePv/XoB8JRyvBy//K4qDDb5VHWrwFHDMPZ/bvvJx4zY3MBELC+UZ9mQPKte2+NhT53fv/d+3/54TEVqaxNhEBnm8GsaiCIxhzmFGOJWUlyzpmkgOJqOj47lC2M3BmQII06q2rVfpW7u5t19j4AP5VthbAz82pI7qXNizQpNjAlQJILuTCFmbHC5gaPiOCchiwdA+VmVh1AJkaioTBKKpsk0rFXMDeGjDlT5KjQBepxdVmvXizzIZZDM+Xq1c0liVGoVk7Iuc9EftbQbuEaYQldMuxfaqdQZu7ebSAAA6gk2axXTCs5ObRjGAZs18gDMGBIuIUNiGN/nGYSZJbCoxNIOuqYE7mLOqK5LdM8RIZhGNdDWWEQsCDxCSOwXoF+ds+oGHRcr2+fny3NSq4gypKGIScWIgo/JT47QF5S4s6jy4xHT/DGCg1IhvwJsAYu0S7x8ilSwAyUsb6Fq+UPvv/H86JJkHLanW1xPb16tf/2H/34V//hA4BRCjDu3npw0kBhAJ+kdFhoa3U57pdXT55Oi2Irl8fqakzGE66ul5J5IHFQgAWeHSmNx0nNlEEMqm15epxyosTB1DvURd1abUkEIHOj8JTSCdkb0ayBpGRO61Xh9VCk1TqmUZNXtw7ddgsz634QMidwyhIdd8Qw9VbBpkKci+SBx50MK2kSHuEeYuwpmFDKwCTL0qWqdvmqTnvXxWDEQWYRi5sGseRerpzIzWs0aBcuEQF4JKT+2RlQ0Y+knbv0sz9FaDOuOzAnCYhBQO7s+C72BYrgLFYa3f8vKUVAe1SFAUJ4dfWlWQMibKVjljIMI4YB2/HULQKAGBiAAUg3MbI1bt96HVFKPh6ruqcknZFPwq0hEOHZI7iRlCBEGtKQE54/x4vnei2Prg9n2xygxez+l1/D61u0w4d/8ejFy8Pjp5eXl/vLq+tXr66P0xJmIGjVYRivDmdQQmKsCpCAcyAB8w1nsfVM5UcfPX708Km7v//5i63T/tPraZoJaK2E+24z9KaiqqEaBoFgNGiWqu7WnMW1Xs/TtB7WgZ8B6gHEib1MZppzIkRXFWtoa5Yyp5xRChILYXecjse5VWVSd3JEmGuzNqu7CUvKmRnOgdQrBuEmHjCPVHi1TWe3V8OWl2jmpNVbNb8p1moWbWrt2uvUlqO7hrfOZguAEQTnIrJZlc16aKZHm0l7WUm4BUUwUzoBbcOwnEzU4HQzcsTpghbAA8LgDHTuSP+hTykBAKsFZV5tjIijg4AstE/9yYLDzI7zXGsdy7Bd2fmWcs6n8t8TQ/vmHREnT3OntQijlPPdeijFzInZ1JkBkJakZq2kokW1Nm9gksRJ6JWlC7pMlx/vHh+fXh6nebaf+9KTh+nudJk4Hj559emjl5eX+2VZ3HSzHYeS52WhkDe/8Pbv/Mbfv/tzXwM+BX4CDACA+tfuZPPNLMNatVzKZjtsz3Z/+en1fj+5+zgMzHzrYhXuROweIGcO9YiAEa0HsuicTAqEad3bsM5kHr28F0TgQEDN4GCmnMswFiThuTV16VcmM1ggUkoZh2K2sqZqvrRmqmFO5hTMROzBWYTh4r0CEIwANXXJkcdx2HLZsHBuNY7u1DqaIlqYK5mZqYf1bkYW6V1x5KZEmSKyyDrlbSkRmdQaFkSHggYT5yyp39dQFc2QM6T7q/pzwYECBCSfagr/ip2aAbrJSTMwAmusDiTo1iKJ4NqsqZmamYcRu1lb6oKAMA9DXsXAbcJsSL31TSAC6vhduomHKOYFWiXJJglIAHjTCKhpCvZIdeDiSU1a5N4yQBxbHexq+WjZ8VjeXA8/nvFJc//w2Xf/9OWbn7m9P877w3J1eWmnzg1yx2cffOHXf+m33vjKN24eka8Dn3TMDqAn2eBmhWF5+OqqHqeZiEourw728uq4VN3tNiXJvfMijFIGVZ+brYSrxkhUNRZ1JmrOh2mBtfCRCu9buyWldJgbRJi0qYW7BxMlTsN2jbMNiHlczpmvp8lqlZLhhtpUPaW8XYc21WY5MYVbVWO2XvQmnFgU2jMZwYAwJ4EAEryKtIKUAGGp6m6BUDuxTpyiqbsHOwcCp6b1U+cDYExI7IkpE4TFyjDnZW6LeefscJaUkAWgEz5OHeJg64b8m4AhTp8sFPiZCz6f9k+Im58zSkarEEAIbspq1LxX2STnhGFMzENJQxmSwaZ6NCyjCXIGJwBIGcwQggjU0Kof6zy1MKzGwsMISXDA1KqqqQMQOgFPQwRwcnC8fvsWHh72zR4utMR4zeV5qjbPlmN/ffj+Dy7HsXjQxe072qqrXezu/tLf+JU3v/p18J2/lt1N8NfBj7ppBHgB5Js9BvYHnY6Tu45D2WxXLy8P+/203YzELAxmnO9WxHS9XxKzum1XuVr0CoTqfrZOQdw0iCm8Ta221bgS6UR9VddeXuTOKackyAk53XxKk6leXx/XbiLZXZtaEk4yJq5RvDRxVRvNojVESjlx7/1lCCdmRwh0iFjFAp6cqhEnKb2k3dTDDIAwOYwcQT2GGuaAu4N65azDBQyKgLNbNFUwOYZUCpdjm9l681JKcAc71LCc+rqxcWT7a2npfidriAnTgsXQw2uJMA4QBXY362xEq4BBAq4aGmTqTZiYYhwky8p8EBJOSRLVmFqlWbm0JMQOSsKSMwsDtNRlXur+eponLSlf0HaXBHAY1daOy4IIZDDDEyh5TuwEdRdhrFK7vlxUqznAL5whSczmtgxF9od5miNJ4pTu33r9/S989Z33voptD9gtJ6ABFL5gn5CusQIoAXF6enq7ejJH2Tx48/767IKZjsflxYvrcSymHu6rVb7Yrc52w/OX0zQrMW1WBUScQOSH2Wqz3VoKtcVCuLi7aV0QZ9tVP1FqbRHdk+1EQnBEoN+rmSAizLXZNC0pGainebkwI4tQ9HKMSBwl5ma4qX7IZWDhkwZANIifl7XBZAiSIApVj0bkiEZZmBBgtoyoqORq0Zqht10CIAf1zIjAvFVVkSQUThx5nQdUjxRDLtVbwv6IPGBp1lzVZV7STNitsVkBP+OzVWDG/qpdHffHRRWJZEyyWhXcqygCbIECbLEJ+Ax2JKwQelRHmJkwOHHK1Ce1JByIpakuFh6JJQ+JhViFrPb2C1erx7Y/THVRKz6uyzq0/+4ObVGDghNRIS4RQsgggjgS8w/+8Lvto6sHFxfW8zacSXju+Rs/9Q2kVL78ha987Ys/X87OkRLscKIh9yLZpjhOx+t9RNvcNWzkdI+PCpazi/TBh8+eP0t5HJdpefHyqi2qrgQaity7GG/fP7t8vn/28rAayvnZYI6h5Kcvrs+348NnR1X3iFu7Ms3Xx/0ybnZmejXXlFMSsmZuhrnBmwBM5tZ6WgIUMAdLGUvOyFncYe4iSh65V7RQCMvazRMpuy2LmZkjiHPJPXpMSYTEkYaUuWzy4BHcFix7b1P4QmIkVFgMiOqaiQ3UvIWTW0iiXqEJCTEeUi6cONiN4v9v711+LEuS887PHu7nnHtvRGRkZlVlVXf1o7rZjyF7pgEuyIU0GAiDgfRvSnsBs5yFtBEgCZKGA4ECmuSQbHaz65mV8bz3PNzdzLTwG1VJcGYw4lJIQy4uApkZN+L4dTc3++z7kfRZ70yJB2RNuzE9lk2/fn2zG8daA86tWVsLory37VlfYujkiwKcMK/b6f714/H2fvEaEjSlfJjSBzB8Z3iqJymgYAEMTEFh7oYw92rOTL3X7CCzWls9zds2V29IwmnKaeQzh4ZJmHPI8bg+3s21etn7uM8VG8JLtRXFtLpGGphH5oGJw3vCDIbHZ1/d/pf/9Kt/8sufDyqnEs1iWep9W5lwe3/Kiffj4Wc//MXPPvkZS8ZWOuQMTOd11hq2spzmx+MJkZhup2I4jEg7EGFZEHQ50l/87ra7sFgLhysLK18cxlcfvyiP82dfPrz/4vDyen9cak7yxetTM392MdTWOrjlh9+/9sBvPrs7Ptzt9pensm3mKhJorRRrG2Aq0g23YY5lQ2yoFbUhSFUkKTcjpimnZjSocBK4s5gmTSY55wKj2j+caAgLRKDVGhQkUGLRDLftFNZsfmhtdRRoh84OEu7cmMOVIqtYc/MQ5sQd+gwmGpNmzUkyQtbiXZUtrDnrNA7DoEbQX3/+xTRNSnnKGY3atoTV3cgX1s3ZHDHj+Lis891yvCvzFsU9ElQ8iuHxdLy4vcF1BvYAA/mcwURXf/jWrDYjRHi0Wjsau0bbynY6bsf7go3GnPeXUz5oygKxLhKn6g836/HNag0X8N0+P6xpiBSIyCEDJaW0U81ESud8NRgeRPHTn3/vf/+X/+b+X//H3/+977HKspX8bDxcXTw8npIOP/vhT3/+yc9fXL/XmxzQfv8Q9BpMT0CdPCgC6zZMo+BxnhC45DhuCCfVq0O6GNPtqYTHMOT9OCURVn3vKi938xdfP/z8R+/jamd3S875qzcPv/ns5pc/fX/I0pqL6DDQ1QeXn9D469/dquq6zgh6c3qeMG1brc1br7kRi6iqoDmOC8JbbbVaqWUcBnXuVVtRFlFWgQpapJQG97VVEcmqHkBrHSrU3Gu1dVuCMYysmYnQitca69zmh9rWpkH7nNmiO1l3PIIyucqg5ISOF0kiTEQRWUSUOAuRRIVFX40QYRZlScSin929uSwX+3GKmJQEbKoEJbidtcjL8X5+eFyXxzJXlCYWgkSZ88iaV8PwuOTDjCRP1RACBCbuAk5AuFFtXre6bW5h7tHczOL4YHc3K+a4vODDTjN2EuTmYO985LaWu7t1q6bj0K7JnB0iAs2SKUihA7OgRXUHG1PjDo1+78X7/+yf/fE//xf/x5cPd//0f/3Fz3/+/JNPPv6TPz+9uv7B9z76wQcvXg1DJk0QPd85el2wf0IjwIagKWAOIg66dvuiLqIer098GHxHxGO+uJgWo1bbtm1lq5qFQac7e3bQ51e707xqrc358y/vf/3Z7fvX+8tXF+ttCXcd6DAlqEyDjPvD7c3NOB1K3T57fZPtRRdotcrCLBhSpOaCGha11HacZ2umqRtanaGCBHBnG4AhRGEqPqRcWwNgsTanXogPg9VqLUi6ZQq8cau0nfzhfjvdb1bblCRzUqEwtggLAzEQiUGDUOt3CkrohkPBDNIwshDuPau1VQJRcHOwWYWpw0LMo1VqRA5xTWQKtA0FsHpzvHtzepy3zawZvKGJDCyjpp3kQVRa5LwYpIK73VlFqzCzCICS5AZe1nU5eqmIEKKoFrXy8THWow0uU5724+Ew7EEU5JpkGIZta6dRWhxbXQcdX16+fHl5rZk8osGJgoXJg8LJlaqTExmFca22evzRH/7Rxx99mNR++j/9uNzR7U36gx/vD7tDyllFoQJNUIEqVN4q0BAokB0ps6ZLzeMwnFb64vbT55dLKh4tvjpaa16dloJ1Kwxmllbr6fbUrcTv7uj+/vST7z8fPro6/ub2r/726904fPLxFXQ8zQ/EnJT3IwN4c3d8+Ww6HcdtPQ7T1dePD1fDlYBaFZAkSI3EltCUGkqzedmOp8WBrLqmGAYTOSvxkpIGqbA7ag0LZRpVKaNNNIq00qKYSVSJPKgRB+cQRotmgHkxDydDChrElQ3cQnoT26NxkCplJRegEvUJleBgB4VHbF4RZk4lzOAUVEoL82S8WtGUFCHFnEs1JZCDZPaa25a2mLf1fl7nrZRWu8YwALAgxJwROadxmhJCUANwWIEXuAWZMA1JvBgZYqO6olUiQJhRo27WFtQN+0kP0+5qf7HfHbrb4zDmi/3FltvpHvvdgwa/un7x4cv3cfkMHLIVbpXQAcsBNHZPZ6i6Rm3raT0uW0R6ef0TYfr6bzLzOA4q8jRcHN7xoU+sWnqySqQn28QAASOBKTOx8O9ev/zyN79+cTner1QcrbVtq7tp9AgmrrVupYQFCEPOu8P48oOrw8cfwda//M3XqvqD71xeXE0Av7lfhWnMNA0M+Oub43tX48Px8OVXa1mOKY9387KTKUKFwZKqszfy1Z2wrW1e67wGwi1xM2suKZGwF4PWYAqiGiAKAnELdXcLphBBSuQiICVMUVsLOLSPUxWyXFKsY3XPRBhS1pSIU0T3laBwzxqcOSm5kxWhJtH6r48cXsPDzNn6CByrUA13W70ZcXHTTKM1ri1qrcNEOYE95lp1LblhrW5F0HKHoXlYQEptsE0sV3bsgkRBgmpom7cSaEQWWgkW3qxVq27V4cQB7nVoRzR4RSsuexmGvN9Nl4fDWlprLUlSTiaUNCVJeT9dX13icIl0ARjCqQaE4QwORD/svLMNCRvcylaWpeXMOWsSktTt1SLCgeh+70Ag7Glh+bcWjec+BEBncJg2+fDFx28ePv30ZnULkG5lFZVl3YRZk7hHEs27tNuNwzQk4ZuHlf7id+5+cz//4KPrq8OAXQJwe7/krGPmi0kA3D3M+wEfv7+7Px6W48O2PNbhWfHChAhxj9YYiBMTEzWzUqpbNzNoEeHBpVqn8hAows37WxYi6v7FzdzDzQKAiIqIMO0HjggwHF69ZTq14ttQmCA9I2RBUDMoCQkUmjOniUVJJHmDzdQ2NovO3Q2HwSL67JkIUwgiPNyDgwKaYrCN1y0kBTONgwoncmmFUTk8Jxd1Lg1uMFRy8kbbVrJvPm7CEwCEYfNa61Y3wIIKiVm0Upo3IkhOAyZxdxGmiDokjzgmZWYzDz6zFVmYQ6z5sq3r1uZlrbVM+ew+dG5RmAMBi3OLohvG8Te3RY6IWn2rLbp7aaYAQkilKx5EmKBP6b98Y/3aDcm6fVA8lWrPrusXu6sXVx9+ff+pcLTamLmVGqhMpFU1aR5ySlprvb9/OJ3WnJnp1f3DqbPXpkFBF7D54bQe9rvErhcZ9+uylufPXmxNmHnaXyzz8bTcjfnKiFvb4oz5duqQ0fB6rsyEMLuptNIdAjzOfjdnDG/Pp6g/MofDEUysKjnlcRyyiCRhEla25kpSd3UtC7zkLERsTmG2NUdSVaTEeRQdKWViFqsAiDOtS6/xhZmX1jyciFICBYcG2MjDgYimO5mCBts2QgwkA3Qng0J8kyAmV3VPRtpiqxDOu3FQTa6hfYip39Ec7ijNtzWqbQFLGe4S4KxZRx3UWzXrDLrwWkpvcSynubmXrZRam5mwGEcptZ7mea3H0+OybYPIuq5YZ0wJtSEqpB9t8QRc6qaIDnKYO4IAFVUVE</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9a49kWXYdttbe596IyMzqqq7q53T3PDiPnhmTImXAQ1KSBVuCH/ITlr5aMCQD8gd/8p/xFxswDBiQYQu0KRuSZRMUJVIjcp497we7e/pR1dVdXe/MjIh7z9l7+cO5kdWkRIocjij3uE4PCjkZkRGZ967Yj7XX3pu/+g9/69KlJ8yslELz4kaSNDOSZiRIEqSRIAyUwUCQAEiAhA5fkBffhgHq/1/o3yRBAMuL6eIpy4MXL2gE+pNJA0UYDUR/44svll+svya4PLb8Tx/4d3kC0H+ri68fnz+1U9brzWa9sWLuxc3NzWgdCTQaDaAZALOOClswBHbMUbi42WYGdIz0f7XACAsKjRCMpo5YwBaQkgaow6n/BA/QAResXEDk9+HJ/rQv2uPzxz5Gw4IpGG2xABc2CQDZjQLUrZZEQASg/h+B/mOklkce/UB/6AKIOpgtdXgSsg5dwkhSBKxbqQ4vPoIU8Pu/vvj38fn/+DGjdf9Iw8ESdaTJPoC4jgBhsSEHbGnBpQAeMLQ8BFIQAPHwMgb1hxeoUVzQaU4tbtfw+6BmgH0AXhevoD+VC/T4/ERO4aPwixf2o1uXJTKChA5CAGKHlQ7xltBxZzgYMII96tKCzo6qA4yF5YvDaxLG/rIgYR3jfAQs++c5Rx2+/9iefShOIcyMh0io25RuwQ6eDgQl0JZ7K1j3pQdfKR5QoCUrWHKDjpuO10NGABopYjgYNzMWp4NNALAmAMwAAAJ+eN1/9vAxyD48p9hFLrlETv0/HaIj6BDsg+LBnC0gE2AgFqh1+2SEE2YwEoaBpNEJmkmSSEPEAYkACAkgRj4yWuO/osvx+PxLOoVO6y5rQVb3Wt3LAY9yOnXEmQDTwmQcTBI7BA2EBqcRbotl6z9rZsaOMRBkwYU/DEiAPzZOP9WnHAKjTlzhEXWxuD8AWLiuDySJHX5u5gZSY7EaSqFYT1wFMFOdugDQDVlmBmBk6QRHf5H+Do/PT/UpZkv4D2BJOoGFjAUO2WKHBczQc0wSDhRPp5mTECEDBGUsMT8AMxKZMkWaKIlgGpIy6ADDC8728fmpPeUQmcl6ZtlxBwCHtBHovJewhGKdN0siAsn0RJJMwcikDl5VghJBIJJGJKTlXTIzjZR0SA6I7FHeowzk8fkpOuWiXoSFqVD3n4ec4EDSQgAyCSRJowBATEgJUCAsFQvJb0TC2D1nEN16wYBMIxtBqRef2pJQgDBjLiWCx1D76TqFPKSYHzRghFFOwqBELjDrJIck5EW8pgskMrvrFEJpBLLXL0UYEoQI5kLHidnda+pQezKkjM7MHig+htpP0Sno9kwXRuxgw6QkCpgUEgJJScsTBCQOpGzn1zppRkE0SJ3N7S5QmVpIXTsUq7oLJkFkf3JQlgStM3WHeO0x2n4aTrdnCyFmi9EShSSYrItxuUDYATC60EMAQAhm4qEs1Vk2SgskQetIDISBPQrszG9/swMKk5ClJcEU6Y85/5+WU7RA5WBlDsZGIJACiby4zxKWQjpA9eirkx3IPJRFOy4CIhC96CkZmRCBFBfOA5YGEw+eNwkTkEhKZoLEzqv5v4or8/j8JE9BR1YvLVELvkiTdCgrdUulBUlUygwJmg51ch0gZFos2aFGuSjMlAaDiUkYTAKNSOUiOJMe1eklWCoNUMrMEHykLnt8PpSncCl/a6mYL1mhZEu0trjMR1KgXuQ8KIRALgmnlgL4Erl1X6zFQorBtKAMlkiAlrHUTEml2JOQDnSKiWSSzIR1k6bHycGH93Sz1UGhxZrpkbpMKS36n/5wx50ODwvK7ksT6oyZhOxPPvzwQajWXzBz8b4LVbLEflJ/veWBJcUVocVWLiB/rAb6UB4Dlmyx+0ks4FhudheZLRDDI3R0OC35QWaP0hJSCh0s0IKcBUYLLC9epdMjKUrKAzAvoIxFUCSgV7HAxyD7MJ/Sg/vOoy5pJPvN5oI9LPT+ge7ghWhWCWDxmTi4tG6kDsIgsT/NDhKQ5ejQVrC4zEXGazKARicXCfgSl+kQnz1OPz+Upxxki3pUHtcCkkck2KMvaRfgOyhpLxLUHp99AJEXuOCF6Hupox6QDQCLa+1FUhjoxuL4QFvJB8/jMuiH8pTu5hZn1elYSBckmrgwXF01q0xwqT31KKrTbwkQyoumgq7izm6VyK6zTVvE2OpP65DxRWC0vFJQCBGC+0EKeYG2x/bsw3oKgIRMBwl2Lw7JtDi/PDQDsKPpUP3OJb1UF2EcDNWCWusYJRdI9R/Wgkbst3soI3MYxs167e4L1gklaVmDqTSDmR2EQ3oMsg/vKVjI1iQo0ZgS2f898LKHwOwQwAl5UAEdkNfBpeg6NqVIUp3oPTwNAd0/fXjr1q1XX3s1I67fuH58dPS5lz/3sZ/5eJvmF194Yb1egSl1LYeUHa2wXlB9ZN4enw/Z6XnA4rMWa3Igax+pdiDQ0EP2JJjdvP2e9E/IDxidDq4EorWb794sPjz19FMPHtz/we/+8Itf/NLDBw+Ojta7/bYYr9+4fvkrl1fr8SPPPv/n//xfeO7ZZ+g90VyQnb0CeyHOfYy2D+EpOBAWC4uQC7VKaon4F7OWPCSHC9e16BMP9fDlx0Ac2uzEiPb6669/+9vfbC2efvqpt95+68Y7t05Pzwg7PzsTFOB+Prt9+3Qo9tZb12/fuf2LX/illz/z6eOT424HddCJ9LoUcFHBx2OofYhO6RpY0C5Ehwu1IS76136nL0pCS/3pEcvRnal1WdGjSjxbxLvvvfP+++9fv3Hj/v2zb3zzu6IoDd5LDQZlpjIXXjciXn3t9dPTh+720osvXr36ZCl+8NwOiov3vDiPVbgfmsN/+srXj09OFuU2L9T/F+1xH0j5LjrT0TVA6t/EkqWyK2WbUi3M/a233vitL/4TyN6+/vY0tWjR/SCA4jaMA4mIVErU6G6F7iC42Wx+4c/8/F/8N//CM8887e5+aMky8tASxUPvMH4sqO1203mG5rm2bE9ffRrY/ASu5ePzB59ysFC2sBpLHnmg7g/aavTUAEAvkC9PO/gwZUj73fbNN9986+03Hz44Xa/Gubab77y730+ZylSvmw+DFaPIudbiGEdrlV6G4jbNE0SJ0PaVb75S6/wf/Qd/5fKVKzoUTgUAeWB78wC1/ONAbWox//aXvvzm2zd++OrrhCLz6OjoYy8+/7nPvfzU1auZae6K9tGXPvcTvc7/fz/lkEJ2QqO7PLuQCKVkOMg5FtnsIYZbODOJOD87+8EPvnf33r0333jj9u073cuaA1KrEdlVs8pERpuMq8Ep1CYiJTsax91u6p1Wg5d5bnG2u3Xr1jzte/mK1D9TRu8fhI6wpS7xh0dsZ9tbX/rqK6+//ub7t+/cvvPgwcPT4pZK4/233775pa++4l5SGJ3HJ8d/4Zf/jU/9zCc/+tInO/Xz+PwJT/lAsI0LehYHkn4JzHChu7jINRfl2Xa7e+fmjffeu/Xtb3/n9u278zRLMpoZQfkij02j0UyKXkiYaxvHUkASZUBr9eMfe+H927ciWousLYfC09OH77136/KVy5vVymg9iDzg6CLx/ECs+Hu+//sAl9/+3itf/O0vf/9338gWly4dKzMTU2vuhGUm5ppjiZDOmk7P9n/37/3aavzHn/nUx//L/+JvPY4C/+TH/+Z/9bfGMi4N5xcS2YWhyKUInoklG1BPA6Ss83x6ej7X/Wuvvvb1V77x4MFpa9FaD+6MYKvN3OqcKRQnTauhmLO4gzBzN0ukEmDupm1Gk1IKCeNg7n50dHR2fr5erWpt6/UaF5M7Hv2KFwFkAu33AuKROvPmrbf+n1/7jW9853fPTs+Hcahz202TQrUFYSkpQEMZ6CCMrWWtmRkPTx+eHA/PPvuk+/pP6Yb8lB7+1le+dHJyCbyYY7aUK+fa5mmfqdVqNPM6z14GI9ydZhH5la9+6Tvf/oEXG8fVrffePz0/y5YkT443MNuf7/fzbAaAGVqt3HpTsaE1kVyv1+fnezDM6IVuFFgMPlib5YVDKRJPTi5duXLppY985N/7d/7y5ctPDEOhmeGQ4B7ANNf9fr9/4tK1wzcvUgS1ePgrv/r3v/r1b717615mEpbKQ5iAQsAMEo1DgbuByIAZxsHNMI6ro6PNz33+M//xf/hXVuPVH/tCp87/6e/89uc+86mrVz/2E7hvH7ZT0Hsxc9FndLFhShmxPT+b9tMzzz1PYpqn7d27Tz39lEDLnOp85/07+2l39+b9CBFyp5eu+kcpPhdagxsjIGStVkoSHMzcPTOnWkn54BFSik6lpkklFcnahHVT4tatO3fu3nvvvVsAf+5nP//pT35iXK+KG9mbCPTOzXdbq2fn5/fu3vv85z577eozgB9MXQIwsyuXnzjfTkbMNcGUIKXRzC0kRhZnZM6V1loZzGhmaBmqbDHVOv/Wb3/1oy88/4Uv/KUf+0L/2q//w6987Vtm+uUv/Jg4y9ybfdCsBj48ivaCLhqjKIsMZZoRNCOHcXX3zp1ozWww2tn52Wq9Otoc331w/ytf/vIPfve1Ns+ZWo3uptZQIxQ6O98rt1CWwRRpxmHwXktKZW1MRkYoCcnCSNQ5QfQ3b5nr0ZKMmnNTKcyI7fnulW9+az9NZ2enoH36U5842hwdHa2naf7qV7+2388gpLh25fK1qxcmrdu8ODs7u3P3XkbWGkujMpZmQbXg0rcMsI8JoZTDCIpOWlnUn1D+oy/+Nt0/88nP9JZVSdGahGvPPEe681+QLux302a9uvnOrf3+7nr9L7aLr772fbp/8uOffvW17/+DX//1K09cuv/wwUeef4704vrXf+Hn33vv/f08/ezn/8yl4yd/Mlj4l3mKMoVEMtSitWm/m6bpyWtPgSillDKcnZ1uNpvtbhstTk/PHzw8/fKXv/zqaz/KlC9CMZvnKjJqCli57aY6jJY1Qyhl0YS7Q7T9ribURwk5iCInkpymrqANQhPghUmDFIGhGA0PTs9e+eZ3vv/DV4fiR8dHLzz33J/75S888/S155599vo7N99++8bR0erGzXc//elPDePRIVCLu/dvfenLr7zz7q3tbt8iASmZB/HlYrohE0WIMFM2pmIcvUnr9cIqwvjurVv/6//2fzj9eH1i5r1zYhjHj3/6Zcj//C///PPPvPAHXeU6PfjRm9ffv/MAyh+98frnPvsH4myad//z3/nbRnv1tTd3c3326acvnayu33j3B7/7hpt9/4dvSXnlyvGP3rqx2+4vXTr67ve+++SVq3/1P/mrwPBHud+h6vwjPfMne4okhdQFF0Qpw3a7u3f79snly0Mpxycnd27fvvLkk5LMfJ72NVpGXn3ySrQU1OZqbvv9nBmLHTSSaDWNWK/HbNEV3Ep6KS2SREIMNKOHAjS3odi8T0AhRstswAj2xvZMM1dqu93tdhMN44Ozhw9PCbz40nOt5htvvf3uO+8fHw1/8c/9sg8FiP63ZU7f+tb3/t7//Y/uPzxtNXthnuxl2KW7lE51CUFoaYqWALboykopVRu8yGhztuKcEs8+/fy9u3dPnjjZnj08e3h2++69lz/x9B+Cs2F1+eVPfvT04fknPvbC5z77Z/+5z4mYfvjqD1/55ne+8rXvRWamIJ0+3K3WgxtXY9nvaygp3r1zfufu2WY1zHNdrcrx0fEfEWR/9//81a9/57sffeHpv/Gf/3Vg9cdHy49//K//zb+xWo1YpjOiFJ+m6c7d9/fnu/XRkZTn59uz09NpmgCOq/HZZ5554YUXeup57eqTZfDz8908VR1aT+apXSgbh6G49WnKaqlao5uQPjFGQnTttiFjkSBFZOTS/VQKh8EiIDFTEZC6JiTXq+Ff+9zLJ5eOv/LVb9545yZp2+3u8uVLT127Wud5GMxM3/r29/6XX/n7t96/W2tKmXEx4UEASrHDlIdHQx/c2MVPTpojQ0r0NKUXR+a5Rstnnn3+ypUr2eL09OHVa0+dn52+8NyTL7z48T/kQn/qU5/75Mee/sIv/tt/EEuy3T74b/+7//Gt6+9Eos51GHyzXu/nauTx0erh6b62WKZHGC8drz/1iRfOt/vLTxzfuffw1vvvfPYzn//D7/Tp6d1f+43fvHv39O690y9/7eubI/vIcy/9mKj54x//+V/4s8fHR2UYgKVL5LVXv/+DH3zvfPtAiVbrPM/37t69e+fuk1evjOPw7rs3b7773ve//8P3b989fXh6//7Ds7Nd5pLB9X4U9MaVbp6A2rIYzUmDLZ2evf2O5vDCYtYCFMyQCaO59YEydF+4s/7CgkoxGDL19o2br772xvu3761X63mqgu7dv7/b74cyrMbx5rvvffWVb333e69Nc/QIaxEGA1BaYWf4+pxvGgH1OeC8UKYfmOBMZArL1CR76ulnTo6fUGKqewNbnfa77Udfeuallz75h1/rJy4/9Qc9lDH/7b/zK6+/8fZQvLiZYRiH46NVcT/fTUNxo9VaW4JENB0fr9eb1ViGO/fP6tzeu33n+jtvPfvCcyfr4wB2MdF6l/Wjc+OdN7/2je/2m9Va/ODV1zbrfOnFT/xJ0FNze+Pm22/deHMYhs366A95Zrl+4+3WpkRevnQZxkzdu3/v7r37d+7cPr1//2M/8/LZ6fn1t95+6WMv/eiNN27ffnee9+S43e6HwR88OO3SDAUAyWDGTKgXLYG5ygPjWGR0pBVrLRetj8MMXKoGLIaOSDN2sUeEhGRlKQDZWoQoQdnMLWOaa1Uigy1anxf54PT0d778jes3br3w/LObzfj1V76z3c0ZQbNDqXaRk2cmegvpBxptUqLB3LDU3jLD3JESZd3mDQPee++9h7fv19bGwUP28uc+u5/bbjv9WHdKwBSR//3/8D994zs/kDCM5f79s2eeulxbTFM9PdtlahiGMrBG7PezpDL4bje9c/MuoO5eabr+zru/8ztfeva5515//Y2z8/Pi9ku//IWjo5PB/SPXnvvBj17933/1H9y+8xCGYbBQ1H38X7/+m7cfnH/6My9/6uOfHP6Yqevc9n/vH/z919+4fv/B6Xa/J3Dt2pVPfOyln/38y+fn+8uXT17+mcW+/vBH3/7+97/D//q/+RvDsAaboXg5muZ2fno+jL4aS6vt0qVLu13bT3s3zC1229oyFDCHu89zQIhMI7MruiXlwZAZAazGUoZhmveHoBtRM8EuoV1vylCshYxGYjdFRh40I3Djaj0YQTIza4Myh8GGoQ97oZGZS1eCu6/GYRzHoZTawtxOT7fb/dSTWYAZiQtZJvp2hEWcslRPSXOMg3VSxN28dL0TS4G5jUOn+XzNlRkEy/SPffKT52enP/uZF/7df/8/++Oi7Itf/PXf/O2v7qf63q07mbp29RKhW3dOn756aSjDe7fv76faf0kzui2zvySNY6FZRFMmYMNoZixerly58vBsO0/Tej1ee+qp87Pdiy8990tf+MI7N979jX/8T6Zpn4oIZQhUKUbq6Gj98z//s1/4xV/8+DMf/YN+z3sPb//GP/6NGzfflWBm41Bu3rpzerqb9i2RPJScy5jF4AOPN8cvvvjis089c+Odt863p0dHR+V8Nw01inNc1TbN213AIEREraHb79+PTBC1pVJmmnZBJMKAWArkoDnzEO7jEGKPznH0YSjnuzrPUcrSFGyDIZbNA/td06ZQssFADF52dT7oeCFjrbFZD9MULcMO7S+9Ya9VmbG4tSZzITnNVcDJyZHVaK2l8mBZ2Xv3AFxEh/1rdToDEtjpjYpknyNSm7t7oTtbI5UE3DkMPHnycgtuVke77flue7rf7U7Pd38UWXnq1HgJABBCfvRnPvXyvbPf+Ef/dJqbpNt3TmttIG7eutepk16lMWMGSkFW9fUg+/0swfv0OstokDHa/N6tO13bHOfT6ekNCftpevfm7aOjzfnZNtR6okOAhlbTXLvd/stf/tqPfvTmX/rL/9anP/1yROx3036/f+rpq9N+/upXvvHVr339/OzBVHdmi7wi+shquKhWF1rbSsznMJcx5mn/7q07EammMqK2WqJpvTYjapXUDkCBudaOPWLe0ouKE65as8fMEak8zLTVEpUZ2aTiNPPeyZmh87qPhJt76a2aMCPJ1dD/VFDabBxSC9UamdkNmIBoyox5jqHYUKwMTmlpOV3kv2hIL6wNaOmWteU833H3UJ6fT60pQmS68zBZ4aKYCwluTCUPXX6QWnQRFASlIpOV9B5fQhG22+/mevNoc3y0Odpu98995HmhvHvrwdvvXc+IG2+/kTE/eeXK8y9+tIzraEv/sxlbq/fvPbxz7/svfuT5S09cMtPxpUsvf/Yz3/v+q7u3rs9TbdEyu9HFhRwQYkpK1ZkpgGFmmYAhQ4IYTM/ipNEQEcy86OPgvXun9++fOglTD2n6GgeCNEXImK3mjevv/cqv/Opzzzx7dj7tdvto7dKlk9Z0+869VqsYvTbtZZkVRYdbGOnmrUnRO7lNEgy7fY2WKUCqO0WtpdbcnqeZQMvWzUxaIANlGI+Oj4+PNmaMjAcP79f9NjMySXYp2SJOc6epl8y7YZMZ3U3KWpNux2vrRfCQMpVCZvdNdGOn4kgOo0dkCu4dzb1gny3QnaMZXRYSoPVo0xyCDcVSanMGWPd1b80XKSXdZU6KLcVusA5yXxwkmuZAis7WJMIk2jIi6aASRoa89FnOkjDtK7A7Pb17+crl3flZneea7Z/85hcfnJ29c+NmixhG+3O/9Is/93N/pq9lEGnB2to0zffu3HnmqSfneTQaqfv37nsxAuM4tBaHJp++AUsSEmlBkJGAkKZMuR3+DsIdUJqbOVtFRqaWQLlX6BSSE6E+tkmZpGUmxAhJ2X3Cfrt/883rc4XRaDo93aWSkJeoLedZlCywSHmqxpHjCushu911wzAmgWnOWnOa1PWKxWUly8lqU8bBaRLTw40AvMcmacZ1Gcdo9dLJ0XqzfnjvwTTtSRs8o2XLhFCKR2RkttRmKJEpwd2GYvu5robYrFbXroxPXN68cf1BRrRUVy6uBq8RggxGS4OYaJ5SjqWk4JajlzlaKT6sWGdBjMB6s5Y01z3J4myR/WNKgxfDYd4al90IyOw2AVIaSBdpmT22X5LRjAsdQe+56fO4lq4YGjIUkUOxTGaotXp29mC/nU+OX3Iv12/evPvggbn3zOv4ZDWUIaIJaNkl79laEvn5z7+8Xq8lJMJkly+frMaV0eY2l1L6L3+YDkEhDWbGlqLULRkRaeaDKBhxdEJCViKajo/t7JTzfJgWkYc/sGkZmpi9Cy0MbIRRSjSlOd2XWQMRiVBkAnKP/ZQRyEh3RusbdGRu48DVoJZttdZ6jRZQIiR3CZjniIQabZORKkOx4j64r9ar/X7qd2U1DAFs93VTvGW0qFn3tOHoaH3p5Lh4ZpsG991+P9dWfNxsyoOHW4BHmzFaCDIvq9F3u6mYD6uxOKapnqyHcdzsp3kow+WTjTn3UwM01xiLb6d5PY6Ref/+/vhklcJuN1978uT2/TPSSextLl7q3JutWq0YCjMyxNaS/dNKZPSoBmCPnZWSGTP7ap8eQ+XSySAheZC4HcZVAhcCYwAR6vZ1npNg59haxQ7z8WZ0L6uVFwOgo83qmaefDum5Z5/ZbMas82tvXH/r7etl9O12f7Q5evrak9fq1cuXn9is110Q884777lbKdaajaO3Fv03NF9WA7amFLoBAxeBCzKPN3RHBlqLCA5CZoZstXEJ077zfwA0FLTofwhImKs4WyhrymgGGpVqDeZtGGy/y+hXDdlqglKyFAM4FJRixWEud+z2SgVNZ+dyZ2vKxDQlqUi1Geaa99jvWfqUiznbaiylcJoiIowcBjfLZ66d3H94RqWRte72U3vqyeOjzbjdWkT0u9tvtpN0roYyU63G4NYb0xOZEbs5zrZTcYfkRkidgZTUIofikcIySJnjyo9GnyL35G6q89zcQWNEIrNFm6fJLCnNM8rAiGxNZCybgHrISECIRLSMFI1GiSalRHPQ1Pe6pNR7XHq4aUsfq5Z2K1v2KpghU7t9DIWlmJTu4+VLl3bbs8wYxtGLi+1jH3vh9HS3Wo3v3nx/v69v/OitH731prKmfLM+unnz5mazeunF569evbY7P4/aXnv9jfffv91nmkzT7M4ImCMjBcCXRtll8Al6/MCQzh5mGbn00AZqRU/fjo9zfVS8KIO7nTZHOjrifk8ILTTvAcE8ChkVACRKaWQLoOUwglQ0kRoGnlzC3FAnRiBTSqw3sVqZMiLFUNTMEKG5atqBjmxoLbsAG8HIbBHFzOpch1JCKl6wwunDGWOhcRj8revvSjg5WRuYiKjzvg7tYauRTky1EXCz3TTXOYZiXV50dr6/fIlonGq0XXvikkVkrTEMZa7t7HzqrQKbdZEwTXF8vGoR89z2U91PTUKrdWpZm3b7eT83swapNtFqi1TIR7rBSQk9Iuz1LhAEe/AhqLXMhDIzWQrdEMFD1or0ZSiRIMiWJVQHpqZPnAfhNCMi1K1WD/LMOBQ/fXh+9epTKTu//s6TTx3Nc/vu979jHKbadtvtOBQfOM/7ea6Xjkfa7uHD0+3O7j244aZp5jxhnmeRU527nKFLfBV9+wJaQ6bcFzQcNM0C0ALaiwMpmjGqIhEBpTZHsVr5POP4SOMmp4oy0smiLF5qCwBHR7kaC6QaUiICJvlh5NhmzfVILxxW1QdcvqRozDAAXjDH3GaRvd0XmZinNFcK24fqpV9zSGyR6qMO/tO/9tdKGbyYUhEypxGRy/jiQ3IGB+h9kA9C6ST7jhNIiTq3MniPQvpyQ1t2Qi1j9LC0DKMXcDLyoOHFQsz2HImM1CNugH0UH3qS35sMKITUd/lYoRunORPL8MmezLa69JJ2j7O8de9iSbohpIge7y9zPhaMLm3OSVsWTwHsFdBK8zkAACAASURBVIjeRzoOdPcyophv1uuhrJ5+6poM716/fnylSKQnZKGMlsU9Ay3CzIEkymBeRt57cJ6qJ5vjlPe1HvupRcQw+LRPEtspdufzNC8jqA9rTZdgy00ilDBb+m4dWopShs2aqyMrjnEYYJmZ004hlcJMrgavM9wxbjS4WTE37XZqs2WoOIbRKZSSPjAiTrczTUdHLpibkNYy97uYZmVLOubq0177fXXXek0BEaozIhAtI0SwtlpWq6H4AAIF3tQZv1Y79dTbUzAOSy5DqAysLRV0ZyneN5Cdn27H1UhDnWPJqI1OwljM6IZEZIJcDW7uda4pRWQmy0CCnZ/ToV5lywJhmjEkOhSakcUJQSEQ7n0WyNKFRSdy6Sh1J8TMRCoPCxG6K4TknYI5YF+SOd0ZTTCtBhb32gThyhNDcbSgjczModhqzTI6yGJkqU6cTTfNdOWZniuElME2gjlGmzINxmwtwTAxBdMAU1Ylg4S5A3Z8vJqj1bnNquuRg9Cq7XbR8w+zZQ7YUhROKDGs1NfwtnhEnbhDwLRPrbBeqwUiMM0ZjTGquMaVDQXbLR7cTynNuFoxldeurDdrUy5CqZqaa50jWtNuF/fvJ4DNEY3c72WGccVx5XWSW2RiKOZFPmAYZIZM7rbY773NGSEIRUBI6PqAhDWkmaAMwLB8kMmIjISRUUWSzuKlFDNzM56bSYim/RwRKSU7VszGwVerlRm9lIyk+TgOkGqLWtUvNMUWLaJlaj81dfbUMJSyGvuOnmUpC2kJCWnqAVe26ESaihUrFJeJCzTLyEi1bpz7SmQIYOs1pm5OkTS6cVj5OOr4uKyOOHgZLWtLOE82A4yJrCGHWyGkuSkNaKq5G0Zodi+SPGrSbD+1wX03tzZbrQIVgcFTaGZ2/6Ej2zCo1r20KtR2X83MndO+CdrtAsgIpdLSxtHWG9ueL3W4nhKPK5axBwxQsowGSpGgTfv0YgRPlZGoc9a5z7AQVtzta3ELadojEoTmyvXIh2fz8ckTGfv9XOc9duetKWvkfqv+JyjRZvbPK4zR9MTlcShsESeXoBzN82gDsc4zvPCJJziM3O/YKuhR7j/cj+Ow5CbCbpJ3O+IwcxjMCUDBaM2Ki1wsNgBaKQWGuebZdlvjUH3uTZoGs2wtprmOwzCuVoTMzN1LsdKL0m5zjbm22iaS42BTZUbPyTXX2iIGd++hHxhLPQ9CtmBPi7wwiRZZ3NxsKCbQzRpzXWy7n1u2iy0JVrj0NzdlythJWBqwOio11M4SbFdOxnFddlPcPa1DKZD2NVcDymhAzFNPYNEi3WBMOuo8Z7o75lmpFk0RPQNmGSBnJpFINSgNyAEtayhPTycjS1nS3lBAcMfJsa/Xvlpba4qWc+23GDSsjrLObFU0KnOazAhztLqoGebZWySNRu8QlFmdZLRaYlxBwYdn6nsdwrzOaLPOtzw7i9oyG0LKBjNevuwgvCAbpyl3O7lprsiG9drPz8KK3CJCrcFHunGeOUWWoicu+fm2kVkiszUxeTFku89xKSDUlOnySTLA3TcrN7JH8eYyaLfdbed2tptJPvJPIKCassRqYI/rM2M1DusBVy8Nqgnw3hnP9+3Bg/OmMNALa+v1IQppbr2dLyLFVtxSTGSGAFWAIfNlyY8baigiYEAT3Qwch9KLZqSZH4AGgIaUG8fRTi6VOmdPUlvLWgPgUHh6Xn0q89QM2rqGApidb+sq4e6tqdVwN7oA1pZItgkhmRskM0/L0kVHgrkZ5O4RWahh5ZuNbda23Wq3b+OAcbDsFLmSsOJGqA0YBpYBhB1d8hPADEOxhE5P67TrQ8mZWiTRGaSDhmjwkrXSHSw+FqtSZpLWGtkAyQY7WkPiekWCVLYareU0qbU0moTNkdNyGP30rNWmYcBmU2h12iua6pxHm7IabTe3cZTEea96nsOI9bg+PZt3cxwf22aDqCx9N7qZLrI1BQQ2ScliymgSx/V6PdilowJYbdFdWUS8++D8fFcvCjq2FB+Xbt6Q9nMcrUqvqbdaz8/3155Y1chekH9wut3P1czoqhWRvfimEJAqpY9PI9TlG4roOZdIgMyU9blFJDKrEL2cCQyDu7vTo2Vk351H92WxTxkMzlIwDIDMzWB5dh6luEEwi5TmzlqThhY5bWMcWGeipMEi0KpqNgPpVooimCHVRtBKmNNgaiylILXdT1aCwmpkcbTotBzLIDOzkvszgDnXUKAMGBy7KTM1FCuFKQBpJI96P1nPqqnojbVLTW9Z/HAgA7OhZiteMvt84OgF3xYcB5WR42Cdr2kTHp72glOAiMyhIFKt5tl51MrW2tGRDyOOjnwo2J231jJqmCuq9pHurMB+mwKdzcHzvaLVzVEh3D/+yZd98FIIYLEl3ekHUxBQjG4eGUa4G6BImKG2vHV/e7Zrh+r5Bzam9G6kzoemgM7GmdHmGtup3nkwn+1ngvs6dwM41+z1nl4U67LDsbi5W/fiUKR61NIp1J5tHIqR8uILxghIkVLkMqYZMrDQxqHwIHZk6blnH+2n2tRmGTtLlNE4t8yACKVaxbjiek13IDnP2k9Zm6J1ao2tKhOtZU9nIlJJBKNlNEUG2Gkq9MwpI8uA1rifanRGtHG3i2gQMLh1RUlrvZ1GHUbTnK1qt9c0hXKJzwB2LqbjLRPL8Ogudwq2Foc7CxDjyPXGJbSWpZh739aVVrTfJYSeRdFRq3bbjIAiW+uuiq2lGcZhyMxxZUrMNQnKuNu1VA97OKw1DisCpWDeR1mKnQ08WODeMAzBDDUwuBlg4H6OyDmBwfnE0WoYbLtvqUeGDIdBykamoFBXs9Bg5gL6s+89mCLhhcWHSERqGMxLn7wBkokl8g8AEWY2EKG+bUBlsEdNnKA5lgmUUikLT4FkpFomjUxQdDNBsQjKqExVGdEqQbVJLRWZsYcXDKMPVKbNLd0QpKA6J9LKgDZzrtkCRP9kAA1q2Iw+l5ibyFyiCMphAkoxM82N0bog2N0177NFTnuZo4CXTrAe3czcMU+amgZHq71AiXkOEErWGn26YU9jFJIWvRNMvRYS0GDGZZh6RuufZdGMqQhOuxYVPmK/ywyYd98AM/WNqhkZTa1KgpEtMoWsCMqNteVqbGXAfso6a7eLYXQTMkTaMFgmducqQ65W5rTVKov7of8nc5EJHDTcB5fVx34iElmbm6f71PLa5dGsV9ZMBGIZt7cMgOwAlMw5DHQ3CtlHR0LdP+7nmJsisRRTJBqWendXqwUMFCJDoa5MRIZK6UUYZmaGDeNSr5QWnyLJ2rLrAs7RTak+ZbK1RuPg7oP1IgwkM2VTtHSzTMxzhhmZAPZz10SCUBu0Dq+9riX0z5MlL6+H2ZCBzWiObJLZktyaQQ0KzLUHA0jJmSZOfe4quVlZoWVAmbXFcFyOjznUjIaJoPcKiu2nxQ70CXW9Xzt1mK7ziOwUF1WKzNTnAueyR1UC2pzdNoWseACUSGJsABkpSVaYi/gHywS6TBnrLHMMoJmvylBbFWKzLtkp1UWOT1FmVgpJdNFD+T1Di/vqaVvmMboDojnLUlzv4mnV2pR5NHqXPncBS5+Gp0RfWt0A50J89lnvBIpZqm/eWaYfKBEpBJZOuL6Zol+jrq+goXXuqEchMCAaaOo1ci6K3s6+CXRSTnJlSjOyIdGF1xB9qW82RDYKwkyjihsNJFukwzpfpcUPqm8MIuFu0ywSXsgRaFiRY3HfaV3woOGJ1erJy8P93WQwGo5W47Unj9erNYCH5/uz893p+W6eeyqqYdFKzUbBNe90et5a6Ow8Nht74sTlOj7uMg1qwG4v6TD7oSdL3agdZEw9NrbD5Ael0It1H9jHpbYwvmVkKRrcCLaWvXBSRgOw2ZRoKbhZOtUCQZmz78eJCoWGIXdRM5oby9rmGbVla0nSDUNhpLa7OhaUoZix8DAfz8Ds5TOhJ8mgSXno1YCAqsy6TP6ZWyOWYWg6iBrMH43z6YqYFKMpS2bv3+3eGaLUQlhcNJZpkZR0sbuYy1jJw0VchC6iigCrc3ihOTMB5VKcBJx0Kyam98+vUr0pVRkZyd7VnIZWgzDzTk8YjdkSlLM7e+XUm6S65s0ARYB9Tgi5atwcXzoa2Wrk+UStHtQj2++P1zway9UnLz/95OWTkw3Bs910tLJ7nmfnW9KGglZTtFLKvJ9qYO0srh6VZWq7jQwJyFTrij3B3boyRboIgw9FE4jZAz+m0kBJkRpEJVtE/35nFgHSkaE5oCHd2RXOdcq5aeyNP511cJjTBC9SXW5DraLBdnWzGYbRSRT3YVDdIeYMwAuneXlHmQNRBpUDEUstMn9AacVItBa9JShTvdWo1kwIDSoOcPDexrEUnpeaINDJei0EBwXQzKg+UAOxEAzLFFvrGxk5kHTvRfA+sM8c7BkFLbL3oizbtM0wrLyXv9gzSUqiEhIjFJIkNx/cZb2RKSKNtQ9TY4umBEytKoVxkLpWE6pzDsUO8/+6zei1H4LIRESSHMP3wfVQ1iPuP2yNq6uXTo4HXb68unxy9MSlk1J8mtr5bjdN826/v33vtK/GMpBkX5UGcZ5Fi3HwcTBxISkicrdTCmVgBrqrdmdreVD9oQfE/WNP685xyfhbdI2aIjthoiWi4EFdH0tWKsiLZS9EJrbbNk1hzos6og8GQBnFzM3m2gREVVtlzg6q2SIu90KFpn0DuBqlytPTumolNRel5P3dF4NbivemGuVizbq37/Y61bcCi4SbdfkAEl64CPaVBM0FeQ8X3BYlhBkJz76sDgBZaOlOqpcYOl0c6mo6OpflFjS4e2aniNGtnZEGN3Ic3GiZGVBw0W44HGTP/iB1jbIVc4fT54heA83WhVqIkBUWkkCEsoZcRiRw6LzrzQ/ItoQ/O7Wz+3eO15fXm+FhZLP9bnv/s599+oXnr/UKWrbct1mKO/cenu2209z7wpRmq8HLYCnNLZgYiokisZs6UQKJPsC6hmWJPAFwGBhB9YvYdY4FmtFH0GTokIL0WdU0QkZ0LKLnUtajEwNSyBmZQTdJLaBUplAxE8Ye+qCz327WIt2tL2WddlFbjCM3Kw6j+Wj7OYcD5xANgiTOcxpQymDj6OhReFmWoEukaXAHVAYfzIQEPFIKuXdJPdcrH/bufQyKoUUfkEKqB3aeXa/ZqQpbPn6PKsLkOJRSeoN4n7EnmFwA3A3D6HWOrgHpjSEsyED0RT+JpoRQ5xiG0omPXk+isZeWWPr7aBjZ/UkmWHIcRJoRmbYYrZ7+ECTXK3vq8njvdJ5aIFlrltHN2CeI28jBSinW5rSqs/O5GFdHw0C7fef9eb5CGpDzVLf7ab/f3r57+t7thz5QYildd4xhKF5Um4qbEAD3c9aqTIgY0MvHkDRXdRqvCzCjVyCLoWYsertD7GNc2h8WfC2kI9BrzYi+zyhFN3dkCqklq2nqJFC/W6SxsDettkB0MTuW5oJxYHHPTDMoMtIJK4WXjoapJo0R0dmWoeR+CkHl+KS4Db1LqUX2iUBKFXrnbZcu88VEm2W4W4+71+sybBfiLWRmfXkmAZpJ2dBDx8yIriVeaB3rI0CF6LPb2T+OVM8VUiTHlR1vfJrYZi3a3aS46NM7jQcsAsbIKEY3ORkBX9w1Ll82EL28tNuqNvnAoagU84CiS6ox14P3JzarMq4GX5efeXLzxvXTqbXVUEC5YVz5PCdlx6vN4GX2trfp4fm8GsvVKydTbbvdfH6+f3B6Wucq6PTs7M698zv3t5IY3uPSYejkc4zDULOtN0aaG+aGcWUJkCrFSZmhVg3OrnmMLuombUBmTqKr+/GlVWLpA2KnLxOkQXDrmWPvFTLvOuPucxnLqDuG+hZBGNn323c+dImxJXfr7UKkevhOY/ECpKRakSkWKylzbtYjiRYy4iQxTSxDWZFAejLdyjKtvXMdolMAemiJQxU1IgRmpveW3VB0JqeLVLo6uG9morqDqwiLbKJ11T9AsBTzohT7xD0Bu13WSHdTpsHd7XjDPWLYeCw7r22asmUaKNBBc0JarQy9+E7VFNLAFJGpYWTpHeZHWaslksBYMJRiVG2MptHVZ0uaMTPmfd7ZT7qyOjnx3KY5Milh9PWVy6upRt23UIh69tplo568tLHi2/301JMn48oNWq389t2Hr75xaxjKfmplcNUWffmjDau10wBmbXNkFreEBqcZVytTKoXWpMTSQQjJMDhb9vERAMxMZiC4n6UpDrsBOw3dpxJCpInwXhXl2MfCUiSLWY1orddMZSQWtqir6jk4SyEBo/VphmXg8P8S9WZLlhxJmp5uZubLObFlJjKxF6pQVd09PcN+Al6QLz1zxRcghSOktHSxZaamqwuFLZEZEWdxd1tUlRfmgQFEIAmIACHIY8dUTf/v/5XY3Go1rQDkl62kxEFQzbZsIUKKsqyaEGtWiUBBCJwEBVwliAOQkZmbdhsE9JNu2qflgORmQADIZGYIqO6RmRsRovpejYUQCYmZHGKQGLiprtqAujJk5hCSpIhBiBEZ3ZGCMAvU6pPgpVggUMWIFtwRUAYSJkVjAlcck/TeBJHAukCMgSUEbvtBAUBo1nJriNSnmEA+JVJBYgaEls3QJeKIOA5BGyxr04bavFZr1jUu/eaT2x+fl8dzxkDgqAVOWxbG4zzc3kxDDPMYkjARImGtU1Vtranqdz99+PB4uW7tiBSiaDPgvreKQ6Ahsblft82siwo6DKxm0iemBNLH1Nbxp30xqrsLdkc2IMI4YK8ARGBGrao70U5EvuiAsJO4zYDBEVGYbJ89IYkwWjEjeOmdGQBAzSRQFBBCNGyqgTvgDs2MBBDgurVxxCGQuiPQ5dpacy5OR3Tw67UwASgDaC66bVUAzE0dUdUYkQXACcTMSDs5AAAI5q66y4j9/w0BxyTA0KNZglAg7oZK1b7QwnI1ZBgjChMSqkIQTJGYMDCigwj5nhWFEk3GeGzuiK5AaCykrgpW1FqzlEgiJgyAWIs1RWQcJNzOU7YKzq+nAQmL6nVdTtdKhF0dR0R2NCYOIEy1uJmToFYoruBeq9emY4qUeFmhbSpISPjhvNQaHuYZCYfAIoQA48CEnGKYhhiiEFIuJedmYDHwtm0/vP/41+8fY+B5jM0cYQ/DikFSZAOPwkW15JqrluopsBm425ad2QFQBJiRus7rpvaiGjv0T7w1IHQJxIggmBICkLX+Ae2DD+qzCfCuApshkSGQyE6+MBESBNidFb1H7hKVFiuKRsACwkiE69pCJGauquMUOHAIiEi1Kgs+PAy1mqop4N0x5OKX67ZuNUZyRDOQFIdm1VS5T1c6xQQOvfD0+QIBI/eEghiYCVnok4fjJ2/Gnx4vOVsIJOQd1Ud0ZoqC1vkiN2GK0ie0PaVPwQHY0QDdwbFVF3YC6iNQcOgzjKWU6rpcPUQ0s6bEgvMI4LQ1KMWseS71/fMm4gjw4y8kEUuxUo0AmEAVHE0CTkPflOC5OLiHsF8GbtCKO3hgQvem2olcEX7zanz/cX16amZrCvLqfnx3uJ0PgxARcQjExLW1ojVnXbdSWnXV94+XIQYkOF+zmu8sE2JkKtSI4O4mubu1puDaoD97O9gLDsWMEZu5MBrAy/4/rwreLDBJQGFggCV7UWVEERoCCtG6aingfRrp7taTtrBTDj1uQl2hoblp8xj9hWHHKJirras6AhNYl1TAWZEFGDBEAXREmIbQWe11tZQwBmlmAPhwP7tZKcrM8wEC85rr8ylLQOYoT89XDuQOv26H6z/YvIGhgVet7hBl16KCIDMHZmJglH/89rPvf/qwlpKLpYiA1MwSQyDscE5tgGal7npcjNhDpro0txVjll7phFFob0Fz1dO5LbmqgSm4UxwwZ4NC2lpK1GeYwHS8JQm0rq23wWXxZg6G/frsYjqAF1IzAoeqNg0sTP2gCRH2CCIkQpIAWB0WqE3z5p/ev3l98CAyT3Ea0jSmnoDUP7Ra9023IXDO/v7D85Bkyw0Ab+fx/oZaU0AqpYUgQwox0OmyjEmgFzJEc1dzKLZbMhFNPQQUxtqsD/OICR0Cogsy70E4MWJKcl5aeZlCz4kE4cl2Rx4LmQGY+0tQfx/+leaBwB2IgQhUd3FRzZkRAvUuEvuInhAATT2rxiiq1qeIBBgjtWqtaQ9iKogl124MK7Vi86rqbscjIVKpRXIubMJEhi9PYwA3U3PqrlnH1loKFAIBOpgNg8+RS13++tPmaMQtJWfGvHsTwKjj4SpM1pUbc4luRurQ36/IJpEodDwLkQHROWGITASnD+Xjc+kMQmsubEi8bRojiLCbx8jDyGA4TNJfYSU3NBCB4Niacxe8iLqHdhTsRgEhtgalNQQ088AgAcEIwJHNzLeNnp8LEf6PcvrkAT/95PbNw+3NcY7CaYhjioC4rjmXuuVly3VZs7by+Hx5PK2ff3I7RF62elmquzc1YVa3FMNlLYdRgpA2U9PAfHuYrlslQHVH3ec988hDxBB21W2XAKGHGgmilwatWqmOhEMi4u7L9XOzMZEwNt81TeadUe1PR+pPp+7W6S03I1OXspyIzJ0Igu26ivfyss+UEUBFEHf8HsxcAvTOMQRw12VpSMDe718A9BD7heXYTCRgDGzuZiCMhNCaixA3B4IhcIwYExEoS4cqXaIplgaAALlU7yR1w5zVEYbATqT4Ig8QIUFiIoJqDmgviL9b86am4AFZGFyxLmaL1+YfH0upTrxvFTaDLSvxTuawQBzAzbbqlCEmOs5UY3B1c2CA2rxTzswGKAQooGTIARW6Xxbc0AzdEWm6meZAJJFcLVD+8CHPUyKk3//m7f3t8TAPKUVGNIDTZT1d1i3nUhoSfHw8PZ4un39y7AL8mtv97WGuerrm2lSYRYiJhlF62Fa/YWLgGEbAjRB6xtsUkRjdIcbeqvuvs+g93AAdAQgxBTfbZ2NAlAKAY97cHK6bIUC/qmHH3GF/ySMwoQNwV3gIu1ppu8JEgED2wk+472uckYjc1JF2f1BPznFAoq4JQrfC9M61Ni/5V7MCODj1MRaD3NyIMBNCKT4PbOAElBIaABEIITOCAwUIgUpRTKiGatolCwIC2uNQgmBnGYgwRkDGzRTROCISE0pbGzkUqz3ybivqChKR2NCoVmvNa/HaPG8+TwzU5TZfrlaKJ0Hu584BDFg8JYzRGJyZe5bPlsHVhgH7ONAMEa0VqOZEnjrjZKgGDMAMS6FfPpR0MnMPgq9vD9OQ7m+mb7589ZfvHm+P08P9UZgdfMst15q30sxKaZd1C4y/fHx+/7jMY6gKzPzxefnrD8+I0F/BbjAMQkRji29fzSmGZd2aKoCPA4l4GojJWSgJKoC61wrdHmLqyH0TA6hBd0wBAjhuW1OHKL3+4SBUyQBcmGqXqvElPB1gJ0vgxb/WM8E6AwS2w2D9/O/qFDh4x177bF8NrGlfJQ1qDkho/ZXR51+E2Ju/HhLTQZUXA8a+41Ae7iTFAIRqGpljFHDQ/uow0qbgHmLnnsF7IUeSkXpYkCs6oCs0VDVPAwo5Bcvqj6dWqh5njkZNWhIYRmrVoAEJmvko1Pd9BgJTtOYE4IZJMN6iREhx7w8OAxLgdW1JWITI3BvW6oheNiPAEHpOeHelAiq06k29FEMEMEwBmoMYuYOht546grhlq9VUdRriq5spJRHCIHx7mJieYgrooKrnZb1cNgRX99a0lLIuVw18umwdTHCHGBiBtFOLaiQsTMOQmChEOR6nMXCt1Vr96en03fvnm5vAiBTZ3Zs5IpqCqjYFkT58BAqu6ltxIuvGMTAo1WoDTzgmrMVSohT6CdmVFUDgPWgLoAPIu37+klazsx0A+yLeHRDdqYEOe0IHbX6VSuBXIr8TrSzwgvb2oZbrHqkNImDWay8RuBPKlhXJmJACITtLd51yqw3IJGDPldiKMhE41qbFTFdHAmbQBkwIBs0BIqSDaGlO2AxCRELadYCGxT2BMwElJMeqTkLobrY/uSWANZewx+AQIiM5mqmrgkS+vw0x9NhRYAeyvSaYw9Z7HEcw3yq4uhq27F0qDOyMNMyHw3w4zqMQI5q55VLC4zJOyERvH45vprGSX7YypjANCQm06fP5SoxuwAzXaylN3eqWK6GPKaQUcrXLWoUoCiEiM+8ECmE33aTIgGSqDb3WymivXg3u/Hy5qne4ruOv1mHPot7U1D1GEgY12IoiYEzUgaLaYEhDCJJzRrJgveZ6VYd9iA8A0JnzPeEZ9+C0Lq7t7nbssXP9x1PPN3ihbsFfUGUAYEYzRyJw7yPrnSKj3smBGdiv6CHus9/e7nfAXEpxidYajiRAsJZGiNpD2s1jInOTUWjBnI0F3KA012YoNDDFgYiRkKgaqavB0lDRY6TjEJigFS3VoGFIWBHcVYS23Kp5aNRzfUo2RkdkYXSwAvt3S9UBQQINyZmByEz7VxZdd46oA0XA++8pEwWBoiqMjUzVm8GalZhH9fOyni+GBK/vJiZUpTcPcwzJHcBxRWXi1vQ4RTV98zCb6umybrl1fMlcQfXpfPn+5/MnD4dxiEEYYB9hlNKYqTXrulxKUVWZ8PY43N0ehijasqmhKJnf3xw+nK5aUBVyU0QwwxipXyDNTRUQrJBvudPbzuRG2KpHoZjCYRyuSwe30QHUXlbcvyQF9098x7T2f7RfbF3dAkcgx10Wd0BEBnNgcOh3Z587dXqrq+KESO69IaOuXHXrTD/KXU1yBERCUzAzJnJ3ubkP8xwREIG02boVEU5BFOC8liVbzjbOdpxjFAWgMCDX1ho5YEyhVBsCp4E5emhais+jONq21qY2DdIHVEPCpqamCMhijnZ+Nma9v+MgIhOZeu1oCkCK6A1LMUHoCHe3HLZs3lOzzACQAJl3/RQaGgMAghCYMwuQpVHO51abtuZYNdfFwd87IsH3P4bXrw63c2pBkGgaa8BuEwAAIABJREFUBhEKwiI8DEMK5AZff/7aAVPgbStrqUJUS95K/vfvn3K1JddSGhEepohITa1FVvOCTYQRcRpTLrWUStQFHNdmwjjGJFG20mrVXNoUw5p1SBgSmYEBmVkzV3UmcGDoYZMGJdvdbWpstZq19boVJkPaRzz+K/WIL7dav3M6DtnfoPuN5rvjiKAfDhByNWBAAEEk4l5MzdwM0aG9bJBxNyJi3EPsAI36EwERESSAqjGjCLYGiEZEXQQSM1QHMCulgQE4tGrLum2bmzoLzDMTU86u5il5GDhX2oNkCULgWtp1beQABDGRVgVzCbitpmIIwOIA3oo18yAogWoFZo+RANHA1BWB3EABSGAIqAzIFCL2dFJ3ZyQgq81bdbXOxDsgBEE0AAERMsdaFAC9WW5WipXiRAAC1ElhIEK8O063h3R7nFKUMYXbm+kwDX02K8yl1KpaSkuYaq3P5+2ybDHSslyF4IefT2uuzFKrnq45iqSb0M/Zy7cZmBgJRKSU8vF5mcbUczlU1d1DohTj6brW1sxMhI9j2FqdAq+LAToTmlKzihBa8yhATjkrOKxrTUmIO6gjagUBqvnOmL3wW+hOhO6wc03et9l3s/R+rXXyCgH2tXC75412jkh3yKaLrV3A79QC7WyFQw+UNMCwr/cdRJBRrYEjkzWDVq02q8WktZZXJAdr4A5FtVTPxW6OSc1Z4LoYgdXWAH2I4rdORNtaiWEYoGwlhq4jmFYXIu8TP4BpFhEYRswrEuHYI94ZopDWRmytwrr6PFLHN8ZEBlgrdHuHMAQhIlDAauauxIhI1bxm7clCDg7I5s5GrRo4CNM0BOEA1j0ilkvbSlFFaCkJ390Mn39yd5zHcYw9YvgwD9OQ+tc4b8Vj8AwFW97K87Jta0bQZcmXy3p3M8YgRBXRH0/bx+fVHBgRmUptnTSRwExEiCw0Rh6S3N3O6FZLdbfDFMHD7TQsy1qLEpOD3t2ly4q1ejNlJu6KsWJTw0ZhwClyh50IsKr1UYJqcYBm8GtUWmfFdg5/7898pzdebjdClEHq1ujlPuvUBJETozCKxFqqvvAaQN3Mj2bOPeWCYP9bAiaSEETC+bIC2KefvT0eD//2b3+9XJfWTGuPOgAAEKtOAZEgBixqghQT3gBQZDBYFtXmztCqDkmI/XIqMeI4ELhpLUPCEFDEawM2JABiXJZebbmqxcaA1NxrMSKMgmh+mHkcuUcpCSNRDy1jdAX1apALAFhrMASsaqWpGgQnNWD0xSEK1GLE0NwcIG8qTJ+/eXN7mGIIKTAApsASuDW9XDdhClEYmRmnIT3cH1OKRATmjtgMwNt6rYSQS922utV6WnKpZVmW94+X61JeP8y1qfTgSaQO7fSBQC0V1At7K3o7sFvPgcVxCN1oum7FBRA8BZEgh0P88OclJWnNkZwI+oIpETTz0uNDDWpRUwfHecbpEMi9qDMCMeueg4d7or4j4L6tGXdbyf7H3tH3WYUTMmpue7ZNn5yREyKRC+OXX3z66dt3f/3uh/Ploq3lWmutaqhqPSZtj/dyMHVmfPf27T/9p3/607/+N/rpfXP9uz/8PUv8/m8fiIp73Rl8RHCQbTNAFYEUIwEYWKsQAqBaU6/Zbm9CM4scaG+5IWcnsOORl4uiExO0YuNA19W24h1IDGLb2lLk09lqczNDtxAxAjuhGQozGDBjiuTuxTsOBkhQimtzc0PDDL+Wf6vVicDRp5FDZCJF8pAYAVW9VXn/y/p8KkwYRWLkKBwCT0OcxxhTBPcUBYlSDLk0Yk6BqhoTqSkhBSHqvjagay6EWtbtpw/n03WD7icNfJhTX0vS7CVuzR0acKAQuIZ2e4zbBqW1IDwMSa2njVhrrqa15c8+nZl5zXUcJG+GQGqmqtYA0ZiQiQILswIAExBjq47YukmREIkE0duW/UUpxBezUy+HtE8sum+HwIwIe1GUQK0aUY8lBN/ntw5AMaZ//Id/ePfmk3dv3j6dn06n88fH54+Pz8u27LtHENzBDMAxJh5SuLk5/vEPv7+7vf/nP/1pHAKz/OXf/3J3d/jyy09//On9+58/5pKBHIilbABuhxsR8VyBCEvRliEN4ODjjEIOhsWsVDeFWiwECBFrwWEkIkpJtNZ1VUQkgFw9iuXqW7bWgBCauqtNkQYhdyBAUgLaR1x7A6A9+A7IfQ52MaoFMIL3KDJAxT1qi4W1mpmFgYSRBTo9vq72+MuViXrkcWB8uJte3R6YMcYwRBlS6M1ySmmeh705cStVW9Paaql2XdZS7JpzXhYm++H98+ma3fchuyoI8ycPB5GgBmZm5mpWawNEJhYhEW5Ty827zT8QNjUiaq3dHiZzv7tJH5/OzXFgloPXYqqGRMLajF07gGPCyAzM1CfvPRecCWMaWtNa28uhghcjGPYDhw7djbj/CpyZXvANM8Xd448O0GPCHIGY6Pe/++b3v/t2mqaH+wcDW5ZtXbf/+//55+9/+FsaghuMU0Kny3KdxzEN6dXDw8PDw+F4MwzT8eYmpBDi8Hd//8cQpFb907/86//5f/3Xn37+yd1u5kGI9tvLGwqiExwn+dW6tVVzwG1rrUIgaO6hUx0Kpdg8E5C1pmGkgL6tSAKTYApsAMuqtVggmBJtSkNg7vSAUa6A1Uvz2ox4Z0LdPAj1sOgYUYFa836JNndi6oJdZAQCM+rrZ1Fh5+EdRATAhhge7saHm2kaUgwd8IEgAkgp8DSNzEwEpbTT+TqkBOjPl+V8Xtdccm65ZPQWI09JzJ0Q1NHcf/j5/OFpFWYiPhzS6bQ5QAxcagNHCUREhBiEmDGlGNMwT6GVkmsDVW/NwHp00vfvPzIqEgizuxfVIATmxIABS1MyRIKOHPYMAHCYptHMmOXh/v67739A6v5E6Ju5iHbvrRMg9H8dmdB/3ZXGOKUByE2taesRQOZODkhwvDn8h7//+2makTAOIxGk4XBs9csvnoH8f/mP/2EcpiDCjOY2DqO5CQdkAsAQ45u3b7rLdRxHBPzrd3/78PHx/v6m1m1Z1piizEe6PaaeiyiISOxqfSGCuR9HqoZDkBicHOLEzXQp2hQEAdRNITdz8i76C5I4YFM2v5m4NZgSjpEGAQmEuPsw1a2tXprXHixlLoHcvKAzAyF6hCC4XpUJ5nF09OtacjNhVCFFR1cScEUTCB18UEhRPrkf747T8TBMQ0wxTlPsAsw4pM6KAfiybNMYmWkY4uWyPJ+Xy5KXdVP1WouZPtwOfcr4+n5+Pmdm1GYOkK+5XxZP56VWJcYYpFUjRi4UhAEhhnA7RwT1vukiyuW6Rsai7bpsKYWffnl8Xlci1I5WIFiz6o7MCNaqCZOS9+ciMQiz98BvDuOUlmW9Lhv43nbh3sz0s4YdQzF3RJAQhOnu7qaU9uHDozAT4/3D7bs3b3746afn55M5BmE1JaK//8O3n3766a46Aai5ObDIN7/5Oo3hzeu3EgLhviauPzG6kdph9y4zQR8DdM/wb3/35ev7f/rP/+X/2I6X//Qf/1HY3Tal5ObYmhI6o2EgM3MDdWKCIaEq9NF9iHg3xHVtSKCOMcC6uLozY6sO4lGoNY/BYwpWvIsZuzlRoTg8b64OSbh1YU3d3CMCBRIOYwyXZdO+iwzxZQeCfDIeAFACCyEHNrPcqpuVYoaq2j65m+7m48PtPI4hhDDGGFMYh8gk5jYOCQGr6rJsAPZ8vpbSLst6Xcq65XWrWymtVjOrTb94e0PELCS8irC7ozAgsZupMbOamdvtNBPTueUgFGJkQjcPgccpHcawNTBtoLqsJcxSqoWBarMP58uWW1EQ730hTLOgQ7MdiOyPOkKf58P5fFKzTl5vuQLg+XIlvHZPwN4dvuBl3XTRoYmQ5B/+7vdffvaFuf/rf//z5Xx9/ebh6en56y+/+OO33xLJ61evjsf5OM8xhpzr73//u2HoS2S7/6s3YzjN01dffEksXZFSBepZMfBi2umjVzDvFd7BwG/vb7744u3HD0+E+tvffv3b330jl7O2sQblvlVOVUMELq7qat61W0YkAmBUs5ohRnCHUgwqgpMDCgJ7TxKFpbntGLe12jrJpA0YLAqS9LwJBLHESE5DRLfw9tXtum0/P16WpblaYBySDDEIpXk6TMPQNRwEiLFv2sJtq6pGN+Ru5h5YxhTnw3BzmPxlRUGtptxKbafz6t4DOPs3sPvHPOey5lpKLrluuSxbMcd//+H09Wd3pZqaIaDt0cOqbVeEqHshATqPxYRMIMwUaRhCEHaHWgqOQ2u1aTtMo4tY8zUvT+cVkMAb9k+F8Lo0JhJBFmKgstkwjYd5Pszz5bq2nKcplVzXsi7r0l+7IVB36Kn2ob+7oaEDWhD57TdfPj2dPv3002+//d2yrNfr+re/fX+YJwC7vbm5vbn79N27aYqvX78ehyGGoGYxRnpp2nZHDu41OaZkDuCg0O+aXw1oCAR9DyYR0q5tAjgMw9gcQ4z/2//+v97d3QGi5GahoYGhOzNkNWkI+3JCZyYkDNHRUXrcqyAgsiAZWvNa+uSaHAyFDMDNq6E211bRQcGsmIEPwo7mXQirPfWToI+PmXOuWg2dlrUQoiBtm4lEOQyXqzbNQjuFMI0JwAMT7KowCoXb+5shhpxzkJBzDRK8r3ivVZurGxMSIRsBelMt1ba1PF2W2tq25VpyLu10zWYOiM+X1fy2Nn335vbLd6+q+uNpuVy2x/Oi6kRUmxbRMQkATiNHCZ1cSDFM0xgCM9mWizZxdzAPQUYDD9r6j7N9olqqgqKpxwTWEJsNiZBxWzdENjORUGsVkXdv3/zl379XbYi71/wwT6XUVTfcZUhHRBY21XXLf/z9bw/zwR2maUSA337z1d/94dvL5frVF5/HFL/44tNhGMcU+zHhnoTRzblI/XghItg+lyOA3e25/8V3icvRyAjQdrDNO1LijmgWx/HdcY7C1/UirfrGGhoqQGlmgEzI5NrAzVicmIy640PBYUjMAqaK0H0Kbg6tqghGdFXI1d2xVjWD/j4F05hIwdCwmLm/TBe1DwZwHg1afnU3v7o/fHw+P56zG6yrecnnRYkxBE59XSA4wnkewjSlGDgFcQBnW65LzUIEjDTPQwyy5kIAEoOROrKbB5GtVDdDoBQFANrj87Zt4Lrkel0qIoTAAHRzGEvTbWuA5OIi9Nmb+3xXH65V3Vzd3M330JeeUFDVzpetD6gREdxb0x4a2G8dQAD0JRdENFU1QGYzR4MgnSZkh7auzQzNaqntfO53BV6vi7D0lLfdqO2wLpt6w/0H7iY1M2Ums/rHP/xhmg7mRkBfffX517/5/P7u3lXDEBHh5nh0QOtFbm+3uloFgD2H5VfnendbIXXfD/Sonl6xd3OKIZCBUn/mWp/UOQAa1Gbu0KpJEHT309qJkn4hGhFCd8s1i6FrF9a0zzWcCE0NEJL0mC4o6oOgKqijqTeFXLync+GLp9cV12a14TjQKFSqbWbasFW9XM+fvrnbVD49HMDtWgszhZHWK65LY6da60mNkI5TeP1wHAILExNSzx8F0KZm3j0XzCR7qCLWWhHQ1FT9umyXZesbdGqzvOVtW5joutbTZUPcJ7CAeF3Kzx8Xa/50yTEIE6+53t/OIYS21fM1z1Mk6g4aYpbaLBFcEcy8lrqCDgEJoVYV9iDSPW1r1ayt84xgUGstxYQgBBnHybRtRa05M4qICKl6a42Y3P35dPK+daJzf+4UOHDsKSfdl8uMMcYU5Q/ffjsMQ5c81bVXLkKixLC7NPZ5QmeDuk2mn2lD600++W4N6UnoL5oCggMBqoHvhnLcf2Ho5ACAtM/1+iJ5M9uKypZdgrW2LzIkQgOwaojYTfRmUKvTPqDr5YzV3NRbQAELEZer6iDc0E2JoDZwo9a0O24IjJABYdsA3FuFOBIqIIGZGYCpfzwtMcnlKrn49dKIIQ2BmYYxIEBr7TjFz97e3d8eSi6I0IdVtzfzNCZVM/PDPPQWrhQ9X1cmrOrVWsmtttYDk7atqHk0Op2vJZcQ6OaQfvxwQSTqW2cdkeCy5q0qIdXWEDHG8Ph8ef/h1FOYl7UeD0MSDlHAIUR2bUNi6AxWt770rQXa5mm4u51r9eMhrnVZl5pGmSc5nzctlrOCsA/w2bt3Nzc3f/4f/3Y6Pe/CuUNf22OmCGSmItJaAwBmUjUJMg5TqBXRS60xijY/3ky/+eqrr774Cndc0BGpz+VhDwXrnoEOxO6hEq6GSEbO2uHuPR8Md/oDCHY7LgJ08h7BFRAdtUOU/VwBdZJ7vwixPwtM1SQ3U6dfOZA99fglm32n2gxYeL8Ue7ffx8kGzd0zIFCt7g7WDBjBKQhrM1WQwHNkYTSBaSAFN4Pz2lz3kI7+Zqqlns/Xf1kWdasKSMjgql5LTZE/e3345NVtjAJuwxCHKPM0xCgpptrUDFLq7iOttX/Y1poDQGvW3fC1tU5PiODj42Jmt8dhnlKIIQiZuSMGBlUTZESstTZ1JkKE06XVqhnzMI6XSzYzIrzmOoKHEHJpYHp/OyybrmuexoCO7thqcw/CGJiQKAa+LquqtsKOwCRuGiO5mamfzpd5nqdpqKU0bXnbuluREDiE3pnX/lsMDiDjGLQ5M4uIu93f33/++WdPj09vP3n1m6+/HodxT0FDeEnp6ZSYAWDnwPtGtS609JqOBoqGve9ysr7blqg3buiABP0BhAhGRH3nONAOGv3P4+W2C6f97kV3kCEF78gaYYjhzav7y3U9nS4AgAF62ocTlNbfsiAs5ibEjthac0dTcMdWfP8mNDf3+TAcp2Sqxyn99MvJHcumtTnK/nVlBnYAxiGGt1/cbKX0GMtARNp6xMLdOBzfDEMKMUgInALHOExjvDlMMYba1BxVbZ6GEBgBiXFZsvcwBPU111zKupatqJk21VYLmC253h7iYU6quG5l30/Xv9q4L/hBIi2VmbbSdt2gf7URiHBIEoRjCCxcW72Zh/ub+XTNy6pmFMMQBMxMW0sx3N+lGHieWJtJYHdtiuMktWBQ7/FgT09PIgQOX3395eV0+eHnHwiAmN09pWRq67b09tS0GxSltfJ8OgURYg4S5vnw7u3b4+GmVxvvjJkBIApRD0EkIO97wwmx53RQ/xPIXjIo3Q2I3PzXKLyXgdzOg9AeCrWTHd1YtM/dduMJAVo/gICGgATy+du7dauPp3x/NxNQCnTWpurzlL756pMffv5wumYGNAZyMPectRt8hyGGEJ6fr10VefvmLm+rmvUqNo3T/YG23LaSUwwAfe2jAvakz56R5NRAmFkkgrNUdwS0iGEe4v3NUYhDDFMKITAxJ5HDYTocBldfc+vq7zCmvJVlywQYo0hgV1u2au61tpzrdSuIeBjjh6fny3Vbc81ZP/vk5vmcETFIn9N1myOwUDcEEtE4ABH1ycWWW4wR9rBIi4wQAwGhcAiSIobAjB2JkRhoiIIIQbgvb4nCAH66rtVhHONB0rbmYQiqPh/mw+Hgbtu2uuk4pvv7u3FOZna9XGutTZWZc0ZiJsQCxXsPKoO5T+PwxZdfvHp49frhlYToALUZku+WEgQiUtzvl47a/nodGQI5OSkqOfZdpLBD/QTkZD3yCRB64mFv+V9W2+iL2uXo3LVBB0Tn/aj1mCUkcCKUplCrIvrlsjERM7RWg0Ct7a/f/UIMt4cDET0+n0OMpdavv3j96s1DkPDz+/eB6PPP3i7L9f0vj0PASFyVSzNb6/l8RuUQg0hIsZrpZDKm2NxDkF/LNwCkRDGYgnt1Q5+G8TgOKQ7CHAOnGA6HcR4iC7MIE29bZYkpBbeGSOu2rtvW1McUzAy7Ptt3i9S25YKAjPbx+bws+eeP1600cPi37x7fvD50Et3dhRGAzK1WkNALuufSonBuPebZmxpA7fSfg7u5BEJAVS0N1jUD4hADgJsZ7041uC51KeXTN8fH51PfNOEGgIJYY0zDMNaWS16ncXr47LMYAjPHGN+OnwDCd99911qdpunp6XkcUi6FmWKIxHSY55ubm2XbPnv37nA4xJBwpwG6sdF7awMvKS99ygV91Roi9ajAPnI1QIJfXYgIBNQNsIY9zRQdAPK2pW6bUe894gvfvZdl971s0o4oAfc7xSkIyoePTzGGGHqomZ7PioRDYnccx/jbrz8Vsj/9+QchmEYG98fTUmsNUQhxGsOHp6en56tpW9fl83evD8fxn//078IYI0kQc0wpEvE4pJtxaOBbruiu/QvRzMGI4OaGEWDLTZsQMjMNKfRzxUStKTGHGFtt65rdYUhYamml9bs6xjB1b4qqFl9zbq215luu7l7zeiqtVv3xl1NthgAGHiODGTFtpc0pzGPUZtqvU/dcVZhu5kGtXZYiLIcxxBh6h7u4qboE7B7GyDIkvLubny/5uhQEcHVhYOY4pI/n/G9/e/r2q4efP1zWrcbIWt1C65To4XBUjcMwpjQ8PDykFLv+1FmAb775be++7+/OTdu2rUT86uFhzduQxnEatWkIIhK6P4jAezAiEroi0gtFhmigu8WXEBDdEBmx9bclkjshIakZEWmvpmZEvC83RsRSW2vX6XAAMzUbUgR0U9fW0hC7YG8vRC9h58aNgEUgMkqMXfiC/T2BgMjzOCxbPi/lX/71r2/uEqMepvj29c0PP35Uz+um4NK0Pj/bttW7mzh7Ol/Leckfns5V/dXD7TTG6zXfHscUg4ox4bXUlwgP4t1GA7XoNEcCuDmEm3lqDUoBAxSm7nzkwMK8bsUBO7fjBmve+vXf1/6MKSLj+byWqutatlwAYR7jltfL5fLh6fp8Kf0aCSKI3tRFSERK0dKMhYNImHlZS2+O5xGQsDUz5zElJOyIrDa7u52HJOtaOjCN4DFGYSPEwN3ryKVWa7KVdlr16SkvW3m6lMtiW3YmDIfAiOPx2PfCPDy8iymCIyBpjyo3d1ACxJ6vTni8ucUdWUVijmnsDVIIhER9ux66G/QVcp2u6n6uvWxgDztF7M9IQ8T9muveJVR0UnS0vkwYwJkYrY88HBFDSOu2hlxyydM0dZ5q73qv6/EwI/VAp5fAYgcDUFUmcgBJMbEI7juZiRmESVtttZpCMfjlua8LoR9+elQAYSmt5WJjiqqlOQrJWrI5/PTLY1+8fL5Wg8jEW645awhIRLU2IcLI0IAJa6vgNs7BzHKh06mUkonIgVPiEJOrVtUYRwc38y1nVSEEoH79Q0pxSKHWtmylqeZcS1MHG4Z4nGMM+OOPP5+v2+Npq81YCNxJoDYvtS1L7r+dgQUQVdVfYjV3IXk3ISHxrsX0WSsjztNMiGtutVRVYiKK0tSaWqvNzXOuZum6FvULIonwdz+ex3mOYTeAz8fb42EOIaaUxnGCfYIA2kzJqPtzXyjzftReTHF7KBgi9AWNZI6EvgubCI5OiNaNddp7JO8V8+Vuwx3ncCL/1SrQO+Zm/YXn4OBeQggsAu6AziwAVJper1tu7TDOyMhIuVYCzLX1WwDBqzYhAiJTAPJSQdWkGQgSIvfANMJ4e+BtI2Rp6tCzjhD7o0ybunsKGIYBkALQgUJRv709Eq+fvHq4vx9//OH9lvXnx2chGsfoqkQYQjjOQYRbUwRTZlVUw6DUHAPTmj2mAO6m+uFxmzcNgYLw4i7CuTQASFEQKQRuTWMcmur5fAUkt2oOzHx/OwFg03Y5nZ9q3Up7Puedm0AydAAQpqq4Zh9nYiJHQqBhDOtani8bAKbI/cDVokQkjEDUM2ER0cw+Pj6NSQR9c2d3M01xZGZC6HqogyN4FHr35ijMb+7HwO2XX56GQXpi3jgMDw+v/AVP7GK47wYuUEciY2YzFUEgZnNgMv2fZEbneLE746A7erFL6+5EhK5dgfU9Ohr30HBzc4AowVwRkUXcPJfa4zN6jI2bdeDzfLncHI89ek8tM7G5xZQeHx/BIaWBCa+XZT4c1nVdkeZpIKLWzMhCCNoaMPbwKZEgxAHBAFmEarOffskp8DCOpemuSjiYQhoTAeSamSimEQBLXqbB//GPX37x2Zv/+v/+f3e3rx7u0o8/P+WqZp61ltq6yDrPcsMhCJ1zCUQkGKP01FMJDIBBWISEpandHD0IEfE0JuFfCz+4+7rmZc0pCqLnbVu2WpvWsqYUt6yHafz6y9enX5Zp4J8/PP/l+6dSrZfX3gb3rTMx8HXN6w81RAkiMQjgTS7th/cnIhxTHIfYtF2u9TDFXnXcDImmMTJhjDIMwbzn7nqfhsxj2o+K9AEJv31z0wG4cDt++OVRXZlwnIbj8WYcByYiYt9FxZ33s529BPPO4xM2BAFEMmvdqfSrtRz1RS0C7pu3e56sm6lj78NwF6qwszuI5kBaa+s9l3vLJYicT6clL1HiOE7PpydVPR5uQqRlyaVUAJjmaVmW4+GYSx5Sui7rZbnc3d6uyzaMyQBKznd3t8wUQrgsawqct1xyjinO8+juwsRI6ApBOMShcSvZXJK6pGFQM3SXEIQ5hAigr+JUG5UG1+vpze0wDTKP6e7+/h9+/8Vf/vrzn/78ITduQKZ90xKwUK3++HR6fHw+TvHhdhrnEIRxl0IwBHFHEazVVVtTDcJMAgi1aX+O16o9KW0YhmlIxESEpbQDhy3XIUZmYqnr9fz+PQkTcyh9z5e6NkB0desnXrWnuzsgDGqZaghhWbO6a1UPtOW85VKqIsKyOSP2O2oYU1Mn5nkahFkCgxshARgLg1utjV4KkzCZ4X/78/ev39x9+uZmLYpI4zS8e/v29uZ2nucgBNhNkeBg2l4gCNwBvf5EdOogRo+C9B6JDUige56xKSpY3+bn5j3DA9zBkYj3H</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9V5BtSXYdtvbOPO6auuXt87b9mO6ZbgxnBoMhQDiCpCiJMiRF6UOhCIYUIX4p9KEI6k9fkj7EPykgSmKQIRoFCIAQCXAwBhjvGm3e637e1KuqV/baYzJzb32cc+t1Y173dHO6B0NF75ioqXvr9jl5Mldus/bK+4CP7CP7yD6yj+wj+8g+so/sI/vIPrKP7CP7yD6yj+wj+8g+so/sI/vI/v9utL6+3mq1Ll86Nd+bKVz1cHt/e2eXmJaWVy1TUZXrq4svPv9slsaqCuDw4GBr844vy/bMzPnLL+0NqvubD6zR9bWNo8Fke2dzcW5mfn557+CoyAfnzpzLS3f/wf0Tq4tLi6s37t4t8vzE+rox0d3Ne+LdxfPnjgaj+w8eLM/Prq2duHX37nB4+NxTT02K6tbtO1GSLM3PEdvrN64x9PLFiwdH/Qc72/O9mdmZmX/9B7/LSdXtdjq9zvaDvaOjkULgbBIZKLwCIkVRxknifSCIYYYhFQUoBIWKApULsSWAADWGZ+cWT546d+70iYPBaHf/cGGms7G+cuve1mA4sZE9c2LDuXJnf0DQU+uLAN3Z3PW+OrE6b6Pkwc5hZPnc6bWyDK9cvSbBnTp5am154fb9B3lezs12Lp4+dePe5sHRKIn4wpmNh7sHN+89iCP77BPnVfmb3/shVBeXFk9vrGw+eLh3NJhpZ09cOLV32H+wc6Ti11bm5mZ6r7xx01XV2VOrZ0+fvnL97sFhvyzz1eWFuZnO9Tub+aRYmJ954sKZrZ39nd0DZr1w9pRhe/XGLag+88SFhYX5H7zyxsHR0Hl3Ym25k8VXrl6xcTrTm7109vThYHjrzhZbvnh6fXVl+Zvfffnqa9+1kUbW9hbWRLMsbbVa2YmN1SKvbt66McoHTJpXrnKTOEoJcvnMxcFo4DUW72Z73bXleebotStv2r/zX//tSV4uLc698LGLZ86e3N8ffPlLX7334OH5S0+sb6xX5WRxYeEzn/0LbwPn7m+jt4H4k382W2Nq3/76r24ffs3bEbdsf6t89eWtOImiPO1lmQABtpiMjg773ZnZSZ4TfBzHTjSxzCbOi4ohLuh4nCcxCAyEpYW5X/vLf/3jL34egCt9lBiAAGxt73vnT55cqe/b7096vVbz+6DozaQ/OrbtnYPVlfkf8wABD7a31zdW61d/+Idf+9hzz80v9ADsbO3FsZ1bmK3/tPuwv7Tcq3+/9ubti+dWYVMAo5Hf2tq6eP4kGABefvn1hV77xJnTAKAKQj1+AA8fbC+vNzc6PBhvbe+cObnW6maA//q//r2F5Y3Lz34SgC/Ku5v7586v15/83re/+7v/+H+ZnUe73f74p3+DolOrq6vrG/MAoPjKv/6D0WQP5G8/3B6O9tZXz6wvdH/xF//6y9/6A5OtznXjjbOX6ut892t/RF/5yr/Ismw4GN7f3B4NxvMLPfX+9ddfj6L4wqVLZ8+dKovq0sXT6yefeU+L/1O33/zN/+7G/q1qqAd75UZv7uS5mYzS7a3SEA8HfSJeXFo8Ojx0vlJrx0XZSpPEJGWRE0HBeT4xrN5LK4k+9ekXfu2v/e0/df2yRJJ8uI9w8HBnmMvp02v1y6rUOKHHfnLYH3V7nenvpWjozTaI37y3vXFy9T3dzwO2+fUbf/S1lpWVjZOrJ8+V46pwVW+2Mx0GHtx67f/+B//zwjJ3uzOf/cLfXFp5KsosAAhu3rxjZWKM3N66c+3O9WF58B/+6r9PGhZXnnzl5e8++8nngbgZ5/4QUPObv/k/ddK0O9O+cO7UmbMnVbF32J9MQulkMBjO9jqLiwt7e4cnT58/3hx/tna4v5e1WscvL118/u716w8Pt8dDP9/pzc12OU4P94oyn+STfHV1NY1tWeRRkvoEY5e30syCNLigkBAACYLY0NrG+sc/+Zml9dPHV1bBZFxmrWZNysJZaz7wx9ndHSwuL8zOdo/fMfYx85yPXRSbJG0WryjQ7tg0jeqXvnSz843Dc+PcxNG73ZKPfytPnjozONhrtbqjcdmb76XT6wMwFrOLy1//8m9lbW61Oi/+/H9sIgawtblLWq2sr/Z6yWtXb2ztb55dPzvKD9MsGRyVUZKevfA00EyUBKTtJGklFljqLSz1Fur3D0+sLz3z9OWHu/v37t7/wQ9e/eHLb7Cxc3O9r3z5X/z8F379/U3hh2NzC4tuMo5a7fplu4OLF1c2b9/KaTw7H58+37r66uFoOAjOzXTac73OaDzw3tvYjsphe5Y6NpPCUxKTD1VwUIVKFCdPPvfnnnz+88d3OTgczc912p0EQJn7JLNJ+q6L929kVYWlpZn696IIafp4HFd5mbXf5lTTaayWADawSQRgZ2t3vptGnS6Am3/yKoI7sb4cL8zDxscL/3ZLAFx69rwbhKi39KN/fv3731BREfB0g+1sHaxtNJ/8xje+cTgYfPb5T6+ceGrz/7lBGLWyjcWlEwB2b19dOvMEAJ7e1gJHQAHULncuzubmM8wvbpw/s/7kpVO/+zv/8trVqxcvX2x3u7/z2//4c5//tV6v/Z6m8MM0G6fl4DCZmQMAXN+44FdfXZpMfKuVvPnG3ujQL891Hzzcb7cziMvzPIi4opJSsnYa9aCcViMBfPBS+RBbu3Hi9M//0qNd5J3MzzXhA4oks48ZxAdh8SP3gXcCGYA4e8fIfbyQR/uDlbUGAd/5w698/4evVVUeWaNKAplpd2dmZzfW1i9dOD2zOIv0LYtI81HvMVc+PBhfu3ZHoSFAAt164wenTj2zstYknTtbu1madLobKyeeGu7en0lnF5ayUxvP138djso/BVsLzL7l5T6QAB0gibKNE2c3/ov/6vm//7/+vatXrjzx1DPtTvLNr//+Zz7/6932B7+z35eRNcnM3I3rXzp/4YvAxqWNjc3nkrub+wsryZuvFm7ibSuOrQHBeeecq7x47yzbditmFPkYRGoNwJjttv7ib/zVpz/9S/WVQ4AxsBEDqMoQJ+ZnI1l4N3twf2txfm52ofGL/Tt3r1594+atW2VZBAnBB+d9kiRxnMVJ2mq1ejPtT33iY5/5C59/ByfX2Nx8m0hUKQQ1HJ+9/IlHf1OsrC2tLD137+5OlYcoaa+srFHIt299r6zmTl9+8twzH/tTVzN/9+/+3be8bE3TNwXG9e8rq2dG/f2t7e3Ll59cW1u+cf21k6fO/+Sz85NZAezOz58Evgf8EfDg7OnF1354mA9sMalGk2IyzqPIrK8ujkfjoqycD5Wi1Y2ZKQwgQQghtrq8svFf/jf/4/LGBYC3Hmx3ux1+lLvAWH7nAfys2N1b906c3jDRI4975Xvf/eZ3vndwdDSejIt8MpqMyzLXIM5Xo9G4PxwcHhxu7+5t374/OdhrhSJbWHynzHtyuHXj+qtxzGvrJ88/8eKjP9QfLwNM1p5p2yRb6CVXbnwXoXvh6U8/9lLvFBEI6Ozu9XtZdOfuXReiyaR69pkXwObEqaLMj5Js9h3+ww/bcuAqsA7cAeaB6Cs/ePnnP/Hsg8mtJInGA8/EaRKVeZVlGROJqjVcVmFc+LTdliTMLXT7myNVT3HnP/3b/3190dvXr525cPGDH6x+iLXTZFQklk+dPfn2d8ev/MnLo9HQVaWrCu9D5RxBvTGiEoKoUmlM5cphf/DmjZt/3M6eOP/yL372E/HJiz/q3r793e8Cqkreh8eMIOn0subXV6/fIJ6b7c2802jfLfNYWuwBeOmlF1566QWXuz/88td6s7MrS4sbJ0+8l4n4EOzvAS3gItAFUo/+l778u1d+4O5f7Xt7EDQJwVWuSuI0ODeeTA77dqbbPRyM+mUZRxFV6sY+3oizcWQz++TZXwCwe7C3NL/4oYAMHyLIdrZ2j7Oxt9orX/3D3f2H3jvvKxERcSH4yBqVEFS996JgTyqOVIoq3yXa2n54Z3Prk0+dv3hmef7Jp0ENVm5cu90/2CdiVVj7uATxLe7+1r3bv/LZn2/1uo/5GIB3x9lbLcqiX/jiFwDs7g3yYT/rPi51/BAtB74MdIB1YBtoAR+3uL83DC/+2tk7bxzeuzemXAsXRoPx0uJ8ZEzlqzRJJ0V5NC4sEDMF722l+w8OIsMzM8vnnnjyT25/af0kAb/w032Wn8hcEcpy8liQ4faV67evj8cT51wIHipBhKDMDEDViwRRAbF49d6gVFV4X92+q2Xp3rx192PbR8998QtABuD8xTNMEhREZnFh8d1HRSr5cNIyHXQe/4H3XUktLb6jb/wwjYBV4AQwD9Tk2eFt/zurG0trS6duXPlhpNHRuHy4tZ/ZuCgq530rzYK4vb2+ZRO1DIGcODeoTKrt5bmnn/25jTWZwSjFn3mu+T5sa3NnbWMlSn/UbQiO9m/f3dzZ3c/L0nunKvX/mNkQKQmCKoSgBAWpivceABFCUeR7+/ujyWg4HGftzsUXP1df1FWVYUNKSfJjSIb15ZUrb7zy2T//773TBz6siv0DMVeWUUPGp8AzQAR8H6iAALyyZLHXK4DxQrY+UDqY7PlSWt20ciUppWk0Hk2CaBANXtptG7ctAiKkrWjl2cufBb7dxSxw+c/4Id+PrW2sPO7tIR5u5zuH127dGIxGzocgAVBVUSXDxExQCKRuRDGDAIXUvV5RBF8VZRGCq4rJ1tbDOoe49cYbZVG0W0aFR6P83QdmJJpbmHuXD/yM4mzQH8z0Og3Immy6JlMuoXHNM21kTy1Uk4PqV375Cfxy+p3/95/+/X/2W2kSuyrPWkkWR6VDnLLjajIeFWVIZyjK5PAoH4/uff2Pf2/9nDuz9smf2Rl4z1bgcAeT0ehoq9/fr5wPIiKiqqpCBGYmJg0BABGIiJmYiQhEqgKCiErwlQqVhd69f+/gxuvz559KklYSWWOMIT5/7ol3H4TPBzOrZ9/lAz+jszzz1srlbdl0B0A1mbxxJX/1lVdu3r4/KYqNlT/+m3/1L3zqxRcfPHz46huvizHtLI3iOKgYJ0JallJ4cgdMFVoRV1T+wb/48vLqyl/5T6LV3m3g7SqBf5tsF/u7+e2d7d293cPdsixBpKJBPKCqMEzGMJN6gIiZ1TCDYGqcAUQKQIP3gREg3u0fHBwcHM2fx/qZk8awNcYYu3D6qeaG71BBv/QLf+X73/r91TPvOFA77A+73Qz83gEX3p3f+0lMBfTjSKvtrd1vf/Pb3/nOD3cP+mVVxHG0f3jw3/4Pb3z62Uv/wV/+5Yd7O7v7e9aayNr+oCq9BG9NlAVXYqytNGmniRONu2jPxT/8xr1f+ZXTP+Z+79lEwD9Nxq28ChNj4XSWLM24VzYfbqsqAT4EDaIAERGRYSZo7b6MGmYARFy7NjCIVLwIe+dFfOXGk5FhA+Dw3psheMAQ483vfenS879Y5Eizx48lTA7X1k8+/m8AANs9rkXrVtk7W6gKE6cfHsiAx4CswrVJNZxtNEgPXTnjefMb3/3yg3v9E3Px2bPzp9YWT548Wbrqu69c/crXv7W+sj4cj9I0CxLySp1HYmPEwakjwAWfFxQv2PlL5uTZ2XAE4AJwCLxbbvFjTTzY/jRBtofBfYQKc88CGTrthY3Vmc1biTUhBO+dQGtdkGFmJlWtoaZEUCUGETW5GkEVCM6RBOdDkKIorl1/Y35p/tvf/gZIgwoRFUUBvCPIAAx2H6ydfvpdRmxdkYsiybJ3BxkAE6cAxJUcfchCmbdYjItxDEFOGBKWowQLs8uH+0enZtyvPH/+0x+7HK0vY34R1j53fum3v3rlySef+pMrr7nMF0UxHOdBdLYXaWxHQyFCmiSxJYpDENndOjAhA579yQf5KBjI21ilD80WMTOPoz+pCQigwnDPwDPBuSASAKgqU+23oAqto6QChNqTAWAiKBRBVcWr954IIfjDw8Pe6sbSwryJYiUYa577uR9D/cy9K8gA2ChN3xef+NME2aObIpvOKZypokhPzHXbWcvAQAj9AaI222y+14qsNdYORpNiMsrznIjLovDOV1VFQMgi74IeyE7llp44+9nfqAnnDy4T+Om5NMbsClABFYZ33PCASX0IlXeqYCKvCiJuFlaZmEBgEVE2BAUxMSME0aAgEYFIiCIrIknSRtxaWlm0kRUKxhjwTyqesD8jqrL3bjP29p/7XJvvdm49OPTIXphdg6fNN+90WulCN73z5pU4Tl2V53lOqsxwzhVFZZit4TRrLc7PfeLFz/YWkuXLh8vxxwEA/h1x9s6No4Pdw/mlJtq60kXJT19bMA/0gSOMjkpXAZKXLoRAXAvsQQQmAqDQGnKi4DprIxhmAqmIqIdCRRUwRCH40Xg42b574/qbMAxVNaiG23H3XUWUUoHjt75R5S7OHs3Jz2i9+a72heeWDu4dvjkcDMXYa6++fPGZy9WkaC/OP/XMxe1/9XVVlqB5UdkoztIkhMDQtZWFX/mLf/Xppz9mY5t1G3w8OPz2+tz5Wob1eHscyIb9cbfXPgaZOv9nAbIKmABD+DHGo8qVZVWN80JV6rMOAFk2bIx4DyU2pCIAMcMwK8EyhCASJAQ0aRtA8D70j/Zff+UHk/EIbCIbc2yroPE7DyUfjLKZP90HeAQyV43H+b8Rzj6g9rD4wI9TqDqnUfRuN1hYPNHfvHt2ubs0b0jbOHXu7GwPaQzQz336M1/81Vn46ve/8tU//v73jTGucidOLf+lf+evX3jqT4tV1uceLy4oRsO08/hWXXDanSrwJqNJq9OiqVZCnPK7Dvv9mi9ViOLHrnC+jYyAEt4hz6uymOSTsnJ1HqaqRLCRNSCvwswECAAos6Ga1zCsLogEEamrURBUVYIq0O60sU/Oh9L7jnY7s2vvMs4fBdnbLIrbs/H7w1n/aNCbnfnJQRaqysTxY0EG4PEgG+xgpmHDv//K9zDoxx6jQT9uzc8ejcP2nuHJRDiEeSyfAIpf+o/+xsL83Je++Z3F5e7nvvDLPwqydxiZwPA7gQyAOR6bVq1OIx8f9/vtTsRR653+q38zs+9wSgCygwyAAwKc07J0vqoqpwiEGi3KzJY5hCCi1hJURISJiJiZmBmKID74oKpKbAhQUlUFOp3ekz/3C67c39pqld5Z+SCe5X19ujf7Xpub/cNBb+4dP2wev0nfyb6L4iC/18qe7gL3rlz97dtvjhIeTNo0GOvlC3OTzb3N/aFWu5WLoMUzly+iv4WYPvlLn93uT05dfPKZj7+3olImMO8ZK/ToEdq9n66qgFvAGCgAj8qVZVE5V/mKVJkAEJFaY4gohNDUm1BVIY6YqG4SSAjee1FRgTFMREG8Chuuk7rhXLd18ezp0ajf7XwAHe33hDPvnI3eRwoyGRWPBdl4MGjPTN/3RX047MfZCHD3vzM+8ZnLQAu4jNvXPn55+OrVH46qar4700u77JlyP790ohevlOIRtxBbEIHNr/21/+y9Dxv8ATukD82OEI6gHgBcVVUuL0rnQxAlIiYY4igygEgQBVQ1SACaXicTQTVoXWMCUGZWRQhBTUTWlvnozT/6qmgRp60u0eLiIjAAZgABKkChAqqzQEAUpFACBKqoqbs6syKCsQBhNHpPOJuC7L3W/63O4wH0CGTAewMZsP/g6vd3Ihrvfev7i0v38/740saMefHZ8yvt/+13fmvuzJwtnAwG586dHD88eLh7//7e9u7X/lWrFT373JOLLzzzb1UxrYAAAd4DgDFwvllLVYCQWECBh6h2UU0gHgpUhYSQV76qggsCqDEUWWuYQwgKJSJRkSDWRtPOJquK9wKoiBIzs3HOSQAxWzYgjEeDIOVkXLjg+/2x39u37TAtMKbpOVODp+YNbZ6ixhkDYCAABB/eV9z8EDsBf8oGd29t3bljqtHWGy/Twtz64tziyol/9E/+5b2727mvWll6b2erDH51cSFfk6pjd/d3//d/+E8nY7cwu/Sf/61/d6bHIXg82MbsCO1TKA+QnHkPtz0ucNz0ZwAC8tyXDqCq8iIqoiKiSg0HSkTEhoiYY2usjShisIExqBNQIqhCFBKgBJWGOZUArTHU/FRVKCnV8FARJULNsYqonQAmh9tB1UdwUEEIyEuoVD6MyxCCh6hhtpaJSERBRCDRIKLMxGwME6CVc3W+r4BhC0UQEVVjrDFGFSIS2dgYb4yd6WaGCEHAUyxBwYAYQKGomROoggRKQP2YBPVQA0VVVT9NXqMC+m/e/z8vnfglwAGrwPrbP1Avc37jBy9/9ff/ZSuhUX8/Mzqv+sfXt/7gD364vXfIzHnur9+7eTAYtDL7g1evuSC3DvZeff32/c2DSVUeHB39w3/2z0NwR/2j5z95/onz66fWb9tWF4MrePpXUWyNdjc7810I1AcfREVL5yvngvcAE0OEVEQBgFVrADCIAQLYGkZDSxFAdSlHzEpgtr5eDlcHbVPHKDBBCXWsQhABKYI2rSHUnUhVRVPx1al886fGM6gCXtVCbRkjNyhHqMYIVXC+KCsRLZz4oCpKUMvGqQD1OXuVIAplYmYikAuuck4FSs0jKJEGIaLIxsbYGuLGRJ1WSwHi2HmB5tTsLxBURYmJiUIQhaiINriFiKhK7S2JWFUHw2F9rq4FhOkjeSDAO4iADUSggiBQQASqqtDmGTQvyrp5rErGMim898SkClVlNklizdwIYOCNN3bv3r+RL81X28Pf2zksP3bq08AAmAUC+k1rRFWLovzWH3/zYH+TuqmNOZjkGz+8MRwUYJ4U+WJv1hBOL69kcaSK4bDcO5rcvPNqmJACy70ZErp18/7hYFC6cmdn8Pr6jaefWT+1OrcyP784eA2mc+X7b37q8x8Hs6iqiPPinPNVqKeKVKXxLIR6spSIBGQYxoVyHKSdZVSTTQQRahrWAJF3jplZAQYzA1R/c0fj0aAaVAlSI7gBF5HWJGltBFIS1C1KVZUGcQrVIKIqijJF5UxeYjKEFC6EVkyt2DJbZsdKRBARgAxzvZsItXCDRINzoaoqkGUiJQZsfX1jImsjYwwUEkJsbeWFbQoyWzsP9g73AUBUavBCAWLCdLqkWUAhkDTBdfqQeZ7bQ/zeHE4CMZDBZ9UhC4RAorDMbFiDgImnM1vvtLpDFlkrot57Ylg2tXqzbtyqci0UQL+Hnjs4mEty0z/8webtvD03PvdxBvaAFHlSjrSut5VUgzpXVa64t7mrq72ZXufqmw/KQShLl1dlEJ3rzBRFOdPtEplOmgZJtjb3xWsIoiKJjSd57ryvXDUqS2B4404Rc5CyzGZ6vZ37UWd2Z2fn4ebe7Mqs96EqXemcc857FZU6lKDWB4KbDUUNbpTIOf9wvz/T6XTbCYgGozzPKy+iQUK9oZtNrTPtdGGuS/WC6DQoqohKDSppNm2z7+ubNwuD6SCOf6oAdT9cVaBQQ5ohzHDci9BJnDE8Kt3Dfu6DY7gqiAQFQMQgCkGSJLLMChUfyqosSh9HpGxUQE2axVGUWGvrdgETdVrtJE1GeVkWhbFxVZVNfJz2R4lIakxAoaQQKKBS+2eq215KxACRFfQrcIwFoAcbOV/wtCZBva8IUFGosabe3SCAATJRbABNaj7dMEBRWU7GZT2zPqhIMGzkobR5I27NtNKb125u2aPyM788C2wDXWRHSWQg1H9ITHVlJJ/5cy+A3O3bd0NZdNoplW4wGvUn41aUTCbjynseG+/8YTXspJmrXOWl9EUvaY0nufcepEHEh1D6CtAbD8aajnorRzZJekWZpHT37v2DSR+gEEQ0QJkIIrWauY7fWu9KBupwxoCoiqjl0lV+rFZJr93YunJrqypDWVRBgkgAUTuNn7qw1jmzPhiWtZ9rkr4mMZPad6mIQrXOxRRSw4dAID3ezjXGmmsI1e4OADQoJrABDI6XYjcXVyecbB2U46IaOh9CUFFiwwbwqqrWGGLSIEXliqIMPgRr1EOFqZEKURynxto6knovzvsgUlUyLguTpHEUAaSQJuDXo6n/D1Q/XJ19Uu3Jp8NVwBhjX/tq0p2hT3z8VWAz4KnROKxceOmtSdP7S/4TpPJGWXkogmiQ0gsRobN8JsHyi5fcRufM7s721/6v7b/2Nz4FHAADWA84pK3u4gpwWfNXnU9/4c9/xvtPnf/EOWDre1+++1v/9Cv9l69aZh+CSCir3DC7shBNCCxSGQERqQSARIQJxuDk6bVWK929t3fz1kNhHYyKysvOvfHH5hac94/cfz1VDAKrqRdWARiFEngqcWBVQGa7mdQhQYgNGbbGQJrUhHud9DPPX1pd6jFbkNapmTbYITUIIdTKQmXWxtEBdYhpXpA2QQlNDwlEBFFlUO08RLTOVRyZI6VYo3YWry/ZJwodFf5oUjjXXJqURJQJ1lpAK+/yoigKR8zei4hGsbVsQ/DEUZLEBECF2fggk0kRiERho4iI2RjUl6zrlUelJ9UTxKpEEBgGKemx5ogIRGz/yT/+drsTzz4brRmX4nMrF869L1z9qHEW2xC0XnAxqkLE0BEo6bV7ukydpDM47G/tPFxbYbg2IgdUvcUO8G3gBGXPLJ/fP7p33XkH7AHrz39h5tq1+9eu3IgtGcOA8d5FUSIhCsGTMbGxQsy1kg9eg8aRPT2/+ht/6Yu9uZn7d7eHg2Exyq/d2g9O10+stGc71to6ZKgomOu1JdA0QaubN3UCMk08oE1MgZJyYLHWGmOYlRgIrAje+267ZaMYdTwBHdf901dNn7FxYDWFSkr6KMJyTU+pKjdAl1ptSEpgFan9BQPK5JVGahyZdi86L3w4Lu89PDpErkqkEIhIsNZawyGEPC8meeklWGIfhMgmcWatDcHHkQXUexfExMZEkWVmH8QHX1QSpa4GWOPblYiacfM0/6zLHYairqfQzEHt2Kx3wVc6+v7n00/9pZ8QYY0lKedlvZ2IVMEStNw/MoYr5w0bzkJvrnewO1pbOY9oF8iBBGBgFfhHwN8C4sC2RmQAACAASURBVNmTLwJbwNeAwcOdfHdv1E5TViRRZLN0MBqncRwZ40JoJWlB7HxVKxGUWVV67e6TT589fWEFEnW7XUBDCCGo9y6KImMsoMpQBZtabNqk2kQMOt6uUBAZiEhNEDQRBgRSVmY2xAwiKIPVEgXh0vkajqoNLgFSEEMVYGJlUqgRlprB0DpWahM0RRRsaiUbNd6W64kkAwD1qRKt3yVAHdiBYaXTzjqt1FquHQ4TiYpC4yiCal4WeVF5H8gYgJlNEmdZGgNCUMNcVYWK6WSxqBomYwxCIKLIGjYktRunOpPQ6dZp3NrxhNX1cn00gRp/R0xkVTVN7LMfFMgAICMaADCGVOsCRUQg6lqzNBlLt+eyrfabr+8tt83SWQccjsCD8kZn9DHbXd4f/qP5BdtuDpvc+d7t6nv/3A0Oh2mSqg/EOtPpOucBWZybH4yHnayVxPFgPGIoMUE4ipK5bu8Tn1s7+8wssHDvyn1XCjFbiziJanKqSfYbeqpOwxTKx1LAOi09nql604jUk6eiRIz5mfal08s7e/28qAyTqooPVYOzWhzdCFenkZCY66SehGBE6swfInUYhapyHa5BYBwvX4MzOqY7lBqNohJ8kEIMAkoveUVemBkssJacV8PGGKqcy/MySIiiiNka5jhO4jgi0uA9k4iEYuJn2h0iqpxzPqiqMRZVMIbz0fhw2BcRCQ17GEVmbXXNGFNVxdHBjnOV98EHD1E2FBkDJlIixtLKaTBZECYTBxy9/QtdfhLrED2sM+vj2E0s6QKBdluxvXb79ty57KXP/x1gVDy8UoaFYXzHLryhk6da7nzeermNCfBwe5Bs38Pmzv7ebijGRRInasI4z3udmSxNjoZD78t2ltrIGMPWzoQQrKmpJuq225OdZPf+mMQFrw3tUBdsVFdubESFlJRrVQwaSqHBWPBaOR1PCsvcm8mIJAhMnYOoGCUFlhe7SwszWRpv709ArN6Xoahc4DqGkxKbaSlW373GjFEVBpS5KR+ndVndzlGlJvufhl0CwFzL/4ejwWjYr1dcpCGu8m4rPTXvKplUgvpMgCFmQNUY8t7nRVVWzjBFNoqMsZE1hg2ThEqCqGrlvXNCXSY2znnnnIraKIqDuoCjw/0Hd2/keemCU4FoSNPW0sIiGw7e9Q8e5HnhnQ8SCNpqZRLFxFT7P+9WTZzZLGuxsZjsoPVB4cySYQStK3QGC0vEDEqBrnPl/ddGv/7rdRO6ky5fLO5d5zDH4TyV2XgyOTiI78V3N87T698+2t/k7YcYDSdSVQzmCETp3tHhbHfGGpOXkzhOW2mmrEkchRCISDQEL1Fkl2bm80MjCLU/qnXLqDMh1K03GKUm64KqMrgpDb2Tza3R9k6/ci7L4pOrnbXlebCXBgLNAcjaV7WyNIriUKfHxGXl6/MdykxAva11euUaTdLkOFChmk4jklr/qnXZQIKm1FVCgzAQE6HIRwe7D0IQmXIeKuoG6XwWddJURGJLNrI+BOec935KoBLX8ctQZI1hqNZiDvigXtUHZWYmC8B771wACWtzCtQHESWt+UIVgJ0PzlVxmhpjuO7DM0iJFMzHjpwA9cEZZDaOE1W5e2/71OUP8MQsgZVhVEAkKmwyAD1gcufONbvgNoujXvr3Ov5zsBeNMS1ZxM48BWMIM3Z2tHfu2oPy9rW7O5s7eT7xzknw3lcKXezNbe/vHvSP4ihWRV4WSRRZY42JiOCDUyVRSaNoeX52wkxNtXdciQPQ2oFAufZmCgXxcSwS1Zu3d67f3B0OR1FESda6eefeM5dOXLqwYSMjIlwncNpE1CS2kWVxIGuYuKg8Gi8JNFlfU5gxkQJBUHuxRrEvAB7xtHU4rKnaaS7U8Bx1/WaMrdMk1MMFEVNe6cGoVJjKuSAgRnDSytrLS900zgwRESZ5Phj0i2JclWWRF0Hrp2YnwQdYa9kaEETV+1BVFdc+NIQQNPeYSFZyVLFzPqiIgSmq0IGyMcZYZhCYSGi6BQHUojfxFQHWGA6C+5u7pz5AmBmGAFJXV0SkYaLs9igN672nYjsn5lt7k8k/+M3/4/T6E899ct0ii6QrpCqYybK+TW7e3Dna74/Ho6J0EBGR0pUSwiRJl+cXt/d287JsZ6kqjfJJFEVZw9QGwyaKYma2SXTMPTU6PjluXx63f5spkSm9QaD+YPSNb/3AF+Wff+GpC2dOvH5v+8Zm9fqbd+MkOX92ZfoxCJo+ZBwZZiYShiHmsgpBgoFpOP+33obqOYHKtI2pzWHdusAFmsy/DrVNh4SpDrt16Lc2IjpuGtS9CEtk+xNfutHO4WiUF1nSOX9m48Tq+mxvjtkGCQoUZXHUPxznw52tB5u37x4M+5UqMXvR4IMmcVQf9RSpfCjL0nsf28h5NxzlRekcc3e2leeuf1gqhQByXmo9m2FDxMShPlCFpmCoXTFCCCDYugLaenjwwaFsasccpYgqfAWUKaufS1eO7r+U9/PF9vWrV964efdazNmLLzzfbWez7Wy0v3/31nVfFMFXVeXq5VFRhvHq947252fmlucXDvr9UZ6nSeqcFxXnfGSNYVZFbKM4jgWYKgumFd10PPUSP2oG1YOdepJ797d7UfTFz770zPn1dG3+3Cef3r9156vff+OwX1QuxHbKSFLjpyJr49jmVVVrIYrCicJS7YDq9IqoaRNMazBGE7AhDX8+bUfXyDwe+HErVRvvwDay9bahun5RiqI44mzi9HAw3u+PZ3srT1166tzJs7O9nrVREHU+KEnpqnExLvxk4+TJ1cXlG1ff2NrfzTWQV2UhBZu6HYvgfV6UkzwnY50PQcQHqSof+lIfxROwQirnATAZYy0xETGTNFU2aj9LAkhwAGzNEe3uDz5IhBlCqKe1yT/ASqJCCqLYxout9dnEt16Y7X/pDx/ujfYP9wb9/IVPPq3Li3euXYsiMagm+SQEYUaQRnDCxD74vaODdtaa7fYUmhdFXRdaw4aZlOMoNsYwQetI2BRt08yMprCqa3Gq5VNo/ByBlKwPX3zpRUvh2t37T1ln5hYXTpz+ZF59+eWbKh5kiQAhrVvEBGM4jiyTJyZiLl1ohBKqxHTcD3+EJaIaZNBjiEOVGg/XlLto+gJ1c71GHkhJrbF1R692p1EUt9IOU1QW5eFw0pvdePLSsxdOnevN9JhYVCV4UXXiW4lvt1pO3MzMbDttW7LxtTd3h4dj50Y5MZM1hhm1dqOs3CQvbJQGCUUVisqFoEGm/+oClEBF5Wp/Zm1ENYyoOWJFDaUMIpLgVWGJiYX7wx/zRR3vz6xF6ZrbCSlrXQ0YMNlm4SOmpaWFZ5555mtf+/pcrzMcjl595dVbaavLfm6xw6xxZAAKotZQpU3zxBobgp8U46IsZ7ozq4vLxhgVrdU6AOIostaqal45ZEaViKmhZKfL2mRFxwKc4w6JAJCNTmtupn16uTfKxyZKH9y4HciwpaoYR5GZEmNNHCbAWkpjW8dmY6zz4n3A9EuTqYkfmBa8U59a409q+oKYocoypZ3AdCwUqmOjkEKUoGwMsyUOJGTYtNNOlrSKohyMxnHce+6ZT188cyGNYmJiNXUHEsGzwkuIoVEUx1FsV62vvLjAd68/HA5ckKCwbJlZISLsvRRFydHEebVRJLViUnVafEChZVmJKjMZGzcedsq81LuqVhsE8VCxRASmvKg+SJzVaKq3Zy3WJHAjT6fgpSY8jcETly8e7O+/9tqV2FrLNBgPk05rMhlDqd3KDs1YxAeBOC+qDMRx3E5TBZx3ZVnkxaTTblfBqUgSR4attVZFisoN86Ld7jZEf51M1+qCWklQVwBcd8ubFJtYVWhp/USsZDppzyhOnl5fWwXZ/s0bZ1bmIssKmvL3zcwSUZbYJkIyu6A+SH3xxh1xLf+Y8l11sqwANRUuNW1j1LJ9kFIjej2O9yAADFIYa40xBDCbNE7SpA3FeDypKnnyiScvX3hyptMp8zz4AGMIRMwGEcgAWlVDQ7aTJLGdlXUtR5N8eDRxLne+DGIiy8QiqDubzkueF7mHNFliLS6j2qOpIi+rOrLbKGZiMChg6sumVBKgElTFAsSGgvNAdfxvC/zElkxrJAZQf50BcRNNjIFonUij1UpfeulT62ur3/vBn0zyvHIyLCoybCJutxJmBphEndQaGq6qEja2kY2jpBHeKCJjApFhG9lIoczGuVB538UUTZAp2Qo0aQ8aSUbTD0ZsoyASKIS2jvf7w90K2ur2x4gVKfda7ReeuXCkCCJNtTqVVjAjiW2TRDKH4CvncXxGd0qxTvsxtRqGpv6z+RAgtUJBEXSqbnxEzzYdfSjIsLFRRCVZMkmUkmqR5+NJPju7ev7sxfnevBPng6+cZx/q9rkhGydsoghQH8ZMIbPp8twizl3Kh/3heDiqCilD7QYECJUPIXgvLFqWVRVQ+fpYlNYiMAaUULkgosaQsTEZqhOH8LYz73UhIyEE2zRGlICHwAf1haAp2NRxaMon1FQ7mgQ2EEzdoaCslZGJlchVQYFKXCVJL22ZMrfWeheiONZI8nHOpIA6Ceo1MtbaKIgIJEta9VcWigYVDSE4H6qymjIJUDA1rqH2bvW61Tm5QhGrXT9xCd1OtX1ve39nHHRSylzcwkhgDtC3E6YRGwSpWw51r0anhFuaRA3xBfKiVeXria4z/gbKTYOGwErSdJrru8s0sk4lgE31q6oEbuLQtKkPY6yNDNvYRkwoi3xSFCq6unxicX4BhCIvRpNxVVUa1DAbtmmWtUwnTVuGzWDg8zJPIk3jztLSan7hiX7/8GgyrkIBcF26+CDO1TIniISyCmXlFKgTTp1W7z6EOhHlJj9j4VC78akvA4hVVYK3SjDEYPQf7PTWPyicZajXo3H3ddAwUybLkApqqa/SaJhfefNaMSmVEFm2s1WUpWTTEIqmORQQWUvEolp7EhF18C3OiDAcjSamSOIkiSOIGhsZExX5OB8X1JRpUwEGUe3am9ZjrWGEguho96BdvtJ78ql47WJ3Mt6vdpz18cU5wPX3yoFUvvZBjZ8RAgsJoSHd0jSqr8pMoigqP/We9Oj+9TtNOt8UJgSSmserdz7VCG5Yt7depJHbkhIoihJmNsaID0VRuspZmy7OL1hjJ/kkn4yqPHe+EC81+5V1eszGWpNm7dL19ncPj/yhTXo27bRnFzbOnj8Y9vPtHc9co7zuMxCZ2JpGKICmY9t0Y0njyM52WgpRUGSjposZqJmn5ke9Z9QHbwnETGzs3Qd7z66/I3DevzVl0zREEWoOr26vGNOosXx4/eqb9+5t+tKRhTFhMCmKKqx3ZisXmKOyylkRGxvZqHS5IRYVrmULhjtZu+lEgiSIMWyMUWjl3PBoDLx1leuKjo4djzZcATGzIQMIjvbQng++Gym2tu9GCc0tzsVZ9+Tssg/uwe6mkDRoUGn8IwFEaRIxk4SGwSgqj4YFVQU/Cn4NsBuQ13neNAVrEHnMwUxJWJouba0CJCLYKDGGDZEL3rmyKkPanm9lreCq4H0oJvBFBKbYEpESxXESfFXkYza21e7u7iQ3b92s7FG3t9CdSXvLyyfPnx/m5bAsmWqhnYoKAUkcp5XvT8pjUqheVkN0Zn0xS2JRJYDZsjFwvmm8TL9bod4nqhqCt/UpUSa9ev3Bsy98kDBrvqRGp8IDQ1MRgoFIHVKG48H16zdroT55GeWjIvchDIteEnlb5iNXOOM1bbWzNC2qHAwJQdgwMCnyTqsTR5EqnA8ArImYuXJeREb9kQRle8ze15BjojBd1oZlX1k+fVTcb7cYs7OgbHFpUfbnsrWs3e3w/Dw6p5DNWuCUodtb92hacE57QUSgOLaGEQIxmAh5UdUpPNM0+2sKx7c3wKd08XQ9HnF709K0ucOUTaubFxRFUUPjqDrn88L15tuRMcG7qnIKirOejay1NoriNE0YHIJ3riyLYZx2WjMLuSb3t3YXPAd0Z3rxwvLy0tJDv3fAzCEEYngvzgdDyJLIsiGaNkBUQTTTSed73dFk4p1opsSmPubePOyjoEl1mA3eszQJKN3dPBxNPqiqMwDTzgumcw0CG0w9K4hAPBqNR8OBShAJRV70D4rgMJ64/tGhBJ9lSTdqBR+YuJWl1ljnfL1stcpoOBoWVaUiAJIoMTYipcpVAE1Gha88apYW06duxnM8F5RmnYQSNzy0S4voLAPAXKpJtrUz2t8bgVMM9lE+RLGJhQsnT53TY3pr+kOhsTXG1KIwUkVRONGpgmaKpmnK30zFtM/UELdTLvmYW8aUcaPjpZvGWrZRxEQAMZP3UpTS7cy0ssyJLSTmtLewsra0vNabm+12sjSN4pSytum2Y0Mh+KrT7swtLAZXjUeDohgFV2StdGa2N9PqsDESgoh6L5WrgnMRU2SNIa79cy2v7rZT50NZOeedihpj2Njpjjp+yiY/A0iCs8Y0VVdRVoOx77Q+kJLz+PuZGoc2zW7ouBNTwyVN0ySJxuO8LIrRZEKqflA5I5NJFcs4tQkYJQBoHMftrNX33jlPQBQZqE7Kgphac4spR3VK4ENw3hGRy11ZlFErQb14DcR4KikkARS4eXPzQPbo4T2cPwEwMMDRISyliyvSSjEzh91d7B3Bpkg3zMzpOL5XFvmU621imzEcRzwpqP46zrz0Un/dgE59+pQirjtPtXetqyQlIZl6sWnp1PTsppP1aMoYUBgTgcgyw9oQALKzvbko6Y6c7ZcybymOY8OhHA0H+cD7SiUksW232tZEYGPSdHl+rpPFfryfH7qxnYmSuNXpttvD4qhyvgpBnA/BB4LGkW0nseHJdMCIY9NtZ/W/XFGHETAbEwGPDgfWIt7jgiD4yjb9MpD3YTDsry99IGey6e3bd6rRIzreq/X8GWaARKSonIaQxtHe4dBpCDPJ/vhwtT0nPhg2xBwZ08myvCzKsvAiBDLGiEhRlaPxME7SiG0URS4473wSJ0EkH5fdeTRBkx6J2pvJIFXFnZu3pZ2dW1vMK58hB3JUR+InxnKrncG70dFBK4t5+lUlWZaVRVFnWlRzboA1HEcWcHUGnJc+BI2mnaa64d6QG/X5zWlYrA88HeNo2nuqR0l6XK80sbMJrVEUtdKsHcUTLVQpa83MzMxXYveHeVGOulE8GFTj4cHWzuZwcKRBrLVZEre7WafdabdnO92luW6y2sv2Hu6xt/mQiyoGEBkWX3rvAKqcr5wDEBtOYxMbno4D7SzutLKyciGo8/6YoBaF9xJCcJOyqEI7S20ckyEiOO9tkracK5jJuTAaDYB3+2aYdzF9hKx6nhgapvHRTAvPJmSBFSLQqfAvSFk5y8Zr6CykQQSFEmyEaCIFE1TEGJOmaSfLnKtU1PmQtlMCjDG1RkYoqFrnvYgwG6iOR5O3jI+mJzxqHwQBM8mFs6d6Pl+9cE5m5oAJYNDN4giH+3sG4+6ciWPlVhvTr7IijpqjKkLKUFUmJqIktlPpEVXOOx9SRNNpqXFUnzkDjk8CTCduGs2boQFvgWDNkCopqSoMsbXcsu1oflGcHxwVRYXFxbl2kvqqiKiYnzOpqba3Hty/f2+cV504mevOGOa8LB5sPTRmd3lpeZ24lURri73i8F7LCNSPR64qKxUP7wBmw/7/Y+09miTLsjOx78onXXvIjJRVWbox1d1QA3IwAkYuZkGazYZm/HU0bmhGLsgFbcgFCXDIBggMgAYaVdWlK1Xo8HD55FWHi+cemVUogCCBa7nw8Eh3f+H3vHOP+L7veF83jXW+J2SsRKyV5IZxklJNh30GFFVT1m3eGoBxBi6Vs36+LMu6MQ774xzgGeOcKw5O5KXW0pquvEPL+Y3Bu3cHpwW6TPfOgO7EtX6gW/gmEKLzrmJLrGVgXVXmzsj4FsbMuveD89seYEs+GrKYRXVlRKzzEOltT4lCCAxMCjns9631q2ptTFtx0VEpffDWWe8RCNZagEnJCag2Fe02btsEYDtXgS0/U1kzHufo4F4gYIx0NHkrI/HcB6yXDQtcb5YYT6HS2defvrw87fdjCju2SAed5CxWcks549wab5zbfSg6f3qHje0uaNe9wR1kiQAG3gHmQHcn7Y6X0jU0GIukjLhwWi+KZrFujKVeb5AlUZ6x8TBnzF1fXsxubomPJofTLNKaarRzsnW92bQ+SKmn48lwMJlO9+c3U4RSSWaBYMEoCDDJJXE47zZl3TZGCJYncS9tVrXVcZRlatDPhODWOmO9bV3nODhXVdkUs82mDUKJsmiEEJFWQiomyPsgfbvpQE4AW1yfvvrqEx4NHz+8DzJmszTGrVbz/QcfpQreFG3btMau1sWjx08B1OWiq7zH6ThPdV2XxrbeBWfb/eFdhXYXme34L2C7Ygexqm6C96HDEBLnjfJRYCn5hdOIOlghdvxwIQSgJqOh9cZY15o20ooL4b03ZJSS3AfrrBBCcMGAqqgpEDjrAp67m+PuzGqrmjVVnk2en58/Gg8AAgyo8E3DlGrX5YuX5xGnjx4fiHWFybQpNnkWY0df2h7HBMYQReouFLU+tK3rvBRtW05drbArIHbGs0UpBXTdMMa2trjl8lHo0Bp0dxtTIM/RgS/q1q429bpoiPFef5hmWX+YE/nFspI8un/8tuP9TYibppqvaqw3wteKYdVUL05P01gpxtM4Hu/dm8/PPVfwrfOWM3RwBEvknK+qpqhrChRr1UuiNGps8EnUK4qKc163xjpft613gUnuA1/fbOzaDbiGo8bXcRIZ65XynknvnbTWAaLL8lvjpYxa6wGA6ay/n8Et5vOqrNNhInSe6jyy9cXZWeMRCyTZKAHW8+u6XOXpXpJkSRK7tnj1/BV6e1tG3vagvEsC3jhAOYpN6Xyo61YwLpWUJELrGHEyAXJ72rHdmSK5AMk4YnujydXtbQiWgERHYJBcCSk66HocK8FZILS18T5ILsLWOdAOR7D1K5vbxUBzpaPr2atHsQYs1ucgmq+KKI7K09PVxfX4cNzWbco80Cb9zFbOd03SsCMTgEAsjsTdYRcCtcbeFc26mv9dLYN2Tmxb8MdduIa7wJ/eUMd+I20nUPABDDDWrzf1pqqU1L28HyUxE5KRGo2OJ1OFgGJTY140Ze08Bd5LGAnaSN5c3MzgTDB+vP847U8bb5u2Nr5u25YY6/JmYnDBVa2p69YYm6YilkwwlI3xzrnggvGdQHxrnHNBSAEIIojRXtw/0ArzxUXbWGu99yQkhUCyg3JyRgRWlEVdW5W9mQrIQN+Lu8AFuBJvHJzd9e1+EmBCSA2uwVuEN/zZ6+SgKwZxBLLWNHW7KTZaqiRS4JCkIibWtuJqF7oz1nHEwLd6FmmSTodhvlpUTa2lZhwcptfrhxA4mJSSc+m9N43xzgklgU4P4u4AQiB47+vV+mDaB+ebqkYUIdSXV4ssS/b6ma+a8nZt6np5My/HSVoXKJYgv00Zd0fw1l4YRVp2PohzHghNY7fVc8buvqYt7mcLrdmW9LDjV70GKN0ZYvcGnfTBTmyWhRC8a+p6udk0TTsaj0fDYdobopdAgjOgBso2lr6nWidb1VOsd5jqQ9tsIF61xi9Wmy9fXR5idLB/NBgdYXkhq9J1ODgplYTSccvI26po2rpp4khqDsVhfSiqhjHybuuMGch5p0kpIbJRfDLtjUfT25c3LmJmp+tBAYwx+fDBg1fnV84HzkJVN0ryXu97aoZJrLV6o9hBIYr0m4qLSsrWvmGHnHMhwPVWK2trWDsPdmdnLICwKYrVaiMFj7VWWjjjdKRuZotEagYWtvQtYoz7ECQDZ5yICYEsSYXgm6p03kkSQosuqWOMCcG7irZtrfeEHXWpUwG+Q315a2PBsyxdV3VRLOEKyGjcz7RSs69fTN9+9OCtR9EgX2zK1rRoKoi1dR47zuXO1DqDgFaScVDYpqF1a3cdgY6QuZMF2H381tK2j9hrX8fQ1d52T5IPHeiLJOOCg0KwVbVeb8qqAWOHBycPTh5hbyftHwALhCCjZDJkaZxYax0hUsp7m/cnewf3L68vLmazs+urqDeZ9np5r61stanjyhoAQmmhdfC6sVVR1puizNMokjzRUkkRSVEbwxmzfmtqzvsQAsCVkkyHYrnZVGazaWS2C0MZCJC/+bv/+urf/0+hKsGYtX7/3uPe99XL7j383mxKIeO3nr7/5jNpb/SmA+QyvXfyGBJwJXbAhl06cdctZgCD8zc3c2PbWOuOUikF3xQNgaVxJLjoqCUdEWNbx9wK8DDOhY7ikdDeO4DiOGGAD4EL3jEwCfDWO+t2n8c6bQt0kGgE8l4rkaTZ85tFnPbhYlR1KKr1qmaKm+V6/+kDlkfzX31eN20wDRd1uLMSAiEgdEcfY4yU4oJxs8seq8ZsoWYA7U6ErptzB1tkd4Z2B+Hu+MjghNAdqhRo284IBE4gwNu6LNfrsmnNcLj//rsf9h68MSPRAQyQGiIorlSUhBC6r5HAst5ozx6Np0fsq8+enZ/Nbi61vCdJUmBSdgLcDIDr6CuBamM3VTMxJori6SBvScRp5EPgnIXWAhCCd6OkQiBvcfnl5ViYwcG0qCJDLd1x6wkySnuRjpqqZpyssauq6f0dKnn/8MW6saCMI/idGtudqdEO5IJXL0+ff/csjRW4BCH4IBizzvf7PdF24m9OCOGC644LAiRjfpuiMXSzIYWQUkohiKjTnmGcg3WCrMEaG8I2OKNuZhtt2bMiikKeL4xb1nY8HCJOoYI7M729AYsl9sawfu/Jg9H5eTWfGeukaChsVTEIQNg6qI7BLiUXgsFuhQ7rxjnvZSeWwHYvAd1Bge6yz601ba2OYce/2/UFOFhgO6/AQnDGrNerxXLDRfTh+z99750PvgfmutOS9QHOBAogprQGVxBCcR4z5PmQGFsX683sZZNHvURJIXeQMXhnG2MQLBPSeqpq0xgTx0k/T5sgqbW+1AAAIABJREFUGm+l4EkSeR86CK4xNhCYEN5SdV0PJp4DXHC43ZV0KESltI7irt3uQlgtl/9II3tj8S6mfSM+w86lcV9Uv/zLXxablVK667lKIVoXwFgaxdZY70MgJqXYSp50U9h4153u8rauASWk4J0KFAeElB2wstst29rQzdIlIiAE8p1qjydwlu9NSx3pOJocHMCb8mouMsHu38PeETCAUpDq0aN7Vdt6HzjIOns3DK57SyLygYhIcCHlXc+IN41xvtNs6TR/tmAHgG0tlSjsCmkd9vINAG3XYdriD7Z8LC4E5+Spqcr5YrWu2oP9Bx+896HefyPIMTs744BgkJwz4l3jgzMojgjIwQ+ix2+9987TDxQsNcs0Er2sR4RNUbSmNaZp6tI7R4S6bpabTVU1PoRE634ac8ZBTEtJgOS8rNumNURMKkUQ4AyMNVXj2nZX6Np22CTnIkkzdE2NEFarZacO2l0w2wo/QuxCLeye36Xlrx9/P19Ah+F8IzLjb75OMK6FiKLYOS8YKS5Wm6qqmyzPuGSU8cI0zkIxwaX2wfvgvfcqdHVnx4VQinnnhegw2WAELjscA/fBMsYZwXTwcXSFEeKMd39FF18DnHEmZXR6Pr8q/uo3f+MtNZzCFZBTIO1UHfv7Y8Z5WbZWtMb77ozbqr6ynZ9kTAimlWSwHIwxNMZ77yPFhxxEtCJqaXdOgqiD2O7wXNhBTt5oZ+0qfdgRP7qCkLfFppgviwB1//7j8WiCGmgAATCgqKgtiTzngrgwTWtsKwCh44gDTEIDEcCACXvy+J3F7NTbijFEUQxCVdbWWeeMM07GEWPkfSiqtqjNPqGXxDJOmeDU1T8ZT5PIOl83BiAZJVxGzoW2KqnaNOuVOh7uqvQAYzKKRD/vEYhzFjzfrF8TUu5yyq72dOeS2e5Jtitu/tDCtq8Xu8Fgd3Z2Z6IcUfTTjz/WUXL66lVdVzc388a4w6N9a11VtybYyppVxaVIpYhCXcWmzqwfIggmCRSC3SoJemgVOe8AxpkA561zrfXjg8HDJ/ejPMZue9lO2K6zvC3dDsxbitNkb38sdYTWIclQniF7DAjgFunop//id87O5qY1EGLbfiEK26gdnLFhHOlM3R/mbwffi/Svb/2Nc8r795QAt7DuCPpLpupOtonxLemkG3/JiF7nlG8wUbbXDEbCwXfwGlNXq9VmXbbD0fF0PDZ1Yet1pGUUy2K9urm5cN5qHaV5T8VJ3VhnmratvfVp0h+N9/PpPcSdw8Vgb3J0/OD82a+9d1IIyZX33RQy54PzXnDORKwCVOvIeuIcmlgvTRoXblabQNBKtcaWdRMIUgrd69et3YQlCIF5LiXnO/g2IEe5/s9/761ff/bXBAZO0zyI7xvZnbLoDwSq/gF6VSmw2b0Z270oAEBoX3797Ha+uHfy4Ojo/jfffpNmw5/9fPDs2bOzi2tjjTEmeGJMQErinOfDRbU+my/D1U0iWKKk5ixSUgqphGg9q511xAKX3HOupCPx4OTw3Z++s80Mdxg9bNVuulLotj6R9tJskE/2R03TxIKx5AH4Es0rxBOAASo6fietPzerYlff3xYFu+g9j+TJwRTT6b9Lc7z6Dv3+7xfh6y+/7ZODs6iWsA7xaKj7dTeG8HV6ybAtZ9BOyQOv79k7gAZnAsQokLNVWSzXZYB+dP/+3jANZsngoeLlvHr+4tnZ1ZX3Xuno+Pje0cmJ0lxqGbhYbRZnl6/i028ODh689fQjHOYAMMT+/sny6iWcl4mOtBZCWGet7ZIZIgpgEThvja/b1rStYyp4ypOkMi540los1kXdGArElNjbH14fDkAkGHqJ7o17aRLrSEohnBcSQDR6yhgYI85EFr95PP4jVwTGOunwnal1ji3cnl+9eHlqne+dDAIzJ8fHv/vbvyk5VVV5en7tvQdRmqablpxpSSdasjjKibjz1gV/09Qnx4O03//8y5ecS4ZSSKlUJGVIudISWsdKxXTX7N763dfAQmzpuRBcBm5ul5u9w8l6tVm05ni0QPIQ62+gC/AJkAFI0v5iVdydcGAMYUt86iuFWEJo3NuHWyNL8GT8NCasl6gDyhrGgfetwq4Uu6uMbK19F5ltS8ls63AQOlAJ70pFgXlvi7Jebepeb3y8N1LctlXpiTabxcX11dXtzDM0zvjWjGzNhWMg17o4UaPpqG6bxc1ssZxtisWHH/6OejAGMNk/THojGyzzQSstpYD3FKyUkdqieKg1tijLqirbpq+zOEqEgiQhpZCMBSGkc6Erf+f9/ME7x01jlJRKKyllFGmlFQcTgm29lVKiyyCub4v/lxHF/19WpzLCX9tZl2masih+/vFHt7dLojAYjx89fCCFMG319MnDxXJRlfWmKJSML29nTCQhBGuZc4YxppQ0BocH4//6v/q3wePzL/8baymKcyEjQAQSPnTN0F33cKdBsS1EdL1vbAsFbIsFVR//5AnSXHJumgYwQI3+IZYX6HmIDICMNHYpzbYWsYtXKQQYi3oBEnDAfI7eEJMpKuO4k1kPsoFQNW377Nj2VoFtgNvFbAwMu+L/Xf0WnKODPwv4ujWbdVnW9t6018+TqlxfXlzUdWOMaRqfjUeD8YALmLaVjK1X8yTWgXgkZJLFURwnSdq25YvnX642m5+b38/fPsRQJHl/tbgSndI26zgmTIgtBpiIrGmL0pdl31o7zJJ0MGZKr4smz9dFVYuza++DdwGKK6WjJBKCR1GslOSMs278JxjuJkemcdy2NWNstij/6cwMdd2EgDzOILrswgMA5IOH9+EsA6SKVSQhuG+a9brgQvz849+QUhPRV988//y7NWNeylgoqbWm4I1ttXT/7r/4V48enpjW/ebPPvw/f/GXxjRp1u/n4yTNhBRCSAbOhWgN0U5QuLMI2hFDOuVHBpBZJ0ogjQGSopLTHiCAAphgeIRyhgwAGHHrPKjjJG4lUIgCGC+NmdY1NAECscKqxHqBNPXDkWsWUsbQGixmUqdSax1JKb1zVVM2pg1hlwFsPe3WlMOO0hB2SgLOmGJTLNZF2RgGJqV2tnl1db24vNpPevvD6SjOYhVxza0Sq/VydlFN9/fSLCvLqm5sW7fEeKRz46vTs1dgv/j9/N+ycZqmWbERWmmtYy5kp2rcwfi895wxyUJjqDXW+dD9VgkZyOko3s+zh6t7IXgwhBCE0lIISK+UVEpjG8lua1hbOxv0kvmq9o6ubtaXL/5qOhp0ovNS8LANUYkz7omsMQC44FoJ0bWbIr0L8SWcwZY3R9dn87/4m2cgSrIsjhMi6tqODPTwcHz06EGSZrABAmjN7ez61enLSEeTyUGa6DgS17MVyENIxqCkBCFwRsa+/fSxCfrTr86DD3uH93u9rynw1rSLxaUQR6kaCC7A2OlVszI3u3Zi2FWMd8UsCgQapOrdw2hy3NU5LSK0l98qIXmSw19h8ghSAhWQns+K//jXL3YpJnwIwXvGGSN23NP3ReD5FFGCcQ4pECnEUkwyUVuYFiFg9PTtex/gb63581+/vDizrmMToWySpnXOe+wEkAEvOUu5U2azWReb0rTWEVgnmOcoihHvy2jqHbu6aOeCS+Z5YK1pPa0bX2i9qVrigriMtAZEJiOZpvPV7JNPf/n++7/ReX0ulJQaxH0IvBOkdsEFUsEFziiQ92R9aFsb1hVVdjZfbZo2TTNiygaaLxuprDe2tLGz2jIlnexkKTlHINSN3NrZZJQ/O70VQi7X9d/8+sVwuLcpKueD4uHlxSxPs9lyU9eWMTTV+r23DpvWffD08NHJ4fnV9Xs//W3QHLVFOv7TP/7z/enksy+fL9fN89ObyainJJI4/vjjf/by1emjByez+a0S0lgHHsHWAOB8XdXn5+eLxfq99z6Iomg4HKisHyUXPlAsIqV1JwISDMaT/u/8/N3zq9n948Ozm9m9o0mep1XlBnHmfFsUS6VUHMdg5Exz+up5v5cLTqN+TkCWSEAwTkrworRChr1+P+llo/0jYA8A9CA6OYGZgSusFigvkOXd7djLepGWZWU5I2PMzbzMU51nSaCwKJtNbQZSIlIQhD4HAU0FWAxHSEfwJXo/TiQbP/pgPDn4/KvPNmXhAs0WbVG1pl1pKaqmjZVwPiSKq4zZerkuNq2xUsVJnGoV52n085/8XL9diOWsvr6obufB2a3MBXHpQ3GzCGDGOZFnLM1VL2NxlkRRGvWKanU9O9+b7RvTWuMCBcZkoC1lC4wRgxTdwAFGYD4EY8k6YtbNZsvT6/nF7cYSbWrnvWeCj3oZ4yg3UitWr6mfsqLxvViUbYg0q8qwtbPDvRHoOZfCe0ghZ2tXNoxDr4tl1QimFVj09uM9Yz33+ccfPXl5dvUbH72NNMtzDfTBOFILMIIkJi5nxZMHR6tNdXAwXc4ulZK9PI/iaG9/b7Ve7U0norNvF8DIN+3NzdXZ+cXJvUc6SvNervIRpF6uqq4O2onaOxeUFtNxNhik84Uc9pPLa0xG+ZO3Hnzy15+T1GnaZxRccF1EIJWGaft5wjmbjHPn2WgQWQutBOC5sEqGewejfi/j2+FoDrCAgs4BibFAADAGYgAHxwd7k4HWBuSXq6Lfw/H+eDSMncN8vrgpzaBuIThCgAkwAU2DcoXeANEe4nQ3YOXHVm/y/k9++/S7L08vLzyRVoi46Pcy53q9VBjjMiWGGk2hZTQ9edybTo/ee/sdfbKbYNS0OP2ufvbF7ZmqVmvfmuA8d0QE7wwoqABzu/DzdR1p2euz/kjtjXtZzzvXNrUPTgjOuVRSKqkAxqToQEpCCK215EJHzAVWt9a50Iv0IEvKfnKzWI56mZLNzbxQQh1O9+NEvfz2apyHy5V6MI1fXdvjsZwtQy9Dwd3Wzk6O97rTJAS01jUhgOnWeuMQJem9/QGj7MOnRy8vbqe96aMH+2VdIT0ALO93QNM1kPn19bry5nIFJh4/2C/LTd4fLGaXgjMXAudCKW2dz/NeT0s4S84TQlU3r169Kso6TlLOWNIbgjFY9+zlqdYJ6wYugxHoyYPx/Qd7xlghhA+eAgkpTu4d1kXxxZcvlZJSaCkUbWUgSCqplOxA1d3NSgTvQ9O2xhKFoLVKkhSsa8+KLrUEOLACixE2EG5X4U+1UkQtEZrWaq2jSHc6tzbgm4vV2/sp+hEowARAwANFhbJAsUZ/hKQCrhAEPKFtUJaoq6ZuOJf60Xu4//jkvX/GubpaX/dHo4PJO/cevDXI1d8zf/b1iiOcjJLsycm9HooCdW1bG1zwPoRA3rm6Mut1vVlXddHY21sqamudOBiRkq0xwQcht4szDqG6Rr7gPE6SJE44I6mZJ1jriEkpI6V9Ful+ng0G/cDV9e2CCD5QpBQxJXjbuUEpFRF0JEIgrcTWzkZHUzAE75wNdV0n/eG9w73ZYt2P3XSU5Xk86evDh/t1Uz9+OEGcH0x6QAYsu2G85c1ttqe/+u6yami12fzknXv3jkZ1tb+opLVeCO69S+OUCASeRpLapr69YVwSaLVZnZ9fjMf7cZwMBiMoCcbJmLKswdAJ6HnvrW0PD0eDQW6M01pZ58HAwZRWH334zhdfvmzqIsuGnTYSD4hizQQpJSKlpRTcEwWyjsBQVQZCBeuUUlmud0GqB5bAFEhAczANle4wxUCnHCyEs6GozHSSaCWJYKzzPnx30/zq+e3DHhsmAlxAachuuBOHbTA7h0NRtk3rSTAArfXWWApBSJm1xZQRTp4cv/PBf/nOj8Rwf+9awxegErlENOmUX1UICIQQ4AOMGVTtYVG3q2J2M19crjaFc+t1GazrZf2e9YRudmJHdAAX1jvvbBInSZwmiWZgWoILHbiM0lxFCcpCcNJSWue999YFLX3TWs4ZQXQSgj6QEOQ8k5xZT1LQrgrLJwCCd977sqz6o/Dh2/vfvAx+JE8Oh0VVH92fAvlklCLeB9x0v/PbXTvAvrqYP42Hv/ri7GBvutmY994+jnrxk4cHX78qjQuC87Y1vX6v02L59X/8s5d/8xdRbzA6Ot47OlkVm9nt4q23P4qiRKUJuAAXTPg4ToiCEMoHsrbt92IffKR1XdVaK2udktKHwID+oKcj7R1Z28ZxDACMa620ZoLzKJJExBgPwVd1m0JXTdvLk1hb74zIJRC2TQ1bQkVADyzvxNTf3NIojlq7QiDrfCetF2ndGGetLz09K1AYdz/3h+NcUGCtARGXEQS5VXF+vZytK+OJC067oV1KiDyNiIz//M8OOMPx4zc+7QIYAgl+ZBFQAhVcDd8iOJCHCGAA15Bi2w2kABdgG/QU9nRksnvL9Hgve/lqcT6zri55nhkXWmvhnPfeBXIBxAW8t9ZHMeeMCSFirXp5L8/TwWAko9gY09QVEXGGujF1XRMhUDDWC87B1R0wWHDmA5OC1YYixe6q/ZlgcOR9CFVVCbIiHU4GizRK0vGI3VxDTAHZH2dAArSIxwDQzhHlwM31rMry9dnV+p//7N3nL8vhvT2AJXuHe8WldZ5zvinK+/fuEYVEqb/5xR+Vxca4U/r0UwhRQuj+KDgXRxFUtJ3YxZiUQgjNOXPehhA+ePchF1wptWzX/UFujI0iZayVQsZxlMSyaZgPvtNj7QAuSaI571SCyFon4KuqkVKUVTsc8KO9vUgzqLtvwEAw0AasBwy3g1RDCb5FfE+n408+f6UEJyKlpNaKcZjWGusY4IU6bzAriqN1ezRMpjmX3WxMY2a3m5fXq3VtIJSQssu6KdiIEYPj8FGSIbrrvyyBC+AW1QDpPUAADnAgD3LwFsGD/Na8tiMvsRWU8A53G9r5M+6RBWgOMIxylkUP017Nr5eLWileluuyqhPtjbWtMY21jHMhtSJSKvIB1lgpOpASXPC3s+tCwNuGupE6nRoasRCCsR6MCyGIOGfkiGkJ5ylRLATO2J0/A6JItqZloKJqOAwgRn0lsjGQ9vqb7eEiuwim6F5yfjabjllZFsvCPX91c3LQe3gyrqsFcADcAgmFTi6VlZsiimMK/nhv9Etrgg/eB+t9ualOF5tRb/EX/9v/TOXv/Sz/l2I4Aujs9Pzb754LIYQU3lilxJPH986uLgXnxtpI682m0DpqmlZpqZQ8Ptr/9RfPe71xR3MlCQaWJDr4DmxPdd1yQm2cqk1RNXkaD8dTY1eoCyQBqOCMvV1yLsTePiCBBGBgBbABBgD2xiNjPREpIYXgnAGEpjXWBSkYAY5ws/GfPZu9v59+dL+334/g/c2iuFy1pUj4eCjjiCvd8chDW1NV1KYRrH04mGDSAwxwCayBDWyDFiC/naaIrmkQds0VbCEYuIN8EILverbbCjUFBIJmGIht4TfzGCm008Em8PqyLDftprbOi/GgMW3dNK1pKAQluZRppLULtqoa0zZNXa3j6PZWZ0k86WXjyRhSM5D3hEBSMKLgrCciLlUgCI7gmZRU1qwn0A1feG1nvSxZFy1ATWMlDwBEFgG97szY/S8LBFS3SAfAzavzhfXq/OLGWLqerX7y7jHS7GivD4iuc7Ipyq71VDW14Hy1XPj5rANPBArOuaK1xobg/WZ2/Zd/+L/cnL/62b/4g72Th3/0H/50sZgnSe69IaI4iuJEc8aJyPmglWpam2fZpigirYxxSZoEH0xbRlFMICm4kEJy3voQArXGEaE2zlnftFZwVlb1H/3iT371y08Yw0j3HMMomb49fnJZnSV7f/jRx+999PEHiAZg4+03AAz3JkRwNiSpBtA2rVeirtpAJKXsohyhxOXGrqtiVroHA3m03zMyt6N+LDXXkgvBtsJUCC5DmmC9FEqmB/sAB25AG5S3ODsNG8sPjqEMrId3W3hVB17jfPtPMIhdiyUEWAfv4T1CgPcAg5DI7xAaATAgoNGlc6um3jSucVBK9vp5a2zT1HXdWNf2ojSKYyW5d4YxzykEF5ramaa0tdLM5VksNARj3lnnbaJVnqXEqEsFvOVS8kDQkkeMBpGsU2jpXtvZZJidXS0ZWN3Y63nXFejuHkNVxVIAt6FsebZ48XJ2ck/e3s5PL5abCl99d/bxh28tV6v337oHqMHReOfzerPbBWfceucCGGdnpxf1y6+6UroPaKw3zkdaDmMtOKxxzz/7m8uXLwYP3/vF//1p25YEGGellMbyprFRpH03SpJz55ySsmntoJ+XZW1aK4VwznlvOOtwUOQDOeed9Na0PsimrlvrtJKRVnXdWEenV0XTuj94+mHl6l++mmsx/Oryhf3y6//+f/zDt09O+gfpRx98+N77Hz46mXoKLy5vrPOREmkcMUAqZdqmrhsiiiMVAjnvrXUMtDbh06v6mxv3U5Udn4w5tvo5u04mA2NMAGlPCrk/GuBoAhBQY7HCy8s//evvBGMfO6HyBCHAOHKORMT7B4jTDpwGZ1E3CDU4gTMED+9gPZyFcWQ9kxxxBEEwgGaAARps/Px68/K2WDsm42yg4ijSadZTSkZxdHL/gRT3k0hFEpFWUoosieMkVkIEgg9BCdnvZ3mWci6HhgZl2xpDTEaRaI1/fP/e3ujIbPaJS81okvCB98MJAXpdla/tbDrpg84YQ2v8t6+WgHHrSvYd2uub23I/tcurmfMsKquX53Ni+vOvn1/PipuVZaDHJ5PnVLH+FBDgIwDl1Tw7iL55ftnNPWCcO+dXF+fXX35mnfUBzgdH1I+T/YHoRVKwriSIcrX6/E/+bLFqidB1Kjsp/Ma0cRS1xnTgGe+JC94ao5W6rubdj4zxtq2LYq2koEDB+6o2XIqyaDxUVTWMZCBKYkXBM1DEMuKzq3JR2JLgxqm61xu/ff/3/9v5vxc+bq/pf/j6k/SPbh73o5UtHr23JzgnoiSWBLLWbYrKWMcZRVoRqK6aumkJHTSYF44WjT0EvxsW8AbJhAhgXLA0P7h3hLgHeFiHRbG+WW1Wxcvr9bo09w8GWZyAMRUP9j/+HYwfvZEMVKhKVGvYEsWcyhWcJ9uYprHOOhcEQz+xCB66xX22DfJWbCUHvaPJ+3v3tVJpmvfznuCcmJhOx+++/VAp6b2NJJuMx1GaQCvkGZj8W4Tdf/hygOn79Ws7O5iO8FpICAg31/PyuF88f35ZtrS/P//u1W0Sx6vl8uX5srHsV5+dTacDrdijR4dHB/2yzIAB0E11xdWseJRUX7+4PdgfOeuSLGnappfos6a2LljnW2uMDb1YasEF42AgIPhQO8xKH4JnvJuWHLoB3mVZDQf9pmmEEM65TtHVO5JSrDblelPcaXSZtlksl7ObmZTjomqklOuiUjqrqnYwiECUxAqck7U9nezHx//m0fsvN7P//cWfLZefLprq+UJroX734cefzOcPuVn5igHelWUVR3FOwelIUiDjXFW1UnDfie+BQqCyanYYH0agtrXbDiYD3yG1aTvcM4AojmIxzAEFWJiAoi1WVVO2q1X5uaVNbafj6XC8f3zv0feMDABLkaXI9gDArdjsEq5p59c3m1euabup1qvG9spmWEpYgT2JOgKbjO/fn8rIOsfBuFB5lvNIQ2oQkKXgQF0j0uD/VDPKJSAh0td2du9wSui2DyGEm7PbVeEGs/kXz66FTGN98fJ8ncT1i1cXZVFUrR8Pk4/fvz9frj54eg+pOj4YdphOIAJub5e1UksCGw363pdKirZp0rzXzWlzIbTOt85Jw2LFwYgzQQTnaWOZId6N2euwFqDAOeq62d+bLFerDl4nhXDed6jA2c3i6vp2B9zqQF3hiy+/jJKPqsbHWm/KZihTxlkSyeARR8p5VG0jGV82i786/4IJsZf0j7P0rf7of/3mz61d/odnv1Lx4J3Jg5fF5mf33/rm5tV1cZOkGedCCuER6qqpmjaJtGlaoi2wfFM0dzgOEGuMDSHwrbTra2n5baTFMEgjDHJAAA3WRZgtrm6XdWO0FFmk8mzQnxz3Rntxr//D7fveVg5wGAMiHh/qoMzq1puaBd86tzDm/DY8EVFsFHjUIIq1iPoZhALjcB4hQDLkyWvcW/KjxZR/7HptZ+necKf2Rq1tX5zeWqRNO/v2xW2UmuVqs9i0vUQqwR6f7BnbPDrZf3J/T0k/fbAH6HRvBADFAvleM7tabGxRXe6N834v36xqrcTs+touZzuNP2ZsqI1lwEE/FbvygyPMa1hnicDFdjocCMdHYx9IStEaO+j1mqaNIm1aK6UIIXjnvHVMCMm2fXIGeB/qxjRNqCJjnBOcaSm1lhSglQShruuz9elekv3l+a9/+8H7gyjzCEoqJZR1Hr7etO3zVTLOJn95+klP6YQizqCEBIPzxCmEQFGmhTEAjHU+UFU3QkZbY2JoW+dDYKGTF+mgScS240+YFOxw2IfMAEJb4PLqyxdnpzdzH0hL1R+Mju492Ts6YZL/gEH7Y4sDEunBwVNMljNjWqVkCHR9c1PXpc3jWEowZgkqNBA54gQAIg7vYS1CC653JcMGVYl0+nd/lgXU/387AxsytuXbW9N+92qWDe/NZjdN65M03NyuHxztaY38MP3pR0//4leffvj0fjbIQmjApkAN9AGcX62Oo96X310UlavK8rd+8qhy0tRaSr66nR33095wWNXXoZsaFJDHuhNLB8ETVRaLpvU+cPn6LwkhHB5MAOKMdc2AsipjrWpjIq2sdb08uRMg6oJtH4LWuqyMDcw5H2stJIsjrZWwNnDGgBCaoNTwJ8fvfLFccxFtzOK/+/T/+E/v//OPH/7rX379Ky5UT0evFs+ui8sn+wezqhglPaWE3CqctbGSAHQkOxn5pjY+hBA6fBvrgOGtdd4HKcUWywvgNaoRvSjOpiMgBgqcX5w/e/ni6qY1nnPR6</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nOy9aYxlSXYe9p0TcZe3v9wra8vaq7t6q9maPTPchqI8NCWKokjJskzZgGEthqBf/iMYBgwb/mf/MwTYhEH/sC1blmCSsob7kEMNNXtPd0/XVHXte1Vm5frWu0TEOf5x78uqme5md8/ULDL6ZAL53n333Ygb94uzfOdEJPChfCgfyofyoXwoH8qH8qF8KB/Kh/KhfCgfyofyoXwoH8qH8qF8KB/K/9+F/uO/88vHjx3Ji6Is3CTPv/G1b42mWX+u3251nCvY2M98+iOLi31SKFSBVqPV7/VExZVOVButuRt3dq9cv+l9uXb40Dj39+/fbSV2dfXQ7mgyHu2tHT4Eju8/eNBtx8fWTty592AwGi4vLHQ63Tv3H+TT8amTx8sy3L53t91I1o4ee7CxubHx4NyZk0navn7rlojOz/WtkbeufJvEnjlzxge6cvXKjavfUnWHjvR//q8cFc6/8qfuzTcviXJCERHAFJSC82VesLFxZEMIIQSyUAGBoKTQ0jlVSiwTk6gSkCbxyuGT83Pzx46sjifZvfXNfrtx7Oih2/fXR+NcRFZXliLD69t7zhVHV5essXc3drxzB5Z63Xb31oMNw3xqbbUowsWrN4oyP3rkyKm1tRt3bu/sDPpz3VNHD99+8HBnd9JqxccPrW7ubN+8s5Ek5rkzp5j5z770ZcPxwuL84ZWF++ubw/G0kabnzhzb3Rs93NxVldWl/nx/7sKV6+PR5NTxg0cPH/725Rvbe8OyyE+sHVmY6128eiPLioV+58zJo3fub9y+v5FYfu6Zk8bYb1+5KSIvPHtyYW7uwlvXH23ugClinU5GcZrEJlluNY8sz+2MJre3hmLNqbVDaWL+9ef+tWqRpMmZMy/GcfP6zTtFmTFT5jIV9aGIbdzt9JbnF3b3BkGzZmvx6IGVTqfz6utv2jid6zTPPXt6e3ds/+av/fJf/ZW/BbQq3L3657/zuT/4N925xZc+8lJwLs+zv/rX/vaPdiq8s4TyN/7pf/vMi62f/tlfAKKvvfz1z/3eF4KaRtloJTFZmjgJmdva2u515wQKX4BATfW5crAe0BAmWVGWrtuKjWHnQiM1J06e++wv/50ja8cAIKiqJxsB2Nsdi9L8fD1KeYE0qTsyGOa9bvr2Dl68eOXcuTPvdRN+Z2+wtLxQvf3iF7/ywnPn+vNdAPfvrTcb6dxCv/pob2fan29Wr69du33q1CHAAhjsFevrD44eXGh0uwC+9a1LBxZ6y4cOArh3597W1s75j75Yfev6tTsnTx2t+7xX3H9w/9zZEzD4yhd+d37xwOlDazS3AACbD/Oc0iMHqjO7cdFs5d25pV/4hf8wl/61a9cLNy3ddHu4xWwGg41uu/3pl19pNbp3bz6Mmu7jr/w80ADw6he/cOzU2YXV1eo69H/9n7/pvJ/vtT/xkbNLh18Cwhf/6Lf/7M9fXT26dvLEcQXarfQTL3/mO8fnTeCFv3gEfxii7s0Lv3314TeCkfF2eOvCZqfRbKLRThreiZpkPNwZj6b9+fnRcKzqozjKXWgkURzF06xkqBeZTLI4gggMY+3o4b//j/8Jos53tTMal512/AO9lWI0uf1w48yZE9XbybhotZN3PHM6mjY7NeCKHCG4Ziuq3t678+Dw0YP7F0yaEcw7dNuXGA7H84ttAGGyd+ni64cPHu0fOgEA97+OeAFLdTe++dWv/8nnfmNh0c4vHvrYK7+k9tBw8ODZk0f+/GtfG07HYHQT7fe74EZQOTp/eOHoycedbANU9/Phg127tnak2WqF4N+4dPf+57/hSycShuPM3bju8vzcc+cm0+m3XvvzFz/yk0909ccAZAAoeuGFv3nt8s4b17403MsmA2nMNQ+eT9nHt65NWEfTSdbpdrvtlrgiqPGWfShLskZB6pWImeOIiEAk7Wbj+eeffzvIXIl9kEkAm6d/Hzdv3Dm2dnQfZAD2QfZki0UWkobZB9n6w+0DqwtABGCwO+40on2QAUg6rXdrzsaoQHbr+s2Nh/ebaRQTwa1jehFpgYVP7J/57MmDfwpJk8TaqNVutzr9YvJwPM3jqLEy33m0d39l5ch4PCpc9vyZ092l4wAGW9u9xYX9TsKhDFg9OGdf+eTPA2Fn81q/2z5xYm00nj56tEkmWn+4/XBjd3FpY23t6HgyLYY3k+7x739Mn7r8yq/9veyfTV4dflW9pI0ERWOUSVE4cVkIWFpcIPUgjeK04Ewb0kgiKjSy7ITEOSKEIEls1k6cPX76E09eeTgqup0kigHAlRLF/NRB5gspgh4/UZszV0iU8JMn7Lc4HU+b7eb+8SLTA6sL+297c+3vofVjJ48fO3l84/JrzSbDZuj1AAYK5AFpE0BjcbnfjFS9ophbPglgPJoMd/deeeUTkPL3//Th3jRjkU99+rPVBXfWN+YPrOxfX3OhlOMIqGw8YOaXzs4vAQBkfXdn5dyzp3e2d7721W+8+cYla8zygaUvff3CZ3568e3T/Ucid25cm19abddT9t7RY/Gt631JR3OLyeIhWX9t4PJpnpcry3PNJNobjL33No7H+ajXi1pJO5D3JCi9clCvTGi1Wh975edXj5+qrh8C8izrdhrV2zIv4vSdrdj3I6Nh2enG9okj3wWyJ+VJkAFIGvQuJ5bY3kKzgSSBD1DAMGwEvKvdXznbAQrgEADgHrCBtMb95//VbxUuwFGPCDK+d+1er9M+/uzzACaDXa/otBtH5mtPLh8MngQZAEof387+bT4EDgAEPjC3iDng0OFw5sSh3/md3792+ZIEt7Cy8q9/73MvvfTJI2tr79bjH5ocPXEKoZi92zjzcXPl4tHh8Eq7k7z65R12vLoyd/f+pjVGQpnnWRDk44kR02jEFE15GhFRFKtzgVmaaeO558+ffb72l4PAGLTaDczM1lMBmXdqo+8AR6dbP3tXaJS8G27ej+j45uXpNHu0Pbjz4FFkjLG8MxhPpoVIyPIMSmy41UwPHVg5e/rYoQOLWGgCCVBpyy5wE1iHKPgYUINMJ8XecBKEOlGaIL59+eraqXOIEgCTwfjClRte/KGl/tbDjbRzMmrEaa9XdyfMLvyE7ONsdfZiF4iANmCSzvG/9ev/+R/+7v/77Te/QcYePLT65oWvb2xuf/zjH/0+BuXpSBnK+7e+dPzkx4HV5bh9/lP2zv271nAoaTLNyyIwUxzbvCiclzKIMEWxbabsJ8HlnkmJlQw/c/LUr/+D//LJgTFP6JSnaCi/C2RPyvcDsvGda6+99sbuYFI692hrL0kSY3lra3c4HouiKPIsL6Aagieg15u7dPVmt93qtpKjq/1OYk+dWsbBLgrCwyGOPQOsAcDeA7QWqZXMpzRpJllRapSsPfuRqsXgkcaxylRUXr34zZXmStR4QlnqO4AMT+BsX+b2X2XDRwGtU2dfYujN2zdeeunj51/66NVr1weD7V5v4W1f/KHJPcDHsR4/+UngSzv4w3ksnj839+Veb+OuMBkRHU3GvXar2+ns7W2LKKlkmfSa6XjIJpMgQVki0s9+9pde/tm/AWCwtQUT9eZmM1KB70e/PCFvV2NPUe5eeOON11+/c+9RUM2yLIh2VEfj0db2jqhIkKLMgxdRkeABMobXH9oNQ4bo9r12p5leuHzzuROrxxfm7NlngBVgD5MpGj1EMYBJmT8aThvdKG08jiqMBWx8aGX+4d5O6SbPnjldHXfDQdTtvdu4vR1nj6XRXQawsbmzuTsWtYcPHo0bredfmH9aw/Q9yWtADBwBviq4x5j88b8a/fW/duLVizeMsVPnCUiiSCWwMUWR2SgxXE4K75yqiGe/empp69YuE833j9UgG2S9bgtx43EjTw8YPziQPbhy+a23Ll+6csMJM2M8HKXNdDwe7+zsTKZjIoJqddtBRINnYgk+KybihQ0Fcdm0sbmtj7aH66cP/1SvieNt4ABaNWPnpvnlK9eUoErOhe9q/a1rl+aa/ZNrZ1hrCEXdHt5d/iKcVXLy5JGTJ/8OgAtvXuy2G8PR+PkXfyS8xg7wm4AFCPgbwKcYd/7Zb/2LycD/5m/c0WQSQjOEUGRFs9nwvhxPxq1m1G537m1sTcqyEcUooJk4DUnHJI30xRd/bne0pzqe7x3+UdzO9y4hd+O9R+O9nWs3buwNp0kjDXnpvLPeFC7Pi0yCJyJVUfEKQAOgIECDeBdC8F6ZiYkIWub5UjvB3grwJFDy3fUHzhXGECml6XdEIfeuXjh59MSJsy+89e1Lu9ib6x7Ee8l742xfnn/h3Ps/+WnLDvA68FFgEQBwBMDAT5rto6/81IFvfu3y1du5n+pkXJbjLE0TJjLWNJuN3b3BNCsakY2YvC8xlZ313bQRHzm2dvjUwQfjL5xZPQD8u4Szh/c2Vg+v9A4c+tKf/dn6+qYovCuz6UQB73xZFiF41QCQSFAIFAQFgUkBVXEqQZSCd6XjiEwZivWdAR5tIHsLjVPAA0CBZ5ZPnLCsKkTEx9dOPNmHw6efB3w2Ggx2tp554SfeT7c/AM5+pDIPfBwYAQR0gQFw8RH+oDEXxnlnbzfEeXM6LbYf7fS7nTwvnPe9bms6ngyG4ziKAdgIQZ2b+rRtO8u98x/7ifl2mO+8+KQ/+uMvZZavHl4BcPWbX7/81uWsKI2xzhXOOWuNSPDBQQQAQYHK6CmDFGDDTKrqNQQlDhKC92xUQtgeDe9uD45sXMexe4ACCfAMkLMrNWIVGoymq9/Zk2xz68q9ex957v1ath9nnBXAk4RCF+gC3wCGQARcOW1P4uzl8ebedOyLMU0GhQjSJCrLMopsGtmiKNkYV3oNwSZxc86SGsuJlK2l9gngi8BJ4MS7tv/jJ3EjBRDG4ytXrg5GI5FgjPHOiQqRFQlQUQITgYQgChCIGKTMRESQ4EVEmVSCD8EyAZpn+aW9yRFpA58FCLgH3MO3rxfOxzYiNSLfTew1lg68tHTg/ffcFlmWNGYusCroB+W3fnB5R9bq47MXOdA+3cl/83NX8h0ppsV0Mm020zSOSg3tZiNNYiUkJA3CaDiaZlloMJGMt3Rn8+Y/+9//j7PnGx97/j3y3D+eYtrtPJsWpWNmqHjnFAqoahABE5RUVAEQAURcBdAEVZEQRJWURUVDCIYY5IK7O5yimJtFQIcBlI1RUCImJj738Z/Zb90XwRrzQRUU1yALHnW//h2Qne094DlgTbBk0IgpYRURdJopNBjLSRwbaxkaJBQ+lI6ynMZbkm+ahkkj4WsXr331848u3XgV+Oc/6rv5XuThg/shBCIS8T54qAJQrdCmqqpSR4iGiIiYQEwqIhJEVFUIEA0SgkIk6DgvXruzjuHOfhPxiWfBYGJmqrKoldhkH2QF3rfwo/UNoGJFgPDd4et3SXD+/V/6ByFl4YaD3flZtcw3Xs9uvTUYjvKApNFII8vWmEaaJnEUGZs77wMZNJI4tYD11IwsVGGlezRaPdO78sYmsPxUOibvMXJPU/7k//nnk+kEAEFDrZ8AUogCAlVRERVVENQQYsvMlVbTCosVGgmqKqpQQun8+qP1we5gv5U//p3/mw0xERu+8KXPPXrw4Lv7Ucr777NdPrACIJtOG80mzLvz3yJgNpEFoN5VVVk/XLkDlHFyipL1ynn/0hf/7R/93pedl36/n0TxZz71yVNrB7/x+mv3Hj6M4igr/TjzISCOUo2jIhQgck7Y+GQx7h6h/oEoLfrAkbc5gh9YvMP+eEyG41b3e8lqv0+5f+XiaDS2kbWGRSCqUCWDuhBVARKoqgAQMmQNJYZKkFOgAh+pQqFCZCrVB8B7cd71nkhQ3n9wj4iFwMzdueXlg28jL55kHN9LeGvjEYBGs/leJz72BH+4IBsDXwHyHDlwCkCEZ6sPvvaVzzvnFub6TLR6YG1zt5ifX/mV/+Qf/qO/9w8//crPNFrdovR5lsVGIkNZ7rPcRZGNmILLdzfy628+2JsOgFPfJ8gAPDkeP1CQAeh05qw17VbHWENU28qqRBgzpKlK5bExCAARMRFURARa5Ucq06n1FRRBgyv93UuvIdutGjq2tqYEEGxkjz77ib+wU+8tdnHl6RiOH5hEwCsAUuz77A+Ag+V4Y7C71W53rTXem29863peum9evLnQb//ln/ro+Reea/eWTp+5+0ef/8M8m2SZ8z5YRlmWrGTHceH9yZ858ZmfrK65Drxr6KRByLxzGUXwtbvxw5ROI2FGFFkmBryKAGAiBaBQhNoqSiC2IASFV4iqCkSFlMDQKjCgKvCrkel8ubO5fuT8p6uGSp8LIYD4XW7/A8mPM68BDSDzdmWzAXzpc39yJU2bnbRx7vTZa7c2v/XoUu7KJIrXH9m3rt9dO/hvz50+evDQgZ//zF/+48//3niUNRLb7nSff/HZ1dXeT3zyF1u9ZeDfAk0g/wtABuAdQTbYHfTmej98kAF445tfs1EU2ajWUBpQxW+qoqFSVFoDSQmkiiAaVBWqUuk2VhCRKogBAaA12Ub8+JYuXroIY9kaRDTeud+eP/T+O5mNs0arsZ++29vc/rHGGRnkl7+VLi1j/kkofGRjM7p18ZvTyeQf/Oqv9p/7xM8C/9lk+x//F//13igTuEJw8657tL13am3z537m5V/47C/+9m//yxOnn/m1/+Dv9pYOPJG8/PSj3avLc+9Q2g+gmIyT1jtbwNFwup9x39ve7S/88Jje8fpD78q5fnd9Y1NFvAQVpQpTGiSIqNS+PgggQIkoKLxURwkEJpYKZagOUFAlCDNL8Ni6i7R58+7DMnhRIpvAxh8IZAAa7e9w3fpLCx9YJbqi/KBf+Z7F3b8WldtPgKwOcC5945I6H4J85bXX609aC//j//BfdVMTfN5vmo+fWvyZF4+Eyc4//xe/1Wq3PvNz/97f/rv/aW9p9bsy5Mtzp9/eqHoH4N1ABqDTfezL7oMslE8/4Nx4uPVdR9pL/W6nAZVsMhEVCbVjT0AdYdaBJFC5ZswAFKSCakEXiJgNE4uIas3eElMICmiZZ2WRo71w/Nnnm43YS5hmhQ8/dLvp8jxK31kBvF3ECUffRxe3H1z+5pef/4mXnjhUXe2rN669BZUkjr7wzTfv3P5v/v5/9Fdx7BTaB/7J3/+1/+l/++2//Mnnf/r8GV5axGT82uX7e8PhuZc+1uotvs9m30+Uo85R9Pi0zfW7SweOVK/9dGrfM6h6f7Ky+rY+m0av1y98UKgEFQ0iGlkGICpU2T+AmUlATKSobSez+sBgIjLMhqj0wYdgrWEiMAeVsvSqEq/UIefZwyuxz8ia+fQDxJXvJh8MZzOQvXd91mBv2uu/w3CLD2zfq3pQPO5cvnnjBqEY37rWXl4ADgICGOD67/7en7DhOI4m06LI81cvXMTgM3jj61juHPmJ8/9d21AaI04RpUimH3nl/OaYlg6/g94CAC1A30uw+STIAOyDDMDTAtm7SbvTUTYAqUoIIiFQHKsiBGVSqIoqgcgYAkSFlYjZEAkxCExkDBtrg4j3LkQ2MpaZVJDlZZZPp7euNE99HMCpk6fb3W42GswvPIVKsPfGWT7N02atwyTPOG1UIJuOx832OxiXasXE20EW8rFJ2+8NMmB09cqNr39hEqXPnD7c/ugvzA5fBRqb975670qpQiHgxbUzZ9fWrBQOiOZ6cAIs03N/CZf/dG97t/Q7y4stHDy71H/3lr4nkP0oxY+uXLmysbk1Gg4BhCAiArCKigQwE5GGoESWLVSq1ACgxMzECiEiEJIoAjDJM+9CZA2BAJoWRZ4VGw9uH5/rYmFBwcPBBIAxDYwfIkorhw+zMHXfv4MCAKj6ozAEMkA8+yBgPH5vnO2DDAA/oULfEWR424qJfTHp+yKWdGvz1a98fvfOpePnX55/DDKMHk46q8nF1wv1RGDNw2effw6xebC1/saFC4Phlknsz/4SYellnH1l+me/K6XDR36EhUz74gEGPGCByrXVWRWdzIojAAj8ALmg4lAhlbmrEpSQynma3r159dHDh/c3NsuyhCIEkSorIBKCMFVhpEpQaxREwQcirkg1Zg6iCpUgxnAnaYmqK4sgkWUCUVn4aV6G4KEeiJfmepvthvMOGuAdTApSoDLOAOqMaWWYa0RVwQURYGpQwsMHdf6HH29eq+jWd5Tf+V/+aZntjnY3mmkrMkt3v/yN17/+epblIYTReDo3107jdDVaiZJEm/xHr17qLzVPHj3U9mUU83A63Lhxc6XXQvzcwaMraM2jMXni2uOZe8eAAxjIUU4QAoJICGVRBhUi9l4k+KAgJQVVjnX1y0wEA1LVynsmBRkmgI0hwzaKbGQNjAEzjKnXGjBDFWFaJbuhgAhUEQSW0RIgAhzKUp0KUBGuIBUFY/8JqndBlRTqXIAiqIoIlOqrqqhUKoV8cJFaQxREWEIggsJYCyJV8cF78a24Sd3O7l6Q4IUiEnFBsrz0ISAEwLcbjVajNZ4MIxtBFCKoODoGtFJjDCJIAAgk9d0xYBRczSKP3ENQFMUPFGcBUGAIBKAAbu7IzasXLx87dJ7TyVLjKLACzGEMgLLJ9Df+5/91PgkaJr1uswz21a9fKMvXidQwjSZj70VCARUTN1aWDxdFdvvulZNYPrzYLMrxpCz6ve71a7eL6fDoiyPsbKI1DyeIbgAM0dlIKbyCFAL1EkIIQcrSF6ULwSu4KiSYkQOs1dMGExklkBKzMDOIap1DRgUEESEhCSKurA2KYa6MFIGZIVrRXaI1YUUADCOJFLEBAoqyLOtSngpcCkCFiFQJpF6UOLY2NswgVkVlNKnWLBREqv6LSghChlXEe4BIgxKRtVaVQpAsy1uNRiNNXKs5yTIJnilS0cL5PHcopshHIPR73SiJmo1W7lw+2tTKEFdZLQUIrBQw41NQZb6EWNmyBildUIGIjCYT6yeXLCUOBUuszkARQgATBOYxRUlMQJ1DI1CV0NCiLEWhKkwmioyI+uAZrKSVSxBFhlNBo3S4cOP+3qU31k+faRe4vrcjS4cWgAxooG0wYO+cy/KRG/VaSavV2Lo9Vj/Os8IFH0dmmmdJlAbvBLqzvfXq5QuT6fj4wR5jIU10HNlyko3zoszK21dvZ5vrZ1/+NJIBZB4OIKkUApRQ3URQqEoQH8Q775zzwWtAUF89WxUoESQEECmBhEhBXJZlXvhup22MIagqgQLNoqJKrVXUPAGGDajyZjBTSRUytObuVUDUmo46KeBDNg27oqJc86+AqKiEuggDqorSBxunSkxsCCQCMlWF2RPcPhEEIXgmK6oaAjOFCgrEsWWAyqIcTyZzhtM0KctSoExEDAkymk4He8NelCAEY2wQO5q66Z1b24Md0pl/RiAlYlDtlNX5hYpSUSgRk6pQ7b5Np7ktWl+xOBohdQBNFsIkAkFFVdQwAaSqtatQf00qcoaUrLUi4r2oiqqp9CmRzqpUVESQG6ZovHesp2PBw9//w/tJS37x1xOP6xYAeoCgRTIISZreuXP70HJ/NNnZ3sobSQheN3e3gooXPbq86oOLbJREZHwJX0zzIo5Nr9MaTaZOJEbj2PGTk+GAkgKxQe84xruQXEOo3GEfpMrJ+BBENAQpCleUZRCp3gIQqVOElSNSWTEirsbBh/Dw0aDdSnrtJggPNna3dkfOSQg+BKnNGCi2fPjg/NJCn6kau2rAVUSq60tNzitEE0bfqFEdOtmr+cFqPj/5owBZG6dxU5gIhtlqrXsBUgMQU40CAoAQxLBA1UtggkLL0gNsOGEmEZlOp7HhJE3i2HovbAiKIDKdFoPRqNls2CiKDZfFNCt8d36elEBVroqqTAMRAOKqw9UUrgvdKgSymR1kw9aBC2wnsBFezt2wKIpWK7HNRu3QGaovxQaws+V5laNnLAigGATwjOkYZOsPgigAEfGBDbPk2m/MZT5a7a9tt6cSxn63aRePABNgC2jBTlqL6b//1z/9+mu9a2/cGA52XeGHk2kapeNsOs6zRtKwxlSxUyNOVhcWmkkynebr27s7w2G7lWxubd2Y3G+nz7db/eHk/mjjYWf1ENqdG6+/6V2o3FRRVZHKsyEAYIVoUFRzuSIyVWY8OeRx0ScxUcWDLvQss3o/VcXm9uaVW4+Kwud5KeJF1Bg+cqD//Jmjc90khDxUD6M2hRXrULtUlcYCNAhyIgQttPKx91mvqmVUGUkolNT53HknRCBmIq1uS6SCnogAtV0WkUqHaQgOwmRVQlnmbCiNIkUoCj+p3UijAkMMwAcpynIyzaZZlogStJk2s3LsvDfWErCPJ6KZHp+9qvLxAhiiOmKoE2LEzOb5Ez85lezo6n2g+DdfuPfsS8e5dRK2A9uB6YDboBaoBTSBFEiBBIiBqIIawE+ADEAaya7CMyuxqnpRTyzx4oGoubrcjA/OrXZs79JXx8+df55oCnQBB4w5MvMHJufO//qnfuZgt7+wuDK/dGjp0aON7b3hcDrtpo1+u+dDsMZGxgJqbdzvdDa2tntLSzfuPLx9b/vilbvX7jzcHgxiq/1uswNC/0wrjHdG4yoe2p9yjIpUqnIw9c/j10TMtS2iii+va54JgI2Mqc+n7b3x3rjQoM57AES0NNf6yZfPLcz1jDVMzIaZDBlmZsPMzNW16hfMBGZjiDkQe2KwIWZUn1UvqD6h6hgROa/jUT7J8jzLJtMpNCRxVGms6sc5FySo1Bo5BK8i+5aXocSsKkVRqKo1Jo5iMsyGrbWW0UrjdiNppKmqOC8B5IOQjRSCGt1MDNQDVI3LE69AxAQQ8wyQTM55c+DA2vr64OBHxI+OvvDi3wJ/39k6GqoTrhuuFm9RxAGch6wgUBTF29tb84fRajS1bJJZASKgD9wENij6qUMnnjv70oEzZ1aOP9e5cOHKZK9sNxqxjZ0PPoQkjpktAc00YYq86t1b2+pNGiXjSTEe5722XZhvtxqJXe6Y7mYI9zQAACAASURBVOp4c0OJDBHYGOb6GVZP2jATVYeJ6j/MXBGb1fkwVS1qjdV6RJkI2BlOd/amQSomHSKBiE4fX2000hqpvI/dukWq63Ro/ykRkc4cwIrGYKqMUv3cKqRTVdpKDNLpJN/bG2b5NM8yEUmSKLJGFAxVFReC977KbEKCD14kqO6XbisACT4vihBCZG2SNpiZ2cSRsYabadRrpa1Ww9ioKMtJ7nIXTGRVddYzQhV9PKFuad9LrGZz/fDrvy54C1U/ic52/hE6R79fhFUSJ8yFKhsoEVfmJp/mGGcCZWY08v5878qrRev8ydbSPeBNoPVo1y7OzTEuAi3gNHAs6tiTz7x+9vzC3r0pQYvSMVOQMGKbJqkxVgFroqtX7hal67WaPoSFTr8Mfjjy08xNJpN0/T6auWbBNFiUDaqxquwVaWUoa0ejLi8lQyogUiizKhG4jh+UmUWVURdtEcMYttZyGUBkrDXGKqh0nupnUaOFMHNbSEWIuS6uEAIJqsZEUdVRKARUFYZBWFln1geGCIYotjZJmBCgEll2vhQJIMtAgFQEWWXCqhXCIQQFBIFCMNaIcBAhSFaUzoVGo+yIGK48ImJmAN5751ySKhEVWbY3yeeiiFgBEgVBVAFWIkuAQoKTOq6pnYHHDC5AcRwTkVVVDbK/e8fTkJRoVMVZxhCEqng+StT2xBWlLwu9o8PRJBuHVm/ecbq1U+7qVbPVp3A+a1861NoGHgG9S/fuXH91mMQJE/IyM2yIyAdflKkx1vmSLEbTyYH+XGTjsvCZKwbDURS3B+NJf9yen0y2HgwGj4Zzxxdr4orAWoXDEOV990uVmFW00ieoalKZWFWNYQmhLteSqngQSqRKR1bm53utW3e33roZDFPwEsQ5L1XAxKb6W3nrVRE1mI2qVGU5JFAr1QpLnu3LWpdakKpiVsc4C/CUmWuelAiW2VoWEeddEqwiVBscBAkzpQXvvReFCrMhIgQFBwohhFCUzpmQ586HEEez+lsiVXiRoijipIyjuN9tFOCNjY3tnU3U2fqgomnaOHv2jDUmz8Yb928VZeFdtVJB4iiKo6jiiIj40LFnGMYatqUHsAM8rQ0NOsxbolCBEpghIBa2vQBsRsn8jRt3n/9UbyH+ewAmD18rygZLEWxcWj/fOrA3tGhtAXr99ubXf8tTkTYbRiWE4HwooGTYhuCrRIsyJ2xL58fTMi/LLM+mLu9krfWNwYHlhd3BcHu3HI6yeSwxQanysCslBiNUk+4gJVUlw4+5bgk6HBTDSbHUb60udwrvsqLg/UhelQiddqPTbkwyd/P+EEREPhShLH2lFXhmYZQUQrMV4SBwxXiCQcpCWoVwAjAgj/3/KjKZ1TETGyYFhsO96XhIpJGlOLIE9c6V1kjQIKGKfEWE2XgJpQ8hhMr1MsSiWlFrRemc8wicFUVwXhOIhkoV+hDK0hdFYaZTSSWyUbuB+w8nOxsPQQqlKkzO09SfOGGsgcIXk6IofOkq1iaxgFJF3IJYgidjbKPZBBPGj9B+WjiLwMyiwsrEosokNiWgD3CWr9+7MvrEs1FVld9anfP3tonSFT0f+WSymw/WO39y7ebR49G3vrh358oOgGaahKClKySQD8GLU1epC8ryIol4mjsouVB6DVCUpb9+c6fd7WzuZg83JsfXjs+CfWilpaqYkvdtIhhcUWYAVDHNyus3d+8/2IqT+MJbdxb6jY+cW+v2m0VZ1AQuo6KKiLiZJCaKVBRGAS6crxezEYgr8qwCJxNUCaIVuKSmTARV1oFJQUTCNTGkmPk9UKkTUKQQ8YaRxjY3zETWkIg457wXAD4EHwLAoupd8CFENllc6HdbLfLivCtKV5ZFphiHkPvgvCudh0pFqBLBe8mdd86XZeF8iJJGxCaJ40BRZRbrINfDeZdoYoxla7ksmGmmjOtsWRWJeO9im1gbWRG9dffBsWefeUo4A4hBwsbU1BsT4ooKmewN9g6cTu8V22ny33/tD9LPfvIXbWS810RbAJT1wNxyN+/e/dbGxv29bFISYDhqpsl4CgKFIEEkqDLZ0ntAmBMALhTelYXLc+eyPLtxd3dnMG41Ws04OXfu3CzEri0fVVXOVJMHqoRZgpkUXsK3Lly/em19banVskoRNja2v1wUP/3Ki3ESe19W36koCABJbCxTqTDMZExReFFlCBFXFNk+r1QNDbRKMz5eEFJxyJUXuM/q7iecqq9XKQEANrJpYtvNdDgcivhqBpXOV+Sy90FUFSTBF943kubxo0dOHlvrtVvBhTwvvPjJaDLY3dna3lrf2pYQyrKUyicUYWOYTRVvSZAQShc0SltJ2tKknxdOAA3Bi0aBSheqYNxU66L26TVVJSVwpb6Dd0RkDRuF3L2/eezZpwYzENVTvqZsKWSK6R6l8Zw9La3uYPTnScIbdx/8y4e//8LHVo00FrurFYvqSn/j1v379x5NtodFkRtjnHe9dtcHVxQuTSIfAFLL8d5kzGyYyAdXusKFEMQXrszdlKC7g7EIrawsmlZUkzz6RE4HNSMFAZGKElczlbC7O/ja119/7siBX/3My/1Dy/By6+76hZsP7j4YnDi+CC3rKY06OWIjawyTD1UpzrTwKqLWUBU17GOGZsXSVdyH2XzXGctUd6kKbOtO1kxUpSoUxIijxFqOY7KMEARQUUgIAJjIh4r2J+dlsbfw0rnnnj11+sDychzFpQ9lUTr148l4MBkMtreuXbv6cH3dOyci1tpKy8eRIbBz3nmvxM4VRSBr7FyvbbJpUGSTUkIQkPMBADOzNYwqFAYpaaXPACUm0uAdAFvFGA83dp8eyiqWUx7PYFTJE4RpghB66WKU/bS/qUcXb1y4dPXmv7xHpC8+98yZ08dbrdaN2/euX78lhZvsTXzweZlZ5n67l8TpZJIRQVQNsTHkg4sMK4L3pWggiGFaXOg/d+7EkbVDSRKVpT9z5niz2wIpql0mFISqFqJ2eqWO9ytHGwrd3N47urTw8Rde9D6AgcXFY0urUWw//41ry0tJIzW1ozWjOmJro8jkZa0R88KLqpkhpB4ArUv4taIb6gL+imCqtW1ltkipqrChusyGZpmciooyUbXfq3qqniogIhKUDQWRMAtoDy4devn8R1969oUDyytJnFaRTRD16vMynxSTwWi70+s0L17a2t4uyzJJYoCc86piDfsgrnSIohBQwgvs6pF2Y6oP7+Wo9T5K55kgbIyJqOZfKnqymiDEBFFUW69ZBTHz1s7oaeKMuV5yTESsEK48yIryjCjp0nKI5IUXWusbm/cebg8G09ffvMykzVb7ypWrDBrsDIMXa2zwbppnO8Odxf6SNeSCa0QJGSPiuq2miEyzSRDPRM00WenP/6W/8tNrxw9HUYTK2FT5yZn7r4+VxXeUaj7J2hvg3MnjRTa9syHtTjK69cDBLM53ESaqWp/JNQdOgLGcRHZEnomYbelDEI0ww9gMJlRXOVBdiFhvVYD6eK3s9HHyqO6gVmUmM+gpwYTgnSu9L4MPilkKgyh4gcIYXppb/sRHXj7/7HMHlg7EcWrYVEXbwqQizbTZ0U6v02ukTYD12xezIpeWxJENErwXJmU2IEiQAC5KN3G+ZJeXIXgJogJlcOl8RYUYY6niuQMpaVV3UM8eggQHVVtt8jEcZ08TZ5ZRas3iKRFDRInYKKmFqCoMmLrdzsc+en77j74grdi74urV60EQxVaDTgdTQ7bT6lZ1LLuDvWbabDXbu4OdkjllxEmDjSuKvJHEkeU4irvt1pnzp06cPsbMdfA/8xiAWXFe/RBr0rGu76F6bCACpQOdZsn6yvPPkBEcPJhCYGKE7PB8txlxfakZipTIGkpiW7l/xnDpNISa2kDFaFYmufbiBTXuaVZfBtQObeUmojanFetSezpESsSGicgQAxq0dGXwoSJMrLEVb8bM/U7voy989KMvnF9eWGJUKDaGVUQN4EEIPiJEzU4jbVgTuTJcv3bZlS6OoiB1TZthU/GFwXsvvDPMBuOs8EWWeRFV1YAwyQpVEJONYkbFKYc6YKbHPyJBVSyRIdI8d08TZxxB8zpUrwI6Q7WBAjQIsZAaENbWjnzqlU+8/sYbWV7GkclKTyCXldNRYdjPd/vWLlgTDcY7j7YfHVo53G13B+Oh864hgYnTJG6kCcGwoYXF/ulzJ601dRpcCVzV5ZGyYv+ZEiCzzK9hEswMXEVUUW9hocAk+PF0XHZ7bXTbaHYwyn7u5Rc3smzoSuxryprbpDSxqAMe9kF8EKIqupzVNFSeKs2mXqUQHytREECsJCyQ/dlRAZqZoMSGrIlAsDXBoVAQM4itYWPZOSGiOIrPnDj7wrnnD60eYeYyL1zwVCe9mIhjg0J9ng9jjTvtzrFDJ7yTyWi8vvnAe28N+xAgai1bNqLivBtN/d5oOslLqfcfkkorl6UXqCGyNgYzUaiD+joRVL8RCaJScR0mBPf9L/9/QhLQaDaEXPsgtWtrDFTFVDaCovjcc2d7/d6Xvvy1wXBUlp6BkCPPiyjioixazU5koiS2e8PdR9uPjqwebqTNaT41RFFkMUvpWEvHz6z1F/rVJkxUh2+zjHQVBuw/1rp0CQwVxozcqnNA3Ep9WT7c2mTb77YOYPcRyjGCQZpm0ykzqypJTeRXQWsSRzQjPEIIpQt1LUPtEFckGhEQoMQVlzGjyMBcqSLiKgEgFe/EFZq58qcrQ6YhKITJMCGy1lrLvk7xKQIRLc4tnj119tDq4ShKnHdOgi+99yFOktjGbEwUxzaOQ3DBTcRFzbR76vjZIsuzr2V5OQkhOO+cCypiDJGnKh+nAueFCcQwagENkLLap0gN26iutaPZfdb5qNkSZAl2v3YJeFTtk/g0pFFvVV1P4lncVZdHWUCqBYSGQMTrm9vOBe+9NcYyRuNCFUwmL/MkTpnRa/ebjdZ4PCxc0Wt30iQJIZTOqYoiBAkRJ4tHluqCOaV9YDNIZu+r2SaiXBXQqarWnFat6WZporjb2rg1eOZoAnZY6WP9/vooK/azAnWl0L7CoTQxdVkesRNXlIGIVGmfkKuArVDmGqK121ZHJ1RtgUdECsOQWbTJM2UHQDWEoEFVDSOyJo4iYwyD2bCIaJA4io8cPHL44OFG2ihdOZlmRTEt8oIVxtpG2ux2+3HaSOJmK7jBXp5nI2LTbnRPnnxme2fr8pU3fXDeh9w5V3o0EmOIQXXMUnuPdeKCiEIVf1gytoromWjfYaiz6cRVHXmwmJUPDNe3ugeeFs7SmadMANVGojZPBFaCAepqsPVH21ev3phmGREzaT4p86ysUOLKUuFG46mXENs4SWJAijJ33hFQuNKH2no2O81Ot7WvrKvsDKtK5ZNWgSaBZmQszdICtetdF0hTnUkPZjIt1jfvn1rqAn5Y+NyHmdml/QynzkxEI41n6SBSQeEcUCsynaGRHhMXwCwyqbwvrfUbM7QqtKiCU5qBH6BQl01XlBFZNtZaCIIqa8WxUKvRPLR6qN/tOOeLPC/zSXCOJAQfphOfT6fExkaRTZJmZ2402NkbPJxkedwohWlx+cDW7qNH6/eKwjsXcucAidkyaem9iDyOnxUKdFtpv9Oq8mTWRFW5BIiqRzDLObECgATvLRRsmNnevr/5wgfYoO/9CIFmUKtY0jpUt0CAGpCWRf7Gty5ubW55EcNEIeSPXO23qHqoCvqd3s5wZ288MMzNNE3i2DD74NuNFjFVXKhNIrAhrqgwqgn0elwqSICwb8GV9gn9KnFIZm5hud2dg4lgmg8uXO6lcVlOi8l2sno4HpZcBmioKYlZTDEjeilNImIWCUwQUJ6VNcFWK75ZlX+VICfMcD+bfDONWnl4Ui+Hpv2ixepadWxAZn8leb38hEmCEKHfnV9cWDDEZTZ2eR7KnImiKOGGaSsJWNVPJ6M4slG3lzR627euDSaPovak3WlHaby0srK7uzWZDPOyUZZeQmgmcRoZUpEZ9ViptjSOTq6tSKgSqcTGMHFVyaFaZWErfQYmEoUPzlZOALF8883bL3zsKWKM9od6Brh9W6OgKj6Q3d3Bw/v3iZlFNHg3kuBnKlhVJEzzrJGkc91+ZOw4y6Z5lmZpv9tLFAS44BViTOQFRVk2qz0d6jjuCfpKUCcyiajm9Wi29QmMiQ8ffw7J44KogytzaXmo09RoYQHNVtpcPXpA4bL7d2+6spghRgElsBIlkWEmkRoW08JXw72PocpPrGNd1OnRGdCrrHz9uUJAXDuTtQblWfSsAJgNkQ2iohDREDwzqYhhs7i4NNfrkSIvfAjKccNGcRKnaZqkaRNEwbm8mI7He/04TZst2M7tRw+TCZZF2i2TNhppkg72trKscN47HyKDTiNpJoWhfJ8NYmiv04isHWZ56UIjFWLLxswiZzz2iWsNrz54q7OS7M2dyXAq3eZTWOQO5N+RFMbMRavgNWO/oeyc894F5713MaJiVFq2TDDGBPEMyvPcd0LEUbvVMWyG00lWZI0isTaiKldtYmvMNMtH42m/3vbicQAJEsiMiqgX6syWq4EExIzl5TVYW9ejV3JgZT4W2ICYEa3U4VE0d+jswXzr6oMHd3TGDgKAahRZa9hVi9iAPHfV3ndMFUcx4ypmwdD+C8xKtDGrdq/CC4HWpCee1GjV0nEyUQKyIUhVKx5ESDVNGweWVnrtnqckkxDFSb/XTpOIWSNro8iACWqSHIPReDTaSZvd3vyCZZ5m46JotBoRk1bzfZLleenLMohoEnEztrE1XFJVxcaWW43UOedD8D4AMMYQm0pbP4aAau2jE4l3lg1XM78oitE46zbf9f/pfRBJK8b9CZzNSIXaWNXZ/LSRRtYCIl6M2CzL57s9kCRxkhfixVFAnme21Yk45iaBKctz511ZOjKURAkryNq98XDfh9inY+sWgaoGmysjSaQ622wCMDaNe30MH2GuBazMzk8wf3C2Xus7YvB08fRCWWxuPMATIDCG44izgpgYhKzwImq50gD7rjOIZhuE1B2rkVX1SfcPzoZOiVihswChzsCSsXHKNlKlEGb7swD97tzK0oqN24PMDJwsJlHajCPSaT4ajzLRwJBGo9lqdlrNqHSl+LLXbvc77Y3t9XJkMpuW5dQwiWI0ySbTYlqUeVG2mo25Tmu+43MfssIptJEm/U4jiELZeT+znFHlJaqSiHqRalEhMRGp987ayFb2xDs/Gg+x/FRwNgMTuNYdT/pqT9CclTENQRqaFFkuQYwxIspMzbQ5yUZBxIfgXJEkDatRI26EEIIPxlpLVkSZufQ+kBKRVE69zLaVqNOKorpPsNN+5yow5lk2uHuj102RZWhUWysEgP6Cf/DWO/js1ua6itQOC8EaTuJ67pJSXjrvJa5zAvsms64tmykw6Ax01YjoPvIep2GrjaRm5p8AJQWZ2FYUv9T1jGqNWVpcme8tlMEO8pLIGZLhYDocbm9tPZpMxlC1xnbajeWl5W5/PjZNwKexXew3Jzsl8t3xdlKSsDXWRpPxeDCeTLJWnrtGGqcRdxvx7jQufRCRbis11rjMFd6VzlVxJBsrQbPCe18MJ2Wj4brtZhzDkiUiCc4mScO7koiCD5Pp6Il/KPYBcQXQk+/JVP+KHGBwFQfMXDRwvXRWYJiDaEKxUR4XGTMZZoaplgpaY5z3lbMp4v+/9t6rR7ItOxP7tj0ufERmZGZluVu3bl3X7NvdZDtySJAUSRkIA80AkgBB/0hPo9+gF71IgjTQkJBGEmZIcbpFtr99bd1y6TP8MdtvPZyIrKpmswUO+CTUQiFRWRmmMs46ay/zfd/iTGZpRilrr0fwkYKBwhjjefzxzz52JI77PcKYalSeZ3mS7sSYtmCemyJvy6gFaMDs6Qu93+/3O8mWbF8CDWABDlBg9KoKMACA5Z3eZrXEbipECElkSzEnhBLdzp5edn+3zrN1+zYz3aZou5hG0MJUt265A3m03dhtercVom1PtxC2pLuICM7F3nDSzXMGu9ejnSyzan3y4uT04iJ62ktlnkkEbDb1pno86M/39g5GjEue9PO0JyPn0RNfaxsD4Uz4ENZlvamaWuddm3AquikrJDdeUkYmgy6nrKzXtTJKGwICShgT2vjZ1XrTGFA+HkZKSJcyygID9cFzinatAYmIV2fPZrePuv2OBDzQNJYwTghyQQDYuBuOE7Qb1tzuxqPbdAytTDIJEITucjICQrf15va+JCAUMYBG3yo+q+htsNa1feuImCbJar0GEGNs0e4xbjHyWZYREOed856gTYSZ1c3nXzxb1NVkf1LWZaD4nffev390C1u09K782Ea7ltGJGAlzcX88/PzJE/rgbrLlM/df2UATgQ2wAlJAAg7IASRCrm86rQAlJGnH2wSEEGu9sX4H5Nkiadt2GbZVQOtVZFu/oUUPEbJt9hAg3oDKt97WDvBijATBxxbM6MOWmppnxWS81+nk3U5BOKmr9Xw1X69N2rmd58OOjNKXVi+q2szLsqqVlOlwMJZJkmVFmmYMhiZEe6opFYyD0FKp1aaumo42WZaxIuGdlLMkEQlNpAghGOe989b4tsNMKC8XpVpUwXjKmBZESZGljnMOBu8cDVa3DE2ANJvl+uLxs8fPADCgk2iqZydf/GhdOwCCGO6XenH61cd/04Z8Zte2vJyffrVZlwC8Xvvquro+OX/68UvpbkJe/gH5lW83ZaVqpSodQ3TB8x0RKE0SwbfBzDobtkrS22cRQihFCG3+xATjnPIQY8GTpqoGRfGd9z68c3i4bUO9bCVsXWcXXkADKajMusV8NosxAg1Qvx66CNAF+kAHkMA1cOUXj+fz613JuX1UKvnWpwh1Pmhjd/iPVjmhzQm3Ua2NsnEXsOLOpXcl2bYL0p6u2B2pdDuDQnAuhBC8a9MDSsmwPxqPx0W3l2YJYrAm9IrR/buPjo4eic505fPztZkvV8Eqp9V8sZov57opabTdXrcYTCNPCUsoo+0RRAmz1peN2VRaaRNiTBlyyaIzJJLL+XJTKeeCdaHR2vsQEa2j5by0SvaSg14+qTexaYyxLYIkeh+4dQ5UtB983ehAJLtR3aadrNsh9NzaVoZEMinzXuJenNmAhIKIXip62px7awGIpCcSJEm1XsxaVDJuDoWbFG3XqgWAgLquy2XNPPEsIEQqKSUkgnLGOnlXW+t9dN5772IUIQb4yBiLMfoQGKUA4YxKIZPAWJq99dbt6f5enqW9Tqdlj8Wd0u/uyMS2J0EQA+JG94b5erk4vb76IFi4JXxAkgBh8fzF8PY9oMD1EwiG/hHAgTtYfe4qHbZLk8g27SJo87MtRT1ErV1oJQtwE41epf/uHvvydNy2DEHI7tRoX5uQdu4EQiklMXrvnDXBGedd21FjjE9Gk8l4nKU5lSzjeZqOCOAae7GqzaoqrakshE9Y1Jyxq8X8sy9Mzvm9O1HK7njv8DIYB4SordOIkVDqPW2M3zS2bEy3E1PBB5nYaNfeLNo5KTnXzBjvg+eRM8plJsbDQb93EIwO8zPrnHfe+9jOGTmjNGzbflhvSq1Mkb8muhHCboDSfhsJZfxV/bwQW8jTzbegjIMItNBk4JVq4OZpLSiOqEbpWuc0dVvQHGsTdkZZmiSJTMt640PQ1qZpTrCDOCEKLgINznrGOefsaLT/7rfeOZxO0iyL27FN3DXWd8GMbIf3iAQxeBOEqRhLf/nFZ9P9iQ+ACSCw86sQ43DUh2+wPHPLFd+fAC3VFKAsKTp0RoLfnoFtGy2R/OZojpE02uwKyBb6FhBJK3QQtifo7snb1GzbcIm7oLeNeIg+gvgASknwMUbvfLDaWaONiwiU0jwrjm/dOTw4ZpNhS+UmBqgNM7aQrkeqIG3S63FacFeF+Vm2qa+urn6GqCw/uP0o7477ulpulpRS65wP28mHsXFT67Ixxvoi54NOqj3WFkrDeutdCDFSutXG4owXg2R8mHez3umXpzSGGFtyf5t2Ev71j77xs198bJ0jIFqb0XjYHb0mIzjd30+zl7W9FLTf77/aZOtkiY4vqzMuhJQSLEHUL/nLWw8ju2ohglB4V24qo12eBuc9wY6WG9vUkudZWtWV914b7ZwVQlDCXHDee8lFCNF5L9OUgLz/4TuD0cC5GLy/4RTtysFd+rkrVdoAE0rVTcKi3BhvihRqc2nXPZF0jEEx3QsvTun+vltWkTAkcutkWITzUzrap6Au+lf1RqRkbW+5JU4p7XY/u/GnXc257XK09+C2xozYuWLEyxM5xkhobFWnHBwlDPDOBGuNtca6EJHK9NHbH/zWh98obu9tyxUHeCAEwkW36NBIe12lreeMERKK7iBJO9nF6Wx+/fGzE51M79250xsd+GBr2wjBw+728d5XjVmXjTK2yJNeyrno9T2hV7HWduVU+z+0zksZ28ZRU9Xu+syT6I0lbItFa0MNf+vRR598/qX3HoQYY7PBQZG+JoXXH7+2XB1E3rp979V/EPng9XpMTo/fBizcBjHsPk3yOm2dAMQ26vzswhrnRev6sXWzLVaZxVSmWZpp01hnXfAEcN6G4AFY76wJlDFK4EOgQK/XCz5S2gaONjPb9jW2l7NtBLTX2ZKh5J1ufqbiaDgMwRAqlvNVUZBibx+nl+vrxUDm/MEdgL9UIzTq6bOv7suUtQdiuMFNRsEZJcSFbc+ibkyIYNveBQEiQjvR3+aLLcAgbNUQXvW81u8iCAkgrVBDK9LRUqMQgnNGaaut40y8+/DD3//+H7717nsva+Jt7ixAKGOyJ9KO88aZEAKAJC36w/He9Pizx58+Oz09uTjtj/f7eU6oiL5dDtVus4g+BOdcpUzV6F6RC4FeJnKWEsRFqV0IjTJSiJaEHACr4vnT8/2u796erjJpYYHtfRNj5GmWyyRRjaI0GGtXq00//0chPgkQiuhf8bNdvdlWqN7+/BefnD57gp4MRgAAIABJREFU7px3zvq4HefHGNquNAERnKVJGqOPMWpjYhERg2ASFM6GEEOeyDZbtjYAIC3UIZCIEHw74wy7nCi2EjytKh1VGI+7mtpg9Giyv1xc+Zh7Q2pS4/l5nhdgBNPpThxvdw3lZLZYHlerTOaV0dhKdVAgcM4YA+yWmdQo69vDrk3md/n/rtAlN12PGF/WmHgZ/Vo4y84jCQUFAyExkOitcbUyzof9ydH3v/17H339Wy/r47bmb98uBDgbYwCBTDJKSACSDJ1ur9MdgLJ1WW3mL67OR2xvHCLxzlnjdkp/JATnI6zzVWMbYyijPLLITZ6mXMha2arRIXhtXJFHwnjwcMqTPvUhbCmF8eZyE8o4T5K0bRk4H9arFV63iH9fexn/yeshjQBEb6pf/vwXZVn7YENE8IFQ7HSVWmEJSgiVggsupBAEYJQLkRDKYqQhIktTwUV8mT3HlvgSYgghRpCtgk9EiHHXAYgeMfjIgkPKAxFCyIOjA+/dej4rhh3CkRQStw8GX7sHFEACFK8szBImCG3M/mBCQNqGVysCxBgTjN5kso223vlWdm3HDo9hV0m2lWe4ycGwuyjbTJLedGe381AQRhnjjMborFXaKOMI4e89+vDhg0co2Na3AmC3hyZIBKXYaq+ElrRNRcqyXBb9/mT/3r2HD956yFxdXj2JaplnSZEXADHG+BAJovXeu9CYUDWqqo113jhXNbppNCO038lGvcK6YLQNIFwmAIsg3lo1X6p1hZdYRwICzjjP8y5wTiglLqzWS79rhrUfmd+pXMZXOtWvfsUuTL3WpwV2ykLtF3aDvQEAhCRJ7t65vZgvv3p2ejKfSZGAxIv1+paPe70+owwElFDGOKU0xsAYa2GILWBMSCEY3RW0kXEO3LSndr9doNvIvQ0RBPSGbhLAhVVOJgnJO4iSSvKXP/h5kqZ/+J/+KTB8iZl7zXSSD4IDKAQXzoQ2b6eglBIhGKJriw+lnfORi22lu0vjsJ1l4qYaaG+RGF9+eDtMZtteRqtRHAmhiIghGG1byYLp9Pbb9x4knNrrpeAMeY7oQ7lyVjNCCBeEUOe8945TxikBleAMHGAAp105eev+O+enz7xewumkm6VZTinzzntvt7wOIPjYaKuMNcZlXEgho4cxhiJ289RYZ6wDIJOU8MQ615Qbv166pmKtwPmuR8MPhuneqPf0SaSEOgJVbdjOR1p7qbX3ysn3K19/vVG++zF7pdi8aWORBw8eCJnuTw//j//rr0/Ol4Qxpepny0+PB+P3bh0XaU4oFYwxxtqS1jolZbYFlBGE6FvFvHhDfNhNeLZgL4pdMCG77TLtKQfrHCLV3gcPGDcYDc9ns4vL2dc/eAfBgQIvR5H05YgzbFgiQwCil1w0WkUAhMQIRomU7QiEgRBjvXU+jQK7A2TXwKBbeUaQXZG5KxZwMwzbQTzaepmy6LdrAkPwxmilbJb3P3jv/dvTEXFrUy1ZXoTF1eXscjGbM07yrFsM+pTIWilvdAghTfJed5QP9kATyG1jfTo9PLp19/mXP3JeR0AIKdoxZYigIUYaQwzRW+edh3PRe89F5JRo6xlBkaabWnsf2nMnHw5OrFvXJSKiZEkiGKetKA4IOCH0T/7kw7/52/8nkkgJvX/wj7gjrA9sdn51ow0bgRjq8t/93z+smub48OjrH+1dzVbL8hdC5t2ea+rqrFzPPvvkvcOjg8GYMiaECMESSrTVlDLORABIaCUBovNBcE453V0Wsmt3bqMYBQLdrpxpewyg0MbCR+N9r+hgfHgcnUUcXK244Gg0XpvxtvvCJ0ACpYlg2gUQyumrESgSQlPJ22SMEBqcF953SDSA2WI+t6FsF9l2Z+U2P8OuW7Z9yZ1zEhAwxhjhNDrjg1JGaXfr8OjB7cN+TgTWnHCj7PnV1ZPnzxbrDaO06PTuknvD0YhLgKFalueXzxORjceHh4d3xd4ECeAhuvn+9Oji+SfeaLIlCCa0vYd9CF4Hn4TAnQ8uIFDmA4GxOsI6TwjLkySTaeNcC1A/mA437xwQ7wljvUR2enmaZ0kiGGXO87aSOqSURg9KqXX/iOtOaOtUu1B4EyL9ixcno8GwyDtpmhhVEcIY45yLSKQQaa83NE5/tlg+n89vj4eJEJKSiOiDN9bESDhnlNIIYq1rtcUY30rqYztJ3eb+cTcQCO1ZuT1HqYuhdcciEwBZK3e5UJ1OoRo1v16MijuvKN4fAdW2j12uWCIabXcZLgDCCKGghIVhJgtGVSQC5Bsd8V1pwTQCfRLFErvuStwy6XZH6E7UZQsFegmdi7vfgoJSJhkQbHTW1Uo7Fyej8aCXV5vZSpeUkGWlz66XJkYieVnXtsStaDgPgKOU9gaFMury7Ozq+mw2u3j07jfye4dgQIHRaNzpjdoTmTIuOWeMCkocSLtrlQvufGyUsYEULOGCM86C9soY530MnhISAwgjWZFNb020sZIzISWjjEvBOaMglJLtpykFa4KnlF1crR/94zma9y6GyNvcFrv2N2Iu5f6dwfX1TAh5uD8qip+3C5IZ5VImMbrYxCzPy83mR8+fJpwVqewlWTdNu0nWLWLBikiI8x6ILSWdMt6Sy+POt2LY+jjiFjoTtgQPAEGVdX16FVPW1qTn59c8yfbyzCjlQwAM8OoenW18cwGU86ZS8LtmMDDNs8loBGM+8P4PB4Mfn8yeXNr/eMKAGusVaHY3HW4g/MvBF3AT3uJNZw83M4C2jbybohBQIhhDK0NgdF0p60OapFzIxfL6yZPPiQ0EUmT9/ek4yYUPXjcqeqtMFZwLkWZZ3h10y9Vqs1yenHzhvXkP3ykeHIKh2xskWceExjoXIyWMUcKE4DwSRwlnjFIeIqnqpqxUr9tP0yLp5KnztXHWOblRfEvyIFykUnJCkSapELJtqe/k9nZ+VmSJMirGcHFd/uO5Ga7nqwgyCDxJHGFse6+GMJnuIeKWlIRwkKi0bb2QEAZCfWCcZ2nKpMyaJl+tZsrH6LHY6LisMrEYZEWRJJILyVgmfY9mNvi6NkD0Hjaw4BFerpuMJIZdKIuUkOCcbZp8MqpV452mcHujzsP7PVIU85OL0cEEkK/42XrXpMX55XxTa+E8nKtqsy4bRshk0MPhAZxBgv473T84vf6Dn1jUK6xKRAtJCA+ebhVc0KqVtqiRmyoGLQUvxsjjTsGqrUVJiwSPgQTvrFW1KqsmREooNzauNM6u6oELd8edfpoLygVPokCFUC0XMdjxeEA5NdZa64KPaZoarZ48+7JW9tv8j9K746TtatU1CGGcE8KNc9YFSiKjZIt2EMSFoLUJYCLJJGMhRCd4mmajkWuJXwRgXFDGWIiMccrYDjC8LR+3ftbrZbNl4z05OV/+n//b/9LpFt5641wieNU0lFDrvPcBBFrrVHDGaZ7Jfq+jmuboYOKDM8b1u51np1eJlHWjlbHzRXW9qASnQiajYb+uVZom3vsQwtcf3bn9zkPiHVyAM0ob2iogEoIYvVNaa2uV81YrdXx0cHFxTRkvii5lzDu7Dn7TWCbAeQhlPXRF7/l1PFlIwUALKnqn51cEXmnXKkkxhpvchwAM/m7qlfWTe/fQLDB/VnBdLp7LMikEQWKA8pVK+mZNh/3Xf/lxWTYf3p4gLb548vHPH78QFPsqvnXrCISirLHXw9EYF5Nf/Gj2QT/FIEPgKpLQhldERHhyIyJ7w5dHBPGezDa8aqy1Ztv/2xWiRUJzFoSrFstNWSkpu4kQ1jkQeTy9N1b1mBG6mvtyrhOOhAPe1rrc1EmA8jA+GuNCjIQKLhlzOL8++eSTH3/U/yPEyIVgjFImGBMRxBhnnacEghFGaYjB+QjKfCSEScoTpWql9EYZ5Uk7mAqgkVKldbnphghuCN0iaWNLVm2U3/rZZNB7/Oya86TRNkb4kJW6VppzYk8u1nleLJYb7z3nvKkW33z/btmoh/emd+7funhxOr3/28AK2ACTr56e5L3e4ycn64356sXFZNQn3nMa377/tS+/evL2W3evr68IoUmaAhxWA1FV9XyxpjsNxapaNaoKwTPGBZd//Gff/73vfue/+Rf/7WpZpUngPBdceu+ByJlI8lwwlhfpdL93cTWfDMaLTQgRup6N+t2ry/O98VAwOh52Imi34ACnFIJRvV5VjUk7PTQbIJH9jjBNiIG16GLUgAYs0AHaY1RCL3tF1k3Fdz76EPu3331wvaw3JCAIClNv/YydY7SP0fSiOH+bxCTvwnPORS6KLO90i16e5UBYbZbXy+u6qRAQ6bbB4T3K2hrTWLXuFplB7GRCa2Os7cmCw1MfCUR/eHgwvff22+8dT6fvRgLTuMuzq8efLE+f2XrTVqmRUhbgZsury0VjXEiE7PVEkjKZOElommnbvDh7uv/ki9F4ChBrbQQo5TFS5wIIbbt9rVCvda5RRucOlIdINmVZleW61o0nm9quG13bOBn3vY9K6VSSxQbTobxamL2hnG9cN6dam62fHewPESPh1HtEkNOZanRAJGXVGMOyTpIX4cHxuFaGhM7X3n/ri6endx7eAe1MD9u6gQMZsFlXXqTmy+fL73z9QaX0dH/v+vKkxRQQyjrd7vnlxXg4JIQBET6Aoqya1WoFwgAwxrKik2UdpZUx+p98/5v/1X/xn0VCf+db3/pX/+ovlNZJUjApAbtT4CSEcgLqQ8izBDEWRVoqNNqFSBkTRZ4xSjtFZj3Nc+4dGGMhOiazq6uT8epYK5ekCfKU5BlzDvBgXUAC41cKFwCYzxZMiE4mOpJBzx58cP/0+kIbwzhD1JApuhlsAygcT/7wdx6S6gQFgRzxw4/efW1/KNLp7SmAZvnLj3+6qTY38CHBxdHe+GDU2z+6XRQZ/7t74hTAfhV2ye+MD/vo9Mn87FSva6dtcIF7H7QJ642IsITa2Yp0O7HfQ9GVeZbkg9VyuVzO8rwDQnwIAKWMt1KzjHDvrffbOpgSEMIoT3wMTVOpunHBee8SIbVgzJAuF3ujHii11Xkn1cbKvX5sGjrsBOfRyyILu3Pz1sE4Agje+ai1IaTTLTKlnRS8kyYP7oyjMx8+On787GLcG46OJ+PVEnQfMMjaNV0zIK+urlaVs2GzN+y+dW+6WC3TonN5FhmjPgTKOGfc2jAa9gd5CqW88zH6TdUY4yIioYQxgUBMsJzJb3//g//6v/xnebd7PZu//+47/+bf/qVuKp1mQiSMM2e340tKSYhENUoK0egm73RXVfAhxIiWf8EZl4L5gBBiuyOgbhpv4+nipPuTv5ncul2qSi1NlmVFtwvOALNbyvTaQqqrqzliPOhKW16JJoHzQPAhCsEgOQqJvSFmV2jW4B1yewoxBK0guij+HrpiNnjvW7+/OX3y5dMvlNHD7vB73/oe6/+mjiR+7U5KYXF71C3e7t4eYVOaqrGN0cYZY51yTaM2a9WUSl9f68Wadnt0PE4Ox0Unp8QboxGiTAQXghAWEb0LQlLBeCQxRBJi5JTlRU4ZWy4WpowIuiXHA5CcZpJzkXLGeSJABCWm3dVCGQ0BkjPrAxe7OmBwNIkxBu+c9U3TdEf0wd3pbLFZrcLRtJ+nst/pF+PxZLM+vDMC8smos8OXUgCLk+vh5ODjL86cp1WjP3zncG9/cP/23vWGaOvaUXeepiAsxBh18/zFV0nRyYouF+Lq+rqqFGEJY4zSNvclv/u7H/3zf/pn2XBQLlbr9Uom5Ou/9eiv/urHTVNmaS5lGrwDsJ2ME2jl8lG6KXVfiBhdN0+EZHkmBWeJlJQzagMijLWciUaZbqdnanoxvxoO+5GIwcGgLssXTx/vTQ+TPN0ORl+aA8JyXVJKF6Va1avcTOYrZ1ywzhvvt3WiYEg70Aqra0iJyR6yIbjYrn151aKG0Ug6AO0e3ftovH/+7KuD+w/Bb5xsjRBB+/hNZoEKsYbV4BajAoMUMUjnpXWF9zAWSmNTN/PN7Hp1fbmslrVZr4ILisIV0nVdWataG9ou547ROWesFoKlSRoZGBPWeUqJ0tq7mVWbYSfNM5EkKSN0u6klROdt2ZgeJz5uu5YxREajC5RROA9B465LRMYE0QcXfCirejRxbz3Yl0/DoEPeOh6vymp4OAaKYT8FnQKhP20/ggZwQPXsdMFE/6e/PP3w0Z3VZvnowSHS7MG9AzzbaOs5Z0rpbrcTY4zO//Vf/K8Xn38cuexO9vdu3X56MbcuJByMcR+i8+GDd27/5//sP5KDAZStG7VcLc8uzt9//+Ff//VPtKqNaZIkJYS2q8BD9M66TdVMp0OlTUtl63UySkmRp5xRzlkL3PY+lLUqMlorc7gn8+O9+dXVi029N540jend+1py/tns6vKoSJFkEPGmzAQ4oIWQdaMbxGc/fPq1ddx4IaVsGrMsFcoGLEIZBI/IoCyWC9QbdIcoOmANNOACjIZqUNe2abQxhJDi7vt4610k+cHDD3bvtQHOgUvoHNn9XUz1QAAC4AELWESHYBEsokeMoB48gnJw1g6y4ANCgFLoptmgON7vD/e7ZyfXs4uV1qaZzRuT65H3tSkbnVLng3fBaK2dd9FbLoo0y9JUeuecMevlPEZvO0VCe4J1uJBtw9l6V9Y6MuNo2ukkPm71lEIknMEHMEa0IYl82Y0sGKXOhxh9XTckGpDeoDebjoasO+7BAmOApMPOdrka7QJAOQNPwMzVXKX5uqzVw/t7X35Vy/EUYHww7i+sdZ5SWpbl0eERSOzn2eeffdzUjXbV7Hr++c9/fqY4oZIQRtDKXoajo4ns9WBdWZaL5bxczxulD+7e6vaK1aqsynWSFoSyYM1WGT9GbSyjxFrvfAghdIrUB1JkCVrRhRibxiKNdW0El5tScRISLjrd7mh/rzvotdjK5ODeKMbNfNHdFyAE/GYaC4BIzqtGS85P5jq9KA/3xzHEsmpOSvPes4tsIOEsXIRI0FI3lYG/wOIKypelMjGAUOecMtY5RwmVkumvfjKql/jwt3eF/wlQAktAwwSQ5zsue1sq33Ta4o4sFYEd9T4EgMF7UIYQQIAYECyiA40okoKP7kguM3l+siqNkayjtVmreVmVLPPKKG1NWZUheG2MdybhRZYITaKyHsED0KbRStgskSGEQONuVGxdsMah5cpHQkkIEZwz50KawAcQQl5CZ5NEaKsRUSvNYAB0ehJ8BGS8m+8+8TYFXbVouifPrwaDYaPUfG3I2ezhnfHoaLxeXQETYAVwbUwIoIRsyjJJk+jd3qATW1xoCM6HVaM2OiOCEEq99yEaQogPEc4542bz2fz6TEiaJEmayIPpZL2plG5UU2V5D0BAIJH4EOvaAMS17JSIbiobHaVswWjRBxhjGSPauLrWStt2OzFjmQ9BaZUIzlACMp1M+HKx+2VrIAfmQB+Qg2HP++AQhOSMUOcc5UxZN1vVf/Xp2cNpZ5IhSyTxHvCgFImA0/X17PR6vax0ACGUuN0iKclYtyOdt/Qag+UeBsfbmr2Z4/w5Vgp7hzABPmxVXXYkZ1AGSkEJGN2plkQEYDvhoC/RDS5AaWgNG+ADImS/f1ukBnJ+trTRL+YXi9I1zbKQfWtc2ZiqrtoZsdHaecNJkhWJ5kEbG4PnlLkQgnfO+RbGSQHBhXPWWhdj5FyESBglIRLOotLgjLQDj5d+1i3SdakJQdNo0u5442KXWGxBFtAKiQ3ra5oVIKdPTmaTBicXM85Yo9QHbx8A+XTc34V6vy43bX+0aRRj9Prqcvnki9g25mPUztbKOUS23VYUKN1yS53Ws/ny8uqsKpejvb0sTUPE4dH+Z58/jTFU1VomGaWsBf5wQurahuB9K8rlkXSE9a5d6eR8DMqEiLoxxjibBMnZ9Uo/28x/+bMn2v5ov1cEgTuHx8cHt0ladTvy7l2aTm/txv/d9tfv9QrvwUjIMwkCb73yri6b0vovVs4l/ijIkQ8JqlREFiKriVLq5HJxcrWpbWRCQHDKBcAQnPQ2bGz0bjzeQ7dVH6+wXuPZ6Y9++tj78K1HnPRzxAjr4cMWGEk5hIAQkBys9TYCAD6g3ZsZ48sHg8JHOA/rYS18BE1JlsluV10sF8uFC+tSWSGYj33rg1bKOJsmWSIpocwYa33oFtmwm7U7XwhFKgVjglEaI1M2RCBP847klXYUrMgzamWaSIB3E9In8dZQ9gQDqV762bCfn14sCUHVuCcnq98FEA0IgEotynQ4Ba42a9Udz754erE/2ZvPFy/OlvO1e/Ji9sffe2+5Xt9/6xAQ2f4IAPwcLL+6WhBCrXcuRErZky+/Kh9/4nwMEc5H40IkhBFO6Ha/kDZGCHn+7OmPf/iDwHlZLupGxfkqTRNr7PRgGmMghGrdaFWnedFuiQOIMd5YRwlV2oQgtno8IWjjQZg12jpmTWNccNYlkteNna3Vx48vvXdH9+9/OX/8k09f/M69u3/75Q/K5Sf9/c63v/m1j77x3kdf+5D2x22i1naqiWR5KmMEoaRpGqUtYuSJXFgsL2ruVebVw/180pHemdm8vNhYJQraTXmWMpkQwQkQvSNaqaak2hdFDpa0tyUWpb5ebxbl06u1Mrh3NM4TSeG9j1lvLz9+G0kBAkQPp6ArmBLUIAZ4h+DhLGz79wDGkCagDBFwBkoH4yP3mqQrG43MJc+6SWePCcow7A/TLBkw9tvf/Gb18AGiS1OZ551Otxh2u90iydPE+UAZzdKMMRKjdx4hEsJFJNIG2yh3dLhXKWOqOUA5iUNJWNDoWkSKsn7pZ5NhDzgFgXX+/LoGqvK67Ow1dn15OdvcGVYXz6+1Dk2jnp4stKE///TJ9aLOFCZ9ef/O3uMnDdIxQNrUdXE2H+6Jn336gnHurIuUeOfM8nr+4pl1znpvQ/AhDroDY4RtRYkRGeNJIuvV6s//+/9ODofjo4P+5FCvNvt748aYfq83Pdg7PTnnXNbVWiQJidQHz2OMgDZOCtZoGwKLAT54IFS1AqFV2bgglFKMCgBZKghBNCGhMgT1ZD2/akqR5Pt5/uH07plIvjj9yQt6+ed//jf54HiyR7/79e/xnDZOtyVFkgogWOfrWnvvKONCsBixLNVqs6nW1elc3Z+kHRZUIHG4n0pJZcIYA22l5iJBDGmKJElIwGi4XSWuPCq1Wda60WVpZqY/FHcXuvZqORlNxt/5D/AajCQi1LANTI3FeVzOoq19Y5yunfc+BMlZnltkGWKA0rpqahuRSFcUfNS7kw85k/1ur1t02xpfiEQm6fvvvNWoJk1EfzJGmoJzsH/AJuAE+PUSelPz8lUO9gaRMAKPFn2qr2dL1Rmtv3hyUTZhbzL76vmcczGfz5+dzMsqPH52/fD+AQHu3Rr39nvjZQ70gE1bHJ1fb7jonl9v7h0fWOfSLNVaFUXRMmqc88pY5YLJOxu1aEX9ZZILIWMkpXJWqVA381V9cDu9nC3E0XS9KfM8++1v/da/bZr5YmOsaqoyyzvBtwucmdJGSlHWCjQJMShtEU1Za8b4umykZMq4US8HQppKIDplMsrvTe5/+96jf/1VfVKerDafr/SmdO5bx++R/GB/EPvDd19c/OCnP/xi4Vb33j4UWYIYpOQxQilVVo3gvG3kERJDCGWlVsqvVP104XrC7e337x/10dJNt96xRSuBMZJ3BoMuDvYBCZRYruP51dnVvGlMwliv2zm6dT/SOL846R1MXncyAAS0QFIgAboTkp8T1+jL84vTp0GZGCxHzIzrN4YhVo1Za9sgSYq8O9g74OkUhFJCCc+zgmcZshSBIU8A9JRGKn8zsPAfbvKlnx0dTAjQ7ozxwZ2eLBYbk54ufvnFOeEFY6dPTpaJ5CdnV95azuq3jkffeP/O2eX8/YeHIMl0r+0CrAEGXF1eNyBzxvho2DVqLQVrGrUlbYP4AONcY8Ps7LkLEYRF0EabGEOW5uA2o+y7f/xH840KIThn2wNx2O/vTSe//0+++z/9z3/hnK/rNRdSShlCsAabjer1snKmk8Jp7ZQ2wZu60YmUZaVHScEpy1IRArKUG42rVckJeb66SM6KEEJCxZBb5OLz0ydGZYmXb+8ds2K/IG/9yaNv/+9f/HBZlgd5wrngjDgPrazzPs/TTaNaKbLgw6ZuYqQ+kKXxjXai63yMaPXN6Y7sFNvlNURwdjTdhxgAAWqFk5NPn56eXi98iIzGxfnTxcWt6eGt4WCYpr+2P3tjOSZHgMzG+wVkub42VRkQdAizdU2CD4RaWgSReMK6JA56OUkzUAYfYB3gIRnojrGWMngN9pvf8R9sL/2sszdoc/YYo9bmycnMhGy5uXp6ukzzsFytnIfkmI7yw72D1Xpz73h4+9Y4elNMJ0AiRyMAbrXgxWB5cT1b6bK5fnA86nY7c11Kwc5PTsz8glLaIvuMC9oFSnmLyTJGddN8vV6tlrPBtFfcviWKThGo96YVzTPGMs6ssYe3Dvf29q4urxqlCFkwRgNIJy+eP1+8/16ureM+lJWy1iutlbJN6nwIglEvWCKZ8xCMqeAWq0Vlq5yRf/P0b/7g3tcbXx/2x7nIXIibUEdzela6B713Xpjy3z39BSXRassYGCMxEmsNiST4KHLKNAsxeO2dD0pZLrcXLALa2BBu9Fp3UIwtlBuTTldM94AEWOD5yfMvn764vDYuEEIZZVmWeKOcUSG68BpI6e8zCrG39x7dm19ZY7hgWpnzi4tys0jTvJOmaPE51BHmQTwQIRnSdMsnoBbBgwJGQSn0foPMivkNIjf/334GNsSOTmiN/vyry87o+PrqAgSTntiUm0d3DxgLnbT39Q8f/OBHv3j/4W3SKw5UBewBqn3vk7Pl4WH66Zdn1</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nGS7Sa8125YdNGax1oqIvfepvvMV993ylZnPmcYoEzuVlDZYSCBkOhbChgZCQhZYCDASQgYhoEWTBr8EOvSQDB3LSiynMCid7+Urbv1V55xdRcRaa85JY1+DLa/ebuwiYo+Yc8wxxqS/+pf/zVJKcOp1/cnHd3/pX/sLn372SRqHv/t//8n/8bf+1s2kn332aUnR1nUcyu12/OlPf+zWmRAeYG51bT0c9HiYn572bV1ub7bjOIR7eF9WG4fMTJo0Jd0MQxqH4/6IMHP0bgGosLl3CxVZ6rrMNQ9Tr+ehZDd7Oi7jUFQlAgRYBJGczosKVFMppbfFLIggwuHGxClpbV2EGGDitRkohEiEWjfr7ggVqmsLhFuE92YuTB6otXkQAHdXFWYW4XCUnIKYmciNmJm5mwFRq203uShXIwBEHOEEELA0Q4AYwsJC1lyzDDk368u8zrVnVRaehgz3tfk4JI+Yrq4FePf2besdkHHMRGxmAYR7baaqES5My9qTciDMopSkKfVWAZjFslZmVk3MFACBLDxrAkDkvYcIiMV6i/CUMgJLrdaNiHJOObGDmajWSiweYAKBQUDAzESV4BYR5gAiIojXZekuIsjCkhge5g5QhJ+Xpnkomoe6rJ+8uP5X//zvf/LZx2UYvnr79Hf+zh+kON/ffagaSTUnGVR/+P1PZTNK76CABcpG50Pp7Xhad2Ma803SFFaB0JT3h/P+uJ/XJqrbsQwlp2mHaZfXlpQporu32oNQl9XgjCiavEDgeRxzSkkppwxRZoQTogcwXr28br0tT8xc65qzBqikRIgIdwMJDyWttffuSfl6SGvtKWXAhkKn8xIAATmFiIowC0eEMC9rbbU3qwRmpmVeHVGUW7d1XbtZSjqUwkxAhJsI5yQg6sHruhJoHAuIidl7L0kDUBUPCFOSqK3X1omQcjYLolDm6fqGI/S0Z9GhFCJPKd/dXZnRvCwpJTOPCPPYH+ZpGlVoKJMqp9Q0JXjv5qrMLMq8tn61ycNSwDBz0dR7E4pmjDAmJkmJjAksen19O5T8+PhOmYehBFGYmVkuuTUD4fr6mpjm08xCEUTEQAA53ElSX1skLjm9/OSn337xD3pJgJuDmMMslLY5A27dg2b507/1p1rtz2/Gf/1f+XM/+PH3n47zw/70v/3vf/vxza//hd/9zU8+/d7pvLiRctlt0suX9yyCdW3zarWhVWb2QLibdRFRVRB3s+NpFU1ZZTMOSUiEPajVen56MuvCDKJ5Xoip1paSABGBoGhrDUSAPKJbEJMARIiwpJpLPh33y/lMTGadAkRY6qIk3Z2JhNFaN48kGEpiJnNDoLZKoJxVVBlISXNKrCzMzQAwEXq3YSxESJKGcdhuxqRyvZtu7u6EkBIhPAJm5u7KBMA8EIagcG/dmvWcdJkXIIgRgaW2uizL2kHk3ntvrfbW6lzr5ur5Z7//b+/fvd+//ZWm5O5rbfO8rmtd1rbWHmBQrGslUGutm09jEWZVkpTqupSsTGLuAINJCK1VMwdBhAlgQiCGYVRBq52Y1mVuRkPW3ltr1lsTJWGNCBFhgps5EG4AAd4bzBHhvbuH92ZEFHDrpimVrACOx0NrKzP17sQc5pJkM2Uzcwcx1rnKT378w/ur6V/6vd/+U7/1G4fT4lb/4O/9/W+/+tW/+Gd/+qPf+OHr90+Hw7nPgiU++fRut92S9/BLkwAT1dYNedxeKRvc56W59QAdT0c3lKEgaLvbjMPgABGFoxsQ3d1EOKXEBEmZiZJKzqmbHY+nACehbl6GIUBMUOVusSxVVZkREYkiAPcYVMFEIGEWVevOHKoZ4d083N29DHm3GVp3IiHybp5z7t1YSIkijEUBPs9LVlbVAJQlZTGHW2w3RTUJc4CEKIBScs55KFlEiSAiY9ZSiohEeOumIsoUAYAjOjMJs5l5BBEQ7oYh5c//+A/M1mVel2XtvS+1rUtd1tXdzRFAb52IkvIwlKRSsnqEioKQU9rsdr13BKz3ubaiQsy9O4u0bpIyHPOyVvNxKMLMLMxorXsQUbh7a0ZMhFiW2loX1TGnpXZzZ1Dvzf07skEBEdlMpbXuCDdzkJu7NwKYKRzMHICbMXOtFgERWWqTf/af+af//O/99u/9/u9a8Pl0+OWXX3391Ze//f37Tz777HCc3z08nOfTzdXwk994vtteASQcREwqXISYhKKt9du3D3/yxZvM5u7H88ogTdJbF6ZxKMTcWjsc53mp07QZSuq9gRggEC44UNWk6gFmKjntthtiYkSrrRQhot49ACHqjtZqUk0q4Z4TExMFmIKJRYiZhMnDa+sIpMQRsa7NHCrs4ee5Wu9hzuTh8IiUkuYxJyRmDyQlJgbBLcwNHqJKQDeUokysIgEW1WaGQEqq4OJwlZxySmkzFlFNOauklJOKlJKW6imlXAYmHsZhyLTsv1ByEREiFk5CBLRew2JttffuEdN4AbMkFXcQMwIebhbdoraWVNa1iTBFgIWJ3NzcS0qAz/O6riuzuEfrfRwHJjazpKqq7l5rZSZRiYje24U0h9uFeKmwgSm8m2sSD0ga1roKvHsQ0Lu5u0f4BbkRTNCUhMjDiWgchyGJ/Bt/8Z/79JNX759Ov/zV5+syf/HV1z96tfnxj39wOBxqq4fT4cWz8ep6aIYICGEYMyIgCeQgOcyRiyiHrYvmgVg//cmf2d28bKd34zSUpKLqgd57KWnIKpKubl9087qc3QEgqXigdRdGADklZlnWJWsaxzwMyYk54G4IEiV3iIDAOTETiYiKMnMu2d3i0tUcZmbdEUHMAoAQQbW13j0nJiBA0zS13kuRde2n8wmACAlzzrmZAQwAHkHoFiDAvbZYq4EiibTewmIYC0DvH/ezR85DgJm9Nw8Esbp7752ImFmFmIkCmiVn7d1yyiQ6lBygnFRViSWnlLJmVVU269b6eVnO87LUHu4ennKybiBqreUkvUfvTZhzSWGhmq+utr2bqNSlDkVTyszUuk3TOI7DaV4jWDgQNE2Dma9rdTBT5LI168uyioqHM3Ft1trigBAbkYfXZVFlZiYWYoL72i08wp0ILKQiACLAQkkU4LWb/Ad/5S++fffui89/db3Nh+P8089e/Nk/97vjNJQiKUkpfnez7Q3zsry63928uEVO0ARlBPd1teV4PC/mSKqb7fb+B78TXg4P3zLqMKhHnM8rECBmQsopQPO8WJuTiIfXtfZuvZuHXyaaMmybNSGkrB4IkPVGzCKsykTMTDlpa631vpnyWg3uqoIIQlyoHDFbt5zk+mazLuZwFQn4BV6imlTM3Hq/DJWtVnNHQC4fQdrNRS7FI8YitXYCiFCyhjshwMRAEEQYbhFgJkR0a2PJjgu5CHdngqp6RG9dRIlpGgdCICAiICJQTkIsmlIS9iAiyjnnpNNQLvOBCBDem4Hi/cNxXtd5Xs/Lcp7bvC4q2s1r6yWp+Xf00czMnYmDiJncjIgOh8Myt3HMjiglrWubl5VFkwqA83JmgjuYYN1YmBmqKkQsCEPrtbWgYEO0Zq0aROhyDQBrqrX37h5GBCEyDzNf5rM+v79C4KPvvXToq/vt7/35f/kXP/vjNr+/3o3d+lBymF5thh9//zalse5bUqftBFFEAyig1lf3GhzH/dP8x3+3dT/t35Gmy+1m4HxciWiaCtYGarW3sZRu1FoXoZSzuxOhR/fFa+3W+1DS+8ejCk/DkETc3QFlISZ3W9YuQuGxLC0n8QBRhAFM6AEiBoiJhedzdfdLX+AQEe5O4e7RhVmUhQUU41CS9W6IQEpifR1Kyint9wdRBUtKUBEW1LUnFU0Swe7eLTgA1d1WW+8RIOZuLkTBYb0DSCkRYV5aBBDmwad5FZAoE5EK5rlqSqoc7gCVJLUj5ayMtXlOkZJmz0y4/96P8Pw3vvyD/3X/+C4iRLh57S3m45lVk8q61lr7brdNScyMWM3DzFSZiQAoq05ovSchs8vzySKUshz2x+ZRpqSq89JyyqrUaqvN3YMZIEqc8kAMDiLJmM9L70xMYQYiBVs3B8QJQTW6KnOQRcj/9N//tVevXim1j17uNGlvrS57Zmhm87lgFJaShrX5u7dPFwaQEPAOs3cPi5u9+PFPzg8Pl+thdOstpcTA+Ty32rtZSTKWvK4tvA9DuWgq7i5MxDTPq5uDkFgi0FoLN2YJdwovWUSEmJQlwt0BkAghImc1dybqZuGIQDcHoMLuTkR3Lz4Zbl6082NOkktmETPPic368bgAiKDaexJmZesBomkztbaCOALL0i8CWG1+4c5M3M1BJMwRdPm6AMLhiMu0GyAEHN+pH8TEzGbGwtvtSCAmarV2dyKflwYi6wYEE6lKOJwoPNa6qqoHiClA4ZSSjJ/8NvhmjEOvZ1GdxlEkacq73ZhTAiEirK9rXfb707zMx+Ns7sywbj1CmQmkKgARUW1GImEOIjO3bofTXNfOwkmEGa27CPfuzBSBpNy7nc8VDAqPCGEBo1YnREpCwq2apJxSGcah945w82jdqP3yf9E8rmuF5MNh3u8fG+R03H/8ybPnLz5Ap/fffH04nXOSVm0ayjhtNs9u4d2XTjYbWD/74ds//MPDaS45BUEopZTMam8ehO+6hvXLGBIAE4mwpkQRJNxaZ6KLLkoAQBZdSFlYVb33IJBHDzCFeVjtacjWGwVSkiASZjcPol5bEITFwwWQPCACFL21cFtqL6WokDCOp3pBuVkwE8FB4hYBDw8RYUa3ENVe12a+rj0lUpEIEJN1eJgwMyOCRCTc+qVJIea5EkvJKSde1paShDuIUyqtVwKbGcEA8oikiZiS0rra2o0QpRRlOp5myQXhkgYGrattNhsi771Pm2FZ2sNh/vbN07fvn1qNn3z/RVK62Q1J3M0JFAg3n5clAAC99dq6hYskZdasJedhGJiprQ0U87yUoazLwsTEPE6j974/r3p5pEumCBbuZuvSiFlFIsIDIrKunYR32815Xt36dne1rCuih1nKKediSPKf/7W/3C3CcTrVabs5LOfzeYab5ivi3XI+vX7zbehmd/eCAbjlnNJ2B2un8/nd40EIfjhttlfhhoj5PLv7yw8/3O/3zEyc4DZOEwvXtSKimxMhAOvu4bV3hAuzsphbzqkMAwIRLkJvH445SRLp5mtdCRASCyeQMohZVRDERCRkvauIh7t5Lqq5aJ5UIvwi+0NZWIhZIgIIjyCSm7u7+TznnNydKFQvzzwThVl4eEoa7hGorasIC4fD3My8lCSqvdlFLavdlqWaGTNnFSJiESBYlInMaa1mFhFu5iISxDmXbr40EGiYBo5gYhL2CA/66s2hVTPKiHQ1TVfXz1knhlzdfhBc5kpk9aqkVy+fb8bpcG7n6sdzJQoRZhZVJaKkklLabaeSswojrPXqbnVty1rN3NwpglWudhMTiyoRLWtTEevVWjcPAmpv89wQMm0KE9UWeRjNelI51d5aXCr7ZQjozYi8ZC1Z5mV9fHzSh/36wfPhXCNnev32zbt3+9PxdDXl4/4hUL768ouJ62lvkbbFbJtJE2M9IiDEVu0YC88dDCLVMtykHGHH99/W5TwOI0UViePpPBQVEetgiTJsgGh1IaJB9GLniCp1Xte6ri3nJEytOcLdY9xcpTYPQ+69195VlCgiiJiImOC9Wy45NNxdRFlinttul60eezOiaK0FRJWWpalaaz0Q4bzZ6HI6i5IKM2vrMOu9+2bS1iLcmMk6NGmARAUgsyhDiWURIbCYGVFYjxWRRJFlM41uvZknVSDMSUDHuc+rMSyn1AxaxrVRBIkRB6uQ6VanG0l7q/Plukn5/mZ7Wm2zubm9fbb99LeA0PffTnefANji3fbueHi3mQbu2Hhw/ubz+Xx+/bAfhpS7hcaUMpUEIMDCvN1mFhnKEAQLRLelzoenfesVJKXkpfar3bbXutsM794/HU5tSJpUIwLEwpq4nuZ5qet2M45jOs/zWBIx7q5Kra6a5trJiRhJaByH03lJSUtKiRf5L/6z/+h6QynLXNv5tJxOR2t9revD8fDu9ZtnI01jIdi0ubu/TsJkZkJKkNpaTjoOWsbh5uNPDq9fB2cpu9fvTvdX5frZ/fk8J+XDsd6/euV1qd32xyXndPfis+nq5Xn/moiEL/w0iAiACA/D5MRwB2EaRmbqbVXhvH22nA4B0qQM7+YXrWKtnZgjAEJWZRYQIvx4OLqFR4Bwc30DuPtl+o7WTVhAXpsFPCl3i95tnZcy6LKsvTkxmXsSNXczJ6bvbDwG3FNKl8E+EO4w78tSASKWlBI4hYc59aBa/dxiWas7tRCj3Cx5um3dOm3y+LxcPd/cvBKYOc7HQ/MI8+YEGkw3745+/8Fnd7d3NO+jB13fgwQAMH395ZeRp3NLZXMT7k+H4/Fcn99dDTmNhaZhvL7Znue1rj1AAFq1QNzeXolIb31tlnK6v38OiqtpFKG6rrWuRDgcT717OJyRWMEhrCCYBQBhJgKxjNvpQp6nadNqZ0ar62Y7pZzg3nsz7+EOQFPRb14frks+1b7fn+bzubZ+OB5TQos+cbm9ffHweFxqvS+5MwhLIu69FaVpzAtF6/3hzWN+OrVu9fyW9SjeH08SsxPCg3NO0WpOaVnmLG51KS8+iMOBJImgZJ1rUyKLEAKD13Vm5ggPD1Ji0EVl7fYuwnGZ+cuQ1Lt1AuXkrfXamjCbOhMzS85ExAi7iI77wyEn7a3+QwvS6moqxAymcHMiAZyFrfs4lHVtRJxVLrJFFmndwCQMFnZHBGr33peUM5OPm62kdjzO1H2znebzjOAgitAONkgqhSlIRlZCul5OT7WuhNpUIgafH5nDwwlizSLCrO/XWBqhn3/1s5//0T+wLDyv9fW7fRm30zT+4Ic/2g7pm2+/ZfBc/f27h8enw/t37++28sHdMFyPu7vn8N77xSnr7hBWYT6e15JzVokBQ0m1zlnTOJbRvQ3dLCIuDkD03qgzDb7UPo5wD/PYjBPBj+f18ekBefPpx9+bT/sUWobiHqUIe1tOC7NeqoYKg3A+neW//ut/aZxkafM05d3V9XlZlX0zjWaelYj0/fsn6PZ4Pq3rYVdgnZp5UfEIMz/O59Npefni+nA4WQQhem3d+uk0p5RqNfeu7IfjcTNt7+5fKLnPh/N+D3IBejhfnKAIFXbEpUo5YhwHMLmDEAS4m1k0Myau60KgAGq3i+WXS2qtR0CVhem0dooQpaEUpmAmcyAYADELCwEXS3GcpmVtQhaUhLn3JiIWoaw9KNwjaK3tkntIyq07EVqHGTycWap5EomI5bywsvfeukkq7pdf2FMqZdqV6w9ah+jIFNHn7e0H45CLdlv3whSsPcbbV99PpRzOfm4I54h2s8nmFsA8L4fD09Nh3u8PT/vDmzdv3j+dHx+PZdpy+LocPv3o1YtnN+u6dLNS0vu3j9OUwrx2S0mTJgKJMjyASFlUUzez1lkoPCBp2mwuRavkUkpOKlmTKK3LUpuXkt6/39de19q3UxHynHg9H/q6GCKJhHfrlhMnVQ8zc6EgIhHpfZW/+Z/++ze3JU8iKaskm09JpRRxWARuN9PV1abyWHgdSj88zeel996TqggR07pa680scs7KwkS5KAsJwr2/fHHv0XdXQ6tG5N4bEG2d3ZYkRISkqsIRwUzhoXmDaBGRVIjYevT+HXcGwh3ugTAV0iRmLiwpZ3Nq3cbNVWsri9TaAJh7uJs5CzNLrS0iiOBuSTWIKSLc19oYXrKChJjCAwgiCMN6ZyICVCTnxIQIqPBmu+lu4ZTHqfWg8FKKO8bN1TRtNeeURtIU4FxGzbvrlx9utne9dxl2ZlbrenP/ir3fvvhEU6a0LeO02V6/+Oj7uVwtTfZP79jtepeuJgm3IfOu5KHg9np7Op5AQFuPx32JJfnyqy+/vX95/zu//89f3X90+/Ljj3/4pz784W/Hev7imze3N1djYUe6f/GhR02cPXBRg3vrHlSSbrZjYmnORLDeVTQn9QBTNItpKiC+2U2ECML1VJZ1jUuwQUhZcs6baYgITQnhRJySkog7ZeUAuXtv63mpenh8fX/3smx2ZV5a669e3L59eH9eKoVy9FJSGvKvf/G2recffPQsiZDQNGhSUmWQbDclKamoiJj7stb9/nSRkxD+5v1DSenx6TxkkZTCI+fSm/Xw42ndTQMQvZkIDyW1bnU5MLMI9SDp3c1EBH7BR3Q3AjOjtrCwoWQV7r331gC0ujBTXddu7ha991wUiPOyJr1MigyiIauZWWsipCq9925hFq3P4zR5Z2aiiAgvJVn37r7bbnMZ948PKQuxdKdSRotOQFJ16FL92Qe/MX30U0CxfHV482ZZaoZq1iSZymY+PITVN29fq+a7+/sPPv5s//C2Ledaa85aSt5cvdDtM6zrm2++KEmHaUu+BuUyFfMYp82V6jSkoZTZx+fPdnVdDo/v7m52n397yBLr09ty/QH+4bHhT7/r8vc/P/2ZzzyrffXtm2l3KyrbMY03d+fXv7p69tHx8c06H4NcNGM+GPFuLMR0OLUgBqhkmFlOCknXN4NZZxJWXWpHuLfe2M3a/oiU+DzXkjk8AkFAI0btQ9GhyLqySpP/8X/4D7HZoBu6SyJiEUYYhHk3DuM4nBabj4fr7WYchmk7bq/Gm6tdHgcaMokk0FjyMORccik5qXp4mHs4RwSit8YkLNx6lDKNn/4WLYdwb836d8Geiy9/aZ0iopfRP8AXEUiFAUQ4gcBUVIiRk67VQOTu7s4iEV5yiX/YZGttmsRLgCDBcWHxSrV2ZgahlBSBnFN4bLabaSzrsgLUrSf9zjkgZiIKsA53y/lgEcSJAudlsdYj3MGkm9u7l5tPfwcQgKC7tn+IsHFUBI9XL3JSTeLgDz/63kff/8H1i+/Z+Thudq1ZKttnn/xkuHrOZQKAWGGdONX5fDyfl4o83U7bl7evPmOZgsr11c2wvX71vY/Wtf7RL79Cmb738vm7908Pjw+3uysdHMhAf/f1n7z99vNI18MoedzUroe5sZa1U6JBp+tWffvqw824ax1r9XHabjdXzZ1Zd7tNa15bY9FcypD0fF5qszIO1j0P48sXd711AkQ4wASj8N7a+Ty33i7UhQLKINDFZa+ty3/7X/57UEF3MMMhYIDJaWnr/e3tpRdOJTnFaVlvbrZOTB65FDDBgwAighCYwQiLeVkv8YF1rWGuosHImkEB2PrwZl3mdW3hLsweDqAkTVl7925+sSg1JdXBrbfWzEKERKRWZyaCMXNKutZmzViZCa11QhCFO5gZQFLWpLE6DCI6DFJb762r0AVw7kEEFhFCSqmb1dpbazkrwN0i3EAAwlqry57Ckqr1LpqIk+YkkiVN293L7fVzGq//v3LCMO9rW59aX72vrGm4vpvuPkxjBhE4cdlAy7DbDLvtd+8A0Nd1nt+/fffm9RfHpWuedlc3Lz746Pr2Wb66s/PT9tWnefdsc/0MOm7Hcjo+3V1fb3e77TRup0HQHt+80VgVdUx2vSvRTzrsnMun3//RcnjHot/7ye/o9kbGm7R7Dr3CdO/n0+7+483VTb7/YJqmZa4gbs2urrY5MQLNrKRMzHXtOadlqfO8rOvqbkRUhuHl/e04ju6RlFSwzMs8r+6WcnKLiDDztTb1/YlHv4TZrMfFKyhZP7q/C4QbJslDTpP1XJQpn85LuR5RFCVj7fAaFgQCO0CcqBQlDEQ0lYwwYmnm8zonSTnruq5FhRL3bt1typpSJpHzXCmQUuqtiwjAvS0Acs5MtNSKQDXsijJk7eYehBAVD4SF9Q6VzKkuK10yFiwIEAmTM5M7cim11gi4N5BeosjWW07laX+w3nNK4zS4fRdzYb6EVFHJ3IM1gcjd5tNxbR6sKU8pKzHo5h69QhNOj9Ukj1f13RfXu2sdB4RgtwPtAKCuKDeAPX71ayfdbIZydYu2IgkABJ2OJwN9+Nlv7K5uVTWVSYShCmB68TEAe/ym91ZdRPXFi+/lrA5+PO0//uijzd33dvY+jiekkp9Nr+7u7p89fPv6cVlqa+sHn/yk94p6QN7hHznTzS22r757oenG2tO79zkLM3LZPT08gUCM6I7w3dWz3r4268xchs3Vdjqe5rU7rIfHBW2bCXVd12anwxFExJqSDkNWBODea0dE68bMw3aL+xcgxnxEXUEDRkZd0dp6OC5LYxGUAWNBLOidzAG/PMbmPZeMAIg4AUytuaHXtSaxz798S0S3V+NmGpOKJnKntbZoDRa5pAgHUa2mCUnVvQdwntslRMHw1i+5xdCx3H30g3Z8OLz/VoS2m3GprXVPysxS1xqEbrCLOYJuHebmjtV6TnJRenNOCMrDOIWdz5diCSZY2EWBbD0cIcxuvdbuILNQYeLorRMWgGv96nw6Ut7M87m2dljlN3/8ybPPvg++B/rj5384xq5cip1mP3x72B89cPfqOXSE97qcpVUhO59Ox6e3vZtoOR3269o2u+2zF99D66f94+Pbrz78wY9luhZRP57WZT3N/f37xwDP5/3nvT4/Hm+ut+5ItUEL2kl32w+zesd6fvrqzf7m5i4XIzvMj8fx2QdABxTbZxeM9Xe/fPvtr57dbOtyNjAQx/Np7T0x5zGbUzPsD485p2XxacinS059SPO8WnhK2i2IaBwGFtXeRESF94fzsqy1dvmv/sa/Izlz2q3zycychMebX//y67/3f/5MHMdz38+9v38Y0dGt1Saahu2IzQYeaB0AhJEyphFJpKQkBAs3zyWNwyCa52VWASGNg95sh1KSxSUwIyJUsjJxLiknDZCZAybE3W1Z6sWluaRTSilDFhVxNyBOD2/qfAYTExAuwq1bXGI9Kg/7elpMBEKuqjmJiCgzC7lHycXcIwjh3epFz3UPIGprTNzd3UmEL+s2RLi0+G5OOpTxKicit6ulmjsAACAASURBVLAF0cLWh/dvzqfDupxh67LMt9cvKU8Av3/7+v3DcUrQYUJf5vNce0dwKtu+nPs8i2YPyLgTLmZ9nDbPP/p4e3MnXr37MIyUpJ0eI3yeq4Uc9k9ff/mrw9Pj+fjevU5FJZogXr56mW4/kpHAUR/eCzGGDfJzGtjm89Wm7KZEKSFtUpbD6y+++OP/Z0yUhFD3iBNrbKdxnWdzI2Ack3sMiZMqSyLiZTm3Wi96+LMXHxwPJ1ItKq03d5/GvC7L43G+vb1KqQBUWw8gZ1Wm4/lMy+f/s0KshrV5qX1ew1j/wc9+/vR0vrneEPCbP/3ppG1IWjYDpgILEIMSQKgLsoIUuAQXCGFIFA+n1rxbm4ZSmyH86biQE1EbShai5nGeV/fYTBmgCMrlO/lqXRsziFiY52WhC0UCRFMEmCKptt57b0QM7xaRc/5u2Yh4XiroErANM1PRALn3krR3uwT01rXmnJe1qoio9N4B7q0RIRdp1ZIqKKxfshfImgIBgois1Xc3L6uTr+eIdTmdWYWB2m1t3J0cJOX65sWn95/8GMDDN1++f/eNSuluvdn17U0WeXp6eP32/Y9//KNlqWWYrq6u0maLf/x8/bP/q54e83TTnc7znJJewoYQ2YzJ6oJozDyM26fHhw8//kR2r/6Rd58BBgYgUB/qvObrLTAA/embr0vZDDdb9Lp//frqeqqHff7gNwEB4vzrv+PBdT23VsNWiiChVpsQzBozt9a7heapFPRa3T2ndLUdH54Ovdkwppzy4/4cQFGubS2b2w8+/v4f/eHfVjEiivBmHvO8DtP17ub61bPN+9dvQJSH8ep2Ws4HZkYZoQl1hTteXOM4Ywgw4XCGMHJBYYTidHYn1nTYH3s3Ye7N4AZmkcQi7oGI6bJvp7rWxuwEtFqBCDiREqHWBhCImJBT4pTn8+yI1mpKaRxyrY1ZL3LxvFQRYeaSZak9gnLJxtS60QUsoHEaT8eZ2FRVch5Zwi0iRPK8zBRBTNZcVEAEwMOFhYGltazCJBegHx6+Jsnbq7vT/qTKl9snzNtJ54rmqmWsy3L5w09zff7y48Pj25iPvRv7RlLe7K5uWsyrHQ9PCP/q8JjHLZOq8rNnd0gZwNV2R5vy+v3D22+/kfFmQCmllDKUIc2nw8vn9+nmJfyw/+qL3uanh/d3w4Q0AAowMAEVMECQN3p+wsGwCxjOx8ckjDYi315dr2DOtx/g8O7h9a8C3de5W7Pe3CIltFbZ2VrjkojTMAgzaavvH751yDAUN8NOg1I3ysO01LrMJ2a+RCKChnDg+pU7yd/8j/+qskgqQcJpCC0JkSRKScMwCBMYORVOeTnOdX+K3jUnjAW9IgJrhwDTCA90a4/H+Xja70/vHx7mWpuZgGozYspKCOScv0uaEi5lrHcjkLlbeG8WlyUL5ks+R1XGaWxmEZdAEZjZPDzg3ls3XEAB5JziUnZAl4jrMGQEkvClwrVm7t9lLtpSA0EIsEQ38x4RJSURSiLMbO6XFkxEm812HAePuJgQ5kHhxGjdInyznSK4tt5DtpuNm9Xl0Or5lz/7ea91OT3sHx+f3b/cXd8eDsfzeQbL8+fP1/V82O8//fSTJHHY7xn9+bP77bN7nx8pTwBy8vdv3p3O85TRKY1l2F7d3N5cJS2Hp8fzWs8P77/81S+msdTW2rzfysolIAAMCKAADDiQaLhFUbS2PD24+bjdSQQUKLdop69//Ys/+eUvkq6P7x+YIeQq4eGtVYAQ3qyXrEw4HpegIJLNVErOOUkEzPq6rPf3V+Nmpxyi8uz+3q0TydPj/tn9TXn22wNW+Zt//d/KQ56X/vbxlFSYYvvRR1QGdl7mNY+5u8Cid2c4mIdxxFhQFLWBHR7IA3LGunzz+ddv3j0yxeF0pnBVLHM385xzKRkgM9td3bh3BBGCCMSp9WbmQiBivaguzG622e6mu/ukvMxza72bq9A4DK1VN9fEvdswDPO8lpRS0ta7inqE9U7EKgyHI4pePG8gAvQddFTZAkLfqRtZ0zAmFSaWda0WCASDQeDLkTEPU06l28UyRK9ryozAhb6c58U9EL237uHWTFTysEkcx+Nh6djubodxePP6K2t1e3V9/9H3n99fodXx/sO7l9+7evYSbeU8XEAGADpun73qx/dPh/Nv/VO/e3Vzs5m2tS6nw1Pv9vLl8+PptK7zr7/48nRatrudWeTlINRRFLgCYG//aP/uqyEZUgEozk8IB6lokt0tljPS+Pjt13U9efS7mylrOZ5OHqGaAiR8ibFQVunmTLgM8sMwLGvt5iwJFMJRayNhb3Wz2wB4enhotQ3TMOaUhPKz+8M3v5D/7m/8uwb6+a+/efvtt9OYD+f69PbQjoenp8dvn5oZdtNwOp5abUEgorrWnDNKhgDVUCuEUBuar/Nc55VE3EKYmUnou6SNMIWHpNH60mq9rHQDUWvvrZYhM1O4gyAsw1BIRHP21pb5zESqqRslpUsjDoACLNRqS6oiAuKcVIRyLrlkd7++vqltBSLl3M0Y7gE3JyYmXOKNKSkCwtTcrTfRFA4QMxGCNcklPOZuFihlw9ubvhxh7m4sxIHWO4BuPdyzMhFyUmZ2R7NIqnkoRNx7LWIsOm2uSfT67qXmDMky/P+0jPOAf+Jsp3x7c5eu7tGXda1MvNld3d7ezqeDR+wPx6+/+koukUwR0jTdfQBRIIAjT1fD9adII5av0Cvl3Jc6n0+//NXnCTFOYz3tj6fTcb8vKcv47PkHHz+9f9fbeZ7nrMIcypxUIsyagUlEAEo519pbt6x8Oq/d+jQNbW3DZnr3bp+S3FxNr98+nc9nd+utvf7lz1tdFOFJ82evrvmDm9cPx198/v765pndjFYbtYX0irWwHFr12nwoKQixNjrOyAnzpXVaO6/uHk7DMJzOc13aOKTrzQ7eLTw8WmtKlFUvW5bMHO6t+4W/uwcBImIeomru67KGdRCpCNxXC7cOKtYWUs1JejfrPSc1j3VdAyTMqaS+ru5QofBqZip8of/C0pe1d+MAJ74sBhOQkq5rc3NiqWvr7tZ6GYqqgBgXJTkiUT/vX8v8uMkJ19uHr79hYSZiYzdrvQtDmXqQuzEJE7L4enqzHnFY7P7lR/vD6XT8WvLm+YuXr7/8E5UciO/96Df/SWz9Y2e8y+P65tc/f/3+IatEmDvlJCL+9u27u92YEq+14zQn1c8+eoHlEMdOSWAdecC0PP78T2arH3z4I1vmb77+cp7Xw37/s7X9uefP847xtqZh2AylxPzl51/kYdqvq/ssSgKZ11qU6LKqSJSSNsHd7fV8OgvRea7DMKg4sbY+P7x9x0nnmYgkJ1qblVKa0Ytn4+s3b+W/+U/+CqvmYXtc6jIvr9+9+/b14f7u+mqg/Wm+GtPVi928P89rBS4SZhcm3UwggOP/ZetNfnRLt/Su1b3vu/f+mmhOm83Nm7etunWLwq6yDEhYMtgWHsCEARMLCzFgghhhMWFSfw2SZSRgaEQjBggwGNlV5bp16zaZefJknnOij+/b3977bdZaDHakQBYxipAiQqEda7/NWs/zeyAEqKXmOuVlmQuAocNSSkrdx3/1D8erq7zUtX2P+HS0EsZVLsJIhJBLTTEws6oCQDNrTWtrrSmv3glERwI3VyXG1bM6dF0I62kdmcnMgEgk5lwYMaUQt1svBdG1qarlXJEgyJN5B/CJ3GBrN04opuTuq2PRHUqp4M5MTW3lbKhpreV0HPPDvXR9qRWQTRUAhQkccm0OmKsyAZKjGWHrAnQCblZyrvOh5QfA+PnP/9Xx5tvD/fXNt29vPry/v76t03E+PmzOLv/lOtMMlDaRz3YDIV6cn3WBAMzUY5TtZnBzJEGwZ+fbZxcDoFTF8fDw5u31PE0wT45wc3N3ONU0nK9iPkS6OD+/ePUxIGHTUs3B3KzUhkjLvBzGJQR2WDWBUKuysJkCUintMBUhiJFrqysIwpp2SRzh7OLZ88uz9+/f95suEB3GPPRd03qaCtbf/ney2QL2X3z1zbtv3vYRO6aXL5+HQLeHuTb86Y8/ebg7NHMRWHLdn/XD2RbSDgjBDZpBqXU8Xd8czBQRtNmqY5IgKZA7xiStKhG1VnfDwMws6A6rRwndAamZozshOLqpI9HqSGMmU5sqsLcQGADNWhCu1bs+xijHcQHXdeepaqsTWhhjGtxqKdWeWrXQrH1nLkQWzrmsSkYiREQJkpfs4GAOjFqt7yILl2IxSm3NDYWxma4K+lqKg0voWilqysRNtSisJqJSTEJEQnBVBXUcpyUG3g7JafPi09/tz8+//tUvHu+uW1M1RJbUb9So32x+8gd/9C9XWysgEdoCInC8hqEDV5ChPdz99ss3QQARn12cd0nC/my8fRxPRyFMgVOSGLvDeJzn7CgpDcS8nI7qgICn0xT7LhCTyPl+d3t/Z3m6vbkGxD6KgW0TBqwGeJoaEHUpvH1320X63scvEPT4ODbTvotq4KY5l5iSSCxl1qr9trfalpxFaJwWka6Hlz8DmO03v77cd6+enYcggNAMatVnl88hxX6zOY6nw3FCcIehnYreX6ftACmBOhguuQE4uC+5IpiaE7GrmtDQxdyaGayX/9YaEagyggMROErkmiuBIa3ifVsH6OBmju5u7kRMzjFGRChZmxox1tKeWnbmLLKO24sZIprhvEwpBFypD65VXZglCKK3pqgmzISgpkPfA0ApFQkjCyKV1iSJA7SqDqaKwqzeSvUQAyOpG4u4mrs7uBACAQMnBO7T6TSbGYISiKMjmBCbNVNDF7T55u2fXrSfaDlhOwZiAVGAZXxAlu7i/OrrL83p/OKy6+La44A637z99TQeg+DlfpO2rwGfA6icv371Op+9fAm0A/DDu998++uvptOpVPvse68fDo99P4i06TSP09IP/el08+ziEkh2KdzeXh8fH+ZbZI5DF0XCbrt/qI1CN08jESzZY4jrU1WgRKi17jra7bpalvXs//zigskfx7nWJkLznIlKEDT3+TTvLy9FCBFIIv/xf/73gRFC3833u+0QhR38OC7rc787lC5EK9W9IQCJaGtEoZTaxQQhgCm0Wudl6IK7TXM2M1N7PJ52Q8eEEoKZT6dJ3cFBmGKKbmsTDVZWxWobEpHY9XnJq6XBzIkodcnMzJDI3dcKxhgjEpvpil5azdGtqZpF4XU+uTpjHbyU1qWIiIhk6PAkAEE1FyZCcmJXa2ZR1g9q2lJM4L6ucwBITAAr1krVFBFEIiCCqwgzoTmuZowgEQFWM0htFZFjEjULIe56YeY+ooQo5HV6CGK9OEIjr2ZFJHX7S61tmUZtCzrEYQMAEHi8f3z79svT8fFx1s3mMvY7gAbACR3TDko+XL+dS727f2TGj1+/2AzbL9+8QQ7omqfj/d3dN+/vtrtdl7q6TMgMbupYpuN2u9ttunE8np1d7nfbm7u7aZ60Zkbr+95d3aB4BPAYYEhRghDi42FEon673X//+8erd6nfurYUud90XZAllxA5T5MBxSB5yfzH/+A/BAKQGMpJCGPXG4TAbm6bLnzz7up0PMYYEGxemjD1wzCfFjAf+gSma0XELjLx8TS1tallvtuk87O9I7j7bkjC0jscZ+u7GFMAgNpaNX8SFZshooPXUpiIGFdHEjHXUsARCITAzZlBhFUdkE1bKSWGgCI1l/XabQ4ATkxMRELWDJAc3FZ5qzuukB/wEASAYHVTVnVwZgGA9aIMSGbuvm7i0JrmUmMQREQEEUY3VW2q2nwpjQCeGCngiJSCDPuLl3/wd05XXxyO89rwGyITgTC7VS2jewM3YSKEObcUmIXnealtiTF+77PP4/5i3TbL4Xh/9wF1MafL1589/+QHAA0gACDGkB/v33/z1YtPPt323d3N+7u7x64bUh9TTKdxdMDtdhOxBmqR6HSaui41VSY2q123CTHEFIUDICzTPM+LASDofmAhVAUg2u82QoZuwlSqm7sQxSjzdLJ5ctN5WtZTuDkxYlEVInMg9hTC0oz/wX/y70cRKKfpeJyzjpPuf/L78WIz3d5bK12i99cPhKD1ifDRaqu19l3q+g6QQBjWVx+otbYfZF4WJE4hSOpiCjHGze/8Yaoncn/xySfgDQDMVFaYjqswSRQ3B1+nZ6BN15G2BDHzqsYItLpzkVy9qZlWJgJ3c3f1kMTMmUhN3T2lwOhETMjVGiGnLubciCjGGITctNtdaGu5ZACiQIEFnrB0GGM3z9N6VwAAf7pFkoOvGl1f2Ue+NmIoxEDIEvu0PUu7S141EdpCHa2cSp5XcpGgpxRjFEKotSJCEEqJwX3ThVwqetMy5aJEmLrN+Dj+6s//9P7921bL3fW3S3M1IqQuxl/++S+uvnkzzcsXv/rV3d19SgEBus225qUsRzU/2+9FEgBI5NMpD+eXu6EXltT1AEYkkXxtN+bqrZV+sw2E0/i42W5i7HMp1YME2g07AzDL1pYYghAxozatTWNMDjBNOXWb8XSs1RjRVB0JHWtVQFwHx+guCADeoPiwHe5vHrTV5esvCDVXvLk9BvTtpndTib1VnacZu5hS6vuhlSrbHnZ7cIGLDdS8vH/vrQ3DsOQWu/7ucOoEd5seHj4g0Vhr2mz6GO7fvQ2CZsRELNHNXDUEqbUROiCu7ufVPAwA7s5IzOxmq8KWEZoBIhKHfohlqTm3FON4mglBVVtrIQZ3XPKyjkGCSddFBzNVQAwhTIc7cwwiCACEHILW5ojabNEsQfJSmdEcmCFIcLemFkJY775NHSkYEMaB44DSz7CJXXd+tk3kh/dfHm6v6nh69r0f9S+1VGUJEihKgMg2LyEvrRQmL/PcJW/VunYsqucdz0paxndvfpmXqU7HFnYPt98SmmPqhgGtXH/9G81ZHU53HzYp7vfb65t7RmJop8fH1myaHghpt9/t9vuzl8/Hq/f3j2OfdjHBeDhqLeDjobY07ADY6lgdHE/73ZbTcP8wvnh+VuaUS1UcipM2ba7PLi9iIFR7fDz4d93rttTjaT48Pm77VEybcQqhqapWtdbH3rQtOddqstn0QAJsUBrF9Pz5Z7xpsDmXuysWqurnZ2f3h7HcHYY+pkhdjP1mM8/zbtPD2SWEFwAbWD5c/eY301ymaTEAMGNCqyV0m7zMb3/5FzF1fWQ9PJY8x8Ddpm9FY5Q8L2uTTEJycHSvulaXKSKaEQIiEyMiqBkRxUDuhE1bUwAEZ4MK7oQWGIlJmNRhmvI6YkJCAFpyDiJA1J5cBgSARLSCu1Y8IIk4ghojhzKPxAyEhH724oXm5XD3SETNBSBS6NJ+67RBEKU4leJNzVuxE0JrpvcnPJTNx89fen+RBkjEQD0Agx6Ad5SWmJeOCEXa3b0ZgFaQsYfW8sx5SeSuc9oMdXN2e3ePYAHrMAiLeRvnWYMMkXm36TdDUm09lG/fvr25jfuhv3z2bMn14XCackOi8bcna7NwVNPTcZzH8e7+4dl5X/Oi7mdnl7zdlHzwNi2ZBZR1Irq8PD+/v7tlVOYu1xKDzONYiEhC13W7KLXW8TixSIypLvNSaoqhS4GQAVUbMXEuJTB1KdY6iZsjIRgAoJpdvfstRwkhNoAlt9PxNB4mtDpO+ac/+HjoNyGG1fXG+z2E3wNgAIBu9+zZA9UxJbm+PT4730xLA4dStKpu+ti0nWYo5arrZRiGh8eTmfGMKQmDVzU3dzB7WqWoNX04TkmkS+L+VAeoDQDAV/wOlNIQzKyYaYrBAJrqJnVq1nIjBGFCxLm03W6vNedaj2NmRCSM7ujuaDEEVWPxoe8d2Ayou8Tnn+pv/wR0pk+eh+NJJYzXdyJMxL963z76/Md9lwyciLy5Qq11WpZld7Y1taVVcO8S227jAIAr1hUBCEDnpTI+xKHj1LWlSkj7/dbNUUIctgQeQxhPcwqsLefx0Bq6aZ3uCTmx1nK/VARk1DJVu/vwFcXd9cN0PB53m25/fnl9+0iEl5cXJGE6HdGeVcdaHaHVBiIhdsPrj5NOR0S0PI4Pte/61hBQ2RRC9+rTi/12y+G5xNRRPRxnYQ7CzAwoOc8YQyJxUAmRARBwQV8308OY+xTMVtCpMQKFLi/LeJrFtLE2kOSGu0G7yLX64eEeiS62aWAoJYt026HbbAYHEiIiOn/2EVz+a//fFg+//mvPt9s3f/q/ne+H3NDMgqC7JgEzlwinMTNBCBvs+h3y4fhYlpq17odeWExVzZkQ3M3s5uH0L/7y7WZIv/vDj1MUM48BQUTNm61OT49RzNzUmUXdSCFIUHdtCgiEARHNfTN0bk0davHIiEjEnCLWWtAJWdCrNgTZ4m7Hc3YjGA8pJtVij4fl8YRwHySEMJRWv/rqNzdL9/Of/fC05BhQhFjk/GxzZLi/fRzHpd/0Z+ebh4dpPM0fru6//va6FVXT9TVupUpkRg4hAOJ+v01R9ruN2okQUgrqjZmqem5kYR838mxI+cg23VtZnGzXm5DVqrskOYVlOdAOueHDeDB314oSzQGQrJVvP9wM2+F4GDU/Ptv3z15/fny8XU5TqaXv+y6otQUNOjTnNB9us/KyPztN+eL5a5awlIW8bLZ9YMzFyBuD51JZYojdNGU3XZZl6MK01L7vWRDNFcgdhr6flgVM+yHRceb/4j/9D2LXw/Y1hoF1DDF0wYckfZfcPAVmljmXs+2QukTIHMKw3eNH/+b/z5AkdqerL81bLQUM1I2e/q2y2/QvXn+iVmrV1G3GbI8Po7sNSQgJAdXd1ADRHZrZ1e3jthdEFwlDlxC85CIiIuzmjpRzXve9UrT5embDELnr+/X3EK7aEFCzJAxghADg5rouLyIhRG7NY0xIXGsJzq2WWopAFcaaSz4+JmEDTN1WecNhs0DY7Lf9pht6AYBpWVzRAVM3dH1aqh6O07t3tw8PJ0DIy5JzyXmZpjIvy3xacm3WTNUd7OHh8TSevn337pe//OK3X759+83VN+9ubu4OapBrZSZANNWQurA5u3j5Sdqcuy2oJUWKggDeRQyMu43sN0OKgQm2fRfYNU/IUmsdNptnF2fXHz6M05xYHw/jy4+/36duOj3eP46leQygRv126xBiYNPl/rCotVbmzXYDdTYtBADgCMawgiK9liwhPCn5Uh+EzE3dmdjca1M1sNZISIgdaMlFzAzQ4PEraHUV9cGQQp/Caab9prRK4xwCpn4TQ7deAAEQ7v9P0AyMoA61gjoAlFq2Qzdn+nBz7GNkQgAvzZY8MWH1gzd399ur9/fH5Zv31+ebtP38IwT6jqFCq8ZHS2tVP3n94jCexjmL4MVu6BIjPWllW6sS0wqHDoHVWl5aDAGQx9NEiGBWzbAUdUTwcV7cQIIQg1ZlciQSETcza0tuCKZmeZ4IoamWkJq5luwIFeuSK3LH28vC6fPfOa/tqRkRAoW4P57yw2E2m011npeScykVEBGIWBCdWJpWr1qbEmFDlgAppnghrVmpNUZr7qY6Ho95Wa4+XCExIp6fby/O9peX+912WIivHlu25xT61A7nA8Ayq1rfUc6263nTRa1miPOsCnFWd6Hy8O11Gxl1GLaHpaUOWyn7Zy+Px0Oj3AXg0Prdi09+8jOw6cOXvw6yLfX+9nae5vl0uH513oNrrZkItLWUqItcq6m2aXxoyg44nQ4xSN+leSk5L81cWIYhnMaZETEKE8WAsu0jgEFk2HUQArhBUYAG55s41VhK38UPt8fVQCvM6dVLkGS331KXoAG4QlMAUIO8TMfDlJuf7xI6ffTpJzdXH9g89WFeltIas8QuAMAPPnt1eT4EYkRUUyZifqL51NZKbVH4/GLfdeHut1fLUh7AL3hbHK6ubwPjq+c7hLV/EVtTIdInXqFHZpLgIiGEcTytsttcGgIAd2qlVE0pqkLFFiQwatGymqzMlIJ0XV/UwJVIAWnJLW72I+3zZMSt66MwqllWOxznUs3UQoiqDRGZiZljjLwy1QrkXJ/GhIBNFZVay6Z6cXHRdbLMZZrnlc/daiVhYlHz1tr93f2XX77Z7XZnZ2evP3rxyetntRZVNe8zdznXwbzjhRCZHVEJKQ0iIlEwK8NUECt1AHYkQfecAZfHw1fT1cWmr2oSX5w9v3h3vEqvzqB7DgBJ/jJ18PGrT7/6+t237z6ktGH3pkagCNL3kdyWXGvTEAOtqLXSUkrgmosCMqAzGwsHSU1PXT+UnJdccimCfQfnOxAEjAAIvkDqwSq4QdeBG9+PKeRSDYDSEIF1ev8GVfsUIAgsDYhctbZm6sjUkXkcEFbuWOljUncAaM3maTqjYdj2hJ6Y1wlB1/fMVEqVvveSu75frh82Q7JaUhRhPE4LIL35xdtxmsHts1eXl2d9DCLCsn8pKMvNmxiiCJm5meHqV4KARERs2tS8OUJraLjdDDFwM0OkUisAxiAIUJsSS2vm2Hbbi+PhliQpEMWu9C/n4ubeibfattvtN++uHx5Py5K32y0TLmXxZmdn21KKm7dmMYm2Ns8L4roGC6zjb3AhTF26uDibTvM6pXAAcCThFGLOubVS8mpN9XE8jcfpiy++Ors4/8Hnn756cdFFWpaWlUp69XKrfrrq+2DupmZAZtYlOUtxTL7M6GgikmKY55xrhT6oUSMuWUu+Ptjjy1DTHS2JxP389Yv6cHtzdfXivD8bJCSxarUZEzl6qzXn7I4AMOcaCB0sMNZWc64AZYVjM7Opcn++Haaqte+Cu06TC2wHCOcAR4AG4GAGVMAUJAIqHJeH60PfdyFaWKGl90dtlR2gKTiAO7ihxJbrUhqRhMh5yQS+TKf9dmvaJCXTggQvn52rmea2qAMCAa09fC3a9d1yOhIS1Farnu1SLg0Rtpvu62+Obz88emvf++jixz94HZhXnKKZ+zy2VkIM3A/zcdSSYx+b+ul0ApyGvmuGjqFLfsqtVNsOHXnrNMf4SQAAIABJREFU+ziOEwK21sCRmTiIaW3NQxBv+fh4XXIB4rh/7fG8GSC2JGG7HZzkizcfptNSW6Wn4BTIuXRdNwxDU5umRarFEHMprbUupRAjM6lpSKLNEanvOwkxBJ2XOcXY9900LSmmUlot1Rxqa62qBCbkUjQEfrx/+Ke3NxcXz3/+8x+fbZJpaZouPvqc/fVy++3p/gP4yu0jESylCuF+34kwIZSmmz6kyMMmgVozcIhNVYjmxXor7fpdOrsAr3nJzDHEvhv2dRmnlhHUgZelpsjuiIICaLX5KuZDcrcUAwu7QWnFqgfh2/dflNLOLs5M2+781fNPf1+AGeAEgAABgIBm0AxVQXoYp3o/BaFh01lV1TadTnNWRmzggw5gWkqZc3E7HcYpV2Xi3iUJAgoRqOrQ98jkSQ1IMcYOhUjR7u6OjHZ+ti2tedNQVzIB5lyWvAwpELa7U/vy7d00zZsUPv7ecxFqxfpdWslItTVYTmm3afOyjCOCIxM6AigTVZeHw6JuJPFs6IWXpsbWkHxZMqxrCIC7TlNuzSVQYDEt3TCYNuZO9q+8fyEp7QGaQYxpLvb2mw/LnDeb7nBUdchL3mw2u13sUkpdh+NERCJCzIQYQiSOZqRm2sx9JYDacTw9Poxmbcm5lLLOymrTdZd319XjCADAYE+QSTX166ur/+Xm9kc//v5f/8Ofu+px0k2/xYsfng/b+eprRzO1J7sNsLm5s0Tuhzidlra00ykjeExRS4lR3L1LEpnAax7v3Jppvfjs57D5/sMv/jETtWZubmDC4KYpcm2tAaKjCDerTtBJMvPURQTQY1thBLU1EV6mmRCbHpesAmUBUqgNfI3VeFrh4f1VHnNV3XQJ3FUbIaihu4kwYljNbWuay2E+IcCuDw/jqWbYbvquYyJOkXIpzen29uHFs/3d3ZUgD9tESNteWmu1lKbOALo+yApTbq3hu9vx5v6ISC/Ouhc/uBAJ1/djDGEpJeXAggAYhJspTlOruuoF3BxpBfZCIguEAMHda5mJwLTNtYQggNhKqxVFEMhbLeNh6oYkuz0hznMOwttnr9rm49T32qyUjMiPx/z+6v40nUQoBDkcRiZPXQ/gy1IdIE1lOi2tNUeIsWutIXIupdWVDaJNVdXAPMRw//DYpU4VHMkdiLg2ra0Rhb5Lqpaam7XaDAFZAgAitFxrWfK/+LNf3d0d/+bf+GvM0PdBlfjsRzGmm69+SYjbTZdzNXJXWpalZDw7H0qp6JBLJcRSTk4c+sFrGTa9m5d5VsZcm6nt1eHwBYK15sRkDmBG6M0gBUEvTmGzjWau1Nb8K3Ndd4a+71VVW1OF2pQlhNSj69fffMV//F/+x9D1sBL1HaBWIIZF22kR5sBMUbSqW11yI5LddtP1fRRBIiTkrq9V179mv+tNXRhy0cvzzTjlUgqzXJ7vL843ly9e1JxXc0et1cwjS1UruS5LC5Ec8OEwfbgbf/v19fEwfvpq/8nr55+8Oksx5tqmudVWEXzYpBgCgiNzrQ3AWIJZQ4AUpbYG7jFGlnWDxSAoEnc/+1ubfpfHKwJA5BhTipxzRVjZkE+5P7td12qVfu/7T6di61hd3R8P+cs37x/u75ecg6Tbu8dWMwsHCUsutbbIouan01hqnU7ZAedpPo7H+TSVWpnBwUzdzIB46Pr7+/vxeHp8PKqaA665SGbempn5vJTa1AFqaWsSAJKsZWpqTe3u5v6LN+8++ujl648/ItkAGHaXbnV6vCm5hkAreLsfYmCZl0rEiLAGD4iQBCJ3dKuqNS8511xLrSrC8/37+fGq1YJoq+wxpBCFAUybNjVEZx7OX32Wx1t3ZwTz9epv6G5u2pSYtVYHn6cZGYRB/PYOnxxsBmqgBofFzJkRAYAYDAFMjQDR3Ftzt8YrkZzQayP0nMtuswmbPYx5mYswPRzn43FGxA3pzcOhj3w8vY8SAgdDYCQJ66ERiSs4nub8cMh/+eW76bS8frHrUuyHTS5aqrFAYHp+MVzfPd485L7vYeWcwar2dLVSq4UoBoSE/WbIS7GqSC5CplpLefjF/2otEwgLtFqbm63voloIvMwOQMPmYrj8bPnwG9m/bM5RwF3nuS4V3n+4H49HNc25llzcrB86ptha06a73T6lrmlD5GWpx8No5oCu1XKtaypZabUVq62YwXSaVsb2Cqt3RCYwUzUIganxsixupuatKTFpUzVrzbW5IwEoINxc3fzDf/SPgeiv/Ct/ACAApb/8OOda7t+ge9elVpVIXNVVi1ZH0tbMrZdkgCI8nUrVJiQhBgAd+kRIanqa8qppiIEAzFVLAyAngpSCmU2nu/r2eH75arx/n0tt6inymqDAFAh9misSaWsr64SIBShABXDXZWHhpk8SF1cABjA019ZcHW7uj0MS6g1DkBhADQyW3GrVu4fD9c1jjB/cTYjMeOjhfN8fp3zzcDJ1TvjqYjfnEoRDFCI+HCcJYs2dYFzszdsP7vpynz753Y932622epxyLvY4nlpdUda45DbNZc7tbNcHIVXrhx2z5XnByIREHKyVw+NYck6pS8LLUqZ5CVHacsfCgH1ib9XdFMmRgIHMvO/TshSrp4erL6rHGHa5lLPzfeiSLsv128NSSqvVAGopSJBCIgo558DCIq22ORd3MvXTaam1mvuqKkZkJii12boWqeaKqoZggFirFqhIHEXULecFHdWd0JjX1iYSYlNrTZu2VTyCyIiAZONx+m/+2//pxbOzTz56dn97x8Q+XEqb63TLDETo2gCw3wzLNK/qmdu7k5oCeF0agoM7eG3N+i4hQFMz881mqDk3M2Le9NEUOAmCu1M1V6sMrtoOj7fCxGZN12sp1lbNQZ/UWcAsueRVBC8NYqi1lhqEgJEMCRC6iEWt6bLMhJi6ZEZRxl3fxS64r4lyYOrE2HFMfbq7fhi6TUjdPGWCepzgfL+5ONuU/BC6kHqspq6OYG7+OOVvPtwvc3XwaSnzsnz6Yv+zH398frYLIVA/LIcDEMeldh0HWcMWWpdkGvLjcb482zCTmyFaq6rmjFCaAubaqrDEwMuSCSMC7HbbzdnFzft3BhJ4ZQRRXrIZq1nXdSVnM5cYiMG1Dc8+oRDFqVYNHXDoHg7flmVZYwPNDRWVPc8LS6jaELB486msIRQiIfVbVXo8+mE+B9wi9evstlnITeYiTSv7uDu7gDCT3UF9p3pyb2bo5q3VmALAWo4ICKUUUwdCFgH1uTZAEolmfng8/sN/9D/8/b/3d8+2gxA/Hs3PPmKsbXpcf7aV0loD0FKqKcUggO7ODsCArNbUIqNbnaYKRCmKlpyruptNU9d1c86oLQrFOIQUFXg53pu7sINTECaCJTfkGIin02xu4NqqNvfnFztVmJYiV3f5+RmnvgMhaI2I87JE96a2LKW1tt0MxikvOmy2a4bLyqFTNURMMQLT813/+ix+uB9zLWa63XbHU/7yYeq68PrF2Xa/Px4OBlBDI6Cv3t/95ZcfplM2NxFB8i7JZx+/2O92pdm8zAPQajCJkZlCawqI++3Qd10pZZxyFFAzMJ+nCRyAkCWSVTONIubgjn0nAJBi4Bjh7HJzuJ/mXHJOYSi1xRAQQZxKyWvW5LpPOWLXbdX8/NmF1watvf9wmKd5fdG1mbCsWHhAzLmkFIQDk6Ru8zjF24d4ffzBMW+WSkAbkAgApbirITMCuDglTAB5no4e+0EAQUsRGNnvMf8K67dod2bewLQpEbWstTY3N3MOAREdYPUUIJk2/eKLr//7//Gf/Ht/999ALwAeU8+X34N2CghVlcmbNUQg8GFINfuS1cAJ0BFSWt1lJS+w3W9rabUtgghgIYaylHmeRTrEKiLCehrvl2wiVJsCApo6IlEQBm1tqrlPUiutfemOqDQXRDeT3TYhZIAIzcAM3IOwmiGymXWbjSFdv79Sw44h9NHUeDUsm8a+gy6AhOevXnz74cPvfP+j68fjh6vDcTztNts+rY1YOo5zrWDelqJX4/Lrtzfj8VAV+yS1VhGuWQ/j8slHFIWL1zrPgFBzTZEBNAYGBDUkETEbOl+hoSLs4CGEOVdf/aDATbXWyswxhFytaR0f5m5ZELyUkrpUagNDDAzuhBAQLEYkR0ARcgqh36Dzw+1DiiEEubs/rKkrCMAxeHZkVHNdSkod4LDYxcP44utfhWM9r40kIAdAfrpZqUOM6MaOT0mSa88xpsEAVNfAqdj8stolxM+BTxRumN9B+Quza0c2c0Kq3pq29ZXIpYUYtFYgEhZi+uUvv/7bf/OPLs+3hHCals3lCxuvlscPwth36XiazDBGGI/jk8l+9dMXiInzVNecxof7h2EYhKhpcScS2wwRAQ7jabvfGVIpmQC7TlQtiAijGrh7KdnMYpAYOYRgvhAFSqStxRRaqQAmu97xxfehZDjewRP1kMhhWbKE0O/Ob2/vljkjYb/ZdikAYGsaAsd+ByGAO3CEfcxfv/3y5rEDurjYHx4PVzePH728uHj+7OHxuOTCBHePi8WLX/zmz6a6xMTPN935bvvu+jA3vdz3P/3RR+udBcCbQj8kwIwEKYZpzkPfLUs2N3AYNtu8zCLUdUMu2cxFGFzdobVCRNvd1q05IIHHIGtLuNRcSjs727VaRHDNx0QEBHJo4EgryD2F8dSAYZmLq7aWSn1Kc0bEWttUiiPG0DV69uXV9vr4Mvslp6QGboAMSKttANQBDJDAEZCAGMxWuTD4mme9vvX0HakGAIWd92b7yX9o/FPaPZgH0yr0TyP9ptXSmhZVMGQJJEFrUaQQZJ7zP/+z3/71v/qTUrKqucHm4iMdrxGceMXt0jJXAFgTioa+N20xABMFxjT0LDQeZhaMgduJUhI1r7WYwXYb+4jjNKvBUmrfd2A2T/M+7QihVkVy0za1xhQWqkwcI5ZqXT8Q6lRLCEHmpQ0P99Pjo0ADxJUM0KqGFFHS3c3d7fU1Or58ef5UYTEECWssHCBAtesvvl6WskvxcSxX42SufeK+l8M4ZfWHnDuWb98/mpdTnafTvNvJT370w++9ODe3zXBdlnLxbDtst/M8L2Xed31pdjxO6yD6MM7bITn4sN3MpxM41LKmObd5OqlDP3SRIwClgQ73N4EpL4uZrcj70jzFqE2J+OXzs9ZUzYdNv8yVY9SSm1pKAgalNQmUsw7gALYZxA2W6WTmTNz3aZ7nWioxFz1/8/CjN++kaIzdebdLAGAKbsACgE+uCV8Tb3CVzD1JwGteQx2BVukWAACYPdWZGRAAMrgDdS/AX4A6urXwEg7/cwj/hzYlt7p6sACB2M2bqpv+3//8l//6H/3uZjPkXGsrmYjiRsvopuiA5ERIhNg8pADgRAxEeZmBsCk0VUesuWgjCkkV+oHrUkurazsjBc7VmIHQVTUITaf5bD/My5GQY+pq05xLCAHAy6mxYK0FwYVZ2yytKeRxSASYAH1ZMhpRisfJTtMhUhu6pLXNp0WEgvTWjAJ8h7pUYN7v9pqvc9V5XoDMG5SqucHVzcM4v38YZ3By84vLXrz8/k9fPd9vLp9dtKqE+PnHz2OUGMPpOHaB+xBXIzFEaXMNjNRFMxOiVgsCxC448DRNfWJ3lzDwi+/D8DPwb2Aew3gqZW619X1c5hoChyhVtVWVQOu5qu87Ql8TdB18vc0JC5PXam9vbn/vUyJhcHfBpdTAskANIdZam9FhefXm9sdj2SKdNmkbNskQrAIh2FNwLdiazgiwRlev76M2cAcWIHwqP0dAAKQ1XRqezBFrVTo8VSkjGhtuff9vgc+0/BPVgi5mzRyFxNERsdT27dsPh/H0yccviBZ37xPPh3453p/G4obbXa+5quEKM6ylbvZnghUxudk0LyIR3GMK1pRQibkUK7W11voUzH2aSq3VTJkoCjcANZtOMzFr092Lj7rE1+/eTtNMse9SNLU12D0Kp5Rks00QENRABFojqJz607wcHk+AEncBVPskm6Hvhg4ctRRABsYnn/B2k7bbl4LTND5M9f72kEu5uxunOS9LVjVAYqYk8mzoP/342fPLs2UppRRiEkRiiSGuZvRSdc0gWnKtVRGhmdZiu13nDlabIzLhkgsztmbb3QZkAy4ACxjA8QHcCCkE9lWQiYTMUBugr5CfUk3N157InKfIFCNhw6YKhB+up//9T779/A90K1HdGEGYRMjMTqfTnOOvvv3hN/eXzSTUX73cvDnVbWt/2xFIwBRCAKDvVqYGAAAE7k+FRQxEa30B0lMJEoKt3CIHUHADRDAHBCD6bkUEIGDHMz/7Wy/DzZs3f1q0lewiyQCRGRwBMC/5zdsrYYzCrenjo/XNzX3o4jjlZSlR2NxzLhwCC5dpLAQOmJcixCKUCzkiiQhTbY1IYmTTWppGLIgGbiJhdXmREK/EJDNmHh8+lMAAvhm60mw8nZhkLtBHx8DmLg4EKBAMarOqJF1ZLwQAXUBvGqIEZuIARLDbc16AAaoBgC8F7w9G8uu3N1988fXD8TSe5tOUHcBqJQqX57uzbUpBPnl1fnG+HYYBAImKOaTAaIi0mt4cAJbSgloVcvMGFkIIsWv1+BS/KhSJ1DxF1maqcDpNRAseH3L5kxCCMJlVd5cQS65ECIh5yblUcOIA1hTc3cmRwFsSWt3FQeD+MNem/+wv3v3ll1fv3n345NPXTBQlqlqKpKaPd+XX377+MH2O4lDnN1/+4r3+M9n9lVc/BZGn89Yq/1mrhwIAwpNjCoEEEJ7WtrXU1iBHBTAHt/9XKuoAhOAIiIAO5t/VLgHGl7H/d3/qN3/+xdetuSG6QxejmTVVJqq1qiqlJAB96reXH0/5ptQmxO5emu52A5GUXKYnii+kFM7Ott3wbJ4OtTx6s363Xb0ZjuCKw25flqWUhoBdH0OIp9PUFLoUd7vdw91ddQU3VaiwxlYiEfQpNvUhugiZW61NpOugF3h4BEyUok4zqPZd9/J50FJyqafTEoR47f8vE1xcgmZwh0W/eXvzy1+/fXiY57KM00QA1byWQkiboft7/9F/tnn5/bf/138l7AxsZimwmm+GtDRdSgkkYc1ma1WtEUqIkvp4PM7WHKPnZZYQarOuS2BFUlfneXUQuOnKFBACYWAyM1c14mCGzEIMtVREJKTV297a6ja2ec4pSNPWVAm9Nkfwu4fxX/z6Xc7+/v3Vj3/82ZLr3cPYWtttEiN9ffvpu8NHHMhcQxw++vG/Mz78ztnz32MGcFiZTSxPp1agp9JxB8SnQCZ3AHsqsqcv1zJyQHz6/OkO4d/dDPC7b1/56Q539bNPnv3bP57/699ezQ7NFJnJ3FupcdPtd8P5fjvszwEIoEFpU7HEMmw5MM+5qDmBsUiMxmjLUlutMyDzseZ5GDp30DrnuThSCLwd0rIUM++60NQcfZpmYXHQmvPVvAQGXkMkAc0hBDmdFiJCWjVXhBxj4M2WpY4nnGx8OG3OA3iblyXGfilthfjMSyklg8ucCxBGNUGGkj9cHb96f/twGM0AAwWT3W7IS04IH718sQ3h5z/9Xnn47cavLvb7aRkTizarrQkRh7DUxkBByMCh1qomQqt3PHV9bk0Iuy6uvMWVbNDUEqABeWtNGzgiY83VBQC8qcKaZmjtyciEuKog3RUMiaCutz11czWnUpQIzNhNmfDNt7c393M1+4tf/OqP/vD3u6EbjydEYuF+89nbmwvkvtUaYggBNsPzTz5+XiqUtnai4LyDv/ET6Pfwm2/gz7+FxYEZAL6rpO/2P3RAAvjuuEb8XUysA8vTwe7/IerNeizLsjShNe29zzn3Xrtm5mYRPkR4hEdmRk5VmVldMyqqqG6pWzSUEJNEA2KQuiRUoh9A9AMv/BIekHiHhwIh1DS0BFlNJV3VlVNlDBnhER4+T2Z27z3T3nutxcMx73aZXG7uD+ZmOmft/X3rG96gzzfzb3lYEQTBkJ/qb75/9+WU/9Hjy+wOi+LNAVarZr1embuVTKGzOdO47xLnXKZJmyVoSq06pEbmGaZc02pNWqdSEXGaR3PebleRQpkrCjNzbNclX63X7O7gFNjMhR2QBBGpGDGauiPC8j9x6LrGzAAICWut8zQQdjXPMk3TumvaNs7j4dCPDM7SlKqrLs2zR2FetW5WSjmMWR34xf6rp6+fPr9E9K7rVqu07rjrtlEiqZ29dXbYHxixbeLVqwevntpqlVKQpu3iWx9Mz7/cX76OMTg4EqmjIJIICyBBra5gVkuSkK3M89ykJIIAOM+Tap36XgSlaYehL9lVlUUAoeRKRmYGjhKEmQh9iZ91XwTllRTdQc2YiIm02gKuwd0divrDZxdWrtzw8eOnP/vpJ7/9u98/P98S0pzLt7+++eWj7i8/7btVChHcgQliAynC1QGAwBS+/1b9tV/7AtLRLfzsZvO7n1yBIgDCqyvYDYB8PbSAwOya4GB+M6vo+uFbKDdAAAMAIIIFyb4BDgAI2bsvpr8Jq8qv/nR2yNNQDYXlvfdumtaLy/005RT7kudVuUIAM0CErmsJwdyZESmZ9TEEdIhtI9H6vm+6I3BjCftdH1JsUuzHPPajuuW5AmItlsmTCCCmtCJUgGmaMziUrEvSdFFDXsKYyEpxAxFmAkIQlMbUJIb5MERGxFBKEYacawycGc0BiYZcP7r/3ByaNo3D5G7HXXPn1tGdt46BOZfqSLnWYparCxqAtSHkAIqmCP08hMM+zwsl6G2QXFyIY2K16wgC1UmIhnFquxUguZZcihk5kjkF6EqdECOqEzBgISJw8zetJYSEDABecgEEJsy5LNaVGH1pYwV3YQIgCY2NhxjjnEspdZjKvh+P16Igbv7Df/rPfvUH3zw9PQZzR2/W8Y/+UJ+9HPcFukZMARAEISXoEjQJGoEPTp7D7inkB0mvfv2DH8VHv/WkQqmABv0E5gsFfv07M5AA2DXeBAD0N+za8lAtuBUBF+hq12NvOVJn3Nrqb0P3SF/+OXFQpSalb334Hriv152pjtNQ5sl2L8kLMUYS9zJndWARARgByRzBwDEaTDG15oaO/aE3U1MfZ7VaN5uVWYgRAbCWiRGJMc/OUUs1JOyakKtVrSUXiByETc0NEL1JEUCnWZlZhPi/+6//I0EHwLLUcgmXkolZq5V5DoJBwotd/7OPH/fDbGa1KDOcHa1+6/v3bt86S103DePhMNZacy3giuh1rm/ffm+1PS3j0AbJWlW19DvVEpgkhBTDtfuNuZ+G4gUVtie3iGUcDuNcCFBkoTAR3aJ2gCaBzXUcJ7DrrRdzQMIUgoi423Iz8OtJsHDvuFofaS3MRIRL27epHx9vmXCei5uKyOW+/8kvvhzHAsQc2qEfq8F3vvMNCEHiOYCH5O+cxSdPqVuFkzVsV7BdwbqD7RpOjuB8Be/JTz6+/8nrV4cO1HL4YvxgcnADZpgLDDO4gZZrxEB0/SThm0G1oAeH6yNy+bgmOPDNhEOg5e8BHULx47L7MfuoTr/2Nz78/d/93tGmQ0St1Qymw5XunxHLjbdvRTZVm+ZcinHgIKxqc87gKgKMWF0IUWIa+4OZAZiqmWnO5lZqtRCEWFZNVHMi0jrv+wGRJHbCSLi0siIhVDUinOZZmBEZEAh8P0wEZrTZEkkSXjqd3yjRjNyK+uePXv/orz6/2vW1FgY/Wcdf/fDOD75zt12tICZ4+8b23gdNamopUCEgJ5H1KsVmJbfuxRjKrKgegGOUccrTXKYpj3NFJEQgsKOuZQ3TnOH2b8jd38qlaim1zITAhF2MMJbdcIFSh2mq6ikGCUKEbiAxCMtSTB1EkHmpaY4pNU1aOI4yj8Rk5sKUUpNSJKZxHGpVd0OkhSBVcxaG6yh3+LMf/uj//id/DuAARcer3F/eenv8W7/TnnYQA6QAwkAEpjBn2BqU8eEnT97bl19dhfRyfnfJVReBGOBkBaigFRxABNBB8xv0gNfDDK+3Um9Qp4Hb9UFJAEzAASSAhOs/sHB38jVf/02r5fbNoz/6u7+7XrUpNW3brjcrsDLtr4SdEGsVcxzGogohct+P+6EAYEgRkMdhGobRct9sb8Vb31wMNcuKfbXuyBcIq9M4u9uYK3Motc6lApCZzePoVhHg5HjdRHGEJgVVI6J3Pvjmar12c3NjRAFkGAfTWqqC4/rGGR+uELwvQ6n68MXVzz962DWha5ujNnzj3s2T4w0JB0JggFrBAKaxiZxzzHmuM3AQZHz01afx0edNEzPCPGeKYMYiVKwWqnGWFKI6jLkaes21a2P/iz+t4CFENQ3CWnKuObXvUjPdOOvAoZg6Sq2FmAgpRC5TVqsxJlUHMHcy96IKGdabDsDneWZiCSElKdWY2NlrrfM0hRiEqagRUYoSRIgK/Ys0Gfc//V/+93UT3/v6vZjaamrDFcOL2yfvPr1cTQXmDEwQAsQAN8KzUuP5u3/rtAOOX72avq62qMJBGDYdHDXw+gDE12OsKvgETQfmAAaqi8vizW4Ar49OgH/JgxAD0r9EFRIQPFB657j79h///b/93t1397u9AUQERQT3yHa0Wo3j3F8+ZhF3v47EQLAyc2DLSrzMfgYUAgVkBQ4hMhNGclVg9iWO5VoGig6cUqx97TY3mkjj4dIc1qtY1CUkhdJ2R1VfW4ZnD+93bWpb6YfMTPzf/Bf/LgH0/bBab5qjDRwfyzy9fHWhpT56ufvxXz8w1X/r7/7Br/zW989bapqYczU1CcHU0BxNrR8vLvYASiy5ZEYKEpskBSo6LQIeQjJVB5jLnFAWucSUsyzAn5gZQxO06lj0sh9rya9fP351sYtBnNHMTJ1ImD3PxQFijLFpai3gkEsxM0JSs+vVP</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAM0AAABsCAIAAABGnqF1AAAgAElEQVR4nIS5ScyleZbedf7zO9/53m+O+GLIiJyqMiurqqur2u7qbgxuQ5cR9gKBaSMheYXEKCEhFrlg6RUSCJCQF5aMkBoJS4BsWq6ubldP1Vk5VY6RGRFfxDfd+d53fv8zC9zQxkI8y3OW53eeI50Hee+rruxkvdx91bYvdYurqvS45Yz1ssw7YqymXGJwbYubPcqyaDydceq1Cg5mD0SQXF1+HvJw1y5Y0N1cz72E47OexRtB02w4uJkvb+e32xWkaR6HB4DMoJe1tcjG6PLm8wd3ThgO2tbULfZYx3SAqazbllFJaeqhyytppDy/+1B1O4dbgGQQwrObfLWZJ4GIIwz0ZL4sf/V7v8XQ/T98/+9S28bx+c123euloNuuVW0tCNtvNm2xpVe3T8DB/bv3HLFAXX82uHz6rKnsblO10tw5zihlQLRTZrNvB5MJD8zBwajTvC7X220dBWnV6jhxWS8e9ImD5LXH94OgUpLsyiJgEnQvy3BA+uXeXb9sT8+mmND9uiQUWW0Rhv4oNNqDc1ojgmgoKAmpt76ptXadNdaB7Q1i572RiFEe8qyqS0CeUw4ey3ZbS51Xe+M1xlQQEkUhR5EyLfYsTaO6UlXTCo4pxVEYYMI9KASGR2K7b0IeWq04Y4xzh8CBtgqv1gXCuu2Uxk1Z1945xnzXYCEooQYw9LK0LMskyzCSYZgW1YYx3+aR0d5byhgLYg6A44i1deuxqqraGaEUiiIa9WScsKaz5N133+VU8CDZ7C8JIIpTAABHGUm62jnQLDBJzAim3rs0izkjlBqKuOpMOuhT0lNd3bXWgcK8REHVdp3gggodxJk0q6dPn84mKUYdYB+F40Fw2OuNETZakwBmynSbak25AZLJpuFRLKit2krWnoV4uVmXxZZxvC+usz6stjXGLh7087xFVsXxQARpXuy7Rl0tP76e/xgh6VByu7xpm6qXqCxOoiSaz8tdXmAinPar+YYAHg+GTWtYAvvl6uYib41nlIQxZZHAjHNKe4M+5lRKqaVvarvd7Hr9EQ9pWcrtqohCwTjZr5WRerOqi3Kb77eZCAXPwsyNZ4JwJDhDnqRZfHWRZ1mQZCHymBISxoJgjD1rSsMo4TwkPmwb6b0nmDqNOWc8YEHIOyk7UzunjZOU0SSMGSVWaSF8FDHOeRIH43GWhpF3GHlEKSGMAcbFbi87xDkmDFjAvAXCCSUh8Qhhp52jgjHqsedtZxAAwYAIUIE6uUZgnXdpOLAaMxxbi5WpQiEwjrAN6loihCkhQmRBkvazHsbeGt91DUZUdxZR57FyhrQV45QGEcaYGKeqWpJ//z/423m56cXDKCZpOpF6Y2AdRh48p6E20jQFUA6cBZSZzbLd78uqdk2tsjTFBEntZOe227nVutU3eVmPpwJhRZh/+eJlLySAufNYGxMLENT0RtO82hPWcjyaDl/pmlgwJtVWtlWShEW52xVFWZYHB5EQeHFdamWyQaplhRFjDC2WZb6rsmx4dNyXtmq6zqrBbDQuqvlyOY/FMAqSzX63WVeAg7PT06oxbd1ybq0ispVVXarG90dpURTrxR45DIa2qvUWkozPjgZNtV8u5G5fnt0dH80Gi9scg3n06hkXti2bctsEgmMaAELjrI8MxCwuyv1kks2Oo9FwolTtbWHaoNWy1i+d8RjC4Zh4cIYsVMu0tlXpjARGuda2rTXnopNdkdddZ7TVQUK1Mghr2WmPLOeEUNQUPktGsukQliICRwzGgDwF57HwN7dbgmnXdB55DOAs5pxHKW6b1tg6jLgHouuOcmI607o2yUIeUNmqtm21sWFICAvikHEWBDQFTQhO4ziWpgOsBeFNBR55qxBg7Ry2Uljv2m7jqfKobRsFQLMsEiHqpNOtJxzv13WUUoelQ9q0pNxX5N/5d/8qqC7pcev22/3Hyu2s1tYj5J0IbGel3MsoigmJowBnUZBX7W5bcRbef/TNXvpqWV4tN8+1qdIRbs22rndNlccRu/h6OxxkygJFIo6cbFwYRzSgZbkJRFc2jWzdzdV8uXpBudRGe4+yZOQMJY4prbquaVrdi49wQNqmc8gBEo20m3WOEO33sVZJmfuq3ak2//Zbvz4aPF4sbijLrm+X15ebWX80nSR1W6y388HgOMviMI6d1Zw4bVxeFLJTndS9UZwMEqu7OOAiYsNBvypra5TSXimMUbRa7TttLcIiTLtOvfOdV45Ox9vdvquUQzqKbdFKwl3XYW3i8fRwu9236ro3SpbrdStdPz4aTpXjOx+Qol1mIyK7ssyd1hYAY0QRgJRN1ZTOy7pute2YIB4sYE0oCkPGODa+EyS1xgPYfhoBWFlr443zhnLsNWqqmlHGhWCciUAgsFqqTirdybQXWOeMMUp2ndSMB3Wrm0rJBjswSRIxjBlliDAuWN3I/b5uO6V8ZUgpIjeZpoP+uMm1B4OwooGnnAoRN00R95DqpNGwW1pMgTOhlMasI4gV+4IHjGAitbbGBCKKYkz+w//obyENVbNuq7lUZcKSfhjLCgRxsgFZdwGhvXiACC/3bbFVZS6LrcrimIomCJ3Trm22VbVHYWn8Pssio9WuKLyzi2VVbHhCpxc3z+M41YYq1dzebrabNt/opnW7cnswzjD31/M1YWK1yPNiTwQpyl0aUcas5/Xly0W/H5VbezQb31yvjKZpdPDi6mkan44HJwHW+2peSSxlC27tHQI9Ohwfi6TJJmFeV1EUEovjMJWNm8yCOw8PHtz77mg0HQxRUVdZL+iPo8NxL06yuiyGw6RuW4wAjNfaVlXbdnXTSFm3oyTWtaYiVFYlCW6qFhPSdbDf5e9893VljKp2XnXQNgcHExaKrm5GgyMaexT4Xnaq1DziyerGr+eOMUIJNtoobbQ2xnUet0EKzoGFzmmCAFnvrPGcY2dlK6umrbxFBBAQq7UmgENGwzBEYJrCeot4SJpaeoMAW6MM4zgMKcbIeu+8sd63BpSUmJG2aZTqECZWG+9907T7olEa1V293m6ULSxuW1laDVrh4XBc5aVUKk0potZ7mmUsTlKHDCBPKdMKxRl1EhijXDBvoa6MVhYjSgVYDUHIRMCV9OS/fPfveKIQ6XhSDzJCfRhHbNjDo0NLieICyw47SzHxplG29lUhgzDI+kPbmabaKaOrvFKqrZptEDjr/G7XFnvlJTmYjQDVk4O4q6KuJpt1iQlJEoF8QGi0rzZNUSR9X5edELrZmZil+1XXC/H0ODTG163x3kdhTDh3ysquqVULrn98POIB6kWTyWDqyG2QkP1+x8mubllnzGR8nwQtgV5Ij2zHer2TptVV0YIWVSE///zi5noB4IBA1ylt3XSW9nvp5csb1enFurq53jLMJ7NJry8wReVeCU6+/fqrAOz6ejmfrzeLwlhPEU+DmBBzerePkXXtZjCgk+EwGYTbGsoCtdKnKck3t1pO86rQat/kSO2iIIwE41b5qu6kalkIjdrVjfSWtpVBBGkFPETeIgBMCDZGl2WDMR0mQ0qwMbnHRlurNBIUIYK6SjV1x0IQBGMAIMAo82ARYb0sQ5Qq7UXgtJLeWu+QN66qG62t1aZtG+tNq2xerfNmY3yd53nAKGcRpwlyjCDcVdZYSzgVoucUeCAOSWd1yGNMXJsj2aq6RJwJRFzXyrbVGFNAoLSjFPqDWAgsG0f+vd/+LUo4wT5IvCfeeVTliglsLQogSsIwDsOqawm4QZYEhDUdGQ1nsYi0bpgHsNqxveB4n5eY2yCidalkI/tpmiVJOkhu51VTWanLspC3l/XxWT/AUVN2ak/G2VE/mihTjw/5yeHdLOojq4Mh+fCz50YrzBnxAvu4kxAQTjoswfZ60a7YpfGgKMpOPp2vFy9e7iMhmsrcPfv2V19dBAydHDx6cP6dw+kD66gI04BNmrKKM8y4ASRJaGYHYVO2IiZFvk8igYBXZReGwmjtvG2koUQQ4NLIkPNIJL1sFAcBI8RIHYgIc6zbTsS86+psGIxHB03niYfOmuVuv5q3XumqMp0UVaWLnSny69nh8Hg8poJrXAvOyh1UZYsRzau8bgocWOSgabS13jskODISWe+sdVXdmZZQEgiKKPEAzoNsGo0AdOcDOtBad1ozxBHHUhrwjiAspYwC0lZNkXdl2REqtJLe+YiHbdMoo8HYptPgLSLgiZK2VKb03jIeUCy8s9YbKQExFaaGcuqcxEwTgpq2YNwiT+Okh4yQrUFUmkaIgHRt13UGAZRl58EyjuNE8EQXhSaUkf/qv/6fMK2rplAS8lppq7X0q2XVFh4UT9MwHQkAn69UkctYRE2nQ8YGWbha7vO8Wm2LRu8Mq+tOlnlT7MtyV917eBCKKIyjy8Xi9iKXXXVzXWZD9tlHe9N6D66fDrNw5EkVx4nou5vbHQAwAZo2L64X5bagLN5ui4cPh4Hwq922qsughxllHrGyahgeOGi7Sg8nx06390++//DBL/fSw3vHb/XSkzg9S9IxJvzlzecXL/+IcQ60DWOxm69nkzgbBHUOjIvD07A3YFVpV+uyLsrRcKo9nhxOiMPEE+0086QqW+IBEej1o8VuDQ5pY8LI3nlwVFd2tyyzNDHOeY/7Kd1t1j//09XL57sozfJqT3gz7BtvkQgdEyLuUyULcGndFbtV0zWSC0yZ7aRW2sdR5Kz31hFORExNY6tKFlXdSQOWDMJQKUsxtkqVXWMM1lY7Z7Uyu7wE4q1HmCCtbBxTo31VS6NM1TSccgSec+KMd9qEQcAEcdZ5YN46xlAUiKaxdVs3teykbzttLd1tTdt6wmQQdxg8sgEm2BjJmB0MPUEEKNOd1dIUO9UUhNIgiEjTtF1rAFHvXH8gtJGM4sV813VOGSDvvvsu5wf93itdeyErQ7inJC73miHAAUbM7/I8r0vQOMB8Ohz1sliqpigLq02vJ7wD27LFpbROWd9SwrwKNmu1zSUL+YuvZFF2nXJZH2UDnoj+q4/vdo1eLYtalUYU+zZvazkZ9e/eH7V639XgbDUaD7PBcLu53Ww7bQ2jEQAIEvVHwWZjhAUaV4EgadSVdQUoPTp4B7uQuZ7gKbTdH/zBP3jy9L2bl09mQYY0ivqIdros7OJ2kavt7TLf3UrCiFFos6peXMzbsguj9OVyJTu1WRdxwPqziIV+2D+IOBdM3L1zoIwyEvaVrJrmYHRY7Kqb24Uggtiga0pEdDzobdZNvvYBY21XxCEx2jy4dz6ZTZMEvPHbXTMa06rU19dFU7hQcCqwd8CYsNYbo7M0oIx2jSTIO+eqvN4VretsP4tikVgLzvogDBhhDkNdKSGYNdaZDlNctV3aw85AsVVlmYO3UhrnUJamSnV1XTGGsx5OMuKc7mUBeB9ESVMrhDCnuGuUcVh13hlrjBOc103rnSEOZME8M1wQ5xDGXluLceos5iJignvn2sZq01HurTNta8EjTK2IEKMcozjf12Vb3NwuyLvvvgsAAJAkD8bj1wfZm/1sjL1vu6JRsq11byS0BqkRy8TLm2KzlsrbfF+lqRhP+hEjUSrSvijqnUMaPF4t6rZCVnlZI1XRplNZ1OuP4vE0Bgx7Wey3+dn55ODYSajiiFjACFuPGvBuMECEtNloeHO76TrIwv6kPyEoBMyRc2Uu1087DqpF5c1NUdbt4SxYLcuqenp59Yvf/Sf/aPn0ixdf/onZdV21rS6X5WZXdUWuys1t6aUTIbr4YpevwSvrwIcimfanIaH9tK+wOzjgj1470BJefet8OHScoeub9STtjwa96WQEQKtSfv38mfWaMlK1JUJ4PO5NZkE/i403m8VGNY5xECkGrJMoVhLdLkoWjBjnVbm9uW2zZKy7dnlT6Zpa5xxS1rsgpP1BggkilNW18hYZZxDgLEkJwqNxMhkMwfq2lVI6QiAIOaGuLZu6dFp1Te045SKg1hrZWHAekNUKdbVOeqlHGpC3FpyDtM8o4x5kWXd1q/dFW9RVGEaDXo9TwRhuG9m1CCPkHSDqwXCkoqa2N4t910LER0ZihJFWYjI4yutVWzrGweCWhiTgYV11da28wVGGw4RwEpdlh4HUdX1zc/v/cPYXFCXZ6WL1ORHKO2AhAwoijBCHrlQZE0d30vFhL+2NeA+lh70w49EwRJ4M0oSRqKl237p//2g6SQa4MtteKOJIE6TyZt9sW9IwFqLDUxOPcBzw8YSvd63pZFnttNSTabZcFbe35aCfcG+PT6I4ana7uqtdyqPxAS53CFG32+e6Uhk+2FUqZGQzrz/77HoxX63aNWoqmhfOVDVrltUy13mrKQ4cT9F8Pbfrslvv4yxMJ6nT3HocJwEW6HqxOD09larbrovb661WEeoCDuzRnftJLzEWvKXeOkFQkrKIBsNBn8VmkFIuREDh5YubYtdJrTHDDuDweFDsTFVV2XB4e33RC/zLy+5okk57MWWBbUKrkPNatbbtpEfgvPLgtUSEYIKBB7SfJsQxTFE/S8MwEIxb47uuowS0Mx6BU9RqwJgSgqMkAPCbVY0wNQ5RirTRUiImgAfee6Q0JoTUnW0755xTxnvgWjltDSVECJr1M4IQpWS3qyhnWpumVRSYt0hKZaxJwswoI3jSG0a93sH56Tc+/+xzEZsgZttdJWtvnXfeeqe0tKNh5o3f7jpjPRdis1sQTMi/+qNXW7XYVy+L8qIsv67rZ95fC1G1srFaBQmjYeAMLoqWMJiM+/1pRjAjwvcOojgWVriy2a2269HxMI6ZIawp7WR8nA2nbW44pOfH54wEJHBhyofj5Ic/eLtUumvy2eyoNb6TqNp3/WSAadB2ar+vsjAxnV7cFh4IYLOZe8wcE0BY4sl+ehJiILRu796f+gj7CoVDOhpztWpFh2Pv+mHIjgZ6JHeFbb1FEHEIAi7GU7YvOyCIR0GapSDIvqmrslmsNsvtrqs7znlRSkCEImJbfdCfMiGytPf100XAeEDYtiyCIB30kqo0wDCNmSDhpD/yiM4XOWep88g41x9wLmC7LtOMC0rTLI0FQUyc3E3abndw9ED5FXK0LnRVtnVlVOcFTrAhTSGVNqcnI2LxZJoxHwQ0BEul1ADOGO3ANW3rnEeYOselUUIEFDNt0dVNsd5VnFkgmIV4v62tx5yKTtp83yKPCSJSacp8FFGnGCWcEtGqareVyjjvXNdJ55wIhDYGEDgNAROqs9qC1g4hdng8ZQwms5OD8UE/G9+sPuQc2tYtLisljVEaETI7EkGAgiAud918sVsv97t9xRkdj2ckxGIwJFJXxW7JqGu6Egzp9c86qa1qRRAUtVyvciYoFzEPmefWgGpU3UpdKFmXlbPly+tn68Wq6sxuW9RVPRhnTb1P2GDY6x0eH35y8fmz66/vHB6X0q2rajQYDydpUcy9t+v5LggYZRYBAHK7bUUDYIwELCzzJhSW1CQeJM7QstJ13uSFSXkshU572LR3SVfPi5VVdZBToVA7TNJ7Q5wgVZN8V0ltKIQBDqzyed22Up6cnxRFo7AFDLKTVVE2slpvdknIgygcZ72YhA6706OJ4Jw6uNqUhIdStb1Q3G5u9l3ZeZXLcrHeNGUVRpEu9L4pm6bWnW0qFSdidjocD4dNVW6KbjIdnpweiiC+XSwCkVEcxVncla1RNt/5/aZy2jutsUfgAbyj4KcHgyhg2NOmrp3FlNK6youiRsgDIO8tJqiTOt/XGLu28ZwFWtYvnl2VVUkJYUiUXTPsn4eC3s7XZd0igH4ahiHR2lonCWZcMGdab9B63ZRF670FpjvTGAmYkFbqkAWCRkYjDwhjoq1zzlnnkiiKMnJ8cIeKQwQ7qeuuVd7RkAVGaYQQxbiurVS6KjqltJI6S5nT3ntF/pv/9n9ApGY86o+zJA3SceqQDciIhaTcb4zzZV5zJpQKHFCp9XK10s5QSrR1Zb5fb/Kbm5vFfLHfVuV+jxEY8Pluf3JwVLV5bRdpmCmgy8VV02nmwzQmdx5Mnr54cXOz9F5whhlzeW5Hk2G3cV4H2+0uTSLvceqj8fjeqlgjx4qSSt22dVUUMO09uHhxsbtB53ffcGnFsd3crlTE4jv9upHLdW3bwjVFkXcCA0OCYCRY2B8DT6JnT16W++aVwdHrjx9RT7xDgPw3z+8/PL03SQbYRkkY3z86ssjv99XR4Khpu0p5Zcy+2rAkOO4Nt/l6vtyHDCinUnbX6wWiKI6iNOpR7HsHyeHhdLvIuxqDhjgeJ2lU7bpRX5S5clbEYS/iOKbhPq9iwimlcRjGYRAIOpkMp7NBL4sYFgQYxYgwiGJR101d11XVACZAwGhLMPGatbW21idZZKw1xhS73FiHCOzX8kd/42/LTj1/9pQQFgXUWM0ZYZ4ToNYYYw04RjB1xmw3DaK+UzbPGwAoirqTFoBIabTWxjkHnmBMGeactW3XdobTiHp9fXsF1EYxRFEgOKfMi5AdHAx4gDCCwTCZTuLp4eDtb99LEhTHmO6KZjQScSp4zJVx23WexNiQgtKeiGcYZmLad4CdQb0s7lSxXv6kbdalYLJTbSutVL1+cqNFP01q1baqbqrWdfgX7Oe+c688Ovns2af7urz7yp2u3ijflQ19+uXl5bPFaJTu1tvXHh1fz9fXz+r1bfPg5I6ITXOlXj6vuMDjcf/ieqXBZAcGlzIIY4HJJx/tfvLT9yYj4i1vau25OrkzI127WLTLzR6Ii5LU6DwTCaKSBEEIolPexX5/szg9HyxXFVf0ZHAc4N4rZ72TmSrK8tH5WdU0RVl88vyjN+/dP0zDh4+nv/fHX+ybYn694b0DLrpNtXW5X2KyWW8ogntHdzx0t/leANqtm+wkOTzoIxg3ddvk8uxkMozMxeq5c/vdlgB0zKTgdL3abQXlaXuYPjo/xMm9fhSEVV1t95u8NP20F0eEIuSQ1VYjCtSDMzbgIjk++8b3fmN7/bQo5l8/eaa8sVrneYEpy9Ig3266slGtVsa2rQnDIUL82bPLxc0KM7oJAu/teJyMs37IucPW2Eq1EPV6srVZHEutjXKIcLDUKa2l5wQwRch53TnKSH8U1JUEBwgD1ur66usoSEKUKeOCxB5Oj5tdg2DMqBgezJCzVVFoIwYpVE1jGHZe5yUjD+8/+Js/+s3xYOJbuy/Xl7fX3kXO3KnKgVJTRHqYiKa2CBHrndN2Orm33S/Lct82EiPQeh2IQGlV1d12U/hOTqeDw6PJLDuYiH5ZlYNshIUF55MBmd+sb27m2AlOURiRxW2xnter2y6imdW02rv5fFd02yyLnHLJMCi2lnK/mHdKWinrougMpHVTPXh8hgIe9ZJ9fblYbKJRWHvkOr3cGh6YThkFTIRBZzEVKRKYC6HU7qP3F6o1IQ9ng/Hb77yZJmKxyznldx+e9mKOgXz45dM+E/izl794+mJTFAGhlzdFZQ1lRRrwy8W8KnKj7cnhXUZpXjbzxSoNE0r9KB1Op71hcHB0+PD3/ulPdk29yJfzxRoZHpN4OhjHNE6CqDdlcRbEZiJQlAbMG0yQU7oZDTPsAGEQIW9VK6W1YK0D2ZnhYOQsfv0H/waQMOwf9WevCCxvr27BWu98vx9aZInVYLXDoLUDYxRKv/+DX3nyyXvzy6fglOk6J5u2qSmC3W57e7tVUm82e2ORQ6osu7pujfEBY6rTRrquc844KhgB6pzDCKIkCLk4OMwOZ7M33jw7vzP69INfECImQ94bxXHUq1dunB1OZ6ecjBjpyV213dRH05N4cidguNyXVxcr8rd+9Bvf+v4PwbswfW0yGr+8XeDu/MmTxc2LF5SS+fIGeXdyNP7wFx9R71jIKWXF1vd4WC8Wp70jzvymuSaMKtVxZh8cP06zcRomx4PDs+khIWJv8mF0V5Hi6nLpDLPKEYbLUoGEyWBKPYlZPx1DbxrdrhaYKQK022rqendeucMpME6dM/3hULa43xNhbGQny6axVt8sv5oMIrDo5dPNV59txgeIcSiLThtb5J1Uzkg7OxuND3vHZ3E6YE8/3x6EUYhRRui4n16Xq/cXX6fjXi8AMbtHxPnZ2etp//T6kz8ev/W9777xZhREl+v1Rx9+OBlkZd143ZwMB0IcZulwxNBqvW6s1GDOH5xqpVOefnHxNUMEKe2UV50MgujewfnhwQwsRKOobdoybzkaSNuQTGf9YRj3+XiWhjyIudf1eBpTQrXWVVN5cEIggoS3rq6ag/M3/+9fQL74squ7QRoQRGTd8IBODofMQiN1U3fW+l0Fk3H27MnPAFwQ8jASlHrO2XCSUoG0VtaYMI7Gw37K2CCLxoN+lgQIvFU6DkUo+MHRwePHjxkh988nZ6eTu0eH5w/GJ6fDw8FoNJnyzl9evxyMBk5ysGy/LEJMCSHXF9dfffrBpz9/78lXz4htOJi67LJ0ylE8Gc7Ib/3oR1KVg57n4RFAoqUAH3/5xZffefuN7XZzdHT4u7/7j5yHJAreevPV9z76aL9Z93uDt9/5JePp4fTw65efXt7Ot5uirSVyRITJ5ODooD89GYy6fP/p+sX1y23M0+urxWgUEsO6VgJorbu61uf3X8+7mzAz+6rY7orNsgoCfDAaHE5mB/eT/Xad9QaLmzzNwrzYzsY83xuPKPas2OdAbL6tJ6OYcdF2cnndUMKaRld7XVYtJRDFPODcWlwXZrsrXnxx/XB2/sNX73//tXtfz7cP7516jH/vZx9/586dCHPm4z997+lodvzFl8/TgSg0Hx+ePV1c/fyLP6PcaddQ7L/14PE4GX758nKcJL/2g79U1PJyvTg+OD6ejr7x2jcublZxSH7jN3/72bOvx9NDY/X06PDu+X3GGY+w9340mrzy4M3R4V9JuGplHWePIRgAPoVgCEEKsiaY7/Z5pxoKWEpDETfWA9AwDAaHr/w5ZpaL6P43frVYX1OMQoEZxtt1GWPsgGiHwPtezJRsACTmTIiAEoYpjeI06eWq5QQAACAASURBVGcYU8Zo0kuHg/G9e2enJ9MoIA/Oj9/+zusPTsZRwPuD+LXXH3z3O989fvDqg8fnp+f3Y8DT6UxwVxclczQMImv8cr1GEGCkgbSTLCWEr+eLMl8eDZO8aqMoePXReZal/UEf0leFSD95sqH7Aq1W9aefb3/p+3B5fT0dnO5ZjpxhIkyS3mAweOP1N3RbDdLMEazb9nazup2vGqlF0AMeONpPe9+qijmjm0Cw+Wo+Pf5V4GfodhneQJKe/cq/8o7VrSABhHsawTfPvomFb3VZyfqzr95DBDGRKKnLvY7DoC0MH4g4ji5vru+epVbVceT365LiMK+rtsUhxueHD++d3P/kq8+D0MgOosyd3x3aLcvi0KDgebnixEtZVDud9j3BmHpylI2Zooez0yfl9vUf/ksPDF52nbJa7cr/5X9776//+rd+/sGT3/3JL9LeqMpXDx+/5jmqzJOrFx+mQWy0wg7fPX31X/7NfxNxQQb/uwjD4cMfvmbgk8uPB734erUTSfVbf+23m90WYPSbv/lv0XAG4P/e3//Pu/qTXtyPKQsntFnVpvUHg56VAbQR9EMQAwAFIAFw1DuDdNB3X6J8TRmLu9ZYT7RmXPT7IwAA0AAMgFzfLB/0jl1bTDIehGfL1Qor7azrJ9G+bGOeRqFQugy4GA2zkFDraJImRjeD4Ww8iKVUAHizXtZFURZ+0o9Gh/12u33vg0/qsnKYYhoE9Ml0usVgXr64ev+DTz0iszujk4PJ5XzeGqh2xW6rjg/TJI16vbipyvVyngRwPDuLkiRJs3R8gMMInIOIAZT1bvf1k6/oN994nE2GL15e2T/6cLlbq6L6zvd/+fz83nq7G/Z602H/9ccPqqp69uzi5h9f3Ds9+PXvvzmf344mQ+/9YDj60V/7O3W9++QXP71zcHhw922A8J8t3skd9ubb6E/+ofFrIfjb77wF4X1ov3IatOs+f/aLiAdHg+GXFxfCsqZV1Injo5lCLXYi4elBMD7oH90sVkXRvP3oG4fjo/e++JPeAU+T/pvf+NfAdkVb1M1KlcYUw3t3HjdnXx+NZq9+79+G8tOLp5/PV2tt3NPnTwKSSYDR+O7x0dlrj76BvIPBvTfecv/gd36HROTR+dFApJyRh/eOvvziq93i5SwKUr/76UfPvv+D7x8fHLENwhge3nvtr/zaX5co+rM/+f2qaB4cn3328//5Jz/9sS3R8fhkMBj84qvP6A/S7EB8/eXvPXj0awCg1AoZkvJsmPZRx8rlliG/KpdubYmzstPPr38/m06yQWTBbVcVwhTbJ+vtygMwHmqpwiCuKy2sVXob9i+902JwDwD6UwQArz6+A1YDJaNhtFys10V3vSg9Ru+89dor904vbzfbfTEZZ2na89ZZZxbLbRqgNAmcM+NBMs3cZ0/Xo15gjPn4Zx/Pd+X989P7D+4//+IT6dH85mZ+c6mlWmz+r/CSuUo//erWOoQxP570t1uRRIF3eLfcqHbnsJocnlAhwKLe0RBEBM0aAgHsPvjd++//TCtF337n/tcXu/Eg41i9cXcSkMnJlJ6fvgk4ARAAcHJ2DACPX3sEAAAVQHJ/ePAX04M4nv3S9/7GvxAqrH/2x/84JrCtr1kgzDb09gkW/MPPfuYNfXw+vbxZLta749HdfdUEIhRxVOit1oSH1WXxcj9vStcq2XSmebFadFYA45utu50vNuV/56xb3naTQ/HqK6PlMv/q85uXi6tHRzOAJ+Dy57dXbRusV7uitAgsDjjiwaq9vc0LbPn22U+vrp49vby9dzb57je/9f4Hnz559sJ4PDw4FnE2G4jn1ztnyg8/fP9k5HZd4ZC9evHk7/33f7cXh1HGb+riO9/9IbJkVzVVZ3/11/51IFNQ/6MsXlwvtwJx0C+Bnf3D3/n7IsDDca8nks6VmUBx2+v1ZtE4jg8eg+f5kw9YEHjljK7229u8qiLGMPIIs2K118bGB1Pbbi20nXF/Nr8I+8PZ2e3oYHC1fDYevQUhb1vRNgXyfHDyyke//yf/608+fOXOMEpiEOL0Gw9OVQseIMhASqi3g6BvnW/aHLS6fLmNk+z8bFTs9tjZNKSP7t1vHQcO5z/4Pkij55dd03z46UUvSc7uT06mB5v5+v3PX3qAyXg8nI7T1b6TcthnjNgO89Vtu2v0JIgc+MV8dfjoPoRT8ADQqd110S2apkHeLwESAAZA/wVW/n+1g/bTYrfLjr4NcPjPatuf3Vzf1Npv8t2+WzBWCX5AcRBz/PL6qu5qZ+zbb/7ScnMTB73p8GSv3B//6f+R9FCr1eKL/ODorqC2rHSc8vH9enkrB4Meh7EHdLu7LRb49AQfHh1cPLvsHUQY+8ODoLhJn7z4chJm947uXO/KAl/fXLSuEs5D1h9EcbIr1nm3IJ70ohOH9e36RVXoNExef/XR/PLGG0uZ4JxaIJSgy8troNhqCGIwvr17cJzLqqvb3ihQYDUAxcJpU25LFNGTg+zVg/ttYxui54vlZDB47ejECvb08go79Ma9UxIJ0WPj2R2AQ4C1qi55ch9gCOABBgAYwOyf/KP1bk8B4rRPTdMpCERACc6b9quLq6rueEQdx5bWLE5EQJpanh8fxSSWpSaQTA6Onj+7/OCDDxilv/Ir75y9+W2AIQAC0AAGgAOsABrIV0A5BFN1+zU/+TaAAygAFIAGiAAYQANwABACPHcvv9w3uh8L6bDz6OXlcrMrzu9MDmdHbVtfLopeFkz6IRXk5dPrTV5Npocnr7xS7q6Mc4PjGaAAlAE+dPn1z977opGOAvQA+F9ARwIQAASg/rxO/rzlAPA/z1kHxv7TDz7+ZSWHd98BiAGKP/zZR3VthtNpXqlpbzAePpyvniusJDBLLEVRv5+FYgSkFOn051/9HDPWKYUq38+yfVx+651f3i8u3//oY6PaXDe9JKWQKNgQF89G7LXj2YPjB188u/zem98ui1K17Ytf3H7x9GvXooum+PSLbRAnQFRbua6pw8h3XcRoQDz4ktbKlOXTWnZ1rQPOym310c8/TgKhtX306lHb1JdPLxgnmUCrPDcecEQxdUVeBAQjJLa3rSQtS2iYwWaXOyO5jRotv1peb1fNuthNBpnBqlGdsVh16juPH85Gs8b4qxdX42wEoYTmhiffA+AALYCB5jOphFFqVbhG0XGsBxHRftCWDRPAsFld797/+EuEcf84mR5NW4XzuhxOuPH+avUiRkPfMbDy6xcv0zj6S7/y3bR/MBgMfFmgqIFGQzoD8AAE4ABgnq8bHrowTvjJL//5ZNP/D/s4x2dkCAa6NqxqSNMHLHo1iW1ba+fj0cxcb7MAg8e3t7XF4v7Do2x2BGGSkFQaW5e5hSLLJgAxZhkom6UpBWj/ec4EAAAsADqACUDwF1r/L8gAgK/y+tnLhbPu4a4ap7Onz2+369XXL9bFz7/AxL/1xoOqztsKdn7taD3pzYwdvryZ35Y/bioTRM/X+9tQROUuv32mJ4cmHsEnlz+uVhp4N9/KSYKIDdZXTV3ve7Pu1XvnWKAnm8/n5d46+Zd/8FchSwCat9/7w48+/uz9Ty+tqjdV1XWKMiaCUHmJGfIepAJtEDhEfNC1rVIuYD4KKUXEaHV2OH39jXfqYuudaYstFcxiX6FOOgBpCyhem54u13WfRuvabG6LscOPXj1fLBb7Tb5cmh3tvHKjXjgaZ47iznRQKyyys0dviyS6uvjSQPdyddUnFcY+iXoAC/B7KNfLZxfLbQOYFk338WcXB4P4rYd5FMXr3LlM5GW93e4FI/uuFR29erk8enCIunaxsIJSMiLpsJXaNLtuu97sRLDdF8Nhc3b/0fHxwf7Fl3XbxvEVBue0lwYDwc+fPRPMP+yatm27VgKgw1nmHbA4BoSBzyBC1c2tsb6fxcAotLW0SBkXI816IyDR4maDvd1czAFwPD0Ehw5n94EeA9j88uOqXXlXOasJTW7nqzStAnGlu/ZmW5nljrz77n8KEP05NzlAA+AB+gCXABMADIABLID5c2OTAA6gA9jurj763T/602eXy9v1GiNntOtqSYi7nW+2213Xdtv1sq4XnJJyq22OU9JrpRQJN0aezt6oK7ld7pRWoeD7jazKPQm87UDW0NRKdvp4mPXDmAC8/ujxG6+8WuTN1fX64ubiq89uAczdw8P91fNk9upmMb+6ut23ggUJ45RgrJSmIkSGpL1BkgwWqy6Mh1kWATP5prDGT8bJ4STTtaTh4LVvfhubohdCHEfL9TavlDFWe6i0tdb3woh7PB0mccZv9nVVamPtvqo94MksdVbmhTwa33/86B42enmxNlrFoudDMhzxSu3X5fzoaDYdjqP0kOMQBAbwgELomjiIpdZAIutJV5fWGkIJ9yUB/9XlZl90CPk4DWlEMSEU+fVmd3OzHs7Gr5y/fnv7PImi3kB0BTR1czjKDgaxbIuLZ19fXnx9dnZnfP+d7e2yyPdhGo4ffhuk/PijjwKKh70MYVTu92VVGWuzEJXbZb5Zza+vuZU//+CTTz768PPPv/j5+x/tN8v9dpkOpi+ePb98+tlP/+D3n3zx5adfPhXMC0qK7fJ2vu/qLuDUyOqLTz9t2+r0YOgVXF1d74vCWCylv7zdHByfgdXk3f/kb4JIAAjAFuAaQAHEAAB2D3gGoAAwAPkL15OCvl5fXqxvrlf7tlW+6VTXtEwg7a3qiFPSe88oyRJxNB2MpwMpYdxLZ6ePLQrWmy1C5OpiXRR1kknQHrcmjBlyNOABkpRZulqUAqMsTU8mg0EWXdyU3jmE8GZbXb1YcxM2hczC/pdPnv7ZB59hXW93+YvL9XInjSpl0xqrmQgwoE7r1199q27lF18+B+fSLANnVNcyAOIgJDQLWd2Zjz69WM9fnMyi5aa8vJojDCgmUlrlLGBkJASMds6nSfBivm5qax22ui2LUmtblzbgwTe/ewcH4Bgu925bFLu6HQzDuoEvP38+6kWzcYyA85BC8A7AAvbXQFMIODiSRPzq8nKzrznns4NpkqZ1Z1RdkKCfpoGzNo3CQS/e5XuEaRQHrTW7zU7rMoxEIJhzvly1435v0IviSKRxPBwNhQhPpjHiLh2PB/1eML0PUEFbp0niAE8O73jTJBFHVl1cLpQ2YcCUUhdXa++14GFe5ILjpm4AeU7RYpWv1murpfdwdbvu2prw4PRo6qwDSq6v1ov54sf/5A9apbTS61LGIQMs2rZJkljL9unTC+t8FEfkL791fn4agLwGUUFbgu6AdQCB3Vzg2AGMADQABXAACAAANt3yZVPtLq+uVuVu17TI8dnw8O7h4cnR0SAIjUXeo6NJ741HJzxgZd6WlXIkvpoXspOqq9L+0OG6rNf5bjvpZ2+/8XpTq/WmPJyMHt0bH83Gb3/re7uq3m/3d08Pq9ZIqYb9ZF90m9XmlXt33nrrTUDIegKISKUvr5da+yCMAqaM7hjxvZgBYED4jXvjbz0e3D8MArs9SPjtblW1JcU2ZIwwzBA5Px5po/uhYxQIWGMkSyZ1VRgnpXHGeaUt5ZjGwbqqvr5ddsop44yydW1Ua8tlt53LJAuQAOTNn/344vZq44kPsziOgtVi01TlIIsenD9g2mKHQRwBDCE4g+3XUM5h/EvaLJWtR+mo67T1sCtq64kyQDgDa421gAgXXFr54nY7vTtLksA6IwLeH6TlrsMtxCKtmy4MgjAIvPOU0rbTXdsSWQsqwTQQngF4wlkv68/uPORhjMB55sKApgJu5pswiqz1n3/14umLRdKflvtd1bTjYcY4z5KwVU4wQglymC7mSy7ComrrquYUQEvrSad0WXVxyHZFezAKxjFqlQ14fH09L4pdW9f79c3tzUvyX/xn//H/Sdib9Niypddha/fRnz7bm/fevO92r6l61ZAySakoybRoAjJFCjYgTWyP/AM88dgTTw3YgD3yxIYNTQwDpiFAgGyJlmmBtFlVrGI91qu6fZN95mmj3a0HJ+PWZZGwAonEOXnixImz97e/b31rrYicHP+aK19Q3SLJyqsLWTwBchpt4CqwBNj8IskBAOGZ40EtN83J4vTtyZv5zQV4k0fR8cFnBzs7nbFcJNPpsLOoGmMcZBTtTne8q3zbPHnyoBiON5uVM9o6P5DRVbValBvf+YCw3Oi3Z8s3b94vbuZSintHe0ryPM8ZwcnZVfCOclU33Xy+Xq/mum0RHIcNCKAsieS0iEcDJWVEhby3l/32954WGZ8ejT/98ni1MY2numklCYmKRoNskCedI4RnO3c+oYSYQOvOV2VljTPelo0um855T7nQAe3aNp0xxjnnKGW6ta4L1DPvwBhNUnb6dkWNSXJufPAgO4NDLph1drw3GeeDfPdTKAVQwAMKyT6wgD0z5dlgMhWB1FXLBTO6IyBZopSUnYFz7uJ6dXI2v5zXjTXj2Xi1KqM0r9bVxcnVUEZ7k93peDTJJAVL4ojScL1oEGwsSJFHQkbIC7AasGB36pvXYvgQHFwFqSTTmqtoOoy7puuMi6RI0zhSXPtwfTXnKhrncadN4KMoZkqI9ycXTEZM8MXV9e7B3qOjmWBkODsaT2az6ejLb33raH+ynF93bfeTr9+9ePny5OSkqRuhVKKYMy373d/5m8Iv3zx/6bQoRqnkEaICaEBpuDwlZK0v3rGwwvoFugu/fnv16kfr0/dvXj1bLddJOmmaMi1SlarY01jQtmvWq3lVLdZN2znSOa6i4s7BQZGw47t3794/LOv21fOXXaN1R7pKe+ud64gjAOk602nDmMgiOh4kWZ7fvbObJMnZ1coHQhAoQdPU69UmeEsoj5VM4kgIyiiNJImliJQaZNI6MBHNxurd6YWkdPzprwHlm1fXjhV5HFvdSqEYF+PJ8PjRZ11XWwNjdCCkadrgDOcseNSV9oI4H0BDvW44hOLSwQIkTRNvnGCMeAghqCOmsr61g8mgbJpy1WxWdTDh8uwySvnRnYlvmp1hBG+wvkazxOa9Wb5ktq7XIZnd59k3I452fek8iiIbjyeHh/tpGq9Xa0pJ2+m27TZlczVfv319Vq2qq7Prrm4Z44+eHO4dZdwSeDksokQywtSD4wejQiWxjKSgeYE4B3JgClQiz4AWaAAKWdBiJEZDVeSD4wcTyaTgR3f2mVDf+PLbXutIwgXqaMLVYL26QQhHe5ObxWq1XI+Gyb2jw2EqBnkikxSE7e/v5+P9fO/BJIuX86tqszBtOx5Eu5OM0DAbF8Z59r2/8bS8uSyKpCo3u8MBSTKwcPX1V1QHQS0iNb9YpplEsOXNzcX5+XyxnC/LVtthFqWSFowUKsqypLWEE74/GRZ5Xmu71l2WivnVtWs3PtjF4maxKrMktcZIFd05/mz36MH944eD8TCELo4UPCKl0iQdF/EXj/a/eHykYvn63XWrDRCqsjraGw3yZFPWnNIojmIlKSWRYEksOKXWWs6oM23dausAuKrctE39t3/n7yAa4uz56zdnb95f27bljKaJIqDDyUHTNF2ry/UVgmeCE3jBiRSCEEoJ851l1nsXlBAxqNZd2WpnHPHghPBAYiWVSpJISKGGw4kOpG6CitI0i2tdaWOGo2z/4DDlYuf+PwBZwFWwpFmeE29IcC/fvn728vmILXSjpZKj2d0QPKfeOpdFYjTIeaKGs8y2tjOubXXTGUp4MYomk/RgmD1+9Cgioa58W5ksjRjlQnCODt4qQbR11FjalXAbhBuQDagDBKBAI4ABY0CC7wAj5A/TvYfRNO5uliKbppHKU661pYxSEoaJfPTwzoPPv1uuNjc315yLyVCNB6lg0Fqbtrq5PrfO+7b++tmL6/kylX6UsScP9trOcpUMB3nbdvzzL3/j5OWPX7x4v7czev7yNB/Nd/JstjtCV3a15gGr+Xx2d4pgN1VJ4ENAlkhCmHH+cJJ88flRWdplZa7X1f70ePfRrwI4/AI/+JP/7cWzn86GqRT8ZtM2jbbeBHjt6kW9mCnStMvVfJ7IdDrbJ8wfP0iGcTFftXkaD4rYNgslHSHr5WI1nEwmIzIYFFLJxaoCoSAsTVTXaQJIQQJBqTVzRCWRJ1Q3dWDR6dvzL5/ewfAA9vSHP3q2XBnGcuI3nHDOXNe4q4sz3TbeGqUkFcxbm+dxsKHtdEoJQPI08s77YAUX1mOxWduFrUnwJOSRJIREiWSUBCJVlK3KxjnHOGeE08DzLK/LuaDkxdcv4yf3gFNUG78sKaVxkULr5apeLDYXVzdHg3yyVzQtqc6eJXE2GiVMMAIK23Yd3ZhOKrm3O3EK0bpyteWNh8D+8Z3F+TUZZAlRfMhNZ1hE26YsNwHeVHVzfbMxHruzcZGK569PkzT75P5+VXd3HtyDkkgS4DEQAyUQAAAR8GD3Gw+w+vmGxwd3Hnh2vthYq9uzy3Meq+kd8/mTY9ettG67znIZpQmNHAIVnY9fvviZdu70/fu67R4/eeBqf7WsuBAUtO26xbJk/873foX6alO2baNHxfDhg3u6XHEqMR7SpmGMVk3HmlZG6s3bS8WZ9TjanxweH7qume4ek52RbDfvr9dciHW1fPXqxdXNmeL05PwqTVNKfRRHTCQ3i9UoL2KJgGBoe3r53NhNYPr8/elivrRsJVhIOA9Wd13ng5uvjIrzopgMhhNChZIJ4dEwT9M0YYwPh8V0MmqNy5PoYGc0nYybkNi21lo754dFNhrE88Xi4f292YPPT3/wQ0HMuiZd16ZJKqTw2jDOgtVc8OlsL05jRhkhIBDOmvF44kGMtkoJKbjgIlaCC8UIzeJEUhpTNkoTKQTnPEoHsZRRnBqjTdda4+JU+WC8pYIJEdE7B3ufH+7HXbU5PzOgbdPZzmht5vN5U9fzxcYa5015c3N9dXk937R7k3w9n2+x9tXVVbtptdZSJZM8YibMhsU4z1IVUe+JMTuDYaxYJBhC6NrG6A5ewztCSL3ZXFxcn13cpLE8Pz1fb1ZV0+YRPX9/cn16prRVcgEsUF3DbyAANFtCFNEkmx4xbjmj97/xW6kIQqqua4PuZg+O733x+MHeJM8HWcTT3QFzpDFhsntACHv55vwvfvZqU5U383UcK0qotc4FRoG6adk//kf/vi4Xu/tHv//7v7/7xW9ePv/RYFwgG6MsiaJe6yiOk/EAs50dRQdFPEiT5OgAbV0ubgQNQqBcrIfj6fXlfDCeELsO7erN2xex5Dwqnv38pz5Q64gQkpLQtsYRU63X61XTuU5wPikySXjEC9t2dd0ul+W04M7qpq2d3uSRJ7BNvSFeZ4kkMjOeRRxRmtcdTZP8wd2Dg88eDvPi/qOHu1nMVfbJwyeTQfbgwfHb9+emk8ff/D1VPb++uVpV1FoEAM4GBAIEUDAuhBKcyigmhFISCBOTnTuddmXZCupHg9jZQBj13lFC8jyfDPJhFiupGOcBYrZ3987B5Pp6IQSNo9havdk0sPCdpkwEa/eG6fH+Ybq7E1HPuKCMzK+uu66ZjrI8i+/tT6VkaZ7nw/33795dnJ1rrYdZ5HRbNU2SD+4f39WtOTk5S6NEMCqlGg2yaa5A+KP7u5ILyen55bzTrq2r1oXZbETBCKV5oqwxl9drbezudOhBu87KKJoN0zRRy3WVUrBgYC2iFLwAml6GygBADFVxACBKWRHHsRKxoMvz96xZi/Ge4qkUjBBuLI0TRbO83TSdFw6s0269WiVxtLczoYQZMBXHbdPxTz+59/k//G0kd4FTmJc7dycYjEEVIgKE0FxFjIAzIODwPuAkBE5fwLn9p1+gW/nFtZTporZKZlk8cdXS8Ky5eF1XjbPn+9NpEieEUc4ni+vzSHQL64WXhUhrXbmbYCXbG+bOhfnGzu7Ey6YMgW6qhlIWRZljcVOXo0HmrKmq5d5ELapyMsm+fvGubbu9nUmzrkclhwiI7hSPP/lsf4nKgCfIdzgDBQUg42RTm/EgLxtr2g6UCBFzJaqqLgZZCKypSx9Ckg9VHOmuXly8gHVFxlIlVSSNCcY6cBLHkZBpCIER/dmD/Ztl8/zd9Xp9mUWzJBb5cDctRm/evHr36q23njEiWEhEtpMXk9kQcQracZLwprqTZNA1CElI8BYzxetNs67rp4/uRpzUdbOzM0QcITBwDpV+I8043HxTlc477ycHE91UrbFMKGdMZY3RlnJIFW9W1XrVllU9GaQe9NGDoygtOOdRJOPcCYpVWW4iHit5fn4VxWo/kYgHiD4BEsDA/hh8S8JnQHHLyW+ulKLq7j5Uwd+fvH//YuovOkOdaRVzcZo4xxMnitnRw2jSdrapNtNJKjkB6O5s0rLR+/evpZLsv/nv/geIMfDCvn9mV0s23IG1EAkYh+6o6ZDuYDgEBsAWP6bIBZIIDLDh4mK5rto//vEbQtTTX/l7o4PPb87fZVG8XC4mo9wYe+few5tVJaVkvs1SOb8qp4PUeBBDR9kkiuLluhtmcRxLwWlZ6bPL1cHuKFGsavSm8fsH94yuGm2zAbn/6C41Yb4sOQ2MYl02uaKu7Vari3xvDxhBJcjGSBjm16/fvHKVfvjdL+HJv/6jn3noSMVMRuPZbpalzjnKyM50L0tV29Z5XhhttDGEhCKLjAsu0MEgjRW31lnrQChABoNimNA8ix98cnx0/8mqXM8G6eX1qmmtNe56XparFXF6MMyzNM2zXAhxZ2+aKBELgjgBc5ASAZAcioMRU1vKY1C5KTfe+TxNxpMRywdQEdIESQo1Betme9PdPHHWUcakjKzW14vSOdd0zgd4IqmIGeWRlDKSdw92pOBFlhbT4d4oL2tdDPK9nYkQLIpkpFSRRZeXCxuQRgkDpfkOcAp/CXgQQJcwS33+zKzfnzz76uLqxjXN4vK8vr6Sgu7v7sRpJpiQUSyEACFJlJHxHZ7cSVK/WS6++53v7I5VkWfO073DO2meT0dZWZUc1fcBg/WqqRrrZJqffAAAIABJREFUfPP23eDJ7wIAzhEPEaeAAGIgATZmNRf5ADSHkM3LZ+uyhHX7+w9+JRoTT+bvfjI++uLJd74LyNGf/1+T3aOmrlsTiNVd2VmrLzdtnsRxLAfG5VIxJj2w0C2h+d3dQZZESqqTsxtjw/HhNB1MXr07M/XNoMhM146zXdiIJ4OHj74FJXDx0raW393Hav3qq59BjyB3eqXfBndqjIW3gMTwwXAw+8GrpWDt3kgOZ0W9viyGvG1ZZ8NsMkgV5UKenl+Vdec8aTVABKNdlMaTVG02LWXWOzBK2qZ8+uTwky8eIcT/9x99v6maYZHu70ymk/Gf/vDr89Mrxf2D411OZRwLpZL9o4ODoSwiguBgLRggBSKGpkIaQURyYoBCIr2T/BxNXVYNZQqdgydwFkognmL5AoNcHex/Y3eGqgNlKAZYL8vFyludJLFudaldkcZRniJQMOj1qq5bU1ZNY/Iii2NFCZmOBz6MuGK27R4/eVA3uu3sxfW7YW0mDz8Fpbi8AOdoWufY6ekFTyaD8e7q1ddGMUoCI8F05dq01gOEt10H+CzN1mXN2+eUC0LC04f3RD7anajl9U3T2tmTbwKAb5eLFQcIpMT+nXw3gMQgs56PHQIGkMAKAFADtdAtNh4Rx2Ie70/jMEMyAJ7ePQCA1bsfAADGAA4fPrp+fzK9/3hxcR3L0DW6al2W5FkxLlcXk/FAEBSTo2c//+lkNPAhgLD7R7t3j/b+tQ+cc6nk1fU8Foxy7sG/eHysjo4gvsinADZwG2Q539sHJEY7x39rD8vXi3fPuq6hwM69EclyQlhrOrz8IRCkWF9fvGPRRCT7ainG2X6nVz7oYO2daTrcP8BmfTAb/Oirn1uHu3fvvju5jNtQl0272XBGGGOcUVBwyk8vV+Pzxby8SfPR/tHjy8v3fn359uSKQOiuDl4c7O6E4BNBJpPR4Z3RdKcAc6AcxCMArUbVwXWoHIYFwAEDzDCNMP9z3pnzq4W2nlGaZVEkVRLfWBvak6ssGxAREAApoXYwTbLZN+DewnW8M4k2aJ2p22Vlx4O0agwFCcEnSSyijFDivQMhfDaF5Ny06YkPQahYHU926XQH2AdqhJewDoSz6fAgkOWmsvXl/u6EM268m9/MW2PzPJNSOeequi6KARB0V19dV11nVKQooZS+SdNECtV2zelffDUoMsr4aDBg//l/8V+CbeXLADIAGPRLMAsMAAGYrbEYyIEZ0jGiBLxD9i0ICvEU2Plg3ogG+x8eQyDhEqZ+8/wnO7OZdU5wWUwOxjv3Vjfvm7phjK3Wm9W63J1kxgXJaKC8LJvRZNK0ZlU2cSxHRaKSIgQM8gTDo97HokABWXy0AO4gknE+yMa76e4eZAa1e/76q/dvTxer6od/8bP3F+eUtIub66vr+cnZ9fXKUD6Yjoq/+/f/XrT7HUQzFGMBaq0XPEzHeVWtwVWqxN5s6H2oO8OETGMZKbmu2rPLxWq5nk1zawyDPr2s1uv2i0/Sl2/PA+hgMJyN8+M742GRFKMZn06hYgQLlcIFcAqp4CwYg5IA4BqQBYjGasGFLLJ4OMiTVOVpJrN8tVhsF+GqrFfzheKBMQLlwJ4CEeguWAlvQBmkZFmWFgXNiniURVmcSimESCa7igLwXApwAsahxhzGGZ3mA+sCSyKwBtggk/AUlJnFuu00I+CCO+eN87tHDxFsmkZKSsbAgChWktG0SAkgBa2rMgBxLF0gddUY573TxrQ+mM16aZznQHbbYpANcIFwDjkBDnr7hgEiwPXAkAAS2ACu9zZttzlg0JVwHZJdc/5STMfauHK9un+0J6Ps8M5xrcNPfvz9m/eLLC9qKnisqKkff3Jnd5xfzDfjIssnx769uJivq8YMMrlclVGcmbrb/eK77btn7fOvhw8PgAVQARIQwA4Q9WaTQwgAl4AARgC+ePrp3mzv2fPn//Rfff83/q3v/Gf/6X8MFZ396E+fnaz+jz96/u7E/9u//j0IAywBCeyy2e6j2beAN8uv/nQ2HV8vqyRJqVQPH8529pumbrXuhJR5lg2Gw1GRtl17s9ic1pngV9OREioOoLPJ4GBvcvzg+N6Dg9PXL6LD3wAAvIBQoClYgIhgLdIMnAN3gBjsGjDoLpGmMB2kIpRLycFjdGYYcbQaRZoDaBp4C8nAPhi0HOAQZ6hb6BaUIJ8AgA2QAowL7eEqsCCHOZyDlBAFMMC4zcefAY28fo7mBrwFHcJYWIe2a9oGPnCpApjuNp4l8/lyU26yNI4E2WzaxXwVhNzf3+261jnnnWWMB/jNekMAT5hSfDIdcUbjNKFMvH/3fnsfl1MgBxQwBsmBCUBuvXgAQIECEEAFXMEv0GoQAx+weovYY/0yXJ8SqkE54l3MXzIRICWLkziPOKftZiX2jkV6l7s1TPnp599e13XoyuPj4+Bda8jx8YM0leeXF4RKUHXv3uHOZBBJdnq+oEwOUfNYRolEzGBXWJ7Yq9PV+2fxuADNAQEA0Lc9yu0FCst4mk3u/u3H33ocquUf/vFX33z8cLj3rXxv8vb11dXCPD0e/o3f+r3eh0L7gwAYRrmG9pNRpq2va723v+udm05mnUVdN0xmq01nXGiNXW66x48+3R3LPFMH+9MvP/vku994eP9oT0oZC5bGkmQ54AACugsoMAPMQFPwBqYFZ9tLSwAF7qEKxBFkBjEGTQEC/gByD8khmALbh7qDyEAMQIa38pF/CTIDDiHaWwMXAEpAHMChZogTOAslkcYQAoSCJYABPKABDUaQHsBTkBKX8/nFfF1umrrrjBdSSEaiSBZFaruKEVDqu7r++ueviIx3Z+P/9wdfbao2TZQQnHEhBeecDYtEcJYlsZA8LQpCKLy9uLjiQA1Q4AYYwF+ADoEKoEACxEAALMB7KT0FPUU8RHMGHmE0BgiKHaI4QKEEsECk4DpwCd9B5pCIi0+ADDjbfXDIfC2w+WQv52Icp/nO48/RlOCqvXq/Ox7nD78EpsA1sIm6zejTHIiAArgAONorRBnGMz6WI3gED1wBU0D0XpIPWwyMAQ+MfvM3f+OPf3T2/Pnbe1+uf/QnX/3hH/35OGO//x/8A0ADDhgCLdD9wuYaPx09mWF5Nl+f1M3mz37yJtjq+GivaVpj3NXFqfeoV1wHMR4maU5sE70/03lePHj8AF3ZaL2uCPKcigIgt4MGAJfwHrQCIuAOVAk0gN5mX2BrOB0ALRADLZABFlgCHBgCACrgGEAvU7agCTAFAnAfagkYAMAeyHY8LMCR3wXOAAMmgRgYfJQLGRSAFiwCSuzL8f4eEF7/yT9/9e7k6HAvi5UnGBLe6a4pq7enF3mSDIf55WJtjTFtvVlincdyNuGcAhyhNQ6j8SBOYnAGQk3diVyORwUJIeCXN9N7ztCniq3hNgAeeA8oIAI0kAMEiIAOUEAHBCACLvprDkI/ixxgwE0/tR0AdCuo+KPa1wEZkAIdQIAWEIDtxz0AHOB9lrV9oGxB5La+k36HrW0uwDZ/+M9/cnm9+Ye/9enp9eZ/+Wffn46K//A/+Y8AAyz6CWaAB0yPBCKgBhp0HbQ2y40PAGCtc8EZAxKM925QZMF7HyAYfXt2NR4NucykoFfn78HkwdPPIAC6HahJP5IW5jmEAhigAQIIBAOSAhYwsBYg4DvABpD9eNJbJ71rwMZAAlwhaACoa6SfAgBOgBGQfDQRClgBEtCABRogBoYA+et80dvxvOl30Lh+XpXl+zevLpdlXbebTTWdDk3bqCj+5NHjd2/exTHTdX023xwd7mbFoCgyH2Qs2Mn5+Ww2VCmzjknKvPWDYV5V7V977cmHIrI9uW1JqoEacEAKaGCxZRD6mU76r6SAGyAAVz3LQPrYlf2e4XY9qS0h54AWoIC8nWDY/uDbYlD1w53cIhJYYNi3BVeA7E2/AQh96APoXv74+fuTxT/+R7/L8+Fd8ezXPj94/Mke0AAboAE8MOjXxjaOHWAABygoBVWJfLqdBgWPtgIYZADh8BbOwcmwXFwvyq7pQK6cc+Vm89l3fh3qCPoVJEN7gygHJFACVwgWrUEUIzh4B+ZBtnk0APfBzwECbKAXIATiw/UZDOjAJDAHbmAagEIUSA+B58AMIP1a3Y5VBXhg2f+x6SfougcJvE9+NcAA3n/9y1saazpKJ8MnCk+y0fzk7cnpedt16ezQdI7HhZBcSHFyekE5i+Ok2mzOzi4iQdebujN+s1mlWWatYYQPhoWQ0mhDQngNJIC9xWcAsOyftv3QE8D16QT9ZJN+SrbDQT4KuwZI+4hJ+p237qutZdL32Y71gUj7Q3UfpS7ftx3blJP2Z9ICw95KftEfahvKDAiABlp32j57+fZq1X3v7/9ev3JeAxRQgASq/rS3H0f6aJ4Ci/5TticWA2sA6Eo4B2NhDHywdfnqdBHHygV1eHiHT8ZoG0gOeQgI4BkQAHmbqLxFCBARKLv9akFDG1ACsc3oCrjqpzwgOBB2m56DA0n75coQWhAGZ8G2BZL1wwI4jcBBPNgAdgnO4R0CwHjfw7nb+qAbcAoqb98IAQj4FlT0u5FfTIdeYzl3Llwvm+lsP4T2/Gx+cbOxZqWb8uXrax/c/Tt7eZGx4LRxHmQ4KmaTMaV8VbUhBBLCK0ABoedjtzVrO+iuvwy6t5TcdgPoJ0D3yY/2T7dB4/sSJvrsst2zAwTgAQsEIAWq2+QB318RUwEW6PolqIC6L6NRD1aqfuHqvvCRHmP19ejy5X//T/73X/niwWefHm+qjuSf5HtH8D8H3WKmGpCA70sG7X9U3/eUgAIyYHl7QCxvpxkGvgNlaFtwBq7MyUYcPp2/+LNRJsnudxCeIbSg23WSA7aPFQowOA2WAhb1CusKwwEIB+GQHF0JDwgFfh84BaZADLwHcqDscV7o14CHt6ACyIEG1RycwWp0BhTgAoSAczCGwBA0nEcIEAKUg0m4DkwhBAQDayAjWAtCYC0QwBV0C+/RdHA+BOscofDX84VKsjRNjSFn5+eEOEbcarlZbTaEyvlyNZ0M00iKONvd3RkfHaFrALpZlLyHR9s1nQAZUH2Euj6UPNpHvemDSfZKFPvLHMcHPNf1uEoCa8ABEVD2OdIBJaD7BCn6Swg1MO7fK4A54Pvj2z6TtYD9KC+WQIAz/frmgIOMquqqswfk4JPCLGA6YAP64UYV/8ZN9Q+2GBxe0xAcIQACgqcUiNLtty7d1yNEX/34z4pUfPnbT0EegaBHpeQWPpIVYOEqsBwYA2skAskEmPZ1Yw0iEI8ADlxhuUSkIVLoFtKD7QAGbgVGgBwYADFodwtDYZEOAQ5FIW7QtIhz6AbGwgfEA+gKvoWzCARdCUbgKXgF3UFFCB5NC+du4QrhiAWaGiFs5qs0TWhW8Hyne/PVzu4OAqs3S0/4MKFRmnRNyzmbzabFaLpeXlNChMrevHn76s37TdXc++bvAC0rv942klFf1M5uubRf8BqiT1Tb1eluscLtdBKg/qiesv731mTC+2K66DPcpp+87Bb53tY70hepbSxWfXYhPVBTPQFhgRd94rG3ibAtwSgIRTlHGsO0AEM2+PZ3vxMP94AdiJ1fYM6/ZrO6M52u1+sqBB98AIgLjgRyenZeN00SJVXTNFVNGDHGWmsAojvrvHfOW+v3C/bv3X1qHTu5WH65usTg7snJ1Wg8SmLWh6y6HdgPi/G23dm2MttGYQA5v82yocRwD4jgl9AdqiXiDl2NrsNsD+Yc1kDEEBJMAAHGo2uRpYADU5AUbAQO+BqBoLqC0QhAFEMJWA2tQRlqBwYIAdOhXINTBAJrISQGE9QA4/lwAHh0G5hGSQZnAR/HKoQQRyNWDJJqlbadp1zFEcUweAMun372MJodVO/fAYApL6+uOEwJEfqJR298iz4CZ76H2KTv6bZMR9vjbtM/3SZ22oO5beGXfQNo+gKqYW/Aj/vEuYW39vYEQglrUNaIIqgOlMM70Abegw4BYH4FQsAktDWNEYmCM5AChIMRBEAebIHmr/+7x381pLwzzm/9QY5zzkVsdCeVMiYIQQO4szbLsrpuqqpx3ltjK19bG6I4arsmhOBcCN51xgQXWt0Zba5NAHB0/OmLt2+b+SJWyR/8wT8NoHVdWmMiyeM0m0wnu7s7u7t7+/u7eRZ/FH8fthbo0F2jK5EMoJdIDgGgGGIdEBx4BJWhruAdogjBY3GNOIZ32JQQsr2+iPICWQytodZwHbzvayhFCAgB5Qa6BaFg5HZiobCegwCg8D4EQozB9dntPKsIXQUuEQKkhJTwntSWpDE6A2u8c6eX5drgs/siigUMINRi7f7l//Q/Pv306XH+g7OTk/ViyWEMhAXWgARCnyd0n7ravs//ANLRd2ehh1bLvpKe9XybAwx8ACVABFfDe8DBzdF18A6egG3AE7AWUsAacI6mAggohQciDsHgDRBAKQLgAugMAMY76E6gjgEIvwLdamIGzTUYBY176eKvhJgxXAjKGCFdWXfOOKUoFxAyBeA9cS5Y21FCNutN23Vt20rOjRKEMGOMdY4xHgKx1rkAhOC8JyCEkNp4+NXD7/6th09OkEVAMciLqjPCmO88nT55/PD5s2cv3744f/ti3VrvAuMsS7ODw8MvvvjsyeMH/QlGwD7UDsgLUCCJAQ1do+3AKXyH2mLvMeYvwBmaCghIM7QlogRFCiCiCdIYhKCpQQl0h0jAatAAwhHFoBybG0QJAmAtmPBtSasFohghQDIER5jAeg3ad9+6Ajx0Bx8gGJxHFN1WD+9AHS3y+0yuVkuuKBiFlKirlLSff/oJGHRTLZfrs8slB9lWqK7PQLJvNxzQAeYXyBoMKOFa+ACR3XYidQnOIDVg0dZ92hMwDQiBUhAEjIEJ+A6MIopvd3EeTAIRQgulAI5M9ChtW6kHQAEE4AbtAoxi/VPICaIdiCnMBiI/eXXivD84OOLpAPGtuuq0ZlL+1Thj7LZHIYQwisCIc/7Dq0Iq1nbeh0iJqu6cC1rbpjXWBimIDxBcAIFS17Y2BDAmfLCc0AAGb8K6JsPB6auXWZ4V978ZS3KzaqqqXt5016+XOe2e7vuzTbx8bUMI1rrlYr5ar37+9ddxknz5rS//7t/5mx9OE3ILIk/hl6AUeQGjQQKgcfGzYDQZTxA0jEZbgjN4h7rBcABC0ZUQCsMhqAcTt/XRGBAHeAQHJcEirG9gLCihSYQsQWOx9TxKDt1CKRgLAhiLSEAoUIYQ4B0IBQWcR3BgHFLBaeTxIJaQElaDEMz2JQl39/fhLLru+N7+dFxwqATI4TtQe9vcmQpwcAFtA6kQAjwAA+PAGNoWUQRp4CwIQAIchV6BSUQJ2g2iIUDQVkgScAGvQXPAg6rbykgigICF26K83kAbJDF4DMbBJFZzSIUk6S98zxDv3lbg5gLuEraFMTDLw/tH/88f/wgi26WRihWArmn/1//5n8x297/93V8dTj4QpABAaA8iCUHoqqqmRGT57T0mOGMhQElhXdDaWOcA6kNgjDmHAEIIAbh1wTs4F5wPzsE5FwIB4RfX873h/h/8ix/cPxz8zv0vpsPs7cXSO395XR+ouTEdj4brijPGrPPBh4BAfSCCBO9fv3x5/uSTvf2/dBcmuBbVBsEjzRGl8BZcglDiIwSPvEDXwmi4AN0gimAtKEGagivoDh7gEZwDoTD6FpZZA6NBNJxFpOA9YgVrISlYjK5F3cIap70LQcYecPAUJiBSsBaUgXh4C++gIjgL7+AcpIAksB04QBicRiCgDISDiSjNgUsezt6Q4RDewBqoFJzCORgDEDAGp5EVILwH9RoD3veYpM+C9rbbh0OUARRmg0EGogAHIoAWIFitkBZgDGQrdTu4C3gPxyFiiBTy7i0WTBkI67HLXwbw24BjFuYKyT6An3799R/9q3/JGbMBVd2REGajfDm//vlP/4ILnhSj4/vH3/jyyzT/+J4lNEmLJP1L5ZWLeDiwm7IOXjNGM5VSQqxNtbF13ThjO8BZGG09PAhRMvahdS6E4ELA6cm7vYefD8eT+boBxNGd/Z+8vKZ0rb3wRAphuUrLFpQxDs8VGw7S/b39O0cHnz39TMYxfnkrsb6EB0jAzRW4ggBA4ANAUWsggHIgwGoUAxiLKILzqCtwjU4jKxAcuIAPsBahBqPwHgASBpFCd9gmeO/RVQi0l0FHzBmmDYIDBJgHoWhbAGAEPsAHxDFCAPGoNwCBsWAMzi1PlsPpLkIFztE0kBEYQxQzCk6KHGnR82f2lo6Kt2yegV2DxD1WUz2FkQBNz6tticQapE91cBCqP5qALWEcKMVgBghUc7c4Z3cCMACbgRUYm/7WSLjt0sXkr4z7L20c2W2VDAjOGgDW265pGIOQE2ssYaSp29Ozr198/dX/+S/+mRBxFKnxdDLbOTi6d288nownU8r+kiqqolxFv3wLHWftcrVcLzd1U3ed9j4Yo30gxtjlYt60mlKutb1ebADc2x//8KuX7dXLg/3Zdz8/cG3y/PXp+frm2188ufPJrz753nE+HP8bvll1ARjQDiKHqdDUcBq6AaMQAkKiKUE5Ni2sDR4kiVBuIDnoGPQQ4hLtOeDQrMAVvINgyFJ0HdoOjEMKdB2sxdbfs/07AQRB00BKuBrbf9TDGSgFp/AeUXRr99AG1sM5wIMwUHsbZKCgZDiI4SpQAhtACIyFFGgr3WkS3M9B015N5706ZnpSre2VSt3HgekFpS1xtc1kqn+J9m3EhwmLeq5ry7humVv116D17gIq7YmVX36tT2++p2BuRbr/9r/+r26uLnwg1mqtrWD86OgwiZRxviqrm9WSeickF0IxYiMlOxcoWN22jBJKSJINCCH5YJQPxpPJaLazu7s7i6JURf9/RMhft9me3DGwDXjuFi9ZzLrKNtoO92cfqZy3mykXXV3FWcoYA2sB0i42NBhZZJAEZgPdIBYIgLcIFPAwLZoWKkew6Bp4h634KgQIg0hBPOo1EEAoCIXkCID3YAQhwAcQwLrb5jEEaA2hYDrEEaAQNESEpoKgCEDdgBBICe+gLQQDYaBAWgAedQspoFt4wGjEEQjgA5gAE2g2pupEHAfrLRiHMVARkAEUuAYkwHtWbEtq1H2Dib5LWPatw1bhVj3vRXvGfNs0jAALbADfWz/GPZfRfTQxAdgANUgLr0HtB2oUQK+Ib08j6eP4gyxrjdYA0doYa7112yvMEAIhhHJeZKnudIADYB06Y60NlFPOqOCh68xmtWyb6uryzIMa60iAUrJuGsYoZ6BUcM6jKAnwBDSOI6UiLmUcSUrocDCMEskJYRRRJAEw6p0LdRcorKuu5stVlI2EitnXL8DYqBiaZkEoIeBRsYPQKk6Dy5NswFLAc0YJR4CIQTnYHIkEJSDqljnSNaIEUsJ6BAIWQWtwBc5hWligngMBnN+KV5xBCDQ1ZAxvAAIZI3igQ1NDSXjfbjZKaRJJUIY4hSYwBsUQ5RpthRCCDU5r76yxQUou4hgBqDcwFoTackMoZVKAC3gCa0CAunPeGesFZ8EaErzRNYc6AKKP1GvZc6rtRzR900dY2cec77vCKaCAsmf8h0AAGsABNwDvaZGtUr4EUoD2CtIcSPvGVkPeBypgA1wArudpNWARCAhHOEXgoAwg8BqE6rMrb2tGCeek6xzgBOeUUGM1CaS11hvLOaNUCsG9F855EEdArScwsJ4IRgJhAAkeAChlW8AfEEIg1lnnfLCO8RBAiO90VxGERnHGhOmaQZ7EMeCclqIzQTBvDEwIzgRBuqa1o52kM9ZTQDsK6hEICINHcF3XBSeUcjGIqwlTSqQMQcN7MA8u+vuCbYWTAXgLOgAslIetwQVAYA34FFhDN3AKKt7ewwZNia5F3UvD1iGKEaewHWzTtVoRgoAoyxFxMIE4gm2QjrA8A6VIYngLSojWXBBQJSHAGLoOlIFQUApCOSPOWtvYrjOBsOCdVEKpiBEwSlttFJPaudWq5L1vpO7TxhwAoIAcWPXEWNK7arccW9ZLBU3PliV9YW16+ZL0sZL2PBz6j4h7XjfrD7i15Vx9RPB+0Bg0EIEoYAEi+x5iKwBDxkuEoJ11NjjvvQtCIk4yAtu0LQkIwQYbOg/dEspAqOg6w0UAoUxIRQ0AqSKAhECIt4IyRqGkBGUBIN4TBJAQwDkjnItAWAgugIFyRhnjlBKAU2O9tUFwEgj1nnTOgNLBcECp8AQ00EiqOE0D9YxT4olUihDOhRRRCjDGpDVBN6WinsUSXCNY0K2UHAFDoAH9oG8OwOWtFswDUCJYyBiBAwyEAxmSGHF5y0Q4gFQgBO0agmFyoKIYxgABXMB7BILV2la1MedxomBvoDvsPwK5i82fQTLoFs5BcDQdnEUkwDm0AeEsTxEcZQaA7jqjjbfOOGMtBqORbmuhlOSEw5egO33xorceFbcGy/twMf18b+Xt6KObonGg+0g/2f6F9g6+BADCAmTUC6N1j9UaQPXYXwG6L6zbD/J9WKv+gQXGfZNLgApYAwGCeB+sttq6LfwwxjVNEydxkmSUti2xRhtrrCOBB0Z5cL5zrQUhzlmjW4KtuKyY4LCBcsI5B2FCKsaINZaAEOKkihklnDHvvQeiOEmSSAoWwAJRgPOw1htKWJLEMXjwa0Z8UQyETCjzjJEkSSglUZQTSrq2a+rKW+tc3HGQ0HIuuIyDd44w5oGgYQ1k00ORrBdOTJ/m0/6lBFiDKCBGWIASQMOdg+Ug4rZDJB5F0XulJOCQTntgDfgOhMF0fHqXhw7WwjncXGBxjoHDen5LalgHm0CKUJauqbmU1njvXbMuB3kWvGUyiihMR</t>
   </si>
   <si>
     <t>Tanmay Maheshwari</t>
@@ -759,7 +879,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1115,9 +1235,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
@@ -1168,10 +1293,10 @@
         <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="H2" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I2" s="2">
         <v>45575</v>
@@ -1194,10 +1319,10 @@
         <v>219</v>
       </c>
       <c r="G3" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I3" s="2">
         <v>45575</v>
@@ -1220,10 +1345,10 @@
         <v>219</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H4" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I4" s="2">
         <v>45575</v>
@@ -1246,10 +1371,10 @@
         <v>219</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H5" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I5" s="2">
         <v>45575</v>
@@ -1272,10 +1397,10 @@
         <v>219</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H6" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I6" s="2">
         <v>45575</v>
@@ -1298,10 +1423,10 @@
         <v>219</v>
       </c>
       <c r="G7" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H7" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="I7" s="2">
         <v>45575</v>
@@ -1324,10 +1449,10 @@
         <v>219</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H8" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="I8" s="2">
         <v>45575</v>
@@ -1350,10 +1475,10 @@
         <v>219</v>
       </c>
       <c r="G9" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H9" t="s">
-        <v>234</v>
+        <v>274</v>
       </c>
       <c r="I9" s="2">
         <v>45575</v>
@@ -1375,8 +1500,11 @@
       <c r="D10" t="s">
         <v>220</v>
       </c>
+      <c r="E10" t="s">
+        <v>222</v>
+      </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="I10" s="2">
         <v>45575</v>
@@ -1395,8 +1523,11 @@
       <c r="D11" t="s">
         <v>220</v>
       </c>
+      <c r="E11" t="s">
+        <v>223</v>
+      </c>
       <c r="G11" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="I11" s="2">
         <v>45575</v>
@@ -1415,8 +1546,11 @@
       <c r="D12" t="s">
         <v>220</v>
       </c>
+      <c r="E12" t="s">
+        <v>224</v>
+      </c>
       <c r="G12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="I12" s="2">
         <v>45575</v>
@@ -1435,8 +1569,11 @@
       <c r="D13" t="s">
         <v>220</v>
       </c>
+      <c r="E13" t="s">
+        <v>225</v>
+      </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="I13" s="2">
         <v>45575</v>
@@ -1455,8 +1592,11 @@
       <c r="D14" t="s">
         <v>220</v>
       </c>
+      <c r="E14" t="s">
+        <v>226</v>
+      </c>
       <c r="G14" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="I14" s="2">
         <v>45575</v>
@@ -1475,8 +1615,11 @@
       <c r="D15" t="s">
         <v>220</v>
       </c>
+      <c r="E15" t="s">
+        <v>227</v>
+      </c>
       <c r="G15" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="I15" s="2">
         <v>45575</v>
@@ -1496,10 +1639,10 @@
         <v>220</v>
       </c>
       <c r="G16" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H16" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I16" s="2">
         <v>45575</v>
@@ -1522,10 +1665,10 @@
         <v>220</v>
       </c>
       <c r="G17" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H17" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="I17" s="2">
         <v>45575</v>
@@ -1548,10 +1691,10 @@
         <v>220</v>
       </c>
       <c r="G18" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H18" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I18" s="2">
         <v>45575</v>
@@ -1574,10 +1717,10 @@
         <v>220</v>
       </c>
       <c r="G19" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H19" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I19" s="2">
         <v>45575</v>
@@ -1600,10 +1743,10 @@
         <v>220</v>
       </c>
       <c r="G20" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H20" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="I20" s="2">
         <v>45575</v>
@@ -1626,10 +1769,10 @@
         <v>220</v>
       </c>
       <c r="G21" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H21" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="I21" s="2">
         <v>45575</v>
@@ -1652,10 +1795,10 @@
         <v>220</v>
       </c>
       <c r="G22" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H22" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I22" s="2">
         <v>45575</v>
@@ -1678,10 +1821,10 @@
         <v>220</v>
       </c>
       <c r="G23" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H23" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I23" s="2">
         <v>45575</v>
@@ -1704,10 +1847,10 @@
         <v>221</v>
       </c>
       <c r="G24" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="H24" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I24" s="2">
         <v>45575</v>
@@ -1730,10 +1873,10 @@
         <v>221</v>
       </c>
       <c r="G25" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="H25" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I25" s="2">
         <v>45575</v>
@@ -1756,10 +1899,10 @@
         <v>221</v>
       </c>
       <c r="G26" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H26" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I26" s="2">
         <v>45575</v>
@@ -1782,10 +1925,10 @@
         <v>221</v>
       </c>
       <c r="G27" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H27" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="I27" s="2">
         <v>45575</v>
@@ -1808,10 +1951,10 @@
         <v>220</v>
       </c>
       <c r="G28" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H28" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="I28" s="2">
         <v>45575</v>
@@ -1834,10 +1977,10 @@
         <v>220</v>
       </c>
       <c r="G29" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H29" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="I29" s="2">
         <v>45575</v>
@@ -1859,11 +2002,14 @@
       <c r="D30" t="s">
         <v>220</v>
       </c>
+      <c r="E30" t="s">
+        <v>228</v>
+      </c>
       <c r="G30" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H30" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="I30" s="2">
         <v>45575</v>
@@ -1885,11 +2031,14 @@
       <c r="D31" t="s">
         <v>220</v>
       </c>
+      <c r="E31" t="s">
+        <v>229</v>
+      </c>
       <c r="G31" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H31" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I31" s="2">
         <v>45575</v>
@@ -1912,10 +2061,10 @@
         <v>220</v>
       </c>
       <c r="G32" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H32" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="I32" s="2">
         <v>45575</v>
@@ -1938,10 +2087,10 @@
         <v>220</v>
       </c>
       <c r="G33" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H33" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I33" s="2">
         <v>45575</v>
@@ -1964,10 +2113,10 @@
         <v>220</v>
       </c>
       <c r="G34" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H34" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I34" s="2">
         <v>45575</v>
@@ -1990,10 +2139,10 @@
         <v>220</v>
       </c>
       <c r="G35" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H35" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="I35" s="2">
         <v>45575</v>
@@ -2016,10 +2165,10 @@
         <v>220</v>
       </c>
       <c r="G36" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H36" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I36" s="2">
         <v>45575</v>
@@ -2042,10 +2191,10 @@
         <v>220</v>
       </c>
       <c r="G37" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H37" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I37" s="2">
         <v>45575</v>
@@ -2068,10 +2217,10 @@
         <v>220</v>
       </c>
       <c r="G38" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H38" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I38" s="2">
         <v>45575</v>
@@ -2094,10 +2243,10 @@
         <v>220</v>
       </c>
       <c r="G39" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H39" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I39" s="2">
         <v>45575</v>
@@ -2120,10 +2269,10 @@
         <v>220</v>
       </c>
       <c r="G40" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H40" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I40" s="2">
         <v>45575</v>
@@ -2146,7 +2295,7 @@
         <v>219</v>
       </c>
       <c r="G41" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="I41" s="2">
         <v>45575</v>
@@ -2169,10 +2318,10 @@
         <v>220</v>
       </c>
       <c r="G42" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H42" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I42" s="2">
         <v>45575</v>
@@ -2195,10 +2344,10 @@
         <v>220</v>
       </c>
       <c r="G43" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H43" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I43" s="2">
         <v>45575</v>
@@ -2221,10 +2370,10 @@
         <v>220</v>
       </c>
       <c r="G44" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H44" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="I44" s="2">
         <v>45575</v>
@@ -2247,10 +2396,10 @@
         <v>220</v>
       </c>
       <c r="G45" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H45" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I45" s="2">
         <v>45575</v>
@@ -2273,10 +2422,10 @@
         <v>220</v>
       </c>
       <c r="G46" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H46" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I46" s="2">
         <v>45575</v>
@@ -2299,10 +2448,10 @@
         <v>220</v>
       </c>
       <c r="G47" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H47" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I47" s="2">
         <v>45575</v>
@@ -2325,10 +2474,10 @@
         <v>220</v>
       </c>
       <c r="G48" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H48" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I48" s="2">
         <v>45575</v>
@@ -2351,10 +2500,10 @@
         <v>220</v>
       </c>
       <c r="G49" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H49" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I49" s="2">
         <v>45575</v>
@@ -2377,10 +2526,10 @@
         <v>220</v>
       </c>
       <c r="G50" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H50" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I50" s="2">
         <v>45575</v>
@@ -2403,10 +2552,10 @@
         <v>220</v>
       </c>
       <c r="G51" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H51" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I51" s="2">
         <v>45575</v>
@@ -2429,10 +2578,10 @@
         <v>220</v>
       </c>
       <c r="G52" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H52" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I52" s="2">
         <v>45575</v>
@@ -2455,10 +2604,10 @@
         <v>220</v>
       </c>
       <c r="G53" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H53" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="I53" s="2">
         <v>45575</v>
@@ -2481,10 +2630,10 @@
         <v>220</v>
       </c>
       <c r="G54" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H54" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I54" s="2">
         <v>45575</v>
@@ -2507,10 +2656,10 @@
         <v>220</v>
       </c>
       <c r="G55" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H55" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I55" s="2">
         <v>45575</v>
@@ -2533,10 +2682,10 @@
         <v>220</v>
       </c>
       <c r="G56" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H56" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I56" s="2">
         <v>45575</v>
@@ -2559,10 +2708,10 @@
         <v>220</v>
       </c>
       <c r="G57" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H57" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I57" s="2">
         <v>45575</v>
@@ -2585,10 +2734,10 @@
         <v>220</v>
       </c>
       <c r="G58" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H58" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I58" s="2">
         <v>45575</v>
@@ -2611,10 +2760,10 @@
         <v>220</v>
       </c>
       <c r="G59" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H59" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I59" s="2">
         <v>45575</v>
@@ -2637,10 +2786,10 @@
         <v>220</v>
       </c>
       <c r="G60" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H60" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I60" s="2">
         <v>45575</v>
@@ -2663,10 +2812,10 @@
         <v>220</v>
       </c>
       <c r="G61" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H61" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I61" s="2">
         <v>45575</v>
@@ -2689,10 +2838,10 @@
         <v>220</v>
       </c>
       <c r="G62" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H62" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="I62" s="2">
         <v>45575</v>
@@ -2715,10 +2864,10 @@
         <v>220</v>
       </c>
       <c r="G63" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H63" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I63" s="2">
         <v>45575</v>
@@ -2741,10 +2890,10 @@
         <v>220</v>
       </c>
       <c r="G64" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H64" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I64" s="2">
         <v>45575</v>
@@ -2767,10 +2916,10 @@
         <v>220</v>
       </c>
       <c r="G65" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H65" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I65" s="2">
         <v>45575</v>
@@ -2793,10 +2942,10 @@
         <v>220</v>
       </c>
       <c r="G66" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H66" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I66" s="2">
         <v>45575</v>
@@ -2819,10 +2968,10 @@
         <v>220</v>
       </c>
       <c r="G67" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H67" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I67" s="2">
         <v>45575</v>
@@ -2844,11 +2993,14 @@
       <c r="D68" t="s">
         <v>220</v>
       </c>
+      <c r="E68" t="s">
+        <v>230</v>
+      </c>
       <c r="G68" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H68" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I68" s="2">
         <v>45575</v>
@@ -2870,11 +3022,14 @@
       <c r="D69" t="s">
         <v>220</v>
       </c>
+      <c r="E69" t="s">
+        <v>231</v>
+      </c>
       <c r="G69" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H69" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I69" s="2">
         <v>45575</v>
@@ -2896,11 +3051,14 @@
       <c r="D70" t="s">
         <v>220</v>
       </c>
+      <c r="E70" t="s">
+        <v>232</v>
+      </c>
       <c r="G70" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H70" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I70" s="2">
         <v>45575</v>
@@ -2922,11 +3080,14 @@
       <c r="D71" t="s">
         <v>220</v>
       </c>
+      <c r="E71" t="s">
+        <v>233</v>
+      </c>
       <c r="G71" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H71" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="I71" s="2">
         <v>45575</v>
@@ -2948,11 +3109,14 @@
       <c r="D72" t="s">
         <v>220</v>
       </c>
+      <c r="E72" t="s">
+        <v>234</v>
+      </c>
       <c r="G72" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H72" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I72" s="2">
         <v>45575</v>
@@ -2974,11 +3138,14 @@
       <c r="D73" t="s">
         <v>220</v>
       </c>
+      <c r="E73" t="s">
+        <v>235</v>
+      </c>
       <c r="G73" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H73" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I73" s="2">
         <v>45575</v>
@@ -3000,11 +3167,14 @@
       <c r="D74" t="s">
         <v>220</v>
       </c>
+      <c r="E74" t="s">
+        <v>236</v>
+      </c>
       <c r="G74" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H74" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I74" s="2">
         <v>45575</v>
@@ -3026,11 +3196,14 @@
       <c r="D75" t="s">
         <v>220</v>
       </c>
+      <c r="E75" t="s">
+        <v>237</v>
+      </c>
       <c r="G75" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H75" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I75" s="2">
         <v>45575</v>
@@ -3052,11 +3225,14 @@
       <c r="D76" t="s">
         <v>220</v>
       </c>
+      <c r="E76" t="s">
+        <v>238</v>
+      </c>
       <c r="G76" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H76" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I76" s="2">
         <v>45575</v>
@@ -3078,11 +3254,14 @@
       <c r="D77" t="s">
         <v>220</v>
       </c>
+      <c r="E77" t="s">
+        <v>239</v>
+      </c>
       <c r="G77" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H77" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I77" s="2">
         <v>45575</v>
@@ -3104,11 +3283,14 @@
       <c r="D78" t="s">
         <v>220</v>
       </c>
+      <c r="E78" t="s">
+        <v>240</v>
+      </c>
       <c r="G78" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H78" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I78" s="2">
         <v>45575</v>
@@ -3130,11 +3312,14 @@
       <c r="D79" t="s">
         <v>220</v>
       </c>
+      <c r="E79" t="s">
+        <v>241</v>
+      </c>
       <c r="G79" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H79" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="I79" s="2">
         <v>45575</v>
@@ -3156,11 +3341,14 @@
       <c r="D80" t="s">
         <v>220</v>
       </c>
+      <c r="E80" t="s">
+        <v>242</v>
+      </c>
       <c r="G80" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H80" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I80" s="2">
         <v>45575</v>
@@ -3182,11 +3370,14 @@
       <c r="D81" t="s">
         <v>220</v>
       </c>
+      <c r="E81" t="s">
+        <v>243</v>
+      </c>
       <c r="G81" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H81" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="I81" s="2">
         <v>45575</v>
@@ -3208,11 +3399,14 @@
       <c r="D82" t="s">
         <v>220</v>
       </c>
+      <c r="E82" t="s">
+        <v>244</v>
+      </c>
       <c r="G82" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H82" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I82" s="2">
         <v>45575</v>
@@ -3234,11 +3428,14 @@
       <c r="D83" t="s">
         <v>220</v>
       </c>
+      <c r="E83" t="s">
+        <v>245</v>
+      </c>
       <c r="G83" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H83" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I83" s="2">
         <v>45575</v>
@@ -3260,11 +3457,14 @@
       <c r="D84" t="s">
         <v>220</v>
       </c>
+      <c r="E84" t="s">
+        <v>246</v>
+      </c>
       <c r="G84" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H84" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I84" s="2">
         <v>45575</v>
@@ -3287,10 +3487,10 @@
         <v>220</v>
       </c>
       <c r="G85" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H85" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I85" s="2">
         <v>45575</v>
@@ -3313,10 +3513,10 @@
         <v>220</v>
       </c>
       <c r="G86" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H86" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I86" s="2">
         <v>45575</v>
@@ -3339,10 +3539,10 @@
         <v>220</v>
       </c>
       <c r="G87" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H87" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I87" s="2">
         <v>45575</v>
@@ -3365,10 +3565,10 @@
         <v>220</v>
       </c>
       <c r="G88" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H88" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I88" s="2">
         <v>45575</v>
@@ -3391,10 +3591,10 @@
         <v>220</v>
       </c>
       <c r="G89" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H89" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I89" s="2">
         <v>45575</v>
@@ -3417,10 +3617,10 @@
         <v>220</v>
       </c>
       <c r="G90" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H90" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="I90" s="2">
         <v>45575</v>
@@ -3443,10 +3643,10 @@
         <v>220</v>
       </c>
       <c r="G91" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H91" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I91" s="2">
         <v>45575</v>
@@ -3469,10 +3669,10 @@
         <v>220</v>
       </c>
       <c r="G92" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H92" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I92" s="2">
         <v>45575</v>
@@ -3495,10 +3695,10 @@
         <v>220</v>
       </c>
       <c r="G93" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H93" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I93" s="2">
         <v>45575</v>
@@ -3521,10 +3721,10 @@
         <v>220</v>
       </c>
       <c r="G94" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H94" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I94" s="2">
         <v>45575</v>
@@ -3547,10 +3747,10 @@
         <v>220</v>
       </c>
       <c r="G95" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H95" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I95" s="2">
         <v>45575</v>
@@ -3573,10 +3773,10 @@
         <v>220</v>
       </c>
       <c r="G96" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H96" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I96" s="2">
         <v>45575</v>
@@ -3599,10 +3799,10 @@
         <v>220</v>
       </c>
       <c r="G97" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H97" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I97" s="2">
         <v>45575</v>
@@ -3625,10 +3825,10 @@
         <v>220</v>
       </c>
       <c r="G98" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H98" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I98" s="2">
         <v>45575</v>
@@ -3651,10 +3851,10 @@
         <v>220</v>
       </c>
       <c r="G99" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H99" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I99" s="2">
         <v>45575</v>
@@ -3677,10 +3877,10 @@
         <v>220</v>
       </c>
       <c r="G100" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H100" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I100" s="2">
         <v>45575</v>
@@ -3703,10 +3903,10 @@
         <v>220</v>
       </c>
       <c r="G101" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H101" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I101" s="2">
         <v>45575</v>
@@ -3729,10 +3929,10 @@
         <v>220</v>
       </c>
       <c r="G102" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H102" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I102" s="2">
         <v>45575</v>
@@ -3755,10 +3955,10 @@
         <v>220</v>
       </c>
       <c r="G103" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="H103" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I103" s="2">
         <v>45575</v>
@@ -3781,10 +3981,10 @@
         <v>220</v>
       </c>
       <c r="G104" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H104" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I104" s="2">
         <v>45575</v>
@@ -3807,10 +4007,10 @@
         <v>220</v>
       </c>
       <c r="G105" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H105" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I105" s="2">
         <v>45575</v>
@@ -3833,10 +4033,10 @@
         <v>220</v>
       </c>
       <c r="G106" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H106" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I106" s="2">
         <v>45575</v>
@@ -3859,10 +4059,10 @@
         <v>220</v>
       </c>
       <c r="G107" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H107" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I107" s="2">
         <v>45575</v>
@@ -3885,10 +4085,10 @@
         <v>220</v>
       </c>
       <c r="G108" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H108" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I108" s="2">
         <v>45575</v>
@@ -3911,10 +4111,10 @@
         <v>220</v>
       </c>
       <c r="G109" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H109" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I109" s="2">
         <v>45575</v>
@@ -3937,10 +4137,10 @@
         <v>220</v>
       </c>
       <c r="G110" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H110" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I110" s="2">
         <v>45575</v>
@@ -3963,10 +4163,10 @@
         <v>220</v>
       </c>
       <c r="G111" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H111" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I111" s="2">
         <v>45575</v>
@@ -3989,10 +4189,10 @@
         <v>220</v>
       </c>
       <c r="G112" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H112" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I112" s="2">
         <v>45575</v>
@@ -4015,10 +4215,10 @@
         <v>220</v>
       </c>
       <c r="G113" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H113" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I113" s="2">
         <v>45575</v>
@@ -4041,10 +4241,10 @@
         <v>220</v>
       </c>
       <c r="G114" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H114" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I114" s="2">
         <v>45575</v>
@@ -4067,10 +4267,10 @@
         <v>220</v>
       </c>
       <c r="G115" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H115" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I115" s="2">
         <v>45575</v>
@@ -4093,10 +4293,10 @@
         <v>220</v>
       </c>
       <c r="G116" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H116" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I116" s="2">
         <v>45575</v>
@@ -4119,10 +4319,10 @@
         <v>220</v>
       </c>
       <c r="G117" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H117" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I117" s="2">
         <v>45575</v>
@@ -4145,10 +4345,10 @@
         <v>220</v>
       </c>
       <c r="G118" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H118" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I118" s="2">
         <v>45575</v>
@@ -4171,10 +4371,10 @@
         <v>220</v>
       </c>
       <c r="G119" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H119" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I119" s="2">
         <v>45575</v>
@@ -4197,10 +4397,10 @@
         <v>220</v>
       </c>
       <c r="G120" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H120" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I120" s="2">
         <v>45575</v>
@@ -4223,10 +4423,10 @@
         <v>220</v>
       </c>
       <c r="G121" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H121" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I121" s="2">
         <v>45575</v>
@@ -4249,10 +4449,10 @@
         <v>220</v>
       </c>
       <c r="G122" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H122" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="I122" s="2">
         <v>45575</v>
@@ -4275,10 +4475,10 @@
         <v>220</v>
       </c>
       <c r="G123" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H123" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I123" s="2">
         <v>45575</v>
@@ -4301,10 +4501,10 @@
         <v>220</v>
       </c>
       <c r="G124" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H124" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I124" s="2">
         <v>45575</v>
@@ -4327,10 +4527,10 @@
         <v>220</v>
       </c>
       <c r="G125" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H125" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I125" s="2">
         <v>45575</v>
@@ -4353,10 +4553,10 @@
         <v>220</v>
       </c>
       <c r="G126" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="H126" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I126" s="2">
         <v>45575</v>
@@ -4379,10 +4579,10 @@
         <v>220</v>
       </c>
       <c r="G127" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H127" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I127" s="2">
         <v>45575</v>
@@ -4405,10 +4605,10 @@
         <v>220</v>
       </c>
       <c r="G128" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H128" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I128" s="2">
         <v>45575</v>
@@ -4431,10 +4631,10 @@
         <v>220</v>
       </c>
       <c r="G129" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H129" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I129" s="2">
         <v>45575</v>
@@ -4457,10 +4657,10 @@
         <v>220</v>
       </c>
       <c r="G130" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H130" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I130" s="2">
         <v>45575</v>
@@ -4483,10 +4683,10 @@
         <v>220</v>
       </c>
       <c r="G131" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H131" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I131" s="2">
         <v>45575</v>
@@ -4509,10 +4709,10 @@
         <v>220</v>
       </c>
       <c r="G132" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H132" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I132" s="2">
         <v>45575</v>
@@ -4535,10 +4735,10 @@
         <v>220</v>
       </c>
       <c r="G133" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H133" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="I133" s="2">
         <v>45575</v>
@@ -4561,10 +4761,10 @@
         <v>220</v>
       </c>
       <c r="G134" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H134" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I134" s="2">
         <v>45575</v>
@@ -4587,10 +4787,10 @@
         <v>220</v>
       </c>
       <c r="G135" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H135" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I135" s="2">
         <v>45575</v>
@@ -4613,10 +4813,10 @@
         <v>220</v>
       </c>
       <c r="G136" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H136" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I136" s="2">
         <v>45575</v>
@@ -4639,10 +4839,10 @@
         <v>220</v>
       </c>
       <c r="G137" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H137" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I137" s="2">
         <v>45575</v>
@@ -4665,10 +4865,10 @@
         <v>220</v>
       </c>
       <c r="G138" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H138" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I138" s="2">
         <v>45575</v>
@@ -4691,10 +4891,10 @@
         <v>220</v>
       </c>
       <c r="G139" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H139" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I139" s="2">
         <v>45575</v>
@@ -4717,10 +4917,10 @@
         <v>220</v>
       </c>
       <c r="G140" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H140" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I140" s="2">
         <v>45575</v>
@@ -4743,10 +4943,10 @@
         <v>220</v>
       </c>
       <c r="G141" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H141" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I141" s="2">
         <v>45575</v>
@@ -4769,10 +4969,10 @@
         <v>220</v>
       </c>
       <c r="G142" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H142" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I142" s="2">
         <v>45575</v>
@@ -4795,10 +4995,10 @@
         <v>220</v>
       </c>
       <c r="G143" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H143" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I143" s="2">
         <v>45575</v>
@@ -4821,10 +5021,10 @@
         <v>220</v>
       </c>
       <c r="G144" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H144" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I144" s="2">
         <v>45575</v>
@@ -4847,10 +5047,10 @@
         <v>220</v>
       </c>
       <c r="G145" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H145" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="I145" s="2">
         <v>45575</v>
@@ -4873,10 +5073,10 @@
         <v>220</v>
       </c>
       <c r="G146" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H146" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I146" s="2">
         <v>45575</v>
@@ -4899,10 +5099,10 @@
         <v>220</v>
       </c>
       <c r="G147" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H147" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I147" s="2">
         <v>45575</v>
@@ -4925,10 +5125,10 @@
         <v>220</v>
       </c>
       <c r="G148" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H148" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I148" s="2">
         <v>45575</v>
@@ -4951,10 +5151,10 @@
         <v>220</v>
       </c>
       <c r="G149" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H149" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I149" s="2">
         <v>45575</v>
@@ -4976,11 +5176,14 @@
       <c r="D150" t="s">
         <v>220</v>
       </c>
+      <c r="E150" t="s">
+        <v>247</v>
+      </c>
       <c r="G150" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H150" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I150" s="2">
         <v>45575</v>
@@ -5002,11 +5205,14 @@
       <c r="D151" t="s">
         <v>220</v>
       </c>
+      <c r="E151" t="s">
+        <v>248</v>
+      </c>
       <c r="G151" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H151" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I151" s="2">
         <v>45575</v>
@@ -5028,11 +5234,14 @@
       <c r="D152" t="s">
         <v>220</v>
       </c>
+      <c r="E152" t="s">
+        <v>249</v>
+      </c>
       <c r="G152" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H152" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I152" s="2">
         <v>45575</v>
@@ -5054,11 +5263,14 @@
       <c r="D153" t="s">
         <v>220</v>
       </c>
+      <c r="E153" t="s">
+        <v>250</v>
+      </c>
       <c r="G153" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H153" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I153" s="2">
         <v>45575</v>
@@ -5080,11 +5292,14 @@
       <c r="D154" t="s">
         <v>220</v>
       </c>
+      <c r="E154" t="s">
+        <v>251</v>
+      </c>
       <c r="G154" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H154" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I154" s="2">
         <v>45575</v>
@@ -5106,11 +5321,14 @@
       <c r="D155" t="s">
         <v>220</v>
       </c>
+      <c r="E155" t="s">
+        <v>252</v>
+      </c>
       <c r="G155" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H155" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I155" s="2">
         <v>45575</v>
@@ -5132,11 +5350,14 @@
       <c r="D156" t="s">
         <v>220</v>
       </c>
+      <c r="E156" t="s">
+        <v>253</v>
+      </c>
       <c r="G156" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H156" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I156" s="2">
         <v>45575</v>
@@ -5158,11 +5379,14 @@
       <c r="D157" t="s">
         <v>220</v>
       </c>
+      <c r="E157" t="s">
+        <v>254</v>
+      </c>
       <c r="G157" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H157" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="I157" s="2">
         <v>45575</v>
@@ -5184,11 +5408,14 @@
       <c r="D158" t="s">
         <v>220</v>
       </c>
+      <c r="E158" t="s">
+        <v>255</v>
+      </c>
       <c r="G158" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H158" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I158" s="2">
         <v>45575</v>
@@ -5210,11 +5437,14 @@
       <c r="D159" t="s">
         <v>220</v>
       </c>
+      <c r="E159" t="s">
+        <v>256</v>
+      </c>
       <c r="G159" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H159" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I159" s="2">
         <v>45575</v>
@@ -5236,11 +5466,14 @@
       <c r="D160" t="s">
         <v>220</v>
       </c>
+      <c r="E160" t="s">
+        <v>257</v>
+      </c>
       <c r="G160" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="H160" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I160" s="2">
         <v>45575</v>
@@ -5262,11 +5495,14 @@
       <c r="D161" t="s">
         <v>220</v>
       </c>
+      <c r="E161" t="s">
+        <v>258</v>
+      </c>
       <c r="G161" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H161" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="I161" s="2">
         <v>45575</v>
@@ -5288,11 +5524,14 @@
       <c r="D162" t="s">
         <v>220</v>
       </c>
+      <c r="E162" t="s">
+        <v>259</v>
+      </c>
       <c r="G162" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H162" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I162" s="2">
         <v>45575</v>
@@ -5314,11 +5553,14 @@
       <c r="D163" t="s">
         <v>220</v>
       </c>
+      <c r="E163" t="s">
+        <v>260</v>
+      </c>
       <c r="G163" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H163" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I163" s="2">
         <v>45575</v>
@@ -5340,11 +5582,14 @@
       <c r="D164" t="s">
         <v>220</v>
       </c>
+      <c r="E164" t="s">
+        <v>261</v>
+      </c>
       <c r="G164" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="H164" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I164" s="2">
         <v>45575</v>
@@ -5367,10 +5612,10 @@
         <v>220</v>
       </c>
       <c r="G165" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H165" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I165" s="2">
         <v>45575</v>
@@ -5393,10 +5638,10 @@
         <v>220</v>
       </c>
       <c r="G166" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H166" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I166" s="2">
         <v>45575</v>
@@ -5419,10 +5664,10 @@
         <v>220</v>
       </c>
       <c r="G167" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H167" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I167" s="2">
         <v>45575</v>
@@ -5445,10 +5690,10 @@
         <v>220</v>
       </c>
       <c r="G168" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H168" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I168" s="2">
         <v>45575</v>
@@ -5471,10 +5716,10 @@
         <v>220</v>
       </c>
       <c r="G169" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H169" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="I169" s="2">
         <v>45575</v>
@@ -5497,10 +5742,10 @@
         <v>220</v>
       </c>
       <c r="G170" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H170" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I170" s="2">
         <v>45575</v>
@@ -5523,10 +5768,10 @@
         <v>220</v>
       </c>
       <c r="G171" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H171" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I171" s="2">
         <v>45575</v>
@@ -5549,10 +5794,10 @@
         <v>220</v>
       </c>
       <c r="G172" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H172" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="I172" s="2">
         <v>45575</v>
@@ -5575,10 +5820,10 @@
         <v>220</v>
       </c>
       <c r="G173" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H173" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I173" s="2">
         <v>45575</v>
@@ -5601,10 +5846,10 @@
         <v>220</v>
       </c>
       <c r="G174" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H174" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I174" s="2">
         <v>45575</v>
@@ -5627,10 +5872,10 @@
         <v>220</v>
       </c>
       <c r="G175" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="H175" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="I175" s="2">
         <v>45575</v>
@@ -5653,10 +5898,10 @@
         <v>220</v>
       </c>
       <c r="G176" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H176" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I176" s="2">
         <v>45575</v>
@@ -5679,10 +5924,10 @@
         <v>220</v>
       </c>
       <c r="G177" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H177" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I177" s="2">
         <v>45575</v>
@@ -5705,10 +5950,10 @@
         <v>220</v>
       </c>
       <c r="G178" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H178" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I178" s="2">
         <v>45575</v>
@@ -5731,10 +5976,10 @@
         <v>220</v>
       </c>
       <c r="G179" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H179" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I179" s="2">
         <v>45575</v>
@@ -5757,10 +6002,10 @@
         <v>220</v>
       </c>
       <c r="G180" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H180" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I180" s="2">
         <v>45575</v>
@@ -5783,10 +6028,10 @@
         <v>220</v>
       </c>
       <c r="G181" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H181" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I181" s="2">
         <v>45575</v>
@@ -5809,10 +6054,10 @@
         <v>220</v>
       </c>
       <c r="G182" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H182" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I182" s="2">
         <v>45575</v>
@@ -5835,10 +6080,10 @@
         <v>220</v>
       </c>
       <c r="G183" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="H183" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I183" s="2">
         <v>45575</v>

</xml_diff>